<commit_message>
Updated latest code for create property class file
</commit_message>
<xml_diff>
--- a/src/main/resources/InputTestdata/Listing details.xlsx
+++ b/src/main/resources/InputTestdata/Listing details.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\I500647\eclipse-workspace\Manoj\Web_Automation_WordPress\src\main\resources\InputTestdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr documentId="13_ncr:1_{C694C11D-452B-4719-BC0C-B79C05301BA8}" revIDLastSave="0" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="46"/>
+  <xr:revisionPtr documentId="13_ncr:1_{BBA761E0-93CC-4972-8F5A-F1F544EEA47B}" revIDLastSave="0" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="46"/>
   <bookViews>
-    <workbookView activeTab="1" windowHeight="12576" windowWidth="23256" xWindow="-108" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}" yWindow="-108"/>
+    <workbookView windowHeight="12576" windowWidth="23256" xWindow="-108" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}" yWindow="-108"/>
   </bookViews>
   <sheets>
     <sheet name="Backlog" r:id="rId1" sheetId="1"/>
@@ -19,21 +19,21 @@
     <sheet name="Agency login" r:id="rId4" sheetId="4"/>
   </sheets>
   <definedNames>
-    <definedName hidden="1" localSheetId="0" name="_xlnm._FilterDatabase">Backlog!$A$1:$AB$1</definedName>
+    <definedName hidden="1" localSheetId="0" name="_xlnm._FilterDatabase">Backlog!$A$1:$AB$52</definedName>
     <definedName hidden="1" localSheetId="1" name="_xlnm._FilterDatabase">Listing!$E$1:$E$32</definedName>
     <definedName hidden="1" localSheetId="1" name="Z_A7754112_A52F_4ABC_8778_92F04773E53C_.wvu.FilterData">Listing!$A$1:$AE$32</definedName>
     <definedName hidden="1" localSheetId="1" name="Z_C25CEB9E_BEC1_4982_90C4_50C84EE1B82A_.wvu.FilterData">Listing!$A$1:$AE$32</definedName>
   </definedNames>
   <calcPr calcId="0"/>
   <customWorkbookViews>
+    <customWorkbookView activeSheetId="0" guid="{C25CEB9E-BEC1-4982-90C4-50C84EE1B82A}" maximized="1" name="Filter 2" windowHeight="0" windowWidth="0"/>
     <customWorkbookView activeSheetId="0" guid="{A7754112-A52F-4ABC-8778-92F04773E53C}" maximized="1" name="Filter 1" windowHeight="0" windowWidth="0"/>
-    <customWorkbookView activeSheetId="0" guid="{C25CEB9E-BEC1-4982-90C4-50C84EE1B82A}" maximized="1" name="Filter 2" windowHeight="0" windowWidth="0"/>
   </customWorkbookViews>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1148" uniqueCount="372">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1168" uniqueCount="371">
   <si>
     <t>ID</t>
   </si>
@@ -701,6 +701,9 @@
     <t>OFF THE MARKET</t>
   </si>
   <si>
+    <t>NEW</t>
+  </si>
+  <si>
     <t>https://www.allhomes.com.au/14-mottram-street-taylor-act-2913</t>
   </si>
   <si>
@@ -761,16 +764,13 @@
     <t>https://www.allhomes.com.au/taylor-act-2913?tid=179295362</t>
   </si>
   <si>
-    <t>NEW</t>
-  </si>
-  <si>
     <t>32</t>
   </si>
   <si>
     <t>14 Mottram Street, Taylor ACT 2913</t>
   </si>
   <si>
-    <t>Block/House:450/ 248</t>
+    <t>Block/House: 450/ 248</t>
   </si>
   <si>
     <t>m² approx</t>
@@ -829,7 +829,7 @@
     <t>Belconnen</t>
   </si>
   <si>
-    <t>Block/House:667/ 225</t>
+    <t>Block/House: 667/ 225</t>
   </si>
   <si>
     <t xml:space="preserve">4	4	9	0	0	0	</t>
@@ -853,7 +853,7 @@
     <t>34</t>
   </si>
   <si>
-    <t>Block/House:337/ 200</t>
+    <t>Block/House: 337/ 200</t>
   </si>
   <si>
     <t xml:space="preserve">4	1	5	0	0	0	</t>
@@ -883,7 +883,7 @@
     <t>Franklin</t>
   </si>
   <si>
-    <t>Block/House:1.04/ 110</t>
+    <t>Block/House: 1.04/ 110</t>
   </si>
   <si>
     <t xml:space="preserve">4	2	9	0	0	0	</t>
@@ -919,7 +919,7 @@
     <t>27 Irinyili Street, Bonner ACT 2914</t>
   </si>
   <si>
-    <t>Block/House:242/ 128</t>
+    <t>Block/House: 242/ 128</t>
   </si>
   <si>
     <t xml:space="preserve">5	7	9	0	0	0	</t>
@@ -943,7 +943,7 @@
     <t>(no street name provided), Whitlam ACT 2611</t>
   </si>
   <si>
-    <t>Other</t>
+    <t>Others</t>
   </si>
   <si>
     <t>Molonglo Valley</t>
@@ -969,9 +969,6 @@
   </si>
   <si>
     <t>95/235 Flemington Road, Franklin ACT 2913</t>
-  </si>
-  <si>
-    <t>Unit / Apartment</t>
   </si>
   <si>
     <t>Enjoy being located in a prime and central location, this spacious Franklin loft house offers a central lifestyle being located just minutes from the tram line, local schools, shops and The Gungahlin Town Centre!
@@ -1002,7 +999,7 @@
     <t>39</t>
   </si>
   <si>
-    <t>Block/House:175/ -</t>
+    <t>Block/House: 175/ -</t>
   </si>
   <si>
     <t>Constrction Price  $289,000
@@ -1018,7 +1015,7 @@
     <t>Coombs</t>
   </si>
   <si>
-    <t>Block/House:612/ -</t>
+    <t>Block/House: 612/ -</t>
   </si>
   <si>
     <t xml:space="preserve">1	1	7	9	0	0	0	</t>
@@ -1039,7 +1036,7 @@
     <t>41</t>
   </si>
   <si>
-    <t>Block/House:420/ 220</t>
+    <t>Block/House: 420/ 220</t>
   </si>
   <si>
     <t xml:space="preserve"> Throsby ACT 2914</t>
@@ -1083,10 +1080,13 @@
     <t>Lawrenson Circuit, Jacka ACT 2914</t>
   </si>
   <si>
+    <t>Town house</t>
+  </si>
+  <si>
     <t>Jacka</t>
   </si>
   <si>
-    <t>Block/House:94/ -</t>
+    <t>Block/House: 94/ -</t>
   </si>
   <si>
     <t xml:space="preserve">5	4	9	0	0	0	</t>
@@ -1114,7 +1114,7 @@
     <t>North Canberra</t>
   </si>
   <si>
-    <t>Block/House:83/ -</t>
+    <t>Block/House: 83/ -</t>
   </si>
   <si>
     <t xml:space="preserve">4	8	3	0	0	0	</t>
@@ -1153,7 +1153,7 @@
     <t>12 Ledgar Rise, Taylor ACT 2913</t>
   </si>
   <si>
-    <t>Block/House:540/ 288</t>
+    <t>Block/House: 540/ 288</t>
   </si>
   <si>
     <t xml:space="preserve">9	6	9	0	0	0	</t>
@@ -1200,7 +1200,7 @@
     <t>19/16 David Miller Crescent, Casey ACT 2913</t>
   </si>
   <si>
-    <t>Block/House:5282/ 92</t>
+    <t>Block/House: 5282/ 92</t>
   </si>
   <si>
     <t xml:space="preserve">3	8	5	0	0	0	</t>
@@ -1237,7 +1237,7 @@
     <t>19 Charles Perkins Circuit, Bonner ACT 2914</t>
   </si>
   <si>
-    <t>Block/House:426/ 238</t>
+    <t>Block/House: 426/ 238</t>
   </si>
   <si>
     <t xml:space="preserve">8	3	0	0	0	0	</t>
@@ -1279,7 +1279,7 @@
     <t>47</t>
   </si>
   <si>
-    <t>Block/House:240/ -</t>
+    <t>Block/House: 240/ -</t>
   </si>
   <si>
     <t xml:space="preserve">5	9	9	0	0	0	</t>
@@ -1301,7 +1301,7 @@
     <t>5 Kaylock Street, Strathnairn ACT 2615</t>
   </si>
   <si>
-    <t>Block/House:612/ 250</t>
+    <t>Block/House: 612/ 250</t>
   </si>
   <si>
     <t xml:space="preserve">9	2	5	0	0	0	</t>
@@ -1335,7 +1335,7 @@
     <t>MacGregor</t>
   </si>
   <si>
-    <t>Block/House:470/ -</t>
+    <t>Block/House: 470/ -</t>
   </si>
   <si>
     <t xml:space="preserve">6	9	9	0	0	0	</t>
@@ -1355,10 +1355,7 @@
     <t>48 Asimus Avenue, Strathnairn ACT 2615</t>
   </si>
   <si>
-    <t>Land</t>
-  </si>
-  <si>
-    <t>Block/House:649/ -</t>
+    <t>Block/House: 649/ -</t>
   </si>
   <si>
     <t xml:space="preserve">9	5	0	0	0	0	</t>
@@ -1374,7 +1371,7 @@
     <t>51</t>
   </si>
   <si>
-    <t>Block/House:570/ 260</t>
+    <t>Block/House: 570/ 260</t>
   </si>
   <si>
     <t xml:space="preserve">9	9	9	0	0	0	</t>
@@ -1581,7 +1578,7 @@
       <name val="Arial"/>
     </font>
   </fonts>
-  <fills count="12">
+  <fills count="14">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1643,6 +1640,16 @@
         <bgColor indexed="2"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor indexed="2"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="mediumGray">
+        <bgColor indexed="2"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -1656,7 +1663,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
   </cellStyleXfs>
-  <cellXfs count="63">
+  <cellXfs count="64">
     <xf applyAlignment="1" applyFont="1" borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
     <xf applyAlignment="1" applyFill="1" applyFont="1" borderId="0" fillId="3" fontId="1" numFmtId="0" xfId="0">
       <alignment horizontal="center"/>
@@ -1792,6 +1799,7 @@
     <xf applyFill="1" borderId="0" fillId="9" fontId="0" numFmtId="0" xfId="0"/>
     <xf applyFill="1" borderId="0" fillId="10" fontId="0" numFmtId="0" xfId="0"/>
     <xf applyFill="1" borderId="0" fillId="11" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyFill="true" borderId="0" fillId="13" fontId="0" numFmtId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle builtinId="0" name="Normal" xfId="0"/>
@@ -2029,9 +2037,9 @@
   </sheetPr>
   <dimension ref="A1:AC52"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane activePane="bottomLeft" state="frozen" topLeftCell="A29" ySplit="1"/>
-      <selection activeCell="B56" pane="bottomLeft" sqref="B56"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane activePane="bottomLeft" state="frozen" topLeftCell="A32" ySplit="1"/>
+      <selection activeCell="B57" pane="bottomLeft" sqref="B57"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr customHeight="1" defaultColWidth="14.44140625" defaultRowHeight="15.75"/>
@@ -3460,10 +3468,10 @@
         <v>32</v>
       </c>
       <c r="B33" t="s">
-        <v>222</v>
-      </c>
-      <c r="D33" s="59" t="s">
-        <v>371</v>
+        <v>223</v>
+      </c>
+      <c r="D33" s="60" t="s">
+        <v>370</v>
       </c>
       <c r="F33" s="29" t="s">
         <v>85</v>
@@ -3480,10 +3488,10 @@
         <v>33</v>
       </c>
       <c r="B34" t="s">
-        <v>223</v>
-      </c>
-      <c r="D34" s="59" t="s">
-        <v>371</v>
+        <v>224</v>
+      </c>
+      <c r="D34" s="60" t="s">
+        <v>370</v>
       </c>
       <c r="F34" s="29" t="s">
         <v>85</v>
@@ -3500,10 +3508,10 @@
         <v>34</v>
       </c>
       <c r="B35" t="s">
-        <v>224</v>
-      </c>
-      <c r="D35" s="59" t="s">
-        <v>371</v>
+        <v>225</v>
+      </c>
+      <c r="D35" s="60" t="s">
+        <v>370</v>
       </c>
       <c r="F35" s="29" t="s">
         <v>85</v>
@@ -3520,10 +3528,10 @@
         <v>35</v>
       </c>
       <c r="B36" t="s">
-        <v>225</v>
-      </c>
-      <c r="D36" s="59" t="s">
-        <v>371</v>
+        <v>226</v>
+      </c>
+      <c r="D36" s="60" t="s">
+        <v>370</v>
       </c>
       <c r="F36" s="29" t="s">
         <v>85</v>
@@ -3540,10 +3548,10 @@
         <v>36</v>
       </c>
       <c r="B37" t="s">
-        <v>226</v>
-      </c>
-      <c r="D37" s="59" t="s">
-        <v>371</v>
+        <v>227</v>
+      </c>
+      <c r="D37" s="60" t="s">
+        <v>370</v>
       </c>
       <c r="F37" s="29" t="s">
         <v>85</v>
@@ -3560,9 +3568,9 @@
         <v>37</v>
       </c>
       <c r="B38" t="s">
-        <v>227</v>
-      </c>
-      <c r="D38" s="59" t="s">
+        <v>228</v>
+      </c>
+      <c r="D38" s="60" t="s">
         <v>15</v>
       </c>
       <c r="F38" s="29" t="s">
@@ -3580,10 +3588,10 @@
         <v>38</v>
       </c>
       <c r="B39" t="s">
-        <v>228</v>
-      </c>
-      <c r="D39" s="59" t="s">
-        <v>15</v>
+        <v>229</v>
+      </c>
+      <c r="D39" s="60" t="s">
+        <v>370</v>
       </c>
       <c r="F39" s="29" t="s">
         <v>85</v>
@@ -3600,10 +3608,10 @@
         <v>39</v>
       </c>
       <c r="B40" t="s">
-        <v>229</v>
-      </c>
-      <c r="D40" s="59" t="s">
-        <v>15</v>
+        <v>230</v>
+      </c>
+      <c r="D40" s="60" t="s">
+        <v>370</v>
       </c>
       <c r="F40" s="29" t="s">
         <v>85</v>
@@ -3620,9 +3628,9 @@
         <v>40</v>
       </c>
       <c r="B41" t="s">
-        <v>230</v>
-      </c>
-      <c r="D41" s="59" t="s">
+        <v>231</v>
+      </c>
+      <c r="D41" s="60" t="s">
         <v>15</v>
       </c>
       <c r="F41" s="29" t="s">
@@ -3640,10 +3648,10 @@
         <v>41</v>
       </c>
       <c r="B42" t="s">
-        <v>231</v>
-      </c>
-      <c r="D42" s="59" t="s">
-        <v>15</v>
+        <v>232</v>
+      </c>
+      <c r="D42" s="60" t="s">
+        <v>370</v>
       </c>
       <c r="F42" s="29" t="s">
         <v>85</v>
@@ -3660,10 +3668,10 @@
         <v>42</v>
       </c>
       <c r="B43" t="s">
-        <v>232</v>
-      </c>
-      <c r="D43" s="59" t="s">
-        <v>15</v>
+        <v>233</v>
+      </c>
+      <c r="D43" s="60" t="s">
+        <v>370</v>
       </c>
       <c r="F43" s="29" t="s">
         <v>85</v>
@@ -3680,9 +3688,9 @@
         <v>43</v>
       </c>
       <c r="B44" t="s">
-        <v>233</v>
-      </c>
-      <c r="D44" s="59" t="s">
+        <v>234</v>
+      </c>
+      <c r="D44" s="60" t="s">
         <v>15</v>
       </c>
       <c r="F44" s="29" t="s">
@@ -3700,10 +3708,10 @@
         <v>44</v>
       </c>
       <c r="B45" t="s">
-        <v>234</v>
-      </c>
-      <c r="D45" s="60" t="s">
-        <v>15</v>
+        <v>235</v>
+      </c>
+      <c r="D45" s="61" t="s">
+        <v>370</v>
       </c>
       <c r="F45" s="29" t="s">
         <v>85</v>
@@ -3720,10 +3728,10 @@
         <v>45</v>
       </c>
       <c r="B46" t="s">
-        <v>235</v>
-      </c>
-      <c r="D46" s="60" t="s">
-        <v>15</v>
+        <v>236</v>
+      </c>
+      <c r="D46" s="61" t="s">
+        <v>370</v>
       </c>
       <c r="F46" s="29" t="s">
         <v>85</v>
@@ -3740,9 +3748,9 @@
         <v>46</v>
       </c>
       <c r="B47" t="s">
-        <v>236</v>
-      </c>
-      <c r="D47" s="60" t="s">
+        <v>237</v>
+      </c>
+      <c r="D47" s="61" t="s">
         <v>15</v>
       </c>
       <c r="F47" s="29" t="s">
@@ -3760,10 +3768,10 @@
         <v>47</v>
       </c>
       <c r="B48" t="s">
-        <v>237</v>
-      </c>
-      <c r="D48" s="61" t="s">
-        <v>15</v>
+        <v>238</v>
+      </c>
+      <c r="D48" s="62" t="s">
+        <v>370</v>
       </c>
       <c r="F48" s="29" t="s">
         <v>110</v>
@@ -3780,10 +3788,10 @@
         <v>48</v>
       </c>
       <c r="B49" t="s">
-        <v>238</v>
-      </c>
-      <c r="D49" s="61" t="s">
-        <v>15</v>
+        <v>239</v>
+      </c>
+      <c r="D49" s="62" t="s">
+        <v>370</v>
       </c>
       <c r="F49" s="29" t="s">
         <v>110</v>
@@ -3800,9 +3808,9 @@
         <v>49</v>
       </c>
       <c r="B50" t="s">
-        <v>239</v>
-      </c>
-      <c r="D50" s="61" t="s">
+        <v>240</v>
+      </c>
+      <c r="D50" s="62" t="s">
         <v>15</v>
       </c>
       <c r="F50" s="29" t="s">
@@ -3820,10 +3828,10 @@
         <v>50</v>
       </c>
       <c r="B51" t="s">
-        <v>240</v>
-      </c>
-      <c r="D51" s="61" t="s">
-        <v>15</v>
+        <v>241</v>
+      </c>
+      <c r="D51" s="62" t="s">
+        <v>370</v>
       </c>
       <c r="F51" s="29" t="s">
         <v>110</v>
@@ -3840,10 +3848,10 @@
         <v>51</v>
       </c>
       <c r="B52" t="s">
-        <v>241</v>
-      </c>
-      <c r="D52" s="61" t="s">
-        <v>15</v>
+        <v>242</v>
+      </c>
+      <c r="D52" s="62" t="s">
+        <v>370</v>
       </c>
       <c r="F52" s="29" t="s">
         <v>110</v>
@@ -3932,8 +3940,8 @@
   </sheetPr>
   <dimension ref="A1:AK52"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
-      <selection activeCell="B53" sqref="B53"/>
+    <sheetView topLeftCell="A25" workbookViewId="0">
+      <selection activeCell="C37" sqref="C37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr customHeight="1" defaultColWidth="14.44140625" defaultRowHeight="15.75"/>
@@ -6195,7 +6203,7 @@
       <c r="A31" s="29">
         <v>30</v>
       </c>
-      <c r="B31" s="62" t="s">
+      <c r="B31" s="59" t="s">
         <v>218</v>
       </c>
       <c r="C31" s="29" t="s">
@@ -6204,8 +6212,8 @@
       <c r="D31" s="29" t="s">
         <v>80</v>
       </c>
-      <c r="E31" s="62" t="s">
-        <v>242</v>
+      <c r="E31" s="59" t="s">
+        <v>222</v>
       </c>
       <c r="F31" s="31" t="s">
         <v>121</v>
@@ -6339,12 +6347,12 @@
       <c r="AI32" s="29"/>
       <c r="AJ32" s="29"/>
     </row>
-    <row ht="13.2" r="33" spans="1:21">
+    <row r="33">
       <c r="A33" t="s">
         <v>243</v>
       </c>
       <c r="B33" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
       <c r="C33" t="s">
         <v>244</v>
@@ -6398,12 +6406,12 @@
         <v>11</v>
       </c>
     </row>
-    <row ht="13.2" r="34" spans="1:21">
+    <row r="34">
       <c r="A34" t="s">
         <v>254</v>
       </c>
       <c r="B34" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
       <c r="C34" t="s">
         <v>103</v>
@@ -6457,12 +6465,12 @@
         <v>11</v>
       </c>
     </row>
-    <row ht="13.2" r="35" spans="1:21">
+    <row r="35">
       <c r="A35" t="s">
         <v>261</v>
       </c>
       <c r="B35" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
       <c r="C35" t="s">
         <v>93</v>
@@ -6516,12 +6524,12 @@
         <v>11</v>
       </c>
     </row>
-    <row ht="13.2" r="36" spans="1:21">
+    <row r="36">
       <c r="A36" t="s">
         <v>267</v>
       </c>
       <c r="B36" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
       <c r="C36" t="s">
         <v>268</v>
@@ -6575,12 +6583,12 @@
         <v>11</v>
       </c>
     </row>
-    <row ht="13.2" r="37" spans="1:21">
+    <row r="37">
       <c r="A37" t="s">
         <v>274</v>
       </c>
       <c r="B37" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
       <c r="C37" t="s">
         <v>275</v>
@@ -6634,7 +6642,7 @@
         <v>11</v>
       </c>
     </row>
-    <row ht="13.2" r="38" spans="1:21">
+    <row r="38">
       <c r="A38" t="s">
         <v>280</v>
       </c>
@@ -6693,18 +6701,18 @@
         <v>11</v>
       </c>
     </row>
-    <row ht="13.2" r="39" spans="1:21">
+    <row r="39">
       <c r="A39" t="s">
         <v>288</v>
       </c>
       <c r="B39" t="s">
-        <v>15</v>
+        <v>370</v>
       </c>
       <c r="C39" t="s">
         <v>289</v>
       </c>
       <c r="D39" t="s">
-        <v>290</v>
+        <v>80</v>
       </c>
       <c r="E39" t="s">
         <v>81</v>
@@ -6743,7 +6751,7 @@
         <v>289</v>
       </c>
       <c r="S39" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="T39" t="s">
         <v>85</v>
@@ -6752,18 +6760,18 @@
         <v>11</v>
       </c>
     </row>
-    <row ht="13.2" r="40" spans="1:21">
+    <row r="40">
       <c r="A40" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="B40" t="s">
-        <v>15</v>
+        <v>370</v>
       </c>
       <c r="C40" t="s">
         <v>93</v>
       </c>
       <c r="D40" t="s">
-        <v>220</v>
+        <v>88</v>
       </c>
       <c r="E40" t="s">
         <v>219</v>
@@ -6775,7 +6783,7 @@
         <v>89</v>
       </c>
       <c r="H40" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="I40" t="s">
         <v>246</v>
@@ -6802,7 +6810,7 @@
         <v>265</v>
       </c>
       <c r="S40" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="T40" t="s">
         <v>85</v>
@@ -6811,18 +6819,18 @@
         <v>11</v>
       </c>
     </row>
-    <row ht="13.2" r="41" spans="1:21">
+    <row r="41">
       <c r="A41" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="B41" t="s">
         <v>15</v>
       </c>
       <c r="C41" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="D41" t="s">
-        <v>220</v>
+        <v>88</v>
       </c>
       <c r="E41" t="s">
         <v>219</v>
@@ -6831,37 +6839,37 @@
         <v>283</v>
       </c>
       <c r="G41" t="s">
+        <v>296</v>
+      </c>
+      <c r="H41" t="s">
         <v>297</v>
-      </c>
-      <c r="H41" t="s">
-        <v>298</v>
       </c>
       <c r="I41" t="s">
         <v>246</v>
       </c>
       <c r="K41" t="s">
+        <v>298</v>
+      </c>
+      <c r="L41" t="s">
         <v>299</v>
       </c>
-      <c r="L41" t="s">
+      <c r="M41" t="s">
         <v>300</v>
-      </c>
-      <c r="M41" t="s">
-        <v>301</v>
       </c>
       <c r="N41" t="s">
         <v>250</v>
       </c>
       <c r="P41" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="Q41" t="s">
         <v>252</v>
       </c>
       <c r="R41" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="S41" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="T41" t="s">
         <v>85</v>
@@ -6870,12 +6878,12 @@
         <v>11</v>
       </c>
     </row>
-    <row ht="13.2" r="42" spans="1:21">
+    <row r="42">
       <c r="A42" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="B42" t="s">
-        <v>15</v>
+        <v>370</v>
       </c>
       <c r="C42" t="s">
         <v>139</v>
@@ -6893,7 +6901,7 @@
         <v>141</v>
       </c>
       <c r="H42" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="I42" t="s">
         <v>246</v>
@@ -6917,10 +6925,10 @@
         <v>252</v>
       </c>
       <c r="R42" t="s">
+        <v>305</v>
+      </c>
+      <c r="S42" t="s">
         <v>306</v>
-      </c>
-      <c r="S42" t="s">
-        <v>307</v>
       </c>
       <c r="T42" t="s">
         <v>85</v>
@@ -6929,18 +6937,18 @@
         <v>11</v>
       </c>
     </row>
-    <row ht="13.2" r="43" spans="1:21">
+    <row r="43">
       <c r="A43" t="s">
+        <v>307</v>
+      </c>
+      <c r="B43" t="s">
+        <v>370</v>
+      </c>
+      <c r="C43" t="s">
         <v>308</v>
       </c>
-      <c r="B43" t="s">
-        <v>15</v>
-      </c>
-      <c r="C43" t="s">
+      <c r="D43" t="s">
         <v>309</v>
-      </c>
-      <c r="D43" t="s">
-        <v>98</v>
       </c>
       <c r="E43" t="s">
         <v>81</v>
@@ -6976,7 +6984,7 @@
         <v>314</v>
       </c>
       <c r="R43" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="S43" t="s">
         <v>315</v>
@@ -6988,7 +6996,7 @@
         <v>11</v>
       </c>
     </row>
-    <row ht="13.2" r="44" spans="1:21">
+    <row r="44">
       <c r="A44" t="s">
         <v>316</v>
       </c>
@@ -7047,12 +7055,12 @@
         <v>11</v>
       </c>
     </row>
-    <row ht="13.2" r="45" spans="1:21">
+    <row r="45">
       <c r="A45" t="s">
         <v>323</v>
       </c>
       <c r="B45" t="s">
-        <v>15</v>
+        <v>370</v>
       </c>
       <c r="C45" t="s">
         <v>324</v>
@@ -7106,12 +7114,12 @@
         <v>40</v>
       </c>
     </row>
-    <row ht="13.2" r="46" spans="1:21">
+    <row r="46">
       <c r="A46" t="s">
         <v>329</v>
       </c>
       <c r="B46" t="s">
-        <v>15</v>
+        <v>370</v>
       </c>
       <c r="C46" t="s">
         <v>330</v>
@@ -7165,7 +7173,7 @@
         <v>40</v>
       </c>
     </row>
-    <row ht="13.2" r="47" spans="1:21">
+    <row r="47">
       <c r="A47" t="s">
         <v>335</v>
       </c>
@@ -7224,18 +7232,18 @@
         <v>40</v>
       </c>
     </row>
-    <row ht="13.2" r="48" spans="1:21">
+    <row r="48">
       <c r="A48" t="s">
         <v>341</v>
       </c>
       <c r="B48" t="s">
-        <v>15</v>
+        <v>370</v>
       </c>
       <c r="C48" t="s">
         <v>93</v>
       </c>
       <c r="D48" t="s">
-        <v>220</v>
+        <v>88</v>
       </c>
       <c r="E48" t="s">
         <v>81</v>
@@ -7283,12 +7291,12 @@
         <v>19</v>
       </c>
     </row>
-    <row ht="13.2" r="49" spans="1:21">
+    <row r="49">
       <c r="A49" t="s">
         <v>346</v>
       </c>
       <c r="B49" t="s">
-        <v>15</v>
+        <v>370</v>
       </c>
       <c r="C49" t="s">
         <v>347</v>
@@ -7318,7 +7326,7 @@
         <v>350</v>
       </c>
       <c r="M49" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="N49" t="s">
         <v>252</v>
@@ -7342,7 +7350,7 @@
         <v>19</v>
       </c>
     </row>
-    <row ht="13.2" r="50" spans="1:21">
+    <row r="50">
       <c r="A50" t="s">
         <v>352</v>
       </c>
@@ -7401,18 +7409,18 @@
         <v>19</v>
       </c>
     </row>
-    <row ht="13.2" r="51" spans="1:21">
+    <row r="51">
       <c r="A51" t="s">
         <v>359</v>
       </c>
       <c r="B51" t="s">
-        <v>15</v>
+        <v>370</v>
       </c>
       <c r="C51" t="s">
         <v>360</v>
       </c>
       <c r="D51" t="s">
-        <v>361</v>
+        <v>282</v>
       </c>
       <c r="E51" t="s">
         <v>81</v>
@@ -7424,16 +7432,16 @@
         <v>106</v>
       </c>
       <c r="H51" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
       <c r="I51" t="s">
         <v>246</v>
       </c>
       <c r="K51" t="s">
+        <v>362</v>
+      </c>
+      <c r="L51" t="s">
         <v>363</v>
-      </c>
-      <c r="L51" t="s">
-        <v>364</v>
       </c>
       <c r="M51" t="s">
         <v>247</v>
@@ -7451,7 +7459,7 @@
         <v>360</v>
       </c>
       <c r="S51" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
       <c r="T51" t="s">
         <v>110</v>
@@ -7460,12 +7468,12 @@
         <v>19</v>
       </c>
     </row>
-    <row ht="13.2" r="52" spans="1:21">
+    <row r="52">
       <c r="A52" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
       <c r="B52" t="s">
-        <v>15</v>
+        <v>370</v>
       </c>
       <c r="C52" t="s">
         <v>93</v>
@@ -7483,16 +7491,16 @@
         <v>89</v>
       </c>
       <c r="H52" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
       <c r="I52" t="s">
         <v>246</v>
       </c>
       <c r="K52" t="s">
+        <v>367</v>
+      </c>
+      <c r="L52" t="s">
         <v>368</v>
-      </c>
-      <c r="L52" t="s">
-        <v>369</v>
       </c>
       <c r="M52" t="s">
         <v>249</v>
@@ -7510,7 +7518,7 @@
         <v>265</v>
       </c>
       <c r="S52" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
       <c r="T52" t="s">
         <v>110</v>
@@ -7522,6 +7530,10 @@
   </sheetData>
   <autoFilter ref="E1:E32" xr:uid="{00000000-0009-0000-0000-000001000000}"/>
   <customSheetViews>
+    <customSheetView filter="1" guid="{C25CEB9E-BEC1-4982-90C4-50C84EE1B82A}" showAutoFilter="1">
+      <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+      <autoFilter ref="A1:AD33" xr:uid="{00000000-0000-0000-0000-000000000000}"/>
+    </customSheetView>
     <customSheetView filter="1" guid="{A7754112-A52F-4ABC-8778-92F04773E53C}" showAutoFilter="1">
       <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
       <autoFilter ref="A1:AD33" xr:uid="{00000000-0000-0000-0000-000000000000}">
@@ -7531,10 +7543,6 @@
           </filters>
         </filterColumn>
       </autoFilter>
-    </customSheetView>
-    <customSheetView filter="1" guid="{C25CEB9E-BEC1-4982-90C4-50C84EE1B82A}" showAutoFilter="1">
-      <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
-      <autoFilter ref="A1:AD33" xr:uid="{00000000-0000-0000-0000-000000000000}"/>
     </customSheetView>
   </customSheetViews>
   <conditionalFormatting sqref="A1:AJ1">

</xml_diff>

<commit_message>
Updated code for excluding Rented Property, add property URL in List sheet and fixed the price Issue while creating a new property
</commit_message>
<xml_diff>
--- a/src/main/resources/InputTestdata/Listing details.xlsx
+++ b/src/main/resources/InputTestdata/Listing details.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Athavan\git\777Homes-business\src\main\resources\InputTestdata\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\manoj\git\777Homes-business\src\main\resources\InputTestdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4A89832B-1EA9-4B8D-8062-3A8BAA211E1F}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FE70CD77-5E20-4D2D-8166-66B54985D1A6}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="20715" windowHeight="13276" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Backlog" sheetId="1" r:id="rId1"/>
@@ -20,20 +20,20 @@
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Backlog!$A$1:$AB$52</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Listing!$A$1:$AE$68</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Listing!$AF$1:$AF$68</definedName>
     <definedName name="Z_A7754112_A52F_4ABC_8778_92F04773E53C_.wvu.FilterData" localSheetId="1" hidden="1">Listing!$A$1:$AE$32</definedName>
     <definedName name="Z_C25CEB9E_BEC1_4982_90C4_50C84EE1B82A_.wvu.FilterData" localSheetId="1" hidden="1">Listing!$A$1:$AE$32</definedName>
   </definedNames>
   <calcPr calcId="0"/>
   <customWorkbookViews>
+    <customWorkbookView name="Filter 2" guid="{C25CEB9E-BEC1-4982-90C4-50C84EE1B82A}" maximized="1" windowWidth="0" windowHeight="0" activeSheetId="0"/>
     <customWorkbookView name="Filter 1" guid="{A7754112-A52F-4ABC-8778-92F04773E53C}" maximized="1" windowWidth="0" windowHeight="0" activeSheetId="0"/>
-    <customWorkbookView name="Filter 2" guid="{C25CEB9E-BEC1-4982-90C4-50C84EE1B82A}" maximized="1" windowWidth="0" windowHeight="0" activeSheetId="0"/>
   </customWorkbookViews>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1553" uniqueCount="486">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1557" uniqueCount="491">
   <si>
     <t>ID</t>
   </si>
@@ -2075,9 +2075,6 @@
 Single storey, separate-title offering in one of the most premium suburbs in Canberra.</t>
   </si>
   <si>
-    <t>Rent</t>
-  </si>
-  <si>
     <t>Draft</t>
   </si>
   <si>
@@ -2088,6 +2085,24 @@
   </si>
   <si>
     <t>799,000+</t>
+  </si>
+  <si>
+    <t>Rented</t>
+  </si>
+  <si>
+    <t>Property URL</t>
+  </si>
+  <si>
+    <t>https://www.777homes.com.au/property/25-braine-street-page-act-2614-2/</t>
+  </si>
+  <si>
+    <t>https://www.777homes.com.au/property/6-summerhayes-st…aylor-act-2913-2/</t>
+  </si>
+  <si>
+    <t>https://www.777homes.com.au/property/227-sculthorpe-a…itlam-act-2611-2/</t>
+  </si>
+  <si>
+    <t>L</t>
   </si>
 </sst>
 </file>
@@ -2736,21 +2751,21 @@
       <selection pane="bottomLeft" activeCell="J2" sqref="J2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.46484375" defaultRowHeight="15.75" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15.75" customHeight="1"/>
   <cols>
     <col min="1" max="1" width="9.33203125" customWidth="1" collapsed="1"/>
     <col min="2" max="2" width="77.6640625" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="8.46484375" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="15.46484375" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="22.1328125" style="58" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="21.86328125" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="56.86328125" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="10.86328125" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="17.86328125" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="22.53125" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="8.44140625" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="15.44140625" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="22.109375" style="58" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="21.88671875" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="56.88671875" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="10.88671875" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="17.88671875" customWidth="1" collapsed="1"/>
+    <col min="11" max="11" width="22.5546875" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:28" ht="13.9">
+    <row r="1" spans="1:28" ht="13.8">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2800,7 +2815,7 @@
         <v>11</v>
       </c>
       <c r="H2" s="6" t="s">
-        <v>483</v>
+        <v>482</v>
       </c>
       <c r="I2" s="7"/>
       <c r="J2" s="63" t="s">
@@ -2827,7 +2842,7 @@
       <c r="AA2" s="7"/>
       <c r="AB2" s="7"/>
     </row>
-    <row r="3" spans="1:28" ht="13.9">
+    <row r="3" spans="1:28" ht="13.8">
       <c r="A3" s="2">
         <v>2</v>
       </c>
@@ -2850,7 +2865,7 @@
         <v>11</v>
       </c>
       <c r="H3" s="6" t="s">
-        <v>483</v>
+        <v>482</v>
       </c>
       <c r="I3" s="7"/>
       <c r="J3" s="4"/>
@@ -2898,7 +2913,7 @@
         <v>11</v>
       </c>
       <c r="H4" s="6" t="s">
-        <v>483</v>
+        <v>482</v>
       </c>
       <c r="I4" s="7"/>
       <c r="J4" s="4"/>
@@ -2923,7 +2938,7 @@
       <c r="AA4" s="7"/>
       <c r="AB4" s="7"/>
     </row>
-    <row r="5" spans="1:28" ht="13.9">
+    <row r="5" spans="1:28" ht="13.8">
       <c r="A5" s="10">
         <v>4</v>
       </c>
@@ -2946,7 +2961,7 @@
         <v>11</v>
       </c>
       <c r="H5" s="6" t="s">
-        <v>483</v>
+        <v>482</v>
       </c>
       <c r="I5" s="7"/>
       <c r="J5" s="4"/>
@@ -2971,7 +2986,7 @@
       <c r="AA5" s="7"/>
       <c r="AB5" s="7"/>
     </row>
-    <row r="6" spans="1:28" ht="13.9">
+    <row r="6" spans="1:28" ht="13.8">
       <c r="A6" s="10">
         <v>5</v>
       </c>
@@ -2992,7 +3007,7 @@
         <v>19</v>
       </c>
       <c r="H6" s="63" t="s">
-        <v>484</v>
+        <v>483</v>
       </c>
       <c r="I6" s="10"/>
       <c r="J6" s="10"/>
@@ -3015,7 +3030,7 @@
       <c r="AA6" s="10"/>
       <c r="AB6" s="10"/>
     </row>
-    <row r="7" spans="1:28" ht="13.9">
+    <row r="7" spans="1:28" ht="13.8">
       <c r="A7" s="10">
         <v>6</v>
       </c>
@@ -3036,7 +3051,7 @@
         <v>19</v>
       </c>
       <c r="H7" s="63" t="s">
-        <v>484</v>
+        <v>483</v>
       </c>
       <c r="I7" s="7"/>
       <c r="J7" s="7"/>
@@ -3059,7 +3074,7 @@
       <c r="AA7" s="7"/>
       <c r="AB7" s="7"/>
     </row>
-    <row r="8" spans="1:28" ht="13.9">
+    <row r="8" spans="1:28" ht="13.8">
       <c r="A8" s="10">
         <v>7</v>
       </c>
@@ -3080,7 +3095,7 @@
         <v>19</v>
       </c>
       <c r="H8" s="63" t="s">
-        <v>484</v>
+        <v>483</v>
       </c>
       <c r="I8" s="7"/>
       <c r="J8" s="7"/>
@@ -3103,7 +3118,7 @@
       <c r="AA8" s="7"/>
       <c r="AB8" s="7"/>
     </row>
-    <row r="9" spans="1:28" ht="13.9">
+    <row r="9" spans="1:28" ht="13.8">
       <c r="A9" s="10">
         <v>8</v>
       </c>
@@ -3124,7 +3139,7 @@
         <v>19</v>
       </c>
       <c r="H9" s="63" t="s">
-        <v>484</v>
+        <v>483</v>
       </c>
       <c r="I9" s="7"/>
       <c r="J9" s="7"/>
@@ -3147,7 +3162,7 @@
       <c r="AA9" s="7"/>
       <c r="AB9" s="7"/>
     </row>
-    <row r="10" spans="1:28" ht="13.9">
+    <row r="10" spans="1:28" ht="13.8">
       <c r="A10" s="10">
         <v>9</v>
       </c>
@@ -3168,7 +3183,7 @@
         <v>19</v>
       </c>
       <c r="H10" s="63" t="s">
-        <v>484</v>
+        <v>483</v>
       </c>
       <c r="I10" s="7"/>
       <c r="J10" s="7"/>
@@ -3191,7 +3206,7 @@
       <c r="AA10" s="7"/>
       <c r="AB10" s="7"/>
     </row>
-    <row r="11" spans="1:28" ht="13.9">
+    <row r="11" spans="1:28" ht="13.8">
       <c r="A11" s="10">
         <v>10</v>
       </c>
@@ -3212,7 +3227,7 @@
         <v>19</v>
       </c>
       <c r="H11" s="63" t="s">
-        <v>484</v>
+        <v>483</v>
       </c>
       <c r="I11" s="7"/>
       <c r="J11" s="7"/>
@@ -3235,7 +3250,7 @@
       <c r="AA11" s="7"/>
       <c r="AB11" s="7"/>
     </row>
-    <row r="12" spans="1:28" ht="13.9">
+    <row r="12" spans="1:28" ht="13.8">
       <c r="A12" s="10">
         <v>11</v>
       </c>
@@ -3256,7 +3271,7 @@
         <v>19</v>
       </c>
       <c r="H12" s="63" t="s">
-        <v>484</v>
+        <v>483</v>
       </c>
       <c r="I12" s="7"/>
       <c r="J12" s="7"/>
@@ -3279,7 +3294,7 @@
       <c r="AA12" s="7"/>
       <c r="AB12" s="7"/>
     </row>
-    <row r="13" spans="1:28" ht="13.9">
+    <row r="13" spans="1:28" ht="13.8">
       <c r="A13" s="10">
         <v>12</v>
       </c>
@@ -3300,7 +3315,7 @@
         <v>19</v>
       </c>
       <c r="H13" s="63" t="s">
-        <v>484</v>
+        <v>483</v>
       </c>
       <c r="I13" s="7"/>
       <c r="J13" s="7"/>
@@ -3323,7 +3338,7 @@
       <c r="AA13" s="7"/>
       <c r="AB13" s="7"/>
     </row>
-    <row r="14" spans="1:28" ht="13.9">
+    <row r="14" spans="1:28" ht="13.8">
       <c r="A14" s="10">
         <v>13</v>
       </c>
@@ -3344,7 +3359,7 @@
         <v>19</v>
       </c>
       <c r="H14" s="63" t="s">
-        <v>484</v>
+        <v>483</v>
       </c>
       <c r="I14" s="7"/>
       <c r="J14" s="7"/>
@@ -3367,7 +3382,7 @@
       <c r="AA14" s="7"/>
       <c r="AB14" s="7"/>
     </row>
-    <row r="15" spans="1:28" ht="13.9">
+    <row r="15" spans="1:28" ht="13.8">
       <c r="A15" s="10">
         <v>14</v>
       </c>
@@ -3388,7 +3403,7 @@
         <v>19</v>
       </c>
       <c r="H15" s="63" t="s">
-        <v>484</v>
+        <v>483</v>
       </c>
       <c r="I15" s="7"/>
       <c r="J15" s="7"/>
@@ -3411,7 +3426,7 @@
       <c r="AA15" s="7"/>
       <c r="AB15" s="7"/>
     </row>
-    <row r="16" spans="1:28" ht="13.9">
+    <row r="16" spans="1:28" ht="13.8">
       <c r="A16" s="10">
         <v>15</v>
       </c>
@@ -3432,7 +3447,7 @@
         <v>19</v>
       </c>
       <c r="H16" s="63" t="s">
-        <v>484</v>
+        <v>483</v>
       </c>
       <c r="I16" s="7"/>
       <c r="J16" s="7"/>
@@ -3455,7 +3470,7 @@
       <c r="AA16" s="7"/>
       <c r="AB16" s="7"/>
     </row>
-    <row r="17" spans="1:28" ht="13.9">
+    <row r="17" spans="1:28" ht="13.8">
       <c r="A17" s="10">
         <v>16</v>
       </c>
@@ -3476,7 +3491,7 @@
         <v>19</v>
       </c>
       <c r="H17" s="63" t="s">
-        <v>484</v>
+        <v>483</v>
       </c>
       <c r="I17" s="7"/>
       <c r="J17" s="7"/>
@@ -3499,7 +3514,7 @@
       <c r="AA17" s="7"/>
       <c r="AB17" s="7"/>
     </row>
-    <row r="18" spans="1:28" ht="13.9">
+    <row r="18" spans="1:28" ht="13.8">
       <c r="A18" s="10">
         <v>17</v>
       </c>
@@ -3520,7 +3535,7 @@
         <v>19</v>
       </c>
       <c r="H18" s="63" t="s">
-        <v>484</v>
+        <v>483</v>
       </c>
       <c r="I18" s="7"/>
       <c r="J18" s="7"/>
@@ -3543,7 +3558,7 @@
       <c r="AA18" s="7"/>
       <c r="AB18" s="7"/>
     </row>
-    <row r="19" spans="1:28" ht="13.9">
+    <row r="19" spans="1:28" ht="13.8">
       <c r="A19" s="10">
         <v>18</v>
       </c>
@@ -3564,7 +3579,7 @@
         <v>19</v>
       </c>
       <c r="H19" s="63" t="s">
-        <v>484</v>
+        <v>483</v>
       </c>
       <c r="I19" s="7"/>
       <c r="J19" s="7"/>
@@ -3587,7 +3602,7 @@
       <c r="AA19" s="7"/>
       <c r="AB19" s="7"/>
     </row>
-    <row r="20" spans="1:28" ht="13.9">
+    <row r="20" spans="1:28" ht="13.8">
       <c r="A20" s="10">
         <v>19</v>
       </c>
@@ -3608,7 +3623,7 @@
         <v>19</v>
       </c>
       <c r="H20" s="63" t="s">
-        <v>484</v>
+        <v>483</v>
       </c>
       <c r="I20" s="7"/>
       <c r="J20" s="7"/>
@@ -3631,7 +3646,7 @@
       <c r="AA20" s="7"/>
       <c r="AB20" s="7"/>
     </row>
-    <row r="21" spans="1:28" ht="13.9">
+    <row r="21" spans="1:28" ht="13.8">
       <c r="A21" s="10">
         <v>20</v>
       </c>
@@ -3652,7 +3667,7 @@
         <v>19</v>
       </c>
       <c r="H21" s="63" t="s">
-        <v>484</v>
+        <v>483</v>
       </c>
       <c r="I21" s="7"/>
       <c r="J21" s="7"/>
@@ -3675,7 +3690,7 @@
       <c r="AA21" s="7"/>
       <c r="AB21" s="7"/>
     </row>
-    <row r="22" spans="1:28" ht="13.9">
+    <row r="22" spans="1:28" ht="13.8">
       <c r="A22" s="10">
         <v>21</v>
       </c>
@@ -3696,7 +3711,7 @@
         <v>19</v>
       </c>
       <c r="H22" s="63" t="s">
-        <v>484</v>
+        <v>483</v>
       </c>
       <c r="I22" s="7"/>
       <c r="J22" s="7"/>
@@ -3719,7 +3734,7 @@
       <c r="AA22" s="7"/>
       <c r="AB22" s="7"/>
     </row>
-    <row r="23" spans="1:28" ht="13.9">
+    <row r="23" spans="1:28" ht="13.8">
       <c r="A23" s="10">
         <v>22</v>
       </c>
@@ -3740,7 +3755,7 @@
         <v>19</v>
       </c>
       <c r="H23" s="63" t="s">
-        <v>484</v>
+        <v>483</v>
       </c>
       <c r="I23" s="7"/>
       <c r="J23" s="7"/>
@@ -3763,7 +3778,7 @@
       <c r="AA23" s="7"/>
       <c r="AB23" s="7"/>
     </row>
-    <row r="24" spans="1:28" ht="13.9">
+    <row r="24" spans="1:28" ht="13.8">
       <c r="A24" s="10">
         <v>23</v>
       </c>
@@ -3784,7 +3799,7 @@
         <v>19</v>
       </c>
       <c r="H24" s="63" t="s">
-        <v>484</v>
+        <v>483</v>
       </c>
       <c r="I24" s="7"/>
       <c r="J24" s="7"/>
@@ -3807,7 +3822,7 @@
       <c r="AA24" s="7"/>
       <c r="AB24" s="7"/>
     </row>
-    <row r="25" spans="1:28" ht="13.9">
+    <row r="25" spans="1:28" ht="13.8">
       <c r="A25" s="10">
         <v>24</v>
       </c>
@@ -3851,7 +3866,7 @@
       <c r="AA25" s="7"/>
       <c r="AB25" s="7"/>
     </row>
-    <row r="26" spans="1:28" ht="13.9">
+    <row r="26" spans="1:28" ht="13.8">
       <c r="A26" s="10">
         <v>25</v>
       </c>
@@ -3895,7 +3910,7 @@
       <c r="AA26" s="7"/>
       <c r="AB26" s="7"/>
     </row>
-    <row r="27" spans="1:28" ht="13.9">
+    <row r="27" spans="1:28" ht="13.8">
       <c r="A27" s="10">
         <v>26</v>
       </c>
@@ -3939,7 +3954,7 @@
       <c r="AA27" s="7"/>
       <c r="AB27" s="7"/>
     </row>
-    <row r="28" spans="1:28" ht="13.9">
+    <row r="28" spans="1:28" ht="13.8">
       <c r="A28" s="10">
         <v>27</v>
       </c>
@@ -3983,7 +3998,7 @@
       <c r="AA28" s="7"/>
       <c r="AB28" s="7"/>
     </row>
-    <row r="29" spans="1:28" ht="13.9">
+    <row r="29" spans="1:28" ht="13.8">
       <c r="A29" s="10">
         <v>28</v>
       </c>
@@ -4027,7 +4042,7 @@
       <c r="AA29" s="7"/>
       <c r="AB29" s="7"/>
     </row>
-    <row r="30" spans="1:28" ht="13.9">
+    <row r="30" spans="1:28" ht="13.8">
       <c r="A30" s="10">
         <v>29</v>
       </c>
@@ -4071,7 +4086,7 @@
       <c r="AA30" s="7"/>
       <c r="AB30" s="7"/>
     </row>
-    <row r="31" spans="1:28" ht="13.9">
+    <row r="31" spans="1:28" ht="13.8">
       <c r="A31" s="4">
         <v>30</v>
       </c>
@@ -4115,7 +4130,7 @@
       <c r="AA31" s="7"/>
       <c r="AB31" s="7"/>
     </row>
-    <row r="32" spans="1:28" ht="13.9">
+    <row r="32" spans="1:28" ht="13.8">
       <c r="A32" s="4">
         <v>31</v>
       </c>
@@ -4159,7 +4174,7 @@
       <c r="AA32" s="7"/>
       <c r="AB32" s="7"/>
     </row>
-    <row r="33" spans="1:8" s="4" customFormat="1" ht="13.5">
+    <row r="33" spans="1:8" s="4" customFormat="1" ht="13.8">
       <c r="A33" s="4">
         <v>32</v>
       </c>
@@ -4176,10 +4191,10 @@
         <v>11</v>
       </c>
       <c r="H33" s="4" t="s">
-        <v>483</v>
-      </c>
-    </row>
-    <row r="34" spans="1:8" s="4" customFormat="1" ht="13.5">
+        <v>482</v>
+      </c>
+    </row>
+    <row r="34" spans="1:8" s="4" customFormat="1" ht="13.8">
       <c r="A34" s="4">
         <v>33</v>
       </c>
@@ -4196,10 +4211,10 @@
         <v>11</v>
       </c>
       <c r="H34" s="4" t="s">
-        <v>483</v>
-      </c>
-    </row>
-    <row r="35" spans="1:8" s="4" customFormat="1" ht="12.75">
+        <v>482</v>
+      </c>
+    </row>
+    <row r="35" spans="1:8" s="4" customFormat="1" ht="13.2">
       <c r="A35" s="4">
         <v>34</v>
       </c>
@@ -4216,10 +4231,10 @@
         <v>11</v>
       </c>
       <c r="H35" s="4" t="s">
-        <v>483</v>
-      </c>
-    </row>
-    <row r="36" spans="1:8" s="4" customFormat="1" ht="12.75">
+        <v>482</v>
+      </c>
+    </row>
+    <row r="36" spans="1:8" s="4" customFormat="1" ht="13.2">
       <c r="A36" s="4">
         <v>35</v>
       </c>
@@ -4236,10 +4251,10 @@
         <v>11</v>
       </c>
       <c r="H36" s="4" t="s">
-        <v>483</v>
-      </c>
-    </row>
-    <row r="37" spans="1:8" s="4" customFormat="1" ht="12.75">
+        <v>482</v>
+      </c>
+    </row>
+    <row r="37" spans="1:8" s="4" customFormat="1" ht="13.2">
       <c r="A37" s="4">
         <v>36</v>
       </c>
@@ -4256,10 +4271,10 @@
         <v>11</v>
       </c>
       <c r="H37" s="4" t="s">
-        <v>483</v>
-      </c>
-    </row>
-    <row r="38" spans="1:8" s="4" customFormat="1" ht="12.75">
+        <v>482</v>
+      </c>
+    </row>
+    <row r="38" spans="1:8" s="4" customFormat="1" ht="13.2">
       <c r="A38" s="4">
         <v>37</v>
       </c>
@@ -4276,10 +4291,10 @@
         <v>11</v>
       </c>
       <c r="H38" s="4" t="s">
-        <v>483</v>
-      </c>
-    </row>
-    <row r="39" spans="1:8" s="4" customFormat="1" ht="12.75">
+        <v>482</v>
+      </c>
+    </row>
+    <row r="39" spans="1:8" s="4" customFormat="1" ht="13.2">
       <c r="A39" s="4">
         <v>38</v>
       </c>
@@ -4296,10 +4311,10 @@
         <v>11</v>
       </c>
       <c r="H39" s="4" t="s">
-        <v>483</v>
-      </c>
-    </row>
-    <row r="40" spans="1:8" s="4" customFormat="1" ht="12.75">
+        <v>482</v>
+      </c>
+    </row>
+    <row r="40" spans="1:8" s="4" customFormat="1" ht="13.2">
       <c r="A40" s="4">
         <v>39</v>
       </c>
@@ -4316,10 +4331,10 @@
         <v>11</v>
       </c>
       <c r="H40" s="4" t="s">
-        <v>483</v>
-      </c>
-    </row>
-    <row r="41" spans="1:8" s="4" customFormat="1" ht="12.75">
+        <v>482</v>
+      </c>
+    </row>
+    <row r="41" spans="1:8" s="4" customFormat="1" ht="13.2">
       <c r="A41" s="4">
         <v>40</v>
       </c>
@@ -4336,10 +4351,10 @@
         <v>11</v>
       </c>
       <c r="H41" s="4" t="s">
-        <v>483</v>
-      </c>
-    </row>
-    <row r="42" spans="1:8" s="4" customFormat="1" ht="12.75">
+        <v>482</v>
+      </c>
+    </row>
+    <row r="42" spans="1:8" s="4" customFormat="1" ht="13.2">
       <c r="A42" s="4">
         <v>41</v>
       </c>
@@ -4356,10 +4371,10 @@
         <v>11</v>
       </c>
       <c r="H42" s="4" t="s">
-        <v>483</v>
-      </c>
-    </row>
-    <row r="43" spans="1:8" s="4" customFormat="1" ht="12.75">
+        <v>482</v>
+      </c>
+    </row>
+    <row r="43" spans="1:8" s="4" customFormat="1" ht="13.2">
       <c r="A43" s="4">
         <v>42</v>
       </c>
@@ -4376,10 +4391,10 @@
         <v>11</v>
       </c>
       <c r="H43" s="4" t="s">
-        <v>483</v>
-      </c>
-    </row>
-    <row r="44" spans="1:8" s="4" customFormat="1" ht="12.75">
+        <v>482</v>
+      </c>
+    </row>
+    <row r="44" spans="1:8" s="4" customFormat="1" ht="13.2">
       <c r="A44" s="4">
         <v>43</v>
       </c>
@@ -4396,10 +4411,10 @@
         <v>11</v>
       </c>
       <c r="H44" s="4" t="s">
-        <v>483</v>
-      </c>
-    </row>
-    <row r="45" spans="1:8" s="4" customFormat="1" ht="12.75">
+        <v>482</v>
+      </c>
+    </row>
+    <row r="45" spans="1:8" s="4" customFormat="1" ht="13.2">
       <c r="A45" s="4">
         <v>44</v>
       </c>
@@ -4419,7 +4434,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="46" spans="1:8" s="4" customFormat="1" ht="12.75">
+    <row r="46" spans="1:8" s="4" customFormat="1" ht="13.2">
       <c r="A46" s="4">
         <v>45</v>
       </c>
@@ -4439,7 +4454,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="47" spans="1:8" s="4" customFormat="1" ht="12.75">
+    <row r="47" spans="1:8" s="4" customFormat="1" ht="13.2">
       <c r="A47" s="4">
         <v>46</v>
       </c>
@@ -4459,7 +4474,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="48" spans="1:8" s="4" customFormat="1" ht="12.75">
+    <row r="48" spans="1:8" s="4" customFormat="1" ht="13.2">
       <c r="A48" s="4">
         <v>47</v>
       </c>
@@ -4476,10 +4491,10 @@
         <v>19</v>
       </c>
       <c r="H48" s="4" t="s">
-        <v>484</v>
-      </c>
-    </row>
-    <row r="49" spans="1:8" s="4" customFormat="1" ht="12.75">
+        <v>483</v>
+      </c>
+    </row>
+    <row r="49" spans="1:8" s="4" customFormat="1" ht="13.2">
       <c r="A49" s="4">
         <v>48</v>
       </c>
@@ -4496,10 +4511,10 @@
         <v>19</v>
       </c>
       <c r="H49" s="4" t="s">
-        <v>484</v>
-      </c>
-    </row>
-    <row r="50" spans="1:8" s="4" customFormat="1" ht="12.75">
+        <v>483</v>
+      </c>
+    </row>
+    <row r="50" spans="1:8" s="4" customFormat="1" ht="13.2">
       <c r="A50" s="4">
         <v>49</v>
       </c>
@@ -4516,10 +4531,10 @@
         <v>19</v>
       </c>
       <c r="H50" s="4" t="s">
-        <v>484</v>
-      </c>
-    </row>
-    <row r="51" spans="1:8" s="4" customFormat="1" ht="12.75">
+        <v>483</v>
+      </c>
+    </row>
+    <row r="51" spans="1:8" s="4" customFormat="1" ht="13.2">
       <c r="A51" s="4">
         <v>50</v>
       </c>
@@ -4536,10 +4551,10 @@
         <v>19</v>
       </c>
       <c r="H51" s="4" t="s">
-        <v>484</v>
-      </c>
-    </row>
-    <row r="52" spans="1:8" s="4" customFormat="1" ht="12.75">
+        <v>483</v>
+      </c>
+    </row>
+    <row r="52" spans="1:8" s="4" customFormat="1" ht="13.2">
       <c r="A52" s="4">
         <v>51</v>
       </c>
@@ -4556,7 +4571,7 @@
         <v>19</v>
       </c>
       <c r="H52" s="4" t="s">
-        <v>484</v>
+        <v>483</v>
       </c>
     </row>
     <row r="53" spans="1:8" s="4" customFormat="1" ht="15.75" customHeight="1">
@@ -4579,7 +4594,7 @@
         <v>369</v>
       </c>
     </row>
-    <row r="54" spans="1:8" ht="12.75">
+    <row r="54" spans="1:8" ht="13.2">
       <c r="A54">
         <v>53</v>
       </c>
@@ -4599,7 +4614,7 @@
         <v>369</v>
       </c>
     </row>
-    <row r="55" spans="1:8" s="4" customFormat="1" ht="12.75">
+    <row r="55" spans="1:8" s="4" customFormat="1" ht="13.2">
       <c r="A55" s="4">
         <v>54</v>
       </c>
@@ -4619,7 +4634,7 @@
         <v>369</v>
       </c>
     </row>
-    <row r="56" spans="1:8" s="4" customFormat="1" ht="12.75">
+    <row r="56" spans="1:8" s="4" customFormat="1" ht="13.2">
       <c r="A56" s="4">
         <v>55</v>
       </c>
@@ -4627,7 +4642,7 @@
         <v>377</v>
       </c>
       <c r="D56" s="16" t="s">
-        <v>9</v>
+        <v>481</v>
       </c>
       <c r="F56" s="4" t="s">
         <v>85</v>
@@ -4639,7 +4654,7 @@
         <v>369</v>
       </c>
     </row>
-    <row r="57" spans="1:8" s="4" customFormat="1" ht="12.75">
+    <row r="57" spans="1:8" s="4" customFormat="1" ht="13.2">
       <c r="A57" s="4">
         <v>56</v>
       </c>
@@ -4659,7 +4674,7 @@
         <v>369</v>
       </c>
     </row>
-    <row r="58" spans="1:8" s="4" customFormat="1" ht="12.75">
+    <row r="58" spans="1:8" s="4" customFormat="1" ht="13.2">
       <c r="A58" s="4">
         <v>57</v>
       </c>
@@ -4679,7 +4694,7 @@
         <v>369</v>
       </c>
     </row>
-    <row r="59" spans="1:8" s="4" customFormat="1" ht="12.75">
+    <row r="59" spans="1:8" s="4" customFormat="1" ht="13.2">
       <c r="A59" s="4">
         <v>58</v>
       </c>
@@ -4699,7 +4714,7 @@
         <v>369</v>
       </c>
     </row>
-    <row r="60" spans="1:8" s="4" customFormat="1" ht="12.75">
+    <row r="60" spans="1:8" s="4" customFormat="1" ht="13.2">
       <c r="A60" s="4">
         <v>59</v>
       </c>
@@ -4719,7 +4734,7 @@
         <v>369</v>
       </c>
     </row>
-    <row r="61" spans="1:8" s="4" customFormat="1" ht="12.75">
+    <row r="61" spans="1:8" s="4" customFormat="1" ht="13.2">
       <c r="A61" s="4">
         <v>60</v>
       </c>
@@ -4739,7 +4754,7 @@
         <v>369</v>
       </c>
     </row>
-    <row r="62" spans="1:8" s="4" customFormat="1" ht="12.75">
+    <row r="62" spans="1:8" s="4" customFormat="1" ht="13.2">
       <c r="A62" s="4">
         <v>61</v>
       </c>
@@ -4756,10 +4771,10 @@
         <v>11</v>
       </c>
       <c r="H62" s="4" t="s">
-        <v>483</v>
-      </c>
-    </row>
-    <row r="63" spans="1:8" s="4" customFormat="1" ht="12.75">
+        <v>482</v>
+      </c>
+    </row>
+    <row r="63" spans="1:8" s="4" customFormat="1" ht="13.2">
       <c r="A63" s="4">
         <v>62</v>
       </c>
@@ -4776,10 +4791,10 @@
         <v>11</v>
       </c>
       <c r="H63" s="4" t="s">
-        <v>483</v>
-      </c>
-    </row>
-    <row r="64" spans="1:8" s="4" customFormat="1" ht="12.75">
+        <v>482</v>
+      </c>
+    </row>
+    <row r="64" spans="1:8" s="4" customFormat="1" ht="13.2">
       <c r="A64" s="4">
         <v>63</v>
       </c>
@@ -4796,10 +4811,10 @@
         <v>11</v>
       </c>
       <c r="H64" s="4" t="s">
-        <v>483</v>
-      </c>
-    </row>
-    <row r="65" spans="1:8" s="4" customFormat="1" ht="12.75">
+        <v>482</v>
+      </c>
+    </row>
+    <row r="65" spans="1:8" s="4" customFormat="1" ht="13.2">
       <c r="A65" s="4">
         <v>64</v>
       </c>
@@ -4816,10 +4831,10 @@
         <v>11</v>
       </c>
       <c r="H65" s="4" t="s">
-        <v>483</v>
-      </c>
-    </row>
-    <row r="66" spans="1:8" s="4" customFormat="1" ht="12.75">
+        <v>482</v>
+      </c>
+    </row>
+    <row r="66" spans="1:8" s="4" customFormat="1" ht="13.2">
       <c r="A66" s="4">
         <v>65</v>
       </c>
@@ -4827,7 +4842,7 @@
         <v>387</v>
       </c>
       <c r="D66" s="4" t="s">
-        <v>9</v>
+        <v>481</v>
       </c>
       <c r="F66" s="4" t="s">
         <v>85</v>
@@ -4839,7 +4854,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="67" spans="1:8" s="4" customFormat="1" ht="12.75">
+    <row r="67" spans="1:8" s="4" customFormat="1" ht="13.2">
       <c r="A67" s="4">
         <v>66</v>
       </c>
@@ -4847,7 +4862,7 @@
         <v>388</v>
       </c>
       <c r="D67" s="4" t="s">
-        <v>9</v>
+        <v>481</v>
       </c>
       <c r="F67" s="4" t="s">
         <v>110</v>
@@ -4856,10 +4871,10 @@
         <v>19</v>
       </c>
       <c r="H67" s="4" t="s">
-        <v>484</v>
-      </c>
-    </row>
-    <row r="68" spans="1:8" s="4" customFormat="1" ht="12.75">
+        <v>483</v>
+      </c>
+    </row>
+    <row r="68" spans="1:8" s="4" customFormat="1" ht="13.2">
       <c r="A68" s="4">
         <v>67</v>
       </c>
@@ -4867,7 +4882,7 @@
         <v>389</v>
       </c>
       <c r="D68" s="4" t="s">
-        <v>9</v>
+        <v>481</v>
       </c>
       <c r="F68" s="4" t="s">
         <v>110</v>
@@ -4876,7 +4891,7 @@
         <v>19</v>
       </c>
       <c r="H68" s="4" t="s">
-        <v>484</v>
+        <v>483</v>
       </c>
     </row>
   </sheetData>
@@ -4961,34 +4976,35 @@
   </sheetPr>
   <dimension ref="A1:AJ68"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="K13" workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="AD2" sqref="AD2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.46484375" defaultRowHeight="15.75" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15.75" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="14.86328125" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="18.1328125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" width="14.88671875" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="18.109375" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="3" max="3" width="53.6640625" customWidth="1" collapsed="1"/>
     <col min="4" max="4" width="25.33203125" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="19.53125" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="19.5546875" customWidth="1" collapsed="1"/>
     <col min="6" max="6" width="19.6640625" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="18.53125" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="18.5546875" customWidth="1" collapsed="1"/>
     <col min="8" max="8" width="32.33203125" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="20.53125" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="21.1328125" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="20.5546875" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="21.109375" customWidth="1" collapsed="1"/>
     <col min="11" max="11" width="28.6640625" customWidth="1" collapsed="1"/>
-    <col min="12" max="12" width="37.53125" customWidth="1" collapsed="1"/>
+    <col min="12" max="12" width="37.5546875" customWidth="1" collapsed="1"/>
     <col min="16" max="17" width="18.6640625" customWidth="1" collapsed="1"/>
-    <col min="18" max="18" width="47.86328125" customWidth="1" collapsed="1"/>
-    <col min="19" max="19" width="77.53125" customWidth="1" collapsed="1"/>
+    <col min="18" max="18" width="47.88671875" customWidth="1" collapsed="1"/>
+    <col min="19" max="19" width="77.5546875" customWidth="1" collapsed="1"/>
     <col min="20" max="20" width="24" customWidth="1" collapsed="1"/>
     <col min="21" max="21" width="18.6640625" customWidth="1" collapsed="1"/>
-    <col min="22" max="22" width="19.1328125" customWidth="1" collapsed="1"/>
+    <col min="22" max="22" width="19.109375" customWidth="1" collapsed="1"/>
     <col min="23" max="31" width="19.33203125" customWidth="1" collapsed="1"/>
+    <col min="32" max="32" width="62.44140625" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:36" ht="27.75">
+    <row r="1" spans="1:36" ht="27.6">
       <c r="A1" s="1" t="s">
         <v>49</v>
       </c>
@@ -5068,7 +5084,7 @@
         <v>73</v>
       </c>
       <c r="AA1" s="1" t="s">
-        <v>74</v>
+        <v>490</v>
       </c>
       <c r="AB1" s="1" t="s">
         <v>75</v>
@@ -5082,7 +5098,9 @@
       <c r="AE1" s="1" t="s">
         <v>78</v>
       </c>
-      <c r="AF1" s="27"/>
+      <c r="AF1" s="27" t="s">
+        <v>486</v>
+      </c>
       <c r="AG1" s="27"/>
       <c r="AH1" s="27"/>
       <c r="AI1" s="27"/>
@@ -5261,7 +5279,7 @@
         <v>799000</v>
       </c>
       <c r="L4" s="28" t="s">
-        <v>485</v>
+        <v>484</v>
       </c>
       <c r="M4" s="28">
         <v>4</v>
@@ -7401,7 +7419,7 @@
       <c r="AI32" s="28"/>
       <c r="AJ32" s="28"/>
     </row>
-    <row r="33" spans="1:21" s="28" customFormat="1" ht="13.5">
+    <row r="33" spans="1:21" s="28" customFormat="1" ht="13.8">
       <c r="A33" s="28" t="s">
         <v>240</v>
       </c>
@@ -7460,7 +7478,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="34" spans="1:21" s="28" customFormat="1" ht="13.5">
+    <row r="34" spans="1:21" s="28" customFormat="1" ht="13.8">
       <c r="A34" s="28" t="s">
         <v>251</v>
       </c>
@@ -7519,7 +7537,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="35" spans="1:21" s="28" customFormat="1" ht="13.5">
+    <row r="35" spans="1:21" s="28" customFormat="1" ht="13.8">
       <c r="A35" s="28" t="s">
         <v>258</v>
       </c>
@@ -7578,7 +7596,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="36" spans="1:21" s="28" customFormat="1" ht="13.5">
+    <row r="36" spans="1:21" s="28" customFormat="1" ht="13.8">
       <c r="A36" s="28" t="s">
         <v>264</v>
       </c>
@@ -7637,7 +7655,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="37" spans="1:21" s="28" customFormat="1" ht="13.5">
+    <row r="37" spans="1:21" s="28" customFormat="1" ht="13.8">
       <c r="A37" s="28" t="s">
         <v>271</v>
       </c>
@@ -7696,7 +7714,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="38" spans="1:21" s="28" customFormat="1" ht="13.5">
+    <row r="38" spans="1:21" s="28" customFormat="1" ht="13.8">
       <c r="A38" s="28" t="s">
         <v>277</v>
       </c>
@@ -7755,7 +7773,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="39" spans="1:21" s="28" customFormat="1" ht="13.5">
+    <row r="39" spans="1:21" s="28" customFormat="1" ht="13.8">
       <c r="A39" s="28" t="s">
         <v>285</v>
       </c>
@@ -7814,7 +7832,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="40" spans="1:21" s="28" customFormat="1" ht="13.5">
+    <row r="40" spans="1:21" s="28" customFormat="1" ht="13.8">
       <c r="A40" s="28" t="s">
         <v>288</v>
       </c>
@@ -7873,7 +7891,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="41" spans="1:21" s="28" customFormat="1" ht="13.5">
+    <row r="41" spans="1:21" s="28" customFormat="1" ht="13.8">
       <c r="A41" s="28" t="s">
         <v>291</v>
       </c>
@@ -7932,7 +7950,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="42" spans="1:21" s="28" customFormat="1" ht="13.5">
+    <row r="42" spans="1:21" s="28" customFormat="1" ht="13.8">
       <c r="A42" s="28" t="s">
         <v>300</v>
       </c>
@@ -7991,7 +8009,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="43" spans="1:21" s="28" customFormat="1" ht="13.5">
+    <row r="43" spans="1:21" s="28" customFormat="1" ht="13.8">
       <c r="A43" s="28" t="s">
         <v>304</v>
       </c>
@@ -8050,7 +8068,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="44" spans="1:21" s="28" customFormat="1" ht="13.5">
+    <row r="44" spans="1:21" s="28" customFormat="1" ht="13.8">
       <c r="A44" s="28" t="s">
         <v>313</v>
       </c>
@@ -8109,7 +8127,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="45" spans="1:21" s="28" customFormat="1" ht="13.5">
+    <row r="45" spans="1:21" s="28" customFormat="1" ht="13.8">
       <c r="A45" s="28" t="s">
         <v>320</v>
       </c>
@@ -8168,7 +8186,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="46" spans="1:21" s="28" customFormat="1" ht="13.5">
+    <row r="46" spans="1:21" s="28" customFormat="1" ht="13.8">
       <c r="A46" s="28" t="s">
         <v>326</v>
       </c>
@@ -8227,7 +8245,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="47" spans="1:21" s="28" customFormat="1" ht="13.5">
+    <row r="47" spans="1:21" s="28" customFormat="1" ht="13.8">
       <c r="A47" s="28" t="s">
         <v>332</v>
       </c>
@@ -8286,7 +8304,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="48" spans="1:21" s="28" customFormat="1" ht="13.5">
+    <row r="48" spans="1:21" s="28" customFormat="1" ht="13.8">
       <c r="A48" s="28" t="s">
         <v>338</v>
       </c>
@@ -8345,7 +8363,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="49" spans="1:21" s="28" customFormat="1" ht="13.5">
+    <row r="49" spans="1:21" s="28" customFormat="1" ht="13.8">
       <c r="A49" s="28" t="s">
         <v>343</v>
       </c>
@@ -8404,7 +8422,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="50" spans="1:21" s="28" customFormat="1" ht="13.5">
+    <row r="50" spans="1:21" s="28" customFormat="1" ht="13.8">
       <c r="A50" s="28" t="s">
         <v>349</v>
       </c>
@@ -8463,7 +8481,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="51" spans="1:21" s="28" customFormat="1" ht="13.5">
+    <row r="51" spans="1:21" s="28" customFormat="1" ht="13.8">
       <c r="A51" s="28" t="s">
         <v>355</v>
       </c>
@@ -8522,7 +8540,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="52" spans="1:21" s="28" customFormat="1" ht="13.5">
+    <row r="52" spans="1:21" s="28" customFormat="1" ht="13.8">
       <c r="A52" s="28" t="s">
         <v>361</v>
       </c>
@@ -8581,7 +8599,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="53" spans="1:21" s="28" customFormat="1" ht="13.5">
+    <row r="53" spans="1:21" s="28" customFormat="1" ht="13.8">
       <c r="A53" s="28" t="s">
         <v>390</v>
       </c>
@@ -8640,12 +8658,12 @@
         <v>371</v>
       </c>
     </row>
-    <row r="54" spans="1:21" ht="12.75">
+    <row r="54" spans="1:21" ht="13.2">
       <c r="A54" t="s">
         <v>396</v>
       </c>
       <c r="B54" t="s">
-        <v>482</v>
+        <v>481</v>
       </c>
       <c r="C54" t="s">
         <v>397</v>
@@ -8699,7 +8717,7 @@
         <v>371</v>
       </c>
     </row>
-    <row r="55" spans="1:21" s="28" customFormat="1" ht="13.5">
+    <row r="55" spans="1:21" s="28" customFormat="1" ht="13.8">
       <c r="A55" s="28" t="s">
         <v>400</v>
       </c>
@@ -8758,12 +8776,12 @@
         <v>371</v>
       </c>
     </row>
-    <row r="56" spans="1:21" s="28" customFormat="1" ht="13.5">
+    <row r="56" spans="1:21" s="28" customFormat="1" ht="13.8">
       <c r="A56" s="28" t="s">
         <v>406</v>
       </c>
       <c r="B56" s="28" t="s">
-        <v>9</v>
+        <v>481</v>
       </c>
       <c r="C56" s="28" t="s">
         <v>407</v>
@@ -8817,12 +8835,12 @@
         <v>371</v>
       </c>
     </row>
-    <row r="57" spans="1:21" s="28" customFormat="1" ht="13.5">
+    <row r="57" spans="1:21" s="28" customFormat="1" ht="13.8">
       <c r="A57" s="28" t="s">
         <v>411</v>
       </c>
       <c r="B57" s="28" t="s">
-        <v>9</v>
+        <v>15</v>
       </c>
       <c r="C57" s="28" t="s">
         <v>412</v>
@@ -8831,7 +8849,7 @@
         <v>88</v>
       </c>
       <c r="E57" s="28" t="s">
-        <v>481</v>
+        <v>485</v>
       </c>
       <c r="F57" s="28" t="s">
         <v>252</v>
@@ -8876,7 +8894,7 @@
         <v>371</v>
       </c>
     </row>
-    <row r="58" spans="1:21" s="28" customFormat="1" ht="13.5">
+    <row r="58" spans="1:21" s="28" customFormat="1" ht="13.8">
       <c r="A58" s="28" t="s">
         <v>418</v>
       </c>
@@ -8890,7 +8908,7 @@
         <v>80</v>
       </c>
       <c r="E58" s="28" t="s">
-        <v>481</v>
+        <v>485</v>
       </c>
       <c r="F58" s="28" t="s">
         <v>82</v>
@@ -8935,7 +8953,7 @@
         <v>371</v>
       </c>
     </row>
-    <row r="59" spans="1:21" s="28" customFormat="1" ht="13.5">
+    <row r="59" spans="1:21" s="28" customFormat="1" ht="13.8">
       <c r="A59" s="28" t="s">
         <v>424</v>
       </c>
@@ -8994,7 +9012,7 @@
         <v>371</v>
       </c>
     </row>
-    <row r="60" spans="1:21" s="28" customFormat="1" ht="13.5">
+    <row r="60" spans="1:21" s="28" customFormat="1" ht="13.8">
       <c r="A60" s="28" t="s">
         <v>431</v>
       </c>
@@ -9053,7 +9071,7 @@
         <v>371</v>
       </c>
     </row>
-    <row r="61" spans="1:21" s="28" customFormat="1" ht="13.5">
+    <row r="61" spans="1:21" s="28" customFormat="1" ht="13.8">
       <c r="A61" s="28" t="s">
         <v>438</v>
       </c>
@@ -9112,7 +9130,7 @@
         <v>371</v>
       </c>
     </row>
-    <row r="62" spans="1:21" s="28" customFormat="1" ht="13.5">
+    <row r="62" spans="1:21" s="28" customFormat="1" ht="13.8">
       <c r="A62" s="28" t="s">
         <v>444</v>
       </c>
@@ -9171,7 +9189,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="63" spans="1:21" s="28" customFormat="1" ht="13.5">
+    <row r="63" spans="1:21" s="28" customFormat="1" ht="13.8">
       <c r="A63" s="28" t="s">
         <v>447</v>
       </c>
@@ -9230,7 +9248,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="64" spans="1:21" s="28" customFormat="1" ht="13.5">
+    <row r="64" spans="1:21" s="28" customFormat="1" ht="13.8">
       <c r="A64" s="28" t="s">
         <v>452</v>
       </c>
@@ -9289,7 +9307,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="65" spans="1:21" s="28" customFormat="1" ht="13.5">
+    <row r="65" spans="1:32" s="28" customFormat="1" ht="13.8">
       <c r="A65" s="28" t="s">
         <v>458</v>
       </c>
@@ -9348,12 +9366,12 @@
         <v>11</v>
       </c>
     </row>
-    <row r="66" spans="1:21" s="28" customFormat="1" ht="13.5">
+    <row r="66" spans="1:32" s="28" customFormat="1" ht="13.8">
       <c r="A66" s="28" t="s">
         <v>463</v>
       </c>
       <c r="B66" s="28" t="s">
-        <v>9</v>
+        <v>481</v>
       </c>
       <c r="C66" s="28" t="s">
         <v>464</v>
@@ -9406,13 +9424,16 @@
       <c r="U66" s="28" t="s">
         <v>40</v>
       </c>
-    </row>
-    <row r="67" spans="1:21" s="28" customFormat="1" ht="13.5">
+      <c r="AF66" t="s">
+        <v>488</v>
+      </c>
+    </row>
+    <row r="67" spans="1:32" s="28" customFormat="1" ht="13.8">
       <c r="A67" s="28" t="s">
         <v>469</v>
       </c>
       <c r="B67" s="28" t="s">
-        <v>9</v>
+        <v>481</v>
       </c>
       <c r="C67" s="28" t="s">
         <v>470</v>
@@ -9465,13 +9486,16 @@
       <c r="U67" s="28" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="68" spans="1:21" s="28" customFormat="1" ht="13.5">
+      <c r="AF67" t="s">
+        <v>487</v>
+      </c>
+    </row>
+    <row r="68" spans="1:32" s="28" customFormat="1" ht="13.8">
       <c r="A68" s="28" t="s">
         <v>475</v>
       </c>
       <c r="B68" s="28" t="s">
-        <v>9</v>
+        <v>481</v>
       </c>
       <c r="C68" s="28" t="s">
         <v>476</v>
@@ -9524,10 +9548,16 @@
       <c r="U68" s="28" t="s">
         <v>19</v>
       </c>
+      <c r="AF68" t="s">
+        <v>489</v>
+      </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:AE68" xr:uid="{3EAC26A4-0215-4509-8AC1-88A18A1CA423}"/>
   <customSheetViews>
+    <customSheetView guid="{C25CEB9E-BEC1-4982-90C4-50C84EE1B82A}" filter="1" showAutoFilter="1">
+      <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+      <autoFilter ref="A1:AD33" xr:uid="{00000000-0000-0000-0000-000000000000}"/>
+    </customSheetView>
     <customSheetView guid="{A7754112-A52F-4ABC-8778-92F04773E53C}" filter="1" showAutoFilter="1">
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <autoFilter ref="A1:AD33" xr:uid="{00000000-0000-0000-0000-000000000000}">
@@ -9537,10 +9567,6 @@
           </filters>
         </filterColumn>
       </autoFilter>
-    </customSheetView>
-    <customSheetView guid="{C25CEB9E-BEC1-4982-90C4-50C84EE1B82A}" filter="1" showAutoFilter="1">
-      <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-      <autoFilter ref="A1:AD33" xr:uid="{00000000-0000-0000-0000-000000000000}"/>
     </customSheetView>
   </customSheetViews>
   <conditionalFormatting sqref="A1:AJ1">
@@ -9614,23 +9640,23 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.46484375" defaultRowHeight="15.75" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15.75" customHeight="1"/>
   <cols>
     <col min="1" max="1" width="16" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="14.53125" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="14.5546875" customWidth="1" collapsed="1"/>
     <col min="4" max="4" width="16.6640625" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="14.53125" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="14.5546875" customWidth="1" collapsed="1"/>
     <col min="9" max="9" width="13.33203125" customWidth="1" collapsed="1"/>
-    <col min="15" max="15" width="20.86328125" customWidth="1" collapsed="1"/>
-    <col min="21" max="21" width="19.1328125" customWidth="1" collapsed="1"/>
+    <col min="15" max="15" width="20.88671875" customWidth="1" collapsed="1"/>
+    <col min="21" max="21" width="19.109375" customWidth="1" collapsed="1"/>
     <col min="22" max="22" width="19.33203125" customWidth="1" collapsed="1"/>
-    <col min="23" max="23" width="20.1328125" customWidth="1" collapsed="1"/>
+    <col min="23" max="23" width="20.109375" customWidth="1" collapsed="1"/>
     <col min="24" max="24" width="19.6640625" customWidth="1" collapsed="1"/>
-    <col min="26" max="26" width="15.86328125" customWidth="1" collapsed="1"/>
-    <col min="27" max="27" width="13.46484375" customWidth="1" collapsed="1"/>
+    <col min="26" max="26" width="15.88671875" customWidth="1" collapsed="1"/>
+    <col min="27" max="27" width="13.44140625" customWidth="1" collapsed="1"/>
     <col min="28" max="28" width="15.33203125" customWidth="1" collapsed="1"/>
-    <col min="29" max="29" width="16.1328125" customWidth="1" collapsed="1"/>
-    <col min="30" max="30" width="15.86328125" customWidth="1" collapsed="1"/>
+    <col min="29" max="29" width="16.109375" customWidth="1" collapsed="1"/>
+    <col min="30" max="30" width="15.88671875" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:35" ht="15.75" customHeight="1">
@@ -9753,16 +9779,16 @@
       <selection pane="bottomLeft" activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.46484375" defaultRowHeight="15.75" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15.75" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="44.86328125" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="17.1328125" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="26.46484375" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="36.1328125" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="51.1328125" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" width="44.88671875" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="17.109375" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="26.44140625" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="36.109375" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="51.109375" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:26" ht="13.9">
+    <row r="1" spans="1:26" ht="13.8">
       <c r="A1" s="45" t="s">
         <v>197</v>
       </c>

</xml_diff>

<commit_message>
Script (5) -run -20/05/2021
</commit_message>
<xml_diff>
--- a/src/main/resources/InputTestdata/Listing details.xlsx
+++ b/src/main/resources/InputTestdata/Listing details.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Athavan\git\777Homes-business\src\main\resources\InputTestdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B70E921D-2A27-4A64-842E-C75FF4498955}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{30C4D70A-DB1D-4B22-AB91-82331DAFC9B7}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="20715" windowHeight="13276" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="20715" windowHeight="13276" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Backlog" sheetId="1" r:id="rId1"/>
@@ -26,14 +26,14 @@
   </definedNames>
   <calcPr calcId="0"/>
   <customWorkbookViews>
+    <customWorkbookView name="Filter 2" guid="{C25CEB9E-BEC1-4982-90C4-50C84EE1B82A}" maximized="1" windowWidth="0" windowHeight="0" activeSheetId="0"/>
     <customWorkbookView name="Filter 1" guid="{A7754112-A52F-4ABC-8778-92F04773E53C}" maximized="1" windowWidth="0" windowHeight="0" activeSheetId="0"/>
-    <customWorkbookView name="Filter 2" guid="{C25CEB9E-BEC1-4982-90C4-50C84EE1B82A}" maximized="1" windowWidth="0" windowHeight="0" activeSheetId="0"/>
   </customWorkbookViews>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1941" uniqueCount="614">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1967" uniqueCount="632">
   <si>
     <t>ID</t>
   </si>
@@ -2301,9 +2301,6 @@
     <t>163 Oodgeroo Avenue, Franklin ACT 2913</t>
   </si>
   <si>
-    <t>NEW</t>
-  </si>
-  <si>
     <t>Block/House: 330/ 146</t>
   </si>
   <si>
@@ -2744,6 +2741,63 @@
 Nett rental yield: 4.5%
 Call Serene 0497565143 to see this compact beauty today!</t>
   </si>
+  <si>
+    <t>https://www.777homes.com.au/?post_type=property&amp;p=6800&amp;preview=true</t>
+  </si>
+  <si>
+    <t>https://www.777homes.com.au/?post_type=property&amp;p=6802&amp;preview=true</t>
+  </si>
+  <si>
+    <t>https://www.777homes.com.au/?post_type=property&amp;p=6804&amp;preview=true</t>
+  </si>
+  <si>
+    <t>https://www.777homes.com.au/?post_type=property&amp;p=6806&amp;preview=true</t>
+  </si>
+  <si>
+    <t>https://www.777homes.com.au/?post_type=property&amp;p=6810&amp;preview=true</t>
+  </si>
+  <si>
+    <t>https://www.777homes.com.au/?post_type=property&amp;p=6812&amp;preview=true</t>
+  </si>
+  <si>
+    <t>https://www.777homes.com.au/?post_type=property&amp;p=6814&amp;preview=true</t>
+  </si>
+  <si>
+    <t>https://www.777homes.com.au/?post_type=property&amp;p=6816&amp;preview=true</t>
+  </si>
+  <si>
+    <t>https://www.777homes.com.au/?post_type=property&amp;p=6818&amp;preview=true</t>
+  </si>
+  <si>
+    <t>https://www.777homes.com.au/?post_type=property&amp;p=6820&amp;preview=true</t>
+  </si>
+  <si>
+    <t>https://www.777homes.com.au/?post_type=property&amp;p=6822&amp;preview=true</t>
+  </si>
+  <si>
+    <t>https://www.777homes.com.au/?post_type=property&amp;p=6824&amp;preview=true</t>
+  </si>
+  <si>
+    <t>https://www.777homes.com.au/?post_type=property&amp;p=6826&amp;preview=true</t>
+  </si>
+  <si>
+    <t>https://www.777homes.com.au/?post_type=property&amp;p=6828&amp;preview=true</t>
+  </si>
+  <si>
+    <t>https://www.777homes.com.au/?post_type=property&amp;p=6830&amp;preview=true</t>
+  </si>
+  <si>
+    <t>https://www.777homes.com.au/?post_type=property&amp;p=6832&amp;preview=true</t>
+  </si>
+  <si>
+    <t>https://www.777homes.com.au/?post_type=property&amp;p=6834&amp;preview=true</t>
+  </si>
+  <si>
+    <t>https://www.777homes.com.au/?post_type=property&amp;p=6836&amp;preview=true</t>
+  </si>
+  <si>
+    <t>https://www.777homes.com.au/property/227-sculthorpe-avenue-whitlam-act-2611/</t>
+  </si>
 </sst>
 </file>
 
@@ -2752,7 +2806,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0"/>
   </numFmts>
-  <fonts count="31">
+  <fonts count="32">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -2928,8 +2982,14 @@
       <color theme="10"/>
       <name val="Arial"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="18">
+  <fills count="19">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -3024,6 +3084,12 @@
         <bgColor indexed="2"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -3038,7 +3104,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="30" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="73">
+  <cellXfs count="75">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -3196,6 +3262,8 @@
     <xf numFmtId="0" fontId="0" fillId="15" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="16" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="17" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="31" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="18" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -3432,11 +3500,11 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:AB85"/>
+  <dimension ref="A1:AB86"/>
   <sheetViews>
-    <sheetView topLeftCell="E1" workbookViewId="0">
+    <sheetView topLeftCell="C1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A56" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F74" sqref="F74"/>
+      <selection pane="bottomLeft" activeCell="G88" sqref="G88"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.3984375" defaultRowHeight="15.75" customHeight="1"/>
@@ -5508,8 +5576,11 @@
       <c r="B68" t="s">
         <v>502</v>
       </c>
+      <c r="C68" s="62" t="s">
+        <v>629</v>
+      </c>
       <c r="D68" s="70" t="s">
-        <v>13</v>
+        <v>450</v>
       </c>
       <c r="G68" t="s">
         <v>9</v>
@@ -5525,8 +5596,11 @@
       <c r="B69" t="s">
         <v>503</v>
       </c>
+      <c r="C69" s="62" t="s">
+        <v>613</v>
+      </c>
       <c r="D69" s="70" t="s">
-        <v>13</v>
+        <v>450</v>
       </c>
       <c r="G69" t="s">
         <v>9</v>
@@ -5542,8 +5616,11 @@
       <c r="B70" t="s">
         <v>504</v>
       </c>
+      <c r="C70" t="s">
+        <v>614</v>
+      </c>
       <c r="D70" s="70" t="s">
-        <v>13</v>
+        <v>450</v>
       </c>
       <c r="G70" t="s">
         <v>9</v>
@@ -5559,8 +5636,11 @@
       <c r="B71" t="s">
         <v>505</v>
       </c>
+      <c r="C71" t="s">
+        <v>615</v>
+      </c>
       <c r="D71" s="70" t="s">
-        <v>13</v>
+        <v>450</v>
       </c>
       <c r="G71" t="s">
         <v>9</v>
@@ -5576,8 +5656,11 @@
       <c r="B72" t="s">
         <v>506</v>
       </c>
+      <c r="C72" t="s">
+        <v>616</v>
+      </c>
       <c r="D72" s="70" t="s">
-        <v>13</v>
+        <v>450</v>
       </c>
       <c r="G72" t="s">
         <v>9</v>
@@ -5593,8 +5676,11 @@
       <c r="B73" t="s">
         <v>507</v>
       </c>
+      <c r="C73" t="s">
+        <v>630</v>
+      </c>
       <c r="D73" s="71" t="s">
-        <v>13</v>
+        <v>450</v>
       </c>
       <c r="G73" t="s">
         <v>17</v>
@@ -5610,8 +5696,11 @@
       <c r="B74" t="s">
         <v>508</v>
       </c>
+      <c r="C74" t="s">
+        <v>617</v>
+      </c>
       <c r="D74" s="71" t="s">
-        <v>13</v>
+        <v>450</v>
       </c>
       <c r="G74" t="s">
         <v>17</v>
@@ -5627,8 +5716,11 @@
       <c r="B75" t="s">
         <v>509</v>
       </c>
+      <c r="C75" t="s">
+        <v>618</v>
+      </c>
       <c r="D75" s="71" t="s">
-        <v>13</v>
+        <v>450</v>
       </c>
       <c r="G75" t="s">
         <v>17</v>
@@ -5644,8 +5736,11 @@
       <c r="B76" t="s">
         <v>510</v>
       </c>
+      <c r="C76" t="s">
+        <v>619</v>
+      </c>
       <c r="D76" s="71" t="s">
-        <v>13</v>
+        <v>450</v>
       </c>
       <c r="G76" t="s">
         <v>17</v>
@@ -5661,8 +5756,11 @@
       <c r="B77" t="s">
         <v>511</v>
       </c>
+      <c r="C77" t="s">
+        <v>620</v>
+      </c>
       <c r="D77" s="71" t="s">
-        <v>13</v>
+        <v>450</v>
       </c>
       <c r="G77" t="s">
         <v>17</v>
@@ -5678,8 +5776,11 @@
       <c r="B78" t="s">
         <v>512</v>
       </c>
+      <c r="C78" t="s">
+        <v>621</v>
+      </c>
       <c r="D78" s="71" t="s">
-        <v>13</v>
+        <v>450</v>
       </c>
       <c r="G78" t="s">
         <v>17</v>
@@ -5695,8 +5796,11 @@
       <c r="B79" t="s">
         <v>513</v>
       </c>
+      <c r="C79" t="s">
+        <v>622</v>
+      </c>
       <c r="D79" s="71" t="s">
-        <v>13</v>
+        <v>450</v>
       </c>
       <c r="G79" t="s">
         <v>17</v>
@@ -5712,8 +5816,11 @@
       <c r="B80" t="s">
         <v>514</v>
       </c>
+      <c r="C80" t="s">
+        <v>623</v>
+      </c>
       <c r="D80" s="71" t="s">
-        <v>13</v>
+        <v>450</v>
       </c>
       <c r="G80" t="s">
         <v>17</v>
@@ -5729,8 +5836,11 @@
       <c r="B81" t="s">
         <v>515</v>
       </c>
+      <c r="C81" t="s">
+        <v>624</v>
+      </c>
       <c r="D81" s="71" t="s">
-        <v>13</v>
+        <v>450</v>
       </c>
       <c r="G81" t="s">
         <v>17</v>
@@ -5746,8 +5856,11 @@
       <c r="B82" t="s">
         <v>516</v>
       </c>
+      <c r="C82" t="s">
+        <v>625</v>
+      </c>
       <c r="D82" s="71" t="s">
-        <v>13</v>
+        <v>450</v>
       </c>
       <c r="G82" t="s">
         <v>17</v>
@@ -5763,8 +5876,11 @@
       <c r="B83" t="s">
         <v>517</v>
       </c>
+      <c r="C83" t="s">
+        <v>626</v>
+      </c>
       <c r="D83" s="71" t="s">
-        <v>13</v>
+        <v>450</v>
       </c>
       <c r="G83" t="s">
         <v>17</v>
@@ -5780,8 +5896,11 @@
       <c r="B84" t="s">
         <v>518</v>
       </c>
+      <c r="C84" t="s">
+        <v>627</v>
+      </c>
       <c r="D84" s="71" t="s">
-        <v>13</v>
+        <v>450</v>
       </c>
       <c r="G84" t="s">
         <v>17</v>
@@ -5797,13 +5916,33 @@
       <c r="B85" t="s">
         <v>519</v>
       </c>
+      <c r="C85" t="s">
+        <v>628</v>
+      </c>
       <c r="D85" s="71" t="s">
-        <v>13</v>
+        <v>450</v>
       </c>
       <c r="G85" t="s">
         <v>17</v>
       </c>
       <c r="H85" t="s">
+        <v>452</v>
+      </c>
+    </row>
+    <row r="86" spans="1:8" ht="15.75" customHeight="1">
+      <c r="A86">
+        <v>85</v>
+      </c>
+      <c r="C86" t="s">
+        <v>631</v>
+      </c>
+      <c r="D86" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="G86" t="s">
+        <v>17</v>
+      </c>
+      <c r="H86" t="s">
         <v>452</v>
       </c>
     </row>
@@ -5875,9 +6014,11 @@
     <hyperlink ref="B54" r:id="rId64" xr:uid="{00000000-0004-0000-0000-00003F000000}"/>
     <hyperlink ref="B42" r:id="rId65" xr:uid="{00000000-0004-0000-0000-000040000000}"/>
     <hyperlink ref="J2" r:id="rId66" xr:uid="{00000000-0004-0000-0000-000041000000}"/>
+    <hyperlink ref="C69" r:id="rId67" xr:uid="{9DAE03A7-93E8-4507-BD6C-AC4013ECD47F}"/>
+    <hyperlink ref="C68" r:id="rId68" xr:uid="{66B9A9CA-DF82-46B6-9C5A-C5709E2FF1AE}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId67"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId69"/>
 </worksheet>
 </file>
 
@@ -5886,10 +6027,10 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:AI85"/>
+  <dimension ref="A1:AI86"/>
   <sheetViews>
-    <sheetView topLeftCell="S64" workbookViewId="0">
-      <selection activeCell="V89" sqref="V89"/>
+    <sheetView tabSelected="1" topLeftCell="A61" workbookViewId="0">
+      <selection activeCell="C54" sqref="C54"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.3984375" defaultRowHeight="15.75" customHeight="1"/>
@@ -10372,12 +10513,12 @@
         <v>17</v>
       </c>
     </row>
-    <row r="68" spans="1:21" ht="12.75">
+    <row r="68" spans="1:21" ht="13.5">
       <c r="A68" t="s">
         <v>522</v>
       </c>
       <c r="B68" t="s">
-        <v>13</v>
+        <v>450</v>
       </c>
       <c r="C68" t="s">
         <v>523</v>
@@ -10386,7 +10527,7 @@
         <v>86</v>
       </c>
       <c r="E68" t="s">
-        <v>524</v>
+        <v>79</v>
       </c>
       <c r="F68" t="s">
         <v>80</v>
@@ -10395,7 +10536,7 @@
         <v>244</v>
       </c>
       <c r="H68" t="s">
-        <v>525</v>
+        <v>524</v>
       </c>
       <c r="I68" t="s">
         <v>221</v>
@@ -10404,7 +10545,7 @@
         <v>222</v>
       </c>
       <c r="L68" t="s">
-        <v>526</v>
+        <v>525</v>
       </c>
       <c r="M68" t="s">
         <v>225</v>
@@ -10422,24 +10563,24 @@
         <v>523</v>
       </c>
       <c r="S68" t="s">
-        <v>527</v>
-      </c>
-      <c r="T68" t="s">
-        <v>222</v>
+        <v>526</v>
+      </c>
+      <c r="T68" s="28" t="s">
+        <v>83</v>
       </c>
       <c r="U68" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="69" spans="1:21" ht="12.75">
+    <row r="69" spans="1:21" ht="13.5">
       <c r="A69" t="s">
+        <v>527</v>
+      </c>
+      <c r="B69" t="s">
+        <v>450</v>
+      </c>
+      <c r="C69" t="s">
         <v>528</v>
-      </c>
-      <c r="B69" t="s">
-        <v>13</v>
-      </c>
-      <c r="C69" t="s">
-        <v>529</v>
       </c>
       <c r="D69" t="s">
         <v>284</v>
@@ -10478,27 +10619,27 @@
         <v>289</v>
       </c>
       <c r="R69" t="s">
+        <v>528</v>
+      </c>
+      <c r="S69" t="s">
         <v>529</v>
       </c>
-      <c r="S69" t="s">
-        <v>530</v>
-      </c>
-      <c r="T69" t="s">
-        <v>222</v>
+      <c r="T69" s="28" t="s">
+        <v>83</v>
       </c>
       <c r="U69" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="70" spans="1:21" ht="12.75">
+    <row r="70" spans="1:21" ht="13.5">
       <c r="A70" t="s">
+        <v>530</v>
+      </c>
+      <c r="B70" t="s">
+        <v>450</v>
+      </c>
+      <c r="C70" t="s">
         <v>531</v>
-      </c>
-      <c r="B70" t="s">
-        <v>13</v>
-      </c>
-      <c r="C70" t="s">
-        <v>532</v>
       </c>
       <c r="D70" t="s">
         <v>86</v>
@@ -10513,16 +10654,16 @@
         <v>120</v>
       </c>
       <c r="H70" t="s">
-        <v>533</v>
+        <v>532</v>
       </c>
       <c r="I70" t="s">
         <v>221</v>
       </c>
       <c r="K70" t="s">
+        <v>533</v>
+      </c>
+      <c r="L70" t="s">
         <v>534</v>
-      </c>
-      <c r="L70" t="s">
-        <v>535</v>
       </c>
       <c r="M70" t="s">
         <v>227</v>
@@ -10537,27 +10678,27 @@
         <v>227</v>
       </c>
       <c r="R70" t="s">
-        <v>532</v>
+        <v>531</v>
       </c>
       <c r="S70" t="s">
-        <v>536</v>
-      </c>
-      <c r="T70" t="s">
-        <v>222</v>
+        <v>535</v>
+      </c>
+      <c r="T70" s="28" t="s">
+        <v>83</v>
       </c>
       <c r="U70" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="71" spans="1:21" ht="12.75">
+    <row r="71" spans="1:21" ht="13.5">
       <c r="A71" t="s">
+        <v>536</v>
+      </c>
+      <c r="B71" t="s">
+        <v>450</v>
+      </c>
+      <c r="C71" t="s">
         <v>537</v>
-      </c>
-      <c r="B71" t="s">
-        <v>13</v>
-      </c>
-      <c r="C71" t="s">
-        <v>538</v>
       </c>
       <c r="D71" t="s">
         <v>86</v>
@@ -10572,7 +10713,7 @@
         <v>126</v>
       </c>
       <c r="H71" t="s">
-        <v>539</v>
+        <v>538</v>
       </c>
       <c r="I71" t="s">
         <v>221</v>
@@ -10581,7 +10722,7 @@
         <v>324</v>
       </c>
       <c r="L71" t="s">
-        <v>540</v>
+        <v>539</v>
       </c>
       <c r="M71" t="s">
         <v>275</v>
@@ -10596,24 +10737,24 @@
         <v>227</v>
       </c>
       <c r="R71" t="s">
-        <v>538</v>
+        <v>537</v>
       </c>
       <c r="S71" t="s">
-        <v>541</v>
-      </c>
-      <c r="T71" t="s">
-        <v>222</v>
+        <v>540</v>
+      </c>
+      <c r="T71" s="28" t="s">
+        <v>83</v>
       </c>
       <c r="U71" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="72" spans="1:21" ht="12.75">
+    <row r="72" spans="1:21" ht="13.5">
       <c r="A72" t="s">
-        <v>542</v>
+        <v>541</v>
       </c>
       <c r="B72" t="s">
-        <v>13</v>
+        <v>450</v>
       </c>
       <c r="C72" t="s">
         <v>101</v>
@@ -10631,7 +10772,7 @@
         <v>104</v>
       </c>
       <c r="H72" t="s">
-        <v>543</v>
+        <v>542</v>
       </c>
       <c r="I72" t="s">
         <v>221</v>
@@ -10658,21 +10799,21 @@
         <v>234</v>
       </c>
       <c r="S72" t="s">
-        <v>544</v>
-      </c>
-      <c r="T72" t="s">
-        <v>222</v>
+        <v>543</v>
+      </c>
+      <c r="T72" s="28" t="s">
+        <v>83</v>
       </c>
       <c r="U72" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="73" spans="1:21" ht="12.75">
+    <row r="73" spans="1:21" ht="13.5">
       <c r="A73" t="s">
-        <v>545</v>
+        <v>544</v>
       </c>
       <c r="B73" t="s">
-        <v>13</v>
+        <v>450</v>
       </c>
       <c r="C73" t="s">
         <v>91</v>
@@ -10681,7 +10822,7 @@
         <v>86</v>
       </c>
       <c r="E73" t="s">
-        <v>524</v>
+        <v>79</v>
       </c>
       <c r="F73" t="s">
         <v>80</v>
@@ -10690,7 +10831,7 @@
         <v>87</v>
       </c>
       <c r="H73" t="s">
-        <v>546</v>
+        <v>545</v>
       </c>
       <c r="I73" t="s">
         <v>221</v>
@@ -10699,7 +10840,7 @@
         <v>471</v>
       </c>
       <c r="L73" t="s">
-        <v>547</v>
+        <v>546</v>
       </c>
       <c r="M73" t="s">
         <v>225</v>
@@ -10717,24 +10858,24 @@
         <v>240</v>
       </c>
       <c r="S73" t="s">
-        <v>548</v>
-      </c>
-      <c r="T73" t="s">
-        <v>222</v>
+        <v>547</v>
+      </c>
+      <c r="T73" s="28" t="s">
+        <v>108</v>
       </c>
       <c r="U73" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="74" spans="1:21" ht="12.75">
+    <row r="74" spans="1:21" ht="13.5">
       <c r="A74" t="s">
+        <v>548</v>
+      </c>
+      <c r="B74" t="s">
+        <v>450</v>
+      </c>
+      <c r="C74" t="s">
         <v>549</v>
-      </c>
-      <c r="B74" t="s">
-        <v>13</v>
-      </c>
-      <c r="C74" t="s">
-        <v>550</v>
       </c>
       <c r="D74" t="s">
         <v>284</v>
@@ -10749,16 +10890,16 @@
         <v>244</v>
       </c>
       <c r="H74" t="s">
-        <v>551</v>
+        <v>550</v>
       </c>
       <c r="I74" t="s">
         <v>221</v>
       </c>
       <c r="K74" t="s">
+        <v>551</v>
+      </c>
+      <c r="L74" t="s">
         <v>552</v>
-      </c>
-      <c r="L74" t="s">
-        <v>553</v>
       </c>
       <c r="M74" t="s">
         <v>224</v>
@@ -10773,27 +10914,27 @@
         <v>222</v>
       </c>
       <c r="R74" t="s">
-        <v>550</v>
+        <v>549</v>
       </c>
       <c r="S74" t="s">
-        <v>554</v>
-      </c>
-      <c r="T74" t="s">
-        <v>222</v>
+        <v>553</v>
+      </c>
+      <c r="T74" s="28" t="s">
+        <v>108</v>
       </c>
       <c r="U74" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="75" spans="1:21" ht="12.75">
+    <row r="75" spans="1:21" ht="13.5">
       <c r="A75" t="s">
+        <v>554</v>
+      </c>
+      <c r="B75" t="s">
+        <v>450</v>
+      </c>
+      <c r="C75" t="s">
         <v>555</v>
-      </c>
-      <c r="B75" t="s">
-        <v>13</v>
-      </c>
-      <c r="C75" t="s">
-        <v>556</v>
       </c>
       <c r="D75" t="s">
         <v>86</v>
@@ -10808,16 +10949,16 @@
         <v>259</v>
       </c>
       <c r="H75" t="s">
-        <v>557</v>
+        <v>556</v>
       </c>
       <c r="I75" t="s">
         <v>221</v>
       </c>
       <c r="K75" t="s">
+        <v>557</v>
+      </c>
+      <c r="L75" t="s">
         <v>558</v>
-      </c>
-      <c r="L75" t="s">
-        <v>559</v>
       </c>
       <c r="M75" t="s">
         <v>225</v>
@@ -10832,24 +10973,24 @@
         <v>227</v>
       </c>
       <c r="R75" t="s">
-        <v>556</v>
+        <v>555</v>
       </c>
       <c r="S75" t="s">
-        <v>560</v>
-      </c>
-      <c r="T75" t="s">
-        <v>222</v>
+        <v>559</v>
+      </c>
+      <c r="T75" s="28" t="s">
+        <v>108</v>
       </c>
       <c r="U75" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="76" spans="1:21" ht="12.75">
+    <row r="76" spans="1:21" ht="13.5">
       <c r="A76" t="s">
-        <v>561</v>
+        <v>560</v>
       </c>
       <c r="B76" t="s">
-        <v>13</v>
+        <v>450</v>
       </c>
       <c r="C76" t="s">
         <v>91</v>
@@ -10867,16 +11008,16 @@
         <v>87</v>
       </c>
       <c r="H76" t="s">
-        <v>562</v>
+        <v>561</v>
       </c>
       <c r="I76" t="s">
         <v>221</v>
       </c>
       <c r="K76" t="s">
+        <v>562</v>
+      </c>
+      <c r="L76" t="s">
         <v>563</v>
-      </c>
-      <c r="L76" t="s">
-        <v>564</v>
       </c>
       <c r="M76" t="s">
         <v>275</v>
@@ -10894,24 +11035,24 @@
         <v>240</v>
       </c>
       <c r="S76" t="s">
-        <v>565</v>
-      </c>
-      <c r="T76" t="s">
-        <v>222</v>
+        <v>564</v>
+      </c>
+      <c r="T76" s="28" t="s">
+        <v>108</v>
       </c>
       <c r="U76" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="77" spans="1:21" ht="12.75">
+    <row r="77" spans="1:21" ht="13.5">
       <c r="A77" t="s">
+        <v>565</v>
+      </c>
+      <c r="B77" t="s">
+        <v>450</v>
+      </c>
+      <c r="C77" t="s">
         <v>566</v>
-      </c>
-      <c r="B77" t="s">
-        <v>13</v>
-      </c>
-      <c r="C77" t="s">
-        <v>567</v>
       </c>
       <c r="D77" t="s">
         <v>284</v>
@@ -10923,19 +11064,19 @@
         <v>230</v>
       </c>
       <c r="G77" t="s">
+        <v>567</v>
+      </c>
+      <c r="H77" t="s">
         <v>568</v>
-      </c>
-      <c r="H77" t="s">
-        <v>569</v>
       </c>
       <c r="I77" t="s">
         <v>221</v>
       </c>
       <c r="K77" t="s">
+        <v>569</v>
+      </c>
+      <c r="L77" t="s">
         <v>570</v>
-      </c>
-      <c r="L77" t="s">
-        <v>571</v>
       </c>
       <c r="M77" t="s">
         <v>227</v>
@@ -10950,27 +11091,27 @@
         <v>289</v>
       </c>
       <c r="R77" t="s">
-        <v>567</v>
+        <v>566</v>
       </c>
       <c r="S77" t="s">
-        <v>572</v>
-      </c>
-      <c r="T77" t="s">
-        <v>222</v>
+        <v>571</v>
+      </c>
+      <c r="T77" s="28" t="s">
+        <v>108</v>
       </c>
       <c r="U77" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="78" spans="1:21" ht="12.75">
+    <row r="78" spans="1:21" ht="13.5">
       <c r="A78" t="s">
+        <v>572</v>
+      </c>
+      <c r="B78" t="s">
+        <v>450</v>
+      </c>
+      <c r="C78" t="s">
         <v>573</v>
-      </c>
-      <c r="B78" t="s">
-        <v>13</v>
-      </c>
-      <c r="C78" t="s">
-        <v>574</v>
       </c>
       <c r="D78" t="s">
         <v>86</v>
@@ -10985,7 +11126,7 @@
         <v>104</v>
       </c>
       <c r="H78" t="s">
-        <v>575</v>
+        <v>574</v>
       </c>
       <c r="I78" t="s">
         <v>221</v>
@@ -11009,27 +11150,27 @@
         <v>227</v>
       </c>
       <c r="R78" t="s">
-        <v>574</v>
+        <v>573</v>
       </c>
       <c r="S78" t="s">
-        <v>576</v>
-      </c>
-      <c r="T78" t="s">
-        <v>222</v>
+        <v>575</v>
+      </c>
+      <c r="T78" s="28" t="s">
+        <v>108</v>
       </c>
       <c r="U78" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="79" spans="1:21" ht="12.75">
+    <row r="79" spans="1:21" ht="13.5">
       <c r="A79" t="s">
+        <v>576</v>
+      </c>
+      <c r="B79" t="s">
+        <v>450</v>
+      </c>
+      <c r="C79" t="s">
         <v>577</v>
-      </c>
-      <c r="B79" t="s">
-        <v>13</v>
-      </c>
-      <c r="C79" t="s">
-        <v>578</v>
       </c>
       <c r="D79" t="s">
         <v>78</v>
@@ -11044,16 +11185,16 @@
         <v>230</v>
       </c>
       <c r="H79" t="s">
-        <v>579</v>
+        <v>578</v>
       </c>
       <c r="I79" t="s">
         <v>221</v>
       </c>
       <c r="K79" t="s">
+        <v>579</v>
+      </c>
+      <c r="L79" t="s">
         <v>580</v>
-      </c>
-      <c r="L79" t="s">
-        <v>581</v>
       </c>
       <c r="M79" t="s">
         <v>227</v>
@@ -11068,27 +11209,27 @@
         <v>222</v>
       </c>
       <c r="R79" t="s">
-        <v>578</v>
+        <v>577</v>
       </c>
       <c r="S79" t="s">
-        <v>582</v>
-      </c>
-      <c r="T79" t="s">
-        <v>222</v>
+        <v>581</v>
+      </c>
+      <c r="T79" s="28" t="s">
+        <v>108</v>
       </c>
       <c r="U79" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="80" spans="1:21" ht="12.75">
+    <row r="80" spans="1:21" ht="13.5">
       <c r="A80" t="s">
+        <v>582</v>
+      </c>
+      <c r="B80" t="s">
+        <v>450</v>
+      </c>
+      <c r="C80" t="s">
         <v>583</v>
-      </c>
-      <c r="B80" t="s">
-        <v>13</v>
-      </c>
-      <c r="C80" t="s">
-        <v>584</v>
       </c>
       <c r="D80" t="s">
         <v>284</v>
@@ -11103,16 +11244,16 @@
         <v>271</v>
       </c>
       <c r="H80" t="s">
-        <v>585</v>
+        <v>584</v>
       </c>
       <c r="I80" t="s">
         <v>221</v>
       </c>
       <c r="K80" t="s">
+        <v>585</v>
+      </c>
+      <c r="L80" t="s">
         <v>586</v>
-      </c>
-      <c r="L80" t="s">
-        <v>587</v>
       </c>
       <c r="M80" t="s">
         <v>225</v>
@@ -11127,24 +11268,24 @@
         <v>227</v>
       </c>
       <c r="R80" t="s">
+        <v>587</v>
+      </c>
+      <c r="S80" t="s">
         <v>588</v>
       </c>
-      <c r="S80" t="s">
-        <v>589</v>
-      </c>
-      <c r="T80" t="s">
-        <v>222</v>
+      <c r="T80" s="28" t="s">
+        <v>108</v>
       </c>
       <c r="U80" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="81" spans="1:21" ht="12.75">
+    <row r="81" spans="1:21" ht="13.5">
       <c r="A81" t="s">
-        <v>590</v>
+        <v>589</v>
       </c>
       <c r="B81" t="s">
-        <v>13</v>
+        <v>450</v>
       </c>
       <c r="C81" t="s">
         <v>91</v>
@@ -11162,16 +11303,16 @@
         <v>87</v>
       </c>
       <c r="H81" t="s">
-        <v>591</v>
+        <v>590</v>
       </c>
       <c r="I81" t="s">
         <v>221</v>
       </c>
       <c r="K81" t="s">
+        <v>591</v>
+      </c>
+      <c r="L81" t="s">
         <v>592</v>
-      </c>
-      <c r="L81" t="s">
-        <v>593</v>
       </c>
       <c r="M81" t="s">
         <v>275</v>
@@ -11189,21 +11330,21 @@
         <v>240</v>
       </c>
       <c r="S81" t="s">
-        <v>594</v>
-      </c>
-      <c r="T81" t="s">
-        <v>222</v>
+        <v>593</v>
+      </c>
+      <c r="T81" s="28" t="s">
+        <v>108</v>
       </c>
       <c r="U81" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="82" spans="1:21" ht="12.75">
+    <row r="82" spans="1:21" ht="13.5">
       <c r="A82" t="s">
-        <v>595</v>
+        <v>594</v>
       </c>
       <c r="B82" t="s">
-        <v>13</v>
+        <v>450</v>
       </c>
       <c r="C82" t="s">
         <v>130</v>
@@ -11221,16 +11362,16 @@
         <v>132</v>
       </c>
       <c r="H82" t="s">
-        <v>596</v>
+        <v>595</v>
       </c>
       <c r="I82" t="s">
         <v>221</v>
       </c>
       <c r="K82" t="s">
+        <v>596</v>
+      </c>
+      <c r="L82" t="s">
         <v>597</v>
-      </c>
-      <c r="L82" t="s">
-        <v>598</v>
       </c>
       <c r="M82" t="s">
         <v>224</v>
@@ -11248,21 +11389,21 @@
         <v>280</v>
       </c>
       <c r="S82" t="s">
-        <v>599</v>
-      </c>
-      <c r="T82" t="s">
-        <v>222</v>
+        <v>598</v>
+      </c>
+      <c r="T82" s="28" t="s">
+        <v>108</v>
       </c>
       <c r="U82" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="83" spans="1:21" ht="12.75">
+    <row r="83" spans="1:21" ht="13.5">
       <c r="A83" t="s">
-        <v>600</v>
+        <v>599</v>
       </c>
       <c r="B83" t="s">
-        <v>13</v>
+        <v>450</v>
       </c>
       <c r="C83" t="s">
         <v>101</v>
@@ -11289,7 +11430,7 @@
         <v>475</v>
       </c>
       <c r="L83" t="s">
-        <v>601</v>
+        <v>600</v>
       </c>
       <c r="M83" t="s">
         <v>224</v>
@@ -11307,21 +11448,21 @@
         <v>234</v>
       </c>
       <c r="S83" t="s">
-        <v>602</v>
-      </c>
-      <c r="T83" t="s">
-        <v>222</v>
+        <v>601</v>
+      </c>
+      <c r="T83" s="28" t="s">
+        <v>108</v>
       </c>
       <c r="U83" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="84" spans="1:21" ht="12.75">
+    <row r="84" spans="1:21" ht="13.5">
       <c r="A84" t="s">
-        <v>603</v>
+        <v>602</v>
       </c>
       <c r="B84" t="s">
-        <v>13</v>
+        <v>450</v>
       </c>
       <c r="C84" t="s">
         <v>118</v>
@@ -11339,16 +11480,16 @@
         <v>120</v>
       </c>
       <c r="H84" t="s">
-        <v>604</v>
+        <v>603</v>
       </c>
       <c r="I84" t="s">
         <v>221</v>
       </c>
       <c r="K84" t="s">
+        <v>585</v>
+      </c>
+      <c r="L84" t="s">
         <v>586</v>
-      </c>
-      <c r="L84" t="s">
-        <v>587</v>
       </c>
       <c r="M84" t="s">
         <v>224</v>
@@ -11363,27 +11504,27 @@
         <v>227</v>
       </c>
       <c r="R84" t="s">
+        <v>604</v>
+      </c>
+      <c r="S84" t="s">
         <v>605</v>
       </c>
-      <c r="S84" t="s">
-        <v>606</v>
-      </c>
-      <c r="T84" t="s">
-        <v>222</v>
+      <c r="T84" s="28" t="s">
+        <v>108</v>
       </c>
       <c r="U84" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="85" spans="1:21" ht="12.75">
+    <row r="85" spans="1:21" ht="13.5">
       <c r="A85" t="s">
+        <v>606</v>
+      </c>
+      <c r="B85" t="s">
+        <v>450</v>
+      </c>
+      <c r="C85" t="s">
         <v>607</v>
-      </c>
-      <c r="B85" t="s">
-        <v>13</v>
-      </c>
-      <c r="C85" t="s">
-        <v>608</v>
       </c>
       <c r="D85" t="s">
         <v>78</v>
@@ -11395,19 +11536,19 @@
         <v>520</v>
       </c>
       <c r="G85" t="s">
+        <v>608</v>
+      </c>
+      <c r="H85" t="s">
         <v>609</v>
-      </c>
-      <c r="H85" t="s">
-        <v>610</v>
       </c>
       <c r="I85" t="s">
         <v>221</v>
       </c>
       <c r="K85" t="s">
+        <v>610</v>
+      </c>
+      <c r="L85" t="s">
         <v>611</v>
-      </c>
-      <c r="L85" t="s">
-        <v>612</v>
       </c>
       <c r="M85" t="s">
         <v>289</v>
@@ -11422,20 +11563,57 @@
         <v>222</v>
       </c>
       <c r="R85" t="s">
-        <v>608</v>
+        <v>607</v>
       </c>
       <c r="S85" t="s">
-        <v>613</v>
-      </c>
-      <c r="T85" t="s">
-        <v>222</v>
+        <v>612</v>
+      </c>
+      <c r="T85" s="28" t="s">
+        <v>108</v>
       </c>
       <c r="U85" t="s">
         <v>17</v>
       </c>
     </row>
+    <row r="86" spans="1:21" ht="15.75" customHeight="1">
+      <c r="A86">
+        <v>85</v>
+      </c>
+      <c r="B86" t="s">
+        <v>7</v>
+      </c>
+      <c r="C86" t="s">
+        <v>555</v>
+      </c>
+      <c r="D86" s="73" t="s">
+        <v>86</v>
+      </c>
+      <c r="E86" s="73" t="s">
+        <v>79</v>
+      </c>
+      <c r="F86" s="74"/>
+      <c r="G86" s="74"/>
+      <c r="H86" s="74"/>
+      <c r="I86" s="74"/>
+      <c r="J86" s="74"/>
+      <c r="K86" s="74"/>
+      <c r="L86" s="74"/>
+      <c r="M86" s="74"/>
+      <c r="N86" s="74"/>
+      <c r="O86" s="74"/>
+      <c r="P86" s="74"/>
+      <c r="Q86" s="74"/>
+      <c r="R86" s="74"/>
+      <c r="S86" s="74"/>
+      <c r="T86" s="74"/>
+      <c r="U86" s="74"/>
+    </row>
   </sheetData>
   <customSheetViews>
+    <customSheetView guid="{C25CEB9E-BEC1-4982-90C4-50C84EE1B82A}" filter="1" showAutoFilter="1">
+      <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+      <autoFilter ref="A1:AD33" xr:uid="{00000000-0000-0000-0000-000000000000}"/>
+    </customSheetView>
     <customSheetView guid="{A7754112-A52F-4ABC-8778-92F04773E53C}" filter="1" showAutoFilter="1">
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <autoFilter ref="A1:AD33" xr:uid="{00000000-0000-0000-0000-000000000000}">
@@ -11445,10 +11623,6 @@
           </filters>
         </filterColumn>
       </autoFilter>
-    </customSheetView>
-    <customSheetView guid="{C25CEB9E-BEC1-4982-90C4-50C84EE1B82A}" filter="1" showAutoFilter="1">
-      <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-      <autoFilter ref="A1:AD33" xr:uid="{00000000-0000-0000-0000-000000000000}"/>
     </customSheetView>
   </customSheetViews>
   <conditionalFormatting sqref="A1:AI1">
@@ -11656,7 +11830,7 @@
   </sheetPr>
   <dimension ref="A1:Z6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="C6" sqref="C6"/>
     </sheetView>

</xml_diff>

<commit_message>
Manual check and updated -24/05/2021
</commit_message>
<xml_diff>
--- a/src/main/resources/InputTestdata/Listing details.xlsx
+++ b/src/main/resources/InputTestdata/Listing details.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Athavan\git\777Homes-business\src\main\resources\InputTestdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{30C4D70A-DB1D-4B22-AB91-82331DAFC9B7}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A1A5BEE4-3CB7-4BFD-9E99-B5BE3ADE53D5}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="20715" windowHeight="13276" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -21,19 +21,30 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Backlog!$A$1:$AB$52</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Listing!#REF!</definedName>
-    <definedName name="Z_A7754112_A52F_4ABC_8778_92F04773E53C_.wvu.FilterData" localSheetId="1" hidden="1">Listing!$A$1:$AE$32</definedName>
-    <definedName name="Z_C25CEB9E_BEC1_4982_90C4_50C84EE1B82A_.wvu.FilterData" localSheetId="1" hidden="1">Listing!$A$1:$AE$32</definedName>
+    <definedName name="Z_A7754112_A52F_4ABC_8778_92F04773E53C_.wvu.FilterData" localSheetId="1" hidden="1">Listing!$A$1:$AG$32</definedName>
+    <definedName name="Z_C25CEB9E_BEC1_4982_90C4_50C84EE1B82A_.wvu.FilterData" localSheetId="1" hidden="1">Listing!$A$1:$AG$32</definedName>
   </definedNames>
-  <calcPr calcId="0"/>
+  <calcPr calcId="191029"/>
   <customWorkbookViews>
+    <customWorkbookView name="Filter 1" guid="{A7754112-A52F-4ABC-8778-92F04773E53C}" maximized="1" windowWidth="0" windowHeight="0" activeSheetId="0"/>
     <customWorkbookView name="Filter 2" guid="{C25CEB9E-BEC1-4982-90C4-50C84EE1B82A}" maximized="1" windowWidth="0" windowHeight="0" activeSheetId="0"/>
-    <customWorkbookView name="Filter 1" guid="{A7754112-A52F-4ABC-8778-92F04773E53C}" maximized="1" windowWidth="0" windowHeight="0" activeSheetId="0"/>
   </customWorkbookViews>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1967" uniqueCount="632">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1986" uniqueCount="634">
   <si>
     <t>ID</t>
   </si>
@@ -2254,9 +2265,6 @@
     <t>https://www.allhomes.com.au/unit-22-22-henry-kendall-street-franklin-act-2913</t>
   </si>
   <si>
-    <t>https://www.allhomes.com.au/227-sculthorpe-avenue-whitlam-act-2611</t>
-  </si>
-  <si>
     <t>https://www.allhomes.com.au/taylor-act-2913?tid=179140230</t>
   </si>
   <si>
@@ -2343,14 +2351,6 @@
     <t>9/4 Lawrenson Circuit, Jacka ACT 2914</t>
   </si>
   <si>
-    <t>A beautiful family home close to Amaroo school &amp; shops
-This brilliantly designed 3-bedroom single storey home is just the ticket for the astute buyers for their home or investment. It has individuality, space and style.
-The residence features a modern kitchen with stone bench-top and ample cupboard space. Great sized living space and a splendid layout offer up a practical and light filled pleasant place to live and entertain.
-Central heating and Energy Efficiency Rating of 6.0 means that you will be cozy during the extreme Canberra weather.
-Features:
-Property information</t>
-  </si>
-  <si>
     <t>69</t>
   </si>
   <si>
@@ -2417,10 +2417,6 @@
   </si>
   <si>
     <t>Block/House: 450/ 220</t>
-  </si>
-  <si>
-    <t>New Door Properties is proud to present you this modern house and land package.
-This sleek single-level home promotes easy family living and entertaining on a block of 450 m2(approx.). Immaculate from start to finish, enjoy a modern, cleverly considered floorplan hosting a formal lounge room and an open plan family and meals area leading out to the undercover alfresco entertaining area combining indoor/outdoor living.</t>
   </si>
   <si>
     <t>72</t>
@@ -2566,10 +2562,6 @@
     <t>Block/House: 362/ 190</t>
   </si>
   <si>
-    <t>Opens to be held at Pro Hart Ave, Block 17 Section 23, Ginninderry Residences, Strathnairn.  (Opposite the Land sales office)
-Completion estimated to be last quarter of 2021.</t>
-  </si>
-  <si>
     <t>78</t>
   </si>
   <si>
@@ -2796,7 +2788,100 @@
     <t>https://www.777homes.com.au/?post_type=property&amp;p=6836&amp;preview=true</t>
   </si>
   <si>
-    <t>https://www.777homes.com.au/property/227-sculthorpe-avenue-whitlam-act-2611/</t>
+    <t>https://www.allhomes.com.au/sculthorpe-avenue-whitlam-act-2611?tid=179490568</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Checked by </t>
+  </si>
+  <si>
+    <t>Checked by Date</t>
+  </si>
+  <si>
+    <t>Athavan</t>
+  </si>
+  <si>
+    <t>Start Living Your Dream! Last 2 H&amp;L Packages left!
+Opens to be held at Pro Hart Ave, Block 17 Section 23, Ginninderry Residences, Strathnairn.  (Opposite the Land sales office)
+Completion estimated to be last quarter of 2021.
+Affordable luxury is now within your reach. Located in the fast growing Strathnairn, this 362 sqm block will surely make your dreams come true. This property is also in prime location, situated closely to the Community Recreation Park, a golf course, schools and shopping centres, this surely is the perfect place to build your dream home.
+This house boast a beautiful floorplan with four well-sized bedrooms, two bathrooms, a magnificent kitchen and living room with a lock up garage space, and an open carport. A modern and well-designed home that has a striking abundance of space and light, perfect for gorgeous family or astute investment. One lock-up garage for the everyday automobile and one long car spot perfect for that holidaying caravan or boat.
+Features Include:
+- Stone bench throughout kitchens and walk-in pantry
+- Stainless steel appliances in both kitchens
+- Floor to Ceiling tiles in all bathrooms
+- 2.55m Ceiling in main residence
+- Walk-in pantry
+- Large master and ensuite
+- Walk in robes to master suite
+- Double garage with internal access to rear
+- Plumbed fridge connections
+- Few minutes to local shopping centre (KIPPAX)
+- 15 minutes to the City
+Standard progress payments, on a split contract. Save on Stamp Duty if eligible. 
+*Picture is inspiration and/or artist impression. Full quote to be provided upon non-obligatory discussion.</t>
+  </si>
+  <si>
+    <t>HOME SWEET HOME
+A beautiful family home close to Amaroo school &amp; shops
+This brilliantly designed 3-bedroom single storey home is just the ticket for the astute buyers for their home or investment. It has individuality, space and style.
+The residence features a modern kitchen with stone bench-top and ample cupboard space. Great sized living space and a splendid layout offer up a practical and light filled pleasant place to live and entertain.
+Central heating and Energy Efficiency Rating of 6.0 means that you will be cozy during the extreme Canberra weather.
+Features:
+Three Bedrooms
+Low maintenance backyard with ample space for kids.
+Close walk to Amaroo school which is one of the great public schools in ACT
+Close walk to Amaroo Village Shops which includes Coles supermarket, Gym, Coffee Guru, Asian / Indian Grocery Store
+Spacious open-plan living and dining
+Ducted Gas heating
+Split cooling system
+5 KW solar system
+Separate laundry
+Stone bench-tops
+Bosch Dishwasher
+Alarm system
+Large master bedroom, ensuite and mirrored built in robe
+Generous 2nd and 3rd bedroom with built in robe
+Single garage with remote control access
+Extra storage and concrete around
+Extra two car parking in front of the house
+NBN
+Property information
+Rates : $428 quarterly (approx.)
+Body Corporate : $507 quarterly (approx.)
+EER 6.0</t>
+  </si>
+  <si>
+    <t>House and Land Package
+New Door Properties is proud to present you this modern house and land package.
+This sleek single-level home promotes easy family living and entertaining on a block of 450 m2(approx.). Immaculate from start to finish, enjoy a modern, cleverly considered floorplan hosting a formal lounge room and an open plan family and meals area leading out to the undercover alfresco entertaining area combining indoor/outdoor living.   
+The modern kitchen boasts quality stainless steel appliances, 40 mm stone benchtops with waterfalls, walk in pantry and plenty of storage. Other features include High ceilings, Reverse-cycle ducted air-conditioning and a low maintenance yard.
+Features
+• 4 bedrooms
+• 2 bathrooms
+• 2 garage
+• Spacious family &amp; dining
+• 2.55 high ceilings
+• Modern Kitchen with glass splashback
+• Stone benchtops with waterfalls 
+• Bosch  cooktop, oven and ducted range-hood
+• Bosch 600 semi-Integrated dishwasher
+• Built in Microwave
+• Walk in Pantry
+• Ducted reverse cycle heating and cooling with zones
+• Full length tiles and tub in main bathroom
+• LED lights throughout the house
+• Video intercom
+• Spacious laundry 
+• Rain water tank
+* Photos from the prevoius project of the builder.
+Property information
+Land Size : 450m2 (approx..)
+Living : 172 m2 (approx..)
+Garage : 38 m2 (approx..)
+Alfresco : 8 m2 (approx..)
+Porch : 2 m2 (approx..)
+Total living : 220 m2 ( approx..)
+EER 6 stars</t>
   </si>
 </sst>
 </file>
@@ -2806,7 +2891,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0"/>
   </numFmts>
-  <fonts count="32">
+  <fonts count="31">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -2982,14 +3067,8 @@
       <color theme="10"/>
       <name val="Arial"/>
     </font>
-    <font>
-      <sz val="10"/>
-      <color rgb="FF000000"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
   </fonts>
-  <fills count="19">
+  <fills count="16">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -3074,22 +3153,6 @@
         <bgColor indexed="2"/>
       </patternFill>
     </fill>
-    <fill>
-      <patternFill patternType="mediumGray">
-        <bgColor indexed="2"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="mediumGray">
-        <bgColor indexed="2"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -3104,7 +3167,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="30" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="75">
+  <cellXfs count="72">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -3260,10 +3323,9 @@
     <xf numFmtId="0" fontId="0" fillId="13" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="14" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="15" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="16" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="17" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="31" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="18" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="14" fontId="18" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -3500,11 +3562,11 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:AB86"/>
+  <dimension ref="A1:AB85"/>
   <sheetViews>
-    <sheetView topLeftCell="C1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A56" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G88" sqref="G88"/>
+      <selection pane="bottomLeft" activeCell="C75" sqref="C75"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.3984375" defaultRowHeight="15.75" customHeight="1"/>
@@ -5569,103 +5631,118 @@
         <v>452</v>
       </c>
     </row>
-    <row r="68" spans="1:8" ht="12.75">
-      <c r="A68">
+    <row r="68" spans="1:8" s="4" customFormat="1" ht="12.75">
+      <c r="A68" s="4">
         <v>67</v>
       </c>
-      <c r="B68" t="s">
+      <c r="B68" s="4" t="s">
         <v>502</v>
       </c>
-      <c r="C68" s="62" t="s">
-        <v>629</v>
-      </c>
-      <c r="D68" s="70" t="s">
-        <v>450</v>
-      </c>
-      <c r="G68" t="s">
+      <c r="C68" s="4" t="s">
+        <v>625</v>
+      </c>
+      <c r="D68" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="F68" s="4" t="s">
+        <v>83</v>
+      </c>
+      <c r="G68" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="H68" t="s">
+      <c r="H68" s="4" t="s">
         <v>451</v>
       </c>
     </row>
-    <row r="69" spans="1:8" ht="12.75">
-      <c r="A69">
+    <row r="69" spans="1:8" s="4" customFormat="1" ht="12.75">
+      <c r="A69" s="4">
         <v>68</v>
       </c>
-      <c r="B69" t="s">
+      <c r="B69" s="4" t="s">
         <v>503</v>
       </c>
-      <c r="C69" s="62" t="s">
-        <v>613</v>
-      </c>
-      <c r="D69" s="70" t="s">
-        <v>450</v>
-      </c>
-      <c r="G69" t="s">
+      <c r="C69" s="4" t="s">
+        <v>609</v>
+      </c>
+      <c r="D69" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="F69" s="4" t="s">
+        <v>83</v>
+      </c>
+      <c r="G69" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="H69" t="s">
+      <c r="H69" s="4" t="s">
         <v>451</v>
       </c>
     </row>
-    <row r="70" spans="1:8" ht="12.75">
-      <c r="A70">
+    <row r="70" spans="1:8" s="4" customFormat="1" ht="12.75">
+      <c r="A70" s="4">
         <v>69</v>
       </c>
-      <c r="B70" t="s">
+      <c r="B70" s="4" t="s">
         <v>504</v>
       </c>
-      <c r="C70" t="s">
-        <v>614</v>
-      </c>
-      <c r="D70" s="70" t="s">
-        <v>450</v>
-      </c>
-      <c r="G70" t="s">
+      <c r="C70" s="4" t="s">
+        <v>610</v>
+      </c>
+      <c r="D70" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="F70" s="4" t="s">
+        <v>83</v>
+      </c>
+      <c r="G70" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="H70" t="s">
+      <c r="H70" s="4" t="s">
         <v>451</v>
       </c>
     </row>
-    <row r="71" spans="1:8" ht="12.75">
-      <c r="A71">
+    <row r="71" spans="1:8" s="4" customFormat="1" ht="12.75">
+      <c r="A71" s="4">
         <v>70</v>
       </c>
-      <c r="B71" t="s">
+      <c r="B71" s="4" t="s">
         <v>505</v>
       </c>
-      <c r="C71" t="s">
-        <v>615</v>
-      </c>
-      <c r="D71" s="70" t="s">
-        <v>450</v>
-      </c>
-      <c r="G71" t="s">
+      <c r="C71" s="4" t="s">
+        <v>611</v>
+      </c>
+      <c r="D71" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="F71" s="4" t="s">
+        <v>83</v>
+      </c>
+      <c r="G71" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="H71" t="s">
+      <c r="H71" s="4" t="s">
         <v>451</v>
       </c>
     </row>
-    <row r="72" spans="1:8" ht="12.75">
-      <c r="A72">
+    <row r="72" spans="1:8" s="4" customFormat="1" ht="12.75">
+      <c r="A72" s="4">
         <v>71</v>
       </c>
-      <c r="B72" t="s">
+      <c r="B72" s="4" t="s">
         <v>506</v>
       </c>
-      <c r="C72" t="s">
-        <v>616</v>
-      </c>
-      <c r="D72" s="70" t="s">
-        <v>450</v>
-      </c>
-      <c r="G72" t="s">
+      <c r="C72" s="4" t="s">
+        <v>612</v>
+      </c>
+      <c r="D72" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="F72" s="4" t="s">
+        <v>83</v>
+      </c>
+      <c r="G72" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="H72" t="s">
+      <c r="H72" s="4" t="s">
         <v>451</v>
       </c>
     </row>
@@ -5676,11 +5753,14 @@
       <c r="B73" t="s">
         <v>507</v>
       </c>
-      <c r="C73" t="s">
-        <v>630</v>
-      </c>
-      <c r="D73" s="71" t="s">
-        <v>450</v>
+      <c r="C73" s="62" t="s">
+        <v>626</v>
+      </c>
+      <c r="D73" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="F73" s="4" t="s">
+        <v>108</v>
       </c>
       <c r="G73" t="s">
         <v>17</v>
@@ -5697,10 +5777,13 @@
         <v>508</v>
       </c>
       <c r="C74" t="s">
-        <v>617</v>
-      </c>
-      <c r="D74" s="71" t="s">
-        <v>450</v>
+        <v>613</v>
+      </c>
+      <c r="D74" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="F74" s="4" t="s">
+        <v>108</v>
       </c>
       <c r="G74" t="s">
         <v>17</v>
@@ -5709,23 +5792,26 @@
         <v>452</v>
       </c>
     </row>
-    <row r="75" spans="1:8" ht="12.75">
-      <c r="A75">
+    <row r="75" spans="1:8" s="4" customFormat="1" ht="12.75">
+      <c r="A75" s="4">
         <v>74</v>
       </c>
-      <c r="B75" t="s">
-        <v>509</v>
-      </c>
-      <c r="C75" t="s">
-        <v>618</v>
-      </c>
-      <c r="D75" s="71" t="s">
-        <v>450</v>
-      </c>
-      <c r="G75" t="s">
+      <c r="B75" s="4" t="s">
+        <v>627</v>
+      </c>
+      <c r="C75" s="4" t="s">
+        <v>614</v>
+      </c>
+      <c r="D75" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="F75" s="4" t="s">
+        <v>108</v>
+      </c>
+      <c r="G75" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="H75" t="s">
+      <c r="H75" s="4" t="s">
         <v>452</v>
       </c>
     </row>
@@ -5734,13 +5820,16 @@
         <v>75</v>
       </c>
       <c r="B76" t="s">
-        <v>510</v>
+        <v>509</v>
       </c>
       <c r="C76" t="s">
-        <v>619</v>
-      </c>
-      <c r="D76" s="71" t="s">
-        <v>450</v>
+        <v>615</v>
+      </c>
+      <c r="D76" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="F76" s="4" t="s">
+        <v>108</v>
       </c>
       <c r="G76" t="s">
         <v>17</v>
@@ -5754,13 +5843,16 @@
         <v>76</v>
       </c>
       <c r="B77" t="s">
-        <v>511</v>
+        <v>510</v>
       </c>
       <c r="C77" t="s">
-        <v>620</v>
-      </c>
-      <c r="D77" s="71" t="s">
-        <v>450</v>
+        <v>616</v>
+      </c>
+      <c r="D77" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="F77" s="4" t="s">
+        <v>108</v>
       </c>
       <c r="G77" t="s">
         <v>17</v>
@@ -5773,14 +5865,17 @@
       <c r="A78">
         <v>77</v>
       </c>
-      <c r="B78" t="s">
-        <v>512</v>
-      </c>
-      <c r="C78" t="s">
-        <v>621</v>
-      </c>
-      <c r="D78" s="71" t="s">
-        <v>450</v>
+      <c r="B78" s="62" t="s">
+        <v>511</v>
+      </c>
+      <c r="C78" s="62" t="s">
+        <v>617</v>
+      </c>
+      <c r="D78" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="F78" s="4" t="s">
+        <v>108</v>
       </c>
       <c r="G78" t="s">
         <v>17</v>
@@ -5794,13 +5889,16 @@
         <v>78</v>
       </c>
       <c r="B79" t="s">
-        <v>513</v>
+        <v>512</v>
       </c>
       <c r="C79" t="s">
-        <v>622</v>
-      </c>
-      <c r="D79" s="71" t="s">
-        <v>450</v>
+        <v>618</v>
+      </c>
+      <c r="D79" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="F79" s="4" t="s">
+        <v>108</v>
       </c>
       <c r="G79" t="s">
         <v>17</v>
@@ -5814,13 +5912,16 @@
         <v>79</v>
       </c>
       <c r="B80" t="s">
-        <v>514</v>
+        <v>513</v>
       </c>
       <c r="C80" t="s">
-        <v>623</v>
-      </c>
-      <c r="D80" s="71" t="s">
-        <v>450</v>
+        <v>619</v>
+      </c>
+      <c r="D80" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="F80" s="4" t="s">
+        <v>108</v>
       </c>
       <c r="G80" t="s">
         <v>17</v>
@@ -5834,13 +5935,16 @@
         <v>80</v>
       </c>
       <c r="B81" t="s">
-        <v>515</v>
+        <v>514</v>
       </c>
       <c r="C81" t="s">
-        <v>624</v>
-      </c>
-      <c r="D81" s="71" t="s">
-        <v>450</v>
+        <v>620</v>
+      </c>
+      <c r="D81" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="F81" s="4" t="s">
+        <v>108</v>
       </c>
       <c r="G81" t="s">
         <v>17</v>
@@ -5854,13 +5958,16 @@
         <v>81</v>
       </c>
       <c r="B82" t="s">
-        <v>516</v>
+        <v>515</v>
       </c>
       <c r="C82" t="s">
-        <v>625</v>
-      </c>
-      <c r="D82" s="71" t="s">
-        <v>450</v>
+        <v>621</v>
+      </c>
+      <c r="D82" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="F82" s="4" t="s">
+        <v>108</v>
       </c>
       <c r="G82" t="s">
         <v>17</v>
@@ -5874,13 +5981,16 @@
         <v>82</v>
       </c>
       <c r="B83" t="s">
-        <v>517</v>
+        <v>516</v>
       </c>
       <c r="C83" t="s">
-        <v>626</v>
-      </c>
-      <c r="D83" s="71" t="s">
-        <v>450</v>
+        <v>622</v>
+      </c>
+      <c r="D83" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="F83" s="4" t="s">
+        <v>108</v>
       </c>
       <c r="G83" t="s">
         <v>17</v>
@@ -5894,13 +6004,16 @@
         <v>83</v>
       </c>
       <c r="B84" t="s">
-        <v>518</v>
+        <v>517</v>
       </c>
       <c r="C84" t="s">
-        <v>627</v>
-      </c>
-      <c r="D84" s="71" t="s">
-        <v>450</v>
+        <v>623</v>
+      </c>
+      <c r="D84" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="F84" s="4" t="s">
+        <v>108</v>
       </c>
       <c r="G84" t="s">
         <v>17</v>
@@ -5914,35 +6027,21 @@
         <v>84</v>
       </c>
       <c r="B85" t="s">
-        <v>519</v>
+        <v>518</v>
       </c>
       <c r="C85" t="s">
-        <v>628</v>
-      </c>
-      <c r="D85" s="71" t="s">
-        <v>450</v>
+        <v>624</v>
+      </c>
+      <c r="D85" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="F85" s="4" t="s">
+        <v>108</v>
       </c>
       <c r="G85" t="s">
         <v>17</v>
       </c>
       <c r="H85" t="s">
-        <v>452</v>
-      </c>
-    </row>
-    <row r="86" spans="1:8" ht="15.75" customHeight="1">
-      <c r="A86">
-        <v>85</v>
-      </c>
-      <c r="C86" t="s">
-        <v>631</v>
-      </c>
-      <c r="D86" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="G86" t="s">
-        <v>17</v>
-      </c>
-      <c r="H86" t="s">
         <v>452</v>
       </c>
     </row>
@@ -6016,9 +6115,23 @@
     <hyperlink ref="J2" r:id="rId66" xr:uid="{00000000-0004-0000-0000-000041000000}"/>
     <hyperlink ref="C69" r:id="rId67" xr:uid="{9DAE03A7-93E8-4507-BD6C-AC4013ECD47F}"/>
     <hyperlink ref="C68" r:id="rId68" xr:uid="{66B9A9CA-DF82-46B6-9C5A-C5709E2FF1AE}"/>
+    <hyperlink ref="B75" r:id="rId69" xr:uid="{57E7BFEF-6F05-4DA9-A3DE-5B0A0EFED4D9}"/>
+    <hyperlink ref="C75" r:id="rId70" xr:uid="{F4755F93-6E59-4C38-BF66-16746869FDF3}"/>
+    <hyperlink ref="H75" r:id="rId71" xr:uid="{5BFAFD71-42C4-487F-B5E7-1697975992B4}"/>
+    <hyperlink ref="B78" r:id="rId72" xr:uid="{D3DE0D76-2479-4283-B7C7-F11B85797022}"/>
+    <hyperlink ref="C78" r:id="rId73" xr:uid="{FC1D9146-2FDC-4F13-A3C3-51CAB46DEC08}"/>
+    <hyperlink ref="B68" r:id="rId74" xr:uid="{3ED6FAA1-2B0F-4DB9-878E-9640A9C2850D}"/>
+    <hyperlink ref="B69" r:id="rId75" xr:uid="{12DE6CA8-DDC5-4E7B-BD2E-14B105A0DE3B}"/>
+    <hyperlink ref="C70" r:id="rId76" xr:uid="{0419758C-286A-4B76-B8B2-31CC336DEDF1}"/>
+    <hyperlink ref="B70" r:id="rId77" xr:uid="{AC18D1D2-FA3D-4352-A402-35B7AAFE27C0}"/>
+    <hyperlink ref="B71" r:id="rId78" xr:uid="{E8BCA1EF-4E17-4AA7-A2CE-5674FC05ABC3}"/>
+    <hyperlink ref="C71" r:id="rId79" xr:uid="{949AE606-DF4A-48F4-93A0-F148D80842CB}"/>
+    <hyperlink ref="B72" r:id="rId80" xr:uid="{69A93BB5-0295-46D6-8334-45444356E6E9}"/>
+    <hyperlink ref="C72" r:id="rId81" xr:uid="{CA171BC7-126F-4175-8A03-123D5A2C2D8A}"/>
+    <hyperlink ref="C73" r:id="rId82" xr:uid="{FACC205D-E563-4266-8E0D-0794F3D76E98}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId69"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId83"/>
 </worksheet>
 </file>
 
@@ -6027,17 +6140,17 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:AI86"/>
+  <dimension ref="A1:AK85"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A61" workbookViewId="0">
-      <selection activeCell="C54" sqref="C54"/>
+      <selection activeCell="C85" sqref="C85"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.3984375" defaultRowHeight="15.75" customHeight="1"/>
   <cols>
     <col min="1" max="1" width="14.86328125" customWidth="1" collapsed="1"/>
     <col min="2" max="2" width="18.1328125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="53.73046875" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="55.59765625" customWidth="1" collapsed="1"/>
     <col min="4" max="4" width="25.265625" customWidth="1" collapsed="1"/>
     <col min="5" max="5" width="19.59765625" customWidth="1" collapsed="1"/>
     <col min="6" max="6" width="19.73046875" customWidth="1" collapsed="1"/>
@@ -6052,11 +6165,12 @@
     <col min="19" max="19" width="77.59765625" customWidth="1" collapsed="1"/>
     <col min="20" max="20" width="24" customWidth="1" collapsed="1"/>
     <col min="21" max="21" width="18.73046875" customWidth="1" collapsed="1"/>
-    <col min="22" max="22" width="19.1328125" customWidth="1" collapsed="1"/>
-    <col min="23" max="31" width="19.265625" customWidth="1" collapsed="1"/>
+    <col min="22" max="23" width="18.73046875" customWidth="1"/>
+    <col min="24" max="24" width="19.1328125" customWidth="1" collapsed="1"/>
+    <col min="25" max="33" width="19.265625" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:35" ht="27.75">
+    <row r="1" spans="1:37" ht="27.75">
       <c r="A1" s="1" t="s">
         <v>47</v>
       </c>
@@ -6121,41 +6235,47 @@
         <v>66</v>
       </c>
       <c r="V1" s="1" t="s">
+        <v>629</v>
+      </c>
+      <c r="W1" s="1" t="s">
+        <v>628</v>
+      </c>
+      <c r="X1" s="1" t="s">
         <v>67</v>
       </c>
-      <c r="W1" s="1" t="s">
+      <c r="Y1" s="1" t="s">
         <v>68</v>
       </c>
-      <c r="X1" s="1" t="s">
+      <c r="Z1" s="1" t="s">
         <v>69</v>
       </c>
-      <c r="Y1" s="1" t="s">
+      <c r="AA1" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="Z1" s="1" t="s">
+      <c r="AB1" s="1" t="s">
         <v>71</v>
       </c>
-      <c r="AA1" s="1" t="s">
+      <c r="AC1" s="1" t="s">
         <v>455</v>
       </c>
-      <c r="AB1" s="1" t="s">
+      <c r="AD1" s="1" t="s">
         <v>73</v>
       </c>
-      <c r="AC1" s="1" t="s">
+      <c r="AE1" s="1" t="s">
         <v>74</v>
       </c>
-      <c r="AD1" s="1" t="s">
+      <c r="AF1" s="1" t="s">
         <v>75</v>
       </c>
-      <c r="AE1" s="1" t="s">
+      <c r="AG1" s="1" t="s">
         <v>76</v>
       </c>
-      <c r="AF1" s="27"/>
-      <c r="AG1" s="27"/>
       <c r="AH1" s="27"/>
       <c r="AI1" s="27"/>
-    </row>
-    <row r="2" spans="1:35" ht="15" customHeight="1">
+      <c r="AJ1" s="27"/>
+      <c r="AK1" s="27"/>
+    </row>
+    <row r="2" spans="1:37" ht="15" customHeight="1">
       <c r="A2" s="28">
         <v>1</v>
       </c>
@@ -6225,8 +6345,10 @@
       <c r="AG2" s="28"/>
       <c r="AH2" s="28"/>
       <c r="AI2" s="28"/>
-    </row>
-    <row r="3" spans="1:35" ht="15" customHeight="1">
+      <c r="AJ2" s="28"/>
+      <c r="AK2" s="28"/>
+    </row>
+    <row r="3" spans="1:37" ht="15" customHeight="1">
       <c r="A3" s="28">
         <v>2</v>
       </c>
@@ -6296,8 +6418,10 @@
       <c r="AG3" s="28"/>
       <c r="AH3" s="28"/>
       <c r="AI3" s="28"/>
-    </row>
-    <row r="4" spans="1:35" s="28" customFormat="1" ht="15" customHeight="1">
+      <c r="AJ3" s="28"/>
+      <c r="AK3" s="28"/>
+    </row>
+    <row r="4" spans="1:37" s="28" customFormat="1" ht="15" customHeight="1">
       <c r="A4" s="28">
         <v>3</v>
       </c>
@@ -6356,7 +6480,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="5" spans="1:35" ht="15" customHeight="1">
+    <row r="5" spans="1:37" ht="15" customHeight="1">
       <c r="A5" s="28">
         <v>4</v>
       </c>
@@ -6428,8 +6552,10 @@
       <c r="AG5" s="28"/>
       <c r="AH5" s="28"/>
       <c r="AI5" s="28"/>
-    </row>
-    <row r="6" spans="1:35" ht="15" customHeight="1">
+      <c r="AJ5" s="28"/>
+      <c r="AK5" s="28"/>
+    </row>
+    <row r="6" spans="1:37" ht="15" customHeight="1">
       <c r="A6" s="28">
         <v>5</v>
       </c>
@@ -6489,8 +6615,8 @@
       <c r="U6" s="29" t="s">
         <v>109</v>
       </c>
-      <c r="V6" s="28"/>
-      <c r="W6" s="28"/>
+      <c r="V6" s="29"/>
+      <c r="W6" s="29"/>
       <c r="X6" s="28"/>
       <c r="Y6" s="28"/>
       <c r="Z6" s="28"/>
@@ -6503,12 +6629,14 @@
       <c r="AG6" s="28"/>
       <c r="AH6" s="28"/>
       <c r="AI6" s="28"/>
-    </row>
-    <row r="7" spans="1:35" ht="15" customHeight="1">
+      <c r="AJ6" s="28"/>
+      <c r="AK6" s="28"/>
+    </row>
+    <row r="7" spans="1:37" ht="15" customHeight="1">
       <c r="A7" s="28">
         <v>6</v>
       </c>
-      <c r="B7" s="72" t="s">
+      <c r="B7" s="70" t="s">
         <v>458</v>
       </c>
       <c r="C7" s="28" t="s">
@@ -6531,7 +6659,7 @@
       </c>
       <c r="I7" s="28"/>
       <c r="J7" s="28"/>
-      <c r="K7" s="72" t="s">
+      <c r="K7" s="70" t="s">
         <v>462</v>
       </c>
       <c r="L7" s="28" t="s">
@@ -6564,8 +6692,8 @@
       <c r="U7" s="29" t="s">
         <v>109</v>
       </c>
-      <c r="V7" s="28"/>
-      <c r="W7" s="28"/>
+      <c r="V7" s="29"/>
+      <c r="W7" s="29"/>
       <c r="X7" s="28"/>
       <c r="Y7" s="28"/>
       <c r="Z7" s="28"/>
@@ -6578,8 +6706,10 @@
       <c r="AG7" s="28"/>
       <c r="AH7" s="28"/>
       <c r="AI7" s="28"/>
-    </row>
-    <row r="8" spans="1:35" ht="15" customHeight="1">
+      <c r="AJ7" s="28"/>
+      <c r="AK7" s="28"/>
+    </row>
+    <row r="8" spans="1:37" ht="15" customHeight="1">
       <c r="A8" s="28">
         <v>7</v>
       </c>
@@ -6637,8 +6767,8 @@
       <c r="U8" s="29" t="s">
         <v>109</v>
       </c>
-      <c r="V8" s="40"/>
-      <c r="W8" s="40"/>
+      <c r="V8" s="29"/>
+      <c r="W8" s="29"/>
       <c r="X8" s="40"/>
       <c r="Y8" s="40"/>
       <c r="Z8" s="40"/>
@@ -6647,12 +6777,14 @@
       <c r="AC8" s="40"/>
       <c r="AD8" s="40"/>
       <c r="AE8" s="40"/>
-      <c r="AF8" s="41"/>
-      <c r="AG8" s="41"/>
+      <c r="AF8" s="40"/>
+      <c r="AG8" s="40"/>
       <c r="AH8" s="41"/>
       <c r="AI8" s="41"/>
-    </row>
-    <row r="9" spans="1:35" ht="15" customHeight="1">
+      <c r="AJ8" s="41"/>
+      <c r="AK8" s="41"/>
+    </row>
+    <row r="9" spans="1:37" ht="15" customHeight="1">
       <c r="A9" s="28">
         <v>8</v>
       </c>
@@ -6712,8 +6844,8 @@
       <c r="U9" s="29" t="s">
         <v>109</v>
       </c>
-      <c r="V9" s="28"/>
-      <c r="W9" s="28"/>
+      <c r="V9" s="29"/>
+      <c r="W9" s="29"/>
       <c r="X9" s="28"/>
       <c r="Y9" s="28"/>
       <c r="Z9" s="28"/>
@@ -6726,12 +6858,14 @@
       <c r="AG9" s="28"/>
       <c r="AH9" s="28"/>
       <c r="AI9" s="28"/>
-    </row>
-    <row r="10" spans="1:35" ht="15" customHeight="1">
+      <c r="AJ9" s="28"/>
+      <c r="AK9" s="28"/>
+    </row>
+    <row r="10" spans="1:37" ht="15" customHeight="1">
       <c r="A10" s="28">
         <v>9</v>
       </c>
-      <c r="B10" s="72" t="s">
+      <c r="B10" s="70" t="s">
         <v>458</v>
       </c>
       <c r="C10" s="32" t="s">
@@ -6754,7 +6888,7 @@
       </c>
       <c r="I10" s="35"/>
       <c r="J10" s="35"/>
-      <c r="K10" s="72" t="s">
+      <c r="K10" s="70" t="s">
         <v>467</v>
       </c>
       <c r="L10" s="67" t="s">
@@ -6785,8 +6919,8 @@
       <c r="U10" s="29" t="s">
         <v>109</v>
       </c>
-      <c r="V10" s="40"/>
-      <c r="W10" s="40"/>
+      <c r="V10" s="29"/>
+      <c r="W10" s="29"/>
       <c r="X10" s="40"/>
       <c r="Y10" s="40"/>
       <c r="Z10" s="40"/>
@@ -6795,12 +6929,14 @@
       <c r="AC10" s="40"/>
       <c r="AD10" s="40"/>
       <c r="AE10" s="40"/>
-      <c r="AF10" s="41"/>
-      <c r="AG10" s="41"/>
+      <c r="AF10" s="40"/>
+      <c r="AG10" s="40"/>
       <c r="AH10" s="41"/>
       <c r="AI10" s="41"/>
-    </row>
-    <row r="11" spans="1:35" ht="15" customHeight="1">
+      <c r="AJ10" s="41"/>
+      <c r="AK10" s="41"/>
+    </row>
+    <row r="11" spans="1:37" ht="15" customHeight="1">
       <c r="A11" s="28">
         <v>10</v>
       </c>
@@ -6858,28 +6994,30 @@
       <c r="U11" s="29" t="s">
         <v>109</v>
       </c>
-      <c r="V11" s="40"/>
-      <c r="W11" s="40" t="s">
-        <v>124</v>
-      </c>
-      <c r="X11" s="40" t="s">
-        <v>124</v>
-      </c>
+      <c r="V11" s="29"/>
+      <c r="W11" s="29"/>
+      <c r="X11" s="40"/>
       <c r="Y11" s="40" t="s">
         <v>124</v>
       </c>
-      <c r="Z11" s="40"/>
-      <c r="AA11" s="40"/>
+      <c r="Z11" s="40" t="s">
+        <v>124</v>
+      </c>
+      <c r="AA11" s="40" t="s">
+        <v>124</v>
+      </c>
       <c r="AB11" s="40"/>
       <c r="AC11" s="40"/>
       <c r="AD11" s="40"/>
       <c r="AE11" s="40"/>
-      <c r="AF11" s="41"/>
-      <c r="AG11" s="41"/>
+      <c r="AF11" s="40"/>
+      <c r="AG11" s="40"/>
       <c r="AH11" s="41"/>
       <c r="AI11" s="41"/>
-    </row>
-    <row r="12" spans="1:35" ht="15" customHeight="1">
+      <c r="AJ11" s="41"/>
+      <c r="AK11" s="41"/>
+    </row>
+    <row r="12" spans="1:37" ht="15" customHeight="1">
       <c r="A12" s="28">
         <v>11</v>
       </c>
@@ -6937,8 +7075,8 @@
       <c r="U12" s="29" t="s">
         <v>109</v>
       </c>
-      <c r="V12" s="28"/>
-      <c r="W12" s="28"/>
+      <c r="V12" s="29"/>
+      <c r="W12" s="29"/>
       <c r="X12" s="28"/>
       <c r="Y12" s="28"/>
       <c r="Z12" s="28"/>
@@ -6951,12 +7089,14 @@
       <c r="AG12" s="28"/>
       <c r="AH12" s="28"/>
       <c r="AI12" s="28"/>
-    </row>
-    <row r="13" spans="1:35" ht="15" customHeight="1">
+      <c r="AJ12" s="28"/>
+      <c r="AK12" s="28"/>
+    </row>
+    <row r="13" spans="1:37" ht="15" customHeight="1">
       <c r="A13" s="28">
         <v>12</v>
       </c>
-      <c r="B13" s="72" t="s">
+      <c r="B13" s="70" t="s">
         <v>458</v>
       </c>
       <c r="C13" s="28" t="s">
@@ -6981,7 +7121,7 @@
         <v>93</v>
       </c>
       <c r="J13" s="28"/>
-      <c r="K13" s="72" t="s">
+      <c r="K13" s="70" t="s">
         <v>475</v>
       </c>
       <c r="L13" s="28" t="s">
@@ -7012,11 +7152,11 @@
       <c r="U13" s="29" t="s">
         <v>109</v>
       </c>
-      <c r="V13" s="28" t="s">
+      <c r="V13" s="29"/>
+      <c r="W13" s="29"/>
+      <c r="X13" s="28" t="s">
         <v>124</v>
       </c>
-      <c r="W13" s="28"/>
-      <c r="X13" s="28"/>
       <c r="Y13" s="28"/>
       <c r="Z13" s="28"/>
       <c r="AA13" s="28"/>
@@ -7028,8 +7168,10 @@
       <c r="AG13" s="28"/>
       <c r="AH13" s="28"/>
       <c r="AI13" s="28"/>
-    </row>
-    <row r="14" spans="1:35" ht="15" customHeight="1">
+      <c r="AJ13" s="28"/>
+      <c r="AK13" s="28"/>
+    </row>
+    <row r="14" spans="1:37" ht="15" customHeight="1">
       <c r="A14" s="28">
         <v>13</v>
       </c>
@@ -7089,30 +7231,32 @@
       <c r="U14" s="29" t="s">
         <v>109</v>
       </c>
-      <c r="V14" s="28"/>
-      <c r="W14" s="28"/>
+      <c r="V14" s="29"/>
+      <c r="W14" s="29"/>
       <c r="X14" s="28"/>
       <c r="Y14" s="28"/>
       <c r="Z14" s="28"/>
-      <c r="AA14" s="28" t="s">
-        <v>124</v>
-      </c>
+      <c r="AA14" s="28"/>
       <c r="AB14" s="28"/>
       <c r="AC14" s="28" t="s">
         <v>124</v>
       </c>
       <c r="AD14" s="28"/>
-      <c r="AE14" s="28"/>
+      <c r="AE14" s="28" t="s">
+        <v>124</v>
+      </c>
       <c r="AF14" s="28"/>
       <c r="AG14" s="28"/>
       <c r="AH14" s="28"/>
       <c r="AI14" s="28"/>
-    </row>
-    <row r="15" spans="1:35" ht="15" customHeight="1">
+      <c r="AJ14" s="28"/>
+      <c r="AK14" s="28"/>
+    </row>
+    <row r="15" spans="1:37" ht="15" customHeight="1">
       <c r="A15" s="28">
         <v>14</v>
       </c>
-      <c r="B15" s="72" t="s">
+      <c r="B15" s="70" t="s">
         <v>458</v>
       </c>
       <c r="C15" s="28" t="s">
@@ -7135,7 +7279,7 @@
       </c>
       <c r="I15" s="28"/>
       <c r="J15" s="28"/>
-      <c r="K15" s="72" t="s">
+      <c r="K15" s="70" t="s">
         <v>482</v>
       </c>
       <c r="L15" s="28" t="s">
@@ -7166,8 +7310,8 @@
       <c r="U15" s="29" t="s">
         <v>109</v>
       </c>
-      <c r="V15" s="28"/>
-      <c r="W15" s="28"/>
+      <c r="V15" s="29"/>
+      <c r="W15" s="29"/>
       <c r="X15" s="28"/>
       <c r="Y15" s="28"/>
       <c r="Z15" s="28"/>
@@ -7180,8 +7324,10 @@
       <c r="AG15" s="28"/>
       <c r="AH15" s="28"/>
       <c r="AI15" s="28"/>
-    </row>
-    <row r="16" spans="1:35" ht="15" customHeight="1">
+      <c r="AJ15" s="28"/>
+      <c r="AK15" s="28"/>
+    </row>
+    <row r="16" spans="1:37" ht="15" customHeight="1">
       <c r="A16" s="28">
         <v>15</v>
       </c>
@@ -7241,8 +7387,8 @@
       <c r="U16" s="29" t="s">
         <v>109</v>
       </c>
-      <c r="V16" s="28"/>
-      <c r="W16" s="28"/>
+      <c r="V16" s="29"/>
+      <c r="W16" s="29"/>
       <c r="X16" s="28"/>
       <c r="Y16" s="28"/>
       <c r="Z16" s="28"/>
@@ -7255,8 +7401,10 @@
       <c r="AG16" s="28"/>
       <c r="AH16" s="28"/>
       <c r="AI16" s="28"/>
-    </row>
-    <row r="17" spans="1:35" ht="15" customHeight="1">
+      <c r="AJ16" s="28"/>
+      <c r="AK16" s="28"/>
+    </row>
+    <row r="17" spans="1:37" ht="15" customHeight="1">
       <c r="A17" s="28">
         <v>16</v>
       </c>
@@ -7314,8 +7462,8 @@
       <c r="U17" s="29" t="s">
         <v>109</v>
       </c>
-      <c r="V17" s="28"/>
-      <c r="W17" s="28"/>
+      <c r="V17" s="29"/>
+      <c r="W17" s="29"/>
       <c r="X17" s="28"/>
       <c r="Y17" s="28"/>
       <c r="Z17" s="28"/>
@@ -7328,12 +7476,14 @@
       <c r="AG17" s="28"/>
       <c r="AH17" s="28"/>
       <c r="AI17" s="28"/>
-    </row>
-    <row r="18" spans="1:35" ht="15" customHeight="1">
+      <c r="AJ17" s="28"/>
+      <c r="AK17" s="28"/>
+    </row>
+    <row r="18" spans="1:37" ht="15" customHeight="1">
       <c r="A18" s="28">
         <v>17</v>
       </c>
-      <c r="B18" s="72" t="s">
+      <c r="B18" s="70" t="s">
         <v>458</v>
       </c>
       <c r="C18" s="28" t="s">
@@ -7358,7 +7508,7 @@
         <v>93</v>
       </c>
       <c r="J18" s="28"/>
-      <c r="K18" s="72" t="s">
+      <c r="K18" s="70" t="s">
         <v>486</v>
       </c>
       <c r="L18" s="68" t="s">
@@ -7389,8 +7539,8 @@
       <c r="U18" s="29" t="s">
         <v>109</v>
       </c>
-      <c r="V18" s="28"/>
-      <c r="W18" s="28"/>
+      <c r="V18" s="29"/>
+      <c r="W18" s="29"/>
       <c r="X18" s="28"/>
       <c r="Y18" s="28"/>
       <c r="Z18" s="28"/>
@@ -7403,8 +7553,10 @@
       <c r="AG18" s="28"/>
       <c r="AH18" s="28"/>
       <c r="AI18" s="28"/>
-    </row>
-    <row r="19" spans="1:35" ht="15" customHeight="1">
+      <c r="AJ18" s="28"/>
+      <c r="AK18" s="28"/>
+    </row>
+    <row r="19" spans="1:37" ht="15" customHeight="1">
       <c r="A19" s="28">
         <v>18</v>
       </c>
@@ -7460,8 +7612,8 @@
       <c r="U19" s="29" t="s">
         <v>109</v>
       </c>
-      <c r="V19" s="28"/>
-      <c r="W19" s="28"/>
+      <c r="V19" s="29"/>
+      <c r="W19" s="29"/>
       <c r="X19" s="28"/>
       <c r="Y19" s="28"/>
       <c r="Z19" s="28"/>
@@ -7474,8 +7626,10 @@
       <c r="AG19" s="28"/>
       <c r="AH19" s="28"/>
       <c r="AI19" s="28"/>
-    </row>
-    <row r="20" spans="1:35" ht="15" customHeight="1">
+      <c r="AJ19" s="28"/>
+      <c r="AK19" s="28"/>
+    </row>
+    <row r="20" spans="1:37" ht="15" customHeight="1">
       <c r="A20" s="28">
         <v>19</v>
       </c>
@@ -7535,8 +7689,8 @@
       <c r="U20" s="29" t="s">
         <v>109</v>
       </c>
-      <c r="V20" s="28"/>
-      <c r="W20" s="28"/>
+      <c r="V20" s="29"/>
+      <c r="W20" s="29"/>
       <c r="X20" s="28"/>
       <c r="Y20" s="28"/>
       <c r="Z20" s="28"/>
@@ -7549,8 +7703,10 @@
       <c r="AG20" s="28"/>
       <c r="AH20" s="28"/>
       <c r="AI20" s="28"/>
-    </row>
-    <row r="21" spans="1:35" ht="15" customHeight="1">
+      <c r="AJ20" s="28"/>
+      <c r="AK20" s="28"/>
+    </row>
+    <row r="21" spans="1:37" ht="15" customHeight="1">
       <c r="A21" s="28">
         <v>20</v>
       </c>
@@ -7606,8 +7762,8 @@
       <c r="U21" s="29" t="s">
         <v>109</v>
       </c>
-      <c r="V21" s="28"/>
-      <c r="W21" s="28"/>
+      <c r="V21" s="29"/>
+      <c r="W21" s="29"/>
       <c r="X21" s="28"/>
       <c r="Y21" s="28"/>
       <c r="Z21" s="28"/>
@@ -7620,8 +7776,10 @@
       <c r="AG21" s="28"/>
       <c r="AH21" s="28"/>
       <c r="AI21" s="28"/>
-    </row>
-    <row r="22" spans="1:35" ht="15" customHeight="1">
+      <c r="AJ21" s="28"/>
+      <c r="AK21" s="28"/>
+    </row>
+    <row r="22" spans="1:37" ht="15" customHeight="1">
       <c r="A22" s="28">
         <v>21</v>
       </c>
@@ -7683,15 +7841,15 @@
       <c r="U22" s="29" t="s">
         <v>109</v>
       </c>
-      <c r="V22" s="28" t="s">
-        <v>124</v>
-      </c>
-      <c r="W22" s="28"/>
+      <c r="V22" s="29"/>
+      <c r="W22" s="29"/>
       <c r="X22" s="28" t="s">
         <v>124</v>
       </c>
       <c r="Y22" s="28"/>
-      <c r="Z22" s="28"/>
+      <c r="Z22" s="28" t="s">
+        <v>124</v>
+      </c>
       <c r="AA22" s="28"/>
       <c r="AB22" s="28"/>
       <c r="AC22" s="28"/>
@@ -7701,8 +7859,10 @@
       <c r="AG22" s="28"/>
       <c r="AH22" s="28"/>
       <c r="AI22" s="28"/>
-    </row>
-    <row r="23" spans="1:35" ht="15" customHeight="1">
+      <c r="AJ22" s="28"/>
+      <c r="AK22" s="28"/>
+    </row>
+    <row r="23" spans="1:37" ht="15" customHeight="1">
       <c r="A23" s="28">
         <v>22</v>
       </c>
@@ -7760,8 +7920,8 @@
       <c r="U23" s="29" t="s">
         <v>109</v>
       </c>
-      <c r="V23" s="28"/>
-      <c r="W23" s="28"/>
+      <c r="V23" s="29"/>
+      <c r="W23" s="29"/>
       <c r="X23" s="28"/>
       <c r="Y23" s="28"/>
       <c r="Z23" s="28"/>
@@ -7774,12 +7934,14 @@
       <c r="AG23" s="28"/>
       <c r="AH23" s="28"/>
       <c r="AI23" s="28"/>
-    </row>
-    <row r="24" spans="1:35" ht="15" customHeight="1">
+      <c r="AJ23" s="28"/>
+      <c r="AK23" s="28"/>
+    </row>
+    <row r="24" spans="1:37" ht="15" customHeight="1">
       <c r="A24" s="28">
         <v>23</v>
       </c>
-      <c r="B24" s="72" t="s">
+      <c r="B24" s="70" t="s">
         <v>458</v>
       </c>
       <c r="C24" s="28" t="s">
@@ -7804,7 +7966,7 @@
         <v>93</v>
       </c>
       <c r="J24" s="28"/>
-      <c r="K24" s="72" t="s">
+      <c r="K24" s="70" t="s">
         <v>459</v>
       </c>
       <c r="L24" s="28" t="s">
@@ -7837,8 +7999,8 @@
       <c r="U24" s="29" t="s">
         <v>109</v>
       </c>
-      <c r="V24" s="28"/>
-      <c r="W24" s="28"/>
+      <c r="V24" s="29"/>
+      <c r="W24" s="29"/>
       <c r="X24" s="28"/>
       <c r="Y24" s="28"/>
       <c r="Z24" s="28"/>
@@ -7851,8 +8013,10 @@
       <c r="AG24" s="28"/>
       <c r="AH24" s="28"/>
       <c r="AI24" s="28"/>
-    </row>
-    <row r="25" spans="1:35" ht="15" customHeight="1">
+      <c r="AJ24" s="28"/>
+      <c r="AK24" s="28"/>
+    </row>
+    <row r="25" spans="1:37" ht="15" customHeight="1">
       <c r="A25" s="28">
         <v>24</v>
       </c>
@@ -7924,8 +8088,10 @@
       <c r="AG25" s="28"/>
       <c r="AH25" s="28"/>
       <c r="AI25" s="28"/>
-    </row>
-    <row r="26" spans="1:35" ht="15" customHeight="1">
+      <c r="AJ25" s="28"/>
+      <c r="AK25" s="28"/>
+    </row>
+    <row r="26" spans="1:37" ht="15" customHeight="1">
       <c r="A26" s="28">
         <v>25</v>
       </c>
@@ -7999,8 +8165,10 @@
       <c r="AG26" s="28"/>
       <c r="AH26" s="28"/>
       <c r="AI26" s="28"/>
-    </row>
-    <row r="27" spans="1:35" ht="15" customHeight="1">
+      <c r="AJ26" s="28"/>
+      <c r="AK26" s="28"/>
+    </row>
+    <row r="27" spans="1:37" ht="15" customHeight="1">
       <c r="A27" s="28">
         <v>26</v>
       </c>
@@ -8074,12 +8242,14 @@
       <c r="AG27" s="28"/>
       <c r="AH27" s="28"/>
       <c r="AI27" s="28"/>
-    </row>
-    <row r="28" spans="1:35" ht="15" customHeight="1">
+      <c r="AJ27" s="28"/>
+      <c r="AK27" s="28"/>
+    </row>
+    <row r="28" spans="1:37" ht="15" customHeight="1">
       <c r="A28" s="28">
         <v>27</v>
       </c>
-      <c r="B28" s="72" t="s">
+      <c r="B28" s="70" t="s">
         <v>458</v>
       </c>
       <c r="C28" s="28" t="s">
@@ -8104,7 +8274,7 @@
         <v>93</v>
       </c>
       <c r="J28" s="28"/>
-      <c r="K28" s="72" t="s">
+      <c r="K28" s="70" t="s">
         <v>496</v>
       </c>
       <c r="L28" s="68" t="s">
@@ -8149,8 +8319,10 @@
       <c r="AG28" s="28"/>
       <c r="AH28" s="28"/>
       <c r="AI28" s="28"/>
-    </row>
-    <row r="29" spans="1:35" ht="15" customHeight="1">
+      <c r="AJ28" s="28"/>
+      <c r="AK28" s="28"/>
+    </row>
+    <row r="29" spans="1:37" ht="15" customHeight="1">
       <c r="A29" s="28">
         <v>28</v>
       </c>
@@ -8224,8 +8396,10 @@
       <c r="AG29" s="28"/>
       <c r="AH29" s="28"/>
       <c r="AI29" s="28"/>
-    </row>
-    <row r="30" spans="1:35" ht="15" customHeight="1">
+      <c r="AJ29" s="28"/>
+      <c r="AK29" s="28"/>
+    </row>
+    <row r="30" spans="1:37" ht="15" customHeight="1">
       <c r="A30" s="28">
         <v>29</v>
       </c>
@@ -8299,8 +8473,10 @@
       <c r="AG30" s="28"/>
       <c r="AH30" s="28"/>
       <c r="AI30" s="28"/>
-    </row>
-    <row r="31" spans="1:35" ht="15" customHeight="1">
+      <c r="AJ30" s="28"/>
+      <c r="AK30" s="28"/>
+    </row>
+    <row r="31" spans="1:37" ht="15" customHeight="1">
       <c r="A31" s="28">
         <v>30</v>
       </c>
@@ -8372,12 +8548,14 @@
       <c r="AG31" s="28"/>
       <c r="AH31" s="28"/>
       <c r="AI31" s="28"/>
-    </row>
-    <row r="32" spans="1:35" ht="15" customHeight="1">
+      <c r="AJ31" s="28"/>
+      <c r="AK31" s="28"/>
+    </row>
+    <row r="32" spans="1:37" ht="15" customHeight="1">
       <c r="A32" s="28">
         <v>31</v>
       </c>
-      <c r="B32" s="72" t="s">
+      <c r="B32" s="70" t="s">
         <v>458</v>
       </c>
       <c r="C32" s="28" t="s">
@@ -8402,7 +8580,7 @@
         <v>93</v>
       </c>
       <c r="J32" s="28"/>
-      <c r="K32" s="72" t="s">
+      <c r="K32" s="70" t="s">
         <v>404</v>
       </c>
       <c r="L32" s="68" t="s">
@@ -8447,6 +8625,8 @@
       <c r="AG32" s="28"/>
       <c r="AH32" s="28"/>
       <c r="AI32" s="28"/>
+      <c r="AJ32" s="28"/>
+      <c r="AK32" s="28"/>
     </row>
     <row r="33" spans="1:21" s="28" customFormat="1" ht="13.5">
       <c r="A33" s="28" t="s">
@@ -10336,7 +10516,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="65" spans="1:21" s="28" customFormat="1" ht="13.5">
+    <row r="65" spans="1:23" s="28" customFormat="1" ht="13.5">
       <c r="A65" s="28" t="s">
         <v>434</v>
       </c>
@@ -10395,7 +10575,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="66" spans="1:21" s="28" customFormat="1" ht="13.5">
+    <row r="66" spans="1:23" s="28" customFormat="1" ht="13.5">
       <c r="A66" s="28" t="s">
         <v>439</v>
       </c>
@@ -10454,11 +10634,11 @@
         <v>38</v>
       </c>
     </row>
-    <row r="67" spans="1:21" s="28" customFormat="1" ht="13.5">
+    <row r="67" spans="1:23" s="28" customFormat="1" ht="13.5">
       <c r="A67" s="28" t="s">
         <v>445</v>
       </c>
-      <c r="B67" s="72" t="s">
+      <c r="B67" s="70" t="s">
         <v>458</v>
       </c>
       <c r="C67" s="28" t="s">
@@ -10470,41 +10650,41 @@
       <c r="E67" s="28" t="s">
         <v>79</v>
       </c>
-      <c r="F67" s="72" t="s">
+      <c r="F67" s="70" t="s">
         <v>230</v>
       </c>
       <c r="G67" s="28" t="s">
         <v>447</v>
       </c>
-      <c r="H67" s="72" t="s">
+      <c r="H67" s="70" t="s">
         <v>448</v>
       </c>
       <c r="I67" s="28" t="s">
         <v>221</v>
       </c>
-      <c r="K67" s="72" t="s">
+      <c r="K67" s="70" t="s">
         <v>449</v>
       </c>
-      <c r="L67" s="72" t="s">
+      <c r="L67" s="70" t="s">
         <v>140</v>
       </c>
-      <c r="M67" s="72" t="s">
+      <c r="M67" s="70" t="s">
         <v>224</v>
       </c>
-      <c r="N67" s="72" t="s">
+      <c r="N67" s="70" t="s">
         <v>227</v>
       </c>
-      <c r="P67" s="72" t="s">
+      <c r="P67" s="70" t="s">
         <v>222</v>
       </c>
-      <c r="Q67" s="72" t="s">
+      <c r="Q67" s="70" t="s">
         <v>289</v>
       </c>
       <c r="R67" s="28" t="s">
         <v>446</v>
       </c>
-      <c r="S67" s="72" t="s">
-        <v>521</v>
+      <c r="S67" s="70" t="s">
+        <v>520</v>
       </c>
       <c r="T67" s="28" t="s">
         <v>108</v>
@@ -10513,307 +10693,337 @@
         <v>17</v>
       </c>
     </row>
-    <row r="68" spans="1:21" ht="13.5">
-      <c r="A68" t="s">
+    <row r="68" spans="1:23" s="28" customFormat="1" ht="13.5">
+      <c r="A68" s="28" t="s">
+        <v>521</v>
+      </c>
+      <c r="B68" s="28" t="s">
+        <v>7</v>
+      </c>
+      <c r="C68" s="28" t="s">
         <v>522</v>
       </c>
-      <c r="B68" t="s">
-        <v>450</v>
-      </c>
-      <c r="C68" t="s">
+      <c r="D68" s="28" t="s">
+        <v>86</v>
+      </c>
+      <c r="E68" s="28" t="s">
+        <v>79</v>
+      </c>
+      <c r="F68" s="28" t="s">
+        <v>80</v>
+      </c>
+      <c r="G68" s="28" t="s">
+        <v>244</v>
+      </c>
+      <c r="H68" s="28" t="s">
         <v>523</v>
       </c>
-      <c r="D68" t="s">
-        <v>86</v>
-      </c>
-      <c r="E68" t="s">
-        <v>79</v>
-      </c>
-      <c r="F68" t="s">
-        <v>80</v>
-      </c>
-      <c r="G68" t="s">
-        <v>244</v>
-      </c>
-      <c r="H68" t="s">
+      <c r="I68" s="28" t="s">
+        <v>221</v>
+      </c>
+      <c r="K68" s="28" t="s">
+        <v>222</v>
+      </c>
+      <c r="L68" s="28" t="s">
         <v>524</v>
       </c>
-      <c r="I68" t="s">
-        <v>221</v>
-      </c>
-      <c r="K68" t="s">
-        <v>222</v>
-      </c>
-      <c r="L68" t="s">
+      <c r="M68" s="28" t="s">
+        <v>225</v>
+      </c>
+      <c r="N68" s="28" t="s">
+        <v>227</v>
+      </c>
+      <c r="P68" s="28" t="s">
+        <v>226</v>
+      </c>
+      <c r="Q68" s="28" t="s">
+        <v>227</v>
+      </c>
+      <c r="R68" s="28" t="s">
+        <v>522</v>
+      </c>
+      <c r="S68" s="28" t="s">
         <v>525</v>
-      </c>
-      <c r="M68" t="s">
-        <v>225</v>
-      </c>
-      <c r="N68" t="s">
-        <v>227</v>
-      </c>
-      <c r="P68" t="s">
-        <v>226</v>
-      </c>
-      <c r="Q68" t="s">
-        <v>227</v>
-      </c>
-      <c r="R68" t="s">
-        <v>523</v>
-      </c>
-      <c r="S68" t="s">
-        <v>526</v>
       </c>
       <c r="T68" s="28" t="s">
         <v>83</v>
       </c>
-      <c r="U68" t="s">
+      <c r="U68" s="28" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="69" spans="1:21" ht="13.5">
-      <c r="A69" t="s">
+      <c r="V68" s="71">
+        <v>44339</v>
+      </c>
+      <c r="W68" s="28" t="s">
+        <v>630</v>
+      </c>
+    </row>
+    <row r="69" spans="1:23" s="28" customFormat="1" ht="13.5">
+      <c r="A69" s="28" t="s">
+        <v>526</v>
+      </c>
+      <c r="B69" s="28" t="s">
+        <v>7</v>
+      </c>
+      <c r="C69" s="28" t="s">
         <v>527</v>
       </c>
-      <c r="B69" t="s">
-        <v>450</v>
-      </c>
-      <c r="C69" t="s">
-        <v>528</v>
-      </c>
-      <c r="D69" t="s">
+      <c r="D69" s="28" t="s">
         <v>284</v>
       </c>
-      <c r="E69" t="s">
+      <c r="E69" s="28" t="s">
         <v>79</v>
       </c>
-      <c r="F69" t="s">
+      <c r="F69" s="28" t="s">
         <v>80</v>
       </c>
-      <c r="G69" t="s">
+      <c r="G69" s="28" t="s">
         <v>285</v>
       </c>
-      <c r="H69" t="s">
+      <c r="H69" s="28" t="s">
         <v>286</v>
       </c>
-      <c r="I69" t="s">
+      <c r="I69" s="28" t="s">
         <v>221</v>
       </c>
-      <c r="K69" t="s">
+      <c r="K69" s="28" t="s">
         <v>222</v>
       </c>
-      <c r="L69" t="s">
+      <c r="L69" s="28" t="s">
         <v>260</v>
       </c>
-      <c r="M69" t="s">
+      <c r="M69" s="28" t="s">
         <v>225</v>
       </c>
-      <c r="N69" t="s">
+      <c r="N69" s="28" t="s">
         <v>227</v>
       </c>
-      <c r="P69" t="s">
+      <c r="P69" s="28" t="s">
         <v>226</v>
       </c>
-      <c r="Q69" t="s">
+      <c r="Q69" s="28" t="s">
         <v>289</v>
       </c>
-      <c r="R69" t="s">
-        <v>528</v>
-      </c>
-      <c r="S69" t="s">
-        <v>529</v>
+      <c r="R69" s="28" t="s">
+        <v>527</v>
+      </c>
+      <c r="S69" s="28" t="s">
+        <v>632</v>
       </c>
       <c r="T69" s="28" t="s">
         <v>83</v>
       </c>
-      <c r="U69" t="s">
+      <c r="U69" s="28" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="70" spans="1:21" ht="13.5">
-      <c r="A70" t="s">
+      <c r="V69" s="71">
+        <v>44339</v>
+      </c>
+      <c r="W69" s="28" t="s">
+        <v>630</v>
+      </c>
+    </row>
+    <row r="70" spans="1:23" s="28" customFormat="1" ht="13.5">
+      <c r="A70" s="28" t="s">
+        <v>528</v>
+      </c>
+      <c r="B70" s="28" t="s">
+        <v>7</v>
+      </c>
+      <c r="C70" s="28" t="s">
+        <v>529</v>
+      </c>
+      <c r="D70" s="28" t="s">
+        <v>86</v>
+      </c>
+      <c r="E70" s="28" t="s">
+        <v>196</v>
+      </c>
+      <c r="F70" s="28" t="s">
+        <v>258</v>
+      </c>
+      <c r="G70" s="28" t="s">
+        <v>120</v>
+      </c>
+      <c r="H70" s="28" t="s">
         <v>530</v>
       </c>
-      <c r="B70" t="s">
-        <v>450</v>
-      </c>
-      <c r="C70" t="s">
+      <c r="I70" s="28" t="s">
+        <v>221</v>
+      </c>
+      <c r="K70" s="28" t="s">
         <v>531</v>
       </c>
-      <c r="D70" t="s">
-        <v>86</v>
-      </c>
-      <c r="E70" t="s">
-        <v>196</v>
-      </c>
-      <c r="F70" t="s">
-        <v>258</v>
-      </c>
-      <c r="G70" t="s">
-        <v>120</v>
-      </c>
-      <c r="H70" t="s">
+      <c r="L70" s="28" t="s">
         <v>532</v>
       </c>
-      <c r="I70" t="s">
-        <v>221</v>
-      </c>
-      <c r="K70" t="s">
+      <c r="M70" s="28" t="s">
+        <v>227</v>
+      </c>
+      <c r="N70" s="28" t="s">
+        <v>227</v>
+      </c>
+      <c r="P70" s="28" t="s">
+        <v>226</v>
+      </c>
+      <c r="Q70" s="28" t="s">
+        <v>227</v>
+      </c>
+      <c r="R70" s="28" t="s">
+        <v>529</v>
+      </c>
+      <c r="S70" s="28" t="s">
         <v>533</v>
-      </c>
-      <c r="L70" t="s">
-        <v>534</v>
-      </c>
-      <c r="M70" t="s">
-        <v>227</v>
-      </c>
-      <c r="N70" t="s">
-        <v>227</v>
-      </c>
-      <c r="P70" t="s">
-        <v>226</v>
-      </c>
-      <c r="Q70" t="s">
-        <v>227</v>
-      </c>
-      <c r="R70" t="s">
-        <v>531</v>
-      </c>
-      <c r="S70" t="s">
-        <v>535</v>
       </c>
       <c r="T70" s="28" t="s">
         <v>83</v>
       </c>
-      <c r="U70" t="s">
+      <c r="U70" s="28" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="71" spans="1:21" ht="13.5">
-      <c r="A71" t="s">
+      <c r="V70" s="71">
+        <v>44339</v>
+      </c>
+      <c r="W70" s="28" t="s">
+        <v>630</v>
+      </c>
+    </row>
+    <row r="71" spans="1:23" s="28" customFormat="1" ht="13.5">
+      <c r="A71" s="28" t="s">
+        <v>534</v>
+      </c>
+      <c r="B71" s="28" t="s">
+        <v>7</v>
+      </c>
+      <c r="C71" s="28" t="s">
+        <v>535</v>
+      </c>
+      <c r="D71" s="28" t="s">
+        <v>86</v>
+      </c>
+      <c r="E71" s="28" t="s">
+        <v>196</v>
+      </c>
+      <c r="F71" s="28" t="s">
+        <v>80</v>
+      </c>
+      <c r="G71" s="28" t="s">
+        <v>126</v>
+      </c>
+      <c r="H71" s="28" t="s">
         <v>536</v>
       </c>
-      <c r="B71" t="s">
-        <v>450</v>
-      </c>
-      <c r="C71" t="s">
+      <c r="I71" s="28" t="s">
+        <v>221</v>
+      </c>
+      <c r="K71" s="28" t="s">
+        <v>324</v>
+      </c>
+      <c r="L71" s="28" t="s">
         <v>537</v>
       </c>
-      <c r="D71" t="s">
-        <v>86</v>
-      </c>
-      <c r="E71" t="s">
-        <v>196</v>
-      </c>
-      <c r="F71" t="s">
-        <v>80</v>
-      </c>
-      <c r="G71" t="s">
-        <v>126</v>
-      </c>
-      <c r="H71" t="s">
+      <c r="M71" s="28" t="s">
+        <v>275</v>
+      </c>
+      <c r="N71" s="28" t="s">
+        <v>227</v>
+      </c>
+      <c r="P71" s="28" t="s">
+        <v>224</v>
+      </c>
+      <c r="Q71" s="28" t="s">
+        <v>227</v>
+      </c>
+      <c r="R71" s="28" t="s">
+        <v>535</v>
+      </c>
+      <c r="S71" s="28" t="s">
         <v>538</v>
-      </c>
-      <c r="I71" t="s">
-        <v>221</v>
-      </c>
-      <c r="K71" t="s">
-        <v>324</v>
-      </c>
-      <c r="L71" t="s">
-        <v>539</v>
-      </c>
-      <c r="M71" t="s">
-        <v>275</v>
-      </c>
-      <c r="N71" t="s">
-        <v>227</v>
-      </c>
-      <c r="P71" t="s">
-        <v>224</v>
-      </c>
-      <c r="Q71" t="s">
-        <v>227</v>
-      </c>
-      <c r="R71" t="s">
-        <v>537</v>
-      </c>
-      <c r="S71" t="s">
-        <v>540</v>
       </c>
       <c r="T71" s="28" t="s">
         <v>83</v>
       </c>
-      <c r="U71" t="s">
+      <c r="U71" s="28" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="72" spans="1:21" ht="13.5">
-      <c r="A72" t="s">
-        <v>541</v>
-      </c>
-      <c r="B72" t="s">
-        <v>450</v>
-      </c>
-      <c r="C72" t="s">
+      <c r="V71" s="71">
+        <v>44339</v>
+      </c>
+      <c r="W71" s="28" t="s">
+        <v>630</v>
+      </c>
+    </row>
+    <row r="72" spans="1:23" s="28" customFormat="1" ht="13.5">
+      <c r="A72" s="28" t="s">
+        <v>539</v>
+      </c>
+      <c r="B72" s="28" t="s">
+        <v>7</v>
+      </c>
+      <c r="C72" s="28" t="s">
         <v>101</v>
       </c>
-      <c r="D72" t="s">
+      <c r="D72" s="28" t="s">
         <v>86</v>
       </c>
-      <c r="E72" t="s">
+      <c r="E72" s="28" t="s">
         <v>79</v>
       </c>
-      <c r="F72" t="s">
+      <c r="F72" s="28" t="s">
         <v>230</v>
       </c>
-      <c r="G72" t="s">
+      <c r="G72" s="28" t="s">
         <v>104</v>
       </c>
-      <c r="H72" t="s">
-        <v>542</v>
-      </c>
-      <c r="I72" t="s">
+      <c r="H72" s="28" t="s">
+        <v>540</v>
+      </c>
+      <c r="I72" s="28" t="s">
         <v>221</v>
       </c>
-      <c r="K72" t="s">
+      <c r="K72" s="28" t="s">
         <v>222</v>
       </c>
-      <c r="L72" t="s">
+      <c r="L72" s="28" t="s">
         <v>260</v>
       </c>
-      <c r="M72" t="s">
+      <c r="M72" s="28" t="s">
         <v>224</v>
       </c>
-      <c r="N72" t="s">
+      <c r="N72" s="28" t="s">
         <v>227</v>
       </c>
-      <c r="P72" t="s">
+      <c r="P72" s="28" t="s">
         <v>226</v>
       </c>
-      <c r="Q72" t="s">
+      <c r="Q72" s="28" t="s">
         <v>227</v>
       </c>
-      <c r="R72" t="s">
+      <c r="R72" s="28" t="s">
         <v>234</v>
       </c>
-      <c r="S72" t="s">
-        <v>543</v>
+      <c r="S72" s="28" t="s">
+        <v>633</v>
       </c>
       <c r="T72" s="28" t="s">
         <v>83</v>
       </c>
-      <c r="U72" t="s">
+      <c r="U72" s="28" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="73" spans="1:21" ht="13.5">
+      <c r="V72" s="71">
+        <v>44339</v>
+      </c>
+      <c r="W72" s="28" t="s">
+        <v>630</v>
+      </c>
+    </row>
+    <row r="73" spans="1:23" ht="13.5">
       <c r="A73" t="s">
-        <v>544</v>
-      </c>
-      <c r="B73" t="s">
-        <v>450</v>
+        <v>541</v>
+      </c>
+      <c r="B73" s="28" t="s">
+        <v>7</v>
       </c>
       <c r="C73" t="s">
         <v>91</v>
@@ -10831,7 +11041,7 @@
         <v>87</v>
       </c>
       <c r="H73" t="s">
-        <v>545</v>
+        <v>542</v>
       </c>
       <c r="I73" t="s">
         <v>221</v>
@@ -10840,7 +11050,7 @@
         <v>471</v>
       </c>
       <c r="L73" t="s">
-        <v>546</v>
+        <v>543</v>
       </c>
       <c r="M73" t="s">
         <v>225</v>
@@ -10858,7 +11068,7 @@
         <v>240</v>
       </c>
       <c r="S73" t="s">
-        <v>547</v>
+        <v>544</v>
       </c>
       <c r="T73" s="28" t="s">
         <v>108</v>
@@ -10867,15 +11077,15 @@
         <v>17</v>
       </c>
     </row>
-    <row r="74" spans="1:21" ht="13.5">
+    <row r="74" spans="1:23" ht="13.5">
       <c r="A74" t="s">
-        <v>548</v>
-      </c>
-      <c r="B74" t="s">
-        <v>450</v>
+        <v>545</v>
+      </c>
+      <c r="B74" s="28" t="s">
+        <v>7</v>
       </c>
       <c r="C74" t="s">
-        <v>549</v>
+        <v>546</v>
       </c>
       <c r="D74" t="s">
         <v>284</v>
@@ -10890,16 +11100,16 @@
         <v>244</v>
       </c>
       <c r="H74" t="s">
-        <v>550</v>
+        <v>547</v>
       </c>
       <c r="I74" t="s">
         <v>221</v>
       </c>
       <c r="K74" t="s">
-        <v>551</v>
+        <v>548</v>
       </c>
       <c r="L74" t="s">
-        <v>552</v>
+        <v>549</v>
       </c>
       <c r="M74" t="s">
         <v>224</v>
@@ -10914,10 +11124,10 @@
         <v>222</v>
       </c>
       <c r="R74" t="s">
-        <v>549</v>
+        <v>546</v>
       </c>
       <c r="S74" t="s">
-        <v>553</v>
+        <v>550</v>
       </c>
       <c r="T74" s="28" t="s">
         <v>108</v>
@@ -10926,71 +11136,77 @@
         <v>17</v>
       </c>
     </row>
-    <row r="75" spans="1:21" ht="13.5">
-      <c r="A75" t="s">
+    <row r="75" spans="1:23" s="28" customFormat="1" ht="13.5">
+      <c r="A75" s="28" t="s">
+        <v>551</v>
+      </c>
+      <c r="B75" s="28" t="s">
+        <v>7</v>
+      </c>
+      <c r="C75" s="28" t="s">
+        <v>552</v>
+      </c>
+      <c r="D75" s="28" t="s">
+        <v>86</v>
+      </c>
+      <c r="E75" s="28" t="s">
+        <v>79</v>
+      </c>
+      <c r="F75" s="28" t="s">
+        <v>258</v>
+      </c>
+      <c r="G75" s="28" t="s">
+        <v>259</v>
+      </c>
+      <c r="H75" s="28" t="s">
+        <v>553</v>
+      </c>
+      <c r="I75" s="28" t="s">
+        <v>221</v>
+      </c>
+      <c r="K75" s="28" t="s">
         <v>554</v>
       </c>
-      <c r="B75" t="s">
-        <v>450</v>
-      </c>
-      <c r="C75" t="s">
+      <c r="L75" s="28" t="s">
         <v>555</v>
       </c>
-      <c r="D75" t="s">
-        <v>86</v>
-      </c>
-      <c r="E75" t="s">
-        <v>79</v>
-      </c>
-      <c r="F75" t="s">
-        <v>258</v>
-      </c>
-      <c r="G75" t="s">
-        <v>259</v>
-      </c>
-      <c r="H75" t="s">
+      <c r="M75" s="28" t="s">
+        <v>225</v>
+      </c>
+      <c r="N75" s="28" t="s">
+        <v>227</v>
+      </c>
+      <c r="P75" s="28" t="s">
+        <v>226</v>
+      </c>
+      <c r="Q75" s="28" t="s">
+        <v>227</v>
+      </c>
+      <c r="R75" s="28" t="s">
+        <v>552</v>
+      </c>
+      <c r="S75" s="28" t="s">
         <v>556</v>
-      </c>
-      <c r="I75" t="s">
-        <v>221</v>
-      </c>
-      <c r="K75" t="s">
-        <v>557</v>
-      </c>
-      <c r="L75" t="s">
-        <v>558</v>
-      </c>
-      <c r="M75" t="s">
-        <v>225</v>
-      </c>
-      <c r="N75" t="s">
-        <v>227</v>
-      </c>
-      <c r="P75" t="s">
-        <v>226</v>
-      </c>
-      <c r="Q75" t="s">
-        <v>227</v>
-      </c>
-      <c r="R75" t="s">
-        <v>555</v>
-      </c>
-      <c r="S75" t="s">
-        <v>559</v>
       </c>
       <c r="T75" s="28" t="s">
         <v>108</v>
       </c>
-      <c r="U75" t="s">
+      <c r="U75" s="28" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="76" spans="1:21" ht="13.5">
+      <c r="V75" s="71">
+        <v>44339</v>
+      </c>
+      <c r="W75" s="28" t="s">
+        <v>630</v>
+      </c>
+    </row>
+    <row r="76" spans="1:23" ht="13.5">
       <c r="A76" t="s">
-        <v>560</v>
-      </c>
-      <c r="B76" t="s">
-        <v>450</v>
+        <v>557</v>
+      </c>
+      <c r="B76" s="28" t="s">
+        <v>7</v>
       </c>
       <c r="C76" t="s">
         <v>91</v>
@@ -11008,16 +11224,16 @@
         <v>87</v>
       </c>
       <c r="H76" t="s">
-        <v>561</v>
+        <v>558</v>
       </c>
       <c r="I76" t="s">
         <v>221</v>
       </c>
       <c r="K76" t="s">
-        <v>562</v>
+        <v>559</v>
       </c>
       <c r="L76" t="s">
-        <v>563</v>
+        <v>560</v>
       </c>
       <c r="M76" t="s">
         <v>275</v>
@@ -11035,7 +11251,7 @@
         <v>240</v>
       </c>
       <c r="S76" t="s">
-        <v>564</v>
+        <v>561</v>
       </c>
       <c r="T76" s="28" t="s">
         <v>108</v>
@@ -11044,15 +11260,15 @@
         <v>17</v>
       </c>
     </row>
-    <row r="77" spans="1:21" ht="13.5">
+    <row r="77" spans="1:23" ht="13.5">
       <c r="A77" t="s">
-        <v>565</v>
-      </c>
-      <c r="B77" t="s">
-        <v>450</v>
+        <v>562</v>
+      </c>
+      <c r="B77" s="28" t="s">
+        <v>7</v>
       </c>
       <c r="C77" t="s">
-        <v>566</v>
+        <v>563</v>
       </c>
       <c r="D77" t="s">
         <v>284</v>
@@ -11064,19 +11280,19 @@
         <v>230</v>
       </c>
       <c r="G77" t="s">
-        <v>567</v>
+        <v>564</v>
       </c>
       <c r="H77" t="s">
-        <v>568</v>
+        <v>565</v>
       </c>
       <c r="I77" t="s">
         <v>221</v>
       </c>
       <c r="K77" t="s">
-        <v>569</v>
+        <v>566</v>
       </c>
       <c r="L77" t="s">
-        <v>570</v>
+        <v>567</v>
       </c>
       <c r="M77" t="s">
         <v>227</v>
@@ -11091,10 +11307,10 @@
         <v>289</v>
       </c>
       <c r="R77" t="s">
-        <v>566</v>
+        <v>563</v>
       </c>
       <c r="S77" t="s">
-        <v>571</v>
+        <v>568</v>
       </c>
       <c r="T77" s="28" t="s">
         <v>108</v>
@@ -11103,74 +11319,80 @@
         <v>17</v>
       </c>
     </row>
-    <row r="78" spans="1:21" ht="13.5">
-      <c r="A78" t="s">
-        <v>572</v>
-      </c>
-      <c r="B78" t="s">
-        <v>450</v>
-      </c>
-      <c r="C78" t="s">
-        <v>573</v>
-      </c>
-      <c r="D78" t="s">
+    <row r="78" spans="1:23" s="28" customFormat="1" ht="13.5">
+      <c r="A78" s="28" t="s">
+        <v>569</v>
+      </c>
+      <c r="B78" s="28" t="s">
+        <v>7</v>
+      </c>
+      <c r="C78" s="28" t="s">
+        <v>570</v>
+      </c>
+      <c r="D78" s="28" t="s">
         <v>86</v>
       </c>
-      <c r="E78" t="s">
+      <c r="E78" s="28" t="s">
         <v>79</v>
       </c>
-      <c r="F78" t="s">
+      <c r="F78" s="28" t="s">
         <v>230</v>
       </c>
-      <c r="G78" t="s">
+      <c r="G78" s="28" t="s">
         <v>104</v>
       </c>
-      <c r="H78" t="s">
-        <v>574</v>
-      </c>
-      <c r="I78" t="s">
+      <c r="H78" s="28" t="s">
+        <v>571</v>
+      </c>
+      <c r="I78" s="28" t="s">
         <v>221</v>
       </c>
-      <c r="K78" t="s">
+      <c r="K78" s="28" t="s">
         <v>459</v>
       </c>
-      <c r="L78" t="s">
+      <c r="L78" s="28" t="s">
         <v>157</v>
       </c>
-      <c r="M78" t="s">
+      <c r="M78" s="28" t="s">
         <v>224</v>
       </c>
-      <c r="N78" t="s">
+      <c r="N78" s="28" t="s">
         <v>227</v>
       </c>
-      <c r="P78" t="s">
+      <c r="P78" s="28" t="s">
         <v>226</v>
       </c>
-      <c r="Q78" t="s">
+      <c r="Q78" s="28" t="s">
         <v>227</v>
       </c>
-      <c r="R78" t="s">
-        <v>573</v>
-      </c>
-      <c r="S78" t="s">
-        <v>575</v>
+      <c r="R78" s="28" t="s">
+        <v>570</v>
+      </c>
+      <c r="S78" s="28" t="s">
+        <v>631</v>
       </c>
       <c r="T78" s="28" t="s">
         <v>108</v>
       </c>
-      <c r="U78" t="s">
+      <c r="U78" s="28" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="79" spans="1:21" ht="13.5">
+      <c r="V78" s="71">
+        <v>44339</v>
+      </c>
+      <c r="W78" s="28" t="s">
+        <v>630</v>
+      </c>
+    </row>
+    <row r="79" spans="1:23" ht="13.5">
       <c r="A79" t="s">
-        <v>576</v>
-      </c>
-      <c r="B79" t="s">
-        <v>450</v>
+        <v>572</v>
+      </c>
+      <c r="B79" s="28" t="s">
+        <v>7</v>
       </c>
       <c r="C79" t="s">
-        <v>577</v>
+        <v>573</v>
       </c>
       <c r="D79" t="s">
         <v>78</v>
@@ -11185,16 +11407,16 @@
         <v>230</v>
       </c>
       <c r="H79" t="s">
-        <v>578</v>
+        <v>574</v>
       </c>
       <c r="I79" t="s">
         <v>221</v>
       </c>
       <c r="K79" t="s">
-        <v>579</v>
+        <v>575</v>
       </c>
       <c r="L79" t="s">
-        <v>580</v>
+        <v>576</v>
       </c>
       <c r="M79" t="s">
         <v>227</v>
@@ -11209,10 +11431,10 @@
         <v>222</v>
       </c>
       <c r="R79" t="s">
+        <v>573</v>
+      </c>
+      <c r="S79" t="s">
         <v>577</v>
-      </c>
-      <c r="S79" t="s">
-        <v>581</v>
       </c>
       <c r="T79" s="28" t="s">
         <v>108</v>
@@ -11221,15 +11443,15 @@
         <v>17</v>
       </c>
     </row>
-    <row r="80" spans="1:21" ht="13.5">
+    <row r="80" spans="1:23" ht="13.5">
       <c r="A80" t="s">
-        <v>582</v>
-      </c>
-      <c r="B80" t="s">
-        <v>450</v>
+        <v>578</v>
+      </c>
+      <c r="B80" s="28" t="s">
+        <v>7</v>
       </c>
       <c r="C80" t="s">
-        <v>583</v>
+        <v>579</v>
       </c>
       <c r="D80" t="s">
         <v>284</v>
@@ -11244,16 +11466,16 @@
         <v>271</v>
       </c>
       <c r="H80" t="s">
-        <v>584</v>
+        <v>580</v>
       </c>
       <c r="I80" t="s">
         <v>221</v>
       </c>
       <c r="K80" t="s">
-        <v>585</v>
+        <v>581</v>
       </c>
       <c r="L80" t="s">
-        <v>586</v>
+        <v>582</v>
       </c>
       <c r="M80" t="s">
         <v>225</v>
@@ -11268,10 +11490,10 @@
         <v>227</v>
       </c>
       <c r="R80" t="s">
-        <v>587</v>
+        <v>583</v>
       </c>
       <c r="S80" t="s">
-        <v>588</v>
+        <v>584</v>
       </c>
       <c r="T80" s="28" t="s">
         <v>108</v>
@@ -11282,10 +11504,10 @@
     </row>
     <row r="81" spans="1:21" ht="13.5">
       <c r="A81" t="s">
-        <v>589</v>
-      </c>
-      <c r="B81" t="s">
-        <v>450</v>
+        <v>585</v>
+      </c>
+      <c r="B81" s="28" t="s">
+        <v>7</v>
       </c>
       <c r="C81" t="s">
         <v>91</v>
@@ -11303,16 +11525,16 @@
         <v>87</v>
       </c>
       <c r="H81" t="s">
-        <v>590</v>
+        <v>586</v>
       </c>
       <c r="I81" t="s">
         <v>221</v>
       </c>
       <c r="K81" t="s">
-        <v>591</v>
+        <v>587</v>
       </c>
       <c r="L81" t="s">
-        <v>592</v>
+        <v>588</v>
       </c>
       <c r="M81" t="s">
         <v>275</v>
@@ -11330,7 +11552,7 @@
         <v>240</v>
       </c>
       <c r="S81" t="s">
-        <v>593</v>
+        <v>589</v>
       </c>
       <c r="T81" s="28" t="s">
         <v>108</v>
@@ -11341,10 +11563,10 @@
     </row>
     <row r="82" spans="1:21" ht="13.5">
       <c r="A82" t="s">
-        <v>594</v>
-      </c>
-      <c r="B82" t="s">
-        <v>450</v>
+        <v>590</v>
+      </c>
+      <c r="B82" s="28" t="s">
+        <v>7</v>
       </c>
       <c r="C82" t="s">
         <v>130</v>
@@ -11362,16 +11584,16 @@
         <v>132</v>
       </c>
       <c r="H82" t="s">
-        <v>595</v>
+        <v>591</v>
       </c>
       <c r="I82" t="s">
         <v>221</v>
       </c>
       <c r="K82" t="s">
-        <v>596</v>
+        <v>592</v>
       </c>
       <c r="L82" t="s">
-        <v>597</v>
+        <v>593</v>
       </c>
       <c r="M82" t="s">
         <v>224</v>
@@ -11389,7 +11611,7 @@
         <v>280</v>
       </c>
       <c r="S82" t="s">
-        <v>598</v>
+        <v>594</v>
       </c>
       <c r="T82" s="28" t="s">
         <v>108</v>
@@ -11400,10 +11622,10 @@
     </row>
     <row r="83" spans="1:21" ht="13.5">
       <c r="A83" t="s">
-        <v>599</v>
-      </c>
-      <c r="B83" t="s">
-        <v>450</v>
+        <v>595</v>
+      </c>
+      <c r="B83" s="28" t="s">
+        <v>7</v>
       </c>
       <c r="C83" t="s">
         <v>101</v>
@@ -11430,7 +11652,7 @@
         <v>475</v>
       </c>
       <c r="L83" t="s">
-        <v>600</v>
+        <v>596</v>
       </c>
       <c r="M83" t="s">
         <v>224</v>
@@ -11448,7 +11670,7 @@
         <v>234</v>
       </c>
       <c r="S83" t="s">
-        <v>601</v>
+        <v>597</v>
       </c>
       <c r="T83" s="28" t="s">
         <v>108</v>
@@ -11459,10 +11681,10 @@
     </row>
     <row r="84" spans="1:21" ht="13.5">
       <c r="A84" t="s">
-        <v>602</v>
-      </c>
-      <c r="B84" t="s">
-        <v>450</v>
+        <v>598</v>
+      </c>
+      <c r="B84" s="28" t="s">
+        <v>7</v>
       </c>
       <c r="C84" t="s">
         <v>118</v>
@@ -11480,16 +11702,16 @@
         <v>120</v>
       </c>
       <c r="H84" t="s">
-        <v>603</v>
+        <v>599</v>
       </c>
       <c r="I84" t="s">
         <v>221</v>
       </c>
       <c r="K84" t="s">
-        <v>585</v>
+        <v>581</v>
       </c>
       <c r="L84" t="s">
-        <v>586</v>
+        <v>582</v>
       </c>
       <c r="M84" t="s">
         <v>224</v>
@@ -11504,10 +11726,10 @@
         <v>227</v>
       </c>
       <c r="R84" t="s">
-        <v>604</v>
+        <v>600</v>
       </c>
       <c r="S84" t="s">
-        <v>605</v>
+        <v>601</v>
       </c>
       <c r="T84" s="28" t="s">
         <v>108</v>
@@ -11518,13 +11740,13 @@
     </row>
     <row r="85" spans="1:21" ht="13.5">
       <c r="A85" t="s">
-        <v>606</v>
-      </c>
-      <c r="B85" t="s">
-        <v>450</v>
+        <v>602</v>
+      </c>
+      <c r="B85" s="28" t="s">
+        <v>7</v>
       </c>
       <c r="C85" t="s">
-        <v>607</v>
+        <v>603</v>
       </c>
       <c r="D85" t="s">
         <v>78</v>
@@ -11533,22 +11755,22 @@
         <v>196</v>
       </c>
       <c r="F85" t="s">
-        <v>520</v>
+        <v>519</v>
       </c>
       <c r="G85" t="s">
-        <v>608</v>
+        <v>604</v>
       </c>
       <c r="H85" t="s">
-        <v>609</v>
+        <v>605</v>
       </c>
       <c r="I85" t="s">
         <v>221</v>
       </c>
       <c r="K85" t="s">
-        <v>610</v>
+        <v>606</v>
       </c>
       <c r="L85" t="s">
-        <v>611</v>
+        <v>607</v>
       </c>
       <c r="M85" t="s">
         <v>289</v>
@@ -11563,10 +11785,10 @@
         <v>222</v>
       </c>
       <c r="R85" t="s">
-        <v>607</v>
+        <v>603</v>
       </c>
       <c r="S85" t="s">
-        <v>612</v>
+        <v>608</v>
       </c>
       <c r="T85" s="28" t="s">
         <v>108</v>
@@ -11575,45 +11797,8 @@
         <v>17</v>
       </c>
     </row>
-    <row r="86" spans="1:21" ht="15.75" customHeight="1">
-      <c r="A86">
-        <v>85</v>
-      </c>
-      <c r="B86" t="s">
-        <v>7</v>
-      </c>
-      <c r="C86" t="s">
-        <v>555</v>
-      </c>
-      <c r="D86" s="73" t="s">
-        <v>86</v>
-      </c>
-      <c r="E86" s="73" t="s">
-        <v>79</v>
-      </c>
-      <c r="F86" s="74"/>
-      <c r="G86" s="74"/>
-      <c r="H86" s="74"/>
-      <c r="I86" s="74"/>
-      <c r="J86" s="74"/>
-      <c r="K86" s="74"/>
-      <c r="L86" s="74"/>
-      <c r="M86" s="74"/>
-      <c r="N86" s="74"/>
-      <c r="O86" s="74"/>
-      <c r="P86" s="74"/>
-      <c r="Q86" s="74"/>
-      <c r="R86" s="74"/>
-      <c r="S86" s="74"/>
-      <c r="T86" s="74"/>
-      <c r="U86" s="74"/>
-    </row>
   </sheetData>
   <customSheetViews>
-    <customSheetView guid="{C25CEB9E-BEC1-4982-90C4-50C84EE1B82A}" filter="1" showAutoFilter="1">
-      <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-      <autoFilter ref="A1:AD33" xr:uid="{00000000-0000-0000-0000-000000000000}"/>
-    </customSheetView>
     <customSheetView guid="{A7754112-A52F-4ABC-8778-92F04773E53C}" filter="1" showAutoFilter="1">
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <autoFilter ref="A1:AD33" xr:uid="{00000000-0000-0000-0000-000000000000}">
@@ -11624,8 +11809,12 @@
         </filterColumn>
       </autoFilter>
     </customSheetView>
+    <customSheetView guid="{C25CEB9E-BEC1-4982-90C4-50C84EE1B82A}" filter="1" showAutoFilter="1">
+      <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+      <autoFilter ref="A1:AD33" xr:uid="{00000000-0000-0000-0000-000000000000}"/>
+    </customSheetView>
   </customSheetViews>
-  <conditionalFormatting sqref="A1:AI1">
+  <conditionalFormatting sqref="A1:AK1">
     <cfRule type="notContainsBlanks" dxfId="1" priority="1">
       <formula>LEN(TRIM(A1))&gt;0</formula>
     </cfRule>

</xml_diff>

<commit_message>
Added code for updating property page
</commit_message>
<xml_diff>
--- a/src/main/resources/InputTestdata/Listing details.xlsx
+++ b/src/main/resources/InputTestdata/Listing details.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Athavan\git\777Homes-business\src\main\resources\InputTestdata\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\manoj\git\777Homes-business\src\main\resources\InputTestdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ACC34725-D059-4AC7-B460-3ED0B1279E76}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DB59EA50-1A4A-4B74-81A8-904222A3D71B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="20715" windowHeight="13276" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Backlog" sheetId="1" r:id="rId1"/>
@@ -21,19 +21,19 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Backlog!$A$1:$AB$52</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Listing!#REF!</definedName>
-    <definedName name="Z_A7754112_A52F_4ABC_8778_92F04773E53C_.wvu.FilterData" localSheetId="1" hidden="1">Listing!$A$1:$AG$32</definedName>
-    <definedName name="Z_C25CEB9E_BEC1_4982_90C4_50C84EE1B82A_.wvu.FilterData" localSheetId="1" hidden="1">Listing!$A$1:$AG$32</definedName>
+    <definedName name="Z_A7754112_A52F_4ABC_8778_92F04773E53C_.wvu.FilterData" localSheetId="1" hidden="1">Listing!$A$1:$AE$32</definedName>
+    <definedName name="Z_C25CEB9E_BEC1_4982_90C4_50C84EE1B82A_.wvu.FilterData" localSheetId="1" hidden="1">Listing!$A$1:$AE$32</definedName>
   </definedNames>
   <calcPr calcId="181029"/>
   <customWorkbookViews>
+    <customWorkbookView name="Filter 1" guid="{A7754112-A52F-4ABC-8778-92F04773E53C}" maximized="1" windowWidth="0" windowHeight="0" activeSheetId="0"/>
     <customWorkbookView name="Filter 2" guid="{C25CEB9E-BEC1-4982-90C4-50C84EE1B82A}" maximized="1" windowWidth="0" windowHeight="0" activeSheetId="0"/>
-    <customWorkbookView name="Filter 1" guid="{A7754112-A52F-4ABC-8778-92F04773E53C}" maximized="1" windowWidth="0" windowHeight="0" activeSheetId="0"/>
   </customWorkbookViews>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2285" uniqueCount="715">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2276" uniqueCount="707">
   <si>
     <t>ID</t>
   </si>
@@ -1955,9 +1955,6 @@
     <t>Rented</t>
   </si>
   <si>
-    <t>L</t>
-  </si>
-  <si>
     <t>777 URL</t>
   </si>
   <si>
@@ -1985,9 +1982,6 @@
     <t xml:space="preserve">8	2	0	0	0	0	</t>
   </si>
   <si>
-    <t>Strathnairn 2615</t>
-  </si>
-  <si>
     <t>Block/House: 371/ 190</t>
   </si>
   <si>
@@ -2044,9 +2038,6 @@
   </si>
   <si>
     <t xml:space="preserve">6	8	9	0	0	0	</t>
-  </si>
-  <si>
-    <t>Taylor 2913</t>
   </si>
   <si>
     <t>Block/House: 483/ -</t>
@@ -2145,9 +2136,6 @@
   </si>
   <si>
     <t xml:space="preserve">1	0	7	5	0	0	0	</t>
-  </si>
-  <si>
-    <t>Phillip 2606</t>
   </si>
   <si>
     <t>Block/House: 3377/ 104</t>
@@ -2665,15 +2653,6 @@
     <t>https://www.allhomes.com.au/sculthorpe-avenue-whitlam-act-2611?tid=179490568</t>
   </si>
   <si>
-    <t xml:space="preserve">Checked by </t>
-  </si>
-  <si>
-    <t>Checked by Date</t>
-  </si>
-  <si>
-    <t>Athavan</t>
-  </si>
-  <si>
     <t>Start Living Your Dream! Last 2 H&amp;L Packages left!
 Opens to be held at Pro Hart Ave, Block 17 Section 23, Ginninderry Residences, Strathnairn.  (Opposite the Land sales office)
 Completion estimated to be last quarter of 2021.
@@ -2758,13 +2737,7 @@
 EER 6 stars</t>
   </si>
   <si>
-    <t>Turner 2612</t>
-  </si>
-  <si>
     <t>Land</t>
-  </si>
-  <si>
-    <t>Moncrieff 2914</t>
   </si>
   <si>
     <t>Block/House: 651/ -</t>
@@ -3106,9 +3079,6 @@
   </si>
   <si>
     <t>$820,000+</t>
-  </si>
-  <si>
-    <t>NEW</t>
   </si>
   <si>
     <t>Currently Tenanted for $470 per week - A fantastic opportunity to buy for living later on or an investment. You will love this 2-bedroom apartment with its open plan living, dining &amp; kitchen area that flows straight to the tiled balcony through glass sliding doors to enjoy breathtaking views on daily basis. The second bedroom can be used as a home office if you prefer, the choice is yours. Quality appliances include a dishwasher, heating and cooling system, laminated timber floor covering to living area and quality carpet to the bedrooms provide a comfortable lifestyle.
@@ -3327,6 +3297,12 @@
   </si>
   <si>
     <t>https://www.777homes.com.au/?post_type=property&amp;p=7338&amp;preview=true</t>
+  </si>
+  <si>
+    <t>Woden Valley</t>
+  </si>
+  <si>
+    <t>PF - Central A/C</t>
   </si>
 </sst>
 </file>
@@ -3631,7 +3607,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="29" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="74">
+  <cellXfs count="73">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -3773,9 +3749,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="14" fontId="18" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="12" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="13" borderId="0" xfId="0" applyFill="1"/>
@@ -4029,21 +4002,21 @@
       <selection pane="bottomLeft" activeCell="A94" sqref="A94:XFD97"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.46484375" defaultRowHeight="15.75" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15.75" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="9.19921875" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="74.796875" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" width="9.21875" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="74.77734375" customWidth="1" collapsed="1"/>
     <col min="3" max="3" width="65" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="14.53125" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="22.1328125" style="55" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="21.86328125" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="56.86328125" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="10.86328125" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="17.86328125" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="22.53125" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="14.5546875" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="22.109375" style="55" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="21.88671875" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="56.88671875" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="10.88671875" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="17.88671875" customWidth="1" collapsed="1"/>
+    <col min="11" max="11" width="22.5546875" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:28" ht="13.9">
+    <row r="1" spans="1:28" ht="13.8">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -4051,7 +4024,7 @@
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>443</v>
+        <v>442</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>2</v>
@@ -4118,7 +4091,7 @@
       <c r="AA2" s="7"/>
       <c r="AB2" s="7"/>
     </row>
-    <row r="3" spans="1:28" ht="13.9">
+    <row r="3" spans="1:28" ht="13.8">
       <c r="A3" s="2">
         <v>2</v>
       </c>
@@ -4210,7 +4183,7 @@
       <c r="AA4" s="7"/>
       <c r="AB4" s="7"/>
     </row>
-    <row r="5" spans="1:28" ht="13.9">
+    <row r="5" spans="1:28" ht="13.8">
       <c r="A5" s="10">
         <v>4</v>
       </c>
@@ -4256,7 +4229,7 @@
       <c r="AA5" s="7"/>
       <c r="AB5" s="7"/>
     </row>
-    <row r="6" spans="1:28" ht="13.9">
+    <row r="6" spans="1:28" ht="13.8">
       <c r="A6" s="10">
         <v>5</v>
       </c>
@@ -4298,7 +4271,7 @@
       <c r="AA6" s="10"/>
       <c r="AB6" s="10"/>
     </row>
-    <row r="7" spans="1:28" ht="13.9">
+    <row r="7" spans="1:28" ht="13.8">
       <c r="A7" s="10">
         <v>6</v>
       </c>
@@ -4340,7 +4313,7 @@
       <c r="AA7" s="7"/>
       <c r="AB7" s="7"/>
     </row>
-    <row r="8" spans="1:28" ht="13.9">
+    <row r="8" spans="1:28" ht="13.8">
       <c r="A8" s="10">
         <v>7</v>
       </c>
@@ -4382,7 +4355,7 @@
       <c r="AA8" s="7"/>
       <c r="AB8" s="7"/>
     </row>
-    <row r="9" spans="1:28" ht="13.9">
+    <row r="9" spans="1:28" ht="13.8">
       <c r="A9" s="10">
         <v>8</v>
       </c>
@@ -4424,7 +4397,7 @@
       <c r="AA9" s="7"/>
       <c r="AB9" s="7"/>
     </row>
-    <row r="10" spans="1:28" ht="13.9">
+    <row r="10" spans="1:28" ht="13.8">
       <c r="A10" s="10">
         <v>9</v>
       </c>
@@ -4466,7 +4439,7 @@
       <c r="AA10" s="7"/>
       <c r="AB10" s="7"/>
     </row>
-    <row r="11" spans="1:28" ht="13.9">
+    <row r="11" spans="1:28" ht="13.8">
       <c r="A11" s="10">
         <v>10</v>
       </c>
@@ -4508,7 +4481,7 @@
       <c r="AA11" s="7"/>
       <c r="AB11" s="7"/>
     </row>
-    <row r="12" spans="1:28" ht="13.9">
+    <row r="12" spans="1:28" ht="13.8">
       <c r="A12" s="10">
         <v>11</v>
       </c>
@@ -4550,7 +4523,7 @@
       <c r="AA12" s="7"/>
       <c r="AB12" s="7"/>
     </row>
-    <row r="13" spans="1:28" ht="13.9">
+    <row r="13" spans="1:28" ht="13.8">
       <c r="A13" s="10">
         <v>12</v>
       </c>
@@ -4592,7 +4565,7 @@
       <c r="AA13" s="7"/>
       <c r="AB13" s="7"/>
     </row>
-    <row r="14" spans="1:28" ht="13.9">
+    <row r="14" spans="1:28" ht="13.8">
       <c r="A14" s="10">
         <v>13</v>
       </c>
@@ -4634,7 +4607,7 @@
       <c r="AA14" s="7"/>
       <c r="AB14" s="7"/>
     </row>
-    <row r="15" spans="1:28" ht="13.9">
+    <row r="15" spans="1:28" ht="13.8">
       <c r="A15" s="10">
         <v>14</v>
       </c>
@@ -4676,7 +4649,7 @@
       <c r="AA15" s="7"/>
       <c r="AB15" s="7"/>
     </row>
-    <row r="16" spans="1:28" ht="13.9">
+    <row r="16" spans="1:28" ht="13.8">
       <c r="A16" s="10">
         <v>15</v>
       </c>
@@ -4718,7 +4691,7 @@
       <c r="AA16" s="7"/>
       <c r="AB16" s="7"/>
     </row>
-    <row r="17" spans="1:28" ht="13.9">
+    <row r="17" spans="1:28" ht="13.8">
       <c r="A17" s="10">
         <v>16</v>
       </c>
@@ -4760,7 +4733,7 @@
       <c r="AA17" s="7"/>
       <c r="AB17" s="7"/>
     </row>
-    <row r="18" spans="1:28" ht="13.9">
+    <row r="18" spans="1:28" ht="13.8">
       <c r="A18" s="10">
         <v>17</v>
       </c>
@@ -4802,7 +4775,7 @@
       <c r="AA18" s="7"/>
       <c r="AB18" s="7"/>
     </row>
-    <row r="19" spans="1:28" ht="13.9">
+    <row r="19" spans="1:28" ht="13.8">
       <c r="A19" s="10">
         <v>18</v>
       </c>
@@ -4844,7 +4817,7 @@
       <c r="AA19" s="7"/>
       <c r="AB19" s="7"/>
     </row>
-    <row r="20" spans="1:28" ht="13.9">
+    <row r="20" spans="1:28" ht="13.8">
       <c r="A20" s="10">
         <v>19</v>
       </c>
@@ -4886,7 +4859,7 @@
       <c r="AA20" s="7"/>
       <c r="AB20" s="7"/>
     </row>
-    <row r="21" spans="1:28" ht="13.9">
+    <row r="21" spans="1:28" ht="13.8">
       <c r="A21" s="10">
         <v>20</v>
       </c>
@@ -4928,7 +4901,7 @@
       <c r="AA21" s="7"/>
       <c r="AB21" s="7"/>
     </row>
-    <row r="22" spans="1:28" ht="13.9">
+    <row r="22" spans="1:28" ht="13.8">
       <c r="A22" s="10">
         <v>21</v>
       </c>
@@ -4970,7 +4943,7 @@
       <c r="AA22" s="7"/>
       <c r="AB22" s="7"/>
     </row>
-    <row r="23" spans="1:28" ht="13.9">
+    <row r="23" spans="1:28" ht="13.8">
       <c r="A23" s="10">
         <v>22</v>
       </c>
@@ -5012,7 +4985,7 @@
       <c r="AA23" s="7"/>
       <c r="AB23" s="7"/>
     </row>
-    <row r="24" spans="1:28" ht="13.9">
+    <row r="24" spans="1:28" ht="13.8">
       <c r="A24" s="10">
         <v>23</v>
       </c>
@@ -5054,7 +5027,7 @@
       <c r="AA24" s="7"/>
       <c r="AB24" s="7"/>
     </row>
-    <row r="25" spans="1:28" ht="13.9">
+    <row r="25" spans="1:28" ht="13.8">
       <c r="A25" s="10">
         <v>24</v>
       </c>
@@ -5096,7 +5069,7 @@
       <c r="AA25" s="7"/>
       <c r="AB25" s="7"/>
     </row>
-    <row r="26" spans="1:28" ht="13.9">
+    <row r="26" spans="1:28" ht="13.8">
       <c r="A26" s="10">
         <v>25</v>
       </c>
@@ -5138,7 +5111,7 @@
       <c r="AA26" s="7"/>
       <c r="AB26" s="7"/>
     </row>
-    <row r="27" spans="1:28" ht="13.9">
+    <row r="27" spans="1:28" ht="13.8">
       <c r="A27" s="10">
         <v>26</v>
       </c>
@@ -5180,7 +5153,7 @@
       <c r="AA27" s="7"/>
       <c r="AB27" s="7"/>
     </row>
-    <row r="28" spans="1:28" ht="13.9">
+    <row r="28" spans="1:28" ht="13.8">
       <c r="A28" s="10">
         <v>27</v>
       </c>
@@ -5222,7 +5195,7 @@
       <c r="AA28" s="7"/>
       <c r="AB28" s="7"/>
     </row>
-    <row r="29" spans="1:28" ht="13.9">
+    <row r="29" spans="1:28" ht="13.8">
       <c r="A29" s="10">
         <v>28</v>
       </c>
@@ -5264,7 +5237,7 @@
       <c r="AA29" s="7"/>
       <c r="AB29" s="7"/>
     </row>
-    <row r="30" spans="1:28" ht="13.9">
+    <row r="30" spans="1:28" ht="13.8">
       <c r="A30" s="10">
         <v>29</v>
       </c>
@@ -5306,7 +5279,7 @@
       <c r="AA30" s="7"/>
       <c r="AB30" s="7"/>
     </row>
-    <row r="31" spans="1:28" ht="13.9">
+    <row r="31" spans="1:28" ht="13.8">
       <c r="A31" s="4">
         <v>30</v>
       </c>
@@ -5348,7 +5321,7 @@
       <c r="AA31" s="7"/>
       <c r="AB31" s="7"/>
     </row>
-    <row r="32" spans="1:28" ht="13.9">
+    <row r="32" spans="1:28" ht="13.8">
       <c r="A32" s="4">
         <v>31</v>
       </c>
@@ -5390,7 +5363,7 @@
       <c r="AA32" s="7"/>
       <c r="AB32" s="7"/>
     </row>
-    <row r="33" spans="1:8" s="4" customFormat="1" ht="13.5">
+    <row r="33" spans="1:8" s="4" customFormat="1" ht="13.8">
       <c r="A33" s="4">
         <v>32</v>
       </c>
@@ -5410,7 +5383,7 @@
         <v>439</v>
       </c>
     </row>
-    <row r="34" spans="1:8" s="4" customFormat="1" ht="13.5">
+    <row r="34" spans="1:8" s="4" customFormat="1" ht="13.8">
       <c r="A34" s="4">
         <v>33</v>
       </c>
@@ -5430,7 +5403,7 @@
         <v>439</v>
       </c>
     </row>
-    <row r="35" spans="1:8" s="4" customFormat="1" ht="12.75">
+    <row r="35" spans="1:8" s="4" customFormat="1" ht="13.2">
       <c r="A35" s="4">
         <v>34</v>
       </c>
@@ -5450,7 +5423,7 @@
         <v>439</v>
       </c>
     </row>
-    <row r="36" spans="1:8" s="4" customFormat="1" ht="12.75">
+    <row r="36" spans="1:8" s="4" customFormat="1" ht="13.2">
       <c r="A36" s="4">
         <v>35</v>
       </c>
@@ -5470,7 +5443,7 @@
         <v>439</v>
       </c>
     </row>
-    <row r="37" spans="1:8" s="4" customFormat="1" ht="12.75">
+    <row r="37" spans="1:8" s="4" customFormat="1" ht="13.2">
       <c r="A37" s="4">
         <v>36</v>
       </c>
@@ -5490,7 +5463,7 @@
         <v>439</v>
       </c>
     </row>
-    <row r="38" spans="1:8" s="4" customFormat="1" ht="12.75">
+    <row r="38" spans="1:8" s="4" customFormat="1" ht="13.2">
       <c r="A38" s="4">
         <v>37</v>
       </c>
@@ -5510,7 +5483,7 @@
         <v>439</v>
       </c>
     </row>
-    <row r="39" spans="1:8" s="4" customFormat="1" ht="12.75">
+    <row r="39" spans="1:8" s="4" customFormat="1" ht="13.2">
       <c r="A39" s="4">
         <v>38</v>
       </c>
@@ -5530,7 +5503,7 @@
         <v>439</v>
       </c>
     </row>
-    <row r="40" spans="1:8" s="4" customFormat="1" ht="12.75">
+    <row r="40" spans="1:8" s="4" customFormat="1" ht="13.2">
       <c r="A40" s="4">
         <v>39</v>
       </c>
@@ -5550,7 +5523,7 @@
         <v>439</v>
       </c>
     </row>
-    <row r="41" spans="1:8" s="4" customFormat="1" ht="12.75">
+    <row r="41" spans="1:8" s="4" customFormat="1" ht="13.2">
       <c r="A41" s="4">
         <v>40</v>
       </c>
@@ -5570,7 +5543,7 @@
         <v>439</v>
       </c>
     </row>
-    <row r="42" spans="1:8" s="4" customFormat="1" ht="12.75">
+    <row r="42" spans="1:8" s="4" customFormat="1" ht="13.2">
       <c r="A42" s="4">
         <v>41</v>
       </c>
@@ -5590,7 +5563,7 @@
         <v>439</v>
       </c>
     </row>
-    <row r="43" spans="1:8" s="4" customFormat="1" ht="12.75">
+    <row r="43" spans="1:8" s="4" customFormat="1" ht="13.2">
       <c r="A43" s="4">
         <v>42</v>
       </c>
@@ -5610,7 +5583,7 @@
         <v>439</v>
       </c>
     </row>
-    <row r="44" spans="1:8" s="4" customFormat="1" ht="12.75">
+    <row r="44" spans="1:8" s="4" customFormat="1" ht="13.2">
       <c r="A44" s="4">
         <v>43</v>
       </c>
@@ -5630,7 +5603,7 @@
         <v>439</v>
       </c>
     </row>
-    <row r="45" spans="1:8" s="4" customFormat="1" ht="12.75">
+    <row r="45" spans="1:8" s="4" customFormat="1" ht="13.2">
       <c r="A45" s="4">
         <v>44</v>
       </c>
@@ -5650,7 +5623,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="46" spans="1:8" s="4" customFormat="1" ht="12.75">
+    <row r="46" spans="1:8" s="4" customFormat="1" ht="13.2">
       <c r="A46" s="4">
         <v>45</v>
       </c>
@@ -5670,7 +5643,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="47" spans="1:8" s="4" customFormat="1" ht="12.75">
+    <row r="47" spans="1:8" s="4" customFormat="1" ht="13.2">
       <c r="A47" s="4">
         <v>46</v>
       </c>
@@ -5690,7 +5663,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="48" spans="1:8" s="4" customFormat="1" ht="12.75">
+    <row r="48" spans="1:8" s="4" customFormat="1" ht="13.2">
       <c r="A48" s="4">
         <v>47</v>
       </c>
@@ -5710,7 +5683,7 @@
         <v>440</v>
       </c>
     </row>
-    <row r="49" spans="1:8" s="4" customFormat="1" ht="12.75">
+    <row r="49" spans="1:8" s="4" customFormat="1" ht="13.2">
       <c r="A49" s="4">
         <v>48</v>
       </c>
@@ -5730,7 +5703,7 @@
         <v>440</v>
       </c>
     </row>
-    <row r="50" spans="1:8" s="4" customFormat="1" ht="12.75">
+    <row r="50" spans="1:8" s="4" customFormat="1" ht="13.2">
       <c r="A50" s="4">
         <v>49</v>
       </c>
@@ -5750,7 +5723,7 @@
         <v>440</v>
       </c>
     </row>
-    <row r="51" spans="1:8" s="4" customFormat="1" ht="12.75">
+    <row r="51" spans="1:8" s="4" customFormat="1" ht="13.2">
       <c r="A51" s="4">
         <v>50</v>
       </c>
@@ -5770,7 +5743,7 @@
         <v>440</v>
       </c>
     </row>
-    <row r="52" spans="1:8" s="4" customFormat="1" ht="12.75">
+    <row r="52" spans="1:8" s="4" customFormat="1" ht="13.2">
       <c r="A52" s="4">
         <v>51</v>
       </c>
@@ -5810,7 +5783,7 @@
         <v>334</v>
       </c>
     </row>
-    <row r="54" spans="1:8" ht="12.75">
+    <row r="54" spans="1:8" ht="13.2">
       <c r="A54">
         <v>53</v>
       </c>
@@ -5830,7 +5803,7 @@
         <v>334</v>
       </c>
     </row>
-    <row r="55" spans="1:8" s="4" customFormat="1" ht="12.75">
+    <row r="55" spans="1:8" s="4" customFormat="1" ht="13.2">
       <c r="A55" s="4">
         <v>54</v>
       </c>
@@ -5850,7 +5823,7 @@
         <v>334</v>
       </c>
     </row>
-    <row r="56" spans="1:8" s="4" customFormat="1" ht="12.75">
+    <row r="56" spans="1:8" s="4" customFormat="1" ht="13.2">
       <c r="A56" s="4">
         <v>55</v>
       </c>
@@ -5870,7 +5843,7 @@
         <v>334</v>
       </c>
     </row>
-    <row r="57" spans="1:8" s="4" customFormat="1" ht="12.75">
+    <row r="57" spans="1:8" s="4" customFormat="1" ht="13.2">
       <c r="A57" s="4">
         <v>56</v>
       </c>
@@ -5890,7 +5863,7 @@
         <v>334</v>
       </c>
     </row>
-    <row r="58" spans="1:8" s="4" customFormat="1" ht="12.75">
+    <row r="58" spans="1:8" s="4" customFormat="1" ht="13.2">
       <c r="A58" s="4">
         <v>57</v>
       </c>
@@ -5910,7 +5883,7 @@
         <v>334</v>
       </c>
     </row>
-    <row r="59" spans="1:8" s="4" customFormat="1" ht="12.75">
+    <row r="59" spans="1:8" s="4" customFormat="1" ht="13.2">
       <c r="A59" s="4">
         <v>58</v>
       </c>
@@ -5930,7 +5903,7 @@
         <v>334</v>
       </c>
     </row>
-    <row r="60" spans="1:8" s="4" customFormat="1" ht="12.75">
+    <row r="60" spans="1:8" s="4" customFormat="1" ht="13.2">
       <c r="A60" s="4">
         <v>59</v>
       </c>
@@ -5950,7 +5923,7 @@
         <v>334</v>
       </c>
     </row>
-    <row r="61" spans="1:8" s="4" customFormat="1" ht="12.75">
+    <row r="61" spans="1:8" s="4" customFormat="1" ht="13.2">
       <c r="A61" s="4">
         <v>60</v>
       </c>
@@ -5970,7 +5943,7 @@
         <v>334</v>
       </c>
     </row>
-    <row r="62" spans="1:8" s="4" customFormat="1" ht="12.75">
+    <row r="62" spans="1:8" s="4" customFormat="1" ht="13.2">
       <c r="A62" s="4">
         <v>61</v>
       </c>
@@ -5990,7 +5963,7 @@
         <v>439</v>
       </c>
     </row>
-    <row r="63" spans="1:8" s="4" customFormat="1" ht="12.75">
+    <row r="63" spans="1:8" s="4" customFormat="1" ht="13.2">
       <c r="A63" s="4">
         <v>62</v>
       </c>
@@ -6010,7 +5983,7 @@
         <v>439</v>
       </c>
     </row>
-    <row r="64" spans="1:8" s="4" customFormat="1" ht="12.75">
+    <row r="64" spans="1:8" s="4" customFormat="1" ht="13.2">
       <c r="A64" s="4">
         <v>63</v>
       </c>
@@ -6030,7 +6003,7 @@
         <v>439</v>
       </c>
     </row>
-    <row r="65" spans="1:8" s="4" customFormat="1" ht="12.75">
+    <row r="65" spans="1:8" s="4" customFormat="1" ht="13.2">
       <c r="A65" s="4">
         <v>64</v>
       </c>
@@ -6051,7 +6024,7 @@
         <v>439</v>
       </c>
     </row>
-    <row r="66" spans="1:8" s="4" customFormat="1" ht="12.75">
+    <row r="66" spans="1:8" s="4" customFormat="1" ht="13.2">
       <c r="A66" s="4">
         <v>65</v>
       </c>
@@ -6071,7 +6044,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="67" spans="1:8" s="4" customFormat="1" ht="12.75">
+    <row r="67" spans="1:8" s="4" customFormat="1" ht="13.2">
       <c r="A67" s="4">
         <v>66</v>
       </c>
@@ -6091,15 +6064,15 @@
         <v>440</v>
       </c>
     </row>
-    <row r="68" spans="1:8" s="4" customFormat="1" ht="12.75">
+    <row r="68" spans="1:8" s="4" customFormat="1" ht="13.2">
       <c r="A68" s="4">
         <v>67</v>
       </c>
       <c r="B68" s="4" t="s">
-        <v>481</v>
+        <v>477</v>
       </c>
       <c r="C68" s="4" t="s">
-        <v>599</v>
+        <v>595</v>
       </c>
       <c r="D68" s="4" t="s">
         <v>7</v>
@@ -6114,15 +6087,15 @@
         <v>439</v>
       </c>
     </row>
-    <row r="69" spans="1:8" s="4" customFormat="1" ht="12.75">
+    <row r="69" spans="1:8" s="4" customFormat="1" ht="13.2">
       <c r="A69" s="4">
         <v>68</v>
       </c>
       <c r="B69" s="4" t="s">
-        <v>482</v>
+        <v>478</v>
       </c>
       <c r="C69" s="4" t="s">
-        <v>583</v>
+        <v>579</v>
       </c>
       <c r="D69" s="4" t="s">
         <v>15</v>
@@ -6137,15 +6110,15 @@
         <v>439</v>
       </c>
     </row>
-    <row r="70" spans="1:8" s="4" customFormat="1" ht="12.75">
+    <row r="70" spans="1:8" s="4" customFormat="1" ht="13.2">
       <c r="A70" s="4">
         <v>69</v>
       </c>
       <c r="B70" s="4" t="s">
-        <v>483</v>
+        <v>479</v>
       </c>
       <c r="C70" s="4" t="s">
-        <v>584</v>
+        <v>580</v>
       </c>
       <c r="D70" s="4" t="s">
         <v>15</v>
@@ -6160,15 +6133,15 @@
         <v>439</v>
       </c>
     </row>
-    <row r="71" spans="1:8" s="4" customFormat="1" ht="12.75">
+    <row r="71" spans="1:8" s="4" customFormat="1" ht="13.2">
       <c r="A71" s="4">
         <v>70</v>
       </c>
       <c r="B71" s="4" t="s">
-        <v>484</v>
+        <v>480</v>
       </c>
       <c r="C71" s="4" t="s">
-        <v>585</v>
+        <v>581</v>
       </c>
       <c r="D71" s="4" t="s">
         <v>15</v>
@@ -6183,15 +6156,15 @@
         <v>439</v>
       </c>
     </row>
-    <row r="72" spans="1:8" s="4" customFormat="1" ht="12.75">
+    <row r="72" spans="1:8" s="4" customFormat="1" ht="13.2">
       <c r="A72" s="4">
         <v>71</v>
       </c>
       <c r="B72" s="4" t="s">
-        <v>485</v>
+        <v>481</v>
       </c>
       <c r="C72" s="4" t="s">
-        <v>586</v>
+        <v>582</v>
       </c>
       <c r="D72" s="4" t="s">
         <v>7</v>
@@ -6206,15 +6179,15 @@
         <v>439</v>
       </c>
     </row>
-    <row r="73" spans="1:8" ht="12.75">
+    <row r="73" spans="1:8" ht="13.2">
       <c r="A73">
         <v>72</v>
       </c>
       <c r="B73" t="s">
-        <v>486</v>
+        <v>482</v>
       </c>
       <c r="C73" s="59" t="s">
-        <v>600</v>
+        <v>596</v>
       </c>
       <c r="D73" s="4" t="s">
         <v>7</v>
@@ -6229,15 +6202,15 @@
         <v>440</v>
       </c>
     </row>
-    <row r="74" spans="1:8" ht="12.75">
+    <row r="74" spans="1:8" ht="13.2">
       <c r="A74">
         <v>73</v>
       </c>
       <c r="B74" t="s">
-        <v>487</v>
+        <v>483</v>
       </c>
       <c r="C74" t="s">
-        <v>587</v>
+        <v>583</v>
       </c>
       <c r="D74" s="4" t="s">
         <v>7</v>
@@ -6252,15 +6225,15 @@
         <v>440</v>
       </c>
     </row>
-    <row r="75" spans="1:8" s="4" customFormat="1" ht="12.75">
+    <row r="75" spans="1:8" s="4" customFormat="1" ht="13.2">
       <c r="A75" s="4">
         <v>74</v>
       </c>
       <c r="B75" s="4" t="s">
-        <v>601</v>
+        <v>597</v>
       </c>
       <c r="C75" s="4" t="s">
-        <v>588</v>
+        <v>584</v>
       </c>
       <c r="D75" s="4" t="s">
         <v>7</v>
@@ -6275,15 +6248,15 @@
         <v>440</v>
       </c>
     </row>
-    <row r="76" spans="1:8" ht="12.75">
+    <row r="76" spans="1:8" ht="13.2">
       <c r="A76">
         <v>75</v>
       </c>
       <c r="B76" t="s">
-        <v>488</v>
+        <v>484</v>
       </c>
       <c r="C76" t="s">
-        <v>589</v>
+        <v>585</v>
       </c>
       <c r="D76" s="4" t="s">
         <v>7</v>
@@ -6298,15 +6271,15 @@
         <v>440</v>
       </c>
     </row>
-    <row r="77" spans="1:8" ht="12.75">
+    <row r="77" spans="1:8" ht="13.2">
       <c r="A77">
         <v>76</v>
       </c>
       <c r="B77" t="s">
-        <v>489</v>
+        <v>485</v>
       </c>
       <c r="C77" t="s">
-        <v>590</v>
+        <v>586</v>
       </c>
       <c r="D77" s="4" t="s">
         <v>7</v>
@@ -6321,15 +6294,15 @@
         <v>440</v>
       </c>
     </row>
-    <row r="78" spans="1:8" ht="12.75">
+    <row r="78" spans="1:8" ht="13.2">
       <c r="A78">
         <v>77</v>
       </c>
       <c r="B78" s="59" t="s">
-        <v>490</v>
+        <v>486</v>
       </c>
       <c r="C78" s="59" t="s">
-        <v>591</v>
+        <v>587</v>
       </c>
       <c r="D78" s="4" t="s">
         <v>7</v>
@@ -6344,15 +6317,15 @@
         <v>440</v>
       </c>
     </row>
-    <row r="79" spans="1:8" ht="12.75">
+    <row r="79" spans="1:8" ht="13.2">
       <c r="A79">
         <v>78</v>
       </c>
       <c r="B79" t="s">
-        <v>491</v>
+        <v>487</v>
       </c>
       <c r="C79" t="s">
-        <v>592</v>
+        <v>588</v>
       </c>
       <c r="D79" s="4" t="s">
         <v>15</v>
@@ -6367,15 +6340,15 @@
         <v>440</v>
       </c>
     </row>
-    <row r="80" spans="1:8" ht="12.75">
+    <row r="80" spans="1:8" ht="13.2">
       <c r="A80">
         <v>79</v>
       </c>
       <c r="B80" t="s">
-        <v>492</v>
+        <v>488</v>
       </c>
       <c r="C80" t="s">
-        <v>593</v>
+        <v>589</v>
       </c>
       <c r="D80" s="4" t="s">
         <v>7</v>
@@ -6390,15 +6363,15 @@
         <v>440</v>
       </c>
     </row>
-    <row r="81" spans="1:8" ht="12.75">
+    <row r="81" spans="1:8" ht="13.2">
       <c r="A81">
         <v>80</v>
       </c>
       <c r="B81" t="s">
-        <v>493</v>
+        <v>489</v>
       </c>
       <c r="C81" t="s">
-        <v>594</v>
+        <v>590</v>
       </c>
       <c r="D81" s="4" t="s">
         <v>7</v>
@@ -6413,15 +6386,15 @@
         <v>440</v>
       </c>
     </row>
-    <row r="82" spans="1:8" ht="12.75">
+    <row r="82" spans="1:8" ht="13.2">
       <c r="A82">
         <v>81</v>
       </c>
       <c r="B82" t="s">
-        <v>494</v>
+        <v>490</v>
       </c>
       <c r="C82" t="s">
-        <v>595</v>
+        <v>591</v>
       </c>
       <c r="D82" s="4" t="s">
         <v>7</v>
@@ -6436,15 +6409,15 @@
         <v>440</v>
       </c>
     </row>
-    <row r="83" spans="1:8" ht="12.75">
+    <row r="83" spans="1:8" ht="13.2">
       <c r="A83">
         <v>82</v>
       </c>
       <c r="B83" t="s">
-        <v>495</v>
+        <v>491</v>
       </c>
       <c r="C83" t="s">
-        <v>596</v>
+        <v>592</v>
       </c>
       <c r="D83" s="4" t="s">
         <v>7</v>
@@ -6459,15 +6432,15 @@
         <v>440</v>
       </c>
     </row>
-    <row r="84" spans="1:8" ht="12.75">
+    <row r="84" spans="1:8" ht="13.2">
       <c r="A84">
         <v>83</v>
       </c>
       <c r="B84" t="s">
-        <v>496</v>
+        <v>492</v>
       </c>
       <c r="C84" t="s">
-        <v>597</v>
+        <v>593</v>
       </c>
       <c r="D84" s="4" t="s">
         <v>7</v>
@@ -6482,15 +6455,15 @@
         <v>440</v>
       </c>
     </row>
-    <row r="85" spans="1:8" ht="12.75">
+    <row r="85" spans="1:8" ht="13.2">
       <c r="A85">
         <v>84</v>
       </c>
       <c r="B85" s="59" t="s">
-        <v>497</v>
+        <v>493</v>
       </c>
       <c r="C85" t="s">
-        <v>598</v>
+        <v>594</v>
       </c>
       <c r="D85" s="4" t="s">
         <v>7</v>
@@ -6505,17 +6478,17 @@
         <v>440</v>
       </c>
     </row>
-    <row r="86" spans="1:8" ht="12.75">
+    <row r="86" spans="1:8" ht="13.2">
       <c r="A86">
         <v>85</v>
       </c>
       <c r="B86" t="s">
-        <v>618</v>
+        <v>609</v>
       </c>
       <c r="C86" t="s">
-        <v>667</v>
-      </c>
-      <c r="D86" s="64" t="s">
+        <v>658</v>
+      </c>
+      <c r="D86" s="63" t="s">
         <v>438</v>
       </c>
       <c r="G86" t="s">
@@ -6525,17 +6498,17 @@
         <v>439</v>
       </c>
     </row>
-    <row r="87" spans="1:8" ht="12.75">
+    <row r="87" spans="1:8" ht="13.2">
       <c r="A87">
         <v>86</v>
       </c>
       <c r="B87" t="s">
-        <v>619</v>
+        <v>610</v>
       </c>
       <c r="C87" t="s">
-        <v>668</v>
-      </c>
-      <c r="D87" s="65" t="s">
+        <v>659</v>
+      </c>
+      <c r="D87" s="64" t="s">
         <v>438</v>
       </c>
       <c r="G87" t="s">
@@ -6545,17 +6518,17 @@
         <v>39</v>
       </c>
     </row>
-    <row r="88" spans="1:8" ht="12.75">
+    <row r="88" spans="1:8" ht="13.2">
       <c r="A88">
         <v>87</v>
       </c>
       <c r="B88" t="s">
-        <v>620</v>
+        <v>611</v>
       </c>
       <c r="C88" t="s">
-        <v>669</v>
-      </c>
-      <c r="D88" s="65" t="s">
+        <v>660</v>
+      </c>
+      <c r="D88" s="64" t="s">
         <v>438</v>
       </c>
       <c r="G88" t="s">
@@ -6565,17 +6538,17 @@
         <v>39</v>
       </c>
     </row>
-    <row r="89" spans="1:8" ht="12.75">
+    <row r="89" spans="1:8" ht="13.2">
       <c r="A89">
         <v>88</v>
       </c>
       <c r="B89" t="s">
-        <v>621</v>
+        <v>612</v>
       </c>
       <c r="C89" t="s">
-        <v>670</v>
-      </c>
-      <c r="D89" s="65" t="s">
+        <v>661</v>
+      </c>
+      <c r="D89" s="64" t="s">
         <v>438</v>
       </c>
       <c r="G89" t="s">
@@ -6585,17 +6558,17 @@
         <v>39</v>
       </c>
     </row>
-    <row r="90" spans="1:8" ht="12.75">
+    <row r="90" spans="1:8" ht="13.2">
       <c r="A90">
         <v>89</v>
       </c>
       <c r="B90" t="s">
-        <v>622</v>
+        <v>613</v>
       </c>
       <c r="C90" t="s">
-        <v>671</v>
-      </c>
-      <c r="D90" s="66" t="s">
+        <v>662</v>
+      </c>
+      <c r="D90" s="65" t="s">
         <v>438</v>
       </c>
       <c r="G90" t="s">
@@ -6605,17 +6578,17 @@
         <v>440</v>
       </c>
     </row>
-    <row r="91" spans="1:8" ht="12.75">
+    <row r="91" spans="1:8" ht="13.2">
       <c r="A91">
         <v>90</v>
       </c>
       <c r="B91" t="s">
-        <v>623</v>
+        <v>614</v>
       </c>
       <c r="C91" t="s">
-        <v>672</v>
-      </c>
-      <c r="D91" s="66" t="s">
+        <v>663</v>
+      </c>
+      <c r="D91" s="65" t="s">
         <v>438</v>
       </c>
       <c r="G91" t="s">
@@ -6625,17 +6598,17 @@
         <v>440</v>
       </c>
     </row>
-    <row r="92" spans="1:8" ht="12.75">
+    <row r="92" spans="1:8" ht="13.2">
       <c r="A92">
         <v>91</v>
       </c>
       <c r="B92" t="s">
-        <v>624</v>
+        <v>615</v>
       </c>
       <c r="C92" t="s">
-        <v>664</v>
-      </c>
-      <c r="D92" s="66" t="s">
+        <v>655</v>
+      </c>
+      <c r="D92" s="65" t="s">
         <v>438</v>
       </c>
       <c r="G92" t="s">
@@ -6645,17 +6618,17 @@
         <v>440</v>
       </c>
     </row>
-    <row r="93" spans="1:8" ht="12.75">
+    <row r="93" spans="1:8" ht="13.2">
       <c r="A93">
         <v>92</v>
       </c>
       <c r="B93" t="s">
-        <v>625</v>
+        <v>616</v>
       </c>
       <c r="C93" t="s">
-        <v>665</v>
-      </c>
-      <c r="D93" s="66" t="s">
+        <v>656</v>
+      </c>
+      <c r="D93" s="65" t="s">
         <v>438</v>
       </c>
       <c r="G93" t="s">
@@ -6665,17 +6638,17 @@
         <v>440</v>
       </c>
     </row>
-    <row r="94" spans="1:8" ht="12.75">
+    <row r="94" spans="1:8" ht="13.2">
       <c r="A94">
         <v>93</v>
       </c>
       <c r="B94" t="s">
-        <v>673</v>
+        <v>664</v>
       </c>
       <c r="C94" t="s">
-        <v>713</v>
-      </c>
-      <c r="D94" s="67" t="s">
+        <v>703</v>
+      </c>
+      <c r="D94" s="66" t="s">
         <v>438</v>
       </c>
       <c r="G94" t="s">
@@ -6685,17 +6658,17 @@
         <v>439</v>
       </c>
     </row>
-    <row r="95" spans="1:8" ht="12.75">
+    <row r="95" spans="1:8" ht="13.2">
       <c r="A95">
         <v>94</v>
       </c>
       <c r="B95" t="s">
-        <v>674</v>
+        <v>665</v>
       </c>
       <c r="C95" t="s">
-        <v>711</v>
-      </c>
-      <c r="D95" s="67" t="s">
+        <v>701</v>
+      </c>
+      <c r="D95" s="66" t="s">
         <v>438</v>
       </c>
       <c r="G95" t="s">
@@ -6705,17 +6678,17 @@
         <v>439</v>
       </c>
     </row>
-    <row r="96" spans="1:8" ht="12.75">
+    <row r="96" spans="1:8" ht="13.2">
       <c r="A96">
         <v>95</v>
       </c>
       <c r="B96" t="s">
-        <v>675</v>
+        <v>666</v>
       </c>
       <c r="C96" t="s">
-        <v>712</v>
-      </c>
-      <c r="D96" s="67" t="s">
+        <v>702</v>
+      </c>
+      <c r="D96" s="66" t="s">
         <v>438</v>
       </c>
       <c r="G96" t="s">
@@ -6725,17 +6698,17 @@
         <v>439</v>
       </c>
     </row>
-    <row r="97" spans="1:8" ht="12.75">
+    <row r="97" spans="1:8" ht="13.2">
       <c r="A97">
         <v>96</v>
       </c>
       <c r="B97" t="s">
-        <v>705</v>
+        <v>695</v>
       </c>
       <c r="C97" t="s">
-        <v>714</v>
-      </c>
-      <c r="D97" s="72" t="s">
+        <v>704</v>
+      </c>
+      <c r="D97" s="71" t="s">
         <v>438</v>
       </c>
       <c r="G97" t="s">
@@ -6841,37 +6814,37 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:AK97"/>
+  <dimension ref="A1:AI97"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A85" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A91" workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="U105" sqref="U105"/>
+      <selection pane="topRight" activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.46484375" defaultRowHeight="15.75" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15.75" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="14.86328125" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="18.1328125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="55.53125" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="25.19921875" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="19.53125" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="19.796875" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="18.53125" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="32.19921875" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="20.53125" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="21.1328125" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="28.796875" customWidth="1" collapsed="1"/>
-    <col min="12" max="12" width="37.53125" customWidth="1" collapsed="1"/>
-    <col min="16" max="17" width="18.796875" customWidth="1" collapsed="1"/>
-    <col min="18" max="18" width="47.86328125" customWidth="1" collapsed="1"/>
-    <col min="19" max="19" width="77.53125" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" width="14.88671875" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="18.109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="55.5546875" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="25.21875" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="19.5546875" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="19.77734375" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="18.5546875" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="32.21875" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="20.5546875" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="21.109375" customWidth="1" collapsed="1"/>
+    <col min="11" max="11" width="28.77734375" customWidth="1" collapsed="1"/>
+    <col min="12" max="12" width="37.5546875" customWidth="1" collapsed="1"/>
+    <col min="16" max="17" width="18.77734375" customWidth="1" collapsed="1"/>
+    <col min="18" max="18" width="47.88671875" customWidth="1" collapsed="1"/>
+    <col min="19" max="19" width="77.5546875" customWidth="1" collapsed="1"/>
     <col min="20" max="20" width="24" customWidth="1" collapsed="1"/>
-    <col min="21" max="23" width="18.796875" customWidth="1" collapsed="1"/>
-    <col min="24" max="24" width="19.1328125" customWidth="1" collapsed="1"/>
-    <col min="25" max="33" width="19.19921875" customWidth="1" collapsed="1"/>
+    <col min="21" max="21" width="18.77734375" customWidth="1" collapsed="1"/>
+    <col min="22" max="22" width="19.109375" customWidth="1" collapsed="1"/>
+    <col min="23" max="31" width="19.21875" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:37" ht="27.75">
+    <row r="1" spans="1:35" ht="27.6">
       <c r="A1" s="1" t="s">
         <v>47</v>
       </c>
@@ -6936,47 +6909,41 @@
         <v>66</v>
       </c>
       <c r="V1" s="1" t="s">
-        <v>603</v>
+        <v>67</v>
       </c>
       <c r="W1" s="1" t="s">
-        <v>602</v>
+        <v>68</v>
       </c>
       <c r="X1" s="1" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="Y1" s="1" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="Z1" s="1" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="AA1" s="1" t="s">
-        <v>70</v>
+        <v>706</v>
       </c>
       <c r="AB1" s="1" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="AC1" s="1" t="s">
-        <v>442</v>
+        <v>74</v>
       </c>
       <c r="AD1" s="1" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="AE1" s="1" t="s">
-        <v>74</v>
-      </c>
-      <c r="AF1" s="1" t="s">
-        <v>75</v>
-      </c>
-      <c r="AG1" s="1" t="s">
         <v>76</v>
       </c>
+      <c r="AF1" s="27"/>
+      <c r="AG1" s="27"/>
       <c r="AH1" s="27"/>
       <c r="AI1" s="27"/>
-      <c r="AJ1" s="27"/>
-      <c r="AK1" s="27"/>
-    </row>
-    <row r="2" spans="1:37" ht="15" customHeight="1">
+    </row>
+    <row r="2" spans="1:35" ht="15" customHeight="1">
       <c r="A2" s="28">
         <v>1</v>
       </c>
@@ -7046,10 +7013,8 @@
       <c r="AG2" s="28"/>
       <c r="AH2" s="28"/>
       <c r="AI2" s="28"/>
-      <c r="AJ2" s="28"/>
-      <c r="AK2" s="28"/>
-    </row>
-    <row r="3" spans="1:37" ht="15" customHeight="1">
+    </row>
+    <row r="3" spans="1:35" ht="15" customHeight="1">
       <c r="A3" s="28">
         <v>2</v>
       </c>
@@ -7119,15 +7084,13 @@
       <c r="AG3" s="28"/>
       <c r="AH3" s="28"/>
       <c r="AI3" s="28"/>
-      <c r="AJ3" s="28"/>
-      <c r="AK3" s="28"/>
-    </row>
-    <row r="4" spans="1:37" s="28" customFormat="1" ht="15" customHeight="1">
+    </row>
+    <row r="4" spans="1:35" s="28" customFormat="1" ht="15" customHeight="1">
       <c r="A4" s="28">
         <v>3</v>
       </c>
-      <c r="B4" s="73" t="s">
-        <v>676</v>
+      <c r="B4" s="72" t="s">
+        <v>667</v>
       </c>
       <c r="C4" s="28" t="s">
         <v>91</v>
@@ -7135,31 +7098,31 @@
       <c r="D4" s="28" t="s">
         <v>86</v>
       </c>
-      <c r="E4" s="68" t="s">
+      <c r="E4" s="67" t="s">
         <v>184</v>
       </c>
-      <c r="F4" s="68" t="s">
+      <c r="F4" s="67" t="s">
         <v>80</v>
       </c>
       <c r="G4" s="28" t="s">
         <v>87</v>
       </c>
-      <c r="H4" s="68" t="s">
-        <v>678</v>
+      <c r="H4" s="67" t="s">
+        <v>669</v>
       </c>
       <c r="I4" s="28" t="s">
         <v>92</v>
       </c>
-      <c r="K4" s="73" t="s">
-        <v>679</v>
-      </c>
-      <c r="L4" s="68" t="s">
-        <v>680</v>
+      <c r="K4" s="72" t="s">
+        <v>670</v>
+      </c>
+      <c r="L4" s="67" t="s">
+        <v>671</v>
       </c>
       <c r="M4" s="28">
         <v>4</v>
       </c>
-      <c r="N4" s="68" t="s">
+      <c r="N4" s="67" t="s">
         <v>213</v>
       </c>
       <c r="O4" s="28">
@@ -7174,8 +7137,8 @@
       <c r="R4" s="28" t="s">
         <v>93</v>
       </c>
-      <c r="S4" s="68" t="s">
-        <v>677</v>
+      <c r="S4" s="67" t="s">
+        <v>668</v>
       </c>
       <c r="T4" s="28" t="s">
         <v>83</v>
@@ -7184,7 +7147,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="5" spans="1:37" ht="15" customHeight="1">
+    <row r="5" spans="1:35" ht="15" customHeight="1">
       <c r="A5" s="28">
         <v>4</v>
       </c>
@@ -7256,10 +7219,8 @@
       <c r="AG5" s="28"/>
       <c r="AH5" s="28"/>
       <c r="AI5" s="28"/>
-      <c r="AJ5" s="28"/>
-      <c r="AK5" s="28"/>
-    </row>
-    <row r="6" spans="1:37" ht="15" customHeight="1">
+    </row>
+    <row r="6" spans="1:35" ht="15" customHeight="1">
       <c r="A6" s="28">
         <v>5</v>
       </c>
@@ -7319,8 +7280,8 @@
       <c r="U6" s="29" t="s">
         <v>108</v>
       </c>
-      <c r="V6" s="29"/>
-      <c r="W6" s="29"/>
+      <c r="V6" s="28"/>
+      <c r="W6" s="28"/>
       <c r="X6" s="28"/>
       <c r="Y6" s="28"/>
       <c r="Z6" s="28"/>
@@ -7333,15 +7294,13 @@
       <c r="AG6" s="28"/>
       <c r="AH6" s="28"/>
       <c r="AI6" s="28"/>
-      <c r="AJ6" s="28"/>
-      <c r="AK6" s="28"/>
-    </row>
-    <row r="7" spans="1:37" ht="15" customHeight="1">
+    </row>
+    <row r="7" spans="1:35" ht="15" customHeight="1">
       <c r="A7" s="28">
         <v>6</v>
       </c>
-      <c r="B7" s="73" t="s">
-        <v>676</v>
+      <c r="B7" s="72" t="s">
+        <v>667</v>
       </c>
       <c r="C7" s="28" t="s">
         <v>109</v>
@@ -7359,15 +7318,15 @@
         <v>110</v>
       </c>
       <c r="H7" s="28" t="s">
-        <v>446</v>
+        <v>445</v>
       </c>
       <c r="I7" s="28"/>
       <c r="J7" s="28"/>
-      <c r="K7" s="73" t="s">
-        <v>447</v>
-      </c>
-      <c r="L7" s="69" t="s">
-        <v>681</v>
+      <c r="K7" s="72" t="s">
+        <v>446</v>
+      </c>
+      <c r="L7" s="68" t="s">
+        <v>672</v>
       </c>
       <c r="M7" s="28">
         <v>4</v>
@@ -7388,7 +7347,7 @@
         <v>109</v>
       </c>
       <c r="S7" s="31" t="s">
-        <v>445</v>
+        <v>444</v>
       </c>
       <c r="T7" s="28" t="s">
         <v>107</v>
@@ -7396,8 +7355,8 @@
       <c r="U7" s="29" t="s">
         <v>108</v>
       </c>
-      <c r="V7" s="29"/>
-      <c r="W7" s="29"/>
+      <c r="V7" s="28"/>
+      <c r="W7" s="28"/>
       <c r="X7" s="28"/>
       <c r="Y7" s="28"/>
       <c r="Z7" s="28"/>
@@ -7410,10 +7369,8 @@
       <c r="AG7" s="28"/>
       <c r="AH7" s="28"/>
       <c r="AI7" s="28"/>
-      <c r="AJ7" s="28"/>
-      <c r="AK7" s="28"/>
-    </row>
-    <row r="8" spans="1:37" ht="15" customHeight="1">
+    </row>
+    <row r="8" spans="1:35" ht="15" customHeight="1">
       <c r="A8" s="28">
         <v>7</v>
       </c>
@@ -7471,8 +7428,8 @@
       <c r="U8" s="29" t="s">
         <v>108</v>
       </c>
-      <c r="V8" s="29"/>
-      <c r="W8" s="29"/>
+      <c r="V8" s="40"/>
+      <c r="W8" s="40"/>
       <c r="X8" s="40"/>
       <c r="Y8" s="40"/>
       <c r="Z8" s="40"/>
@@ -7481,14 +7438,12 @@
       <c r="AC8" s="40"/>
       <c r="AD8" s="40"/>
       <c r="AE8" s="40"/>
-      <c r="AF8" s="40"/>
-      <c r="AG8" s="40"/>
+      <c r="AF8" s="41"/>
+      <c r="AG8" s="41"/>
       <c r="AH8" s="41"/>
       <c r="AI8" s="41"/>
-      <c r="AJ8" s="41"/>
-      <c r="AK8" s="41"/>
-    </row>
-    <row r="9" spans="1:37" s="28" customFormat="1" ht="15" customHeight="1">
+    </row>
+    <row r="9" spans="1:35" s="28" customFormat="1" ht="15" customHeight="1">
       <c r="A9" s="28">
         <v>8</v>
       </c>
@@ -7505,13 +7460,13 @@
         <v>183</v>
       </c>
       <c r="F9" s="28" t="s">
-        <v>448</v>
+        <v>218</v>
       </c>
       <c r="G9" s="28" t="s">
         <v>103</v>
       </c>
       <c r="H9" s="28" t="s">
-        <v>449</v>
+        <v>447</v>
       </c>
       <c r="I9" s="28" t="s">
         <v>92</v>
@@ -7547,7 +7502,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="10" spans="1:37" s="28" customFormat="1" ht="15" customHeight="1">
+    <row r="10" spans="1:35" s="28" customFormat="1" ht="15" customHeight="1">
       <c r="A10" s="28">
         <v>9</v>
       </c>
@@ -7564,13 +7519,13 @@
         <v>183</v>
       </c>
       <c r="F10" s="28" t="s">
-        <v>608</v>
+        <v>281</v>
       </c>
       <c r="G10" s="28" t="s">
         <v>115</v>
       </c>
       <c r="H10" s="28" t="s">
-        <v>450</v>
+        <v>448</v>
       </c>
       <c r="K10" s="28" t="s">
         <v>210</v>
@@ -7603,12 +7558,12 @@
         <v>108</v>
       </c>
     </row>
-    <row r="11" spans="1:37" ht="15" customHeight="1">
+    <row r="11" spans="1:35" ht="15" customHeight="1">
       <c r="A11" s="28">
         <v>10</v>
       </c>
-      <c r="B11" s="73" t="s">
-        <v>676</v>
+      <c r="B11" s="72" t="s">
+        <v>667</v>
       </c>
       <c r="C11" s="32" t="s">
         <v>116</v>
@@ -7616,7 +7571,7 @@
       <c r="D11" s="33" t="s">
         <v>86</v>
       </c>
-      <c r="E11" s="71" t="s">
+      <c r="E11" s="70" t="s">
         <v>184</v>
       </c>
       <c r="F11" s="30" t="s">
@@ -7625,21 +7580,21 @@
       <c r="G11" s="28" t="s">
         <v>118</v>
       </c>
-      <c r="H11" s="71" t="s">
-        <v>704</v>
+      <c r="H11" s="70" t="s">
+        <v>694</v>
       </c>
       <c r="I11" s="35"/>
       <c r="J11" s="35"/>
-      <c r="K11" s="73" t="s">
+      <c r="K11" s="72" t="s">
         <v>329</v>
       </c>
-      <c r="L11" s="71" t="s">
+      <c r="L11" s="70" t="s">
         <v>330</v>
       </c>
       <c r="M11" s="33">
         <v>4</v>
       </c>
-      <c r="N11" s="71" t="s">
+      <c r="N11" s="70" t="s">
         <v>213</v>
       </c>
       <c r="O11" s="38"/>
@@ -7652,8 +7607,8 @@
       <c r="R11" s="32" t="s">
         <v>119</v>
       </c>
-      <c r="S11" s="71" t="s">
-        <v>703</v>
+      <c r="S11" s="70" t="s">
+        <v>693</v>
       </c>
       <c r="T11" s="28" t="s">
         <v>107</v>
@@ -7661,30 +7616,28 @@
       <c r="U11" s="29" t="s">
         <v>108</v>
       </c>
-      <c r="V11" s="29"/>
-      <c r="W11" s="29"/>
-      <c r="X11" s="40"/>
+      <c r="V11" s="40"/>
+      <c r="W11" s="40" t="s">
+        <v>120</v>
+      </c>
+      <c r="X11" s="40" t="s">
+        <v>120</v>
+      </c>
       <c r="Y11" s="40" t="s">
         <v>120</v>
       </c>
-      <c r="Z11" s="40" t="s">
-        <v>120</v>
-      </c>
-      <c r="AA11" s="40" t="s">
-        <v>120</v>
-      </c>
+      <c r="Z11" s="40"/>
+      <c r="AA11" s="40"/>
       <c r="AB11" s="40"/>
       <c r="AC11" s="40"/>
       <c r="AD11" s="40"/>
       <c r="AE11" s="40"/>
-      <c r="AF11" s="40"/>
-      <c r="AG11" s="40"/>
+      <c r="AF11" s="41"/>
+      <c r="AG11" s="41"/>
       <c r="AH11" s="41"/>
       <c r="AI11" s="41"/>
-      <c r="AJ11" s="41"/>
-      <c r="AK11" s="41"/>
-    </row>
-    <row r="12" spans="1:37" s="28" customFormat="1" ht="15" customHeight="1">
+    </row>
+    <row r="12" spans="1:35" s="28" customFormat="1" ht="15" customHeight="1">
       <c r="A12" s="28">
         <v>11</v>
       </c>
@@ -7707,13 +7660,13 @@
         <v>122</v>
       </c>
       <c r="H12" s="28" t="s">
+        <v>450</v>
+      </c>
+      <c r="K12" s="28" t="s">
+        <v>451</v>
+      </c>
+      <c r="L12" s="28" t="s">
         <v>452</v>
-      </c>
-      <c r="K12" s="28" t="s">
-        <v>453</v>
-      </c>
-      <c r="L12" s="28" t="s">
-        <v>454</v>
       </c>
       <c r="M12" s="28">
         <v>3</v>
@@ -7731,7 +7684,7 @@
         <v>123</v>
       </c>
       <c r="S12" s="28" t="s">
-        <v>451</v>
+        <v>449</v>
       </c>
       <c r="T12" s="28" t="s">
         <v>107</v>
@@ -7740,7 +7693,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="13" spans="1:37" s="28" customFormat="1" ht="15" customHeight="1">
+    <row r="13" spans="1:35" s="28" customFormat="1" ht="15" customHeight="1">
       <c r="A13" s="28">
         <v>12</v>
       </c>
@@ -7751,19 +7704,19 @@
         <v>124</v>
       </c>
       <c r="D13" s="28" t="s">
-        <v>609</v>
+        <v>601</v>
       </c>
       <c r="E13" s="61" t="s">
         <v>183</v>
       </c>
       <c r="F13" s="28" t="s">
-        <v>610</v>
+        <v>80</v>
       </c>
       <c r="G13" s="28" t="s">
         <v>122</v>
       </c>
       <c r="H13" s="28" t="s">
-        <v>611</v>
+        <v>602</v>
       </c>
       <c r="I13" s="28" t="s">
         <v>92</v>
@@ -7795,11 +7748,11 @@
       <c r="U13" s="28" t="s">
         <v>108</v>
       </c>
-      <c r="X13" s="28" t="s">
+      <c r="V13" s="28" t="s">
         <v>120</v>
       </c>
     </row>
-    <row r="14" spans="1:37" s="28" customFormat="1" ht="15" customHeight="1">
+    <row r="14" spans="1:35" s="28" customFormat="1" ht="15" customHeight="1">
       <c r="A14" s="28">
         <v>13</v>
       </c>
@@ -7822,16 +7775,16 @@
         <v>127</v>
       </c>
       <c r="H14" s="28" t="s">
-        <v>457</v>
+        <v>455</v>
       </c>
       <c r="I14" s="28" t="s">
         <v>92</v>
       </c>
       <c r="K14" s="28" t="s">
-        <v>458</v>
+        <v>456</v>
       </c>
       <c r="L14" s="28" t="s">
-        <v>459</v>
+        <v>457</v>
       </c>
       <c r="M14" s="28">
         <v>3</v>
@@ -7849,7 +7802,7 @@
         <v>128</v>
       </c>
       <c r="S14" s="28" t="s">
-        <v>456</v>
+        <v>454</v>
       </c>
       <c r="T14" s="28" t="s">
         <v>107</v>
@@ -7857,19 +7810,19 @@
       <c r="U14" s="28" t="s">
         <v>108</v>
       </c>
+      <c r="AA14" s="28" t="s">
+        <v>120</v>
+      </c>
       <c r="AC14" s="28" t="s">
         <v>120</v>
       </c>
-      <c r="AE14" s="28" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="15" spans="1:37" s="28" customFormat="1" ht="15" customHeight="1">
+    </row>
+    <row r="15" spans="1:35" s="28" customFormat="1" ht="15" customHeight="1">
       <c r="A15" s="28">
         <v>14</v>
       </c>
-      <c r="B15" s="73" t="s">
-        <v>676</v>
+      <c r="B15" s="72" t="s">
+        <v>667</v>
       </c>
       <c r="C15" s="28" t="s">
         <v>100</v>
@@ -7880,17 +7833,17 @@
       <c r="E15" s="28" t="s">
         <v>126</v>
       </c>
-      <c r="F15" s="69" t="s">
+      <c r="F15" s="68" t="s">
         <v>218</v>
       </c>
       <c r="G15" s="28" t="s">
         <v>103</v>
       </c>
       <c r="H15" s="28" t="s">
-        <v>461</v>
-      </c>
-      <c r="K15" s="73" t="s">
-        <v>462</v>
+        <v>459</v>
+      </c>
+      <c r="K15" s="72" t="s">
+        <v>460</v>
       </c>
       <c r="L15" s="28" t="s">
         <v>129</v>
@@ -7911,7 +7864,7 @@
         <v>106</v>
       </c>
       <c r="S15" s="28" t="s">
-        <v>460</v>
+        <v>458</v>
       </c>
       <c r="T15" s="28" t="s">
         <v>107</v>
@@ -7920,7 +7873,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="16" spans="1:37" s="28" customFormat="1" ht="15" customHeight="1">
+    <row r="16" spans="1:35" s="28" customFormat="1" ht="15" customHeight="1">
       <c r="A16" s="28">
         <v>15</v>
       </c>
@@ -7937,13 +7890,13 @@
         <v>183</v>
       </c>
       <c r="F16" s="28" t="s">
-        <v>463</v>
+        <v>80</v>
       </c>
       <c r="G16" s="28" t="s">
         <v>87</v>
       </c>
       <c r="H16" s="28" t="s">
-        <v>464</v>
+        <v>461</v>
       </c>
       <c r="I16" s="28" t="s">
         <v>92</v>
@@ -7979,12 +7932,12 @@
         <v>108</v>
       </c>
     </row>
-    <row r="17" spans="1:37" s="28" customFormat="1" ht="15" customHeight="1">
+    <row r="17" spans="1:35" s="28" customFormat="1" ht="15" customHeight="1">
       <c r="A17" s="28">
         <v>16</v>
       </c>
-      <c r="B17" s="73" t="s">
-        <v>676</v>
+      <c r="B17" s="72" t="s">
+        <v>667</v>
       </c>
       <c r="C17" s="28" t="s">
         <v>131</v>
@@ -7995,16 +7948,16 @@
       <c r="E17" s="28" t="s">
         <v>184</v>
       </c>
-      <c r="F17" s="69" t="s">
+      <c r="F17" s="68" t="s">
         <v>218</v>
       </c>
       <c r="G17" s="28" t="s">
         <v>103</v>
       </c>
       <c r="H17" s="28" t="s">
-        <v>613</v>
-      </c>
-      <c r="K17" s="73" t="s">
+        <v>604</v>
+      </c>
+      <c r="K17" s="72" t="s">
         <v>437</v>
       </c>
       <c r="L17" s="28" t="s">
@@ -8026,7 +7979,7 @@
         <v>131</v>
       </c>
       <c r="S17" s="28" t="s">
-        <v>612</v>
+        <v>603</v>
       </c>
       <c r="T17" s="28" t="s">
         <v>107</v>
@@ -8035,7 +7988,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="18" spans="1:37" s="28" customFormat="1" ht="15" customHeight="1">
+    <row r="18" spans="1:35" s="28" customFormat="1" ht="15" customHeight="1">
       <c r="A18" s="28">
         <v>17</v>
       </c>
@@ -8064,10 +8017,10 @@
         <v>92</v>
       </c>
       <c r="K18" s="28" t="s">
-        <v>466</v>
+        <v>463</v>
       </c>
       <c r="L18" s="28" t="s">
-        <v>467</v>
+        <v>464</v>
       </c>
       <c r="M18" s="28">
         <v>4</v>
@@ -8085,7 +8038,7 @@
         <v>128</v>
       </c>
       <c r="S18" s="28" t="s">
-        <v>465</v>
+        <v>462</v>
       </c>
       <c r="T18" s="28" t="s">
         <v>107</v>
@@ -8094,12 +8047,12 @@
         <v>108</v>
       </c>
     </row>
-    <row r="19" spans="1:37" ht="15" customHeight="1">
+    <row r="19" spans="1:35" ht="15" customHeight="1">
       <c r="A19" s="28">
         <v>18</v>
       </c>
       <c r="B19" s="62" t="s">
-        <v>658</v>
+        <v>649</v>
       </c>
       <c r="C19" s="28" t="s">
         <v>100</v>
@@ -8150,8 +8103,8 @@
       <c r="U19" s="29" t="s">
         <v>108</v>
       </c>
-      <c r="V19" s="29"/>
-      <c r="W19" s="29"/>
+      <c r="V19" s="28"/>
+      <c r="W19" s="28"/>
       <c r="X19" s="28"/>
       <c r="Y19" s="28"/>
       <c r="Z19" s="28"/>
@@ -8164,10 +8117,8 @@
       <c r="AG19" s="28"/>
       <c r="AH19" s="28"/>
       <c r="AI19" s="28"/>
-      <c r="AJ19" s="28"/>
-      <c r="AK19" s="28"/>
-    </row>
-    <row r="20" spans="1:37" ht="15" customHeight="1">
+    </row>
+    <row r="20" spans="1:35" ht="15" customHeight="1">
       <c r="A20" s="28">
         <v>19</v>
       </c>
@@ -8227,8 +8178,8 @@
       <c r="U20" s="29" t="s">
         <v>108</v>
       </c>
-      <c r="V20" s="29"/>
-      <c r="W20" s="29"/>
+      <c r="V20" s="28"/>
+      <c r="W20" s="28"/>
       <c r="X20" s="28"/>
       <c r="Y20" s="28"/>
       <c r="Z20" s="28"/>
@@ -8241,10 +8192,8 @@
       <c r="AG20" s="28"/>
       <c r="AH20" s="28"/>
       <c r="AI20" s="28"/>
-      <c r="AJ20" s="28"/>
-      <c r="AK20" s="28"/>
-    </row>
-    <row r="21" spans="1:37" ht="15" customHeight="1">
+    </row>
+    <row r="21" spans="1:35" ht="15" customHeight="1">
       <c r="A21" s="28">
         <v>20</v>
       </c>
@@ -8300,8 +8249,8 @@
       <c r="U21" s="29" t="s">
         <v>108</v>
       </c>
-      <c r="V21" s="29"/>
-      <c r="W21" s="29"/>
+      <c r="V21" s="28"/>
+      <c r="W21" s="28"/>
       <c r="X21" s="28"/>
       <c r="Y21" s="28"/>
       <c r="Z21" s="28"/>
@@ -8314,10 +8263,8 @@
       <c r="AG21" s="28"/>
       <c r="AH21" s="28"/>
       <c r="AI21" s="28"/>
-      <c r="AJ21" s="28"/>
-      <c r="AK21" s="28"/>
-    </row>
-    <row r="22" spans="1:37" s="28" customFormat="1" ht="15" customHeight="1">
+    </row>
+    <row r="22" spans="1:35" s="28" customFormat="1" ht="15" customHeight="1">
       <c r="A22" s="28">
         <v>21</v>
       </c>
@@ -8340,16 +8287,16 @@
         <v>127</v>
       </c>
       <c r="H22" s="28" t="s">
-        <v>469</v>
+        <v>466</v>
       </c>
       <c r="I22" s="28" t="s">
         <v>92</v>
       </c>
       <c r="K22" s="28" t="s">
-        <v>470</v>
+        <v>467</v>
       </c>
       <c r="L22" s="28" t="s">
-        <v>471</v>
+        <v>468</v>
       </c>
       <c r="M22" s="28">
         <v>3</v>
@@ -8370,7 +8317,7 @@
         <v>140</v>
       </c>
       <c r="S22" s="28" t="s">
-        <v>468</v>
+        <v>465</v>
       </c>
       <c r="T22" s="28" t="s">
         <v>107</v>
@@ -8378,24 +8325,24 @@
       <c r="U22" s="28" t="s">
         <v>108</v>
       </c>
+      <c r="V22" s="28" t="s">
+        <v>120</v>
+      </c>
       <c r="X22" s="28" t="s">
         <v>120</v>
       </c>
-      <c r="Z22" s="28" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="23" spans="1:37" ht="15" customHeight="1">
+    </row>
+    <row r="23" spans="1:35" ht="15" customHeight="1">
       <c r="A23" s="28">
         <v>22</v>
       </c>
-      <c r="B23" s="73" t="s">
-        <v>676</v>
+      <c r="B23" s="72" t="s">
+        <v>667</v>
       </c>
       <c r="C23" s="28" t="s">
         <v>141</v>
       </c>
-      <c r="D23" s="73" t="s">
+      <c r="D23" s="72" t="s">
         <v>86</v>
       </c>
       <c r="E23" s="28" t="s">
@@ -8443,8 +8390,8 @@
       <c r="U23" s="29" t="s">
         <v>108</v>
       </c>
-      <c r="V23" s="29"/>
-      <c r="W23" s="29"/>
+      <c r="V23" s="28"/>
+      <c r="W23" s="28"/>
       <c r="X23" s="28"/>
       <c r="Y23" s="28"/>
       <c r="Z23" s="28"/>
@@ -8457,10 +8404,8 @@
       <c r="AG23" s="28"/>
       <c r="AH23" s="28"/>
       <c r="AI23" s="28"/>
-      <c r="AJ23" s="28"/>
-      <c r="AK23" s="28"/>
-    </row>
-    <row r="24" spans="1:37" s="28" customFormat="1" ht="15" customHeight="1">
+    </row>
+    <row r="24" spans="1:35" s="28" customFormat="1" ht="15" customHeight="1">
       <c r="A24" s="28">
         <v>23</v>
       </c>
@@ -8483,13 +8428,13 @@
         <v>122</v>
       </c>
       <c r="H24" s="28" t="s">
-        <v>473</v>
+        <v>470</v>
       </c>
       <c r="I24" s="28" t="s">
         <v>92</v>
       </c>
       <c r="K24" s="28" t="s">
-        <v>444</v>
+        <v>443</v>
       </c>
       <c r="L24" s="28" t="s">
         <v>146</v>
@@ -8513,7 +8458,7 @@
         <v>123</v>
       </c>
       <c r="S24" s="28" t="s">
-        <v>472</v>
+        <v>469</v>
       </c>
       <c r="T24" s="28" t="s">
         <v>107</v>
@@ -8522,7 +8467,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="25" spans="1:37" ht="15" customHeight="1">
+    <row r="25" spans="1:35" ht="15" customHeight="1">
       <c r="A25" s="28">
         <v>24</v>
       </c>
@@ -8594,15 +8539,13 @@
       <c r="AG25" s="28"/>
       <c r="AH25" s="28"/>
       <c r="AI25" s="28"/>
-      <c r="AJ25" s="28"/>
-      <c r="AK25" s="28"/>
-    </row>
-    <row r="26" spans="1:37" s="28" customFormat="1" ht="15" customHeight="1">
+    </row>
+    <row r="26" spans="1:35" s="28" customFormat="1" ht="15" customHeight="1">
       <c r="A26" s="28">
         <v>25</v>
       </c>
-      <c r="B26" s="73" t="s">
-        <v>676</v>
+      <c r="B26" s="72" t="s">
+        <v>667</v>
       </c>
       <c r="C26" s="28" t="s">
         <v>152</v>
@@ -8620,16 +8563,16 @@
         <v>154</v>
       </c>
       <c r="H26" s="28" t="s">
-        <v>615</v>
+        <v>606</v>
       </c>
       <c r="I26" s="28" t="s">
         <v>92</v>
       </c>
-      <c r="K26" s="73" t="s">
+      <c r="K26" s="72" t="s">
         <v>226</v>
       </c>
       <c r="L26" s="28" t="s">
-        <v>616</v>
+        <v>607</v>
       </c>
       <c r="M26" s="28">
         <v>2</v>
@@ -8647,7 +8590,7 @@
         <v>152</v>
       </c>
       <c r="S26" s="28" t="s">
-        <v>614</v>
+        <v>605</v>
       </c>
       <c r="T26" s="28" t="s">
         <v>83</v>
@@ -8656,12 +8599,12 @@
         <v>151</v>
       </c>
     </row>
-    <row r="27" spans="1:37" ht="15" customHeight="1">
+    <row r="27" spans="1:35" ht="15" customHeight="1">
       <c r="A27" s="28">
         <v>26</v>
       </c>
-      <c r="B27" s="73" t="s">
-        <v>676</v>
+      <c r="B27" s="72" t="s">
+        <v>667</v>
       </c>
       <c r="C27" s="28" t="s">
         <v>155</v>
@@ -8669,8 +8612,8 @@
       <c r="D27" s="28" t="s">
         <v>78</v>
       </c>
-      <c r="E27" s="69" t="s">
-        <v>682</v>
+      <c r="E27" s="68" t="s">
+        <v>79</v>
       </c>
       <c r="F27" s="30" t="s">
         <v>96</v>
@@ -8678,18 +8621,18 @@
       <c r="G27" s="28" t="s">
         <v>80</v>
       </c>
-      <c r="H27" s="69" t="s">
+      <c r="H27" s="68" t="s">
         <v>210</v>
       </c>
       <c r="I27" s="28" t="s">
         <v>92</v>
       </c>
       <c r="J27" s="28"/>
-      <c r="K27" s="73" t="s">
-        <v>684</v>
-      </c>
-      <c r="L27" s="69" t="s">
-        <v>685</v>
+      <c r="K27" s="72" t="s">
+        <v>674</v>
+      </c>
+      <c r="L27" s="68" t="s">
+        <v>675</v>
       </c>
       <c r="M27" s="28">
         <v>2</v>
@@ -8707,8 +8650,8 @@
       <c r="R27" s="28" t="s">
         <v>155</v>
       </c>
-      <c r="S27" s="69" t="s">
-        <v>683</v>
+      <c r="S27" s="68" t="s">
+        <v>673</v>
       </c>
       <c r="T27" s="28" t="s">
         <v>83</v>
@@ -8730,10 +8673,8 @@
       <c r="AG27" s="28"/>
       <c r="AH27" s="28"/>
       <c r="AI27" s="28"/>
-      <c r="AJ27" s="28"/>
-      <c r="AK27" s="28"/>
-    </row>
-    <row r="28" spans="1:37" s="28" customFormat="1" ht="15" customHeight="1">
+    </row>
+    <row r="28" spans="1:35" s="28" customFormat="1" ht="15" customHeight="1">
       <c r="A28" s="28">
         <v>27</v>
       </c>
@@ -8756,16 +8697,16 @@
         <v>148</v>
       </c>
       <c r="H28" s="28" t="s">
-        <v>475</v>
+        <v>472</v>
       </c>
       <c r="I28" s="28" t="s">
         <v>92</v>
       </c>
       <c r="K28" s="28" t="s">
-        <v>476</v>
+        <v>473</v>
       </c>
       <c r="L28" s="28" t="s">
-        <v>617</v>
+        <v>608</v>
       </c>
       <c r="M28" s="28">
         <v>4</v>
@@ -8783,7 +8724,7 @@
         <v>156</v>
       </c>
       <c r="S28" s="28" t="s">
-        <v>474</v>
+        <v>471</v>
       </c>
       <c r="T28" s="28" t="s">
         <v>83</v>
@@ -8792,12 +8733,12 @@
         <v>151</v>
       </c>
     </row>
-    <row r="29" spans="1:37" ht="15" customHeight="1">
+    <row r="29" spans="1:35" ht="15" customHeight="1">
       <c r="A29" s="28">
         <v>28</v>
       </c>
-      <c r="B29" s="73" t="s">
-        <v>676</v>
+      <c r="B29" s="72" t="s">
+        <v>667</v>
       </c>
       <c r="C29" s="28" t="s">
         <v>157</v>
@@ -8805,8 +8746,8 @@
       <c r="D29" s="28" t="s">
         <v>86</v>
       </c>
-      <c r="E29" s="69" t="s">
-        <v>686</v>
+      <c r="E29" s="68" t="s">
+        <v>676</v>
       </c>
       <c r="F29" s="30" t="s">
         <v>96</v>
@@ -8814,18 +8755,18 @@
       <c r="G29" s="28" t="s">
         <v>87</v>
       </c>
-      <c r="H29" s="69" t="s">
-        <v>688</v>
+      <c r="H29" s="68" t="s">
+        <v>678</v>
       </c>
       <c r="I29" s="28" t="s">
         <v>92</v>
       </c>
       <c r="J29" s="28"/>
-      <c r="K29" s="73" t="s">
-        <v>689</v>
-      </c>
-      <c r="L29" s="69" t="s">
-        <v>690</v>
+      <c r="K29" s="72" t="s">
+        <v>679</v>
+      </c>
+      <c r="L29" s="68" t="s">
+        <v>680</v>
       </c>
       <c r="M29" s="28">
         <v>4</v>
@@ -8843,8 +8784,8 @@
       <c r="R29" s="28" t="s">
         <v>157</v>
       </c>
-      <c r="S29" s="69" t="s">
-        <v>687</v>
+      <c r="S29" s="68" t="s">
+        <v>677</v>
       </c>
       <c r="T29" s="28" t="s">
         <v>83</v>
@@ -8866,10 +8807,8 @@
       <c r="AG29" s="28"/>
       <c r="AH29" s="28"/>
       <c r="AI29" s="28"/>
-      <c r="AJ29" s="28"/>
-      <c r="AK29" s="28"/>
-    </row>
-    <row r="30" spans="1:37" s="28" customFormat="1" ht="15" customHeight="1">
+    </row>
+    <row r="30" spans="1:35" s="28" customFormat="1" ht="15" customHeight="1">
       <c r="A30" s="28">
         <v>29</v>
       </c>
@@ -8886,13 +8825,13 @@
         <v>183</v>
       </c>
       <c r="F30" s="28" t="s">
-        <v>477</v>
+        <v>705</v>
       </c>
       <c r="G30" s="28" t="s">
         <v>154</v>
       </c>
       <c r="H30" s="28" t="s">
-        <v>478</v>
+        <v>474</v>
       </c>
       <c r="I30" s="28" t="s">
         <v>92</v>
@@ -8928,12 +8867,12 @@
         <v>151</v>
       </c>
     </row>
-    <row r="31" spans="1:37" ht="15" customHeight="1">
+    <row r="31" spans="1:35" ht="15" customHeight="1">
       <c r="A31" s="28">
         <v>30</v>
       </c>
-      <c r="B31" s="73" t="s">
-        <v>676</v>
+      <c r="B31" s="72" t="s">
+        <v>667</v>
       </c>
       <c r="C31" s="28" t="s">
         <v>159</v>
@@ -8941,7 +8880,7 @@
       <c r="D31" s="28" t="s">
         <v>78</v>
       </c>
-      <c r="E31" s="69" t="s">
+      <c r="E31" s="68" t="s">
         <v>184</v>
       </c>
       <c r="F31" s="30" t="s">
@@ -8950,13 +8889,13 @@
       <c r="G31" s="28" t="s">
         <v>160</v>
       </c>
-      <c r="H31" s="69" t="s">
+      <c r="H31" s="68" t="s">
         <v>210</v>
       </c>
       <c r="I31" s="28"/>
       <c r="J31" s="28"/>
-      <c r="K31" s="73" t="s">
-        <v>692</v>
+      <c r="K31" s="72" t="s">
+        <v>682</v>
       </c>
       <c r="L31" s="28" t="s">
         <v>161</v>
@@ -8968,17 +8907,17 @@
         <v>1</v>
       </c>
       <c r="O31" s="28"/>
-      <c r="P31" s="69" t="s">
+      <c r="P31" s="68" t="s">
         <v>210</v>
       </c>
-      <c r="Q31" s="69" t="s">
+      <c r="Q31" s="68" t="s">
         <v>210</v>
       </c>
       <c r="R31" s="28" t="s">
         <v>159</v>
       </c>
-      <c r="S31" s="69" t="s">
-        <v>691</v>
+      <c r="S31" s="68" t="s">
+        <v>681</v>
       </c>
       <c r="T31" s="28" t="s">
         <v>83</v>
@@ -9000,10 +8939,8 @@
       <c r="AG31" s="28"/>
       <c r="AH31" s="28"/>
       <c r="AI31" s="28"/>
-      <c r="AJ31" s="28"/>
-      <c r="AK31" s="28"/>
-    </row>
-    <row r="32" spans="1:37" s="28" customFormat="1" ht="15" customHeight="1">
+    </row>
+    <row r="32" spans="1:35" s="28" customFormat="1" ht="15" customHeight="1">
       <c r="A32" s="28">
         <v>31</v>
       </c>
@@ -9026,7 +8963,7 @@
         <v>87</v>
       </c>
       <c r="H32" s="28" t="s">
-        <v>480</v>
+        <v>476</v>
       </c>
       <c r="I32" s="28" t="s">
         <v>92</v>
@@ -9053,7 +8990,7 @@
         <v>162</v>
       </c>
       <c r="S32" s="28" t="s">
-        <v>479</v>
+        <v>475</v>
       </c>
       <c r="T32" s="28" t="s">
         <v>83</v>
@@ -9062,7 +8999,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="33" spans="1:21" s="28" customFormat="1" ht="13.5">
+    <row r="33" spans="1:21" s="28" customFormat="1" ht="13.8">
       <c r="A33" s="28" t="s">
         <v>206</v>
       </c>
@@ -9121,7 +9058,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="34" spans="1:21" s="28" customFormat="1" ht="13.5">
+    <row r="34" spans="1:21" s="28" customFormat="1" ht="13.8">
       <c r="A34" s="28" t="s">
         <v>217</v>
       </c>
@@ -9180,7 +9117,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="35" spans="1:21" s="28" customFormat="1" ht="13.5">
+    <row r="35" spans="1:21" s="28" customFormat="1" ht="13.8">
       <c r="A35" s="28" t="s">
         <v>224</v>
       </c>
@@ -9239,7 +9176,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="36" spans="1:21" s="28" customFormat="1" ht="13.5">
+    <row r="36" spans="1:21" s="28" customFormat="1" ht="13.8">
       <c r="A36" s="28" t="s">
         <v>230</v>
       </c>
@@ -9298,7 +9235,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="37" spans="1:21" s="28" customFormat="1" ht="13.5">
+    <row r="37" spans="1:21" s="28" customFormat="1" ht="13.8">
       <c r="A37" s="28" t="s">
         <v>237</v>
       </c>
@@ -9357,7 +9294,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="38" spans="1:21" s="28" customFormat="1" ht="13.5">
+    <row r="38" spans="1:21" s="28" customFormat="1" ht="13.8">
       <c r="A38" s="28" t="s">
         <v>243</v>
       </c>
@@ -9416,7 +9353,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="39" spans="1:21" s="28" customFormat="1" ht="13.5">
+    <row r="39" spans="1:21" s="28" customFormat="1" ht="13.8">
       <c r="A39" s="28" t="s">
         <v>251</v>
       </c>
@@ -9475,7 +9412,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="40" spans="1:21" s="28" customFormat="1" ht="13.5">
+    <row r="40" spans="1:21" s="28" customFormat="1" ht="13.8">
       <c r="A40" s="28" t="s">
         <v>254</v>
       </c>
@@ -9534,7 +9471,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="41" spans="1:21" s="28" customFormat="1" ht="13.5">
+    <row r="41" spans="1:21" s="28" customFormat="1" ht="13.8">
       <c r="A41" s="28" t="s">
         <v>257</v>
       </c>
@@ -9593,7 +9530,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="42" spans="1:21" s="28" customFormat="1" ht="13.5">
+    <row r="42" spans="1:21" s="28" customFormat="1" ht="13.8">
       <c r="A42" s="28" t="s">
         <v>266</v>
       </c>
@@ -9652,7 +9589,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="43" spans="1:21" s="28" customFormat="1" ht="13.5">
+    <row r="43" spans="1:21" s="28" customFormat="1" ht="13.8">
       <c r="A43" s="28" t="s">
         <v>270</v>
       </c>
@@ -9711,7 +9648,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="44" spans="1:21" s="28" customFormat="1" ht="13.5">
+    <row r="44" spans="1:21" s="28" customFormat="1" ht="13.8">
       <c r="A44" s="28" t="s">
         <v>279</v>
       </c>
@@ -9770,7 +9707,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="45" spans="1:21" s="28" customFormat="1" ht="13.5">
+    <row r="45" spans="1:21" s="28" customFormat="1" ht="13.8">
       <c r="A45" s="28" t="s">
         <v>286</v>
       </c>
@@ -9829,7 +9766,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="46" spans="1:21" s="28" customFormat="1" ht="13.5">
+    <row r="46" spans="1:21" s="28" customFormat="1" ht="13.8">
       <c r="A46" s="28" t="s">
         <v>292</v>
       </c>
@@ -9888,7 +9825,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="47" spans="1:21" s="28" customFormat="1" ht="13.5">
+    <row r="47" spans="1:21" s="28" customFormat="1" ht="13.8">
       <c r="A47" s="28" t="s">
         <v>298</v>
       </c>
@@ -9947,7 +9884,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="48" spans="1:21" s="28" customFormat="1" ht="13.5">
+    <row r="48" spans="1:21" s="28" customFormat="1" ht="13.8">
       <c r="A48" s="28" t="s">
         <v>304</v>
       </c>
@@ -10006,7 +9943,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="49" spans="1:21" s="28" customFormat="1" ht="13.5">
+    <row r="49" spans="1:21" s="28" customFormat="1" ht="13.8">
       <c r="A49" s="28" t="s">
         <v>309</v>
       </c>
@@ -10065,7 +10002,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="50" spans="1:21" s="28" customFormat="1" ht="13.5">
+    <row r="50" spans="1:21" s="28" customFormat="1" ht="13.8">
       <c r="A50" s="28" t="s">
         <v>315</v>
       </c>
@@ -10124,7 +10061,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="51" spans="1:21" s="28" customFormat="1" ht="13.5">
+    <row r="51" spans="1:21" s="28" customFormat="1" ht="13.8">
       <c r="A51" s="28" t="s">
         <v>321</v>
       </c>
@@ -10183,7 +10120,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="52" spans="1:21" s="28" customFormat="1" ht="13.5">
+    <row r="52" spans="1:21" s="28" customFormat="1" ht="13.8">
       <c r="A52" s="28" t="s">
         <v>327</v>
       </c>
@@ -10242,7 +10179,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="53" spans="1:21" s="28" customFormat="1" ht="13.5">
+    <row r="53" spans="1:21" s="28" customFormat="1" ht="13.8">
       <c r="A53" s="28" t="s">
         <v>354</v>
       </c>
@@ -10301,7 +10238,7 @@
         <v>336</v>
       </c>
     </row>
-    <row r="54" spans="1:21" ht="12.75">
+    <row r="54" spans="1:21" ht="13.2">
       <c r="A54" t="s">
         <v>360</v>
       </c>
@@ -10360,7 +10297,7 @@
         <v>336</v>
       </c>
     </row>
-    <row r="55" spans="1:21" s="28" customFormat="1" ht="13.5">
+    <row r="55" spans="1:21" s="28" customFormat="1" ht="13.8">
       <c r="A55" s="28" t="s">
         <v>364</v>
       </c>
@@ -10419,7 +10356,7 @@
         <v>336</v>
       </c>
     </row>
-    <row r="56" spans="1:21" s="28" customFormat="1" ht="13.5">
+    <row r="56" spans="1:21" s="28" customFormat="1" ht="13.8">
       <c r="A56" s="28" t="s">
         <v>370</v>
       </c>
@@ -10478,7 +10415,7 @@
         <v>336</v>
       </c>
     </row>
-    <row r="57" spans="1:21" s="28" customFormat="1" ht="13.5">
+    <row r="57" spans="1:21" s="28" customFormat="1" ht="13.8">
       <c r="A57" s="28" t="s">
         <v>375</v>
       </c>
@@ -10537,7 +10474,7 @@
         <v>336</v>
       </c>
     </row>
-    <row r="58" spans="1:21" s="28" customFormat="1" ht="13.5">
+    <row r="58" spans="1:21" s="28" customFormat="1" ht="13.8">
       <c r="A58" s="28" t="s">
         <v>382</v>
       </c>
@@ -10596,7 +10533,7 @@
         <v>336</v>
       </c>
     </row>
-    <row r="59" spans="1:21" s="28" customFormat="1" ht="13.5">
+    <row r="59" spans="1:21" s="28" customFormat="1" ht="13.8">
       <c r="A59" s="28" t="s">
         <v>388</v>
       </c>
@@ -10655,7 +10592,7 @@
         <v>336</v>
       </c>
     </row>
-    <row r="60" spans="1:21" s="28" customFormat="1" ht="13.5">
+    <row r="60" spans="1:21" s="28" customFormat="1" ht="13.8">
       <c r="A60" s="28" t="s">
         <v>395</v>
       </c>
@@ -10714,7 +10651,7 @@
         <v>336</v>
       </c>
     </row>
-    <row r="61" spans="1:21" s="28" customFormat="1" ht="13.5">
+    <row r="61" spans="1:21" s="28" customFormat="1" ht="13.8">
       <c r="A61" s="28" t="s">
         <v>402</v>
       </c>
@@ -10773,7 +10710,7 @@
         <v>336</v>
       </c>
     </row>
-    <row r="62" spans="1:21" s="28" customFormat="1" ht="13.5">
+    <row r="62" spans="1:21" s="28" customFormat="1" ht="13.8">
       <c r="A62" s="28" t="s">
         <v>408</v>
       </c>
@@ -10832,7 +10769,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="63" spans="1:21" s="28" customFormat="1" ht="13.5">
+    <row r="63" spans="1:21" s="28" customFormat="1" ht="13.8">
       <c r="A63" s="28" t="s">
         <v>411</v>
       </c>
@@ -10891,7 +10828,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="64" spans="1:21" s="28" customFormat="1" ht="13.5">
+    <row r="64" spans="1:21" s="28" customFormat="1" ht="13.8">
       <c r="A64" s="28" t="s">
         <v>416</v>
       </c>
@@ -10950,7 +10887,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="65" spans="1:23" s="28" customFormat="1" ht="13.5">
+    <row r="65" spans="1:21" s="28" customFormat="1" ht="13.8">
       <c r="A65" s="28" t="s">
         <v>422</v>
       </c>
@@ -11009,7 +10946,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="66" spans="1:23" s="28" customFormat="1" ht="13.5">
+    <row r="66" spans="1:21" s="28" customFormat="1" ht="13.8">
       <c r="A66" s="28" t="s">
         <v>427</v>
       </c>
@@ -11068,7 +11005,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="67" spans="1:23" s="28" customFormat="1" ht="13.5">
+    <row r="67" spans="1:21" s="28" customFormat="1" ht="13.8">
       <c r="A67" s="28" t="s">
         <v>433</v>
       </c>
@@ -11100,7 +11037,7 @@
         <v>825000</v>
       </c>
       <c r="L67" s="28" t="s">
-        <v>659</v>
+        <v>650</v>
       </c>
       <c r="M67" s="28" t="s">
         <v>212</v>
@@ -11118,7 +11055,7 @@
         <v>434</v>
       </c>
       <c r="S67" s="28" t="s">
-        <v>498</v>
+        <v>494</v>
       </c>
       <c r="T67" s="28" t="s">
         <v>107</v>
@@ -11127,15 +11064,15 @@
         <v>17</v>
       </c>
     </row>
-    <row r="68" spans="1:23" s="28" customFormat="1" ht="13.5">
+    <row r="68" spans="1:21" s="28" customFormat="1" ht="13.8">
       <c r="A68" s="28" t="s">
-        <v>499</v>
+        <v>495</v>
       </c>
       <c r="B68" s="28" t="s">
         <v>7</v>
       </c>
       <c r="C68" s="28" t="s">
-        <v>500</v>
+        <v>496</v>
       </c>
       <c r="D68" s="28" t="s">
         <v>86</v>
@@ -11150,7 +11087,7 @@
         <v>232</v>
       </c>
       <c r="H68" s="28" t="s">
-        <v>501</v>
+        <v>497</v>
       </c>
       <c r="I68" s="28" t="s">
         <v>209</v>
@@ -11159,7 +11096,7 @@
         <v>210</v>
       </c>
       <c r="L68" s="28" t="s">
-        <v>502</v>
+        <v>498</v>
       </c>
       <c r="M68" s="28" t="s">
         <v>213</v>
@@ -11174,10 +11111,10 @@
         <v>215</v>
       </c>
       <c r="R68" s="28" t="s">
-        <v>500</v>
+        <v>496</v>
       </c>
       <c r="S68" s="28" t="s">
-        <v>503</v>
+        <v>499</v>
       </c>
       <c r="T68" s="28" t="s">
         <v>83</v>
@@ -11185,22 +11122,16 @@
       <c r="U68" s="28" t="s">
         <v>9</v>
       </c>
-      <c r="V68" s="63">
-        <v>44339</v>
-      </c>
-      <c r="W68" s="28" t="s">
-        <v>604</v>
-      </c>
-    </row>
-    <row r="69" spans="1:23" s="28" customFormat="1" ht="13.5">
+    </row>
+    <row r="69" spans="1:21" s="28" customFormat="1" ht="13.8">
       <c r="A69" s="28" t="s">
-        <v>504</v>
+        <v>500</v>
       </c>
       <c r="B69" s="28" t="s">
         <v>7</v>
       </c>
       <c r="C69" s="28" t="s">
-        <v>505</v>
+        <v>501</v>
       </c>
       <c r="D69" s="28" t="s">
         <v>272</v>
@@ -11239,10 +11170,10 @@
         <v>277</v>
       </c>
       <c r="R69" s="28" t="s">
-        <v>505</v>
+        <v>501</v>
       </c>
       <c r="S69" s="28" t="s">
-        <v>606</v>
+        <v>599</v>
       </c>
       <c r="T69" s="28" t="s">
         <v>83</v>
@@ -11250,22 +11181,16 @@
       <c r="U69" s="28" t="s">
         <v>9</v>
       </c>
-      <c r="V69" s="63">
-        <v>44339</v>
-      </c>
-      <c r="W69" s="28" t="s">
-        <v>604</v>
-      </c>
-    </row>
-    <row r="70" spans="1:23" s="28" customFormat="1" ht="13.5">
+    </row>
+    <row r="70" spans="1:21" s="28" customFormat="1" ht="13.8">
       <c r="A70" s="28" t="s">
-        <v>506</v>
+        <v>502</v>
       </c>
       <c r="B70" s="28" t="s">
         <v>7</v>
       </c>
       <c r="C70" s="28" t="s">
-        <v>507</v>
+        <v>503</v>
       </c>
       <c r="D70" s="28" t="s">
         <v>86</v>
@@ -11280,16 +11205,16 @@
         <v>118</v>
       </c>
       <c r="H70" s="28" t="s">
-        <v>508</v>
+        <v>504</v>
       </c>
       <c r="I70" s="28" t="s">
         <v>209</v>
       </c>
       <c r="K70" s="28" t="s">
-        <v>509</v>
+        <v>505</v>
       </c>
       <c r="L70" s="28" t="s">
-        <v>510</v>
+        <v>506</v>
       </c>
       <c r="M70" s="28" t="s">
         <v>215</v>
@@ -11304,10 +11229,10 @@
         <v>215</v>
       </c>
       <c r="R70" s="28" t="s">
+        <v>503</v>
+      </c>
+      <c r="S70" s="28" t="s">
         <v>507</v>
-      </c>
-      <c r="S70" s="28" t="s">
-        <v>511</v>
       </c>
       <c r="T70" s="28" t="s">
         <v>83</v>
@@ -11315,22 +11240,16 @@
       <c r="U70" s="28" t="s">
         <v>9</v>
       </c>
-      <c r="V70" s="63">
-        <v>44339</v>
-      </c>
-      <c r="W70" s="28" t="s">
-        <v>604</v>
-      </c>
-    </row>
-    <row r="71" spans="1:23" s="28" customFormat="1" ht="13.5">
+    </row>
+    <row r="71" spans="1:21" s="28" customFormat="1" ht="13.8">
       <c r="A71" s="28" t="s">
-        <v>512</v>
+        <v>508</v>
       </c>
       <c r="B71" s="28" t="s">
         <v>7</v>
       </c>
       <c r="C71" s="28" t="s">
-        <v>513</v>
+        <v>509</v>
       </c>
       <c r="D71" s="28" t="s">
         <v>86</v>
@@ -11345,7 +11264,7 @@
         <v>122</v>
       </c>
       <c r="H71" s="28" t="s">
-        <v>514</v>
+        <v>510</v>
       </c>
       <c r="I71" s="28" t="s">
         <v>209</v>
@@ -11354,7 +11273,7 @@
         <v>312</v>
       </c>
       <c r="L71" s="28" t="s">
-        <v>515</v>
+        <v>511</v>
       </c>
       <c r="M71" s="28" t="s">
         <v>263</v>
@@ -11369,10 +11288,10 @@
         <v>215</v>
       </c>
       <c r="R71" s="28" t="s">
-        <v>513</v>
+        <v>509</v>
       </c>
       <c r="S71" s="28" t="s">
-        <v>516</v>
+        <v>512</v>
       </c>
       <c r="T71" s="28" t="s">
         <v>83</v>
@@ -11380,16 +11299,10 @@
       <c r="U71" s="28" t="s">
         <v>9</v>
       </c>
-      <c r="V71" s="63">
-        <v>44339</v>
-      </c>
-      <c r="W71" s="28" t="s">
-        <v>604</v>
-      </c>
-    </row>
-    <row r="72" spans="1:23" s="28" customFormat="1" ht="13.5">
+    </row>
+    <row r="72" spans="1:21" s="28" customFormat="1" ht="13.8">
       <c r="A72" s="28" t="s">
-        <v>517</v>
+        <v>513</v>
       </c>
       <c r="B72" s="28" t="s">
         <v>7</v>
@@ -11410,7 +11323,7 @@
         <v>103</v>
       </c>
       <c r="H72" s="28" t="s">
-        <v>518</v>
+        <v>514</v>
       </c>
       <c r="I72" s="28" t="s">
         <v>209</v>
@@ -11437,7 +11350,7 @@
         <v>222</v>
       </c>
       <c r="S72" s="28" t="s">
-        <v>607</v>
+        <v>600</v>
       </c>
       <c r="T72" s="28" t="s">
         <v>83</v>
@@ -11445,16 +11358,10 @@
       <c r="U72" s="28" t="s">
         <v>9</v>
       </c>
-      <c r="V72" s="63">
-        <v>44339</v>
-      </c>
-      <c r="W72" s="28" t="s">
-        <v>604</v>
-      </c>
-    </row>
-    <row r="73" spans="1:23" s="28" customFormat="1" ht="13.5">
+    </row>
+    <row r="73" spans="1:21" s="28" customFormat="1" ht="13.8">
       <c r="A73" s="28" t="s">
-        <v>519</v>
+        <v>515</v>
       </c>
       <c r="B73" s="28" t="s">
         <v>7</v>
@@ -11475,16 +11382,16 @@
         <v>87</v>
       </c>
       <c r="H73" s="28" t="s">
-        <v>520</v>
+        <v>516</v>
       </c>
       <c r="I73" s="28" t="s">
         <v>209</v>
       </c>
       <c r="K73" s="28" t="s">
-        <v>453</v>
+        <v>451</v>
       </c>
       <c r="L73" s="28" t="s">
-        <v>521</v>
+        <v>517</v>
       </c>
       <c r="M73" s="28" t="s">
         <v>213</v>
@@ -11502,7 +11409,7 @@
         <v>228</v>
       </c>
       <c r="S73" s="28" t="s">
-        <v>522</v>
+        <v>518</v>
       </c>
       <c r="T73" s="28" t="s">
         <v>107</v>
@@ -11511,15 +11418,15 @@
         <v>17</v>
       </c>
     </row>
-    <row r="74" spans="1:23" s="28" customFormat="1" ht="13.5">
+    <row r="74" spans="1:21" s="28" customFormat="1" ht="13.8">
       <c r="A74" s="28" t="s">
-        <v>523</v>
+        <v>519</v>
       </c>
       <c r="B74" s="28" t="s">
         <v>7</v>
       </c>
       <c r="C74" s="28" t="s">
-        <v>524</v>
+        <v>520</v>
       </c>
       <c r="D74" s="28" t="s">
         <v>272</v>
@@ -11534,16 +11441,16 @@
         <v>232</v>
       </c>
       <c r="H74" s="28" t="s">
-        <v>525</v>
+        <v>521</v>
       </c>
       <c r="I74" s="28" t="s">
         <v>209</v>
       </c>
       <c r="K74" s="28" t="s">
-        <v>526</v>
+        <v>522</v>
       </c>
       <c r="L74" s="28" t="s">
-        <v>527</v>
+        <v>523</v>
       </c>
       <c r="M74" s="28" t="s">
         <v>212</v>
@@ -11558,10 +11465,10 @@
         <v>210</v>
       </c>
       <c r="R74" s="28" t="s">
+        <v>520</v>
+      </c>
+      <c r="S74" s="28" t="s">
         <v>524</v>
-      </c>
-      <c r="S74" s="28" t="s">
-        <v>528</v>
       </c>
       <c r="T74" s="28" t="s">
         <v>107</v>
@@ -11570,15 +11477,15 @@
         <v>17</v>
       </c>
     </row>
-    <row r="75" spans="1:23" s="28" customFormat="1" ht="13.5">
+    <row r="75" spans="1:21" s="28" customFormat="1" ht="13.8">
       <c r="A75" s="28" t="s">
-        <v>529</v>
+        <v>525</v>
       </c>
       <c r="B75" s="28" t="s">
         <v>7</v>
       </c>
       <c r="C75" s="28" t="s">
-        <v>530</v>
+        <v>526</v>
       </c>
       <c r="D75" s="28" t="s">
         <v>86</v>
@@ -11593,16 +11500,16 @@
         <v>247</v>
       </c>
       <c r="H75" s="28" t="s">
-        <v>531</v>
+        <v>527</v>
       </c>
       <c r="I75" s="28" t="s">
         <v>209</v>
       </c>
       <c r="K75" s="28" t="s">
-        <v>532</v>
+        <v>528</v>
       </c>
       <c r="L75" s="28" t="s">
-        <v>533</v>
+        <v>529</v>
       </c>
       <c r="M75" s="28" t="s">
         <v>213</v>
@@ -11617,10 +11524,10 @@
         <v>215</v>
       </c>
       <c r="R75" s="28" t="s">
+        <v>526</v>
+      </c>
+      <c r="S75" s="28" t="s">
         <v>530</v>
-      </c>
-      <c r="S75" s="28" t="s">
-        <v>534</v>
       </c>
       <c r="T75" s="28" t="s">
         <v>107</v>
@@ -11628,16 +11535,10 @@
       <c r="U75" s="28" t="s">
         <v>17</v>
       </c>
-      <c r="V75" s="63">
-        <v>44339</v>
-      </c>
-      <c r="W75" s="28" t="s">
-        <v>604</v>
-      </c>
-    </row>
-    <row r="76" spans="1:23" s="28" customFormat="1" ht="13.5">
+    </row>
+    <row r="76" spans="1:21" s="28" customFormat="1" ht="13.8">
       <c r="A76" s="28" t="s">
-        <v>535</v>
+        <v>531</v>
       </c>
       <c r="B76" s="28" t="s">
         <v>7</v>
@@ -11658,16 +11559,16 @@
         <v>87</v>
       </c>
       <c r="H76" s="28" t="s">
-        <v>536</v>
+        <v>532</v>
       </c>
       <c r="I76" s="28" t="s">
         <v>209</v>
       </c>
       <c r="K76" s="28" t="s">
-        <v>537</v>
+        <v>533</v>
       </c>
       <c r="L76" s="28" t="s">
-        <v>538</v>
+        <v>534</v>
       </c>
       <c r="M76" s="28" t="s">
         <v>263</v>
@@ -11685,7 +11586,7 @@
         <v>228</v>
       </c>
       <c r="S76" s="28" t="s">
-        <v>539</v>
+        <v>535</v>
       </c>
       <c r="T76" s="28" t="s">
         <v>107</v>
@@ -11694,15 +11595,15 @@
         <v>17</v>
       </c>
     </row>
-    <row r="77" spans="1:23" s="28" customFormat="1" ht="13.5">
+    <row r="77" spans="1:21" s="28" customFormat="1" ht="13.8">
       <c r="A77" s="28" t="s">
-        <v>540</v>
+        <v>536</v>
       </c>
       <c r="B77" s="28" t="s">
         <v>7</v>
       </c>
       <c r="C77" s="28" t="s">
-        <v>541</v>
+        <v>537</v>
       </c>
       <c r="D77" s="28" t="s">
         <v>272</v>
@@ -11714,19 +11615,19 @@
         <v>218</v>
       </c>
       <c r="G77" s="28" t="s">
-        <v>542</v>
+        <v>538</v>
       </c>
       <c r="H77" s="28" t="s">
-        <v>543</v>
+        <v>539</v>
       </c>
       <c r="I77" s="28" t="s">
         <v>209</v>
       </c>
       <c r="K77" s="28" t="s">
-        <v>544</v>
+        <v>540</v>
       </c>
       <c r="L77" s="28" t="s">
-        <v>545</v>
+        <v>541</v>
       </c>
       <c r="M77" s="28" t="s">
         <v>215</v>
@@ -11741,10 +11642,10 @@
         <v>277</v>
       </c>
       <c r="R77" s="28" t="s">
-        <v>541</v>
+        <v>537</v>
       </c>
       <c r="S77" s="28" t="s">
-        <v>546</v>
+        <v>542</v>
       </c>
       <c r="T77" s="28" t="s">
         <v>107</v>
@@ -11753,15 +11654,15 @@
         <v>17</v>
       </c>
     </row>
-    <row r="78" spans="1:23" s="28" customFormat="1" ht="13.5">
+    <row r="78" spans="1:21" s="28" customFormat="1" ht="13.8">
       <c r="A78" s="28" t="s">
-        <v>547</v>
+        <v>543</v>
       </c>
       <c r="B78" s="28" t="s">
         <v>7</v>
       </c>
       <c r="C78" s="28" t="s">
-        <v>548</v>
+        <v>544</v>
       </c>
       <c r="D78" s="28" t="s">
         <v>86</v>
@@ -11776,13 +11677,13 @@
         <v>103</v>
       </c>
       <c r="H78" s="28" t="s">
-        <v>549</v>
+        <v>545</v>
       </c>
       <c r="I78" s="28" t="s">
         <v>209</v>
       </c>
       <c r="K78" s="28" t="s">
-        <v>444</v>
+        <v>443</v>
       </c>
       <c r="L78" s="28" t="s">
         <v>150</v>
@@ -11800,10 +11701,10 @@
         <v>215</v>
       </c>
       <c r="R78" s="28" t="s">
-        <v>548</v>
+        <v>544</v>
       </c>
       <c r="S78" s="28" t="s">
-        <v>605</v>
+        <v>598</v>
       </c>
       <c r="T78" s="28" t="s">
         <v>107</v>
@@ -11811,22 +11712,16 @@
       <c r="U78" s="28" t="s">
         <v>17</v>
       </c>
-      <c r="V78" s="63">
-        <v>44339</v>
-      </c>
-      <c r="W78" s="28" t="s">
-        <v>604</v>
-      </c>
-    </row>
-    <row r="79" spans="1:23" s="28" customFormat="1" ht="13.5">
+    </row>
+    <row r="79" spans="1:21" s="28" customFormat="1" ht="13.8">
       <c r="A79" s="28" t="s">
-        <v>550</v>
+        <v>546</v>
       </c>
       <c r="B79" s="28" t="s">
         <v>7</v>
       </c>
       <c r="C79" s="28" t="s">
-        <v>551</v>
+        <v>547</v>
       </c>
       <c r="D79" s="28" t="s">
         <v>78</v>
@@ -11841,16 +11736,16 @@
         <v>218</v>
       </c>
       <c r="H79" s="28" t="s">
-        <v>552</v>
+        <v>548</v>
       </c>
       <c r="I79" s="28" t="s">
         <v>209</v>
       </c>
       <c r="K79" s="28" t="s">
-        <v>553</v>
+        <v>549</v>
       </c>
       <c r="L79" s="28" t="s">
-        <v>554</v>
+        <v>550</v>
       </c>
       <c r="M79" s="28" t="s">
         <v>215</v>
@@ -11865,10 +11760,10 @@
         <v>210</v>
       </c>
       <c r="R79" s="28" t="s">
+        <v>547</v>
+      </c>
+      <c r="S79" s="28" t="s">
         <v>551</v>
-      </c>
-      <c r="S79" s="28" t="s">
-        <v>555</v>
       </c>
       <c r="T79" s="28" t="s">
         <v>107</v>
@@ -11877,15 +11772,15 @@
         <v>17</v>
       </c>
     </row>
-    <row r="80" spans="1:23" s="28" customFormat="1" ht="13.5">
+    <row r="80" spans="1:21" s="28" customFormat="1" ht="13.8">
       <c r="A80" s="28" t="s">
-        <v>556</v>
+        <v>552</v>
       </c>
       <c r="B80" s="28" t="s">
         <v>7</v>
       </c>
       <c r="C80" s="28" t="s">
-        <v>557</v>
+        <v>553</v>
       </c>
       <c r="D80" s="28" t="s">
         <v>272</v>
@@ -11900,16 +11795,16 @@
         <v>259</v>
       </c>
       <c r="H80" s="28" t="s">
-        <v>558</v>
+        <v>554</v>
       </c>
       <c r="I80" s="28" t="s">
         <v>209</v>
       </c>
       <c r="K80" s="28" t="s">
-        <v>559</v>
+        <v>555</v>
       </c>
       <c r="L80" s="28" t="s">
-        <v>560</v>
+        <v>556</v>
       </c>
       <c r="M80" s="28" t="s">
         <v>213</v>
@@ -11924,10 +11819,10 @@
         <v>215</v>
       </c>
       <c r="R80" s="28" t="s">
-        <v>561</v>
+        <v>557</v>
       </c>
       <c r="S80" s="28" t="s">
-        <v>562</v>
+        <v>558</v>
       </c>
       <c r="T80" s="28" t="s">
         <v>107</v>
@@ -11936,9 +11831,9 @@
         <v>17</v>
       </c>
     </row>
-    <row r="81" spans="1:21" s="28" customFormat="1" ht="13.5">
+    <row r="81" spans="1:21" s="28" customFormat="1" ht="13.8">
       <c r="A81" s="28" t="s">
-        <v>563</v>
+        <v>559</v>
       </c>
       <c r="B81" s="28" t="s">
         <v>7</v>
@@ -11959,16 +11854,16 @@
         <v>87</v>
       </c>
       <c r="H81" s="28" t="s">
-        <v>564</v>
+        <v>560</v>
       </c>
       <c r="I81" s="28" t="s">
         <v>209</v>
       </c>
       <c r="K81" s="28" t="s">
-        <v>565</v>
+        <v>561</v>
       </c>
       <c r="L81" s="28" t="s">
-        <v>566</v>
+        <v>562</v>
       </c>
       <c r="M81" s="28" t="s">
         <v>263</v>
@@ -11986,7 +11881,7 @@
         <v>228</v>
       </c>
       <c r="S81" s="28" t="s">
-        <v>567</v>
+        <v>563</v>
       </c>
       <c r="T81" s="28" t="s">
         <v>107</v>
@@ -11995,9 +11890,9 @@
         <v>17</v>
       </c>
     </row>
-    <row r="82" spans="1:21" s="28" customFormat="1" ht="13.5">
+    <row r="82" spans="1:21" s="28" customFormat="1" ht="13.8">
       <c r="A82" s="28" t="s">
-        <v>568</v>
+        <v>564</v>
       </c>
       <c r="B82" s="28" t="s">
         <v>7</v>
@@ -12018,16 +11913,16 @@
         <v>127</v>
       </c>
       <c r="H82" s="28" t="s">
-        <v>569</v>
+        <v>565</v>
       </c>
       <c r="I82" s="28" t="s">
         <v>209</v>
       </c>
       <c r="K82" s="28" t="s">
-        <v>570</v>
+        <v>566</v>
       </c>
       <c r="L82" s="28" t="s">
-        <v>571</v>
+        <v>567</v>
       </c>
       <c r="M82" s="28" t="s">
         <v>212</v>
@@ -12045,7 +11940,7 @@
         <v>268</v>
       </c>
       <c r="S82" s="28" t="s">
-        <v>572</v>
+        <v>568</v>
       </c>
       <c r="T82" s="28" t="s">
         <v>107</v>
@@ -12054,9 +11949,9 @@
         <v>17</v>
       </c>
     </row>
-    <row r="83" spans="1:21" s="28" customFormat="1" ht="13.5">
+    <row r="83" spans="1:21" s="28" customFormat="1" ht="13.8">
       <c r="A83" s="28" t="s">
-        <v>573</v>
+        <v>569</v>
       </c>
       <c r="B83" s="28" t="s">
         <v>7</v>
@@ -12077,16 +11972,16 @@
         <v>103</v>
       </c>
       <c r="H83" s="28" t="s">
-        <v>449</v>
+        <v>447</v>
       </c>
       <c r="I83" s="28" t="s">
         <v>209</v>
       </c>
       <c r="K83" s="28" t="s">
-        <v>455</v>
+        <v>453</v>
       </c>
       <c r="L83" s="28" t="s">
-        <v>574</v>
+        <v>570</v>
       </c>
       <c r="M83" s="28" t="s">
         <v>212</v>
@@ -12104,7 +11999,7 @@
         <v>222</v>
       </c>
       <c r="S83" s="28" t="s">
-        <v>575</v>
+        <v>571</v>
       </c>
       <c r="T83" s="28" t="s">
         <v>107</v>
@@ -12113,9 +12008,9 @@
         <v>17</v>
       </c>
     </row>
-    <row r="84" spans="1:21" s="28" customFormat="1" ht="13.5">
+    <row r="84" spans="1:21" s="28" customFormat="1" ht="13.8">
       <c r="A84" s="28" t="s">
-        <v>576</v>
+        <v>572</v>
       </c>
       <c r="B84" s="28" t="s">
         <v>7</v>
@@ -12136,16 +12031,16 @@
         <v>118</v>
       </c>
       <c r="H84" s="28" t="s">
-        <v>577</v>
+        <v>573</v>
       </c>
       <c r="I84" s="28" t="s">
         <v>209</v>
       </c>
       <c r="K84" s="28" t="s">
-        <v>559</v>
+        <v>555</v>
       </c>
       <c r="L84" s="28" t="s">
-        <v>560</v>
+        <v>556</v>
       </c>
       <c r="M84" s="28" t="s">
         <v>212</v>
@@ -12160,10 +12055,10 @@
         <v>215</v>
       </c>
       <c r="R84" s="28" t="s">
-        <v>578</v>
+        <v>574</v>
       </c>
       <c r="S84" s="28" t="s">
-        <v>579</v>
+        <v>575</v>
       </c>
       <c r="T84" s="28" t="s">
         <v>107</v>
@@ -12172,15 +12067,15 @@
         <v>17</v>
       </c>
     </row>
-    <row r="85" spans="1:21" s="28" customFormat="1" ht="13.5">
+    <row r="85" spans="1:21" s="28" customFormat="1" ht="13.8">
       <c r="A85" s="28" t="s">
-        <v>580</v>
+        <v>576</v>
       </c>
       <c r="B85" s="28" t="s">
         <v>7</v>
       </c>
       <c r="C85" s="28" t="s">
-        <v>581</v>
+        <v>577</v>
       </c>
       <c r="D85" s="28" t="s">
         <v>78</v>
@@ -12192,19 +12087,19 @@
         <v>153</v>
       </c>
       <c r="G85" s="28" t="s">
-        <v>582</v>
+        <v>578</v>
       </c>
       <c r="H85" s="28" t="s">
-        <v>660</v>
+        <v>651</v>
       </c>
       <c r="I85" s="28" t="s">
-        <v>661</v>
+        <v>652</v>
       </c>
       <c r="K85" s="28">
         <v>349000</v>
       </c>
       <c r="L85" s="28" t="s">
-        <v>662</v>
+        <v>653</v>
       </c>
       <c r="M85" s="28">
         <v>1</v>
@@ -12219,10 +12114,10 @@
         <v>277</v>
       </c>
       <c r="R85" s="28" t="s">
-        <v>581</v>
+        <v>577</v>
       </c>
       <c r="S85" s="28" t="s">
-        <v>663</v>
+        <v>654</v>
       </c>
       <c r="T85" s="28" t="s">
         <v>107</v>
@@ -12231,15 +12126,15 @@
         <v>17</v>
       </c>
     </row>
-    <row r="86" spans="1:21" s="28" customFormat="1" ht="13.5">
+    <row r="86" spans="1:21" s="28" customFormat="1" ht="13.8">
       <c r="A86" s="28" t="s">
-        <v>626</v>
+        <v>617</v>
       </c>
       <c r="B86" s="28" t="s">
         <v>7</v>
       </c>
       <c r="C86" s="28" t="s">
-        <v>627</v>
+        <v>618</v>
       </c>
       <c r="D86" s="28" t="s">
         <v>86</v>
@@ -12254,7 +12149,7 @@
         <v>122</v>
       </c>
       <c r="H86" s="28" t="s">
-        <v>628</v>
+        <v>619</v>
       </c>
       <c r="I86" s="28" t="s">
         <v>209</v>
@@ -12263,7 +12158,7 @@
         <v>210</v>
       </c>
       <c r="L86" s="28" t="s">
-        <v>502</v>
+        <v>498</v>
       </c>
       <c r="M86" s="28" t="s">
         <v>212</v>
@@ -12278,10 +12173,10 @@
         <v>215</v>
       </c>
       <c r="R86" s="28" t="s">
-        <v>627</v>
+        <v>618</v>
       </c>
       <c r="S86" s="28" t="s">
-        <v>629</v>
+        <v>620</v>
       </c>
       <c r="T86" s="28" t="s">
         <v>83</v>
@@ -12290,15 +12185,15 @@
         <v>9</v>
       </c>
     </row>
-    <row r="87" spans="1:21" s="28" customFormat="1" ht="13.5">
+    <row r="87" spans="1:21" s="28" customFormat="1" ht="13.8">
       <c r="A87" s="28" t="s">
-        <v>630</v>
+        <v>621</v>
       </c>
       <c r="B87" s="28" t="s">
         <v>7</v>
       </c>
       <c r="C87" s="28" t="s">
-        <v>631</v>
+        <v>622</v>
       </c>
       <c r="D87" s="28" t="s">
         <v>86</v>
@@ -12310,16 +12205,16 @@
         <v>80</v>
       </c>
       <c r="G87" s="28" t="s">
-        <v>632</v>
+        <v>623</v>
       </c>
       <c r="H87" s="28" t="s">
-        <v>633</v>
+        <v>624</v>
       </c>
       <c r="I87" s="28" t="s">
         <v>209</v>
       </c>
       <c r="K87" s="28" t="s">
-        <v>444</v>
+        <v>443</v>
       </c>
       <c r="L87" s="28" t="s">
         <v>150</v>
@@ -12337,10 +12232,10 @@
         <v>215</v>
       </c>
       <c r="R87" s="28" t="s">
-        <v>631</v>
+        <v>622</v>
       </c>
       <c r="S87" s="28" t="s">
-        <v>634</v>
+        <v>625</v>
       </c>
       <c r="T87" s="28" t="s">
         <v>83</v>
@@ -12349,15 +12244,15 @@
         <v>38</v>
       </c>
     </row>
-    <row r="88" spans="1:21" s="28" customFormat="1" ht="13.5">
+    <row r="88" spans="1:21" s="28" customFormat="1" ht="13.8">
       <c r="A88" s="28" t="s">
-        <v>635</v>
+        <v>626</v>
       </c>
       <c r="B88" s="28" t="s">
         <v>7</v>
       </c>
       <c r="C88" s="28" t="s">
-        <v>636</v>
+        <v>627</v>
       </c>
       <c r="D88" s="28" t="s">
         <v>78</v>
@@ -12372,7 +12267,7 @@
         <v>80</v>
       </c>
       <c r="H88" s="28" t="s">
-        <v>637</v>
+        <v>628</v>
       </c>
       <c r="I88" s="28" t="s">
         <v>209</v>
@@ -12396,10 +12291,10 @@
         <v>277</v>
       </c>
       <c r="R88" s="28" t="s">
-        <v>636</v>
+        <v>627</v>
       </c>
       <c r="S88" s="28" t="s">
-        <v>638</v>
+        <v>629</v>
       </c>
       <c r="T88" s="28" t="s">
         <v>83</v>
@@ -12408,15 +12303,15 @@
         <v>38</v>
       </c>
     </row>
-    <row r="89" spans="1:21" s="28" customFormat="1" ht="13.5">
+    <row r="89" spans="1:21" s="28" customFormat="1" ht="13.8">
       <c r="A89" s="28" t="s">
-        <v>639</v>
+        <v>630</v>
       </c>
       <c r="B89" s="28" t="s">
         <v>7</v>
       </c>
       <c r="C89" s="28" t="s">
-        <v>640</v>
+        <v>631</v>
       </c>
       <c r="D89" s="28" t="s">
         <v>86</v>
@@ -12428,10 +12323,10 @@
         <v>80</v>
       </c>
       <c r="G89" s="28" t="s">
-        <v>641</v>
+        <v>632</v>
       </c>
       <c r="H89" s="28" t="s">
-        <v>642</v>
+        <v>633</v>
       </c>
       <c r="I89" s="28" t="s">
         <v>209</v>
@@ -12440,7 +12335,7 @@
         <v>210</v>
       </c>
       <c r="L89" s="28" t="s">
-        <v>643</v>
+        <v>634</v>
       </c>
       <c r="M89" s="28" t="s">
         <v>213</v>
@@ -12455,10 +12350,10 @@
         <v>215</v>
       </c>
       <c r="R89" s="28" t="s">
-        <v>640</v>
+        <v>631</v>
       </c>
       <c r="S89" s="28" t="s">
-        <v>644</v>
+        <v>635</v>
       </c>
       <c r="T89" s="28" t="s">
         <v>83</v>
@@ -12467,15 +12362,15 @@
         <v>38</v>
       </c>
     </row>
-    <row r="90" spans="1:21" s="28" customFormat="1" ht="13.5">
+    <row r="90" spans="1:21" s="28" customFormat="1" ht="13.8">
       <c r="A90" s="28" t="s">
-        <v>645</v>
+        <v>636</v>
       </c>
       <c r="B90" s="28" t="s">
         <v>7</v>
       </c>
       <c r="C90" s="28" t="s">
-        <v>646</v>
+        <v>637</v>
       </c>
       <c r="D90" s="28" t="s">
         <v>86</v>
@@ -12490,7 +12385,7 @@
         <v>87</v>
       </c>
       <c r="H90" s="28" t="s">
-        <v>647</v>
+        <v>638</v>
       </c>
       <c r="I90" s="28" t="s">
         <v>209</v>
@@ -12514,10 +12409,10 @@
         <v>215</v>
       </c>
       <c r="R90" s="28" t="s">
-        <v>646</v>
+        <v>637</v>
       </c>
       <c r="S90" s="28" t="s">
-        <v>648</v>
+        <v>639</v>
       </c>
       <c r="T90" s="28" t="s">
         <v>107</v>
@@ -12526,15 +12421,15 @@
         <v>17</v>
       </c>
     </row>
-    <row r="91" spans="1:21" s="28" customFormat="1" ht="13.5">
+    <row r="91" spans="1:21" s="28" customFormat="1" ht="13.8">
       <c r="A91" s="28" t="s">
-        <v>649</v>
+        <v>640</v>
       </c>
       <c r="B91" s="28" t="s">
         <v>7</v>
       </c>
       <c r="C91" s="28" t="s">
-        <v>650</v>
+        <v>641</v>
       </c>
       <c r="D91" s="28" t="s">
         <v>86</v>
@@ -12549,7 +12444,7 @@
         <v>332</v>
       </c>
       <c r="H91" s="28" t="s">
-        <v>651</v>
+        <v>642</v>
       </c>
       <c r="I91" s="28" t="s">
         <v>209</v>
@@ -12573,10 +12468,10 @@
         <v>277</v>
       </c>
       <c r="R91" s="28" t="s">
-        <v>666</v>
+        <v>657</v>
       </c>
       <c r="S91" s="28" t="s">
-        <v>652</v>
+        <v>643</v>
       </c>
       <c r="T91" s="28" t="s">
         <v>107</v>
@@ -12585,15 +12480,15 @@
         <v>17</v>
       </c>
     </row>
-    <row r="92" spans="1:21" s="28" customFormat="1" ht="13.5">
+    <row r="92" spans="1:21" s="28" customFormat="1" ht="13.8">
       <c r="A92" s="28" t="s">
-        <v>653</v>
+        <v>644</v>
       </c>
       <c r="B92" s="28" t="s">
         <v>7</v>
       </c>
       <c r="C92" s="28" t="s">
-        <v>654</v>
+        <v>645</v>
       </c>
       <c r="D92" s="28" t="s">
         <v>78</v>
@@ -12608,16 +12503,16 @@
         <v>218</v>
       </c>
       <c r="H92" s="28" t="s">
-        <v>552</v>
+        <v>548</v>
       </c>
       <c r="I92" s="28" t="s">
         <v>209</v>
       </c>
       <c r="K92" s="28" t="s">
-        <v>553</v>
+        <v>549</v>
       </c>
       <c r="L92" s="28" t="s">
-        <v>554</v>
+        <v>550</v>
       </c>
       <c r="M92" s="28" t="s">
         <v>215</v>
@@ -12632,10 +12527,10 @@
         <v>210</v>
       </c>
       <c r="R92" s="28" t="s">
-        <v>654</v>
+        <v>645</v>
       </c>
       <c r="S92" s="28" t="s">
-        <v>655</v>
+        <v>646</v>
       </c>
       <c r="T92" s="28" t="s">
         <v>107</v>
@@ -12644,12 +12539,12 @@
         <v>17</v>
       </c>
     </row>
-    <row r="93" spans="1:21" ht="13.5">
+    <row r="93" spans="1:21" ht="13.8">
       <c r="A93" t="s">
-        <v>656</v>
-      </c>
-      <c r="B93" s="70" t="s">
-        <v>676</v>
+        <v>647</v>
+      </c>
+      <c r="B93" t="s">
+        <v>438</v>
       </c>
       <c r="C93" t="s">
         <v>121</v>
@@ -12660,41 +12555,41 @@
       <c r="E93" t="s">
         <v>184</v>
       </c>
-      <c r="F93" s="70" t="s">
+      <c r="F93" s="69" t="s">
         <v>246</v>
       </c>
       <c r="G93" t="s">
         <v>122</v>
       </c>
-      <c r="H93" s="70" t="s">
-        <v>577</v>
+      <c r="H93" s="69" t="s">
+        <v>573</v>
       </c>
       <c r="I93" t="s">
         <v>209</v>
       </c>
-      <c r="K93" s="70" t="s">
-        <v>559</v>
-      </c>
-      <c r="L93" s="70" t="s">
-        <v>560</v>
-      </c>
-      <c r="M93" s="70" t="s">
+      <c r="K93" s="69" t="s">
+        <v>555</v>
+      </c>
+      <c r="L93" s="69" t="s">
+        <v>556</v>
+      </c>
+      <c r="M93" s="69" t="s">
         <v>212</v>
       </c>
-      <c r="N93" s="70" t="s">
+      <c r="N93" s="69" t="s">
         <v>215</v>
       </c>
-      <c r="P93" s="70" t="s">
+      <c r="P93" s="69" t="s">
         <v>214</v>
       </c>
-      <c r="Q93" s="70" t="s">
+      <c r="Q93" s="69" t="s">
         <v>215</v>
       </c>
       <c r="R93" t="s">
-        <v>657</v>
-      </c>
-      <c r="S93" s="70" t="s">
-        <v>579</v>
+        <v>648</v>
+      </c>
+      <c r="S93" s="69" t="s">
+        <v>575</v>
       </c>
       <c r="T93" s="28" t="s">
         <v>107</v>
@@ -12703,15 +12598,15 @@
         <v>17</v>
       </c>
     </row>
-    <row r="94" spans="1:21" ht="13.5">
+    <row r="94" spans="1:21" ht="13.8">
       <c r="A94" t="s">
-        <v>693</v>
+        <v>683</v>
       </c>
       <c r="B94" t="s">
         <v>438</v>
       </c>
       <c r="C94" t="s">
-        <v>694</v>
+        <v>684</v>
       </c>
       <c r="D94" t="s">
         <v>86</v>
@@ -12726,7 +12621,7 @@
         <v>148</v>
       </c>
       <c r="H94" t="s">
-        <v>695</v>
+        <v>685</v>
       </c>
       <c r="I94" t="s">
         <v>209</v>
@@ -12735,7 +12630,7 @@
         <v>210</v>
       </c>
       <c r="L94" t="s">
-        <v>696</v>
+        <v>686</v>
       </c>
       <c r="M94" t="s">
         <v>212</v>
@@ -12750,10 +12645,10 @@
         <v>215</v>
       </c>
       <c r="R94" t="s">
-        <v>694</v>
+        <v>684</v>
       </c>
       <c r="S94" t="s">
-        <v>697</v>
+        <v>687</v>
       </c>
       <c r="T94" s="28" t="s">
         <v>83</v>
@@ -12762,15 +12657,15 @@
         <v>9</v>
       </c>
     </row>
-    <row r="95" spans="1:21" ht="13.5">
+    <row r="95" spans="1:21" ht="13.8">
       <c r="A95" t="s">
-        <v>698</v>
+        <v>688</v>
       </c>
       <c r="B95" t="s">
         <v>438</v>
       </c>
       <c r="C95" t="s">
-        <v>699</v>
+        <v>689</v>
       </c>
       <c r="D95" t="s">
         <v>86</v>
@@ -12791,10 +12686,10 @@
         <v>209</v>
       </c>
       <c r="K95" t="s">
-        <v>444</v>
+        <v>443</v>
       </c>
       <c r="L95" t="s">
-        <v>700</v>
+        <v>690</v>
       </c>
       <c r="M95" t="s">
         <v>212</v>
@@ -12809,10 +12704,10 @@
         <v>215</v>
       </c>
       <c r="R95" t="s">
-        <v>699</v>
+        <v>689</v>
       </c>
       <c r="S95" t="s">
-        <v>701</v>
+        <v>691</v>
       </c>
       <c r="T95" s="28" t="s">
         <v>83</v>
@@ -12821,9 +12716,9 @@
         <v>9</v>
       </c>
     </row>
-    <row r="96" spans="1:21" ht="13.5">
+    <row r="96" spans="1:21" ht="13.8">
       <c r="A96" t="s">
-        <v>702</v>
+        <v>692</v>
       </c>
       <c r="B96" t="s">
         <v>438</v>
@@ -12837,41 +12732,41 @@
       <c r="E96" t="s">
         <v>79</v>
       </c>
-      <c r="F96" s="73" t="s">
+      <c r="F96" s="72" t="s">
         <v>218</v>
       </c>
       <c r="G96" t="s">
         <v>87</v>
       </c>
-      <c r="H96" s="73" t="s">
-        <v>449</v>
+      <c r="H96" s="72" t="s">
+        <v>447</v>
       </c>
       <c r="I96" t="s">
         <v>209</v>
       </c>
-      <c r="K96" s="73" t="s">
-        <v>455</v>
-      </c>
-      <c r="L96" s="73" t="s">
-        <v>574</v>
-      </c>
-      <c r="M96" s="73" t="s">
+      <c r="K96" s="72" t="s">
+        <v>453</v>
+      </c>
+      <c r="L96" s="72" t="s">
+        <v>570</v>
+      </c>
+      <c r="M96" s="72" t="s">
         <v>212</v>
       </c>
-      <c r="N96" s="73" t="s">
+      <c r="N96" s="72" t="s">
         <v>215</v>
       </c>
-      <c r="P96" s="73" t="s">
+      <c r="P96" s="72" t="s">
         <v>210</v>
       </c>
-      <c r="Q96" s="73" t="s">
+      <c r="Q96" s="72" t="s">
         <v>277</v>
       </c>
       <c r="R96" t="s">
         <v>228</v>
       </c>
-      <c r="S96" s="73" t="s">
-        <v>575</v>
+      <c r="S96" s="72" t="s">
+        <v>571</v>
       </c>
       <c r="T96" s="28" t="s">
         <v>83</v>
@@ -12880,15 +12775,15 @@
         <v>9</v>
       </c>
     </row>
-    <row r="97" spans="1:21" ht="13.5">
+    <row r="97" spans="1:21" ht="13.8">
       <c r="A97" t="s">
-        <v>706</v>
+        <v>696</v>
       </c>
       <c r="B97" t="s">
         <v>438</v>
       </c>
       <c r="C97" t="s">
-        <v>707</v>
+        <v>697</v>
       </c>
       <c r="D97" t="s">
         <v>86</v>
@@ -12903,7 +12798,7 @@
         <v>148</v>
       </c>
       <c r="H97" t="s">
-        <v>708</v>
+        <v>698</v>
       </c>
       <c r="I97" t="s">
         <v>209</v>
@@ -12912,7 +12807,7 @@
         <v>210</v>
       </c>
       <c r="L97" t="s">
-        <v>709</v>
+        <v>699</v>
       </c>
       <c r="M97" t="s">
         <v>212</v>
@@ -12927,10 +12822,10 @@
         <v>215</v>
       </c>
       <c r="R97" t="s">
-        <v>707</v>
+        <v>697</v>
       </c>
       <c r="S97" t="s">
-        <v>710</v>
+        <v>700</v>
       </c>
       <c r="T97" s="28" t="s">
         <v>83</v>
@@ -12941,13 +12836,9 @@
     </row>
   </sheetData>
   <customSheetViews>
-    <customSheetView guid="{C25CEB9E-BEC1-4982-90C4-50C84EE1B82A}" filter="1" showAutoFilter="1">
-      <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-      <autoFilter ref="A1:AD33" xr:uid="{38D2612A-9F4E-4B79-B3B7-6162B58C1230}"/>
-    </customSheetView>
     <customSheetView guid="{A7754112-A52F-4ABC-8778-92F04773E53C}" filter="1" showAutoFilter="1">
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-      <autoFilter ref="A1:AD33" xr:uid="{1E224870-A2D2-4119-99A3-9B51FD782071}">
+      <autoFilter ref="A1:AD33" xr:uid="{2452B91A-1092-476C-AA9F-A0F90977EB27}">
         <filterColumn colId="5">
           <filters blank="1">
             <filter val="Strathnairn"/>
@@ -12955,8 +12846,12 @@
         </filterColumn>
       </autoFilter>
     </customSheetView>
+    <customSheetView guid="{C25CEB9E-BEC1-4982-90C4-50C84EE1B82A}" filter="1" showAutoFilter="1">
+      <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+      <autoFilter ref="A1:AD33" xr:uid="{2B19F17B-E94C-4ACA-A398-EF54335794CA}"/>
+    </customSheetView>
   </customSheetViews>
-  <conditionalFormatting sqref="A1:AK1">
+  <conditionalFormatting sqref="A1:AI1">
     <cfRule type="notContainsBlanks" dxfId="1" priority="1">
       <formula>LEN(TRIM(A1))&gt;0</formula>
     </cfRule>
@@ -13026,23 +12921,23 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.46484375" defaultRowHeight="15.75" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15.75" customHeight="1"/>
   <cols>
     <col min="1" max="1" width="16" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="14.53125" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="16.796875" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="14.53125" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="13.19921875" customWidth="1" collapsed="1"/>
-    <col min="15" max="15" width="20.86328125" customWidth="1" collapsed="1"/>
-    <col min="21" max="21" width="19.1328125" customWidth="1" collapsed="1"/>
-    <col min="22" max="22" width="19.19921875" customWidth="1" collapsed="1"/>
-    <col min="23" max="23" width="20.1328125" customWidth="1" collapsed="1"/>
-    <col min="24" max="24" width="19.796875" customWidth="1" collapsed="1"/>
-    <col min="26" max="26" width="15.86328125" customWidth="1" collapsed="1"/>
-    <col min="27" max="27" width="13.46484375" customWidth="1" collapsed="1"/>
-    <col min="28" max="28" width="15.19921875" customWidth="1" collapsed="1"/>
-    <col min="29" max="29" width="16.1328125" customWidth="1" collapsed="1"/>
-    <col min="30" max="30" width="15.86328125" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="14.5546875" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="16.77734375" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="14.5546875" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="13.21875" customWidth="1" collapsed="1"/>
+    <col min="15" max="15" width="20.88671875" customWidth="1" collapsed="1"/>
+    <col min="21" max="21" width="19.109375" customWidth="1" collapsed="1"/>
+    <col min="22" max="22" width="19.21875" customWidth="1" collapsed="1"/>
+    <col min="23" max="23" width="20.109375" customWidth="1" collapsed="1"/>
+    <col min="24" max="24" width="19.77734375" customWidth="1" collapsed="1"/>
+    <col min="26" max="26" width="15.88671875" customWidth="1" collapsed="1"/>
+    <col min="27" max="27" width="13.44140625" customWidth="1" collapsed="1"/>
+    <col min="28" max="28" width="15.21875" customWidth="1" collapsed="1"/>
+    <col min="29" max="29" width="16.109375" customWidth="1" collapsed="1"/>
+    <col min="30" max="30" width="15.88671875" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:35" ht="15.75" customHeight="1">
@@ -13165,16 +13060,16 @@
       <selection pane="bottomLeft" activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.46484375" defaultRowHeight="15.75" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15.75" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="44.86328125" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="17.1328125" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="26.46484375" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="36.1328125" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="51.1328125" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" width="44.88671875" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="17.109375" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="26.44140625" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="36.109375" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="51.109375" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:26" ht="13.9">
+    <row r="1" spans="1:26" ht="13.8">
       <c r="A1" s="42" t="s">
         <v>163</v>
       </c>

</xml_diff>

<commit_message>
Update existing listings 14/06/2021
</commit_message>
<xml_diff>
--- a/src/main/resources/InputTestdata/Listing details.xlsx
+++ b/src/main/resources/InputTestdata/Listing details.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\manoj\git\777Homes-business\src\main\resources\InputTestdata\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Athavan\git\777Homes-2\777Homes-business\src\main\resources\InputTestdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DB59EA50-1A4A-4B74-81A8-904222A3D71B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BA381021-8C8F-4AA4-9D58-4297210F2981}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="20715" windowHeight="13276" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Backlog" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2276" uniqueCount="707">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2288" uniqueCount="718">
   <si>
     <t>ID</t>
   </si>
@@ -3045,9 +3045,6 @@
     <t>https://www.allhomes.com.au/taylor-act-2913?tid=179073334</t>
   </si>
   <si>
-    <t>TO BE UPDATED</t>
-  </si>
-  <si>
     <t>New Door Properties presents this wonderful opportunity to secure a 4 bedroom beautiful home in Taylor.
 This 4 bedroom three bathroom comes with a practical layout and room to entertain and relax, you will feel right at home with the contemporary and neutral decor. You would notice that the inclusion list is quite generous with provision of high standard items. 
 House and Land Package Details:
@@ -3103,9 +3100,6 @@
   </si>
   <si>
     <t>$399,000+</t>
-  </si>
-  <si>
-    <t>NEW PRICE</t>
   </si>
   <si>
     <t>An amazing large home to enjoy living upon completion of this extravagant property nearby multiple walking &amp; bike trails, schools, and shops. All the local amenities are right on your doorstep to build lifetime memories in this amazing home.
@@ -3303,6 +3297,45 @@
   </si>
   <si>
     <t>PF - Central A/C</t>
+  </si>
+  <si>
+    <t>https://www.777homes.com.au/wp-admin/post.php?post=5543&amp;amp;action=edit&amp;amp;classic-editor</t>
+  </si>
+  <si>
+    <t>https://www.777homes.com.au/wp-admin/post.php?post=5525&amp;action=edit&amp;classic-editor</t>
+  </si>
+  <si>
+    <t>https://www.777homes.com.au/wp-admin/post.php?post=5730&amp;action=edit&amp;classic-editor</t>
+  </si>
+  <si>
+    <t>https://www.777homes.com.au/wp-admin/post.php?post=5748&amp;action=edit&amp;classic-editor</t>
+  </si>
+  <si>
+    <t>https://www.777homes.com.au/wp-admin/post.php?post=5762&amp;action=edit&amp;classic-editor</t>
+  </si>
+  <si>
+    <t>https://www.777homes.com.au/wp-admin/post.php?post=6230&amp;action=edit&amp;classic-editor</t>
+  </si>
+  <si>
+    <t>https://www.777homes.com.au/wp-admin/post.php?post=5774&amp;action=edit&amp;classic-editor</t>
+  </si>
+  <si>
+    <t>https://www.777homes.com.au/wp-admin/post.php?post=5786&amp;action=edit&amp;classic-editor</t>
+  </si>
+  <si>
+    <t>https://www.777homes.com.au/wp-admin/post.php?post=6051&amp;action=edit&amp;classic-editor</t>
+  </si>
+  <si>
+    <t>https://www.777homes.com.au/wp-admin/post.php?post=6058&amp;action=edit&amp;classic-editor</t>
+  </si>
+  <si>
+    <t>https://www.777homes.com.au/wp-admin/post.php?post=6070&amp;action=edit&amp;classic-editor</t>
+  </si>
+  <si>
+    <t>https://www.777homes.com.au/wp-admin/post.php?post=6090&amp;action=edit&amp;classic-editor</t>
+  </si>
+  <si>
+    <t>Owner Infor</t>
   </si>
 </sst>
 </file>
@@ -3998,25 +4031,25 @@
   <dimension ref="A1:AB97"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A74" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A94" sqref="A94:XFD97"/>
+      <pane ySplit="1" topLeftCell="A26" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B29" sqref="B29"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15.75" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="14.46484375" defaultRowHeight="15.75" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="9.21875" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="74.77734375" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" width="9.19921875" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="74.796875" customWidth="1" collapsed="1"/>
     <col min="3" max="3" width="65" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="14.5546875" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="22.109375" style="55" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="21.88671875" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="56.88671875" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="10.88671875" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="17.88671875" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="22.5546875" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="14.53125" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="22.1328125" style="55" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="21.86328125" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="56.86328125" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="10.86328125" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="17.86328125" customWidth="1" collapsed="1"/>
+    <col min="11" max="11" width="22.53125" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:28" ht="13.8">
+    <row r="1" spans="1:28" ht="13.9">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -4050,7 +4083,7 @@
       <c r="B2" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="C2" s="4"/>
+      <c r="C2" s="2"/>
       <c r="D2" s="58" t="s">
         <v>15</v>
       </c>
@@ -4091,14 +4124,16 @@
       <c r="AA2" s="7"/>
       <c r="AB2" s="7"/>
     </row>
-    <row r="3" spans="1:28" ht="13.8">
+    <row r="3" spans="1:28" ht="13.9">
       <c r="A3" s="2">
         <v>2</v>
       </c>
       <c r="B3" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="C3" s="4"/>
+      <c r="C3" s="2" t="s">
+        <v>705</v>
+      </c>
       <c r="D3" s="5" t="s">
         <v>15</v>
       </c>
@@ -4144,7 +4179,9 @@
       <c r="B4" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="C4" s="4"/>
+      <c r="C4" s="2" t="s">
+        <v>706</v>
+      </c>
       <c r="D4" s="5" t="s">
         <v>7</v>
       </c>
@@ -4183,14 +4220,14 @@
       <c r="AA4" s="7"/>
       <c r="AB4" s="7"/>
     </row>
-    <row r="5" spans="1:28" ht="13.8">
+    <row r="5" spans="1:28" ht="13.9">
       <c r="A5" s="10">
         <v>4</v>
       </c>
       <c r="B5" s="9" t="s">
         <v>14</v>
       </c>
-      <c r="C5" s="4"/>
+      <c r="C5" s="2"/>
       <c r="D5" s="58" t="s">
         <v>15</v>
       </c>
@@ -4229,14 +4266,16 @@
       <c r="AA5" s="7"/>
       <c r="AB5" s="7"/>
     </row>
-    <row r="6" spans="1:28" ht="13.8">
+    <row r="6" spans="1:28" ht="13.9">
       <c r="A6" s="10">
         <v>5</v>
       </c>
       <c r="B6" s="13" t="s">
         <v>16</v>
       </c>
-      <c r="C6" s="10"/>
+      <c r="C6" s="10" t="s">
+        <v>707</v>
+      </c>
       <c r="D6" s="5" t="s">
         <v>7</v>
       </c>
@@ -4271,14 +4310,16 @@
       <c r="AA6" s="10"/>
       <c r="AB6" s="10"/>
     </row>
-    <row r="7" spans="1:28" ht="13.8">
+    <row r="7" spans="1:28" ht="13.9">
       <c r="A7" s="10">
         <v>6</v>
       </c>
       <c r="B7" s="15" t="s">
         <v>19</v>
       </c>
-      <c r="C7" s="4"/>
+      <c r="C7" s="2" t="s">
+        <v>708</v>
+      </c>
       <c r="D7" s="5" t="s">
         <v>7</v>
       </c>
@@ -4313,14 +4354,14 @@
       <c r="AA7" s="7"/>
       <c r="AB7" s="7"/>
     </row>
-    <row r="8" spans="1:28" ht="13.8">
+    <row r="8" spans="1:28" ht="13.9">
       <c r="A8" s="10">
         <v>7</v>
       </c>
       <c r="B8" s="20" t="s">
         <v>20</v>
       </c>
-      <c r="C8" s="4"/>
+      <c r="C8" s="2"/>
       <c r="D8" s="5" t="s">
         <v>7</v>
       </c>
@@ -4355,14 +4396,14 @@
       <c r="AA8" s="7"/>
       <c r="AB8" s="7"/>
     </row>
-    <row r="9" spans="1:28" ht="13.8">
+    <row r="9" spans="1:28" ht="13.9">
       <c r="A9" s="10">
         <v>8</v>
       </c>
       <c r="B9" s="20" t="s">
         <v>21</v>
       </c>
-      <c r="C9" s="4"/>
+      <c r="C9" s="2"/>
       <c r="D9" s="58" t="s">
         <v>15</v>
       </c>
@@ -4397,14 +4438,14 @@
       <c r="AA9" s="7"/>
       <c r="AB9" s="7"/>
     </row>
-    <row r="10" spans="1:28" ht="13.8">
+    <row r="10" spans="1:28" ht="13.9">
       <c r="A10" s="10">
         <v>9</v>
       </c>
       <c r="B10" s="21" t="s">
         <v>22</v>
       </c>
-      <c r="C10" s="4"/>
+      <c r="C10" s="2"/>
       <c r="D10" s="58" t="s">
         <v>15</v>
       </c>
@@ -4439,14 +4480,16 @@
       <c r="AA10" s="7"/>
       <c r="AB10" s="7"/>
     </row>
-    <row r="11" spans="1:28" ht="13.8">
+    <row r="11" spans="1:28" ht="13.9">
       <c r="A11" s="10">
         <v>10</v>
       </c>
       <c r="B11" s="21" t="s">
         <v>23</v>
       </c>
-      <c r="C11" s="4"/>
+      <c r="C11" s="2" t="s">
+        <v>709</v>
+      </c>
       <c r="D11" s="16" t="s">
         <v>7</v>
       </c>
@@ -4481,14 +4524,14 @@
       <c r="AA11" s="7"/>
       <c r="AB11" s="7"/>
     </row>
-    <row r="12" spans="1:28" ht="13.8">
+    <row r="12" spans="1:28" ht="13.9">
       <c r="A12" s="10">
         <v>11</v>
       </c>
       <c r="B12" s="21" t="s">
         <v>24</v>
       </c>
-      <c r="C12" s="4"/>
+      <c r="C12" s="2"/>
       <c r="D12" s="58" t="s">
         <v>15</v>
       </c>
@@ -4523,14 +4566,14 @@
       <c r="AA12" s="7"/>
       <c r="AB12" s="7"/>
     </row>
-    <row r="13" spans="1:28" ht="13.8">
+    <row r="13" spans="1:28" ht="13.9">
       <c r="A13" s="10">
         <v>12</v>
       </c>
       <c r="B13" s="21" t="s">
         <v>25</v>
       </c>
-      <c r="C13" s="4"/>
+      <c r="C13" s="2"/>
       <c r="D13" s="58" t="s">
         <v>15</v>
       </c>
@@ -4565,14 +4608,14 @@
       <c r="AA13" s="7"/>
       <c r="AB13" s="7"/>
     </row>
-    <row r="14" spans="1:28" ht="13.8">
+    <row r="14" spans="1:28" ht="13.9">
       <c r="A14" s="10">
         <v>13</v>
       </c>
       <c r="B14" s="21" t="s">
         <v>26</v>
       </c>
-      <c r="C14" s="4"/>
+      <c r="C14" s="2"/>
       <c r="D14" s="58" t="s">
         <v>15</v>
       </c>
@@ -4607,14 +4650,16 @@
       <c r="AA14" s="7"/>
       <c r="AB14" s="7"/>
     </row>
-    <row r="15" spans="1:28" ht="13.8">
+    <row r="15" spans="1:28" ht="13.9">
       <c r="A15" s="10">
         <v>14</v>
       </c>
       <c r="B15" s="20" t="s">
         <v>27</v>
       </c>
-      <c r="C15" s="4"/>
+      <c r="C15" s="2" t="s">
+        <v>710</v>
+      </c>
       <c r="D15" s="16" t="s">
         <v>7</v>
       </c>
@@ -4649,14 +4694,14 @@
       <c r="AA15" s="7"/>
       <c r="AB15" s="7"/>
     </row>
-    <row r="16" spans="1:28" ht="13.8">
+    <row r="16" spans="1:28" ht="13.9">
       <c r="A16" s="10">
         <v>15</v>
       </c>
       <c r="B16" s="21" t="s">
         <v>28</v>
       </c>
-      <c r="C16" s="4"/>
+      <c r="C16" s="2"/>
       <c r="D16" s="58" t="s">
         <v>15</v>
       </c>
@@ -4691,14 +4736,16 @@
       <c r="AA16" s="7"/>
       <c r="AB16" s="7"/>
     </row>
-    <row r="17" spans="1:28" ht="13.8">
+    <row r="17" spans="1:28" ht="13.9">
       <c r="A17" s="10">
         <v>16</v>
       </c>
       <c r="B17" s="20" t="s">
         <v>29</v>
       </c>
-      <c r="C17" s="4"/>
+      <c r="C17" s="2" t="s">
+        <v>711</v>
+      </c>
       <c r="D17" s="16" t="s">
         <v>7</v>
       </c>
@@ -4733,14 +4780,14 @@
       <c r="AA17" s="7"/>
       <c r="AB17" s="7"/>
     </row>
-    <row r="18" spans="1:28" ht="13.8">
+    <row r="18" spans="1:28" ht="13.9">
       <c r="A18" s="10">
         <v>17</v>
       </c>
       <c r="B18" s="60" t="s">
         <v>30</v>
       </c>
-      <c r="C18" s="4"/>
+      <c r="C18" s="2"/>
       <c r="D18" s="58" t="s">
         <v>15</v>
       </c>
@@ -4775,14 +4822,14 @@
       <c r="AA18" s="7"/>
       <c r="AB18" s="7"/>
     </row>
-    <row r="19" spans="1:28" ht="13.8">
+    <row r="19" spans="1:28" ht="13.9">
       <c r="A19" s="10">
         <v>18</v>
       </c>
       <c r="B19" s="20" t="s">
         <v>31</v>
       </c>
-      <c r="C19" s="4"/>
+      <c r="C19" s="2"/>
       <c r="D19" s="16" t="s">
         <v>7</v>
       </c>
@@ -4817,14 +4864,14 @@
       <c r="AA19" s="7"/>
       <c r="AB19" s="7"/>
     </row>
-    <row r="20" spans="1:28" ht="13.8">
+    <row r="20" spans="1:28" ht="13.9">
       <c r="A20" s="10">
         <v>19</v>
       </c>
       <c r="B20" s="21" t="s">
         <v>32</v>
       </c>
-      <c r="C20" s="4"/>
+      <c r="C20" s="2"/>
       <c r="D20" s="16" t="s">
         <v>7</v>
       </c>
@@ -4859,14 +4906,14 @@
       <c r="AA20" s="7"/>
       <c r="AB20" s="7"/>
     </row>
-    <row r="21" spans="1:28" ht="13.8">
+    <row r="21" spans="1:28" ht="13.9">
       <c r="A21" s="10">
         <v>20</v>
       </c>
       <c r="B21" s="21" t="s">
         <v>33</v>
       </c>
-      <c r="C21" s="4"/>
+      <c r="C21" s="2"/>
       <c r="D21" s="16" t="s">
         <v>7</v>
       </c>
@@ -4901,14 +4948,14 @@
       <c r="AA21" s="7"/>
       <c r="AB21" s="7"/>
     </row>
-    <row r="22" spans="1:28" ht="13.8">
+    <row r="22" spans="1:28" ht="13.9">
       <c r="A22" s="10">
         <v>21</v>
       </c>
       <c r="B22" s="21" t="s">
         <v>34</v>
       </c>
-      <c r="C22" s="4"/>
+      <c r="C22" s="2"/>
       <c r="D22" s="16" t="s">
         <v>15</v>
       </c>
@@ -4943,14 +4990,16 @@
       <c r="AA22" s="7"/>
       <c r="AB22" s="7"/>
     </row>
-    <row r="23" spans="1:28" ht="13.8">
+    <row r="23" spans="1:28" ht="13.9">
       <c r="A23" s="10">
         <v>22</v>
       </c>
       <c r="B23" s="21" t="s">
         <v>35</v>
       </c>
-      <c r="C23" s="4"/>
+      <c r="C23" s="2" t="s">
+        <v>712</v>
+      </c>
       <c r="D23" s="16" t="s">
         <v>7</v>
       </c>
@@ -4985,14 +5034,14 @@
       <c r="AA23" s="7"/>
       <c r="AB23" s="7"/>
     </row>
-    <row r="24" spans="1:28" ht="13.8">
+    <row r="24" spans="1:28" ht="13.9">
       <c r="A24" s="10">
         <v>23</v>
       </c>
       <c r="B24" s="21" t="s">
         <v>36</v>
       </c>
-      <c r="C24" s="4"/>
+      <c r="C24" s="2"/>
       <c r="D24" s="16" t="s">
         <v>15</v>
       </c>
@@ -5027,14 +5076,14 @@
       <c r="AA24" s="7"/>
       <c r="AB24" s="7"/>
     </row>
-    <row r="25" spans="1:28" ht="13.8">
+    <row r="25" spans="1:28" ht="13.9">
       <c r="A25" s="10">
         <v>24</v>
       </c>
       <c r="B25" s="22" t="s">
         <v>37</v>
       </c>
-      <c r="C25" s="4"/>
+      <c r="C25" s="2"/>
       <c r="D25" s="58" t="s">
         <v>15</v>
       </c>
@@ -5069,14 +5118,16 @@
       <c r="AA25" s="7"/>
       <c r="AB25" s="7"/>
     </row>
-    <row r="26" spans="1:28" ht="13.8">
+    <row r="26" spans="1:28" ht="13.9">
       <c r="A26" s="10">
         <v>25</v>
       </c>
       <c r="B26" s="22" t="s">
         <v>40</v>
       </c>
-      <c r="C26" s="4"/>
+      <c r="C26" s="2" t="s">
+        <v>713</v>
+      </c>
       <c r="D26" s="16" t="s">
         <v>7</v>
       </c>
@@ -5111,14 +5162,16 @@
       <c r="AA26" s="7"/>
       <c r="AB26" s="7"/>
     </row>
-    <row r="27" spans="1:28" ht="13.8">
+    <row r="27" spans="1:28" ht="13.9">
       <c r="A27" s="10">
         <v>26</v>
       </c>
       <c r="B27" s="22" t="s">
         <v>41</v>
       </c>
-      <c r="C27" s="4"/>
+      <c r="C27" s="2" t="s">
+        <v>714</v>
+      </c>
       <c r="D27" s="16" t="s">
         <v>7</v>
       </c>
@@ -5153,14 +5206,14 @@
       <c r="AA27" s="7"/>
       <c r="AB27" s="7"/>
     </row>
-    <row r="28" spans="1:28" ht="13.8">
+    <row r="28" spans="1:28" ht="13.9">
       <c r="A28" s="10">
         <v>27</v>
       </c>
       <c r="B28" s="60" t="s">
         <v>42</v>
       </c>
-      <c r="C28" s="4"/>
+      <c r="C28" s="2"/>
       <c r="D28" s="58" t="s">
         <v>15</v>
       </c>
@@ -5195,14 +5248,16 @@
       <c r="AA28" s="7"/>
       <c r="AB28" s="7"/>
     </row>
-    <row r="29" spans="1:28" ht="13.8">
+    <row r="29" spans="1:28" ht="13.9">
       <c r="A29" s="10">
         <v>28</v>
       </c>
       <c r="B29" s="15" t="s">
         <v>43</v>
       </c>
-      <c r="C29" s="4"/>
+      <c r="C29" s="2" t="s">
+        <v>715</v>
+      </c>
       <c r="D29" s="16" t="s">
         <v>7</v>
       </c>
@@ -5237,14 +5292,14 @@
       <c r="AA29" s="7"/>
       <c r="AB29" s="7"/>
     </row>
-    <row r="30" spans="1:28" ht="13.8">
+    <row r="30" spans="1:28" ht="13.9">
       <c r="A30" s="10">
         <v>29</v>
       </c>
       <c r="B30" s="15" t="s">
         <v>44</v>
       </c>
-      <c r="C30" s="4"/>
+      <c r="C30" s="2"/>
       <c r="D30" s="58" t="s">
         <v>15</v>
       </c>
@@ -5279,14 +5334,16 @@
       <c r="AA30" s="7"/>
       <c r="AB30" s="7"/>
     </row>
-    <row r="31" spans="1:28" ht="13.8">
+    <row r="31" spans="1:28" ht="13.9">
       <c r="A31" s="4">
         <v>30</v>
       </c>
       <c r="B31" s="15" t="s">
         <v>45</v>
       </c>
-      <c r="C31" s="4"/>
+      <c r="C31" s="2" t="s">
+        <v>716</v>
+      </c>
       <c r="D31" s="16" t="s">
         <v>7</v>
       </c>
@@ -5321,7 +5378,7 @@
       <c r="AA31" s="7"/>
       <c r="AB31" s="7"/>
     </row>
-    <row r="32" spans="1:28" ht="13.8">
+    <row r="32" spans="1:28" ht="13.9">
       <c r="A32" s="4">
         <v>31</v>
       </c>
@@ -5363,7 +5420,7 @@
       <c r="AA32" s="7"/>
       <c r="AB32" s="7"/>
     </row>
-    <row r="33" spans="1:8" s="4" customFormat="1" ht="13.8">
+    <row r="33" spans="1:8" s="4" customFormat="1" ht="13.5">
       <c r="A33" s="4">
         <v>32</v>
       </c>
@@ -5383,7 +5440,7 @@
         <v>439</v>
       </c>
     </row>
-    <row r="34" spans="1:8" s="4" customFormat="1" ht="13.8">
+    <row r="34" spans="1:8" s="4" customFormat="1" ht="13.5">
       <c r="A34" s="4">
         <v>33</v>
       </c>
@@ -5403,7 +5460,7 @@
         <v>439</v>
       </c>
     </row>
-    <row r="35" spans="1:8" s="4" customFormat="1" ht="13.2">
+    <row r="35" spans="1:8" s="4" customFormat="1" ht="12.75">
       <c r="A35" s="4">
         <v>34</v>
       </c>
@@ -5423,7 +5480,7 @@
         <v>439</v>
       </c>
     </row>
-    <row r="36" spans="1:8" s="4" customFormat="1" ht="13.2">
+    <row r="36" spans="1:8" s="4" customFormat="1" ht="12.75">
       <c r="A36" s="4">
         <v>35</v>
       </c>
@@ -5443,7 +5500,7 @@
         <v>439</v>
       </c>
     </row>
-    <row r="37" spans="1:8" s="4" customFormat="1" ht="13.2">
+    <row r="37" spans="1:8" s="4" customFormat="1" ht="12.75">
       <c r="A37" s="4">
         <v>36</v>
       </c>
@@ -5463,7 +5520,7 @@
         <v>439</v>
       </c>
     </row>
-    <row r="38" spans="1:8" s="4" customFormat="1" ht="13.2">
+    <row r="38" spans="1:8" s="4" customFormat="1" ht="12.75">
       <c r="A38" s="4">
         <v>37</v>
       </c>
@@ -5483,7 +5540,7 @@
         <v>439</v>
       </c>
     </row>
-    <row r="39" spans="1:8" s="4" customFormat="1" ht="13.2">
+    <row r="39" spans="1:8" s="4" customFormat="1" ht="12.75">
       <c r="A39" s="4">
         <v>38</v>
       </c>
@@ -5503,7 +5560,7 @@
         <v>439</v>
       </c>
     </row>
-    <row r="40" spans="1:8" s="4" customFormat="1" ht="13.2">
+    <row r="40" spans="1:8" s="4" customFormat="1" ht="12.75">
       <c r="A40" s="4">
         <v>39</v>
       </c>
@@ -5523,7 +5580,7 @@
         <v>439</v>
       </c>
     </row>
-    <row r="41" spans="1:8" s="4" customFormat="1" ht="13.2">
+    <row r="41" spans="1:8" s="4" customFormat="1" ht="12.75">
       <c r="A41" s="4">
         <v>40</v>
       </c>
@@ -5543,7 +5600,7 @@
         <v>439</v>
       </c>
     </row>
-    <row r="42" spans="1:8" s="4" customFormat="1" ht="13.2">
+    <row r="42" spans="1:8" s="4" customFormat="1" ht="12.75">
       <c r="A42" s="4">
         <v>41</v>
       </c>
@@ -5563,7 +5620,7 @@
         <v>439</v>
       </c>
     </row>
-    <row r="43" spans="1:8" s="4" customFormat="1" ht="13.2">
+    <row r="43" spans="1:8" s="4" customFormat="1" ht="12.75">
       <c r="A43" s="4">
         <v>42</v>
       </c>
@@ -5583,7 +5640,7 @@
         <v>439</v>
       </c>
     </row>
-    <row r="44" spans="1:8" s="4" customFormat="1" ht="13.2">
+    <row r="44" spans="1:8" s="4" customFormat="1" ht="12.75">
       <c r="A44" s="4">
         <v>43</v>
       </c>
@@ -5603,7 +5660,7 @@
         <v>439</v>
       </c>
     </row>
-    <row r="45" spans="1:8" s="4" customFormat="1" ht="13.2">
+    <row r="45" spans="1:8" s="4" customFormat="1" ht="12.75">
       <c r="A45" s="4">
         <v>44</v>
       </c>
@@ -5623,7 +5680,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="46" spans="1:8" s="4" customFormat="1" ht="13.2">
+    <row r="46" spans="1:8" s="4" customFormat="1" ht="12.75">
       <c r="A46" s="4">
         <v>45</v>
       </c>
@@ -5643,7 +5700,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="47" spans="1:8" s="4" customFormat="1" ht="13.2">
+    <row r="47" spans="1:8" s="4" customFormat="1" ht="12.75">
       <c r="A47" s="4">
         <v>46</v>
       </c>
@@ -5663,7 +5720,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="48" spans="1:8" s="4" customFormat="1" ht="13.2">
+    <row r="48" spans="1:8" s="4" customFormat="1" ht="12.75">
       <c r="A48" s="4">
         <v>47</v>
       </c>
@@ -5683,7 +5740,7 @@
         <v>440</v>
       </c>
     </row>
-    <row r="49" spans="1:8" s="4" customFormat="1" ht="13.2">
+    <row r="49" spans="1:8" s="4" customFormat="1" ht="12.75">
       <c r="A49" s="4">
         <v>48</v>
       </c>
@@ -5703,7 +5760,7 @@
         <v>440</v>
       </c>
     </row>
-    <row r="50" spans="1:8" s="4" customFormat="1" ht="13.2">
+    <row r="50" spans="1:8" s="4" customFormat="1" ht="12.75">
       <c r="A50" s="4">
         <v>49</v>
       </c>
@@ -5723,7 +5780,7 @@
         <v>440</v>
       </c>
     </row>
-    <row r="51" spans="1:8" s="4" customFormat="1" ht="13.2">
+    <row r="51" spans="1:8" s="4" customFormat="1" ht="12.75">
       <c r="A51" s="4">
         <v>50</v>
       </c>
@@ -5743,7 +5800,7 @@
         <v>440</v>
       </c>
     </row>
-    <row r="52" spans="1:8" s="4" customFormat="1" ht="13.2">
+    <row r="52" spans="1:8" s="4" customFormat="1" ht="12.75">
       <c r="A52" s="4">
         <v>51</v>
       </c>
@@ -5783,7 +5840,7 @@
         <v>334</v>
       </c>
     </row>
-    <row r="54" spans="1:8" ht="13.2">
+    <row r="54" spans="1:8" ht="12.75">
       <c r="A54">
         <v>53</v>
       </c>
@@ -5803,7 +5860,7 @@
         <v>334</v>
       </c>
     </row>
-    <row r="55" spans="1:8" s="4" customFormat="1" ht="13.2">
+    <row r="55" spans="1:8" s="4" customFormat="1" ht="12.75">
       <c r="A55" s="4">
         <v>54</v>
       </c>
@@ -5823,7 +5880,7 @@
         <v>334</v>
       </c>
     </row>
-    <row r="56" spans="1:8" s="4" customFormat="1" ht="13.2">
+    <row r="56" spans="1:8" s="4" customFormat="1" ht="12.75">
       <c r="A56" s="4">
         <v>55</v>
       </c>
@@ -5843,7 +5900,7 @@
         <v>334</v>
       </c>
     </row>
-    <row r="57" spans="1:8" s="4" customFormat="1" ht="13.2">
+    <row r="57" spans="1:8" s="4" customFormat="1" ht="12.75">
       <c r="A57" s="4">
         <v>56</v>
       </c>
@@ -5863,7 +5920,7 @@
         <v>334</v>
       </c>
     </row>
-    <row r="58" spans="1:8" s="4" customFormat="1" ht="13.2">
+    <row r="58" spans="1:8" s="4" customFormat="1" ht="12.75">
       <c r="A58" s="4">
         <v>57</v>
       </c>
@@ -5883,7 +5940,7 @@
         <v>334</v>
       </c>
     </row>
-    <row r="59" spans="1:8" s="4" customFormat="1" ht="13.2">
+    <row r="59" spans="1:8" s="4" customFormat="1" ht="12.75">
       <c r="A59" s="4">
         <v>58</v>
       </c>
@@ -5903,7 +5960,7 @@
         <v>334</v>
       </c>
     </row>
-    <row r="60" spans="1:8" s="4" customFormat="1" ht="13.2">
+    <row r="60" spans="1:8" s="4" customFormat="1" ht="12.75">
       <c r="A60" s="4">
         <v>59</v>
       </c>
@@ -5923,7 +5980,7 @@
         <v>334</v>
       </c>
     </row>
-    <row r="61" spans="1:8" s="4" customFormat="1" ht="13.2">
+    <row r="61" spans="1:8" s="4" customFormat="1" ht="12.75">
       <c r="A61" s="4">
         <v>60</v>
       </c>
@@ -5943,7 +6000,7 @@
         <v>334</v>
       </c>
     </row>
-    <row r="62" spans="1:8" s="4" customFormat="1" ht="13.2">
+    <row r="62" spans="1:8" s="4" customFormat="1" ht="12.75">
       <c r="A62" s="4">
         <v>61</v>
       </c>
@@ -5963,7 +6020,7 @@
         <v>439</v>
       </c>
     </row>
-    <row r="63" spans="1:8" s="4" customFormat="1" ht="13.2">
+    <row r="63" spans="1:8" s="4" customFormat="1" ht="12.75">
       <c r="A63" s="4">
         <v>62</v>
       </c>
@@ -5983,7 +6040,7 @@
         <v>439</v>
       </c>
     </row>
-    <row r="64" spans="1:8" s="4" customFormat="1" ht="13.2">
+    <row r="64" spans="1:8" s="4" customFormat="1" ht="12.75">
       <c r="A64" s="4">
         <v>63</v>
       </c>
@@ -6003,7 +6060,7 @@
         <v>439</v>
       </c>
     </row>
-    <row r="65" spans="1:8" s="4" customFormat="1" ht="13.2">
+    <row r="65" spans="1:8" s="4" customFormat="1" ht="12.75">
       <c r="A65" s="4">
         <v>64</v>
       </c>
@@ -6024,7 +6081,7 @@
         <v>439</v>
       </c>
     </row>
-    <row r="66" spans="1:8" s="4" customFormat="1" ht="13.2">
+    <row r="66" spans="1:8" s="4" customFormat="1" ht="12.75">
       <c r="A66" s="4">
         <v>65</v>
       </c>
@@ -6044,7 +6101,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="67" spans="1:8" s="4" customFormat="1" ht="13.2">
+    <row r="67" spans="1:8" s="4" customFormat="1" ht="12.75">
       <c r="A67" s="4">
         <v>66</v>
       </c>
@@ -6064,7 +6121,7 @@
         <v>440</v>
       </c>
     </row>
-    <row r="68" spans="1:8" s="4" customFormat="1" ht="13.2">
+    <row r="68" spans="1:8" s="4" customFormat="1" ht="12.75">
       <c r="A68" s="4">
         <v>67</v>
       </c>
@@ -6087,7 +6144,7 @@
         <v>439</v>
       </c>
     </row>
-    <row r="69" spans="1:8" s="4" customFormat="1" ht="13.2">
+    <row r="69" spans="1:8" s="4" customFormat="1" ht="12.75">
       <c r="A69" s="4">
         <v>68</v>
       </c>
@@ -6110,7 +6167,7 @@
         <v>439</v>
       </c>
     </row>
-    <row r="70" spans="1:8" s="4" customFormat="1" ht="13.2">
+    <row r="70" spans="1:8" s="4" customFormat="1" ht="12.75">
       <c r="A70" s="4">
         <v>69</v>
       </c>
@@ -6133,7 +6190,7 @@
         <v>439</v>
       </c>
     </row>
-    <row r="71" spans="1:8" s="4" customFormat="1" ht="13.2">
+    <row r="71" spans="1:8" s="4" customFormat="1" ht="12.75">
       <c r="A71" s="4">
         <v>70</v>
       </c>
@@ -6156,7 +6213,7 @@
         <v>439</v>
       </c>
     </row>
-    <row r="72" spans="1:8" s="4" customFormat="1" ht="13.2">
+    <row r="72" spans="1:8" s="4" customFormat="1" ht="12.75">
       <c r="A72" s="4">
         <v>71</v>
       </c>
@@ -6179,7 +6236,7 @@
         <v>439</v>
       </c>
     </row>
-    <row r="73" spans="1:8" ht="13.2">
+    <row r="73" spans="1:8" ht="12.75">
       <c r="A73">
         <v>72</v>
       </c>
@@ -6202,7 +6259,7 @@
         <v>440</v>
       </c>
     </row>
-    <row r="74" spans="1:8" ht="13.2">
+    <row r="74" spans="1:8" ht="12.75">
       <c r="A74">
         <v>73</v>
       </c>
@@ -6225,7 +6282,7 @@
         <v>440</v>
       </c>
     </row>
-    <row r="75" spans="1:8" s="4" customFormat="1" ht="13.2">
+    <row r="75" spans="1:8" s="4" customFormat="1" ht="12.75">
       <c r="A75" s="4">
         <v>74</v>
       </c>
@@ -6248,7 +6305,7 @@
         <v>440</v>
       </c>
     </row>
-    <row r="76" spans="1:8" ht="13.2">
+    <row r="76" spans="1:8" ht="12.75">
       <c r="A76">
         <v>75</v>
       </c>
@@ -6271,7 +6328,7 @@
         <v>440</v>
       </c>
     </row>
-    <row r="77" spans="1:8" ht="13.2">
+    <row r="77" spans="1:8" ht="12.75">
       <c r="A77">
         <v>76</v>
       </c>
@@ -6294,7 +6351,7 @@
         <v>440</v>
       </c>
     </row>
-    <row r="78" spans="1:8" ht="13.2">
+    <row r="78" spans="1:8" ht="12.75">
       <c r="A78">
         <v>77</v>
       </c>
@@ -6317,7 +6374,7 @@
         <v>440</v>
       </c>
     </row>
-    <row r="79" spans="1:8" ht="13.2">
+    <row r="79" spans="1:8" ht="12.75">
       <c r="A79">
         <v>78</v>
       </c>
@@ -6340,7 +6397,7 @@
         <v>440</v>
       </c>
     </row>
-    <row r="80" spans="1:8" ht="13.2">
+    <row r="80" spans="1:8" ht="12.75">
       <c r="A80">
         <v>79</v>
       </c>
@@ -6363,7 +6420,7 @@
         <v>440</v>
       </c>
     </row>
-    <row r="81" spans="1:8" ht="13.2">
+    <row r="81" spans="1:8" ht="12.75">
       <c r="A81">
         <v>80</v>
       </c>
@@ -6386,7 +6443,7 @@
         <v>440</v>
       </c>
     </row>
-    <row r="82" spans="1:8" ht="13.2">
+    <row r="82" spans="1:8" ht="12.75">
       <c r="A82">
         <v>81</v>
       </c>
@@ -6409,7 +6466,7 @@
         <v>440</v>
       </c>
     </row>
-    <row r="83" spans="1:8" ht="13.2">
+    <row r="83" spans="1:8" ht="12.75">
       <c r="A83">
         <v>82</v>
       </c>
@@ -6432,7 +6489,7 @@
         <v>440</v>
       </c>
     </row>
-    <row r="84" spans="1:8" ht="13.2">
+    <row r="84" spans="1:8" ht="12.75">
       <c r="A84">
         <v>83</v>
       </c>
@@ -6455,7 +6512,7 @@
         <v>440</v>
       </c>
     </row>
-    <row r="85" spans="1:8" ht="13.2">
+    <row r="85" spans="1:8" ht="12.75">
       <c r="A85">
         <v>84</v>
       </c>
@@ -6478,7 +6535,7 @@
         <v>440</v>
       </c>
     </row>
-    <row r="86" spans="1:8" ht="13.2">
+    <row r="86" spans="1:8" ht="12.75">
       <c r="A86">
         <v>85</v>
       </c>
@@ -6498,7 +6555,7 @@
         <v>439</v>
       </c>
     </row>
-    <row r="87" spans="1:8" ht="13.2">
+    <row r="87" spans="1:8" ht="12.75">
       <c r="A87">
         <v>86</v>
       </c>
@@ -6518,7 +6575,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="88" spans="1:8" ht="13.2">
+    <row r="88" spans="1:8" ht="12.75">
       <c r="A88">
         <v>87</v>
       </c>
@@ -6538,7 +6595,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="89" spans="1:8" ht="13.2">
+    <row r="89" spans="1:8" ht="12.75">
       <c r="A89">
         <v>88</v>
       </c>
@@ -6558,7 +6615,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="90" spans="1:8" ht="13.2">
+    <row r="90" spans="1:8" ht="12.75">
       <c r="A90">
         <v>89</v>
       </c>
@@ -6578,7 +6635,7 @@
         <v>440</v>
       </c>
     </row>
-    <row r="91" spans="1:8" ht="13.2">
+    <row r="91" spans="1:8" ht="12.75">
       <c r="A91">
         <v>90</v>
       </c>
@@ -6598,7 +6655,7 @@
         <v>440</v>
       </c>
     </row>
-    <row r="92" spans="1:8" ht="13.2">
+    <row r="92" spans="1:8" ht="12.75">
       <c r="A92">
         <v>91</v>
       </c>
@@ -6618,7 +6675,7 @@
         <v>440</v>
       </c>
     </row>
-    <row r="93" spans="1:8" ht="13.2">
+    <row r="93" spans="1:8" ht="12.75">
       <c r="A93">
         <v>92</v>
       </c>
@@ -6638,7 +6695,7 @@
         <v>440</v>
       </c>
     </row>
-    <row r="94" spans="1:8" ht="13.2">
+    <row r="94" spans="1:8" ht="12.75">
       <c r="A94">
         <v>93</v>
       </c>
@@ -6646,7 +6703,7 @@
         <v>664</v>
       </c>
       <c r="C94" t="s">
-        <v>703</v>
+        <v>701</v>
       </c>
       <c r="D94" s="66" t="s">
         <v>438</v>
@@ -6658,7 +6715,7 @@
         <v>439</v>
       </c>
     </row>
-    <row r="95" spans="1:8" ht="13.2">
+    <row r="95" spans="1:8" ht="12.75">
       <c r="A95">
         <v>94</v>
       </c>
@@ -6666,7 +6723,7 @@
         <v>665</v>
       </c>
       <c r="C95" t="s">
-        <v>701</v>
+        <v>699</v>
       </c>
       <c r="D95" s="66" t="s">
         <v>438</v>
@@ -6678,7 +6735,7 @@
         <v>439</v>
       </c>
     </row>
-    <row r="96" spans="1:8" ht="13.2">
+    <row r="96" spans="1:8" ht="12.75">
       <c r="A96">
         <v>95</v>
       </c>
@@ -6686,7 +6743,7 @@
         <v>666</v>
       </c>
       <c r="C96" t="s">
-        <v>702</v>
+        <v>700</v>
       </c>
       <c r="D96" s="66" t="s">
         <v>438</v>
@@ -6698,15 +6755,15 @@
         <v>439</v>
       </c>
     </row>
-    <row r="97" spans="1:8" ht="13.2">
+    <row r="97" spans="1:8" ht="12.75">
       <c r="A97">
         <v>96</v>
       </c>
       <c r="B97" t="s">
-        <v>695</v>
+        <v>693</v>
       </c>
       <c r="C97" t="s">
-        <v>704</v>
+        <v>702</v>
       </c>
       <c r="D97" s="71" t="s">
         <v>438</v>
@@ -6816,35 +6873,35 @@
   </sheetPr>
   <dimension ref="A1:AI97"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A91" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="C16" sqref="C16"/>
+      <selection pane="topRight" activeCell="F40" sqref="F40"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15.75" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="14.46484375" defaultRowHeight="15.75" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="14.88671875" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="18.109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="55.5546875" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="25.21875" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="19.5546875" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="19.77734375" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="18.5546875" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="32.21875" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="20.5546875" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="21.109375" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="28.77734375" customWidth="1" collapsed="1"/>
-    <col min="12" max="12" width="37.5546875" customWidth="1" collapsed="1"/>
-    <col min="16" max="17" width="18.77734375" customWidth="1" collapsed="1"/>
-    <col min="18" max="18" width="47.88671875" customWidth="1" collapsed="1"/>
-    <col min="19" max="19" width="77.5546875" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" width="14.86328125" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="18.1328125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="55.53125" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="25.19921875" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="19.53125" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="19.796875" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="18.53125" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="32.19921875" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="20.53125" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="21.1328125" customWidth="1" collapsed="1"/>
+    <col min="11" max="11" width="28.796875" customWidth="1" collapsed="1"/>
+    <col min="12" max="12" width="37.53125" customWidth="1" collapsed="1"/>
+    <col min="16" max="17" width="18.796875" customWidth="1" collapsed="1"/>
+    <col min="18" max="18" width="47.86328125" customWidth="1" collapsed="1"/>
+    <col min="19" max="19" width="77.53125" customWidth="1" collapsed="1"/>
     <col min="20" max="20" width="24" customWidth="1" collapsed="1"/>
-    <col min="21" max="21" width="18.77734375" customWidth="1" collapsed="1"/>
-    <col min="22" max="22" width="19.109375" customWidth="1" collapsed="1"/>
-    <col min="23" max="31" width="19.21875" customWidth="1" collapsed="1"/>
+    <col min="21" max="21" width="18.796875" customWidth="1" collapsed="1"/>
+    <col min="22" max="22" width="19.1328125" customWidth="1" collapsed="1"/>
+    <col min="23" max="31" width="19.19921875" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:35" ht="27.6">
+    <row r="1" spans="1:35" ht="27.75">
       <c r="A1" s="1" t="s">
         <v>47</v>
       </c>
@@ -6924,7 +6981,7 @@
         <v>71</v>
       </c>
       <c r="AA1" s="1" t="s">
-        <v>706</v>
+        <v>704</v>
       </c>
       <c r="AB1" s="1" t="s">
         <v>73</v>
@@ -7089,8 +7146,8 @@
       <c r="A4" s="28">
         <v>3</v>
       </c>
-      <c r="B4" s="72" t="s">
-        <v>667</v>
+      <c r="B4" t="s">
+        <v>7</v>
       </c>
       <c r="C4" s="28" t="s">
         <v>91</v>
@@ -7108,16 +7165,16 @@
         <v>87</v>
       </c>
       <c r="H4" s="67" t="s">
-        <v>669</v>
+        <v>668</v>
       </c>
       <c r="I4" s="28" t="s">
         <v>92</v>
       </c>
       <c r="K4" s="72" t="s">
+        <v>669</v>
+      </c>
+      <c r="L4" s="67" t="s">
         <v>670</v>
-      </c>
-      <c r="L4" s="67" t="s">
-        <v>671</v>
       </c>
       <c r="M4" s="28">
         <v>4</v>
@@ -7138,7 +7195,7 @@
         <v>93</v>
       </c>
       <c r="S4" s="67" t="s">
-        <v>668</v>
+        <v>667</v>
       </c>
       <c r="T4" s="28" t="s">
         <v>83</v>
@@ -7299,8 +7356,8 @@
       <c r="A7" s="28">
         <v>6</v>
       </c>
-      <c r="B7" s="72" t="s">
-        <v>667</v>
+      <c r="B7" t="s">
+        <v>7</v>
       </c>
       <c r="C7" s="28" t="s">
         <v>109</v>
@@ -7326,7 +7383,7 @@
         <v>446</v>
       </c>
       <c r="L7" s="68" t="s">
-        <v>672</v>
+        <v>671</v>
       </c>
       <c r="M7" s="28">
         <v>4</v>
@@ -7562,8 +7619,8 @@
       <c r="A11" s="28">
         <v>10</v>
       </c>
-      <c r="B11" s="72" t="s">
-        <v>667</v>
+      <c r="B11" t="s">
+        <v>7</v>
       </c>
       <c r="C11" s="32" t="s">
         <v>116</v>
@@ -7581,7 +7638,7 @@
         <v>118</v>
       </c>
       <c r="H11" s="70" t="s">
-        <v>694</v>
+        <v>692</v>
       </c>
       <c r="I11" s="35"/>
       <c r="J11" s="35"/>
@@ -7608,7 +7665,7 @@
         <v>119</v>
       </c>
       <c r="S11" s="70" t="s">
-        <v>693</v>
+        <v>691</v>
       </c>
       <c r="T11" s="28" t="s">
         <v>107</v>
@@ -7821,8 +7878,8 @@
       <c r="A15" s="28">
         <v>14</v>
       </c>
-      <c r="B15" s="72" t="s">
-        <v>667</v>
+      <c r="B15" t="s">
+        <v>7</v>
       </c>
       <c r="C15" s="28" t="s">
         <v>100</v>
@@ -7936,8 +7993,8 @@
       <c r="A17" s="28">
         <v>16</v>
       </c>
-      <c r="B17" s="72" t="s">
-        <v>667</v>
+      <c r="B17" t="s">
+        <v>7</v>
       </c>
       <c r="C17" s="28" t="s">
         <v>131</v>
@@ -8336,8 +8393,8 @@
       <c r="A23" s="28">
         <v>22</v>
       </c>
-      <c r="B23" s="72" t="s">
-        <v>667</v>
+      <c r="B23" t="s">
+        <v>7</v>
       </c>
       <c r="C23" s="28" t="s">
         <v>141</v>
@@ -8346,7 +8403,7 @@
         <v>86</v>
       </c>
       <c r="E23" s="28" t="s">
-        <v>101</v>
+        <v>79</v>
       </c>
       <c r="F23" s="30" t="s">
         <v>102</v>
@@ -8523,7 +8580,7 @@
         <v>83</v>
       </c>
       <c r="U25" s="28" t="s">
-        <v>151</v>
+        <v>38</v>
       </c>
       <c r="V25" s="28"/>
       <c r="W25" s="28"/>
@@ -8544,8 +8601,8 @@
       <c r="A26" s="28">
         <v>25</v>
       </c>
-      <c r="B26" s="72" t="s">
-        <v>667</v>
+      <c r="B26" t="s">
+        <v>7</v>
       </c>
       <c r="C26" s="28" t="s">
         <v>152</v>
@@ -8596,15 +8653,15 @@
         <v>83</v>
       </c>
       <c r="U26" s="28" t="s">
-        <v>151</v>
+        <v>38</v>
       </c>
     </row>
     <row r="27" spans="1:35" ht="15" customHeight="1">
       <c r="A27" s="28">
         <v>26</v>
       </c>
-      <c r="B27" s="72" t="s">
-        <v>667</v>
+      <c r="B27" t="s">
+        <v>7</v>
       </c>
       <c r="C27" s="28" t="s">
         <v>155</v>
@@ -8629,10 +8686,10 @@
       </c>
       <c r="J27" s="28"/>
       <c r="K27" s="72" t="s">
+        <v>673</v>
+      </c>
+      <c r="L27" s="68" t="s">
         <v>674</v>
-      </c>
-      <c r="L27" s="68" t="s">
-        <v>675</v>
       </c>
       <c r="M27" s="28">
         <v>2</v>
@@ -8651,13 +8708,13 @@
         <v>155</v>
       </c>
       <c r="S27" s="68" t="s">
-        <v>673</v>
+        <v>672</v>
       </c>
       <c r="T27" s="28" t="s">
         <v>83</v>
       </c>
       <c r="U27" s="28" t="s">
-        <v>151</v>
+        <v>38</v>
       </c>
       <c r="V27" s="28"/>
       <c r="W27" s="28"/>
@@ -8730,15 +8787,15 @@
         <v>83</v>
       </c>
       <c r="U28" s="28" t="s">
-        <v>151</v>
-      </c>
-    </row>
-    <row r="29" spans="1:35" ht="15" customHeight="1">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="29" spans="1:35" s="28" customFormat="1" ht="15" customHeight="1">
       <c r="A29" s="28">
         <v>28</v>
       </c>
-      <c r="B29" s="72" t="s">
-        <v>667</v>
+      <c r="B29" s="61" t="s">
+        <v>183</v>
       </c>
       <c r="C29" s="28" t="s">
         <v>157</v>
@@ -8746,27 +8803,26 @@
       <c r="D29" s="28" t="s">
         <v>86</v>
       </c>
-      <c r="E29" s="68" t="s">
-        <v>676</v>
-      </c>
-      <c r="F29" s="30" t="s">
+      <c r="E29" s="61" t="s">
+        <v>183</v>
+      </c>
+      <c r="F29" s="28" t="s">
         <v>96</v>
       </c>
       <c r="G29" s="28" t="s">
         <v>87</v>
       </c>
-      <c r="H29" s="68" t="s">
-        <v>678</v>
+      <c r="H29" s="28" t="s">
+        <v>676</v>
       </c>
       <c r="I29" s="28" t="s">
         <v>92</v>
       </c>
-      <c r="J29" s="28"/>
-      <c r="K29" s="72" t="s">
-        <v>679</v>
-      </c>
-      <c r="L29" s="68" t="s">
-        <v>680</v>
+      <c r="K29" s="28" t="s">
+        <v>677</v>
+      </c>
+      <c r="L29" s="28" t="s">
+        <v>678</v>
       </c>
       <c r="M29" s="28">
         <v>4</v>
@@ -8774,7 +8830,6 @@
       <c r="N29" s="28">
         <v>3</v>
       </c>
-      <c r="O29" s="28"/>
       <c r="P29" s="28">
         <v>6</v>
       </c>
@@ -8784,29 +8839,15 @@
       <c r="R29" s="28" t="s">
         <v>157</v>
       </c>
-      <c r="S29" s="68" t="s">
-        <v>677</v>
+      <c r="S29" s="28" t="s">
+        <v>675</v>
       </c>
       <c r="T29" s="28" t="s">
-        <v>83</v>
+        <v>717</v>
       </c>
       <c r="U29" s="28" t="s">
-        <v>151</v>
-      </c>
-      <c r="V29" s="28"/>
-      <c r="W29" s="28"/>
-      <c r="X29" s="28"/>
-      <c r="Y29" s="28"/>
-      <c r="Z29" s="28"/>
-      <c r="AA29" s="28"/>
-      <c r="AB29" s="28"/>
-      <c r="AC29" s="28"/>
-      <c r="AD29" s="28"/>
-      <c r="AE29" s="28"/>
-      <c r="AF29" s="28"/>
-      <c r="AG29" s="28"/>
-      <c r="AH29" s="28"/>
-      <c r="AI29" s="28"/>
+        <v>38</v>
+      </c>
     </row>
     <row r="30" spans="1:35" s="28" customFormat="1" ht="15" customHeight="1">
       <c r="A30" s="28">
@@ -8825,7 +8866,7 @@
         <v>183</v>
       </c>
       <c r="F30" s="28" t="s">
-        <v>705</v>
+        <v>703</v>
       </c>
       <c r="G30" s="28" t="s">
         <v>154</v>
@@ -8861,18 +8902,18 @@
         <v>210</v>
       </c>
       <c r="T30" s="28" t="s">
-        <v>83</v>
+        <v>717</v>
       </c>
       <c r="U30" s="28" t="s">
-        <v>151</v>
+        <v>38</v>
       </c>
     </row>
     <row r="31" spans="1:35" ht="15" customHeight="1">
       <c r="A31" s="28">
         <v>30</v>
       </c>
-      <c r="B31" s="72" t="s">
-        <v>667</v>
+      <c r="B31" t="s">
+        <v>7</v>
       </c>
       <c r="C31" s="28" t="s">
         <v>159</v>
@@ -8895,7 +8936,7 @@
       <c r="I31" s="28"/>
       <c r="J31" s="28"/>
       <c r="K31" s="72" t="s">
-        <v>682</v>
+        <v>680</v>
       </c>
       <c r="L31" s="28" t="s">
         <v>161</v>
@@ -8917,13 +8958,13 @@
         <v>159</v>
       </c>
       <c r="S31" s="68" t="s">
-        <v>681</v>
+        <v>679</v>
       </c>
       <c r="T31" s="28" t="s">
-        <v>83</v>
+        <v>717</v>
       </c>
       <c r="U31" s="28" t="s">
-        <v>151</v>
+        <v>38</v>
       </c>
       <c r="V31" s="28"/>
       <c r="W31" s="28"/>
@@ -8999,7 +9040,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="33" spans="1:21" s="28" customFormat="1" ht="13.8">
+    <row r="33" spans="1:21" s="28" customFormat="1" ht="13.5">
       <c r="A33" s="28" t="s">
         <v>206</v>
       </c>
@@ -9058,7 +9099,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="34" spans="1:21" s="28" customFormat="1" ht="13.8">
+    <row r="34" spans="1:21" s="28" customFormat="1" ht="13.5">
       <c r="A34" s="28" t="s">
         <v>217</v>
       </c>
@@ -9117,7 +9158,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="35" spans="1:21" s="28" customFormat="1" ht="13.8">
+    <row r="35" spans="1:21" s="28" customFormat="1" ht="13.5">
       <c r="A35" s="28" t="s">
         <v>224</v>
       </c>
@@ -9176,7 +9217,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="36" spans="1:21" s="28" customFormat="1" ht="13.8">
+    <row r="36" spans="1:21" s="28" customFormat="1" ht="13.5">
       <c r="A36" s="28" t="s">
         <v>230</v>
       </c>
@@ -9235,7 +9276,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="37" spans="1:21" s="28" customFormat="1" ht="13.8">
+    <row r="37" spans="1:21" s="28" customFormat="1" ht="13.5">
       <c r="A37" s="28" t="s">
         <v>237</v>
       </c>
@@ -9294,7 +9335,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="38" spans="1:21" s="28" customFormat="1" ht="13.8">
+    <row r="38" spans="1:21" s="28" customFormat="1" ht="13.5">
       <c r="A38" s="28" t="s">
         <v>243</v>
       </c>
@@ -9353,7 +9394,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="39" spans="1:21" s="28" customFormat="1" ht="13.8">
+    <row r="39" spans="1:21" s="28" customFormat="1" ht="13.5">
       <c r="A39" s="28" t="s">
         <v>251</v>
       </c>
@@ -9412,7 +9453,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="40" spans="1:21" s="28" customFormat="1" ht="13.8">
+    <row r="40" spans="1:21" s="28" customFormat="1" ht="13.5">
       <c r="A40" s="28" t="s">
         <v>254</v>
       </c>
@@ -9471,7 +9512,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="41" spans="1:21" s="28" customFormat="1" ht="13.8">
+    <row r="41" spans="1:21" s="28" customFormat="1" ht="13.5">
       <c r="A41" s="28" t="s">
         <v>257</v>
       </c>
@@ -9530,7 +9571,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="42" spans="1:21" s="28" customFormat="1" ht="13.8">
+    <row r="42" spans="1:21" s="28" customFormat="1" ht="13.5">
       <c r="A42" s="28" t="s">
         <v>266</v>
       </c>
@@ -9589,7 +9630,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="43" spans="1:21" s="28" customFormat="1" ht="13.8">
+    <row r="43" spans="1:21" s="28" customFormat="1" ht="13.5">
       <c r="A43" s="28" t="s">
         <v>270</v>
       </c>
@@ -9648,7 +9689,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="44" spans="1:21" s="28" customFormat="1" ht="13.8">
+    <row r="44" spans="1:21" s="28" customFormat="1" ht="13.5">
       <c r="A44" s="28" t="s">
         <v>279</v>
       </c>
@@ -9707,7 +9748,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="45" spans="1:21" s="28" customFormat="1" ht="13.8">
+    <row r="45" spans="1:21" s="28" customFormat="1" ht="13.5">
       <c r="A45" s="28" t="s">
         <v>286</v>
       </c>
@@ -9766,7 +9807,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="46" spans="1:21" s="28" customFormat="1" ht="13.8">
+    <row r="46" spans="1:21" s="28" customFormat="1" ht="13.5">
       <c r="A46" s="28" t="s">
         <v>292</v>
       </c>
@@ -9825,7 +9866,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="47" spans="1:21" s="28" customFormat="1" ht="13.8">
+    <row r="47" spans="1:21" s="28" customFormat="1" ht="13.5">
       <c r="A47" s="28" t="s">
         <v>298</v>
       </c>
@@ -9884,7 +9925,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="48" spans="1:21" s="28" customFormat="1" ht="13.8">
+    <row r="48" spans="1:21" s="28" customFormat="1" ht="13.5">
       <c r="A48" s="28" t="s">
         <v>304</v>
       </c>
@@ -9943,7 +9984,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="49" spans="1:21" s="28" customFormat="1" ht="13.8">
+    <row r="49" spans="1:21" s="28" customFormat="1" ht="13.5">
       <c r="A49" s="28" t="s">
         <v>309</v>
       </c>
@@ -10002,7 +10043,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="50" spans="1:21" s="28" customFormat="1" ht="13.8">
+    <row r="50" spans="1:21" s="28" customFormat="1" ht="13.5">
       <c r="A50" s="28" t="s">
         <v>315</v>
       </c>
@@ -10061,7 +10102,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="51" spans="1:21" s="28" customFormat="1" ht="13.8">
+    <row r="51" spans="1:21" s="28" customFormat="1" ht="13.5">
       <c r="A51" s="28" t="s">
         <v>321</v>
       </c>
@@ -10120,7 +10161,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="52" spans="1:21" s="28" customFormat="1" ht="13.8">
+    <row r="52" spans="1:21" s="28" customFormat="1" ht="13.5">
       <c r="A52" s="28" t="s">
         <v>327</v>
       </c>
@@ -10179,7 +10220,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="53" spans="1:21" s="28" customFormat="1" ht="13.8">
+    <row r="53" spans="1:21" s="28" customFormat="1" ht="13.5">
       <c r="A53" s="28" t="s">
         <v>354</v>
       </c>
@@ -10238,7 +10279,7 @@
         <v>336</v>
       </c>
     </row>
-    <row r="54" spans="1:21" ht="13.2">
+    <row r="54" spans="1:21" ht="12.75">
       <c r="A54" t="s">
         <v>360</v>
       </c>
@@ -10297,7 +10338,7 @@
         <v>336</v>
       </c>
     </row>
-    <row r="55" spans="1:21" s="28" customFormat="1" ht="13.8">
+    <row r="55" spans="1:21" s="28" customFormat="1" ht="13.5">
       <c r="A55" s="28" t="s">
         <v>364</v>
       </c>
@@ -10356,7 +10397,7 @@
         <v>336</v>
       </c>
     </row>
-    <row r="56" spans="1:21" s="28" customFormat="1" ht="13.8">
+    <row r="56" spans="1:21" s="28" customFormat="1" ht="13.5">
       <c r="A56" s="28" t="s">
         <v>370</v>
       </c>
@@ -10415,7 +10456,7 @@
         <v>336</v>
       </c>
     </row>
-    <row r="57" spans="1:21" s="28" customFormat="1" ht="13.8">
+    <row r="57" spans="1:21" s="28" customFormat="1" ht="13.5">
       <c r="A57" s="28" t="s">
         <v>375</v>
       </c>
@@ -10474,7 +10515,7 @@
         <v>336</v>
       </c>
     </row>
-    <row r="58" spans="1:21" s="28" customFormat="1" ht="13.8">
+    <row r="58" spans="1:21" s="28" customFormat="1" ht="13.5">
       <c r="A58" s="28" t="s">
         <v>382</v>
       </c>
@@ -10533,7 +10574,7 @@
         <v>336</v>
       </c>
     </row>
-    <row r="59" spans="1:21" s="28" customFormat="1" ht="13.8">
+    <row r="59" spans="1:21" s="28" customFormat="1" ht="13.5">
       <c r="A59" s="28" t="s">
         <v>388</v>
       </c>
@@ -10592,7 +10633,7 @@
         <v>336</v>
       </c>
     </row>
-    <row r="60" spans="1:21" s="28" customFormat="1" ht="13.8">
+    <row r="60" spans="1:21" s="28" customFormat="1" ht="13.5">
       <c r="A60" s="28" t="s">
         <v>395</v>
       </c>
@@ -10651,7 +10692,7 @@
         <v>336</v>
       </c>
     </row>
-    <row r="61" spans="1:21" s="28" customFormat="1" ht="13.8">
+    <row r="61" spans="1:21" s="28" customFormat="1" ht="13.5">
       <c r="A61" s="28" t="s">
         <v>402</v>
       </c>
@@ -10710,7 +10751,7 @@
         <v>336</v>
       </c>
     </row>
-    <row r="62" spans="1:21" s="28" customFormat="1" ht="13.8">
+    <row r="62" spans="1:21" s="28" customFormat="1" ht="13.5">
       <c r="A62" s="28" t="s">
         <v>408</v>
       </c>
@@ -10769,7 +10810,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="63" spans="1:21" s="28" customFormat="1" ht="13.8">
+    <row r="63" spans="1:21" s="28" customFormat="1" ht="13.5">
       <c r="A63" s="28" t="s">
         <v>411</v>
       </c>
@@ -10828,7 +10869,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="64" spans="1:21" s="28" customFormat="1" ht="13.8">
+    <row r="64" spans="1:21" s="28" customFormat="1" ht="13.5">
       <c r="A64" s="28" t="s">
         <v>416</v>
       </c>
@@ -10887,7 +10928,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="65" spans="1:21" s="28" customFormat="1" ht="13.8">
+    <row r="65" spans="1:21" s="28" customFormat="1" ht="13.5">
       <c r="A65" s="28" t="s">
         <v>422</v>
       </c>
@@ -10946,7 +10987,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="66" spans="1:21" s="28" customFormat="1" ht="13.8">
+    <row r="66" spans="1:21" s="28" customFormat="1" ht="13.5">
       <c r="A66" s="28" t="s">
         <v>427</v>
       </c>
@@ -11005,7 +11046,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="67" spans="1:21" s="28" customFormat="1" ht="13.8">
+    <row r="67" spans="1:21" s="28" customFormat="1" ht="13.5">
       <c r="A67" s="28" t="s">
         <v>433</v>
       </c>
@@ -11064,7 +11105,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="68" spans="1:21" s="28" customFormat="1" ht="13.8">
+    <row r="68" spans="1:21" s="28" customFormat="1" ht="13.5">
       <c r="A68" s="28" t="s">
         <v>495</v>
       </c>
@@ -11123,7 +11164,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="69" spans="1:21" s="28" customFormat="1" ht="13.8">
+    <row r="69" spans="1:21" s="28" customFormat="1" ht="13.5">
       <c r="A69" s="28" t="s">
         <v>500</v>
       </c>
@@ -11182,7 +11223,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="70" spans="1:21" s="28" customFormat="1" ht="13.8">
+    <row r="70" spans="1:21" s="28" customFormat="1" ht="13.5">
       <c r="A70" s="28" t="s">
         <v>502</v>
       </c>
@@ -11241,7 +11282,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="71" spans="1:21" s="28" customFormat="1" ht="13.8">
+    <row r="71" spans="1:21" s="28" customFormat="1" ht="13.5">
       <c r="A71" s="28" t="s">
         <v>508</v>
       </c>
@@ -11300,7 +11341,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="72" spans="1:21" s="28" customFormat="1" ht="13.8">
+    <row r="72" spans="1:21" s="28" customFormat="1" ht="13.5">
       <c r="A72" s="28" t="s">
         <v>513</v>
       </c>
@@ -11359,7 +11400,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="73" spans="1:21" s="28" customFormat="1" ht="13.8">
+    <row r="73" spans="1:21" s="28" customFormat="1" ht="13.5">
       <c r="A73" s="28" t="s">
         <v>515</v>
       </c>
@@ -11418,7 +11459,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="74" spans="1:21" s="28" customFormat="1" ht="13.8">
+    <row r="74" spans="1:21" s="28" customFormat="1" ht="13.5">
       <c r="A74" s="28" t="s">
         <v>519</v>
       </c>
@@ -11477,7 +11518,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="75" spans="1:21" s="28" customFormat="1" ht="13.8">
+    <row r="75" spans="1:21" s="28" customFormat="1" ht="13.5">
       <c r="A75" s="28" t="s">
         <v>525</v>
       </c>
@@ -11536,7 +11577,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="76" spans="1:21" s="28" customFormat="1" ht="13.8">
+    <row r="76" spans="1:21" s="28" customFormat="1" ht="13.5">
       <c r="A76" s="28" t="s">
         <v>531</v>
       </c>
@@ -11595,7 +11636,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="77" spans="1:21" s="28" customFormat="1" ht="13.8">
+    <row r="77" spans="1:21" s="28" customFormat="1" ht="13.5">
       <c r="A77" s="28" t="s">
         <v>536</v>
       </c>
@@ -11654,7 +11695,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="78" spans="1:21" s="28" customFormat="1" ht="13.8">
+    <row r="78" spans="1:21" s="28" customFormat="1" ht="13.5">
       <c r="A78" s="28" t="s">
         <v>543</v>
       </c>
@@ -11713,7 +11754,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="79" spans="1:21" s="28" customFormat="1" ht="13.8">
+    <row r="79" spans="1:21" s="28" customFormat="1" ht="13.5">
       <c r="A79" s="28" t="s">
         <v>546</v>
       </c>
@@ -11772,7 +11813,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="80" spans="1:21" s="28" customFormat="1" ht="13.8">
+    <row r="80" spans="1:21" s="28" customFormat="1" ht="13.5">
       <c r="A80" s="28" t="s">
         <v>552</v>
       </c>
@@ -11831,7 +11872,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="81" spans="1:21" s="28" customFormat="1" ht="13.8">
+    <row r="81" spans="1:21" s="28" customFormat="1" ht="13.5">
       <c r="A81" s="28" t="s">
         <v>559</v>
       </c>
@@ -11890,7 +11931,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="82" spans="1:21" s="28" customFormat="1" ht="13.8">
+    <row r="82" spans="1:21" s="28" customFormat="1" ht="13.5">
       <c r="A82" s="28" t="s">
         <v>564</v>
       </c>
@@ -11949,7 +11990,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="83" spans="1:21" s="28" customFormat="1" ht="13.8">
+    <row r="83" spans="1:21" s="28" customFormat="1" ht="13.5">
       <c r="A83" s="28" t="s">
         <v>569</v>
       </c>
@@ -12008,7 +12049,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="84" spans="1:21" s="28" customFormat="1" ht="13.8">
+    <row r="84" spans="1:21" s="28" customFormat="1" ht="13.5">
       <c r="A84" s="28" t="s">
         <v>572</v>
       </c>
@@ -12067,7 +12108,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="85" spans="1:21" s="28" customFormat="1" ht="13.8">
+    <row r="85" spans="1:21" s="28" customFormat="1" ht="13.5">
       <c r="A85" s="28" t="s">
         <v>576</v>
       </c>
@@ -12126,7 +12167,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="86" spans="1:21" s="28" customFormat="1" ht="13.8">
+    <row r="86" spans="1:21" s="28" customFormat="1" ht="13.5">
       <c r="A86" s="28" t="s">
         <v>617</v>
       </c>
@@ -12185,7 +12226,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="87" spans="1:21" s="28" customFormat="1" ht="13.8">
+    <row r="87" spans="1:21" s="28" customFormat="1" ht="13.5">
       <c r="A87" s="28" t="s">
         <v>621</v>
       </c>
@@ -12244,7 +12285,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="88" spans="1:21" s="28" customFormat="1" ht="13.8">
+    <row r="88" spans="1:21" s="28" customFormat="1" ht="13.5">
       <c r="A88" s="28" t="s">
         <v>626</v>
       </c>
@@ -12303,7 +12344,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="89" spans="1:21" s="28" customFormat="1" ht="13.8">
+    <row r="89" spans="1:21" s="28" customFormat="1" ht="13.5">
       <c r="A89" s="28" t="s">
         <v>630</v>
       </c>
@@ -12362,7 +12403,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="90" spans="1:21" s="28" customFormat="1" ht="13.8">
+    <row r="90" spans="1:21" s="28" customFormat="1" ht="13.5">
       <c r="A90" s="28" t="s">
         <v>636</v>
       </c>
@@ -12421,7 +12462,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="91" spans="1:21" s="28" customFormat="1" ht="13.8">
+    <row r="91" spans="1:21" s="28" customFormat="1" ht="13.5">
       <c r="A91" s="28" t="s">
         <v>640</v>
       </c>
@@ -12480,7 +12521,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="92" spans="1:21" s="28" customFormat="1" ht="13.8">
+    <row r="92" spans="1:21" s="28" customFormat="1" ht="13.5">
       <c r="A92" s="28" t="s">
         <v>644</v>
       </c>
@@ -12539,12 +12580,12 @@
         <v>17</v>
       </c>
     </row>
-    <row r="93" spans="1:21" ht="13.8">
+    <row r="93" spans="1:21" ht="13.5">
       <c r="A93" t="s">
         <v>647</v>
       </c>
-      <c r="B93" t="s">
-        <v>438</v>
+      <c r="B93" s="28" t="s">
+        <v>7</v>
       </c>
       <c r="C93" t="s">
         <v>121</v>
@@ -12598,15 +12639,15 @@
         <v>17</v>
       </c>
     </row>
-    <row r="94" spans="1:21" ht="13.8">
+    <row r="94" spans="1:21" ht="13.5">
       <c r="A94" t="s">
-        <v>683</v>
-      </c>
-      <c r="B94" t="s">
-        <v>438</v>
+        <v>681</v>
+      </c>
+      <c r="B94" s="28" t="s">
+        <v>7</v>
       </c>
       <c r="C94" t="s">
-        <v>684</v>
+        <v>682</v>
       </c>
       <c r="D94" t="s">
         <v>86</v>
@@ -12621,7 +12662,7 @@
         <v>148</v>
       </c>
       <c r="H94" t="s">
-        <v>685</v>
+        <v>683</v>
       </c>
       <c r="I94" t="s">
         <v>209</v>
@@ -12630,7 +12671,7 @@
         <v>210</v>
       </c>
       <c r="L94" t="s">
-        <v>686</v>
+        <v>684</v>
       </c>
       <c r="M94" t="s">
         <v>212</v>
@@ -12645,10 +12686,10 @@
         <v>215</v>
       </c>
       <c r="R94" t="s">
-        <v>684</v>
+        <v>682</v>
       </c>
       <c r="S94" t="s">
-        <v>687</v>
+        <v>685</v>
       </c>
       <c r="T94" s="28" t="s">
         <v>83</v>
@@ -12657,15 +12698,15 @@
         <v>9</v>
       </c>
     </row>
-    <row r="95" spans="1:21" ht="13.8">
+    <row r="95" spans="1:21" ht="13.5">
       <c r="A95" t="s">
-        <v>688</v>
-      </c>
-      <c r="B95" t="s">
-        <v>438</v>
+        <v>686</v>
+      </c>
+      <c r="B95" s="28" t="s">
+        <v>7</v>
       </c>
       <c r="C95" t="s">
-        <v>689</v>
+        <v>687</v>
       </c>
       <c r="D95" t="s">
         <v>86</v>
@@ -12689,7 +12730,7 @@
         <v>443</v>
       </c>
       <c r="L95" t="s">
-        <v>690</v>
+        <v>688</v>
       </c>
       <c r="M95" t="s">
         <v>212</v>
@@ -12704,10 +12745,10 @@
         <v>215</v>
       </c>
       <c r="R95" t="s">
+        <v>687</v>
+      </c>
+      <c r="S95" t="s">
         <v>689</v>
-      </c>
-      <c r="S95" t="s">
-        <v>691</v>
       </c>
       <c r="T95" s="28" t="s">
         <v>83</v>
@@ -12716,12 +12757,12 @@
         <v>9</v>
       </c>
     </row>
-    <row r="96" spans="1:21" ht="13.8">
+    <row r="96" spans="1:21" ht="13.5">
       <c r="A96" t="s">
-        <v>692</v>
-      </c>
-      <c r="B96" t="s">
-        <v>438</v>
+        <v>690</v>
+      </c>
+      <c r="B96" s="28" t="s">
+        <v>7</v>
       </c>
       <c r="C96" t="s">
         <v>91</v>
@@ -12775,15 +12816,15 @@
         <v>9</v>
       </c>
     </row>
-    <row r="97" spans="1:21" ht="13.8">
+    <row r="97" spans="1:21" ht="13.5">
       <c r="A97" t="s">
-        <v>696</v>
-      </c>
-      <c r="B97" t="s">
-        <v>438</v>
+        <v>694</v>
+      </c>
+      <c r="B97" s="28" t="s">
+        <v>7</v>
       </c>
       <c r="C97" t="s">
-        <v>697</v>
+        <v>695</v>
       </c>
       <c r="D97" t="s">
         <v>86</v>
@@ -12798,7 +12839,7 @@
         <v>148</v>
       </c>
       <c r="H97" t="s">
-        <v>698</v>
+        <v>696</v>
       </c>
       <c r="I97" t="s">
         <v>209</v>
@@ -12807,7 +12848,7 @@
         <v>210</v>
       </c>
       <c r="L97" t="s">
-        <v>699</v>
+        <v>697</v>
       </c>
       <c r="M97" t="s">
         <v>212</v>
@@ -12822,10 +12863,10 @@
         <v>215</v>
       </c>
       <c r="R97" t="s">
-        <v>697</v>
+        <v>695</v>
       </c>
       <c r="S97" t="s">
-        <v>700</v>
+        <v>698</v>
       </c>
       <c r="T97" s="28" t="s">
         <v>83</v>
@@ -12838,7 +12879,7 @@
   <customSheetViews>
     <customSheetView guid="{A7754112-A52F-4ABC-8778-92F04773E53C}" filter="1" showAutoFilter="1">
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-      <autoFilter ref="A1:AD33" xr:uid="{2452B91A-1092-476C-AA9F-A0F90977EB27}">
+      <autoFilter ref="A1:AD33" xr:uid="{6C46D9A0-423D-4209-BC8B-2A919D166CCC}">
         <filterColumn colId="5">
           <filters blank="1">
             <filter val="Strathnairn"/>
@@ -12848,7 +12889,7 @@
     </customSheetView>
     <customSheetView guid="{C25CEB9E-BEC1-4982-90C4-50C84EE1B82A}" filter="1" showAutoFilter="1">
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-      <autoFilter ref="A1:AD33" xr:uid="{2B19F17B-E94C-4ACA-A398-EF54335794CA}"/>
+      <autoFilter ref="A1:AD33" xr:uid="{EFC939B7-DF89-4B3F-B51B-36EEFA6E0F08}"/>
     </customSheetView>
   </customSheetViews>
   <conditionalFormatting sqref="A1:AI1">
@@ -12921,23 +12962,23 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15.75" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="14.46484375" defaultRowHeight="15.75" customHeight="1"/>
   <cols>
     <col min="1" max="1" width="16" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="14.5546875" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="16.77734375" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="14.5546875" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="13.21875" customWidth="1" collapsed="1"/>
-    <col min="15" max="15" width="20.88671875" customWidth="1" collapsed="1"/>
-    <col min="21" max="21" width="19.109375" customWidth="1" collapsed="1"/>
-    <col min="22" max="22" width="19.21875" customWidth="1" collapsed="1"/>
-    <col min="23" max="23" width="20.109375" customWidth="1" collapsed="1"/>
-    <col min="24" max="24" width="19.77734375" customWidth="1" collapsed="1"/>
-    <col min="26" max="26" width="15.88671875" customWidth="1" collapsed="1"/>
-    <col min="27" max="27" width="13.44140625" customWidth="1" collapsed="1"/>
-    <col min="28" max="28" width="15.21875" customWidth="1" collapsed="1"/>
-    <col min="29" max="29" width="16.109375" customWidth="1" collapsed="1"/>
-    <col min="30" max="30" width="15.88671875" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="14.53125" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="16.796875" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="14.53125" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="13.19921875" customWidth="1" collapsed="1"/>
+    <col min="15" max="15" width="20.86328125" customWidth="1" collapsed="1"/>
+    <col min="21" max="21" width="19.1328125" customWidth="1" collapsed="1"/>
+    <col min="22" max="22" width="19.19921875" customWidth="1" collapsed="1"/>
+    <col min="23" max="23" width="20.1328125" customWidth="1" collapsed="1"/>
+    <col min="24" max="24" width="19.796875" customWidth="1" collapsed="1"/>
+    <col min="26" max="26" width="15.86328125" customWidth="1" collapsed="1"/>
+    <col min="27" max="27" width="13.46484375" customWidth="1" collapsed="1"/>
+    <col min="28" max="28" width="15.19921875" customWidth="1" collapsed="1"/>
+    <col min="29" max="29" width="16.1328125" customWidth="1" collapsed="1"/>
+    <col min="30" max="30" width="15.86328125" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:35" ht="15.75" customHeight="1">
@@ -13060,16 +13101,16 @@
       <selection pane="bottomLeft" activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15.75" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="14.46484375" defaultRowHeight="15.75" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="44.88671875" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="17.109375" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="26.44140625" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="36.109375" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="51.109375" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" width="44.86328125" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="17.1328125" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="26.46484375" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="36.1328125" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="51.1328125" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:26" ht="13.8">
+    <row r="1" spans="1:26" ht="13.9">
       <c r="A1" s="42" t="s">
         <v>163</v>
       </c>

</xml_diff>

<commit_message>
Scripts 5 run 20/06/2021
</commit_message>
<xml_diff>
--- a/src/main/resources/InputTestdata/Listing details.xlsx
+++ b/src/main/resources/InputTestdata/Listing details.xlsx
@@ -1,39 +1,39 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24026"/>
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <mc:AlternateContent>
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Athavan\git\777Homes-2\777Homes-business\src\main\resources\InputTestdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7176A150-6395-4026-BB14-892D1F48AE0B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr documentId="13_ncr:1_{30AB22AF-B962-45E9-A187-B441513416E8}" revIDLastSave="0" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="20715" windowHeight="13276" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView activeTab="1" windowHeight="13276" windowWidth="20715" xWindow="-98" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}" yWindow="-98"/>
   </bookViews>
   <sheets>
-    <sheet name="Backlog" sheetId="1" r:id="rId1"/>
-    <sheet name="Listing" sheetId="2" r:id="rId2"/>
-    <sheet name="Tobe-executed" sheetId="3" r:id="rId3"/>
-    <sheet name="Agency login" sheetId="4" r:id="rId4"/>
+    <sheet name="Backlog" r:id="rId1" sheetId="1"/>
+    <sheet name="Listing" r:id="rId2" sheetId="2"/>
+    <sheet name="Tobe-executed" r:id="rId3" sheetId="3"/>
+    <sheet name="Agency login" r:id="rId4" sheetId="4"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Backlog!$A$1:$AB$52</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Listing!#REF!</definedName>
-    <definedName name="Z_A7754112_A52F_4ABC_8778_92F04773E53C_.wvu.FilterData" localSheetId="1" hidden="1">Listing!$A$1:$AE$32</definedName>
-    <definedName name="Z_C25CEB9E_BEC1_4982_90C4_50C84EE1B82A_.wvu.FilterData" localSheetId="1" hidden="1">Listing!$A$1:$AE$32</definedName>
+    <definedName hidden="1" localSheetId="0" name="_xlnm._FilterDatabase">Backlog!$A$1:$AB$52</definedName>
+    <definedName hidden="1" localSheetId="1" name="_xlnm._FilterDatabase">Listing!#REF!</definedName>
+    <definedName hidden="1" localSheetId="1" name="Z_A7754112_A52F_4ABC_8778_92F04773E53C_.wvu.FilterData">Listing!$A$1:$AE$32</definedName>
+    <definedName hidden="1" localSheetId="1" name="Z_C25CEB9E_BEC1_4982_90C4_50C84EE1B82A_.wvu.FilterData">Listing!$A$1:$AE$32</definedName>
   </definedNames>
   <calcPr calcId="181029"/>
   <customWorkbookViews>
-    <customWorkbookView name="Filter 2" guid="{C25CEB9E-BEC1-4982-90C4-50C84EE1B82A}" maximized="1" windowWidth="0" windowHeight="0" activeSheetId="0"/>
-    <customWorkbookView name="Filter 1" guid="{A7754112-A52F-4ABC-8778-92F04773E53C}" maximized="1" windowWidth="0" windowHeight="0" activeSheetId="0"/>
+    <customWorkbookView activeSheetId="0" guid="{A7754112-A52F-4ABC-8778-92F04773E53C}" maximized="1" name="Filter 1" windowHeight="0" windowWidth="0"/>
+    <customWorkbookView activeSheetId="0" guid="{C25CEB9E-BEC1-4982-90C4-50C84EE1B82A}" maximized="1" name="Filter 2" windowHeight="0" windowWidth="0"/>
   </customWorkbookViews>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2322" uniqueCount="717">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2400" uniqueCount="737">
   <si>
     <t>ID</t>
   </si>
@@ -3333,6 +3333,105 @@
   </si>
   <si>
     <t>https://www.777homes.com.au/?post_type=property&amp;p=6070&amp;preview=true</t>
+  </si>
+  <si>
+    <t>https://www.allhomes.com.au/unit-11-15-bill-ferguson-circuit-bonner-act-2914</t>
+  </si>
+  <si>
+    <t>https://www.allhomes.com.au/unit-294-1-anthony-rolfe-avenue-gungahlin-act-2912</t>
+  </si>
+  <si>
+    <t>https://www.allhomes.com.au/14-hartley-street-turner-act-2612</t>
+  </si>
+  <si>
+    <t>98</t>
+  </si>
+  <si>
+    <t>11/15 Bill Ferguson Circuit, Bonner ACT 2914</t>
+  </si>
+  <si>
+    <t>Block/House: 106/ -</t>
+  </si>
+  <si>
+    <t>New Door Properties is proudly presenting this spacious 2-bedroom apartment that has been released to the market, so do not miss out the opportunity.
+Call to all first home buyers and investors!
+This apartment boasts lots of natural light, with spacious open plan living areas that create a sense of space. Also included is a split system air conditioner and you benefit from a good-sized North and South facing balcony. The modern kitchen has stainless steel appliances, combined with stone bench tops and a functional layout that makes life for the chef in the family a bit easier.
+The 2 bedrooms are all a good size, the master with Ensuite and there are robes in each room. The large bathroom also incorporates the European style laundry. Apartment is located on level 2, with secured entrance to the building along with the secured entrance to the car port located in the private complex.
+Easy walking distance to cafes, parks, playing fields and Neville Bonner Primary School is just walkable distance.
+Property Features:
+• Two Spacious Bedrooms
+• Main bedroom with Ensuite &amp; built-in-robe
+• Second bedroom with built-in-robe
+• Spacious Kitchen with ample of storage cupboards
+• Tiled splashback in kitchen
+• 600 mm stainless steel appliances, gas cooktop, oven &amp; dishwasher
+• European laundry in main bathroom
+- Separate two facing balcony
+• Split aircon in Living
+• Secured intercom entrance to the building, and carport
+• Strata fees: $857 per quarter (approx.)
+• Rates: $404 per quarter (approx.)
+Property Information:
+Living : 89 m2 (approx.)
+Balcony : 22 m2 (approx.)
+Storage : 4 m2 (approx.)
+EER : 6 Stars</t>
+  </si>
+  <si>
+    <t>99</t>
+  </si>
+  <si>
+    <t>294/1 Anthony Rolfe Ave, Gungahlin ACT 2912</t>
+  </si>
+  <si>
+    <t>Block/House: 76/ -</t>
+  </si>
+  <si>
+    <t>This is an incredible opportunity to own an apartment in the heart of Gungahlin. A stones throw from all the local amenities including Light Rail. You can't help but smile when you walk into this gorgeous apartment. This north facing apartment showcases some of the best views to Brindabella mountains. An apartment with natural light, its truly has a great feel to it.
+A chance to buy for an investment or living the lifestyle your deserve on daily basis. A short stroll to the heart of the Gungahlin shopping district. If you are an investor, then consider someone else paying off the apartment in the mid term and when you are ready to move in, on reflection it could be the best investment you have ever made.
+On the 5th floor is the Sky Deck. With its; open spaces and separate BBQ areas, , a beautiful infinity pool, with a quality gym and a sitting area which can be used for private functions or parties with friends and family to enjoy and of course incredible views over Yerrabi Pond &amp; Gungahlin Town Centre. This is definitely a lifestyle and an investment in your future. Call us now to view this amazing apartment before you miss this one.
+Property Features Include:
+North facing with beautiful views
+Sunset &amp; water views
+2 Rooms with practical layout
+Walk-in Robe
+Heating &amp; cooling system
+Parking with storage cage
+Intercom access to foyer
+Gym &amp; Function room
+Barbecue area
+Infinity edge Pool &amp; Spa
+Short stroll to Gungahlin Town Centre
+Much more on offer to enjoy living the life style you deserve in this apartment.
+Call us now before you miss this one.</t>
+  </si>
+  <si>
+    <t>100</t>
+  </si>
+  <si>
+    <t>14 Hartley Street, Turner ACT 2612</t>
+  </si>
+  <si>
+    <t>Block/House: 813/ -</t>
+  </si>
+  <si>
+    <t xml:space="preserve">4	7	0	0	0	0	</t>
+  </si>
+  <si>
+    <t>$470,000</t>
+  </si>
+  <si>
+    <t>Located in Unit 21/ 14 Hartley Street, Turner ACT 2612, this unit is one of a kind. A special place for those who want to have a peaceful and comfortable living.
+Enjoy its one spacious bedroom with one living room consists of alluring highlights and with a touch of modern architectural designs. Every corner is filled with natural light and giving you a vacation like vibe.</t>
+  </si>
+  <si>
+    <t>https://www.777homes.com.au/?post_type=property&amp;p=7483&amp;preview=true</t>
+  </si>
+  <si>
+    <t>https://www.777homes.com.au/?post_type=property&amp;p=7485&amp;preview=true</t>
+  </si>
+  <si>
+    <t>https://www.777homes.com.au/?post_type=property&amp;p=7487&amp;preview=true</t>
   </si>
 </sst>
 </file>
@@ -3513,7 +3612,7 @@
       <name val="Arial"/>
     </font>
   </fonts>
-  <fills count="11">
+  <fills count="14">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -3573,6 +3672,21 @@
         <bgColor indexed="2"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="mediumGray">
+        <bgColor indexed="2"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="mediumGray">
+        <bgColor indexed="2"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="mediumGray">
+        <bgColor indexed="2"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -3584,155 +3698,158 @@
     </border>
   </borders>
   <cellStyleXfs count="2">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
+    <xf applyAlignment="0" applyBorder="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="0" fontId="29" numFmtId="0"/>
   </cellStyleXfs>
-  <cellXfs count="63">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+  <cellXfs count="66">
+    <xf applyAlignment="1" applyFont="1" borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyAlignment="1" applyFill="1" applyFont="1" borderId="0" fillId="3" fontId="1" numFmtId="0" xfId="0">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf applyAlignment="1" applyFill="1" applyFont="1" borderId="0" fillId="2" fontId="2" numFmtId="0" xfId="0">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf applyAlignment="1" applyFill="1" applyFont="1" borderId="0" fillId="2" fontId="3" numFmtId="0" xfId="0"/>
+    <xf applyAlignment="1" applyFill="1" applyFont="1" borderId="0" fillId="2" fontId="4" numFmtId="0" xfId="0">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf applyAlignment="1" applyFill="1" applyFont="1" borderId="0" fillId="4" fontId="5" numFmtId="0" xfId="0">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf applyAlignment="1" applyFill="1" applyFont="1" borderId="0" fillId="2" fontId="6" numFmtId="0" xfId="0">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf applyFill="1" applyFont="1" borderId="0" fillId="2" fontId="4" numFmtId="0" xfId="0"/>
+    <xf applyAlignment="1" applyFill="1" applyFont="1" borderId="0" fillId="2" fontId="7" numFmtId="0" xfId="0"/>
+    <xf applyAlignment="1" applyFill="1" applyFont="1" borderId="0" fillId="2" fontId="8" numFmtId="0" xfId="0"/>
+    <xf applyAlignment="1" applyFill="1" applyFont="1" borderId="0" fillId="2" fontId="5" numFmtId="0" xfId="0">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf applyAlignment="1" applyFill="1" applyFont="1" borderId="0" fillId="5" fontId="4" numFmtId="0" xfId="0">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf applyAlignment="1" applyFill="1" applyFont="1" borderId="0" fillId="6" fontId="4" numFmtId="0" xfId="0">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf applyAlignment="1" applyFill="1" applyFont="1" borderId="0" fillId="2" fontId="9" numFmtId="0" xfId="0">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="11" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf applyAlignment="1" applyFill="1" applyFont="1" borderId="0" fillId="2" fontId="10" numFmtId="0" xfId="0"/>
+    <xf applyAlignment="1" applyFill="1" applyFont="1" borderId="0" fillId="2" fontId="11" numFmtId="0" xfId="0"/>
+    <xf applyAlignment="1" applyFill="1" applyFont="1" borderId="0" fillId="4" fontId="4" numFmtId="0" xfId="0">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf applyAlignment="1" applyFill="1" applyFont="1" borderId="0" fillId="2" fontId="4" numFmtId="0" xfId="0">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="13" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="14" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="15" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="16" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="17" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf applyAlignment="1" applyFill="1" applyFont="1" borderId="0" fillId="2" fontId="12" numFmtId="0" xfId="0"/>
+    <xf applyAlignment="1" applyFill="1" applyFont="1" borderId="0" fillId="2" fontId="13" numFmtId="0" xfId="0"/>
+    <xf applyAlignment="1" applyFill="1" applyFont="1" borderId="0" fillId="2" fontId="14" numFmtId="0" xfId="0"/>
+    <xf applyAlignment="1" applyFill="1" applyFont="1" borderId="0" fillId="2" fontId="15" numFmtId="0" xfId="0"/>
+    <xf applyAlignment="1" applyFill="1" applyFont="1" borderId="0" fillId="2" fontId="16" numFmtId="0" xfId="0"/>
+    <xf applyAlignment="1" applyFill="1" applyFont="1" borderId="0" fillId="2" fontId="17" numFmtId="0" xfId="0"/>
+    <xf applyAlignment="1" applyFill="1" applyFont="1" borderId="0" fillId="5" fontId="4" numFmtId="0" xfId="0"/>
+    <xf applyFill="1" applyFont="1" borderId="0" fillId="5" fontId="4" numFmtId="0" xfId="0"/>
+    <xf applyAlignment="1" applyFill="1" applyFont="1" borderId="0" fillId="3" fontId="1" numFmtId="0" xfId="0">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="18" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf applyFill="1" applyFont="1" borderId="0" fillId="3" fontId="7" numFmtId="0" xfId="0"/>
+    <xf applyAlignment="1" applyFill="1" applyFont="1" borderId="0" fillId="2" fontId="18" numFmtId="0" xfId="0">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf applyAlignment="1" applyFill="1" applyFont="1" borderId="0" fillId="2" fontId="19" numFmtId="0" xfId="0">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf applyAlignment="1" applyFill="1" applyFont="1" borderId="0" fillId="2" fontId="20" numFmtId="0" xfId="0">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf applyAlignment="1" applyFill="1" applyFont="1" borderId="0" fillId="2" fontId="21" numFmtId="0" xfId="0">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf applyAlignment="1" applyFill="1" applyFont="1" borderId="0" fillId="2" fontId="18" numFmtId="0" xfId="0">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf applyAlignment="1" applyFill="1" applyFont="1" borderId="0" fillId="2" fontId="22" numFmtId="0" xfId="0">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf applyAlignment="1" applyFill="1" applyFont="1" borderId="0" fillId="2" fontId="23" numFmtId="0" xfId="0">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf applyAlignment="1" applyFill="1" applyFont="1" borderId="0" fillId="2" fontId="22" numFmtId="0" xfId="0">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="3" fontId="23" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf applyAlignment="1" applyFill="1" applyFont="1" applyNumberFormat="1" borderId="0" fillId="2" fontId="23" numFmtId="3" xfId="0">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="164" fontId="23" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf applyAlignment="1" applyFill="1" applyFont="1" applyNumberFormat="1" borderId="0" fillId="2" fontId="23" numFmtId="164" xfId="0">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf applyAlignment="1" applyFill="1" applyFont="1" borderId="0" fillId="2" fontId="22" numFmtId="0" xfId="0">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="24" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf applyAlignment="1" applyFill="1" applyFont="1" borderId="0" fillId="2" fontId="24" numFmtId="0" xfId="0">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf applyAlignment="1" applyFill="1" applyFont="1" borderId="0" fillId="2" fontId="23" numFmtId="0" xfId="0">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf applyAlignment="1" applyFill="1" applyFont="1" borderId="0" fillId="2" fontId="22" numFmtId="0" xfId="0">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf applyAlignment="1" applyFont="1" borderId="0" fillId="0" fontId="7" numFmtId="0" xfId="0">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf applyAlignment="1" applyFill="1" applyFont="1" borderId="0" fillId="5" fontId="17" numFmtId="0" xfId="0">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf applyAlignment="1" applyFill="1" applyFont="1" borderId="0" fillId="5" fontId="17" numFmtId="0" xfId="0">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf applyAlignment="1" applyFill="1" applyFont="1" borderId="0" fillId="5" fontId="4" numFmtId="0" xfId="0">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="25" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf applyAlignment="1" applyFill="1" applyFont="1" borderId="0" fillId="5" fontId="25" numFmtId="0" xfId="0">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="26" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="17" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="12" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="25" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf applyAlignment="1" applyFill="1" applyFont="1" borderId="0" fillId="5" fontId="26" numFmtId="0" xfId="0"/>
+    <xf applyAlignment="1" applyFill="1" applyFont="1" borderId="0" fillId="3" fontId="17" numFmtId="0" xfId="0"/>
+    <xf applyAlignment="1" applyFill="1" applyFont="1" borderId="0" fillId="3" fontId="12" numFmtId="0" xfId="0"/>
+    <xf applyAlignment="1" applyFill="1" applyFont="1" borderId="0" fillId="3" fontId="25" numFmtId="0" xfId="0">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="27" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="28" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf applyAlignment="1" applyFill="1" applyFont="1" borderId="0" fillId="3" fontId="27" numFmtId="0" xfId="0"/>
+    <xf applyAlignment="1" applyFont="1" borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0"/>
+    <xf applyAlignment="1" applyFill="1" applyFont="1" borderId="0" fillId="3" fontId="28" numFmtId="0" xfId="0">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf applyAlignment="1" applyFill="1" applyFont="1" borderId="0" fillId="3" fontId="1" numFmtId="0" xfId="0">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf applyAlignment="1" applyFont="1" borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="29" fillId="2" borderId="0" xfId="1" applyFill="1" applyAlignment="1">
+    <xf applyAlignment="1" applyFill="1" borderId="0" fillId="2" fontId="29" numFmtId="0" xfId="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf applyAlignment="1" applyFill="1" applyFont="1" borderId="0" fillId="7" fontId="2" numFmtId="0" xfId="0">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf applyAlignment="1" applyFill="1" applyFont="1" borderId="0" fillId="8" fontId="5" numFmtId="0" xfId="0">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="29" fillId="2" borderId="0" xfId="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="18" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf applyAlignment="1" borderId="0" fillId="0" fontId="29" numFmtId="0" xfId="1"/>
+    <xf applyAlignment="1" applyFill="1" borderId="0" fillId="2" fontId="29" numFmtId="0" xfId="1"/>
+    <xf applyAlignment="1" applyFill="1" applyFont="1" borderId="0" fillId="9" fontId="18" numFmtId="0" xfId="0">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1"/>
+    <xf applyFill="1" borderId="0" fillId="10" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyFill="1" borderId="0" fillId="11" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyFill="1" borderId="0" fillId="12" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyFill="1" borderId="0" fillId="13" fontId="0" numFmtId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="2">
-    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle builtinId="8" name="Hyperlink" xfId="1"/>
+    <cellStyle builtinId="0" name="Normal" xfId="0"/>
   </cellStyles>
   <dxfs count="2">
     <dxf>
@@ -3752,7 +3869,7 @@
       </fill>
     </dxf>
   </dxfs>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <tableStyles count="0" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium2"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -3876,21 +3993,21 @@
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
-        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cap="flat" cmpd="sng" w="6350">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
           <a:miter lim="800000"/>
         </a:ln>
-        <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cap="flat" cmpd="sng" w="12700">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
           <a:miter lim="800000"/>
         </a:ln>
-        <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cap="flat" cmpd="sng" w="19050">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
@@ -3907,7 +4024,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+            <a:outerShdw algn="ctr" blurRad="57150" dir="5400000" dist="19050" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="63000"/>
               </a:srgbClr>
@@ -3961,32 +4078,32 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:AB98"/>
+  <dimension ref="A1:AC101"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B15" sqref="B15"/>
+    <sheetView workbookViewId="0">
+      <pane activePane="bottomLeft" state="frozen" topLeftCell="A26" ySplit="1"/>
+      <selection activeCell="B15" pane="bottomLeft" sqref="B15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.46484375" defaultRowHeight="15.75" customHeight="1"/>
+  <sheetFormatPr customHeight="1" defaultColWidth="14.46484375" defaultRowHeight="15.75"/>
   <cols>
-    <col min="1" max="1" width="9.19921875" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="74.796875" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="75" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="14.53125" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="22.1328125" style="55" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="21.86328125" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="56.86328125" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="10.86328125" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="17.86328125" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="22.53125" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="9.19921875" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="74.796875" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="75.0" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="14.53125" collapsed="true"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" style="55" width="22.1328125" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" width="21.86328125" collapsed="true"/>
+    <col min="8" max="8" customWidth="true" width="56.86328125" collapsed="true"/>
+    <col min="9" max="9" customWidth="true" width="10.86328125" collapsed="true"/>
+    <col min="10" max="10" customWidth="true" width="17.86328125" collapsed="true"/>
+    <col min="11" max="11" customWidth="true" width="22.53125" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:28" ht="13.9">
+    <row ht="13.9" r="1" spans="1:28">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -4013,7 +4130,7 @@
       </c>
       <c r="J1" s="1"/>
     </row>
-    <row r="2" spans="1:28" ht="15.75" customHeight="1">
+    <row customHeight="1" ht="15.75" r="2" spans="1:28">
       <c r="A2" s="2">
         <v>1</v>
       </c>
@@ -4059,7 +4176,7 @@
       <c r="AA2" s="7"/>
       <c r="AB2" s="7"/>
     </row>
-    <row r="3" spans="1:28" ht="13.9">
+    <row ht="13.9" r="3" spans="1:28">
       <c r="A3" s="2">
         <v>2</v>
       </c>
@@ -4105,7 +4222,7 @@
       <c r="AA3" s="7"/>
       <c r="AB3" s="7"/>
     </row>
-    <row r="4" spans="1:28" ht="15.75" customHeight="1">
+    <row customHeight="1" ht="15.75" r="4" spans="1:28">
       <c r="A4" s="10">
         <v>3</v>
       </c>
@@ -4151,7 +4268,7 @@
       <c r="AA4" s="7"/>
       <c r="AB4" s="7"/>
     </row>
-    <row r="5" spans="1:28" ht="13.9">
+    <row ht="13.9" r="5" spans="1:28">
       <c r="A5" s="10">
         <v>4</v>
       </c>
@@ -4195,7 +4312,7 @@
       <c r="AA5" s="7"/>
       <c r="AB5" s="7"/>
     </row>
-    <row r="6" spans="1:28" ht="13.9">
+    <row ht="13.9" r="6" spans="1:28">
       <c r="A6" s="10">
         <v>5</v>
       </c>
@@ -4239,7 +4356,7 @@
       <c r="AA6" s="10"/>
       <c r="AB6" s="10"/>
     </row>
-    <row r="7" spans="1:28" ht="13.9">
+    <row ht="13.9" r="7" spans="1:28">
       <c r="A7" s="10">
         <v>6</v>
       </c>
@@ -4283,7 +4400,7 @@
       <c r="AA7" s="7"/>
       <c r="AB7" s="7"/>
     </row>
-    <row r="8" spans="1:28" ht="13.9">
+    <row ht="13.9" r="8" spans="1:28">
       <c r="A8" s="10">
         <v>7</v>
       </c>
@@ -4325,7 +4442,7 @@
       <c r="AA8" s="7"/>
       <c r="AB8" s="7"/>
     </row>
-    <row r="9" spans="1:28" ht="13.9">
+    <row ht="13.9" r="9" spans="1:28">
       <c r="A9" s="10">
         <v>8</v>
       </c>
@@ -4367,7 +4484,7 @@
       <c r="AA9" s="7"/>
       <c r="AB9" s="7"/>
     </row>
-    <row r="10" spans="1:28" ht="13.9">
+    <row ht="13.9" r="10" spans="1:28">
       <c r="A10" s="10">
         <v>9</v>
       </c>
@@ -4409,7 +4526,7 @@
       <c r="AA10" s="7"/>
       <c r="AB10" s="7"/>
     </row>
-    <row r="11" spans="1:28" ht="13.9">
+    <row ht="13.9" r="11" spans="1:28">
       <c r="A11" s="10">
         <v>10</v>
       </c>
@@ -4453,7 +4570,7 @@
       <c r="AA11" s="7"/>
       <c r="AB11" s="7"/>
     </row>
-    <row r="12" spans="1:28" ht="13.9">
+    <row ht="13.9" r="12" spans="1:28">
       <c r="A12" s="10">
         <v>11</v>
       </c>
@@ -4495,7 +4612,7 @@
       <c r="AA12" s="7"/>
       <c r="AB12" s="7"/>
     </row>
-    <row r="13" spans="1:28" ht="13.9">
+    <row ht="13.9" r="13" spans="1:28">
       <c r="A13" s="10">
         <v>12</v>
       </c>
@@ -4537,7 +4654,7 @@
       <c r="AA13" s="7"/>
       <c r="AB13" s="7"/>
     </row>
-    <row r="14" spans="1:28" ht="13.9">
+    <row ht="13.9" r="14" spans="1:28">
       <c r="A14" s="10">
         <v>13</v>
       </c>
@@ -4579,7 +4696,7 @@
       <c r="AA14" s="7"/>
       <c r="AB14" s="7"/>
     </row>
-    <row r="15" spans="1:28" ht="13.9">
+    <row ht="13.9" r="15" spans="1:28">
       <c r="A15" s="10">
         <v>14</v>
       </c>
@@ -4623,7 +4740,7 @@
       <c r="AA15" s="7"/>
       <c r="AB15" s="7"/>
     </row>
-    <row r="16" spans="1:28" ht="13.9">
+    <row ht="13.9" r="16" spans="1:28">
       <c r="A16" s="10">
         <v>15</v>
       </c>
@@ -4665,7 +4782,7 @@
       <c r="AA16" s="7"/>
       <c r="AB16" s="7"/>
     </row>
-    <row r="17" spans="1:28" ht="13.9">
+    <row ht="13.9" r="17" spans="1:28">
       <c r="A17" s="10">
         <v>16</v>
       </c>
@@ -4709,7 +4826,7 @@
       <c r="AA17" s="7"/>
       <c r="AB17" s="7"/>
     </row>
-    <row r="18" spans="1:28" ht="13.9">
+    <row ht="13.9" r="18" spans="1:28">
       <c r="A18" s="10">
         <v>17</v>
       </c>
@@ -4751,7 +4868,7 @@
       <c r="AA18" s="7"/>
       <c r="AB18" s="7"/>
     </row>
-    <row r="19" spans="1:28" ht="13.9">
+    <row ht="13.9" r="19" spans="1:28">
       <c r="A19" s="10">
         <v>18</v>
       </c>
@@ -4793,7 +4910,7 @@
       <c r="AA19" s="7"/>
       <c r="AB19" s="7"/>
     </row>
-    <row r="20" spans="1:28" ht="13.9">
+    <row ht="13.9" r="20" spans="1:28">
       <c r="A20" s="10">
         <v>19</v>
       </c>
@@ -4835,7 +4952,7 @@
       <c r="AA20" s="7"/>
       <c r="AB20" s="7"/>
     </row>
-    <row r="21" spans="1:28" ht="13.9">
+    <row ht="13.9" r="21" spans="1:28">
       <c r="A21" s="10">
         <v>20</v>
       </c>
@@ -4877,7 +4994,7 @@
       <c r="AA21" s="7"/>
       <c r="AB21" s="7"/>
     </row>
-    <row r="22" spans="1:28" ht="13.9">
+    <row ht="13.9" r="22" spans="1:28">
       <c r="A22" s="10">
         <v>21</v>
       </c>
@@ -4919,7 +5036,7 @@
       <c r="AA22" s="7"/>
       <c r="AB22" s="7"/>
     </row>
-    <row r="23" spans="1:28" ht="13.9">
+    <row ht="13.9" r="23" spans="1:28">
       <c r="A23" s="10">
         <v>22</v>
       </c>
@@ -4963,7 +5080,7 @@
       <c r="AA23" s="7"/>
       <c r="AB23" s="7"/>
     </row>
-    <row r="24" spans="1:28" ht="13.9">
+    <row ht="13.9" r="24" spans="1:28">
       <c r="A24" s="10">
         <v>23</v>
       </c>
@@ -5005,7 +5122,7 @@
       <c r="AA24" s="7"/>
       <c r="AB24" s="7"/>
     </row>
-    <row r="25" spans="1:28" ht="13.9">
+    <row ht="13.9" r="25" spans="1:28">
       <c r="A25" s="10">
         <v>24</v>
       </c>
@@ -5047,7 +5164,7 @@
       <c r="AA25" s="7"/>
       <c r="AB25" s="7"/>
     </row>
-    <row r="26" spans="1:28" ht="13.9">
+    <row ht="13.9" r="26" spans="1:28">
       <c r="A26" s="10">
         <v>25</v>
       </c>
@@ -5091,7 +5208,7 @@
       <c r="AA26" s="7"/>
       <c r="AB26" s="7"/>
     </row>
-    <row r="27" spans="1:28" ht="13.9">
+    <row ht="13.9" r="27" spans="1:28">
       <c r="A27" s="10">
         <v>26</v>
       </c>
@@ -5135,7 +5252,7 @@
       <c r="AA27" s="7"/>
       <c r="AB27" s="7"/>
     </row>
-    <row r="28" spans="1:28" ht="13.9">
+    <row ht="13.9" r="28" spans="1:28">
       <c r="A28" s="10">
         <v>27</v>
       </c>
@@ -5177,7 +5294,7 @@
       <c r="AA28" s="7"/>
       <c r="AB28" s="7"/>
     </row>
-    <row r="29" spans="1:28" ht="13.9">
+    <row ht="13.9" r="29" spans="1:28">
       <c r="A29" s="10">
         <v>28</v>
       </c>
@@ -5221,7 +5338,7 @@
       <c r="AA29" s="7"/>
       <c r="AB29" s="7"/>
     </row>
-    <row r="30" spans="1:28" ht="13.9">
+    <row ht="13.9" r="30" spans="1:28">
       <c r="A30" s="10">
         <v>29</v>
       </c>
@@ -5263,7 +5380,7 @@
       <c r="AA30" s="7"/>
       <c r="AB30" s="7"/>
     </row>
-    <row r="31" spans="1:28" ht="13.9">
+    <row ht="13.9" r="31" spans="1:28">
       <c r="A31" s="4">
         <v>30</v>
       </c>
@@ -5307,7 +5424,7 @@
       <c r="AA31" s="7"/>
       <c r="AB31" s="7"/>
     </row>
-    <row r="32" spans="1:28" ht="13.9">
+    <row ht="13.9" r="32" spans="1:28">
       <c r="A32" s="4">
         <v>31</v>
       </c>
@@ -5349,7 +5466,7 @@
       <c r="AA32" s="7"/>
       <c r="AB32" s="7"/>
     </row>
-    <row r="33" spans="1:8" s="4" customFormat="1" ht="13.5">
+    <row customFormat="1" ht="13.5" r="33" s="4" spans="1:8">
       <c r="A33" s="4">
         <v>32</v>
       </c>
@@ -5369,7 +5486,7 @@
         <v>434</v>
       </c>
     </row>
-    <row r="34" spans="1:8" s="4" customFormat="1" ht="13.5">
+    <row customFormat="1" ht="13.5" r="34" s="4" spans="1:8">
       <c r="A34" s="4">
         <v>33</v>
       </c>
@@ -5389,7 +5506,7 @@
         <v>434</v>
       </c>
     </row>
-    <row r="35" spans="1:8" s="4" customFormat="1" ht="13.9">
+    <row customFormat="1" ht="13.9" r="35" s="4" spans="1:8">
       <c r="A35" s="4">
         <v>34</v>
       </c>
@@ -5409,7 +5526,7 @@
         <v>434</v>
       </c>
     </row>
-    <row r="36" spans="1:8" s="4" customFormat="1" ht="13.9">
+    <row customFormat="1" ht="13.9" r="36" s="4" spans="1:8">
       <c r="A36" s="4">
         <v>35</v>
       </c>
@@ -5429,7 +5546,7 @@
         <v>434</v>
       </c>
     </row>
-    <row r="37" spans="1:8" s="4" customFormat="1" ht="13.9">
+    <row customFormat="1" ht="13.9" r="37" s="4" spans="1:8">
       <c r="A37" s="4">
         <v>36</v>
       </c>
@@ -5449,7 +5566,7 @@
         <v>434</v>
       </c>
     </row>
-    <row r="38" spans="1:8" s="4" customFormat="1" ht="13.5">
+    <row customFormat="1" ht="13.5" r="38" s="4" spans="1:8">
       <c r="A38" s="4">
         <v>37</v>
       </c>
@@ -5469,7 +5586,7 @@
         <v>434</v>
       </c>
     </row>
-    <row r="39" spans="1:8" s="4" customFormat="1" ht="13.5">
+    <row customFormat="1" ht="13.5" r="39" s="4" spans="1:8">
       <c r="A39" s="4">
         <v>38</v>
       </c>
@@ -5489,7 +5606,7 @@
         <v>434</v>
       </c>
     </row>
-    <row r="40" spans="1:8" s="4" customFormat="1" ht="13.5">
+    <row customFormat="1" ht="13.5" r="40" s="4" spans="1:8">
       <c r="A40" s="4">
         <v>39</v>
       </c>
@@ -5509,7 +5626,7 @@
         <v>434</v>
       </c>
     </row>
-    <row r="41" spans="1:8" s="4" customFormat="1" ht="13.9">
+    <row customFormat="1" ht="13.9" r="41" s="4" spans="1:8">
       <c r="A41" s="4">
         <v>40</v>
       </c>
@@ -5529,7 +5646,7 @@
         <v>434</v>
       </c>
     </row>
-    <row r="42" spans="1:8" s="4" customFormat="1" ht="13.5">
+    <row customFormat="1" ht="13.5" r="42" s="4" spans="1:8">
       <c r="A42" s="4">
         <v>41</v>
       </c>
@@ -5549,7 +5666,7 @@
         <v>434</v>
       </c>
     </row>
-    <row r="43" spans="1:8" s="4" customFormat="1" ht="13.5">
+    <row customFormat="1" ht="13.5" r="43" s="4" spans="1:8">
       <c r="A43" s="4">
         <v>42</v>
       </c>
@@ -5569,7 +5686,7 @@
         <v>434</v>
       </c>
     </row>
-    <row r="44" spans="1:8" s="4" customFormat="1" ht="13.5">
+    <row customFormat="1" ht="13.5" r="44" s="4" spans="1:8">
       <c r="A44" s="4">
         <v>43</v>
       </c>
@@ -5589,7 +5706,7 @@
         <v>434</v>
       </c>
     </row>
-    <row r="45" spans="1:8" s="4" customFormat="1" ht="13.5">
+    <row customFormat="1" ht="13.5" r="45" s="4" spans="1:8">
       <c r="A45" s="4">
         <v>44</v>
       </c>
@@ -5609,7 +5726,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="46" spans="1:8" s="4" customFormat="1" ht="13.5">
+    <row customFormat="1" ht="13.5" r="46" s="4" spans="1:8">
       <c r="A46" s="4">
         <v>45</v>
       </c>
@@ -5629,7 +5746,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="47" spans="1:8" s="4" customFormat="1" ht="13.5">
+    <row customFormat="1" ht="13.5" r="47" s="4" spans="1:8">
       <c r="A47" s="4">
         <v>46</v>
       </c>
@@ -5649,7 +5766,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="48" spans="1:8" s="4" customFormat="1" ht="12.75">
+    <row customFormat="1" ht="12.75" r="48" s="4" spans="1:8">
       <c r="A48" s="4">
         <v>47</v>
       </c>
@@ -5669,7 +5786,7 @@
         <v>435</v>
       </c>
     </row>
-    <row r="49" spans="1:8" s="4" customFormat="1" ht="12.75">
+    <row customFormat="1" ht="12.75" r="49" s="4" spans="1:8">
       <c r="A49" s="4">
         <v>48</v>
       </c>
@@ -5689,7 +5806,7 @@
         <v>435</v>
       </c>
     </row>
-    <row r="50" spans="1:8" s="4" customFormat="1" ht="13.15">
+    <row customFormat="1" ht="13.15" r="50" s="4" spans="1:8">
       <c r="A50" s="4">
         <v>49</v>
       </c>
@@ -5709,7 +5826,7 @@
         <v>435</v>
       </c>
     </row>
-    <row r="51" spans="1:8" s="4" customFormat="1" ht="13.15">
+    <row customFormat="1" ht="13.15" r="51" s="4" spans="1:8">
       <c r="A51" s="4">
         <v>50</v>
       </c>
@@ -5729,7 +5846,7 @@
         <v>435</v>
       </c>
     </row>
-    <row r="52" spans="1:8" s="4" customFormat="1" ht="13.15">
+    <row customFormat="1" ht="13.15" r="52" s="4" spans="1:8">
       <c r="A52" s="4">
         <v>51</v>
       </c>
@@ -5749,7 +5866,7 @@
         <v>435</v>
       </c>
     </row>
-    <row r="53" spans="1:8" s="4" customFormat="1" ht="15.75" customHeight="1">
+    <row customFormat="1" customHeight="1" ht="15.75" r="53" s="4" spans="1:8">
       <c r="A53" s="4">
         <v>52</v>
       </c>
@@ -5769,7 +5886,7 @@
         <v>329</v>
       </c>
     </row>
-    <row r="54" spans="1:8" ht="12.75">
+    <row ht="12.75" r="54" spans="1:8">
       <c r="A54">
         <v>53</v>
       </c>
@@ -5789,7 +5906,7 @@
         <v>329</v>
       </c>
     </row>
-    <row r="55" spans="1:8" s="4" customFormat="1" ht="12.75">
+    <row customFormat="1" ht="12.75" r="55" s="4" spans="1:8">
       <c r="A55" s="4">
         <v>54</v>
       </c>
@@ -5809,7 +5926,7 @@
         <v>329</v>
       </c>
     </row>
-    <row r="56" spans="1:8" s="4" customFormat="1" ht="12.75">
+    <row customFormat="1" ht="12.75" r="56" s="4" spans="1:8">
       <c r="A56" s="4">
         <v>55</v>
       </c>
@@ -5829,7 +5946,7 @@
         <v>329</v>
       </c>
     </row>
-    <row r="57" spans="1:8" s="4" customFormat="1" ht="12.75">
+    <row customFormat="1" ht="12.75" r="57" s="4" spans="1:8">
       <c r="A57" s="4">
         <v>56</v>
       </c>
@@ -5849,7 +5966,7 @@
         <v>329</v>
       </c>
     </row>
-    <row r="58" spans="1:8" s="4" customFormat="1" ht="12.75">
+    <row customFormat="1" ht="12.75" r="58" s="4" spans="1:8">
       <c r="A58" s="4">
         <v>57</v>
       </c>
@@ -5869,7 +5986,7 @@
         <v>329</v>
       </c>
     </row>
-    <row r="59" spans="1:8" s="4" customFormat="1" ht="12.75">
+    <row customFormat="1" ht="12.75" r="59" s="4" spans="1:8">
       <c r="A59" s="4">
         <v>58</v>
       </c>
@@ -5889,7 +6006,7 @@
         <v>329</v>
       </c>
     </row>
-    <row r="60" spans="1:8" s="4" customFormat="1" ht="12.75">
+    <row customFormat="1" ht="12.75" r="60" s="4" spans="1:8">
       <c r="A60" s="4">
         <v>59</v>
       </c>
@@ -5909,7 +6026,7 @@
         <v>329</v>
       </c>
     </row>
-    <row r="61" spans="1:8" s="4" customFormat="1" ht="12.75">
+    <row customFormat="1" ht="12.75" r="61" s="4" spans="1:8">
       <c r="A61" s="4">
         <v>60</v>
       </c>
@@ -5929,7 +6046,7 @@
         <v>329</v>
       </c>
     </row>
-    <row r="62" spans="1:8" s="4" customFormat="1" ht="12.75">
+    <row customFormat="1" ht="12.75" r="62" s="4" spans="1:8">
       <c r="A62" s="4">
         <v>61</v>
       </c>
@@ -5949,7 +6066,7 @@
         <v>434</v>
       </c>
     </row>
-    <row r="63" spans="1:8" s="4" customFormat="1" ht="12.75">
+    <row customFormat="1" ht="12.75" r="63" s="4" spans="1:8">
       <c r="A63" s="4">
         <v>62</v>
       </c>
@@ -5969,7 +6086,7 @@
         <v>434</v>
       </c>
     </row>
-    <row r="64" spans="1:8" s="4" customFormat="1" ht="12.75">
+    <row customFormat="1" ht="12.75" r="64" s="4" spans="1:8">
       <c r="A64" s="4">
         <v>63</v>
       </c>
@@ -5989,7 +6106,7 @@
         <v>434</v>
       </c>
     </row>
-    <row r="65" spans="1:8" s="4" customFormat="1" ht="12.75">
+    <row customFormat="1" ht="12.75" r="65" s="4" spans="1:8">
       <c r="A65" s="4">
         <v>64</v>
       </c>
@@ -5998,7 +6115,7 @@
       </c>
       <c r="C65"/>
       <c r="D65" s="4" t="s">
-        <v>7</v>
+        <v>14</v>
       </c>
       <c r="F65" s="2" t="s">
         <v>700</v>
@@ -6010,7 +6127,7 @@
         <v>434</v>
       </c>
     </row>
-    <row r="66" spans="1:8" s="4" customFormat="1" ht="12.75">
+    <row customFormat="1" ht="12.75" r="66" s="4" spans="1:8">
       <c r="A66" s="4">
         <v>65</v>
       </c>
@@ -6030,7 +6147,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="67" spans="1:8" s="4" customFormat="1" ht="12.75">
+    <row customFormat="1" ht="12.75" r="67" s="4" spans="1:8">
       <c r="A67" s="4">
         <v>66</v>
       </c>
@@ -6050,7 +6167,7 @@
         <v>435</v>
       </c>
     </row>
-    <row r="68" spans="1:8" s="4" customFormat="1" ht="12.75">
+    <row customFormat="1" ht="12.75" r="68" s="4" spans="1:8">
       <c r="A68" s="4">
         <v>67</v>
       </c>
@@ -6073,7 +6190,7 @@
         <v>434</v>
       </c>
     </row>
-    <row r="69" spans="1:8" s="4" customFormat="1" ht="12.75">
+    <row customFormat="1" ht="12.75" r="69" s="4" spans="1:8">
       <c r="A69" s="4">
         <v>68</v>
       </c>
@@ -6096,7 +6213,7 @@
         <v>434</v>
       </c>
     </row>
-    <row r="70" spans="1:8" s="4" customFormat="1" ht="12.75">
+    <row customFormat="1" ht="12.75" r="70" s="4" spans="1:8">
       <c r="A70" s="4">
         <v>69</v>
       </c>
@@ -6119,7 +6236,7 @@
         <v>434</v>
       </c>
     </row>
-    <row r="71" spans="1:8" s="4" customFormat="1" ht="12.75">
+    <row customFormat="1" ht="12.75" r="71" s="4" spans="1:8">
       <c r="A71" s="4">
         <v>70</v>
       </c>
@@ -6142,7 +6259,7 @@
         <v>434</v>
       </c>
     </row>
-    <row r="72" spans="1:8" s="4" customFormat="1" ht="12.75">
+    <row customFormat="1" ht="12.75" r="72" s="4" spans="1:8">
       <c r="A72" s="4">
         <v>71</v>
       </c>
@@ -6165,7 +6282,7 @@
         <v>434</v>
       </c>
     </row>
-    <row r="73" spans="1:8" ht="12.75">
+    <row ht="12.75" r="73" spans="1:8">
       <c r="A73">
         <v>72</v>
       </c>
@@ -6188,7 +6305,7 @@
         <v>435</v>
       </c>
     </row>
-    <row r="74" spans="1:8" ht="12.75">
+    <row ht="12.75" r="74" spans="1:8">
       <c r="A74">
         <v>73</v>
       </c>
@@ -6211,7 +6328,7 @@
         <v>435</v>
       </c>
     </row>
-    <row r="75" spans="1:8" s="4" customFormat="1" ht="12.75">
+    <row customFormat="1" ht="12.75" r="75" s="4" spans="1:8">
       <c r="A75" s="4">
         <v>74</v>
       </c>
@@ -6234,7 +6351,7 @@
         <v>435</v>
       </c>
     </row>
-    <row r="76" spans="1:8" ht="12.75">
+    <row ht="12.75" r="76" spans="1:8">
       <c r="A76">
         <v>75</v>
       </c>
@@ -6257,7 +6374,7 @@
         <v>435</v>
       </c>
     </row>
-    <row r="77" spans="1:8" ht="12.75">
+    <row ht="12.75" r="77" spans="1:8">
       <c r="A77">
         <v>76</v>
       </c>
@@ -6280,7 +6397,7 @@
         <v>435</v>
       </c>
     </row>
-    <row r="78" spans="1:8" ht="12.75">
+    <row ht="12.75" r="78" spans="1:8">
       <c r="A78">
         <v>77</v>
       </c>
@@ -6303,7 +6420,7 @@
         <v>435</v>
       </c>
     </row>
-    <row r="79" spans="1:8" ht="12.75">
+    <row ht="12.75" r="79" spans="1:8">
       <c r="A79">
         <v>78</v>
       </c>
@@ -6326,7 +6443,7 @@
         <v>435</v>
       </c>
     </row>
-    <row r="80" spans="1:8" ht="12.75">
+    <row ht="12.75" r="80" spans="1:8">
       <c r="A80">
         <v>79</v>
       </c>
@@ -6349,7 +6466,7 @@
         <v>435</v>
       </c>
     </row>
-    <row r="81" spans="1:8" ht="12.75">
+    <row ht="12.75" r="81" spans="1:8">
       <c r="A81">
         <v>80</v>
       </c>
@@ -6372,7 +6489,7 @@
         <v>435</v>
       </c>
     </row>
-    <row r="82" spans="1:8" ht="12.75">
+    <row ht="12.75" r="82" spans="1:8">
       <c r="A82">
         <v>81</v>
       </c>
@@ -6395,7 +6512,7 @@
         <v>435</v>
       </c>
     </row>
-    <row r="83" spans="1:8" ht="12.75">
+    <row ht="12.75" r="83" spans="1:8">
       <c r="A83">
         <v>82</v>
       </c>
@@ -6418,7 +6535,7 @@
         <v>435</v>
       </c>
     </row>
-    <row r="84" spans="1:8" ht="12.75">
+    <row ht="12.75" r="84" spans="1:8">
       <c r="A84">
         <v>83</v>
       </c>
@@ -6441,7 +6558,7 @@
         <v>435</v>
       </c>
     </row>
-    <row r="85" spans="1:8" ht="12.75">
+    <row ht="12.75" r="85" spans="1:8">
       <c r="A85">
         <v>84</v>
       </c>
@@ -6464,7 +6581,7 @@
         <v>435</v>
       </c>
     </row>
-    <row r="86" spans="1:8" ht="12.75">
+    <row ht="12.75" r="86" spans="1:8">
       <c r="A86">
         <v>85</v>
       </c>
@@ -6487,7 +6604,7 @@
         <v>434</v>
       </c>
     </row>
-    <row r="87" spans="1:8" ht="12.75">
+    <row ht="12.75" r="87" spans="1:8">
       <c r="A87">
         <v>86</v>
       </c>
@@ -6510,7 +6627,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="88" spans="1:8" ht="12.75">
+    <row ht="12.75" r="88" spans="1:8">
       <c r="A88">
         <v>87</v>
       </c>
@@ -6533,7 +6650,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="89" spans="1:8" ht="12.75">
+    <row ht="12.75" r="89" spans="1:8">
       <c r="A89">
         <v>88</v>
       </c>
@@ -6544,7 +6661,7 @@
         <v>656</v>
       </c>
       <c r="D89" s="4" t="s">
-        <v>7</v>
+        <v>14</v>
       </c>
       <c r="F89" s="2" t="s">
         <v>700</v>
@@ -6556,7 +6673,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="90" spans="1:8" ht="12.75">
+    <row ht="12.75" r="90" spans="1:8">
       <c r="A90">
         <v>89</v>
       </c>
@@ -6579,7 +6696,7 @@
         <v>435</v>
       </c>
     </row>
-    <row r="91" spans="1:8" ht="12.75">
+    <row ht="12.75" r="91" spans="1:8">
       <c r="A91">
         <v>90</v>
       </c>
@@ -6602,7 +6719,7 @@
         <v>435</v>
       </c>
     </row>
-    <row r="92" spans="1:8" ht="12.75">
+    <row ht="12.75" r="92" spans="1:8">
       <c r="A92">
         <v>91</v>
       </c>
@@ -6625,7 +6742,7 @@
         <v>435</v>
       </c>
     </row>
-    <row r="93" spans="1:8" ht="12.75">
+    <row ht="12.75" r="93" spans="1:8">
       <c r="A93">
         <v>92</v>
       </c>
@@ -6648,7 +6765,7 @@
         <v>435</v>
       </c>
     </row>
-    <row r="94" spans="1:8" ht="12.75">
+    <row ht="12.75" r="94" spans="1:8">
       <c r="A94">
         <v>93</v>
       </c>
@@ -6671,7 +6788,7 @@
         <v>434</v>
       </c>
     </row>
-    <row r="95" spans="1:8" ht="12.75">
+    <row ht="12.75" r="95" spans="1:8">
       <c r="A95">
         <v>94</v>
       </c>
@@ -6694,7 +6811,7 @@
         <v>434</v>
       </c>
     </row>
-    <row r="96" spans="1:8" ht="12.75">
+    <row ht="12.75" r="96" spans="1:8">
       <c r="A96">
         <v>95</v>
       </c>
@@ -6717,7 +6834,7 @@
         <v>434</v>
       </c>
     </row>
-    <row r="97" spans="1:8" ht="12.75">
+    <row ht="12.75" r="97" spans="1:8">
       <c r="A97">
         <v>96</v>
       </c>
@@ -6740,7 +6857,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="98" spans="1:8" ht="12.75">
+    <row ht="12.75" r="98" spans="1:8">
       <c r="A98">
         <v>97</v>
       </c>
@@ -6763,138 +6880,198 @@
         <v>435</v>
       </c>
     </row>
+    <row ht="12.75" r="99" spans="1:8">
+      <c r="A99">
+        <v>98</v>
+      </c>
+      <c r="B99" t="s">
+        <v>717</v>
+      </c>
+      <c r="C99" t="s">
+        <v>734</v>
+      </c>
+      <c r="D99" s="63" t="s">
+        <v>433</v>
+      </c>
+      <c r="G99" t="s">
+        <v>8</v>
+      </c>
+      <c r="H99" t="s">
+        <v>434</v>
+      </c>
+    </row>
+    <row ht="12.75" r="100" spans="1:8">
+      <c r="A100">
+        <v>99</v>
+      </c>
+      <c r="B100" t="s">
+        <v>718</v>
+      </c>
+      <c r="C100" t="s">
+        <v>735</v>
+      </c>
+      <c r="D100" s="64" t="s">
+        <v>433</v>
+      </c>
+      <c r="G100" t="s">
+        <v>37</v>
+      </c>
+      <c r="H100" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row ht="12.75" r="101" spans="1:8">
+      <c r="A101">
+        <v>100</v>
+      </c>
+      <c r="B101" t="s">
+        <v>719</v>
+      </c>
+      <c r="C101" t="s">
+        <v>736</v>
+      </c>
+      <c r="D101" s="65" t="s">
+        <v>433</v>
+      </c>
+      <c r="G101" t="s">
+        <v>16</v>
+      </c>
+      <c r="H101" t="s">
+        <v>435</v>
+      </c>
+    </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B2" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
-    <hyperlink ref="B3" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
-    <hyperlink ref="B4" r:id="rId3" xr:uid="{00000000-0004-0000-0000-000002000000}"/>
-    <hyperlink ref="B5" r:id="rId4" xr:uid="{00000000-0004-0000-0000-000003000000}"/>
-    <hyperlink ref="B6" r:id="rId5" xr:uid="{00000000-0004-0000-0000-000004000000}"/>
-    <hyperlink ref="H6" r:id="rId6" xr:uid="{00000000-0004-0000-0000-000005000000}"/>
-    <hyperlink ref="B7" r:id="rId7" xr:uid="{00000000-0004-0000-0000-000006000000}"/>
-    <hyperlink ref="B8" r:id="rId8" xr:uid="{00000000-0004-0000-0000-000007000000}"/>
-    <hyperlink ref="B9" r:id="rId9" xr:uid="{00000000-0004-0000-0000-000008000000}"/>
-    <hyperlink ref="B10" r:id="rId10" xr:uid="{00000000-0004-0000-0000-000009000000}"/>
-    <hyperlink ref="B11" r:id="rId11" xr:uid="{00000000-0004-0000-0000-00000A000000}"/>
-    <hyperlink ref="B12" r:id="rId12" xr:uid="{00000000-0004-0000-0000-00000B000000}"/>
-    <hyperlink ref="B13" r:id="rId13" xr:uid="{00000000-0004-0000-0000-00000C000000}"/>
-    <hyperlink ref="B14" r:id="rId14" xr:uid="{00000000-0004-0000-0000-00000D000000}"/>
-    <hyperlink ref="B15" r:id="rId15" xr:uid="{00000000-0004-0000-0000-00000E000000}"/>
-    <hyperlink ref="B16" r:id="rId16" xr:uid="{00000000-0004-0000-0000-00000F000000}"/>
-    <hyperlink ref="B17" r:id="rId17" xr:uid="{00000000-0004-0000-0000-000010000000}"/>
-    <hyperlink ref="B18" r:id="rId18" xr:uid="{00000000-0004-0000-0000-000011000000}"/>
-    <hyperlink ref="B19" r:id="rId19" xr:uid="{00000000-0004-0000-0000-000012000000}"/>
-    <hyperlink ref="B20" r:id="rId20" xr:uid="{00000000-0004-0000-0000-000013000000}"/>
-    <hyperlink ref="B21" r:id="rId21" xr:uid="{00000000-0004-0000-0000-000014000000}"/>
-    <hyperlink ref="B22" r:id="rId22" xr:uid="{00000000-0004-0000-0000-000015000000}"/>
-    <hyperlink ref="B23" r:id="rId23" xr:uid="{00000000-0004-0000-0000-000016000000}"/>
-    <hyperlink ref="B24" r:id="rId24" xr:uid="{00000000-0004-0000-0000-000017000000}"/>
-    <hyperlink ref="B25" r:id="rId25" xr:uid="{00000000-0004-0000-0000-000018000000}"/>
-    <hyperlink ref="H25" r:id="rId26" xr:uid="{00000000-0004-0000-0000-000019000000}"/>
-    <hyperlink ref="B26" r:id="rId27" xr:uid="{00000000-0004-0000-0000-00001A000000}"/>
-    <hyperlink ref="H26" r:id="rId28" xr:uid="{00000000-0004-0000-0000-00001B000000}"/>
-    <hyperlink ref="B27" r:id="rId29" xr:uid="{00000000-0004-0000-0000-00001C000000}"/>
-    <hyperlink ref="H27" r:id="rId30" xr:uid="{00000000-0004-0000-0000-00001D000000}"/>
-    <hyperlink ref="B28" r:id="rId31" xr:uid="{00000000-0004-0000-0000-00001E000000}"/>
-    <hyperlink ref="H28" r:id="rId32" xr:uid="{00000000-0004-0000-0000-00001F000000}"/>
-    <hyperlink ref="B29" r:id="rId33" xr:uid="{00000000-0004-0000-0000-000020000000}"/>
-    <hyperlink ref="H29" r:id="rId34" xr:uid="{00000000-0004-0000-0000-000021000000}"/>
-    <hyperlink ref="B30" r:id="rId35" xr:uid="{00000000-0004-0000-0000-000022000000}"/>
-    <hyperlink ref="H30" r:id="rId36" xr:uid="{00000000-0004-0000-0000-000023000000}"/>
-    <hyperlink ref="B31" r:id="rId37" xr:uid="{00000000-0004-0000-0000-000024000000}"/>
-    <hyperlink ref="H31" r:id="rId38" xr:uid="{00000000-0004-0000-0000-000025000000}"/>
-    <hyperlink ref="B32" r:id="rId39" xr:uid="{00000000-0004-0000-0000-000026000000}"/>
-    <hyperlink ref="H32" r:id="rId40" xr:uid="{00000000-0004-0000-0000-000027000000}"/>
-    <hyperlink ref="B33" r:id="rId41" xr:uid="{00000000-0004-0000-0000-000028000000}"/>
-    <hyperlink ref="B34" r:id="rId42" xr:uid="{00000000-0004-0000-0000-000029000000}"/>
-    <hyperlink ref="B38" r:id="rId43" xr:uid="{00000000-0004-0000-0000-00002A000000}"/>
-    <hyperlink ref="B45" r:id="rId44" xr:uid="{00000000-0004-0000-0000-00002B000000}"/>
-    <hyperlink ref="B48" r:id="rId45" xr:uid="{00000000-0004-0000-0000-00002C000000}"/>
-    <hyperlink ref="B35" r:id="rId46" xr:uid="{00000000-0004-0000-0000-00002D000000}"/>
-    <hyperlink ref="B52" r:id="rId47" xr:uid="{00000000-0004-0000-0000-00002E000000}"/>
-    <hyperlink ref="B53" r:id="rId48" xr:uid="{00000000-0004-0000-0000-00002F000000}"/>
-    <hyperlink ref="B55" r:id="rId49" xr:uid="{00000000-0004-0000-0000-000030000000}"/>
-    <hyperlink ref="B56" r:id="rId50" xr:uid="{00000000-0004-0000-0000-000031000000}"/>
-    <hyperlink ref="B57" r:id="rId51" xr:uid="{00000000-0004-0000-0000-000032000000}"/>
-    <hyperlink ref="B58" r:id="rId52" xr:uid="{00000000-0004-0000-0000-000033000000}"/>
-    <hyperlink ref="B61" r:id="rId53" xr:uid="{00000000-0004-0000-0000-000034000000}"/>
-    <hyperlink ref="B62" r:id="rId54" xr:uid="{00000000-0004-0000-0000-000035000000}"/>
-    <hyperlink ref="B63" r:id="rId55" xr:uid="{00000000-0004-0000-0000-000036000000}"/>
-    <hyperlink ref="B64" r:id="rId56" xr:uid="{00000000-0004-0000-0000-000037000000}"/>
-    <hyperlink ref="B65" r:id="rId57" xr:uid="{00000000-0004-0000-0000-000038000000}"/>
-    <hyperlink ref="B66" r:id="rId58" xr:uid="{00000000-0004-0000-0000-000039000000}"/>
-    <hyperlink ref="B67" r:id="rId59" xr:uid="{00000000-0004-0000-0000-00003A000000}"/>
-    <hyperlink ref="H7:H24" r:id="rId60" display="https://www.allhomes.com.au/agency/trusted-realtors-570129/" xr:uid="{00000000-0004-0000-0000-00003B000000}"/>
-    <hyperlink ref="B43" r:id="rId61" xr:uid="{00000000-0004-0000-0000-00003C000000}"/>
-    <hyperlink ref="B44" r:id="rId62" xr:uid="{00000000-0004-0000-0000-00003D000000}"/>
-    <hyperlink ref="B46" r:id="rId63" xr:uid="{00000000-0004-0000-0000-00003E000000}"/>
-    <hyperlink ref="B54" r:id="rId64" xr:uid="{00000000-0004-0000-0000-00003F000000}"/>
-    <hyperlink ref="B42" r:id="rId65" xr:uid="{00000000-0004-0000-0000-000040000000}"/>
-    <hyperlink ref="J2" r:id="rId66" xr:uid="{00000000-0004-0000-0000-000041000000}"/>
-    <hyperlink ref="C69" r:id="rId67" xr:uid="{9DAE03A7-93E8-4507-BD6C-AC4013ECD47F}"/>
-    <hyperlink ref="C68" r:id="rId68" xr:uid="{66B9A9CA-DF82-46B6-9C5A-C5709E2FF1AE}"/>
-    <hyperlink ref="B75" r:id="rId69" xr:uid="{57E7BFEF-6F05-4DA9-A3DE-5B0A0EFED4D9}"/>
-    <hyperlink ref="C75" r:id="rId70" xr:uid="{F4755F93-6E59-4C38-BF66-16746869FDF3}"/>
-    <hyperlink ref="H75" r:id="rId71" xr:uid="{5BFAFD71-42C4-487F-B5E7-1697975992B4}"/>
-    <hyperlink ref="B78" r:id="rId72" xr:uid="{D3DE0D76-2479-4283-B7C7-F11B85797022}"/>
-    <hyperlink ref="C78" r:id="rId73" xr:uid="{FC1D9146-2FDC-4F13-A3C3-51CAB46DEC08}"/>
-    <hyperlink ref="B68" r:id="rId74" xr:uid="{3ED6FAA1-2B0F-4DB9-878E-9640A9C2850D}"/>
-    <hyperlink ref="B69" r:id="rId75" xr:uid="{12DE6CA8-DDC5-4E7B-BD2E-14B105A0DE3B}"/>
-    <hyperlink ref="C70" r:id="rId76" xr:uid="{0419758C-286A-4B76-B8B2-31CC336DEDF1}"/>
-    <hyperlink ref="B70" r:id="rId77" xr:uid="{AC18D1D2-FA3D-4352-A402-35B7AAFE27C0}"/>
-    <hyperlink ref="B71" r:id="rId78" xr:uid="{E8BCA1EF-4E17-4AA7-A2CE-5674FC05ABC3}"/>
-    <hyperlink ref="C71" r:id="rId79" xr:uid="{949AE606-DF4A-48F4-93A0-F148D80842CB}"/>
-    <hyperlink ref="B72" r:id="rId80" xr:uid="{69A93BB5-0295-46D6-8334-45444356E6E9}"/>
-    <hyperlink ref="C72" r:id="rId81" xr:uid="{CA171BC7-126F-4175-8A03-123D5A2C2D8A}"/>
-    <hyperlink ref="C73" r:id="rId82" xr:uid="{FACC205D-E563-4266-8E0D-0794F3D76E98}"/>
-    <hyperlink ref="B85" r:id="rId83" xr:uid="{7ABCABC0-A765-435B-AE52-9D27F653E00F}"/>
-    <hyperlink ref="C4" r:id="rId84" xr:uid="{2CD58DBE-98E3-4EDC-898F-088D5F0FCB81}"/>
-    <hyperlink ref="C29" r:id="rId85" xr:uid="{CB7CAD83-ACA3-4309-B102-B0F536FC97E6}"/>
-    <hyperlink ref="C90" r:id="rId86" xr:uid="{B4F55488-2B40-4078-ABF0-4B4254363237}"/>
-    <hyperlink ref="B90" r:id="rId87" xr:uid="{09FEE7FE-E667-40E8-BC22-3FDC999B614F}"/>
-    <hyperlink ref="C15" r:id="rId88" xr:uid="{34F25BA9-B460-46CF-85C0-4AC9D6288B41}"/>
+    <hyperlink r:id="rId1" ref="B2" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
+    <hyperlink r:id="rId2" ref="B3" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
+    <hyperlink r:id="rId3" ref="B4" xr:uid="{00000000-0004-0000-0000-000002000000}"/>
+    <hyperlink r:id="rId4" ref="B5" xr:uid="{00000000-0004-0000-0000-000003000000}"/>
+    <hyperlink r:id="rId5" ref="B6" xr:uid="{00000000-0004-0000-0000-000004000000}"/>
+    <hyperlink r:id="rId6" ref="H6" xr:uid="{00000000-0004-0000-0000-000005000000}"/>
+    <hyperlink r:id="rId7" ref="B7" xr:uid="{00000000-0004-0000-0000-000006000000}"/>
+    <hyperlink r:id="rId8" ref="B8" xr:uid="{00000000-0004-0000-0000-000007000000}"/>
+    <hyperlink r:id="rId9" ref="B9" xr:uid="{00000000-0004-0000-0000-000008000000}"/>
+    <hyperlink r:id="rId10" ref="B10" xr:uid="{00000000-0004-0000-0000-000009000000}"/>
+    <hyperlink r:id="rId11" ref="B11" xr:uid="{00000000-0004-0000-0000-00000A000000}"/>
+    <hyperlink r:id="rId12" ref="B12" xr:uid="{00000000-0004-0000-0000-00000B000000}"/>
+    <hyperlink r:id="rId13" ref="B13" xr:uid="{00000000-0004-0000-0000-00000C000000}"/>
+    <hyperlink r:id="rId14" ref="B14" xr:uid="{00000000-0004-0000-0000-00000D000000}"/>
+    <hyperlink r:id="rId15" ref="B15" xr:uid="{00000000-0004-0000-0000-00000E000000}"/>
+    <hyperlink r:id="rId16" ref="B16" xr:uid="{00000000-0004-0000-0000-00000F000000}"/>
+    <hyperlink r:id="rId17" ref="B17" xr:uid="{00000000-0004-0000-0000-000010000000}"/>
+    <hyperlink r:id="rId18" ref="B18" xr:uid="{00000000-0004-0000-0000-000011000000}"/>
+    <hyperlink r:id="rId19" ref="B19" xr:uid="{00000000-0004-0000-0000-000012000000}"/>
+    <hyperlink r:id="rId20" ref="B20" xr:uid="{00000000-0004-0000-0000-000013000000}"/>
+    <hyperlink r:id="rId21" ref="B21" xr:uid="{00000000-0004-0000-0000-000014000000}"/>
+    <hyperlink r:id="rId22" ref="B22" xr:uid="{00000000-0004-0000-0000-000015000000}"/>
+    <hyperlink r:id="rId23" ref="B23" xr:uid="{00000000-0004-0000-0000-000016000000}"/>
+    <hyperlink r:id="rId24" ref="B24" xr:uid="{00000000-0004-0000-0000-000017000000}"/>
+    <hyperlink r:id="rId25" ref="B25" xr:uid="{00000000-0004-0000-0000-000018000000}"/>
+    <hyperlink r:id="rId26" ref="H25" xr:uid="{00000000-0004-0000-0000-000019000000}"/>
+    <hyperlink r:id="rId27" ref="B26" xr:uid="{00000000-0004-0000-0000-00001A000000}"/>
+    <hyperlink r:id="rId28" ref="H26" xr:uid="{00000000-0004-0000-0000-00001B000000}"/>
+    <hyperlink r:id="rId29" ref="B27" xr:uid="{00000000-0004-0000-0000-00001C000000}"/>
+    <hyperlink r:id="rId30" ref="H27" xr:uid="{00000000-0004-0000-0000-00001D000000}"/>
+    <hyperlink r:id="rId31" ref="B28" xr:uid="{00000000-0004-0000-0000-00001E000000}"/>
+    <hyperlink r:id="rId32" ref="H28" xr:uid="{00000000-0004-0000-0000-00001F000000}"/>
+    <hyperlink r:id="rId33" ref="B29" xr:uid="{00000000-0004-0000-0000-000020000000}"/>
+    <hyperlink r:id="rId34" ref="H29" xr:uid="{00000000-0004-0000-0000-000021000000}"/>
+    <hyperlink r:id="rId35" ref="B30" xr:uid="{00000000-0004-0000-0000-000022000000}"/>
+    <hyperlink r:id="rId36" ref="H30" xr:uid="{00000000-0004-0000-0000-000023000000}"/>
+    <hyperlink r:id="rId37" ref="B31" xr:uid="{00000000-0004-0000-0000-000024000000}"/>
+    <hyperlink r:id="rId38" ref="H31" xr:uid="{00000000-0004-0000-0000-000025000000}"/>
+    <hyperlink r:id="rId39" ref="B32" xr:uid="{00000000-0004-0000-0000-000026000000}"/>
+    <hyperlink r:id="rId40" ref="H32" xr:uid="{00000000-0004-0000-0000-000027000000}"/>
+    <hyperlink r:id="rId41" ref="B33" xr:uid="{00000000-0004-0000-0000-000028000000}"/>
+    <hyperlink r:id="rId42" ref="B34" xr:uid="{00000000-0004-0000-0000-000029000000}"/>
+    <hyperlink r:id="rId43" ref="B38" xr:uid="{00000000-0004-0000-0000-00002A000000}"/>
+    <hyperlink r:id="rId44" ref="B45" xr:uid="{00000000-0004-0000-0000-00002B000000}"/>
+    <hyperlink r:id="rId45" ref="B48" xr:uid="{00000000-0004-0000-0000-00002C000000}"/>
+    <hyperlink r:id="rId46" ref="B35" xr:uid="{00000000-0004-0000-0000-00002D000000}"/>
+    <hyperlink r:id="rId47" ref="B52" xr:uid="{00000000-0004-0000-0000-00002E000000}"/>
+    <hyperlink r:id="rId48" ref="B53" xr:uid="{00000000-0004-0000-0000-00002F000000}"/>
+    <hyperlink r:id="rId49" ref="B55" xr:uid="{00000000-0004-0000-0000-000030000000}"/>
+    <hyperlink r:id="rId50" ref="B56" xr:uid="{00000000-0004-0000-0000-000031000000}"/>
+    <hyperlink r:id="rId51" ref="B57" xr:uid="{00000000-0004-0000-0000-000032000000}"/>
+    <hyperlink r:id="rId52" ref="B58" xr:uid="{00000000-0004-0000-0000-000033000000}"/>
+    <hyperlink r:id="rId53" ref="B61" xr:uid="{00000000-0004-0000-0000-000034000000}"/>
+    <hyperlink r:id="rId54" ref="B62" xr:uid="{00000000-0004-0000-0000-000035000000}"/>
+    <hyperlink r:id="rId55" ref="B63" xr:uid="{00000000-0004-0000-0000-000036000000}"/>
+    <hyperlink r:id="rId56" ref="B64" xr:uid="{00000000-0004-0000-0000-000037000000}"/>
+    <hyperlink r:id="rId57" ref="B65" xr:uid="{00000000-0004-0000-0000-000038000000}"/>
+    <hyperlink r:id="rId58" ref="B66" xr:uid="{00000000-0004-0000-0000-000039000000}"/>
+    <hyperlink r:id="rId59" ref="B67" xr:uid="{00000000-0004-0000-0000-00003A000000}"/>
+    <hyperlink display="https://www.allhomes.com.au/agency/trusted-realtors-570129/" r:id="rId60" ref="H7:H24" xr:uid="{00000000-0004-0000-0000-00003B000000}"/>
+    <hyperlink r:id="rId61" ref="B43" xr:uid="{00000000-0004-0000-0000-00003C000000}"/>
+    <hyperlink r:id="rId62" ref="B44" xr:uid="{00000000-0004-0000-0000-00003D000000}"/>
+    <hyperlink r:id="rId63" ref="B46" xr:uid="{00000000-0004-0000-0000-00003E000000}"/>
+    <hyperlink r:id="rId64" ref="B54" xr:uid="{00000000-0004-0000-0000-00003F000000}"/>
+    <hyperlink r:id="rId65" ref="B42" xr:uid="{00000000-0004-0000-0000-000040000000}"/>
+    <hyperlink r:id="rId66" ref="J2" xr:uid="{00000000-0004-0000-0000-000041000000}"/>
+    <hyperlink r:id="rId67" ref="C69" xr:uid="{9DAE03A7-93E8-4507-BD6C-AC4013ECD47F}"/>
+    <hyperlink r:id="rId68" ref="C68" xr:uid="{66B9A9CA-DF82-46B6-9C5A-C5709E2FF1AE}"/>
+    <hyperlink r:id="rId69" ref="B75" xr:uid="{57E7BFEF-6F05-4DA9-A3DE-5B0A0EFED4D9}"/>
+    <hyperlink r:id="rId70" ref="C75" xr:uid="{F4755F93-6E59-4C38-BF66-16746869FDF3}"/>
+    <hyperlink r:id="rId71" ref="H75" xr:uid="{5BFAFD71-42C4-487F-B5E7-1697975992B4}"/>
+    <hyperlink r:id="rId72" ref="B78" xr:uid="{D3DE0D76-2479-4283-B7C7-F11B85797022}"/>
+    <hyperlink r:id="rId73" ref="C78" xr:uid="{FC1D9146-2FDC-4F13-A3C3-51CAB46DEC08}"/>
+    <hyperlink r:id="rId74" ref="B68" xr:uid="{3ED6FAA1-2B0F-4DB9-878E-9640A9C2850D}"/>
+    <hyperlink r:id="rId75" ref="B69" xr:uid="{12DE6CA8-DDC5-4E7B-BD2E-14B105A0DE3B}"/>
+    <hyperlink r:id="rId76" ref="C70" xr:uid="{0419758C-286A-4B76-B8B2-31CC336DEDF1}"/>
+    <hyperlink r:id="rId77" ref="B70" xr:uid="{AC18D1D2-FA3D-4352-A402-35B7AAFE27C0}"/>
+    <hyperlink r:id="rId78" ref="B71" xr:uid="{E8BCA1EF-4E17-4AA7-A2CE-5674FC05ABC3}"/>
+    <hyperlink r:id="rId79" ref="C71" xr:uid="{949AE606-DF4A-48F4-93A0-F148D80842CB}"/>
+    <hyperlink r:id="rId80" ref="B72" xr:uid="{69A93BB5-0295-46D6-8334-45444356E6E9}"/>
+    <hyperlink r:id="rId81" ref="C72" xr:uid="{CA171BC7-126F-4175-8A03-123D5A2C2D8A}"/>
+    <hyperlink r:id="rId82" ref="C73" xr:uid="{FACC205D-E563-4266-8E0D-0794F3D76E98}"/>
+    <hyperlink r:id="rId83" ref="B85" xr:uid="{7ABCABC0-A765-435B-AE52-9D27F653E00F}"/>
+    <hyperlink r:id="rId84" ref="C4" xr:uid="{2CD58DBE-98E3-4EDC-898F-088D5F0FCB81}"/>
+    <hyperlink r:id="rId85" ref="C29" xr:uid="{CB7CAD83-ACA3-4309-B102-B0F536FC97E6}"/>
+    <hyperlink r:id="rId86" ref="C90" xr:uid="{B4F55488-2B40-4078-ABF0-4B4254363237}"/>
+    <hyperlink r:id="rId87" ref="B90" xr:uid="{09FEE7FE-E667-40E8-BC22-3FDC999B614F}"/>
+    <hyperlink r:id="rId88" ref="C15" xr:uid="{34F25BA9-B460-46CF-85C0-4AC9D6288B41}"/>
   </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId89"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageSetup orientation="portrait" paperSize="9" r:id="rId89"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:AI98"/>
+  <dimension ref="A1:AJ101"/>
   <sheetViews>
-    <sheetView topLeftCell="A76" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="C90" sqref="C90"/>
+    <sheetView tabSelected="1" topLeftCell="A76" workbookViewId="0">
+      <pane activePane="topRight" state="frozen" topLeftCell="R1" xSplit="1"/>
+      <selection activeCell="T106" pane="topRight" sqref="T106"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.46484375" defaultRowHeight="15.75" customHeight="1"/>
+  <sheetFormatPr customHeight="1" defaultColWidth="14.46484375" defaultRowHeight="15.75"/>
   <cols>
-    <col min="1" max="1" width="14.86328125" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="18.1328125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="55.53125" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="25.19921875" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="19.53125" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="19.796875" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="18.53125" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="32.19921875" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="20.53125" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="21.1328125" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="28.796875" customWidth="1" collapsed="1"/>
-    <col min="12" max="12" width="37.53125" customWidth="1" collapsed="1"/>
-    <col min="16" max="17" width="18.796875" customWidth="1" collapsed="1"/>
-    <col min="18" max="18" width="47.86328125" customWidth="1" collapsed="1"/>
-    <col min="19" max="19" width="77.53125" customWidth="1" collapsed="1"/>
-    <col min="20" max="20" width="24" customWidth="1" collapsed="1"/>
-    <col min="21" max="21" width="18.796875" customWidth="1" collapsed="1"/>
-    <col min="22" max="22" width="19.1328125" customWidth="1" collapsed="1"/>
-    <col min="23" max="31" width="19.19921875" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="14.86328125" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="18.1328125" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="55.53125" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="25.19921875" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="19.53125" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" width="19.796875" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" width="18.53125" collapsed="true"/>
+    <col min="8" max="8" customWidth="true" width="32.19921875" collapsed="true"/>
+    <col min="9" max="9" customWidth="true" width="20.53125" collapsed="true"/>
+    <col min="10" max="10" customWidth="true" width="21.1328125" collapsed="true"/>
+    <col min="11" max="11" customWidth="true" width="28.796875" collapsed="true"/>
+    <col min="12" max="12" customWidth="true" width="37.53125" collapsed="true"/>
+    <col min="16" max="17" customWidth="true" width="18.796875" collapsed="true"/>
+    <col min="18" max="18" customWidth="true" width="47.86328125" collapsed="true"/>
+    <col min="19" max="19" customWidth="true" width="77.53125" collapsed="true"/>
+    <col min="20" max="20" customWidth="true" width="24.0" collapsed="true"/>
+    <col min="21" max="21" customWidth="true" width="18.796875" collapsed="true"/>
+    <col min="22" max="22" customWidth="true" width="19.1328125" collapsed="true"/>
+    <col min="23" max="31" customWidth="true" width="19.19921875" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:35" ht="27.75">
+    <row ht="27.75" r="1" spans="1:35">
       <c r="A1" s="1" t="s">
         <v>46</v>
       </c>
@@ -6993,7 +7170,7 @@
       <c r="AH1" s="27"/>
       <c r="AI1" s="27"/>
     </row>
-    <row r="2" spans="1:35" ht="15" customHeight="1">
+    <row customHeight="1" ht="15" r="2" spans="1:35">
       <c r="A2" s="28">
         <v>1</v>
       </c>
@@ -7064,7 +7241,7 @@
       <c r="AH2" s="28"/>
       <c r="AI2" s="28"/>
     </row>
-    <row r="3" spans="1:35" ht="15" customHeight="1">
+    <row customHeight="1" ht="15" r="3" spans="1:35">
       <c r="A3" s="28">
         <v>2</v>
       </c>
@@ -7135,7 +7312,7 @@
       <c r="AH3" s="28"/>
       <c r="AI3" s="28"/>
     </row>
-    <row r="4" spans="1:35" s="28" customFormat="1" ht="15" customHeight="1">
+    <row customFormat="1" customHeight="1" ht="15" r="4" s="28" spans="1:35">
       <c r="A4" s="28">
         <v>3</v>
       </c>
@@ -7197,7 +7374,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="5" spans="1:35" ht="15" customHeight="1">
+    <row customHeight="1" ht="15" r="5" spans="1:35">
       <c r="A5" s="28">
         <v>4</v>
       </c>
@@ -7270,7 +7447,7 @@
       <c r="AH5" s="28"/>
       <c r="AI5" s="28"/>
     </row>
-    <row r="6" spans="1:35" ht="15" customHeight="1">
+    <row customHeight="1" ht="15" r="6" spans="1:35">
       <c r="A6" s="28">
         <v>5</v>
       </c>
@@ -7345,7 +7522,7 @@
       <c r="AH6" s="28"/>
       <c r="AI6" s="28"/>
     </row>
-    <row r="7" spans="1:35" s="28" customFormat="1" ht="15" customHeight="1">
+    <row customFormat="1" customHeight="1" ht="15" r="7" s="28" spans="1:35">
       <c r="A7" s="28">
         <v>6</v>
       </c>
@@ -7404,7 +7581,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="8" spans="1:35" ht="15" customHeight="1">
+    <row customHeight="1" ht="15" r="8" spans="1:35">
       <c r="A8" s="28">
         <v>7</v>
       </c>
@@ -7477,7 +7654,7 @@
       <c r="AH8" s="41"/>
       <c r="AI8" s="41"/>
     </row>
-    <row r="9" spans="1:35" s="28" customFormat="1" ht="15" customHeight="1">
+    <row customFormat="1" customHeight="1" ht="15" r="9" s="28" spans="1:35">
       <c r="A9" s="28">
         <v>8</v>
       </c>
@@ -7536,7 +7713,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="10" spans="1:35" s="28" customFormat="1" ht="15" customHeight="1">
+    <row customFormat="1" customHeight="1" ht="15" r="10" s="28" spans="1:35">
       <c r="A10" s="28">
         <v>9</v>
       </c>
@@ -7592,7 +7769,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="11" spans="1:35" s="28" customFormat="1" ht="15" customHeight="1">
+    <row customFormat="1" customHeight="1" ht="15" r="11" s="28" spans="1:35">
       <c r="A11" s="28">
         <v>10</v>
       </c>
@@ -7657,7 +7834,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="12" spans="1:35" s="28" customFormat="1" ht="15" customHeight="1">
+    <row customFormat="1" customHeight="1" ht="15" r="12" s="28" spans="1:35">
       <c r="A12" s="28">
         <v>11</v>
       </c>
@@ -7713,7 +7890,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="13" spans="1:35" s="28" customFormat="1" ht="15" customHeight="1">
+    <row customFormat="1" customHeight="1" ht="15" r="13" s="28" spans="1:35">
       <c r="A13" s="28">
         <v>12</v>
       </c>
@@ -7772,7 +7949,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="14" spans="1:35" s="28" customFormat="1" ht="15" customHeight="1">
+    <row customFormat="1" customHeight="1" ht="15" r="14" s="28" spans="1:35">
       <c r="A14" s="28">
         <v>13</v>
       </c>
@@ -7837,7 +8014,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="15" spans="1:35" s="28" customFormat="1" ht="15" customHeight="1">
+    <row customFormat="1" customHeight="1" ht="15" r="15" s="28" spans="1:35">
       <c r="A15" s="28">
         <v>14</v>
       </c>
@@ -7896,7 +8073,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="16" spans="1:35" s="28" customFormat="1" ht="15" customHeight="1">
+    <row customFormat="1" customHeight="1" ht="15" r="16" s="28" spans="1:35">
       <c r="A16" s="28">
         <v>15</v>
       </c>
@@ -7955,7 +8132,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="17" spans="1:35" s="28" customFormat="1" ht="15" customHeight="1">
+    <row customFormat="1" customHeight="1" ht="15" r="17" s="28" spans="1:35">
       <c r="A17" s="28">
         <v>16</v>
       </c>
@@ -8011,7 +8188,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="18" spans="1:35" s="28" customFormat="1" ht="15" customHeight="1">
+    <row customFormat="1" customHeight="1" ht="15" r="18" s="28" spans="1:35">
       <c r="A18" s="28">
         <v>17</v>
       </c>
@@ -8070,7 +8247,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="19" spans="1:35" ht="15" customHeight="1">
+    <row customHeight="1" ht="15" r="19" spans="1:35">
       <c r="A19" s="28">
         <v>18</v>
       </c>
@@ -8141,7 +8318,7 @@
       <c r="AH19" s="28"/>
       <c r="AI19" s="28"/>
     </row>
-    <row r="20" spans="1:35" ht="15" customHeight="1">
+    <row customHeight="1" ht="15" r="20" spans="1:35">
       <c r="A20" s="28">
         <v>19</v>
       </c>
@@ -8216,7 +8393,7 @@
       <c r="AH20" s="28"/>
       <c r="AI20" s="28"/>
     </row>
-    <row r="21" spans="1:35" ht="15" customHeight="1">
+    <row customHeight="1" ht="15" r="21" spans="1:35">
       <c r="A21" s="28">
         <v>20</v>
       </c>
@@ -8287,7 +8464,7 @@
       <c r="AH21" s="28"/>
       <c r="AI21" s="28"/>
     </row>
-    <row r="22" spans="1:35" s="28" customFormat="1" ht="15" customHeight="1">
+    <row customFormat="1" customHeight="1" ht="15" r="22" s="28" spans="1:35">
       <c r="A22" s="28">
         <v>21</v>
       </c>
@@ -8355,7 +8532,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="23" spans="1:35" s="28" customFormat="1" ht="15" customHeight="1">
+    <row customFormat="1" customHeight="1" ht="15" r="23" s="28" spans="1:35">
       <c r="A23" s="28">
         <v>22</v>
       </c>
@@ -8411,7 +8588,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="24" spans="1:35" s="28" customFormat="1" ht="15" customHeight="1">
+    <row customFormat="1" customHeight="1" ht="15" r="24" s="28" spans="1:35">
       <c r="A24" s="28">
         <v>23</v>
       </c>
@@ -8473,7 +8650,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="25" spans="1:35" ht="15" customHeight="1">
+    <row customHeight="1" ht="15" r="25" spans="1:35">
       <c r="A25" s="28">
         <v>24</v>
       </c>
@@ -8546,7 +8723,7 @@
       <c r="AH25" s="28"/>
       <c r="AI25" s="28"/>
     </row>
-    <row r="26" spans="1:35" s="28" customFormat="1" ht="15" customHeight="1">
+    <row customFormat="1" customHeight="1" ht="15" r="26" s="28" spans="1:35">
       <c r="A26" s="28">
         <v>25</v>
       </c>
@@ -8605,7 +8782,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="27" spans="1:35" s="28" customFormat="1" ht="15" customHeight="1">
+    <row customFormat="1" customHeight="1" ht="15" r="27" s="28" spans="1:35">
       <c r="A27" s="28">
         <v>26</v>
       </c>
@@ -8664,7 +8841,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="28" spans="1:35" s="28" customFormat="1" ht="15" customHeight="1">
+    <row customFormat="1" customHeight="1" ht="15" r="28" s="28" spans="1:35">
       <c r="A28" s="28">
         <v>27</v>
       </c>
@@ -8723,7 +8900,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="29" spans="1:35" s="28" customFormat="1" ht="15" customHeight="1">
+    <row customFormat="1" customHeight="1" ht="15" r="29" s="28" spans="1:35">
       <c r="A29" s="28">
         <v>28</v>
       </c>
@@ -8782,7 +8959,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="30" spans="1:35" s="28" customFormat="1" ht="15" customHeight="1">
+    <row customFormat="1" customHeight="1" ht="15" r="30" s="28" spans="1:35">
       <c r="A30" s="28">
         <v>29</v>
       </c>
@@ -8841,7 +9018,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="31" spans="1:35" s="28" customFormat="1" ht="15" customHeight="1">
+    <row customFormat="1" customHeight="1" ht="15" r="31" s="28" spans="1:35">
       <c r="A31" s="28">
         <v>30</v>
       </c>
@@ -8897,7 +9074,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="32" spans="1:35" s="28" customFormat="1" ht="15" customHeight="1">
+    <row customFormat="1" customHeight="1" ht="15" r="32" s="28" spans="1:35">
       <c r="A32" s="28">
         <v>31</v>
       </c>
@@ -8956,7 +9133,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="33" spans="1:21" s="28" customFormat="1" ht="13.5">
+    <row customFormat="1" ht="13.5" r="33" s="28" spans="1:21">
       <c r="A33" s="28" t="s">
         <v>201</v>
       </c>
@@ -9015,7 +9192,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="34" spans="1:21" s="28" customFormat="1" ht="13.5">
+    <row customFormat="1" ht="13.5" r="34" s="28" spans="1:21">
       <c r="A34" s="28" t="s">
         <v>212</v>
       </c>
@@ -9074,7 +9251,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="35" spans="1:21" s="28" customFormat="1" ht="13.5">
+    <row customFormat="1" ht="13.5" r="35" s="28" spans="1:21">
       <c r="A35" s="28" t="s">
         <v>219</v>
       </c>
@@ -9133,7 +9310,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="36" spans="1:21" s="28" customFormat="1" ht="13.5">
+    <row customFormat="1" ht="13.5" r="36" s="28" spans="1:21">
       <c r="A36" s="28" t="s">
         <v>225</v>
       </c>
@@ -9192,7 +9369,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="37" spans="1:21" s="28" customFormat="1" ht="13.5">
+    <row customFormat="1" ht="13.5" r="37" s="28" spans="1:21">
       <c r="A37" s="28" t="s">
         <v>232</v>
       </c>
@@ -9251,7 +9428,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="38" spans="1:21" s="28" customFormat="1" ht="13.5">
+    <row customFormat="1" ht="13.5" r="38" s="28" spans="1:21">
       <c r="A38" s="28" t="s">
         <v>238</v>
       </c>
@@ -9310,7 +9487,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="39" spans="1:21" s="28" customFormat="1" ht="13.5">
+    <row customFormat="1" ht="13.5" r="39" s="28" spans="1:21">
       <c r="A39" s="28" t="s">
         <v>246</v>
       </c>
@@ -9369,7 +9546,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="40" spans="1:21" s="28" customFormat="1" ht="13.5">
+    <row customFormat="1" ht="13.5" r="40" s="28" spans="1:21">
       <c r="A40" s="28" t="s">
         <v>249</v>
       </c>
@@ -9428,7 +9605,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="41" spans="1:21" s="28" customFormat="1" ht="13.5">
+    <row customFormat="1" ht="13.5" r="41" s="28" spans="1:21">
       <c r="A41" s="28" t="s">
         <v>252</v>
       </c>
@@ -9487,7 +9664,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="42" spans="1:21" s="28" customFormat="1" ht="13.5">
+    <row customFormat="1" ht="13.5" r="42" s="28" spans="1:21">
       <c r="A42" s="28" t="s">
         <v>261</v>
       </c>
@@ -9546,7 +9723,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="43" spans="1:21" s="28" customFormat="1" ht="13.5">
+    <row customFormat="1" ht="13.5" r="43" s="28" spans="1:21">
       <c r="A43" s="28" t="s">
         <v>265</v>
       </c>
@@ -9605,7 +9782,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="44" spans="1:21" s="28" customFormat="1" ht="13.5">
+    <row customFormat="1" ht="13.5" r="44" s="28" spans="1:21">
       <c r="A44" s="28" t="s">
         <v>274</v>
       </c>
@@ -9664,7 +9841,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="45" spans="1:21" s="28" customFormat="1" ht="13.5">
+    <row customFormat="1" ht="13.5" r="45" s="28" spans="1:21">
       <c r="A45" s="28" t="s">
         <v>281</v>
       </c>
@@ -9723,7 +9900,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="46" spans="1:21" s="28" customFormat="1" ht="13.5">
+    <row customFormat="1" ht="13.5" r="46" s="28" spans="1:21">
       <c r="A46" s="28" t="s">
         <v>287</v>
       </c>
@@ -9782,7 +9959,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="47" spans="1:21" s="28" customFormat="1" ht="13.5">
+    <row customFormat="1" ht="13.5" r="47" s="28" spans="1:21">
       <c r="A47" s="28" t="s">
         <v>293</v>
       </c>
@@ -9841,7 +10018,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="48" spans="1:21" s="28" customFormat="1" ht="13.5">
+    <row customFormat="1" ht="13.5" r="48" s="28" spans="1:21">
       <c r="A48" s="28" t="s">
         <v>299</v>
       </c>
@@ -9900,7 +10077,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="49" spans="1:21" s="28" customFormat="1" ht="13.5">
+    <row customFormat="1" ht="13.5" r="49" s="28" spans="1:21">
       <c r="A49" s="28" t="s">
         <v>304</v>
       </c>
@@ -9959,7 +10136,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="50" spans="1:21" s="28" customFormat="1" ht="13.5">
+    <row customFormat="1" ht="13.5" r="50" s="28" spans="1:21">
       <c r="A50" s="28" t="s">
         <v>310</v>
       </c>
@@ -10018,7 +10195,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="51" spans="1:21" s="28" customFormat="1" ht="13.5">
+    <row customFormat="1" ht="13.5" r="51" s="28" spans="1:21">
       <c r="A51" s="28" t="s">
         <v>316</v>
       </c>
@@ -10077,7 +10254,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="52" spans="1:21" s="28" customFormat="1" ht="13.5">
+    <row customFormat="1" ht="13.5" r="52" s="28" spans="1:21">
       <c r="A52" s="28" t="s">
         <v>322</v>
       </c>
@@ -10136,7 +10313,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="53" spans="1:21" s="28" customFormat="1" ht="13.5">
+    <row customFormat="1" ht="13.5" r="53" s="28" spans="1:21">
       <c r="A53" s="28" t="s">
         <v>349</v>
       </c>
@@ -10195,7 +10372,7 @@
         <v>331</v>
       </c>
     </row>
-    <row r="54" spans="1:21" ht="12.75">
+    <row ht="12.75" r="54" spans="1:21">
       <c r="A54" t="s">
         <v>355</v>
       </c>
@@ -10254,7 +10431,7 @@
         <v>331</v>
       </c>
     </row>
-    <row r="55" spans="1:21" s="28" customFormat="1" ht="13.5">
+    <row customFormat="1" ht="13.5" r="55" s="28" spans="1:21">
       <c r="A55" s="28" t="s">
         <v>359</v>
       </c>
@@ -10313,7 +10490,7 @@
         <v>331</v>
       </c>
     </row>
-    <row r="56" spans="1:21" s="28" customFormat="1" ht="13.5">
+    <row customFormat="1" ht="13.5" r="56" s="28" spans="1:21">
       <c r="A56" s="28" t="s">
         <v>365</v>
       </c>
@@ -10372,7 +10549,7 @@
         <v>331</v>
       </c>
     </row>
-    <row r="57" spans="1:21" s="28" customFormat="1" ht="13.5">
+    <row customFormat="1" ht="13.5" r="57" s="28" spans="1:21">
       <c r="A57" s="28" t="s">
         <v>370</v>
       </c>
@@ -10431,7 +10608,7 @@
         <v>331</v>
       </c>
     </row>
-    <row r="58" spans="1:21" s="28" customFormat="1" ht="13.5">
+    <row customFormat="1" ht="13.5" r="58" s="28" spans="1:21">
       <c r="A58" s="28" t="s">
         <v>377</v>
       </c>
@@ -10490,7 +10667,7 @@
         <v>331</v>
       </c>
     </row>
-    <row r="59" spans="1:21" s="28" customFormat="1" ht="13.5">
+    <row customFormat="1" ht="13.5" r="59" s="28" spans="1:21">
       <c r="A59" s="28" t="s">
         <v>383</v>
       </c>
@@ -10549,7 +10726,7 @@
         <v>331</v>
       </c>
     </row>
-    <row r="60" spans="1:21" s="28" customFormat="1" ht="13.5">
+    <row customFormat="1" ht="13.5" r="60" s="28" spans="1:21">
       <c r="A60" s="28" t="s">
         <v>390</v>
       </c>
@@ -10608,7 +10785,7 @@
         <v>331</v>
       </c>
     </row>
-    <row r="61" spans="1:21" s="28" customFormat="1" ht="13.5">
+    <row customFormat="1" ht="13.5" r="61" s="28" spans="1:21">
       <c r="A61" s="28" t="s">
         <v>397</v>
       </c>
@@ -10667,7 +10844,7 @@
         <v>331</v>
       </c>
     </row>
-    <row r="62" spans="1:21" s="28" customFormat="1" ht="13.5">
+    <row customFormat="1" ht="13.5" r="62" s="28" spans="1:21">
       <c r="A62" s="28" t="s">
         <v>403</v>
       </c>
@@ -10726,7 +10903,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="63" spans="1:21" s="28" customFormat="1" ht="13.5">
+    <row customFormat="1" ht="13.5" r="63" s="28" spans="1:21">
       <c r="A63" s="28" t="s">
         <v>406</v>
       </c>
@@ -10785,7 +10962,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="64" spans="1:21" s="28" customFormat="1" ht="13.5">
+    <row customFormat="1" ht="13.5" r="64" s="28" spans="1:21">
       <c r="A64" s="28" t="s">
         <v>411</v>
       </c>
@@ -10844,7 +11021,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="65" spans="1:21" s="28" customFormat="1" ht="13.5">
+    <row customFormat="1" ht="13.5" r="65" s="28" spans="1:21">
       <c r="A65" s="28" t="s">
         <v>417</v>
       </c>
@@ -10903,7 +11080,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="66" spans="1:21" s="28" customFormat="1" ht="13.5">
+    <row customFormat="1" ht="13.5" r="66" s="28" spans="1:21">
       <c r="A66" s="28" t="s">
         <v>422</v>
       </c>
@@ -10962,7 +11139,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="67" spans="1:21" s="28" customFormat="1" ht="13.5">
+    <row customFormat="1" ht="13.5" r="67" s="28" spans="1:21">
       <c r="A67" s="28" t="s">
         <v>428</v>
       </c>
@@ -11021,7 +11198,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="68" spans="1:21" s="28" customFormat="1" ht="13.5">
+    <row customFormat="1" ht="13.5" r="68" s="28" spans="1:21">
       <c r="A68" s="28" t="s">
         <v>490</v>
       </c>
@@ -11080,7 +11257,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="69" spans="1:21" s="28" customFormat="1" ht="13.5">
+    <row customFormat="1" ht="13.5" r="69" s="28" spans="1:21">
       <c r="A69" s="28" t="s">
         <v>495</v>
       </c>
@@ -11139,7 +11316,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="70" spans="1:21" s="28" customFormat="1" ht="13.5">
+    <row customFormat="1" ht="13.5" r="70" s="28" spans="1:21">
       <c r="A70" s="28" t="s">
         <v>497</v>
       </c>
@@ -11198,7 +11375,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="71" spans="1:21" s="28" customFormat="1" ht="13.5">
+    <row customFormat="1" ht="13.5" r="71" s="28" spans="1:21">
       <c r="A71" s="28" t="s">
         <v>503</v>
       </c>
@@ -11257,7 +11434,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="72" spans="1:21" s="28" customFormat="1" ht="13.5">
+    <row customFormat="1" ht="13.5" r="72" s="28" spans="1:21">
       <c r="A72" s="28" t="s">
         <v>508</v>
       </c>
@@ -11316,7 +11493,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="73" spans="1:21" s="28" customFormat="1" ht="13.5">
+    <row customFormat="1" ht="13.5" r="73" s="28" spans="1:21">
       <c r="A73" s="28" t="s">
         <v>510</v>
       </c>
@@ -11375,7 +11552,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="74" spans="1:21" s="28" customFormat="1" ht="13.5">
+    <row customFormat="1" ht="13.5" r="74" s="28" spans="1:21">
       <c r="A74" s="28" t="s">
         <v>514</v>
       </c>
@@ -11434,7 +11611,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="75" spans="1:21" s="28" customFormat="1" ht="13.5">
+    <row customFormat="1" ht="13.5" r="75" s="28" spans="1:21">
       <c r="A75" s="28" t="s">
         <v>520</v>
       </c>
@@ -11493,7 +11670,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="76" spans="1:21" s="28" customFormat="1" ht="13.5">
+    <row customFormat="1" ht="13.5" r="76" s="28" spans="1:21">
       <c r="A76" s="28" t="s">
         <v>526</v>
       </c>
@@ -11552,7 +11729,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="77" spans="1:21" s="28" customFormat="1" ht="13.5">
+    <row customFormat="1" ht="13.5" r="77" s="28" spans="1:21">
       <c r="A77" s="28" t="s">
         <v>531</v>
       </c>
@@ -11611,7 +11788,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="78" spans="1:21" s="28" customFormat="1" ht="13.5">
+    <row customFormat="1" ht="13.5" r="78" s="28" spans="1:21">
       <c r="A78" s="28" t="s">
         <v>538</v>
       </c>
@@ -11670,7 +11847,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="79" spans="1:21" s="28" customFormat="1" ht="13.5">
+    <row customFormat="1" ht="13.5" r="79" s="28" spans="1:21">
       <c r="A79" s="28" t="s">
         <v>541</v>
       </c>
@@ -11729,7 +11906,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="80" spans="1:21" s="28" customFormat="1" ht="13.5">
+    <row customFormat="1" ht="13.5" r="80" s="28" spans="1:21">
       <c r="A80" s="28" t="s">
         <v>547</v>
       </c>
@@ -11788,7 +11965,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="81" spans="1:21" s="28" customFormat="1" ht="13.5">
+    <row customFormat="1" ht="13.5" r="81" s="28" spans="1:21">
       <c r="A81" s="28" t="s">
         <v>554</v>
       </c>
@@ -11847,7 +12024,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="82" spans="1:21" s="28" customFormat="1" ht="13.5">
+    <row customFormat="1" ht="13.5" r="82" s="28" spans="1:21">
       <c r="A82" s="28" t="s">
         <v>559</v>
       </c>
@@ -11906,7 +12083,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="83" spans="1:21" s="28" customFormat="1" ht="13.5">
+    <row customFormat="1" ht="13.5" r="83" s="28" spans="1:21">
       <c r="A83" s="28" t="s">
         <v>564</v>
       </c>
@@ -11965,7 +12142,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="84" spans="1:21" s="28" customFormat="1" ht="13.5">
+    <row customFormat="1" ht="13.5" r="84" s="28" spans="1:21">
       <c r="A84" s="28" t="s">
         <v>567</v>
       </c>
@@ -12024,7 +12201,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="85" spans="1:21" s="28" customFormat="1" ht="13.5">
+    <row customFormat="1" ht="13.5" r="85" s="28" spans="1:21">
       <c r="A85" s="28" t="s">
         <v>571</v>
       </c>
@@ -12083,7 +12260,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="86" spans="1:21" s="28" customFormat="1" ht="13.5">
+    <row customFormat="1" ht="13.5" r="86" s="28" spans="1:21">
       <c r="A86" s="28" t="s">
         <v>612</v>
       </c>
@@ -12142,7 +12319,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="87" spans="1:21" s="28" customFormat="1" ht="13.5">
+    <row customFormat="1" ht="13.5" r="87" s="28" spans="1:21">
       <c r="A87" s="28" t="s">
         <v>616</v>
       </c>
@@ -12201,7 +12378,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="88" spans="1:21" s="28" customFormat="1" ht="13.5">
+    <row customFormat="1" ht="13.5" r="88" s="28" spans="1:21">
       <c r="A88" s="28" t="s">
         <v>621</v>
       </c>
@@ -12260,7 +12437,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="89" spans="1:21" s="28" customFormat="1" ht="13.5">
+    <row customFormat="1" ht="13.5" r="89" s="28" spans="1:21">
       <c r="A89" s="28" t="s">
         <v>625</v>
       </c>
@@ -12319,7 +12496,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="90" spans="1:21" s="28" customFormat="1" ht="13.5">
+    <row customFormat="1" ht="13.5" r="90" s="28" spans="1:21">
       <c r="A90" s="28" t="s">
         <v>631</v>
       </c>
@@ -12378,7 +12555,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="91" spans="1:21" s="28" customFormat="1" ht="13.5">
+    <row customFormat="1" ht="13.5" r="91" s="28" spans="1:21">
       <c r="A91" s="28" t="s">
         <v>635</v>
       </c>
@@ -12437,7 +12614,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="92" spans="1:21" s="28" customFormat="1" ht="13.5">
+    <row customFormat="1" ht="13.5" r="92" s="28" spans="1:21">
       <c r="A92" s="28" t="s">
         <v>639</v>
       </c>
@@ -12496,7 +12673,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="93" spans="1:21" s="28" customFormat="1" ht="13.5">
+    <row customFormat="1" ht="13.5" r="93" s="28" spans="1:21">
       <c r="A93" s="28" t="s">
         <v>642</v>
       </c>
@@ -12555,7 +12732,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="94" spans="1:21" s="28" customFormat="1" ht="13.5">
+    <row customFormat="1" ht="13.5" r="94" s="28" spans="1:21">
       <c r="A94" s="28" t="s">
         <v>676</v>
       </c>
@@ -12614,7 +12791,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="95" spans="1:21" s="28" customFormat="1" ht="13.5">
+    <row customFormat="1" ht="13.5" r="95" s="28" spans="1:21">
       <c r="A95" s="28" t="s">
         <v>681</v>
       </c>
@@ -12673,7 +12850,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="96" spans="1:21" s="28" customFormat="1" ht="13.5">
+    <row customFormat="1" ht="13.5" r="96" s="28" spans="1:21">
       <c r="A96" s="28" t="s">
         <v>685</v>
       </c>
@@ -12732,7 +12909,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="97" spans="1:21" s="28" customFormat="1" ht="13.5">
+    <row customFormat="1" ht="13.5" r="97" s="28" spans="1:21">
       <c r="A97" s="28" t="s">
         <v>689</v>
       </c>
@@ -12791,7 +12968,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="98" spans="1:21" s="28" customFormat="1" ht="13.5">
+    <row customFormat="1" ht="13.5" r="98" s="28" spans="1:21">
       <c r="A98" s="28" t="s">
         <v>703</v>
       </c>
@@ -12850,15 +13027,188 @@
         <v>16</v>
       </c>
     </row>
+    <row ht="13.5" r="99" spans="1:21">
+      <c r="A99" t="s">
+        <v>720</v>
+      </c>
+      <c r="B99" t="s">
+        <v>433</v>
+      </c>
+      <c r="C99" t="s">
+        <v>721</v>
+      </c>
+      <c r="D99" t="s">
+        <v>77</v>
+      </c>
+      <c r="E99" t="s">
+        <v>78</v>
+      </c>
+      <c r="F99" t="s">
+        <v>79</v>
+      </c>
+      <c r="G99" t="s">
+        <v>144</v>
+      </c>
+      <c r="H99" t="s">
+        <v>722</v>
+      </c>
+      <c r="I99" t="s">
+        <v>204</v>
+      </c>
+      <c r="K99" t="s">
+        <v>205</v>
+      </c>
+      <c r="L99" t="s">
+        <v>243</v>
+      </c>
+      <c r="M99" t="s">
+        <v>210</v>
+      </c>
+      <c r="N99" t="s">
+        <v>210</v>
+      </c>
+      <c r="P99" t="s">
+        <v>209</v>
+      </c>
+      <c r="Q99" t="s">
+        <v>205</v>
+      </c>
+      <c r="R99" t="s">
+        <v>721</v>
+      </c>
+      <c r="S99" t="s">
+        <v>723</v>
+      </c>
+      <c r="T99" s="28" t="s">
+        <v>82</v>
+      </c>
+      <c r="U99" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row ht="13.5" r="100" spans="1:21">
+      <c r="A100" t="s">
+        <v>724</v>
+      </c>
+      <c r="B100" t="s">
+        <v>433</v>
+      </c>
+      <c r="C100" t="s">
+        <v>725</v>
+      </c>
+      <c r="D100" t="s">
+        <v>77</v>
+      </c>
+      <c r="E100" t="s">
+        <v>78</v>
+      </c>
+      <c r="F100" t="s">
+        <v>79</v>
+      </c>
+      <c r="G100" t="s">
+        <v>79</v>
+      </c>
+      <c r="H100" t="s">
+        <v>726</v>
+      </c>
+      <c r="I100" t="s">
+        <v>204</v>
+      </c>
+      <c r="K100" t="s">
+        <v>205</v>
+      </c>
+      <c r="L100" t="s">
+        <v>243</v>
+      </c>
+      <c r="M100" t="s">
+        <v>210</v>
+      </c>
+      <c r="N100" t="s">
+        <v>272</v>
+      </c>
+      <c r="P100" t="s">
+        <v>209</v>
+      </c>
+      <c r="Q100" t="s">
+        <v>272</v>
+      </c>
+      <c r="R100" t="s">
+        <v>725</v>
+      </c>
+      <c r="S100" t="s">
+        <v>727</v>
+      </c>
+      <c r="T100" s="28" t="s">
+        <v>82</v>
+      </c>
+      <c r="U100" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row ht="13.5" r="101" spans="1:21">
+      <c r="A101" t="s">
+        <v>728</v>
+      </c>
+      <c r="B101" t="s">
+        <v>433</v>
+      </c>
+      <c r="C101" t="s">
+        <v>729</v>
+      </c>
+      <c r="D101" t="s">
+        <v>77</v>
+      </c>
+      <c r="E101" t="s">
+        <v>78</v>
+      </c>
+      <c r="F101" t="s">
+        <v>276</v>
+      </c>
+      <c r="G101" t="s">
+        <v>111</v>
+      </c>
+      <c r="H101" t="s">
+        <v>730</v>
+      </c>
+      <c r="I101" t="s">
+        <v>204</v>
+      </c>
+      <c r="K101" t="s">
+        <v>731</v>
+      </c>
+      <c r="L101" t="s">
+        <v>732</v>
+      </c>
+      <c r="M101" t="s">
+        <v>272</v>
+      </c>
+      <c r="N101" t="s">
+        <v>272</v>
+      </c>
+      <c r="P101" t="s">
+        <v>205</v>
+      </c>
+      <c r="Q101" t="s">
+        <v>205</v>
+      </c>
+      <c r="R101" t="s">
+        <v>729</v>
+      </c>
+      <c r="S101" t="s">
+        <v>733</v>
+      </c>
+      <c r="T101" s="28" t="s">
+        <v>104</v>
+      </c>
+      <c r="U101" t="s">
+        <v>16</v>
+      </c>
+    </row>
   </sheetData>
   <customSheetViews>
-    <customSheetView guid="{C25CEB9E-BEC1-4982-90C4-50C84EE1B82A}" filter="1" showAutoFilter="1">
-      <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-      <autoFilter ref="A1:AD33" xr:uid="{B0ED3D05-3B5B-4FB4-9A60-B4383DAB1391}"/>
-    </customSheetView>
-    <customSheetView guid="{A7754112-A52F-4ABC-8778-92F04773E53C}" filter="1" showAutoFilter="1">
-      <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-      <autoFilter ref="A1:AD33" xr:uid="{A8EDCA26-C172-46B6-964C-3378F9082C9B}">
+    <customSheetView filter="1" guid="{A7754112-A52F-4ABC-8778-92F04773E53C}" showAutoFilter="1">
+      <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+      <autoFilter ref="A1:AD33" xr:uid="{8814925C-CAF0-49FB-90A3-CF047BD5F7AB}">
         <filterColumn colId="5">
           <filters blank="1">
             <filter val="Strathnairn"/>
@@ -12866,78 +13216,82 @@
         </filterColumn>
       </autoFilter>
     </customSheetView>
+    <customSheetView filter="1" guid="{C25CEB9E-BEC1-4982-90C4-50C84EE1B82A}" showAutoFilter="1">
+      <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+      <autoFilter ref="A1:AD33" xr:uid="{C85633C5-E7A2-4BE6-9827-6CBA723B2F4B}"/>
+    </customSheetView>
   </customSheetViews>
   <conditionalFormatting sqref="A1:AI1">
-    <cfRule type="notContainsBlanks" dxfId="1" priority="1">
+    <cfRule dxfId="1" priority="1" type="notContainsBlanks">
       <formula>LEN(TRIM(A1))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <hyperlinks>
-    <hyperlink ref="S2" r:id="rId1" xr:uid="{00000000-0004-0000-0100-000000000000}"/>
-    <hyperlink ref="S3" r:id="rId2" xr:uid="{00000000-0004-0000-0100-000001000000}"/>
-    <hyperlink ref="S4" r:id="rId3" xr:uid="{00000000-0004-0000-0100-000002000000}"/>
-    <hyperlink ref="S5" r:id="rId4" xr:uid="{00000000-0004-0000-0100-000003000000}"/>
-    <hyperlink ref="S6" r:id="rId5" xr:uid="{00000000-0004-0000-0100-000004000000}"/>
-    <hyperlink ref="S7" r:id="rId6" xr:uid="{00000000-0004-0000-0100-000006000000}"/>
-    <hyperlink ref="S8" r:id="rId7" xr:uid="{00000000-0004-0000-0100-000008000000}"/>
-    <hyperlink ref="S9" r:id="rId8" xr:uid="{00000000-0004-0000-0100-00000A000000}"/>
-    <hyperlink ref="S10" r:id="rId9" xr:uid="{00000000-0004-0000-0100-00000C000000}"/>
-    <hyperlink ref="S11" r:id="rId10" xr:uid="{00000000-0004-0000-0100-00000E000000}"/>
-    <hyperlink ref="S12" r:id="rId11" xr:uid="{00000000-0004-0000-0100-000010000000}"/>
-    <hyperlink ref="S14" r:id="rId12" xr:uid="{00000000-0004-0000-0100-000014000000}"/>
-    <hyperlink ref="S15" r:id="rId13" xr:uid="{00000000-0004-0000-0100-000016000000}"/>
-    <hyperlink ref="S16" r:id="rId14" xr:uid="{00000000-0004-0000-0100-000018000000}"/>
-    <hyperlink ref="S17" r:id="rId15" xr:uid="{00000000-0004-0000-0100-00001A000000}"/>
-    <hyperlink ref="S18" r:id="rId16" xr:uid="{00000000-0004-0000-0100-00001C000000}"/>
-    <hyperlink ref="S19" r:id="rId17" xr:uid="{00000000-0004-0000-0100-00001E000000}"/>
-    <hyperlink ref="S20" r:id="rId18" xr:uid="{00000000-0004-0000-0100-000020000000}"/>
-    <hyperlink ref="S21" r:id="rId19" xr:uid="{00000000-0004-0000-0100-000022000000}"/>
-    <hyperlink ref="S22" r:id="rId20" xr:uid="{00000000-0004-0000-0100-000024000000}"/>
-    <hyperlink ref="S23" r:id="rId21" xr:uid="{00000000-0004-0000-0100-000026000000}"/>
-    <hyperlink ref="S24" r:id="rId22" xr:uid="{00000000-0004-0000-0100-000028000000}"/>
-    <hyperlink ref="S25" r:id="rId23" xr:uid="{00000000-0004-0000-0100-00002A000000}"/>
-    <hyperlink ref="S26" r:id="rId24" xr:uid="{00000000-0004-0000-0100-00002B000000}"/>
-    <hyperlink ref="S27" r:id="rId25" xr:uid="{00000000-0004-0000-0100-00002C000000}"/>
-    <hyperlink ref="S28" r:id="rId26" xr:uid="{00000000-0004-0000-0100-00002D000000}"/>
-    <hyperlink ref="S29" r:id="rId27" xr:uid="{00000000-0004-0000-0100-00002E000000}"/>
-    <hyperlink ref="S30" r:id="rId28" xr:uid="{00000000-0004-0000-0100-00002F000000}"/>
-    <hyperlink ref="S31" r:id="rId29" xr:uid="{00000000-0004-0000-0100-000030000000}"/>
-    <hyperlink ref="S32" r:id="rId30" xr:uid="{00000000-0004-0000-0100-000031000000}"/>
+    <hyperlink r:id="rId1" ref="S2" xr:uid="{00000000-0004-0000-0100-000000000000}"/>
+    <hyperlink r:id="rId2" ref="S3" xr:uid="{00000000-0004-0000-0100-000001000000}"/>
+    <hyperlink r:id="rId3" ref="S4" xr:uid="{00000000-0004-0000-0100-000002000000}"/>
+    <hyperlink r:id="rId4" ref="S5" xr:uid="{00000000-0004-0000-0100-000003000000}"/>
+    <hyperlink r:id="rId5" ref="S6" xr:uid="{00000000-0004-0000-0100-000004000000}"/>
+    <hyperlink r:id="rId6" ref="S7" xr:uid="{00000000-0004-0000-0100-000006000000}"/>
+    <hyperlink r:id="rId7" ref="S8" xr:uid="{00000000-0004-0000-0100-000008000000}"/>
+    <hyperlink r:id="rId8" ref="S9" xr:uid="{00000000-0004-0000-0100-00000A000000}"/>
+    <hyperlink r:id="rId9" ref="S10" xr:uid="{00000000-0004-0000-0100-00000C000000}"/>
+    <hyperlink r:id="rId10" ref="S11" xr:uid="{00000000-0004-0000-0100-00000E000000}"/>
+    <hyperlink r:id="rId11" ref="S12" xr:uid="{00000000-0004-0000-0100-000010000000}"/>
+    <hyperlink r:id="rId12" ref="S14" xr:uid="{00000000-0004-0000-0100-000014000000}"/>
+    <hyperlink r:id="rId13" ref="S15" xr:uid="{00000000-0004-0000-0100-000016000000}"/>
+    <hyperlink r:id="rId14" ref="S16" xr:uid="{00000000-0004-0000-0100-000018000000}"/>
+    <hyperlink r:id="rId15" ref="S17" xr:uid="{00000000-0004-0000-0100-00001A000000}"/>
+    <hyperlink r:id="rId16" ref="S18" xr:uid="{00000000-0004-0000-0100-00001C000000}"/>
+    <hyperlink r:id="rId17" ref="S19" xr:uid="{00000000-0004-0000-0100-00001E000000}"/>
+    <hyperlink r:id="rId18" ref="S20" xr:uid="{00000000-0004-0000-0100-000020000000}"/>
+    <hyperlink r:id="rId19" ref="S21" xr:uid="{00000000-0004-0000-0100-000022000000}"/>
+    <hyperlink r:id="rId20" ref="S22" xr:uid="{00000000-0004-0000-0100-000024000000}"/>
+    <hyperlink r:id="rId21" ref="S23" xr:uid="{00000000-0004-0000-0100-000026000000}"/>
+    <hyperlink r:id="rId22" ref="S24" xr:uid="{00000000-0004-0000-0100-000028000000}"/>
+    <hyperlink r:id="rId23" ref="S25" xr:uid="{00000000-0004-0000-0100-00002A000000}"/>
+    <hyperlink r:id="rId24" ref="S26" xr:uid="{00000000-0004-0000-0100-00002B000000}"/>
+    <hyperlink r:id="rId25" ref="S27" xr:uid="{00000000-0004-0000-0100-00002C000000}"/>
+    <hyperlink r:id="rId26" ref="S28" xr:uid="{00000000-0004-0000-0100-00002D000000}"/>
+    <hyperlink r:id="rId27" ref="S29" xr:uid="{00000000-0004-0000-0100-00002E000000}"/>
+    <hyperlink r:id="rId28" ref="S30" xr:uid="{00000000-0004-0000-0100-00002F000000}"/>
+    <hyperlink r:id="rId29" ref="S31" xr:uid="{00000000-0004-0000-0100-000030000000}"/>
+    <hyperlink r:id="rId30" ref="S32" xr:uid="{00000000-0004-0000-0100-000031000000}"/>
   </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId31"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageSetup orientation="portrait" paperSize="9" r:id="rId31"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:AI1"/>
+  <dimension ref="A1:AJ1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.46484375" defaultRowHeight="15.75" customHeight="1"/>
+  <sheetFormatPr customHeight="1" defaultColWidth="14.46484375" defaultRowHeight="15.75"/>
   <cols>
-    <col min="1" max="1" width="16" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="14.53125" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="16.796875" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="14.53125" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="13.19921875" customWidth="1" collapsed="1"/>
-    <col min="15" max="15" width="20.86328125" customWidth="1" collapsed="1"/>
-    <col min="21" max="21" width="19.1328125" customWidth="1" collapsed="1"/>
-    <col min="22" max="22" width="19.19921875" customWidth="1" collapsed="1"/>
-    <col min="23" max="23" width="20.1328125" customWidth="1" collapsed="1"/>
-    <col min="24" max="24" width="19.796875" customWidth="1" collapsed="1"/>
-    <col min="26" max="26" width="15.86328125" customWidth="1" collapsed="1"/>
-    <col min="27" max="27" width="13.46484375" customWidth="1" collapsed="1"/>
-    <col min="28" max="28" width="15.19921875" customWidth="1" collapsed="1"/>
-    <col min="29" max="29" width="16.1328125" customWidth="1" collapsed="1"/>
-    <col min="30" max="30" width="15.86328125" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="16.0" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="14.53125" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="16.796875" collapsed="true"/>
+    <col min="8" max="8" customWidth="true" width="14.53125" collapsed="true"/>
+    <col min="9" max="9" customWidth="true" width="13.19921875" collapsed="true"/>
+    <col min="15" max="15" customWidth="true" width="20.86328125" collapsed="true"/>
+    <col min="21" max="21" customWidth="true" width="19.1328125" collapsed="true"/>
+    <col min="22" max="22" customWidth="true" width="19.19921875" collapsed="true"/>
+    <col min="23" max="23" customWidth="true" width="20.1328125" collapsed="true"/>
+    <col min="24" max="24" customWidth="true" width="19.796875" collapsed="true"/>
+    <col min="26" max="26" customWidth="true" width="15.86328125" collapsed="true"/>
+    <col min="27" max="27" customWidth="true" width="13.46484375" collapsed="true"/>
+    <col min="28" max="28" customWidth="true" width="15.19921875" collapsed="true"/>
+    <col min="29" max="29" customWidth="true" width="16.1328125" collapsed="true"/>
+    <col min="30" max="30" customWidth="true" width="15.86328125" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:35" ht="15.75" customHeight="1">
+    <row customHeight="1" ht="15.75" r="1" spans="1:35">
       <c r="A1" s="1" t="s">
         <v>46</v>
       </c>
@@ -13036,37 +13390,37 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A1:AI1">
-    <cfRule type="notContainsBlanks" dxfId="0" priority="1">
+    <cfRule dxfId="0" priority="1" type="notContainsBlanks">
       <formula>LEN(TRIM(A1))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageSetup orientation="portrait" paperSize="9" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:Z6"/>
+  <dimension ref="A1:AA6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C6" sqref="C6"/>
+      <pane activePane="bottomLeft" state="frozen" topLeftCell="A2" ySplit="1"/>
+      <selection activeCell="C6" pane="bottomLeft" sqref="C6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.46484375" defaultRowHeight="15.75" customHeight="1"/>
+  <sheetFormatPr customHeight="1" defaultColWidth="14.46484375" defaultRowHeight="15.75"/>
   <cols>
-    <col min="1" max="1" width="44.86328125" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="17.1328125" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="26.46484375" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="36.1328125" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="51.1328125" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="44.86328125" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="17.1328125" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="26.46484375" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="36.1328125" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="51.1328125" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:26" ht="13.9">
+    <row ht="13.9" r="1" spans="1:26">
       <c r="A1" s="42" t="s">
         <v>158</v>
       </c>
@@ -13089,7 +13443,7 @@
         <v>163</v>
       </c>
     </row>
-    <row r="2" spans="1:26" ht="15.75" customHeight="1">
+    <row customHeight="1" ht="15.75" r="2" spans="1:26">
       <c r="A2" s="43" t="s">
         <v>164</v>
       </c>
@@ -13131,7 +13485,7 @@
       <c r="Y2" s="25"/>
       <c r="Z2" s="25"/>
     </row>
-    <row r="3" spans="1:26" ht="15.75" customHeight="1">
+    <row customHeight="1" ht="15.75" r="3" spans="1:26">
       <c r="A3" s="48" t="s">
         <v>167</v>
       </c>
@@ -13148,7 +13502,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="4" spans="1:26" ht="15.75" customHeight="1">
+    <row customHeight="1" ht="15.75" r="4" spans="1:26">
       <c r="A4" s="48" t="s">
         <v>170</v>
       </c>
@@ -13165,7 +13519,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="5" spans="1:26" ht="15.75" customHeight="1">
+    <row customHeight="1" ht="15.75" r="5" spans="1:26">
       <c r="A5" s="52" t="s">
         <v>173</v>
       </c>
@@ -13182,7 +13536,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="6" spans="1:26" ht="15.75" customHeight="1">
+    <row customHeight="1" ht="15.75" r="6" spans="1:26">
       <c r="A6" t="s">
         <v>334</v>
       </c>
@@ -13201,14 +13555,14 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="E2" r:id="rId1" xr:uid="{00000000-0004-0000-0300-000000000000}"/>
-    <hyperlink ref="E3" r:id="rId2" xr:uid="{00000000-0004-0000-0300-000001000000}"/>
-    <hyperlink ref="E4" r:id="rId3" xr:uid="{00000000-0004-0000-0300-000002000000}"/>
-    <hyperlink ref="E5" r:id="rId4" xr:uid="{00000000-0004-0000-0300-000003000000}"/>
-    <hyperlink ref="D6" r:id="rId5" xr:uid="{00000000-0004-0000-0300-000004000000}"/>
-    <hyperlink ref="E6" r:id="rId6" xr:uid="{00000000-0004-0000-0300-000005000000}"/>
+    <hyperlink r:id="rId1" ref="E2" xr:uid="{00000000-0004-0000-0300-000000000000}"/>
+    <hyperlink r:id="rId2" ref="E3" xr:uid="{00000000-0004-0000-0300-000001000000}"/>
+    <hyperlink r:id="rId3" ref="E4" xr:uid="{00000000-0004-0000-0300-000002000000}"/>
+    <hyperlink r:id="rId4" ref="E5" xr:uid="{00000000-0004-0000-0300-000003000000}"/>
+    <hyperlink r:id="rId5" ref="D6" xr:uid="{00000000-0004-0000-0300-000004000000}"/>
+    <hyperlink r:id="rId6" ref="E6" xr:uid="{00000000-0004-0000-0300-000005000000}"/>
   </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId7"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageSetup orientation="portrait" paperSize="9" r:id="rId7"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Listing(101 & 102) published
</commit_message>
<xml_diff>
--- a/src/main/resources/InputTestdata/Listing details.xlsx
+++ b/src/main/resources/InputTestdata/Listing details.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Athavan\git\777Homes-2\777Homes-business\src\main\resources\InputTestdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{453522B0-1FF7-4160-B30D-C8FF949DC82F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E41B9558-25DA-42DC-A045-5618969E7ABE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="20715" windowHeight="13276" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="20715" windowHeight="13276" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Backlog" sheetId="1" r:id="rId1"/>
@@ -26,8 +26,8 @@
   </definedNames>
   <calcPr calcId="181029"/>
   <customWorkbookViews>
+    <customWorkbookView name="Filter 1" guid="{A7754112-A52F-4ABC-8778-92F04773E53C}" maximized="1" windowWidth="0" windowHeight="0" activeSheetId="0"/>
     <customWorkbookView name="Filter 2" guid="{C25CEB9E-BEC1-4982-90C4-50C84EE1B82A}" maximized="1" windowWidth="0" windowHeight="0" activeSheetId="0"/>
-    <customWorkbookView name="Filter 1" guid="{A7754112-A52F-4ABC-8778-92F04773E53C}" maximized="1" windowWidth="0" windowHeight="0" activeSheetId="0"/>
   </customWorkbookViews>
 </workbook>
 </file>
@@ -3743,7 +3743,7 @@
       <name val="Arial"/>
     </font>
   </fonts>
-  <fills count="12">
+  <fills count="10">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -3798,16 +3798,6 @@
         <bgColor rgb="FFD9EAD3"/>
       </patternFill>
     </fill>
-    <fill>
-      <patternFill patternType="mediumGray">
-        <bgColor indexed="2"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="mediumGray">
-        <bgColor indexed="2"/>
-      </patternFill>
-    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -3822,7 +3812,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="29" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="64">
+  <cellXfs count="62">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -3963,8 +3953,6 @@
     <xf numFmtId="0" fontId="18" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -4203,9 +4191,9 @@
   </sheetPr>
   <dimension ref="A1:AB103"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A38" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D56" sqref="D56"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A74" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D101" sqref="D101:D103"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.46484375" defaultRowHeight="15.75" customHeight="1"/>
@@ -7134,8 +7122,8 @@
       <c r="C102" t="s">
         <v>766</v>
       </c>
-      <c r="D102" s="62" t="s">
-        <v>432</v>
+      <c r="D102" s="4" t="s">
+        <v>7</v>
       </c>
       <c r="F102" s="2" t="s">
         <v>698</v>
@@ -7157,8 +7145,8 @@
       <c r="C103" t="s">
         <v>767</v>
       </c>
-      <c r="D103" s="63" t="s">
-        <v>432</v>
+      <c r="D103" s="4" t="s">
+        <v>7</v>
       </c>
       <c r="F103" s="2" t="s">
         <v>699</v>
@@ -7294,9 +7282,9 @@
   </sheetPr>
   <dimension ref="A1:AI103"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A73" workbookViewId="0">
+    <sheetView topLeftCell="A79" workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="D105" sqref="D105"/>
+      <selection pane="topRight" activeCell="D108" sqref="D108"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.46484375" defaultRowHeight="15.75" customHeight="1"/>
@@ -13437,139 +13425,139 @@
         <v>16</v>
       </c>
     </row>
-    <row r="102" spans="1:21" ht="13.5">
-      <c r="A102" t="s">
+    <row r="102" spans="1:21" s="28" customFormat="1" ht="13.5">
+      <c r="A102" s="28" t="s">
         <v>756</v>
       </c>
-      <c r="B102" s="62" t="s">
+      <c r="B102" s="28" t="s">
         <v>432</v>
       </c>
-      <c r="C102" t="s">
+      <c r="C102" s="28" t="s">
         <v>757</v>
       </c>
-      <c r="D102" t="s">
+      <c r="D102" s="28" t="s">
         <v>84</v>
       </c>
-      <c r="E102" t="s">
+      <c r="E102" s="28" t="s">
         <v>78</v>
       </c>
-      <c r="F102" t="s">
+      <c r="F102" s="28" t="s">
         <v>79</v>
       </c>
-      <c r="G102" t="s">
+      <c r="G102" s="28" t="s">
         <v>758</v>
       </c>
-      <c r="H102" t="s">
+      <c r="H102" s="28" t="s">
         <v>759</v>
       </c>
-      <c r="I102" t="s">
+      <c r="I102" s="28" t="s">
         <v>203</v>
       </c>
-      <c r="K102" t="s">
+      <c r="K102" s="28" t="s">
         <v>204</v>
       </c>
-      <c r="L102" t="s">
+      <c r="L102" s="28" t="s">
         <v>760</v>
       </c>
-      <c r="M102" t="s">
+      <c r="M102" s="28" t="s">
         <v>207</v>
       </c>
-      <c r="N102" t="s">
+      <c r="N102" s="28" t="s">
         <v>209</v>
       </c>
-      <c r="P102" t="s">
+      <c r="P102" s="28" t="s">
         <v>209</v>
       </c>
-      <c r="Q102" t="s">
+      <c r="Q102" s="28" t="s">
         <v>209</v>
       </c>
-      <c r="R102" t="s">
+      <c r="R102" s="28" t="s">
         <v>757</v>
       </c>
-      <c r="S102" t="s">
+      <c r="S102" s="28" t="s">
         <v>761</v>
       </c>
       <c r="T102" s="28" t="s">
         <v>82</v>
       </c>
-      <c r="U102" t="s">
+      <c r="U102" s="28" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="103" spans="1:21" ht="13.5">
-      <c r="A103" t="s">
+    <row r="103" spans="1:21" s="28" customFormat="1" ht="13.5">
+      <c r="A103" s="28" t="s">
         <v>762</v>
       </c>
-      <c r="B103" s="62" t="s">
+      <c r="B103" s="28" t="s">
         <v>432</v>
       </c>
-      <c r="C103" t="s">
+      <c r="C103" s="28" t="s">
         <v>98</v>
       </c>
-      <c r="D103" t="s">
+      <c r="D103" s="28" t="s">
         <v>84</v>
       </c>
       <c r="E103" s="28" t="s">
         <v>78</v>
       </c>
-      <c r="F103" t="s">
+      <c r="F103" s="28" t="s">
         <v>212</v>
       </c>
-      <c r="G103" t="s">
+      <c r="G103" s="28" t="s">
         <v>100</v>
       </c>
-      <c r="H103" t="s">
+      <c r="H103" s="28" t="s">
         <v>763</v>
       </c>
-      <c r="I103" t="s">
+      <c r="I103" s="28" t="s">
         <v>203</v>
       </c>
-      <c r="K103" t="s">
+      <c r="K103" s="28" t="s">
         <v>754</v>
       </c>
-      <c r="L103" t="s">
+      <c r="L103" s="28" t="s">
         <v>764</v>
       </c>
-      <c r="M103" t="s">
+      <c r="M103" s="28" t="s">
         <v>257</v>
       </c>
-      <c r="N103" t="s">
+      <c r="N103" s="28" t="s">
         <v>209</v>
       </c>
-      <c r="P103" t="s">
+      <c r="P103" s="28" t="s">
         <v>208</v>
       </c>
-      <c r="Q103" t="s">
+      <c r="Q103" s="28" t="s">
         <v>209</v>
       </c>
-      <c r="R103" t="s">
+      <c r="R103" s="28" t="s">
         <v>216</v>
       </c>
-      <c r="S103" t="s">
+      <c r="S103" s="28" t="s">
         <v>765</v>
       </c>
       <c r="T103" s="28" t="s">
         <v>104</v>
       </c>
-      <c r="U103" t="s">
+      <c r="U103" s="28" t="s">
         <v>16</v>
       </c>
     </row>
   </sheetData>
   <customSheetViews>
-    <customSheetView guid="{C25CEB9E-BEC1-4982-90C4-50C84EE1B82A}" filter="1" showAutoFilter="1">
-      <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-      <autoFilter ref="A1:AD33" xr:uid="{2EE84BD7-CD08-48B0-9729-062731625796}"/>
-    </customSheetView>
     <customSheetView guid="{A7754112-A52F-4ABC-8778-92F04773E53C}" filter="1" showAutoFilter="1">
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-      <autoFilter ref="A1:AD33" xr:uid="{C561AC0E-FB1D-4B04-95D0-12B66A5A9357}">
+      <autoFilter ref="A1:AD33" xr:uid="{6FC7F231-1C0F-4B9F-9EE9-B10376BF08C8}">
         <filterColumn colId="5">
           <filters blank="1">
             <filter val="Strathnairn"/>
           </filters>
         </filterColumn>
       </autoFilter>
+    </customSheetView>
+    <customSheetView guid="{C25CEB9E-BEC1-4982-90C4-50C84EE1B82A}" filter="1" showAutoFilter="1">
+      <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+      <autoFilter ref="A1:AD33" xr:uid="{2F96F445-D8DF-4A85-B15B-C24EDE52000D}"/>
     </customSheetView>
   </customSheetViews>
   <conditionalFormatting sqref="A1:AI1">

</xml_diff>

<commit_message>
Script (1 to 5) and fixed issues
</commit_message>
<xml_diff>
--- a/src/main/resources/InputTestdata/Listing details.xlsx
+++ b/src/main/resources/InputTestdata/Listing details.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Athavan\git\777Homes-2\777Homes-business\src\main\resources\InputTestdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8FD2FB19-24D9-4B3E-AC43-B139143F73B4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3630B92B-833F-496F-B72E-40EC9AEB0ACD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="20715" windowHeight="13276" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="20715" windowHeight="13276" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Backlog" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2744" uniqueCount="847">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2769" uniqueCount="856">
   <si>
     <t>ID</t>
   </si>
@@ -3934,6 +3934,50 @@
   </si>
   <si>
     <t>Block/House: 4688 / 92</t>
+  </si>
+  <si>
+    <t>https://www.allhomes.com.au/unit-62-100-henry-kendall-street-franklin-act-2913</t>
+  </si>
+  <si>
+    <t>114</t>
+  </si>
+  <si>
+    <t>62/100 Henry Kendall Street, Franklin ACT 2913</t>
+  </si>
+  <si>
+    <t xml:space="preserve">5	0	0	</t>
+  </si>
+  <si>
+    <t>$500 per week</t>
+  </si>
+  <si>
+    <t>This large two-bedroom apartment is located in the beautiful Vista complex in Franklin, close to Gungahlin Marketplace, parks &amp; nature reserves and Light Rail network which can take just minutes to transport you to Gungahlin Town Centre, Mitchell, Inner North or even the Canberra City CBD.
+Situated on the highly desired ground floor with the largest, most private courtyard in the complex, the apartment features quality inclusions, open plan living/dining area, two good sized bedrooms, two bathrooms with heated floor and air-conditioning in the main living area.
+Open plan dining &amp; living area extends through the sliding glass doors onto the alfresco deck which offers you lots of fantastic space for entertaining.
+The property also comes complete with two underground car spaces and a storage cage.
+- High quality finishes throughout
+- Great kitchen with large stone benchtops
+- Open-plan living and dining area
+- Spacious, modern bathrooms with heated flooring
+- Plenty of storage including linen cupboard
+- Bedroom one with walk-in wardrobe &amp; ensuite
+- Bedroom two with built-in wardrobe
+- Air-conditioning in the main living area
+- NBN broadband available
+- Data points and TV points in all bedrooms and living room
+- Undercover parking and lockable storage
+- Close to the Gungahlin Marketplace
+- Close to the Light Rail network
+For any additional information or alternative viewing times, please call Vinko on 0410 636 045.</t>
+  </si>
+  <si>
+    <t>Draft</t>
+  </si>
+  <si>
+    <t>https://www.777homes.com.au/?post_type=property&amp;p=8116&amp;preview=true</t>
+  </si>
+  <si>
+    <t>Rent</t>
   </si>
 </sst>
 </file>
@@ -4106,7 +4150,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="10">
+  <fills count="11">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -4160,6 +4204,11 @@
         <bgColor indexed="2"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="mediumGray">
+        <bgColor indexed="2"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -4174,7 +4223,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="27" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="54">
+  <cellXfs count="55">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -4289,6 +4338,7 @@
     <xf numFmtId="0" fontId="28" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -4525,11 +4575,11 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:AB114"/>
+  <dimension ref="A1:AB115"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A95" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C114" sqref="C114"/>
+      <selection pane="bottomLeft" activeCell="B115" sqref="B115"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.46484375" defaultRowHeight="15.75" customHeight="1"/>
@@ -5669,7 +5719,7 @@
       <c r="C27" s="2" t="s">
         <v>705</v>
       </c>
-      <c r="D27" s="4" t="s">
+      <c r="D27" s="48" t="s">
         <v>14</v>
       </c>
       <c r="E27" s="15"/>
@@ -6262,7 +6312,7 @@
       <c r="A49" s="4">
         <v>48</v>
       </c>
-      <c r="B49" s="4" t="s">
+      <c r="B49" s="46" t="s">
         <v>194</v>
       </c>
       <c r="C49" s="46" t="s">
@@ -6586,7 +6636,7 @@
       <c r="C64" s="46" t="s">
         <v>740</v>
       </c>
-      <c r="D64" s="4" t="s">
+      <c r="D64" s="47" t="s">
         <v>14</v>
       </c>
       <c r="F64" s="2" t="s">
@@ -6630,8 +6680,8 @@
       <c r="C66" s="46" t="s">
         <v>741</v>
       </c>
-      <c r="D66" s="4" t="s">
-        <v>7</v>
+      <c r="D66" s="47" t="s">
+        <v>14</v>
       </c>
       <c r="F66" s="2" t="s">
         <v>691</v>
@@ -6808,7 +6858,7 @@
       <c r="A74">
         <v>73</v>
       </c>
-      <c r="B74" t="s">
+      <c r="B74" s="49" t="s">
         <v>474</v>
       </c>
       <c r="C74" t="s">
@@ -6854,7 +6904,7 @@
       <c r="A76">
         <v>75</v>
       </c>
-      <c r="B76" t="s">
+      <c r="B76" s="49" t="s">
         <v>475</v>
       </c>
       <c r="C76" t="s">
@@ -7136,7 +7186,7 @@
       <c r="C88" t="s">
         <v>650</v>
       </c>
-      <c r="D88" s="4" t="s">
+      <c r="D88" s="47" t="s">
         <v>14</v>
       </c>
       <c r="F88" s="2" t="s">
@@ -7275,7 +7325,7 @@
         <v>687</v>
       </c>
       <c r="D94" s="4" t="s">
-        <v>7</v>
+        <v>14</v>
       </c>
       <c r="F94" s="2" t="s">
         <v>691</v>
@@ -7413,7 +7463,7 @@
         <v>722</v>
       </c>
       <c r="D100" s="4" t="s">
-        <v>7</v>
+        <v>14</v>
       </c>
       <c r="F100" s="2" t="s">
         <v>691</v>
@@ -7596,8 +7646,8 @@
       <c r="C108" t="s">
         <v>803</v>
       </c>
-      <c r="D108" s="47" t="s">
-        <v>14</v>
+      <c r="D108" s="4" t="s">
+        <v>7</v>
       </c>
       <c r="F108" s="2" t="s">
         <v>691</v>
@@ -7745,6 +7795,29 @@
       </c>
       <c r="H114" t="s">
         <v>430</v>
+      </c>
+    </row>
+    <row r="115" spans="1:8" ht="12.75">
+      <c r="A115">
+        <v>114</v>
+      </c>
+      <c r="B115" s="49" t="s">
+        <v>847</v>
+      </c>
+      <c r="C115" t="s">
+        <v>854</v>
+      </c>
+      <c r="D115" s="54" t="s">
+        <v>853</v>
+      </c>
+      <c r="F115" s="2" t="s">
+        <v>691</v>
+      </c>
+      <c r="G115" t="s">
+        <v>328</v>
+      </c>
+      <c r="H115" t="s">
+        <v>326</v>
       </c>
     </row>
   </sheetData>
@@ -7892,9 +7965,13 @@
     <hyperlink ref="C114" r:id="rId141" xr:uid="{6FE6A043-A6B1-44FF-8A45-8C3690323458}"/>
     <hyperlink ref="B113" r:id="rId142" xr:uid="{0F94FF41-1E06-4D7B-B360-1EB377073C87}"/>
     <hyperlink ref="B112" r:id="rId143" xr:uid="{490A5044-10EC-4082-BEC1-14008171D5CF}"/>
+    <hyperlink ref="B49" r:id="rId144" xr:uid="{836EB236-8BF1-4259-B395-AD9FA9DE0AE0}"/>
+    <hyperlink ref="B74" r:id="rId145" xr:uid="{8AA8904A-1CC5-4D06-93EF-66F7FC625199}"/>
+    <hyperlink ref="B76" r:id="rId146" xr:uid="{5743888C-C74A-41C6-ABC5-E9575351702D}"/>
+    <hyperlink ref="B115" r:id="rId147" xr:uid="{27BDB583-8AD0-4B33-BA19-24E42C9E7CE9}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId144"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId148"/>
 </worksheet>
 </file>
 
@@ -7903,11 +7980,11 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:AI114"/>
+  <dimension ref="A1:AI115"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A93" workbookViewId="0">
+    <sheetView topLeftCell="A100" workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="P126" sqref="P126"/>
+      <selection pane="topRight" activeCell="E121" sqref="E121"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.46484375" defaultRowHeight="15.75" customHeight="1"/>
@@ -8178,8 +8255,8 @@
       <c r="A4" s="26">
         <v>3</v>
       </c>
-      <c r="B4" s="26" t="s">
-        <v>7</v>
+      <c r="B4" s="51" t="s">
+        <v>175</v>
       </c>
       <c r="C4" s="26" t="s">
         <v>89</v>
@@ -8187,8 +8264,8 @@
       <c r="D4" s="26" t="s">
         <v>84</v>
       </c>
-      <c r="E4" s="26" t="s">
-        <v>176</v>
+      <c r="E4" s="51" t="s">
+        <v>175</v>
       </c>
       <c r="F4" s="26" t="s">
         <v>79</v>
@@ -8372,8 +8449,8 @@
       <c r="A7" s="26">
         <v>6</v>
       </c>
-      <c r="B7" s="26" t="s">
-        <v>7</v>
+      <c r="B7" s="51" t="s">
+        <v>175</v>
       </c>
       <c r="C7" s="26" t="s">
         <v>103</v>
@@ -8381,8 +8458,8 @@
       <c r="D7" s="26" t="s">
         <v>84</v>
       </c>
-      <c r="E7" s="26" t="s">
-        <v>176</v>
+      <c r="E7" s="51" t="s">
+        <v>175</v>
       </c>
       <c r="F7" s="26" t="s">
         <v>94</v>
@@ -9586,8 +9663,8 @@
       <c r="A27" s="26">
         <v>26</v>
       </c>
-      <c r="B27" s="26" t="s">
-        <v>7</v>
+      <c r="B27" s="51" t="s">
+        <v>175</v>
       </c>
       <c r="C27" s="26" t="s">
         <v>147</v>
@@ -9595,8 +9672,8 @@
       <c r="D27" s="26" t="s">
         <v>77</v>
       </c>
-      <c r="E27" s="26" t="s">
-        <v>176</v>
+      <c r="E27" s="51" t="s">
+        <v>175</v>
       </c>
       <c r="F27" s="26" t="s">
         <v>94</v>
@@ -9822,8 +9899,8 @@
       <c r="A31" s="26">
         <v>30</v>
       </c>
-      <c r="B31" s="26" t="s">
-        <v>7</v>
+      <c r="B31" s="51" t="s">
+        <v>175</v>
       </c>
       <c r="C31" s="26" t="s">
         <v>151</v>
@@ -9831,8 +9908,8 @@
       <c r="D31" s="26" t="s">
         <v>77</v>
       </c>
-      <c r="E31" s="26" t="s">
-        <v>176</v>
+      <c r="E31" s="51" t="s">
+        <v>175</v>
       </c>
       <c r="F31" s="26" t="s">
         <v>108</v>
@@ -10881,8 +10958,8 @@
       <c r="A49" s="26" t="s">
         <v>301</v>
       </c>
-      <c r="B49" s="26" t="s">
-        <v>7</v>
+      <c r="B49" s="51" t="s">
+        <v>175</v>
       </c>
       <c r="C49" s="26" t="s">
         <v>302</v>
@@ -10890,8 +10967,8 @@
       <c r="D49" s="26" t="s">
         <v>84</v>
       </c>
-      <c r="E49" s="26" t="s">
-        <v>78</v>
+      <c r="E49" s="51" t="s">
+        <v>175</v>
       </c>
       <c r="F49" s="26" t="s">
         <v>210</v>
@@ -11707,8 +11784,8 @@
       <c r="A63" s="26" t="s">
         <v>403</v>
       </c>
-      <c r="B63" s="26" t="s">
-        <v>7</v>
+      <c r="B63" s="51" t="s">
+        <v>175</v>
       </c>
       <c r="C63" s="26" t="s">
         <v>404</v>
@@ -11716,8 +11793,8 @@
       <c r="D63" s="26" t="s">
         <v>84</v>
       </c>
-      <c r="E63" s="26" t="s">
-        <v>78</v>
+      <c r="E63" s="51" t="s">
+        <v>175</v>
       </c>
       <c r="F63" s="26" t="s">
         <v>79</v>
@@ -11766,8 +11843,8 @@
       <c r="A64" s="26" t="s">
         <v>408</v>
       </c>
-      <c r="B64" s="26" t="s">
-        <v>7</v>
+      <c r="B64" s="51" t="s">
+        <v>175</v>
       </c>
       <c r="C64" s="26" t="s">
         <v>409</v>
@@ -11775,8 +11852,8 @@
       <c r="D64" s="26" t="s">
         <v>84</v>
       </c>
-      <c r="E64" s="26" t="s">
-        <v>78</v>
+      <c r="E64" s="51" t="s">
+        <v>175</v>
       </c>
       <c r="F64" s="26" t="s">
         <v>410</v>
@@ -11943,8 +12020,8 @@
       <c r="A67" s="26" t="s">
         <v>425</v>
       </c>
-      <c r="B67" s="26" t="s">
-        <v>7</v>
+      <c r="B67" s="51" t="s">
+        <v>175</v>
       </c>
       <c r="C67" s="26" t="s">
         <v>426</v>
@@ -11952,8 +12029,8 @@
       <c r="D67" s="26" t="s">
         <v>84</v>
       </c>
-      <c r="E67" s="26" t="s">
-        <v>78</v>
+      <c r="E67" s="51" t="s">
+        <v>175</v>
       </c>
       <c r="F67" s="26" t="s">
         <v>99</v>
@@ -12002,8 +12079,8 @@
       <c r="A68" s="26" t="s">
         <v>486</v>
       </c>
-      <c r="B68" s="26" t="s">
-        <v>7</v>
+      <c r="B68" s="51" t="s">
+        <v>175</v>
       </c>
       <c r="C68" s="26" t="s">
         <v>487</v>
@@ -12011,8 +12088,8 @@
       <c r="D68" s="26" t="s">
         <v>84</v>
       </c>
-      <c r="E68" s="26" t="s">
-        <v>78</v>
+      <c r="E68" s="51" t="s">
+        <v>175</v>
       </c>
       <c r="F68" s="26" t="s">
         <v>79</v>
@@ -12356,8 +12433,8 @@
       <c r="A74" s="26" t="s">
         <v>510</v>
       </c>
-      <c r="B74" s="26" t="s">
-        <v>7</v>
+      <c r="B74" s="51" t="s">
+        <v>175</v>
       </c>
       <c r="C74" s="26" t="s">
         <v>511</v>
@@ -12365,8 +12442,8 @@
       <c r="D74" s="26" t="s">
         <v>264</v>
       </c>
-      <c r="E74" s="26" t="s">
-        <v>78</v>
+      <c r="E74" s="51" t="s">
+        <v>175</v>
       </c>
       <c r="F74" s="26" t="s">
         <v>79</v>
@@ -12484,7 +12561,7 @@
         <v>84</v>
       </c>
       <c r="E76" s="26" t="s">
-        <v>78</v>
+        <v>176</v>
       </c>
       <c r="F76" s="26" t="s">
         <v>79</v>
@@ -13182,8 +13259,8 @@
       <c r="A88" s="26" t="s">
         <v>617</v>
       </c>
-      <c r="B88" s="26" t="s">
-        <v>7</v>
+      <c r="B88" s="51" t="s">
+        <v>175</v>
       </c>
       <c r="C88" s="26" t="s">
         <v>618</v>
@@ -13191,8 +13268,8 @@
       <c r="D88" s="26" t="s">
         <v>77</v>
       </c>
-      <c r="E88" s="26" t="s">
-        <v>78</v>
+      <c r="E88" s="51" t="s">
+        <v>175</v>
       </c>
       <c r="F88" s="26" t="s">
         <v>79</v>
@@ -14008,8 +14085,8 @@
       <c r="A102" s="26" t="s">
         <v>749</v>
       </c>
-      <c r="B102" s="26" t="s">
-        <v>7</v>
+      <c r="B102" s="51" t="s">
+        <v>175</v>
       </c>
       <c r="C102" s="26" t="s">
         <v>750</v>
@@ -14017,8 +14094,8 @@
       <c r="D102" s="26" t="s">
         <v>84</v>
       </c>
-      <c r="E102" s="26" t="s">
-        <v>78</v>
+      <c r="E102" s="51" t="s">
+        <v>175</v>
       </c>
       <c r="F102" s="26" t="s">
         <v>79</v>
@@ -14372,7 +14449,7 @@
         <v>77</v>
       </c>
       <c r="E108" s="26" t="s">
-        <v>78</v>
+        <v>176</v>
       </c>
       <c r="F108" s="26" t="s">
         <v>79</v>
@@ -14769,17 +14846,76 @@
       </c>
       <c r="U114" s="26" t="s">
         <v>8</v>
+      </c>
+    </row>
+    <row r="115" spans="1:21" ht="13.5">
+      <c r="A115" t="s">
+        <v>848</v>
+      </c>
+      <c r="B115" t="s">
+        <v>853</v>
+      </c>
+      <c r="C115" t="s">
+        <v>849</v>
+      </c>
+      <c r="D115" t="s">
+        <v>77</v>
+      </c>
+      <c r="E115" t="s">
+        <v>855</v>
+      </c>
+      <c r="F115" t="s">
+        <v>79</v>
+      </c>
+      <c r="G115" t="s">
+        <v>224</v>
+      </c>
+      <c r="H115" t="s">
+        <v>202</v>
+      </c>
+      <c r="I115" t="s">
+        <v>201</v>
+      </c>
+      <c r="K115" t="s">
+        <v>850</v>
+      </c>
+      <c r="L115" t="s">
+        <v>851</v>
+      </c>
+      <c r="M115" t="s">
+        <v>207</v>
+      </c>
+      <c r="N115" t="s">
+        <v>269</v>
+      </c>
+      <c r="P115" t="s">
+        <v>202</v>
+      </c>
+      <c r="Q115" t="s">
+        <v>202</v>
+      </c>
+      <c r="R115" t="s">
+        <v>849</v>
+      </c>
+      <c r="S115" t="s">
+        <v>852</v>
+      </c>
+      <c r="T115" s="26" t="s">
+        <v>691</v>
+      </c>
+      <c r="U115" t="s">
+        <v>328</v>
       </c>
     </row>
   </sheetData>
   <customSheetViews>
     <customSheetView guid="{C25CEB9E-BEC1-4982-90C4-50C84EE1B82A}" filter="1" showAutoFilter="1">
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-      <autoFilter ref="A1:AD33" xr:uid="{69AFEFEF-4FE7-42A3-870F-E1C74472621C}"/>
+      <autoFilter ref="A1:AD33" xr:uid="{648BE49C-5618-4C9A-9D28-663898EFD3CD}"/>
     </customSheetView>
     <customSheetView guid="{A7754112-A52F-4ABC-8778-92F04773E53C}" filter="1" showAutoFilter="1">
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-      <autoFilter ref="A1:AD33" xr:uid="{5FAD2C09-3879-46EF-A5B9-9C4BE1C4035F}">
+      <autoFilter ref="A1:AD33" xr:uid="{737C7704-22C4-4848-B912-7D86624B64F0}">
         <filterColumn colId="5">
           <filters blank="1">
             <filter val="Strathnairn"/>

</xml_diff>

<commit_message>
Issues raised by Sangee in fixed (05/09/2021)
</commit_message>
<xml_diff>
--- a/src/main/resources/InputTestdata/Listing details.xlsx
+++ b/src/main/resources/InputTestdata/Listing details.xlsx
@@ -1,39 +1,39 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" mc:Ignorable="x15 xr xr6 xr10 xr2">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24326"/>
   <workbookPr/>
-  <mc:AlternateContent>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Athavan\git\777Homes-2\777Homes-business\src\main\resources\InputTestdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr documentId="13_ncr:1_{EE0A6416-93E3-4F52-B109-CF5899E95993}" revIDLastSave="0" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A2D64A54-914B-428A-BAF1-125CD1510B8A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView windowHeight="15840" windowWidth="29040" xWindow="-120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}" yWindow="-120"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Backlog" r:id="rId1" sheetId="1"/>
-    <sheet name="Listing" r:id="rId2" sheetId="2"/>
-    <sheet name="Tobe-executed" r:id="rId3" sheetId="3"/>
-    <sheet name="Agency login" r:id="rId4" sheetId="4"/>
+    <sheet name="Backlog" sheetId="1" r:id="rId1"/>
+    <sheet name="Listing" sheetId="2" r:id="rId2"/>
+    <sheet name="Tobe-executed" sheetId="3" r:id="rId3"/>
+    <sheet name="Agency login" sheetId="4" r:id="rId4"/>
   </sheets>
   <definedNames>
-    <definedName hidden="1" localSheetId="0" name="_xlnm._FilterDatabase">Backlog!$A$1:$AB$52</definedName>
-    <definedName hidden="1" localSheetId="1" name="_xlnm._FilterDatabase">Listing!#REF!</definedName>
-    <definedName hidden="1" localSheetId="1" name="Z_A7754112_A52F_4ABC_8778_92F04773E53C_.wvu.FilterData">Listing!$A$1:$AE$32</definedName>
-    <definedName hidden="1" localSheetId="1" name="Z_C25CEB9E_BEC1_4982_90C4_50C84EE1B82A_.wvu.FilterData">Listing!$A$1:$AE$32</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Backlog!$A$1:$AB$52</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Listing!#REF!</definedName>
+    <definedName name="Z_A7754112_A52F_4ABC_8778_92F04773E53C_.wvu.FilterData" localSheetId="1" hidden="1">Listing!$A$1:$AE$32</definedName>
+    <definedName name="Z_C25CEB9E_BEC1_4982_90C4_50C84EE1B82A_.wvu.FilterData" localSheetId="1" hidden="1">Listing!$A$1:$AE$32</definedName>
   </definedNames>
   <calcPr calcId="181029"/>
   <customWorkbookViews>
-    <customWorkbookView activeSheetId="0" guid="{A7754112-A52F-4ABC-8778-92F04773E53C}" maximized="1" name="Filter 1" windowHeight="0" windowWidth="0"/>
-    <customWorkbookView activeSheetId="0" guid="{C25CEB9E-BEC1-4982-90C4-50C84EE1B82A}" maximized="1" name="Filter 2" windowHeight="0" windowWidth="0"/>
+    <customWorkbookView name="Filter 2" guid="{C25CEB9E-BEC1-4982-90C4-50C84EE1B82A}" maximized="1" windowWidth="0" windowHeight="0" activeSheetId="0"/>
+    <customWorkbookView name="Filter 1" guid="{A7754112-A52F-4ABC-8778-92F04773E53C}" maximized="1" windowWidth="0" windowHeight="0" activeSheetId="0"/>
   </customWorkbookViews>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3472" uniqueCount="1052">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3470" uniqueCount="1052">
   <si>
     <t>ID</t>
   </si>
@@ -5050,7 +5050,6 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="0"/>
   <fonts count="30">
     <font>
       <sz val="10"/>
@@ -5299,118 +5298,118 @@
     </border>
   </borders>
   <cellStyleXfs count="2">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
-    <xf applyAlignment="0" applyBorder="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="0" fontId="26" numFmtId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="50">
-    <xf applyAlignment="1" applyFont="1" borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyAlignment="1" applyFill="1" applyFont="1" borderId="0" fillId="3" fontId="1" numFmtId="0" xfId="0">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf applyAlignment="1" applyFill="1" applyFont="1" borderId="0" fillId="2" fontId="2" numFmtId="0" xfId="0">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf applyAlignment="1" applyFill="1" applyFont="1" borderId="0" fillId="2" fontId="3" numFmtId="0" xfId="0"/>
-    <xf applyAlignment="1" applyFill="1" applyFont="1" borderId="0" fillId="2" fontId="4" numFmtId="0" xfId="0">
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf applyAlignment="1" applyFill="1" applyFont="1" borderId="0" fillId="2" fontId="6" numFmtId="0" xfId="0">
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf applyFill="1" applyFont="1" borderId="0" fillId="2" fontId="4" numFmtId="0" xfId="0"/>
-    <xf applyAlignment="1" applyFill="1" applyFont="1" borderId="0" fillId="2" fontId="7" numFmtId="0" xfId="0"/>
-    <xf applyAlignment="1" applyFill="1" applyFont="1" borderId="0" fillId="2" fontId="8" numFmtId="0" xfId="0"/>
-    <xf applyAlignment="1" applyFill="1" applyFont="1" borderId="0" fillId="2" fontId="5" numFmtId="0" xfId="0">
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf applyAlignment="1" applyFill="1" applyFont="1" borderId="0" fillId="4" fontId="4" numFmtId="0" xfId="0">
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf applyAlignment="1" applyFill="1" applyFont="1" borderId="0" fillId="5" fontId="4" numFmtId="0" xfId="0">
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf applyAlignment="1" applyFill="1" applyFont="1" borderId="0" fillId="2" fontId="9" numFmtId="0" xfId="0">
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf applyAlignment="1" applyFill="1" applyFont="1" borderId="0" fillId="2" fontId="10" numFmtId="0" xfId="0"/>
-    <xf applyAlignment="1" applyFill="1" applyFont="1" borderId="0" fillId="2" fontId="11" numFmtId="0" xfId="0"/>
-    <xf applyAlignment="1" applyFill="1" applyFont="1" borderId="0" fillId="2" fontId="4" numFmtId="0" xfId="0">
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="11" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf applyAlignment="1" applyFill="1" applyFont="1" borderId="0" fillId="2" fontId="12" numFmtId="0" xfId="0"/>
-    <xf applyAlignment="1" applyFill="1" applyFont="1" borderId="0" fillId="2" fontId="13" numFmtId="0" xfId="0"/>
-    <xf applyAlignment="1" applyFill="1" applyFont="1" borderId="0" fillId="2" fontId="14" numFmtId="0" xfId="0"/>
-    <xf applyAlignment="1" applyFill="1" applyFont="1" borderId="0" fillId="2" fontId="15" numFmtId="0" xfId="0"/>
-    <xf applyAlignment="1" applyFill="1" applyFont="1" borderId="0" fillId="2" fontId="16" numFmtId="0" xfId="0"/>
-    <xf applyAlignment="1" applyFill="1" applyFont="1" borderId="0" fillId="2" fontId="17" numFmtId="0" xfId="0"/>
-    <xf applyAlignment="1" applyFill="1" applyFont="1" borderId="0" fillId="3" fontId="1" numFmtId="0" xfId="0">
+    <xf numFmtId="0" fontId="12" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="13" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="14" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="15" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="16" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="17" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf applyFill="1" applyFont="1" borderId="0" fillId="3" fontId="7" numFmtId="0" xfId="0"/>
-    <xf applyAlignment="1" applyFill="1" applyFont="1" borderId="0" fillId="2" fontId="18" numFmtId="0" xfId="0">
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="18" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf applyAlignment="1" applyFill="1" applyFont="1" borderId="0" fillId="2" fontId="19" numFmtId="0" xfId="0">
+    <xf numFmtId="0" fontId="19" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf applyAlignment="1" applyFill="1" applyFont="1" borderId="0" fillId="2" fontId="20" numFmtId="0" xfId="0">
+    <xf numFmtId="0" fontId="20" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf applyAlignment="1" applyFill="1" applyFont="1" borderId="0" fillId="2" fontId="21" numFmtId="0" xfId="0">
+    <xf numFmtId="0" fontId="21" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf applyAlignment="1" applyFill="1" applyFont="1" borderId="0" fillId="2" fontId="18" numFmtId="0" xfId="0">
+    <xf numFmtId="0" fontId="18" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf applyAlignment="1" applyFill="1" applyFont="1" borderId="0" fillId="2" fontId="22" numFmtId="0" xfId="0">
+    <xf numFmtId="0" fontId="22" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf applyAlignment="1" applyFont="1" borderId="0" fillId="0" fontId="7" numFmtId="0" xfId="0">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf applyAlignment="1" applyFill="1" applyFont="1" borderId="0" fillId="3" fontId="17" numFmtId="0" xfId="0"/>
-    <xf applyAlignment="1" applyFill="1" applyFont="1" borderId="0" fillId="3" fontId="12" numFmtId="0" xfId="0"/>
-    <xf applyAlignment="1" applyFill="1" applyFont="1" borderId="0" fillId="3" fontId="23" numFmtId="0" xfId="0">
+    <xf numFmtId="0" fontId="17" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="12" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="23" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf applyAlignment="1" applyFill="1" applyFont="1" borderId="0" fillId="3" fontId="24" numFmtId="0" xfId="0"/>
-    <xf applyAlignment="1" applyFont="1" borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0"/>
-    <xf applyAlignment="1" applyFill="1" applyFont="1" borderId="0" fillId="3" fontId="25" numFmtId="0" xfId="0">
+    <xf numFmtId="0" fontId="24" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="25" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf applyAlignment="1" applyFill="1" applyFont="1" borderId="0" fillId="3" fontId="1" numFmtId="0" xfId="0">
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf applyAlignment="1" applyFont="1" borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf applyAlignment="1" applyFill="1" borderId="0" fillId="2" fontId="26" numFmtId="0" xfId="1">
+    <xf numFmtId="0" fontId="26" fillId="2" borderId="0" xfId="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf applyAlignment="1" applyFill="1" applyFont="1" borderId="0" fillId="6" fontId="2" numFmtId="0" xfId="0">
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf applyAlignment="1" applyFill="1" applyFont="1" borderId="0" fillId="7" fontId="5" numFmtId="0" xfId="0">
+    <xf numFmtId="0" fontId="5" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf applyAlignment="1" borderId="0" fillId="0" fontId="26" numFmtId="0" xfId="1"/>
-    <xf applyAlignment="1" applyFill="1" borderId="0" fillId="2" fontId="26" numFmtId="0" xfId="1"/>
-    <xf applyAlignment="1" applyFill="1" applyFont="1" borderId="0" fillId="8" fontId="18" numFmtId="0" xfId="0">
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" xfId="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="26" fillId="2" borderId="0" xfId="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="18" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf applyFill="1" borderId="0" fillId="9" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyAlignment="1" applyFill="1" applyFont="1" borderId="0" fillId="2" fontId="27" numFmtId="0" xfId="0">
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="27" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf applyAlignment="1" applyFont="1" borderId="0" fillId="0" fontId="29" numFmtId="0" xfId="0"/>
-    <xf applyAlignment="1" applyFill="1" applyFont="1" borderId="0" fillId="10" fontId="28" numFmtId="0" xfId="0">
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="28" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf applyFill="1" borderId="0" fillId="11" fontId="0" numFmtId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
-    <cellStyle builtinId="8" name="Hyperlink" xfId="1"/>
-    <cellStyle builtinId="0" name="Normal" xfId="0"/>
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="2">
     <dxf>
@@ -5430,7 +5429,7 @@
       </fill>
     </dxf>
   </dxfs>
-  <tableStyles count="0" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium2"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -5554,21 +5553,21 @@
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
-        <a:ln algn="ctr" cap="flat" cmpd="sng" w="6350">
+        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
           <a:miter lim="800000"/>
         </a:ln>
-        <a:ln algn="ctr" cap="flat" cmpd="sng" w="12700">
+        <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
           <a:miter lim="800000"/>
         </a:ln>
-        <a:ln algn="ctr" cap="flat" cmpd="sng" w="19050">
+        <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
@@ -5585,7 +5584,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw algn="ctr" blurRad="57150" dir="5400000" dist="19050" rotWithShape="0">
+            <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="63000"/>
               </a:srgbClr>
@@ -5639,32 +5638,32 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:AC143"/>
+  <dimension ref="A1:AB143"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane activePane="bottomLeft" state="frozen" topLeftCell="A113" ySplit="1"/>
-      <selection activeCell="C130" pane="bottomLeft" sqref="C130"/>
+      <pane ySplit="1" topLeftCell="A122" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C145" sqref="C145"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="14.42578125" defaultRowHeight="15.75"/>
+  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="9.140625" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" width="74.85546875" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="75.0" collapsed="true"/>
-    <col min="4" max="4" customWidth="true" width="14.5703125" collapsed="true"/>
-    <col min="6" max="6" bestFit="true" customWidth="true" style="38" width="22.140625" collapsed="true"/>
-    <col min="7" max="7" customWidth="true" width="21.85546875" collapsed="true"/>
-    <col min="8" max="8" customWidth="true" width="56.85546875" collapsed="true"/>
-    <col min="9" max="9" customWidth="true" width="10.85546875" collapsed="true"/>
-    <col min="10" max="10" customWidth="true" width="17.85546875" collapsed="true"/>
-    <col min="11" max="11" customWidth="true" width="22.5703125" collapsed="true"/>
+    <col min="1" max="1" width="9.140625" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="74.85546875" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="75" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="14.5703125" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="22.140625" style="38" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="21.85546875" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="56.85546875" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="10.85546875" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="17.85546875" customWidth="1" collapsed="1"/>
+    <col min="11" max="11" width="22.5703125" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row ht="15" r="1" spans="1:28">
+    <row r="1" spans="1:28" ht="15">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -5691,7 +5690,7 @@
       </c>
       <c r="J1" s="1"/>
     </row>
-    <row customHeight="1" ht="15.75" r="2" spans="1:28">
+    <row r="2" spans="1:28" ht="15.75" customHeight="1">
       <c r="A2" s="2">
         <v>1</v>
       </c>
@@ -5737,7 +5736,7 @@
       <c r="AA2" s="6"/>
       <c r="AB2" s="6"/>
     </row>
-    <row ht="14.25" r="3" spans="1:28">
+    <row r="3" spans="1:28" ht="14.25">
       <c r="A3" s="2">
         <v>2</v>
       </c>
@@ -5783,7 +5782,7 @@
       <c r="AA3" s="6"/>
       <c r="AB3" s="6"/>
     </row>
-    <row customHeight="1" ht="15.75" r="4" spans="1:28">
+    <row r="4" spans="1:28" ht="15.75" customHeight="1">
       <c r="A4" s="9">
         <v>3</v>
       </c>
@@ -5829,7 +5828,7 @@
       <c r="AA4" s="6"/>
       <c r="AB4" s="6"/>
     </row>
-    <row ht="14.25" r="5" spans="1:28">
+    <row r="5" spans="1:28" ht="14.25">
       <c r="A5" s="9">
         <v>4</v>
       </c>
@@ -5873,7 +5872,7 @@
       <c r="AA5" s="6"/>
       <c r="AB5" s="6"/>
     </row>
-    <row ht="14.25" r="6" spans="1:28">
+    <row r="6" spans="1:28" ht="14.25">
       <c r="A6" s="9">
         <v>5</v>
       </c>
@@ -5917,7 +5916,7 @@
       <c r="AA6" s="9"/>
       <c r="AB6" s="9"/>
     </row>
-    <row ht="14.25" r="7" spans="1:28">
+    <row r="7" spans="1:28" ht="14.25">
       <c r="A7" s="9">
         <v>6</v>
       </c>
@@ -5961,7 +5960,7 @@
       <c r="AA7" s="6"/>
       <c r="AB7" s="6"/>
     </row>
-    <row ht="14.25" r="8" spans="1:28">
+    <row r="8" spans="1:28" ht="14.25">
       <c r="A8" s="9">
         <v>7</v>
       </c>
@@ -6005,7 +6004,7 @@
       <c r="AA8" s="6"/>
       <c r="AB8" s="6"/>
     </row>
-    <row ht="14.25" r="9" spans="1:28">
+    <row r="9" spans="1:28" ht="14.25">
       <c r="A9" s="9">
         <v>8</v>
       </c>
@@ -6047,7 +6046,7 @@
       <c r="AA9" s="6"/>
       <c r="AB9" s="6"/>
     </row>
-    <row ht="14.25" r="10" spans="1:28">
+    <row r="10" spans="1:28" ht="14.25">
       <c r="A10" s="9">
         <v>9</v>
       </c>
@@ -6089,7 +6088,7 @@
       <c r="AA10" s="6"/>
       <c r="AB10" s="6"/>
     </row>
-    <row ht="14.25" r="11" spans="1:28">
+    <row r="11" spans="1:28" ht="14.25">
       <c r="A11" s="9">
         <v>10</v>
       </c>
@@ -6133,7 +6132,7 @@
       <c r="AA11" s="6"/>
       <c r="AB11" s="6"/>
     </row>
-    <row ht="14.25" r="12" spans="1:28">
+    <row r="12" spans="1:28" ht="14.25">
       <c r="A12" s="9">
         <v>11</v>
       </c>
@@ -6175,7 +6174,7 @@
       <c r="AA12" s="6"/>
       <c r="AB12" s="6"/>
     </row>
-    <row ht="14.25" r="13" spans="1:28">
+    <row r="13" spans="1:28" ht="14.25">
       <c r="A13" s="9">
         <v>12</v>
       </c>
@@ -6217,7 +6216,7 @@
       <c r="AA13" s="6"/>
       <c r="AB13" s="6"/>
     </row>
-    <row ht="14.25" r="14" spans="1:28">
+    <row r="14" spans="1:28" ht="14.25">
       <c r="A14" s="9">
         <v>13</v>
       </c>
@@ -6259,7 +6258,7 @@
       <c r="AA14" s="6"/>
       <c r="AB14" s="6"/>
     </row>
-    <row ht="14.25" r="15" spans="1:28">
+    <row r="15" spans="1:28" ht="14.25">
       <c r="A15" s="9">
         <v>14</v>
       </c>
@@ -6303,7 +6302,7 @@
       <c r="AA15" s="6"/>
       <c r="AB15" s="6"/>
     </row>
-    <row ht="14.25" r="16" spans="1:28">
+    <row r="16" spans="1:28" ht="14.25">
       <c r="A16" s="9">
         <v>15</v>
       </c>
@@ -6345,7 +6344,7 @@
       <c r="AA16" s="6"/>
       <c r="AB16" s="6"/>
     </row>
-    <row ht="14.25" r="17" spans="1:28">
+    <row r="17" spans="1:28" ht="14.25">
       <c r="A17" s="9">
         <v>16</v>
       </c>
@@ -6389,7 +6388,7 @@
       <c r="AA17" s="6"/>
       <c r="AB17" s="6"/>
     </row>
-    <row ht="14.25" r="18" spans="1:28">
+    <row r="18" spans="1:28" ht="14.25">
       <c r="A18" s="9">
         <v>17</v>
       </c>
@@ -6431,7 +6430,7 @@
       <c r="AA18" s="6"/>
       <c r="AB18" s="6"/>
     </row>
-    <row ht="14.25" r="19" spans="1:28">
+    <row r="19" spans="1:28" ht="14.25">
       <c r="A19" s="9">
         <v>18</v>
       </c>
@@ -6475,7 +6474,7 @@
       <c r="AA19" s="6"/>
       <c r="AB19" s="6"/>
     </row>
-    <row ht="14.25" r="20" spans="1:28">
+    <row r="20" spans="1:28" ht="14.25">
       <c r="A20" s="9">
         <v>19</v>
       </c>
@@ -6519,7 +6518,7 @@
       <c r="AA20" s="6"/>
       <c r="AB20" s="6"/>
     </row>
-    <row ht="14.25" r="21" spans="1:28">
+    <row r="21" spans="1:28" ht="14.25">
       <c r="A21" s="9">
         <v>20</v>
       </c>
@@ -6563,7 +6562,7 @@
       <c r="AA21" s="6"/>
       <c r="AB21" s="6"/>
     </row>
-    <row ht="14.25" r="22" spans="1:28">
+    <row r="22" spans="1:28" ht="14.25">
       <c r="A22" s="9">
         <v>21</v>
       </c>
@@ -6605,7 +6604,7 @@
       <c r="AA22" s="6"/>
       <c r="AB22" s="6"/>
     </row>
-    <row ht="14.25" r="23" spans="1:28">
+    <row r="23" spans="1:28" ht="14.25">
       <c r="A23" s="9">
         <v>22</v>
       </c>
@@ -6649,7 +6648,7 @@
       <c r="AA23" s="6"/>
       <c r="AB23" s="6"/>
     </row>
-    <row ht="14.25" r="24" spans="1:28">
+    <row r="24" spans="1:28" ht="14.25">
       <c r="A24" s="9">
         <v>23</v>
       </c>
@@ -6691,7 +6690,7 @@
       <c r="AA24" s="6"/>
       <c r="AB24" s="6"/>
     </row>
-    <row ht="14.25" r="25" spans="1:28">
+    <row r="25" spans="1:28" ht="14.25">
       <c r="A25" s="9">
         <v>24</v>
       </c>
@@ -6733,7 +6732,7 @@
       <c r="AA25" s="6"/>
       <c r="AB25" s="6"/>
     </row>
-    <row ht="14.25" r="26" spans="1:28">
+    <row r="26" spans="1:28" ht="14.25">
       <c r="A26" s="9">
         <v>25</v>
       </c>
@@ -6777,7 +6776,7 @@
       <c r="AA26" s="6"/>
       <c r="AB26" s="6"/>
     </row>
-    <row ht="14.25" r="27" spans="1:28">
+    <row r="27" spans="1:28" ht="14.25">
       <c r="A27" s="9">
         <v>26</v>
       </c>
@@ -6821,7 +6820,7 @@
       <c r="AA27" s="6"/>
       <c r="AB27" s="6"/>
     </row>
-    <row ht="14.25" r="28" spans="1:28">
+    <row r="28" spans="1:28" ht="14.25">
       <c r="A28" s="9">
         <v>27</v>
       </c>
@@ -6863,7 +6862,7 @@
       <c r="AA28" s="6"/>
       <c r="AB28" s="6"/>
     </row>
-    <row ht="14.25" r="29" spans="1:28">
+    <row r="29" spans="1:28" ht="14.25">
       <c r="A29" s="9">
         <v>28</v>
       </c>
@@ -6907,7 +6906,7 @@
       <c r="AA29" s="6"/>
       <c r="AB29" s="6"/>
     </row>
-    <row ht="14.25" r="30" spans="1:28">
+    <row r="30" spans="1:28" ht="14.25">
       <c r="A30" s="9">
         <v>29</v>
       </c>
@@ -6949,7 +6948,7 @@
       <c r="AA30" s="6"/>
       <c r="AB30" s="6"/>
     </row>
-    <row ht="14.25" r="31" spans="1:28">
+    <row r="31" spans="1:28" ht="14.25">
       <c r="A31" s="4">
         <v>30</v>
       </c>
@@ -6993,7 +6992,7 @@
       <c r="AA31" s="6"/>
       <c r="AB31" s="6"/>
     </row>
-    <row ht="14.25" r="32" spans="1:28">
+    <row r="32" spans="1:28" ht="14.25">
       <c r="A32" s="4">
         <v>31</v>
       </c>
@@ -7035,7 +7034,7 @@
       <c r="AA32" s="6"/>
       <c r="AB32" s="6"/>
     </row>
-    <row customFormat="1" ht="14.25" r="33" s="4" spans="1:8">
+    <row r="33" spans="1:8" s="4" customFormat="1" ht="14.25">
       <c r="A33" s="4">
         <v>32</v>
       </c>
@@ -7058,7 +7057,7 @@
         <v>430</v>
       </c>
     </row>
-    <row customFormat="1" ht="14.25" r="34" s="4" spans="1:8">
+    <row r="34" spans="1:8" s="4" customFormat="1" ht="14.25">
       <c r="A34" s="4">
         <v>33</v>
       </c>
@@ -7078,7 +7077,7 @@
         <v>430</v>
       </c>
     </row>
-    <row customFormat="1" ht="14.25" r="35" s="4" spans="1:8">
+    <row r="35" spans="1:8" s="4" customFormat="1" ht="14.25">
       <c r="A35" s="4">
         <v>34</v>
       </c>
@@ -7098,7 +7097,7 @@
         <v>430</v>
       </c>
     </row>
-    <row customFormat="1" ht="14.25" r="36" s="4" spans="1:8">
+    <row r="36" spans="1:8" s="4" customFormat="1" ht="14.25">
       <c r="A36" s="4">
         <v>35</v>
       </c>
@@ -7118,7 +7117,7 @@
         <v>430</v>
       </c>
     </row>
-    <row customFormat="1" ht="14.25" r="37" s="4" spans="1:8">
+    <row r="37" spans="1:8" s="4" customFormat="1" ht="14.25">
       <c r="A37" s="4">
         <v>36</v>
       </c>
@@ -7138,7 +7137,7 @@
         <v>430</v>
       </c>
     </row>
-    <row customFormat="1" ht="14.25" r="38" s="4" spans="1:8">
+    <row r="38" spans="1:8" s="4" customFormat="1" ht="14.25">
       <c r="A38" s="4">
         <v>37</v>
       </c>
@@ -7161,17 +7160,17 @@
         <v>430</v>
       </c>
     </row>
-    <row customFormat="1" ht="14.25" r="39" s="4" spans="1:8">
+    <row r="39" spans="1:8" s="4" customFormat="1" ht="14.25">
       <c r="A39" s="4">
         <v>38</v>
       </c>
-      <c r="B39" s="4" t="s">
+      <c r="B39" s="39" t="s">
         <v>184</v>
       </c>
       <c r="C39" s="39" t="s">
         <v>730</v>
       </c>
-      <c r="D39" s="4" t="s">
+      <c r="D39" s="41" t="s">
         <v>14</v>
       </c>
       <c r="F39" s="28" t="s">
@@ -7184,7 +7183,7 @@
         <v>430</v>
       </c>
     </row>
-    <row customFormat="1" ht="14.25" r="40" s="4" spans="1:8">
+    <row r="40" spans="1:8" s="4" customFormat="1" ht="14.25">
       <c r="A40" s="4">
         <v>39</v>
       </c>
@@ -7207,7 +7206,7 @@
         <v>430</v>
       </c>
     </row>
-    <row customFormat="1" ht="14.25" r="41" s="4" spans="1:8">
+    <row r="41" spans="1:8" s="4" customFormat="1" ht="14.25">
       <c r="A41" s="4">
         <v>40</v>
       </c>
@@ -7227,7 +7226,7 @@
         <v>430</v>
       </c>
     </row>
-    <row customFormat="1" ht="14.25" r="42" s="4" spans="1:8">
+    <row r="42" spans="1:8" s="4" customFormat="1" ht="14.25">
       <c r="A42" s="4">
         <v>41</v>
       </c>
@@ -7250,7 +7249,7 @@
         <v>430</v>
       </c>
     </row>
-    <row customFormat="1" ht="14.25" r="43" s="4" spans="1:8">
+    <row r="43" spans="1:8" s="4" customFormat="1" ht="14.25">
       <c r="A43" s="4">
         <v>42</v>
       </c>
@@ -7270,7 +7269,7 @@
         <v>430</v>
       </c>
     </row>
-    <row customFormat="1" ht="14.25" r="44" s="4" spans="1:8">
+    <row r="44" spans="1:8" s="4" customFormat="1" ht="14.25">
       <c r="A44" s="4">
         <v>43</v>
       </c>
@@ -7290,7 +7289,7 @@
         <v>430</v>
       </c>
     </row>
-    <row customFormat="1" ht="14.25" r="45" s="4" spans="1:8">
+    <row r="45" spans="1:8" s="4" customFormat="1" ht="14.25">
       <c r="A45" s="4">
         <v>44</v>
       </c>
@@ -7313,7 +7312,7 @@
         <v>38</v>
       </c>
     </row>
-    <row customFormat="1" ht="14.25" r="46" s="4" spans="1:8">
+    <row r="46" spans="1:8" s="4" customFormat="1" ht="14.25">
       <c r="A46" s="4">
         <v>45</v>
       </c>
@@ -7333,7 +7332,7 @@
         <v>38</v>
       </c>
     </row>
-    <row customFormat="1" ht="14.25" r="47" s="4" spans="1:8">
+    <row r="47" spans="1:8" s="4" customFormat="1" ht="14.25">
       <c r="A47" s="4">
         <v>46</v>
       </c>
@@ -7353,7 +7352,7 @@
         <v>38</v>
       </c>
     </row>
-    <row customFormat="1" ht="12.75" r="48" s="4" spans="1:8">
+    <row r="48" spans="1:8" s="4" customFormat="1" ht="12.75">
       <c r="A48" s="4">
         <v>47</v>
       </c>
@@ -7376,7 +7375,7 @@
         <v>431</v>
       </c>
     </row>
-    <row customFormat="1" ht="12.75" r="49" s="4" spans="1:8">
+    <row r="49" spans="1:8" s="4" customFormat="1" ht="12.75">
       <c r="A49" s="4">
         <v>48</v>
       </c>
@@ -7399,7 +7398,7 @@
         <v>431</v>
       </c>
     </row>
-    <row customFormat="1" ht="12.75" r="50" s="4" spans="1:8">
+    <row r="50" spans="1:8" s="4" customFormat="1" ht="12.75">
       <c r="A50" s="4">
         <v>49</v>
       </c>
@@ -7419,7 +7418,7 @@
         <v>431</v>
       </c>
     </row>
-    <row customFormat="1" ht="12.75" r="51" s="4" spans="1:8">
+    <row r="51" spans="1:8" s="4" customFormat="1" ht="12.75">
       <c r="A51" s="4">
         <v>50</v>
       </c>
@@ -7439,7 +7438,7 @@
         <v>431</v>
       </c>
     </row>
-    <row customFormat="1" ht="12.75" r="52" s="4" spans="1:8">
+    <row r="52" spans="1:8" s="4" customFormat="1" ht="12.75">
       <c r="A52" s="4">
         <v>51</v>
       </c>
@@ -7462,7 +7461,7 @@
         <v>431</v>
       </c>
     </row>
-    <row customFormat="1" customHeight="1" ht="15.75" r="53" s="4" spans="1:8">
+    <row r="53" spans="1:8" s="4" customFormat="1" ht="15.75" customHeight="1">
       <c r="A53" s="4">
         <v>52</v>
       </c>
@@ -7485,7 +7484,7 @@
         <v>326</v>
       </c>
     </row>
-    <row customFormat="1" ht="12.75" r="54" s="4" spans="1:8">
+    <row r="54" spans="1:8" s="4" customFormat="1" ht="12.75">
       <c r="A54" s="4">
         <v>53</v>
       </c>
@@ -7505,7 +7504,7 @@
         <v>326</v>
       </c>
     </row>
-    <row customFormat="1" ht="12.75" r="55" s="4" spans="1:8">
+    <row r="55" spans="1:8" s="4" customFormat="1" ht="12.75">
       <c r="A55" s="4">
         <v>54</v>
       </c>
@@ -7528,7 +7527,7 @@
         <v>326</v>
       </c>
     </row>
-    <row customFormat="1" ht="12.75" r="56" s="4" spans="1:8">
+    <row r="56" spans="1:8" s="4" customFormat="1" ht="12.75">
       <c r="A56" s="4">
         <v>55</v>
       </c>
@@ -7551,7 +7550,7 @@
         <v>326</v>
       </c>
     </row>
-    <row customFormat="1" ht="12.75" r="57" s="4" spans="1:8">
+    <row r="57" spans="1:8" s="4" customFormat="1" ht="12.75">
       <c r="A57" s="4">
         <v>56</v>
       </c>
@@ -7571,7 +7570,7 @@
         <v>326</v>
       </c>
     </row>
-    <row customFormat="1" ht="12.75" r="58" s="4" spans="1:8">
+    <row r="58" spans="1:8" s="4" customFormat="1" ht="12.75">
       <c r="A58" s="4">
         <v>57</v>
       </c>
@@ -7591,7 +7590,7 @@
         <v>326</v>
       </c>
     </row>
-    <row customFormat="1" ht="12.75" r="59" s="4" spans="1:8">
+    <row r="59" spans="1:8" s="4" customFormat="1" ht="12.75">
       <c r="A59" s="4">
         <v>58</v>
       </c>
@@ -7611,7 +7610,7 @@
         <v>326</v>
       </c>
     </row>
-    <row customFormat="1" ht="12.75" r="60" s="4" spans="1:8">
+    <row r="60" spans="1:8" s="4" customFormat="1" ht="12.75">
       <c r="A60" s="4">
         <v>59</v>
       </c>
@@ -7631,7 +7630,7 @@
         <v>326</v>
       </c>
     </row>
-    <row customFormat="1" ht="12.75" r="61" s="4" spans="1:8">
+    <row r="61" spans="1:8" s="4" customFormat="1" ht="12.75">
       <c r="A61" s="4">
         <v>60</v>
       </c>
@@ -7651,7 +7650,7 @@
         <v>326</v>
       </c>
     </row>
-    <row customFormat="1" ht="12.75" r="62" s="4" spans="1:8">
+    <row r="62" spans="1:8" s="4" customFormat="1" ht="12.75">
       <c r="A62" s="4">
         <v>61</v>
       </c>
@@ -7671,7 +7670,7 @@
         <v>430</v>
       </c>
     </row>
-    <row customFormat="1" ht="12.75" r="63" s="4" spans="1:8">
+    <row r="63" spans="1:8" s="4" customFormat="1" ht="12.75">
       <c r="A63" s="4">
         <v>62</v>
       </c>
@@ -7694,7 +7693,7 @@
         <v>430</v>
       </c>
     </row>
-    <row customFormat="1" ht="12.75" r="64" s="4" spans="1:8">
+    <row r="64" spans="1:8" s="4" customFormat="1" ht="12.75">
       <c r="A64" s="4">
         <v>63</v>
       </c>
@@ -7717,7 +7716,7 @@
         <v>430</v>
       </c>
     </row>
-    <row customFormat="1" ht="12.75" r="65" s="4" spans="1:8">
+    <row r="65" spans="1:8" s="4" customFormat="1" ht="12.75">
       <c r="A65" s="4">
         <v>64</v>
       </c>
@@ -7738,7 +7737,7 @@
         <v>430</v>
       </c>
     </row>
-    <row customFormat="1" ht="12.75" r="66" s="4" spans="1:8">
+    <row r="66" spans="1:8" s="4" customFormat="1" ht="12.75">
       <c r="A66" s="4">
         <v>65</v>
       </c>
@@ -7761,7 +7760,7 @@
         <v>38</v>
       </c>
     </row>
-    <row customFormat="1" ht="12.75" r="67" s="4" spans="1:8">
+    <row r="67" spans="1:8" s="4" customFormat="1" ht="12.75">
       <c r="A67" s="4">
         <v>66</v>
       </c>
@@ -7784,7 +7783,7 @@
         <v>431</v>
       </c>
     </row>
-    <row customFormat="1" ht="12.75" r="68" s="4" spans="1:8">
+    <row r="68" spans="1:8" s="4" customFormat="1" ht="12.75">
       <c r="A68" s="4">
         <v>67</v>
       </c>
@@ -7807,7 +7806,7 @@
         <v>430</v>
       </c>
     </row>
-    <row customFormat="1" ht="12.75" r="69" s="4" spans="1:8">
+    <row r="69" spans="1:8" s="4" customFormat="1" ht="12.75">
       <c r="A69" s="4">
         <v>68</v>
       </c>
@@ -7830,7 +7829,7 @@
         <v>430</v>
       </c>
     </row>
-    <row customFormat="1" ht="12.75" r="70" s="4" spans="1:8">
+    <row r="70" spans="1:8" s="4" customFormat="1" ht="12.75">
       <c r="A70" s="4">
         <v>69</v>
       </c>
@@ -7853,7 +7852,7 @@
         <v>430</v>
       </c>
     </row>
-    <row customFormat="1" ht="12.75" r="71" s="4" spans="1:8">
+    <row r="71" spans="1:8" s="4" customFormat="1" ht="12.75">
       <c r="A71" s="4">
         <v>70</v>
       </c>
@@ -7876,7 +7875,7 @@
         <v>430</v>
       </c>
     </row>
-    <row customFormat="1" ht="12.75" r="72" s="4" spans="1:8">
+    <row r="72" spans="1:8" s="4" customFormat="1" ht="12.75">
       <c r="A72" s="4">
         <v>71</v>
       </c>
@@ -7899,7 +7898,7 @@
         <v>430</v>
       </c>
     </row>
-    <row ht="12.75" r="73" spans="1:8">
+    <row r="73" spans="1:8" ht="12.75">
       <c r="A73">
         <v>72</v>
       </c>
@@ -7922,7 +7921,7 @@
         <v>431</v>
       </c>
     </row>
-    <row ht="12.75" r="74" spans="1:8">
+    <row r="74" spans="1:8" ht="12.75">
       <c r="A74">
         <v>73</v>
       </c>
@@ -7945,7 +7944,7 @@
         <v>431</v>
       </c>
     </row>
-    <row customFormat="1" ht="12.75" r="75" s="4" spans="1:8">
+    <row r="75" spans="1:8" s="4" customFormat="1" ht="12.75">
       <c r="A75" s="4">
         <v>74</v>
       </c>
@@ -7968,7 +7967,7 @@
         <v>431</v>
       </c>
     </row>
-    <row ht="12.75" r="76" spans="1:8">
+    <row r="76" spans="1:8" ht="12.75">
       <c r="A76">
         <v>75</v>
       </c>
@@ -7991,7 +7990,7 @@
         <v>431</v>
       </c>
     </row>
-    <row ht="12.75" r="77" spans="1:8">
+    <row r="77" spans="1:8" ht="12.75">
       <c r="A77">
         <v>76</v>
       </c>
@@ -8014,7 +8013,7 @@
         <v>431</v>
       </c>
     </row>
-    <row ht="12.75" r="78" spans="1:8">
+    <row r="78" spans="1:8" ht="12.75">
       <c r="A78">
         <v>77</v>
       </c>
@@ -8037,7 +8036,7 @@
         <v>431</v>
       </c>
     </row>
-    <row ht="12.75" r="79" spans="1:8">
+    <row r="79" spans="1:8" ht="12.75">
       <c r="A79">
         <v>78</v>
       </c>
@@ -8060,7 +8059,7 @@
         <v>431</v>
       </c>
     </row>
-    <row ht="12.75" r="80" spans="1:8">
+    <row r="80" spans="1:8" ht="12.75">
       <c r="A80">
         <v>79</v>
       </c>
@@ -8083,7 +8082,7 @@
         <v>431</v>
       </c>
     </row>
-    <row ht="12.75" r="81" spans="1:8">
+    <row r="81" spans="1:8" ht="12.75">
       <c r="A81">
         <v>80</v>
       </c>
@@ -8106,7 +8105,7 @@
         <v>431</v>
       </c>
     </row>
-    <row ht="12.75" r="82" spans="1:8">
+    <row r="82" spans="1:8" ht="12.75">
       <c r="A82">
         <v>81</v>
       </c>
@@ -8129,7 +8128,7 @@
         <v>431</v>
       </c>
     </row>
-    <row ht="12.75" r="83" spans="1:8">
+    <row r="83" spans="1:8" ht="12.75">
       <c r="A83">
         <v>82</v>
       </c>
@@ -8152,7 +8151,7 @@
         <v>431</v>
       </c>
     </row>
-    <row ht="12.75" r="84" spans="1:8">
+    <row r="84" spans="1:8" ht="12.75">
       <c r="A84">
         <v>83</v>
       </c>
@@ -8175,7 +8174,7 @@
         <v>431</v>
       </c>
     </row>
-    <row ht="12.75" r="85" spans="1:8">
+    <row r="85" spans="1:8" ht="12.75">
       <c r="A85">
         <v>84</v>
       </c>
@@ -8198,7 +8197,7 @@
         <v>431</v>
       </c>
     </row>
-    <row customFormat="1" ht="12.75" r="86" s="4" spans="1:8">
+    <row r="86" spans="1:8" s="4" customFormat="1" ht="12.75">
       <c r="A86" s="4">
         <v>85</v>
       </c>
@@ -8221,7 +8220,7 @@
         <v>430</v>
       </c>
     </row>
-    <row customFormat="1" ht="12.75" r="87" s="4" spans="1:8">
+    <row r="87" spans="1:8" s="4" customFormat="1" ht="12.75">
       <c r="A87" s="4">
         <v>86</v>
       </c>
@@ -8244,7 +8243,7 @@
         <v>38</v>
       </c>
     </row>
-    <row ht="12.75" r="88" spans="1:8">
+    <row r="88" spans="1:8" ht="12.75">
       <c r="A88">
         <v>87</v>
       </c>
@@ -8267,7 +8266,7 @@
         <v>38</v>
       </c>
     </row>
-    <row ht="12.75" r="89" spans="1:8">
+    <row r="89" spans="1:8" ht="12.75">
       <c r="A89">
         <v>88</v>
       </c>
@@ -8290,7 +8289,7 @@
         <v>38</v>
       </c>
     </row>
-    <row ht="12.75" r="90" spans="1:8">
+    <row r="90" spans="1:8" ht="12.75">
       <c r="A90">
         <v>89</v>
       </c>
@@ -8313,7 +8312,7 @@
         <v>431</v>
       </c>
     </row>
-    <row ht="12.75" r="91" spans="1:8">
+    <row r="91" spans="1:8" ht="12.75">
       <c r="A91">
         <v>90</v>
       </c>
@@ -8336,7 +8335,7 @@
         <v>431</v>
       </c>
     </row>
-    <row ht="12.75" r="92" spans="1:8">
+    <row r="92" spans="1:8" ht="12.75">
       <c r="A92">
         <v>91</v>
       </c>
@@ -8359,7 +8358,7 @@
         <v>431</v>
       </c>
     </row>
-    <row ht="12.75" r="93" spans="1:8">
+    <row r="93" spans="1:8" ht="12.75">
       <c r="A93">
         <v>92</v>
       </c>
@@ -8382,7 +8381,7 @@
         <v>431</v>
       </c>
     </row>
-    <row ht="12.75" r="94" spans="1:8">
+    <row r="94" spans="1:8" ht="12.75">
       <c r="A94">
         <v>93</v>
       </c>
@@ -8405,7 +8404,7 @@
         <v>430</v>
       </c>
     </row>
-    <row ht="12.75" r="95" spans="1:8">
+    <row r="95" spans="1:8" ht="12.75">
       <c r="A95">
         <v>94</v>
       </c>
@@ -8428,7 +8427,7 @@
         <v>430</v>
       </c>
     </row>
-    <row ht="12.75" r="96" spans="1:8">
+    <row r="96" spans="1:8" ht="12.75">
       <c r="A96">
         <v>95</v>
       </c>
@@ -8451,7 +8450,7 @@
         <v>430</v>
       </c>
     </row>
-    <row ht="12.75" r="97" spans="1:8">
+    <row r="97" spans="1:8" ht="12.75">
       <c r="A97">
         <v>96</v>
       </c>
@@ -8474,7 +8473,7 @@
         <v>38</v>
       </c>
     </row>
-    <row ht="12.75" r="98" spans="1:8">
+    <row r="98" spans="1:8" ht="12.75">
       <c r="A98">
         <v>97</v>
       </c>
@@ -8497,7 +8496,7 @@
         <v>431</v>
       </c>
     </row>
-    <row ht="12.75" r="99" spans="1:8">
+    <row r="99" spans="1:8" ht="12.75">
       <c r="A99">
         <v>98</v>
       </c>
@@ -8507,8 +8506,8 @@
       <c r="C99" s="42" t="s">
         <v>721</v>
       </c>
-      <c r="D99" s="4" t="s">
-        <v>7</v>
+      <c r="D99" s="40" t="s">
+        <v>14</v>
       </c>
       <c r="F99" s="2" t="s">
         <v>691</v>
@@ -8520,7 +8519,7 @@
         <v>430</v>
       </c>
     </row>
-    <row ht="12.75" r="100" spans="1:8">
+    <row r="100" spans="1:8" ht="12.75">
       <c r="A100">
         <v>99</v>
       </c>
@@ -8543,7 +8542,7 @@
         <v>38</v>
       </c>
     </row>
-    <row ht="12.75" r="101" spans="1:8">
+    <row r="101" spans="1:8" ht="12.75">
       <c r="A101">
         <v>100</v>
       </c>
@@ -8566,7 +8565,7 @@
         <v>431</v>
       </c>
     </row>
-    <row ht="12.75" r="102" spans="1:8">
+    <row r="102" spans="1:8" ht="12.75">
       <c r="A102">
         <v>101</v>
       </c>
@@ -8589,7 +8588,7 @@
         <v>38</v>
       </c>
     </row>
-    <row ht="12.75" r="103" spans="1:8">
+    <row r="103" spans="1:8" ht="12.75">
       <c r="A103">
         <v>102</v>
       </c>
@@ -8612,17 +8611,17 @@
         <v>431</v>
       </c>
     </row>
-    <row ht="12.75" r="104" spans="1:8">
+    <row r="104" spans="1:8" ht="12.75">
       <c r="A104">
         <v>103</v>
       </c>
-      <c r="B104" t="s">
+      <c r="B104" s="42" t="s">
         <v>764</v>
       </c>
       <c r="C104" s="42" t="s">
         <v>770</v>
       </c>
-      <c r="D104" s="4" t="s">
+      <c r="D104" s="40" t="s">
         <v>14</v>
       </c>
       <c r="F104" s="2" t="s">
@@ -8635,18 +8634,18 @@
         <v>38</v>
       </c>
     </row>
-    <row ht="12.75" r="105" spans="1:8">
+    <row r="105" spans="1:8" ht="12.75">
       <c r="A105">
         <v>104</v>
       </c>
       <c r="B105" s="42" t="s">
         <v>771</v>
       </c>
-      <c r="C105" t="s">
+      <c r="C105" s="42" t="s">
         <v>787</v>
       </c>
-      <c r="D105" s="4" t="s">
-        <v>7</v>
+      <c r="D105" s="40" t="s">
+        <v>14</v>
       </c>
       <c r="F105" s="2" t="s">
         <v>691</v>
@@ -8658,7 +8657,7 @@
         <v>38</v>
       </c>
     </row>
-    <row ht="12.75" r="106" spans="1:8">
+    <row r="106" spans="1:8" ht="12.75">
       <c r="A106">
         <v>105</v>
       </c>
@@ -8681,7 +8680,7 @@
         <v>38</v>
       </c>
     </row>
-    <row ht="12.75" r="107" spans="1:8">
+    <row r="107" spans="1:8" ht="12.75">
       <c r="A107">
         <v>106</v>
       </c>
@@ -8704,14 +8703,14 @@
         <v>430</v>
       </c>
     </row>
-    <row ht="12.75" r="108" spans="1:8">
+    <row r="108" spans="1:8" ht="12.75">
       <c r="A108">
         <v>107</v>
       </c>
       <c r="B108" s="42" t="s">
         <v>790</v>
       </c>
-      <c r="C108" t="s">
+      <c r="C108" s="42" t="s">
         <v>803</v>
       </c>
       <c r="D108" s="40" t="s">
@@ -8727,17 +8726,17 @@
         <v>38</v>
       </c>
     </row>
-    <row ht="12.75" r="109" spans="1:8">
+    <row r="109" spans="1:8" ht="12.75">
       <c r="A109">
         <v>108</v>
       </c>
-      <c r="B109" t="s">
+      <c r="B109" s="42" t="s">
         <v>804</v>
       </c>
-      <c r="C109" t="s">
+      <c r="C109" s="42" t="s">
         <v>808</v>
       </c>
-      <c r="D109" s="4" t="s">
+      <c r="D109" s="40" t="s">
         <v>14</v>
       </c>
       <c r="F109" s="2" t="s">
@@ -8750,7 +8749,7 @@
         <v>38</v>
       </c>
     </row>
-    <row ht="12.75" r="110" spans="1:8">
+    <row r="110" spans="1:8" ht="12.75">
       <c r="A110">
         <v>109</v>
       </c>
@@ -8773,7 +8772,7 @@
         <v>431</v>
       </c>
     </row>
-    <row ht="12.75" r="111" spans="1:8">
+    <row r="111" spans="1:8" ht="12.75">
       <c r="A111">
         <v>110</v>
       </c>
@@ -8796,7 +8795,7 @@
         <v>431</v>
       </c>
     </row>
-    <row ht="12.75" r="112" spans="1:8">
+    <row r="112" spans="1:8" ht="12.75">
       <c r="A112">
         <v>111</v>
       </c>
@@ -8819,7 +8818,7 @@
         <v>431</v>
       </c>
     </row>
-    <row ht="12.75" r="113" spans="1:8">
+    <row r="113" spans="1:8" ht="12.75">
       <c r="A113">
         <v>112</v>
       </c>
@@ -8842,7 +8841,7 @@
         <v>431</v>
       </c>
     </row>
-    <row ht="12.75" r="114" spans="1:8">
+    <row r="114" spans="1:8" ht="12.75">
       <c r="A114">
         <v>113</v>
       </c>
@@ -8865,7 +8864,7 @@
         <v>430</v>
       </c>
     </row>
-    <row ht="12.75" r="115" spans="1:8">
+    <row r="115" spans="1:8" ht="12.75">
       <c r="A115">
         <v>114</v>
       </c>
@@ -8888,7 +8887,7 @@
         <v>326</v>
       </c>
     </row>
-    <row ht="12.75" r="116" spans="1:8">
+    <row r="116" spans="1:8" ht="12.75">
       <c r="A116">
         <v>115</v>
       </c>
@@ -8911,7 +8910,7 @@
         <v>430</v>
       </c>
     </row>
-    <row ht="12.75" r="117" spans="1:8">
+    <row r="117" spans="1:8" ht="12.75">
       <c r="A117">
         <v>116</v>
       </c>
@@ -8934,7 +8933,7 @@
         <v>431</v>
       </c>
     </row>
-    <row ht="12.75" r="118" spans="1:8">
+    <row r="118" spans="1:8" ht="12.75">
       <c r="A118">
         <v>117</v>
       </c>
@@ -8954,7 +8953,7 @@
         <v>38</v>
       </c>
     </row>
-    <row ht="12.75" r="119" spans="1:8">
+    <row r="119" spans="1:8" ht="12.75">
       <c r="A119">
         <v>118</v>
       </c>
@@ -8977,7 +8976,7 @@
         <v>431</v>
       </c>
     </row>
-    <row customHeight="1" ht="15.75" r="120" spans="1:8">
+    <row r="120" spans="1:8" ht="15.75" customHeight="1">
       <c r="A120">
         <v>119</v>
       </c>
@@ -9000,7 +8999,7 @@
         <v>887</v>
       </c>
     </row>
-    <row ht="12.75" r="121" spans="1:8">
+    <row r="121" spans="1:8" ht="12.75">
       <c r="A121">
         <v>120</v>
       </c>
@@ -9023,7 +9022,7 @@
         <v>887</v>
       </c>
     </row>
-    <row ht="12.75" r="122" spans="1:8">
+    <row r="122" spans="1:8" ht="12.75">
       <c r="A122">
         <v>121</v>
       </c>
@@ -9046,7 +9045,7 @@
         <v>887</v>
       </c>
     </row>
-    <row ht="12.75" r="123" spans="1:8">
+    <row r="123" spans="1:8" ht="12.75">
       <c r="A123">
         <v>122</v>
       </c>
@@ -9069,7 +9068,7 @@
         <v>887</v>
       </c>
     </row>
-    <row ht="12.75" r="124" spans="1:8">
+    <row r="124" spans="1:8" ht="12.75">
       <c r="A124">
         <v>123</v>
       </c>
@@ -9092,7 +9091,7 @@
         <v>887</v>
       </c>
     </row>
-    <row ht="12.75" r="125" spans="1:8">
+    <row r="125" spans="1:8" ht="12.75">
       <c r="A125">
         <v>124</v>
       </c>
@@ -9115,7 +9114,7 @@
         <v>887</v>
       </c>
     </row>
-    <row ht="12.75" r="126" spans="1:8">
+    <row r="126" spans="1:8" ht="12.75">
       <c r="A126">
         <v>125</v>
       </c>
@@ -9138,7 +9137,7 @@
         <v>887</v>
       </c>
     </row>
-    <row ht="12.75" r="127" spans="1:8">
+    <row r="127" spans="1:8" ht="12.75">
       <c r="A127">
         <v>126</v>
       </c>
@@ -9161,7 +9160,7 @@
         <v>887</v>
       </c>
     </row>
-    <row ht="12.75" r="128" spans="1:8">
+    <row r="128" spans="1:8" ht="12.75">
       <c r="A128">
         <v>127</v>
       </c>
@@ -9184,7 +9183,7 @@
         <v>887</v>
       </c>
     </row>
-    <row ht="12.75" r="129" spans="1:8">
+    <row r="129" spans="1:8" ht="12.75">
       <c r="A129">
         <v>128</v>
       </c>
@@ -9207,7 +9206,7 @@
         <v>887</v>
       </c>
     </row>
-    <row ht="12.75" r="130" spans="1:8">
+    <row r="130" spans="1:8" ht="12.75">
       <c r="A130">
         <v>129</v>
       </c>
@@ -9230,7 +9229,7 @@
         <v>887</v>
       </c>
     </row>
-    <row ht="12.75" r="131" spans="1:8">
+    <row r="131" spans="1:8" ht="12.75">
       <c r="A131">
         <v>130</v>
       </c>
@@ -9253,7 +9252,7 @@
         <v>887</v>
       </c>
     </row>
-    <row ht="12.75" r="132" spans="1:8">
+    <row r="132" spans="1:8" ht="12.75">
       <c r="A132">
         <v>131</v>
       </c>
@@ -9276,7 +9275,7 @@
         <v>887</v>
       </c>
     </row>
-    <row ht="12.75" r="133" spans="1:8">
+    <row r="133" spans="1:8" ht="12.75">
       <c r="A133">
         <v>132</v>
       </c>
@@ -9299,7 +9298,7 @@
         <v>887</v>
       </c>
     </row>
-    <row ht="12.75" r="134" spans="1:8">
+    <row r="134" spans="1:8" ht="12.75">
       <c r="A134">
         <v>133</v>
       </c>
@@ -9322,7 +9321,7 @@
         <v>887</v>
       </c>
     </row>
-    <row ht="12.75" r="135" spans="1:8">
+    <row r="135" spans="1:8" ht="12.75">
       <c r="A135">
         <v>134</v>
       </c>
@@ -9345,7 +9344,7 @@
         <v>887</v>
       </c>
     </row>
-    <row ht="12.75" r="136" spans="1:8">
+    <row r="136" spans="1:8" ht="12.75">
       <c r="A136">
         <v>135</v>
       </c>
@@ -9368,7 +9367,7 @@
         <v>887</v>
       </c>
     </row>
-    <row ht="12.75" r="137" spans="1:8">
+    <row r="137" spans="1:8" ht="12.75">
       <c r="A137">
         <v>136</v>
       </c>
@@ -9391,7 +9390,7 @@
         <v>887</v>
       </c>
     </row>
-    <row ht="12.75" r="138" spans="1:8">
+    <row r="138" spans="1:8" ht="12.75">
       <c r="A138">
         <v>137</v>
       </c>
@@ -9414,7 +9413,7 @@
         <v>887</v>
       </c>
     </row>
-    <row ht="12.75" r="139" spans="1:8">
+    <row r="139" spans="1:8" ht="12.75">
       <c r="A139">
         <v>138</v>
       </c>
@@ -9437,7 +9436,7 @@
         <v>887</v>
       </c>
     </row>
-    <row ht="12.75" r="140" spans="1:8">
+    <row r="140" spans="1:8" ht="12.75">
       <c r="A140">
         <v>139</v>
       </c>
@@ -9460,7 +9459,7 @@
         <v>887</v>
       </c>
     </row>
-    <row ht="12.75" r="141" spans="1:8">
+    <row r="141" spans="1:8" ht="12.75">
       <c r="A141">
         <v>140</v>
       </c>
@@ -9483,7 +9482,7 @@
         <v>887</v>
       </c>
     </row>
-    <row ht="12.75" r="142" spans="1:8">
+    <row r="142" spans="1:8" ht="12.75">
       <c r="A142">
         <v>141</v>
       </c>
@@ -9503,7 +9502,7 @@
         <v>887</v>
       </c>
     </row>
-    <row ht="12.75" r="143" spans="1:8">
+    <row r="143" spans="1:8" ht="12.75">
       <c r="A143">
         <v>142</v>
       </c>
@@ -9525,198 +9524,204 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink r:id="rId1" ref="B2" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
-    <hyperlink r:id="rId2" ref="B3" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
-    <hyperlink r:id="rId3" ref="B4" xr:uid="{00000000-0004-0000-0000-000002000000}"/>
-    <hyperlink r:id="rId4" ref="B5" xr:uid="{00000000-0004-0000-0000-000003000000}"/>
-    <hyperlink r:id="rId5" ref="B6" xr:uid="{00000000-0004-0000-0000-000004000000}"/>
-    <hyperlink r:id="rId6" ref="H6" xr:uid="{00000000-0004-0000-0000-000005000000}"/>
-    <hyperlink r:id="rId7" ref="B7" xr:uid="{00000000-0004-0000-0000-000006000000}"/>
-    <hyperlink r:id="rId8" ref="B8" xr:uid="{00000000-0004-0000-0000-000007000000}"/>
-    <hyperlink r:id="rId9" ref="B9" xr:uid="{00000000-0004-0000-0000-000008000000}"/>
-    <hyperlink r:id="rId10" ref="B10" xr:uid="{00000000-0004-0000-0000-000009000000}"/>
-    <hyperlink r:id="rId11" ref="B11" xr:uid="{00000000-0004-0000-0000-00000A000000}"/>
-    <hyperlink r:id="rId12" ref="B12" xr:uid="{00000000-0004-0000-0000-00000B000000}"/>
-    <hyperlink r:id="rId13" ref="B13" xr:uid="{00000000-0004-0000-0000-00000C000000}"/>
-    <hyperlink r:id="rId14" ref="B14" xr:uid="{00000000-0004-0000-0000-00000D000000}"/>
-    <hyperlink r:id="rId15" ref="B15" xr:uid="{00000000-0004-0000-0000-00000E000000}"/>
-    <hyperlink r:id="rId16" ref="B16" xr:uid="{00000000-0004-0000-0000-00000F000000}"/>
-    <hyperlink r:id="rId17" ref="B17" xr:uid="{00000000-0004-0000-0000-000010000000}"/>
-    <hyperlink r:id="rId18" ref="B18" xr:uid="{00000000-0004-0000-0000-000011000000}"/>
-    <hyperlink r:id="rId19" ref="B19" xr:uid="{00000000-0004-0000-0000-000012000000}"/>
-    <hyperlink r:id="rId20" ref="B20" xr:uid="{00000000-0004-0000-0000-000013000000}"/>
-    <hyperlink r:id="rId21" ref="B21" xr:uid="{00000000-0004-0000-0000-000014000000}"/>
-    <hyperlink r:id="rId22" ref="B22" xr:uid="{00000000-0004-0000-0000-000015000000}"/>
-    <hyperlink r:id="rId23" ref="B23" xr:uid="{00000000-0004-0000-0000-000016000000}"/>
-    <hyperlink r:id="rId24" ref="B24" xr:uid="{00000000-0004-0000-0000-000017000000}"/>
-    <hyperlink r:id="rId25" ref="B25" xr:uid="{00000000-0004-0000-0000-000018000000}"/>
-    <hyperlink r:id="rId26" ref="H25" xr:uid="{00000000-0004-0000-0000-000019000000}"/>
-    <hyperlink r:id="rId27" ref="B26" xr:uid="{00000000-0004-0000-0000-00001A000000}"/>
-    <hyperlink r:id="rId28" ref="H26" xr:uid="{00000000-0004-0000-0000-00001B000000}"/>
-    <hyperlink r:id="rId29" ref="B27" xr:uid="{00000000-0004-0000-0000-00001C000000}"/>
-    <hyperlink r:id="rId30" ref="H27" xr:uid="{00000000-0004-0000-0000-00001D000000}"/>
-    <hyperlink r:id="rId31" ref="B28" xr:uid="{00000000-0004-0000-0000-00001E000000}"/>
-    <hyperlink r:id="rId32" ref="H28" xr:uid="{00000000-0004-0000-0000-00001F000000}"/>
-    <hyperlink r:id="rId33" ref="B29" xr:uid="{00000000-0004-0000-0000-000020000000}"/>
-    <hyperlink r:id="rId34" ref="H29" xr:uid="{00000000-0004-0000-0000-000021000000}"/>
-    <hyperlink r:id="rId35" ref="B30" xr:uid="{00000000-0004-0000-0000-000022000000}"/>
-    <hyperlink r:id="rId36" ref="H30" xr:uid="{00000000-0004-0000-0000-000023000000}"/>
-    <hyperlink r:id="rId37" ref="B31" xr:uid="{00000000-0004-0000-0000-000024000000}"/>
-    <hyperlink r:id="rId38" ref="H31" xr:uid="{00000000-0004-0000-0000-000025000000}"/>
-    <hyperlink r:id="rId39" ref="B32" xr:uid="{00000000-0004-0000-0000-000026000000}"/>
-    <hyperlink r:id="rId40" ref="H32" xr:uid="{00000000-0004-0000-0000-000027000000}"/>
-    <hyperlink r:id="rId41" ref="B33" xr:uid="{00000000-0004-0000-0000-000028000000}"/>
-    <hyperlink r:id="rId42" ref="B34" xr:uid="{00000000-0004-0000-0000-000029000000}"/>
-    <hyperlink r:id="rId43" ref="B38" xr:uid="{00000000-0004-0000-0000-00002A000000}"/>
-    <hyperlink r:id="rId44" ref="B45" xr:uid="{00000000-0004-0000-0000-00002B000000}"/>
-    <hyperlink r:id="rId45" ref="B48" xr:uid="{00000000-0004-0000-0000-00002C000000}"/>
-    <hyperlink r:id="rId46" ref="B35" xr:uid="{00000000-0004-0000-0000-00002D000000}"/>
-    <hyperlink r:id="rId47" ref="B52" xr:uid="{00000000-0004-0000-0000-00002E000000}"/>
-    <hyperlink r:id="rId48" ref="B53" xr:uid="{00000000-0004-0000-0000-00002F000000}"/>
-    <hyperlink r:id="rId49" ref="B55" xr:uid="{00000000-0004-0000-0000-000030000000}"/>
-    <hyperlink r:id="rId50" ref="B56" xr:uid="{00000000-0004-0000-0000-000031000000}"/>
-    <hyperlink r:id="rId51" ref="B57" xr:uid="{00000000-0004-0000-0000-000032000000}"/>
-    <hyperlink r:id="rId52" ref="B58" xr:uid="{00000000-0004-0000-0000-000033000000}"/>
-    <hyperlink r:id="rId53" ref="B61" xr:uid="{00000000-0004-0000-0000-000034000000}"/>
-    <hyperlink r:id="rId54" ref="B62" xr:uid="{00000000-0004-0000-0000-000035000000}"/>
-    <hyperlink r:id="rId55" ref="B63" xr:uid="{00000000-0004-0000-0000-000036000000}"/>
-    <hyperlink r:id="rId56" ref="B64" xr:uid="{00000000-0004-0000-0000-000037000000}"/>
-    <hyperlink r:id="rId57" ref="B65" xr:uid="{00000000-0004-0000-0000-000038000000}"/>
-    <hyperlink r:id="rId58" ref="B66" xr:uid="{00000000-0004-0000-0000-000039000000}"/>
-    <hyperlink r:id="rId59" ref="B67" xr:uid="{00000000-0004-0000-0000-00003A000000}"/>
-    <hyperlink display="https://www.allhomes.com.au/agency/trusted-realtors-570129/" r:id="rId60" ref="H7:H24" xr:uid="{00000000-0004-0000-0000-00003B000000}"/>
-    <hyperlink r:id="rId61" ref="B43" xr:uid="{00000000-0004-0000-0000-00003C000000}"/>
-    <hyperlink r:id="rId62" ref="B44" xr:uid="{00000000-0004-0000-0000-00003D000000}"/>
-    <hyperlink r:id="rId63" ref="B46" xr:uid="{00000000-0004-0000-0000-00003E000000}"/>
-    <hyperlink r:id="rId64" ref="B54" xr:uid="{00000000-0004-0000-0000-00003F000000}"/>
-    <hyperlink r:id="rId65" ref="B42" xr:uid="{00000000-0004-0000-0000-000040000000}"/>
-    <hyperlink r:id="rId66" ref="J2" xr:uid="{00000000-0004-0000-0000-000041000000}"/>
-    <hyperlink r:id="rId67" ref="C69" xr:uid="{9DAE03A7-93E8-4507-BD6C-AC4013ECD47F}"/>
-    <hyperlink r:id="rId68" ref="C68" xr:uid="{66B9A9CA-DF82-46B6-9C5A-C5709E2FF1AE}"/>
-    <hyperlink r:id="rId69" ref="B75" xr:uid="{57E7BFEF-6F05-4DA9-A3DE-5B0A0EFED4D9}"/>
-    <hyperlink r:id="rId70" ref="C75" xr:uid="{F4755F93-6E59-4C38-BF66-16746869FDF3}"/>
-    <hyperlink r:id="rId71" ref="H75" xr:uid="{5BFAFD71-42C4-487F-B5E7-1697975992B4}"/>
-    <hyperlink r:id="rId72" ref="B78" xr:uid="{D3DE0D76-2479-4283-B7C7-F11B85797022}"/>
-    <hyperlink r:id="rId73" ref="C78" xr:uid="{FC1D9146-2FDC-4F13-A3C3-51CAB46DEC08}"/>
-    <hyperlink r:id="rId74" ref="B68" xr:uid="{3ED6FAA1-2B0F-4DB9-878E-9640A9C2850D}"/>
-    <hyperlink r:id="rId75" ref="B69" xr:uid="{12DE6CA8-DDC5-4E7B-BD2E-14B105A0DE3B}"/>
-    <hyperlink r:id="rId76" ref="C70" xr:uid="{0419758C-286A-4B76-B8B2-31CC336DEDF1}"/>
-    <hyperlink r:id="rId77" ref="B70" xr:uid="{AC18D1D2-FA3D-4352-A402-35B7AAFE27C0}"/>
-    <hyperlink r:id="rId78" ref="B71" xr:uid="{E8BCA1EF-4E17-4AA7-A2CE-5674FC05ABC3}"/>
-    <hyperlink r:id="rId79" ref="C71" xr:uid="{949AE606-DF4A-48F4-93A0-F148D80842CB}"/>
-    <hyperlink r:id="rId80" ref="B72" xr:uid="{69A93BB5-0295-46D6-8334-45444356E6E9}"/>
-    <hyperlink r:id="rId81" ref="C72" xr:uid="{CA171BC7-126F-4175-8A03-123D5A2C2D8A}"/>
-    <hyperlink r:id="rId82" ref="C73" xr:uid="{FACC205D-E563-4266-8E0D-0794F3D76E98}"/>
-    <hyperlink r:id="rId83" ref="B85" xr:uid="{7ABCABC0-A765-435B-AE52-9D27F653E00F}"/>
-    <hyperlink r:id="rId84" ref="C4" xr:uid="{2CD58DBE-98E3-4EDC-898F-088D5F0FCB81}"/>
-    <hyperlink r:id="rId85" ref="C29" xr:uid="{CB7CAD83-ACA3-4309-B102-B0F536FC97E6}"/>
-    <hyperlink r:id="rId86" ref="C90" xr:uid="{B4F55488-2B40-4078-ABF0-4B4254363237}"/>
-    <hyperlink r:id="rId87" ref="B90" xr:uid="{09FEE7FE-E667-40E8-BC22-3FDC999B614F}"/>
-    <hyperlink r:id="rId88" ref="C15" xr:uid="{34F25BA9-B460-46CF-85C0-4AC9D6288B41}"/>
-    <hyperlink r:id="rId89" ref="C3" xr:uid="{EBAAEE7A-83B2-457B-8600-89427BF11448}"/>
-    <hyperlink r:id="rId90" ref="C8" xr:uid="{3D3D678C-8F1B-47BC-ACA2-D1CBF5A76F0B}"/>
-    <hyperlink r:id="rId91" ref="C19" xr:uid="{ED2C9A9B-3440-4B4A-91A1-7CAF84972535}"/>
-    <hyperlink r:id="rId92" ref="C20" xr:uid="{E47C999F-11AE-4F93-9032-6E51EB582635}"/>
-    <hyperlink r:id="rId93" ref="C21" xr:uid="{E59411CC-EC13-4665-969A-8D9238CCD0C2}"/>
-    <hyperlink r:id="rId94" ref="C33" xr:uid="{9C953AB9-0076-4477-B52F-C393846B1211}"/>
-    <hyperlink r:id="rId95" ref="C38" xr:uid="{D349EA20-36BF-44C7-A16B-E85B8FE53B2A}"/>
-    <hyperlink r:id="rId96" ref="C39" xr:uid="{DE18DA3B-1A3D-4613-888E-7F506CC87091}"/>
-    <hyperlink r:id="rId97" ref="C40" xr:uid="{0C71282B-049B-4CD1-A090-B66647F2B29B}"/>
-    <hyperlink r:id="rId98" ref="C42" xr:uid="{AD0DC851-DEC5-4ACE-B928-50149068BB70}"/>
-    <hyperlink r:id="rId99" ref="C45" xr:uid="{EB51DFC2-D28F-4E0C-B019-F9954D6C9832}"/>
-    <hyperlink r:id="rId100" ref="C52" xr:uid="{9E5146F6-8EC8-4A2C-B192-C1CCB11CAB8A}"/>
-    <hyperlink r:id="rId101" ref="C48" xr:uid="{31B308E4-DA3E-401B-B796-7D03404228FB}"/>
-    <hyperlink r:id="rId102" ref="C49" xr:uid="{EBAAB9CE-7F91-4628-AF75-32C4EEF948C2}"/>
-    <hyperlink r:id="rId103" ref="C53" xr:uid="{2FF7EB1F-CD56-4E71-AD0F-0D12E8347603}"/>
-    <hyperlink r:id="rId104" ref="C55" xr:uid="{9BD44DCD-EEBB-4649-9792-F3DAC40B3960}"/>
-    <hyperlink r:id="rId105" ref="C63" xr:uid="{9929BCF4-32FD-4143-99F6-FEB21B90BCD7}"/>
-    <hyperlink r:id="rId106" ref="C64" xr:uid="{80B3DEC9-506E-4F3A-B171-A2D71B731577}"/>
-    <hyperlink r:id="rId107" ref="C66" xr:uid="{011D2C70-C541-49D4-894E-FF670D6C19BB}"/>
-    <hyperlink r:id="rId108" ref="C67" xr:uid="{B62DFA3B-60A0-44AA-BF1D-BCA2A049E46C}"/>
-    <hyperlink r:id="rId109" ref="C56" xr:uid="{C98B5D5D-65AB-489D-8160-8F1B41CDE6A7}"/>
-    <hyperlink r:id="rId110" ref="B103" xr:uid="{4D81C408-B745-40E2-B9C7-6E36C45175A7}"/>
-    <hyperlink r:id="rId111" ref="C26" xr:uid="{6A9C6F44-3E7F-47CF-8514-B6609EBEE668}"/>
-    <hyperlink r:id="rId112" ref="C23" xr:uid="{F99F350A-C378-4940-B611-41F47BC3B4B0}"/>
-    <hyperlink r:id="rId113" ref="C103" xr:uid="{3E9C8DCE-ABC0-49DA-B64B-B569BAAE6ED0}"/>
-    <hyperlink r:id="rId114" ref="C104" xr:uid="{E96AA061-2DED-4A35-BE99-8E7E156527EB}"/>
-    <hyperlink r:id="rId115" ref="C102" xr:uid="{4DAA7E56-3BCD-4AF1-B6E7-A26B02A0DA6C}"/>
-    <hyperlink r:id="rId116" ref="C101" xr:uid="{EBE0EC7F-0880-4F4A-991C-2C7C53889923}"/>
-    <hyperlink r:id="rId117" ref="C100" xr:uid="{7AA4A2D0-C18F-4625-A776-6EDD2415E1BC}"/>
-    <hyperlink r:id="rId118" ref="C99" xr:uid="{15BFB680-4225-425B-8826-841A35922C8A}"/>
-    <hyperlink r:id="rId119" ref="B99" xr:uid="{1EF2BF94-D92B-41EF-8B1F-0585F1910B74}"/>
-    <hyperlink r:id="rId120" ref="C97" xr:uid="{6687C5A1-CC2B-49FF-B98D-946AA21B8C55}"/>
-    <hyperlink r:id="rId121" ref="B97" xr:uid="{0411E592-2DE8-4D1D-B66C-46CE99CAA412}"/>
-    <hyperlink r:id="rId122" ref="C96" xr:uid="{A7ED7210-DE23-4760-B67F-78027E9B9B73}"/>
-    <hyperlink r:id="rId123" ref="B96" xr:uid="{992F1752-E440-4347-A698-44C8E60F00BE}"/>
-    <hyperlink r:id="rId124" ref="B102" xr:uid="{A0E03FB2-010F-497D-874D-A0A66FB6303C}"/>
-    <hyperlink r:id="rId125" ref="B101" xr:uid="{165FBF6F-9195-42DA-AC37-C49B2308ACA1}"/>
-    <hyperlink r:id="rId126" ref="B94" xr:uid="{7DB2C8A6-8C43-4818-A7C2-D5E14351114B}"/>
-    <hyperlink r:id="rId127" ref="B93" xr:uid="{EFC122F7-44E7-447B-8F21-BA1503A72780}"/>
-    <hyperlink r:id="rId128" ref="B91" xr:uid="{7AC22E1D-6919-43E6-AD91-1551DBBDE570}"/>
-    <hyperlink r:id="rId129" ref="B88" xr:uid="{FB3E9840-E4E3-4E64-8CCF-2BAEC7024AD6}"/>
-    <hyperlink r:id="rId130" ref="B87" xr:uid="{348337ED-A616-4A9D-A8D3-0091262177C6}"/>
-    <hyperlink r:id="rId131" ref="B86" xr:uid="{CF62843D-4B82-47CB-B74F-D3F292E9603A}"/>
-    <hyperlink r:id="rId132" ref="B84" xr:uid="{9CA10EFF-3943-479E-914B-1D6EE04D75FC}"/>
-    <hyperlink r:id="rId133" ref="C84" xr:uid="{1074AAC9-CCB0-4FFC-9AFB-EFD1363D7538}"/>
-    <hyperlink r:id="rId134" ref="B105" xr:uid="{D6DE2797-5A68-4C1E-9E74-0D323B6ADFA2}"/>
-    <hyperlink r:id="rId135" ref="B106" xr:uid="{1FCAF9BA-00B5-4008-B5C8-E822ABD6BCDD}"/>
-    <hyperlink r:id="rId136" ref="C11" xr:uid="{893B2404-B185-41F7-B397-A3E08B386C5F}"/>
-    <hyperlink r:id="rId137" ref="B107" xr:uid="{B0E609F4-D8A3-433A-BE15-17E4804C6EA3}"/>
-    <hyperlink r:id="rId138" ref="C107" xr:uid="{6793ECA4-A034-42EC-A741-3B0FF42BC11B}"/>
-    <hyperlink r:id="rId139" ref="B108" xr:uid="{4DB78F44-0F08-4561-A0E8-0EE92F9FFECB}"/>
-    <hyperlink r:id="rId140" ref="B114" xr:uid="{27750164-38B8-4B5E-9B5A-E6C71FFFC61F}"/>
-    <hyperlink r:id="rId141" ref="C114" xr:uid="{6FE6A043-A6B1-44FF-8A45-8C3690323458}"/>
-    <hyperlink r:id="rId142" ref="B113" xr:uid="{0F94FF41-1E06-4D7B-B360-1EB377073C87}"/>
-    <hyperlink r:id="rId143" ref="B112" xr:uid="{490A5044-10EC-4082-BEC1-14008171D5CF}"/>
-    <hyperlink r:id="rId144" ref="B49" xr:uid="{836EB236-8BF1-4259-B395-AD9FA9DE0AE0}"/>
-    <hyperlink r:id="rId145" ref="B74" xr:uid="{8AA8904A-1CC5-4D06-93EF-66F7FC625199}"/>
-    <hyperlink r:id="rId146" ref="B76" xr:uid="{5743888C-C74A-41C6-ABC5-E9575351702D}"/>
-    <hyperlink r:id="rId147" ref="B115" xr:uid="{27BDB583-8AD0-4B33-BA19-24E42C9E7CE9}"/>
-    <hyperlink r:id="rId148" ref="B117" xr:uid="{92BA6213-0D94-4C5A-B06A-6FC35C0BECA9}"/>
-    <hyperlink r:id="rId149" ref="B119" xr:uid="{6724AE23-65F5-4D67-ADA6-E20BD420531B}"/>
-    <hyperlink r:id="rId150" ref="C119" xr:uid="{0A5009EB-B388-4AF4-99CE-5813711C2B1E}"/>
-    <hyperlink r:id="rId151" ref="B120" xr:uid="{255CB59B-E711-471E-8ACE-D0ABA408AE96}"/>
+    <hyperlink ref="B2" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
+    <hyperlink ref="B3" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
+    <hyperlink ref="B4" r:id="rId3" xr:uid="{00000000-0004-0000-0000-000002000000}"/>
+    <hyperlink ref="B5" r:id="rId4" xr:uid="{00000000-0004-0000-0000-000003000000}"/>
+    <hyperlink ref="B6" r:id="rId5" xr:uid="{00000000-0004-0000-0000-000004000000}"/>
+    <hyperlink ref="H6" r:id="rId6" xr:uid="{00000000-0004-0000-0000-000005000000}"/>
+    <hyperlink ref="B7" r:id="rId7" xr:uid="{00000000-0004-0000-0000-000006000000}"/>
+    <hyperlink ref="B8" r:id="rId8" xr:uid="{00000000-0004-0000-0000-000007000000}"/>
+    <hyperlink ref="B9" r:id="rId9" xr:uid="{00000000-0004-0000-0000-000008000000}"/>
+    <hyperlink ref="B10" r:id="rId10" xr:uid="{00000000-0004-0000-0000-000009000000}"/>
+    <hyperlink ref="B11" r:id="rId11" xr:uid="{00000000-0004-0000-0000-00000A000000}"/>
+    <hyperlink ref="B12" r:id="rId12" xr:uid="{00000000-0004-0000-0000-00000B000000}"/>
+    <hyperlink ref="B13" r:id="rId13" xr:uid="{00000000-0004-0000-0000-00000C000000}"/>
+    <hyperlink ref="B14" r:id="rId14" xr:uid="{00000000-0004-0000-0000-00000D000000}"/>
+    <hyperlink ref="B15" r:id="rId15" xr:uid="{00000000-0004-0000-0000-00000E000000}"/>
+    <hyperlink ref="B16" r:id="rId16" xr:uid="{00000000-0004-0000-0000-00000F000000}"/>
+    <hyperlink ref="B17" r:id="rId17" xr:uid="{00000000-0004-0000-0000-000010000000}"/>
+    <hyperlink ref="B18" r:id="rId18" xr:uid="{00000000-0004-0000-0000-000011000000}"/>
+    <hyperlink ref="B19" r:id="rId19" xr:uid="{00000000-0004-0000-0000-000012000000}"/>
+    <hyperlink ref="B20" r:id="rId20" xr:uid="{00000000-0004-0000-0000-000013000000}"/>
+    <hyperlink ref="B21" r:id="rId21" xr:uid="{00000000-0004-0000-0000-000014000000}"/>
+    <hyperlink ref="B22" r:id="rId22" xr:uid="{00000000-0004-0000-0000-000015000000}"/>
+    <hyperlink ref="B23" r:id="rId23" xr:uid="{00000000-0004-0000-0000-000016000000}"/>
+    <hyperlink ref="B24" r:id="rId24" xr:uid="{00000000-0004-0000-0000-000017000000}"/>
+    <hyperlink ref="B25" r:id="rId25" xr:uid="{00000000-0004-0000-0000-000018000000}"/>
+    <hyperlink ref="H25" r:id="rId26" xr:uid="{00000000-0004-0000-0000-000019000000}"/>
+    <hyperlink ref="B26" r:id="rId27" xr:uid="{00000000-0004-0000-0000-00001A000000}"/>
+    <hyperlink ref="H26" r:id="rId28" xr:uid="{00000000-0004-0000-0000-00001B000000}"/>
+    <hyperlink ref="B27" r:id="rId29" xr:uid="{00000000-0004-0000-0000-00001C000000}"/>
+    <hyperlink ref="H27" r:id="rId30" xr:uid="{00000000-0004-0000-0000-00001D000000}"/>
+    <hyperlink ref="B28" r:id="rId31" xr:uid="{00000000-0004-0000-0000-00001E000000}"/>
+    <hyperlink ref="H28" r:id="rId32" xr:uid="{00000000-0004-0000-0000-00001F000000}"/>
+    <hyperlink ref="B29" r:id="rId33" xr:uid="{00000000-0004-0000-0000-000020000000}"/>
+    <hyperlink ref="H29" r:id="rId34" xr:uid="{00000000-0004-0000-0000-000021000000}"/>
+    <hyperlink ref="B30" r:id="rId35" xr:uid="{00000000-0004-0000-0000-000022000000}"/>
+    <hyperlink ref="H30" r:id="rId36" xr:uid="{00000000-0004-0000-0000-000023000000}"/>
+    <hyperlink ref="B31" r:id="rId37" xr:uid="{00000000-0004-0000-0000-000024000000}"/>
+    <hyperlink ref="H31" r:id="rId38" xr:uid="{00000000-0004-0000-0000-000025000000}"/>
+    <hyperlink ref="B32" r:id="rId39" xr:uid="{00000000-0004-0000-0000-000026000000}"/>
+    <hyperlink ref="H32" r:id="rId40" xr:uid="{00000000-0004-0000-0000-000027000000}"/>
+    <hyperlink ref="B33" r:id="rId41" xr:uid="{00000000-0004-0000-0000-000028000000}"/>
+    <hyperlink ref="B34" r:id="rId42" xr:uid="{00000000-0004-0000-0000-000029000000}"/>
+    <hyperlink ref="B38" r:id="rId43" xr:uid="{00000000-0004-0000-0000-00002A000000}"/>
+    <hyperlink ref="B45" r:id="rId44" xr:uid="{00000000-0004-0000-0000-00002B000000}"/>
+    <hyperlink ref="B48" r:id="rId45" xr:uid="{00000000-0004-0000-0000-00002C000000}"/>
+    <hyperlink ref="B35" r:id="rId46" xr:uid="{00000000-0004-0000-0000-00002D000000}"/>
+    <hyperlink ref="B52" r:id="rId47" xr:uid="{00000000-0004-0000-0000-00002E000000}"/>
+    <hyperlink ref="B53" r:id="rId48" xr:uid="{00000000-0004-0000-0000-00002F000000}"/>
+    <hyperlink ref="B55" r:id="rId49" xr:uid="{00000000-0004-0000-0000-000030000000}"/>
+    <hyperlink ref="B56" r:id="rId50" xr:uid="{00000000-0004-0000-0000-000031000000}"/>
+    <hyperlink ref="B57" r:id="rId51" xr:uid="{00000000-0004-0000-0000-000032000000}"/>
+    <hyperlink ref="B58" r:id="rId52" xr:uid="{00000000-0004-0000-0000-000033000000}"/>
+    <hyperlink ref="B61" r:id="rId53" xr:uid="{00000000-0004-0000-0000-000034000000}"/>
+    <hyperlink ref="B62" r:id="rId54" xr:uid="{00000000-0004-0000-0000-000035000000}"/>
+    <hyperlink ref="B63" r:id="rId55" xr:uid="{00000000-0004-0000-0000-000036000000}"/>
+    <hyperlink ref="B64" r:id="rId56" xr:uid="{00000000-0004-0000-0000-000037000000}"/>
+    <hyperlink ref="B65" r:id="rId57" xr:uid="{00000000-0004-0000-0000-000038000000}"/>
+    <hyperlink ref="B66" r:id="rId58" xr:uid="{00000000-0004-0000-0000-000039000000}"/>
+    <hyperlink ref="B67" r:id="rId59" xr:uid="{00000000-0004-0000-0000-00003A000000}"/>
+    <hyperlink ref="H7:H24" r:id="rId60" display="https://www.allhomes.com.au/agency/trusted-realtors-570129/" xr:uid="{00000000-0004-0000-0000-00003B000000}"/>
+    <hyperlink ref="B43" r:id="rId61" xr:uid="{00000000-0004-0000-0000-00003C000000}"/>
+    <hyperlink ref="B44" r:id="rId62" xr:uid="{00000000-0004-0000-0000-00003D000000}"/>
+    <hyperlink ref="B46" r:id="rId63" xr:uid="{00000000-0004-0000-0000-00003E000000}"/>
+    <hyperlink ref="B54" r:id="rId64" xr:uid="{00000000-0004-0000-0000-00003F000000}"/>
+    <hyperlink ref="B42" r:id="rId65" xr:uid="{00000000-0004-0000-0000-000040000000}"/>
+    <hyperlink ref="J2" r:id="rId66" xr:uid="{00000000-0004-0000-0000-000041000000}"/>
+    <hyperlink ref="C69" r:id="rId67" xr:uid="{9DAE03A7-93E8-4507-BD6C-AC4013ECD47F}"/>
+    <hyperlink ref="C68" r:id="rId68" xr:uid="{66B9A9CA-DF82-46B6-9C5A-C5709E2FF1AE}"/>
+    <hyperlink ref="B75" r:id="rId69" xr:uid="{57E7BFEF-6F05-4DA9-A3DE-5B0A0EFED4D9}"/>
+    <hyperlink ref="C75" r:id="rId70" xr:uid="{F4755F93-6E59-4C38-BF66-16746869FDF3}"/>
+    <hyperlink ref="H75" r:id="rId71" xr:uid="{5BFAFD71-42C4-487F-B5E7-1697975992B4}"/>
+    <hyperlink ref="B78" r:id="rId72" xr:uid="{D3DE0D76-2479-4283-B7C7-F11B85797022}"/>
+    <hyperlink ref="C78" r:id="rId73" xr:uid="{FC1D9146-2FDC-4F13-A3C3-51CAB46DEC08}"/>
+    <hyperlink ref="B68" r:id="rId74" xr:uid="{3ED6FAA1-2B0F-4DB9-878E-9640A9C2850D}"/>
+    <hyperlink ref="B69" r:id="rId75" xr:uid="{12DE6CA8-DDC5-4E7B-BD2E-14B105A0DE3B}"/>
+    <hyperlink ref="C70" r:id="rId76" xr:uid="{0419758C-286A-4B76-B8B2-31CC336DEDF1}"/>
+    <hyperlink ref="B70" r:id="rId77" xr:uid="{AC18D1D2-FA3D-4352-A402-35B7AAFE27C0}"/>
+    <hyperlink ref="B71" r:id="rId78" xr:uid="{E8BCA1EF-4E17-4AA7-A2CE-5674FC05ABC3}"/>
+    <hyperlink ref="C71" r:id="rId79" xr:uid="{949AE606-DF4A-48F4-93A0-F148D80842CB}"/>
+    <hyperlink ref="B72" r:id="rId80" xr:uid="{69A93BB5-0295-46D6-8334-45444356E6E9}"/>
+    <hyperlink ref="C72" r:id="rId81" xr:uid="{CA171BC7-126F-4175-8A03-123D5A2C2D8A}"/>
+    <hyperlink ref="C73" r:id="rId82" xr:uid="{FACC205D-E563-4266-8E0D-0794F3D76E98}"/>
+    <hyperlink ref="B85" r:id="rId83" xr:uid="{7ABCABC0-A765-435B-AE52-9D27F653E00F}"/>
+    <hyperlink ref="C4" r:id="rId84" xr:uid="{2CD58DBE-98E3-4EDC-898F-088D5F0FCB81}"/>
+    <hyperlink ref="C29" r:id="rId85" xr:uid="{CB7CAD83-ACA3-4309-B102-B0F536FC97E6}"/>
+    <hyperlink ref="C90" r:id="rId86" xr:uid="{B4F55488-2B40-4078-ABF0-4B4254363237}"/>
+    <hyperlink ref="B90" r:id="rId87" xr:uid="{09FEE7FE-E667-40E8-BC22-3FDC999B614F}"/>
+    <hyperlink ref="C15" r:id="rId88" xr:uid="{34F25BA9-B460-46CF-85C0-4AC9D6288B41}"/>
+    <hyperlink ref="C3" r:id="rId89" xr:uid="{EBAAEE7A-83B2-457B-8600-89427BF11448}"/>
+    <hyperlink ref="C8" r:id="rId90" xr:uid="{3D3D678C-8F1B-47BC-ACA2-D1CBF5A76F0B}"/>
+    <hyperlink ref="C19" r:id="rId91" xr:uid="{ED2C9A9B-3440-4B4A-91A1-7CAF84972535}"/>
+    <hyperlink ref="C20" r:id="rId92" xr:uid="{E47C999F-11AE-4F93-9032-6E51EB582635}"/>
+    <hyperlink ref="C21" r:id="rId93" xr:uid="{E59411CC-EC13-4665-969A-8D9238CCD0C2}"/>
+    <hyperlink ref="C33" r:id="rId94" xr:uid="{9C953AB9-0076-4477-B52F-C393846B1211}"/>
+    <hyperlink ref="C38" r:id="rId95" xr:uid="{D349EA20-36BF-44C7-A16B-E85B8FE53B2A}"/>
+    <hyperlink ref="C39" r:id="rId96" xr:uid="{DE18DA3B-1A3D-4613-888E-7F506CC87091}"/>
+    <hyperlink ref="C40" r:id="rId97" xr:uid="{0C71282B-049B-4CD1-A090-B66647F2B29B}"/>
+    <hyperlink ref="C42" r:id="rId98" xr:uid="{AD0DC851-DEC5-4ACE-B928-50149068BB70}"/>
+    <hyperlink ref="C45" r:id="rId99" xr:uid="{EB51DFC2-D28F-4E0C-B019-F9954D6C9832}"/>
+    <hyperlink ref="C52" r:id="rId100" xr:uid="{9E5146F6-8EC8-4A2C-B192-C1CCB11CAB8A}"/>
+    <hyperlink ref="C48" r:id="rId101" xr:uid="{31B308E4-DA3E-401B-B796-7D03404228FB}"/>
+    <hyperlink ref="C49" r:id="rId102" xr:uid="{EBAAB9CE-7F91-4628-AF75-32C4EEF948C2}"/>
+    <hyperlink ref="C53" r:id="rId103" xr:uid="{2FF7EB1F-CD56-4E71-AD0F-0D12E8347603}"/>
+    <hyperlink ref="C55" r:id="rId104" xr:uid="{9BD44DCD-EEBB-4649-9792-F3DAC40B3960}"/>
+    <hyperlink ref="C63" r:id="rId105" xr:uid="{9929BCF4-32FD-4143-99F6-FEB21B90BCD7}"/>
+    <hyperlink ref="C64" r:id="rId106" xr:uid="{80B3DEC9-506E-4F3A-B171-A2D71B731577}"/>
+    <hyperlink ref="C66" r:id="rId107" xr:uid="{011D2C70-C541-49D4-894E-FF670D6C19BB}"/>
+    <hyperlink ref="C67" r:id="rId108" xr:uid="{B62DFA3B-60A0-44AA-BF1D-BCA2A049E46C}"/>
+    <hyperlink ref="C56" r:id="rId109" xr:uid="{C98B5D5D-65AB-489D-8160-8F1B41CDE6A7}"/>
+    <hyperlink ref="B103" r:id="rId110" xr:uid="{4D81C408-B745-40E2-B9C7-6E36C45175A7}"/>
+    <hyperlink ref="C26" r:id="rId111" xr:uid="{6A9C6F44-3E7F-47CF-8514-B6609EBEE668}"/>
+    <hyperlink ref="C23" r:id="rId112" xr:uid="{F99F350A-C378-4940-B611-41F47BC3B4B0}"/>
+    <hyperlink ref="C103" r:id="rId113" xr:uid="{3E9C8DCE-ABC0-49DA-B64B-B569BAAE6ED0}"/>
+    <hyperlink ref="C104" r:id="rId114" xr:uid="{E96AA061-2DED-4A35-BE99-8E7E156527EB}"/>
+    <hyperlink ref="C102" r:id="rId115" xr:uid="{4DAA7E56-3BCD-4AF1-B6E7-A26B02A0DA6C}"/>
+    <hyperlink ref="C101" r:id="rId116" xr:uid="{EBE0EC7F-0880-4F4A-991C-2C7C53889923}"/>
+    <hyperlink ref="C100" r:id="rId117" xr:uid="{7AA4A2D0-C18F-4625-A776-6EDD2415E1BC}"/>
+    <hyperlink ref="C99" r:id="rId118" xr:uid="{15BFB680-4225-425B-8826-841A35922C8A}"/>
+    <hyperlink ref="B99" r:id="rId119" xr:uid="{1EF2BF94-D92B-41EF-8B1F-0585F1910B74}"/>
+    <hyperlink ref="C97" r:id="rId120" xr:uid="{6687C5A1-CC2B-49FF-B98D-946AA21B8C55}"/>
+    <hyperlink ref="B97" r:id="rId121" xr:uid="{0411E592-2DE8-4D1D-B66C-46CE99CAA412}"/>
+    <hyperlink ref="C96" r:id="rId122" xr:uid="{A7ED7210-DE23-4760-B67F-78027E9B9B73}"/>
+    <hyperlink ref="B96" r:id="rId123" xr:uid="{992F1752-E440-4347-A698-44C8E60F00BE}"/>
+    <hyperlink ref="B102" r:id="rId124" xr:uid="{A0E03FB2-010F-497D-874D-A0A66FB6303C}"/>
+    <hyperlink ref="B101" r:id="rId125" xr:uid="{165FBF6F-9195-42DA-AC37-C49B2308ACA1}"/>
+    <hyperlink ref="B94" r:id="rId126" xr:uid="{7DB2C8A6-8C43-4818-A7C2-D5E14351114B}"/>
+    <hyperlink ref="B93" r:id="rId127" xr:uid="{EFC122F7-44E7-447B-8F21-BA1503A72780}"/>
+    <hyperlink ref="B91" r:id="rId128" xr:uid="{7AC22E1D-6919-43E6-AD91-1551DBBDE570}"/>
+    <hyperlink ref="B88" r:id="rId129" xr:uid="{FB3E9840-E4E3-4E64-8CCF-2BAEC7024AD6}"/>
+    <hyperlink ref="B87" r:id="rId130" xr:uid="{348337ED-A616-4A9D-A8D3-0091262177C6}"/>
+    <hyperlink ref="B86" r:id="rId131" xr:uid="{CF62843D-4B82-47CB-B74F-D3F292E9603A}"/>
+    <hyperlink ref="B84" r:id="rId132" xr:uid="{9CA10EFF-3943-479E-914B-1D6EE04D75FC}"/>
+    <hyperlink ref="C84" r:id="rId133" xr:uid="{1074AAC9-CCB0-4FFC-9AFB-EFD1363D7538}"/>
+    <hyperlink ref="B105" r:id="rId134" xr:uid="{D6DE2797-5A68-4C1E-9E74-0D323B6ADFA2}"/>
+    <hyperlink ref="B106" r:id="rId135" xr:uid="{1FCAF9BA-00B5-4008-B5C8-E822ABD6BCDD}"/>
+    <hyperlink ref="C11" r:id="rId136" xr:uid="{893B2404-B185-41F7-B397-A3E08B386C5F}"/>
+    <hyperlink ref="B107" r:id="rId137" xr:uid="{B0E609F4-D8A3-433A-BE15-17E4804C6EA3}"/>
+    <hyperlink ref="C107" r:id="rId138" xr:uid="{6793ECA4-A034-42EC-A741-3B0FF42BC11B}"/>
+    <hyperlink ref="B108" r:id="rId139" xr:uid="{4DB78F44-0F08-4561-A0E8-0EE92F9FFECB}"/>
+    <hyperlink ref="B114" r:id="rId140" xr:uid="{27750164-38B8-4B5E-9B5A-E6C71FFFC61F}"/>
+    <hyperlink ref="C114" r:id="rId141" xr:uid="{6FE6A043-A6B1-44FF-8A45-8C3690323458}"/>
+    <hyperlink ref="B113" r:id="rId142" xr:uid="{0F94FF41-1E06-4D7B-B360-1EB377073C87}"/>
+    <hyperlink ref="B112" r:id="rId143" xr:uid="{490A5044-10EC-4082-BEC1-14008171D5CF}"/>
+    <hyperlink ref="B49" r:id="rId144" xr:uid="{836EB236-8BF1-4259-B395-AD9FA9DE0AE0}"/>
+    <hyperlink ref="B74" r:id="rId145" xr:uid="{8AA8904A-1CC5-4D06-93EF-66F7FC625199}"/>
+    <hyperlink ref="B76" r:id="rId146" xr:uid="{5743888C-C74A-41C6-ABC5-E9575351702D}"/>
+    <hyperlink ref="B115" r:id="rId147" xr:uid="{27BDB583-8AD0-4B33-BA19-24E42C9E7CE9}"/>
+    <hyperlink ref="B117" r:id="rId148" xr:uid="{92BA6213-0D94-4C5A-B06A-6FC35C0BECA9}"/>
+    <hyperlink ref="B119" r:id="rId149" xr:uid="{6724AE23-65F5-4D67-ADA6-E20BD420531B}"/>
+    <hyperlink ref="C119" r:id="rId150" xr:uid="{0A5009EB-B388-4AF4-99CE-5813711C2B1E}"/>
+    <hyperlink ref="B120" r:id="rId151" xr:uid="{255CB59B-E711-471E-8ACE-D0ABA408AE96}"/>
+    <hyperlink ref="B39" r:id="rId152" xr:uid="{39FB4A7C-4EA8-4530-9FE6-2842C777350C}"/>
+    <hyperlink ref="B104" r:id="rId153" xr:uid="{FC8A6FB5-FCCF-409E-9D6D-A93D412B2275}"/>
+    <hyperlink ref="C105" r:id="rId154" xr:uid="{988B91BF-CEBD-44F6-A773-3C87D877BE5A}"/>
+    <hyperlink ref="C108" r:id="rId155" xr:uid="{F0593E1B-3EE0-4DF2-B93E-84A02071630B}"/>
+    <hyperlink ref="B109" r:id="rId156" xr:uid="{601C40E0-818B-457C-9FE7-30D06707CEB7}"/>
+    <hyperlink ref="C109" r:id="rId157" xr:uid="{E1D93474-1A3D-49F1-B191-3C3484679D2D}"/>
   </hyperlinks>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
-  <pageSetup orientation="portrait" paperSize="9" r:id="rId152"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId158"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:AJ143"/>
+  <dimension ref="A1:AI143"/>
   <sheetViews>
-    <sheetView topLeftCell="A110" workbookViewId="0">
-      <pane activePane="topRight" state="frozen" topLeftCell="M1" xSplit="1"/>
-      <selection activeCell="U130" pane="topRight" sqref="U130"/>
+    <sheetView topLeftCell="A113" workbookViewId="0">
+      <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="C145" sqref="C145"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="14.42578125" defaultRowHeight="15.75"/>
+  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="14.85546875" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="18.140625" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" width="55.5703125" collapsed="true"/>
-    <col min="4" max="4" customWidth="true" width="25.140625" collapsed="true"/>
-    <col min="5" max="5" customWidth="true" width="19.5703125" collapsed="true"/>
-    <col min="6" max="6" customWidth="true" width="19.85546875" collapsed="true"/>
-    <col min="7" max="7" customWidth="true" width="18.5703125" collapsed="true"/>
-    <col min="8" max="8" customWidth="true" width="32.140625" collapsed="true"/>
-    <col min="9" max="9" customWidth="true" width="20.5703125" collapsed="true"/>
-    <col min="10" max="10" customWidth="true" width="21.140625" collapsed="true"/>
-    <col min="11" max="11" customWidth="true" width="28.85546875" collapsed="true"/>
-    <col min="12" max="12" customWidth="true" width="37.5703125" collapsed="true"/>
-    <col min="16" max="17" customWidth="true" width="18.85546875" collapsed="true"/>
-    <col min="18" max="18" customWidth="true" width="47.85546875" collapsed="true"/>
-    <col min="19" max="19" customWidth="true" width="77.5703125" collapsed="true"/>
-    <col min="20" max="20" customWidth="true" width="24.0" collapsed="true"/>
-    <col min="21" max="21" customWidth="true" width="18.85546875" collapsed="true"/>
-    <col min="22" max="31" customWidth="true" width="19.140625" collapsed="true"/>
+    <col min="1" max="1" width="14.85546875" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="18.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="55.5703125" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="25.140625" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="19.5703125" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="19.85546875" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="18.5703125" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="32.140625" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="20.5703125" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="21.140625" customWidth="1" collapsed="1"/>
+    <col min="11" max="11" width="28.85546875" customWidth="1" collapsed="1"/>
+    <col min="12" max="12" width="37.5703125" customWidth="1" collapsed="1"/>
+    <col min="16" max="17" width="18.85546875" customWidth="1" collapsed="1"/>
+    <col min="18" max="18" width="47.85546875" customWidth="1" collapsed="1"/>
+    <col min="19" max="19" width="77.5703125" customWidth="1" collapsed="1"/>
+    <col min="20" max="20" width="24" customWidth="1" collapsed="1"/>
+    <col min="21" max="21" width="18.85546875" customWidth="1" collapsed="1"/>
+    <col min="22" max="31" width="19.140625" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row ht="30" r="1" spans="1:35">
+    <row r="1" spans="1:35" ht="30">
       <c r="A1" s="1" t="s">
         <v>46</v>
       </c>
@@ -9815,7 +9820,7 @@
       <c r="AH1" s="23"/>
       <c r="AI1" s="23"/>
     </row>
-    <row customHeight="1" ht="15" r="2" spans="1:35">
+    <row r="2" spans="1:35" ht="15" customHeight="1">
       <c r="A2" s="24">
         <v>1</v>
       </c>
@@ -9886,7 +9891,7 @@
       <c r="AH2" s="24"/>
       <c r="AI2" s="24"/>
     </row>
-    <row customHeight="1" ht="15" r="3" spans="1:35">
+    <row r="3" spans="1:35" ht="15" customHeight="1">
       <c r="A3" s="24">
         <v>2</v>
       </c>
@@ -9957,7 +9962,7 @@
       <c r="AH3" s="24"/>
       <c r="AI3" s="24"/>
     </row>
-    <row customFormat="1" customHeight="1" ht="15" r="4" s="24" spans="1:35">
+    <row r="4" spans="1:35" s="24" customFormat="1" ht="15" customHeight="1">
       <c r="A4" s="24">
         <v>3</v>
       </c>
@@ -10019,7 +10024,7 @@
         <v>8</v>
       </c>
     </row>
-    <row customHeight="1" ht="15" r="5" spans="1:35">
+    <row r="5" spans="1:35" ht="15" customHeight="1">
       <c r="A5" s="24">
         <v>4</v>
       </c>
@@ -10092,7 +10097,7 @@
       <c r="AH5" s="24"/>
       <c r="AI5" s="24"/>
     </row>
-    <row customFormat="1" customHeight="1" ht="15" r="6" s="24" spans="1:35">
+    <row r="6" spans="1:35" s="24" customFormat="1" ht="15" customHeight="1">
       <c r="A6" s="24">
         <v>5</v>
       </c>
@@ -10151,7 +10156,7 @@
         <v>16</v>
       </c>
     </row>
-    <row customFormat="1" customHeight="1" ht="15" r="7" s="24" spans="1:35">
+    <row r="7" spans="1:35" s="24" customFormat="1" ht="15" customHeight="1">
       <c r="A7" s="24">
         <v>6</v>
       </c>
@@ -10210,7 +10215,7 @@
         <v>16</v>
       </c>
     </row>
-    <row customFormat="1" customHeight="1" ht="15" r="8" s="24" spans="1:35">
+    <row r="8" spans="1:35" s="24" customFormat="1" ht="15" customHeight="1">
       <c r="A8" s="24">
         <v>7</v>
       </c>
@@ -10266,7 +10271,7 @@
         <v>16</v>
       </c>
     </row>
-    <row customFormat="1" customHeight="1" ht="15" r="9" s="24" spans="1:35">
+    <row r="9" spans="1:35" s="24" customFormat="1" ht="15" customHeight="1">
       <c r="A9" s="24">
         <v>8</v>
       </c>
@@ -10325,7 +10330,7 @@
         <v>16</v>
       </c>
     </row>
-    <row customFormat="1" customHeight="1" ht="15" r="10" s="24" spans="1:35">
+    <row r="10" spans="1:35" s="24" customFormat="1" ht="15" customHeight="1">
       <c r="A10" s="24">
         <v>9</v>
       </c>
@@ -10381,7 +10386,7 @@
         <v>16</v>
       </c>
     </row>
-    <row customFormat="1" customHeight="1" ht="15" r="11" s="24" spans="1:35">
+    <row r="11" spans="1:35" s="24" customFormat="1" ht="15" customHeight="1">
       <c r="A11" s="24">
         <v>10</v>
       </c>
@@ -10446,7 +10451,7 @@
         <v>114</v>
       </c>
     </row>
-    <row customFormat="1" customHeight="1" ht="15" r="12" s="24" spans="1:35">
+    <row r="12" spans="1:35" s="24" customFormat="1" ht="15" customHeight="1">
       <c r="A12" s="24">
         <v>11</v>
       </c>
@@ -10502,7 +10507,7 @@
         <v>16</v>
       </c>
     </row>
-    <row customFormat="1" customHeight="1" ht="15" r="13" s="24" spans="1:35">
+    <row r="13" spans="1:35" s="24" customFormat="1" ht="15" customHeight="1">
       <c r="A13" s="24">
         <v>12</v>
       </c>
@@ -10561,7 +10566,7 @@
         <v>114</v>
       </c>
     </row>
-    <row customFormat="1" customHeight="1" ht="15" r="14" s="24" spans="1:35">
+    <row r="14" spans="1:35" s="24" customFormat="1" ht="15" customHeight="1">
       <c r="A14" s="24">
         <v>13</v>
       </c>
@@ -10626,7 +10631,7 @@
         <v>114</v>
       </c>
     </row>
-    <row customFormat="1" customHeight="1" ht="15" r="15" s="24" spans="1:35">
+    <row r="15" spans="1:35" s="24" customFormat="1" ht="15" customHeight="1">
       <c r="A15" s="24">
         <v>14</v>
       </c>
@@ -10685,7 +10690,7 @@
         <v>16</v>
       </c>
     </row>
-    <row customFormat="1" customHeight="1" ht="15" r="16" s="24" spans="1:35">
+    <row r="16" spans="1:35" s="24" customFormat="1" ht="15" customHeight="1">
       <c r="A16" s="24">
         <v>15</v>
       </c>
@@ -10744,7 +10749,7 @@
         <v>16</v>
       </c>
     </row>
-    <row customFormat="1" customHeight="1" ht="15" r="17" s="24" spans="1:35">
+    <row r="17" spans="1:35" s="24" customFormat="1" ht="15" customHeight="1">
       <c r="A17" s="24">
         <v>16</v>
       </c>
@@ -10800,7 +10805,7 @@
         <v>16</v>
       </c>
     </row>
-    <row customFormat="1" customHeight="1" ht="15" r="18" s="24" spans="1:35">
+    <row r="18" spans="1:35" s="24" customFormat="1" ht="15" customHeight="1">
       <c r="A18" s="24">
         <v>17</v>
       </c>
@@ -10859,7 +10864,7 @@
         <v>16</v>
       </c>
     </row>
-    <row customFormat="1" customHeight="1" ht="15" r="19" s="24" spans="1:35">
+    <row r="19" spans="1:35" s="24" customFormat="1" ht="15" customHeight="1">
       <c r="A19" s="24">
         <v>18</v>
       </c>
@@ -10912,7 +10917,7 @@
         <v>16</v>
       </c>
     </row>
-    <row customHeight="1" ht="15" r="20" spans="1:35">
+    <row r="20" spans="1:35" ht="15" customHeight="1">
       <c r="A20" s="24">
         <v>19</v>
       </c>
@@ -10987,7 +10992,7 @@
       <c r="AH20" s="24"/>
       <c r="AI20" s="24"/>
     </row>
-    <row customHeight="1" ht="15" r="21" spans="1:35">
+    <row r="21" spans="1:35" ht="15" customHeight="1">
       <c r="A21" s="24">
         <v>20</v>
       </c>
@@ -11058,7 +11063,7 @@
       <c r="AH21" s="24"/>
       <c r="AI21" s="24"/>
     </row>
-    <row customFormat="1" customHeight="1" ht="15" r="22" s="24" spans="1:35">
+    <row r="22" spans="1:35" s="24" customFormat="1" ht="15" customHeight="1">
       <c r="A22" s="24">
         <v>21</v>
       </c>
@@ -11123,7 +11128,7 @@
         <v>114</v>
       </c>
     </row>
-    <row customFormat="1" customHeight="1" ht="15" r="23" s="24" spans="1:35">
+    <row r="23" spans="1:35" s="24" customFormat="1" ht="15" customHeight="1">
       <c r="A23" s="24">
         <v>22</v>
       </c>
@@ -11176,7 +11181,7 @@
         <v>16</v>
       </c>
     </row>
-    <row customFormat="1" customHeight="1" ht="15" r="24" s="24" spans="1:35">
+    <row r="24" spans="1:35" s="24" customFormat="1" ht="15" customHeight="1">
       <c r="A24" s="24">
         <v>23</v>
       </c>
@@ -11235,7 +11240,7 @@
         <v>16</v>
       </c>
     </row>
-    <row customHeight="1" ht="15" r="25" spans="1:35">
+    <row r="25" spans="1:35" ht="15" customHeight="1">
       <c r="A25" s="24">
         <v>24</v>
       </c>
@@ -11306,7 +11311,7 @@
       <c r="AH25" s="24"/>
       <c r="AI25" s="24"/>
     </row>
-    <row customFormat="1" customHeight="1" ht="15" r="26" s="24" spans="1:35">
+    <row r="26" spans="1:35" s="24" customFormat="1" ht="15" customHeight="1">
       <c r="A26" s="24">
         <v>25</v>
       </c>
@@ -11365,7 +11370,7 @@
         <v>37</v>
       </c>
     </row>
-    <row customFormat="1" customHeight="1" ht="15" r="27" s="24" spans="1:35">
+    <row r="27" spans="1:35" s="24" customFormat="1" ht="15" customHeight="1">
       <c r="A27" s="24">
         <v>26</v>
       </c>
@@ -11424,7 +11429,7 @@
         <v>37</v>
       </c>
     </row>
-    <row customFormat="1" customHeight="1" ht="15" r="28" s="24" spans="1:35">
+    <row r="28" spans="1:35" s="24" customFormat="1" ht="15" customHeight="1">
       <c r="A28" s="24">
         <v>27</v>
       </c>
@@ -11483,7 +11488,7 @@
         <v>37</v>
       </c>
     </row>
-    <row customFormat="1" customHeight="1" ht="15" r="29" s="24" spans="1:35">
+    <row r="29" spans="1:35" s="24" customFormat="1" ht="15" customHeight="1">
       <c r="A29" s="24">
         <v>28</v>
       </c>
@@ -11542,7 +11547,7 @@
         <v>37</v>
       </c>
     </row>
-    <row customFormat="1" customHeight="1" ht="15" r="30" s="24" spans="1:35">
+    <row r="30" spans="1:35" s="24" customFormat="1" ht="15" customHeight="1">
       <c r="A30" s="24">
         <v>29</v>
       </c>
@@ -11601,7 +11606,7 @@
         <v>37</v>
       </c>
     </row>
-    <row customFormat="1" customHeight="1" ht="15" r="31" s="24" spans="1:35">
+    <row r="31" spans="1:35" s="24" customFormat="1" ht="15" customHeight="1">
       <c r="A31" s="24">
         <v>30</v>
       </c>
@@ -11657,7 +11662,7 @@
         <v>37</v>
       </c>
     </row>
-    <row customFormat="1" customHeight="1" ht="15" r="32" s="24" spans="1:35">
+    <row r="32" spans="1:35" s="24" customFormat="1" ht="15" customHeight="1">
       <c r="A32" s="24">
         <v>31</v>
       </c>
@@ -11716,7 +11721,7 @@
         <v>37</v>
       </c>
     </row>
-    <row customFormat="1" ht="14.25" r="33" s="24" spans="1:21">
+    <row r="33" spans="1:21" s="24" customFormat="1" ht="14.25">
       <c r="A33" s="24" t="s">
         <v>198</v>
       </c>
@@ -11775,7 +11780,7 @@
         <v>8</v>
       </c>
     </row>
-    <row customFormat="1" ht="14.25" r="34" s="24" spans="1:21">
+    <row r="34" spans="1:21" s="24" customFormat="1" ht="14.25">
       <c r="A34" s="24" t="s">
         <v>209</v>
       </c>
@@ -11834,7 +11839,7 @@
         <v>8</v>
       </c>
     </row>
-    <row customFormat="1" ht="14.25" r="35" s="24" spans="1:21">
+    <row r="35" spans="1:21" s="24" customFormat="1" ht="14.25">
       <c r="A35" s="24" t="s">
         <v>216</v>
       </c>
@@ -11893,7 +11898,7 @@
         <v>8</v>
       </c>
     </row>
-    <row customFormat="1" ht="14.25" r="36" s="24" spans="1:21">
+    <row r="36" spans="1:21" s="24" customFormat="1" ht="14.25">
       <c r="A36" s="24" t="s">
         <v>222</v>
       </c>
@@ -11952,7 +11957,7 @@
         <v>8</v>
       </c>
     </row>
-    <row customFormat="1" ht="14.25" r="37" s="24" spans="1:21">
+    <row r="37" spans="1:21" s="24" customFormat="1" ht="14.25">
       <c r="A37" s="24" t="s">
         <v>229</v>
       </c>
@@ -12011,7 +12016,7 @@
         <v>8</v>
       </c>
     </row>
-    <row customFormat="1" ht="14.25" r="38" s="24" spans="1:21">
+    <row r="38" spans="1:21" s="24" customFormat="1" ht="14.25">
       <c r="A38" s="24" t="s">
         <v>235</v>
       </c>
@@ -12070,12 +12075,12 @@
         <v>8</v>
       </c>
     </row>
-    <row customFormat="1" ht="14.25" r="39" s="24" spans="1:21">
+    <row r="39" spans="1:21" s="24" customFormat="1" ht="14.25">
       <c r="A39" s="24" t="s">
         <v>243</v>
       </c>
-      <c r="B39" s="24" t="s">
-        <v>7</v>
+      <c r="B39" s="44" t="s">
+        <v>175</v>
       </c>
       <c r="C39" s="24" t="s">
         <v>244</v>
@@ -12083,8 +12088,8 @@
       <c r="D39" s="24" t="s">
         <v>77</v>
       </c>
-      <c r="E39" s="24" t="s">
-        <v>78</v>
+      <c r="E39" s="44" t="s">
+        <v>175</v>
       </c>
       <c r="F39" s="24" t="s">
         <v>79</v>
@@ -12129,7 +12134,7 @@
         <v>8</v>
       </c>
     </row>
-    <row customFormat="1" ht="14.25" r="40" s="24" spans="1:21">
+    <row r="40" spans="1:21" s="24" customFormat="1" ht="14.25">
       <c r="A40" s="24" t="s">
         <v>246</v>
       </c>
@@ -12188,7 +12193,7 @@
         <v>8</v>
       </c>
     </row>
-    <row customFormat="1" ht="14.25" r="41" s="24" spans="1:21">
+    <row r="41" spans="1:21" s="24" customFormat="1" ht="14.25">
       <c r="A41" s="24" t="s">
         <v>249</v>
       </c>
@@ -12247,7 +12252,7 @@
         <v>8</v>
       </c>
     </row>
-    <row customFormat="1" ht="14.25" r="42" s="24" spans="1:21">
+    <row r="42" spans="1:21" s="24" customFormat="1" ht="14.25">
       <c r="A42" s="24" t="s">
         <v>258</v>
       </c>
@@ -12306,7 +12311,7 @@
         <v>8</v>
       </c>
     </row>
-    <row customFormat="1" ht="14.25" r="43" s="24" spans="1:21">
+    <row r="43" spans="1:21" s="24" customFormat="1" ht="14.25">
       <c r="A43" s="24" t="s">
         <v>262</v>
       </c>
@@ -12365,7 +12370,7 @@
         <v>8</v>
       </c>
     </row>
-    <row customFormat="1" ht="14.25" r="44" s="24" spans="1:21">
+    <row r="44" spans="1:21" s="24" customFormat="1" ht="14.25">
       <c r="A44" s="24" t="s">
         <v>271</v>
       </c>
@@ -12424,7 +12429,7 @@
         <v>8</v>
       </c>
     </row>
-    <row customFormat="1" ht="14.25" r="45" s="24" spans="1:21">
+    <row r="45" spans="1:21" s="24" customFormat="1" ht="14.25">
       <c r="A45" s="24" t="s">
         <v>278</v>
       </c>
@@ -12483,7 +12488,7 @@
         <v>37</v>
       </c>
     </row>
-    <row customFormat="1" ht="14.25" r="46" s="24" spans="1:21">
+    <row r="46" spans="1:21" s="24" customFormat="1" ht="14.25">
       <c r="A46" s="24" t="s">
         <v>284</v>
       </c>
@@ -12542,7 +12547,7 @@
         <v>37</v>
       </c>
     </row>
-    <row customFormat="1" ht="14.25" r="47" s="24" spans="1:21">
+    <row r="47" spans="1:21" s="24" customFormat="1" ht="14.25">
       <c r="A47" s="24" t="s">
         <v>290</v>
       </c>
@@ -12601,7 +12606,7 @@
         <v>37</v>
       </c>
     </row>
-    <row customFormat="1" ht="14.25" r="48" s="24" spans="1:21">
+    <row r="48" spans="1:21" s="24" customFormat="1" ht="14.25">
       <c r="A48" s="24" t="s">
         <v>296</v>
       </c>
@@ -12660,7 +12665,7 @@
         <v>16</v>
       </c>
     </row>
-    <row customFormat="1" ht="14.25" r="49" s="24" spans="1:21">
+    <row r="49" spans="1:21" s="24" customFormat="1" ht="14.25">
       <c r="A49" s="24" t="s">
         <v>301</v>
       </c>
@@ -12719,7 +12724,7 @@
         <v>16</v>
       </c>
     </row>
-    <row customFormat="1" ht="14.25" r="50" s="24" spans="1:21">
+    <row r="50" spans="1:21" s="24" customFormat="1" ht="14.25">
       <c r="A50" s="24" t="s">
         <v>307</v>
       </c>
@@ -12778,7 +12783,7 @@
         <v>16</v>
       </c>
     </row>
-    <row customFormat="1" ht="14.25" r="51" s="24" spans="1:21">
+    <row r="51" spans="1:21" s="24" customFormat="1" ht="14.25">
       <c r="A51" s="24" t="s">
         <v>313</v>
       </c>
@@ -12837,7 +12842,7 @@
         <v>16</v>
       </c>
     </row>
-    <row customFormat="1" ht="14.25" r="52" s="24" spans="1:21">
+    <row r="52" spans="1:21" s="24" customFormat="1" ht="14.25">
       <c r="A52" s="24" t="s">
         <v>319</v>
       </c>
@@ -12896,7 +12901,7 @@
         <v>16</v>
       </c>
     </row>
-    <row customFormat="1" ht="14.25" r="53" s="24" spans="1:21">
+    <row r="53" spans="1:21" s="24" customFormat="1" ht="14.25">
       <c r="A53" s="24" t="s">
         <v>346</v>
       </c>
@@ -12955,7 +12960,7 @@
         <v>328</v>
       </c>
     </row>
-    <row customFormat="1" ht="14.25" r="54" s="24" spans="1:21">
+    <row r="54" spans="1:21" s="24" customFormat="1" ht="14.25">
       <c r="A54" s="24" t="s">
         <v>352</v>
       </c>
@@ -13014,7 +13019,7 @@
         <v>328</v>
       </c>
     </row>
-    <row customFormat="1" ht="14.25" r="55" s="24" spans="1:21">
+    <row r="55" spans="1:21" s="24" customFormat="1" ht="14.25">
       <c r="A55" s="24" t="s">
         <v>356</v>
       </c>
@@ -13073,7 +13078,7 @@
         <v>328</v>
       </c>
     </row>
-    <row customFormat="1" ht="14.25" r="56" s="24" spans="1:21">
+    <row r="56" spans="1:21" s="24" customFormat="1" ht="14.25">
       <c r="A56" s="24" t="s">
         <v>362</v>
       </c>
@@ -13132,7 +13137,7 @@
         <v>328</v>
       </c>
     </row>
-    <row customFormat="1" ht="14.25" r="57" s="24" spans="1:21">
+    <row r="57" spans="1:21" s="24" customFormat="1" ht="14.25">
       <c r="A57" s="24" t="s">
         <v>367</v>
       </c>
@@ -13191,7 +13196,7 @@
         <v>328</v>
       </c>
     </row>
-    <row customFormat="1" ht="14.25" r="58" s="24" spans="1:21">
+    <row r="58" spans="1:21" s="24" customFormat="1" ht="14.25">
       <c r="A58" s="24" t="s">
         <v>374</v>
       </c>
@@ -13250,7 +13255,7 @@
         <v>328</v>
       </c>
     </row>
-    <row customFormat="1" ht="14.25" r="59" s="24" spans="1:21">
+    <row r="59" spans="1:21" s="24" customFormat="1" ht="14.25">
       <c r="A59" s="24" t="s">
         <v>380</v>
       </c>
@@ -13309,7 +13314,7 @@
         <v>328</v>
       </c>
     </row>
-    <row customFormat="1" ht="14.25" r="60" s="24" spans="1:21">
+    <row r="60" spans="1:21" s="24" customFormat="1" ht="14.25">
       <c r="A60" s="24" t="s">
         <v>387</v>
       </c>
@@ -13368,7 +13373,7 @@
         <v>328</v>
       </c>
     </row>
-    <row customFormat="1" ht="14.25" r="61" s="24" spans="1:21">
+    <row r="61" spans="1:21" s="24" customFormat="1" ht="14.25">
       <c r="A61" s="24" t="s">
         <v>394</v>
       </c>
@@ -13427,7 +13432,7 @@
         <v>328</v>
       </c>
     </row>
-    <row customFormat="1" ht="14.25" r="62" s="24" spans="1:21">
+    <row r="62" spans="1:21" s="24" customFormat="1" ht="14.25">
       <c r="A62" s="24" t="s">
         <v>400</v>
       </c>
@@ -13486,7 +13491,7 @@
         <v>8</v>
       </c>
     </row>
-    <row customFormat="1" ht="14.25" r="63" s="24" spans="1:21">
+    <row r="63" spans="1:21" s="24" customFormat="1" ht="14.25">
       <c r="A63" s="24" t="s">
         <v>403</v>
       </c>
@@ -13545,7 +13550,7 @@
         <v>8</v>
       </c>
     </row>
-    <row customFormat="1" ht="14.25" r="64" s="24" spans="1:21">
+    <row r="64" spans="1:21" s="24" customFormat="1" ht="14.25">
       <c r="A64" s="24" t="s">
         <v>408</v>
       </c>
@@ -13604,7 +13609,7 @@
         <v>8</v>
       </c>
     </row>
-    <row customFormat="1" ht="14.25" r="65" s="24" spans="1:21">
+    <row r="65" spans="1:21" s="24" customFormat="1" ht="14.25">
       <c r="A65" s="24" t="s">
         <v>414</v>
       </c>
@@ -13663,12 +13668,12 @@
         <v>8</v>
       </c>
     </row>
-    <row customFormat="1" ht="14.25" r="66" s="24" spans="1:21">
+    <row r="66" spans="1:21" s="24" customFormat="1" ht="14.25">
       <c r="A66" s="24" t="s">
         <v>419</v>
       </c>
-      <c r="B66" s="24" t="s">
-        <v>7</v>
+      <c r="B66" s="44" t="s">
+        <v>175</v>
       </c>
       <c r="C66" s="24" t="s">
         <v>420</v>
@@ -13676,8 +13681,8 @@
       <c r="D66" s="24" t="s">
         <v>84</v>
       </c>
-      <c r="E66" s="24" t="s">
-        <v>78</v>
+      <c r="E66" s="44" t="s">
+        <v>175</v>
       </c>
       <c r="F66" s="24" t="s">
         <v>79</v>
@@ -13722,7 +13727,7 @@
         <v>37</v>
       </c>
     </row>
-    <row customFormat="1" ht="14.25" r="67" s="24" spans="1:21">
+    <row r="67" spans="1:21" s="24" customFormat="1" ht="14.25">
       <c r="A67" s="24" t="s">
         <v>425</v>
       </c>
@@ -13781,7 +13786,7 @@
         <v>16</v>
       </c>
     </row>
-    <row customFormat="1" ht="14.25" r="68" s="24" spans="1:21">
+    <row r="68" spans="1:21" s="24" customFormat="1" ht="14.25">
       <c r="A68" s="24" t="s">
         <v>486</v>
       </c>
@@ -13840,7 +13845,7 @@
         <v>8</v>
       </c>
     </row>
-    <row customFormat="1" ht="14.25" r="69" s="24" spans="1:21">
+    <row r="69" spans="1:21" s="24" customFormat="1" ht="14.25">
       <c r="A69" s="24" t="s">
         <v>491</v>
       </c>
@@ -13899,7 +13904,7 @@
         <v>8</v>
       </c>
     </row>
-    <row customFormat="1" ht="14.25" r="70" s="24" spans="1:21">
+    <row r="70" spans="1:21" s="24" customFormat="1" ht="14.25">
       <c r="A70" s="24" t="s">
         <v>493</v>
       </c>
@@ -13958,7 +13963,7 @@
         <v>8</v>
       </c>
     </row>
-    <row customFormat="1" ht="14.25" r="71" s="24" spans="1:21">
+    <row r="71" spans="1:21" s="24" customFormat="1" ht="14.25">
       <c r="A71" s="24" t="s">
         <v>499</v>
       </c>
@@ -14017,7 +14022,7 @@
         <v>8</v>
       </c>
     </row>
-    <row customFormat="1" ht="14.25" r="72" s="24" spans="1:21">
+    <row r="72" spans="1:21" s="24" customFormat="1" ht="14.25">
       <c r="A72" s="24" t="s">
         <v>504</v>
       </c>
@@ -14076,7 +14081,7 @@
         <v>8</v>
       </c>
     </row>
-    <row customFormat="1" ht="14.25" r="73" s="24" spans="1:21">
+    <row r="73" spans="1:21" s="24" customFormat="1" ht="14.25">
       <c r="A73" s="24" t="s">
         <v>506</v>
       </c>
@@ -14135,7 +14140,7 @@
         <v>16</v>
       </c>
     </row>
-    <row customFormat="1" ht="14.25" r="74" s="24" spans="1:21">
+    <row r="74" spans="1:21" s="24" customFormat="1" ht="14.25">
       <c r="A74" s="24" t="s">
         <v>510</v>
       </c>
@@ -14194,7 +14199,7 @@
         <v>16</v>
       </c>
     </row>
-    <row customFormat="1" ht="14.25" r="75" s="24" spans="1:21">
+    <row r="75" spans="1:21" s="24" customFormat="1" ht="14.25">
       <c r="A75" s="24" t="s">
         <v>516</v>
       </c>
@@ -14253,7 +14258,7 @@
         <v>16</v>
       </c>
     </row>
-    <row customFormat="1" ht="14.25" r="76" s="24" spans="1:21">
+    <row r="76" spans="1:21" s="24" customFormat="1" ht="14.25">
       <c r="A76" s="24" t="s">
         <v>522</v>
       </c>
@@ -14312,7 +14317,7 @@
         <v>16</v>
       </c>
     </row>
-    <row customFormat="1" ht="14.25" r="77" s="24" spans="1:21">
+    <row r="77" spans="1:21" s="24" customFormat="1" ht="14.25">
       <c r="A77" s="24" t="s">
         <v>527</v>
       </c>
@@ -14371,7 +14376,7 @@
         <v>16</v>
       </c>
     </row>
-    <row customFormat="1" ht="14.25" r="78" s="24" spans="1:21">
+    <row r="78" spans="1:21" s="24" customFormat="1" ht="14.25">
       <c r="A78" s="24" t="s">
         <v>534</v>
       </c>
@@ -14430,7 +14435,7 @@
         <v>16</v>
       </c>
     </row>
-    <row customFormat="1" ht="14.25" r="79" s="24" spans="1:21">
+    <row r="79" spans="1:21" s="24" customFormat="1" ht="14.25">
       <c r="A79" s="24" t="s">
         <v>537</v>
       </c>
@@ -14489,7 +14494,7 @@
         <v>16</v>
       </c>
     </row>
-    <row customFormat="1" ht="14.25" r="80" s="24" spans="1:21">
+    <row r="80" spans="1:21" s="24" customFormat="1" ht="14.25">
       <c r="A80" s="24" t="s">
         <v>543</v>
       </c>
@@ -14548,7 +14553,7 @@
         <v>16</v>
       </c>
     </row>
-    <row customFormat="1" ht="14.25" r="81" s="24" spans="1:21">
+    <row r="81" spans="1:21" s="24" customFormat="1" ht="14.25">
       <c r="A81" s="24" t="s">
         <v>550</v>
       </c>
@@ -14607,7 +14612,7 @@
         <v>16</v>
       </c>
     </row>
-    <row customFormat="1" ht="14.25" r="82" s="24" spans="1:21">
+    <row r="82" spans="1:21" s="24" customFormat="1" ht="14.25">
       <c r="A82" s="24" t="s">
         <v>555</v>
       </c>
@@ -14666,7 +14671,7 @@
         <v>16</v>
       </c>
     </row>
-    <row customFormat="1" ht="14.25" r="83" s="24" spans="1:21">
+    <row r="83" spans="1:21" s="24" customFormat="1" ht="14.25">
       <c r="A83" s="24" t="s">
         <v>560</v>
       </c>
@@ -14725,7 +14730,7 @@
         <v>16</v>
       </c>
     </row>
-    <row customFormat="1" ht="14.25" r="84" s="24" spans="1:21">
+    <row r="84" spans="1:21" s="24" customFormat="1" ht="14.25">
       <c r="A84" s="24" t="s">
         <v>563</v>
       </c>
@@ -14784,7 +14789,7 @@
         <v>16</v>
       </c>
     </row>
-    <row customFormat="1" ht="14.25" r="85" s="24" spans="1:21">
+    <row r="85" spans="1:21" s="24" customFormat="1" ht="14.25">
       <c r="A85" s="24" t="s">
         <v>567</v>
       </c>
@@ -14843,7 +14848,7 @@
         <v>16</v>
       </c>
     </row>
-    <row customFormat="1" ht="14.25" r="86" s="24" spans="1:21">
+    <row r="86" spans="1:21" s="24" customFormat="1" ht="14.25">
       <c r="A86" s="24" t="s">
         <v>608</v>
       </c>
@@ -14902,7 +14907,7 @@
         <v>8</v>
       </c>
     </row>
-    <row customFormat="1" ht="14.25" r="87" s="24" spans="1:21">
+    <row r="87" spans="1:21" s="24" customFormat="1" ht="14.25">
       <c r="A87" s="24" t="s">
         <v>612</v>
       </c>
@@ -14961,7 +14966,7 @@
         <v>37</v>
       </c>
     </row>
-    <row customFormat="1" ht="14.25" r="88" s="24" spans="1:21">
+    <row r="88" spans="1:21" s="24" customFormat="1" ht="14.25">
       <c r="A88" s="24" t="s">
         <v>617</v>
       </c>
@@ -15020,7 +15025,7 @@
         <v>37</v>
       </c>
     </row>
-    <row customFormat="1" ht="14.25" r="89" s="24" spans="1:21">
+    <row r="89" spans="1:21" s="24" customFormat="1" ht="14.25">
       <c r="A89" s="24" t="s">
         <v>621</v>
       </c>
@@ -15079,7 +15084,7 @@
         <v>37</v>
       </c>
     </row>
-    <row customFormat="1" ht="14.25" r="90" s="24" spans="1:21">
+    <row r="90" spans="1:21" s="24" customFormat="1" ht="14.25">
       <c r="A90" s="24" t="s">
         <v>627</v>
       </c>
@@ -15138,7 +15143,7 @@
         <v>16</v>
       </c>
     </row>
-    <row customFormat="1" ht="14.25" r="91" s="24" spans="1:21">
+    <row r="91" spans="1:21" s="24" customFormat="1" ht="14.25">
       <c r="A91" s="24" t="s">
         <v>631</v>
       </c>
@@ -15197,7 +15202,7 @@
         <v>16</v>
       </c>
     </row>
-    <row customFormat="1" ht="14.25" r="92" s="24" spans="1:21">
+    <row r="92" spans="1:21" s="24" customFormat="1" ht="14.25">
       <c r="A92" s="24" t="s">
         <v>635</v>
       </c>
@@ -15256,7 +15261,7 @@
         <v>16</v>
       </c>
     </row>
-    <row customFormat="1" ht="14.25" r="93" s="24" spans="1:21">
+    <row r="93" spans="1:21" s="24" customFormat="1" ht="14.25">
       <c r="A93" s="24" t="s">
         <v>638</v>
       </c>
@@ -15315,7 +15320,7 @@
         <v>16</v>
       </c>
     </row>
-    <row customFormat="1" ht="14.25" r="94" s="24" spans="1:21">
+    <row r="94" spans="1:21" s="24" customFormat="1" ht="14.25">
       <c r="A94" s="24" t="s">
         <v>667</v>
       </c>
@@ -15374,7 +15379,7 @@
         <v>8</v>
       </c>
     </row>
-    <row customFormat="1" ht="14.25" r="95" s="24" spans="1:21">
+    <row r="95" spans="1:21" s="24" customFormat="1" ht="14.25">
       <c r="A95" s="24" t="s">
         <v>672</v>
       </c>
@@ -15433,7 +15438,7 @@
         <v>8</v>
       </c>
     </row>
-    <row customFormat="1" ht="14.25" r="96" s="24" spans="1:21">
+    <row r="96" spans="1:21" s="24" customFormat="1" ht="14.25">
       <c r="A96" s="24" t="s">
         <v>676</v>
       </c>
@@ -15492,7 +15497,7 @@
         <v>8</v>
       </c>
     </row>
-    <row customFormat="1" ht="14.25" r="97" s="24" spans="1:21">
+    <row r="97" spans="1:21" s="24" customFormat="1" ht="14.25">
       <c r="A97" s="24" t="s">
         <v>680</v>
       </c>
@@ -15551,7 +15556,7 @@
         <v>37</v>
       </c>
     </row>
-    <row customFormat="1" ht="14.25" r="98" s="24" spans="1:21">
+    <row r="98" spans="1:21" s="24" customFormat="1" ht="14.25">
       <c r="A98" s="24" t="s">
         <v>694</v>
       </c>
@@ -15610,12 +15615,12 @@
         <v>16</v>
       </c>
     </row>
-    <row customFormat="1" ht="14.25" r="99" s="24" spans="1:21">
+    <row r="99" spans="1:21" s="24" customFormat="1" ht="14.25">
       <c r="A99" s="24" t="s">
         <v>711</v>
       </c>
-      <c r="B99" s="24" t="s">
-        <v>7</v>
+      <c r="B99" s="44" t="s">
+        <v>175</v>
       </c>
       <c r="C99" s="24" t="s">
         <v>712</v>
@@ -15623,8 +15628,8 @@
       <c r="D99" s="24" t="s">
         <v>77</v>
       </c>
-      <c r="E99" s="24" t="s">
-        <v>78</v>
+      <c r="E99" s="44" t="s">
+        <v>175</v>
       </c>
       <c r="F99" s="24" t="s">
         <v>79</v>
@@ -15669,7 +15674,7 @@
         <v>8</v>
       </c>
     </row>
-    <row customFormat="1" ht="14.25" r="100" s="24" spans="1:21">
+    <row r="100" spans="1:21" s="24" customFormat="1" ht="14.25">
       <c r="A100" s="24" t="s">
         <v>715</v>
       </c>
@@ -15728,7 +15733,7 @@
         <v>37</v>
       </c>
     </row>
-    <row customFormat="1" ht="14.25" r="101" s="24" spans="1:21">
+    <row r="101" spans="1:21" s="24" customFormat="1" ht="14.25">
       <c r="A101" s="24" t="s">
         <v>719</v>
       </c>
@@ -15787,7 +15792,7 @@
         <v>16</v>
       </c>
     </row>
-    <row customFormat="1" ht="14.25" r="102" s="24" spans="1:21">
+    <row r="102" spans="1:21" s="24" customFormat="1" ht="14.25">
       <c r="A102" s="24" t="s">
         <v>749</v>
       </c>
@@ -15846,7 +15851,7 @@
         <v>37</v>
       </c>
     </row>
-    <row customFormat="1" ht="14.25" r="103" s="24" spans="1:21">
+    <row r="103" spans="1:21" s="24" customFormat="1" ht="14.25">
       <c r="A103" s="24" t="s">
         <v>755</v>
       </c>
@@ -15905,12 +15910,12 @@
         <v>16</v>
       </c>
     </row>
-    <row customFormat="1" ht="14.25" r="104" s="24" spans="1:21">
+    <row r="104" spans="1:21" s="24" customFormat="1" ht="14.25">
       <c r="A104" s="24" t="s">
         <v>765</v>
       </c>
-      <c r="B104" s="24" t="s">
-        <v>7</v>
+      <c r="B104" s="44" t="s">
+        <v>175</v>
       </c>
       <c r="C104" s="24" t="s">
         <v>766</v>
@@ -15918,8 +15923,8 @@
       <c r="D104" s="24" t="s">
         <v>84</v>
       </c>
-      <c r="E104" s="24" t="s">
-        <v>78</v>
+      <c r="E104" s="44" t="s">
+        <v>175</v>
       </c>
       <c r="F104" s="24" t="s">
         <v>79</v>
@@ -15964,12 +15969,12 @@
         <v>37</v>
       </c>
     </row>
-    <row customFormat="1" ht="14.25" r="105" s="24" spans="1:21">
+    <row r="105" spans="1:21" s="24" customFormat="1" ht="14.25">
       <c r="A105" s="24" t="s">
         <v>775</v>
       </c>
-      <c r="B105" s="24" t="s">
-        <v>7</v>
+      <c r="B105" s="44" t="s">
+        <v>175</v>
       </c>
       <c r="C105" s="24" t="s">
         <v>776</v>
@@ -15977,8 +15982,8 @@
       <c r="D105" s="24" t="s">
         <v>77</v>
       </c>
-      <c r="E105" s="24" t="s">
-        <v>78</v>
+      <c r="E105" s="44" t="s">
+        <v>175</v>
       </c>
       <c r="F105" s="24" t="s">
         <v>79</v>
@@ -16023,7 +16028,7 @@
         <v>37</v>
       </c>
     </row>
-    <row customFormat="1" ht="14.25" r="106" s="24" spans="1:21">
+    <row r="106" spans="1:21" s="24" customFormat="1" ht="14.25">
       <c r="A106" s="24" t="s">
         <v>781</v>
       </c>
@@ -16082,7 +16087,7 @@
         <v>37</v>
       </c>
     </row>
-    <row customFormat="1" ht="14.25" r="107" s="24" spans="1:21">
+    <row r="107" spans="1:21" s="24" customFormat="1" ht="14.25">
       <c r="A107" s="24" t="s">
         <v>791</v>
       </c>
@@ -16141,12 +16146,12 @@
         <v>8</v>
       </c>
     </row>
-    <row customFormat="1" ht="14.25" r="108" s="24" spans="1:21">
+    <row r="108" spans="1:21" s="24" customFormat="1" ht="14.25">
       <c r="A108" s="24" t="s">
         <v>796</v>
       </c>
-      <c r="B108" s="24" t="s">
-        <v>7</v>
+      <c r="B108" s="44" t="s">
+        <v>175</v>
       </c>
       <c r="C108" s="24" t="s">
         <v>797</v>
@@ -16154,8 +16159,8 @@
       <c r="D108" s="24" t="s">
         <v>77</v>
       </c>
-      <c r="E108" s="24" t="s">
-        <v>176</v>
+      <c r="E108" s="44" t="s">
+        <v>175</v>
       </c>
       <c r="F108" s="24" t="s">
         <v>79</v>
@@ -16200,12 +16205,12 @@
         <v>37</v>
       </c>
     </row>
-    <row customFormat="1" ht="14.25" r="109" s="24" spans="1:21">
+    <row r="109" spans="1:21" s="24" customFormat="1" ht="14.25">
       <c r="A109" s="24" t="s">
         <v>805</v>
       </c>
-      <c r="B109" s="24" t="s">
-        <v>7</v>
+      <c r="B109" s="44" t="s">
+        <v>175</v>
       </c>
       <c r="C109" s="24" t="s">
         <v>806</v>
@@ -16259,7 +16264,7 @@
         <v>37</v>
       </c>
     </row>
-    <row customFormat="1" ht="14.25" r="110" s="24" spans="1:21">
+    <row r="110" spans="1:21" s="24" customFormat="1" ht="14.25">
       <c r="A110" s="24" t="s">
         <v>813</v>
       </c>
@@ -16318,7 +16323,7 @@
         <v>16</v>
       </c>
     </row>
-    <row customFormat="1" ht="14.25" r="111" s="24" spans="1:21">
+    <row r="111" spans="1:21" s="24" customFormat="1" ht="14.25">
       <c r="A111" s="24" t="s">
         <v>818</v>
       </c>
@@ -16377,7 +16382,7 @@
         <v>16</v>
       </c>
     </row>
-    <row customFormat="1" ht="14.25" r="112" s="24" spans="1:21">
+    <row r="112" spans="1:21" s="24" customFormat="1" ht="14.25">
       <c r="A112" s="24" t="s">
         <v>823</v>
       </c>
@@ -16436,7 +16441,7 @@
         <v>16</v>
       </c>
     </row>
-    <row customFormat="1" ht="14.25" r="113" s="24" spans="1:21">
+    <row r="113" spans="1:21" s="24" customFormat="1" ht="14.25">
       <c r="A113" s="24" t="s">
         <v>828</v>
       </c>
@@ -16495,7 +16500,7 @@
         <v>16</v>
       </c>
     </row>
-    <row customFormat="1" ht="14.25" r="114" s="24" spans="1:21">
+    <row r="114" spans="1:21" s="24" customFormat="1" ht="14.25">
       <c r="A114" s="24" t="s">
         <v>839</v>
       </c>
@@ -16554,7 +16559,7 @@
         <v>8</v>
       </c>
     </row>
-    <row customFormat="1" ht="14.25" r="115" s="24" spans="1:21">
+    <row r="115" spans="1:21" s="24" customFormat="1" ht="14.25">
       <c r="A115" s="24" t="s">
         <v>848</v>
       </c>
@@ -16613,7 +16618,7 @@
         <v>328</v>
       </c>
     </row>
-    <row customFormat="1" ht="14.25" r="116" s="24" spans="1:21">
+    <row r="116" spans="1:21" s="24" customFormat="1" ht="14.25">
       <c r="A116" s="24" t="s">
         <v>856</v>
       </c>
@@ -16672,7 +16677,7 @@
         <v>8</v>
       </c>
     </row>
-    <row customFormat="1" ht="14.25" r="117" s="24" spans="1:21">
+    <row r="117" spans="1:21" s="24" customFormat="1" ht="14.25">
       <c r="A117" s="24" t="s">
         <v>863</v>
       </c>
@@ -16731,7 +16736,7 @@
         <v>16</v>
       </c>
     </row>
-    <row customFormat="1" ht="14.25" r="118" s="24" spans="1:21">
+    <row r="118" spans="1:21" s="24" customFormat="1" ht="14.25">
       <c r="A118" s="24" t="s">
         <v>872</v>
       </c>
@@ -16790,7 +16795,7 @@
         <v>37</v>
       </c>
     </row>
-    <row customFormat="1" ht="14.25" r="119" s="24" spans="1:21">
+    <row r="119" spans="1:21" s="24" customFormat="1" ht="14.25">
       <c r="A119" s="24" t="s">
         <v>876</v>
       </c>
@@ -16849,7 +16854,7 @@
         <v>16</v>
       </c>
     </row>
-    <row ht="12.75" r="120" spans="1:21">
+    <row r="120" spans="1:21" ht="12.75">
       <c r="A120">
         <v>119</v>
       </c>
@@ -16908,7 +16913,7 @@
         <v>884</v>
       </c>
     </row>
-    <row ht="12.75" r="121" spans="1:21">
+    <row r="121" spans="1:21" ht="12.75">
       <c r="A121" t="s">
         <v>917</v>
       </c>
@@ -16967,7 +16972,7 @@
         <v>884</v>
       </c>
     </row>
-    <row ht="12.75" r="122" spans="1:21">
+    <row r="122" spans="1:21" ht="12.75">
       <c r="A122" t="s">
         <v>922</v>
       </c>
@@ -17026,7 +17031,7 @@
         <v>884</v>
       </c>
     </row>
-    <row ht="12.75" r="123" spans="1:21">
+    <row r="123" spans="1:21" ht="12.75">
       <c r="A123" t="s">
         <v>929</v>
       </c>
@@ -17085,7 +17090,7 @@
         <v>884</v>
       </c>
     </row>
-    <row ht="12.75" r="124" spans="1:21">
+    <row r="124" spans="1:21" ht="12.75">
       <c r="A124" t="s">
         <v>934</v>
       </c>
@@ -17144,7 +17149,7 @@
         <v>884</v>
       </c>
     </row>
-    <row ht="12.75" r="125" spans="1:21">
+    <row r="125" spans="1:21" ht="12.75">
       <c r="A125" t="s">
         <v>937</v>
       </c>
@@ -17203,7 +17208,7 @@
         <v>884</v>
       </c>
     </row>
-    <row ht="12.75" r="126" spans="1:21">
+    <row r="126" spans="1:21" ht="12.75">
       <c r="A126" t="s">
         <v>941</v>
       </c>
@@ -17262,7 +17267,7 @@
         <v>884</v>
       </c>
     </row>
-    <row ht="12.75" r="127" spans="1:21">
+    <row r="127" spans="1:21" ht="12.75">
       <c r="A127" t="s">
         <v>947</v>
       </c>
@@ -17321,7 +17326,7 @@
         <v>884</v>
       </c>
     </row>
-    <row ht="12.75" r="128" spans="1:21">
+    <row r="128" spans="1:21" ht="12.75">
       <c r="A128" t="s">
         <v>953</v>
       </c>
@@ -17380,7 +17385,7 @@
         <v>884</v>
       </c>
     </row>
-    <row ht="12.75" r="129" spans="1:21">
+    <row r="129" spans="1:21" ht="12.75">
       <c r="A129" t="s">
         <v>958</v>
       </c>
@@ -17439,7 +17444,7 @@
         <v>884</v>
       </c>
     </row>
-    <row ht="12.75" r="130" spans="1:21">
+    <row r="130" spans="1:21" ht="12.75">
       <c r="A130" t="s">
         <v>963</v>
       </c>
@@ -17498,7 +17503,7 @@
         <v>884</v>
       </c>
     </row>
-    <row ht="12.75" r="131" spans="1:21">
+    <row r="131" spans="1:21" ht="12.75">
       <c r="A131" t="s">
         <v>967</v>
       </c>
@@ -17557,7 +17562,7 @@
         <v>884</v>
       </c>
     </row>
-    <row ht="12.75" r="132" spans="1:21">
+    <row r="132" spans="1:21" ht="12.75">
       <c r="A132" t="s">
         <v>970</v>
       </c>
@@ -17616,7 +17621,7 @@
         <v>884</v>
       </c>
     </row>
-    <row ht="12.75" r="133" spans="1:21">
+    <row r="133" spans="1:21" ht="12.75">
       <c r="A133" t="s">
         <v>974</v>
       </c>
@@ -17675,7 +17680,7 @@
         <v>884</v>
       </c>
     </row>
-    <row ht="12.75" r="134" spans="1:21">
+    <row r="134" spans="1:21" ht="12.75">
       <c r="A134" t="s">
         <v>979</v>
       </c>
@@ -17734,7 +17739,7 @@
         <v>884</v>
       </c>
     </row>
-    <row ht="12.75" r="135" spans="1:21">
+    <row r="135" spans="1:21" ht="12.75">
       <c r="A135" t="s">
         <v>982</v>
       </c>
@@ -17793,7 +17798,7 @@
         <v>884</v>
       </c>
     </row>
-    <row ht="12.75" r="136" spans="1:21">
+    <row r="136" spans="1:21" ht="12.75">
       <c r="A136" t="s">
         <v>987</v>
       </c>
@@ -17852,7 +17857,7 @@
         <v>884</v>
       </c>
     </row>
-    <row ht="12.75" r="137" spans="1:21">
+    <row r="137" spans="1:21" ht="12.75">
       <c r="A137" t="s">
         <v>993</v>
       </c>
@@ -17911,7 +17916,7 @@
         <v>884</v>
       </c>
     </row>
-    <row ht="12.75" r="138" spans="1:21">
+    <row r="138" spans="1:21" ht="12.75">
       <c r="A138" t="s">
         <v>999</v>
       </c>
@@ -17970,7 +17975,7 @@
         <v>884</v>
       </c>
     </row>
-    <row ht="12.75" r="139" spans="1:21">
+    <row r="139" spans="1:21" ht="12.75">
       <c r="A139" t="s">
         <v>1004</v>
       </c>
@@ -18029,7 +18034,7 @@
         <v>884</v>
       </c>
     </row>
-    <row ht="12.75" r="140" spans="1:21">
+    <row r="140" spans="1:21" ht="12.75">
       <c r="A140" t="s">
         <v>1008</v>
       </c>
@@ -18088,7 +18093,7 @@
         <v>884</v>
       </c>
     </row>
-    <row ht="12.75" r="141" spans="1:21">
+    <row r="141" spans="1:21" ht="12.75">
       <c r="A141" t="s">
         <v>1014</v>
       </c>
@@ -18147,7 +18152,7 @@
         <v>884</v>
       </c>
     </row>
-    <row customFormat="1" ht="14.25" r="142" s="24" spans="1:21">
+    <row r="142" spans="1:21" s="24" customFormat="1" ht="14.25">
       <c r="A142" s="24" t="s">
         <v>1019</v>
       </c>
@@ -18160,8 +18165,8 @@
       <c r="D142" s="24" t="s">
         <v>84</v>
       </c>
-      <c r="E142" s="44" t="s">
-        <v>175</v>
+      <c r="E142" t="s">
+        <v>78</v>
       </c>
       <c r="F142" s="24" t="s">
         <v>79</v>
@@ -18206,7 +18211,7 @@
         <v>884</v>
       </c>
     </row>
-    <row customFormat="1" ht="14.25" r="143" s="24" spans="1:21">
+    <row r="143" spans="1:21" s="24" customFormat="1" ht="14.25">
       <c r="A143" s="24" t="s">
         <v>1024</v>
       </c>
@@ -18219,8 +18224,8 @@
       <c r="D143" s="24" t="s">
         <v>77</v>
       </c>
-      <c r="E143" s="44" t="s">
-        <v>175</v>
+      <c r="E143" t="s">
+        <v>78</v>
       </c>
       <c r="F143" s="24" t="s">
         <v>238</v>
@@ -18267,9 +18272,13 @@
     </row>
   </sheetData>
   <customSheetViews>
-    <customSheetView filter="1" guid="{A7754112-A52F-4ABC-8778-92F04773E53C}" showAutoFilter="1">
-      <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
-      <autoFilter ref="A1:AD33" xr:uid="{A49EF74B-1004-4B97-B748-EDB857996977}">
+    <customSheetView guid="{C25CEB9E-BEC1-4982-90C4-50C84EE1B82A}" filter="1" showAutoFilter="1">
+      <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+      <autoFilter ref="A1:AD33" xr:uid="{46DFB8EC-B9DE-4DA0-897F-8BA479564939}"/>
+    </customSheetView>
+    <customSheetView guid="{A7754112-A52F-4ABC-8778-92F04773E53C}" filter="1" showAutoFilter="1">
+      <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+      <autoFilter ref="A1:AD33" xr:uid="{7C2225CF-E3B8-4D32-8047-690012F4B453}">
         <filterColumn colId="5">
           <filters blank="1">
             <filter val="Strathnairn"/>
@@ -18277,81 +18286,77 @@
         </filterColumn>
       </autoFilter>
     </customSheetView>
-    <customSheetView filter="1" guid="{C25CEB9E-BEC1-4982-90C4-50C84EE1B82A}" showAutoFilter="1">
-      <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
-      <autoFilter ref="A1:AD33" xr:uid="{2BCDFFB2-08C1-4FB5-8831-76A4EEA3B232}"/>
-    </customSheetView>
   </customSheetViews>
   <conditionalFormatting sqref="A1:AI1">
-    <cfRule dxfId="1" priority="1" type="notContainsBlanks">
+    <cfRule type="notContainsBlanks" dxfId="1" priority="1">
       <formula>LEN(TRIM(A1))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <hyperlinks>
-    <hyperlink r:id="rId1" ref="S2" xr:uid="{00000000-0004-0000-0100-000000000000}"/>
-    <hyperlink r:id="rId2" ref="S3" xr:uid="{00000000-0004-0000-0100-000001000000}"/>
-    <hyperlink r:id="rId3" ref="S4" xr:uid="{00000000-0004-0000-0100-000002000000}"/>
-    <hyperlink r:id="rId4" ref="S5" xr:uid="{00000000-0004-0000-0100-000003000000}"/>
-    <hyperlink r:id="rId5" ref="S6" xr:uid="{00000000-0004-0000-0100-000004000000}"/>
-    <hyperlink r:id="rId6" ref="S7" xr:uid="{00000000-0004-0000-0100-000006000000}"/>
-    <hyperlink r:id="rId7" ref="S8" xr:uid="{00000000-0004-0000-0100-000008000000}"/>
-    <hyperlink r:id="rId8" ref="S9" xr:uid="{00000000-0004-0000-0100-00000A000000}"/>
-    <hyperlink r:id="rId9" ref="S10" xr:uid="{00000000-0004-0000-0100-00000C000000}"/>
-    <hyperlink r:id="rId10" ref="S11" xr:uid="{00000000-0004-0000-0100-00000E000000}"/>
-    <hyperlink r:id="rId11" ref="S12" xr:uid="{00000000-0004-0000-0100-000010000000}"/>
-    <hyperlink r:id="rId12" ref="S14" xr:uid="{00000000-0004-0000-0100-000014000000}"/>
-    <hyperlink r:id="rId13" ref="S15" xr:uid="{00000000-0004-0000-0100-000016000000}"/>
-    <hyperlink r:id="rId14" ref="S16" xr:uid="{00000000-0004-0000-0100-000018000000}"/>
-    <hyperlink r:id="rId15" ref="S17" xr:uid="{00000000-0004-0000-0100-00001A000000}"/>
-    <hyperlink r:id="rId16" ref="S18" xr:uid="{00000000-0004-0000-0100-00001C000000}"/>
-    <hyperlink display="https://www.allhomes.com.au/strathnairn-act-2615?tid=178720657" r:id="rId17" ref="S19" xr:uid="{00000000-0004-0000-0100-00001E000000}"/>
-    <hyperlink r:id="rId18" ref="S20" xr:uid="{00000000-0004-0000-0100-000020000000}"/>
-    <hyperlink r:id="rId19" ref="S21" xr:uid="{00000000-0004-0000-0100-000022000000}"/>
-    <hyperlink r:id="rId20" ref="S22" xr:uid="{00000000-0004-0000-0100-000024000000}"/>
-    <hyperlink r:id="rId21" ref="S32" xr:uid="{00000000-0004-0000-0100-000031000000}"/>
-    <hyperlink r:id="rId22" ref="S31" xr:uid="{00000000-0004-0000-0100-000030000000}"/>
-    <hyperlink r:id="rId23" ref="S30" xr:uid="{00000000-0004-0000-0100-00002F000000}"/>
-    <hyperlink r:id="rId24" ref="S29" xr:uid="{00000000-0004-0000-0100-00002E000000}"/>
-    <hyperlink r:id="rId25" ref="S28" xr:uid="{00000000-0004-0000-0100-00002D000000}"/>
-    <hyperlink r:id="rId26" ref="S27" xr:uid="{00000000-0004-0000-0100-00002C000000}"/>
-    <hyperlink r:id="rId27" ref="S26" xr:uid="{00000000-0004-0000-0100-00002B000000}"/>
-    <hyperlink r:id="rId28" ref="S25" xr:uid="{00000000-0004-0000-0100-00002A000000}"/>
-    <hyperlink r:id="rId29" ref="S24" xr:uid="{00000000-0004-0000-0100-000028000000}"/>
-    <hyperlink display="https://www.allhomes.com.au/ginninderra-estate-act-2615?tid=174799089" r:id="rId30" ref="S23" xr:uid="{00000000-0004-0000-0100-000026000000}"/>
+    <hyperlink ref="S2" r:id="rId1" xr:uid="{00000000-0004-0000-0100-000000000000}"/>
+    <hyperlink ref="S3" r:id="rId2" xr:uid="{00000000-0004-0000-0100-000001000000}"/>
+    <hyperlink ref="S4" r:id="rId3" xr:uid="{00000000-0004-0000-0100-000002000000}"/>
+    <hyperlink ref="S5" r:id="rId4" xr:uid="{00000000-0004-0000-0100-000003000000}"/>
+    <hyperlink ref="S6" r:id="rId5" xr:uid="{00000000-0004-0000-0100-000004000000}"/>
+    <hyperlink ref="S7" r:id="rId6" xr:uid="{00000000-0004-0000-0100-000006000000}"/>
+    <hyperlink ref="S8" r:id="rId7" xr:uid="{00000000-0004-0000-0100-000008000000}"/>
+    <hyperlink ref="S9" r:id="rId8" xr:uid="{00000000-0004-0000-0100-00000A000000}"/>
+    <hyperlink ref="S10" r:id="rId9" xr:uid="{00000000-0004-0000-0100-00000C000000}"/>
+    <hyperlink ref="S11" r:id="rId10" xr:uid="{00000000-0004-0000-0100-00000E000000}"/>
+    <hyperlink ref="S12" r:id="rId11" xr:uid="{00000000-0004-0000-0100-000010000000}"/>
+    <hyperlink ref="S14" r:id="rId12" xr:uid="{00000000-0004-0000-0100-000014000000}"/>
+    <hyperlink ref="S15" r:id="rId13" xr:uid="{00000000-0004-0000-0100-000016000000}"/>
+    <hyperlink ref="S16" r:id="rId14" xr:uid="{00000000-0004-0000-0100-000018000000}"/>
+    <hyperlink ref="S17" r:id="rId15" xr:uid="{00000000-0004-0000-0100-00001A000000}"/>
+    <hyperlink ref="S18" r:id="rId16" xr:uid="{00000000-0004-0000-0100-00001C000000}"/>
+    <hyperlink ref="S19" r:id="rId17" display="https://www.allhomes.com.au/strathnairn-act-2615?tid=178720657" xr:uid="{00000000-0004-0000-0100-00001E000000}"/>
+    <hyperlink ref="S20" r:id="rId18" xr:uid="{00000000-0004-0000-0100-000020000000}"/>
+    <hyperlink ref="S21" r:id="rId19" xr:uid="{00000000-0004-0000-0100-000022000000}"/>
+    <hyperlink ref="S22" r:id="rId20" xr:uid="{00000000-0004-0000-0100-000024000000}"/>
+    <hyperlink ref="S32" r:id="rId21" xr:uid="{00000000-0004-0000-0100-000031000000}"/>
+    <hyperlink ref="S31" r:id="rId22" xr:uid="{00000000-0004-0000-0100-000030000000}"/>
+    <hyperlink ref="S30" r:id="rId23" xr:uid="{00000000-0004-0000-0100-00002F000000}"/>
+    <hyperlink ref="S29" r:id="rId24" xr:uid="{00000000-0004-0000-0100-00002E000000}"/>
+    <hyperlink ref="S28" r:id="rId25" xr:uid="{00000000-0004-0000-0100-00002D000000}"/>
+    <hyperlink ref="S27" r:id="rId26" xr:uid="{00000000-0004-0000-0100-00002C000000}"/>
+    <hyperlink ref="S26" r:id="rId27" xr:uid="{00000000-0004-0000-0100-00002B000000}"/>
+    <hyperlink ref="S25" r:id="rId28" xr:uid="{00000000-0004-0000-0100-00002A000000}"/>
+    <hyperlink ref="S24" r:id="rId29" xr:uid="{00000000-0004-0000-0100-000028000000}"/>
+    <hyperlink ref="S23" r:id="rId30" display="https://www.allhomes.com.au/ginninderra-estate-act-2615?tid=174799089" xr:uid="{00000000-0004-0000-0100-000026000000}"/>
   </hyperlinks>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
-  <pageSetup orientation="portrait" paperSize="9" r:id="rId31"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId31"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:AJ1"/>
+  <dimension ref="A1:AI1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="14.42578125" defaultRowHeight="15.75"/>
+  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="16.0" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" width="14.5703125" collapsed="true"/>
-    <col min="4" max="4" customWidth="true" width="16.85546875" collapsed="true"/>
-    <col min="8" max="8" customWidth="true" width="14.5703125" collapsed="true"/>
-    <col min="9" max="9" customWidth="true" width="13.140625" collapsed="true"/>
-    <col min="15" max="15" customWidth="true" width="20.85546875" collapsed="true"/>
-    <col min="21" max="22" customWidth="true" width="19.140625" collapsed="true"/>
-    <col min="23" max="23" customWidth="true" width="20.140625" collapsed="true"/>
-    <col min="24" max="24" customWidth="true" width="19.85546875" collapsed="true"/>
-    <col min="26" max="26" customWidth="true" width="15.85546875" collapsed="true"/>
-    <col min="27" max="27" customWidth="true" width="13.42578125" collapsed="true"/>
-    <col min="28" max="28" customWidth="true" width="15.140625" collapsed="true"/>
-    <col min="29" max="29" customWidth="true" width="16.140625" collapsed="true"/>
-    <col min="30" max="30" customWidth="true" width="15.85546875" collapsed="true"/>
+    <col min="1" max="1" width="16" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="14.5703125" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="16.85546875" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="14.5703125" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="13.140625" customWidth="1" collapsed="1"/>
+    <col min="15" max="15" width="20.85546875" customWidth="1" collapsed="1"/>
+    <col min="21" max="22" width="19.140625" customWidth="1" collapsed="1"/>
+    <col min="23" max="23" width="20.140625" customWidth="1" collapsed="1"/>
+    <col min="24" max="24" width="19.85546875" customWidth="1" collapsed="1"/>
+    <col min="26" max="26" width="15.85546875" customWidth="1" collapsed="1"/>
+    <col min="27" max="27" width="13.42578125" customWidth="1" collapsed="1"/>
+    <col min="28" max="28" width="15.140625" customWidth="1" collapsed="1"/>
+    <col min="29" max="29" width="16.140625" customWidth="1" collapsed="1"/>
+    <col min="30" max="30" width="15.85546875" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row customHeight="1" ht="15.75" r="1" spans="1:35">
+    <row r="1" spans="1:35" ht="15.75" customHeight="1">
       <c r="A1" s="1" t="s">
         <v>46</v>
       </c>
@@ -18450,37 +18455,37 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A1:AI1">
-    <cfRule dxfId="0" priority="1" type="notContainsBlanks">
+    <cfRule type="notContainsBlanks" dxfId="0" priority="1">
       <formula>LEN(TRIM(A1))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
-  <pageSetup orientation="portrait" paperSize="9" r:id="rId1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:H7"/>
+  <dimension ref="A1:G7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane activePane="bottomLeft" state="frozen" topLeftCell="A2" ySplit="1"/>
-      <selection activeCell="B7" pane="bottomLeft" sqref="B7"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D18" sqref="D18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="14.42578125" defaultRowHeight="15.75"/>
+  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="44.85546875" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="19.5703125" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" width="26.42578125" collapsed="true"/>
-    <col min="4" max="4" customWidth="true" width="36.140625" collapsed="true"/>
-    <col min="5" max="5" bestFit="true" customWidth="true" width="53.7109375" collapsed="true"/>
+    <col min="1" max="1" width="44.85546875" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="19.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="26.42578125" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="36.140625" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="53.7109375" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row ht="15" r="1" spans="1:7">
+    <row r="1" spans="1:7" ht="15">
       <c r="A1" s="30" t="s">
         <v>155</v>
       </c>
@@ -18503,7 +18508,7 @@
         <v>160</v>
       </c>
     </row>
-    <row customFormat="1" customHeight="1" ht="15.75" r="2" s="31" spans="1:7">
+    <row r="2" spans="1:7" s="31" customFormat="1" ht="15.75" customHeight="1">
       <c r="A2" s="31" t="s">
         <v>161</v>
       </c>
@@ -18526,7 +18531,7 @@
         <v>7</v>
       </c>
     </row>
-    <row customHeight="1" ht="15.75" r="3" spans="1:7">
+    <row r="3" spans="1:7" ht="15.75" customHeight="1">
       <c r="A3" s="31" t="s">
         <v>164</v>
       </c>
@@ -18543,7 +18548,7 @@
         <v>17</v>
       </c>
     </row>
-    <row customHeight="1" ht="15.75" r="4" spans="1:7">
+    <row r="4" spans="1:7" ht="15.75" customHeight="1">
       <c r="A4" s="31" t="s">
         <v>167</v>
       </c>
@@ -18560,7 +18565,7 @@
         <v>38</v>
       </c>
     </row>
-    <row customHeight="1" ht="15.75" r="5" spans="1:7">
+    <row r="5" spans="1:7" ht="15.75" customHeight="1">
       <c r="A5" s="35" t="s">
         <v>170</v>
       </c>
@@ -18577,7 +18582,7 @@
         <v>9</v>
       </c>
     </row>
-    <row customHeight="1" ht="15.75" r="6" spans="1:7">
+    <row r="6" spans="1:7" ht="15.75" customHeight="1">
       <c r="A6" t="s">
         <v>331</v>
       </c>
@@ -18594,7 +18599,7 @@
         <v>326</v>
       </c>
     </row>
-    <row customHeight="1" ht="15.75" r="7" spans="1:7">
+    <row r="7" spans="1:7" ht="15.75" customHeight="1">
       <c r="A7" s="47" t="s">
         <v>883</v>
       </c>
@@ -18613,16 +18618,16 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink r:id="rId1" ref="E2" xr:uid="{00000000-0004-0000-0300-000000000000}"/>
-    <hyperlink r:id="rId2" ref="E3" xr:uid="{00000000-0004-0000-0300-000001000000}"/>
-    <hyperlink r:id="rId3" ref="E4" xr:uid="{00000000-0004-0000-0300-000002000000}"/>
-    <hyperlink r:id="rId4" ref="E5" xr:uid="{00000000-0004-0000-0300-000003000000}"/>
-    <hyperlink r:id="rId5" ref="D6" xr:uid="{00000000-0004-0000-0300-000004000000}"/>
-    <hyperlink r:id="rId6" ref="E6" xr:uid="{00000000-0004-0000-0300-000005000000}"/>
-    <hyperlink r:id="rId7" ref="D7" xr:uid="{B34712F5-65E4-4DA3-B4D8-B5E126A91A19}"/>
-    <hyperlink r:id="rId8" ref="E7" xr:uid="{FAD2E722-F8D2-45E6-8DA2-DA530385A188}"/>
+    <hyperlink ref="E2" r:id="rId1" xr:uid="{00000000-0004-0000-0300-000000000000}"/>
+    <hyperlink ref="E3" r:id="rId2" xr:uid="{00000000-0004-0000-0300-000001000000}"/>
+    <hyperlink ref="E4" r:id="rId3" xr:uid="{00000000-0004-0000-0300-000002000000}"/>
+    <hyperlink ref="E5" r:id="rId4" xr:uid="{00000000-0004-0000-0300-000003000000}"/>
+    <hyperlink ref="D6" r:id="rId5" xr:uid="{00000000-0004-0000-0300-000004000000}"/>
+    <hyperlink ref="E6" r:id="rId6" xr:uid="{00000000-0004-0000-0300-000005000000}"/>
+    <hyperlink ref="D7" r:id="rId7" xr:uid="{B34712F5-65E4-4DA3-B4D8-B5E126A91A19}"/>
+    <hyperlink ref="E7" r:id="rId8" xr:uid="{FAD2E722-F8D2-45E6-8DA2-DA530385A188}"/>
   </hyperlinks>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
-  <pageSetup orientation="portrait" paperSize="9" r:id="rId9"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId9"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Scripts run (new listings)
</commit_message>
<xml_diff>
--- a/src/main/resources/InputTestdata/Listing details.xlsx
+++ b/src/main/resources/InputTestdata/Listing details.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Athavan\git\777Homes-2\777Homes-business\src\main\resources\InputTestdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EB074CDA-BACE-4B22-B76D-2C16A4404222}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{39C2DA6A-495D-4131-A512-45180B1D5B14}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Backlog" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3472" uniqueCount="1055">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3522" uniqueCount="1070">
   <si>
     <t>ID</t>
   </si>
@@ -4217,9 +4217,6 @@
     <t>https://www.allhomes.com.au/94-roden-cutler-drive-bonner-act-2914</t>
   </si>
   <si>
-    <t>https://www.allhomes.com.au/unit-14-85-holborow-avenue-denman-prospect-act-2611?tid=179787734</t>
-  </si>
-  <si>
     <t>155 Lawrence Wackett Crescent, Theodore ACT 2905</t>
   </si>
   <si>
@@ -5053,6 +5050,86 @@
   </si>
   <si>
     <t>https://cbrhome.flywheelstaging.com/?post_type=property&amp;p=8303&amp;preview=true</t>
+  </si>
+  <si>
+    <t>https://www.allhomes.com.au/unit-14-85-holborow-avenue-denman-prospect-act-2611</t>
+  </si>
+  <si>
+    <t>https://www.allhomes.com.au/7-carinya-street-queanbeyan-nsw-2620</t>
+  </si>
+  <si>
+    <t>https://www.allhomes.com.au/road-south-jerrabomberra-nsw-2620?tid=179875289</t>
+  </si>
+  <si>
+    <t>143</t>
+  </si>
+  <si>
+    <t>7 - 9 Carinya Street, Queanbeyan NSW 2620</t>
+  </si>
+  <si>
+    <t>Queanbeyan</t>
+  </si>
+  <si>
+    <t>Block/House: 1342/ -</t>
+  </si>
+  <si>
+    <t>An amazing opportunity to develop 2-blocks of lands near the CBD area. Total land size is 1,342 sqm approximate. Here are the facts and features to consider:
+&gt;&gt; 7 Carinya Street - 715 sqm, vacant land only. Rented for $200 p/m
+&gt;&gt; 9 Carinya Street - 627 sqm, 4-bedroom house, Rented for $275p/w
+&gt;&gt; Zone B3 - Commercial Core
+Permitted with Consent:
+Centre-based childcare facilities
+Commercial premises
+Community facilities
+Educational establishments
+Entertainment facilities
+Function centres
+Hotel or motel accommodation
+Information and education facilities
+Medical centres
+Oyster aquaculture
+Passenger transport facilities
+Recreation facilities (indoor)
+Registered clubs
+Respite Day care centres
+Restricted premises; Roads
+Tank-based aquaculture.
+What’s Nearby:
+- Queanbeyan Riverside Caravan Park
+- Queanbeyan District Hospital &amp; Health Service
+- Police Station
+- Peppertree Lodge
+- Riverside Football Stadium
+- Woolworths, Kmart, Coles, Aldi, Bharat Bazar
+- Queanbeyan Riverside Plaza
+- Hungry Jack’s, McDonald’s
+- Dan Murphy’s
+Call Shaun for further details to discuss this opportunity before you miss out.</t>
+  </si>
+  <si>
+    <t>144</t>
+  </si>
+  <si>
+    <t>Road, South Jerrabomberra NSW 2620</t>
+  </si>
+  <si>
+    <t>South Jerrabomberra</t>
+  </si>
+  <si>
+    <t>Block/House: 129/ -</t>
+  </si>
+  <si>
+    <t>The Opportunity: 3 bedroom 2 bathroom and a double lock-up garage, a rare product on a separate title with no body corporate fees. Most of all, it being in the south, such a location highly sought after but rarely found. Today, you can own a pocket of South Jerra, what an opportunity!
+The Dream: Precious gem that will inspire you to live life to the fullest, low maintenance weekend cleaning, and endless sunsets with sparkling.</t>
+  </si>
+  <si>
+    <t>Draft</t>
+  </si>
+  <si>
+    <t>https://www.777homes.com.au/?post_type=property&amp;p=8691&amp;preview=true</t>
+  </si>
+  <si>
+    <t>https://www.777homes.com.au/?post_type=property&amp;p=8689&amp;preview=true</t>
   </si>
 </sst>
 </file>
@@ -5225,7 +5302,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="10">
+  <fills count="11">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -5279,6 +5356,11 @@
         <bgColor indexed="2"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="mediumGray">
+        <bgColor indexed="2"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -5293,7 +5375,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="26" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="48">
+  <cellXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -5394,6 +5476,7 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="28" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -5630,11 +5713,11 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:AB143"/>
+  <dimension ref="A1:AB145"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A116" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D150" sqref="D150"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A113" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F148" sqref="F148"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1"/>
@@ -7136,7 +7219,7 @@
         <v>729</v>
       </c>
       <c r="D38" s="4" t="s">
-        <v>7</v>
+        <v>14</v>
       </c>
       <c r="F38" s="28" t="s">
         <v>691</v>
@@ -7182,7 +7265,7 @@
         <v>731</v>
       </c>
       <c r="D40" s="4" t="s">
-        <v>7</v>
+        <v>14</v>
       </c>
       <c r="F40" s="28" t="s">
         <v>691</v>
@@ -7874,7 +7957,7 @@
         <v>573</v>
       </c>
       <c r="D72" s="4" t="s">
-        <v>7</v>
+        <v>14</v>
       </c>
       <c r="F72" s="2" t="s">
         <v>691</v>
@@ -8426,7 +8509,7 @@
         <v>686</v>
       </c>
       <c r="D96" s="4" t="s">
-        <v>7</v>
+        <v>14</v>
       </c>
       <c r="F96" s="2" t="s">
         <v>691</v>
@@ -8840,7 +8923,7 @@
         <v>841</v>
       </c>
       <c r="D114" s="4" t="s">
-        <v>7</v>
+        <v>14</v>
       </c>
       <c r="F114" s="2" t="s">
         <v>691</v>
@@ -8863,7 +8946,7 @@
         <v>853</v>
       </c>
       <c r="D115" s="4" t="s">
-        <v>7</v>
+        <v>14</v>
       </c>
       <c r="F115" s="2" t="s">
         <v>691</v>
@@ -8886,7 +8969,7 @@
         <v>861</v>
       </c>
       <c r="D116" s="4" t="s">
-        <v>7</v>
+        <v>14</v>
       </c>
       <c r="F116" s="2" t="s">
         <v>691</v>
@@ -8932,7 +9015,7 @@
         <v>14</v>
       </c>
       <c r="F118" s="2" t="s">
-        <v>691</v>
+        <v>1052</v>
       </c>
       <c r="G118" t="s">
         <v>37</v>
@@ -8972,7 +9055,7 @@
         <v>888</v>
       </c>
       <c r="C120" s="42" t="s">
-        <v>1029</v>
+        <v>1028</v>
       </c>
       <c r="D120" s="4" t="s">
         <v>7</v>
@@ -8981,7 +9064,7 @@
         <v>692</v>
       </c>
       <c r="G120" t="s">
-        <v>1051</v>
+        <v>1050</v>
       </c>
       <c r="H120" t="s">
         <v>887</v>
@@ -8995,7 +9078,7 @@
         <v>889</v>
       </c>
       <c r="C121" t="s">
-        <v>1030</v>
+        <v>1029</v>
       </c>
       <c r="D121" s="4" t="s">
         <v>7</v>
@@ -9004,7 +9087,7 @@
         <v>692</v>
       </c>
       <c r="G121" t="s">
-        <v>1051</v>
+        <v>1050</v>
       </c>
       <c r="H121" t="s">
         <v>887</v>
@@ -9018,7 +9101,7 @@
         <v>890</v>
       </c>
       <c r="C122" s="42" t="s">
-        <v>1031</v>
+        <v>1030</v>
       </c>
       <c r="D122" s="4" t="s">
         <v>7</v>
@@ -9027,7 +9110,7 @@
         <v>692</v>
       </c>
       <c r="G122" t="s">
-        <v>1051</v>
+        <v>1050</v>
       </c>
       <c r="H122" t="s">
         <v>887</v>
@@ -9041,7 +9124,7 @@
         <v>891</v>
       </c>
       <c r="C123" s="42" t="s">
-        <v>1032</v>
+        <v>1031</v>
       </c>
       <c r="D123" s="4" t="s">
         <v>7</v>
@@ -9050,7 +9133,7 @@
         <v>692</v>
       </c>
       <c r="G123" t="s">
-        <v>1051</v>
+        <v>1050</v>
       </c>
       <c r="H123" t="s">
         <v>887</v>
@@ -9064,7 +9147,7 @@
         <v>892</v>
       </c>
       <c r="C124" s="42" t="s">
-        <v>1033</v>
+        <v>1032</v>
       </c>
       <c r="D124" s="4" t="s">
         <v>7</v>
@@ -9073,7 +9156,7 @@
         <v>692</v>
       </c>
       <c r="G124" t="s">
-        <v>1051</v>
+        <v>1050</v>
       </c>
       <c r="H124" t="s">
         <v>887</v>
@@ -9087,7 +9170,7 @@
         <v>893</v>
       </c>
       <c r="C125" s="42" t="s">
-        <v>1034</v>
+        <v>1033</v>
       </c>
       <c r="D125" s="4" t="s">
         <v>7</v>
@@ -9096,7 +9179,7 @@
         <v>692</v>
       </c>
       <c r="G125" t="s">
-        <v>1051</v>
+        <v>1050</v>
       </c>
       <c r="H125" t="s">
         <v>887</v>
@@ -9110,7 +9193,7 @@
         <v>894</v>
       </c>
       <c r="C126" s="42" t="s">
-        <v>1035</v>
+        <v>1034</v>
       </c>
       <c r="D126" s="4" t="s">
         <v>7</v>
@@ -9119,7 +9202,7 @@
         <v>692</v>
       </c>
       <c r="G126" t="s">
-        <v>1051</v>
+        <v>1050</v>
       </c>
       <c r="H126" t="s">
         <v>887</v>
@@ -9133,7 +9216,7 @@
         <v>895</v>
       </c>
       <c r="C127" s="42" t="s">
-        <v>1036</v>
+        <v>1035</v>
       </c>
       <c r="D127" s="4" t="s">
         <v>7</v>
@@ -9142,7 +9225,7 @@
         <v>692</v>
       </c>
       <c r="G127" t="s">
-        <v>1051</v>
+        <v>1050</v>
       </c>
       <c r="H127" t="s">
         <v>887</v>
@@ -9156,7 +9239,7 @@
         <v>896</v>
       </c>
       <c r="C128" s="42" t="s">
-        <v>1048</v>
+        <v>1047</v>
       </c>
       <c r="D128" s="4" t="s">
         <v>7</v>
@@ -9165,7 +9248,7 @@
         <v>692</v>
       </c>
       <c r="G128" t="s">
-        <v>1051</v>
+        <v>1050</v>
       </c>
       <c r="H128" t="s">
         <v>887</v>
@@ -9179,7 +9262,7 @@
         <v>897</v>
       </c>
       <c r="C129" t="s">
-        <v>1049</v>
+        <v>1048</v>
       </c>
       <c r="D129" s="4" t="s">
         <v>7</v>
@@ -9188,7 +9271,7 @@
         <v>692</v>
       </c>
       <c r="G129" t="s">
-        <v>1051</v>
+        <v>1050</v>
       </c>
       <c r="H129" t="s">
         <v>887</v>
@@ -9202,7 +9285,7 @@
         <v>898</v>
       </c>
       <c r="C130" s="42" t="s">
-        <v>1050</v>
+        <v>1049</v>
       </c>
       <c r="D130" s="4" t="s">
         <v>7</v>
@@ -9211,7 +9294,7 @@
         <v>692</v>
       </c>
       <c r="G130" t="s">
-        <v>1051</v>
+        <v>1050</v>
       </c>
       <c r="H130" t="s">
         <v>887</v>
@@ -9225,7 +9308,7 @@
         <v>899</v>
       </c>
       <c r="C131" s="42" t="s">
-        <v>1037</v>
+        <v>1036</v>
       </c>
       <c r="D131" s="4" t="s">
         <v>7</v>
@@ -9234,7 +9317,7 @@
         <v>692</v>
       </c>
       <c r="G131" t="s">
-        <v>1051</v>
+        <v>1050</v>
       </c>
       <c r="H131" t="s">
         <v>887</v>
@@ -9248,7 +9331,7 @@
         <v>900</v>
       </c>
       <c r="C132" s="42" t="s">
-        <v>1038</v>
+        <v>1037</v>
       </c>
       <c r="D132" s="4" t="s">
         <v>7</v>
@@ -9257,7 +9340,7 @@
         <v>692</v>
       </c>
       <c r="G132" t="s">
-        <v>1051</v>
+        <v>1050</v>
       </c>
       <c r="H132" t="s">
         <v>887</v>
@@ -9271,7 +9354,7 @@
         <v>901</v>
       </c>
       <c r="C133" s="42" t="s">
-        <v>1039</v>
+        <v>1038</v>
       </c>
       <c r="D133" s="4" t="s">
         <v>7</v>
@@ -9280,7 +9363,7 @@
         <v>692</v>
       </c>
       <c r="G133" t="s">
-        <v>1051</v>
+        <v>1050</v>
       </c>
       <c r="H133" t="s">
         <v>887</v>
@@ -9294,7 +9377,7 @@
         <v>902</v>
       </c>
       <c r="C134" t="s">
-        <v>1040</v>
+        <v>1039</v>
       </c>
       <c r="D134" s="4" t="s">
         <v>7</v>
@@ -9303,7 +9386,7 @@
         <v>692</v>
       </c>
       <c r="G134" t="s">
-        <v>1051</v>
+        <v>1050</v>
       </c>
       <c r="H134" t="s">
         <v>887</v>
@@ -9317,7 +9400,7 @@
         <v>903</v>
       </c>
       <c r="C135" t="s">
-        <v>1041</v>
+        <v>1040</v>
       </c>
       <c r="D135" s="4" t="s">
         <v>7</v>
@@ -9326,7 +9409,7 @@
         <v>692</v>
       </c>
       <c r="G135" t="s">
-        <v>1051</v>
+        <v>1050</v>
       </c>
       <c r="H135" t="s">
         <v>887</v>
@@ -9340,7 +9423,7 @@
         <v>904</v>
       </c>
       <c r="C136" s="42" t="s">
-        <v>1042</v>
+        <v>1041</v>
       </c>
       <c r="D136" s="4" t="s">
         <v>7</v>
@@ -9349,7 +9432,7 @@
         <v>692</v>
       </c>
       <c r="G136" t="s">
-        <v>1051</v>
+        <v>1050</v>
       </c>
       <c r="H136" t="s">
         <v>887</v>
@@ -9363,7 +9446,7 @@
         <v>905</v>
       </c>
       <c r="C137" s="42" t="s">
-        <v>1043</v>
+        <v>1042</v>
       </c>
       <c r="D137" s="4" t="s">
         <v>7</v>
@@ -9372,7 +9455,7 @@
         <v>692</v>
       </c>
       <c r="G137" t="s">
-        <v>1051</v>
+        <v>1050</v>
       </c>
       <c r="H137" t="s">
         <v>887</v>
@@ -9386,7 +9469,7 @@
         <v>906</v>
       </c>
       <c r="C138" t="s">
-        <v>1044</v>
+        <v>1043</v>
       </c>
       <c r="D138" s="4" t="s">
         <v>7</v>
@@ -9395,7 +9478,7 @@
         <v>692</v>
       </c>
       <c r="G138" t="s">
-        <v>1051</v>
+        <v>1050</v>
       </c>
       <c r="H138" t="s">
         <v>887</v>
@@ -9409,7 +9492,7 @@
         <v>907</v>
       </c>
       <c r="C139" t="s">
-        <v>1045</v>
+        <v>1044</v>
       </c>
       <c r="D139" s="4" t="s">
         <v>7</v>
@@ -9418,7 +9501,7 @@
         <v>692</v>
       </c>
       <c r="G139" t="s">
-        <v>1051</v>
+        <v>1050</v>
       </c>
       <c r="H139" t="s">
         <v>887</v>
@@ -9432,7 +9515,7 @@
         <v>908</v>
       </c>
       <c r="C140" t="s">
-        <v>1046</v>
+        <v>1045</v>
       </c>
       <c r="D140" s="4" t="s">
         <v>7</v>
@@ -9441,7 +9524,7 @@
         <v>692</v>
       </c>
       <c r="G140" t="s">
-        <v>1051</v>
+        <v>1050</v>
       </c>
       <c r="H140" t="s">
         <v>887</v>
@@ -9455,7 +9538,7 @@
         <v>909</v>
       </c>
       <c r="C141" s="42" t="s">
-        <v>1047</v>
+        <v>1046</v>
       </c>
       <c r="D141" s="4" t="s">
         <v>7</v>
@@ -9464,7 +9547,7 @@
         <v>692</v>
       </c>
       <c r="G141" t="s">
-        <v>1051</v>
+        <v>1050</v>
       </c>
       <c r="H141" t="s">
         <v>887</v>
@@ -9478,7 +9561,7 @@
         <v>910</v>
       </c>
       <c r="C142" t="s">
-        <v>1052</v>
+        <v>1051</v>
       </c>
       <c r="D142" s="40" t="s">
         <v>14</v>
@@ -9487,7 +9570,7 @@
         <v>692</v>
       </c>
       <c r="G142" t="s">
-        <v>1051</v>
+        <v>1050</v>
       </c>
       <c r="H142" t="s">
         <v>887</v>
@@ -9497,11 +9580,11 @@
       <c r="A143">
         <v>142</v>
       </c>
-      <c r="B143" t="s">
-        <v>911</v>
+      <c r="B143" s="42" t="s">
+        <v>1054</v>
       </c>
       <c r="C143" t="s">
-        <v>1054</v>
+        <v>1053</v>
       </c>
       <c r="D143" s="40" t="s">
         <v>14</v>
@@ -9510,10 +9593,56 @@
         <v>692</v>
       </c>
       <c r="G143" t="s">
-        <v>1051</v>
+        <v>1050</v>
       </c>
       <c r="H143" t="s">
         <v>887</v>
+      </c>
+    </row>
+    <row r="144" spans="1:8" ht="12.75">
+      <c r="A144">
+        <v>143</v>
+      </c>
+      <c r="B144" s="42" t="s">
+        <v>1055</v>
+      </c>
+      <c r="C144" t="s">
+        <v>1069</v>
+      </c>
+      <c r="D144" s="48" t="s">
+        <v>1067</v>
+      </c>
+      <c r="F144" s="2" t="s">
+        <v>1052</v>
+      </c>
+      <c r="G144" t="s">
+        <v>37</v>
+      </c>
+      <c r="H144" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="145" spans="1:8" ht="12.75">
+      <c r="A145">
+        <v>144</v>
+      </c>
+      <c r="B145" t="s">
+        <v>1056</v>
+      </c>
+      <c r="C145" t="s">
+        <v>1068</v>
+      </c>
+      <c r="D145" s="48" t="s">
+        <v>1067</v>
+      </c>
+      <c r="F145" s="2" t="s">
+        <v>692</v>
+      </c>
+      <c r="G145" t="s">
+        <v>16</v>
+      </c>
+      <c r="H145" t="s">
+        <v>431</v>
       </c>
     </row>
   </sheetData>
@@ -9692,9 +9821,11 @@
     <hyperlink ref="C136" r:id="rId172" xr:uid="{E14EBE84-3FBA-44D8-B082-69967148B456}"/>
     <hyperlink ref="C137" r:id="rId173" xr:uid="{CC0D1827-F782-476A-9312-1BAA88B7D496}"/>
     <hyperlink ref="C141" r:id="rId174" xr:uid="{1528B515-167A-4838-B645-B63CD0312C05}"/>
+    <hyperlink ref="B143" r:id="rId175" xr:uid="{50B775B1-8A20-4A55-90CA-EC152D3C2098}"/>
+    <hyperlink ref="B144" r:id="rId176" xr:uid="{F6EFF9E5-8AC0-4C40-A2A8-62DF9BB671E9}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId175"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId177"/>
 </worksheet>
 </file>
 
@@ -9703,11 +9834,11 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:AI143"/>
+  <dimension ref="A1:AI145"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A113" workbookViewId="0">
+    <sheetView topLeftCell="A113" workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="E146" sqref="E146"/>
+      <selection pane="topRight" activeCell="C148" sqref="C148"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1"/>
@@ -16873,7 +17004,7 @@
         <v>7</v>
       </c>
       <c r="C120" s="24" t="s">
-        <v>912</v>
+        <v>911</v>
       </c>
       <c r="D120" s="24" t="s">
         <v>84</v>
@@ -16882,10 +17013,10 @@
         <v>78</v>
       </c>
       <c r="F120" s="24" t="s">
+        <v>912</v>
+      </c>
+      <c r="G120" s="24" t="s">
         <v>913</v>
-      </c>
-      <c r="G120" s="24" t="s">
-        <v>914</v>
       </c>
       <c r="H120" s="24" t="s">
         <v>202</v>
@@ -16897,7 +17028,7 @@
         <v>202</v>
       </c>
       <c r="L120" s="24" t="s">
-        <v>915</v>
+        <v>914</v>
       </c>
       <c r="M120" s="24" t="s">
         <v>205</v>
@@ -16912,27 +17043,27 @@
         <v>202</v>
       </c>
       <c r="R120" s="24" t="s">
-        <v>912</v>
+        <v>911</v>
       </c>
       <c r="S120" s="24" t="s">
-        <v>916</v>
+        <v>915</v>
       </c>
       <c r="T120" s="24" t="s">
         <v>692</v>
       </c>
       <c r="U120" s="24" t="s">
-        <v>1051</v>
+        <v>1050</v>
       </c>
     </row>
     <row r="121" spans="1:21" s="24" customFormat="1" ht="14.25">
       <c r="A121" s="24" t="s">
-        <v>917</v>
+        <v>916</v>
       </c>
       <c r="B121" s="24" t="s">
         <v>7</v>
       </c>
       <c r="C121" s="24" t="s">
-        <v>918</v>
+        <v>917</v>
       </c>
       <c r="D121" s="24" t="s">
         <v>84</v>
@@ -16944,10 +17075,10 @@
         <v>210</v>
       </c>
       <c r="G121" s="24" t="s">
+        <v>918</v>
+      </c>
+      <c r="H121" s="24" t="s">
         <v>919</v>
-      </c>
-      <c r="H121" s="24" t="s">
-        <v>920</v>
       </c>
       <c r="I121" s="24" t="s">
         <v>201</v>
@@ -16956,7 +17087,7 @@
         <v>202</v>
       </c>
       <c r="L121" s="24" t="s">
-        <v>915</v>
+        <v>914</v>
       </c>
       <c r="M121" s="24" t="s">
         <v>204</v>
@@ -16971,27 +17102,27 @@
         <v>207</v>
       </c>
       <c r="R121" s="24" t="s">
-        <v>918</v>
+        <v>917</v>
       </c>
       <c r="S121" s="24" t="s">
-        <v>921</v>
+        <v>920</v>
       </c>
       <c r="T121" s="24" t="s">
         <v>692</v>
       </c>
       <c r="U121" s="24" t="s">
-        <v>1051</v>
+        <v>1050</v>
       </c>
     </row>
     <row r="122" spans="1:21" s="24" customFormat="1" ht="14.25">
       <c r="A122" s="24" t="s">
-        <v>922</v>
+        <v>921</v>
       </c>
       <c r="B122" s="24" t="s">
         <v>7</v>
       </c>
       <c r="C122" s="24" t="s">
-        <v>923</v>
+        <v>922</v>
       </c>
       <c r="D122" s="24" t="s">
         <v>77</v>
@@ -17000,13 +17131,13 @@
         <v>78</v>
       </c>
       <c r="F122" s="24" t="s">
+        <v>923</v>
+      </c>
+      <c r="G122" s="24" t="s">
         <v>924</v>
       </c>
-      <c r="G122" s="24" t="s">
+      <c r="H122" s="24" t="s">
         <v>925</v>
-      </c>
-      <c r="H122" s="24" t="s">
-        <v>926</v>
       </c>
       <c r="I122" s="24" t="s">
         <v>201</v>
@@ -17015,7 +17146,7 @@
         <v>212</v>
       </c>
       <c r="L122" s="24" t="s">
-        <v>927</v>
+        <v>926</v>
       </c>
       <c r="M122" s="24" t="s">
         <v>207</v>
@@ -17030,27 +17161,27 @@
         <v>202</v>
       </c>
       <c r="R122" s="24" t="s">
-        <v>923</v>
+        <v>922</v>
       </c>
       <c r="S122" s="24" t="s">
-        <v>928</v>
+        <v>927</v>
       </c>
       <c r="T122" s="24" t="s">
         <v>692</v>
       </c>
       <c r="U122" s="24" t="s">
-        <v>1051</v>
+        <v>1050</v>
       </c>
     </row>
     <row r="123" spans="1:21" s="24" customFormat="1" ht="14.25">
       <c r="A123" s="24" t="s">
-        <v>929</v>
+        <v>928</v>
       </c>
       <c r="B123" s="24" t="s">
         <v>7</v>
       </c>
       <c r="C123" s="24" t="s">
-        <v>930</v>
+        <v>929</v>
       </c>
       <c r="D123" s="24" t="s">
         <v>84</v>
@@ -17071,10 +17202,10 @@
         <v>201</v>
       </c>
       <c r="K123" s="24" t="s">
+        <v>930</v>
+      </c>
+      <c r="L123" s="24" t="s">
         <v>931</v>
-      </c>
-      <c r="L123" s="24" t="s">
-        <v>932</v>
       </c>
       <c r="M123" s="24" t="s">
         <v>206</v>
@@ -17089,27 +17220,27 @@
         <v>202</v>
       </c>
       <c r="R123" s="24" t="s">
-        <v>930</v>
+        <v>929</v>
       </c>
       <c r="S123" s="24" t="s">
-        <v>933</v>
+        <v>932</v>
       </c>
       <c r="T123" s="24" t="s">
         <v>692</v>
       </c>
       <c r="U123" s="24" t="s">
-        <v>1051</v>
+        <v>1050</v>
       </c>
     </row>
     <row r="124" spans="1:21" s="24" customFormat="1" ht="14.25">
       <c r="A124" s="24" t="s">
-        <v>934</v>
+        <v>933</v>
       </c>
       <c r="B124" s="24" t="s">
         <v>7</v>
       </c>
       <c r="C124" s="24" t="s">
-        <v>935</v>
+        <v>934</v>
       </c>
       <c r="D124" s="24" t="s">
         <v>84</v>
@@ -17148,27 +17279,27 @@
         <v>269</v>
       </c>
       <c r="R124" s="24" t="s">
+        <v>934</v>
+      </c>
+      <c r="S124" s="24" t="s">
         <v>935</v>
-      </c>
-      <c r="S124" s="24" t="s">
-        <v>936</v>
       </c>
       <c r="T124" s="24" t="s">
         <v>692</v>
       </c>
       <c r="U124" s="24" t="s">
-        <v>1051</v>
+        <v>1050</v>
       </c>
     </row>
     <row r="125" spans="1:21" s="24" customFormat="1" ht="14.25">
       <c r="A125" s="24" t="s">
-        <v>937</v>
+        <v>936</v>
       </c>
       <c r="B125" s="24" t="s">
         <v>7</v>
       </c>
       <c r="C125" s="24" t="s">
-        <v>938</v>
+        <v>937</v>
       </c>
       <c r="D125" s="24" t="s">
         <v>77</v>
@@ -17177,10 +17308,10 @@
         <v>78</v>
       </c>
       <c r="F125" s="24" t="s">
-        <v>913</v>
+        <v>912</v>
       </c>
       <c r="G125" s="24" t="s">
-        <v>939</v>
+        <v>938</v>
       </c>
       <c r="H125" s="24" t="s">
         <v>202</v>
@@ -17207,27 +17338,27 @@
         <v>269</v>
       </c>
       <c r="R125" s="24" t="s">
-        <v>938</v>
+        <v>937</v>
       </c>
       <c r="S125" s="24" t="s">
-        <v>940</v>
+        <v>939</v>
       </c>
       <c r="T125" s="24" t="s">
         <v>692</v>
       </c>
       <c r="U125" s="24" t="s">
-        <v>1051</v>
+        <v>1050</v>
       </c>
     </row>
     <row r="126" spans="1:21" s="24" customFormat="1" ht="14.25">
       <c r="A126" s="24" t="s">
-        <v>941</v>
+        <v>940</v>
       </c>
       <c r="B126" s="24" t="s">
         <v>7</v>
       </c>
       <c r="C126" s="24" t="s">
-        <v>942</v>
+        <v>941</v>
       </c>
       <c r="D126" s="24" t="s">
         <v>77</v>
@@ -17248,10 +17379,10 @@
         <v>201</v>
       </c>
       <c r="K126" s="24" t="s">
+        <v>942</v>
+      </c>
+      <c r="L126" s="24" t="s">
         <v>943</v>
-      </c>
-      <c r="L126" s="24" t="s">
-        <v>944</v>
       </c>
       <c r="M126" s="24" t="s">
         <v>269</v>
@@ -17260,33 +17391,33 @@
         <v>269</v>
       </c>
       <c r="P126" s="24" t="s">
-        <v>945</v>
+        <v>944</v>
       </c>
       <c r="Q126" s="24" t="s">
         <v>269</v>
       </c>
       <c r="R126" s="24" t="s">
-        <v>942</v>
+        <v>941</v>
       </c>
       <c r="S126" s="24" t="s">
-        <v>946</v>
+        <v>945</v>
       </c>
       <c r="T126" s="24" t="s">
         <v>692</v>
       </c>
       <c r="U126" s="24" t="s">
-        <v>1051</v>
+        <v>1050</v>
       </c>
     </row>
     <row r="127" spans="1:21" s="24" customFormat="1" ht="14.25">
       <c r="A127" s="24" t="s">
-        <v>947</v>
+        <v>946</v>
       </c>
       <c r="B127" s="24" t="s">
         <v>7</v>
       </c>
       <c r="C127" s="24" t="s">
-        <v>948</v>
+        <v>947</v>
       </c>
       <c r="D127" s="24" t="s">
         <v>84</v>
@@ -17301,16 +17432,16 @@
         <v>85</v>
       </c>
       <c r="H127" s="24" t="s">
-        <v>949</v>
+        <v>948</v>
       </c>
       <c r="I127" s="24" t="s">
         <v>201</v>
       </c>
       <c r="K127" s="24" t="s">
+        <v>949</v>
+      </c>
+      <c r="L127" s="24" t="s">
         <v>950</v>
-      </c>
-      <c r="L127" s="24" t="s">
-        <v>951</v>
       </c>
       <c r="M127" s="24" t="s">
         <v>204</v>
@@ -17325,27 +17456,27 @@
         <v>207</v>
       </c>
       <c r="R127" s="24" t="s">
-        <v>948</v>
+        <v>947</v>
       </c>
       <c r="S127" s="24" t="s">
-        <v>952</v>
+        <v>951</v>
       </c>
       <c r="T127" s="24" t="s">
         <v>692</v>
       </c>
       <c r="U127" s="24" t="s">
-        <v>1051</v>
+        <v>1050</v>
       </c>
     </row>
     <row r="128" spans="1:21" s="24" customFormat="1" ht="14.25">
       <c r="A128" s="24" t="s">
-        <v>953</v>
+        <v>952</v>
       </c>
       <c r="B128" s="24" t="s">
         <v>7</v>
       </c>
       <c r="C128" s="24" t="s">
-        <v>954</v>
+        <v>953</v>
       </c>
       <c r="D128" s="24" t="s">
         <v>77</v>
@@ -17360,7 +17491,7 @@
         <v>85</v>
       </c>
       <c r="H128" s="24" t="s">
-        <v>955</v>
+        <v>954</v>
       </c>
       <c r="I128" s="24" t="s">
         <v>201</v>
@@ -17369,7 +17500,7 @@
         <v>359</v>
       </c>
       <c r="L128" s="24" t="s">
-        <v>956</v>
+        <v>955</v>
       </c>
       <c r="M128" s="24" t="s">
         <v>207</v>
@@ -17384,27 +17515,27 @@
         <v>202</v>
       </c>
       <c r="R128" s="24" t="s">
-        <v>954</v>
+        <v>953</v>
       </c>
       <c r="S128" s="24" t="s">
-        <v>957</v>
+        <v>956</v>
       </c>
       <c r="T128" s="24" t="s">
         <v>692</v>
       </c>
       <c r="U128" s="24" t="s">
-        <v>1051</v>
+        <v>1050</v>
       </c>
     </row>
     <row r="129" spans="1:21" s="24" customFormat="1" ht="14.25">
       <c r="A129" s="24" t="s">
-        <v>958</v>
+        <v>957</v>
       </c>
       <c r="B129" s="24" t="s">
         <v>7</v>
       </c>
       <c r="C129" s="24" t="s">
-        <v>959</v>
+        <v>958</v>
       </c>
       <c r="D129" s="24" t="s">
         <v>77</v>
@@ -17419,7 +17550,7 @@
         <v>85</v>
       </c>
       <c r="H129" s="24" t="s">
-        <v>960</v>
+        <v>959</v>
       </c>
       <c r="I129" s="24" t="s">
         <v>201</v>
@@ -17428,7 +17559,7 @@
         <v>364</v>
       </c>
       <c r="L129" s="24" t="s">
-        <v>961</v>
+        <v>960</v>
       </c>
       <c r="M129" s="24" t="s">
         <v>269</v>
@@ -17443,27 +17574,27 @@
         <v>202</v>
       </c>
       <c r="R129" s="24" t="s">
-        <v>959</v>
+        <v>958</v>
       </c>
       <c r="S129" s="24" t="s">
-        <v>962</v>
+        <v>961</v>
       </c>
       <c r="T129" s="24" t="s">
         <v>692</v>
       </c>
       <c r="U129" s="24" t="s">
-        <v>1051</v>
+        <v>1050</v>
       </c>
     </row>
     <row r="130" spans="1:21" s="24" customFormat="1" ht="14.25">
       <c r="A130" s="24" t="s">
-        <v>963</v>
+        <v>962</v>
       </c>
       <c r="B130" s="24" t="s">
         <v>7</v>
       </c>
       <c r="C130" s="24" t="s">
-        <v>964</v>
+        <v>963</v>
       </c>
       <c r="D130" s="24" t="s">
         <v>84</v>
@@ -17475,7 +17606,7 @@
         <v>410</v>
       </c>
       <c r="G130" s="24" t="s">
-        <v>965</v>
+        <v>964</v>
       </c>
       <c r="H130" s="24" t="s">
         <v>202</v>
@@ -17502,27 +17633,27 @@
         <v>207</v>
       </c>
       <c r="R130" s="24" t="s">
-        <v>964</v>
+        <v>963</v>
       </c>
       <c r="S130" s="24" t="s">
-        <v>966</v>
+        <v>965</v>
       </c>
       <c r="T130" s="24" t="s">
         <v>692</v>
       </c>
       <c r="U130" s="24" t="s">
-        <v>1051</v>
+        <v>1050</v>
       </c>
     </row>
     <row r="131" spans="1:21" s="24" customFormat="1" ht="14.25">
       <c r="A131" s="24" t="s">
-        <v>967</v>
+        <v>966</v>
       </c>
       <c r="B131" s="24" t="s">
         <v>7</v>
       </c>
       <c r="C131" s="24" t="s">
-        <v>968</v>
+        <v>967</v>
       </c>
       <c r="D131" s="24" t="s">
         <v>84</v>
@@ -17561,27 +17692,27 @@
         <v>205</v>
       </c>
       <c r="R131" s="24" t="s">
+        <v>967</v>
+      </c>
+      <c r="S131" s="24" t="s">
         <v>968</v>
-      </c>
-      <c r="S131" s="24" t="s">
-        <v>969</v>
       </c>
       <c r="T131" s="24" t="s">
         <v>692</v>
       </c>
       <c r="U131" s="24" t="s">
-        <v>1051</v>
+        <v>1050</v>
       </c>
     </row>
     <row r="132" spans="1:21" s="24" customFormat="1" ht="14.25">
       <c r="A132" s="24" t="s">
-        <v>970</v>
+        <v>969</v>
       </c>
       <c r="B132" s="24" t="s">
         <v>7</v>
       </c>
       <c r="C132" s="24" t="s">
-        <v>971</v>
+        <v>970</v>
       </c>
       <c r="D132" s="24" t="s">
         <v>84</v>
@@ -17605,7 +17736,7 @@
         <v>202</v>
       </c>
       <c r="L132" s="24" t="s">
-        <v>972</v>
+        <v>971</v>
       </c>
       <c r="M132" s="24" t="s">
         <v>255</v>
@@ -17620,27 +17751,27 @@
         <v>207</v>
       </c>
       <c r="R132" s="24" t="s">
-        <v>971</v>
+        <v>970</v>
       </c>
       <c r="S132" s="24" t="s">
-        <v>973</v>
+        <v>972</v>
       </c>
       <c r="T132" s="24" t="s">
         <v>692</v>
       </c>
       <c r="U132" s="24" t="s">
-        <v>1051</v>
+        <v>1050</v>
       </c>
     </row>
     <row r="133" spans="1:21" s="24" customFormat="1" ht="14.25">
       <c r="A133" s="24" t="s">
-        <v>974</v>
+        <v>973</v>
       </c>
       <c r="B133" s="24" t="s">
         <v>7</v>
       </c>
       <c r="C133" s="24" t="s">
-        <v>975</v>
+        <v>974</v>
       </c>
       <c r="D133" s="24" t="s">
         <v>77</v>
@@ -17661,10 +17792,10 @@
         <v>201</v>
       </c>
       <c r="K133" s="24" t="s">
+        <v>975</v>
+      </c>
+      <c r="L133" s="24" t="s">
         <v>976</v>
-      </c>
-      <c r="L133" s="24" t="s">
-        <v>977</v>
       </c>
       <c r="M133" s="24" t="s">
         <v>269</v>
@@ -17673,33 +17804,33 @@
         <v>269</v>
       </c>
       <c r="P133" s="24" t="s">
-        <v>945</v>
+        <v>944</v>
       </c>
       <c r="Q133" s="24" t="s">
         <v>269</v>
       </c>
       <c r="R133" s="24" t="s">
-        <v>975</v>
+        <v>974</v>
       </c>
       <c r="S133" s="24" t="s">
-        <v>978</v>
+        <v>977</v>
       </c>
       <c r="T133" s="24" t="s">
         <v>692</v>
       </c>
       <c r="U133" s="24" t="s">
-        <v>1051</v>
+        <v>1050</v>
       </c>
     </row>
     <row r="134" spans="1:21" s="24" customFormat="1" ht="14.25">
       <c r="A134" s="24" t="s">
-        <v>979</v>
+        <v>978</v>
       </c>
       <c r="B134" s="24" t="s">
         <v>7</v>
       </c>
       <c r="C134" s="24" t="s">
-        <v>980</v>
+        <v>979</v>
       </c>
       <c r="D134" s="24" t="s">
         <v>84</v>
@@ -17738,27 +17869,27 @@
         <v>207</v>
       </c>
       <c r="R134" s="24" t="s">
+        <v>979</v>
+      </c>
+      <c r="S134" s="24" t="s">
         <v>980</v>
-      </c>
-      <c r="S134" s="24" t="s">
-        <v>981</v>
       </c>
       <c r="T134" s="24" t="s">
         <v>692</v>
       </c>
       <c r="U134" s="24" t="s">
-        <v>1051</v>
+        <v>1050</v>
       </c>
     </row>
     <row r="135" spans="1:21" s="24" customFormat="1" ht="14.25">
       <c r="A135" s="24" t="s">
-        <v>982</v>
+        <v>981</v>
       </c>
       <c r="B135" s="24" t="s">
         <v>7</v>
       </c>
       <c r="C135" s="24" t="s">
-        <v>983</v>
+        <v>982</v>
       </c>
       <c r="D135" s="24" t="s">
         <v>84</v>
@@ -17779,10 +17910,10 @@
         <v>201</v>
       </c>
       <c r="K135" s="24" t="s">
+        <v>983</v>
+      </c>
+      <c r="L135" s="24" t="s">
         <v>984</v>
-      </c>
-      <c r="L135" s="24" t="s">
-        <v>985</v>
       </c>
       <c r="M135" s="24" t="s">
         <v>204</v>
@@ -17797,27 +17928,27 @@
         <v>207</v>
       </c>
       <c r="R135" s="24" t="s">
-        <v>983</v>
+        <v>982</v>
       </c>
       <c r="S135" s="24" t="s">
-        <v>986</v>
+        <v>985</v>
       </c>
       <c r="T135" s="24" t="s">
         <v>692</v>
       </c>
       <c r="U135" s="24" t="s">
-        <v>1051</v>
+        <v>1050</v>
       </c>
     </row>
     <row r="136" spans="1:21" s="24" customFormat="1" ht="14.25">
       <c r="A136" s="24" t="s">
-        <v>987</v>
+        <v>986</v>
       </c>
       <c r="B136" s="24" t="s">
         <v>7</v>
       </c>
       <c r="C136" s="24" t="s">
-        <v>988</v>
+        <v>987</v>
       </c>
       <c r="D136" s="24" t="s">
         <v>84</v>
@@ -17832,16 +17963,16 @@
         <v>239</v>
       </c>
       <c r="H136" s="24" t="s">
-        <v>989</v>
+        <v>988</v>
       </c>
       <c r="I136" s="24" t="s">
         <v>201</v>
       </c>
       <c r="K136" s="24" t="s">
+        <v>989</v>
+      </c>
+      <c r="L136" s="24" t="s">
         <v>990</v>
-      </c>
-      <c r="L136" s="24" t="s">
-        <v>991</v>
       </c>
       <c r="M136" s="24" t="s">
         <v>204</v>
@@ -17856,27 +17987,27 @@
         <v>207</v>
       </c>
       <c r="R136" s="24" t="s">
-        <v>988</v>
+        <v>987</v>
       </c>
       <c r="S136" s="24" t="s">
-        <v>992</v>
+        <v>991</v>
       </c>
       <c r="T136" s="24" t="s">
         <v>692</v>
       </c>
       <c r="U136" s="24" t="s">
-        <v>1051</v>
+        <v>1050</v>
       </c>
     </row>
     <row r="137" spans="1:21" s="24" customFormat="1" ht="14.25">
       <c r="A137" s="24" t="s">
-        <v>993</v>
+        <v>992</v>
       </c>
       <c r="B137" s="24" t="s">
         <v>7</v>
       </c>
       <c r="C137" s="24" t="s">
-        <v>994</v>
+        <v>993</v>
       </c>
       <c r="D137" s="24" t="s">
         <v>84</v>
@@ -17891,16 +18022,16 @@
         <v>85</v>
       </c>
       <c r="H137" s="24" t="s">
-        <v>995</v>
+        <v>994</v>
       </c>
       <c r="I137" s="24" t="s">
         <v>201</v>
       </c>
       <c r="K137" s="24" t="s">
+        <v>995</v>
+      </c>
+      <c r="L137" s="24" t="s">
         <v>996</v>
-      </c>
-      <c r="L137" s="24" t="s">
-        <v>997</v>
       </c>
       <c r="M137" s="24" t="s">
         <v>204</v>
@@ -17909,33 +18040,33 @@
         <v>207</v>
       </c>
       <c r="P137" s="24" t="s">
-        <v>945</v>
+        <v>944</v>
       </c>
       <c r="Q137" s="24" t="s">
         <v>207</v>
       </c>
       <c r="R137" s="24" t="s">
-        <v>994</v>
+        <v>993</v>
       </c>
       <c r="S137" s="24" t="s">
-        <v>998</v>
+        <v>997</v>
       </c>
       <c r="T137" s="24" t="s">
         <v>692</v>
       </c>
       <c r="U137" s="24" t="s">
-        <v>1051</v>
+        <v>1050</v>
       </c>
     </row>
     <row r="138" spans="1:21" s="24" customFormat="1" ht="14.25">
       <c r="A138" s="24" t="s">
-        <v>999</v>
+        <v>998</v>
       </c>
       <c r="B138" s="24" t="s">
         <v>7</v>
       </c>
       <c r="C138" s="24" t="s">
-        <v>1000</v>
+        <v>999</v>
       </c>
       <c r="D138" s="24" t="s">
         <v>84</v>
@@ -17944,13 +18075,13 @@
         <v>176</v>
       </c>
       <c r="F138" s="24" t="s">
-        <v>913</v>
+        <v>912</v>
       </c>
       <c r="G138" s="24" t="s">
+        <v>1000</v>
+      </c>
+      <c r="H138" s="24" t="s">
         <v>1001</v>
-      </c>
-      <c r="H138" s="24" t="s">
-        <v>1002</v>
       </c>
       <c r="I138" s="24" t="s">
         <v>201</v>
@@ -17974,27 +18105,27 @@
         <v>205</v>
       </c>
       <c r="R138" s="24" t="s">
-        <v>1000</v>
+        <v>999</v>
       </c>
       <c r="S138" s="24" t="s">
-        <v>1003</v>
+        <v>1002</v>
       </c>
       <c r="T138" s="24" t="s">
         <v>692</v>
       </c>
       <c r="U138" s="24" t="s">
-        <v>1051</v>
+        <v>1050</v>
       </c>
     </row>
     <row r="139" spans="1:21" s="24" customFormat="1" ht="14.25">
       <c r="A139" s="24" t="s">
-        <v>1004</v>
+        <v>1003</v>
       </c>
       <c r="B139" s="24" t="s">
         <v>7</v>
       </c>
       <c r="C139" s="24" t="s">
-        <v>1005</v>
+        <v>1004</v>
       </c>
       <c r="D139" s="24" t="s">
         <v>77</v>
@@ -18018,7 +18149,7 @@
         <v>310</v>
       </c>
       <c r="L139" s="24" t="s">
-        <v>1006</v>
+        <v>1005</v>
       </c>
       <c r="M139" s="24" t="s">
         <v>207</v>
@@ -18033,27 +18164,27 @@
         <v>269</v>
       </c>
       <c r="R139" s="24" t="s">
-        <v>1005</v>
+        <v>1004</v>
       </c>
       <c r="S139" s="24" t="s">
-        <v>1007</v>
+        <v>1006</v>
       </c>
       <c r="T139" s="24" t="s">
         <v>692</v>
       </c>
       <c r="U139" s="24" t="s">
-        <v>1051</v>
+        <v>1050</v>
       </c>
     </row>
     <row r="140" spans="1:21" s="24" customFormat="1" ht="14.25">
       <c r="A140" s="24" t="s">
-        <v>1008</v>
+        <v>1007</v>
       </c>
       <c r="B140" s="24" t="s">
         <v>7</v>
       </c>
       <c r="C140" s="24" t="s">
-        <v>1009</v>
+        <v>1008</v>
       </c>
       <c r="D140" s="24" t="s">
         <v>84</v>
@@ -18068,16 +18199,16 @@
         <v>100</v>
       </c>
       <c r="H140" s="24" t="s">
-        <v>1010</v>
+        <v>1009</v>
       </c>
       <c r="I140" s="24" t="s">
         <v>201</v>
       </c>
       <c r="K140" s="24" t="s">
+        <v>1010</v>
+      </c>
+      <c r="L140" s="24" t="s">
         <v>1011</v>
-      </c>
-      <c r="L140" s="24" t="s">
-        <v>1012</v>
       </c>
       <c r="M140" s="24" t="s">
         <v>204</v>
@@ -18092,27 +18223,27 @@
         <v>207</v>
       </c>
       <c r="R140" s="24" t="s">
-        <v>1009</v>
+        <v>1008</v>
       </c>
       <c r="S140" s="24" t="s">
-        <v>1013</v>
+        <v>1012</v>
       </c>
       <c r="T140" s="24" t="s">
         <v>692</v>
       </c>
       <c r="U140" s="24" t="s">
-        <v>1051</v>
+        <v>1050</v>
       </c>
     </row>
     <row r="141" spans="1:21" s="24" customFormat="1" ht="14.25">
       <c r="A141" s="24" t="s">
-        <v>1014</v>
+        <v>1013</v>
       </c>
       <c r="B141" s="24" t="s">
         <v>7</v>
       </c>
       <c r="C141" s="24" t="s">
-        <v>1015</v>
+        <v>1014</v>
       </c>
       <c r="D141" s="24" t="s">
         <v>84</v>
@@ -18124,10 +18255,10 @@
         <v>238</v>
       </c>
       <c r="G141" s="24" t="s">
+        <v>1015</v>
+      </c>
+      <c r="H141" s="24" t="s">
         <v>1016</v>
-      </c>
-      <c r="H141" s="24" t="s">
-        <v>1017</v>
       </c>
       <c r="I141" s="24" t="s">
         <v>201</v>
@@ -18151,27 +18282,27 @@
         <v>207</v>
       </c>
       <c r="R141" s="24" t="s">
-        <v>1015</v>
+        <v>1014</v>
       </c>
       <c r="S141" s="24" t="s">
-        <v>1018</v>
+        <v>1017</v>
       </c>
       <c r="T141" s="24" t="s">
         <v>692</v>
       </c>
       <c r="U141" s="24" t="s">
-        <v>1051</v>
+        <v>1050</v>
       </c>
     </row>
     <row r="142" spans="1:21" s="24" customFormat="1" ht="14.25">
       <c r="A142" s="24" t="s">
-        <v>1019</v>
+        <v>1018</v>
       </c>
       <c r="B142" s="44" t="s">
         <v>175</v>
       </c>
       <c r="C142" s="24" t="s">
-        <v>1020</v>
+        <v>1019</v>
       </c>
       <c r="D142" s="24" t="s">
         <v>84</v>
@@ -18192,10 +18323,10 @@
         <v>201</v>
       </c>
       <c r="K142" s="24" t="s">
+        <v>1020</v>
+      </c>
+      <c r="L142" s="24" t="s">
         <v>1021</v>
-      </c>
-      <c r="L142" s="24" t="s">
-        <v>1022</v>
       </c>
       <c r="M142" s="24" t="s">
         <v>204</v>
@@ -18210,27 +18341,27 @@
         <v>207</v>
       </c>
       <c r="R142" s="24" t="s">
-        <v>1020</v>
+        <v>1019</v>
       </c>
       <c r="S142" s="24" t="s">
-        <v>1023</v>
+        <v>1022</v>
       </c>
       <c r="T142" s="24" t="s">
         <v>692</v>
       </c>
       <c r="U142" s="24" t="s">
-        <v>1051</v>
+        <v>1050</v>
       </c>
     </row>
     <row r="143" spans="1:21" s="24" customFormat="1" ht="14.25">
       <c r="A143" s="24" t="s">
-        <v>1024</v>
+        <v>1023</v>
       </c>
       <c r="B143" s="44" t="s">
         <v>175</v>
       </c>
       <c r="C143" s="24" t="s">
-        <v>1025</v>
+        <v>1024</v>
       </c>
       <c r="D143" s="24" t="s">
         <v>77</v>
@@ -18242,7 +18373,7 @@
         <v>238</v>
       </c>
       <c r="G143" s="24" t="s">
-        <v>1016</v>
+        <v>1015</v>
       </c>
       <c r="H143" s="24" t="s">
         <v>202</v>
@@ -18251,10 +18382,10 @@
         <v>201</v>
       </c>
       <c r="K143" s="24" t="s">
+        <v>1025</v>
+      </c>
+      <c r="L143" s="24" t="s">
         <v>1026</v>
-      </c>
-      <c r="L143" s="24" t="s">
-        <v>1027</v>
       </c>
       <c r="M143" s="24" t="s">
         <v>205</v>
@@ -18263,29 +18394,147 @@
         <v>205</v>
       </c>
       <c r="P143" s="24" t="s">
-        <v>945</v>
+        <v>944</v>
       </c>
       <c r="Q143" s="24" t="s">
         <v>269</v>
       </c>
       <c r="R143" s="24" t="s">
-        <v>1025</v>
+        <v>1024</v>
       </c>
       <c r="S143" s="24" t="s">
-        <v>1028</v>
+        <v>1027</v>
       </c>
       <c r="T143" s="24" t="s">
-        <v>1053</v>
+        <v>1052</v>
       </c>
       <c r="U143" s="24" t="s">
         <v>37</v>
+      </c>
+    </row>
+    <row r="144" spans="1:21" ht="12.75">
+      <c r="A144" t="s">
+        <v>1057</v>
+      </c>
+      <c r="B144" t="s">
+        <v>1067</v>
+      </c>
+      <c r="C144" t="s">
+        <v>1058</v>
+      </c>
+      <c r="D144" t="s">
+        <v>237</v>
+      </c>
+      <c r="E144" t="s">
+        <v>78</v>
+      </c>
+      <c r="F144" t="s">
+        <v>410</v>
+      </c>
+      <c r="G144" t="s">
+        <v>1059</v>
+      </c>
+      <c r="H144" t="s">
+        <v>1060</v>
+      </c>
+      <c r="I144" t="s">
+        <v>201</v>
+      </c>
+      <c r="K144" t="s">
+        <v>202</v>
+      </c>
+      <c r="L144" t="s">
+        <v>240</v>
+      </c>
+      <c r="M144" t="s">
+        <v>202</v>
+      </c>
+      <c r="N144" t="s">
+        <v>202</v>
+      </c>
+      <c r="P144" t="s">
+        <v>202</v>
+      </c>
+      <c r="Q144" t="s">
+        <v>202</v>
+      </c>
+      <c r="R144" t="s">
+        <v>1058</v>
+      </c>
+      <c r="S144" t="s">
+        <v>1061</v>
+      </c>
+      <c r="T144" t="s">
+        <v>691</v>
+      </c>
+      <c r="U144" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="145" spans="1:21" ht="12.75">
+      <c r="A145" t="s">
+        <v>1062</v>
+      </c>
+      <c r="B145" t="s">
+        <v>1067</v>
+      </c>
+      <c r="C145" t="s">
+        <v>1063</v>
+      </c>
+      <c r="D145" t="s">
+        <v>84</v>
+      </c>
+      <c r="E145" t="s">
+        <v>78</v>
+      </c>
+      <c r="F145" t="s">
+        <v>410</v>
+      </c>
+      <c r="G145" t="s">
+        <v>1064</v>
+      </c>
+      <c r="H145" t="s">
+        <v>1065</v>
+      </c>
+      <c r="I145" t="s">
+        <v>201</v>
+      </c>
+      <c r="K145" t="s">
+        <v>513</v>
+      </c>
+      <c r="L145" t="s">
+        <v>514</v>
+      </c>
+      <c r="M145" t="s">
+        <v>205</v>
+      </c>
+      <c r="N145" t="s">
+        <v>207</v>
+      </c>
+      <c r="P145" t="s">
+        <v>202</v>
+      </c>
+      <c r="Q145" t="s">
+        <v>207</v>
+      </c>
+      <c r="R145" t="s">
+        <v>1063</v>
+      </c>
+      <c r="S145" t="s">
+        <v>1066</v>
+      </c>
+      <c r="T145" t="s">
+        <v>692</v>
+      </c>
+      <c r="U145" t="s">
+        <v>16</v>
       </c>
     </row>
   </sheetData>
   <customSheetViews>
     <customSheetView guid="{A7754112-A52F-4ABC-8778-92F04773E53C}" filter="1" showAutoFilter="1">
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-      <autoFilter ref="A1:AD33" xr:uid="{36770BF8-1D1F-439E-9B25-E527A790BBD3}">
+      <autoFilter ref="A1:AD33" xr:uid="{DB2A4052-19CB-4E4A-B3F4-2EEEA3E82EE2}">
         <filterColumn colId="5">
           <filters blank="1">
             <filter val="Strathnairn"/>
@@ -18295,7 +18544,7 @@
     </customSheetView>
     <customSheetView guid="{C25CEB9E-BEC1-4982-90C4-50C84EE1B82A}" filter="1" showAutoFilter="1">
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-      <autoFilter ref="A1:AD33" xr:uid="{941BCCD3-8FDC-4F1C-BC41-4DD572BE9B8E}"/>
+      <autoFilter ref="A1:AD33" xr:uid="{BD0AF5FF-FB2E-4C3A-A319-B574FCDF1049}"/>
     </customSheetView>
   </customSheetViews>
   <conditionalFormatting sqref="A1:AI1">

</xml_diff>

<commit_message>
Fixed as per check-updates script
</commit_message>
<xml_diff>
--- a/src/main/resources/InputTestdata/Listing details.xlsx
+++ b/src/main/resources/InputTestdata/Listing details.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Athavan\git\777Homes-2\777Homes-business\src\main\resources\InputTestdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{17B9F445-2725-4368-8165-4140CE326DBC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1D886A65-3E22-4EDF-A644-172D4F627A2F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,14 +20,14 @@
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Backlog!$A$1:$AB$52</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Listing!#REF!</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Listing!$E$1:$E$145</definedName>
     <definedName name="Z_A7754112_A52F_4ABC_8778_92F04773E53C_.wvu.FilterData" localSheetId="1" hidden="1">Listing!$A$1:$AE$32</definedName>
     <definedName name="Z_C25CEB9E_BEC1_4982_90C4_50C84EE1B82A_.wvu.FilterData" localSheetId="1" hidden="1">Listing!$A$1:$AE$32</definedName>
   </definedNames>
   <calcPr calcId="181029"/>
   <customWorkbookViews>
+    <customWorkbookView name="Filter 1" guid="{A7754112-A52F-4ABC-8778-92F04773E53C}" maximized="1" windowWidth="0" windowHeight="0" activeSheetId="0"/>
     <customWorkbookView name="Filter 2" guid="{C25CEB9E-BEC1-4982-90C4-50C84EE1B82A}" maximized="1" windowWidth="0" windowHeight="0" activeSheetId="0"/>
-    <customWorkbookView name="Filter 1" guid="{A7754112-A52F-4ABC-8778-92F04773E53C}" maximized="1" windowWidth="0" windowHeight="0" activeSheetId="0"/>
   </customWorkbookViews>
 </workbook>
 </file>
@@ -5336,7 +5336,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="11">
+  <fills count="10">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -5390,11 +5390,6 @@
         <bgColor indexed="2"/>
       </patternFill>
     </fill>
-    <fill>
-      <patternFill patternType="mediumGray">
-        <bgColor indexed="2"/>
-      </patternFill>
-    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -5409,7 +5404,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="48">
+  <cellXfs count="47">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -5502,12 +5497,11 @@
     <xf numFmtId="0" fontId="18" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="26" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="27" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -5747,8 +5741,8 @@
   <dimension ref="A1:AB145"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A128" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D153" sqref="D153"/>
+      <pane ySplit="1" topLeftCell="A20" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C23" sqref="C23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1"/>
@@ -6453,7 +6447,7 @@
       <c r="B17" s="18" t="s">
         <v>28</v>
       </c>
-      <c r="C17" s="2" t="s">
+      <c r="C17" s="38" t="s">
         <v>699</v>
       </c>
       <c r="D17" s="4" t="s">
@@ -6710,7 +6704,7 @@
       <c r="A23" s="9">
         <v>22</v>
       </c>
-      <c r="B23" s="19" t="s">
+      <c r="B23" s="42" t="s">
         <v>34</v>
       </c>
       <c r="C23" s="38" t="s">
@@ -9856,9 +9850,10 @@
     <hyperlink ref="B144" r:id="rId176" xr:uid="{F6EFF9E5-8AC0-4C40-A2A8-62DF9BB671E9}"/>
     <hyperlink ref="C145" r:id="rId177" xr:uid="{DE56B3AC-2F1A-494E-A9CD-9C972DA863E2}"/>
     <hyperlink ref="B145" r:id="rId178" xr:uid="{F783979B-F441-49BC-98C4-8448098CBBC1}"/>
+    <hyperlink ref="C17" r:id="rId179" xr:uid="{DBE3D417-C525-4AE7-BA26-A27F8BD7B6D3}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId179"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId180"/>
 </worksheet>
 </file>
 
@@ -9871,7 +9866,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A131" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="S154" sqref="S154"/>
+      <selection pane="bottomLeft" activeCell="D23" sqref="D23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1"/>
@@ -10297,7 +10292,7 @@
       <c r="H6" s="24" t="s">
         <v>839</v>
       </c>
-      <c r="K6" s="44" t="s">
+      <c r="K6" s="24" t="s">
         <v>656</v>
       </c>
       <c r="L6" s="24" t="s">
@@ -10394,13 +10389,13 @@
       <c r="A8" s="24">
         <v>7</v>
       </c>
-      <c r="B8" s="47" t="s">
-        <v>1063</v>
+      <c r="B8" s="24" t="s">
+        <v>7</v>
       </c>
       <c r="C8" s="24" t="s">
         <v>98</v>
       </c>
-      <c r="D8" s="47" t="s">
+      <c r="D8" s="24" t="s">
         <v>84</v>
       </c>
       <c r="E8" s="24" t="s">
@@ -10928,8 +10923,8 @@
       <c r="A17" s="24">
         <v>16</v>
       </c>
-      <c r="B17" s="47" t="s">
-        <v>1063</v>
+      <c r="B17" s="24" t="s">
+        <v>7</v>
       </c>
       <c r="C17" s="24" t="s">
         <v>124</v>
@@ -10949,7 +10944,7 @@
       <c r="H17" s="24" t="s">
         <v>592</v>
       </c>
-      <c r="K17" s="47" t="s">
+      <c r="K17" s="24" t="s">
         <v>426</v>
       </c>
       <c r="L17" s="24" t="s">
@@ -11043,7 +11038,7 @@
       <c r="A19" s="24">
         <v>18</v>
       </c>
-      <c r="B19" s="47" t="s">
+      <c r="B19" s="46" t="s">
         <v>1063</v>
       </c>
       <c r="C19" s="24" t="s">
@@ -11052,7 +11047,7 @@
       <c r="D19" s="24" t="s">
         <v>84</v>
       </c>
-      <c r="E19" s="47" t="s">
+      <c r="E19" s="46" t="s">
         <v>173</v>
       </c>
       <c r="F19" s="24" t="s">
@@ -11061,13 +11056,13 @@
       <c r="G19" s="24" t="s">
         <v>100</v>
       </c>
-      <c r="H19" s="47" t="s">
+      <c r="H19" s="46" t="s">
         <v>1065</v>
       </c>
-      <c r="K19" s="47" t="s">
+      <c r="K19" s="46" t="s">
         <v>313</v>
       </c>
-      <c r="L19" s="47" t="s">
+      <c r="L19" s="46" t="s">
         <v>1066</v>
       </c>
       <c r="M19" s="24">
@@ -11085,7 +11080,7 @@
       <c r="R19" s="24" t="s">
         <v>101</v>
       </c>
-      <c r="S19" s="47" t="s">
+      <c r="S19" s="46" t="s">
         <v>1064</v>
       </c>
       <c r="T19" s="24" t="s">
@@ -11174,7 +11169,7 @@
       <c r="A21" s="24">
         <v>20</v>
       </c>
-      <c r="B21" s="47" t="s">
+      <c r="B21" s="46" t="s">
         <v>1063</v>
       </c>
       <c r="C21" s="24" t="s">
@@ -11183,7 +11178,7 @@
       <c r="D21" s="24" t="s">
         <v>84</v>
       </c>
-      <c r="E21" s="47" t="s">
+      <c r="E21" s="46" t="s">
         <v>173</v>
       </c>
       <c r="F21" s="24" t="s">
@@ -11192,15 +11187,15 @@
       <c r="G21" s="24" t="s">
         <v>100</v>
       </c>
-      <c r="H21" s="47" t="s">
+      <c r="H21" s="46" t="s">
         <v>1068</v>
       </c>
       <c r="I21" s="24"/>
       <c r="J21" s="24"/>
-      <c r="K21" s="47" t="s">
+      <c r="K21" s="46" t="s">
         <v>431</v>
       </c>
-      <c r="L21" s="47" t="s">
+      <c r="L21" s="46" t="s">
         <v>1069</v>
       </c>
       <c r="M21" s="24">
@@ -11210,16 +11205,16 @@
         <v>2</v>
       </c>
       <c r="O21" s="24"/>
-      <c r="P21" s="47" t="s">
+      <c r="P21" s="46" t="s">
         <v>203</v>
       </c>
-      <c r="Q21" s="47" t="s">
+      <c r="Q21" s="46" t="s">
         <v>204</v>
       </c>
       <c r="R21" s="24" t="s">
         <v>101</v>
       </c>
-      <c r="S21" s="47" t="s">
+      <c r="S21" s="46" t="s">
         <v>1067</v>
       </c>
       <c r="T21" s="24" t="s">
@@ -11312,13 +11307,13 @@
       <c r="A23" s="24">
         <v>22</v>
       </c>
-      <c r="B23" s="47" t="s">
-        <v>1063</v>
+      <c r="B23" s="24" t="s">
+        <v>7</v>
       </c>
       <c r="C23" s="24" t="s">
         <v>131</v>
       </c>
-      <c r="D23" s="47" t="s">
+      <c r="D23" s="24" t="s">
         <v>84</v>
       </c>
       <c r="E23" s="24" t="s">
@@ -16702,7 +16697,7 @@
       <c r="G114" s="24" t="s">
         <v>526</v>
       </c>
-      <c r="H114" s="45" t="s">
+      <c r="H114" s="44" t="s">
         <v>842</v>
       </c>
       <c r="I114" s="24" t="s">
@@ -16743,8 +16738,8 @@
       <c r="A115" s="24" t="s">
         <v>844</v>
       </c>
-      <c r="B115" s="24" t="s">
-        <v>7</v>
+      <c r="B115" s="43" t="s">
+        <v>386</v>
       </c>
       <c r="C115" s="24" t="s">
         <v>845</v>
@@ -16752,8 +16747,8 @@
       <c r="D115" s="24" t="s">
         <v>77</v>
       </c>
-      <c r="E115" s="24" t="s">
-        <v>850</v>
+      <c r="E115" s="43" t="s">
+        <v>386</v>
       </c>
       <c r="F115" s="24" t="s">
         <v>79</v>
@@ -16871,7 +16866,7 @@
         <v>77</v>
       </c>
       <c r="E117" s="24" t="s">
-        <v>78</v>
+        <v>850</v>
       </c>
       <c r="F117" s="24" t="s">
         <v>270</v>
@@ -18569,20 +18564,21 @@
       </c>
     </row>
   </sheetData>
+  <autoFilter ref="E1:E145" xr:uid="{00000000-0001-0000-0100-000000000000}"/>
   <customSheetViews>
-    <customSheetView guid="{C25CEB9E-BEC1-4982-90C4-50C84EE1B82A}" filter="1" showAutoFilter="1">
-      <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-      <autoFilter ref="A1:AD33" xr:uid="{6B9F424A-224D-4695-8A09-000DF7216673}"/>
-    </customSheetView>
     <customSheetView guid="{A7754112-A52F-4ABC-8778-92F04773E53C}" filter="1" showAutoFilter="1">
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-      <autoFilter ref="A1:AD33" xr:uid="{671E895F-8D13-45E4-9257-5D01F3EC168C}">
+      <autoFilter ref="A1:AD33" xr:uid="{D459F44F-61CA-4CC4-9ED5-4470B90B89A5}">
         <filterColumn colId="5">
           <filters blank="1">
             <filter val="Strathnairn"/>
           </filters>
         </filterColumn>
       </autoFilter>
+    </customSheetView>
+    <customSheetView guid="{C25CEB9E-BEC1-4982-90C4-50C84EE1B82A}" filter="1" showAutoFilter="1">
+      <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+      <autoFilter ref="A1:AD33" xr:uid="{233D75FB-5D27-4ACD-82C0-573AE156D5F1}"/>
     </customSheetView>
   </customSheetViews>
   <conditionalFormatting sqref="A1:AI1">
@@ -18899,10 +18895,10 @@
       </c>
     </row>
     <row r="7" spans="1:7" ht="15.75" customHeight="1">
-      <c r="A7" s="46" t="s">
+      <c r="A7" s="45" t="s">
         <v>879</v>
       </c>
-      <c r="B7" s="46" t="s">
+      <c r="B7" s="45" t="s">
         <v>880</v>
       </c>
       <c r="C7" t="s">

</xml_diff>

<commit_message>
Add new property 21/09/2021
</commit_message>
<xml_diff>
--- a/src/main/resources/InputTestdata/Listing details.xlsx
+++ b/src/main/resources/InputTestdata/Listing details.xlsx
@@ -1,39 +1,39 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24326"/>
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <mc:AlternateContent>
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Athavan\git\777Homes-2\777Homes-business\src\main\resources\InputTestdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{41C5971F-9F6D-4674-ACDB-8941AB3E8E65}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr documentId="13_ncr:1_{61F3BAB8-8A9D-43F6-9E0A-B63C75C062AD}" revIDLastSave="0" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView windowHeight="15840" windowWidth="29040" xWindow="-120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}" yWindow="-120"/>
   </bookViews>
   <sheets>
-    <sheet name="Backlog" sheetId="1" r:id="rId1"/>
-    <sheet name="Listing" sheetId="2" r:id="rId2"/>
-    <sheet name="Tobe-executed" sheetId="3" r:id="rId3"/>
-    <sheet name="Agency login" sheetId="4" r:id="rId4"/>
+    <sheet name="Backlog" r:id="rId1" sheetId="1"/>
+    <sheet name="Listing" r:id="rId2" sheetId="2"/>
+    <sheet name="Tobe-executed" r:id="rId3" sheetId="3"/>
+    <sheet name="Agency login" r:id="rId4" sheetId="4"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Backlog!$A$1:$AB$52</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Listing!$E$1:$E$145</definedName>
-    <definedName name="Z_A7754112_A52F_4ABC_8778_92F04773E53C_.wvu.FilterData" localSheetId="1" hidden="1">Listing!$A$1:$AE$32</definedName>
-    <definedName name="Z_C25CEB9E_BEC1_4982_90C4_50C84EE1B82A_.wvu.FilterData" localSheetId="1" hidden="1">Listing!$A$1:$AE$32</definedName>
+    <definedName hidden="1" localSheetId="0" name="_xlnm._FilterDatabase">Backlog!$A$1:$AB$52</definedName>
+    <definedName hidden="1" localSheetId="1" name="_xlnm._FilterDatabase">Listing!$E$1:$E$145</definedName>
+    <definedName hidden="1" localSheetId="1" name="Z_A7754112_A52F_4ABC_8778_92F04773E53C_.wvu.FilterData">Listing!$A$1:$AE$32</definedName>
+    <definedName hidden="1" localSheetId="1" name="Z_C25CEB9E_BEC1_4982_90C4_50C84EE1B82A_.wvu.FilterData">Listing!$A$1:$AE$32</definedName>
   </definedNames>
   <calcPr calcId="181029"/>
   <customWorkbookViews>
-    <customWorkbookView name="Filter 1" guid="{A7754112-A52F-4ABC-8778-92F04773E53C}" maximized="1" windowWidth="0" windowHeight="0" activeSheetId="0"/>
-    <customWorkbookView name="Filter 2" guid="{C25CEB9E-BEC1-4982-90C4-50C84EE1B82A}" maximized="1" windowWidth="0" windowHeight="0" activeSheetId="0"/>
+    <customWorkbookView activeSheetId="0" guid="{A7754112-A52F-4ABC-8778-92F04773E53C}" maximized="1" name="Filter 1" windowHeight="0" windowWidth="0"/>
+    <customWorkbookView activeSheetId="0" guid="{C25CEB9E-BEC1-4982-90C4-50C84EE1B82A}" maximized="1" name="Filter 2" windowHeight="0" windowWidth="0"/>
   </customWorkbookViews>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3622" uniqueCount="1101">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3649" uniqueCount="1107">
   <si>
     <t>ID</t>
   </si>
@@ -5289,9 +5289,6 @@
     <t>https://www.777homes.com.au/?post_type=property&amp;p=8748&amp;preview=true</t>
   </si>
   <si>
-    <t>TO BE UPDATED</t>
-  </si>
-  <si>
     <t>In line with new Covid Guidelines, after 17/09/21 11:59pm, Real estate agents are allowed to conduct in-person house inspections by private appointment. Only household members will be permitted to attend an appointment with one agent. Please contact us for your inspection.
 The Opportunity: Enjoy the space, light and comfort of a welcoming home in the MOLONGLO VALLEY- where the ribbon cannot be bluer than blue.
 Feel the difference with a carefully curated material palette, your customised lifestyle ideas, from your wildest dreams onto an actual concrete plan. Design your plan, build it, and move into it!
@@ -5358,11 +5355,61 @@
 - 800 meters to Well station drive light rail station
 - 3.23 km from Gungahlin marketplace</t>
   </si>
+  <si>
+    <t>https://www.allhomes.com.au/13-porter-street-wright-act-2611</t>
+  </si>
+  <si>
+    <t>149</t>
+  </si>
+  <si>
+    <t>13 Porter Street, Wright ACT 2611</t>
+  </si>
+  <si>
+    <t>Block/House: 574/ 334</t>
+  </si>
+  <si>
+    <t>~ Forthcoming Auction ~
+Bookings by appointments open. Please call Anish on 0450 865 524 to book your slot.
+Immediately impressive, this impressive home oozes street appeal, with beautifully landscaped gardens and arguably one of the best views in the suburb. This brand-new home has been thoughtfully designed to offer a low-maintenance lifestyle without compromising on the best of indoor and outdoor living.
+Well-suited to families of all ages, the home is spread across two levels with 334m2 of space on offer. The lower level has a superb feeling of space with an oversized front door leading to a grand entry and soaring ceilings. An impressive hallway leads to the separate lounge room and master downstairs with walk-in-robe and ensuite. Stairway leading upstairs opens up a whole new level of impressiveness.
+Seamlessly connecting indoor and outdoor living, the dining area opens to a secluded tiled entertainment area. The family room connects to a covered entertaining area with plenty of space to entertain family and friends.
+Sure to impress the MasterChef in any family, the huge kitchen provides ample bench and storage space including a walk-in pantry and island bench, and quality inclusions such as 40mm natural stone benchtops, soft close drawers, built-in oven and a 5 burner gas stove.
+Upstairs, an open living area provides a great break away space for the kids and the three guest bedrooms are each a generous size and are serviced by the substantial main bathroom and additional ensuite. The master suite is a haven for parents and features a private balcony with views to Molonglo Valley and telstra tower.
+To increase the comfort and enjoyment of the home, additional features include double glazed windows and doors, ducted reverse cycle heating and cooling, hybrid flooring and quality carpet, a double automatic garage with internal entry.
+Positioned within walking distance to local parks, schools and public transport, this luxurious home has it all.
+Features include:
+-Large living areas
+-Formal lounge or media room positioned at the front of the home
+-Separate guest suite with ensuite
+-Master suite with built in robes and stunning ensuite
+-Open plan living &amp; dining flows through to a covered alfresco area
+-Kitchen with natural stone benchtops, walk in pantry and quality appliances
+-Gas cooking
+-Quality carpets throughout, hybrid laminate living areas
+-Level rear yard with manicured lawn
+-Large frontage
+-Intercom
+-Water tank
+-Zoned gas reverse cycle heating &amp; cooling
+-Double lock up garage with internal access
+-Positioned close to Denman School, Wright private school, Stromlo leisure centre.
+Easy access to major arterial roads allows a short commute to the City, Woden Shopping Centre or the Belconnen Town Centre. Call Anish now on 0450 865 524 before you miss out.
+Land - 574 m2
+GFA - 334 m2
+EER: 6.0</t>
+  </si>
+  <si>
+    <t>Draft</t>
+  </si>
+  <si>
+    <t>https://www.777homes.com.au/?post_type=property&amp;p=8847&amp;preview=true</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="0"/>
   <fonts count="28">
     <font>
       <sz val="10"/>
@@ -5523,7 +5570,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="11">
+  <fills count="10">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -5577,11 +5624,6 @@
         <bgColor indexed="2"/>
       </patternFill>
     </fill>
-    <fill>
-      <patternFill patternType="mediumGray">
-        <bgColor indexed="2"/>
-      </patternFill>
-    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -5593,112 +5635,111 @@
     </border>
   </borders>
   <cellStyleXfs count="2">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
+    <xf applyAlignment="0" applyBorder="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="0" fontId="25" numFmtId="0"/>
   </cellStyleXfs>
-  <cellXfs count="48">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+  <cellXfs count="47">
+    <xf applyAlignment="1" applyFont="1" borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyAlignment="1" applyFill="1" applyFont="1" borderId="0" fillId="3" fontId="1" numFmtId="0" xfId="0">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf applyAlignment="1" applyFill="1" applyFont="1" borderId="0" fillId="2" fontId="2" numFmtId="0" xfId="0">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf applyAlignment="1" applyFill="1" applyFont="1" borderId="0" fillId="2" fontId="3" numFmtId="0" xfId="0"/>
+    <xf applyAlignment="1" applyFill="1" applyFont="1" borderId="0" fillId="2" fontId="4" numFmtId="0" xfId="0">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf applyAlignment="1" applyFill="1" applyFont="1" borderId="0" fillId="2" fontId="6" numFmtId="0" xfId="0">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf applyFill="1" applyFont="1" borderId="0" fillId="2" fontId="4" numFmtId="0" xfId="0"/>
+    <xf applyAlignment="1" applyFill="1" applyFont="1" borderId="0" fillId="2" fontId="7" numFmtId="0" xfId="0"/>
+    <xf applyAlignment="1" applyFill="1" applyFont="1" borderId="0" fillId="2" fontId="8" numFmtId="0" xfId="0"/>
+    <xf applyAlignment="1" applyFill="1" applyFont="1" borderId="0" fillId="2" fontId="5" numFmtId="0" xfId="0">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf applyAlignment="1" applyFill="1" applyFont="1" borderId="0" fillId="4" fontId="4" numFmtId="0" xfId="0">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf applyAlignment="1" applyFill="1" applyFont="1" borderId="0" fillId="5" fontId="4" numFmtId="0" xfId="0">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf applyAlignment="1" applyFill="1" applyFont="1" borderId="0" fillId="2" fontId="9" numFmtId="0" xfId="0">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="11" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf applyAlignment="1" applyFill="1" applyFont="1" borderId="0" fillId="2" fontId="10" numFmtId="0" xfId="0"/>
+    <xf applyAlignment="1" applyFill="1" applyFont="1" borderId="0" fillId="2" fontId="11" numFmtId="0" xfId="0"/>
+    <xf applyAlignment="1" applyFill="1" applyFont="1" borderId="0" fillId="2" fontId="4" numFmtId="0" xfId="0">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="13" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="14" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="15" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="16" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="17" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf applyAlignment="1" applyFill="1" applyFont="1" borderId="0" fillId="2" fontId="12" numFmtId="0" xfId="0"/>
+    <xf applyAlignment="1" applyFill="1" applyFont="1" borderId="0" fillId="2" fontId="13" numFmtId="0" xfId="0"/>
+    <xf applyAlignment="1" applyFill="1" applyFont="1" borderId="0" fillId="2" fontId="14" numFmtId="0" xfId="0"/>
+    <xf applyAlignment="1" applyFill="1" applyFont="1" borderId="0" fillId="2" fontId="15" numFmtId="0" xfId="0"/>
+    <xf applyAlignment="1" applyFill="1" applyFont="1" borderId="0" fillId="2" fontId="16" numFmtId="0" xfId="0"/>
+    <xf applyAlignment="1" applyFill="1" applyFont="1" borderId="0" fillId="2" fontId="17" numFmtId="0" xfId="0"/>
+    <xf applyAlignment="1" applyFill="1" applyFont="1" borderId="0" fillId="3" fontId="1" numFmtId="0" xfId="0">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="18" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf applyFill="1" applyFont="1" borderId="0" fillId="3" fontId="7" numFmtId="0" xfId="0"/>
+    <xf applyAlignment="1" applyFill="1" applyFont="1" borderId="0" fillId="2" fontId="18" numFmtId="0" xfId="0">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf applyAlignment="1" applyFill="1" applyFont="1" borderId="0" fillId="2" fontId="19" numFmtId="0" xfId="0">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf applyAlignment="1" applyFill="1" applyFont="1" borderId="0" fillId="2" fontId="20" numFmtId="0" xfId="0">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf applyAlignment="1" applyFill="1" applyFont="1" borderId="0" fillId="2" fontId="18" numFmtId="0" xfId="0">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf applyAlignment="1" applyFill="1" applyFont="1" borderId="0" fillId="2" fontId="21" numFmtId="0" xfId="0">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf applyAlignment="1" applyFont="1" borderId="0" fillId="0" fontId="7" numFmtId="0" xfId="0">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="12" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="22" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf applyAlignment="1" applyFill="1" applyFont="1" borderId="0" fillId="3" fontId="17" numFmtId="0" xfId="0"/>
+    <xf applyAlignment="1" applyFill="1" applyFont="1" borderId="0" fillId="3" fontId="12" numFmtId="0" xfId="0"/>
+    <xf applyAlignment="1" applyFill="1" applyFont="1" borderId="0" fillId="3" fontId="22" numFmtId="0" xfId="0">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="24" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf applyAlignment="1" applyFill="1" applyFont="1" borderId="0" fillId="3" fontId="23" numFmtId="0" xfId="0"/>
+    <xf applyAlignment="1" applyFont="1" borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0"/>
+    <xf applyAlignment="1" applyFill="1" applyFont="1" borderId="0" fillId="3" fontId="24" numFmtId="0" xfId="0">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf applyAlignment="1" applyFill="1" applyFont="1" borderId="0" fillId="3" fontId="1" numFmtId="0" xfId="0">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf applyAlignment="1" applyFont="1" borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="25" fillId="2" borderId="0" xfId="1" applyFill="1" applyAlignment="1">
+    <xf applyAlignment="1" applyFill="1" borderId="0" fillId="2" fontId="25" numFmtId="0" xfId="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf applyAlignment="1" applyFill="1" applyFont="1" borderId="0" fillId="6" fontId="2" numFmtId="0" xfId="0">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf applyAlignment="1" applyFill="1" applyFont="1" borderId="0" fillId="7" fontId="5" numFmtId="0" xfId="0">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" xfId="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="25" fillId="2" borderId="0" xfId="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="18" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf applyAlignment="1" borderId="0" fillId="0" fontId="25" numFmtId="0" xfId="1"/>
+    <xf applyAlignment="1" applyFill="1" borderId="0" fillId="2" fontId="25" numFmtId="0" xfId="1"/>
+    <xf applyAlignment="1" applyFill="1" applyFont="1" borderId="0" fillId="8" fontId="18" numFmtId="0" xfId="0">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="26" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf applyAlignment="1" applyFill="1" applyFont="1" borderId="0" fillId="2" fontId="26" numFmtId="0" xfId="0">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1"/>
+    <xf applyAlignment="1" applyFont="1" borderId="0" fillId="0" fontId="27" numFmtId="0" xfId="0"/>
+    <xf applyFill="1" borderId="0" fillId="9" fontId="0" numFmtId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="2">
-    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle builtinId="8" name="Hyperlink" xfId="1"/>
+    <cellStyle builtinId="0" name="Normal" xfId="0"/>
   </cellStyles>
   <dxfs count="2">
     <dxf>
@@ -5718,7 +5759,7 @@
       </fill>
     </dxf>
   </dxfs>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <tableStyles count="0" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium2"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -5842,21 +5883,21 @@
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
-        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cap="flat" cmpd="sng" w="6350">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
           <a:miter lim="800000"/>
         </a:ln>
-        <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cap="flat" cmpd="sng" w="12700">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
           <a:miter lim="800000"/>
         </a:ln>
-        <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cap="flat" cmpd="sng" w="19050">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
@@ -5873,7 +5914,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+            <a:outerShdw algn="ctr" blurRad="57150" dir="5400000" dist="19050" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="63000"/>
               </a:srgbClr>
@@ -5927,32 +5968,32 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:AB149"/>
+  <dimension ref="A1:AC150"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A125" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D149" sqref="D149"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane activePane="bottomLeft" state="frozen" topLeftCell="A137" ySplit="1"/>
+      <selection activeCell="B150" pane="bottomLeft" sqref="B150"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1"/>
+  <sheetFormatPr customHeight="1" defaultColWidth="14.42578125" defaultRowHeight="15.75"/>
   <cols>
-    <col min="1" max="1" width="9.140625" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="74.85546875" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="75" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="14.5703125" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="22.140625" style="37" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="21.85546875" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="56.85546875" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="10.85546875" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="17.85546875" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="22.5703125" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="9.140625" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="74.85546875" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="75.0" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="14.5703125" collapsed="true"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" style="37" width="22.140625" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" width="21.85546875" collapsed="true"/>
+    <col min="8" max="8" customWidth="true" width="56.85546875" collapsed="true"/>
+    <col min="9" max="9" customWidth="true" width="10.85546875" collapsed="true"/>
+    <col min="10" max="10" customWidth="true" width="17.85546875" collapsed="true"/>
+    <col min="11" max="11" customWidth="true" width="22.5703125" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:28" ht="15">
+    <row ht="15" r="1" spans="1:28">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -5979,7 +6020,7 @@
       </c>
       <c r="J1" s="1"/>
     </row>
-    <row r="2" spans="1:28" ht="15.75" customHeight="1">
+    <row customHeight="1" ht="15.75" r="2" spans="1:28">
       <c r="A2" s="2">
         <v>1</v>
       </c>
@@ -6025,7 +6066,7 @@
       <c r="AA2" s="6"/>
       <c r="AB2" s="6"/>
     </row>
-    <row r="3" spans="1:28" ht="14.25">
+    <row ht="14.25" r="3" spans="1:28">
       <c r="A3" s="2">
         <v>2</v>
       </c>
@@ -6071,7 +6112,7 @@
       <c r="AA3" s="6"/>
       <c r="AB3" s="6"/>
     </row>
-    <row r="4" spans="1:28" ht="15.75" customHeight="1">
+    <row customHeight="1" ht="15.75" r="4" spans="1:28">
       <c r="A4" s="9">
         <v>3</v>
       </c>
@@ -6117,7 +6158,7 @@
       <c r="AA4" s="6"/>
       <c r="AB4" s="6"/>
     </row>
-    <row r="5" spans="1:28" ht="14.25">
+    <row ht="14.25" r="5" spans="1:28">
       <c r="A5" s="9">
         <v>4</v>
       </c>
@@ -6161,7 +6202,7 @@
       <c r="AA5" s="6"/>
       <c r="AB5" s="6"/>
     </row>
-    <row r="6" spans="1:28" ht="14.25">
+    <row ht="14.25" r="6" spans="1:28">
       <c r="A6" s="9">
         <v>5</v>
       </c>
@@ -6205,7 +6246,7 @@
       <c r="AA6" s="9"/>
       <c r="AB6" s="9"/>
     </row>
-    <row r="7" spans="1:28" ht="14.25">
+    <row ht="14.25" r="7" spans="1:28">
       <c r="A7" s="9">
         <v>6</v>
       </c>
@@ -6249,7 +6290,7 @@
       <c r="AA7" s="6"/>
       <c r="AB7" s="6"/>
     </row>
-    <row r="8" spans="1:28" ht="14.25">
+    <row ht="14.25" r="8" spans="1:28">
       <c r="A8" s="9">
         <v>7</v>
       </c>
@@ -6293,7 +6334,7 @@
       <c r="AA8" s="6"/>
       <c r="AB8" s="6"/>
     </row>
-    <row r="9" spans="1:28" ht="14.25">
+    <row ht="14.25" r="9" spans="1:28">
       <c r="A9" s="9">
         <v>8</v>
       </c>
@@ -6335,7 +6376,7 @@
       <c r="AA9" s="6"/>
       <c r="AB9" s="6"/>
     </row>
-    <row r="10" spans="1:28" ht="14.25">
+    <row ht="14.25" r="10" spans="1:28">
       <c r="A10" s="9">
         <v>9</v>
       </c>
@@ -6377,7 +6418,7 @@
       <c r="AA10" s="6"/>
       <c r="AB10" s="6"/>
     </row>
-    <row r="11" spans="1:28" ht="14.25">
+    <row ht="14.25" r="11" spans="1:28">
       <c r="A11" s="9">
         <v>10</v>
       </c>
@@ -6421,7 +6462,7 @@
       <c r="AA11" s="6"/>
       <c r="AB11" s="6"/>
     </row>
-    <row r="12" spans="1:28" ht="14.25">
+    <row ht="14.25" r="12" spans="1:28">
       <c r="A12" s="9">
         <v>11</v>
       </c>
@@ -6463,7 +6504,7 @@
       <c r="AA12" s="6"/>
       <c r="AB12" s="6"/>
     </row>
-    <row r="13" spans="1:28" ht="14.25">
+    <row ht="14.25" r="13" spans="1:28">
       <c r="A13" s="9">
         <v>12</v>
       </c>
@@ -6505,7 +6546,7 @@
       <c r="AA13" s="6"/>
       <c r="AB13" s="6"/>
     </row>
-    <row r="14" spans="1:28" ht="14.25">
+    <row ht="14.25" r="14" spans="1:28">
       <c r="A14" s="9">
         <v>13</v>
       </c>
@@ -6547,7 +6588,7 @@
       <c r="AA14" s="6"/>
       <c r="AB14" s="6"/>
     </row>
-    <row r="15" spans="1:28" ht="14.25">
+    <row ht="14.25" r="15" spans="1:28">
       <c r="A15" s="9">
         <v>14</v>
       </c>
@@ -6591,7 +6632,7 @@
       <c r="AA15" s="6"/>
       <c r="AB15" s="6"/>
     </row>
-    <row r="16" spans="1:28" ht="14.25">
+    <row ht="14.25" r="16" spans="1:28">
       <c r="A16" s="9">
         <v>15</v>
       </c>
@@ -6633,7 +6674,7 @@
       <c r="AA16" s="6"/>
       <c r="AB16" s="6"/>
     </row>
-    <row r="17" spans="1:28" ht="14.25">
+    <row ht="14.25" r="17" spans="1:28">
       <c r="A17" s="9">
         <v>16</v>
       </c>
@@ -6677,7 +6718,7 @@
       <c r="AA17" s="6"/>
       <c r="AB17" s="6"/>
     </row>
-    <row r="18" spans="1:28" ht="14.25">
+    <row ht="14.25" r="18" spans="1:28">
       <c r="A18" s="9">
         <v>17</v>
       </c>
@@ -6719,7 +6760,7 @@
       <c r="AA18" s="6"/>
       <c r="AB18" s="6"/>
     </row>
-    <row r="19" spans="1:28" ht="14.25">
+    <row ht="14.25" r="19" spans="1:28">
       <c r="A19" s="9">
         <v>18</v>
       </c>
@@ -6763,7 +6804,7 @@
       <c r="AA19" s="6"/>
       <c r="AB19" s="6"/>
     </row>
-    <row r="20" spans="1:28" ht="14.25">
+    <row ht="14.25" r="20" spans="1:28">
       <c r="A20" s="9">
         <v>19</v>
       </c>
@@ -6807,7 +6848,7 @@
       <c r="AA20" s="6"/>
       <c r="AB20" s="6"/>
     </row>
-    <row r="21" spans="1:28" ht="14.25">
+    <row ht="14.25" r="21" spans="1:28">
       <c r="A21" s="9">
         <v>20</v>
       </c>
@@ -6851,7 +6892,7 @@
       <c r="AA21" s="6"/>
       <c r="AB21" s="6"/>
     </row>
-    <row r="22" spans="1:28" ht="14.25">
+    <row ht="14.25" r="22" spans="1:28">
       <c r="A22" s="9">
         <v>21</v>
       </c>
@@ -6893,7 +6934,7 @@
       <c r="AA22" s="6"/>
       <c r="AB22" s="6"/>
     </row>
-    <row r="23" spans="1:28" ht="14.25">
+    <row ht="14.25" r="23" spans="1:28">
       <c r="A23" s="9">
         <v>22</v>
       </c>
@@ -6937,7 +6978,7 @@
       <c r="AA23" s="6"/>
       <c r="AB23" s="6"/>
     </row>
-    <row r="24" spans="1:28" ht="14.25">
+    <row ht="14.25" r="24" spans="1:28">
       <c r="A24" s="9">
         <v>23</v>
       </c>
@@ -6979,7 +7020,7 @@
       <c r="AA24" s="6"/>
       <c r="AB24" s="6"/>
     </row>
-    <row r="25" spans="1:28" ht="14.25">
+    <row ht="14.25" r="25" spans="1:28">
       <c r="A25" s="9">
         <v>24</v>
       </c>
@@ -7021,7 +7062,7 @@
       <c r="AA25" s="6"/>
       <c r="AB25" s="6"/>
     </row>
-    <row r="26" spans="1:28" ht="14.25">
+    <row ht="14.25" r="26" spans="1:28">
       <c r="A26" s="9">
         <v>25</v>
       </c>
@@ -7065,7 +7106,7 @@
       <c r="AA26" s="6"/>
       <c r="AB26" s="6"/>
     </row>
-    <row r="27" spans="1:28" ht="14.25">
+    <row ht="14.25" r="27" spans="1:28">
       <c r="A27" s="9">
         <v>26</v>
       </c>
@@ -7109,7 +7150,7 @@
       <c r="AA27" s="6"/>
       <c r="AB27" s="6"/>
     </row>
-    <row r="28" spans="1:28" ht="14.25">
+    <row ht="14.25" r="28" spans="1:28">
       <c r="A28" s="9">
         <v>27</v>
       </c>
@@ -7151,7 +7192,7 @@
       <c r="AA28" s="6"/>
       <c r="AB28" s="6"/>
     </row>
-    <row r="29" spans="1:28" ht="14.25">
+    <row ht="14.25" r="29" spans="1:28">
       <c r="A29" s="9">
         <v>28</v>
       </c>
@@ -7195,7 +7236,7 @@
       <c r="AA29" s="6"/>
       <c r="AB29" s="6"/>
     </row>
-    <row r="30" spans="1:28" ht="14.25">
+    <row ht="14.25" r="30" spans="1:28">
       <c r="A30" s="9">
         <v>29</v>
       </c>
@@ -7237,7 +7278,7 @@
       <c r="AA30" s="6"/>
       <c r="AB30" s="6"/>
     </row>
-    <row r="31" spans="1:28" ht="14.25">
+    <row ht="14.25" r="31" spans="1:28">
       <c r="A31" s="4">
         <v>30</v>
       </c>
@@ -7281,7 +7322,7 @@
       <c r="AA31" s="6"/>
       <c r="AB31" s="6"/>
     </row>
-    <row r="32" spans="1:28" ht="14.25">
+    <row ht="14.25" r="32" spans="1:28">
       <c r="A32" s="4">
         <v>31</v>
       </c>
@@ -7323,7 +7364,7 @@
       <c r="AA32" s="6"/>
       <c r="AB32" s="6"/>
     </row>
-    <row r="33" spans="1:8" s="4" customFormat="1" ht="14.25">
+    <row customFormat="1" ht="14.25" r="33" s="4" spans="1:8">
       <c r="A33" s="4">
         <v>32</v>
       </c>
@@ -7346,7 +7387,7 @@
         <v>427</v>
       </c>
     </row>
-    <row r="34" spans="1:8" s="4" customFormat="1" ht="14.25">
+    <row customFormat="1" ht="14.25" r="34" s="4" spans="1:8">
       <c r="A34" s="4">
         <v>33</v>
       </c>
@@ -7366,7 +7407,7 @@
         <v>427</v>
       </c>
     </row>
-    <row r="35" spans="1:8" s="4" customFormat="1" ht="14.25">
+    <row customFormat="1" ht="14.25" r="35" s="4" spans="1:8">
       <c r="A35" s="4">
         <v>34</v>
       </c>
@@ -7386,7 +7427,7 @@
         <v>427</v>
       </c>
     </row>
-    <row r="36" spans="1:8" s="4" customFormat="1" ht="14.25">
+    <row customFormat="1" ht="14.25" r="36" s="4" spans="1:8">
       <c r="A36" s="4">
         <v>35</v>
       </c>
@@ -7406,7 +7447,7 @@
         <v>427</v>
       </c>
     </row>
-    <row r="37" spans="1:8" s="4" customFormat="1" ht="14.25">
+    <row customFormat="1" ht="14.25" r="37" s="4" spans="1:8">
       <c r="A37" s="4">
         <v>36</v>
       </c>
@@ -7426,7 +7467,7 @@
         <v>427</v>
       </c>
     </row>
-    <row r="38" spans="1:8" s="4" customFormat="1" ht="14.25">
+    <row customFormat="1" ht="14.25" r="38" s="4" spans="1:8">
       <c r="A38" s="4">
         <v>37</v>
       </c>
@@ -7449,7 +7490,7 @@
         <v>427</v>
       </c>
     </row>
-    <row r="39" spans="1:8" s="4" customFormat="1" ht="14.25">
+    <row customFormat="1" ht="14.25" r="39" s="4" spans="1:8">
       <c r="A39" s="4">
         <v>38</v>
       </c>
@@ -7472,7 +7513,7 @@
         <v>427</v>
       </c>
     </row>
-    <row r="40" spans="1:8" s="4" customFormat="1" ht="14.25">
+    <row customFormat="1" ht="14.25" r="40" s="4" spans="1:8">
       <c r="A40" s="4">
         <v>39</v>
       </c>
@@ -7495,7 +7536,7 @@
         <v>427</v>
       </c>
     </row>
-    <row r="41" spans="1:8" s="4" customFormat="1" ht="14.25">
+    <row customFormat="1" ht="14.25" r="41" s="4" spans="1:8">
       <c r="A41" s="4">
         <v>40</v>
       </c>
@@ -7515,7 +7556,7 @@
         <v>427</v>
       </c>
     </row>
-    <row r="42" spans="1:8" s="4" customFormat="1" ht="14.25">
+    <row customFormat="1" ht="14.25" r="42" s="4" spans="1:8">
       <c r="A42" s="4">
         <v>41</v>
       </c>
@@ -7538,7 +7579,7 @@
         <v>427</v>
       </c>
     </row>
-    <row r="43" spans="1:8" s="4" customFormat="1" ht="14.25">
+    <row customFormat="1" ht="14.25" r="43" s="4" spans="1:8">
       <c r="A43" s="4">
         <v>42</v>
       </c>
@@ -7558,7 +7599,7 @@
         <v>427</v>
       </c>
     </row>
-    <row r="44" spans="1:8" s="4" customFormat="1" ht="14.25">
+    <row customFormat="1" ht="14.25" r="44" s="4" spans="1:8">
       <c r="A44" s="4">
         <v>43</v>
       </c>
@@ -7578,7 +7619,7 @@
         <v>427</v>
       </c>
     </row>
-    <row r="45" spans="1:8" s="4" customFormat="1" ht="14.25">
+    <row customFormat="1" ht="14.25" r="45" s="4" spans="1:8">
       <c r="A45" s="4">
         <v>44</v>
       </c>
@@ -7601,7 +7642,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="46" spans="1:8" s="4" customFormat="1" ht="14.25">
+    <row customFormat="1" ht="14.25" r="46" s="4" spans="1:8">
       <c r="A46" s="4">
         <v>45</v>
       </c>
@@ -7621,7 +7662,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="47" spans="1:8" s="4" customFormat="1" ht="14.25">
+    <row customFormat="1" ht="14.25" r="47" s="4" spans="1:8">
       <c r="A47" s="4">
         <v>46</v>
       </c>
@@ -7641,7 +7682,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="48" spans="1:8" s="4" customFormat="1" ht="12.75">
+    <row customFormat="1" ht="12.75" r="48" s="4" spans="1:8">
       <c r="A48" s="4">
         <v>47</v>
       </c>
@@ -7664,7 +7705,7 @@
         <v>428</v>
       </c>
     </row>
-    <row r="49" spans="1:8" s="4" customFormat="1" ht="12.75">
+    <row customFormat="1" ht="12.75" r="49" s="4" spans="1:8">
       <c r="A49" s="4">
         <v>48</v>
       </c>
@@ -7687,7 +7728,7 @@
         <v>428</v>
       </c>
     </row>
-    <row r="50" spans="1:8" s="4" customFormat="1" ht="12.75">
+    <row customFormat="1" ht="12.75" r="50" s="4" spans="1:8">
       <c r="A50" s="4">
         <v>49</v>
       </c>
@@ -7707,7 +7748,7 @@
         <v>428</v>
       </c>
     </row>
-    <row r="51" spans="1:8" s="4" customFormat="1" ht="12.75">
+    <row customFormat="1" ht="12.75" r="51" s="4" spans="1:8">
       <c r="A51" s="4">
         <v>50</v>
       </c>
@@ -7727,7 +7768,7 @@
         <v>428</v>
       </c>
     </row>
-    <row r="52" spans="1:8" s="4" customFormat="1" ht="12.75">
+    <row customFormat="1" ht="12.75" r="52" s="4" spans="1:8">
       <c r="A52" s="4">
         <v>51</v>
       </c>
@@ -7750,7 +7791,7 @@
         <v>428</v>
       </c>
     </row>
-    <row r="53" spans="1:8" s="4" customFormat="1" ht="15.75" customHeight="1">
+    <row customFormat="1" customHeight="1" ht="15.75" r="53" s="4" spans="1:8">
       <c r="A53" s="4">
         <v>52</v>
       </c>
@@ -7773,7 +7814,7 @@
         <v>323</v>
       </c>
     </row>
-    <row r="54" spans="1:8" s="4" customFormat="1" ht="12.75">
+    <row customFormat="1" ht="12.75" r="54" s="4" spans="1:8">
       <c r="A54" s="4">
         <v>53</v>
       </c>
@@ -7793,7 +7834,7 @@
         <v>323</v>
       </c>
     </row>
-    <row r="55" spans="1:8" s="4" customFormat="1" ht="12.75">
+    <row customFormat="1" ht="12.75" r="55" s="4" spans="1:8">
       <c r="A55" s="4">
         <v>54</v>
       </c>
@@ -7816,7 +7857,7 @@
         <v>323</v>
       </c>
     </row>
-    <row r="56" spans="1:8" s="4" customFormat="1" ht="12.75">
+    <row customFormat="1" ht="12.75" r="56" s="4" spans="1:8">
       <c r="A56" s="4">
         <v>55</v>
       </c>
@@ -7827,7 +7868,7 @@
         <v>756</v>
       </c>
       <c r="D56" s="4" t="s">
-        <v>7</v>
+        <v>14</v>
       </c>
       <c r="F56" s="2" t="s">
         <v>686</v>
@@ -7839,7 +7880,7 @@
         <v>323</v>
       </c>
     </row>
-    <row r="57" spans="1:8" s="4" customFormat="1" ht="12.75">
+    <row customFormat="1" ht="12.75" r="57" s="4" spans="1:8">
       <c r="A57" s="4">
         <v>56</v>
       </c>
@@ -7859,7 +7900,7 @@
         <v>323</v>
       </c>
     </row>
-    <row r="58" spans="1:8" s="4" customFormat="1" ht="12.75">
+    <row customFormat="1" ht="12.75" r="58" s="4" spans="1:8">
       <c r="A58" s="4">
         <v>57</v>
       </c>
@@ -7879,7 +7920,7 @@
         <v>323</v>
       </c>
     </row>
-    <row r="59" spans="1:8" s="4" customFormat="1" ht="12.75">
+    <row customFormat="1" ht="12.75" r="59" s="4" spans="1:8">
       <c r="A59" s="4">
         <v>58</v>
       </c>
@@ -7899,7 +7940,7 @@
         <v>323</v>
       </c>
     </row>
-    <row r="60" spans="1:8" s="4" customFormat="1" ht="12.75">
+    <row customFormat="1" ht="12.75" r="60" s="4" spans="1:8">
       <c r="A60" s="4">
         <v>59</v>
       </c>
@@ -7919,7 +7960,7 @@
         <v>323</v>
       </c>
     </row>
-    <row r="61" spans="1:8" s="4" customFormat="1" ht="12.75">
+    <row customFormat="1" ht="12.75" r="61" s="4" spans="1:8">
       <c r="A61" s="4">
         <v>60</v>
       </c>
@@ -7939,7 +7980,7 @@
         <v>323</v>
       </c>
     </row>
-    <row r="62" spans="1:8" s="4" customFormat="1" ht="12.75">
+    <row customFormat="1" ht="12.75" r="62" s="4" spans="1:8">
       <c r="A62" s="4">
         <v>61</v>
       </c>
@@ -7959,7 +8000,7 @@
         <v>427</v>
       </c>
     </row>
-    <row r="63" spans="1:8" s="4" customFormat="1" ht="12.75">
+    <row customFormat="1" ht="12.75" r="63" s="4" spans="1:8">
       <c r="A63" s="4">
         <v>62</v>
       </c>
@@ -7982,7 +8023,7 @@
         <v>427</v>
       </c>
     </row>
-    <row r="64" spans="1:8" s="4" customFormat="1" ht="12.75">
+    <row customFormat="1" ht="12.75" r="64" s="4" spans="1:8">
       <c r="A64" s="4">
         <v>63</v>
       </c>
@@ -8005,7 +8046,7 @@
         <v>427</v>
       </c>
     </row>
-    <row r="65" spans="1:8" s="4" customFormat="1" ht="12.75">
+    <row customFormat="1" ht="12.75" r="65" s="4" spans="1:8">
       <c r="A65" s="4">
         <v>64</v>
       </c>
@@ -8026,7 +8067,7 @@
         <v>427</v>
       </c>
     </row>
-    <row r="66" spans="1:8" s="4" customFormat="1" ht="12.75">
+    <row customFormat="1" ht="12.75" r="66" s="4" spans="1:8">
       <c r="A66" s="4">
         <v>65</v>
       </c>
@@ -8049,7 +8090,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="67" spans="1:8" s="4" customFormat="1" ht="12.75">
+    <row customFormat="1" ht="12.75" r="67" s="4" spans="1:8">
       <c r="A67" s="4">
         <v>66</v>
       </c>
@@ -8072,7 +8113,7 @@
         <v>428</v>
       </c>
     </row>
-    <row r="68" spans="1:8" s="4" customFormat="1" ht="12.75">
+    <row customFormat="1" ht="12.75" r="68" s="4" spans="1:8">
       <c r="A68" s="4">
         <v>67</v>
       </c>
@@ -8095,7 +8136,7 @@
         <v>427</v>
       </c>
     </row>
-    <row r="69" spans="1:8" s="4" customFormat="1" ht="12.75">
+    <row customFormat="1" ht="12.75" r="69" s="4" spans="1:8">
       <c r="A69" s="4">
         <v>68</v>
       </c>
@@ -8118,7 +8159,7 @@
         <v>427</v>
       </c>
     </row>
-    <row r="70" spans="1:8" s="4" customFormat="1" ht="12.75">
+    <row customFormat="1" ht="12.75" r="70" s="4" spans="1:8">
       <c r="A70" s="4">
         <v>69</v>
       </c>
@@ -8141,7 +8182,7 @@
         <v>427</v>
       </c>
     </row>
-    <row r="71" spans="1:8" s="4" customFormat="1" ht="12.75">
+    <row customFormat="1" ht="12.75" r="71" s="4" spans="1:8">
       <c r="A71" s="4">
         <v>70</v>
       </c>
@@ -8164,7 +8205,7 @@
         <v>427</v>
       </c>
     </row>
-    <row r="72" spans="1:8" s="4" customFormat="1" ht="12.75">
+    <row customFormat="1" ht="12.75" r="72" s="4" spans="1:8">
       <c r="A72" s="4">
         <v>71</v>
       </c>
@@ -8187,7 +8228,7 @@
         <v>427</v>
       </c>
     </row>
-    <row r="73" spans="1:8" ht="12.75">
+    <row ht="12.75" r="73" spans="1:8">
       <c r="A73">
         <v>72</v>
       </c>
@@ -8210,7 +8251,7 @@
         <v>428</v>
       </c>
     </row>
-    <row r="74" spans="1:8" ht="12.75">
+    <row ht="12.75" r="74" spans="1:8">
       <c r="A74">
         <v>73</v>
       </c>
@@ -8233,7 +8274,7 @@
         <v>428</v>
       </c>
     </row>
-    <row r="75" spans="1:8" s="4" customFormat="1" ht="12.75">
+    <row customFormat="1" ht="12.75" r="75" s="4" spans="1:8">
       <c r="A75" s="4">
         <v>74</v>
       </c>
@@ -8256,7 +8297,7 @@
         <v>428</v>
       </c>
     </row>
-    <row r="76" spans="1:8" ht="12.75">
+    <row ht="12.75" r="76" spans="1:8">
       <c r="A76">
         <v>75</v>
       </c>
@@ -8279,7 +8320,7 @@
         <v>428</v>
       </c>
     </row>
-    <row r="77" spans="1:8" ht="12.75">
+    <row ht="12.75" r="77" spans="1:8">
       <c r="A77">
         <v>76</v>
       </c>
@@ -8302,7 +8343,7 @@
         <v>428</v>
       </c>
     </row>
-    <row r="78" spans="1:8" ht="12.75">
+    <row ht="12.75" r="78" spans="1:8">
       <c r="A78">
         <v>77</v>
       </c>
@@ -8325,7 +8366,7 @@
         <v>428</v>
       </c>
     </row>
-    <row r="79" spans="1:8" ht="12.75">
+    <row ht="12.75" r="79" spans="1:8">
       <c r="A79">
         <v>78</v>
       </c>
@@ -8348,7 +8389,7 @@
         <v>428</v>
       </c>
     </row>
-    <row r="80" spans="1:8" ht="12.75">
+    <row ht="12.75" r="80" spans="1:8">
       <c r="A80">
         <v>79</v>
       </c>
@@ -8371,7 +8412,7 @@
         <v>428</v>
       </c>
     </row>
-    <row r="81" spans="1:8" ht="12.75">
+    <row ht="12.75" r="81" spans="1:8">
       <c r="A81">
         <v>80</v>
       </c>
@@ -8394,7 +8435,7 @@
         <v>428</v>
       </c>
     </row>
-    <row r="82" spans="1:8" ht="12.75">
+    <row ht="12.75" r="82" spans="1:8">
       <c r="A82">
         <v>81</v>
       </c>
@@ -8417,7 +8458,7 @@
         <v>428</v>
       </c>
     </row>
-    <row r="83" spans="1:8" ht="12.75">
+    <row ht="12.75" r="83" spans="1:8">
       <c r="A83">
         <v>82</v>
       </c>
@@ -8440,7 +8481,7 @@
         <v>428</v>
       </c>
     </row>
-    <row r="84" spans="1:8" ht="12.75">
+    <row ht="12.75" r="84" spans="1:8">
       <c r="A84">
         <v>83</v>
       </c>
@@ -8463,7 +8504,7 @@
         <v>428</v>
       </c>
     </row>
-    <row r="85" spans="1:8" ht="12.75">
+    <row ht="12.75" r="85" spans="1:8">
       <c r="A85">
         <v>84</v>
       </c>
@@ -8486,7 +8527,7 @@
         <v>428</v>
       </c>
     </row>
-    <row r="86" spans="1:8" s="4" customFormat="1" ht="12.75">
+    <row customFormat="1" ht="12.75" r="86" s="4" spans="1:8">
       <c r="A86" s="4">
         <v>85</v>
       </c>
@@ -8509,7 +8550,7 @@
         <v>427</v>
       </c>
     </row>
-    <row r="87" spans="1:8" s="4" customFormat="1" ht="12.75">
+    <row customFormat="1" ht="12.75" r="87" s="4" spans="1:8">
       <c r="A87" s="4">
         <v>86</v>
       </c>
@@ -8532,7 +8573,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="88" spans="1:8" ht="12.75">
+    <row ht="12.75" r="88" spans="1:8">
       <c r="A88">
         <v>87</v>
       </c>
@@ -8555,7 +8596,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="89" spans="1:8" ht="12.75">
+    <row ht="12.75" r="89" spans="1:8">
       <c r="A89">
         <v>88</v>
       </c>
@@ -8578,7 +8619,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="90" spans="1:8" ht="12.75">
+    <row ht="12.75" r="90" spans="1:8">
       <c r="A90">
         <v>89</v>
       </c>
@@ -8601,7 +8642,7 @@
         <v>428</v>
       </c>
     </row>
-    <row r="91" spans="1:8" ht="12.75">
+    <row ht="12.75" r="91" spans="1:8">
       <c r="A91">
         <v>90</v>
       </c>
@@ -8624,7 +8665,7 @@
         <v>428</v>
       </c>
     </row>
-    <row r="92" spans="1:8" ht="12.75">
+    <row ht="12.75" r="92" spans="1:8">
       <c r="A92">
         <v>91</v>
       </c>
@@ -8647,7 +8688,7 @@
         <v>428</v>
       </c>
     </row>
-    <row r="93" spans="1:8" ht="12.75">
+    <row ht="12.75" r="93" spans="1:8">
       <c r="A93">
         <v>92</v>
       </c>
@@ -8670,7 +8711,7 @@
         <v>428</v>
       </c>
     </row>
-    <row r="94" spans="1:8" ht="12.75">
+    <row ht="12.75" r="94" spans="1:8">
       <c r="A94">
         <v>93</v>
       </c>
@@ -8693,7 +8734,7 @@
         <v>427</v>
       </c>
     </row>
-    <row r="95" spans="1:8" ht="12.75">
+    <row ht="12.75" r="95" spans="1:8">
       <c r="A95">
         <v>94</v>
       </c>
@@ -8716,7 +8757,7 @@
         <v>427</v>
       </c>
     </row>
-    <row r="96" spans="1:8" ht="12.75">
+    <row ht="12.75" r="96" spans="1:8">
       <c r="A96">
         <v>95</v>
       </c>
@@ -8739,7 +8780,7 @@
         <v>427</v>
       </c>
     </row>
-    <row r="97" spans="1:8" ht="12.75">
+    <row ht="12.75" r="97" spans="1:8">
       <c r="A97">
         <v>96</v>
       </c>
@@ -8762,7 +8803,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="98" spans="1:8" ht="12.75">
+    <row ht="12.75" r="98" spans="1:8">
       <c r="A98">
         <v>97</v>
       </c>
@@ -8785,7 +8826,7 @@
         <v>428</v>
       </c>
     </row>
-    <row r="99" spans="1:8" ht="12.75">
+    <row ht="12.75" r="99" spans="1:8">
       <c r="A99">
         <v>98</v>
       </c>
@@ -8808,7 +8849,7 @@
         <v>427</v>
       </c>
     </row>
-    <row r="100" spans="1:8" ht="12.75">
+    <row ht="12.75" r="100" spans="1:8">
       <c r="A100">
         <v>99</v>
       </c>
@@ -8831,7 +8872,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="101" spans="1:8" ht="12.75">
+    <row ht="12.75" r="101" spans="1:8">
       <c r="A101">
         <v>100</v>
       </c>
@@ -8854,7 +8895,7 @@
         <v>428</v>
       </c>
     </row>
-    <row r="102" spans="1:8" ht="12.75">
+    <row ht="12.75" r="102" spans="1:8">
       <c r="A102">
         <v>101</v>
       </c>
@@ -8877,7 +8918,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="103" spans="1:8" ht="12.75">
+    <row ht="12.75" r="103" spans="1:8">
       <c r="A103">
         <v>102</v>
       </c>
@@ -8900,7 +8941,7 @@
         <v>428</v>
       </c>
     </row>
-    <row r="104" spans="1:8" ht="12.75">
+    <row ht="12.75" r="104" spans="1:8">
       <c r="A104">
         <v>103</v>
       </c>
@@ -8923,7 +8964,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="105" spans="1:8" ht="12.75">
+    <row ht="12.75" r="105" spans="1:8">
       <c r="A105">
         <v>104</v>
       </c>
@@ -8946,7 +8987,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="106" spans="1:8" ht="12.75">
+    <row ht="12.75" r="106" spans="1:8">
       <c r="A106">
         <v>105</v>
       </c>
@@ -8969,7 +9010,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="107" spans="1:8" ht="12.75">
+    <row ht="12.75" r="107" spans="1:8">
       <c r="A107">
         <v>106</v>
       </c>
@@ -8992,7 +9033,7 @@
         <v>427</v>
       </c>
     </row>
-    <row r="108" spans="1:8" ht="12.75">
+    <row ht="12.75" r="108" spans="1:8">
       <c r="A108">
         <v>107</v>
       </c>
@@ -9015,7 +9056,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="109" spans="1:8" ht="12.75">
+    <row ht="12.75" r="109" spans="1:8">
       <c r="A109">
         <v>108</v>
       </c>
@@ -9038,7 +9079,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="110" spans="1:8" ht="12.75">
+    <row ht="12.75" r="110" spans="1:8">
       <c r="A110">
         <v>109</v>
       </c>
@@ -9061,7 +9102,7 @@
         <v>428</v>
       </c>
     </row>
-    <row r="111" spans="1:8" ht="12.75">
+    <row ht="12.75" r="111" spans="1:8">
       <c r="A111">
         <v>110</v>
       </c>
@@ -9084,7 +9125,7 @@
         <v>428</v>
       </c>
     </row>
-    <row r="112" spans="1:8" ht="12.75">
+    <row ht="12.75" r="112" spans="1:8">
       <c r="A112">
         <v>111</v>
       </c>
@@ -9107,7 +9148,7 @@
         <v>428</v>
       </c>
     </row>
-    <row r="113" spans="1:8" ht="12.75">
+    <row ht="12.75" r="113" spans="1:8">
       <c r="A113">
         <v>112</v>
       </c>
@@ -9130,7 +9171,7 @@
         <v>428</v>
       </c>
     </row>
-    <row r="114" spans="1:8" ht="12.75">
+    <row ht="12.75" r="114" spans="1:8">
       <c r="A114">
         <v>113</v>
       </c>
@@ -9153,7 +9194,7 @@
         <v>427</v>
       </c>
     </row>
-    <row r="115" spans="1:8" ht="12.75">
+    <row ht="12.75" r="115" spans="1:8">
       <c r="A115">
         <v>114</v>
       </c>
@@ -9176,7 +9217,7 @@
         <v>323</v>
       </c>
     </row>
-    <row r="116" spans="1:8" ht="12.75">
+    <row ht="12.75" r="116" spans="1:8">
       <c r="A116">
         <v>115</v>
       </c>
@@ -9199,7 +9240,7 @@
         <v>427</v>
       </c>
     </row>
-    <row r="117" spans="1:8" ht="12.75">
+    <row ht="12.75" r="117" spans="1:8">
       <c r="A117">
         <v>116</v>
       </c>
@@ -9222,7 +9263,7 @@
         <v>428</v>
       </c>
     </row>
-    <row r="118" spans="1:8" ht="12.75">
+    <row ht="12.75" r="118" spans="1:8">
       <c r="A118">
         <v>117</v>
       </c>
@@ -9242,7 +9283,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="119" spans="1:8" ht="12.75">
+    <row ht="12.75" r="119" spans="1:8">
       <c r="A119">
         <v>118</v>
       </c>
@@ -9265,7 +9306,7 @@
         <v>428</v>
       </c>
     </row>
-    <row r="120" spans="1:8" ht="15.75" customHeight="1">
+    <row customHeight="1" ht="15.75" r="120" spans="1:8">
       <c r="A120">
         <v>119</v>
       </c>
@@ -9288,7 +9329,7 @@
         <v>881</v>
       </c>
     </row>
-    <row r="121" spans="1:8" ht="12.75">
+    <row ht="12.75" r="121" spans="1:8">
       <c r="A121">
         <v>120</v>
       </c>
@@ -9311,7 +9352,7 @@
         <v>881</v>
       </c>
     </row>
-    <row r="122" spans="1:8" ht="12.75">
+    <row ht="12.75" r="122" spans="1:8">
       <c r="A122">
         <v>121</v>
       </c>
@@ -9334,7 +9375,7 @@
         <v>881</v>
       </c>
     </row>
-    <row r="123" spans="1:8" ht="12.75">
+    <row ht="12.75" r="123" spans="1:8">
       <c r="A123">
         <v>122</v>
       </c>
@@ -9357,7 +9398,7 @@
         <v>881</v>
       </c>
     </row>
-    <row r="124" spans="1:8" ht="12.75">
+    <row ht="12.75" r="124" spans="1:8">
       <c r="A124">
         <v>123</v>
       </c>
@@ -9380,7 +9421,7 @@
         <v>881</v>
       </c>
     </row>
-    <row r="125" spans="1:8" ht="12.75">
+    <row ht="12.75" r="125" spans="1:8">
       <c r="A125">
         <v>124</v>
       </c>
@@ -9403,7 +9444,7 @@
         <v>881</v>
       </c>
     </row>
-    <row r="126" spans="1:8" ht="12.75">
+    <row ht="12.75" r="126" spans="1:8">
       <c r="A126">
         <v>125</v>
       </c>
@@ -9426,7 +9467,7 @@
         <v>881</v>
       </c>
     </row>
-    <row r="127" spans="1:8" ht="12.75">
+    <row ht="12.75" r="127" spans="1:8">
       <c r="A127">
         <v>126</v>
       </c>
@@ -9449,7 +9490,7 @@
         <v>881</v>
       </c>
     </row>
-    <row r="128" spans="1:8" ht="12.75">
+    <row ht="12.75" r="128" spans="1:8">
       <c r="A128">
         <v>127</v>
       </c>
@@ -9472,7 +9513,7 @@
         <v>881</v>
       </c>
     </row>
-    <row r="129" spans="1:8" ht="12.75">
+    <row ht="12.75" r="129" spans="1:8">
       <c r="A129">
         <v>128</v>
       </c>
@@ -9495,7 +9536,7 @@
         <v>881</v>
       </c>
     </row>
-    <row r="130" spans="1:8" ht="12.75">
+    <row ht="12.75" r="130" spans="1:8">
       <c r="A130">
         <v>129</v>
       </c>
@@ -9518,7 +9559,7 @@
         <v>881</v>
       </c>
     </row>
-    <row r="131" spans="1:8" ht="12.75">
+    <row ht="12.75" r="131" spans="1:8">
       <c r="A131">
         <v>130</v>
       </c>
@@ -9541,7 +9582,7 @@
         <v>881</v>
       </c>
     </row>
-    <row r="132" spans="1:8" ht="12.75">
+    <row ht="12.75" r="132" spans="1:8">
       <c r="A132">
         <v>131</v>
       </c>
@@ -9564,7 +9605,7 @@
         <v>881</v>
       </c>
     </row>
-    <row r="133" spans="1:8" ht="12.75">
+    <row ht="12.75" r="133" spans="1:8">
       <c r="A133">
         <v>132</v>
       </c>
@@ -9587,7 +9628,7 @@
         <v>881</v>
       </c>
     </row>
-    <row r="134" spans="1:8" ht="12.75">
+    <row ht="12.75" r="134" spans="1:8">
       <c r="A134">
         <v>133</v>
       </c>
@@ -9610,7 +9651,7 @@
         <v>881</v>
       </c>
     </row>
-    <row r="135" spans="1:8" ht="12.75">
+    <row ht="12.75" r="135" spans="1:8">
       <c r="A135">
         <v>134</v>
       </c>
@@ -9633,7 +9674,7 @@
         <v>881</v>
       </c>
     </row>
-    <row r="136" spans="1:8" ht="12.75">
+    <row ht="12.75" r="136" spans="1:8">
       <c r="A136">
         <v>135</v>
       </c>
@@ -9656,7 +9697,7 @@
         <v>881</v>
       </c>
     </row>
-    <row r="137" spans="1:8" ht="12.75">
+    <row ht="12.75" r="137" spans="1:8">
       <c r="A137">
         <v>136</v>
       </c>
@@ -9679,7 +9720,7 @@
         <v>881</v>
       </c>
     </row>
-    <row r="138" spans="1:8" ht="12.75">
+    <row ht="12.75" r="138" spans="1:8">
       <c r="A138">
         <v>137</v>
       </c>
@@ -9702,7 +9743,7 @@
         <v>881</v>
       </c>
     </row>
-    <row r="139" spans="1:8" ht="12.75">
+    <row ht="12.75" r="139" spans="1:8">
       <c r="A139">
         <v>138</v>
       </c>
@@ -9725,7 +9766,7 @@
         <v>881</v>
       </c>
     </row>
-    <row r="140" spans="1:8" ht="12.75">
+    <row ht="12.75" r="140" spans="1:8">
       <c r="A140">
         <v>139</v>
       </c>
@@ -9748,7 +9789,7 @@
         <v>881</v>
       </c>
     </row>
-    <row r="141" spans="1:8" ht="12.75">
+    <row ht="12.75" r="141" spans="1:8">
       <c r="A141">
         <v>140</v>
       </c>
@@ -9771,7 +9812,7 @@
         <v>881</v>
       </c>
     </row>
-    <row r="142" spans="1:8" ht="12.75">
+    <row ht="12.75" r="142" spans="1:8">
       <c r="A142">
         <v>141</v>
       </c>
@@ -9794,7 +9835,7 @@
         <v>881</v>
       </c>
     </row>
-    <row r="143" spans="1:8" ht="12.75">
+    <row ht="12.75" r="143" spans="1:8">
       <c r="A143">
         <v>142</v>
       </c>
@@ -9817,7 +9858,7 @@
         <v>881</v>
       </c>
     </row>
-    <row r="144" spans="1:8" ht="12.75">
+    <row ht="12.75" r="144" spans="1:8">
       <c r="A144">
         <v>143</v>
       </c>
@@ -9840,7 +9881,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="145" spans="1:8" ht="12.75">
+    <row ht="12.75" r="145" spans="1:8">
       <c r="A145">
         <v>144</v>
       </c>
@@ -9863,7 +9904,7 @@
         <v>428</v>
       </c>
     </row>
-    <row r="146" spans="1:8" ht="12.75">
+    <row ht="12.75" r="146" spans="1:8">
       <c r="A146">
         <v>145</v>
       </c>
@@ -9886,7 +9927,7 @@
         <v>427</v>
       </c>
     </row>
-    <row r="147" spans="1:8" ht="12.75">
+    <row ht="12.75" r="147" spans="1:8">
       <c r="A147">
         <v>146</v>
       </c>
@@ -9909,7 +9950,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="148" spans="1:8" ht="12.75">
+    <row ht="12.75" r="148" spans="1:8">
       <c r="A148">
         <v>147</v>
       </c>
@@ -9932,7 +9973,7 @@
         <v>881</v>
       </c>
     </row>
-    <row r="149" spans="1:8" ht="12.75">
+    <row ht="12.75" r="149" spans="1:8">
       <c r="A149">
         <v>148</v>
       </c>
@@ -9955,237 +9996,261 @@
         <v>881</v>
       </c>
     </row>
+    <row ht="12.75" r="150" spans="1:8">
+      <c r="A150">
+        <v>149</v>
+      </c>
+      <c r="B150" s="41" t="s">
+        <v>1100</v>
+      </c>
+      <c r="C150" t="s">
+        <v>1106</v>
+      </c>
+      <c r="D150" s="46" t="s">
+        <v>1105</v>
+      </c>
+      <c r="F150" s="2" t="s">
+        <v>687</v>
+      </c>
+      <c r="G150" t="s">
+        <v>1044</v>
+      </c>
+      <c r="H150" t="s">
+        <v>881</v>
+      </c>
+    </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B2" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
-    <hyperlink ref="B3" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
-    <hyperlink ref="B4" r:id="rId3" xr:uid="{00000000-0004-0000-0000-000002000000}"/>
-    <hyperlink ref="B5" r:id="rId4" xr:uid="{00000000-0004-0000-0000-000003000000}"/>
-    <hyperlink ref="B6" r:id="rId5" xr:uid="{00000000-0004-0000-0000-000004000000}"/>
-    <hyperlink ref="H6" r:id="rId6" xr:uid="{00000000-0004-0000-0000-000005000000}"/>
-    <hyperlink ref="B7" r:id="rId7" xr:uid="{00000000-0004-0000-0000-000006000000}"/>
-    <hyperlink ref="B8" r:id="rId8" xr:uid="{00000000-0004-0000-0000-000007000000}"/>
-    <hyperlink ref="B9" r:id="rId9" xr:uid="{00000000-0004-0000-0000-000008000000}"/>
-    <hyperlink ref="B10" r:id="rId10" xr:uid="{00000000-0004-0000-0000-000009000000}"/>
-    <hyperlink ref="B11" r:id="rId11" xr:uid="{00000000-0004-0000-0000-00000A000000}"/>
-    <hyperlink ref="B12" r:id="rId12" xr:uid="{00000000-0004-0000-0000-00000B000000}"/>
-    <hyperlink ref="B13" r:id="rId13" xr:uid="{00000000-0004-0000-0000-00000C000000}"/>
-    <hyperlink ref="B14" r:id="rId14" xr:uid="{00000000-0004-0000-0000-00000D000000}"/>
-    <hyperlink ref="B15" r:id="rId15" xr:uid="{00000000-0004-0000-0000-00000E000000}"/>
-    <hyperlink ref="B16" r:id="rId16" xr:uid="{00000000-0004-0000-0000-00000F000000}"/>
-    <hyperlink ref="B17" r:id="rId17" xr:uid="{00000000-0004-0000-0000-000010000000}"/>
-    <hyperlink ref="B18" r:id="rId18" xr:uid="{00000000-0004-0000-0000-000011000000}"/>
-    <hyperlink ref="B19" r:id="rId19" xr:uid="{00000000-0004-0000-0000-000012000000}"/>
-    <hyperlink ref="B20" r:id="rId20" xr:uid="{00000000-0004-0000-0000-000013000000}"/>
-    <hyperlink ref="B21" r:id="rId21" xr:uid="{00000000-0004-0000-0000-000014000000}"/>
-    <hyperlink ref="B22" r:id="rId22" xr:uid="{00000000-0004-0000-0000-000015000000}"/>
-    <hyperlink ref="B23" r:id="rId23" xr:uid="{00000000-0004-0000-0000-000016000000}"/>
-    <hyperlink ref="B24" r:id="rId24" xr:uid="{00000000-0004-0000-0000-000017000000}"/>
-    <hyperlink ref="B25" r:id="rId25" xr:uid="{00000000-0004-0000-0000-000018000000}"/>
-    <hyperlink ref="H25" r:id="rId26" xr:uid="{00000000-0004-0000-0000-000019000000}"/>
-    <hyperlink ref="B26" r:id="rId27" xr:uid="{00000000-0004-0000-0000-00001A000000}"/>
-    <hyperlink ref="H26" r:id="rId28" xr:uid="{00000000-0004-0000-0000-00001B000000}"/>
-    <hyperlink ref="B27" r:id="rId29" xr:uid="{00000000-0004-0000-0000-00001C000000}"/>
-    <hyperlink ref="H27" r:id="rId30" xr:uid="{00000000-0004-0000-0000-00001D000000}"/>
-    <hyperlink ref="B28" r:id="rId31" xr:uid="{00000000-0004-0000-0000-00001E000000}"/>
-    <hyperlink ref="H28" r:id="rId32" xr:uid="{00000000-0004-0000-0000-00001F000000}"/>
-    <hyperlink ref="B29" r:id="rId33" xr:uid="{00000000-0004-0000-0000-000020000000}"/>
-    <hyperlink ref="H29" r:id="rId34" xr:uid="{00000000-0004-0000-0000-000021000000}"/>
-    <hyperlink ref="B30" r:id="rId35" xr:uid="{00000000-0004-0000-0000-000022000000}"/>
-    <hyperlink ref="H30" r:id="rId36" xr:uid="{00000000-0004-0000-0000-000023000000}"/>
-    <hyperlink ref="B31" r:id="rId37" xr:uid="{00000000-0004-0000-0000-000024000000}"/>
-    <hyperlink ref="H31" r:id="rId38" xr:uid="{00000000-0004-0000-0000-000025000000}"/>
-    <hyperlink ref="B32" r:id="rId39" xr:uid="{00000000-0004-0000-0000-000026000000}"/>
-    <hyperlink ref="H32" r:id="rId40" xr:uid="{00000000-0004-0000-0000-000027000000}"/>
-    <hyperlink ref="B33" r:id="rId41" xr:uid="{00000000-0004-0000-0000-000028000000}"/>
-    <hyperlink ref="B34" r:id="rId42" xr:uid="{00000000-0004-0000-0000-000029000000}"/>
-    <hyperlink ref="B38" r:id="rId43" xr:uid="{00000000-0004-0000-0000-00002A000000}"/>
-    <hyperlink ref="B45" r:id="rId44" xr:uid="{00000000-0004-0000-0000-00002B000000}"/>
-    <hyperlink ref="B48" r:id="rId45" xr:uid="{00000000-0004-0000-0000-00002C000000}"/>
-    <hyperlink ref="B35" r:id="rId46" xr:uid="{00000000-0004-0000-0000-00002D000000}"/>
-    <hyperlink ref="B52" r:id="rId47" xr:uid="{00000000-0004-0000-0000-00002E000000}"/>
-    <hyperlink ref="B53" r:id="rId48" xr:uid="{00000000-0004-0000-0000-00002F000000}"/>
-    <hyperlink ref="B55" r:id="rId49" xr:uid="{00000000-0004-0000-0000-000030000000}"/>
-    <hyperlink ref="B56" r:id="rId50" xr:uid="{00000000-0004-0000-0000-000031000000}"/>
-    <hyperlink ref="B57" r:id="rId51" xr:uid="{00000000-0004-0000-0000-000032000000}"/>
-    <hyperlink ref="B58" r:id="rId52" xr:uid="{00000000-0004-0000-0000-000033000000}"/>
-    <hyperlink ref="B61" r:id="rId53" xr:uid="{00000000-0004-0000-0000-000034000000}"/>
-    <hyperlink ref="B62" r:id="rId54" xr:uid="{00000000-0004-0000-0000-000035000000}"/>
-    <hyperlink ref="B63" r:id="rId55" xr:uid="{00000000-0004-0000-0000-000036000000}"/>
-    <hyperlink ref="B64" r:id="rId56" xr:uid="{00000000-0004-0000-0000-000037000000}"/>
-    <hyperlink ref="B65" r:id="rId57" xr:uid="{00000000-0004-0000-0000-000038000000}"/>
-    <hyperlink ref="B66" r:id="rId58" xr:uid="{00000000-0004-0000-0000-000039000000}"/>
-    <hyperlink ref="B67" r:id="rId59" xr:uid="{00000000-0004-0000-0000-00003A000000}"/>
-    <hyperlink ref="H7:H24" r:id="rId60" display="https://www.allhomes.com.au/agency/trusted-realtors-570129/" xr:uid="{00000000-0004-0000-0000-00003B000000}"/>
-    <hyperlink ref="B43" r:id="rId61" xr:uid="{00000000-0004-0000-0000-00003C000000}"/>
-    <hyperlink ref="B44" r:id="rId62" xr:uid="{00000000-0004-0000-0000-00003D000000}"/>
-    <hyperlink ref="B46" r:id="rId63" xr:uid="{00000000-0004-0000-0000-00003E000000}"/>
-    <hyperlink ref="B54" r:id="rId64" xr:uid="{00000000-0004-0000-0000-00003F000000}"/>
-    <hyperlink ref="B42" r:id="rId65" xr:uid="{00000000-0004-0000-0000-000040000000}"/>
-    <hyperlink ref="J2" r:id="rId66" xr:uid="{00000000-0004-0000-0000-000041000000}"/>
-    <hyperlink ref="C69" r:id="rId67" xr:uid="{9DAE03A7-93E8-4507-BD6C-AC4013ECD47F}"/>
-    <hyperlink ref="C68" r:id="rId68" xr:uid="{66B9A9CA-DF82-46B6-9C5A-C5709E2FF1AE}"/>
-    <hyperlink ref="B75" r:id="rId69" xr:uid="{57E7BFEF-6F05-4DA9-A3DE-5B0A0EFED4D9}"/>
-    <hyperlink ref="C75" r:id="rId70" xr:uid="{F4755F93-6E59-4C38-BF66-16746869FDF3}"/>
-    <hyperlink ref="H75" r:id="rId71" xr:uid="{5BFAFD71-42C4-487F-B5E7-1697975992B4}"/>
-    <hyperlink ref="B78" r:id="rId72" xr:uid="{D3DE0D76-2479-4283-B7C7-F11B85797022}"/>
-    <hyperlink ref="C78" r:id="rId73" xr:uid="{FC1D9146-2FDC-4F13-A3C3-51CAB46DEC08}"/>
-    <hyperlink ref="B68" r:id="rId74" xr:uid="{3ED6FAA1-2B0F-4DB9-878E-9640A9C2850D}"/>
-    <hyperlink ref="B69" r:id="rId75" xr:uid="{12DE6CA8-DDC5-4E7B-BD2E-14B105A0DE3B}"/>
-    <hyperlink ref="C70" r:id="rId76" xr:uid="{0419758C-286A-4B76-B8B2-31CC336DEDF1}"/>
-    <hyperlink ref="B70" r:id="rId77" xr:uid="{AC18D1D2-FA3D-4352-A402-35B7AAFE27C0}"/>
-    <hyperlink ref="B71" r:id="rId78" xr:uid="{E8BCA1EF-4E17-4AA7-A2CE-5674FC05ABC3}"/>
-    <hyperlink ref="C71" r:id="rId79" xr:uid="{949AE606-DF4A-48F4-93A0-F148D80842CB}"/>
-    <hyperlink ref="B72" r:id="rId80" xr:uid="{69A93BB5-0295-46D6-8334-45444356E6E9}"/>
-    <hyperlink ref="C72" r:id="rId81" xr:uid="{CA171BC7-126F-4175-8A03-123D5A2C2D8A}"/>
-    <hyperlink ref="C73" r:id="rId82" xr:uid="{FACC205D-E563-4266-8E0D-0794F3D76E98}"/>
-    <hyperlink ref="B85" r:id="rId83" xr:uid="{7ABCABC0-A765-435B-AE52-9D27F653E00F}"/>
-    <hyperlink ref="C4" r:id="rId84" xr:uid="{2CD58DBE-98E3-4EDC-898F-088D5F0FCB81}"/>
-    <hyperlink ref="C29" r:id="rId85" xr:uid="{CB7CAD83-ACA3-4309-B102-B0F536FC97E6}"/>
-    <hyperlink ref="C90" r:id="rId86" xr:uid="{B4F55488-2B40-4078-ABF0-4B4254363237}"/>
-    <hyperlink ref="B90" r:id="rId87" xr:uid="{09FEE7FE-E667-40E8-BC22-3FDC999B614F}"/>
-    <hyperlink ref="C15" r:id="rId88" xr:uid="{34F25BA9-B460-46CF-85C0-4AC9D6288B41}"/>
-    <hyperlink ref="C3" r:id="rId89" xr:uid="{EBAAEE7A-83B2-457B-8600-89427BF11448}"/>
-    <hyperlink ref="C8" r:id="rId90" xr:uid="{3D3D678C-8F1B-47BC-ACA2-D1CBF5A76F0B}"/>
-    <hyperlink ref="C19" r:id="rId91" xr:uid="{ED2C9A9B-3440-4B4A-91A1-7CAF84972535}"/>
-    <hyperlink ref="C20" r:id="rId92" xr:uid="{E47C999F-11AE-4F93-9032-6E51EB582635}"/>
-    <hyperlink ref="C21" r:id="rId93" xr:uid="{E59411CC-EC13-4665-969A-8D9238CCD0C2}"/>
-    <hyperlink ref="C33" r:id="rId94" xr:uid="{9C953AB9-0076-4477-B52F-C393846B1211}"/>
-    <hyperlink ref="C38" r:id="rId95" xr:uid="{D349EA20-36BF-44C7-A16B-E85B8FE53B2A}"/>
-    <hyperlink ref="C39" r:id="rId96" xr:uid="{DE18DA3B-1A3D-4613-888E-7F506CC87091}"/>
-    <hyperlink ref="C40" r:id="rId97" xr:uid="{0C71282B-049B-4CD1-A090-B66647F2B29B}"/>
-    <hyperlink ref="C42" r:id="rId98" xr:uid="{AD0DC851-DEC5-4ACE-B928-50149068BB70}"/>
-    <hyperlink ref="C45" r:id="rId99" xr:uid="{EB51DFC2-D28F-4E0C-B019-F9954D6C9832}"/>
-    <hyperlink ref="C52" r:id="rId100" xr:uid="{9E5146F6-8EC8-4A2C-B192-C1CCB11CAB8A}"/>
-    <hyperlink ref="C48" r:id="rId101" xr:uid="{31B308E4-DA3E-401B-B796-7D03404228FB}"/>
-    <hyperlink ref="C49" r:id="rId102" xr:uid="{EBAAB9CE-7F91-4628-AF75-32C4EEF948C2}"/>
-    <hyperlink ref="C53" r:id="rId103" xr:uid="{2FF7EB1F-CD56-4E71-AD0F-0D12E8347603}"/>
-    <hyperlink ref="C55" r:id="rId104" xr:uid="{9BD44DCD-EEBB-4649-9792-F3DAC40B3960}"/>
-    <hyperlink ref="C63" r:id="rId105" xr:uid="{9929BCF4-32FD-4143-99F6-FEB21B90BCD7}"/>
-    <hyperlink ref="C64" r:id="rId106" xr:uid="{80B3DEC9-506E-4F3A-B171-A2D71B731577}"/>
-    <hyperlink ref="C66" r:id="rId107" xr:uid="{011D2C70-C541-49D4-894E-FF670D6C19BB}"/>
-    <hyperlink ref="C67" r:id="rId108" xr:uid="{B62DFA3B-60A0-44AA-BF1D-BCA2A049E46C}"/>
-    <hyperlink ref="C56" r:id="rId109" xr:uid="{C98B5D5D-65AB-489D-8160-8F1B41CDE6A7}"/>
-    <hyperlink ref="B103" r:id="rId110" xr:uid="{4D81C408-B745-40E2-B9C7-6E36C45175A7}"/>
-    <hyperlink ref="C26" r:id="rId111" xr:uid="{6A9C6F44-3E7F-47CF-8514-B6609EBEE668}"/>
-    <hyperlink ref="C23" r:id="rId112" xr:uid="{F99F350A-C378-4940-B611-41F47BC3B4B0}"/>
-    <hyperlink ref="C103" r:id="rId113" xr:uid="{3E9C8DCE-ABC0-49DA-B64B-B569BAAE6ED0}"/>
-    <hyperlink ref="C104" r:id="rId114" xr:uid="{E96AA061-2DED-4A35-BE99-8E7E156527EB}"/>
-    <hyperlink ref="C102" r:id="rId115" xr:uid="{4DAA7E56-3BCD-4AF1-B6E7-A26B02A0DA6C}"/>
-    <hyperlink ref="C101" r:id="rId116" xr:uid="{EBE0EC7F-0880-4F4A-991C-2C7C53889923}"/>
-    <hyperlink ref="C100" r:id="rId117" xr:uid="{7AA4A2D0-C18F-4625-A776-6EDD2415E1BC}"/>
-    <hyperlink ref="C99" r:id="rId118" xr:uid="{15BFB680-4225-425B-8826-841A35922C8A}"/>
-    <hyperlink ref="B99" r:id="rId119" xr:uid="{1EF2BF94-D92B-41EF-8B1F-0585F1910B74}"/>
-    <hyperlink ref="C97" r:id="rId120" xr:uid="{6687C5A1-CC2B-49FF-B98D-946AA21B8C55}"/>
-    <hyperlink ref="B97" r:id="rId121" xr:uid="{0411E592-2DE8-4D1D-B66C-46CE99CAA412}"/>
-    <hyperlink ref="C96" r:id="rId122" xr:uid="{A7ED7210-DE23-4760-B67F-78027E9B9B73}"/>
-    <hyperlink ref="B96" r:id="rId123" xr:uid="{992F1752-E440-4347-A698-44C8E60F00BE}"/>
-    <hyperlink ref="B102" r:id="rId124" xr:uid="{A0E03FB2-010F-497D-874D-A0A66FB6303C}"/>
-    <hyperlink ref="B101" r:id="rId125" xr:uid="{165FBF6F-9195-42DA-AC37-C49B2308ACA1}"/>
-    <hyperlink ref="B94" r:id="rId126" xr:uid="{7DB2C8A6-8C43-4818-A7C2-D5E14351114B}"/>
-    <hyperlink ref="B93" r:id="rId127" xr:uid="{EFC122F7-44E7-447B-8F21-BA1503A72780}"/>
-    <hyperlink ref="B91" r:id="rId128" xr:uid="{7AC22E1D-6919-43E6-AD91-1551DBBDE570}"/>
-    <hyperlink ref="B88" r:id="rId129" xr:uid="{FB3E9840-E4E3-4E64-8CCF-2BAEC7024AD6}"/>
-    <hyperlink ref="B87" r:id="rId130" xr:uid="{348337ED-A616-4A9D-A8D3-0091262177C6}"/>
-    <hyperlink ref="B86" r:id="rId131" xr:uid="{CF62843D-4B82-47CB-B74F-D3F292E9603A}"/>
-    <hyperlink ref="B84" r:id="rId132" xr:uid="{9CA10EFF-3943-479E-914B-1D6EE04D75FC}"/>
-    <hyperlink ref="C84" r:id="rId133" xr:uid="{1074AAC9-CCB0-4FFC-9AFB-EFD1363D7538}"/>
-    <hyperlink ref="B105" r:id="rId134" xr:uid="{D6DE2797-5A68-4C1E-9E74-0D323B6ADFA2}"/>
-    <hyperlink ref="B106" r:id="rId135" xr:uid="{1FCAF9BA-00B5-4008-B5C8-E822ABD6BCDD}"/>
-    <hyperlink ref="C11" r:id="rId136" xr:uid="{893B2404-B185-41F7-B397-A3E08B386C5F}"/>
-    <hyperlink ref="B107" r:id="rId137" xr:uid="{B0E609F4-D8A3-433A-BE15-17E4804C6EA3}"/>
-    <hyperlink ref="C107" r:id="rId138" xr:uid="{6793ECA4-A034-42EC-A741-3B0FF42BC11B}"/>
-    <hyperlink ref="B108" r:id="rId139" xr:uid="{4DB78F44-0F08-4561-A0E8-0EE92F9FFECB}"/>
-    <hyperlink ref="B114" r:id="rId140" xr:uid="{27750164-38B8-4B5E-9B5A-E6C71FFFC61F}"/>
-    <hyperlink ref="C114" r:id="rId141" xr:uid="{6FE6A043-A6B1-44FF-8A45-8C3690323458}"/>
-    <hyperlink ref="B113" r:id="rId142" xr:uid="{0F94FF41-1E06-4D7B-B360-1EB377073C87}"/>
-    <hyperlink ref="B112" r:id="rId143" xr:uid="{490A5044-10EC-4082-BEC1-14008171D5CF}"/>
-    <hyperlink ref="B49" r:id="rId144" xr:uid="{836EB236-8BF1-4259-B395-AD9FA9DE0AE0}"/>
-    <hyperlink ref="B74" r:id="rId145" xr:uid="{8AA8904A-1CC5-4D06-93EF-66F7FC625199}"/>
-    <hyperlink ref="B76" r:id="rId146" xr:uid="{5743888C-C74A-41C6-ABC5-E9575351702D}"/>
-    <hyperlink ref="B115" r:id="rId147" xr:uid="{27BDB583-8AD0-4B33-BA19-24E42C9E7CE9}"/>
-    <hyperlink ref="B117" r:id="rId148" xr:uid="{92BA6213-0D94-4C5A-B06A-6FC35C0BECA9}"/>
-    <hyperlink ref="B119" r:id="rId149" xr:uid="{6724AE23-65F5-4D67-ADA6-E20BD420531B}"/>
-    <hyperlink ref="C119" r:id="rId150" xr:uid="{0A5009EB-B388-4AF4-99CE-5813711C2B1E}"/>
-    <hyperlink ref="B120" r:id="rId151" xr:uid="{255CB59B-E711-471E-8ACE-D0ABA408AE96}"/>
-    <hyperlink ref="B39" r:id="rId152" xr:uid="{39FB4A7C-4EA8-4530-9FE6-2842C777350C}"/>
-    <hyperlink ref="B104" r:id="rId153" xr:uid="{FC8A6FB5-FCCF-409E-9D6D-A93D412B2275}"/>
-    <hyperlink ref="C105" r:id="rId154" xr:uid="{988B91BF-CEBD-44F6-A773-3C87D877BE5A}"/>
-    <hyperlink ref="C108" r:id="rId155" xr:uid="{F0593E1B-3EE0-4DF2-B93E-84A02071630B}"/>
-    <hyperlink ref="B109" r:id="rId156" xr:uid="{601C40E0-818B-457C-9FE7-30D06707CEB7}"/>
-    <hyperlink ref="C109" r:id="rId157" xr:uid="{E1D93474-1A3D-49F1-B191-3C3484679D2D}"/>
-    <hyperlink ref="C83" r:id="rId158" xr:uid="{B0D57129-C33F-45FF-B844-E7642495443D}"/>
-    <hyperlink ref="B83" r:id="rId159" xr:uid="{7DCBF3E6-0CD2-475D-AE1F-56469491B512}"/>
-    <hyperlink ref="C120" r:id="rId160" xr:uid="{F24698EA-BA1A-4C92-8B6D-72A40DDDD7A3}"/>
-    <hyperlink ref="C122" r:id="rId161" xr:uid="{BAC9069D-9D63-415D-B933-A4F86CB8C587}"/>
-    <hyperlink ref="C123" r:id="rId162" xr:uid="{140A866C-FAC2-4A61-BA7E-0AFB9A05FD2F}"/>
-    <hyperlink ref="C124" r:id="rId163" xr:uid="{6EA83FA2-D552-4B23-98A9-6C5EFC3BC2CA}"/>
-    <hyperlink ref="C125" r:id="rId164" xr:uid="{E34375AF-4BB2-420C-887F-8D684FC72F4C}"/>
-    <hyperlink ref="C126" r:id="rId165" xr:uid="{CB74A187-1404-4E3B-B1EF-E6C50CF09D3E}"/>
-    <hyperlink ref="C127" r:id="rId166" xr:uid="{B0565FA3-8BDF-4E3B-9814-B9F51432FA7D}"/>
-    <hyperlink ref="C128" r:id="rId167" xr:uid="{8504A7CE-7DD9-4C74-83D8-90E0745EAB21}"/>
-    <hyperlink ref="C130" r:id="rId168" xr:uid="{D3DDF4DA-6F84-4EAF-BA60-77D926C7C2AC}"/>
-    <hyperlink ref="C131" r:id="rId169" xr:uid="{060B4F44-BF89-4037-9E74-C61E23C6AAC9}"/>
-    <hyperlink ref="C132" r:id="rId170" xr:uid="{8FD9E395-82BD-4EEA-89E9-166FDA928F87}"/>
-    <hyperlink ref="C133" r:id="rId171" xr:uid="{3669E93D-A9CE-4C72-B1DD-98E95312A18C}"/>
-    <hyperlink ref="C136" r:id="rId172" xr:uid="{E14EBE84-3FBA-44D8-B082-69967148B456}"/>
-    <hyperlink ref="C137" r:id="rId173" xr:uid="{CC0D1827-F782-476A-9312-1BAA88B7D496}"/>
-    <hyperlink ref="C141" r:id="rId174" xr:uid="{1528B515-167A-4838-B645-B63CD0312C05}"/>
-    <hyperlink ref="B143" r:id="rId175" xr:uid="{50B775B1-8A20-4A55-90CA-EC152D3C2098}"/>
-    <hyperlink ref="B144" r:id="rId176" xr:uid="{F6EFF9E5-8AC0-4C40-A2A8-62DF9BB671E9}"/>
-    <hyperlink ref="C145" r:id="rId177" xr:uid="{DE56B3AC-2F1A-494E-A9CD-9C972DA863E2}"/>
-    <hyperlink ref="B145" r:id="rId178" xr:uid="{F783979B-F441-49BC-98C4-8448098CBBC1}"/>
-    <hyperlink ref="C17" r:id="rId179" xr:uid="{DBE3D417-C525-4AE7-BA26-A27F8BD7B6D3}"/>
-    <hyperlink ref="B121" r:id="rId180" xr:uid="{BF1CBD80-282B-4284-A960-458EE8D86966}"/>
-    <hyperlink ref="C146" r:id="rId181" xr:uid="{3FA9DCB7-198C-457D-99E0-AF0A29EDEAF1}"/>
-    <hyperlink ref="B146" r:id="rId182" xr:uid="{6B057403-173E-478A-AFE1-5BA96D6006F7}"/>
-    <hyperlink ref="C147" r:id="rId183" xr:uid="{FBD8EA4A-7B80-4D87-BD4D-6D3DDE043E14}"/>
-    <hyperlink ref="B147" r:id="rId184" xr:uid="{F9D4FD4A-592C-4041-AD52-AAD4E4FECD78}"/>
-    <hyperlink ref="C148" r:id="rId185" xr:uid="{EF3F39F0-4058-49A5-8980-E800B6F200B5}"/>
-    <hyperlink ref="B148" r:id="rId186" xr:uid="{513D1B27-06CF-4F01-AD66-B1DDDB3DF171}"/>
-    <hyperlink ref="C149" r:id="rId187" xr:uid="{BFCDD610-AD9F-445C-AAE8-66DB3CD722A6}"/>
-    <hyperlink ref="B149" r:id="rId188" xr:uid="{1567BEF7-2918-4A3A-89A1-A37D6C6B5419}"/>
+    <hyperlink r:id="rId1" ref="B2" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
+    <hyperlink r:id="rId2" ref="B3" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
+    <hyperlink r:id="rId3" ref="B4" xr:uid="{00000000-0004-0000-0000-000002000000}"/>
+    <hyperlink r:id="rId4" ref="B5" xr:uid="{00000000-0004-0000-0000-000003000000}"/>
+    <hyperlink r:id="rId5" ref="B6" xr:uid="{00000000-0004-0000-0000-000004000000}"/>
+    <hyperlink r:id="rId6" ref="H6" xr:uid="{00000000-0004-0000-0000-000005000000}"/>
+    <hyperlink r:id="rId7" ref="B7" xr:uid="{00000000-0004-0000-0000-000006000000}"/>
+    <hyperlink r:id="rId8" ref="B8" xr:uid="{00000000-0004-0000-0000-000007000000}"/>
+    <hyperlink r:id="rId9" ref="B9" xr:uid="{00000000-0004-0000-0000-000008000000}"/>
+    <hyperlink r:id="rId10" ref="B10" xr:uid="{00000000-0004-0000-0000-000009000000}"/>
+    <hyperlink r:id="rId11" ref="B11" xr:uid="{00000000-0004-0000-0000-00000A000000}"/>
+    <hyperlink r:id="rId12" ref="B12" xr:uid="{00000000-0004-0000-0000-00000B000000}"/>
+    <hyperlink r:id="rId13" ref="B13" xr:uid="{00000000-0004-0000-0000-00000C000000}"/>
+    <hyperlink r:id="rId14" ref="B14" xr:uid="{00000000-0004-0000-0000-00000D000000}"/>
+    <hyperlink r:id="rId15" ref="B15" xr:uid="{00000000-0004-0000-0000-00000E000000}"/>
+    <hyperlink r:id="rId16" ref="B16" xr:uid="{00000000-0004-0000-0000-00000F000000}"/>
+    <hyperlink r:id="rId17" ref="B17" xr:uid="{00000000-0004-0000-0000-000010000000}"/>
+    <hyperlink r:id="rId18" ref="B18" xr:uid="{00000000-0004-0000-0000-000011000000}"/>
+    <hyperlink r:id="rId19" ref="B19" xr:uid="{00000000-0004-0000-0000-000012000000}"/>
+    <hyperlink r:id="rId20" ref="B20" xr:uid="{00000000-0004-0000-0000-000013000000}"/>
+    <hyperlink r:id="rId21" ref="B21" xr:uid="{00000000-0004-0000-0000-000014000000}"/>
+    <hyperlink r:id="rId22" ref="B22" xr:uid="{00000000-0004-0000-0000-000015000000}"/>
+    <hyperlink r:id="rId23" ref="B23" xr:uid="{00000000-0004-0000-0000-000016000000}"/>
+    <hyperlink r:id="rId24" ref="B24" xr:uid="{00000000-0004-0000-0000-000017000000}"/>
+    <hyperlink r:id="rId25" ref="B25" xr:uid="{00000000-0004-0000-0000-000018000000}"/>
+    <hyperlink r:id="rId26" ref="H25" xr:uid="{00000000-0004-0000-0000-000019000000}"/>
+    <hyperlink r:id="rId27" ref="B26" xr:uid="{00000000-0004-0000-0000-00001A000000}"/>
+    <hyperlink r:id="rId28" ref="H26" xr:uid="{00000000-0004-0000-0000-00001B000000}"/>
+    <hyperlink r:id="rId29" ref="B27" xr:uid="{00000000-0004-0000-0000-00001C000000}"/>
+    <hyperlink r:id="rId30" ref="H27" xr:uid="{00000000-0004-0000-0000-00001D000000}"/>
+    <hyperlink r:id="rId31" ref="B28" xr:uid="{00000000-0004-0000-0000-00001E000000}"/>
+    <hyperlink r:id="rId32" ref="H28" xr:uid="{00000000-0004-0000-0000-00001F000000}"/>
+    <hyperlink r:id="rId33" ref="B29" xr:uid="{00000000-0004-0000-0000-000020000000}"/>
+    <hyperlink r:id="rId34" ref="H29" xr:uid="{00000000-0004-0000-0000-000021000000}"/>
+    <hyperlink r:id="rId35" ref="B30" xr:uid="{00000000-0004-0000-0000-000022000000}"/>
+    <hyperlink r:id="rId36" ref="H30" xr:uid="{00000000-0004-0000-0000-000023000000}"/>
+    <hyperlink r:id="rId37" ref="B31" xr:uid="{00000000-0004-0000-0000-000024000000}"/>
+    <hyperlink r:id="rId38" ref="H31" xr:uid="{00000000-0004-0000-0000-000025000000}"/>
+    <hyperlink r:id="rId39" ref="B32" xr:uid="{00000000-0004-0000-0000-000026000000}"/>
+    <hyperlink r:id="rId40" ref="H32" xr:uid="{00000000-0004-0000-0000-000027000000}"/>
+    <hyperlink r:id="rId41" ref="B33" xr:uid="{00000000-0004-0000-0000-000028000000}"/>
+    <hyperlink r:id="rId42" ref="B34" xr:uid="{00000000-0004-0000-0000-000029000000}"/>
+    <hyperlink r:id="rId43" ref="B38" xr:uid="{00000000-0004-0000-0000-00002A000000}"/>
+    <hyperlink r:id="rId44" ref="B45" xr:uid="{00000000-0004-0000-0000-00002B000000}"/>
+    <hyperlink r:id="rId45" ref="B48" xr:uid="{00000000-0004-0000-0000-00002C000000}"/>
+    <hyperlink r:id="rId46" ref="B35" xr:uid="{00000000-0004-0000-0000-00002D000000}"/>
+    <hyperlink r:id="rId47" ref="B52" xr:uid="{00000000-0004-0000-0000-00002E000000}"/>
+    <hyperlink r:id="rId48" ref="B53" xr:uid="{00000000-0004-0000-0000-00002F000000}"/>
+    <hyperlink r:id="rId49" ref="B55" xr:uid="{00000000-0004-0000-0000-000030000000}"/>
+    <hyperlink r:id="rId50" ref="B56" xr:uid="{00000000-0004-0000-0000-000031000000}"/>
+    <hyperlink r:id="rId51" ref="B57" xr:uid="{00000000-0004-0000-0000-000032000000}"/>
+    <hyperlink r:id="rId52" ref="B58" xr:uid="{00000000-0004-0000-0000-000033000000}"/>
+    <hyperlink r:id="rId53" ref="B61" xr:uid="{00000000-0004-0000-0000-000034000000}"/>
+    <hyperlink r:id="rId54" ref="B62" xr:uid="{00000000-0004-0000-0000-000035000000}"/>
+    <hyperlink r:id="rId55" ref="B63" xr:uid="{00000000-0004-0000-0000-000036000000}"/>
+    <hyperlink r:id="rId56" ref="B64" xr:uid="{00000000-0004-0000-0000-000037000000}"/>
+    <hyperlink r:id="rId57" ref="B65" xr:uid="{00000000-0004-0000-0000-000038000000}"/>
+    <hyperlink r:id="rId58" ref="B66" xr:uid="{00000000-0004-0000-0000-000039000000}"/>
+    <hyperlink r:id="rId59" ref="B67" xr:uid="{00000000-0004-0000-0000-00003A000000}"/>
+    <hyperlink display="https://www.allhomes.com.au/agency/trusted-realtors-570129/" r:id="rId60" ref="H7:H24" xr:uid="{00000000-0004-0000-0000-00003B000000}"/>
+    <hyperlink r:id="rId61" ref="B43" xr:uid="{00000000-0004-0000-0000-00003C000000}"/>
+    <hyperlink r:id="rId62" ref="B44" xr:uid="{00000000-0004-0000-0000-00003D000000}"/>
+    <hyperlink r:id="rId63" ref="B46" xr:uid="{00000000-0004-0000-0000-00003E000000}"/>
+    <hyperlink r:id="rId64" ref="B54" xr:uid="{00000000-0004-0000-0000-00003F000000}"/>
+    <hyperlink r:id="rId65" ref="B42" xr:uid="{00000000-0004-0000-0000-000040000000}"/>
+    <hyperlink r:id="rId66" ref="J2" xr:uid="{00000000-0004-0000-0000-000041000000}"/>
+    <hyperlink r:id="rId67" ref="C69" xr:uid="{9DAE03A7-93E8-4507-BD6C-AC4013ECD47F}"/>
+    <hyperlink r:id="rId68" ref="C68" xr:uid="{66B9A9CA-DF82-46B6-9C5A-C5709E2FF1AE}"/>
+    <hyperlink r:id="rId69" ref="B75" xr:uid="{57E7BFEF-6F05-4DA9-A3DE-5B0A0EFED4D9}"/>
+    <hyperlink r:id="rId70" ref="C75" xr:uid="{F4755F93-6E59-4C38-BF66-16746869FDF3}"/>
+    <hyperlink r:id="rId71" ref="H75" xr:uid="{5BFAFD71-42C4-487F-B5E7-1697975992B4}"/>
+    <hyperlink r:id="rId72" ref="B78" xr:uid="{D3DE0D76-2479-4283-B7C7-F11B85797022}"/>
+    <hyperlink r:id="rId73" ref="C78" xr:uid="{FC1D9146-2FDC-4F13-A3C3-51CAB46DEC08}"/>
+    <hyperlink r:id="rId74" ref="B68" xr:uid="{3ED6FAA1-2B0F-4DB9-878E-9640A9C2850D}"/>
+    <hyperlink r:id="rId75" ref="B69" xr:uid="{12DE6CA8-DDC5-4E7B-BD2E-14B105A0DE3B}"/>
+    <hyperlink r:id="rId76" ref="C70" xr:uid="{0419758C-286A-4B76-B8B2-31CC336DEDF1}"/>
+    <hyperlink r:id="rId77" ref="B70" xr:uid="{AC18D1D2-FA3D-4352-A402-35B7AAFE27C0}"/>
+    <hyperlink r:id="rId78" ref="B71" xr:uid="{E8BCA1EF-4E17-4AA7-A2CE-5674FC05ABC3}"/>
+    <hyperlink r:id="rId79" ref="C71" xr:uid="{949AE606-DF4A-48F4-93A0-F148D80842CB}"/>
+    <hyperlink r:id="rId80" ref="B72" xr:uid="{69A93BB5-0295-46D6-8334-45444356E6E9}"/>
+    <hyperlink r:id="rId81" ref="C72" xr:uid="{CA171BC7-126F-4175-8A03-123D5A2C2D8A}"/>
+    <hyperlink r:id="rId82" ref="C73" xr:uid="{FACC205D-E563-4266-8E0D-0794F3D76E98}"/>
+    <hyperlink r:id="rId83" ref="B85" xr:uid="{7ABCABC0-A765-435B-AE52-9D27F653E00F}"/>
+    <hyperlink r:id="rId84" ref="C4" xr:uid="{2CD58DBE-98E3-4EDC-898F-088D5F0FCB81}"/>
+    <hyperlink r:id="rId85" ref="C29" xr:uid="{CB7CAD83-ACA3-4309-B102-B0F536FC97E6}"/>
+    <hyperlink r:id="rId86" ref="C90" xr:uid="{B4F55488-2B40-4078-ABF0-4B4254363237}"/>
+    <hyperlink r:id="rId87" ref="B90" xr:uid="{09FEE7FE-E667-40E8-BC22-3FDC999B614F}"/>
+    <hyperlink r:id="rId88" ref="C15" xr:uid="{34F25BA9-B460-46CF-85C0-4AC9D6288B41}"/>
+    <hyperlink r:id="rId89" ref="C3" xr:uid="{EBAAEE7A-83B2-457B-8600-89427BF11448}"/>
+    <hyperlink r:id="rId90" ref="C8" xr:uid="{3D3D678C-8F1B-47BC-ACA2-D1CBF5A76F0B}"/>
+    <hyperlink r:id="rId91" ref="C19" xr:uid="{ED2C9A9B-3440-4B4A-91A1-7CAF84972535}"/>
+    <hyperlink r:id="rId92" ref="C20" xr:uid="{E47C999F-11AE-4F93-9032-6E51EB582635}"/>
+    <hyperlink r:id="rId93" ref="C21" xr:uid="{E59411CC-EC13-4665-969A-8D9238CCD0C2}"/>
+    <hyperlink r:id="rId94" ref="C33" xr:uid="{9C953AB9-0076-4477-B52F-C393846B1211}"/>
+    <hyperlink r:id="rId95" ref="C38" xr:uid="{D349EA20-36BF-44C7-A16B-E85B8FE53B2A}"/>
+    <hyperlink r:id="rId96" ref="C39" xr:uid="{DE18DA3B-1A3D-4613-888E-7F506CC87091}"/>
+    <hyperlink r:id="rId97" ref="C40" xr:uid="{0C71282B-049B-4CD1-A090-B66647F2B29B}"/>
+    <hyperlink r:id="rId98" ref="C42" xr:uid="{AD0DC851-DEC5-4ACE-B928-50149068BB70}"/>
+    <hyperlink r:id="rId99" ref="C45" xr:uid="{EB51DFC2-D28F-4E0C-B019-F9954D6C9832}"/>
+    <hyperlink r:id="rId100" ref="C52" xr:uid="{9E5146F6-8EC8-4A2C-B192-C1CCB11CAB8A}"/>
+    <hyperlink r:id="rId101" ref="C48" xr:uid="{31B308E4-DA3E-401B-B796-7D03404228FB}"/>
+    <hyperlink r:id="rId102" ref="C49" xr:uid="{EBAAB9CE-7F91-4628-AF75-32C4EEF948C2}"/>
+    <hyperlink r:id="rId103" ref="C53" xr:uid="{2FF7EB1F-CD56-4E71-AD0F-0D12E8347603}"/>
+    <hyperlink r:id="rId104" ref="C55" xr:uid="{9BD44DCD-EEBB-4649-9792-F3DAC40B3960}"/>
+    <hyperlink r:id="rId105" ref="C63" xr:uid="{9929BCF4-32FD-4143-99F6-FEB21B90BCD7}"/>
+    <hyperlink r:id="rId106" ref="C64" xr:uid="{80B3DEC9-506E-4F3A-B171-A2D71B731577}"/>
+    <hyperlink r:id="rId107" ref="C66" xr:uid="{011D2C70-C541-49D4-894E-FF670D6C19BB}"/>
+    <hyperlink r:id="rId108" ref="C67" xr:uid="{B62DFA3B-60A0-44AA-BF1D-BCA2A049E46C}"/>
+    <hyperlink r:id="rId109" ref="C56" xr:uid="{C98B5D5D-65AB-489D-8160-8F1B41CDE6A7}"/>
+    <hyperlink r:id="rId110" ref="B103" xr:uid="{4D81C408-B745-40E2-B9C7-6E36C45175A7}"/>
+    <hyperlink r:id="rId111" ref="C26" xr:uid="{6A9C6F44-3E7F-47CF-8514-B6609EBEE668}"/>
+    <hyperlink r:id="rId112" ref="C23" xr:uid="{F99F350A-C378-4940-B611-41F47BC3B4B0}"/>
+    <hyperlink r:id="rId113" ref="C103" xr:uid="{3E9C8DCE-ABC0-49DA-B64B-B569BAAE6ED0}"/>
+    <hyperlink r:id="rId114" ref="C104" xr:uid="{E96AA061-2DED-4A35-BE99-8E7E156527EB}"/>
+    <hyperlink r:id="rId115" ref="C102" xr:uid="{4DAA7E56-3BCD-4AF1-B6E7-A26B02A0DA6C}"/>
+    <hyperlink r:id="rId116" ref="C101" xr:uid="{EBE0EC7F-0880-4F4A-991C-2C7C53889923}"/>
+    <hyperlink r:id="rId117" ref="C100" xr:uid="{7AA4A2D0-C18F-4625-A776-6EDD2415E1BC}"/>
+    <hyperlink r:id="rId118" ref="C99" xr:uid="{15BFB680-4225-425B-8826-841A35922C8A}"/>
+    <hyperlink r:id="rId119" ref="B99" xr:uid="{1EF2BF94-D92B-41EF-8B1F-0585F1910B74}"/>
+    <hyperlink r:id="rId120" ref="C97" xr:uid="{6687C5A1-CC2B-49FF-B98D-946AA21B8C55}"/>
+    <hyperlink r:id="rId121" ref="B97" xr:uid="{0411E592-2DE8-4D1D-B66C-46CE99CAA412}"/>
+    <hyperlink r:id="rId122" ref="C96" xr:uid="{A7ED7210-DE23-4760-B67F-78027E9B9B73}"/>
+    <hyperlink r:id="rId123" ref="B96" xr:uid="{992F1752-E440-4347-A698-44C8E60F00BE}"/>
+    <hyperlink r:id="rId124" ref="B102" xr:uid="{A0E03FB2-010F-497D-874D-A0A66FB6303C}"/>
+    <hyperlink r:id="rId125" ref="B101" xr:uid="{165FBF6F-9195-42DA-AC37-C49B2308ACA1}"/>
+    <hyperlink r:id="rId126" ref="B94" xr:uid="{7DB2C8A6-8C43-4818-A7C2-D5E14351114B}"/>
+    <hyperlink r:id="rId127" ref="B93" xr:uid="{EFC122F7-44E7-447B-8F21-BA1503A72780}"/>
+    <hyperlink r:id="rId128" ref="B91" xr:uid="{7AC22E1D-6919-43E6-AD91-1551DBBDE570}"/>
+    <hyperlink r:id="rId129" ref="B88" xr:uid="{FB3E9840-E4E3-4E64-8CCF-2BAEC7024AD6}"/>
+    <hyperlink r:id="rId130" ref="B87" xr:uid="{348337ED-A616-4A9D-A8D3-0091262177C6}"/>
+    <hyperlink r:id="rId131" ref="B86" xr:uid="{CF62843D-4B82-47CB-B74F-D3F292E9603A}"/>
+    <hyperlink r:id="rId132" ref="B84" xr:uid="{9CA10EFF-3943-479E-914B-1D6EE04D75FC}"/>
+    <hyperlink r:id="rId133" ref="C84" xr:uid="{1074AAC9-CCB0-4FFC-9AFB-EFD1363D7538}"/>
+    <hyperlink r:id="rId134" ref="B105" xr:uid="{D6DE2797-5A68-4C1E-9E74-0D323B6ADFA2}"/>
+    <hyperlink r:id="rId135" ref="B106" xr:uid="{1FCAF9BA-00B5-4008-B5C8-E822ABD6BCDD}"/>
+    <hyperlink r:id="rId136" ref="C11" xr:uid="{893B2404-B185-41F7-B397-A3E08B386C5F}"/>
+    <hyperlink r:id="rId137" ref="B107" xr:uid="{B0E609F4-D8A3-433A-BE15-17E4804C6EA3}"/>
+    <hyperlink r:id="rId138" ref="C107" xr:uid="{6793ECA4-A034-42EC-A741-3B0FF42BC11B}"/>
+    <hyperlink r:id="rId139" ref="B108" xr:uid="{4DB78F44-0F08-4561-A0E8-0EE92F9FFECB}"/>
+    <hyperlink r:id="rId140" ref="B114" xr:uid="{27750164-38B8-4B5E-9B5A-E6C71FFFC61F}"/>
+    <hyperlink r:id="rId141" ref="C114" xr:uid="{6FE6A043-A6B1-44FF-8A45-8C3690323458}"/>
+    <hyperlink r:id="rId142" ref="B113" xr:uid="{0F94FF41-1E06-4D7B-B360-1EB377073C87}"/>
+    <hyperlink r:id="rId143" ref="B112" xr:uid="{490A5044-10EC-4082-BEC1-14008171D5CF}"/>
+    <hyperlink r:id="rId144" ref="B49" xr:uid="{836EB236-8BF1-4259-B395-AD9FA9DE0AE0}"/>
+    <hyperlink r:id="rId145" ref="B74" xr:uid="{8AA8904A-1CC5-4D06-93EF-66F7FC625199}"/>
+    <hyperlink r:id="rId146" ref="B76" xr:uid="{5743888C-C74A-41C6-ABC5-E9575351702D}"/>
+    <hyperlink r:id="rId147" ref="B115" xr:uid="{27BDB583-8AD0-4B33-BA19-24E42C9E7CE9}"/>
+    <hyperlink r:id="rId148" ref="B117" xr:uid="{92BA6213-0D94-4C5A-B06A-6FC35C0BECA9}"/>
+    <hyperlink r:id="rId149" ref="B119" xr:uid="{6724AE23-65F5-4D67-ADA6-E20BD420531B}"/>
+    <hyperlink r:id="rId150" ref="C119" xr:uid="{0A5009EB-B388-4AF4-99CE-5813711C2B1E}"/>
+    <hyperlink r:id="rId151" ref="B120" xr:uid="{255CB59B-E711-471E-8ACE-D0ABA408AE96}"/>
+    <hyperlink r:id="rId152" ref="B39" xr:uid="{39FB4A7C-4EA8-4530-9FE6-2842C777350C}"/>
+    <hyperlink r:id="rId153" ref="B104" xr:uid="{FC8A6FB5-FCCF-409E-9D6D-A93D412B2275}"/>
+    <hyperlink r:id="rId154" ref="C105" xr:uid="{988B91BF-CEBD-44F6-A773-3C87D877BE5A}"/>
+    <hyperlink r:id="rId155" ref="C108" xr:uid="{F0593E1B-3EE0-4DF2-B93E-84A02071630B}"/>
+    <hyperlink r:id="rId156" ref="B109" xr:uid="{601C40E0-818B-457C-9FE7-30D06707CEB7}"/>
+    <hyperlink r:id="rId157" ref="C109" xr:uid="{E1D93474-1A3D-49F1-B191-3C3484679D2D}"/>
+    <hyperlink r:id="rId158" ref="C83" xr:uid="{B0D57129-C33F-45FF-B844-E7642495443D}"/>
+    <hyperlink r:id="rId159" ref="B83" xr:uid="{7DCBF3E6-0CD2-475D-AE1F-56469491B512}"/>
+    <hyperlink r:id="rId160" ref="C120" xr:uid="{F24698EA-BA1A-4C92-8B6D-72A40DDDD7A3}"/>
+    <hyperlink r:id="rId161" ref="C122" xr:uid="{BAC9069D-9D63-415D-B933-A4F86CB8C587}"/>
+    <hyperlink r:id="rId162" ref="C123" xr:uid="{140A866C-FAC2-4A61-BA7E-0AFB9A05FD2F}"/>
+    <hyperlink r:id="rId163" ref="C124" xr:uid="{6EA83FA2-D552-4B23-98A9-6C5EFC3BC2CA}"/>
+    <hyperlink r:id="rId164" ref="C125" xr:uid="{E34375AF-4BB2-420C-887F-8D684FC72F4C}"/>
+    <hyperlink r:id="rId165" ref="C126" xr:uid="{CB74A187-1404-4E3B-B1EF-E6C50CF09D3E}"/>
+    <hyperlink r:id="rId166" ref="C127" xr:uid="{B0565FA3-8BDF-4E3B-9814-B9F51432FA7D}"/>
+    <hyperlink r:id="rId167" ref="C128" xr:uid="{8504A7CE-7DD9-4C74-83D8-90E0745EAB21}"/>
+    <hyperlink r:id="rId168" ref="C130" xr:uid="{D3DDF4DA-6F84-4EAF-BA60-77D926C7C2AC}"/>
+    <hyperlink r:id="rId169" ref="C131" xr:uid="{060B4F44-BF89-4037-9E74-C61E23C6AAC9}"/>
+    <hyperlink r:id="rId170" ref="C132" xr:uid="{8FD9E395-82BD-4EEA-89E9-166FDA928F87}"/>
+    <hyperlink r:id="rId171" ref="C133" xr:uid="{3669E93D-A9CE-4C72-B1DD-98E95312A18C}"/>
+    <hyperlink r:id="rId172" ref="C136" xr:uid="{E14EBE84-3FBA-44D8-B082-69967148B456}"/>
+    <hyperlink r:id="rId173" ref="C137" xr:uid="{CC0D1827-F782-476A-9312-1BAA88B7D496}"/>
+    <hyperlink r:id="rId174" ref="C141" xr:uid="{1528B515-167A-4838-B645-B63CD0312C05}"/>
+    <hyperlink r:id="rId175" ref="B143" xr:uid="{50B775B1-8A20-4A55-90CA-EC152D3C2098}"/>
+    <hyperlink r:id="rId176" ref="B144" xr:uid="{F6EFF9E5-8AC0-4C40-A2A8-62DF9BB671E9}"/>
+    <hyperlink r:id="rId177" ref="C145" xr:uid="{DE56B3AC-2F1A-494E-A9CD-9C972DA863E2}"/>
+    <hyperlink r:id="rId178" ref="B145" xr:uid="{F783979B-F441-49BC-98C4-8448098CBBC1}"/>
+    <hyperlink r:id="rId179" ref="C17" xr:uid="{DBE3D417-C525-4AE7-BA26-A27F8BD7B6D3}"/>
+    <hyperlink r:id="rId180" ref="B121" xr:uid="{BF1CBD80-282B-4284-A960-458EE8D86966}"/>
+    <hyperlink r:id="rId181" ref="C146" xr:uid="{3FA9DCB7-198C-457D-99E0-AF0A29EDEAF1}"/>
+    <hyperlink r:id="rId182" ref="B146" xr:uid="{6B057403-173E-478A-AFE1-5BA96D6006F7}"/>
+    <hyperlink r:id="rId183" ref="C147" xr:uid="{FBD8EA4A-7B80-4D87-BD4D-6D3DDE043E14}"/>
+    <hyperlink r:id="rId184" ref="B147" xr:uid="{F9D4FD4A-592C-4041-AD52-AAD4E4FECD78}"/>
+    <hyperlink r:id="rId185" ref="C148" xr:uid="{EF3F39F0-4058-49A5-8980-E800B6F200B5}"/>
+    <hyperlink r:id="rId186" ref="B148" xr:uid="{513D1B27-06CF-4F01-AD66-B1DDDB3DF171}"/>
+    <hyperlink r:id="rId187" ref="C149" xr:uid="{BFCDD610-AD9F-445C-AAE8-66DB3CD722A6}"/>
+    <hyperlink r:id="rId188" ref="B149" xr:uid="{1567BEF7-2918-4A3A-89A1-A37D6C6B5419}"/>
+    <hyperlink r:id="rId189" ref="B150" xr:uid="{233679EA-F519-4185-AA17-F008EE8DA109}"/>
   </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId189"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageSetup orientation="portrait" paperSize="9" r:id="rId190"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:AI149"/>
+  <dimension ref="A1:AJ150"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E24" sqref="E24"/>
+    <sheetView topLeftCell="E1" workbookViewId="0">
+      <pane activePane="bottomLeft" state="frozen" topLeftCell="A134" ySplit="1"/>
+      <selection activeCell="R155" pane="bottomLeft" sqref="R155"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1"/>
+  <sheetFormatPr customHeight="1" defaultColWidth="14.42578125" defaultRowHeight="15.75"/>
   <cols>
-    <col min="1" max="1" width="14.85546875" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="18.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="55.5703125" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="25.140625" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="19.5703125" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="19.85546875" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="18.5703125" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="32.140625" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="20.5703125" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="21.140625" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="28.85546875" customWidth="1" collapsed="1"/>
-    <col min="12" max="12" width="37.5703125" customWidth="1" collapsed="1"/>
-    <col min="16" max="17" width="18.85546875" customWidth="1" collapsed="1"/>
-    <col min="18" max="18" width="47.85546875" customWidth="1" collapsed="1"/>
-    <col min="19" max="19" width="77.5703125" customWidth="1" collapsed="1"/>
-    <col min="20" max="20" width="24" customWidth="1" collapsed="1"/>
-    <col min="21" max="21" width="18.85546875" customWidth="1" collapsed="1"/>
-    <col min="22" max="31" width="19.140625" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="14.85546875" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="18.140625" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="55.5703125" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="25.140625" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="19.5703125" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" width="19.85546875" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" width="18.5703125" collapsed="true"/>
+    <col min="8" max="8" customWidth="true" width="32.140625" collapsed="true"/>
+    <col min="9" max="9" customWidth="true" width="20.5703125" collapsed="true"/>
+    <col min="10" max="10" customWidth="true" width="21.140625" collapsed="true"/>
+    <col min="11" max="11" customWidth="true" width="28.85546875" collapsed="true"/>
+    <col min="12" max="12" customWidth="true" width="37.5703125" collapsed="true"/>
+    <col min="16" max="17" customWidth="true" width="18.85546875" collapsed="true"/>
+    <col min="18" max="18" customWidth="true" width="47.85546875" collapsed="true"/>
+    <col min="19" max="19" customWidth="true" width="77.5703125" collapsed="true"/>
+    <col min="20" max="20" customWidth="true" width="24.0" collapsed="true"/>
+    <col min="21" max="21" customWidth="true" width="18.85546875" collapsed="true"/>
+    <col min="22" max="31" customWidth="true" width="19.140625" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:35" ht="30">
+    <row ht="30" r="1" spans="1:35">
       <c r="A1" s="1" t="s">
         <v>46</v>
       </c>
@@ -10284,7 +10349,7 @@
       <c r="AH1" s="23"/>
       <c r="AI1" s="23"/>
     </row>
-    <row r="2" spans="1:35" ht="15" customHeight="1">
+    <row customHeight="1" ht="15" r="2" spans="1:35">
       <c r="A2" s="24">
         <v>1</v>
       </c>
@@ -10355,7 +10420,7 @@
       <c r="AH2" s="24"/>
       <c r="AI2" s="24"/>
     </row>
-    <row r="3" spans="1:35" ht="15" customHeight="1">
+    <row customHeight="1" ht="15" r="3" spans="1:35">
       <c r="A3" s="24">
         <v>2</v>
       </c>
@@ -10426,7 +10491,7 @@
       <c r="AH3" s="24"/>
       <c r="AI3" s="24"/>
     </row>
-    <row r="4" spans="1:35" s="24" customFormat="1" ht="15" customHeight="1">
+    <row customFormat="1" customHeight="1" ht="15" r="4" s="24" spans="1:35">
       <c r="A4" s="24">
         <v>3</v>
       </c>
@@ -10488,7 +10553,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="5" spans="1:35" ht="15" customHeight="1">
+    <row customHeight="1" ht="15" r="5" spans="1:35">
       <c r="A5" s="24">
         <v>4</v>
       </c>
@@ -10561,7 +10626,7 @@
       <c r="AH5" s="24"/>
       <c r="AI5" s="24"/>
     </row>
-    <row r="6" spans="1:35" s="24" customFormat="1" ht="15" customHeight="1">
+    <row customFormat="1" customHeight="1" ht="15" r="6" s="24" spans="1:35">
       <c r="A6" s="24">
         <v>5</v>
       </c>
@@ -10620,7 +10685,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="7" spans="1:35" s="24" customFormat="1" ht="15" customHeight="1">
+    <row customFormat="1" customHeight="1" ht="15" r="7" s="24" spans="1:35">
       <c r="A7" s="24">
         <v>6</v>
       </c>
@@ -10679,7 +10744,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="8" spans="1:35" s="24" customFormat="1" ht="15" customHeight="1">
+    <row customFormat="1" customHeight="1" ht="15" r="8" s="24" spans="1:35">
       <c r="A8" s="24">
         <v>7</v>
       </c>
@@ -10735,7 +10800,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="9" spans="1:35" s="24" customFormat="1" ht="15" customHeight="1">
+    <row customFormat="1" customHeight="1" ht="15" r="9" s="24" spans="1:35">
       <c r="A9" s="24">
         <v>8</v>
       </c>
@@ -10794,7 +10859,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="10" spans="1:35" s="24" customFormat="1" ht="15" customHeight="1">
+    <row customFormat="1" customHeight="1" ht="15" r="10" s="24" spans="1:35">
       <c r="A10" s="24">
         <v>9</v>
       </c>
@@ -10850,17 +10915,17 @@
         <v>16</v>
       </c>
     </row>
-    <row r="11" spans="1:35" s="24" customFormat="1" ht="15" customHeight="1">
+    <row customFormat="1" customHeight="1" ht="15" r="11" s="24" spans="1:35">
       <c r="A11" s="24">
         <v>10</v>
       </c>
-      <c r="B11" s="47" t="s">
-        <v>1093</v>
+      <c r="B11" s="24" t="s">
+        <v>7</v>
       </c>
       <c r="C11" s="24" t="s">
         <v>110</v>
       </c>
-      <c r="D11" s="47" t="s">
+      <c r="D11" s="24" t="s">
         <v>234</v>
       </c>
       <c r="E11" s="24" t="s">
@@ -10872,14 +10937,14 @@
       <c r="G11" s="24" t="s">
         <v>112</v>
       </c>
-      <c r="H11" s="47" t="s">
+      <c r="H11" s="24" t="s">
+        <v>1094</v>
+      </c>
+      <c r="K11" s="24" t="s">
+        <v>426</v>
+      </c>
+      <c r="L11" s="24" t="s">
         <v>1095</v>
-      </c>
-      <c r="K11" s="47" t="s">
-        <v>426</v>
-      </c>
-      <c r="L11" s="47" t="s">
-        <v>1096</v>
       </c>
       <c r="M11" s="24">
         <v>4</v>
@@ -10896,8 +10961,8 @@
       <c r="R11" s="24" t="s">
         <v>113</v>
       </c>
-      <c r="S11" s="47" t="s">
-        <v>1094</v>
+      <c r="S11" s="24" t="s">
+        <v>1093</v>
       </c>
       <c r="T11" s="24" t="s">
         <v>102</v>
@@ -10915,7 +10980,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="12" spans="1:35" s="24" customFormat="1" ht="15" customHeight="1">
+    <row customFormat="1" customHeight="1" ht="15" r="12" s="24" spans="1:35">
       <c r="A12" s="24">
         <v>11</v>
       </c>
@@ -10971,7 +11036,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="13" spans="1:35" s="24" customFormat="1" ht="15" customHeight="1">
+    <row customFormat="1" customHeight="1" ht="15" r="13" s="24" spans="1:35">
       <c r="A13" s="24">
         <v>12</v>
       </c>
@@ -11030,7 +11095,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="14" spans="1:35" s="24" customFormat="1" ht="15" customHeight="1">
+    <row customFormat="1" customHeight="1" ht="15" r="14" s="24" spans="1:35">
       <c r="A14" s="24">
         <v>13</v>
       </c>
@@ -11095,7 +11160,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="15" spans="1:35" s="24" customFormat="1" ht="15" customHeight="1">
+    <row customFormat="1" customHeight="1" ht="15" r="15" s="24" spans="1:35">
       <c r="A15" s="24">
         <v>14</v>
       </c>
@@ -11154,7 +11219,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="16" spans="1:35" s="24" customFormat="1" ht="15" customHeight="1">
+    <row customFormat="1" customHeight="1" ht="15" r="16" s="24" spans="1:35">
       <c r="A16" s="24">
         <v>15</v>
       </c>
@@ -11213,7 +11278,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="17" spans="1:35" s="24" customFormat="1" ht="15" customHeight="1">
+    <row customFormat="1" customHeight="1" ht="15" r="17" s="24" spans="1:35">
       <c r="A17" s="24">
         <v>16</v>
       </c>
@@ -11269,7 +11334,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="18" spans="1:35" s="24" customFormat="1" ht="15" customHeight="1">
+    <row customFormat="1" customHeight="1" ht="15" r="18" s="24" spans="1:35">
       <c r="A18" s="24">
         <v>17</v>
       </c>
@@ -11328,12 +11393,12 @@
         <v>16</v>
       </c>
     </row>
-    <row r="19" spans="1:35" s="24" customFormat="1" ht="15" customHeight="1">
+    <row customFormat="1" customHeight="1" ht="15" r="19" s="24" spans="1:35">
       <c r="A19" s="24">
         <v>18</v>
       </c>
-      <c r="B19" s="47" t="s">
-        <v>1093</v>
+      <c r="B19" s="24" t="s">
+        <v>7</v>
       </c>
       <c r="C19" s="24" t="s">
         <v>98</v>
@@ -11353,10 +11418,10 @@
       <c r="H19" s="24" t="s">
         <v>1062</v>
       </c>
-      <c r="K19" s="47" t="s">
+      <c r="K19" s="24" t="s">
         <v>313</v>
       </c>
-      <c r="L19" s="46" t="s">
+      <c r="L19" s="24" t="s">
         <v>1063</v>
       </c>
       <c r="M19" s="24">
@@ -11374,7 +11439,7 @@
       <c r="R19" s="24" t="s">
         <v>101</v>
       </c>
-      <c r="S19" s="46" t="s">
+      <c r="S19" s="24" t="s">
         <v>1061</v>
       </c>
       <c r="T19" s="24" t="s">
@@ -11384,7 +11449,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="20" spans="1:35" ht="15" customHeight="1">
+    <row customHeight="1" ht="15" r="20" spans="1:35">
       <c r="A20" s="24">
         <v>19</v>
       </c>
@@ -11459,12 +11524,12 @@
       <c r="AH20" s="24"/>
       <c r="AI20" s="24"/>
     </row>
-    <row r="21" spans="1:35" ht="15" customHeight="1">
+    <row customFormat="1" customHeight="1" ht="15" r="21" s="24" spans="1:35">
       <c r="A21" s="24">
         <v>20</v>
       </c>
-      <c r="B21" s="47" t="s">
-        <v>1093</v>
+      <c r="B21" s="24" t="s">
+        <v>7</v>
       </c>
       <c r="C21" s="24" t="s">
         <v>98</v>
@@ -11484,12 +11549,10 @@
       <c r="H21" s="24" t="s">
         <v>1065</v>
       </c>
-      <c r="I21" s="24"/>
-      <c r="J21" s="24"/>
-      <c r="K21" s="47" t="s">
+      <c r="K21" s="24" t="s">
         <v>431</v>
       </c>
-      <c r="L21" s="46" t="s">
+      <c r="L21" s="24" t="s">
         <v>1066</v>
       </c>
       <c r="M21" s="24">
@@ -11498,17 +11561,16 @@
       <c r="N21" s="24">
         <v>2</v>
       </c>
-      <c r="O21" s="24"/>
-      <c r="P21" s="46" t="s">
+      <c r="P21" s="24" t="s">
         <v>203</v>
       </c>
-      <c r="Q21" s="46" t="s">
+      <c r="Q21" s="24" t="s">
         <v>204</v>
       </c>
       <c r="R21" s="24" t="s">
         <v>101</v>
       </c>
-      <c r="S21" s="46" t="s">
+      <c r="S21" s="24" t="s">
         <v>1064</v>
       </c>
       <c r="T21" s="24" t="s">
@@ -11517,22 +11579,8 @@
       <c r="U21" s="24" t="s">
         <v>16</v>
       </c>
-      <c r="V21" s="24"/>
-      <c r="W21" s="24"/>
-      <c r="X21" s="24"/>
-      <c r="Y21" s="24"/>
-      <c r="Z21" s="24"/>
-      <c r="AA21" s="24"/>
-      <c r="AB21" s="24"/>
-      <c r="AC21" s="24"/>
-      <c r="AD21" s="24"/>
-      <c r="AE21" s="24"/>
-      <c r="AF21" s="24"/>
-      <c r="AG21" s="24"/>
-      <c r="AH21" s="24"/>
-      <c r="AI21" s="24"/>
-    </row>
-    <row r="22" spans="1:35" s="24" customFormat="1" ht="15" customHeight="1">
+    </row>
+    <row customFormat="1" customHeight="1" ht="15" r="22" s="24" spans="1:35">
       <c r="A22" s="24">
         <v>21</v>
       </c>
@@ -11597,7 +11645,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="23" spans="1:35" s="24" customFormat="1" ht="15" customHeight="1">
+    <row customFormat="1" customHeight="1" ht="15" r="23" s="24" spans="1:35">
       <c r="A23" s="24">
         <v>22</v>
       </c>
@@ -11650,7 +11698,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="24" spans="1:35" s="24" customFormat="1" ht="15" customHeight="1">
+    <row customFormat="1" customHeight="1" ht="15" r="24" s="24" spans="1:35">
       <c r="A24" s="24">
         <v>23</v>
       </c>
@@ -11709,7 +11757,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="25" spans="1:35" ht="15" customHeight="1">
+    <row customHeight="1" ht="15" r="25" spans="1:35">
       <c r="A25" s="24">
         <v>24</v>
       </c>
@@ -11780,7 +11828,7 @@
       <c r="AH25" s="24"/>
       <c r="AI25" s="24"/>
     </row>
-    <row r="26" spans="1:35" s="24" customFormat="1" ht="15" customHeight="1">
+    <row customFormat="1" customHeight="1" ht="15" r="26" s="24" spans="1:35">
       <c r="A26" s="24">
         <v>25</v>
       </c>
@@ -11839,7 +11887,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="27" spans="1:35" s="24" customFormat="1" ht="15" customHeight="1">
+    <row customFormat="1" customHeight="1" ht="15" r="27" s="24" spans="1:35">
       <c r="A27" s="24">
         <v>26</v>
       </c>
@@ -11898,7 +11946,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="28" spans="1:35" s="24" customFormat="1" ht="15" customHeight="1">
+    <row customFormat="1" customHeight="1" ht="15" r="28" s="24" spans="1:35">
       <c r="A28" s="24">
         <v>27</v>
       </c>
@@ -11957,7 +12005,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="29" spans="1:35" s="24" customFormat="1" ht="15" customHeight="1">
+    <row customFormat="1" customHeight="1" ht="15" r="29" s="24" spans="1:35">
       <c r="A29" s="24">
         <v>28</v>
       </c>
@@ -12016,7 +12064,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="30" spans="1:35" s="24" customFormat="1" ht="15" customHeight="1">
+    <row customFormat="1" customHeight="1" ht="15" r="30" s="24" spans="1:35">
       <c r="A30" s="24">
         <v>29</v>
       </c>
@@ -12075,7 +12123,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="31" spans="1:35" s="24" customFormat="1" ht="15" customHeight="1">
+    <row customFormat="1" customHeight="1" ht="15" r="31" s="24" spans="1:35">
       <c r="A31" s="24">
         <v>30</v>
       </c>
@@ -12131,7 +12179,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="32" spans="1:35" s="24" customFormat="1" ht="15" customHeight="1">
+    <row customFormat="1" customHeight="1" ht="15" r="32" s="24" spans="1:35">
       <c r="A32" s="24">
         <v>31</v>
       </c>
@@ -12190,7 +12238,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="33" spans="1:21" s="24" customFormat="1" ht="14.25">
+    <row customFormat="1" ht="14.25" r="33" s="24" spans="1:21">
       <c r="A33" s="24" t="s">
         <v>195</v>
       </c>
@@ -12249,7 +12297,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="34" spans="1:21" s="24" customFormat="1" ht="14.25">
+    <row customFormat="1" ht="14.25" r="34" s="24" spans="1:21">
       <c r="A34" s="24" t="s">
         <v>206</v>
       </c>
@@ -12308,7 +12356,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="35" spans="1:21" s="24" customFormat="1" ht="14.25">
+    <row customFormat="1" ht="14.25" r="35" s="24" spans="1:21">
       <c r="A35" s="24" t="s">
         <v>213</v>
       </c>
@@ -12367,7 +12415,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="36" spans="1:21" s="24" customFormat="1" ht="14.25">
+    <row customFormat="1" ht="14.25" r="36" s="24" spans="1:21">
       <c r="A36" s="24" t="s">
         <v>219</v>
       </c>
@@ -12426,7 +12474,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="37" spans="1:21" s="24" customFormat="1" ht="14.25">
+    <row customFormat="1" ht="14.25" r="37" s="24" spans="1:21">
       <c r="A37" s="24" t="s">
         <v>226</v>
       </c>
@@ -12485,7 +12533,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="38" spans="1:21" s="24" customFormat="1" ht="14.25">
+    <row customFormat="1" ht="14.25" r="38" s="24" spans="1:21">
       <c r="A38" s="24" t="s">
         <v>232</v>
       </c>
@@ -12544,7 +12592,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="39" spans="1:21" s="24" customFormat="1" ht="14.25">
+    <row customFormat="1" ht="14.25" r="39" s="24" spans="1:21">
       <c r="A39" s="24" t="s">
         <v>240</v>
       </c>
@@ -12603,7 +12651,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="40" spans="1:21" s="24" customFormat="1" ht="14.25">
+    <row customFormat="1" ht="14.25" r="40" s="24" spans="1:21">
       <c r="A40" s="24" t="s">
         <v>243</v>
       </c>
@@ -12662,7 +12710,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="41" spans="1:21" s="24" customFormat="1" ht="14.25">
+    <row customFormat="1" ht="14.25" r="41" s="24" spans="1:21">
       <c r="A41" s="24" t="s">
         <v>246</v>
       </c>
@@ -12721,7 +12769,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="42" spans="1:21" s="24" customFormat="1" ht="14.25">
+    <row customFormat="1" ht="14.25" r="42" s="24" spans="1:21">
       <c r="A42" s="24" t="s">
         <v>255</v>
       </c>
@@ -12780,7 +12828,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="43" spans="1:21" s="24" customFormat="1" ht="14.25">
+    <row customFormat="1" ht="14.25" r="43" s="24" spans="1:21">
       <c r="A43" s="24" t="s">
         <v>259</v>
       </c>
@@ -12839,7 +12887,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="44" spans="1:21" s="24" customFormat="1" ht="14.25">
+    <row customFormat="1" ht="14.25" r="44" s="24" spans="1:21">
       <c r="A44" s="24" t="s">
         <v>268</v>
       </c>
@@ -12898,7 +12946,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="45" spans="1:21" s="24" customFormat="1" ht="14.25">
+    <row customFormat="1" ht="14.25" r="45" s="24" spans="1:21">
       <c r="A45" s="24" t="s">
         <v>275</v>
       </c>
@@ -12957,7 +13005,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="46" spans="1:21" s="24" customFormat="1" ht="14.25">
+    <row customFormat="1" ht="14.25" r="46" s="24" spans="1:21">
       <c r="A46" s="24" t="s">
         <v>281</v>
       </c>
@@ -13016,7 +13064,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="47" spans="1:21" s="24" customFormat="1" ht="14.25">
+    <row customFormat="1" ht="14.25" r="47" s="24" spans="1:21">
       <c r="A47" s="24" t="s">
         <v>287</v>
       </c>
@@ -13075,7 +13123,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="48" spans="1:21" s="24" customFormat="1" ht="14.25">
+    <row customFormat="1" ht="14.25" r="48" s="24" spans="1:21">
       <c r="A48" s="24" t="s">
         <v>293</v>
       </c>
@@ -13134,7 +13182,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="49" spans="1:21" s="24" customFormat="1" ht="14.25">
+    <row customFormat="1" ht="14.25" r="49" s="24" spans="1:21">
       <c r="A49" s="24" t="s">
         <v>298</v>
       </c>
@@ -13193,7 +13241,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="50" spans="1:21" s="24" customFormat="1" ht="14.25">
+    <row customFormat="1" ht="14.25" r="50" s="24" spans="1:21">
       <c r="A50" s="24" t="s">
         <v>304</v>
       </c>
@@ -13252,7 +13300,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="51" spans="1:21" s="24" customFormat="1" ht="14.25">
+    <row customFormat="1" ht="14.25" r="51" s="24" spans="1:21">
       <c r="A51" s="24" t="s">
         <v>310</v>
       </c>
@@ -13311,7 +13359,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="52" spans="1:21" s="24" customFormat="1" ht="14.25">
+    <row customFormat="1" ht="14.25" r="52" s="24" spans="1:21">
       <c r="A52" s="24" t="s">
         <v>316</v>
       </c>
@@ -13370,7 +13418,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="53" spans="1:21" s="24" customFormat="1" ht="14.25">
+    <row customFormat="1" ht="14.25" r="53" s="24" spans="1:21">
       <c r="A53" s="24" t="s">
         <v>343</v>
       </c>
@@ -13429,7 +13477,7 @@
         <v>325</v>
       </c>
     </row>
-    <row r="54" spans="1:21" s="24" customFormat="1" ht="14.25">
+    <row customFormat="1" ht="14.25" r="54" s="24" spans="1:21">
       <c r="A54" s="24" t="s">
         <v>349</v>
       </c>
@@ -13488,7 +13536,7 @@
         <v>325</v>
       </c>
     </row>
-    <row r="55" spans="1:21" s="24" customFormat="1" ht="14.25">
+    <row customFormat="1" ht="14.25" r="55" s="24" spans="1:21">
       <c r="A55" s="24" t="s">
         <v>353</v>
       </c>
@@ -13547,7 +13595,7 @@
         <v>325</v>
       </c>
     </row>
-    <row r="56" spans="1:21" s="24" customFormat="1" ht="14.25">
+    <row customFormat="1" ht="14.25" r="56" s="24" spans="1:21">
       <c r="A56" s="24" t="s">
         <v>359</v>
       </c>
@@ -13606,7 +13654,7 @@
         <v>325</v>
       </c>
     </row>
-    <row r="57" spans="1:21" s="24" customFormat="1" ht="14.25">
+    <row customFormat="1" ht="14.25" r="57" s="24" spans="1:21">
       <c r="A57" s="24" t="s">
         <v>364</v>
       </c>
@@ -13665,7 +13713,7 @@
         <v>325</v>
       </c>
     </row>
-    <row r="58" spans="1:21" s="24" customFormat="1" ht="14.25">
+    <row customFormat="1" ht="14.25" r="58" s="24" spans="1:21">
       <c r="A58" s="24" t="s">
         <v>371</v>
       </c>
@@ -13724,7 +13772,7 @@
         <v>325</v>
       </c>
     </row>
-    <row r="59" spans="1:21" s="24" customFormat="1" ht="14.25">
+    <row customFormat="1" ht="14.25" r="59" s="24" spans="1:21">
       <c r="A59" s="24" t="s">
         <v>377</v>
       </c>
@@ -13783,7 +13831,7 @@
         <v>325</v>
       </c>
     </row>
-    <row r="60" spans="1:21" s="24" customFormat="1" ht="14.25">
+    <row customFormat="1" ht="14.25" r="60" s="24" spans="1:21">
       <c r="A60" s="24" t="s">
         <v>384</v>
       </c>
@@ -13842,7 +13890,7 @@
         <v>325</v>
       </c>
     </row>
-    <row r="61" spans="1:21" s="24" customFormat="1" ht="14.25">
+    <row customFormat="1" ht="14.25" r="61" s="24" spans="1:21">
       <c r="A61" s="24" t="s">
         <v>391</v>
       </c>
@@ -13901,7 +13949,7 @@
         <v>325</v>
       </c>
     </row>
-    <row r="62" spans="1:21" s="24" customFormat="1" ht="14.25">
+    <row customFormat="1" ht="14.25" r="62" s="24" spans="1:21">
       <c r="A62" s="24" t="s">
         <v>397</v>
       </c>
@@ -13960,7 +14008,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="63" spans="1:21" s="24" customFormat="1" ht="14.25">
+    <row customFormat="1" ht="14.25" r="63" s="24" spans="1:21">
       <c r="A63" s="24" t="s">
         <v>400</v>
       </c>
@@ -14019,7 +14067,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="64" spans="1:21" s="24" customFormat="1" ht="14.25">
+    <row customFormat="1" ht="14.25" r="64" s="24" spans="1:21">
       <c r="A64" s="24" t="s">
         <v>405</v>
       </c>
@@ -14078,7 +14126,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="65" spans="1:21" s="24" customFormat="1" ht="14.25">
+    <row customFormat="1" ht="14.25" r="65" s="24" spans="1:21">
       <c r="A65" s="24" t="s">
         <v>411</v>
       </c>
@@ -14137,7 +14185,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="66" spans="1:21" s="24" customFormat="1" ht="14.25">
+    <row customFormat="1" ht="14.25" r="66" s="24" spans="1:21">
       <c r="A66" s="24" t="s">
         <v>416</v>
       </c>
@@ -14196,7 +14244,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="67" spans="1:21" s="24" customFormat="1" ht="14.25">
+    <row customFormat="1" ht="14.25" r="67" s="24" spans="1:21">
       <c r="A67" s="24" t="s">
         <v>422</v>
       </c>
@@ -14255,7 +14303,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="68" spans="1:21" s="24" customFormat="1" ht="14.25">
+    <row customFormat="1" ht="14.25" r="68" s="24" spans="1:21">
       <c r="A68" s="24" t="s">
         <v>483</v>
       </c>
@@ -14314,7 +14362,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="69" spans="1:21" s="24" customFormat="1" ht="14.25">
+    <row customFormat="1" ht="14.25" r="69" s="24" spans="1:21">
       <c r="A69" s="24" t="s">
         <v>488</v>
       </c>
@@ -14373,7 +14421,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="70" spans="1:21" s="24" customFormat="1" ht="14.25">
+    <row customFormat="1" ht="14.25" r="70" s="24" spans="1:21">
       <c r="A70" s="24" t="s">
         <v>490</v>
       </c>
@@ -14432,7 +14480,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="71" spans="1:21" s="24" customFormat="1" ht="14.25">
+    <row customFormat="1" ht="14.25" r="71" s="24" spans="1:21">
       <c r="A71" s="24" t="s">
         <v>496</v>
       </c>
@@ -14491,7 +14539,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="72" spans="1:21" s="24" customFormat="1" ht="14.25">
+    <row customFormat="1" ht="14.25" r="72" s="24" spans="1:21">
       <c r="A72" s="24" t="s">
         <v>501</v>
       </c>
@@ -14550,7 +14598,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="73" spans="1:21" s="24" customFormat="1" ht="14.25">
+    <row customFormat="1" ht="14.25" r="73" s="24" spans="1:21">
       <c r="A73" s="24" t="s">
         <v>503</v>
       </c>
@@ -14609,7 +14657,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="74" spans="1:21" s="24" customFormat="1" ht="14.25">
+    <row customFormat="1" ht="14.25" r="74" s="24" spans="1:21">
       <c r="A74" s="24" t="s">
         <v>507</v>
       </c>
@@ -14668,7 +14716,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="75" spans="1:21" s="24" customFormat="1" ht="14.25">
+    <row customFormat="1" ht="14.25" r="75" s="24" spans="1:21">
       <c r="A75" s="24" t="s">
         <v>513</v>
       </c>
@@ -14727,7 +14775,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="76" spans="1:21" s="24" customFormat="1" ht="14.25">
+    <row customFormat="1" ht="14.25" r="76" s="24" spans="1:21">
       <c r="A76" s="24" t="s">
         <v>519</v>
       </c>
@@ -14786,7 +14834,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="77" spans="1:21" s="24" customFormat="1" ht="14.25">
+    <row customFormat="1" ht="14.25" r="77" s="24" spans="1:21">
       <c r="A77" s="24" t="s">
         <v>524</v>
       </c>
@@ -14845,7 +14893,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="78" spans="1:21" s="24" customFormat="1" ht="14.25">
+    <row customFormat="1" ht="14.25" r="78" s="24" spans="1:21">
       <c r="A78" s="24" t="s">
         <v>531</v>
       </c>
@@ -14904,7 +14952,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="79" spans="1:21" s="24" customFormat="1" ht="14.25">
+    <row customFormat="1" ht="14.25" r="79" s="24" spans="1:21">
       <c r="A79" s="24" t="s">
         <v>534</v>
       </c>
@@ -14963,7 +15011,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="80" spans="1:21" s="24" customFormat="1" ht="14.25">
+    <row customFormat="1" ht="14.25" r="80" s="24" spans="1:21">
       <c r="A80" s="24" t="s">
         <v>540</v>
       </c>
@@ -15022,7 +15070,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="81" spans="1:21" s="24" customFormat="1" ht="14.25">
+    <row customFormat="1" ht="14.25" r="81" s="24" spans="1:21">
       <c r="A81" s="24" t="s">
         <v>547</v>
       </c>
@@ -15081,7 +15129,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="82" spans="1:21" s="24" customFormat="1" ht="14.25">
+    <row customFormat="1" ht="14.25" r="82" s="24" spans="1:21">
       <c r="A82" s="24" t="s">
         <v>552</v>
       </c>
@@ -15140,7 +15188,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="83" spans="1:21" s="24" customFormat="1" ht="14.25">
+    <row customFormat="1" ht="14.25" r="83" s="24" spans="1:21">
       <c r="A83" s="24" t="s">
         <v>557</v>
       </c>
@@ -15199,7 +15247,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="84" spans="1:21" s="24" customFormat="1" ht="14.25">
+    <row customFormat="1" ht="14.25" r="84" s="24" spans="1:21">
       <c r="A84" s="24" t="s">
         <v>560</v>
       </c>
@@ -15258,7 +15306,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="85" spans="1:21" s="24" customFormat="1" ht="14.25">
+    <row customFormat="1" ht="14.25" r="85" s="24" spans="1:21">
       <c r="A85" s="24" t="s">
         <v>564</v>
       </c>
@@ -15317,7 +15365,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="86" spans="1:21" s="24" customFormat="1" ht="14.25">
+    <row customFormat="1" ht="14.25" r="86" s="24" spans="1:21">
       <c r="A86" s="24" t="s">
         <v>605</v>
       </c>
@@ -15376,7 +15424,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="87" spans="1:21" s="24" customFormat="1" ht="14.25">
+    <row customFormat="1" ht="14.25" r="87" s="24" spans="1:21">
       <c r="A87" s="24" t="s">
         <v>609</v>
       </c>
@@ -15435,7 +15483,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="88" spans="1:21" s="24" customFormat="1" ht="14.25">
+    <row customFormat="1" ht="14.25" r="88" s="24" spans="1:21">
       <c r="A88" s="24" t="s">
         <v>614</v>
       </c>
@@ -15494,7 +15542,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="89" spans="1:21" s="24" customFormat="1" ht="14.25">
+    <row customFormat="1" ht="14.25" r="89" s="24" spans="1:21">
       <c r="A89" s="24" t="s">
         <v>618</v>
       </c>
@@ -15553,7 +15601,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="90" spans="1:21" s="24" customFormat="1" ht="14.25">
+    <row customFormat="1" ht="14.25" r="90" s="24" spans="1:21">
       <c r="A90" s="24" t="s">
         <v>624</v>
       </c>
@@ -15612,7 +15660,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="91" spans="1:21" s="24" customFormat="1" ht="14.25">
+    <row customFormat="1" ht="14.25" r="91" s="24" spans="1:21">
       <c r="A91" s="24" t="s">
         <v>628</v>
       </c>
@@ -15671,7 +15719,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="92" spans="1:21" s="24" customFormat="1" ht="14.25">
+    <row customFormat="1" ht="14.25" r="92" s="24" spans="1:21">
       <c r="A92" s="24" t="s">
         <v>632</v>
       </c>
@@ -15730,7 +15778,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="93" spans="1:21" s="24" customFormat="1" ht="14.25">
+    <row customFormat="1" ht="14.25" r="93" s="24" spans="1:21">
       <c r="A93" s="24" t="s">
         <v>635</v>
       </c>
@@ -15789,7 +15837,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="94" spans="1:21" s="24" customFormat="1" ht="14.25">
+    <row customFormat="1" ht="14.25" r="94" s="24" spans="1:21">
       <c r="A94" s="24" t="s">
         <v>664</v>
       </c>
@@ -15848,7 +15896,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="95" spans="1:21" s="24" customFormat="1" ht="14.25">
+    <row customFormat="1" ht="14.25" r="95" s="24" spans="1:21">
       <c r="A95" s="24" t="s">
         <v>669</v>
       </c>
@@ -15907,7 +15955,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="96" spans="1:21" s="24" customFormat="1" ht="14.25">
+    <row customFormat="1" ht="14.25" r="96" s="24" spans="1:21">
       <c r="A96" s="24" t="s">
         <v>673</v>
       </c>
@@ -15966,7 +16014,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="97" spans="1:21" s="24" customFormat="1" ht="14.25">
+    <row customFormat="1" ht="14.25" r="97" s="24" spans="1:21">
       <c r="A97" s="24" t="s">
         <v>675</v>
       </c>
@@ -16025,7 +16073,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="98" spans="1:21" s="24" customFormat="1" ht="14.25">
+    <row customFormat="1" ht="14.25" r="98" s="24" spans="1:21">
       <c r="A98" s="24" t="s">
         <v>689</v>
       </c>
@@ -16084,7 +16132,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="99" spans="1:21" s="24" customFormat="1" ht="14.25">
+    <row customFormat="1" ht="14.25" r="99" s="24" spans="1:21">
       <c r="A99" s="24" t="s">
         <v>706</v>
       </c>
@@ -16143,7 +16191,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="100" spans="1:21" s="24" customFormat="1" ht="14.25">
+    <row customFormat="1" ht="14.25" r="100" s="24" spans="1:21">
       <c r="A100" s="24" t="s">
         <v>710</v>
       </c>
@@ -16202,7 +16250,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="101" spans="1:21" s="24" customFormat="1" ht="14.25">
+    <row customFormat="1" ht="14.25" r="101" s="24" spans="1:21">
       <c r="A101" s="24" t="s">
         <v>714</v>
       </c>
@@ -16261,7 +16309,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="102" spans="1:21" s="24" customFormat="1" ht="14.25">
+    <row customFormat="1" ht="14.25" r="102" s="24" spans="1:21">
       <c r="A102" s="24" t="s">
         <v>744</v>
       </c>
@@ -16320,7 +16368,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="103" spans="1:21" s="24" customFormat="1" ht="14.25">
+    <row customFormat="1" ht="14.25" r="103" s="24" spans="1:21">
       <c r="A103" s="24" t="s">
         <v>750</v>
       </c>
@@ -16379,7 +16427,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="104" spans="1:21" s="24" customFormat="1" ht="14.25">
+    <row customFormat="1" ht="14.25" r="104" s="24" spans="1:21">
       <c r="A104" s="24" t="s">
         <v>759</v>
       </c>
@@ -16438,7 +16486,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="105" spans="1:21" s="24" customFormat="1" ht="14.25">
+    <row customFormat="1" ht="14.25" r="105" s="24" spans="1:21">
       <c r="A105" s="24" t="s">
         <v>769</v>
       </c>
@@ -16497,7 +16545,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="106" spans="1:21" s="24" customFormat="1" ht="14.25">
+    <row customFormat="1" ht="14.25" r="106" s="24" spans="1:21">
       <c r="A106" s="24" t="s">
         <v>775</v>
       </c>
@@ -16556,7 +16604,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="107" spans="1:21" s="24" customFormat="1" ht="14.25">
+    <row customFormat="1" ht="14.25" r="107" s="24" spans="1:21">
       <c r="A107" s="24" t="s">
         <v>785</v>
       </c>
@@ -16615,7 +16663,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="108" spans="1:21" s="24" customFormat="1" ht="14.25">
+    <row customFormat="1" ht="14.25" r="108" s="24" spans="1:21">
       <c r="A108" s="24" t="s">
         <v>790</v>
       </c>
@@ -16674,7 +16722,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="109" spans="1:21" s="24" customFormat="1" ht="14.25">
+    <row customFormat="1" ht="14.25" r="109" s="24" spans="1:21">
       <c r="A109" s="24" t="s">
         <v>799</v>
       </c>
@@ -16733,7 +16781,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="110" spans="1:21" s="24" customFormat="1" ht="14.25">
+    <row customFormat="1" ht="14.25" r="110" s="24" spans="1:21">
       <c r="A110" s="24" t="s">
         <v>807</v>
       </c>
@@ -16792,7 +16840,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="111" spans="1:21" s="24" customFormat="1" ht="14.25">
+    <row customFormat="1" ht="14.25" r="111" s="24" spans="1:21">
       <c r="A111" s="24" t="s">
         <v>812</v>
       </c>
@@ -16851,7 +16899,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="112" spans="1:21" s="24" customFormat="1" ht="14.25">
+    <row customFormat="1" ht="14.25" r="112" s="24" spans="1:21">
       <c r="A112" s="24" t="s">
         <v>817</v>
       </c>
@@ -16910,7 +16958,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="113" spans="1:21" s="24" customFormat="1" ht="14.25">
+    <row customFormat="1" ht="14.25" r="113" s="24" spans="1:21">
       <c r="A113" s="24" t="s">
         <v>822</v>
       </c>
@@ -16969,7 +17017,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="114" spans="1:21" s="24" customFormat="1" ht="14.25">
+    <row customFormat="1" ht="14.25" r="114" s="24" spans="1:21">
       <c r="A114" s="24" t="s">
         <v>833</v>
       </c>
@@ -17028,7 +17076,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="115" spans="1:21" s="24" customFormat="1" ht="14.25">
+    <row customFormat="1" ht="14.25" r="115" s="24" spans="1:21">
       <c r="A115" s="24" t="s">
         <v>842</v>
       </c>
@@ -17087,7 +17135,7 @@
         <v>325</v>
       </c>
     </row>
-    <row r="116" spans="1:21" s="24" customFormat="1" ht="14.25">
+    <row customFormat="1" ht="14.25" r="116" s="24" spans="1:21">
       <c r="A116" s="24" t="s">
         <v>850</v>
       </c>
@@ -17146,7 +17194,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="117" spans="1:21" s="24" customFormat="1" ht="14.25">
+    <row customFormat="1" ht="14.25" r="117" s="24" spans="1:21">
       <c r="A117" s="24" t="s">
         <v>857</v>
       </c>
@@ -17205,7 +17253,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="118" spans="1:21" s="24" customFormat="1" ht="14.25">
+    <row customFormat="1" ht="14.25" r="118" s="24" spans="1:21">
       <c r="A118" s="24" t="s">
         <v>866</v>
       </c>
@@ -17264,7 +17312,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="119" spans="1:21" s="24" customFormat="1" ht="14.25">
+    <row customFormat="1" ht="14.25" r="119" s="24" spans="1:21">
       <c r="A119" s="24" t="s">
         <v>870</v>
       </c>
@@ -17323,7 +17371,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="120" spans="1:21" s="24" customFormat="1" ht="14.25">
+    <row customFormat="1" ht="14.25" r="120" s="24" spans="1:21">
       <c r="A120" s="24">
         <v>119</v>
       </c>
@@ -17382,7 +17430,7 @@
         <v>1044</v>
       </c>
     </row>
-    <row r="121" spans="1:21" s="24" customFormat="1" ht="14.25">
+    <row customFormat="1" ht="14.25" r="121" s="24" spans="1:21">
       <c r="A121" s="24" t="s">
         <v>910</v>
       </c>
@@ -17441,7 +17489,7 @@
         <v>1044</v>
       </c>
     </row>
-    <row r="122" spans="1:21" s="24" customFormat="1" ht="14.25">
+    <row customFormat="1" ht="14.25" r="122" s="24" spans="1:21">
       <c r="A122" s="24" t="s">
         <v>915</v>
       </c>
@@ -17500,7 +17548,7 @@
         <v>1044</v>
       </c>
     </row>
-    <row r="123" spans="1:21" s="24" customFormat="1" ht="14.25">
+    <row customFormat="1" ht="14.25" r="123" s="24" spans="1:21">
       <c r="A123" s="24" t="s">
         <v>922</v>
       </c>
@@ -17559,7 +17607,7 @@
         <v>1044</v>
       </c>
     </row>
-    <row r="124" spans="1:21" s="24" customFormat="1" ht="14.25">
+    <row customFormat="1" ht="14.25" r="124" s="24" spans="1:21">
       <c r="A124" s="24" t="s">
         <v>927</v>
       </c>
@@ -17618,7 +17666,7 @@
         <v>1044</v>
       </c>
     </row>
-    <row r="125" spans="1:21" s="24" customFormat="1" ht="14.25">
+    <row customFormat="1" ht="14.25" r="125" s="24" spans="1:21">
       <c r="A125" s="24" t="s">
         <v>930</v>
       </c>
@@ -17677,7 +17725,7 @@
         <v>1044</v>
       </c>
     </row>
-    <row r="126" spans="1:21" s="24" customFormat="1" ht="14.25">
+    <row customFormat="1" ht="14.25" r="126" s="24" spans="1:21">
       <c r="A126" s="24" t="s">
         <v>934</v>
       </c>
@@ -17736,7 +17784,7 @@
         <v>1044</v>
       </c>
     </row>
-    <row r="127" spans="1:21" s="24" customFormat="1" ht="14.25">
+    <row customFormat="1" ht="14.25" r="127" s="24" spans="1:21">
       <c r="A127" s="24" t="s">
         <v>940</v>
       </c>
@@ -17795,7 +17843,7 @@
         <v>1044</v>
       </c>
     </row>
-    <row r="128" spans="1:21" s="24" customFormat="1" ht="14.25">
+    <row customFormat="1" ht="14.25" r="128" s="24" spans="1:21">
       <c r="A128" s="24" t="s">
         <v>946</v>
       </c>
@@ -17854,7 +17902,7 @@
         <v>1044</v>
       </c>
     </row>
-    <row r="129" spans="1:21" s="24" customFormat="1" ht="14.25">
+    <row customFormat="1" ht="14.25" r="129" s="24" spans="1:21">
       <c r="A129" s="24" t="s">
         <v>951</v>
       </c>
@@ -17913,7 +17961,7 @@
         <v>1044</v>
       </c>
     </row>
-    <row r="130" spans="1:21" s="24" customFormat="1" ht="14.25">
+    <row customFormat="1" ht="14.25" r="130" s="24" spans="1:21">
       <c r="A130" s="24" t="s">
         <v>956</v>
       </c>
@@ -17972,7 +18020,7 @@
         <v>1044</v>
       </c>
     </row>
-    <row r="131" spans="1:21" s="24" customFormat="1" ht="14.25">
+    <row customFormat="1" ht="14.25" r="131" s="24" spans="1:21">
       <c r="A131" s="24" t="s">
         <v>960</v>
       </c>
@@ -18031,7 +18079,7 @@
         <v>1044</v>
       </c>
     </row>
-    <row r="132" spans="1:21" s="24" customFormat="1" ht="14.25">
+    <row customFormat="1" ht="14.25" r="132" s="24" spans="1:21">
       <c r="A132" s="24" t="s">
         <v>963</v>
       </c>
@@ -18090,7 +18138,7 @@
         <v>1044</v>
       </c>
     </row>
-    <row r="133" spans="1:21" s="24" customFormat="1" ht="14.25">
+    <row customFormat="1" ht="14.25" r="133" s="24" spans="1:21">
       <c r="A133" s="24" t="s">
         <v>967</v>
       </c>
@@ -18149,7 +18197,7 @@
         <v>1044</v>
       </c>
     </row>
-    <row r="134" spans="1:21" s="24" customFormat="1" ht="14.25">
+    <row customFormat="1" ht="14.25" r="134" s="24" spans="1:21">
       <c r="A134" s="24" t="s">
         <v>972</v>
       </c>
@@ -18208,7 +18256,7 @@
         <v>1044</v>
       </c>
     </row>
-    <row r="135" spans="1:21" s="24" customFormat="1" ht="14.25">
+    <row customFormat="1" ht="14.25" r="135" s="24" spans="1:21">
       <c r="A135" s="24" t="s">
         <v>975</v>
       </c>
@@ -18267,7 +18315,7 @@
         <v>1044</v>
       </c>
     </row>
-    <row r="136" spans="1:21" s="24" customFormat="1" ht="14.25">
+    <row customFormat="1" ht="14.25" r="136" s="24" spans="1:21">
       <c r="A136" s="24" t="s">
         <v>980</v>
       </c>
@@ -18326,7 +18374,7 @@
         <v>1044</v>
       </c>
     </row>
-    <row r="137" spans="1:21" s="24" customFormat="1" ht="14.25">
+    <row customFormat="1" ht="14.25" r="137" s="24" spans="1:21">
       <c r="A137" s="24" t="s">
         <v>986</v>
       </c>
@@ -18385,7 +18433,7 @@
         <v>1044</v>
       </c>
     </row>
-    <row r="138" spans="1:21" s="24" customFormat="1" ht="14.25">
+    <row customFormat="1" ht="14.25" r="138" s="24" spans="1:21">
       <c r="A138" s="24" t="s">
         <v>992</v>
       </c>
@@ -18444,7 +18492,7 @@
         <v>1044</v>
       </c>
     </row>
-    <row r="139" spans="1:21" s="24" customFormat="1" ht="14.25">
+    <row customFormat="1" ht="14.25" r="139" s="24" spans="1:21">
       <c r="A139" s="24" t="s">
         <v>997</v>
       </c>
@@ -18503,7 +18551,7 @@
         <v>1044</v>
       </c>
     </row>
-    <row r="140" spans="1:21" s="24" customFormat="1" ht="14.25">
+    <row customFormat="1" ht="14.25" r="140" s="24" spans="1:21">
       <c r="A140" s="24" t="s">
         <v>1001</v>
       </c>
@@ -18562,7 +18610,7 @@
         <v>1044</v>
       </c>
     </row>
-    <row r="141" spans="1:21" s="24" customFormat="1" ht="14.25">
+    <row customFormat="1" ht="14.25" r="141" s="24" spans="1:21">
       <c r="A141" s="24" t="s">
         <v>1007</v>
       </c>
@@ -18621,7 +18669,7 @@
         <v>1044</v>
       </c>
     </row>
-    <row r="142" spans="1:21" s="24" customFormat="1" ht="14.25">
+    <row customFormat="1" ht="14.25" r="142" s="24" spans="1:21">
       <c r="A142" s="24" t="s">
         <v>1012</v>
       </c>
@@ -18680,7 +18728,7 @@
         <v>1044</v>
       </c>
     </row>
-    <row r="143" spans="1:21" s="24" customFormat="1" ht="14.25">
+    <row customFormat="1" ht="14.25" r="143" s="24" spans="1:21">
       <c r="A143" s="24" t="s">
         <v>1017</v>
       </c>
@@ -18739,7 +18787,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="144" spans="1:21" s="24" customFormat="1" ht="14.25">
+    <row customFormat="1" ht="14.25" r="144" s="24" spans="1:21">
       <c r="A144" s="24" t="s">
         <v>1051</v>
       </c>
@@ -18798,7 +18846,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="145" spans="1:21" s="24" customFormat="1" ht="14.25">
+    <row customFormat="1" ht="14.25" r="145" s="24" spans="1:21">
       <c r="A145" s="24" t="s">
         <v>1056</v>
       </c>
@@ -18857,7 +18905,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="146" spans="1:21" s="24" customFormat="1" ht="14.25">
+    <row customFormat="1" ht="14.25" r="146" s="24" spans="1:21">
       <c r="A146" s="24" t="s">
         <v>1073</v>
       </c>
@@ -18916,7 +18964,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="147" spans="1:21" s="24" customFormat="1" ht="14.25">
+    <row customFormat="1" ht="14.25" r="147" s="24" spans="1:21">
       <c r="A147" s="24" t="s">
         <v>1078</v>
       </c>
@@ -18975,7 +19023,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="148" spans="1:21" s="24" customFormat="1" ht="14.25">
+    <row customFormat="1" ht="14.25" r="148" s="24" spans="1:21">
       <c r="A148" s="24" t="s">
         <v>1082</v>
       </c>
@@ -19034,15 +19082,15 @@
         <v>1044</v>
       </c>
     </row>
-    <row r="149" spans="1:21" s="24" customFormat="1" ht="14.25">
+    <row customFormat="1" ht="14.25" r="149" s="24" spans="1:21">
       <c r="A149" s="24" t="s">
-        <v>1097</v>
+        <v>1096</v>
       </c>
       <c r="B149" s="24" t="s">
         <v>7</v>
       </c>
       <c r="C149" s="24" t="s">
-        <v>1098</v>
+        <v>1097</v>
       </c>
       <c r="D149" s="24" t="s">
         <v>84</v>
@@ -19057,7 +19105,7 @@
         <v>104</v>
       </c>
       <c r="H149" s="24" t="s">
-        <v>1099</v>
+        <v>1098</v>
       </c>
       <c r="I149" s="24" t="s">
         <v>198</v>
@@ -19081,24 +19129,83 @@
         <v>266</v>
       </c>
       <c r="R149" s="24" t="s">
-        <v>1098</v>
+        <v>1097</v>
       </c>
       <c r="S149" s="24" t="s">
-        <v>1100</v>
+        <v>1099</v>
       </c>
       <c r="T149" s="24" t="s">
         <v>687</v>
       </c>
       <c r="U149" s="24" t="s">
+        <v>1044</v>
+      </c>
+    </row>
+    <row ht="14.25" r="150" spans="1:21">
+      <c r="A150" t="s">
+        <v>1101</v>
+      </c>
+      <c r="B150" t="s">
+        <v>1105</v>
+      </c>
+      <c r="C150" t="s">
+        <v>1102</v>
+      </c>
+      <c r="D150" t="s">
+        <v>84</v>
+      </c>
+      <c r="E150" t="s">
+        <v>78</v>
+      </c>
+      <c r="F150" t="s">
+        <v>235</v>
+      </c>
+      <c r="G150" t="s">
+        <v>112</v>
+      </c>
+      <c r="H150" t="s">
+        <v>1103</v>
+      </c>
+      <c r="I150" t="s">
+        <v>198</v>
+      </c>
+      <c r="K150" t="s">
+        <v>199</v>
+      </c>
+      <c r="L150" t="s">
+        <v>908</v>
+      </c>
+      <c r="M150" t="s">
+        <v>201</v>
+      </c>
+      <c r="N150" t="s">
+        <v>202</v>
+      </c>
+      <c r="P150" t="s">
+        <v>203</v>
+      </c>
+      <c r="Q150" t="s">
+        <v>204</v>
+      </c>
+      <c r="R150" t="s">
+        <v>1102</v>
+      </c>
+      <c r="S150" t="s">
+        <v>1104</v>
+      </c>
+      <c r="T150" s="24" t="s">
+        <v>687</v>
+      </c>
+      <c r="U150" t="s">
         <v>1044</v>
       </c>
     </row>
   </sheetData>
   <autoFilter ref="E1:E145" xr:uid="{00000000-0001-0000-0100-000000000000}"/>
   <customSheetViews>
-    <customSheetView guid="{A7754112-A52F-4ABC-8778-92F04773E53C}" filter="1" showAutoFilter="1">
-      <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-      <autoFilter ref="A1:AD33" xr:uid="{7F4EDE8C-81BA-40FB-A06E-FAFFDDC51A0F}">
+    <customSheetView filter="1" guid="{A7754112-A52F-4ABC-8778-92F04773E53C}" showAutoFilter="1">
+      <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+      <autoFilter ref="A1:AD33" xr:uid="{3170E001-C29F-4BEB-A877-F6985A9C8695}">
         <filterColumn colId="5">
           <filters blank="1">
             <filter val="Strathnairn"/>
@@ -19106,82 +19213,82 @@
         </filterColumn>
       </autoFilter>
     </customSheetView>
-    <customSheetView guid="{C25CEB9E-BEC1-4982-90C4-50C84EE1B82A}" filter="1" showAutoFilter="1">
-      <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-      <autoFilter ref="A1:AD33" xr:uid="{3F009389-08EB-4D30-AB3E-8136F1D928C3}"/>
+    <customSheetView filter="1" guid="{C25CEB9E-BEC1-4982-90C4-50C84EE1B82A}" showAutoFilter="1">
+      <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+      <autoFilter ref="A1:AD33" xr:uid="{A95EB127-FF80-4452-8922-E4548A997664}"/>
     </customSheetView>
   </customSheetViews>
   <conditionalFormatting sqref="A1:AI1">
-    <cfRule type="notContainsBlanks" dxfId="1" priority="1">
+    <cfRule dxfId="1" priority="1" type="notContainsBlanks">
       <formula>LEN(TRIM(A1))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <hyperlinks>
-    <hyperlink ref="S2" r:id="rId1" xr:uid="{00000000-0004-0000-0100-000000000000}"/>
-    <hyperlink ref="S3" r:id="rId2" xr:uid="{00000000-0004-0000-0100-000001000000}"/>
-    <hyperlink ref="S4" r:id="rId3" xr:uid="{00000000-0004-0000-0100-000002000000}"/>
-    <hyperlink ref="S5" r:id="rId4" xr:uid="{00000000-0004-0000-0100-000003000000}"/>
-    <hyperlink ref="S6" r:id="rId5" xr:uid="{00000000-0004-0000-0100-000004000000}"/>
-    <hyperlink ref="S7" r:id="rId6" xr:uid="{00000000-0004-0000-0100-000006000000}"/>
-    <hyperlink ref="S8" r:id="rId7" xr:uid="{00000000-0004-0000-0100-000008000000}"/>
-    <hyperlink ref="S9" r:id="rId8" xr:uid="{00000000-0004-0000-0100-00000A000000}"/>
-    <hyperlink ref="S10" r:id="rId9" xr:uid="{00000000-0004-0000-0100-00000C000000}"/>
-    <hyperlink ref="S11" r:id="rId10" xr:uid="{00000000-0004-0000-0100-00000E000000}"/>
-    <hyperlink ref="S12" r:id="rId11" xr:uid="{00000000-0004-0000-0100-000010000000}"/>
-    <hyperlink ref="S14" r:id="rId12" xr:uid="{00000000-0004-0000-0100-000014000000}"/>
-    <hyperlink ref="S15" r:id="rId13" xr:uid="{00000000-0004-0000-0100-000016000000}"/>
-    <hyperlink ref="S16" r:id="rId14" xr:uid="{00000000-0004-0000-0100-000018000000}"/>
-    <hyperlink ref="S17" r:id="rId15" xr:uid="{00000000-0004-0000-0100-00001A000000}"/>
-    <hyperlink ref="S18" r:id="rId16" xr:uid="{00000000-0004-0000-0100-00001C000000}"/>
-    <hyperlink ref="S19" r:id="rId17" display="https://www.allhomes.com.au/strathnairn-act-2615?tid=178720657" xr:uid="{00000000-0004-0000-0100-00001E000000}"/>
-    <hyperlink ref="S20" r:id="rId18" xr:uid="{00000000-0004-0000-0100-000020000000}"/>
-    <hyperlink ref="S21" r:id="rId19" xr:uid="{00000000-0004-0000-0100-000022000000}"/>
-    <hyperlink ref="S22" r:id="rId20" xr:uid="{00000000-0004-0000-0100-000024000000}"/>
-    <hyperlink ref="S32" r:id="rId21" xr:uid="{00000000-0004-0000-0100-000031000000}"/>
-    <hyperlink ref="S31" r:id="rId22" xr:uid="{00000000-0004-0000-0100-000030000000}"/>
-    <hyperlink ref="S30" r:id="rId23" xr:uid="{00000000-0004-0000-0100-00002F000000}"/>
-    <hyperlink ref="S29" r:id="rId24" xr:uid="{00000000-0004-0000-0100-00002E000000}"/>
-    <hyperlink ref="S28" r:id="rId25" xr:uid="{00000000-0004-0000-0100-00002D000000}"/>
-    <hyperlink ref="S27" r:id="rId26" xr:uid="{00000000-0004-0000-0100-00002C000000}"/>
-    <hyperlink ref="S26" r:id="rId27" xr:uid="{00000000-0004-0000-0100-00002B000000}"/>
-    <hyperlink ref="S25" r:id="rId28" xr:uid="{00000000-0004-0000-0100-00002A000000}"/>
-    <hyperlink ref="S24" r:id="rId29" xr:uid="{00000000-0004-0000-0100-000028000000}"/>
-    <hyperlink ref="S23" r:id="rId30" display="https://www.allhomes.com.au/ginninderra-estate-act-2615?tid=174799089" xr:uid="{00000000-0004-0000-0100-000026000000}"/>
-    <hyperlink ref="F145" r:id="rId31" display="https://www.allhomes.com.au/browse-sale/greater-queanbeyan-queanbeyan-region-nsw/" xr:uid="{4A50D1D1-69A3-4F14-AFDA-4A60EE9976C1}"/>
+    <hyperlink r:id="rId1" ref="S2" xr:uid="{00000000-0004-0000-0100-000000000000}"/>
+    <hyperlink r:id="rId2" ref="S3" xr:uid="{00000000-0004-0000-0100-000001000000}"/>
+    <hyperlink r:id="rId3" ref="S4" xr:uid="{00000000-0004-0000-0100-000002000000}"/>
+    <hyperlink r:id="rId4" ref="S5" xr:uid="{00000000-0004-0000-0100-000003000000}"/>
+    <hyperlink r:id="rId5" ref="S6" xr:uid="{00000000-0004-0000-0100-000004000000}"/>
+    <hyperlink r:id="rId6" ref="S7" xr:uid="{00000000-0004-0000-0100-000006000000}"/>
+    <hyperlink r:id="rId7" ref="S8" xr:uid="{00000000-0004-0000-0100-000008000000}"/>
+    <hyperlink r:id="rId8" ref="S9" xr:uid="{00000000-0004-0000-0100-00000A000000}"/>
+    <hyperlink r:id="rId9" ref="S10" xr:uid="{00000000-0004-0000-0100-00000C000000}"/>
+    <hyperlink r:id="rId10" ref="S11" xr:uid="{00000000-0004-0000-0100-00000E000000}"/>
+    <hyperlink r:id="rId11" ref="S12" xr:uid="{00000000-0004-0000-0100-000010000000}"/>
+    <hyperlink r:id="rId12" ref="S14" xr:uid="{00000000-0004-0000-0100-000014000000}"/>
+    <hyperlink r:id="rId13" ref="S15" xr:uid="{00000000-0004-0000-0100-000016000000}"/>
+    <hyperlink r:id="rId14" ref="S16" xr:uid="{00000000-0004-0000-0100-000018000000}"/>
+    <hyperlink r:id="rId15" ref="S17" xr:uid="{00000000-0004-0000-0100-00001A000000}"/>
+    <hyperlink r:id="rId16" ref="S18" xr:uid="{00000000-0004-0000-0100-00001C000000}"/>
+    <hyperlink display="https://www.allhomes.com.au/strathnairn-act-2615?tid=178720657" r:id="rId17" ref="S19" xr:uid="{00000000-0004-0000-0100-00001E000000}"/>
+    <hyperlink r:id="rId18" ref="S20" xr:uid="{00000000-0004-0000-0100-000020000000}"/>
+    <hyperlink r:id="rId19" ref="S21" xr:uid="{00000000-0004-0000-0100-000022000000}"/>
+    <hyperlink r:id="rId20" ref="S22" xr:uid="{00000000-0004-0000-0100-000024000000}"/>
+    <hyperlink r:id="rId21" ref="S32" xr:uid="{00000000-0004-0000-0100-000031000000}"/>
+    <hyperlink r:id="rId22" ref="S31" xr:uid="{00000000-0004-0000-0100-000030000000}"/>
+    <hyperlink r:id="rId23" ref="S30" xr:uid="{00000000-0004-0000-0100-00002F000000}"/>
+    <hyperlink r:id="rId24" ref="S29" xr:uid="{00000000-0004-0000-0100-00002E000000}"/>
+    <hyperlink r:id="rId25" ref="S28" xr:uid="{00000000-0004-0000-0100-00002D000000}"/>
+    <hyperlink r:id="rId26" ref="S27" xr:uid="{00000000-0004-0000-0100-00002C000000}"/>
+    <hyperlink r:id="rId27" ref="S26" xr:uid="{00000000-0004-0000-0100-00002B000000}"/>
+    <hyperlink r:id="rId28" ref="S25" xr:uid="{00000000-0004-0000-0100-00002A000000}"/>
+    <hyperlink r:id="rId29" ref="S24" xr:uid="{00000000-0004-0000-0100-000028000000}"/>
+    <hyperlink display="https://www.allhomes.com.au/ginninderra-estate-act-2615?tid=174799089" r:id="rId30" ref="S23" xr:uid="{00000000-0004-0000-0100-000026000000}"/>
+    <hyperlink display="https://www.allhomes.com.au/browse-sale/greater-queanbeyan-queanbeyan-region-nsw/" r:id="rId31" ref="F145" xr:uid="{4A50D1D1-69A3-4F14-AFDA-4A60EE9976C1}"/>
   </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId32"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageSetup orientation="portrait" paperSize="9" r:id="rId32"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:AI1"/>
+  <dimension ref="A1:AJ1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1"/>
+  <sheetFormatPr customHeight="1" defaultColWidth="14.42578125" defaultRowHeight="15.75"/>
   <cols>
-    <col min="1" max="1" width="16" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="14.5703125" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="16.85546875" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="14.5703125" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="13.140625" customWidth="1" collapsed="1"/>
-    <col min="15" max="15" width="20.85546875" customWidth="1" collapsed="1"/>
-    <col min="21" max="22" width="19.140625" customWidth="1" collapsed="1"/>
-    <col min="23" max="23" width="20.140625" customWidth="1" collapsed="1"/>
-    <col min="24" max="24" width="19.85546875" customWidth="1" collapsed="1"/>
-    <col min="26" max="26" width="15.85546875" customWidth="1" collapsed="1"/>
-    <col min="27" max="27" width="13.42578125" customWidth="1" collapsed="1"/>
-    <col min="28" max="28" width="15.140625" customWidth="1" collapsed="1"/>
-    <col min="29" max="29" width="16.140625" customWidth="1" collapsed="1"/>
-    <col min="30" max="30" width="15.85546875" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="16.0" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="14.5703125" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="16.85546875" collapsed="true"/>
+    <col min="8" max="8" customWidth="true" width="14.5703125" collapsed="true"/>
+    <col min="9" max="9" customWidth="true" width="13.140625" collapsed="true"/>
+    <col min="15" max="15" customWidth="true" width="20.85546875" collapsed="true"/>
+    <col min="21" max="22" customWidth="true" width="19.140625" collapsed="true"/>
+    <col min="23" max="23" customWidth="true" width="20.140625" collapsed="true"/>
+    <col min="24" max="24" customWidth="true" width="19.85546875" collapsed="true"/>
+    <col min="26" max="26" customWidth="true" width="15.85546875" collapsed="true"/>
+    <col min="27" max="27" customWidth="true" width="13.42578125" collapsed="true"/>
+    <col min="28" max="28" customWidth="true" width="15.140625" collapsed="true"/>
+    <col min="29" max="29" customWidth="true" width="16.140625" collapsed="true"/>
+    <col min="30" max="30" customWidth="true" width="15.85546875" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:35" ht="15.75" customHeight="1">
+    <row customHeight="1" ht="15.75" r="1" spans="1:35">
       <c r="A1" s="1" t="s">
         <v>46</v>
       </c>
@@ -19280,37 +19387,37 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A1:AI1">
-    <cfRule type="notContainsBlanks" dxfId="0" priority="1">
+    <cfRule dxfId="0" priority="1" type="notContainsBlanks">
       <formula>LEN(TRIM(A1))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageSetup orientation="portrait" paperSize="9" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:G7"/>
+  <dimension ref="A1:H7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D18" sqref="D18"/>
+      <pane activePane="bottomLeft" state="frozen" topLeftCell="A2" ySplit="1"/>
+      <selection activeCell="D18" pane="bottomLeft" sqref="D18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1"/>
+  <sheetFormatPr customHeight="1" defaultColWidth="14.42578125" defaultRowHeight="15.75"/>
   <cols>
-    <col min="1" max="1" width="44.85546875" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="19.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="26.42578125" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="36.140625" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="53.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="44.85546875" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="19.5703125" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="26.42578125" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="36.140625" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="53.7109375" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="15">
+    <row ht="15" r="1" spans="1:7">
       <c r="A1" s="29" t="s">
         <v>152</v>
       </c>
@@ -19333,7 +19440,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="2" spans="1:7" s="30" customFormat="1" ht="15.75" customHeight="1">
+    <row customFormat="1" customHeight="1" ht="15.75" r="2" s="30" spans="1:7">
       <c r="A2" s="30" t="s">
         <v>158</v>
       </c>
@@ -19356,7 +19463,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:7" ht="15.75" customHeight="1">
+    <row customHeight="1" ht="15.75" r="3" spans="1:7">
       <c r="A3" s="30" t="s">
         <v>161</v>
       </c>
@@ -19373,7 +19480,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="4" spans="1:7" ht="15.75" customHeight="1">
+    <row customHeight="1" ht="15.75" r="4" spans="1:7">
       <c r="A4" s="30" t="s">
         <v>164</v>
       </c>
@@ -19390,7 +19497,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="5" spans="1:7" ht="15.75" customHeight="1">
+    <row customHeight="1" ht="15.75" r="5" spans="1:7">
       <c r="A5" s="34" t="s">
         <v>167</v>
       </c>
@@ -19407,7 +19514,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="6" spans="1:7" ht="15.75" customHeight="1">
+    <row customHeight="1" ht="15.75" r="6" spans="1:7">
       <c r="A6" t="s">
         <v>328</v>
       </c>
@@ -19424,7 +19531,7 @@
         <v>323</v>
       </c>
     </row>
-    <row r="7" spans="1:7" ht="15.75" customHeight="1">
+    <row customHeight="1" ht="15.75" r="7" spans="1:7">
       <c r="A7" s="45" t="s">
         <v>877</v>
       </c>
@@ -19443,16 +19550,16 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="E2" r:id="rId1" xr:uid="{00000000-0004-0000-0300-000000000000}"/>
-    <hyperlink ref="E3" r:id="rId2" xr:uid="{00000000-0004-0000-0300-000001000000}"/>
-    <hyperlink ref="E4" r:id="rId3" xr:uid="{00000000-0004-0000-0300-000002000000}"/>
-    <hyperlink ref="E5" r:id="rId4" xr:uid="{00000000-0004-0000-0300-000003000000}"/>
-    <hyperlink ref="D6" r:id="rId5" xr:uid="{00000000-0004-0000-0300-000004000000}"/>
-    <hyperlink ref="E6" r:id="rId6" xr:uid="{00000000-0004-0000-0300-000005000000}"/>
-    <hyperlink ref="D7" r:id="rId7" xr:uid="{B34712F5-65E4-4DA3-B4D8-B5E126A91A19}"/>
-    <hyperlink ref="E7" r:id="rId8" xr:uid="{FAD2E722-F8D2-45E6-8DA2-DA530385A188}"/>
+    <hyperlink r:id="rId1" ref="E2" xr:uid="{00000000-0004-0000-0300-000000000000}"/>
+    <hyperlink r:id="rId2" ref="E3" xr:uid="{00000000-0004-0000-0300-000001000000}"/>
+    <hyperlink r:id="rId3" ref="E4" xr:uid="{00000000-0004-0000-0300-000002000000}"/>
+    <hyperlink r:id="rId4" ref="E5" xr:uid="{00000000-0004-0000-0300-000003000000}"/>
+    <hyperlink r:id="rId5" ref="D6" xr:uid="{00000000-0004-0000-0300-000004000000}"/>
+    <hyperlink r:id="rId6" ref="E6" xr:uid="{00000000-0004-0000-0300-000005000000}"/>
+    <hyperlink r:id="rId7" ref="D7" xr:uid="{B34712F5-65E4-4DA3-B4D8-B5E126A91A19}"/>
+    <hyperlink r:id="rId8" ref="E7" xr:uid="{FAD2E722-F8D2-45E6-8DA2-DA530385A188}"/>
   </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId9"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageSetup orientation="portrait" paperSize="9" r:id="rId9"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
New listing check script run 23/09/2021
</commit_message>
<xml_diff>
--- a/src/main/resources/InputTestdata/Listing details.xlsx
+++ b/src/main/resources/InputTestdata/Listing details.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Athavan\git\777Homes-2\777Homes-business\src\main\resources\InputTestdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr documentId="13_ncr:1_{61F3BAB8-8A9D-43F6-9E0A-B63C75C062AD}" revIDLastSave="0" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47"/>
+  <xr:revisionPtr documentId="13_ncr:1_{A4E7D451-5509-43D9-A984-65D982E26BBC}" revIDLastSave="0" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47"/>
   <bookViews>
     <workbookView windowHeight="15840" windowWidth="29040" xWindow="-120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}" yWindow="-120"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3649" uniqueCount="1107">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3703" uniqueCount="1123">
   <si>
     <t>ID</t>
   </si>
@@ -5399,10 +5399,119 @@
 EER: 6.0</t>
   </si>
   <si>
+    <t>https://www.777homes.com.au/?post_type=property&amp;p=8847&amp;preview=true</t>
+  </si>
+  <si>
+    <t>https://www.allhomes.com.au/39-mccredie-street-taylor-act-2913</t>
+  </si>
+  <si>
+    <t>https://www.allhomes.com.au/unit-68-17-medley-street-chifley-act-2606</t>
+  </si>
+  <si>
+    <t>150</t>
+  </si>
+  <si>
+    <t>39 McCredie Street, Taylor ACT 2913</t>
+  </si>
+  <si>
+    <t>NEW</t>
+  </si>
+  <si>
+    <t>Block/House: 555/ 315</t>
+  </si>
+  <si>
+    <t>Upcoming Auction</t>
+  </si>
+  <si>
+    <t>DUE TO COVID RESTRICTIONS - YOU MUST CALL TO BOOK IN FOR THE TIME SLOT TO VIEW 1 ON 1.
+Please contact Gurjant 0497 000 007 or Abhi 0404 525 998 for further details or to arrange your personal inspection.
+New Door properties is proud to present 39 McCredie Street in the picturesque suburb - Taylor.
+There are plenty of features in this house to make a blanket statement about it being "breathtaking". Upon viewing this property, you will appreciate the love and care by which the first owner has kept the home. This architect designed home stands out with its modern detailed facade, and a commitment to high end inclusions and finishes to the very last detail it is now ready and waiting for those who are looking for a beautiful new family home in a popular location.
+Offering a stunning, North facing formal living area, four bedrooms including spacious master suite, theatre room, spacious family and dining area, common sitting room all unfolding over two levels, and provides superlative comfort and luxury.
+Open plan casual living can only be described as spectacular, the magnificent kitchen showcases a stone island bench with waterfalls. Top of the range appliances include Bosch oven, microwave, 900 mm cooktop, Fisher and Paykel dishwasher &amp; Schweigen range-hood. Comfort is assured throughout by the ducted reverse cycle air conditioning system with two zones.
+Casual living is continuous with an outdoor space designed for entertainment with the family. Also, nature is just on the doorstep of this fabulous location, with a walking/cycling pathway running along with parameter, park is just on a walking distance. Taylor school is only a short walk away &amp; It is just a short drive to all the facilities of Gungahlin marketplace and the light rail terminals.
+Property Features:
+• Modern façade
+• Four bedrooms
+• Extra-large master bedroom with balcony
+• Three bathroom
+• Rumpus/ Theatre room
+• Multiple living areas
+• Electric fire place
+• Quality timber features
+• LED lights throughout the house
+• Video intercom
+• Stone island bench with waterfalls
+• Walk in pantry with all custom joinery
+• Schweigen under-mount ducted range-hood
+• Fisher &amp; Paykel double door dishwasher
+• Bosch induction cooktop
+• Bosch twin 600 mm oven &amp; Microwave
+• Timber Flooring in living areas
+• Carpet in bedrooms
+• Separate laundry
+• Quality bathrooms with Phoenix tap-ware
+• Heated towel rails
+• 2.70 m ceiling in lower living
+• 2.55 m ceiling in upper living
+• Double glazed windows
+• 6 Security Cameras
+• Ducted reverse cycle heating and cooling with zones
+• Separate hot water systems for upstairs and downstairs
+• Tiled alfresco with custom joinery
+• Low maintenance landscaped backyard.
+• Concrete all around the house.
+• Rainwater tank
+• Double garage
+• NBN connected
+Property Information :
+• Lower Living : 141.20 m2 (approx...)
+• Upper Living : 92.32 m2 (approx...)
+• Garage : 43.73 m2 (approx...)
+• Alfresco : 25.27 m2 (approx...)
+• Balcony : 7.27 m2 (approx...)
+• Porch : 5.86 m2 (approx...)
+• House Size : 315.64 m2 (approx...)
+• Block Size : 555.00 m2 (approx..)</t>
+  </si>
+  <si>
+    <t>151</t>
+  </si>
+  <si>
+    <t>68/17 Medley Street, Chifley ACT 2606</t>
+  </si>
+  <si>
+    <t>Chifley</t>
+  </si>
+  <si>
+    <t xml:space="preserve">3	3	9	0	0	0	</t>
+  </si>
+  <si>
+    <t>Offers over $339,000</t>
+  </si>
+  <si>
+    <t>Due to the current ACT lockdown restrictions we are only doing opens by private appointments. Please Call Anish on 0450865524 to book your appointment.
+This delightful top floor, two bedroom apartment is conveniently located at the end of the complex adjacent to parkland and walking tracks and all within a few minutes of the Woden Town Centre.
+The unit has a generous kitchen with ample cupboard space. Light filled living and dining area leads to a generous balcony. Both bedrooms include built-in wardrobes, with bathroom centrally located between the bedrooms. A double carport and storage cupboard and abundant visitor car parks complete the charm of this entry level apartment.
+If you are a first home buyer or looking to invest you can't go past this opportunity.
+Potential rental return $450 a week. Call Anish now on 0450865524 before you miss this opportunity.
+Features
+- Light-filled top floor two bedroom apartment with leafy outlook
+- Two bedrooms with built-in wardrobes
+- Spacious balcony
+- Double carport and storage shed
+- Visitor car parks
+- Close proximity to Woden Town Centre, Westfield Woden, cafes and bars
+- The Canberra Hospital nearby</t>
+  </si>
+  <si>
     <t>Draft</t>
   </si>
   <si>
-    <t>https://www.777homes.com.au/?post_type=property&amp;p=8847&amp;preview=true</t>
+    <t>https://www.777homes.com.au/?post_type=property&amp;p=8875&amp;preview=true</t>
+  </si>
+  <si>
+    <t>https://www.777homes.com.au/?post_type=property&amp;p=8877&amp;preview=true</t>
   </si>
 </sst>
 </file>
@@ -5570,7 +5679,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="10">
+  <fills count="13">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -5624,6 +5733,21 @@
         <bgColor indexed="2"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="mediumGray">
+        <bgColor indexed="2"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor indexed="2"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="mediumGray">
+        <bgColor indexed="2"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -5638,7 +5762,7 @@
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
     <xf applyAlignment="0" applyBorder="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="0" fontId="25" numFmtId="0"/>
   </cellStyleXfs>
-  <cellXfs count="47">
+  <cellXfs count="49">
     <xf applyAlignment="1" applyFont="1" borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
     <xf applyAlignment="1" applyFill="1" applyFont="1" borderId="0" fillId="3" fontId="1" numFmtId="0" xfId="0">
       <alignment horizontal="center"/>
@@ -5736,6 +5860,8 @@
     </xf>
     <xf applyAlignment="1" applyFont="1" borderId="0" fillId="0" fontId="27" numFmtId="0" xfId="0"/>
     <xf applyFill="1" borderId="0" fillId="9" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyFill="1" borderId="0" fillId="10" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyFill="true" borderId="0" fillId="12" fontId="0" numFmtId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle builtinId="8" name="Hyperlink" xfId="1"/>
@@ -5972,11 +6098,11 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:AC150"/>
+  <dimension ref="A1:AC152"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane activePane="bottomLeft" state="frozen" topLeftCell="A137" ySplit="1"/>
-      <selection activeCell="B150" pane="bottomLeft" sqref="B150"/>
+      <selection activeCell="F155" pane="bottomLeft" sqref="F155"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr customHeight="1" defaultColWidth="14.42578125" defaultRowHeight="15.75"/>
@@ -9570,7 +9696,7 @@
         <v>1030</v>
       </c>
       <c r="D131" s="4" t="s">
-        <v>7</v>
+        <v>14</v>
       </c>
       <c r="F131" s="2" t="s">
         <v>687</v>
@@ -10004,10 +10130,10 @@
         <v>1100</v>
       </c>
       <c r="C150" t="s">
-        <v>1106</v>
-      </c>
-      <c r="D150" s="46" t="s">
         <v>1105</v>
+      </c>
+      <c r="D150" s="4" t="s">
+        <v>7</v>
       </c>
       <c r="F150" s="2" t="s">
         <v>687</v>
@@ -10016,6 +10142,52 @@
         <v>1044</v>
       </c>
       <c r="H150" t="s">
+        <v>881</v>
+      </c>
+    </row>
+    <row ht="12.75" r="151" spans="1:8">
+      <c r="A151">
+        <v>150</v>
+      </c>
+      <c r="B151" t="s">
+        <v>1106</v>
+      </c>
+      <c r="C151" t="s">
+        <v>1121</v>
+      </c>
+      <c r="D151" s="46" t="s">
+        <v>1120</v>
+      </c>
+      <c r="F151" s="2" t="s">
+        <v>1046</v>
+      </c>
+      <c r="G151" t="s">
+        <v>8</v>
+      </c>
+      <c r="H151" t="s">
+        <v>427</v>
+      </c>
+    </row>
+    <row ht="12.75" r="152" spans="1:8">
+      <c r="A152">
+        <v>151</v>
+      </c>
+      <c r="B152" t="s">
+        <v>1107</v>
+      </c>
+      <c r="C152" t="s">
+        <v>1122</v>
+      </c>
+      <c r="D152" s="47" t="s">
+        <v>1120</v>
+      </c>
+      <c r="F152" s="2" t="s">
+        <v>687</v>
+      </c>
+      <c r="G152" t="s">
+        <v>1044</v>
+      </c>
+      <c r="H152" t="s">
         <v>881</v>
       </c>
     </row>
@@ -10221,11 +10393,11 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:AJ150"/>
+  <dimension ref="A1:AJ152"/>
   <sheetViews>
-    <sheetView topLeftCell="E1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane activePane="bottomLeft" state="frozen" topLeftCell="A134" ySplit="1"/>
-      <selection activeCell="R155" pane="bottomLeft" sqref="R155"/>
+      <selection activeCell="D161" pane="bottomLeft" sqref="D161"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr customHeight="1" defaultColWidth="14.42578125" defaultRowHeight="15.75"/>
@@ -19141,62 +19313,180 @@
         <v>1044</v>
       </c>
     </row>
-    <row ht="14.25" r="150" spans="1:21">
-      <c r="A150" t="s">
+    <row customFormat="1" ht="14.25" r="150" s="24" spans="1:21">
+      <c r="A150" s="24" t="s">
         <v>1101</v>
       </c>
-      <c r="B150" t="s">
-        <v>1105</v>
-      </c>
-      <c r="C150" t="s">
+      <c r="B150" s="24" t="s">
+        <v>7</v>
+      </c>
+      <c r="C150" s="24" t="s">
         <v>1102</v>
       </c>
-      <c r="D150" t="s">
+      <c r="D150" s="24" t="s">
         <v>84</v>
       </c>
-      <c r="E150" t="s">
+      <c r="E150" s="24" t="s">
         <v>78</v>
       </c>
-      <c r="F150" t="s">
+      <c r="F150" s="24" t="s">
         <v>235</v>
       </c>
-      <c r="G150" t="s">
+      <c r="G150" s="24" t="s">
         <v>112</v>
       </c>
-      <c r="H150" t="s">
+      <c r="H150" s="24" t="s">
         <v>1103</v>
       </c>
-      <c r="I150" t="s">
+      <c r="I150" s="24" t="s">
         <v>198</v>
       </c>
-      <c r="K150" t="s">
+      <c r="K150" s="24" t="s">
         <v>199</v>
       </c>
-      <c r="L150" t="s">
+      <c r="L150" s="24" t="s">
         <v>908</v>
       </c>
-      <c r="M150" t="s">
+      <c r="M150" s="24" t="s">
         <v>201</v>
       </c>
-      <c r="N150" t="s">
+      <c r="N150" s="24" t="s">
         <v>202</v>
       </c>
-      <c r="P150" t="s">
+      <c r="P150" s="24" t="s">
         <v>203</v>
       </c>
-      <c r="Q150" t="s">
+      <c r="Q150" s="24" t="s">
         <v>204</v>
       </c>
-      <c r="R150" t="s">
+      <c r="R150" s="24" t="s">
         <v>1102</v>
       </c>
-      <c r="S150" t="s">
+      <c r="S150" s="24" t="s">
         <v>1104</v>
       </c>
       <c r="T150" s="24" t="s">
         <v>687</v>
       </c>
-      <c r="U150" t="s">
+      <c r="U150" s="24" t="s">
+        <v>1044</v>
+      </c>
+    </row>
+    <row r="151">
+      <c r="A151" t="s">
+        <v>1108</v>
+      </c>
+      <c r="B151" t="s">
+        <v>1120</v>
+      </c>
+      <c r="C151" t="s">
+        <v>1109</v>
+      </c>
+      <c r="D151" t="s">
+        <v>84</v>
+      </c>
+      <c r="E151" t="s">
+        <v>78</v>
+      </c>
+      <c r="F151" t="s">
+        <v>79</v>
+      </c>
+      <c r="G151" t="s">
+        <v>85</v>
+      </c>
+      <c r="H151" t="s">
+        <v>1111</v>
+      </c>
+      <c r="I151" t="s">
+        <v>198</v>
+      </c>
+      <c r="K151" t="s">
+        <v>199</v>
+      </c>
+      <c r="L151" t="s">
+        <v>1112</v>
+      </c>
+      <c r="M151" t="s">
+        <v>201</v>
+      </c>
+      <c r="N151" t="s">
+        <v>202</v>
+      </c>
+      <c r="P151" t="s">
+        <v>203</v>
+      </c>
+      <c r="Q151" t="s">
+        <v>204</v>
+      </c>
+      <c r="R151" t="s">
+        <v>1109</v>
+      </c>
+      <c r="S151" t="s">
+        <v>1113</v>
+      </c>
+      <c r="T151" t="s">
+        <v>1046</v>
+      </c>
+      <c r="U151" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="152">
+      <c r="A152" t="s">
+        <v>1114</v>
+      </c>
+      <c r="B152" t="s">
+        <v>1120</v>
+      </c>
+      <c r="C152" t="s">
+        <v>1115</v>
+      </c>
+      <c r="D152" t="s">
+        <v>77</v>
+      </c>
+      <c r="E152" t="s">
+        <v>78</v>
+      </c>
+      <c r="F152" t="s">
+        <v>684</v>
+      </c>
+      <c r="G152" t="s">
+        <v>1116</v>
+      </c>
+      <c r="H152" t="s">
+        <v>199</v>
+      </c>
+      <c r="I152" t="s">
+        <v>198</v>
+      </c>
+      <c r="K152" t="s">
+        <v>1117</v>
+      </c>
+      <c r="L152" t="s">
+        <v>1118</v>
+      </c>
+      <c r="M152" t="s">
+        <v>204</v>
+      </c>
+      <c r="N152" t="s">
+        <v>266</v>
+      </c>
+      <c r="P152" t="s">
+        <v>252</v>
+      </c>
+      <c r="Q152" t="s">
+        <v>204</v>
+      </c>
+      <c r="R152" t="s">
+        <v>1115</v>
+      </c>
+      <c r="S152" t="s">
+        <v>1119</v>
+      </c>
+      <c r="T152" t="s">
+        <v>687</v>
+      </c>
+      <c r="U152" t="s">
         <v>1044</v>
       </c>
     </row>
@@ -19205,7 +19495,7 @@
   <customSheetViews>
     <customSheetView filter="1" guid="{A7754112-A52F-4ABC-8778-92F04773E53C}" showAutoFilter="1">
       <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
-      <autoFilter ref="A1:AD33" xr:uid="{3170E001-C29F-4BEB-A877-F6985A9C8695}">
+      <autoFilter ref="A1:AD33" xr:uid="{50AC9568-35DE-4B86-9AD0-75B55D6D263E}">
         <filterColumn colId="5">
           <filters blank="1">
             <filter val="Strathnairn"/>
@@ -19215,7 +19505,7 @@
     </customSheetView>
     <customSheetView filter="1" guid="{C25CEB9E-BEC1-4982-90C4-50C84EE1B82A}" showAutoFilter="1">
       <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
-      <autoFilter ref="A1:AD33" xr:uid="{A95EB127-FF80-4452-8922-E4548A997664}"/>
+      <autoFilter ref="A1:AD33" xr:uid="{CC0452E8-80BB-42E2-9DA0-FBE75D4E7806}"/>
     </customSheetView>
   </customSheetViews>
   <conditionalFormatting sqref="A1:AI1">

</xml_diff>

<commit_message>
New property script run 27/09/2021
</commit_message>
<xml_diff>
--- a/src/main/resources/InputTestdata/Listing details.xlsx
+++ b/src/main/resources/InputTestdata/Listing details.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Athavan\git\777Homes-2\777Homes-business\src\main\resources\InputTestdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr documentId="13_ncr:1_{A4E7D451-5509-43D9-A984-65D982E26BBC}" revIDLastSave="0" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47"/>
+  <xr:revisionPtr documentId="13_ncr:1_{008756E1-6CFA-4503-B13A-646A05FBAFEE}" revIDLastSave="0" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47"/>
   <bookViews>
     <workbookView windowHeight="15840" windowWidth="29040" xWindow="-120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}" yWindow="-120"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3703" uniqueCount="1123">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3725" uniqueCount="1129">
   <si>
     <t>ID</t>
   </si>
@@ -5412,9 +5412,6 @@
   </si>
   <si>
     <t>39 McCredie Street, Taylor ACT 2913</t>
-  </si>
-  <si>
-    <t>NEW</t>
   </si>
   <si>
     <t>Block/House: 555/ 315</t>
@@ -5505,13 +5502,48 @@
 - The Canberra Hospital nearby</t>
   </si>
   <si>
+    <t>https://www.777homes.com.au/?post_type=property&amp;p=8875&amp;preview=true</t>
+  </si>
+  <si>
+    <t>https://www.777homes.com.au/?post_type=property&amp;p=8877&amp;preview=true</t>
+  </si>
+  <si>
+    <t>https://www.allhomes.com.au/unit-5-92-casey-crescent-calwell-act-2905</t>
+  </si>
+  <si>
+    <t>152</t>
+  </si>
+  <si>
+    <t>5/92 Casey Crescent, Calwell ACT 2905</t>
+  </si>
+  <si>
+    <t>NEW</t>
+  </si>
+  <si>
+    <t>Calwell</t>
+  </si>
+  <si>
+    <t>Bookings by appointment. Limited appointments available on Saturday 25th September from 10:30am onwards. Please call Alvin on 0426 146 118 to book your slot.
+Situated within one of Calwell's best known townhouse complexes, 'Narona Park,' this quality and attractive three bedroom, ensuite free-standing townhouse is a must see. Although considered within the well maintained complex, unit 5 doesn't have neighbours on either sides.
+Offering open plan living areas, lounge at the front of the house overlooks charming front courtyard garden. The tiled kitchen overlooks the immaculate and secure rear garden and adjoins both the dining and family area, allowing you to keep an eye on the kids when preparing your meals. With a gas cooktop, electric oven and dishwasher (all stainless steel), generous storage and a breakfast bar you will quickly discover this is a practical and functional area too.
+Boasting a choice of superb alfresco entertaining spaces, this single level townhouse showcases generous proportions and a host of quality inclusions. It's set back from the street in a quiet complex a stroll from local shops, schools, parks and transport.
+- Spacious lounge room and all bedrooms with quality bamboo flooring
+- All-weather patio with speakers, LED lights and heating
+- North facing courtyard, manicured gardens and outdoor seven seat Jacuzzi
+- Light filled gas kitchen with a breakfast bar and dishwasher
+- Well scaled bedrooms, master with ensuite and walk-in robe
+- Family sized main bathroom with large corner bath and separate w/c
+- Excellent opportunity for downsizers or first homebuyers
+- Security Alarm, ducted air conditioning/heating, garden sheds, ducted vacuum
+- Internal entry to double automated garage, secure side access
+- Close to Calwell Shopping Centre, sport fields and eateries
+- CCTV Camera, near new Bamboo flooring, fresh paint throughout</t>
+  </si>
+  <si>
     <t>Draft</t>
   </si>
   <si>
-    <t>https://www.777homes.com.au/?post_type=property&amp;p=8875&amp;preview=true</t>
-  </si>
-  <si>
-    <t>https://www.777homes.com.au/?post_type=property&amp;p=8877&amp;preview=true</t>
+    <t>https://www.777homes.com.au/?post_type=property&amp;p=8946&amp;preview=true</t>
   </si>
 </sst>
 </file>
@@ -5679,7 +5711,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="13">
+  <fills count="12">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -5734,11 +5766,6 @@
       </patternFill>
     </fill>
     <fill>
-      <patternFill patternType="mediumGray">
-        <bgColor indexed="2"/>
-      </patternFill>
-    </fill>
-    <fill>
       <patternFill patternType="none">
         <bgColor indexed="2"/>
       </patternFill>
@@ -5762,7 +5789,7 @@
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
     <xf applyAlignment="0" applyBorder="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="0" fontId="25" numFmtId="0"/>
   </cellStyleXfs>
-  <cellXfs count="49">
+  <cellXfs count="48">
     <xf applyAlignment="1" applyFont="1" borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
     <xf applyAlignment="1" applyFill="1" applyFont="1" borderId="0" fillId="3" fontId="1" numFmtId="0" xfId="0">
       <alignment horizontal="center"/>
@@ -5860,8 +5887,7 @@
     </xf>
     <xf applyAlignment="1" applyFont="1" borderId="0" fillId="0" fontId="27" numFmtId="0" xfId="0"/>
     <xf applyFill="1" borderId="0" fillId="9" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyFill="1" borderId="0" fillId="10" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyFill="true" borderId="0" fillId="12" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyFill="true" borderId="0" fillId="11" fontId="0" numFmtId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle builtinId="8" name="Hyperlink" xfId="1"/>
@@ -6098,11 +6124,11 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:AC152"/>
+  <dimension ref="A1:AC153"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane activePane="bottomLeft" state="frozen" topLeftCell="A137" ySplit="1"/>
-      <selection activeCell="F155" pane="bottomLeft" sqref="F155"/>
+      <pane activePane="bottomLeft" state="frozen" topLeftCell="A131" ySplit="1"/>
+      <selection activeCell="E158" pane="bottomLeft" sqref="E158"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr customHeight="1" defaultColWidth="14.42578125" defaultRowHeight="15.75"/>
@@ -10153,10 +10179,10 @@
         <v>1106</v>
       </c>
       <c r="C151" t="s">
-        <v>1121</v>
-      </c>
-      <c r="D151" s="46" t="s">
-        <v>1120</v>
+        <v>1119</v>
+      </c>
+      <c r="D151" s="4" t="s">
+        <v>7</v>
       </c>
       <c r="F151" s="2" t="s">
         <v>1046</v>
@@ -10176,10 +10202,10 @@
         <v>1107</v>
       </c>
       <c r="C152" t="s">
-        <v>1122</v>
-      </c>
-      <c r="D152" s="47" t="s">
         <v>1120</v>
+      </c>
+      <c r="D152" s="4" t="s">
+        <v>7</v>
       </c>
       <c r="F152" s="2" t="s">
         <v>687</v>
@@ -10188,6 +10214,29 @@
         <v>1044</v>
       </c>
       <c r="H152" t="s">
+        <v>881</v>
+      </c>
+    </row>
+    <row ht="12.75" r="153" spans="1:8">
+      <c r="A153">
+        <v>152</v>
+      </c>
+      <c r="B153" t="s">
+        <v>1121</v>
+      </c>
+      <c r="C153" t="s">
+        <v>1128</v>
+      </c>
+      <c r="D153" s="46" t="s">
+        <v>1127</v>
+      </c>
+      <c r="F153" s="2" t="s">
+        <v>687</v>
+      </c>
+      <c r="G153" t="s">
+        <v>1044</v>
+      </c>
+      <c r="H153" t="s">
         <v>881</v>
       </c>
     </row>
@@ -10393,11 +10442,11 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:AJ152"/>
+  <dimension ref="A1:AJ153"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane activePane="bottomLeft" state="frozen" topLeftCell="A134" ySplit="1"/>
-      <selection activeCell="D161" pane="bottomLeft" sqref="D161"/>
+      <selection activeCell="C159" pane="bottomLeft" sqref="C159"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr customHeight="1" defaultColWidth="14.42578125" defaultRowHeight="15.75"/>
@@ -19372,121 +19421,180 @@
         <v>1044</v>
       </c>
     </row>
-    <row r="151">
-      <c r="A151" t="s">
+    <row customFormat="1" ht="14.25" r="151" s="24" spans="1:21">
+      <c r="A151" s="24" t="s">
         <v>1108</v>
       </c>
-      <c r="B151" t="s">
-        <v>1120</v>
-      </c>
-      <c r="C151" t="s">
+      <c r="B151" s="24" t="s">
+        <v>7</v>
+      </c>
+      <c r="C151" s="24" t="s">
         <v>1109</v>
       </c>
-      <c r="D151" t="s">
+      <c r="D151" s="24" t="s">
         <v>84</v>
       </c>
-      <c r="E151" t="s">
+      <c r="E151" s="24" t="s">
         <v>78</v>
       </c>
-      <c r="F151" t="s">
+      <c r="F151" s="24" t="s">
         <v>79</v>
       </c>
-      <c r="G151" t="s">
+      <c r="G151" s="24" t="s">
         <v>85</v>
       </c>
-      <c r="H151" t="s">
+      <c r="H151" s="24" t="s">
+        <v>1110</v>
+      </c>
+      <c r="I151" s="24" t="s">
+        <v>198</v>
+      </c>
+      <c r="K151" s="24" t="s">
+        <v>199</v>
+      </c>
+      <c r="L151" s="24" t="s">
         <v>1111</v>
       </c>
-      <c r="I151" t="s">
+      <c r="M151" s="24" t="s">
+        <v>201</v>
+      </c>
+      <c r="N151" s="24" t="s">
+        <v>202</v>
+      </c>
+      <c r="P151" s="24" t="s">
+        <v>203</v>
+      </c>
+      <c r="Q151" s="24" t="s">
+        <v>204</v>
+      </c>
+      <c r="R151" s="24" t="s">
+        <v>1109</v>
+      </c>
+      <c r="S151" s="24" t="s">
+        <v>1112</v>
+      </c>
+      <c r="T151" s="24" t="s">
+        <v>1046</v>
+      </c>
+      <c r="U151" s="24" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row customFormat="1" ht="14.25" r="152" s="24" spans="1:21">
+      <c r="A152" s="24" t="s">
+        <v>1113</v>
+      </c>
+      <c r="B152" s="24" t="s">
+        <v>7</v>
+      </c>
+      <c r="C152" s="24" t="s">
+        <v>1114</v>
+      </c>
+      <c r="D152" s="24" t="s">
+        <v>77</v>
+      </c>
+      <c r="E152" s="24" t="s">
+        <v>78</v>
+      </c>
+      <c r="F152" s="24" t="s">
+        <v>684</v>
+      </c>
+      <c r="G152" s="24" t="s">
+        <v>1115</v>
+      </c>
+      <c r="H152" s="24" t="s">
+        <v>199</v>
+      </c>
+      <c r="I152" s="24" t="s">
         <v>198</v>
       </c>
-      <c r="K151" t="s">
+      <c r="K152" s="24" t="s">
+        <v>1116</v>
+      </c>
+      <c r="L152" s="24" t="s">
+        <v>1117</v>
+      </c>
+      <c r="M152" s="24" t="s">
+        <v>204</v>
+      </c>
+      <c r="N152" s="24" t="s">
+        <v>266</v>
+      </c>
+      <c r="P152" s="24" t="s">
+        <v>252</v>
+      </c>
+      <c r="Q152" s="24" t="s">
+        <v>204</v>
+      </c>
+      <c r="R152" s="24" t="s">
+        <v>1114</v>
+      </c>
+      <c r="S152" s="24" t="s">
+        <v>1118</v>
+      </c>
+      <c r="T152" s="24" t="s">
+        <v>687</v>
+      </c>
+      <c r="U152" s="24" t="s">
+        <v>1044</v>
+      </c>
+    </row>
+    <row r="153">
+      <c r="A153" t="s">
+        <v>1122</v>
+      </c>
+      <c r="B153" t="s">
+        <v>1127</v>
+      </c>
+      <c r="C153" t="s">
+        <v>1123</v>
+      </c>
+      <c r="D153" t="s">
+        <v>77</v>
+      </c>
+      <c r="E153" t="s">
+        <v>78</v>
+      </c>
+      <c r="F153" t="s">
+        <v>906</v>
+      </c>
+      <c r="G153" t="s">
+        <v>1125</v>
+      </c>
+      <c r="H153" t="s">
         <v>199</v>
       </c>
-      <c r="L151" t="s">
-        <v>1112</v>
-      </c>
-      <c r="M151" t="s">
+      <c r="I153" t="s">
+        <v>198</v>
+      </c>
+      <c r="K153" t="s">
+        <v>199</v>
+      </c>
+      <c r="L153" t="s">
+        <v>237</v>
+      </c>
+      <c r="M153" t="s">
+        <v>202</v>
+      </c>
+      <c r="N153" t="s">
+        <v>204</v>
+      </c>
+      <c r="P153" t="s">
         <v>201</v>
       </c>
-      <c r="N151" t="s">
-        <v>202</v>
-      </c>
-      <c r="P151" t="s">
-        <v>203</v>
-      </c>
-      <c r="Q151" t="s">
+      <c r="Q153" t="s">
         <v>204</v>
       </c>
-      <c r="R151" t="s">
-        <v>1109</v>
-      </c>
-      <c r="S151" t="s">
-        <v>1113</v>
-      </c>
-      <c r="T151" t="s">
-        <v>1046</v>
-      </c>
-      <c r="U151" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="152">
-      <c r="A152" t="s">
-        <v>1114</v>
-      </c>
-      <c r="B152" t="s">
-        <v>1120</v>
-      </c>
-      <c r="C152" t="s">
-        <v>1115</v>
-      </c>
-      <c r="D152" t="s">
-        <v>77</v>
-      </c>
-      <c r="E152" t="s">
-        <v>78</v>
-      </c>
-      <c r="F152" t="s">
-        <v>684</v>
-      </c>
-      <c r="G152" t="s">
-        <v>1116</v>
-      </c>
-      <c r="H152" t="s">
-        <v>199</v>
-      </c>
-      <c r="I152" t="s">
-        <v>198</v>
-      </c>
-      <c r="K152" t="s">
-        <v>1117</v>
-      </c>
-      <c r="L152" t="s">
-        <v>1118</v>
-      </c>
-      <c r="M152" t="s">
-        <v>204</v>
-      </c>
-      <c r="N152" t="s">
-        <v>266</v>
-      </c>
-      <c r="P152" t="s">
-        <v>252</v>
-      </c>
-      <c r="Q152" t="s">
-        <v>204</v>
-      </c>
-      <c r="R152" t="s">
-        <v>1115</v>
-      </c>
-      <c r="S152" t="s">
-        <v>1119</v>
-      </c>
-      <c r="T152" t="s">
+      <c r="R153" t="s">
+        <v>1123</v>
+      </c>
+      <c r="S153" t="s">
+        <v>1126</v>
+      </c>
+      <c r="T153" t="s">
         <v>687</v>
       </c>
-      <c r="U152" t="s">
+      <c r="U153" t="s">
         <v>1044</v>
       </c>
     </row>
@@ -19495,7 +19603,7 @@
   <customSheetViews>
     <customSheetView filter="1" guid="{A7754112-A52F-4ABC-8778-92F04773E53C}" showAutoFilter="1">
       <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
-      <autoFilter ref="A1:AD33" xr:uid="{50AC9568-35DE-4B86-9AD0-75B55D6D263E}">
+      <autoFilter ref="A1:AD33" xr:uid="{37B0B7DD-C8E3-4D3D-97C5-3A0B3A6F3541}">
         <filterColumn colId="5">
           <filters blank="1">
             <filter val="Strathnairn"/>
@@ -19505,7 +19613,7 @@
     </customSheetView>
     <customSheetView filter="1" guid="{C25CEB9E-BEC1-4982-90C4-50C84EE1B82A}" showAutoFilter="1">
       <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
-      <autoFilter ref="A1:AD33" xr:uid="{CC0452E8-80BB-42E2-9DA0-FBE75D4E7806}"/>
+      <autoFilter ref="A1:AD33" xr:uid="{D44D412F-5057-48D7-A789-A8DDFB1D2F9E}"/>
     </customSheetView>
   </customSheetViews>
   <conditionalFormatting sqref="A1:AI1">

</xml_diff>

<commit_message>
Checked existing listings 27/09/2021
</commit_message>
<xml_diff>
--- a/src/main/resources/InputTestdata/Listing details.xlsx
+++ b/src/main/resources/InputTestdata/Listing details.xlsx
@@ -1,39 +1,39 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" mc:Ignorable="x15 xr xr6 xr10 xr2">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24326"/>
   <workbookPr/>
-  <mc:AlternateContent>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Athavan\git\777Homes-2\777Homes-business\src\main\resources\InputTestdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr documentId="13_ncr:1_{008756E1-6CFA-4503-B13A-646A05FBAFEE}" revIDLastSave="0" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{431F0D31-8EFC-4FC3-99E1-9F37481A0E3C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView windowHeight="15840" windowWidth="29040" xWindow="-120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}" yWindow="-120"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Backlog" r:id="rId1" sheetId="1"/>
-    <sheet name="Listing" r:id="rId2" sheetId="2"/>
-    <sheet name="Tobe-executed" r:id="rId3" sheetId="3"/>
-    <sheet name="Agency login" r:id="rId4" sheetId="4"/>
+    <sheet name="Backlog" sheetId="1" r:id="rId1"/>
+    <sheet name="Listing" sheetId="2" r:id="rId2"/>
+    <sheet name="Tobe-executed" sheetId="3" r:id="rId3"/>
+    <sheet name="Agency login" sheetId="4" r:id="rId4"/>
   </sheets>
   <definedNames>
-    <definedName hidden="1" localSheetId="0" name="_xlnm._FilterDatabase">Backlog!$A$1:$AB$52</definedName>
-    <definedName hidden="1" localSheetId="1" name="_xlnm._FilterDatabase">Listing!$E$1:$E$145</definedName>
-    <definedName hidden="1" localSheetId="1" name="Z_A7754112_A52F_4ABC_8778_92F04773E53C_.wvu.FilterData">Listing!$A$1:$AE$32</definedName>
-    <definedName hidden="1" localSheetId="1" name="Z_C25CEB9E_BEC1_4982_90C4_50C84EE1B82A_.wvu.FilterData">Listing!$A$1:$AE$32</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Backlog!$A$1:$AB$52</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Listing!$E$1:$E$145</definedName>
+    <definedName name="Z_A7754112_A52F_4ABC_8778_92F04773E53C_.wvu.FilterData" localSheetId="1" hidden="1">Listing!$A$1:$AE$32</definedName>
+    <definedName name="Z_C25CEB9E_BEC1_4982_90C4_50C84EE1B82A_.wvu.FilterData" localSheetId="1" hidden="1">Listing!$A$1:$AE$32</definedName>
   </definedNames>
   <calcPr calcId="181029"/>
   <customWorkbookViews>
-    <customWorkbookView activeSheetId="0" guid="{A7754112-A52F-4ABC-8778-92F04773E53C}" maximized="1" name="Filter 1" windowHeight="0" windowWidth="0"/>
-    <customWorkbookView activeSheetId="0" guid="{C25CEB9E-BEC1-4982-90C4-50C84EE1B82A}" maximized="1" name="Filter 2" windowHeight="0" windowWidth="0"/>
+    <customWorkbookView name="Filter 2" guid="{C25CEB9E-BEC1-4982-90C4-50C84EE1B82A}" maximized="1" windowWidth="0" windowHeight="0" activeSheetId="0"/>
+    <customWorkbookView name="Filter 1" guid="{A7754112-A52F-4ABC-8778-92F04773E53C}" maximized="1" windowWidth="0" windowHeight="0" activeSheetId="0"/>
   </customWorkbookViews>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3725" uniqueCount="1129">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3724" uniqueCount="1128">
   <si>
     <t>ID</t>
   </si>
@@ -5511,13 +5511,16 @@
     <t>https://www.allhomes.com.au/unit-5-92-casey-crescent-calwell-act-2905</t>
   </si>
   <si>
+    <t>https://www.777homes.com.au/?post_type=property&amp;p=8946&amp;preview=true</t>
+  </si>
+  <si>
+    <t>TO BE UPDATED</t>
+  </si>
+  <si>
     <t>152</t>
   </si>
   <si>
     <t>5/92 Casey Crescent, Calwell ACT 2905</t>
-  </si>
-  <si>
-    <t>NEW</t>
   </si>
   <si>
     <t>Calwell</t>
@@ -5539,18 +5542,11 @@
 - Close to Calwell Shopping Centre, sport fields and eateries
 - CCTV Camera, near new Bamboo flooring, fresh paint throughout</t>
   </si>
-  <si>
-    <t>Draft</t>
-  </si>
-  <si>
-    <t>https://www.777homes.com.au/?post_type=property&amp;p=8946&amp;preview=true</t>
-  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="0"/>
   <fonts count="28">
     <font>
       <sz val="10"/>
@@ -5711,7 +5707,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="12">
+  <fills count="11">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -5766,13 +5762,9 @@
       </patternFill>
     </fill>
     <fill>
-      <patternFill patternType="none">
-        <bgColor indexed="2"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="mediumGray">
-        <bgColor indexed="2"/>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC00000"/>
+        <bgColor rgb="FFD9EAD3"/>
       </patternFill>
     </fill>
   </fills>
@@ -5786,112 +5778,114 @@
     </border>
   </borders>
   <cellStyleXfs count="2">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
-    <xf applyAlignment="0" applyBorder="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="0" fontId="25" numFmtId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="48">
-    <xf applyAlignment="1" applyFont="1" borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyAlignment="1" applyFill="1" applyFont="1" borderId="0" fillId="3" fontId="1" numFmtId="0" xfId="0">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf applyAlignment="1" applyFill="1" applyFont="1" borderId="0" fillId="2" fontId="2" numFmtId="0" xfId="0">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf applyAlignment="1" applyFill="1" applyFont="1" borderId="0" fillId="2" fontId="3" numFmtId="0" xfId="0"/>
-    <xf applyAlignment="1" applyFill="1" applyFont="1" borderId="0" fillId="2" fontId="4" numFmtId="0" xfId="0">
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf applyAlignment="1" applyFill="1" applyFont="1" borderId="0" fillId="2" fontId="6" numFmtId="0" xfId="0">
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf applyFill="1" applyFont="1" borderId="0" fillId="2" fontId="4" numFmtId="0" xfId="0"/>
-    <xf applyAlignment="1" applyFill="1" applyFont="1" borderId="0" fillId="2" fontId="7" numFmtId="0" xfId="0"/>
-    <xf applyAlignment="1" applyFill="1" applyFont="1" borderId="0" fillId="2" fontId="8" numFmtId="0" xfId="0"/>
-    <xf applyAlignment="1" applyFill="1" applyFont="1" borderId="0" fillId="2" fontId="5" numFmtId="0" xfId="0">
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf applyAlignment="1" applyFill="1" applyFont="1" borderId="0" fillId="4" fontId="4" numFmtId="0" xfId="0">
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf applyAlignment="1" applyFill="1" applyFont="1" borderId="0" fillId="5" fontId="4" numFmtId="0" xfId="0">
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf applyAlignment="1" applyFill="1" applyFont="1" borderId="0" fillId="2" fontId="9" numFmtId="0" xfId="0">
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf applyAlignment="1" applyFill="1" applyFont="1" borderId="0" fillId="2" fontId="10" numFmtId="0" xfId="0"/>
-    <xf applyAlignment="1" applyFill="1" applyFont="1" borderId="0" fillId="2" fontId="11" numFmtId="0" xfId="0"/>
-    <xf applyAlignment="1" applyFill="1" applyFont="1" borderId="0" fillId="2" fontId="4" numFmtId="0" xfId="0">
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="11" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf applyAlignment="1" applyFill="1" applyFont="1" borderId="0" fillId="2" fontId="12" numFmtId="0" xfId="0"/>
-    <xf applyAlignment="1" applyFill="1" applyFont="1" borderId="0" fillId="2" fontId="13" numFmtId="0" xfId="0"/>
-    <xf applyAlignment="1" applyFill="1" applyFont="1" borderId="0" fillId="2" fontId="14" numFmtId="0" xfId="0"/>
-    <xf applyAlignment="1" applyFill="1" applyFont="1" borderId="0" fillId="2" fontId="15" numFmtId="0" xfId="0"/>
-    <xf applyAlignment="1" applyFill="1" applyFont="1" borderId="0" fillId="2" fontId="16" numFmtId="0" xfId="0"/>
-    <xf applyAlignment="1" applyFill="1" applyFont="1" borderId="0" fillId="2" fontId="17" numFmtId="0" xfId="0"/>
-    <xf applyAlignment="1" applyFill="1" applyFont="1" borderId="0" fillId="3" fontId="1" numFmtId="0" xfId="0">
+    <xf numFmtId="0" fontId="12" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="13" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="14" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="15" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="16" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="17" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf applyFill="1" applyFont="1" borderId="0" fillId="3" fontId="7" numFmtId="0" xfId="0"/>
-    <xf applyAlignment="1" applyFill="1" applyFont="1" borderId="0" fillId="2" fontId="18" numFmtId="0" xfId="0">
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="18" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf applyAlignment="1" applyFill="1" applyFont="1" borderId="0" fillId="2" fontId="19" numFmtId="0" xfId="0">
+    <xf numFmtId="0" fontId="19" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf applyAlignment="1" applyFill="1" applyFont="1" borderId="0" fillId="2" fontId="20" numFmtId="0" xfId="0">
+    <xf numFmtId="0" fontId="20" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf applyAlignment="1" applyFill="1" applyFont="1" borderId="0" fillId="2" fontId="18" numFmtId="0" xfId="0">
+    <xf numFmtId="0" fontId="18" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf applyAlignment="1" applyFill="1" applyFont="1" borderId="0" fillId="2" fontId="21" numFmtId="0" xfId="0">
+    <xf numFmtId="0" fontId="21" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf applyAlignment="1" applyFont="1" borderId="0" fillId="0" fontId="7" numFmtId="0" xfId="0">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf applyAlignment="1" applyFill="1" applyFont="1" borderId="0" fillId="3" fontId="17" numFmtId="0" xfId="0"/>
-    <xf applyAlignment="1" applyFill="1" applyFont="1" borderId="0" fillId="3" fontId="12" numFmtId="0" xfId="0"/>
-    <xf applyAlignment="1" applyFill="1" applyFont="1" borderId="0" fillId="3" fontId="22" numFmtId="0" xfId="0">
+    <xf numFmtId="0" fontId="17" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="12" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="22" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf applyAlignment="1" applyFill="1" applyFont="1" borderId="0" fillId="3" fontId="23" numFmtId="0" xfId="0"/>
-    <xf applyAlignment="1" applyFont="1" borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0"/>
-    <xf applyAlignment="1" applyFill="1" applyFont="1" borderId="0" fillId="3" fontId="24" numFmtId="0" xfId="0">
+    <xf numFmtId="0" fontId="23" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="24" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf applyAlignment="1" applyFill="1" applyFont="1" borderId="0" fillId="3" fontId="1" numFmtId="0" xfId="0">
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf applyAlignment="1" applyFont="1" borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf applyAlignment="1" applyFill="1" borderId="0" fillId="2" fontId="25" numFmtId="0" xfId="1">
+    <xf numFmtId="0" fontId="25" fillId="2" borderId="0" xfId="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf applyAlignment="1" applyFill="1" applyFont="1" borderId="0" fillId="6" fontId="2" numFmtId="0" xfId="0">
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf applyAlignment="1" applyFill="1" applyFont="1" borderId="0" fillId="7" fontId="5" numFmtId="0" xfId="0">
+    <xf numFmtId="0" fontId="5" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf applyAlignment="1" borderId="0" fillId="0" fontId="25" numFmtId="0" xfId="1"/>
-    <xf applyAlignment="1" applyFill="1" borderId="0" fillId="2" fontId="25" numFmtId="0" xfId="1"/>
-    <xf applyAlignment="1" applyFill="1" applyFont="1" borderId="0" fillId="8" fontId="18" numFmtId="0" xfId="0">
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" xfId="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="25" fillId="2" borderId="0" xfId="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="18" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf applyAlignment="1" applyFill="1" applyFont="1" borderId="0" fillId="2" fontId="26" numFmtId="0" xfId="0">
+    <xf numFmtId="0" fontId="26" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf applyAlignment="1" applyFont="1" borderId="0" fillId="0" fontId="27" numFmtId="0" xfId="0"/>
-    <xf applyFill="1" borderId="0" fillId="9" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyFill="true" borderId="0" fillId="11" fontId="0" numFmtId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="18" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
-    <cellStyle builtinId="8" name="Hyperlink" xfId="1"/>
-    <cellStyle builtinId="0" name="Normal" xfId="0"/>
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="2">
     <dxf>
@@ -5911,7 +5905,7 @@
       </fill>
     </dxf>
   </dxfs>
-  <tableStyles count="0" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium2"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -6035,21 +6029,21 @@
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
-        <a:ln algn="ctr" cap="flat" cmpd="sng" w="6350">
+        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
           <a:miter lim="800000"/>
         </a:ln>
-        <a:ln algn="ctr" cap="flat" cmpd="sng" w="12700">
+        <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
           <a:miter lim="800000"/>
         </a:ln>
-        <a:ln algn="ctr" cap="flat" cmpd="sng" w="19050">
+        <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
@@ -6066,7 +6060,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw algn="ctr" blurRad="57150" dir="5400000" dist="19050" rotWithShape="0">
+            <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="63000"/>
               </a:srgbClr>
@@ -6120,32 +6114,32 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:AC153"/>
+  <dimension ref="A1:AB153"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane activePane="bottomLeft" state="frozen" topLeftCell="A131" ySplit="1"/>
-      <selection activeCell="E158" pane="bottomLeft" sqref="E158"/>
+    <sheetView workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B23" sqref="B23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="14.42578125" defaultRowHeight="15.75"/>
+  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="9.140625" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" width="74.85546875" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="75.0" collapsed="true"/>
-    <col min="4" max="4" customWidth="true" width="14.5703125" collapsed="true"/>
-    <col min="6" max="6" bestFit="true" customWidth="true" style="37" width="22.140625" collapsed="true"/>
-    <col min="7" max="7" customWidth="true" width="21.85546875" collapsed="true"/>
-    <col min="8" max="8" customWidth="true" width="56.85546875" collapsed="true"/>
-    <col min="9" max="9" customWidth="true" width="10.85546875" collapsed="true"/>
-    <col min="10" max="10" customWidth="true" width="17.85546875" collapsed="true"/>
-    <col min="11" max="11" customWidth="true" width="22.5703125" collapsed="true"/>
+    <col min="1" max="1" width="9.140625" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="74.85546875" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="75" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="14.5703125" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="22.140625" style="37" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="21.85546875" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="56.85546875" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="10.85546875" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="17.85546875" customWidth="1" collapsed="1"/>
+    <col min="11" max="11" width="22.5703125" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row ht="15" r="1" spans="1:28">
+    <row r="1" spans="1:28" ht="15">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -6172,7 +6166,7 @@
       </c>
       <c r="J1" s="1"/>
     </row>
-    <row customHeight="1" ht="15.75" r="2" spans="1:28">
+    <row r="2" spans="1:28" ht="15.75" customHeight="1">
       <c r="A2" s="2">
         <v>1</v>
       </c>
@@ -6218,7 +6212,7 @@
       <c r="AA2" s="6"/>
       <c r="AB2" s="6"/>
     </row>
-    <row ht="14.25" r="3" spans="1:28">
+    <row r="3" spans="1:28" ht="14.25">
       <c r="A3" s="2">
         <v>2</v>
       </c>
@@ -6264,7 +6258,7 @@
       <c r="AA3" s="6"/>
       <c r="AB3" s="6"/>
     </row>
-    <row customHeight="1" ht="15.75" r="4" spans="1:28">
+    <row r="4" spans="1:28" ht="15.75" customHeight="1">
       <c r="A4" s="9">
         <v>3</v>
       </c>
@@ -6310,7 +6304,7 @@
       <c r="AA4" s="6"/>
       <c r="AB4" s="6"/>
     </row>
-    <row ht="14.25" r="5" spans="1:28">
+    <row r="5" spans="1:28" ht="14.25">
       <c r="A5" s="9">
         <v>4</v>
       </c>
@@ -6354,7 +6348,7 @@
       <c r="AA5" s="6"/>
       <c r="AB5" s="6"/>
     </row>
-    <row ht="14.25" r="6" spans="1:28">
+    <row r="6" spans="1:28" ht="14.25">
       <c r="A6" s="9">
         <v>5</v>
       </c>
@@ -6398,7 +6392,7 @@
       <c r="AA6" s="9"/>
       <c r="AB6" s="9"/>
     </row>
-    <row ht="14.25" r="7" spans="1:28">
+    <row r="7" spans="1:28" ht="14.25">
       <c r="A7" s="9">
         <v>6</v>
       </c>
@@ -6442,7 +6436,7 @@
       <c r="AA7" s="6"/>
       <c r="AB7" s="6"/>
     </row>
-    <row ht="14.25" r="8" spans="1:28">
+    <row r="8" spans="1:28" ht="14.25">
       <c r="A8" s="9">
         <v>7</v>
       </c>
@@ -6486,7 +6480,7 @@
       <c r="AA8" s="6"/>
       <c r="AB8" s="6"/>
     </row>
-    <row ht="14.25" r="9" spans="1:28">
+    <row r="9" spans="1:28" ht="14.25">
       <c r="A9" s="9">
         <v>8</v>
       </c>
@@ -6528,7 +6522,7 @@
       <c r="AA9" s="6"/>
       <c r="AB9" s="6"/>
     </row>
-    <row ht="14.25" r="10" spans="1:28">
+    <row r="10" spans="1:28" ht="14.25">
       <c r="A10" s="9">
         <v>9</v>
       </c>
@@ -6570,7 +6564,7 @@
       <c r="AA10" s="6"/>
       <c r="AB10" s="6"/>
     </row>
-    <row ht="14.25" r="11" spans="1:28">
+    <row r="11" spans="1:28" ht="14.25">
       <c r="A11" s="9">
         <v>10</v>
       </c>
@@ -6614,7 +6608,7 @@
       <c r="AA11" s="6"/>
       <c r="AB11" s="6"/>
     </row>
-    <row ht="14.25" r="12" spans="1:28">
+    <row r="12" spans="1:28" ht="14.25">
       <c r="A12" s="9">
         <v>11</v>
       </c>
@@ -6656,7 +6650,7 @@
       <c r="AA12" s="6"/>
       <c r="AB12" s="6"/>
     </row>
-    <row ht="14.25" r="13" spans="1:28">
+    <row r="13" spans="1:28" ht="14.25">
       <c r="A13" s="9">
         <v>12</v>
       </c>
@@ -6698,7 +6692,7 @@
       <c r="AA13" s="6"/>
       <c r="AB13" s="6"/>
     </row>
-    <row ht="14.25" r="14" spans="1:28">
+    <row r="14" spans="1:28" ht="14.25">
       <c r="A14" s="9">
         <v>13</v>
       </c>
@@ -6740,7 +6734,7 @@
       <c r="AA14" s="6"/>
       <c r="AB14" s="6"/>
     </row>
-    <row ht="14.25" r="15" spans="1:28">
+    <row r="15" spans="1:28" ht="14.25">
       <c r="A15" s="9">
         <v>14</v>
       </c>
@@ -6784,7 +6778,7 @@
       <c r="AA15" s="6"/>
       <c r="AB15" s="6"/>
     </row>
-    <row ht="14.25" r="16" spans="1:28">
+    <row r="16" spans="1:28" ht="14.25">
       <c r="A16" s="9">
         <v>15</v>
       </c>
@@ -6826,7 +6820,7 @@
       <c r="AA16" s="6"/>
       <c r="AB16" s="6"/>
     </row>
-    <row ht="14.25" r="17" spans="1:28">
+    <row r="17" spans="1:28" ht="14.25">
       <c r="A17" s="9">
         <v>16</v>
       </c>
@@ -6870,7 +6864,7 @@
       <c r="AA17" s="6"/>
       <c r="AB17" s="6"/>
     </row>
-    <row ht="14.25" r="18" spans="1:28">
+    <row r="18" spans="1:28" ht="14.25">
       <c r="A18" s="9">
         <v>17</v>
       </c>
@@ -6912,7 +6906,7 @@
       <c r="AA18" s="6"/>
       <c r="AB18" s="6"/>
     </row>
-    <row ht="14.25" r="19" spans="1:28">
+    <row r="19" spans="1:28" ht="14.25">
       <c r="A19" s="9">
         <v>18</v>
       </c>
@@ -6956,7 +6950,7 @@
       <c r="AA19" s="6"/>
       <c r="AB19" s="6"/>
     </row>
-    <row ht="14.25" r="20" spans="1:28">
+    <row r="20" spans="1:28" ht="14.25">
       <c r="A20" s="9">
         <v>19</v>
       </c>
@@ -7000,7 +6994,7 @@
       <c r="AA20" s="6"/>
       <c r="AB20" s="6"/>
     </row>
-    <row ht="14.25" r="21" spans="1:28">
+    <row r="21" spans="1:28" ht="14.25">
       <c r="A21" s="9">
         <v>20</v>
       </c>
@@ -7044,7 +7038,7 @@
       <c r="AA21" s="6"/>
       <c r="AB21" s="6"/>
     </row>
-    <row ht="14.25" r="22" spans="1:28">
+    <row r="22" spans="1:28" ht="14.25">
       <c r="A22" s="9">
         <v>21</v>
       </c>
@@ -7086,7 +7080,7 @@
       <c r="AA22" s="6"/>
       <c r="AB22" s="6"/>
     </row>
-    <row ht="14.25" r="23" spans="1:28">
+    <row r="23" spans="1:28" ht="14.25">
       <c r="A23" s="9">
         <v>22</v>
       </c>
@@ -7130,7 +7124,7 @@
       <c r="AA23" s="6"/>
       <c r="AB23" s="6"/>
     </row>
-    <row ht="14.25" r="24" spans="1:28">
+    <row r="24" spans="1:28" ht="14.25">
       <c r="A24" s="9">
         <v>23</v>
       </c>
@@ -7172,7 +7166,7 @@
       <c r="AA24" s="6"/>
       <c r="AB24" s="6"/>
     </row>
-    <row ht="14.25" r="25" spans="1:28">
+    <row r="25" spans="1:28" ht="14.25">
       <c r="A25" s="9">
         <v>24</v>
       </c>
@@ -7214,7 +7208,7 @@
       <c r="AA25" s="6"/>
       <c r="AB25" s="6"/>
     </row>
-    <row ht="14.25" r="26" spans="1:28">
+    <row r="26" spans="1:28" ht="14.25">
       <c r="A26" s="9">
         <v>25</v>
       </c>
@@ -7258,7 +7252,7 @@
       <c r="AA26" s="6"/>
       <c r="AB26" s="6"/>
     </row>
-    <row ht="14.25" r="27" spans="1:28">
+    <row r="27" spans="1:28" ht="14.25">
       <c r="A27" s="9">
         <v>26</v>
       </c>
@@ -7302,7 +7296,7 @@
       <c r="AA27" s="6"/>
       <c r="AB27" s="6"/>
     </row>
-    <row ht="14.25" r="28" spans="1:28">
+    <row r="28" spans="1:28" ht="14.25">
       <c r="A28" s="9">
         <v>27</v>
       </c>
@@ -7344,7 +7338,7 @@
       <c r="AA28" s="6"/>
       <c r="AB28" s="6"/>
     </row>
-    <row ht="14.25" r="29" spans="1:28">
+    <row r="29" spans="1:28" ht="14.25">
       <c r="A29" s="9">
         <v>28</v>
       </c>
@@ -7388,7 +7382,7 @@
       <c r="AA29" s="6"/>
       <c r="AB29" s="6"/>
     </row>
-    <row ht="14.25" r="30" spans="1:28">
+    <row r="30" spans="1:28" ht="14.25">
       <c r="A30" s="9">
         <v>29</v>
       </c>
@@ -7430,7 +7424,7 @@
       <c r="AA30" s="6"/>
       <c r="AB30" s="6"/>
     </row>
-    <row ht="14.25" r="31" spans="1:28">
+    <row r="31" spans="1:28" ht="14.25">
       <c r="A31" s="4">
         <v>30</v>
       </c>
@@ -7474,7 +7468,7 @@
       <c r="AA31" s="6"/>
       <c r="AB31" s="6"/>
     </row>
-    <row ht="14.25" r="32" spans="1:28">
+    <row r="32" spans="1:28" ht="14.25">
       <c r="A32" s="4">
         <v>31</v>
       </c>
@@ -7516,7 +7510,7 @@
       <c r="AA32" s="6"/>
       <c r="AB32" s="6"/>
     </row>
-    <row customFormat="1" ht="14.25" r="33" s="4" spans="1:8">
+    <row r="33" spans="1:8" s="4" customFormat="1" ht="14.25">
       <c r="A33" s="4">
         <v>32</v>
       </c>
@@ -7539,7 +7533,7 @@
         <v>427</v>
       </c>
     </row>
-    <row customFormat="1" ht="14.25" r="34" s="4" spans="1:8">
+    <row r="34" spans="1:8" s="4" customFormat="1" ht="14.25">
       <c r="A34" s="4">
         <v>33</v>
       </c>
@@ -7559,7 +7553,7 @@
         <v>427</v>
       </c>
     </row>
-    <row customFormat="1" ht="14.25" r="35" s="4" spans="1:8">
+    <row r="35" spans="1:8" s="4" customFormat="1" ht="14.25">
       <c r="A35" s="4">
         <v>34</v>
       </c>
@@ -7579,7 +7573,7 @@
         <v>427</v>
       </c>
     </row>
-    <row customFormat="1" ht="14.25" r="36" s="4" spans="1:8">
+    <row r="36" spans="1:8" s="4" customFormat="1" ht="14.25">
       <c r="A36" s="4">
         <v>35</v>
       </c>
@@ -7599,7 +7593,7 @@
         <v>427</v>
       </c>
     </row>
-    <row customFormat="1" ht="14.25" r="37" s="4" spans="1:8">
+    <row r="37" spans="1:8" s="4" customFormat="1" ht="14.25">
       <c r="A37" s="4">
         <v>36</v>
       </c>
@@ -7619,7 +7613,7 @@
         <v>427</v>
       </c>
     </row>
-    <row customFormat="1" ht="14.25" r="38" s="4" spans="1:8">
+    <row r="38" spans="1:8" s="4" customFormat="1" ht="14.25">
       <c r="A38" s="4">
         <v>37</v>
       </c>
@@ -7642,7 +7636,7 @@
         <v>427</v>
       </c>
     </row>
-    <row customFormat="1" ht="14.25" r="39" s="4" spans="1:8">
+    <row r="39" spans="1:8" s="4" customFormat="1" ht="14.25">
       <c r="A39" s="4">
         <v>38</v>
       </c>
@@ -7665,7 +7659,7 @@
         <v>427</v>
       </c>
     </row>
-    <row customFormat="1" ht="14.25" r="40" s="4" spans="1:8">
+    <row r="40" spans="1:8" s="4" customFormat="1" ht="14.25">
       <c r="A40" s="4">
         <v>39</v>
       </c>
@@ -7688,7 +7682,7 @@
         <v>427</v>
       </c>
     </row>
-    <row customFormat="1" ht="14.25" r="41" s="4" spans="1:8">
+    <row r="41" spans="1:8" s="4" customFormat="1" ht="14.25">
       <c r="A41" s="4">
         <v>40</v>
       </c>
@@ -7708,7 +7702,7 @@
         <v>427</v>
       </c>
     </row>
-    <row customFormat="1" ht="14.25" r="42" s="4" spans="1:8">
+    <row r="42" spans="1:8" s="4" customFormat="1" ht="14.25">
       <c r="A42" s="4">
         <v>41</v>
       </c>
@@ -7731,7 +7725,7 @@
         <v>427</v>
       </c>
     </row>
-    <row customFormat="1" ht="14.25" r="43" s="4" spans="1:8">
+    <row r="43" spans="1:8" s="4" customFormat="1" ht="14.25">
       <c r="A43" s="4">
         <v>42</v>
       </c>
@@ -7751,7 +7745,7 @@
         <v>427</v>
       </c>
     </row>
-    <row customFormat="1" ht="14.25" r="44" s="4" spans="1:8">
+    <row r="44" spans="1:8" s="4" customFormat="1" ht="14.25">
       <c r="A44" s="4">
         <v>43</v>
       </c>
@@ -7771,7 +7765,7 @@
         <v>427</v>
       </c>
     </row>
-    <row customFormat="1" ht="14.25" r="45" s="4" spans="1:8">
+    <row r="45" spans="1:8" s="4" customFormat="1" ht="14.25">
       <c r="A45" s="4">
         <v>44</v>
       </c>
@@ -7794,7 +7788,7 @@
         <v>38</v>
       </c>
     </row>
-    <row customFormat="1" ht="14.25" r="46" s="4" spans="1:8">
+    <row r="46" spans="1:8" s="4" customFormat="1" ht="14.25">
       <c r="A46" s="4">
         <v>45</v>
       </c>
@@ -7814,7 +7808,7 @@
         <v>38</v>
       </c>
     </row>
-    <row customFormat="1" ht="14.25" r="47" s="4" spans="1:8">
+    <row r="47" spans="1:8" s="4" customFormat="1" ht="14.25">
       <c r="A47" s="4">
         <v>46</v>
       </c>
@@ -7834,7 +7828,7 @@
         <v>38</v>
       </c>
     </row>
-    <row customFormat="1" ht="12.75" r="48" s="4" spans="1:8">
+    <row r="48" spans="1:8" s="4" customFormat="1" ht="12.75">
       <c r="A48" s="4">
         <v>47</v>
       </c>
@@ -7857,7 +7851,7 @@
         <v>428</v>
       </c>
     </row>
-    <row customFormat="1" ht="12.75" r="49" s="4" spans="1:8">
+    <row r="49" spans="1:8" s="4" customFormat="1" ht="12.75">
       <c r="A49" s="4">
         <v>48</v>
       </c>
@@ -7880,7 +7874,7 @@
         <v>428</v>
       </c>
     </row>
-    <row customFormat="1" ht="12.75" r="50" s="4" spans="1:8">
+    <row r="50" spans="1:8" s="4" customFormat="1" ht="12.75">
       <c r="A50" s="4">
         <v>49</v>
       </c>
@@ -7900,7 +7894,7 @@
         <v>428</v>
       </c>
     </row>
-    <row customFormat="1" ht="12.75" r="51" s="4" spans="1:8">
+    <row r="51" spans="1:8" s="4" customFormat="1" ht="12.75">
       <c r="A51" s="4">
         <v>50</v>
       </c>
@@ -7920,7 +7914,7 @@
         <v>428</v>
       </c>
     </row>
-    <row customFormat="1" ht="12.75" r="52" s="4" spans="1:8">
+    <row r="52" spans="1:8" s="4" customFormat="1" ht="12.75">
       <c r="A52" s="4">
         <v>51</v>
       </c>
@@ -7943,7 +7937,7 @@
         <v>428</v>
       </c>
     </row>
-    <row customFormat="1" customHeight="1" ht="15.75" r="53" s="4" spans="1:8">
+    <row r="53" spans="1:8" s="4" customFormat="1" ht="15.75" customHeight="1">
       <c r="A53" s="4">
         <v>52</v>
       </c>
@@ -7966,7 +7960,7 @@
         <v>323</v>
       </c>
     </row>
-    <row customFormat="1" ht="12.75" r="54" s="4" spans="1:8">
+    <row r="54" spans="1:8" s="4" customFormat="1" ht="12.75">
       <c r="A54" s="4">
         <v>53</v>
       </c>
@@ -7986,7 +7980,7 @@
         <v>323</v>
       </c>
     </row>
-    <row customFormat="1" ht="12.75" r="55" s="4" spans="1:8">
+    <row r="55" spans="1:8" s="4" customFormat="1" ht="12.75">
       <c r="A55" s="4">
         <v>54</v>
       </c>
@@ -8009,7 +8003,7 @@
         <v>323</v>
       </c>
     </row>
-    <row customFormat="1" ht="12.75" r="56" s="4" spans="1:8">
+    <row r="56" spans="1:8" s="4" customFormat="1" ht="12.75">
       <c r="A56" s="4">
         <v>55</v>
       </c>
@@ -8032,7 +8026,7 @@
         <v>323</v>
       </c>
     </row>
-    <row customFormat="1" ht="12.75" r="57" s="4" spans="1:8">
+    <row r="57" spans="1:8" s="4" customFormat="1" ht="12.75">
       <c r="A57" s="4">
         <v>56</v>
       </c>
@@ -8052,7 +8046,7 @@
         <v>323</v>
       </c>
     </row>
-    <row customFormat="1" ht="12.75" r="58" s="4" spans="1:8">
+    <row r="58" spans="1:8" s="4" customFormat="1" ht="12.75">
       <c r="A58" s="4">
         <v>57</v>
       </c>
@@ -8072,7 +8066,7 @@
         <v>323</v>
       </c>
     </row>
-    <row customFormat="1" ht="12.75" r="59" s="4" spans="1:8">
+    <row r="59" spans="1:8" s="4" customFormat="1" ht="12.75">
       <c r="A59" s="4">
         <v>58</v>
       </c>
@@ -8092,7 +8086,7 @@
         <v>323</v>
       </c>
     </row>
-    <row customFormat="1" ht="12.75" r="60" s="4" spans="1:8">
+    <row r="60" spans="1:8" s="4" customFormat="1" ht="12.75">
       <c r="A60" s="4">
         <v>59</v>
       </c>
@@ -8112,7 +8106,7 @@
         <v>323</v>
       </c>
     </row>
-    <row customFormat="1" ht="12.75" r="61" s="4" spans="1:8">
+    <row r="61" spans="1:8" s="4" customFormat="1" ht="12.75">
       <c r="A61" s="4">
         <v>60</v>
       </c>
@@ -8132,7 +8126,7 @@
         <v>323</v>
       </c>
     </row>
-    <row customFormat="1" ht="12.75" r="62" s="4" spans="1:8">
+    <row r="62" spans="1:8" s="4" customFormat="1" ht="12.75">
       <c r="A62" s="4">
         <v>61</v>
       </c>
@@ -8152,7 +8146,7 @@
         <v>427</v>
       </c>
     </row>
-    <row customFormat="1" ht="12.75" r="63" s="4" spans="1:8">
+    <row r="63" spans="1:8" s="4" customFormat="1" ht="12.75">
       <c r="A63" s="4">
         <v>62</v>
       </c>
@@ -8175,7 +8169,7 @@
         <v>427</v>
       </c>
     </row>
-    <row customFormat="1" ht="12.75" r="64" s="4" spans="1:8">
+    <row r="64" spans="1:8" s="4" customFormat="1" ht="12.75">
       <c r="A64" s="4">
         <v>63</v>
       </c>
@@ -8198,7 +8192,7 @@
         <v>427</v>
       </c>
     </row>
-    <row customFormat="1" ht="12.75" r="65" s="4" spans="1:8">
+    <row r="65" spans="1:8" s="4" customFormat="1" ht="12.75">
       <c r="A65" s="4">
         <v>64</v>
       </c>
@@ -8219,7 +8213,7 @@
         <v>427</v>
       </c>
     </row>
-    <row customFormat="1" ht="12.75" r="66" s="4" spans="1:8">
+    <row r="66" spans="1:8" s="4" customFormat="1" ht="12.75">
       <c r="A66" s="4">
         <v>65</v>
       </c>
@@ -8242,7 +8236,7 @@
         <v>38</v>
       </c>
     </row>
-    <row customFormat="1" ht="12.75" r="67" s="4" spans="1:8">
+    <row r="67" spans="1:8" s="4" customFormat="1" ht="12.75">
       <c r="A67" s="4">
         <v>66</v>
       </c>
@@ -8265,7 +8259,7 @@
         <v>428</v>
       </c>
     </row>
-    <row customFormat="1" ht="12.75" r="68" s="4" spans="1:8">
+    <row r="68" spans="1:8" s="4" customFormat="1" ht="12.75">
       <c r="A68" s="4">
         <v>67</v>
       </c>
@@ -8288,7 +8282,7 @@
         <v>427</v>
       </c>
     </row>
-    <row customFormat="1" ht="12.75" r="69" s="4" spans="1:8">
+    <row r="69" spans="1:8" s="4" customFormat="1" ht="12.75">
       <c r="A69" s="4">
         <v>68</v>
       </c>
@@ -8311,7 +8305,7 @@
         <v>427</v>
       </c>
     </row>
-    <row customFormat="1" ht="12.75" r="70" s="4" spans="1:8">
+    <row r="70" spans="1:8" s="4" customFormat="1" ht="12.75">
       <c r="A70" s="4">
         <v>69</v>
       </c>
@@ -8334,7 +8328,7 @@
         <v>427</v>
       </c>
     </row>
-    <row customFormat="1" ht="12.75" r="71" s="4" spans="1:8">
+    <row r="71" spans="1:8" s="4" customFormat="1" ht="12.75">
       <c r="A71" s="4">
         <v>70</v>
       </c>
@@ -8357,7 +8351,7 @@
         <v>427</v>
       </c>
     </row>
-    <row customFormat="1" ht="12.75" r="72" s="4" spans="1:8">
+    <row r="72" spans="1:8" s="4" customFormat="1" ht="12.75">
       <c r="A72" s="4">
         <v>71</v>
       </c>
@@ -8380,7 +8374,7 @@
         <v>427</v>
       </c>
     </row>
-    <row ht="12.75" r="73" spans="1:8">
+    <row r="73" spans="1:8" ht="12.75">
       <c r="A73">
         <v>72</v>
       </c>
@@ -8403,7 +8397,7 @@
         <v>428</v>
       </c>
     </row>
-    <row ht="12.75" r="74" spans="1:8">
+    <row r="74" spans="1:8" ht="12.75">
       <c r="A74">
         <v>73</v>
       </c>
@@ -8426,7 +8420,7 @@
         <v>428</v>
       </c>
     </row>
-    <row customFormat="1" ht="12.75" r="75" s="4" spans="1:8">
+    <row r="75" spans="1:8" s="4" customFormat="1" ht="12.75">
       <c r="A75" s="4">
         <v>74</v>
       </c>
@@ -8449,7 +8443,7 @@
         <v>428</v>
       </c>
     </row>
-    <row ht="12.75" r="76" spans="1:8">
+    <row r="76" spans="1:8" ht="12.75">
       <c r="A76">
         <v>75</v>
       </c>
@@ -8472,7 +8466,7 @@
         <v>428</v>
       </c>
     </row>
-    <row ht="12.75" r="77" spans="1:8">
+    <row r="77" spans="1:8" ht="12.75">
       <c r="A77">
         <v>76</v>
       </c>
@@ -8495,7 +8489,7 @@
         <v>428</v>
       </c>
     </row>
-    <row ht="12.75" r="78" spans="1:8">
+    <row r="78" spans="1:8" ht="12.75">
       <c r="A78">
         <v>77</v>
       </c>
@@ -8518,7 +8512,7 @@
         <v>428</v>
       </c>
     </row>
-    <row ht="12.75" r="79" spans="1:8">
+    <row r="79" spans="1:8" ht="12.75">
       <c r="A79">
         <v>78</v>
       </c>
@@ -8541,7 +8535,7 @@
         <v>428</v>
       </c>
     </row>
-    <row ht="12.75" r="80" spans="1:8">
+    <row r="80" spans="1:8" ht="12.75">
       <c r="A80">
         <v>79</v>
       </c>
@@ -8564,7 +8558,7 @@
         <v>428</v>
       </c>
     </row>
-    <row ht="12.75" r="81" spans="1:8">
+    <row r="81" spans="1:8" ht="12.75">
       <c r="A81">
         <v>80</v>
       </c>
@@ -8587,7 +8581,7 @@
         <v>428</v>
       </c>
     </row>
-    <row ht="12.75" r="82" spans="1:8">
+    <row r="82" spans="1:8" ht="12.75">
       <c r="A82">
         <v>81</v>
       </c>
@@ -8610,7 +8604,7 @@
         <v>428</v>
       </c>
     </row>
-    <row ht="12.75" r="83" spans="1:8">
+    <row r="83" spans="1:8" ht="12.75">
       <c r="A83">
         <v>82</v>
       </c>
@@ -8633,7 +8627,7 @@
         <v>428</v>
       </c>
     </row>
-    <row ht="12.75" r="84" spans="1:8">
+    <row r="84" spans="1:8" ht="12.75">
       <c r="A84">
         <v>83</v>
       </c>
@@ -8656,7 +8650,7 @@
         <v>428</v>
       </c>
     </row>
-    <row ht="12.75" r="85" spans="1:8">
+    <row r="85" spans="1:8" ht="12.75">
       <c r="A85">
         <v>84</v>
       </c>
@@ -8679,7 +8673,7 @@
         <v>428</v>
       </c>
     </row>
-    <row customFormat="1" ht="12.75" r="86" s="4" spans="1:8">
+    <row r="86" spans="1:8" s="4" customFormat="1" ht="12.75">
       <c r="A86" s="4">
         <v>85</v>
       </c>
@@ -8702,7 +8696,7 @@
         <v>427</v>
       </c>
     </row>
-    <row customFormat="1" ht="12.75" r="87" s="4" spans="1:8">
+    <row r="87" spans="1:8" s="4" customFormat="1" ht="12.75">
       <c r="A87" s="4">
         <v>86</v>
       </c>
@@ -8725,7 +8719,7 @@
         <v>38</v>
       </c>
     </row>
-    <row ht="12.75" r="88" spans="1:8">
+    <row r="88" spans="1:8" ht="12.75">
       <c r="A88">
         <v>87</v>
       </c>
@@ -8748,7 +8742,7 @@
         <v>38</v>
       </c>
     </row>
-    <row ht="12.75" r="89" spans="1:8">
+    <row r="89" spans="1:8" ht="12.75">
       <c r="A89">
         <v>88</v>
       </c>
@@ -8771,7 +8765,7 @@
         <v>38</v>
       </c>
     </row>
-    <row ht="12.75" r="90" spans="1:8">
+    <row r="90" spans="1:8" ht="12.75">
       <c r="A90">
         <v>89</v>
       </c>
@@ -8794,7 +8788,7 @@
         <v>428</v>
       </c>
     </row>
-    <row ht="12.75" r="91" spans="1:8">
+    <row r="91" spans="1:8" ht="12.75">
       <c r="A91">
         <v>90</v>
       </c>
@@ -8817,7 +8811,7 @@
         <v>428</v>
       </c>
     </row>
-    <row ht="12.75" r="92" spans="1:8">
+    <row r="92" spans="1:8" ht="12.75">
       <c r="A92">
         <v>91</v>
       </c>
@@ -8840,7 +8834,7 @@
         <v>428</v>
       </c>
     </row>
-    <row ht="12.75" r="93" spans="1:8">
+    <row r="93" spans="1:8" ht="12.75">
       <c r="A93">
         <v>92</v>
       </c>
@@ -8863,7 +8857,7 @@
         <v>428</v>
       </c>
     </row>
-    <row ht="12.75" r="94" spans="1:8">
+    <row r="94" spans="1:8" ht="12.75">
       <c r="A94">
         <v>93</v>
       </c>
@@ -8886,7 +8880,7 @@
         <v>427</v>
       </c>
     </row>
-    <row ht="12.75" r="95" spans="1:8">
+    <row r="95" spans="1:8" ht="12.75">
       <c r="A95">
         <v>94</v>
       </c>
@@ -8909,7 +8903,7 @@
         <v>427</v>
       </c>
     </row>
-    <row ht="12.75" r="96" spans="1:8">
+    <row r="96" spans="1:8" ht="12.75">
       <c r="A96">
         <v>95</v>
       </c>
@@ -8932,7 +8926,7 @@
         <v>427</v>
       </c>
     </row>
-    <row ht="12.75" r="97" spans="1:8">
+    <row r="97" spans="1:8" ht="12.75">
       <c r="A97">
         <v>96</v>
       </c>
@@ -8955,7 +8949,7 @@
         <v>38</v>
       </c>
     </row>
-    <row ht="12.75" r="98" spans="1:8">
+    <row r="98" spans="1:8" ht="12.75">
       <c r="A98">
         <v>97</v>
       </c>
@@ -8978,7 +8972,7 @@
         <v>428</v>
       </c>
     </row>
-    <row ht="12.75" r="99" spans="1:8">
+    <row r="99" spans="1:8" ht="12.75">
       <c r="A99">
         <v>98</v>
       </c>
@@ -9001,7 +8995,7 @@
         <v>427</v>
       </c>
     </row>
-    <row ht="12.75" r="100" spans="1:8">
+    <row r="100" spans="1:8" ht="12.75">
       <c r="A100">
         <v>99</v>
       </c>
@@ -9024,7 +9018,7 @@
         <v>38</v>
       </c>
     </row>
-    <row ht="12.75" r="101" spans="1:8">
+    <row r="101" spans="1:8" ht="12.75">
       <c r="A101">
         <v>100</v>
       </c>
@@ -9047,7 +9041,7 @@
         <v>428</v>
       </c>
     </row>
-    <row ht="12.75" r="102" spans="1:8">
+    <row r="102" spans="1:8" ht="12.75">
       <c r="A102">
         <v>101</v>
       </c>
@@ -9070,7 +9064,7 @@
         <v>38</v>
       </c>
     </row>
-    <row ht="12.75" r="103" spans="1:8">
+    <row r="103" spans="1:8" ht="12.75">
       <c r="A103">
         <v>102</v>
       </c>
@@ -9093,7 +9087,7 @@
         <v>428</v>
       </c>
     </row>
-    <row ht="12.75" r="104" spans="1:8">
+    <row r="104" spans="1:8" ht="12.75">
       <c r="A104">
         <v>103</v>
       </c>
@@ -9116,7 +9110,7 @@
         <v>38</v>
       </c>
     </row>
-    <row ht="12.75" r="105" spans="1:8">
+    <row r="105" spans="1:8" ht="12.75">
       <c r="A105">
         <v>104</v>
       </c>
@@ -9139,7 +9133,7 @@
         <v>38</v>
       </c>
     </row>
-    <row ht="12.75" r="106" spans="1:8">
+    <row r="106" spans="1:8" ht="12.75">
       <c r="A106">
         <v>105</v>
       </c>
@@ -9162,7 +9156,7 @@
         <v>38</v>
       </c>
     </row>
-    <row ht="12.75" r="107" spans="1:8">
+    <row r="107" spans="1:8" ht="12.75">
       <c r="A107">
         <v>106</v>
       </c>
@@ -9185,7 +9179,7 @@
         <v>427</v>
       </c>
     </row>
-    <row ht="12.75" r="108" spans="1:8">
+    <row r="108" spans="1:8" ht="12.75">
       <c r="A108">
         <v>107</v>
       </c>
@@ -9208,7 +9202,7 @@
         <v>38</v>
       </c>
     </row>
-    <row ht="12.75" r="109" spans="1:8">
+    <row r="109" spans="1:8" ht="12.75">
       <c r="A109">
         <v>108</v>
       </c>
@@ -9231,7 +9225,7 @@
         <v>38</v>
       </c>
     </row>
-    <row ht="12.75" r="110" spans="1:8">
+    <row r="110" spans="1:8" ht="12.75">
       <c r="A110">
         <v>109</v>
       </c>
@@ -9254,7 +9248,7 @@
         <v>428</v>
       </c>
     </row>
-    <row ht="12.75" r="111" spans="1:8">
+    <row r="111" spans="1:8" ht="12.75">
       <c r="A111">
         <v>110</v>
       </c>
@@ -9277,7 +9271,7 @@
         <v>428</v>
       </c>
     </row>
-    <row ht="12.75" r="112" spans="1:8">
+    <row r="112" spans="1:8" ht="12.75">
       <c r="A112">
         <v>111</v>
       </c>
@@ -9300,7 +9294,7 @@
         <v>428</v>
       </c>
     </row>
-    <row ht="12.75" r="113" spans="1:8">
+    <row r="113" spans="1:8" ht="12.75">
       <c r="A113">
         <v>112</v>
       </c>
@@ -9323,7 +9317,7 @@
         <v>428</v>
       </c>
     </row>
-    <row ht="12.75" r="114" spans="1:8">
+    <row r="114" spans="1:8" ht="12.75">
       <c r="A114">
         <v>113</v>
       </c>
@@ -9346,7 +9340,7 @@
         <v>427</v>
       </c>
     </row>
-    <row ht="12.75" r="115" spans="1:8">
+    <row r="115" spans="1:8" ht="12.75">
       <c r="A115">
         <v>114</v>
       </c>
@@ -9369,7 +9363,7 @@
         <v>323</v>
       </c>
     </row>
-    <row ht="12.75" r="116" spans="1:8">
+    <row r="116" spans="1:8" ht="12.75">
       <c r="A116">
         <v>115</v>
       </c>
@@ -9392,7 +9386,7 @@
         <v>427</v>
       </c>
     </row>
-    <row ht="12.75" r="117" spans="1:8">
+    <row r="117" spans="1:8" ht="12.75">
       <c r="A117">
         <v>116</v>
       </c>
@@ -9415,7 +9409,7 @@
         <v>428</v>
       </c>
     </row>
-    <row ht="12.75" r="118" spans="1:8">
+    <row r="118" spans="1:8" ht="12.75">
       <c r="A118">
         <v>117</v>
       </c>
@@ -9435,7 +9429,7 @@
         <v>38</v>
       </c>
     </row>
-    <row ht="12.75" r="119" spans="1:8">
+    <row r="119" spans="1:8" ht="12.75">
       <c r="A119">
         <v>118</v>
       </c>
@@ -9458,7 +9452,7 @@
         <v>428</v>
       </c>
     </row>
-    <row customHeight="1" ht="15.75" r="120" spans="1:8">
+    <row r="120" spans="1:8" ht="15.75" customHeight="1">
       <c r="A120">
         <v>119</v>
       </c>
@@ -9481,7 +9475,7 @@
         <v>881</v>
       </c>
     </row>
-    <row ht="12.75" r="121" spans="1:8">
+    <row r="121" spans="1:8" ht="12.75">
       <c r="A121">
         <v>120</v>
       </c>
@@ -9504,7 +9498,7 @@
         <v>881</v>
       </c>
     </row>
-    <row ht="12.75" r="122" spans="1:8">
+    <row r="122" spans="1:8" ht="12.75">
       <c r="A122">
         <v>121</v>
       </c>
@@ -9527,7 +9521,7 @@
         <v>881</v>
       </c>
     </row>
-    <row ht="12.75" r="123" spans="1:8">
+    <row r="123" spans="1:8" ht="12.75">
       <c r="A123">
         <v>122</v>
       </c>
@@ -9550,7 +9544,7 @@
         <v>881</v>
       </c>
     </row>
-    <row ht="12.75" r="124" spans="1:8">
+    <row r="124" spans="1:8" ht="12.75">
       <c r="A124">
         <v>123</v>
       </c>
@@ -9573,7 +9567,7 @@
         <v>881</v>
       </c>
     </row>
-    <row ht="12.75" r="125" spans="1:8">
+    <row r="125" spans="1:8" ht="12.75">
       <c r="A125">
         <v>124</v>
       </c>
@@ -9596,7 +9590,7 @@
         <v>881</v>
       </c>
     </row>
-    <row ht="12.75" r="126" spans="1:8">
+    <row r="126" spans="1:8" ht="12.75">
       <c r="A126">
         <v>125</v>
       </c>
@@ -9619,7 +9613,7 @@
         <v>881</v>
       </c>
     </row>
-    <row ht="12.75" r="127" spans="1:8">
+    <row r="127" spans="1:8" ht="12.75">
       <c r="A127">
         <v>126</v>
       </c>
@@ -9642,7 +9636,7 @@
         <v>881</v>
       </c>
     </row>
-    <row ht="12.75" r="128" spans="1:8">
+    <row r="128" spans="1:8" ht="12.75">
       <c r="A128">
         <v>127</v>
       </c>
@@ -9665,7 +9659,7 @@
         <v>881</v>
       </c>
     </row>
-    <row ht="12.75" r="129" spans="1:8">
+    <row r="129" spans="1:8" ht="12.75">
       <c r="A129">
         <v>128</v>
       </c>
@@ -9688,7 +9682,7 @@
         <v>881</v>
       </c>
     </row>
-    <row ht="12.75" r="130" spans="1:8">
+    <row r="130" spans="1:8" ht="12.75">
       <c r="A130">
         <v>129</v>
       </c>
@@ -9711,7 +9705,7 @@
         <v>881</v>
       </c>
     </row>
-    <row ht="12.75" r="131" spans="1:8">
+    <row r="131" spans="1:8" ht="12.75">
       <c r="A131">
         <v>130</v>
       </c>
@@ -9734,7 +9728,7 @@
         <v>881</v>
       </c>
     </row>
-    <row ht="12.75" r="132" spans="1:8">
+    <row r="132" spans="1:8" ht="12.75">
       <c r="A132">
         <v>131</v>
       </c>
@@ -9757,7 +9751,7 @@
         <v>881</v>
       </c>
     </row>
-    <row ht="12.75" r="133" spans="1:8">
+    <row r="133" spans="1:8" ht="12.75">
       <c r="A133">
         <v>132</v>
       </c>
@@ -9780,7 +9774,7 @@
         <v>881</v>
       </c>
     </row>
-    <row ht="12.75" r="134" spans="1:8">
+    <row r="134" spans="1:8" ht="12.75">
       <c r="A134">
         <v>133</v>
       </c>
@@ -9803,7 +9797,7 @@
         <v>881</v>
       </c>
     </row>
-    <row ht="12.75" r="135" spans="1:8">
+    <row r="135" spans="1:8" ht="12.75">
       <c r="A135">
         <v>134</v>
       </c>
@@ -9826,7 +9820,7 @@
         <v>881</v>
       </c>
     </row>
-    <row ht="12.75" r="136" spans="1:8">
+    <row r="136" spans="1:8" ht="12.75">
       <c r="A136">
         <v>135</v>
       </c>
@@ -9849,7 +9843,7 @@
         <v>881</v>
       </c>
     </row>
-    <row ht="12.75" r="137" spans="1:8">
+    <row r="137" spans="1:8" ht="12.75">
       <c r="A137">
         <v>136</v>
       </c>
@@ -9872,7 +9866,7 @@
         <v>881</v>
       </c>
     </row>
-    <row ht="12.75" r="138" spans="1:8">
+    <row r="138" spans="1:8" ht="12.75">
       <c r="A138">
         <v>137</v>
       </c>
@@ -9895,7 +9889,7 @@
         <v>881</v>
       </c>
     </row>
-    <row ht="12.75" r="139" spans="1:8">
+    <row r="139" spans="1:8" ht="12.75">
       <c r="A139">
         <v>138</v>
       </c>
@@ -9918,7 +9912,7 @@
         <v>881</v>
       </c>
     </row>
-    <row ht="12.75" r="140" spans="1:8">
+    <row r="140" spans="1:8" ht="12.75">
       <c r="A140">
         <v>139</v>
       </c>
@@ -9941,7 +9935,7 @@
         <v>881</v>
       </c>
     </row>
-    <row ht="12.75" r="141" spans="1:8">
+    <row r="141" spans="1:8" ht="12.75">
       <c r="A141">
         <v>140</v>
       </c>
@@ -9964,7 +9958,7 @@
         <v>881</v>
       </c>
     </row>
-    <row ht="12.75" r="142" spans="1:8">
+    <row r="142" spans="1:8" ht="12.75">
       <c r="A142">
         <v>141</v>
       </c>
@@ -9987,7 +9981,7 @@
         <v>881</v>
       </c>
     </row>
-    <row ht="12.75" r="143" spans="1:8">
+    <row r="143" spans="1:8" ht="12.75">
       <c r="A143">
         <v>142</v>
       </c>
@@ -10010,7 +10004,7 @@
         <v>881</v>
       </c>
     </row>
-    <row ht="12.75" r="144" spans="1:8">
+    <row r="144" spans="1:8" ht="12.75">
       <c r="A144">
         <v>143</v>
       </c>
@@ -10033,7 +10027,7 @@
         <v>38</v>
       </c>
     </row>
-    <row ht="12.75" r="145" spans="1:8">
+    <row r="145" spans="1:8" ht="12.75">
       <c r="A145">
         <v>144</v>
       </c>
@@ -10056,7 +10050,7 @@
         <v>428</v>
       </c>
     </row>
-    <row ht="12.75" r="146" spans="1:8">
+    <row r="146" spans="1:8" ht="12.75">
       <c r="A146">
         <v>145</v>
       </c>
@@ -10079,7 +10073,7 @@
         <v>427</v>
       </c>
     </row>
-    <row ht="12.75" r="147" spans="1:8">
+    <row r="147" spans="1:8" ht="12.75">
       <c r="A147">
         <v>146</v>
       </c>
@@ -10102,7 +10096,7 @@
         <v>38</v>
       </c>
     </row>
-    <row ht="12.75" r="148" spans="1:8">
+    <row r="148" spans="1:8" ht="12.75">
       <c r="A148">
         <v>147</v>
       </c>
@@ -10125,7 +10119,7 @@
         <v>881</v>
       </c>
     </row>
-    <row ht="12.75" r="149" spans="1:8">
+    <row r="149" spans="1:8" ht="12.75">
       <c r="A149">
         <v>148</v>
       </c>
@@ -10148,7 +10142,7 @@
         <v>881</v>
       </c>
     </row>
-    <row ht="12.75" r="150" spans="1:8">
+    <row r="150" spans="1:8" ht="12.75">
       <c r="A150">
         <v>149</v>
       </c>
@@ -10171,7 +10165,7 @@
         <v>881</v>
       </c>
     </row>
-    <row ht="12.75" r="151" spans="1:8">
+    <row r="151" spans="1:8" ht="12.75">
       <c r="A151">
         <v>150</v>
       </c>
@@ -10194,7 +10188,7 @@
         <v>427</v>
       </c>
     </row>
-    <row ht="12.75" r="152" spans="1:8">
+    <row r="152" spans="1:8" ht="12.75">
       <c r="A152">
         <v>151</v>
       </c>
@@ -10217,18 +10211,18 @@
         <v>881</v>
       </c>
     </row>
-    <row ht="12.75" r="153" spans="1:8">
+    <row r="153" spans="1:8" ht="12.75">
       <c r="A153">
         <v>152</v>
       </c>
-      <c r="B153" t="s">
+      <c r="B153" s="41" t="s">
         <v>1121</v>
       </c>
-      <c r="C153" t="s">
-        <v>1128</v>
-      </c>
-      <c r="D153" s="46" t="s">
-        <v>1127</v>
+      <c r="C153" s="41" t="s">
+        <v>1122</v>
+      </c>
+      <c r="D153" s="4" t="s">
+        <v>7</v>
       </c>
       <c r="F153" s="2" t="s">
         <v>687</v>
@@ -10242,236 +10236,238 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink r:id="rId1" ref="B2" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
-    <hyperlink r:id="rId2" ref="B3" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
-    <hyperlink r:id="rId3" ref="B4" xr:uid="{00000000-0004-0000-0000-000002000000}"/>
-    <hyperlink r:id="rId4" ref="B5" xr:uid="{00000000-0004-0000-0000-000003000000}"/>
-    <hyperlink r:id="rId5" ref="B6" xr:uid="{00000000-0004-0000-0000-000004000000}"/>
-    <hyperlink r:id="rId6" ref="H6" xr:uid="{00000000-0004-0000-0000-000005000000}"/>
-    <hyperlink r:id="rId7" ref="B7" xr:uid="{00000000-0004-0000-0000-000006000000}"/>
-    <hyperlink r:id="rId8" ref="B8" xr:uid="{00000000-0004-0000-0000-000007000000}"/>
-    <hyperlink r:id="rId9" ref="B9" xr:uid="{00000000-0004-0000-0000-000008000000}"/>
-    <hyperlink r:id="rId10" ref="B10" xr:uid="{00000000-0004-0000-0000-000009000000}"/>
-    <hyperlink r:id="rId11" ref="B11" xr:uid="{00000000-0004-0000-0000-00000A000000}"/>
-    <hyperlink r:id="rId12" ref="B12" xr:uid="{00000000-0004-0000-0000-00000B000000}"/>
-    <hyperlink r:id="rId13" ref="B13" xr:uid="{00000000-0004-0000-0000-00000C000000}"/>
-    <hyperlink r:id="rId14" ref="B14" xr:uid="{00000000-0004-0000-0000-00000D000000}"/>
-    <hyperlink r:id="rId15" ref="B15" xr:uid="{00000000-0004-0000-0000-00000E000000}"/>
-    <hyperlink r:id="rId16" ref="B16" xr:uid="{00000000-0004-0000-0000-00000F000000}"/>
-    <hyperlink r:id="rId17" ref="B17" xr:uid="{00000000-0004-0000-0000-000010000000}"/>
-    <hyperlink r:id="rId18" ref="B18" xr:uid="{00000000-0004-0000-0000-000011000000}"/>
-    <hyperlink r:id="rId19" ref="B19" xr:uid="{00000000-0004-0000-0000-000012000000}"/>
-    <hyperlink r:id="rId20" ref="B20" xr:uid="{00000000-0004-0000-0000-000013000000}"/>
-    <hyperlink r:id="rId21" ref="B21" xr:uid="{00000000-0004-0000-0000-000014000000}"/>
-    <hyperlink r:id="rId22" ref="B22" xr:uid="{00000000-0004-0000-0000-000015000000}"/>
-    <hyperlink r:id="rId23" ref="B23" xr:uid="{00000000-0004-0000-0000-000016000000}"/>
-    <hyperlink r:id="rId24" ref="B24" xr:uid="{00000000-0004-0000-0000-000017000000}"/>
-    <hyperlink r:id="rId25" ref="B25" xr:uid="{00000000-0004-0000-0000-000018000000}"/>
-    <hyperlink r:id="rId26" ref="H25" xr:uid="{00000000-0004-0000-0000-000019000000}"/>
-    <hyperlink r:id="rId27" ref="B26" xr:uid="{00000000-0004-0000-0000-00001A000000}"/>
-    <hyperlink r:id="rId28" ref="H26" xr:uid="{00000000-0004-0000-0000-00001B000000}"/>
-    <hyperlink r:id="rId29" ref="B27" xr:uid="{00000000-0004-0000-0000-00001C000000}"/>
-    <hyperlink r:id="rId30" ref="H27" xr:uid="{00000000-0004-0000-0000-00001D000000}"/>
-    <hyperlink r:id="rId31" ref="B28" xr:uid="{00000000-0004-0000-0000-00001E000000}"/>
-    <hyperlink r:id="rId32" ref="H28" xr:uid="{00000000-0004-0000-0000-00001F000000}"/>
-    <hyperlink r:id="rId33" ref="B29" xr:uid="{00000000-0004-0000-0000-000020000000}"/>
-    <hyperlink r:id="rId34" ref="H29" xr:uid="{00000000-0004-0000-0000-000021000000}"/>
-    <hyperlink r:id="rId35" ref="B30" xr:uid="{00000000-0004-0000-0000-000022000000}"/>
-    <hyperlink r:id="rId36" ref="H30" xr:uid="{00000000-0004-0000-0000-000023000000}"/>
-    <hyperlink r:id="rId37" ref="B31" xr:uid="{00000000-0004-0000-0000-000024000000}"/>
-    <hyperlink r:id="rId38" ref="H31" xr:uid="{00000000-0004-0000-0000-000025000000}"/>
-    <hyperlink r:id="rId39" ref="B32" xr:uid="{00000000-0004-0000-0000-000026000000}"/>
-    <hyperlink r:id="rId40" ref="H32" xr:uid="{00000000-0004-0000-0000-000027000000}"/>
-    <hyperlink r:id="rId41" ref="B33" xr:uid="{00000000-0004-0000-0000-000028000000}"/>
-    <hyperlink r:id="rId42" ref="B34" xr:uid="{00000000-0004-0000-0000-000029000000}"/>
-    <hyperlink r:id="rId43" ref="B38" xr:uid="{00000000-0004-0000-0000-00002A000000}"/>
-    <hyperlink r:id="rId44" ref="B45" xr:uid="{00000000-0004-0000-0000-00002B000000}"/>
-    <hyperlink r:id="rId45" ref="B48" xr:uid="{00000000-0004-0000-0000-00002C000000}"/>
-    <hyperlink r:id="rId46" ref="B35" xr:uid="{00000000-0004-0000-0000-00002D000000}"/>
-    <hyperlink r:id="rId47" ref="B52" xr:uid="{00000000-0004-0000-0000-00002E000000}"/>
-    <hyperlink r:id="rId48" ref="B53" xr:uid="{00000000-0004-0000-0000-00002F000000}"/>
-    <hyperlink r:id="rId49" ref="B55" xr:uid="{00000000-0004-0000-0000-000030000000}"/>
-    <hyperlink r:id="rId50" ref="B56" xr:uid="{00000000-0004-0000-0000-000031000000}"/>
-    <hyperlink r:id="rId51" ref="B57" xr:uid="{00000000-0004-0000-0000-000032000000}"/>
-    <hyperlink r:id="rId52" ref="B58" xr:uid="{00000000-0004-0000-0000-000033000000}"/>
-    <hyperlink r:id="rId53" ref="B61" xr:uid="{00000000-0004-0000-0000-000034000000}"/>
-    <hyperlink r:id="rId54" ref="B62" xr:uid="{00000000-0004-0000-0000-000035000000}"/>
-    <hyperlink r:id="rId55" ref="B63" xr:uid="{00000000-0004-0000-0000-000036000000}"/>
-    <hyperlink r:id="rId56" ref="B64" xr:uid="{00000000-0004-0000-0000-000037000000}"/>
-    <hyperlink r:id="rId57" ref="B65" xr:uid="{00000000-0004-0000-0000-000038000000}"/>
-    <hyperlink r:id="rId58" ref="B66" xr:uid="{00000000-0004-0000-0000-000039000000}"/>
-    <hyperlink r:id="rId59" ref="B67" xr:uid="{00000000-0004-0000-0000-00003A000000}"/>
-    <hyperlink display="https://www.allhomes.com.au/agency/trusted-realtors-570129/" r:id="rId60" ref="H7:H24" xr:uid="{00000000-0004-0000-0000-00003B000000}"/>
-    <hyperlink r:id="rId61" ref="B43" xr:uid="{00000000-0004-0000-0000-00003C000000}"/>
-    <hyperlink r:id="rId62" ref="B44" xr:uid="{00000000-0004-0000-0000-00003D000000}"/>
-    <hyperlink r:id="rId63" ref="B46" xr:uid="{00000000-0004-0000-0000-00003E000000}"/>
-    <hyperlink r:id="rId64" ref="B54" xr:uid="{00000000-0004-0000-0000-00003F000000}"/>
-    <hyperlink r:id="rId65" ref="B42" xr:uid="{00000000-0004-0000-0000-000040000000}"/>
-    <hyperlink r:id="rId66" ref="J2" xr:uid="{00000000-0004-0000-0000-000041000000}"/>
-    <hyperlink r:id="rId67" ref="C69" xr:uid="{9DAE03A7-93E8-4507-BD6C-AC4013ECD47F}"/>
-    <hyperlink r:id="rId68" ref="C68" xr:uid="{66B9A9CA-DF82-46B6-9C5A-C5709E2FF1AE}"/>
-    <hyperlink r:id="rId69" ref="B75" xr:uid="{57E7BFEF-6F05-4DA9-A3DE-5B0A0EFED4D9}"/>
-    <hyperlink r:id="rId70" ref="C75" xr:uid="{F4755F93-6E59-4C38-BF66-16746869FDF3}"/>
-    <hyperlink r:id="rId71" ref="H75" xr:uid="{5BFAFD71-42C4-487F-B5E7-1697975992B4}"/>
-    <hyperlink r:id="rId72" ref="B78" xr:uid="{D3DE0D76-2479-4283-B7C7-F11B85797022}"/>
-    <hyperlink r:id="rId73" ref="C78" xr:uid="{FC1D9146-2FDC-4F13-A3C3-51CAB46DEC08}"/>
-    <hyperlink r:id="rId74" ref="B68" xr:uid="{3ED6FAA1-2B0F-4DB9-878E-9640A9C2850D}"/>
-    <hyperlink r:id="rId75" ref="B69" xr:uid="{12DE6CA8-DDC5-4E7B-BD2E-14B105A0DE3B}"/>
-    <hyperlink r:id="rId76" ref="C70" xr:uid="{0419758C-286A-4B76-B8B2-31CC336DEDF1}"/>
-    <hyperlink r:id="rId77" ref="B70" xr:uid="{AC18D1D2-FA3D-4352-A402-35B7AAFE27C0}"/>
-    <hyperlink r:id="rId78" ref="B71" xr:uid="{E8BCA1EF-4E17-4AA7-A2CE-5674FC05ABC3}"/>
-    <hyperlink r:id="rId79" ref="C71" xr:uid="{949AE606-DF4A-48F4-93A0-F148D80842CB}"/>
-    <hyperlink r:id="rId80" ref="B72" xr:uid="{69A93BB5-0295-46D6-8334-45444356E6E9}"/>
-    <hyperlink r:id="rId81" ref="C72" xr:uid="{CA171BC7-126F-4175-8A03-123D5A2C2D8A}"/>
-    <hyperlink r:id="rId82" ref="C73" xr:uid="{FACC205D-E563-4266-8E0D-0794F3D76E98}"/>
-    <hyperlink r:id="rId83" ref="B85" xr:uid="{7ABCABC0-A765-435B-AE52-9D27F653E00F}"/>
-    <hyperlink r:id="rId84" ref="C4" xr:uid="{2CD58DBE-98E3-4EDC-898F-088D5F0FCB81}"/>
-    <hyperlink r:id="rId85" ref="C29" xr:uid="{CB7CAD83-ACA3-4309-B102-B0F536FC97E6}"/>
-    <hyperlink r:id="rId86" ref="C90" xr:uid="{B4F55488-2B40-4078-ABF0-4B4254363237}"/>
-    <hyperlink r:id="rId87" ref="B90" xr:uid="{09FEE7FE-E667-40E8-BC22-3FDC999B614F}"/>
-    <hyperlink r:id="rId88" ref="C15" xr:uid="{34F25BA9-B460-46CF-85C0-4AC9D6288B41}"/>
-    <hyperlink r:id="rId89" ref="C3" xr:uid="{EBAAEE7A-83B2-457B-8600-89427BF11448}"/>
-    <hyperlink r:id="rId90" ref="C8" xr:uid="{3D3D678C-8F1B-47BC-ACA2-D1CBF5A76F0B}"/>
-    <hyperlink r:id="rId91" ref="C19" xr:uid="{ED2C9A9B-3440-4B4A-91A1-7CAF84972535}"/>
-    <hyperlink r:id="rId92" ref="C20" xr:uid="{E47C999F-11AE-4F93-9032-6E51EB582635}"/>
-    <hyperlink r:id="rId93" ref="C21" xr:uid="{E59411CC-EC13-4665-969A-8D9238CCD0C2}"/>
-    <hyperlink r:id="rId94" ref="C33" xr:uid="{9C953AB9-0076-4477-B52F-C393846B1211}"/>
-    <hyperlink r:id="rId95" ref="C38" xr:uid="{D349EA20-36BF-44C7-A16B-E85B8FE53B2A}"/>
-    <hyperlink r:id="rId96" ref="C39" xr:uid="{DE18DA3B-1A3D-4613-888E-7F506CC87091}"/>
-    <hyperlink r:id="rId97" ref="C40" xr:uid="{0C71282B-049B-4CD1-A090-B66647F2B29B}"/>
-    <hyperlink r:id="rId98" ref="C42" xr:uid="{AD0DC851-DEC5-4ACE-B928-50149068BB70}"/>
-    <hyperlink r:id="rId99" ref="C45" xr:uid="{EB51DFC2-D28F-4E0C-B019-F9954D6C9832}"/>
-    <hyperlink r:id="rId100" ref="C52" xr:uid="{9E5146F6-8EC8-4A2C-B192-C1CCB11CAB8A}"/>
-    <hyperlink r:id="rId101" ref="C48" xr:uid="{31B308E4-DA3E-401B-B796-7D03404228FB}"/>
-    <hyperlink r:id="rId102" ref="C49" xr:uid="{EBAAB9CE-7F91-4628-AF75-32C4EEF948C2}"/>
-    <hyperlink r:id="rId103" ref="C53" xr:uid="{2FF7EB1F-CD56-4E71-AD0F-0D12E8347603}"/>
-    <hyperlink r:id="rId104" ref="C55" xr:uid="{9BD44DCD-EEBB-4649-9792-F3DAC40B3960}"/>
-    <hyperlink r:id="rId105" ref="C63" xr:uid="{9929BCF4-32FD-4143-99F6-FEB21B90BCD7}"/>
-    <hyperlink r:id="rId106" ref="C64" xr:uid="{80B3DEC9-506E-4F3A-B171-A2D71B731577}"/>
-    <hyperlink r:id="rId107" ref="C66" xr:uid="{011D2C70-C541-49D4-894E-FF670D6C19BB}"/>
-    <hyperlink r:id="rId108" ref="C67" xr:uid="{B62DFA3B-60A0-44AA-BF1D-BCA2A049E46C}"/>
-    <hyperlink r:id="rId109" ref="C56" xr:uid="{C98B5D5D-65AB-489D-8160-8F1B41CDE6A7}"/>
-    <hyperlink r:id="rId110" ref="B103" xr:uid="{4D81C408-B745-40E2-B9C7-6E36C45175A7}"/>
-    <hyperlink r:id="rId111" ref="C26" xr:uid="{6A9C6F44-3E7F-47CF-8514-B6609EBEE668}"/>
-    <hyperlink r:id="rId112" ref="C23" xr:uid="{F99F350A-C378-4940-B611-41F47BC3B4B0}"/>
-    <hyperlink r:id="rId113" ref="C103" xr:uid="{3E9C8DCE-ABC0-49DA-B64B-B569BAAE6ED0}"/>
-    <hyperlink r:id="rId114" ref="C104" xr:uid="{E96AA061-2DED-4A35-BE99-8E7E156527EB}"/>
-    <hyperlink r:id="rId115" ref="C102" xr:uid="{4DAA7E56-3BCD-4AF1-B6E7-A26B02A0DA6C}"/>
-    <hyperlink r:id="rId116" ref="C101" xr:uid="{EBE0EC7F-0880-4F4A-991C-2C7C53889923}"/>
-    <hyperlink r:id="rId117" ref="C100" xr:uid="{7AA4A2D0-C18F-4625-A776-6EDD2415E1BC}"/>
-    <hyperlink r:id="rId118" ref="C99" xr:uid="{15BFB680-4225-425B-8826-841A35922C8A}"/>
-    <hyperlink r:id="rId119" ref="B99" xr:uid="{1EF2BF94-D92B-41EF-8B1F-0585F1910B74}"/>
-    <hyperlink r:id="rId120" ref="C97" xr:uid="{6687C5A1-CC2B-49FF-B98D-946AA21B8C55}"/>
-    <hyperlink r:id="rId121" ref="B97" xr:uid="{0411E592-2DE8-4D1D-B66C-46CE99CAA412}"/>
-    <hyperlink r:id="rId122" ref="C96" xr:uid="{A7ED7210-DE23-4760-B67F-78027E9B9B73}"/>
-    <hyperlink r:id="rId123" ref="B96" xr:uid="{992F1752-E440-4347-A698-44C8E60F00BE}"/>
-    <hyperlink r:id="rId124" ref="B102" xr:uid="{A0E03FB2-010F-497D-874D-A0A66FB6303C}"/>
-    <hyperlink r:id="rId125" ref="B101" xr:uid="{165FBF6F-9195-42DA-AC37-C49B2308ACA1}"/>
-    <hyperlink r:id="rId126" ref="B94" xr:uid="{7DB2C8A6-8C43-4818-A7C2-D5E14351114B}"/>
-    <hyperlink r:id="rId127" ref="B93" xr:uid="{EFC122F7-44E7-447B-8F21-BA1503A72780}"/>
-    <hyperlink r:id="rId128" ref="B91" xr:uid="{7AC22E1D-6919-43E6-AD91-1551DBBDE570}"/>
-    <hyperlink r:id="rId129" ref="B88" xr:uid="{FB3E9840-E4E3-4E64-8CCF-2BAEC7024AD6}"/>
-    <hyperlink r:id="rId130" ref="B87" xr:uid="{348337ED-A616-4A9D-A8D3-0091262177C6}"/>
-    <hyperlink r:id="rId131" ref="B86" xr:uid="{CF62843D-4B82-47CB-B74F-D3F292E9603A}"/>
-    <hyperlink r:id="rId132" ref="B84" xr:uid="{9CA10EFF-3943-479E-914B-1D6EE04D75FC}"/>
-    <hyperlink r:id="rId133" ref="C84" xr:uid="{1074AAC9-CCB0-4FFC-9AFB-EFD1363D7538}"/>
-    <hyperlink r:id="rId134" ref="B105" xr:uid="{D6DE2797-5A68-4C1E-9E74-0D323B6ADFA2}"/>
-    <hyperlink r:id="rId135" ref="B106" xr:uid="{1FCAF9BA-00B5-4008-B5C8-E822ABD6BCDD}"/>
-    <hyperlink r:id="rId136" ref="C11" xr:uid="{893B2404-B185-41F7-B397-A3E08B386C5F}"/>
-    <hyperlink r:id="rId137" ref="B107" xr:uid="{B0E609F4-D8A3-433A-BE15-17E4804C6EA3}"/>
-    <hyperlink r:id="rId138" ref="C107" xr:uid="{6793ECA4-A034-42EC-A741-3B0FF42BC11B}"/>
-    <hyperlink r:id="rId139" ref="B108" xr:uid="{4DB78F44-0F08-4561-A0E8-0EE92F9FFECB}"/>
-    <hyperlink r:id="rId140" ref="B114" xr:uid="{27750164-38B8-4B5E-9B5A-E6C71FFFC61F}"/>
-    <hyperlink r:id="rId141" ref="C114" xr:uid="{6FE6A043-A6B1-44FF-8A45-8C3690323458}"/>
-    <hyperlink r:id="rId142" ref="B113" xr:uid="{0F94FF41-1E06-4D7B-B360-1EB377073C87}"/>
-    <hyperlink r:id="rId143" ref="B112" xr:uid="{490A5044-10EC-4082-BEC1-14008171D5CF}"/>
-    <hyperlink r:id="rId144" ref="B49" xr:uid="{836EB236-8BF1-4259-B395-AD9FA9DE0AE0}"/>
-    <hyperlink r:id="rId145" ref="B74" xr:uid="{8AA8904A-1CC5-4D06-93EF-66F7FC625199}"/>
-    <hyperlink r:id="rId146" ref="B76" xr:uid="{5743888C-C74A-41C6-ABC5-E9575351702D}"/>
-    <hyperlink r:id="rId147" ref="B115" xr:uid="{27BDB583-8AD0-4B33-BA19-24E42C9E7CE9}"/>
-    <hyperlink r:id="rId148" ref="B117" xr:uid="{92BA6213-0D94-4C5A-B06A-6FC35C0BECA9}"/>
-    <hyperlink r:id="rId149" ref="B119" xr:uid="{6724AE23-65F5-4D67-ADA6-E20BD420531B}"/>
-    <hyperlink r:id="rId150" ref="C119" xr:uid="{0A5009EB-B388-4AF4-99CE-5813711C2B1E}"/>
-    <hyperlink r:id="rId151" ref="B120" xr:uid="{255CB59B-E711-471E-8ACE-D0ABA408AE96}"/>
-    <hyperlink r:id="rId152" ref="B39" xr:uid="{39FB4A7C-4EA8-4530-9FE6-2842C777350C}"/>
-    <hyperlink r:id="rId153" ref="B104" xr:uid="{FC8A6FB5-FCCF-409E-9D6D-A93D412B2275}"/>
-    <hyperlink r:id="rId154" ref="C105" xr:uid="{988B91BF-CEBD-44F6-A773-3C87D877BE5A}"/>
-    <hyperlink r:id="rId155" ref="C108" xr:uid="{F0593E1B-3EE0-4DF2-B93E-84A02071630B}"/>
-    <hyperlink r:id="rId156" ref="B109" xr:uid="{601C40E0-818B-457C-9FE7-30D06707CEB7}"/>
-    <hyperlink r:id="rId157" ref="C109" xr:uid="{E1D93474-1A3D-49F1-B191-3C3484679D2D}"/>
-    <hyperlink r:id="rId158" ref="C83" xr:uid="{B0D57129-C33F-45FF-B844-E7642495443D}"/>
-    <hyperlink r:id="rId159" ref="B83" xr:uid="{7DCBF3E6-0CD2-475D-AE1F-56469491B512}"/>
-    <hyperlink r:id="rId160" ref="C120" xr:uid="{F24698EA-BA1A-4C92-8B6D-72A40DDDD7A3}"/>
-    <hyperlink r:id="rId161" ref="C122" xr:uid="{BAC9069D-9D63-415D-B933-A4F86CB8C587}"/>
-    <hyperlink r:id="rId162" ref="C123" xr:uid="{140A866C-FAC2-4A61-BA7E-0AFB9A05FD2F}"/>
-    <hyperlink r:id="rId163" ref="C124" xr:uid="{6EA83FA2-D552-4B23-98A9-6C5EFC3BC2CA}"/>
-    <hyperlink r:id="rId164" ref="C125" xr:uid="{E34375AF-4BB2-420C-887F-8D684FC72F4C}"/>
-    <hyperlink r:id="rId165" ref="C126" xr:uid="{CB74A187-1404-4E3B-B1EF-E6C50CF09D3E}"/>
-    <hyperlink r:id="rId166" ref="C127" xr:uid="{B0565FA3-8BDF-4E3B-9814-B9F51432FA7D}"/>
-    <hyperlink r:id="rId167" ref="C128" xr:uid="{8504A7CE-7DD9-4C74-83D8-90E0745EAB21}"/>
-    <hyperlink r:id="rId168" ref="C130" xr:uid="{D3DDF4DA-6F84-4EAF-BA60-77D926C7C2AC}"/>
-    <hyperlink r:id="rId169" ref="C131" xr:uid="{060B4F44-BF89-4037-9E74-C61E23C6AAC9}"/>
-    <hyperlink r:id="rId170" ref="C132" xr:uid="{8FD9E395-82BD-4EEA-89E9-166FDA928F87}"/>
-    <hyperlink r:id="rId171" ref="C133" xr:uid="{3669E93D-A9CE-4C72-B1DD-98E95312A18C}"/>
-    <hyperlink r:id="rId172" ref="C136" xr:uid="{E14EBE84-3FBA-44D8-B082-69967148B456}"/>
-    <hyperlink r:id="rId173" ref="C137" xr:uid="{CC0D1827-F782-476A-9312-1BAA88B7D496}"/>
-    <hyperlink r:id="rId174" ref="C141" xr:uid="{1528B515-167A-4838-B645-B63CD0312C05}"/>
-    <hyperlink r:id="rId175" ref="B143" xr:uid="{50B775B1-8A20-4A55-90CA-EC152D3C2098}"/>
-    <hyperlink r:id="rId176" ref="B144" xr:uid="{F6EFF9E5-8AC0-4C40-A2A8-62DF9BB671E9}"/>
-    <hyperlink r:id="rId177" ref="C145" xr:uid="{DE56B3AC-2F1A-494E-A9CD-9C972DA863E2}"/>
-    <hyperlink r:id="rId178" ref="B145" xr:uid="{F783979B-F441-49BC-98C4-8448098CBBC1}"/>
-    <hyperlink r:id="rId179" ref="C17" xr:uid="{DBE3D417-C525-4AE7-BA26-A27F8BD7B6D3}"/>
-    <hyperlink r:id="rId180" ref="B121" xr:uid="{BF1CBD80-282B-4284-A960-458EE8D86966}"/>
-    <hyperlink r:id="rId181" ref="C146" xr:uid="{3FA9DCB7-198C-457D-99E0-AF0A29EDEAF1}"/>
-    <hyperlink r:id="rId182" ref="B146" xr:uid="{6B057403-173E-478A-AFE1-5BA96D6006F7}"/>
-    <hyperlink r:id="rId183" ref="C147" xr:uid="{FBD8EA4A-7B80-4D87-BD4D-6D3DDE043E14}"/>
-    <hyperlink r:id="rId184" ref="B147" xr:uid="{F9D4FD4A-592C-4041-AD52-AAD4E4FECD78}"/>
-    <hyperlink r:id="rId185" ref="C148" xr:uid="{EF3F39F0-4058-49A5-8980-E800B6F200B5}"/>
-    <hyperlink r:id="rId186" ref="B148" xr:uid="{513D1B27-06CF-4F01-AD66-B1DDDB3DF171}"/>
-    <hyperlink r:id="rId187" ref="C149" xr:uid="{BFCDD610-AD9F-445C-AAE8-66DB3CD722A6}"/>
-    <hyperlink r:id="rId188" ref="B149" xr:uid="{1567BEF7-2918-4A3A-89A1-A37D6C6B5419}"/>
-    <hyperlink r:id="rId189" ref="B150" xr:uid="{233679EA-F519-4185-AA17-F008EE8DA109}"/>
+    <hyperlink ref="B2" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
+    <hyperlink ref="B3" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
+    <hyperlink ref="B4" r:id="rId3" xr:uid="{00000000-0004-0000-0000-000002000000}"/>
+    <hyperlink ref="B5" r:id="rId4" xr:uid="{00000000-0004-0000-0000-000003000000}"/>
+    <hyperlink ref="B6" r:id="rId5" xr:uid="{00000000-0004-0000-0000-000004000000}"/>
+    <hyperlink ref="H6" r:id="rId6" xr:uid="{00000000-0004-0000-0000-000005000000}"/>
+    <hyperlink ref="B7" r:id="rId7" xr:uid="{00000000-0004-0000-0000-000006000000}"/>
+    <hyperlink ref="B8" r:id="rId8" xr:uid="{00000000-0004-0000-0000-000007000000}"/>
+    <hyperlink ref="B9" r:id="rId9" xr:uid="{00000000-0004-0000-0000-000008000000}"/>
+    <hyperlink ref="B10" r:id="rId10" xr:uid="{00000000-0004-0000-0000-000009000000}"/>
+    <hyperlink ref="B11" r:id="rId11" xr:uid="{00000000-0004-0000-0000-00000A000000}"/>
+    <hyperlink ref="B12" r:id="rId12" xr:uid="{00000000-0004-0000-0000-00000B000000}"/>
+    <hyperlink ref="B13" r:id="rId13" xr:uid="{00000000-0004-0000-0000-00000C000000}"/>
+    <hyperlink ref="B14" r:id="rId14" xr:uid="{00000000-0004-0000-0000-00000D000000}"/>
+    <hyperlink ref="B15" r:id="rId15" xr:uid="{00000000-0004-0000-0000-00000E000000}"/>
+    <hyperlink ref="B16" r:id="rId16" xr:uid="{00000000-0004-0000-0000-00000F000000}"/>
+    <hyperlink ref="B17" r:id="rId17" xr:uid="{00000000-0004-0000-0000-000010000000}"/>
+    <hyperlink ref="B18" r:id="rId18" xr:uid="{00000000-0004-0000-0000-000011000000}"/>
+    <hyperlink ref="B19" r:id="rId19" xr:uid="{00000000-0004-0000-0000-000012000000}"/>
+    <hyperlink ref="B20" r:id="rId20" xr:uid="{00000000-0004-0000-0000-000013000000}"/>
+    <hyperlink ref="B21" r:id="rId21" xr:uid="{00000000-0004-0000-0000-000014000000}"/>
+    <hyperlink ref="B22" r:id="rId22" xr:uid="{00000000-0004-0000-0000-000015000000}"/>
+    <hyperlink ref="B23" r:id="rId23" xr:uid="{00000000-0004-0000-0000-000016000000}"/>
+    <hyperlink ref="B24" r:id="rId24" xr:uid="{00000000-0004-0000-0000-000017000000}"/>
+    <hyperlink ref="B25" r:id="rId25" xr:uid="{00000000-0004-0000-0000-000018000000}"/>
+    <hyperlink ref="H25" r:id="rId26" xr:uid="{00000000-0004-0000-0000-000019000000}"/>
+    <hyperlink ref="B26" r:id="rId27" xr:uid="{00000000-0004-0000-0000-00001A000000}"/>
+    <hyperlink ref="H26" r:id="rId28" xr:uid="{00000000-0004-0000-0000-00001B000000}"/>
+    <hyperlink ref="B27" r:id="rId29" xr:uid="{00000000-0004-0000-0000-00001C000000}"/>
+    <hyperlink ref="H27" r:id="rId30" xr:uid="{00000000-0004-0000-0000-00001D000000}"/>
+    <hyperlink ref="B28" r:id="rId31" xr:uid="{00000000-0004-0000-0000-00001E000000}"/>
+    <hyperlink ref="H28" r:id="rId32" xr:uid="{00000000-0004-0000-0000-00001F000000}"/>
+    <hyperlink ref="B29" r:id="rId33" xr:uid="{00000000-0004-0000-0000-000020000000}"/>
+    <hyperlink ref="H29" r:id="rId34" xr:uid="{00000000-0004-0000-0000-000021000000}"/>
+    <hyperlink ref="B30" r:id="rId35" xr:uid="{00000000-0004-0000-0000-000022000000}"/>
+    <hyperlink ref="H30" r:id="rId36" xr:uid="{00000000-0004-0000-0000-000023000000}"/>
+    <hyperlink ref="B31" r:id="rId37" xr:uid="{00000000-0004-0000-0000-000024000000}"/>
+    <hyperlink ref="H31" r:id="rId38" xr:uid="{00000000-0004-0000-0000-000025000000}"/>
+    <hyperlink ref="B32" r:id="rId39" xr:uid="{00000000-0004-0000-0000-000026000000}"/>
+    <hyperlink ref="H32" r:id="rId40" xr:uid="{00000000-0004-0000-0000-000027000000}"/>
+    <hyperlink ref="B33" r:id="rId41" xr:uid="{00000000-0004-0000-0000-000028000000}"/>
+    <hyperlink ref="B34" r:id="rId42" xr:uid="{00000000-0004-0000-0000-000029000000}"/>
+    <hyperlink ref="B38" r:id="rId43" xr:uid="{00000000-0004-0000-0000-00002A000000}"/>
+    <hyperlink ref="B45" r:id="rId44" xr:uid="{00000000-0004-0000-0000-00002B000000}"/>
+    <hyperlink ref="B48" r:id="rId45" xr:uid="{00000000-0004-0000-0000-00002C000000}"/>
+    <hyperlink ref="B35" r:id="rId46" xr:uid="{00000000-0004-0000-0000-00002D000000}"/>
+    <hyperlink ref="B52" r:id="rId47" xr:uid="{00000000-0004-0000-0000-00002E000000}"/>
+    <hyperlink ref="B53" r:id="rId48" xr:uid="{00000000-0004-0000-0000-00002F000000}"/>
+    <hyperlink ref="B55" r:id="rId49" xr:uid="{00000000-0004-0000-0000-000030000000}"/>
+    <hyperlink ref="B56" r:id="rId50" xr:uid="{00000000-0004-0000-0000-000031000000}"/>
+    <hyperlink ref="B57" r:id="rId51" xr:uid="{00000000-0004-0000-0000-000032000000}"/>
+    <hyperlink ref="B58" r:id="rId52" xr:uid="{00000000-0004-0000-0000-000033000000}"/>
+    <hyperlink ref="B61" r:id="rId53" xr:uid="{00000000-0004-0000-0000-000034000000}"/>
+    <hyperlink ref="B62" r:id="rId54" xr:uid="{00000000-0004-0000-0000-000035000000}"/>
+    <hyperlink ref="B63" r:id="rId55" xr:uid="{00000000-0004-0000-0000-000036000000}"/>
+    <hyperlink ref="B64" r:id="rId56" xr:uid="{00000000-0004-0000-0000-000037000000}"/>
+    <hyperlink ref="B65" r:id="rId57" xr:uid="{00000000-0004-0000-0000-000038000000}"/>
+    <hyperlink ref="B66" r:id="rId58" xr:uid="{00000000-0004-0000-0000-000039000000}"/>
+    <hyperlink ref="B67" r:id="rId59" xr:uid="{00000000-0004-0000-0000-00003A000000}"/>
+    <hyperlink ref="H7:H24" r:id="rId60" display="https://www.allhomes.com.au/agency/trusted-realtors-570129/" xr:uid="{00000000-0004-0000-0000-00003B000000}"/>
+    <hyperlink ref="B43" r:id="rId61" xr:uid="{00000000-0004-0000-0000-00003C000000}"/>
+    <hyperlink ref="B44" r:id="rId62" xr:uid="{00000000-0004-0000-0000-00003D000000}"/>
+    <hyperlink ref="B46" r:id="rId63" xr:uid="{00000000-0004-0000-0000-00003E000000}"/>
+    <hyperlink ref="B54" r:id="rId64" xr:uid="{00000000-0004-0000-0000-00003F000000}"/>
+    <hyperlink ref="B42" r:id="rId65" xr:uid="{00000000-0004-0000-0000-000040000000}"/>
+    <hyperlink ref="J2" r:id="rId66" xr:uid="{00000000-0004-0000-0000-000041000000}"/>
+    <hyperlink ref="C69" r:id="rId67" xr:uid="{9DAE03A7-93E8-4507-BD6C-AC4013ECD47F}"/>
+    <hyperlink ref="C68" r:id="rId68" xr:uid="{66B9A9CA-DF82-46B6-9C5A-C5709E2FF1AE}"/>
+    <hyperlink ref="B75" r:id="rId69" xr:uid="{57E7BFEF-6F05-4DA9-A3DE-5B0A0EFED4D9}"/>
+    <hyperlink ref="C75" r:id="rId70" xr:uid="{F4755F93-6E59-4C38-BF66-16746869FDF3}"/>
+    <hyperlink ref="H75" r:id="rId71" xr:uid="{5BFAFD71-42C4-487F-B5E7-1697975992B4}"/>
+    <hyperlink ref="B78" r:id="rId72" xr:uid="{D3DE0D76-2479-4283-B7C7-F11B85797022}"/>
+    <hyperlink ref="C78" r:id="rId73" xr:uid="{FC1D9146-2FDC-4F13-A3C3-51CAB46DEC08}"/>
+    <hyperlink ref="B68" r:id="rId74" xr:uid="{3ED6FAA1-2B0F-4DB9-878E-9640A9C2850D}"/>
+    <hyperlink ref="B69" r:id="rId75" xr:uid="{12DE6CA8-DDC5-4E7B-BD2E-14B105A0DE3B}"/>
+    <hyperlink ref="C70" r:id="rId76" xr:uid="{0419758C-286A-4B76-B8B2-31CC336DEDF1}"/>
+    <hyperlink ref="B70" r:id="rId77" xr:uid="{AC18D1D2-FA3D-4352-A402-35B7AAFE27C0}"/>
+    <hyperlink ref="B71" r:id="rId78" xr:uid="{E8BCA1EF-4E17-4AA7-A2CE-5674FC05ABC3}"/>
+    <hyperlink ref="C71" r:id="rId79" xr:uid="{949AE606-DF4A-48F4-93A0-F148D80842CB}"/>
+    <hyperlink ref="B72" r:id="rId80" xr:uid="{69A93BB5-0295-46D6-8334-45444356E6E9}"/>
+    <hyperlink ref="C72" r:id="rId81" xr:uid="{CA171BC7-126F-4175-8A03-123D5A2C2D8A}"/>
+    <hyperlink ref="C73" r:id="rId82" xr:uid="{FACC205D-E563-4266-8E0D-0794F3D76E98}"/>
+    <hyperlink ref="B85" r:id="rId83" xr:uid="{7ABCABC0-A765-435B-AE52-9D27F653E00F}"/>
+    <hyperlink ref="C4" r:id="rId84" xr:uid="{2CD58DBE-98E3-4EDC-898F-088D5F0FCB81}"/>
+    <hyperlink ref="C29" r:id="rId85" xr:uid="{CB7CAD83-ACA3-4309-B102-B0F536FC97E6}"/>
+    <hyperlink ref="C90" r:id="rId86" xr:uid="{B4F55488-2B40-4078-ABF0-4B4254363237}"/>
+    <hyperlink ref="B90" r:id="rId87" xr:uid="{09FEE7FE-E667-40E8-BC22-3FDC999B614F}"/>
+    <hyperlink ref="C15" r:id="rId88" xr:uid="{34F25BA9-B460-46CF-85C0-4AC9D6288B41}"/>
+    <hyperlink ref="C3" r:id="rId89" xr:uid="{EBAAEE7A-83B2-457B-8600-89427BF11448}"/>
+    <hyperlink ref="C8" r:id="rId90" xr:uid="{3D3D678C-8F1B-47BC-ACA2-D1CBF5A76F0B}"/>
+    <hyperlink ref="C19" r:id="rId91" xr:uid="{ED2C9A9B-3440-4B4A-91A1-7CAF84972535}"/>
+    <hyperlink ref="C20" r:id="rId92" xr:uid="{E47C999F-11AE-4F93-9032-6E51EB582635}"/>
+    <hyperlink ref="C21" r:id="rId93" xr:uid="{E59411CC-EC13-4665-969A-8D9238CCD0C2}"/>
+    <hyperlink ref="C33" r:id="rId94" xr:uid="{9C953AB9-0076-4477-B52F-C393846B1211}"/>
+    <hyperlink ref="C38" r:id="rId95" xr:uid="{D349EA20-36BF-44C7-A16B-E85B8FE53B2A}"/>
+    <hyperlink ref="C39" r:id="rId96" xr:uid="{DE18DA3B-1A3D-4613-888E-7F506CC87091}"/>
+    <hyperlink ref="C40" r:id="rId97" xr:uid="{0C71282B-049B-4CD1-A090-B66647F2B29B}"/>
+    <hyperlink ref="C42" r:id="rId98" xr:uid="{AD0DC851-DEC5-4ACE-B928-50149068BB70}"/>
+    <hyperlink ref="C45" r:id="rId99" xr:uid="{EB51DFC2-D28F-4E0C-B019-F9954D6C9832}"/>
+    <hyperlink ref="C52" r:id="rId100" xr:uid="{9E5146F6-8EC8-4A2C-B192-C1CCB11CAB8A}"/>
+    <hyperlink ref="C48" r:id="rId101" xr:uid="{31B308E4-DA3E-401B-B796-7D03404228FB}"/>
+    <hyperlink ref="C49" r:id="rId102" xr:uid="{EBAAB9CE-7F91-4628-AF75-32C4EEF948C2}"/>
+    <hyperlink ref="C53" r:id="rId103" xr:uid="{2FF7EB1F-CD56-4E71-AD0F-0D12E8347603}"/>
+    <hyperlink ref="C55" r:id="rId104" xr:uid="{9BD44DCD-EEBB-4649-9792-F3DAC40B3960}"/>
+    <hyperlink ref="C63" r:id="rId105" xr:uid="{9929BCF4-32FD-4143-99F6-FEB21B90BCD7}"/>
+    <hyperlink ref="C64" r:id="rId106" xr:uid="{80B3DEC9-506E-4F3A-B171-A2D71B731577}"/>
+    <hyperlink ref="C66" r:id="rId107" xr:uid="{011D2C70-C541-49D4-894E-FF670D6C19BB}"/>
+    <hyperlink ref="C67" r:id="rId108" xr:uid="{B62DFA3B-60A0-44AA-BF1D-BCA2A049E46C}"/>
+    <hyperlink ref="C56" r:id="rId109" xr:uid="{C98B5D5D-65AB-489D-8160-8F1B41CDE6A7}"/>
+    <hyperlink ref="B103" r:id="rId110" xr:uid="{4D81C408-B745-40E2-B9C7-6E36C45175A7}"/>
+    <hyperlink ref="C26" r:id="rId111" xr:uid="{6A9C6F44-3E7F-47CF-8514-B6609EBEE668}"/>
+    <hyperlink ref="C23" r:id="rId112" xr:uid="{F99F350A-C378-4940-B611-41F47BC3B4B0}"/>
+    <hyperlink ref="C103" r:id="rId113" xr:uid="{3E9C8DCE-ABC0-49DA-B64B-B569BAAE6ED0}"/>
+    <hyperlink ref="C104" r:id="rId114" xr:uid="{E96AA061-2DED-4A35-BE99-8E7E156527EB}"/>
+    <hyperlink ref="C102" r:id="rId115" xr:uid="{4DAA7E56-3BCD-4AF1-B6E7-A26B02A0DA6C}"/>
+    <hyperlink ref="C101" r:id="rId116" xr:uid="{EBE0EC7F-0880-4F4A-991C-2C7C53889923}"/>
+    <hyperlink ref="C100" r:id="rId117" xr:uid="{7AA4A2D0-C18F-4625-A776-6EDD2415E1BC}"/>
+    <hyperlink ref="C99" r:id="rId118" xr:uid="{15BFB680-4225-425B-8826-841A35922C8A}"/>
+    <hyperlink ref="B99" r:id="rId119" xr:uid="{1EF2BF94-D92B-41EF-8B1F-0585F1910B74}"/>
+    <hyperlink ref="C97" r:id="rId120" xr:uid="{6687C5A1-CC2B-49FF-B98D-946AA21B8C55}"/>
+    <hyperlink ref="B97" r:id="rId121" xr:uid="{0411E592-2DE8-4D1D-B66C-46CE99CAA412}"/>
+    <hyperlink ref="C96" r:id="rId122" xr:uid="{A7ED7210-DE23-4760-B67F-78027E9B9B73}"/>
+    <hyperlink ref="B96" r:id="rId123" xr:uid="{992F1752-E440-4347-A698-44C8E60F00BE}"/>
+    <hyperlink ref="B102" r:id="rId124" xr:uid="{A0E03FB2-010F-497D-874D-A0A66FB6303C}"/>
+    <hyperlink ref="B101" r:id="rId125" xr:uid="{165FBF6F-9195-42DA-AC37-C49B2308ACA1}"/>
+    <hyperlink ref="B94" r:id="rId126" xr:uid="{7DB2C8A6-8C43-4818-A7C2-D5E14351114B}"/>
+    <hyperlink ref="B93" r:id="rId127" xr:uid="{EFC122F7-44E7-447B-8F21-BA1503A72780}"/>
+    <hyperlink ref="B91" r:id="rId128" xr:uid="{7AC22E1D-6919-43E6-AD91-1551DBBDE570}"/>
+    <hyperlink ref="B88" r:id="rId129" xr:uid="{FB3E9840-E4E3-4E64-8CCF-2BAEC7024AD6}"/>
+    <hyperlink ref="B87" r:id="rId130" xr:uid="{348337ED-A616-4A9D-A8D3-0091262177C6}"/>
+    <hyperlink ref="B86" r:id="rId131" xr:uid="{CF62843D-4B82-47CB-B74F-D3F292E9603A}"/>
+    <hyperlink ref="B84" r:id="rId132" xr:uid="{9CA10EFF-3943-479E-914B-1D6EE04D75FC}"/>
+    <hyperlink ref="C84" r:id="rId133" xr:uid="{1074AAC9-CCB0-4FFC-9AFB-EFD1363D7538}"/>
+    <hyperlink ref="B105" r:id="rId134" xr:uid="{D6DE2797-5A68-4C1E-9E74-0D323B6ADFA2}"/>
+    <hyperlink ref="B106" r:id="rId135" xr:uid="{1FCAF9BA-00B5-4008-B5C8-E822ABD6BCDD}"/>
+    <hyperlink ref="C11" r:id="rId136" xr:uid="{893B2404-B185-41F7-B397-A3E08B386C5F}"/>
+    <hyperlink ref="B107" r:id="rId137" xr:uid="{B0E609F4-D8A3-433A-BE15-17E4804C6EA3}"/>
+    <hyperlink ref="C107" r:id="rId138" xr:uid="{6793ECA4-A034-42EC-A741-3B0FF42BC11B}"/>
+    <hyperlink ref="B108" r:id="rId139" xr:uid="{4DB78F44-0F08-4561-A0E8-0EE92F9FFECB}"/>
+    <hyperlink ref="B114" r:id="rId140" xr:uid="{27750164-38B8-4B5E-9B5A-E6C71FFFC61F}"/>
+    <hyperlink ref="C114" r:id="rId141" xr:uid="{6FE6A043-A6B1-44FF-8A45-8C3690323458}"/>
+    <hyperlink ref="B113" r:id="rId142" xr:uid="{0F94FF41-1E06-4D7B-B360-1EB377073C87}"/>
+    <hyperlink ref="B112" r:id="rId143" xr:uid="{490A5044-10EC-4082-BEC1-14008171D5CF}"/>
+    <hyperlink ref="B49" r:id="rId144" xr:uid="{836EB236-8BF1-4259-B395-AD9FA9DE0AE0}"/>
+    <hyperlink ref="B74" r:id="rId145" xr:uid="{8AA8904A-1CC5-4D06-93EF-66F7FC625199}"/>
+    <hyperlink ref="B76" r:id="rId146" xr:uid="{5743888C-C74A-41C6-ABC5-E9575351702D}"/>
+    <hyperlink ref="B115" r:id="rId147" xr:uid="{27BDB583-8AD0-4B33-BA19-24E42C9E7CE9}"/>
+    <hyperlink ref="B117" r:id="rId148" xr:uid="{92BA6213-0D94-4C5A-B06A-6FC35C0BECA9}"/>
+    <hyperlink ref="B119" r:id="rId149" xr:uid="{6724AE23-65F5-4D67-ADA6-E20BD420531B}"/>
+    <hyperlink ref="C119" r:id="rId150" xr:uid="{0A5009EB-B388-4AF4-99CE-5813711C2B1E}"/>
+    <hyperlink ref="B120" r:id="rId151" xr:uid="{255CB59B-E711-471E-8ACE-D0ABA408AE96}"/>
+    <hyperlink ref="B39" r:id="rId152" xr:uid="{39FB4A7C-4EA8-4530-9FE6-2842C777350C}"/>
+    <hyperlink ref="B104" r:id="rId153" xr:uid="{FC8A6FB5-FCCF-409E-9D6D-A93D412B2275}"/>
+    <hyperlink ref="C105" r:id="rId154" xr:uid="{988B91BF-CEBD-44F6-A773-3C87D877BE5A}"/>
+    <hyperlink ref="C108" r:id="rId155" xr:uid="{F0593E1B-3EE0-4DF2-B93E-84A02071630B}"/>
+    <hyperlink ref="B109" r:id="rId156" xr:uid="{601C40E0-818B-457C-9FE7-30D06707CEB7}"/>
+    <hyperlink ref="C109" r:id="rId157" xr:uid="{E1D93474-1A3D-49F1-B191-3C3484679D2D}"/>
+    <hyperlink ref="C83" r:id="rId158" xr:uid="{B0D57129-C33F-45FF-B844-E7642495443D}"/>
+    <hyperlink ref="B83" r:id="rId159" xr:uid="{7DCBF3E6-0CD2-475D-AE1F-56469491B512}"/>
+    <hyperlink ref="C120" r:id="rId160" xr:uid="{F24698EA-BA1A-4C92-8B6D-72A40DDDD7A3}"/>
+    <hyperlink ref="C122" r:id="rId161" xr:uid="{BAC9069D-9D63-415D-B933-A4F86CB8C587}"/>
+    <hyperlink ref="C123" r:id="rId162" xr:uid="{140A866C-FAC2-4A61-BA7E-0AFB9A05FD2F}"/>
+    <hyperlink ref="C124" r:id="rId163" xr:uid="{6EA83FA2-D552-4B23-98A9-6C5EFC3BC2CA}"/>
+    <hyperlink ref="C125" r:id="rId164" xr:uid="{E34375AF-4BB2-420C-887F-8D684FC72F4C}"/>
+    <hyperlink ref="C126" r:id="rId165" xr:uid="{CB74A187-1404-4E3B-B1EF-E6C50CF09D3E}"/>
+    <hyperlink ref="C127" r:id="rId166" xr:uid="{B0565FA3-8BDF-4E3B-9814-B9F51432FA7D}"/>
+    <hyperlink ref="C128" r:id="rId167" xr:uid="{8504A7CE-7DD9-4C74-83D8-90E0745EAB21}"/>
+    <hyperlink ref="C130" r:id="rId168" xr:uid="{D3DDF4DA-6F84-4EAF-BA60-77D926C7C2AC}"/>
+    <hyperlink ref="C131" r:id="rId169" xr:uid="{060B4F44-BF89-4037-9E74-C61E23C6AAC9}"/>
+    <hyperlink ref="C132" r:id="rId170" xr:uid="{8FD9E395-82BD-4EEA-89E9-166FDA928F87}"/>
+    <hyperlink ref="C133" r:id="rId171" xr:uid="{3669E93D-A9CE-4C72-B1DD-98E95312A18C}"/>
+    <hyperlink ref="C136" r:id="rId172" xr:uid="{E14EBE84-3FBA-44D8-B082-69967148B456}"/>
+    <hyperlink ref="C137" r:id="rId173" xr:uid="{CC0D1827-F782-476A-9312-1BAA88B7D496}"/>
+    <hyperlink ref="C141" r:id="rId174" xr:uid="{1528B515-167A-4838-B645-B63CD0312C05}"/>
+    <hyperlink ref="B143" r:id="rId175" xr:uid="{50B775B1-8A20-4A55-90CA-EC152D3C2098}"/>
+    <hyperlink ref="B144" r:id="rId176" xr:uid="{F6EFF9E5-8AC0-4C40-A2A8-62DF9BB671E9}"/>
+    <hyperlink ref="C145" r:id="rId177" xr:uid="{DE56B3AC-2F1A-494E-A9CD-9C972DA863E2}"/>
+    <hyperlink ref="B145" r:id="rId178" xr:uid="{F783979B-F441-49BC-98C4-8448098CBBC1}"/>
+    <hyperlink ref="C17" r:id="rId179" xr:uid="{DBE3D417-C525-4AE7-BA26-A27F8BD7B6D3}"/>
+    <hyperlink ref="B121" r:id="rId180" xr:uid="{BF1CBD80-282B-4284-A960-458EE8D86966}"/>
+    <hyperlink ref="C146" r:id="rId181" xr:uid="{3FA9DCB7-198C-457D-99E0-AF0A29EDEAF1}"/>
+    <hyperlink ref="B146" r:id="rId182" xr:uid="{6B057403-173E-478A-AFE1-5BA96D6006F7}"/>
+    <hyperlink ref="C147" r:id="rId183" xr:uid="{FBD8EA4A-7B80-4D87-BD4D-6D3DDE043E14}"/>
+    <hyperlink ref="B147" r:id="rId184" xr:uid="{F9D4FD4A-592C-4041-AD52-AAD4E4FECD78}"/>
+    <hyperlink ref="C148" r:id="rId185" xr:uid="{EF3F39F0-4058-49A5-8980-E800B6F200B5}"/>
+    <hyperlink ref="B148" r:id="rId186" xr:uid="{513D1B27-06CF-4F01-AD66-B1DDDB3DF171}"/>
+    <hyperlink ref="C149" r:id="rId187" xr:uid="{BFCDD610-AD9F-445C-AAE8-66DB3CD722A6}"/>
+    <hyperlink ref="B149" r:id="rId188" xr:uid="{1567BEF7-2918-4A3A-89A1-A37D6C6B5419}"/>
+    <hyperlink ref="B150" r:id="rId189" xr:uid="{233679EA-F519-4185-AA17-F008EE8DA109}"/>
+    <hyperlink ref="C153" r:id="rId190" xr:uid="{D979C888-F3D2-4FAE-9C96-C32136017BEF}"/>
+    <hyperlink ref="B153" r:id="rId191" xr:uid="{F7FA0B04-B8E5-4470-AA22-DE86ABDF6874}"/>
   </hyperlinks>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
-  <pageSetup orientation="portrait" paperSize="9" r:id="rId190"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId192"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:AJ153"/>
+  <dimension ref="A1:AI153"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane activePane="bottomLeft" state="frozen" topLeftCell="A134" ySplit="1"/>
-      <selection activeCell="C159" pane="bottomLeft" sqref="C159"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C19" sqref="C19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="14.42578125" defaultRowHeight="15.75"/>
+  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="14.85546875" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="18.140625" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" width="55.5703125" collapsed="true"/>
-    <col min="4" max="4" customWidth="true" width="25.140625" collapsed="true"/>
-    <col min="5" max="5" customWidth="true" width="19.5703125" collapsed="true"/>
-    <col min="6" max="6" customWidth="true" width="19.85546875" collapsed="true"/>
-    <col min="7" max="7" customWidth="true" width="18.5703125" collapsed="true"/>
-    <col min="8" max="8" customWidth="true" width="32.140625" collapsed="true"/>
-    <col min="9" max="9" customWidth="true" width="20.5703125" collapsed="true"/>
-    <col min="10" max="10" customWidth="true" width="21.140625" collapsed="true"/>
-    <col min="11" max="11" customWidth="true" width="28.85546875" collapsed="true"/>
-    <col min="12" max="12" customWidth="true" width="37.5703125" collapsed="true"/>
-    <col min="16" max="17" customWidth="true" width="18.85546875" collapsed="true"/>
-    <col min="18" max="18" customWidth="true" width="47.85546875" collapsed="true"/>
-    <col min="19" max="19" customWidth="true" width="77.5703125" collapsed="true"/>
-    <col min="20" max="20" customWidth="true" width="24.0" collapsed="true"/>
-    <col min="21" max="21" customWidth="true" width="18.85546875" collapsed="true"/>
-    <col min="22" max="31" customWidth="true" width="19.140625" collapsed="true"/>
+    <col min="1" max="1" width="14.85546875" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="18.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="55.5703125" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="25.140625" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="19.5703125" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="19.85546875" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="18.5703125" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="32.140625" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="20.5703125" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="21.140625" customWidth="1" collapsed="1"/>
+    <col min="11" max="11" width="28.85546875" customWidth="1" collapsed="1"/>
+    <col min="12" max="12" width="37.5703125" customWidth="1" collapsed="1"/>
+    <col min="16" max="17" width="18.85546875" customWidth="1" collapsed="1"/>
+    <col min="18" max="18" width="47.85546875" customWidth="1" collapsed="1"/>
+    <col min="19" max="19" width="77.5703125" customWidth="1" collapsed="1"/>
+    <col min="20" max="20" width="24" customWidth="1" collapsed="1"/>
+    <col min="21" max="21" width="18.85546875" customWidth="1" collapsed="1"/>
+    <col min="22" max="31" width="19.140625" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row ht="30" r="1" spans="1:35">
+    <row r="1" spans="1:35" ht="30">
       <c r="A1" s="1" t="s">
         <v>46</v>
       </c>
@@ -10570,7 +10566,7 @@
       <c r="AH1" s="23"/>
       <c r="AI1" s="23"/>
     </row>
-    <row customHeight="1" ht="15" r="2" spans="1:35">
+    <row r="2" spans="1:35" ht="15" customHeight="1">
       <c r="A2" s="24">
         <v>1</v>
       </c>
@@ -10641,7 +10637,7 @@
       <c r="AH2" s="24"/>
       <c r="AI2" s="24"/>
     </row>
-    <row customHeight="1" ht="15" r="3" spans="1:35">
+    <row r="3" spans="1:35" ht="15" customHeight="1">
       <c r="A3" s="24">
         <v>2</v>
       </c>
@@ -10712,7 +10708,7 @@
       <c r="AH3" s="24"/>
       <c r="AI3" s="24"/>
     </row>
-    <row customFormat="1" customHeight="1" ht="15" r="4" s="24" spans="1:35">
+    <row r="4" spans="1:35" s="24" customFormat="1" ht="15" customHeight="1">
       <c r="A4" s="24">
         <v>3</v>
       </c>
@@ -10774,7 +10770,7 @@
         <v>8</v>
       </c>
     </row>
-    <row customHeight="1" ht="15" r="5" spans="1:35">
+    <row r="5" spans="1:35" ht="15" customHeight="1">
       <c r="A5" s="24">
         <v>4</v>
       </c>
@@ -10847,7 +10843,7 @@
       <c r="AH5" s="24"/>
       <c r="AI5" s="24"/>
     </row>
-    <row customFormat="1" customHeight="1" ht="15" r="6" s="24" spans="1:35">
+    <row r="6" spans="1:35" s="24" customFormat="1" ht="15" customHeight="1">
       <c r="A6" s="24">
         <v>5</v>
       </c>
@@ -10906,7 +10902,7 @@
         <v>16</v>
       </c>
     </row>
-    <row customFormat="1" customHeight="1" ht="15" r="7" s="24" spans="1:35">
+    <row r="7" spans="1:35" s="24" customFormat="1" ht="15" customHeight="1">
       <c r="A7" s="24">
         <v>6</v>
       </c>
@@ -10965,7 +10961,7 @@
         <v>16</v>
       </c>
     </row>
-    <row customFormat="1" customHeight="1" ht="15" r="8" s="24" spans="1:35">
+    <row r="8" spans="1:35" s="24" customFormat="1" ht="15" customHeight="1">
       <c r="A8" s="24">
         <v>7</v>
       </c>
@@ -11021,7 +11017,7 @@
         <v>16</v>
       </c>
     </row>
-    <row customFormat="1" customHeight="1" ht="15" r="9" s="24" spans="1:35">
+    <row r="9" spans="1:35" s="24" customFormat="1" ht="15" customHeight="1">
       <c r="A9" s="24">
         <v>8</v>
       </c>
@@ -11080,7 +11076,7 @@
         <v>16</v>
       </c>
     </row>
-    <row customFormat="1" customHeight="1" ht="15" r="10" s="24" spans="1:35">
+    <row r="10" spans="1:35" s="24" customFormat="1" ht="15" customHeight="1">
       <c r="A10" s="24">
         <v>9</v>
       </c>
@@ -11136,12 +11132,12 @@
         <v>16</v>
       </c>
     </row>
-    <row customFormat="1" customHeight="1" ht="15" r="11" s="24" spans="1:35">
+    <row r="11" spans="1:35" s="24" customFormat="1" ht="15" customHeight="1">
       <c r="A11" s="24">
         <v>10</v>
       </c>
-      <c r="B11" s="24" t="s">
-        <v>7</v>
+      <c r="B11" s="46" t="s">
+        <v>1123</v>
       </c>
       <c r="C11" s="24" t="s">
         <v>110</v>
@@ -11182,7 +11178,7 @@
       <c r="R11" s="24" t="s">
         <v>113</v>
       </c>
-      <c r="S11" s="24" t="s">
+      <c r="S11" s="47" t="s">
         <v>1093</v>
       </c>
       <c r="T11" s="24" t="s">
@@ -11201,7 +11197,7 @@
         <v>114</v>
       </c>
     </row>
-    <row customFormat="1" customHeight="1" ht="15" r="12" s="24" spans="1:35">
+    <row r="12" spans="1:35" s="24" customFormat="1" ht="15" customHeight="1">
       <c r="A12" s="24">
         <v>11</v>
       </c>
@@ -11257,7 +11253,7 @@
         <v>16</v>
       </c>
     </row>
-    <row customFormat="1" customHeight="1" ht="15" r="13" s="24" spans="1:35">
+    <row r="13" spans="1:35" s="24" customFormat="1" ht="15" customHeight="1">
       <c r="A13" s="24">
         <v>12</v>
       </c>
@@ -11316,7 +11312,7 @@
         <v>114</v>
       </c>
     </row>
-    <row customFormat="1" customHeight="1" ht="15" r="14" s="24" spans="1:35">
+    <row r="14" spans="1:35" s="24" customFormat="1" ht="15" customHeight="1">
       <c r="A14" s="24">
         <v>13</v>
       </c>
@@ -11381,7 +11377,7 @@
         <v>114</v>
       </c>
     </row>
-    <row customFormat="1" customHeight="1" ht="15" r="15" s="24" spans="1:35">
+    <row r="15" spans="1:35" s="24" customFormat="1" ht="15" customHeight="1">
       <c r="A15" s="24">
         <v>14</v>
       </c>
@@ -11440,7 +11436,7 @@
         <v>16</v>
       </c>
     </row>
-    <row customFormat="1" customHeight="1" ht="15" r="16" s="24" spans="1:35">
+    <row r="16" spans="1:35" s="24" customFormat="1" ht="15" customHeight="1">
       <c r="A16" s="24">
         <v>15</v>
       </c>
@@ -11499,7 +11495,7 @@
         <v>16</v>
       </c>
     </row>
-    <row customFormat="1" customHeight="1" ht="15" r="17" s="24" spans="1:35">
+    <row r="17" spans="1:35" s="24" customFormat="1" ht="15" customHeight="1">
       <c r="A17" s="24">
         <v>16</v>
       </c>
@@ -11555,7 +11551,7 @@
         <v>16</v>
       </c>
     </row>
-    <row customFormat="1" customHeight="1" ht="15" r="18" s="24" spans="1:35">
+    <row r="18" spans="1:35" s="24" customFormat="1" ht="15" customHeight="1">
       <c r="A18" s="24">
         <v>17</v>
       </c>
@@ -11614,7 +11610,7 @@
         <v>16</v>
       </c>
     </row>
-    <row customFormat="1" customHeight="1" ht="15" r="19" s="24" spans="1:35">
+    <row r="19" spans="1:35" s="24" customFormat="1" ht="15" customHeight="1">
       <c r="A19" s="24">
         <v>18</v>
       </c>
@@ -11670,7 +11666,7 @@
         <v>16</v>
       </c>
     </row>
-    <row customHeight="1" ht="15" r="20" spans="1:35">
+    <row r="20" spans="1:35" ht="15" customHeight="1">
       <c r="A20" s="24">
         <v>19</v>
       </c>
@@ -11745,7 +11741,7 @@
       <c r="AH20" s="24"/>
       <c r="AI20" s="24"/>
     </row>
-    <row customFormat="1" customHeight="1" ht="15" r="21" s="24" spans="1:35">
+    <row r="21" spans="1:35" s="24" customFormat="1" ht="15" customHeight="1">
       <c r="A21" s="24">
         <v>20</v>
       </c>
@@ -11801,7 +11797,7 @@
         <v>16</v>
       </c>
     </row>
-    <row customFormat="1" customHeight="1" ht="15" r="22" s="24" spans="1:35">
+    <row r="22" spans="1:35" s="24" customFormat="1" ht="15" customHeight="1">
       <c r="A22" s="24">
         <v>21</v>
       </c>
@@ -11866,7 +11862,7 @@
         <v>114</v>
       </c>
     </row>
-    <row customFormat="1" customHeight="1" ht="15" r="23" s="24" spans="1:35">
+    <row r="23" spans="1:35" s="24" customFormat="1" ht="15" customHeight="1">
       <c r="A23" s="24">
         <v>22</v>
       </c>
@@ -11919,7 +11915,7 @@
         <v>16</v>
       </c>
     </row>
-    <row customFormat="1" customHeight="1" ht="15" r="24" s="24" spans="1:35">
+    <row r="24" spans="1:35" s="24" customFormat="1" ht="15" customHeight="1">
       <c r="A24" s="24">
         <v>23</v>
       </c>
@@ -11978,7 +11974,7 @@
         <v>16</v>
       </c>
     </row>
-    <row customHeight="1" ht="15" r="25" spans="1:35">
+    <row r="25" spans="1:35" ht="15" customHeight="1">
       <c r="A25" s="24">
         <v>24</v>
       </c>
@@ -12049,7 +12045,7 @@
       <c r="AH25" s="24"/>
       <c r="AI25" s="24"/>
     </row>
-    <row customFormat="1" customHeight="1" ht="15" r="26" s="24" spans="1:35">
+    <row r="26" spans="1:35" s="24" customFormat="1" ht="15" customHeight="1">
       <c r="A26" s="24">
         <v>25</v>
       </c>
@@ -12108,7 +12104,7 @@
         <v>37</v>
       </c>
     </row>
-    <row customFormat="1" customHeight="1" ht="15" r="27" s="24" spans="1:35">
+    <row r="27" spans="1:35" s="24" customFormat="1" ht="15" customHeight="1">
       <c r="A27" s="24">
         <v>26</v>
       </c>
@@ -12167,7 +12163,7 @@
         <v>37</v>
       </c>
     </row>
-    <row customFormat="1" customHeight="1" ht="15" r="28" s="24" spans="1:35">
+    <row r="28" spans="1:35" s="24" customFormat="1" ht="15" customHeight="1">
       <c r="A28" s="24">
         <v>27</v>
       </c>
@@ -12226,7 +12222,7 @@
         <v>37</v>
       </c>
     </row>
-    <row customFormat="1" customHeight="1" ht="15" r="29" s="24" spans="1:35">
+    <row r="29" spans="1:35" s="24" customFormat="1" ht="15" customHeight="1">
       <c r="A29" s="24">
         <v>28</v>
       </c>
@@ -12285,7 +12281,7 @@
         <v>37</v>
       </c>
     </row>
-    <row customFormat="1" customHeight="1" ht="15" r="30" s="24" spans="1:35">
+    <row r="30" spans="1:35" s="24" customFormat="1" ht="15" customHeight="1">
       <c r="A30" s="24">
         <v>29</v>
       </c>
@@ -12344,7 +12340,7 @@
         <v>37</v>
       </c>
     </row>
-    <row customFormat="1" customHeight="1" ht="15" r="31" s="24" spans="1:35">
+    <row r="31" spans="1:35" s="24" customFormat="1" ht="15" customHeight="1">
       <c r="A31" s="24">
         <v>30</v>
       </c>
@@ -12400,7 +12396,7 @@
         <v>37</v>
       </c>
     </row>
-    <row customFormat="1" customHeight="1" ht="15" r="32" s="24" spans="1:35">
+    <row r="32" spans="1:35" s="24" customFormat="1" ht="15" customHeight="1">
       <c r="A32" s="24">
         <v>31</v>
       </c>
@@ -12459,7 +12455,7 @@
         <v>37</v>
       </c>
     </row>
-    <row customFormat="1" ht="14.25" r="33" s="24" spans="1:21">
+    <row r="33" spans="1:21" s="24" customFormat="1" ht="14.25">
       <c r="A33" s="24" t="s">
         <v>195</v>
       </c>
@@ -12518,7 +12514,7 @@
         <v>8</v>
       </c>
     </row>
-    <row customFormat="1" ht="14.25" r="34" s="24" spans="1:21">
+    <row r="34" spans="1:21" s="24" customFormat="1" ht="14.25">
       <c r="A34" s="24" t="s">
         <v>206</v>
       </c>
@@ -12577,7 +12573,7 @@
         <v>8</v>
       </c>
     </row>
-    <row customFormat="1" ht="14.25" r="35" s="24" spans="1:21">
+    <row r="35" spans="1:21" s="24" customFormat="1" ht="14.25">
       <c r="A35" s="24" t="s">
         <v>213</v>
       </c>
@@ -12636,7 +12632,7 @@
         <v>8</v>
       </c>
     </row>
-    <row customFormat="1" ht="14.25" r="36" s="24" spans="1:21">
+    <row r="36" spans="1:21" s="24" customFormat="1" ht="14.25">
       <c r="A36" s="24" t="s">
         <v>219</v>
       </c>
@@ -12695,7 +12691,7 @@
         <v>8</v>
       </c>
     </row>
-    <row customFormat="1" ht="14.25" r="37" s="24" spans="1:21">
+    <row r="37" spans="1:21" s="24" customFormat="1" ht="14.25">
       <c r="A37" s="24" t="s">
         <v>226</v>
       </c>
@@ -12754,7 +12750,7 @@
         <v>8</v>
       </c>
     </row>
-    <row customFormat="1" ht="14.25" r="38" s="24" spans="1:21">
+    <row r="38" spans="1:21" s="24" customFormat="1" ht="14.25">
       <c r="A38" s="24" t="s">
         <v>232</v>
       </c>
@@ -12813,7 +12809,7 @@
         <v>8</v>
       </c>
     </row>
-    <row customFormat="1" ht="14.25" r="39" s="24" spans="1:21">
+    <row r="39" spans="1:21" s="24" customFormat="1" ht="14.25">
       <c r="A39" s="24" t="s">
         <v>240</v>
       </c>
@@ -12872,7 +12868,7 @@
         <v>8</v>
       </c>
     </row>
-    <row customFormat="1" ht="14.25" r="40" s="24" spans="1:21">
+    <row r="40" spans="1:21" s="24" customFormat="1" ht="14.25">
       <c r="A40" s="24" t="s">
         <v>243</v>
       </c>
@@ -12931,7 +12927,7 @@
         <v>8</v>
       </c>
     </row>
-    <row customFormat="1" ht="14.25" r="41" s="24" spans="1:21">
+    <row r="41" spans="1:21" s="24" customFormat="1" ht="14.25">
       <c r="A41" s="24" t="s">
         <v>246</v>
       </c>
@@ -12990,7 +12986,7 @@
         <v>8</v>
       </c>
     </row>
-    <row customFormat="1" ht="14.25" r="42" s="24" spans="1:21">
+    <row r="42" spans="1:21" s="24" customFormat="1" ht="14.25">
       <c r="A42" s="24" t="s">
         <v>255</v>
       </c>
@@ -13049,7 +13045,7 @@
         <v>8</v>
       </c>
     </row>
-    <row customFormat="1" ht="14.25" r="43" s="24" spans="1:21">
+    <row r="43" spans="1:21" s="24" customFormat="1" ht="14.25">
       <c r="A43" s="24" t="s">
         <v>259</v>
       </c>
@@ -13108,7 +13104,7 @@
         <v>8</v>
       </c>
     </row>
-    <row customFormat="1" ht="14.25" r="44" s="24" spans="1:21">
+    <row r="44" spans="1:21" s="24" customFormat="1" ht="14.25">
       <c r="A44" s="24" t="s">
         <v>268</v>
       </c>
@@ -13167,7 +13163,7 @@
         <v>8</v>
       </c>
     </row>
-    <row customFormat="1" ht="14.25" r="45" s="24" spans="1:21">
+    <row r="45" spans="1:21" s="24" customFormat="1" ht="14.25">
       <c r="A45" s="24" t="s">
         <v>275</v>
       </c>
@@ -13226,7 +13222,7 @@
         <v>37</v>
       </c>
     </row>
-    <row customFormat="1" ht="14.25" r="46" s="24" spans="1:21">
+    <row r="46" spans="1:21" s="24" customFormat="1" ht="14.25">
       <c r="A46" s="24" t="s">
         <v>281</v>
       </c>
@@ -13285,7 +13281,7 @@
         <v>37</v>
       </c>
     </row>
-    <row customFormat="1" ht="14.25" r="47" s="24" spans="1:21">
+    <row r="47" spans="1:21" s="24" customFormat="1" ht="14.25">
       <c r="A47" s="24" t="s">
         <v>287</v>
       </c>
@@ -13344,7 +13340,7 @@
         <v>37</v>
       </c>
     </row>
-    <row customFormat="1" ht="14.25" r="48" s="24" spans="1:21">
+    <row r="48" spans="1:21" s="24" customFormat="1" ht="14.25">
       <c r="A48" s="24" t="s">
         <v>293</v>
       </c>
@@ -13403,7 +13399,7 @@
         <v>16</v>
       </c>
     </row>
-    <row customFormat="1" ht="14.25" r="49" s="24" spans="1:21">
+    <row r="49" spans="1:21" s="24" customFormat="1" ht="14.25">
       <c r="A49" s="24" t="s">
         <v>298</v>
       </c>
@@ -13462,7 +13458,7 @@
         <v>16</v>
       </c>
     </row>
-    <row customFormat="1" ht="14.25" r="50" s="24" spans="1:21">
+    <row r="50" spans="1:21" s="24" customFormat="1" ht="14.25">
       <c r="A50" s="24" t="s">
         <v>304</v>
       </c>
@@ -13521,7 +13517,7 @@
         <v>16</v>
       </c>
     </row>
-    <row customFormat="1" ht="14.25" r="51" s="24" spans="1:21">
+    <row r="51" spans="1:21" s="24" customFormat="1" ht="14.25">
       <c r="A51" s="24" t="s">
         <v>310</v>
       </c>
@@ -13580,7 +13576,7 @@
         <v>16</v>
       </c>
     </row>
-    <row customFormat="1" ht="14.25" r="52" s="24" spans="1:21">
+    <row r="52" spans="1:21" s="24" customFormat="1" ht="14.25">
       <c r="A52" s="24" t="s">
         <v>316</v>
       </c>
@@ -13639,7 +13635,7 @@
         <v>16</v>
       </c>
     </row>
-    <row customFormat="1" ht="14.25" r="53" s="24" spans="1:21">
+    <row r="53" spans="1:21" s="24" customFormat="1" ht="14.25">
       <c r="A53" s="24" t="s">
         <v>343</v>
       </c>
@@ -13698,7 +13694,7 @@
         <v>325</v>
       </c>
     </row>
-    <row customFormat="1" ht="14.25" r="54" s="24" spans="1:21">
+    <row r="54" spans="1:21" s="24" customFormat="1" ht="14.25">
       <c r="A54" s="24" t="s">
         <v>349</v>
       </c>
@@ -13757,7 +13753,7 @@
         <v>325</v>
       </c>
     </row>
-    <row customFormat="1" ht="14.25" r="55" s="24" spans="1:21">
+    <row r="55" spans="1:21" s="24" customFormat="1" ht="14.25">
       <c r="A55" s="24" t="s">
         <v>353</v>
       </c>
@@ -13816,7 +13812,7 @@
         <v>325</v>
       </c>
     </row>
-    <row customFormat="1" ht="14.25" r="56" s="24" spans="1:21">
+    <row r="56" spans="1:21" s="24" customFormat="1" ht="14.25">
       <c r="A56" s="24" t="s">
         <v>359</v>
       </c>
@@ -13875,7 +13871,7 @@
         <v>325</v>
       </c>
     </row>
-    <row customFormat="1" ht="14.25" r="57" s="24" spans="1:21">
+    <row r="57" spans="1:21" s="24" customFormat="1" ht="14.25">
       <c r="A57" s="24" t="s">
         <v>364</v>
       </c>
@@ -13934,7 +13930,7 @@
         <v>325</v>
       </c>
     </row>
-    <row customFormat="1" ht="14.25" r="58" s="24" spans="1:21">
+    <row r="58" spans="1:21" s="24" customFormat="1" ht="14.25">
       <c r="A58" s="24" t="s">
         <v>371</v>
       </c>
@@ -13993,7 +13989,7 @@
         <v>325</v>
       </c>
     </row>
-    <row customFormat="1" ht="14.25" r="59" s="24" spans="1:21">
+    <row r="59" spans="1:21" s="24" customFormat="1" ht="14.25">
       <c r="A59" s="24" t="s">
         <v>377</v>
       </c>
@@ -14052,7 +14048,7 @@
         <v>325</v>
       </c>
     </row>
-    <row customFormat="1" ht="14.25" r="60" s="24" spans="1:21">
+    <row r="60" spans="1:21" s="24" customFormat="1" ht="14.25">
       <c r="A60" s="24" t="s">
         <v>384</v>
       </c>
@@ -14111,7 +14107,7 @@
         <v>325</v>
       </c>
     </row>
-    <row customFormat="1" ht="14.25" r="61" s="24" spans="1:21">
+    <row r="61" spans="1:21" s="24" customFormat="1" ht="14.25">
       <c r="A61" s="24" t="s">
         <v>391</v>
       </c>
@@ -14170,7 +14166,7 @@
         <v>325</v>
       </c>
     </row>
-    <row customFormat="1" ht="14.25" r="62" s="24" spans="1:21">
+    <row r="62" spans="1:21" s="24" customFormat="1" ht="14.25">
       <c r="A62" s="24" t="s">
         <v>397</v>
       </c>
@@ -14229,7 +14225,7 @@
         <v>8</v>
       </c>
     </row>
-    <row customFormat="1" ht="14.25" r="63" s="24" spans="1:21">
+    <row r="63" spans="1:21" s="24" customFormat="1" ht="14.25">
       <c r="A63" s="24" t="s">
         <v>400</v>
       </c>
@@ -14288,7 +14284,7 @@
         <v>8</v>
       </c>
     </row>
-    <row customFormat="1" ht="14.25" r="64" s="24" spans="1:21">
+    <row r="64" spans="1:21" s="24" customFormat="1" ht="14.25">
       <c r="A64" s="24" t="s">
         <v>405</v>
       </c>
@@ -14347,7 +14343,7 @@
         <v>8</v>
       </c>
     </row>
-    <row customFormat="1" ht="14.25" r="65" s="24" spans="1:21">
+    <row r="65" spans="1:21" s="24" customFormat="1" ht="14.25">
       <c r="A65" s="24" t="s">
         <v>411</v>
       </c>
@@ -14406,7 +14402,7 @@
         <v>8</v>
       </c>
     </row>
-    <row customFormat="1" ht="14.25" r="66" s="24" spans="1:21">
+    <row r="66" spans="1:21" s="24" customFormat="1" ht="14.25">
       <c r="A66" s="24" t="s">
         <v>416</v>
       </c>
@@ -14465,7 +14461,7 @@
         <v>37</v>
       </c>
     </row>
-    <row customFormat="1" ht="14.25" r="67" s="24" spans="1:21">
+    <row r="67" spans="1:21" s="24" customFormat="1" ht="14.25">
       <c r="A67" s="24" t="s">
         <v>422</v>
       </c>
@@ -14524,7 +14520,7 @@
         <v>16</v>
       </c>
     </row>
-    <row customFormat="1" ht="14.25" r="68" s="24" spans="1:21">
+    <row r="68" spans="1:21" s="24" customFormat="1" ht="14.25">
       <c r="A68" s="24" t="s">
         <v>483</v>
       </c>
@@ -14583,7 +14579,7 @@
         <v>8</v>
       </c>
     </row>
-    <row customFormat="1" ht="14.25" r="69" s="24" spans="1:21">
+    <row r="69" spans="1:21" s="24" customFormat="1" ht="14.25">
       <c r="A69" s="24" t="s">
         <v>488</v>
       </c>
@@ -14642,7 +14638,7 @@
         <v>8</v>
       </c>
     </row>
-    <row customFormat="1" ht="14.25" r="70" s="24" spans="1:21">
+    <row r="70" spans="1:21" s="24" customFormat="1" ht="14.25">
       <c r="A70" s="24" t="s">
         <v>490</v>
       </c>
@@ -14701,7 +14697,7 @@
         <v>8</v>
       </c>
     </row>
-    <row customFormat="1" ht="14.25" r="71" s="24" spans="1:21">
+    <row r="71" spans="1:21" s="24" customFormat="1" ht="14.25">
       <c r="A71" s="24" t="s">
         <v>496</v>
       </c>
@@ -14760,7 +14756,7 @@
         <v>8</v>
       </c>
     </row>
-    <row customFormat="1" ht="14.25" r="72" s="24" spans="1:21">
+    <row r="72" spans="1:21" s="24" customFormat="1" ht="14.25">
       <c r="A72" s="24" t="s">
         <v>501</v>
       </c>
@@ -14819,7 +14815,7 @@
         <v>8</v>
       </c>
     </row>
-    <row customFormat="1" ht="14.25" r="73" s="24" spans="1:21">
+    <row r="73" spans="1:21" s="24" customFormat="1" ht="14.25">
       <c r="A73" s="24" t="s">
         <v>503</v>
       </c>
@@ -14878,7 +14874,7 @@
         <v>16</v>
       </c>
     </row>
-    <row customFormat="1" ht="14.25" r="74" s="24" spans="1:21">
+    <row r="74" spans="1:21" s="24" customFormat="1" ht="14.25">
       <c r="A74" s="24" t="s">
         <v>507</v>
       </c>
@@ -14937,7 +14933,7 @@
         <v>16</v>
       </c>
     </row>
-    <row customFormat="1" ht="14.25" r="75" s="24" spans="1:21">
+    <row r="75" spans="1:21" s="24" customFormat="1" ht="14.25">
       <c r="A75" s="24" t="s">
         <v>513</v>
       </c>
@@ -14996,7 +14992,7 @@
         <v>16</v>
       </c>
     </row>
-    <row customFormat="1" ht="14.25" r="76" s="24" spans="1:21">
+    <row r="76" spans="1:21" s="24" customFormat="1" ht="14.25">
       <c r="A76" s="24" t="s">
         <v>519</v>
       </c>
@@ -15055,7 +15051,7 @@
         <v>16</v>
       </c>
     </row>
-    <row customFormat="1" ht="14.25" r="77" s="24" spans="1:21">
+    <row r="77" spans="1:21" s="24" customFormat="1" ht="14.25">
       <c r="A77" s="24" t="s">
         <v>524</v>
       </c>
@@ -15114,7 +15110,7 @@
         <v>16</v>
       </c>
     </row>
-    <row customFormat="1" ht="14.25" r="78" s="24" spans="1:21">
+    <row r="78" spans="1:21" s="24" customFormat="1" ht="14.25">
       <c r="A78" s="24" t="s">
         <v>531</v>
       </c>
@@ -15173,7 +15169,7 @@
         <v>16</v>
       </c>
     </row>
-    <row customFormat="1" ht="14.25" r="79" s="24" spans="1:21">
+    <row r="79" spans="1:21" s="24" customFormat="1" ht="14.25">
       <c r="A79" s="24" t="s">
         <v>534</v>
       </c>
@@ -15232,7 +15228,7 @@
         <v>16</v>
       </c>
     </row>
-    <row customFormat="1" ht="14.25" r="80" s="24" spans="1:21">
+    <row r="80" spans="1:21" s="24" customFormat="1" ht="14.25">
       <c r="A80" s="24" t="s">
         <v>540</v>
       </c>
@@ -15291,7 +15287,7 @@
         <v>16</v>
       </c>
     </row>
-    <row customFormat="1" ht="14.25" r="81" s="24" spans="1:21">
+    <row r="81" spans="1:21" s="24" customFormat="1" ht="14.25">
       <c r="A81" s="24" t="s">
         <v>547</v>
       </c>
@@ -15350,7 +15346,7 @@
         <v>16</v>
       </c>
     </row>
-    <row customFormat="1" ht="14.25" r="82" s="24" spans="1:21">
+    <row r="82" spans="1:21" s="24" customFormat="1" ht="14.25">
       <c r="A82" s="24" t="s">
         <v>552</v>
       </c>
@@ -15409,7 +15405,7 @@
         <v>16</v>
       </c>
     </row>
-    <row customFormat="1" ht="14.25" r="83" s="24" spans="1:21">
+    <row r="83" spans="1:21" s="24" customFormat="1" ht="14.25">
       <c r="A83" s="24" t="s">
         <v>557</v>
       </c>
@@ -15468,7 +15464,7 @@
         <v>16</v>
       </c>
     </row>
-    <row customFormat="1" ht="14.25" r="84" s="24" spans="1:21">
+    <row r="84" spans="1:21" s="24" customFormat="1" ht="14.25">
       <c r="A84" s="24" t="s">
         <v>560</v>
       </c>
@@ -15527,7 +15523,7 @@
         <v>16</v>
       </c>
     </row>
-    <row customFormat="1" ht="14.25" r="85" s="24" spans="1:21">
+    <row r="85" spans="1:21" s="24" customFormat="1" ht="14.25">
       <c r="A85" s="24" t="s">
         <v>564</v>
       </c>
@@ -15586,7 +15582,7 @@
         <v>16</v>
       </c>
     </row>
-    <row customFormat="1" ht="14.25" r="86" s="24" spans="1:21">
+    <row r="86" spans="1:21" s="24" customFormat="1" ht="14.25">
       <c r="A86" s="24" t="s">
         <v>605</v>
       </c>
@@ -15645,7 +15641,7 @@
         <v>8</v>
       </c>
     </row>
-    <row customFormat="1" ht="14.25" r="87" s="24" spans="1:21">
+    <row r="87" spans="1:21" s="24" customFormat="1" ht="14.25">
       <c r="A87" s="24" t="s">
         <v>609</v>
       </c>
@@ -15704,7 +15700,7 @@
         <v>37</v>
       </c>
     </row>
-    <row customFormat="1" ht="14.25" r="88" s="24" spans="1:21">
+    <row r="88" spans="1:21" s="24" customFormat="1" ht="14.25">
       <c r="A88" s="24" t="s">
         <v>614</v>
       </c>
@@ -15763,7 +15759,7 @@
         <v>37</v>
       </c>
     </row>
-    <row customFormat="1" ht="14.25" r="89" s="24" spans="1:21">
+    <row r="89" spans="1:21" s="24" customFormat="1" ht="14.25">
       <c r="A89" s="24" t="s">
         <v>618</v>
       </c>
@@ -15822,7 +15818,7 @@
         <v>37</v>
       </c>
     </row>
-    <row customFormat="1" ht="14.25" r="90" s="24" spans="1:21">
+    <row r="90" spans="1:21" s="24" customFormat="1" ht="14.25">
       <c r="A90" s="24" t="s">
         <v>624</v>
       </c>
@@ -15881,7 +15877,7 @@
         <v>16</v>
       </c>
     </row>
-    <row customFormat="1" ht="14.25" r="91" s="24" spans="1:21">
+    <row r="91" spans="1:21" s="24" customFormat="1" ht="14.25">
       <c r="A91" s="24" t="s">
         <v>628</v>
       </c>
@@ -15940,7 +15936,7 @@
         <v>16</v>
       </c>
     </row>
-    <row customFormat="1" ht="14.25" r="92" s="24" spans="1:21">
+    <row r="92" spans="1:21" s="24" customFormat="1" ht="14.25">
       <c r="A92" s="24" t="s">
         <v>632</v>
       </c>
@@ -15999,7 +15995,7 @@
         <v>16</v>
       </c>
     </row>
-    <row customFormat="1" ht="14.25" r="93" s="24" spans="1:21">
+    <row r="93" spans="1:21" s="24" customFormat="1" ht="14.25">
       <c r="A93" s="24" t="s">
         <v>635</v>
       </c>
@@ -16058,7 +16054,7 @@
         <v>16</v>
       </c>
     </row>
-    <row customFormat="1" ht="14.25" r="94" s="24" spans="1:21">
+    <row r="94" spans="1:21" s="24" customFormat="1" ht="14.25">
       <c r="A94" s="24" t="s">
         <v>664</v>
       </c>
@@ -16117,7 +16113,7 @@
         <v>8</v>
       </c>
     </row>
-    <row customFormat="1" ht="14.25" r="95" s="24" spans="1:21">
+    <row r="95" spans="1:21" s="24" customFormat="1" ht="14.25">
       <c r="A95" s="24" t="s">
         <v>669</v>
       </c>
@@ -16176,7 +16172,7 @@
         <v>8</v>
       </c>
     </row>
-    <row customFormat="1" ht="14.25" r="96" s="24" spans="1:21">
+    <row r="96" spans="1:21" s="24" customFormat="1" ht="14.25">
       <c r="A96" s="24" t="s">
         <v>673</v>
       </c>
@@ -16235,7 +16231,7 @@
         <v>8</v>
       </c>
     </row>
-    <row customFormat="1" ht="14.25" r="97" s="24" spans="1:21">
+    <row r="97" spans="1:21" s="24" customFormat="1" ht="14.25">
       <c r="A97" s="24" t="s">
         <v>675</v>
       </c>
@@ -16294,7 +16290,7 @@
         <v>37</v>
       </c>
     </row>
-    <row customFormat="1" ht="14.25" r="98" s="24" spans="1:21">
+    <row r="98" spans="1:21" s="24" customFormat="1" ht="14.25">
       <c r="A98" s="24" t="s">
         <v>689</v>
       </c>
@@ -16353,7 +16349,7 @@
         <v>16</v>
       </c>
     </row>
-    <row customFormat="1" ht="14.25" r="99" s="24" spans="1:21">
+    <row r="99" spans="1:21" s="24" customFormat="1" ht="14.25">
       <c r="A99" s="24" t="s">
         <v>706</v>
       </c>
@@ -16412,7 +16408,7 @@
         <v>8</v>
       </c>
     </row>
-    <row customFormat="1" ht="14.25" r="100" s="24" spans="1:21">
+    <row r="100" spans="1:21" s="24" customFormat="1" ht="14.25">
       <c r="A100" s="24" t="s">
         <v>710</v>
       </c>
@@ -16471,7 +16467,7 @@
         <v>37</v>
       </c>
     </row>
-    <row customFormat="1" ht="14.25" r="101" s="24" spans="1:21">
+    <row r="101" spans="1:21" s="24" customFormat="1" ht="14.25">
       <c r="A101" s="24" t="s">
         <v>714</v>
       </c>
@@ -16530,7 +16526,7 @@
         <v>16</v>
       </c>
     </row>
-    <row customFormat="1" ht="14.25" r="102" s="24" spans="1:21">
+    <row r="102" spans="1:21" s="24" customFormat="1" ht="14.25">
       <c r="A102" s="24" t="s">
         <v>744</v>
       </c>
@@ -16589,7 +16585,7 @@
         <v>37</v>
       </c>
     </row>
-    <row customFormat="1" ht="14.25" r="103" s="24" spans="1:21">
+    <row r="103" spans="1:21" s="24" customFormat="1" ht="14.25">
       <c r="A103" s="24" t="s">
         <v>750</v>
       </c>
@@ -16648,7 +16644,7 @@
         <v>16</v>
       </c>
     </row>
-    <row customFormat="1" ht="14.25" r="104" s="24" spans="1:21">
+    <row r="104" spans="1:21" s="24" customFormat="1" ht="14.25">
       <c r="A104" s="24" t="s">
         <v>759</v>
       </c>
@@ -16707,7 +16703,7 @@
         <v>37</v>
       </c>
     </row>
-    <row customFormat="1" ht="14.25" r="105" s="24" spans="1:21">
+    <row r="105" spans="1:21" s="24" customFormat="1" ht="14.25">
       <c r="A105" s="24" t="s">
         <v>769</v>
       </c>
@@ -16766,7 +16762,7 @@
         <v>37</v>
       </c>
     </row>
-    <row customFormat="1" ht="14.25" r="106" s="24" spans="1:21">
+    <row r="106" spans="1:21" s="24" customFormat="1" ht="14.25">
       <c r="A106" s="24" t="s">
         <v>775</v>
       </c>
@@ -16825,7 +16821,7 @@
         <v>37</v>
       </c>
     </row>
-    <row customFormat="1" ht="14.25" r="107" s="24" spans="1:21">
+    <row r="107" spans="1:21" s="24" customFormat="1" ht="14.25">
       <c r="A107" s="24" t="s">
         <v>785</v>
       </c>
@@ -16884,7 +16880,7 @@
         <v>8</v>
       </c>
     </row>
-    <row customFormat="1" ht="14.25" r="108" s="24" spans="1:21">
+    <row r="108" spans="1:21" s="24" customFormat="1" ht="14.25">
       <c r="A108" s="24" t="s">
         <v>790</v>
       </c>
@@ -16943,7 +16939,7 @@
         <v>37</v>
       </c>
     </row>
-    <row customFormat="1" ht="14.25" r="109" s="24" spans="1:21">
+    <row r="109" spans="1:21" s="24" customFormat="1" ht="14.25">
       <c r="A109" s="24" t="s">
         <v>799</v>
       </c>
@@ -17002,7 +16998,7 @@
         <v>37</v>
       </c>
     </row>
-    <row customFormat="1" ht="14.25" r="110" s="24" spans="1:21">
+    <row r="110" spans="1:21" s="24" customFormat="1" ht="14.25">
       <c r="A110" s="24" t="s">
         <v>807</v>
       </c>
@@ -17061,7 +17057,7 @@
         <v>16</v>
       </c>
     </row>
-    <row customFormat="1" ht="14.25" r="111" s="24" spans="1:21">
+    <row r="111" spans="1:21" s="24" customFormat="1" ht="14.25">
       <c r="A111" s="24" t="s">
         <v>812</v>
       </c>
@@ -17120,7 +17116,7 @@
         <v>16</v>
       </c>
     </row>
-    <row customFormat="1" ht="14.25" r="112" s="24" spans="1:21">
+    <row r="112" spans="1:21" s="24" customFormat="1" ht="14.25">
       <c r="A112" s="24" t="s">
         <v>817</v>
       </c>
@@ -17179,7 +17175,7 @@
         <v>16</v>
       </c>
     </row>
-    <row customFormat="1" ht="14.25" r="113" s="24" spans="1:21">
+    <row r="113" spans="1:21" s="24" customFormat="1" ht="14.25">
       <c r="A113" s="24" t="s">
         <v>822</v>
       </c>
@@ -17238,7 +17234,7 @@
         <v>16</v>
       </c>
     </row>
-    <row customFormat="1" ht="14.25" r="114" s="24" spans="1:21">
+    <row r="114" spans="1:21" s="24" customFormat="1" ht="14.25">
       <c r="A114" s="24" t="s">
         <v>833</v>
       </c>
@@ -17297,7 +17293,7 @@
         <v>8</v>
       </c>
     </row>
-    <row customFormat="1" ht="14.25" r="115" s="24" spans="1:21">
+    <row r="115" spans="1:21" s="24" customFormat="1" ht="14.25">
       <c r="A115" s="24" t="s">
         <v>842</v>
       </c>
@@ -17356,7 +17352,7 @@
         <v>325</v>
       </c>
     </row>
-    <row customFormat="1" ht="14.25" r="116" s="24" spans="1:21">
+    <row r="116" spans="1:21" s="24" customFormat="1" ht="14.25">
       <c r="A116" s="24" t="s">
         <v>850</v>
       </c>
@@ -17415,7 +17411,7 @@
         <v>8</v>
       </c>
     </row>
-    <row customFormat="1" ht="14.25" r="117" s="24" spans="1:21">
+    <row r="117" spans="1:21" s="24" customFormat="1" ht="14.25">
       <c r="A117" s="24" t="s">
         <v>857</v>
       </c>
@@ -17474,7 +17470,7 @@
         <v>16</v>
       </c>
     </row>
-    <row customFormat="1" ht="14.25" r="118" s="24" spans="1:21">
+    <row r="118" spans="1:21" s="24" customFormat="1" ht="14.25">
       <c r="A118" s="24" t="s">
         <v>866</v>
       </c>
@@ -17533,7 +17529,7 @@
         <v>37</v>
       </c>
     </row>
-    <row customFormat="1" ht="14.25" r="119" s="24" spans="1:21">
+    <row r="119" spans="1:21" s="24" customFormat="1" ht="14.25">
       <c r="A119" s="24" t="s">
         <v>870</v>
       </c>
@@ -17592,7 +17588,7 @@
         <v>16</v>
       </c>
     </row>
-    <row customFormat="1" ht="14.25" r="120" s="24" spans="1:21">
+    <row r="120" spans="1:21" s="24" customFormat="1" ht="14.25">
       <c r="A120" s="24">
         <v>119</v>
       </c>
@@ -17651,7 +17647,7 @@
         <v>1044</v>
       </c>
     </row>
-    <row customFormat="1" ht="14.25" r="121" s="24" spans="1:21">
+    <row r="121" spans="1:21" s="24" customFormat="1" ht="14.25">
       <c r="A121" s="24" t="s">
         <v>910</v>
       </c>
@@ -17710,7 +17706,7 @@
         <v>1044</v>
       </c>
     </row>
-    <row customFormat="1" ht="14.25" r="122" s="24" spans="1:21">
+    <row r="122" spans="1:21" s="24" customFormat="1" ht="14.25">
       <c r="A122" s="24" t="s">
         <v>915</v>
       </c>
@@ -17769,7 +17765,7 @@
         <v>1044</v>
       </c>
     </row>
-    <row customFormat="1" ht="14.25" r="123" s="24" spans="1:21">
+    <row r="123" spans="1:21" s="24" customFormat="1" ht="14.25">
       <c r="A123" s="24" t="s">
         <v>922</v>
       </c>
@@ -17828,7 +17824,7 @@
         <v>1044</v>
       </c>
     </row>
-    <row customFormat="1" ht="14.25" r="124" s="24" spans="1:21">
+    <row r="124" spans="1:21" s="24" customFormat="1" ht="14.25">
       <c r="A124" s="24" t="s">
         <v>927</v>
       </c>
@@ -17887,7 +17883,7 @@
         <v>1044</v>
       </c>
     </row>
-    <row customFormat="1" ht="14.25" r="125" s="24" spans="1:21">
+    <row r="125" spans="1:21" s="24" customFormat="1" ht="14.25">
       <c r="A125" s="24" t="s">
         <v>930</v>
       </c>
@@ -17946,7 +17942,7 @@
         <v>1044</v>
       </c>
     </row>
-    <row customFormat="1" ht="14.25" r="126" s="24" spans="1:21">
+    <row r="126" spans="1:21" s="24" customFormat="1" ht="14.25">
       <c r="A126" s="24" t="s">
         <v>934</v>
       </c>
@@ -18005,7 +18001,7 @@
         <v>1044</v>
       </c>
     </row>
-    <row customFormat="1" ht="14.25" r="127" s="24" spans="1:21">
+    <row r="127" spans="1:21" s="24" customFormat="1" ht="14.25">
       <c r="A127" s="24" t="s">
         <v>940</v>
       </c>
@@ -18064,7 +18060,7 @@
         <v>1044</v>
       </c>
     </row>
-    <row customFormat="1" ht="14.25" r="128" s="24" spans="1:21">
+    <row r="128" spans="1:21" s="24" customFormat="1" ht="14.25">
       <c r="A128" s="24" t="s">
         <v>946</v>
       </c>
@@ -18123,7 +18119,7 @@
         <v>1044</v>
       </c>
     </row>
-    <row customFormat="1" ht="14.25" r="129" s="24" spans="1:21">
+    <row r="129" spans="1:21" s="24" customFormat="1" ht="14.25">
       <c r="A129" s="24" t="s">
         <v>951</v>
       </c>
@@ -18182,7 +18178,7 @@
         <v>1044</v>
       </c>
     </row>
-    <row customFormat="1" ht="14.25" r="130" s="24" spans="1:21">
+    <row r="130" spans="1:21" s="24" customFormat="1" ht="14.25">
       <c r="A130" s="24" t="s">
         <v>956</v>
       </c>
@@ -18241,7 +18237,7 @@
         <v>1044</v>
       </c>
     </row>
-    <row customFormat="1" ht="14.25" r="131" s="24" spans="1:21">
+    <row r="131" spans="1:21" s="24" customFormat="1" ht="14.25">
       <c r="A131" s="24" t="s">
         <v>960</v>
       </c>
@@ -18300,7 +18296,7 @@
         <v>1044</v>
       </c>
     </row>
-    <row customFormat="1" ht="14.25" r="132" s="24" spans="1:21">
+    <row r="132" spans="1:21" s="24" customFormat="1" ht="14.25">
       <c r="A132" s="24" t="s">
         <v>963</v>
       </c>
@@ -18359,7 +18355,7 @@
         <v>1044</v>
       </c>
     </row>
-    <row customFormat="1" ht="14.25" r="133" s="24" spans="1:21">
+    <row r="133" spans="1:21" s="24" customFormat="1" ht="14.25">
       <c r="A133" s="24" t="s">
         <v>967</v>
       </c>
@@ -18418,7 +18414,7 @@
         <v>1044</v>
       </c>
     </row>
-    <row customFormat="1" ht="14.25" r="134" s="24" spans="1:21">
+    <row r="134" spans="1:21" s="24" customFormat="1" ht="14.25">
       <c r="A134" s="24" t="s">
         <v>972</v>
       </c>
@@ -18477,7 +18473,7 @@
         <v>1044</v>
       </c>
     </row>
-    <row customFormat="1" ht="14.25" r="135" s="24" spans="1:21">
+    <row r="135" spans="1:21" s="24" customFormat="1" ht="14.25">
       <c r="A135" s="24" t="s">
         <v>975</v>
       </c>
@@ -18536,7 +18532,7 @@
         <v>1044</v>
       </c>
     </row>
-    <row customFormat="1" ht="14.25" r="136" s="24" spans="1:21">
+    <row r="136" spans="1:21" s="24" customFormat="1" ht="14.25">
       <c r="A136" s="24" t="s">
         <v>980</v>
       </c>
@@ -18595,7 +18591,7 @@
         <v>1044</v>
       </c>
     </row>
-    <row customFormat="1" ht="14.25" r="137" s="24" spans="1:21">
+    <row r="137" spans="1:21" s="24" customFormat="1" ht="14.25">
       <c r="A137" s="24" t="s">
         <v>986</v>
       </c>
@@ -18654,7 +18650,7 @@
         <v>1044</v>
       </c>
     </row>
-    <row customFormat="1" ht="14.25" r="138" s="24" spans="1:21">
+    <row r="138" spans="1:21" s="24" customFormat="1" ht="14.25">
       <c r="A138" s="24" t="s">
         <v>992</v>
       </c>
@@ -18713,7 +18709,7 @@
         <v>1044</v>
       </c>
     </row>
-    <row customFormat="1" ht="14.25" r="139" s="24" spans="1:21">
+    <row r="139" spans="1:21" s="24" customFormat="1" ht="14.25">
       <c r="A139" s="24" t="s">
         <v>997</v>
       </c>
@@ -18772,7 +18768,7 @@
         <v>1044</v>
       </c>
     </row>
-    <row customFormat="1" ht="14.25" r="140" s="24" spans="1:21">
+    <row r="140" spans="1:21" s="24" customFormat="1" ht="14.25">
       <c r="A140" s="24" t="s">
         <v>1001</v>
       </c>
@@ -18831,7 +18827,7 @@
         <v>1044</v>
       </c>
     </row>
-    <row customFormat="1" ht="14.25" r="141" s="24" spans="1:21">
+    <row r="141" spans="1:21" s="24" customFormat="1" ht="14.25">
       <c r="A141" s="24" t="s">
         <v>1007</v>
       </c>
@@ -18890,7 +18886,7 @@
         <v>1044</v>
       </c>
     </row>
-    <row customFormat="1" ht="14.25" r="142" s="24" spans="1:21">
+    <row r="142" spans="1:21" s="24" customFormat="1" ht="14.25">
       <c r="A142" s="24" t="s">
         <v>1012</v>
       </c>
@@ -18949,7 +18945,7 @@
         <v>1044</v>
       </c>
     </row>
-    <row customFormat="1" ht="14.25" r="143" s="24" spans="1:21">
+    <row r="143" spans="1:21" s="24" customFormat="1" ht="14.25">
       <c r="A143" s="24" t="s">
         <v>1017</v>
       </c>
@@ -19008,7 +19004,7 @@
         <v>37</v>
       </c>
     </row>
-    <row customFormat="1" ht="14.25" r="144" s="24" spans="1:21">
+    <row r="144" spans="1:21" s="24" customFormat="1" ht="14.25">
       <c r="A144" s="24" t="s">
         <v>1051</v>
       </c>
@@ -19067,7 +19063,7 @@
         <v>37</v>
       </c>
     </row>
-    <row customFormat="1" ht="14.25" r="145" s="24" spans="1:21">
+    <row r="145" spans="1:21" s="24" customFormat="1" ht="14.25">
       <c r="A145" s="24" t="s">
         <v>1056</v>
       </c>
@@ -19126,7 +19122,7 @@
         <v>16</v>
       </c>
     </row>
-    <row customFormat="1" ht="14.25" r="146" s="24" spans="1:21">
+    <row r="146" spans="1:21" s="24" customFormat="1" ht="14.25">
       <c r="A146" s="24" t="s">
         <v>1073</v>
       </c>
@@ -19185,7 +19181,7 @@
         <v>8</v>
       </c>
     </row>
-    <row customFormat="1" ht="14.25" r="147" s="24" spans="1:21">
+    <row r="147" spans="1:21" s="24" customFormat="1" ht="14.25">
       <c r="A147" s="24" t="s">
         <v>1078</v>
       </c>
@@ -19244,7 +19240,7 @@
         <v>37</v>
       </c>
     </row>
-    <row customFormat="1" ht="14.25" r="148" s="24" spans="1:21">
+    <row r="148" spans="1:21" s="24" customFormat="1" ht="14.25">
       <c r="A148" s="24" t="s">
         <v>1082</v>
       </c>
@@ -19303,7 +19299,7 @@
         <v>1044</v>
       </c>
     </row>
-    <row customFormat="1" ht="14.25" r="149" s="24" spans="1:21">
+    <row r="149" spans="1:21" s="24" customFormat="1" ht="14.25">
       <c r="A149" s="24" t="s">
         <v>1096</v>
       </c>
@@ -19362,7 +19358,7 @@
         <v>1044</v>
       </c>
     </row>
-    <row customFormat="1" ht="14.25" r="150" s="24" spans="1:21">
+    <row r="150" spans="1:21" s="24" customFormat="1" ht="14.25">
       <c r="A150" s="24" t="s">
         <v>1101</v>
       </c>
@@ -19421,7 +19417,7 @@
         <v>1044</v>
       </c>
     </row>
-    <row customFormat="1" ht="14.25" r="151" s="24" spans="1:21">
+    <row r="151" spans="1:21" s="24" customFormat="1" ht="14.25">
       <c r="A151" s="24" t="s">
         <v>1108</v>
       </c>
@@ -19480,7 +19476,7 @@
         <v>8</v>
       </c>
     </row>
-    <row customFormat="1" ht="14.25" r="152" s="24" spans="1:21">
+    <row r="152" spans="1:21" s="24" customFormat="1" ht="14.25">
       <c r="A152" s="24" t="s">
         <v>1113</v>
       </c>
@@ -19539,71 +19535,75 @@
         <v>1044</v>
       </c>
     </row>
-    <row r="153">
-      <c r="A153" t="s">
-        <v>1122</v>
-      </c>
-      <c r="B153" t="s">
+    <row r="153" spans="1:21" s="24" customFormat="1" ht="14.25">
+      <c r="A153" s="24" t="s">
+        <v>1124</v>
+      </c>
+      <c r="B153" s="24" t="s">
+        <v>7</v>
+      </c>
+      <c r="C153" s="24" t="s">
+        <v>1125</v>
+      </c>
+      <c r="D153" s="24" t="s">
+        <v>77</v>
+      </c>
+      <c r="E153" s="24" t="s">
+        <v>78</v>
+      </c>
+      <c r="F153" s="24" t="s">
+        <v>906</v>
+      </c>
+      <c r="G153" s="24" t="s">
+        <v>1126</v>
+      </c>
+      <c r="H153" s="24" t="s">
+        <v>199</v>
+      </c>
+      <c r="I153" s="24" t="s">
+        <v>198</v>
+      </c>
+      <c r="K153" s="24" t="s">
+        <v>199</v>
+      </c>
+      <c r="L153" s="24" t="s">
+        <v>237</v>
+      </c>
+      <c r="M153" s="24" t="s">
+        <v>202</v>
+      </c>
+      <c r="N153" s="24" t="s">
+        <v>204</v>
+      </c>
+      <c r="P153" s="24" t="s">
+        <v>201</v>
+      </c>
+      <c r="Q153" s="24" t="s">
+        <v>204</v>
+      </c>
+      <c r="R153" s="24" t="s">
+        <v>1125</v>
+      </c>
+      <c r="S153" s="24" t="s">
         <v>1127</v>
       </c>
-      <c r="C153" t="s">
-        <v>1123</v>
-      </c>
-      <c r="D153" t="s">
-        <v>77</v>
-      </c>
-      <c r="E153" t="s">
-        <v>78</v>
-      </c>
-      <c r="F153" t="s">
-        <v>906</v>
-      </c>
-      <c r="G153" t="s">
-        <v>1125</v>
-      </c>
-      <c r="H153" t="s">
-        <v>199</v>
-      </c>
-      <c r="I153" t="s">
-        <v>198</v>
-      </c>
-      <c r="K153" t="s">
-        <v>199</v>
-      </c>
-      <c r="L153" t="s">
-        <v>237</v>
-      </c>
-      <c r="M153" t="s">
-        <v>202</v>
-      </c>
-      <c r="N153" t="s">
-        <v>204</v>
-      </c>
-      <c r="P153" t="s">
-        <v>201</v>
-      </c>
-      <c r="Q153" t="s">
-        <v>204</v>
-      </c>
-      <c r="R153" t="s">
-        <v>1123</v>
-      </c>
-      <c r="S153" t="s">
-        <v>1126</v>
-      </c>
-      <c r="T153" t="s">
+      <c r="T153" s="24" t="s">
         <v>687</v>
       </c>
-      <c r="U153" t="s">
+      <c r="U153" s="24" t="s">
         <v>1044</v>
       </c>
     </row>
   </sheetData>
   <autoFilter ref="E1:E145" xr:uid="{00000000-0001-0000-0100-000000000000}"/>
   <customSheetViews>
-    <customSheetView filter="1" guid="{A7754112-A52F-4ABC-8778-92F04773E53C}" showAutoFilter="1">
-      <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
-      <autoFilter ref="A1:AD33" xr:uid="{37B0B7DD-C8E3-4D3D-97C5-3A0B3A6F3541}">
+    <customSheetView guid="{C25CEB9E-BEC1-4982-90C4-50C84EE1B82A}" filter="1" showAutoFilter="1">
+      <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+      <autoFilter ref="A1:AD33" xr:uid="{90701E33-9B9E-47AF-9FB1-DF354111A6C2}"/>
+    </customSheetView>
+    <customSheetView guid="{A7754112-A52F-4ABC-8778-92F04773E53C}" filter="1" showAutoFilter="1">
+      <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+      <autoFilter ref="A1:AD33" xr:uid="{1C0CC383-E312-4807-81FF-2D69453F21A9}">
         <filterColumn colId="5">
           <filters blank="1">
             <filter val="Strathnairn"/>
@@ -19611,82 +19611,78 @@
         </filterColumn>
       </autoFilter>
     </customSheetView>
-    <customSheetView filter="1" guid="{C25CEB9E-BEC1-4982-90C4-50C84EE1B82A}" showAutoFilter="1">
-      <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
-      <autoFilter ref="A1:AD33" xr:uid="{D44D412F-5057-48D7-A789-A8DDFB1D2F9E}"/>
-    </customSheetView>
   </customSheetViews>
   <conditionalFormatting sqref="A1:AI1">
-    <cfRule dxfId="1" priority="1" type="notContainsBlanks">
+    <cfRule type="notContainsBlanks" dxfId="1" priority="1">
       <formula>LEN(TRIM(A1))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <hyperlinks>
-    <hyperlink r:id="rId1" ref="S2" xr:uid="{00000000-0004-0000-0100-000000000000}"/>
-    <hyperlink r:id="rId2" ref="S3" xr:uid="{00000000-0004-0000-0100-000001000000}"/>
-    <hyperlink r:id="rId3" ref="S4" xr:uid="{00000000-0004-0000-0100-000002000000}"/>
-    <hyperlink r:id="rId4" ref="S5" xr:uid="{00000000-0004-0000-0100-000003000000}"/>
-    <hyperlink r:id="rId5" ref="S6" xr:uid="{00000000-0004-0000-0100-000004000000}"/>
-    <hyperlink r:id="rId6" ref="S7" xr:uid="{00000000-0004-0000-0100-000006000000}"/>
-    <hyperlink r:id="rId7" ref="S8" xr:uid="{00000000-0004-0000-0100-000008000000}"/>
-    <hyperlink r:id="rId8" ref="S9" xr:uid="{00000000-0004-0000-0100-00000A000000}"/>
-    <hyperlink r:id="rId9" ref="S10" xr:uid="{00000000-0004-0000-0100-00000C000000}"/>
-    <hyperlink r:id="rId10" ref="S11" xr:uid="{00000000-0004-0000-0100-00000E000000}"/>
-    <hyperlink r:id="rId11" ref="S12" xr:uid="{00000000-0004-0000-0100-000010000000}"/>
-    <hyperlink r:id="rId12" ref="S14" xr:uid="{00000000-0004-0000-0100-000014000000}"/>
-    <hyperlink r:id="rId13" ref="S15" xr:uid="{00000000-0004-0000-0100-000016000000}"/>
-    <hyperlink r:id="rId14" ref="S16" xr:uid="{00000000-0004-0000-0100-000018000000}"/>
-    <hyperlink r:id="rId15" ref="S17" xr:uid="{00000000-0004-0000-0100-00001A000000}"/>
-    <hyperlink r:id="rId16" ref="S18" xr:uid="{00000000-0004-0000-0100-00001C000000}"/>
-    <hyperlink display="https://www.allhomes.com.au/strathnairn-act-2615?tid=178720657" r:id="rId17" ref="S19" xr:uid="{00000000-0004-0000-0100-00001E000000}"/>
-    <hyperlink r:id="rId18" ref="S20" xr:uid="{00000000-0004-0000-0100-000020000000}"/>
-    <hyperlink r:id="rId19" ref="S21" xr:uid="{00000000-0004-0000-0100-000022000000}"/>
-    <hyperlink r:id="rId20" ref="S22" xr:uid="{00000000-0004-0000-0100-000024000000}"/>
-    <hyperlink r:id="rId21" ref="S32" xr:uid="{00000000-0004-0000-0100-000031000000}"/>
-    <hyperlink r:id="rId22" ref="S31" xr:uid="{00000000-0004-0000-0100-000030000000}"/>
-    <hyperlink r:id="rId23" ref="S30" xr:uid="{00000000-0004-0000-0100-00002F000000}"/>
-    <hyperlink r:id="rId24" ref="S29" xr:uid="{00000000-0004-0000-0100-00002E000000}"/>
-    <hyperlink r:id="rId25" ref="S28" xr:uid="{00000000-0004-0000-0100-00002D000000}"/>
-    <hyperlink r:id="rId26" ref="S27" xr:uid="{00000000-0004-0000-0100-00002C000000}"/>
-    <hyperlink r:id="rId27" ref="S26" xr:uid="{00000000-0004-0000-0100-00002B000000}"/>
-    <hyperlink r:id="rId28" ref="S25" xr:uid="{00000000-0004-0000-0100-00002A000000}"/>
-    <hyperlink r:id="rId29" ref="S24" xr:uid="{00000000-0004-0000-0100-000028000000}"/>
-    <hyperlink display="https://www.allhomes.com.au/ginninderra-estate-act-2615?tid=174799089" r:id="rId30" ref="S23" xr:uid="{00000000-0004-0000-0100-000026000000}"/>
-    <hyperlink display="https://www.allhomes.com.au/browse-sale/greater-queanbeyan-queanbeyan-region-nsw/" r:id="rId31" ref="F145" xr:uid="{4A50D1D1-69A3-4F14-AFDA-4A60EE9976C1}"/>
+    <hyperlink ref="S2" r:id="rId1" xr:uid="{00000000-0004-0000-0100-000000000000}"/>
+    <hyperlink ref="S3" r:id="rId2" xr:uid="{00000000-0004-0000-0100-000001000000}"/>
+    <hyperlink ref="S4" r:id="rId3" xr:uid="{00000000-0004-0000-0100-000002000000}"/>
+    <hyperlink ref="S5" r:id="rId4" xr:uid="{00000000-0004-0000-0100-000003000000}"/>
+    <hyperlink ref="S6" r:id="rId5" xr:uid="{00000000-0004-0000-0100-000004000000}"/>
+    <hyperlink ref="S7" r:id="rId6" xr:uid="{00000000-0004-0000-0100-000006000000}"/>
+    <hyperlink ref="S8" r:id="rId7" xr:uid="{00000000-0004-0000-0100-000008000000}"/>
+    <hyperlink ref="S9" r:id="rId8" xr:uid="{00000000-0004-0000-0100-00000A000000}"/>
+    <hyperlink ref="S10" r:id="rId9" xr:uid="{00000000-0004-0000-0100-00000C000000}"/>
+    <hyperlink ref="S11" r:id="rId10" xr:uid="{00000000-0004-0000-0100-00000E000000}"/>
+    <hyperlink ref="S12" r:id="rId11" xr:uid="{00000000-0004-0000-0100-000010000000}"/>
+    <hyperlink ref="S14" r:id="rId12" xr:uid="{00000000-0004-0000-0100-000014000000}"/>
+    <hyperlink ref="S15" r:id="rId13" xr:uid="{00000000-0004-0000-0100-000016000000}"/>
+    <hyperlink ref="S16" r:id="rId14" xr:uid="{00000000-0004-0000-0100-000018000000}"/>
+    <hyperlink ref="S17" r:id="rId15" xr:uid="{00000000-0004-0000-0100-00001A000000}"/>
+    <hyperlink ref="S18" r:id="rId16" xr:uid="{00000000-0004-0000-0100-00001C000000}"/>
+    <hyperlink ref="S19" r:id="rId17" display="https://www.allhomes.com.au/strathnairn-act-2615?tid=178720657" xr:uid="{00000000-0004-0000-0100-00001E000000}"/>
+    <hyperlink ref="S20" r:id="rId18" xr:uid="{00000000-0004-0000-0100-000020000000}"/>
+    <hyperlink ref="S21" r:id="rId19" xr:uid="{00000000-0004-0000-0100-000022000000}"/>
+    <hyperlink ref="S22" r:id="rId20" xr:uid="{00000000-0004-0000-0100-000024000000}"/>
+    <hyperlink ref="S32" r:id="rId21" xr:uid="{00000000-0004-0000-0100-000031000000}"/>
+    <hyperlink ref="S31" r:id="rId22" xr:uid="{00000000-0004-0000-0100-000030000000}"/>
+    <hyperlink ref="S30" r:id="rId23" xr:uid="{00000000-0004-0000-0100-00002F000000}"/>
+    <hyperlink ref="S29" r:id="rId24" xr:uid="{00000000-0004-0000-0100-00002E000000}"/>
+    <hyperlink ref="S28" r:id="rId25" xr:uid="{00000000-0004-0000-0100-00002D000000}"/>
+    <hyperlink ref="S27" r:id="rId26" xr:uid="{00000000-0004-0000-0100-00002C000000}"/>
+    <hyperlink ref="S26" r:id="rId27" xr:uid="{00000000-0004-0000-0100-00002B000000}"/>
+    <hyperlink ref="S25" r:id="rId28" xr:uid="{00000000-0004-0000-0100-00002A000000}"/>
+    <hyperlink ref="S24" r:id="rId29" xr:uid="{00000000-0004-0000-0100-000028000000}"/>
+    <hyperlink ref="S23" r:id="rId30" display="https://www.allhomes.com.au/ginninderra-estate-act-2615?tid=174799089" xr:uid="{00000000-0004-0000-0100-000026000000}"/>
+    <hyperlink ref="F145" r:id="rId31" display="https://www.allhomes.com.au/browse-sale/greater-queanbeyan-queanbeyan-region-nsw/" xr:uid="{4A50D1D1-69A3-4F14-AFDA-4A60EE9976C1}"/>
   </hyperlinks>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
-  <pageSetup orientation="portrait" paperSize="9" r:id="rId32"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId32"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:AJ1"/>
+  <dimension ref="A1:AI1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="14.42578125" defaultRowHeight="15.75"/>
+  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="16.0" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" width="14.5703125" collapsed="true"/>
-    <col min="4" max="4" customWidth="true" width="16.85546875" collapsed="true"/>
-    <col min="8" max="8" customWidth="true" width="14.5703125" collapsed="true"/>
-    <col min="9" max="9" customWidth="true" width="13.140625" collapsed="true"/>
-    <col min="15" max="15" customWidth="true" width="20.85546875" collapsed="true"/>
-    <col min="21" max="22" customWidth="true" width="19.140625" collapsed="true"/>
-    <col min="23" max="23" customWidth="true" width="20.140625" collapsed="true"/>
-    <col min="24" max="24" customWidth="true" width="19.85546875" collapsed="true"/>
-    <col min="26" max="26" customWidth="true" width="15.85546875" collapsed="true"/>
-    <col min="27" max="27" customWidth="true" width="13.42578125" collapsed="true"/>
-    <col min="28" max="28" customWidth="true" width="15.140625" collapsed="true"/>
-    <col min="29" max="29" customWidth="true" width="16.140625" collapsed="true"/>
-    <col min="30" max="30" customWidth="true" width="15.85546875" collapsed="true"/>
+    <col min="1" max="1" width="16" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="14.5703125" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="16.85546875" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="14.5703125" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="13.140625" customWidth="1" collapsed="1"/>
+    <col min="15" max="15" width="20.85546875" customWidth="1" collapsed="1"/>
+    <col min="21" max="22" width="19.140625" customWidth="1" collapsed="1"/>
+    <col min="23" max="23" width="20.140625" customWidth="1" collapsed="1"/>
+    <col min="24" max="24" width="19.85546875" customWidth="1" collapsed="1"/>
+    <col min="26" max="26" width="15.85546875" customWidth="1" collapsed="1"/>
+    <col min="27" max="27" width="13.42578125" customWidth="1" collapsed="1"/>
+    <col min="28" max="28" width="15.140625" customWidth="1" collapsed="1"/>
+    <col min="29" max="29" width="16.140625" customWidth="1" collapsed="1"/>
+    <col min="30" max="30" width="15.85546875" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row customHeight="1" ht="15.75" r="1" spans="1:35">
+    <row r="1" spans="1:35" ht="15.75" customHeight="1">
       <c r="A1" s="1" t="s">
         <v>46</v>
       </c>
@@ -19785,37 +19781,37 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A1:AI1">
-    <cfRule dxfId="0" priority="1" type="notContainsBlanks">
+    <cfRule type="notContainsBlanks" dxfId="0" priority="1">
       <formula>LEN(TRIM(A1))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
-  <pageSetup orientation="portrait" paperSize="9" r:id="rId1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:H7"/>
+  <dimension ref="A1:G7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane activePane="bottomLeft" state="frozen" topLeftCell="A2" ySplit="1"/>
-      <selection activeCell="D18" pane="bottomLeft" sqref="D18"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D18" sqref="D18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="14.42578125" defaultRowHeight="15.75"/>
+  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="44.85546875" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="19.5703125" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" width="26.42578125" collapsed="true"/>
-    <col min="4" max="4" customWidth="true" width="36.140625" collapsed="true"/>
-    <col min="5" max="5" bestFit="true" customWidth="true" width="53.7109375" collapsed="true"/>
+    <col min="1" max="1" width="44.85546875" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="19.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="26.42578125" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="36.140625" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="53.7109375" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row ht="15" r="1" spans="1:7">
+    <row r="1" spans="1:7" ht="15">
       <c r="A1" s="29" t="s">
         <v>152</v>
       </c>
@@ -19838,7 +19834,7 @@
         <v>157</v>
       </c>
     </row>
-    <row customFormat="1" customHeight="1" ht="15.75" r="2" s="30" spans="1:7">
+    <row r="2" spans="1:7" s="30" customFormat="1" ht="15.75" customHeight="1">
       <c r="A2" s="30" t="s">
         <v>158</v>
       </c>
@@ -19861,7 +19857,7 @@
         <v>7</v>
       </c>
     </row>
-    <row customHeight="1" ht="15.75" r="3" spans="1:7">
+    <row r="3" spans="1:7" ht="15.75" customHeight="1">
       <c r="A3" s="30" t="s">
         <v>161</v>
       </c>
@@ -19878,7 +19874,7 @@
         <v>17</v>
       </c>
     </row>
-    <row customHeight="1" ht="15.75" r="4" spans="1:7">
+    <row r="4" spans="1:7" ht="15.75" customHeight="1">
       <c r="A4" s="30" t="s">
         <v>164</v>
       </c>
@@ -19895,7 +19891,7 @@
         <v>38</v>
       </c>
     </row>
-    <row customHeight="1" ht="15.75" r="5" spans="1:7">
+    <row r="5" spans="1:7" ht="15.75" customHeight="1">
       <c r="A5" s="34" t="s">
         <v>167</v>
       </c>
@@ -19912,7 +19908,7 @@
         <v>9</v>
       </c>
     </row>
-    <row customHeight="1" ht="15.75" r="6" spans="1:7">
+    <row r="6" spans="1:7" ht="15.75" customHeight="1">
       <c r="A6" t="s">
         <v>328</v>
       </c>
@@ -19929,7 +19925,7 @@
         <v>323</v>
       </c>
     </row>
-    <row customHeight="1" ht="15.75" r="7" spans="1:7">
+    <row r="7" spans="1:7" ht="15.75" customHeight="1">
       <c r="A7" s="45" t="s">
         <v>877</v>
       </c>
@@ -19948,16 +19944,16 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink r:id="rId1" ref="E2" xr:uid="{00000000-0004-0000-0300-000000000000}"/>
-    <hyperlink r:id="rId2" ref="E3" xr:uid="{00000000-0004-0000-0300-000001000000}"/>
-    <hyperlink r:id="rId3" ref="E4" xr:uid="{00000000-0004-0000-0300-000002000000}"/>
-    <hyperlink r:id="rId4" ref="E5" xr:uid="{00000000-0004-0000-0300-000003000000}"/>
-    <hyperlink r:id="rId5" ref="D6" xr:uid="{00000000-0004-0000-0300-000004000000}"/>
-    <hyperlink r:id="rId6" ref="E6" xr:uid="{00000000-0004-0000-0300-000005000000}"/>
-    <hyperlink r:id="rId7" ref="D7" xr:uid="{B34712F5-65E4-4DA3-B4D8-B5E126A91A19}"/>
-    <hyperlink r:id="rId8" ref="E7" xr:uid="{FAD2E722-F8D2-45E6-8DA2-DA530385A188}"/>
+    <hyperlink ref="E2" r:id="rId1" xr:uid="{00000000-0004-0000-0300-000000000000}"/>
+    <hyperlink ref="E3" r:id="rId2" xr:uid="{00000000-0004-0000-0300-000001000000}"/>
+    <hyperlink ref="E4" r:id="rId3" xr:uid="{00000000-0004-0000-0300-000002000000}"/>
+    <hyperlink ref="E5" r:id="rId4" xr:uid="{00000000-0004-0000-0300-000003000000}"/>
+    <hyperlink ref="D6" r:id="rId5" xr:uid="{00000000-0004-0000-0300-000004000000}"/>
+    <hyperlink ref="E6" r:id="rId6" xr:uid="{00000000-0004-0000-0300-000005000000}"/>
+    <hyperlink ref="D7" r:id="rId7" xr:uid="{B34712F5-65E4-4DA3-B4D8-B5E126A91A19}"/>
+    <hyperlink ref="E7" r:id="rId8" xr:uid="{FAD2E722-F8D2-45E6-8DA2-DA530385A188}"/>
   </hyperlinks>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
-  <pageSetup orientation="portrait" paperSize="9" r:id="rId9"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId9"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
New listing script run 03/10/2021
</commit_message>
<xml_diff>
--- a/src/main/resources/InputTestdata/Listing details.xlsx
+++ b/src/main/resources/InputTestdata/Listing details.xlsx
@@ -1,39 +1,39 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24326"/>
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <mc:AlternateContent>
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Athavan\git\777Homes-2\777Homes-business\src\main\resources\InputTestdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{431F0D31-8EFC-4FC3-99E1-9F37481A0E3C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr documentId="13_ncr:1_{B4E9023C-3712-4FFB-96E4-4FE2861542A7}" revIDLastSave="0" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView windowHeight="15840" windowWidth="29040" xWindow="-120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}" yWindow="-120"/>
   </bookViews>
   <sheets>
-    <sheet name="Backlog" sheetId="1" r:id="rId1"/>
-    <sheet name="Listing" sheetId="2" r:id="rId2"/>
-    <sheet name="Tobe-executed" sheetId="3" r:id="rId3"/>
-    <sheet name="Agency login" sheetId="4" r:id="rId4"/>
+    <sheet name="Backlog" r:id="rId1" sheetId="1"/>
+    <sheet name="Listing" r:id="rId2" sheetId="2"/>
+    <sheet name="Tobe-executed" r:id="rId3" sheetId="3"/>
+    <sheet name="Agency login" r:id="rId4" sheetId="4"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Backlog!$A$1:$AB$52</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Listing!$E$1:$E$145</definedName>
-    <definedName name="Z_A7754112_A52F_4ABC_8778_92F04773E53C_.wvu.FilterData" localSheetId="1" hidden="1">Listing!$A$1:$AE$32</definedName>
-    <definedName name="Z_C25CEB9E_BEC1_4982_90C4_50C84EE1B82A_.wvu.FilterData" localSheetId="1" hidden="1">Listing!$A$1:$AE$32</definedName>
+    <definedName hidden="1" localSheetId="0" name="_xlnm._FilterDatabase">Backlog!$A$1:$AB$52</definedName>
+    <definedName hidden="1" localSheetId="1" name="_xlnm._FilterDatabase">Listing!$E$1:$E$145</definedName>
+    <definedName hidden="1" localSheetId="1" name="Z_A7754112_A52F_4ABC_8778_92F04773E53C_.wvu.FilterData">Listing!$A$1:$AE$32</definedName>
+    <definedName hidden="1" localSheetId="1" name="Z_C25CEB9E_BEC1_4982_90C4_50C84EE1B82A_.wvu.FilterData">Listing!$A$1:$AE$32</definedName>
   </definedNames>
   <calcPr calcId="181029"/>
   <customWorkbookViews>
-    <customWorkbookView name="Filter 2" guid="{C25CEB9E-BEC1-4982-90C4-50C84EE1B82A}" maximized="1" windowWidth="0" windowHeight="0" activeSheetId="0"/>
-    <customWorkbookView name="Filter 1" guid="{A7754112-A52F-4ABC-8778-92F04773E53C}" maximized="1" windowWidth="0" windowHeight="0" activeSheetId="0"/>
+    <customWorkbookView activeSheetId="0" guid="{C25CEB9E-BEC1-4982-90C4-50C84EE1B82A}" maximized="1" name="Filter 2" windowHeight="0" windowWidth="0"/>
+    <customWorkbookView activeSheetId="0" guid="{A7754112-A52F-4ABC-8778-92F04773E53C}" maximized="1" name="Filter 1" windowHeight="0" windowWidth="0"/>
   </customWorkbookViews>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3724" uniqueCount="1128">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3831" uniqueCount="1149">
   <si>
     <t>ID</t>
   </si>
@@ -5514,9 +5514,6 @@
     <t>https://www.777homes.com.au/?post_type=property&amp;p=8946&amp;preview=true</t>
   </si>
   <si>
-    <t>TO BE UPDATED</t>
-  </si>
-  <si>
     <t>152</t>
   </si>
   <si>
@@ -5542,11 +5539,131 @@
 - Close to Calwell Shopping Centre, sport fields and eateries
 - CCTV Camera, near new Bamboo flooring, fresh paint throughout</t>
   </si>
+  <si>
+    <t>https://www.allhomes.com.au/unit-39-1-bon-scott-crescent-moncrieff-act-2914</t>
+  </si>
+  <si>
+    <t>https://www.allhomes.com.au/unit-171-259-northbourne-avenue-lyneham-act-2602</t>
+  </si>
+  <si>
+    <t>https://www.allhomes.com.au/unit-53-9-felstead-vista-denman-prospect-act-2611</t>
+  </si>
+  <si>
+    <t>https://www.allhomes.com.au/19-mari-funaki-street-whitlam-act-2611</t>
+  </si>
+  <si>
+    <t>https://www.allhomes.com.au/strathnairn-act-2615?tid=178913671</t>
+  </si>
+  <si>
+    <t>153</t>
+  </si>
+  <si>
+    <t>39/1 Bon Scott Crescent, Moncrieff ACT 2914</t>
+  </si>
+  <si>
+    <t>Block/House: 1.03/ 144</t>
+  </si>
+  <si>
+    <t>New Door Properties is proud to present this townhouse located in one of the most sought-after pockets in the suburb of Moncrieff. Designed with practicality and comfort in mind, this 144 sqm home is presented with beautiful modern finishes throughout. The open-plan design features a complete family living. Opportunity not to be missed by people buying their first home or wanting to add to their investment portfolio.
+What you get:
+3 bed | 2.5 bath | 2 car garage
+- Spacious three bedroom townhouse set in 'The Reserve'
+- Built in robes in all bedrooms and carpet to floors
+- Master bedroom with walk in robe and ensuite
+- Spacious living with modern finishes, and drenched with natural light
+- Open plan kitchen with spacious walk in pantry
+- Gas cooktop, electric oven, ducted rangehood and dishwasher
+- Separate powder room with a small vanity
+- Ducted reverse cycle heating and cooling
+- European style laundry
+- Low maintenance courtyard and tiled alfresco
+- Double lockup garage with internal access
+Property Information:
+- Rates: $460 per quarter (approx.)
+- Land Tax: $587.25 per quarter (approx.)
+- Body corporate $577 per quarter (approx.)
+- Total floor area: 108sqm approx.
+- Garage: 36sqm approx.
+- Total Residence: 144sqm approx.
+- Rental estimate: $620 - $640 per week
+- EER: 5.5 Stars
+- Year Build: 2017
+Location:
+- Moncrieff is located in North Gungahlin and is bound by Horse Park Drive. It is located approximately 5Km north of
+the Gungahlin Town Centre
+- Close proximity to Margaret Hendry School and Amaroo School
+- Close drive to Gungahlin centre and Amaroo shopping centre
+- Easy access to public transport options
+- Close proximity to very popular Moncrieff Community Recreation Park and walking strips
+To Know more call Yash Sethi 0406551043 or Abhi Parashar 0404525998
+Disclaimer: New Door Properties and the vendor cannot warrant the accuracy of the information provided and will not accept any liability for loss or damage for any errors or misstatements in the information. Some images may be digitally styled/furnished for illustration purposes. Images and floor plans should be treated as a guide only. Purchasers should rely on their own independent enquiries or contact the agent for more information.</t>
+  </si>
+  <si>
+    <t>154</t>
+  </si>
+  <si>
+    <t>171/259 Northbourne Avenue, Lyneham ACT 2602</t>
+  </si>
+  <si>
+    <t>$323,000</t>
+  </si>
+  <si>
+    <t>155</t>
+  </si>
+  <si>
+    <t>53/9 Felstead Vista, Denman Prospect ACT 2611</t>
+  </si>
+  <si>
+    <t xml:space="preserve">7	6	9	0	0	0	</t>
+  </si>
+  <si>
+    <t>Offers over $769,000</t>
+  </si>
+  <si>
+    <t>Due to the current ACT lockdown restrictions we are only doing opens by private appointments. Please Call Alvin on 0426 146 118 to book your appointment.
+Have you been searching for your first ever home? Well time to stop. Quality meets space and potential. You will find the balance of nature, luxury, amenity and practicality you have been searching for.
+- Enjoy a barbecue with friends to the best views of Molonglo.
+- Escape in the tranquillity of your natural surroundings
+- Ride your bike through Stromlo Forest Park
+- Take a walk through the National Arboretum
+- Stroll across Denman Village shops
+- Meticulously designed with close Proximity to Canberra's major urban centres
+The facade maximises on aspect, privacy and spectacular views of the surrounding valley, while allowing natural light to flow throughout the interiors.
+Luxury features include;
+- Three bedrooms, Master bedroom with ensuite
+- Two bathrooms and powder with vanity.
+- Well appointed interiors complemented by outdoor spaces.
+- Quality stainless steel appliances
+- Ducted reverse cycle heating and cooling
+- Double glazed windows and sliding doors
+- Extra large double garage with internal access and two extra allocated parking space.
+Denman Prospect is quickly becoming a wonderful hotbed of entrepreneurial growth and houses and townhouses are going fast in this becoming area, be a part of it and have the benefit of a well designed strongly built townhouse.
+EER - 6.0
+Town house size- 157 sqm
+Double garage- 35 sqm
+Total - 192 sqm</t>
+  </si>
+  <si>
+    <t>157</t>
+  </si>
+  <si>
+    <t>Draft</t>
+  </si>
+  <si>
+    <t>https://www.777homes.com.au/?post_type=property&amp;p=9020&amp;preview=true</t>
+  </si>
+  <si>
+    <t>https://www.777homes.com.au/?post_type=property&amp;p=9022&amp;preview=true</t>
+  </si>
+  <si>
+    <t>https://www.777homes.com.au/?post_type=property&amp;p=9024&amp;preview=true</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="0"/>
   <fonts count="28">
     <font>
       <sz val="10"/>
@@ -5707,7 +5824,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="11">
+  <fills count="10">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -5761,12 +5878,6 @@
         <bgColor indexed="2"/>
       </patternFill>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC00000"/>
-        <bgColor rgb="FFD9EAD3"/>
-      </patternFill>
-    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -5778,114 +5889,111 @@
     </border>
   </borders>
   <cellStyleXfs count="2">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
+    <xf applyAlignment="0" applyBorder="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="0" fontId="25" numFmtId="0"/>
   </cellStyleXfs>
-  <cellXfs count="48">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+  <cellXfs count="47">
+    <xf applyAlignment="1" applyFont="1" borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyAlignment="1" applyFill="1" applyFont="1" borderId="0" fillId="3" fontId="1" numFmtId="0" xfId="0">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf applyAlignment="1" applyFill="1" applyFont="1" borderId="0" fillId="2" fontId="2" numFmtId="0" xfId="0">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf applyAlignment="1" applyFill="1" applyFont="1" borderId="0" fillId="2" fontId="3" numFmtId="0" xfId="0"/>
+    <xf applyAlignment="1" applyFill="1" applyFont="1" borderId="0" fillId="2" fontId="4" numFmtId="0" xfId="0">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf applyAlignment="1" applyFill="1" applyFont="1" borderId="0" fillId="2" fontId="6" numFmtId="0" xfId="0">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf applyFill="1" applyFont="1" borderId="0" fillId="2" fontId="4" numFmtId="0" xfId="0"/>
+    <xf applyAlignment="1" applyFill="1" applyFont="1" borderId="0" fillId="2" fontId="7" numFmtId="0" xfId="0"/>
+    <xf applyAlignment="1" applyFill="1" applyFont="1" borderId="0" fillId="2" fontId="8" numFmtId="0" xfId="0"/>
+    <xf applyAlignment="1" applyFill="1" applyFont="1" borderId="0" fillId="2" fontId="5" numFmtId="0" xfId="0">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf applyAlignment="1" applyFill="1" applyFont="1" borderId="0" fillId="4" fontId="4" numFmtId="0" xfId="0">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf applyAlignment="1" applyFill="1" applyFont="1" borderId="0" fillId="5" fontId="4" numFmtId="0" xfId="0">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf applyAlignment="1" applyFill="1" applyFont="1" borderId="0" fillId="2" fontId="9" numFmtId="0" xfId="0">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="11" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf applyAlignment="1" applyFill="1" applyFont="1" borderId="0" fillId="2" fontId="10" numFmtId="0" xfId="0"/>
+    <xf applyAlignment="1" applyFill="1" applyFont="1" borderId="0" fillId="2" fontId="11" numFmtId="0" xfId="0"/>
+    <xf applyAlignment="1" applyFill="1" applyFont="1" borderId="0" fillId="2" fontId="4" numFmtId="0" xfId="0">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="13" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="14" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="15" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="16" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="17" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf applyAlignment="1" applyFill="1" applyFont="1" borderId="0" fillId="2" fontId="12" numFmtId="0" xfId="0"/>
+    <xf applyAlignment="1" applyFill="1" applyFont="1" borderId="0" fillId="2" fontId="13" numFmtId="0" xfId="0"/>
+    <xf applyAlignment="1" applyFill="1" applyFont="1" borderId="0" fillId="2" fontId="14" numFmtId="0" xfId="0"/>
+    <xf applyAlignment="1" applyFill="1" applyFont="1" borderId="0" fillId="2" fontId="15" numFmtId="0" xfId="0"/>
+    <xf applyAlignment="1" applyFill="1" applyFont="1" borderId="0" fillId="2" fontId="16" numFmtId="0" xfId="0"/>
+    <xf applyAlignment="1" applyFill="1" applyFont="1" borderId="0" fillId="2" fontId="17" numFmtId="0" xfId="0"/>
+    <xf applyAlignment="1" applyFill="1" applyFont="1" borderId="0" fillId="3" fontId="1" numFmtId="0" xfId="0">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="18" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf applyFill="1" applyFont="1" borderId="0" fillId="3" fontId="7" numFmtId="0" xfId="0"/>
+    <xf applyAlignment="1" applyFill="1" applyFont="1" borderId="0" fillId="2" fontId="18" numFmtId="0" xfId="0">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf applyAlignment="1" applyFill="1" applyFont="1" borderId="0" fillId="2" fontId="19" numFmtId="0" xfId="0">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf applyAlignment="1" applyFill="1" applyFont="1" borderId="0" fillId="2" fontId="20" numFmtId="0" xfId="0">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf applyAlignment="1" applyFill="1" applyFont="1" borderId="0" fillId="2" fontId="18" numFmtId="0" xfId="0">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf applyAlignment="1" applyFill="1" applyFont="1" borderId="0" fillId="2" fontId="21" numFmtId="0" xfId="0">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf applyAlignment="1" applyFont="1" borderId="0" fillId="0" fontId="7" numFmtId="0" xfId="0">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="12" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="22" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf applyAlignment="1" applyFill="1" applyFont="1" borderId="0" fillId="3" fontId="17" numFmtId="0" xfId="0"/>
+    <xf applyAlignment="1" applyFill="1" applyFont="1" borderId="0" fillId="3" fontId="12" numFmtId="0" xfId="0"/>
+    <xf applyAlignment="1" applyFill="1" applyFont="1" borderId="0" fillId="3" fontId="22" numFmtId="0" xfId="0">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="24" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf applyAlignment="1" applyFill="1" applyFont="1" borderId="0" fillId="3" fontId="23" numFmtId="0" xfId="0"/>
+    <xf applyAlignment="1" applyFont="1" borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0"/>
+    <xf applyAlignment="1" applyFill="1" applyFont="1" borderId="0" fillId="3" fontId="24" numFmtId="0" xfId="0">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf applyAlignment="1" applyFill="1" applyFont="1" borderId="0" fillId="3" fontId="1" numFmtId="0" xfId="0">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf applyAlignment="1" applyFont="1" borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="25" fillId="2" borderId="0" xfId="1" applyFill="1" applyAlignment="1">
+    <xf applyAlignment="1" applyFill="1" borderId="0" fillId="2" fontId="25" numFmtId="0" xfId="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf applyAlignment="1" applyFill="1" applyFont="1" borderId="0" fillId="6" fontId="2" numFmtId="0" xfId="0">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf applyAlignment="1" applyFill="1" applyFont="1" borderId="0" fillId="7" fontId="5" numFmtId="0" xfId="0">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" xfId="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="25" fillId="2" borderId="0" xfId="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="18" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf applyAlignment="1" borderId="0" fillId="0" fontId="25" numFmtId="0" xfId="1"/>
+    <xf applyAlignment="1" applyFill="1" borderId="0" fillId="2" fontId="25" numFmtId="0" xfId="1"/>
+    <xf applyAlignment="1" applyFill="1" applyFont="1" borderId="0" fillId="8" fontId="18" numFmtId="0" xfId="0">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="26" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf applyAlignment="1" applyFill="1" applyFont="1" borderId="0" fillId="2" fontId="26" numFmtId="0" xfId="0">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="18" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
+    <xf applyAlignment="1" applyFont="1" borderId="0" fillId="0" fontId="27" numFmtId="0" xfId="0"/>
+    <xf applyFill="1" borderId="0" fillId="9" fontId="0" numFmtId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="2">
-    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle builtinId="8" name="Hyperlink" xfId="1"/>
+    <cellStyle builtinId="0" name="Normal" xfId="0"/>
   </cellStyles>
   <dxfs count="2">
     <dxf>
@@ -5905,7 +6013,7 @@
       </fill>
     </dxf>
   </dxfs>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <tableStyles count="0" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium2"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -6029,21 +6137,21 @@
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
-        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cap="flat" cmpd="sng" w="6350">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
           <a:miter lim="800000"/>
         </a:ln>
-        <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cap="flat" cmpd="sng" w="12700">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
           <a:miter lim="800000"/>
         </a:ln>
-        <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cap="flat" cmpd="sng" w="19050">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
@@ -6060,7 +6168,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+            <a:outerShdw algn="ctr" blurRad="57150" dir="5400000" dist="19050" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="63000"/>
               </a:srgbClr>
@@ -6114,32 +6222,32 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:AB153"/>
+  <dimension ref="A1:AC158"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B23" sqref="B23"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane activePane="bottomLeft" state="frozen" topLeftCell="A139" ySplit="1"/>
+      <selection activeCell="C168" pane="bottomLeft" sqref="C168"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1"/>
+  <sheetFormatPr customHeight="1" defaultColWidth="14.42578125" defaultRowHeight="15.75"/>
   <cols>
-    <col min="1" max="1" width="9.140625" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="74.85546875" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="75" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="14.5703125" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="22.140625" style="37" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="21.85546875" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="56.85546875" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="10.85546875" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="17.85546875" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="22.5703125" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="9.140625" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="74.85546875" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="75.0" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="14.5703125" collapsed="true"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" style="37" width="22.140625" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" width="21.85546875" collapsed="true"/>
+    <col min="8" max="8" customWidth="true" width="56.85546875" collapsed="true"/>
+    <col min="9" max="9" customWidth="true" width="10.85546875" collapsed="true"/>
+    <col min="10" max="10" customWidth="true" width="17.85546875" collapsed="true"/>
+    <col min="11" max="11" customWidth="true" width="22.5703125" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:28" ht="15">
+    <row ht="15" r="1" spans="1:28">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -6166,7 +6274,7 @@
       </c>
       <c r="J1" s="1"/>
     </row>
-    <row r="2" spans="1:28" ht="15.75" customHeight="1">
+    <row customHeight="1" ht="15.75" r="2" spans="1:28">
       <c r="A2" s="2">
         <v>1</v>
       </c>
@@ -6212,7 +6320,7 @@
       <c r="AA2" s="6"/>
       <c r="AB2" s="6"/>
     </row>
-    <row r="3" spans="1:28" ht="14.25">
+    <row ht="14.25" r="3" spans="1:28">
       <c r="A3" s="2">
         <v>2</v>
       </c>
@@ -6258,7 +6366,7 @@
       <c r="AA3" s="6"/>
       <c r="AB3" s="6"/>
     </row>
-    <row r="4" spans="1:28" ht="15.75" customHeight="1">
+    <row customHeight="1" ht="15.75" r="4" spans="1:28">
       <c r="A4" s="9">
         <v>3</v>
       </c>
@@ -6304,7 +6412,7 @@
       <c r="AA4" s="6"/>
       <c r="AB4" s="6"/>
     </row>
-    <row r="5" spans="1:28" ht="14.25">
+    <row ht="14.25" r="5" spans="1:28">
       <c r="A5" s="9">
         <v>4</v>
       </c>
@@ -6348,7 +6456,7 @@
       <c r="AA5" s="6"/>
       <c r="AB5" s="6"/>
     </row>
-    <row r="6" spans="1:28" ht="14.25">
+    <row ht="14.25" r="6" spans="1:28">
       <c r="A6" s="9">
         <v>5</v>
       </c>
@@ -6392,7 +6500,7 @@
       <c r="AA6" s="9"/>
       <c r="AB6" s="9"/>
     </row>
-    <row r="7" spans="1:28" ht="14.25">
+    <row ht="14.25" r="7" spans="1:28">
       <c r="A7" s="9">
         <v>6</v>
       </c>
@@ -6436,7 +6544,7 @@
       <c r="AA7" s="6"/>
       <c r="AB7" s="6"/>
     </row>
-    <row r="8" spans="1:28" ht="14.25">
+    <row ht="14.25" r="8" spans="1:28">
       <c r="A8" s="9">
         <v>7</v>
       </c>
@@ -6480,7 +6588,7 @@
       <c r="AA8" s="6"/>
       <c r="AB8" s="6"/>
     </row>
-    <row r="9" spans="1:28" ht="14.25">
+    <row ht="14.25" r="9" spans="1:28">
       <c r="A9" s="9">
         <v>8</v>
       </c>
@@ -6522,7 +6630,7 @@
       <c r="AA9" s="6"/>
       <c r="AB9" s="6"/>
     </row>
-    <row r="10" spans="1:28" ht="14.25">
+    <row ht="14.25" r="10" spans="1:28">
       <c r="A10" s="9">
         <v>9</v>
       </c>
@@ -6564,7 +6672,7 @@
       <c r="AA10" s="6"/>
       <c r="AB10" s="6"/>
     </row>
-    <row r="11" spans="1:28" ht="14.25">
+    <row ht="14.25" r="11" spans="1:28">
       <c r="A11" s="9">
         <v>10</v>
       </c>
@@ -6608,7 +6716,7 @@
       <c r="AA11" s="6"/>
       <c r="AB11" s="6"/>
     </row>
-    <row r="12" spans="1:28" ht="14.25">
+    <row ht="14.25" r="12" spans="1:28">
       <c r="A12" s="9">
         <v>11</v>
       </c>
@@ -6650,7 +6758,7 @@
       <c r="AA12" s="6"/>
       <c r="AB12" s="6"/>
     </row>
-    <row r="13" spans="1:28" ht="14.25">
+    <row ht="14.25" r="13" spans="1:28">
       <c r="A13" s="9">
         <v>12</v>
       </c>
@@ -6692,7 +6800,7 @@
       <c r="AA13" s="6"/>
       <c r="AB13" s="6"/>
     </row>
-    <row r="14" spans="1:28" ht="14.25">
+    <row ht="14.25" r="14" spans="1:28">
       <c r="A14" s="9">
         <v>13</v>
       </c>
@@ -6734,7 +6842,7 @@
       <c r="AA14" s="6"/>
       <c r="AB14" s="6"/>
     </row>
-    <row r="15" spans="1:28" ht="14.25">
+    <row ht="14.25" r="15" spans="1:28">
       <c r="A15" s="9">
         <v>14</v>
       </c>
@@ -6778,7 +6886,7 @@
       <c r="AA15" s="6"/>
       <c r="AB15" s="6"/>
     </row>
-    <row r="16" spans="1:28" ht="14.25">
+    <row ht="14.25" r="16" spans="1:28">
       <c r="A16" s="9">
         <v>15</v>
       </c>
@@ -6820,7 +6928,7 @@
       <c r="AA16" s="6"/>
       <c r="AB16" s="6"/>
     </row>
-    <row r="17" spans="1:28" ht="14.25">
+    <row ht="14.25" r="17" spans="1:28">
       <c r="A17" s="9">
         <v>16</v>
       </c>
@@ -6831,7 +6939,7 @@
         <v>697</v>
       </c>
       <c r="D17" s="4" t="s">
-        <v>7</v>
+        <v>14</v>
       </c>
       <c r="E17" s="15"/>
       <c r="F17" s="27" t="s">
@@ -6864,7 +6972,7 @@
       <c r="AA17" s="6"/>
       <c r="AB17" s="6"/>
     </row>
-    <row r="18" spans="1:28" ht="14.25">
+    <row ht="14.25" r="18" spans="1:28">
       <c r="A18" s="9">
         <v>17</v>
       </c>
@@ -6906,7 +7014,7 @@
       <c r="AA18" s="6"/>
       <c r="AB18" s="6"/>
     </row>
-    <row r="19" spans="1:28" ht="14.25">
+    <row ht="14.25" r="19" spans="1:28">
       <c r="A19" s="9">
         <v>18</v>
       </c>
@@ -6950,7 +7058,7 @@
       <c r="AA19" s="6"/>
       <c r="AB19" s="6"/>
     </row>
-    <row r="20" spans="1:28" ht="14.25">
+    <row ht="14.25" r="20" spans="1:28">
       <c r="A20" s="9">
         <v>19</v>
       </c>
@@ -6994,7 +7102,7 @@
       <c r="AA20" s="6"/>
       <c r="AB20" s="6"/>
     </row>
-    <row r="21" spans="1:28" ht="14.25">
+    <row ht="14.25" r="21" spans="1:28">
       <c r="A21" s="9">
         <v>20</v>
       </c>
@@ -7038,7 +7146,7 @@
       <c r="AA21" s="6"/>
       <c r="AB21" s="6"/>
     </row>
-    <row r="22" spans="1:28" ht="14.25">
+    <row ht="14.25" r="22" spans="1:28">
       <c r="A22" s="9">
         <v>21</v>
       </c>
@@ -7080,7 +7188,7 @@
       <c r="AA22" s="6"/>
       <c r="AB22" s="6"/>
     </row>
-    <row r="23" spans="1:28" ht="14.25">
+    <row ht="14.25" r="23" spans="1:28">
       <c r="A23" s="9">
         <v>22</v>
       </c>
@@ -7124,7 +7232,7 @@
       <c r="AA23" s="6"/>
       <c r="AB23" s="6"/>
     </row>
-    <row r="24" spans="1:28" ht="14.25">
+    <row ht="14.25" r="24" spans="1:28">
       <c r="A24" s="9">
         <v>23</v>
       </c>
@@ -7166,7 +7274,7 @@
       <c r="AA24" s="6"/>
       <c r="AB24" s="6"/>
     </row>
-    <row r="25" spans="1:28" ht="14.25">
+    <row ht="14.25" r="25" spans="1:28">
       <c r="A25" s="9">
         <v>24</v>
       </c>
@@ -7208,7 +7316,7 @@
       <c r="AA25" s="6"/>
       <c r="AB25" s="6"/>
     </row>
-    <row r="26" spans="1:28" ht="14.25">
+    <row ht="14.25" r="26" spans="1:28">
       <c r="A26" s="9">
         <v>25</v>
       </c>
@@ -7252,7 +7360,7 @@
       <c r="AA26" s="6"/>
       <c r="AB26" s="6"/>
     </row>
-    <row r="27" spans="1:28" ht="14.25">
+    <row ht="14.25" r="27" spans="1:28">
       <c r="A27" s="9">
         <v>26</v>
       </c>
@@ -7296,7 +7404,7 @@
       <c r="AA27" s="6"/>
       <c r="AB27" s="6"/>
     </row>
-    <row r="28" spans="1:28" ht="14.25">
+    <row ht="14.25" r="28" spans="1:28">
       <c r="A28" s="9">
         <v>27</v>
       </c>
@@ -7338,7 +7446,7 @@
       <c r="AA28" s="6"/>
       <c r="AB28" s="6"/>
     </row>
-    <row r="29" spans="1:28" ht="14.25">
+    <row ht="14.25" r="29" spans="1:28">
       <c r="A29" s="9">
         <v>28</v>
       </c>
@@ -7382,7 +7490,7 @@
       <c r="AA29" s="6"/>
       <c r="AB29" s="6"/>
     </row>
-    <row r="30" spans="1:28" ht="14.25">
+    <row ht="14.25" r="30" spans="1:28">
       <c r="A30" s="9">
         <v>29</v>
       </c>
@@ -7424,7 +7532,7 @@
       <c r="AA30" s="6"/>
       <c r="AB30" s="6"/>
     </row>
-    <row r="31" spans="1:28" ht="14.25">
+    <row ht="14.25" r="31" spans="1:28">
       <c r="A31" s="4">
         <v>30</v>
       </c>
@@ -7468,7 +7576,7 @@
       <c r="AA31" s="6"/>
       <c r="AB31" s="6"/>
     </row>
-    <row r="32" spans="1:28" ht="14.25">
+    <row ht="14.25" r="32" spans="1:28">
       <c r="A32" s="4">
         <v>31</v>
       </c>
@@ -7510,7 +7618,7 @@
       <c r="AA32" s="6"/>
       <c r="AB32" s="6"/>
     </row>
-    <row r="33" spans="1:8" s="4" customFormat="1" ht="14.25">
+    <row customFormat="1" ht="14.25" r="33" s="4" spans="1:8">
       <c r="A33" s="4">
         <v>32</v>
       </c>
@@ -7533,7 +7641,7 @@
         <v>427</v>
       </c>
     </row>
-    <row r="34" spans="1:8" s="4" customFormat="1" ht="14.25">
+    <row customFormat="1" ht="14.25" r="34" s="4" spans="1:8">
       <c r="A34" s="4">
         <v>33</v>
       </c>
@@ -7553,7 +7661,7 @@
         <v>427</v>
       </c>
     </row>
-    <row r="35" spans="1:8" s="4" customFormat="1" ht="14.25">
+    <row customFormat="1" ht="14.25" r="35" s="4" spans="1:8">
       <c r="A35" s="4">
         <v>34</v>
       </c>
@@ -7573,7 +7681,7 @@
         <v>427</v>
       </c>
     </row>
-    <row r="36" spans="1:8" s="4" customFormat="1" ht="14.25">
+    <row customFormat="1" ht="14.25" r="36" s="4" spans="1:8">
       <c r="A36" s="4">
         <v>35</v>
       </c>
@@ -7593,7 +7701,7 @@
         <v>427</v>
       </c>
     </row>
-    <row r="37" spans="1:8" s="4" customFormat="1" ht="14.25">
+    <row customFormat="1" ht="14.25" r="37" s="4" spans="1:8">
       <c r="A37" s="4">
         <v>36</v>
       </c>
@@ -7613,7 +7721,7 @@
         <v>427</v>
       </c>
     </row>
-    <row r="38" spans="1:8" s="4" customFormat="1" ht="14.25">
+    <row customFormat="1" ht="14.25" r="38" s="4" spans="1:8">
       <c r="A38" s="4">
         <v>37</v>
       </c>
@@ -7636,7 +7744,7 @@
         <v>427</v>
       </c>
     </row>
-    <row r="39" spans="1:8" s="4" customFormat="1" ht="14.25">
+    <row customFormat="1" ht="14.25" r="39" s="4" spans="1:8">
       <c r="A39" s="4">
         <v>38</v>
       </c>
@@ -7659,7 +7767,7 @@
         <v>427</v>
       </c>
     </row>
-    <row r="40" spans="1:8" s="4" customFormat="1" ht="14.25">
+    <row customFormat="1" ht="14.25" r="40" s="4" spans="1:8">
       <c r="A40" s="4">
         <v>39</v>
       </c>
@@ -7682,7 +7790,7 @@
         <v>427</v>
       </c>
     </row>
-    <row r="41" spans="1:8" s="4" customFormat="1" ht="14.25">
+    <row customFormat="1" ht="14.25" r="41" s="4" spans="1:8">
       <c r="A41" s="4">
         <v>40</v>
       </c>
@@ -7702,7 +7810,7 @@
         <v>427</v>
       </c>
     </row>
-    <row r="42" spans="1:8" s="4" customFormat="1" ht="14.25">
+    <row customFormat="1" ht="14.25" r="42" s="4" spans="1:8">
       <c r="A42" s="4">
         <v>41</v>
       </c>
@@ -7725,7 +7833,7 @@
         <v>427</v>
       </c>
     </row>
-    <row r="43" spans="1:8" s="4" customFormat="1" ht="14.25">
+    <row customFormat="1" ht="14.25" r="43" s="4" spans="1:8">
       <c r="A43" s="4">
         <v>42</v>
       </c>
@@ -7745,7 +7853,7 @@
         <v>427</v>
       </c>
     </row>
-    <row r="44" spans="1:8" s="4" customFormat="1" ht="14.25">
+    <row customFormat="1" ht="14.25" r="44" s="4" spans="1:8">
       <c r="A44" s="4">
         <v>43</v>
       </c>
@@ -7765,7 +7873,7 @@
         <v>427</v>
       </c>
     </row>
-    <row r="45" spans="1:8" s="4" customFormat="1" ht="14.25">
+    <row customFormat="1" ht="14.25" r="45" s="4" spans="1:8">
       <c r="A45" s="4">
         <v>44</v>
       </c>
@@ -7776,7 +7884,7 @@
         <v>728</v>
       </c>
       <c r="D45" s="4" t="s">
-        <v>7</v>
+        <v>14</v>
       </c>
       <c r="F45" s="27" t="s">
         <v>686</v>
@@ -7788,7 +7896,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="46" spans="1:8" s="4" customFormat="1" ht="14.25">
+    <row customFormat="1" ht="14.25" r="46" s="4" spans="1:8">
       <c r="A46" s="4">
         <v>45</v>
       </c>
@@ -7808,7 +7916,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="47" spans="1:8" s="4" customFormat="1" ht="14.25">
+    <row customFormat="1" ht="14.25" r="47" s="4" spans="1:8">
       <c r="A47" s="4">
         <v>46</v>
       </c>
@@ -7828,7 +7936,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="48" spans="1:8" s="4" customFormat="1" ht="12.75">
+    <row customFormat="1" ht="12.75" r="48" s="4" spans="1:8">
       <c r="A48" s="4">
         <v>47</v>
       </c>
@@ -7851,7 +7959,7 @@
         <v>428</v>
       </c>
     </row>
-    <row r="49" spans="1:8" s="4" customFormat="1" ht="12.75">
+    <row customFormat="1" ht="12.75" r="49" s="4" spans="1:8">
       <c r="A49" s="4">
         <v>48</v>
       </c>
@@ -7874,7 +7982,7 @@
         <v>428</v>
       </c>
     </row>
-    <row r="50" spans="1:8" s="4" customFormat="1" ht="12.75">
+    <row customFormat="1" ht="12.75" r="50" s="4" spans="1:8">
       <c r="A50" s="4">
         <v>49</v>
       </c>
@@ -7894,7 +8002,7 @@
         <v>428</v>
       </c>
     </row>
-    <row r="51" spans="1:8" s="4" customFormat="1" ht="12.75">
+    <row customFormat="1" ht="12.75" r="51" s="4" spans="1:8">
       <c r="A51" s="4">
         <v>50</v>
       </c>
@@ -7914,7 +8022,7 @@
         <v>428</v>
       </c>
     </row>
-    <row r="52" spans="1:8" s="4" customFormat="1" ht="12.75">
+    <row customFormat="1" ht="12.75" r="52" s="4" spans="1:8">
       <c r="A52" s="4">
         <v>51</v>
       </c>
@@ -7937,7 +8045,7 @@
         <v>428</v>
       </c>
     </row>
-    <row r="53" spans="1:8" s="4" customFormat="1" ht="15.75" customHeight="1">
+    <row customFormat="1" customHeight="1" ht="15.75" r="53" s="4" spans="1:8">
       <c r="A53" s="4">
         <v>52</v>
       </c>
@@ -7960,7 +8068,7 @@
         <v>323</v>
       </c>
     </row>
-    <row r="54" spans="1:8" s="4" customFormat="1" ht="12.75">
+    <row customFormat="1" ht="12.75" r="54" s="4" spans="1:8">
       <c r="A54" s="4">
         <v>53</v>
       </c>
@@ -7980,7 +8088,7 @@
         <v>323</v>
       </c>
     </row>
-    <row r="55" spans="1:8" s="4" customFormat="1" ht="12.75">
+    <row customFormat="1" ht="12.75" r="55" s="4" spans="1:8">
       <c r="A55" s="4">
         <v>54</v>
       </c>
@@ -8003,7 +8111,7 @@
         <v>323</v>
       </c>
     </row>
-    <row r="56" spans="1:8" s="4" customFormat="1" ht="12.75">
+    <row customFormat="1" ht="12.75" r="56" s="4" spans="1:8">
       <c r="A56" s="4">
         <v>55</v>
       </c>
@@ -8026,7 +8134,7 @@
         <v>323</v>
       </c>
     </row>
-    <row r="57" spans="1:8" s="4" customFormat="1" ht="12.75">
+    <row customFormat="1" ht="12.75" r="57" s="4" spans="1:8">
       <c r="A57" s="4">
         <v>56</v>
       </c>
@@ -8046,7 +8154,7 @@
         <v>323</v>
       </c>
     </row>
-    <row r="58" spans="1:8" s="4" customFormat="1" ht="12.75">
+    <row customFormat="1" ht="12.75" r="58" s="4" spans="1:8">
       <c r="A58" s="4">
         <v>57</v>
       </c>
@@ -8066,7 +8174,7 @@
         <v>323</v>
       </c>
     </row>
-    <row r="59" spans="1:8" s="4" customFormat="1" ht="12.75">
+    <row customFormat="1" ht="12.75" r="59" s="4" spans="1:8">
       <c r="A59" s="4">
         <v>58</v>
       </c>
@@ -8086,7 +8194,7 @@
         <v>323</v>
       </c>
     </row>
-    <row r="60" spans="1:8" s="4" customFormat="1" ht="12.75">
+    <row customFormat="1" ht="12.75" r="60" s="4" spans="1:8">
       <c r="A60" s="4">
         <v>59</v>
       </c>
@@ -8106,7 +8214,7 @@
         <v>323</v>
       </c>
     </row>
-    <row r="61" spans="1:8" s="4" customFormat="1" ht="12.75">
+    <row customFormat="1" ht="12.75" r="61" s="4" spans="1:8">
       <c r="A61" s="4">
         <v>60</v>
       </c>
@@ -8126,7 +8234,7 @@
         <v>323</v>
       </c>
     </row>
-    <row r="62" spans="1:8" s="4" customFormat="1" ht="12.75">
+    <row customFormat="1" ht="12.75" r="62" s="4" spans="1:8">
       <c r="A62" s="4">
         <v>61</v>
       </c>
@@ -8146,7 +8254,7 @@
         <v>427</v>
       </c>
     </row>
-    <row r="63" spans="1:8" s="4" customFormat="1" ht="12.75">
+    <row customFormat="1" ht="12.75" r="63" s="4" spans="1:8">
       <c r="A63" s="4">
         <v>62</v>
       </c>
@@ -8169,7 +8277,7 @@
         <v>427</v>
       </c>
     </row>
-    <row r="64" spans="1:8" s="4" customFormat="1" ht="12.75">
+    <row customFormat="1" ht="12.75" r="64" s="4" spans="1:8">
       <c r="A64" s="4">
         <v>63</v>
       </c>
@@ -8192,7 +8300,7 @@
         <v>427</v>
       </c>
     </row>
-    <row r="65" spans="1:8" s="4" customFormat="1" ht="12.75">
+    <row customFormat="1" ht="12.75" r="65" s="4" spans="1:8">
       <c r="A65" s="4">
         <v>64</v>
       </c>
@@ -8213,7 +8321,7 @@
         <v>427</v>
       </c>
     </row>
-    <row r="66" spans="1:8" s="4" customFormat="1" ht="12.75">
+    <row customFormat="1" ht="12.75" r="66" s="4" spans="1:8">
       <c r="A66" s="4">
         <v>65</v>
       </c>
@@ -8236,7 +8344,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="67" spans="1:8" s="4" customFormat="1" ht="12.75">
+    <row customFormat="1" ht="12.75" r="67" s="4" spans="1:8">
       <c r="A67" s="4">
         <v>66</v>
       </c>
@@ -8259,7 +8367,7 @@
         <v>428</v>
       </c>
     </row>
-    <row r="68" spans="1:8" s="4" customFormat="1" ht="12.75">
+    <row customFormat="1" ht="12.75" r="68" s="4" spans="1:8">
       <c r="A68" s="4">
         <v>67</v>
       </c>
@@ -8282,7 +8390,7 @@
         <v>427</v>
       </c>
     </row>
-    <row r="69" spans="1:8" s="4" customFormat="1" ht="12.75">
+    <row customFormat="1" ht="12.75" r="69" s="4" spans="1:8">
       <c r="A69" s="4">
         <v>68</v>
       </c>
@@ -8305,7 +8413,7 @@
         <v>427</v>
       </c>
     </row>
-    <row r="70" spans="1:8" s="4" customFormat="1" ht="12.75">
+    <row customFormat="1" ht="12.75" r="70" s="4" spans="1:8">
       <c r="A70" s="4">
         <v>69</v>
       </c>
@@ -8328,7 +8436,7 @@
         <v>427</v>
       </c>
     </row>
-    <row r="71" spans="1:8" s="4" customFormat="1" ht="12.75">
+    <row customFormat="1" ht="12.75" r="71" s="4" spans="1:8">
       <c r="A71" s="4">
         <v>70</v>
       </c>
@@ -8351,7 +8459,7 @@
         <v>427</v>
       </c>
     </row>
-    <row r="72" spans="1:8" s="4" customFormat="1" ht="12.75">
+    <row customFormat="1" ht="12.75" r="72" s="4" spans="1:8">
       <c r="A72" s="4">
         <v>71</v>
       </c>
@@ -8374,7 +8482,7 @@
         <v>427</v>
       </c>
     </row>
-    <row r="73" spans="1:8" ht="12.75">
+    <row ht="12.75" r="73" spans="1:8">
       <c r="A73">
         <v>72</v>
       </c>
@@ -8397,7 +8505,7 @@
         <v>428</v>
       </c>
     </row>
-    <row r="74" spans="1:8" ht="12.75">
+    <row ht="12.75" r="74" spans="1:8">
       <c r="A74">
         <v>73</v>
       </c>
@@ -8420,7 +8528,7 @@
         <v>428</v>
       </c>
     </row>
-    <row r="75" spans="1:8" s="4" customFormat="1" ht="12.75">
+    <row customFormat="1" ht="12.75" r="75" s="4" spans="1:8">
       <c r="A75" s="4">
         <v>74</v>
       </c>
@@ -8443,7 +8551,7 @@
         <v>428</v>
       </c>
     </row>
-    <row r="76" spans="1:8" ht="12.75">
+    <row ht="12.75" r="76" spans="1:8">
       <c r="A76">
         <v>75</v>
       </c>
@@ -8466,7 +8574,7 @@
         <v>428</v>
       </c>
     </row>
-    <row r="77" spans="1:8" ht="12.75">
+    <row ht="12.75" r="77" spans="1:8">
       <c r="A77">
         <v>76</v>
       </c>
@@ -8489,7 +8597,7 @@
         <v>428</v>
       </c>
     </row>
-    <row r="78" spans="1:8" ht="12.75">
+    <row ht="12.75" r="78" spans="1:8">
       <c r="A78">
         <v>77</v>
       </c>
@@ -8512,7 +8620,7 @@
         <v>428</v>
       </c>
     </row>
-    <row r="79" spans="1:8" ht="12.75">
+    <row ht="12.75" r="79" spans="1:8">
       <c r="A79">
         <v>78</v>
       </c>
@@ -8535,7 +8643,7 @@
         <v>428</v>
       </c>
     </row>
-    <row r="80" spans="1:8" ht="12.75">
+    <row ht="12.75" r="80" spans="1:8">
       <c r="A80">
         <v>79</v>
       </c>
@@ -8558,7 +8666,7 @@
         <v>428</v>
       </c>
     </row>
-    <row r="81" spans="1:8" ht="12.75">
+    <row ht="12.75" r="81" spans="1:8">
       <c r="A81">
         <v>80</v>
       </c>
@@ -8581,7 +8689,7 @@
         <v>428</v>
       </c>
     </row>
-    <row r="82" spans="1:8" ht="12.75">
+    <row ht="12.75" r="82" spans="1:8">
       <c r="A82">
         <v>81</v>
       </c>
@@ -8604,7 +8712,7 @@
         <v>428</v>
       </c>
     </row>
-    <row r="83" spans="1:8" ht="12.75">
+    <row ht="12.75" r="83" spans="1:8">
       <c r="A83">
         <v>82</v>
       </c>
@@ -8627,7 +8735,7 @@
         <v>428</v>
       </c>
     </row>
-    <row r="84" spans="1:8" ht="12.75">
+    <row ht="12.75" r="84" spans="1:8">
       <c r="A84">
         <v>83</v>
       </c>
@@ -8650,7 +8758,7 @@
         <v>428</v>
       </c>
     </row>
-    <row r="85" spans="1:8" ht="12.75">
+    <row ht="12.75" r="85" spans="1:8">
       <c r="A85">
         <v>84</v>
       </c>
@@ -8673,7 +8781,7 @@
         <v>428</v>
       </c>
     </row>
-    <row r="86" spans="1:8" s="4" customFormat="1" ht="12.75">
+    <row customFormat="1" ht="12.75" r="86" s="4" spans="1:8">
       <c r="A86" s="4">
         <v>85</v>
       </c>
@@ -8696,7 +8804,7 @@
         <v>427</v>
       </c>
     </row>
-    <row r="87" spans="1:8" s="4" customFormat="1" ht="12.75">
+    <row customFormat="1" ht="12.75" r="87" s="4" spans="1:8">
       <c r="A87" s="4">
         <v>86</v>
       </c>
@@ -8719,7 +8827,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="88" spans="1:8" ht="12.75">
+    <row ht="12.75" r="88" spans="1:8">
       <c r="A88">
         <v>87</v>
       </c>
@@ -8742,7 +8850,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="89" spans="1:8" ht="12.75">
+    <row ht="12.75" r="89" spans="1:8">
       <c r="A89">
         <v>88</v>
       </c>
@@ -8765,7 +8873,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="90" spans="1:8" ht="12.75">
+    <row ht="12.75" r="90" spans="1:8">
       <c r="A90">
         <v>89</v>
       </c>
@@ -8788,7 +8896,7 @@
         <v>428</v>
       </c>
     </row>
-    <row r="91" spans="1:8" ht="12.75">
+    <row ht="12.75" r="91" spans="1:8">
       <c r="A91">
         <v>90</v>
       </c>
@@ -8811,7 +8919,7 @@
         <v>428</v>
       </c>
     </row>
-    <row r="92" spans="1:8" ht="12.75">
+    <row ht="12.75" r="92" spans="1:8">
       <c r="A92">
         <v>91</v>
       </c>
@@ -8834,14 +8942,14 @@
         <v>428</v>
       </c>
     </row>
-    <row r="93" spans="1:8" ht="12.75">
+    <row ht="12.75" r="93" spans="1:8">
       <c r="A93">
         <v>92</v>
       </c>
       <c r="B93" s="41" t="s">
         <v>604</v>
       </c>
-      <c r="C93" t="s">
+      <c r="C93" s="41" t="s">
         <v>643</v>
       </c>
       <c r="D93" s="4" t="s">
@@ -8857,7 +8965,7 @@
         <v>428</v>
       </c>
     </row>
-    <row r="94" spans="1:8" ht="12.75">
+    <row ht="12.75" r="94" spans="1:8">
       <c r="A94">
         <v>93</v>
       </c>
@@ -8876,11 +8984,11 @@
       <c r="G94" t="s">
         <v>8</v>
       </c>
-      <c r="H94" t="s">
+      <c r="H94" s="41" t="s">
         <v>427</v>
       </c>
     </row>
-    <row r="95" spans="1:8" ht="12.75">
+    <row ht="12.75" r="95" spans="1:8">
       <c r="A95">
         <v>94</v>
       </c>
@@ -8903,7 +9011,7 @@
         <v>427</v>
       </c>
     </row>
-    <row r="96" spans="1:8" ht="12.75">
+    <row ht="12.75" r="96" spans="1:8">
       <c r="A96">
         <v>95</v>
       </c>
@@ -8926,7 +9034,7 @@
         <v>427</v>
       </c>
     </row>
-    <row r="97" spans="1:8" ht="12.75">
+    <row ht="12.75" r="97" spans="1:8">
       <c r="A97">
         <v>96</v>
       </c>
@@ -8949,7 +9057,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="98" spans="1:8" ht="12.75">
+    <row ht="12.75" r="98" spans="1:8">
       <c r="A98">
         <v>97</v>
       </c>
@@ -8972,7 +9080,7 @@
         <v>428</v>
       </c>
     </row>
-    <row r="99" spans="1:8" ht="12.75">
+    <row ht="12.75" r="99" spans="1:8">
       <c r="A99">
         <v>98</v>
       </c>
@@ -8995,7 +9103,7 @@
         <v>427</v>
       </c>
     </row>
-    <row r="100" spans="1:8" ht="12.75">
+    <row ht="12.75" r="100" spans="1:8">
       <c r="A100">
         <v>99</v>
       </c>
@@ -9018,7 +9126,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="101" spans="1:8" ht="12.75">
+    <row ht="12.75" r="101" spans="1:8">
       <c r="A101">
         <v>100</v>
       </c>
@@ -9041,7 +9149,7 @@
         <v>428</v>
       </c>
     </row>
-    <row r="102" spans="1:8" ht="12.75">
+    <row ht="12.75" r="102" spans="1:8">
       <c r="A102">
         <v>101</v>
       </c>
@@ -9064,7 +9172,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="103" spans="1:8" ht="12.75">
+    <row ht="12.75" r="103" spans="1:8">
       <c r="A103">
         <v>102</v>
       </c>
@@ -9087,7 +9195,7 @@
         <v>428</v>
       </c>
     </row>
-    <row r="104" spans="1:8" ht="12.75">
+    <row ht="12.75" r="104" spans="1:8">
       <c r="A104">
         <v>103</v>
       </c>
@@ -9110,7 +9218,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="105" spans="1:8" ht="12.75">
+    <row ht="12.75" r="105" spans="1:8">
       <c r="A105">
         <v>104</v>
       </c>
@@ -9133,7 +9241,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="106" spans="1:8" ht="12.75">
+    <row ht="12.75" r="106" spans="1:8">
       <c r="A106">
         <v>105</v>
       </c>
@@ -9144,7 +9252,7 @@
         <v>782</v>
       </c>
       <c r="D106" s="4" t="s">
-        <v>7</v>
+        <v>14</v>
       </c>
       <c r="F106" s="2" t="s">
         <v>686</v>
@@ -9156,7 +9264,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="107" spans="1:8" ht="12.75">
+    <row ht="12.75" r="107" spans="1:8">
       <c r="A107">
         <v>106</v>
       </c>
@@ -9179,7 +9287,7 @@
         <v>427</v>
       </c>
     </row>
-    <row r="108" spans="1:8" ht="12.75">
+    <row ht="12.75" r="108" spans="1:8">
       <c r="A108">
         <v>107</v>
       </c>
@@ -9202,7 +9310,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="109" spans="1:8" ht="12.75">
+    <row ht="12.75" r="109" spans="1:8">
       <c r="A109">
         <v>108</v>
       </c>
@@ -9225,7 +9333,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="110" spans="1:8" ht="12.75">
+    <row ht="12.75" r="110" spans="1:8">
       <c r="A110">
         <v>109</v>
       </c>
@@ -9248,7 +9356,7 @@
         <v>428</v>
       </c>
     </row>
-    <row r="111" spans="1:8" ht="12.75">
+    <row ht="12.75" r="111" spans="1:8">
       <c r="A111">
         <v>110</v>
       </c>
@@ -9271,7 +9379,7 @@
         <v>428</v>
       </c>
     </row>
-    <row r="112" spans="1:8" ht="12.75">
+    <row ht="12.75" r="112" spans="1:8">
       <c r="A112">
         <v>111</v>
       </c>
@@ -9294,7 +9402,7 @@
         <v>428</v>
       </c>
     </row>
-    <row r="113" spans="1:8" ht="12.75">
+    <row ht="12.75" r="113" spans="1:8">
       <c r="A113">
         <v>112</v>
       </c>
@@ -9317,7 +9425,7 @@
         <v>428</v>
       </c>
     </row>
-    <row r="114" spans="1:8" ht="12.75">
+    <row ht="12.75" r="114" spans="1:8">
       <c r="A114">
         <v>113</v>
       </c>
@@ -9340,7 +9448,7 @@
         <v>427</v>
       </c>
     </row>
-    <row r="115" spans="1:8" ht="12.75">
+    <row ht="12.75" r="115" spans="1:8">
       <c r="A115">
         <v>114</v>
       </c>
@@ -9363,7 +9471,7 @@
         <v>323</v>
       </c>
     </row>
-    <row r="116" spans="1:8" ht="12.75">
+    <row ht="12.75" r="116" spans="1:8">
       <c r="A116">
         <v>115</v>
       </c>
@@ -9386,7 +9494,7 @@
         <v>427</v>
       </c>
     </row>
-    <row r="117" spans="1:8" ht="12.75">
+    <row ht="12.75" r="117" spans="1:8">
       <c r="A117">
         <v>116</v>
       </c>
@@ -9409,7 +9517,7 @@
         <v>428</v>
       </c>
     </row>
-    <row r="118" spans="1:8" ht="12.75">
+    <row ht="12.75" r="118" spans="1:8">
       <c r="A118">
         <v>117</v>
       </c>
@@ -9429,7 +9537,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="119" spans="1:8" ht="12.75">
+    <row ht="12.75" r="119" spans="1:8">
       <c r="A119">
         <v>118</v>
       </c>
@@ -9452,7 +9560,7 @@
         <v>428</v>
       </c>
     </row>
-    <row r="120" spans="1:8" ht="15.75" customHeight="1">
+    <row customHeight="1" ht="15.75" r="120" spans="1:8">
       <c r="A120">
         <v>119</v>
       </c>
@@ -9475,7 +9583,7 @@
         <v>881</v>
       </c>
     </row>
-    <row r="121" spans="1:8" ht="12.75">
+    <row ht="12.75" r="121" spans="1:8">
       <c r="A121">
         <v>120</v>
       </c>
@@ -9498,7 +9606,7 @@
         <v>881</v>
       </c>
     </row>
-    <row r="122" spans="1:8" ht="12.75">
+    <row ht="12.75" r="122" spans="1:8">
       <c r="A122">
         <v>121</v>
       </c>
@@ -9521,7 +9629,7 @@
         <v>881</v>
       </c>
     </row>
-    <row r="123" spans="1:8" ht="12.75">
+    <row ht="12.75" r="123" spans="1:8">
       <c r="A123">
         <v>122</v>
       </c>
@@ -9544,7 +9652,7 @@
         <v>881</v>
       </c>
     </row>
-    <row r="124" spans="1:8" ht="12.75">
+    <row ht="12.75" r="124" spans="1:8">
       <c r="A124">
         <v>123</v>
       </c>
@@ -9567,7 +9675,7 @@
         <v>881</v>
       </c>
     </row>
-    <row r="125" spans="1:8" ht="12.75">
+    <row ht="12.75" r="125" spans="1:8">
       <c r="A125">
         <v>124</v>
       </c>
@@ -9590,7 +9698,7 @@
         <v>881</v>
       </c>
     </row>
-    <row r="126" spans="1:8" ht="12.75">
+    <row ht="12.75" r="126" spans="1:8">
       <c r="A126">
         <v>125</v>
       </c>
@@ -9613,7 +9721,7 @@
         <v>881</v>
       </c>
     </row>
-    <row r="127" spans="1:8" ht="12.75">
+    <row ht="12.75" r="127" spans="1:8">
       <c r="A127">
         <v>126</v>
       </c>
@@ -9636,7 +9744,7 @@
         <v>881</v>
       </c>
     </row>
-    <row r="128" spans="1:8" ht="12.75">
+    <row ht="12.75" r="128" spans="1:8">
       <c r="A128">
         <v>127</v>
       </c>
@@ -9659,7 +9767,7 @@
         <v>881</v>
       </c>
     </row>
-    <row r="129" spans="1:8" ht="12.75">
+    <row ht="12.75" r="129" spans="1:8">
       <c r="A129">
         <v>128</v>
       </c>
@@ -9682,7 +9790,7 @@
         <v>881</v>
       </c>
     </row>
-    <row r="130" spans="1:8" ht="12.75">
+    <row ht="12.75" r="130" spans="1:8">
       <c r="A130">
         <v>129</v>
       </c>
@@ -9693,7 +9801,7 @@
         <v>1043</v>
       </c>
       <c r="D130" s="4" t="s">
-        <v>7</v>
+        <v>14</v>
       </c>
       <c r="F130" s="2" t="s">
         <v>687</v>
@@ -9705,7 +9813,7 @@
         <v>881</v>
       </c>
     </row>
-    <row r="131" spans="1:8" ht="12.75">
+    <row ht="12.75" r="131" spans="1:8">
       <c r="A131">
         <v>130</v>
       </c>
@@ -9728,7 +9836,7 @@
         <v>881</v>
       </c>
     </row>
-    <row r="132" spans="1:8" ht="12.75">
+    <row ht="12.75" r="132" spans="1:8">
       <c r="A132">
         <v>131</v>
       </c>
@@ -9751,7 +9859,7 @@
         <v>881</v>
       </c>
     </row>
-    <row r="133" spans="1:8" ht="12.75">
+    <row ht="12.75" r="133" spans="1:8">
       <c r="A133">
         <v>132</v>
       </c>
@@ -9774,7 +9882,7 @@
         <v>881</v>
       </c>
     </row>
-    <row r="134" spans="1:8" ht="12.75">
+    <row ht="12.75" r="134" spans="1:8">
       <c r="A134">
         <v>133</v>
       </c>
@@ -9797,7 +9905,7 @@
         <v>881</v>
       </c>
     </row>
-    <row r="135" spans="1:8" ht="12.75">
+    <row ht="12.75" r="135" spans="1:8">
       <c r="A135">
         <v>134</v>
       </c>
@@ -9820,7 +9928,7 @@
         <v>881</v>
       </c>
     </row>
-    <row r="136" spans="1:8" ht="12.75">
+    <row ht="12.75" r="136" spans="1:8">
       <c r="A136">
         <v>135</v>
       </c>
@@ -9843,7 +9951,7 @@
         <v>881</v>
       </c>
     </row>
-    <row r="137" spans="1:8" ht="12.75">
+    <row ht="12.75" r="137" spans="1:8">
       <c r="A137">
         <v>136</v>
       </c>
@@ -9866,7 +9974,7 @@
         <v>881</v>
       </c>
     </row>
-    <row r="138" spans="1:8" ht="12.75">
+    <row ht="12.75" r="138" spans="1:8">
       <c r="A138">
         <v>137</v>
       </c>
@@ -9889,7 +9997,7 @@
         <v>881</v>
       </c>
     </row>
-    <row r="139" spans="1:8" ht="12.75">
+    <row ht="12.75" r="139" spans="1:8">
       <c r="A139">
         <v>138</v>
       </c>
@@ -9912,7 +10020,7 @@
         <v>881</v>
       </c>
     </row>
-    <row r="140" spans="1:8" ht="12.75">
+    <row ht="12.75" r="140" spans="1:8">
       <c r="A140">
         <v>139</v>
       </c>
@@ -9935,7 +10043,7 @@
         <v>881</v>
       </c>
     </row>
-    <row r="141" spans="1:8" ht="12.75">
+    <row ht="12.75" r="141" spans="1:8">
       <c r="A141">
         <v>140</v>
       </c>
@@ -9958,7 +10066,7 @@
         <v>881</v>
       </c>
     </row>
-    <row r="142" spans="1:8" ht="12.75">
+    <row ht="12.75" r="142" spans="1:8">
       <c r="A142">
         <v>141</v>
       </c>
@@ -9981,7 +10089,7 @@
         <v>881</v>
       </c>
     </row>
-    <row r="143" spans="1:8" ht="12.75">
+    <row ht="12.75" r="143" spans="1:8">
       <c r="A143">
         <v>142</v>
       </c>
@@ -10004,7 +10112,7 @@
         <v>881</v>
       </c>
     </row>
-    <row r="144" spans="1:8" ht="12.75">
+    <row ht="12.75" r="144" spans="1:8">
       <c r="A144">
         <v>143</v>
       </c>
@@ -10027,7 +10135,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="145" spans="1:8" ht="12.75">
+    <row ht="12.75" r="145" spans="1:8">
       <c r="A145">
         <v>144</v>
       </c>
@@ -10050,7 +10158,7 @@
         <v>428</v>
       </c>
     </row>
-    <row r="146" spans="1:8" ht="12.75">
+    <row ht="12.75" r="146" spans="1:8">
       <c r="A146">
         <v>145</v>
       </c>
@@ -10073,7 +10181,7 @@
         <v>427</v>
       </c>
     </row>
-    <row r="147" spans="1:8" ht="12.75">
+    <row ht="12.75" r="147" spans="1:8">
       <c r="A147">
         <v>146</v>
       </c>
@@ -10096,7 +10204,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="148" spans="1:8" ht="12.75">
+    <row ht="12.75" r="148" spans="1:8">
       <c r="A148">
         <v>147</v>
       </c>
@@ -10119,7 +10227,7 @@
         <v>881</v>
       </c>
     </row>
-    <row r="149" spans="1:8" ht="12.75">
+    <row ht="12.75" r="149" spans="1:8">
       <c r="A149">
         <v>148</v>
       </c>
@@ -10142,7 +10250,7 @@
         <v>881</v>
       </c>
     </row>
-    <row r="150" spans="1:8" ht="12.75">
+    <row ht="12.75" r="150" spans="1:8">
       <c r="A150">
         <v>149</v>
       </c>
@@ -10165,7 +10273,7 @@
         <v>881</v>
       </c>
     </row>
-    <row r="151" spans="1:8" ht="12.75">
+    <row ht="12.75" r="151" spans="1:8">
       <c r="A151">
         <v>150</v>
       </c>
@@ -10188,7 +10296,7 @@
         <v>427</v>
       </c>
     </row>
-    <row r="152" spans="1:8" ht="12.75">
+    <row ht="12.75" r="152" spans="1:8">
       <c r="A152">
         <v>151</v>
       </c>
@@ -10211,7 +10319,7 @@
         <v>881</v>
       </c>
     </row>
-    <row r="153" spans="1:8" ht="12.75">
+    <row ht="12.75" r="153" spans="1:8">
       <c r="A153">
         <v>152</v>
       </c>
@@ -10234,240 +10342,356 @@
         <v>881</v>
       </c>
     </row>
+    <row ht="12.75" r="154" spans="1:8">
+      <c r="A154">
+        <v>153</v>
+      </c>
+      <c r="B154" s="41" t="s">
+        <v>1127</v>
+      </c>
+      <c r="C154" t="s">
+        <v>1146</v>
+      </c>
+      <c r="D154" s="46" t="s">
+        <v>1145</v>
+      </c>
+      <c r="F154" s="2" t="s">
+        <v>1046</v>
+      </c>
+      <c r="G154" t="s">
+        <v>8</v>
+      </c>
+      <c r="H154" t="s">
+        <v>427</v>
+      </c>
+    </row>
+    <row ht="12.75" r="155" spans="1:8">
+      <c r="A155">
+        <v>154</v>
+      </c>
+      <c r="B155" s="41" t="s">
+        <v>1128</v>
+      </c>
+      <c r="D155" s="39" t="s">
+        <v>14</v>
+      </c>
+      <c r="F155" s="2" t="s">
+        <v>1046</v>
+      </c>
+      <c r="G155" t="s">
+        <v>37</v>
+      </c>
+      <c r="H155" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row ht="12.75" r="156" spans="1:8">
+      <c r="A156">
+        <v>155</v>
+      </c>
+      <c r="B156" s="41" t="s">
+        <v>1129</v>
+      </c>
+      <c r="C156" t="s">
+        <v>1147</v>
+      </c>
+      <c r="D156" s="46" t="s">
+        <v>1145</v>
+      </c>
+      <c r="F156" s="2" t="s">
+        <v>687</v>
+      </c>
+      <c r="G156" t="s">
+        <v>1044</v>
+      </c>
+      <c r="H156" t="s">
+        <v>881</v>
+      </c>
+    </row>
+    <row ht="12.75" r="157" spans="1:8">
+      <c r="A157">
+        <v>156</v>
+      </c>
+      <c r="B157" s="41" t="s">
+        <v>1130</v>
+      </c>
+      <c r="D157" s="39" t="s">
+        <v>14</v>
+      </c>
+      <c r="F157" s="2" t="s">
+        <v>687</v>
+      </c>
+      <c r="G157" t="s">
+        <v>1044</v>
+      </c>
+      <c r="H157" t="s">
+        <v>881</v>
+      </c>
+    </row>
+    <row ht="12.75" r="158" spans="1:8">
+      <c r="A158">
+        <v>157</v>
+      </c>
+      <c r="B158" s="41" t="s">
+        <v>1131</v>
+      </c>
+      <c r="C158" t="s">
+        <v>1148</v>
+      </c>
+      <c r="D158" s="46" t="s">
+        <v>1145</v>
+      </c>
+      <c r="F158" s="2" t="s">
+        <v>687</v>
+      </c>
+      <c r="G158" t="s">
+        <v>16</v>
+      </c>
+      <c r="H158" t="s">
+        <v>428</v>
+      </c>
+    </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B2" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
-    <hyperlink ref="B3" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
-    <hyperlink ref="B4" r:id="rId3" xr:uid="{00000000-0004-0000-0000-000002000000}"/>
-    <hyperlink ref="B5" r:id="rId4" xr:uid="{00000000-0004-0000-0000-000003000000}"/>
-    <hyperlink ref="B6" r:id="rId5" xr:uid="{00000000-0004-0000-0000-000004000000}"/>
-    <hyperlink ref="H6" r:id="rId6" xr:uid="{00000000-0004-0000-0000-000005000000}"/>
-    <hyperlink ref="B7" r:id="rId7" xr:uid="{00000000-0004-0000-0000-000006000000}"/>
-    <hyperlink ref="B8" r:id="rId8" xr:uid="{00000000-0004-0000-0000-000007000000}"/>
-    <hyperlink ref="B9" r:id="rId9" xr:uid="{00000000-0004-0000-0000-000008000000}"/>
-    <hyperlink ref="B10" r:id="rId10" xr:uid="{00000000-0004-0000-0000-000009000000}"/>
-    <hyperlink ref="B11" r:id="rId11" xr:uid="{00000000-0004-0000-0000-00000A000000}"/>
-    <hyperlink ref="B12" r:id="rId12" xr:uid="{00000000-0004-0000-0000-00000B000000}"/>
-    <hyperlink ref="B13" r:id="rId13" xr:uid="{00000000-0004-0000-0000-00000C000000}"/>
-    <hyperlink ref="B14" r:id="rId14" xr:uid="{00000000-0004-0000-0000-00000D000000}"/>
-    <hyperlink ref="B15" r:id="rId15" xr:uid="{00000000-0004-0000-0000-00000E000000}"/>
-    <hyperlink ref="B16" r:id="rId16" xr:uid="{00000000-0004-0000-0000-00000F000000}"/>
-    <hyperlink ref="B17" r:id="rId17" xr:uid="{00000000-0004-0000-0000-000010000000}"/>
-    <hyperlink ref="B18" r:id="rId18" xr:uid="{00000000-0004-0000-0000-000011000000}"/>
-    <hyperlink ref="B19" r:id="rId19" xr:uid="{00000000-0004-0000-0000-000012000000}"/>
-    <hyperlink ref="B20" r:id="rId20" xr:uid="{00000000-0004-0000-0000-000013000000}"/>
-    <hyperlink ref="B21" r:id="rId21" xr:uid="{00000000-0004-0000-0000-000014000000}"/>
-    <hyperlink ref="B22" r:id="rId22" xr:uid="{00000000-0004-0000-0000-000015000000}"/>
-    <hyperlink ref="B23" r:id="rId23" xr:uid="{00000000-0004-0000-0000-000016000000}"/>
-    <hyperlink ref="B24" r:id="rId24" xr:uid="{00000000-0004-0000-0000-000017000000}"/>
-    <hyperlink ref="B25" r:id="rId25" xr:uid="{00000000-0004-0000-0000-000018000000}"/>
-    <hyperlink ref="H25" r:id="rId26" xr:uid="{00000000-0004-0000-0000-000019000000}"/>
-    <hyperlink ref="B26" r:id="rId27" xr:uid="{00000000-0004-0000-0000-00001A000000}"/>
-    <hyperlink ref="H26" r:id="rId28" xr:uid="{00000000-0004-0000-0000-00001B000000}"/>
-    <hyperlink ref="B27" r:id="rId29" xr:uid="{00000000-0004-0000-0000-00001C000000}"/>
-    <hyperlink ref="H27" r:id="rId30" xr:uid="{00000000-0004-0000-0000-00001D000000}"/>
-    <hyperlink ref="B28" r:id="rId31" xr:uid="{00000000-0004-0000-0000-00001E000000}"/>
-    <hyperlink ref="H28" r:id="rId32" xr:uid="{00000000-0004-0000-0000-00001F000000}"/>
-    <hyperlink ref="B29" r:id="rId33" xr:uid="{00000000-0004-0000-0000-000020000000}"/>
-    <hyperlink ref="H29" r:id="rId34" xr:uid="{00000000-0004-0000-0000-000021000000}"/>
-    <hyperlink ref="B30" r:id="rId35" xr:uid="{00000000-0004-0000-0000-000022000000}"/>
-    <hyperlink ref="H30" r:id="rId36" xr:uid="{00000000-0004-0000-0000-000023000000}"/>
-    <hyperlink ref="B31" r:id="rId37" xr:uid="{00000000-0004-0000-0000-000024000000}"/>
-    <hyperlink ref="H31" r:id="rId38" xr:uid="{00000000-0004-0000-0000-000025000000}"/>
-    <hyperlink ref="B32" r:id="rId39" xr:uid="{00000000-0004-0000-0000-000026000000}"/>
-    <hyperlink ref="H32" r:id="rId40" xr:uid="{00000000-0004-0000-0000-000027000000}"/>
-    <hyperlink ref="B33" r:id="rId41" xr:uid="{00000000-0004-0000-0000-000028000000}"/>
-    <hyperlink ref="B34" r:id="rId42" xr:uid="{00000000-0004-0000-0000-000029000000}"/>
-    <hyperlink ref="B38" r:id="rId43" xr:uid="{00000000-0004-0000-0000-00002A000000}"/>
-    <hyperlink ref="B45" r:id="rId44" xr:uid="{00000000-0004-0000-0000-00002B000000}"/>
-    <hyperlink ref="B48" r:id="rId45" xr:uid="{00000000-0004-0000-0000-00002C000000}"/>
-    <hyperlink ref="B35" r:id="rId46" xr:uid="{00000000-0004-0000-0000-00002D000000}"/>
-    <hyperlink ref="B52" r:id="rId47" xr:uid="{00000000-0004-0000-0000-00002E000000}"/>
-    <hyperlink ref="B53" r:id="rId48" xr:uid="{00000000-0004-0000-0000-00002F000000}"/>
-    <hyperlink ref="B55" r:id="rId49" xr:uid="{00000000-0004-0000-0000-000030000000}"/>
-    <hyperlink ref="B56" r:id="rId50" xr:uid="{00000000-0004-0000-0000-000031000000}"/>
-    <hyperlink ref="B57" r:id="rId51" xr:uid="{00000000-0004-0000-0000-000032000000}"/>
-    <hyperlink ref="B58" r:id="rId52" xr:uid="{00000000-0004-0000-0000-000033000000}"/>
-    <hyperlink ref="B61" r:id="rId53" xr:uid="{00000000-0004-0000-0000-000034000000}"/>
-    <hyperlink ref="B62" r:id="rId54" xr:uid="{00000000-0004-0000-0000-000035000000}"/>
-    <hyperlink ref="B63" r:id="rId55" xr:uid="{00000000-0004-0000-0000-000036000000}"/>
-    <hyperlink ref="B64" r:id="rId56" xr:uid="{00000000-0004-0000-0000-000037000000}"/>
-    <hyperlink ref="B65" r:id="rId57" xr:uid="{00000000-0004-0000-0000-000038000000}"/>
-    <hyperlink ref="B66" r:id="rId58" xr:uid="{00000000-0004-0000-0000-000039000000}"/>
-    <hyperlink ref="B67" r:id="rId59" xr:uid="{00000000-0004-0000-0000-00003A000000}"/>
-    <hyperlink ref="H7:H24" r:id="rId60" display="https://www.allhomes.com.au/agency/trusted-realtors-570129/" xr:uid="{00000000-0004-0000-0000-00003B000000}"/>
-    <hyperlink ref="B43" r:id="rId61" xr:uid="{00000000-0004-0000-0000-00003C000000}"/>
-    <hyperlink ref="B44" r:id="rId62" xr:uid="{00000000-0004-0000-0000-00003D000000}"/>
-    <hyperlink ref="B46" r:id="rId63" xr:uid="{00000000-0004-0000-0000-00003E000000}"/>
-    <hyperlink ref="B54" r:id="rId64" xr:uid="{00000000-0004-0000-0000-00003F000000}"/>
-    <hyperlink ref="B42" r:id="rId65" xr:uid="{00000000-0004-0000-0000-000040000000}"/>
-    <hyperlink ref="J2" r:id="rId66" xr:uid="{00000000-0004-0000-0000-000041000000}"/>
-    <hyperlink ref="C69" r:id="rId67" xr:uid="{9DAE03A7-93E8-4507-BD6C-AC4013ECD47F}"/>
-    <hyperlink ref="C68" r:id="rId68" xr:uid="{66B9A9CA-DF82-46B6-9C5A-C5709E2FF1AE}"/>
-    <hyperlink ref="B75" r:id="rId69" xr:uid="{57E7BFEF-6F05-4DA9-A3DE-5B0A0EFED4D9}"/>
-    <hyperlink ref="C75" r:id="rId70" xr:uid="{F4755F93-6E59-4C38-BF66-16746869FDF3}"/>
-    <hyperlink ref="H75" r:id="rId71" xr:uid="{5BFAFD71-42C4-487F-B5E7-1697975992B4}"/>
-    <hyperlink ref="B78" r:id="rId72" xr:uid="{D3DE0D76-2479-4283-B7C7-F11B85797022}"/>
-    <hyperlink ref="C78" r:id="rId73" xr:uid="{FC1D9146-2FDC-4F13-A3C3-51CAB46DEC08}"/>
-    <hyperlink ref="B68" r:id="rId74" xr:uid="{3ED6FAA1-2B0F-4DB9-878E-9640A9C2850D}"/>
-    <hyperlink ref="B69" r:id="rId75" xr:uid="{12DE6CA8-DDC5-4E7B-BD2E-14B105A0DE3B}"/>
-    <hyperlink ref="C70" r:id="rId76" xr:uid="{0419758C-286A-4B76-B8B2-31CC336DEDF1}"/>
-    <hyperlink ref="B70" r:id="rId77" xr:uid="{AC18D1D2-FA3D-4352-A402-35B7AAFE27C0}"/>
-    <hyperlink ref="B71" r:id="rId78" xr:uid="{E8BCA1EF-4E17-4AA7-A2CE-5674FC05ABC3}"/>
-    <hyperlink ref="C71" r:id="rId79" xr:uid="{949AE606-DF4A-48F4-93A0-F148D80842CB}"/>
-    <hyperlink ref="B72" r:id="rId80" xr:uid="{69A93BB5-0295-46D6-8334-45444356E6E9}"/>
-    <hyperlink ref="C72" r:id="rId81" xr:uid="{CA171BC7-126F-4175-8A03-123D5A2C2D8A}"/>
-    <hyperlink ref="C73" r:id="rId82" xr:uid="{FACC205D-E563-4266-8E0D-0794F3D76E98}"/>
-    <hyperlink ref="B85" r:id="rId83" xr:uid="{7ABCABC0-A765-435B-AE52-9D27F653E00F}"/>
-    <hyperlink ref="C4" r:id="rId84" xr:uid="{2CD58DBE-98E3-4EDC-898F-088D5F0FCB81}"/>
-    <hyperlink ref="C29" r:id="rId85" xr:uid="{CB7CAD83-ACA3-4309-B102-B0F536FC97E6}"/>
-    <hyperlink ref="C90" r:id="rId86" xr:uid="{B4F55488-2B40-4078-ABF0-4B4254363237}"/>
-    <hyperlink ref="B90" r:id="rId87" xr:uid="{09FEE7FE-E667-40E8-BC22-3FDC999B614F}"/>
-    <hyperlink ref="C15" r:id="rId88" xr:uid="{34F25BA9-B460-46CF-85C0-4AC9D6288B41}"/>
-    <hyperlink ref="C3" r:id="rId89" xr:uid="{EBAAEE7A-83B2-457B-8600-89427BF11448}"/>
-    <hyperlink ref="C8" r:id="rId90" xr:uid="{3D3D678C-8F1B-47BC-ACA2-D1CBF5A76F0B}"/>
-    <hyperlink ref="C19" r:id="rId91" xr:uid="{ED2C9A9B-3440-4B4A-91A1-7CAF84972535}"/>
-    <hyperlink ref="C20" r:id="rId92" xr:uid="{E47C999F-11AE-4F93-9032-6E51EB582635}"/>
-    <hyperlink ref="C21" r:id="rId93" xr:uid="{E59411CC-EC13-4665-969A-8D9238CCD0C2}"/>
-    <hyperlink ref="C33" r:id="rId94" xr:uid="{9C953AB9-0076-4477-B52F-C393846B1211}"/>
-    <hyperlink ref="C38" r:id="rId95" xr:uid="{D349EA20-36BF-44C7-A16B-E85B8FE53B2A}"/>
-    <hyperlink ref="C39" r:id="rId96" xr:uid="{DE18DA3B-1A3D-4613-888E-7F506CC87091}"/>
-    <hyperlink ref="C40" r:id="rId97" xr:uid="{0C71282B-049B-4CD1-A090-B66647F2B29B}"/>
-    <hyperlink ref="C42" r:id="rId98" xr:uid="{AD0DC851-DEC5-4ACE-B928-50149068BB70}"/>
-    <hyperlink ref="C45" r:id="rId99" xr:uid="{EB51DFC2-D28F-4E0C-B019-F9954D6C9832}"/>
-    <hyperlink ref="C52" r:id="rId100" xr:uid="{9E5146F6-8EC8-4A2C-B192-C1CCB11CAB8A}"/>
-    <hyperlink ref="C48" r:id="rId101" xr:uid="{31B308E4-DA3E-401B-B796-7D03404228FB}"/>
-    <hyperlink ref="C49" r:id="rId102" xr:uid="{EBAAB9CE-7F91-4628-AF75-32C4EEF948C2}"/>
-    <hyperlink ref="C53" r:id="rId103" xr:uid="{2FF7EB1F-CD56-4E71-AD0F-0D12E8347603}"/>
-    <hyperlink ref="C55" r:id="rId104" xr:uid="{9BD44DCD-EEBB-4649-9792-F3DAC40B3960}"/>
-    <hyperlink ref="C63" r:id="rId105" xr:uid="{9929BCF4-32FD-4143-99F6-FEB21B90BCD7}"/>
-    <hyperlink ref="C64" r:id="rId106" xr:uid="{80B3DEC9-506E-4F3A-B171-A2D71B731577}"/>
-    <hyperlink ref="C66" r:id="rId107" xr:uid="{011D2C70-C541-49D4-894E-FF670D6C19BB}"/>
-    <hyperlink ref="C67" r:id="rId108" xr:uid="{B62DFA3B-60A0-44AA-BF1D-BCA2A049E46C}"/>
-    <hyperlink ref="C56" r:id="rId109" xr:uid="{C98B5D5D-65AB-489D-8160-8F1B41CDE6A7}"/>
-    <hyperlink ref="B103" r:id="rId110" xr:uid="{4D81C408-B745-40E2-B9C7-6E36C45175A7}"/>
-    <hyperlink ref="C26" r:id="rId111" xr:uid="{6A9C6F44-3E7F-47CF-8514-B6609EBEE668}"/>
-    <hyperlink ref="C23" r:id="rId112" xr:uid="{F99F350A-C378-4940-B611-41F47BC3B4B0}"/>
-    <hyperlink ref="C103" r:id="rId113" xr:uid="{3E9C8DCE-ABC0-49DA-B64B-B569BAAE6ED0}"/>
-    <hyperlink ref="C104" r:id="rId114" xr:uid="{E96AA061-2DED-4A35-BE99-8E7E156527EB}"/>
-    <hyperlink ref="C102" r:id="rId115" xr:uid="{4DAA7E56-3BCD-4AF1-B6E7-A26B02A0DA6C}"/>
-    <hyperlink ref="C101" r:id="rId116" xr:uid="{EBE0EC7F-0880-4F4A-991C-2C7C53889923}"/>
-    <hyperlink ref="C100" r:id="rId117" xr:uid="{7AA4A2D0-C18F-4625-A776-6EDD2415E1BC}"/>
-    <hyperlink ref="C99" r:id="rId118" xr:uid="{15BFB680-4225-425B-8826-841A35922C8A}"/>
-    <hyperlink ref="B99" r:id="rId119" xr:uid="{1EF2BF94-D92B-41EF-8B1F-0585F1910B74}"/>
-    <hyperlink ref="C97" r:id="rId120" xr:uid="{6687C5A1-CC2B-49FF-B98D-946AA21B8C55}"/>
-    <hyperlink ref="B97" r:id="rId121" xr:uid="{0411E592-2DE8-4D1D-B66C-46CE99CAA412}"/>
-    <hyperlink ref="C96" r:id="rId122" xr:uid="{A7ED7210-DE23-4760-B67F-78027E9B9B73}"/>
-    <hyperlink ref="B96" r:id="rId123" xr:uid="{992F1752-E440-4347-A698-44C8E60F00BE}"/>
-    <hyperlink ref="B102" r:id="rId124" xr:uid="{A0E03FB2-010F-497D-874D-A0A66FB6303C}"/>
-    <hyperlink ref="B101" r:id="rId125" xr:uid="{165FBF6F-9195-42DA-AC37-C49B2308ACA1}"/>
-    <hyperlink ref="B94" r:id="rId126" xr:uid="{7DB2C8A6-8C43-4818-A7C2-D5E14351114B}"/>
-    <hyperlink ref="B93" r:id="rId127" xr:uid="{EFC122F7-44E7-447B-8F21-BA1503A72780}"/>
-    <hyperlink ref="B91" r:id="rId128" xr:uid="{7AC22E1D-6919-43E6-AD91-1551DBBDE570}"/>
-    <hyperlink ref="B88" r:id="rId129" xr:uid="{FB3E9840-E4E3-4E64-8CCF-2BAEC7024AD6}"/>
-    <hyperlink ref="B87" r:id="rId130" xr:uid="{348337ED-A616-4A9D-A8D3-0091262177C6}"/>
-    <hyperlink ref="B86" r:id="rId131" xr:uid="{CF62843D-4B82-47CB-B74F-D3F292E9603A}"/>
-    <hyperlink ref="B84" r:id="rId132" xr:uid="{9CA10EFF-3943-479E-914B-1D6EE04D75FC}"/>
-    <hyperlink ref="C84" r:id="rId133" xr:uid="{1074AAC9-CCB0-4FFC-9AFB-EFD1363D7538}"/>
-    <hyperlink ref="B105" r:id="rId134" xr:uid="{D6DE2797-5A68-4C1E-9E74-0D323B6ADFA2}"/>
-    <hyperlink ref="B106" r:id="rId135" xr:uid="{1FCAF9BA-00B5-4008-B5C8-E822ABD6BCDD}"/>
-    <hyperlink ref="C11" r:id="rId136" xr:uid="{893B2404-B185-41F7-B397-A3E08B386C5F}"/>
-    <hyperlink ref="B107" r:id="rId137" xr:uid="{B0E609F4-D8A3-433A-BE15-17E4804C6EA3}"/>
-    <hyperlink ref="C107" r:id="rId138" xr:uid="{6793ECA4-A034-42EC-A741-3B0FF42BC11B}"/>
-    <hyperlink ref="B108" r:id="rId139" xr:uid="{4DB78F44-0F08-4561-A0E8-0EE92F9FFECB}"/>
-    <hyperlink ref="B114" r:id="rId140" xr:uid="{27750164-38B8-4B5E-9B5A-E6C71FFFC61F}"/>
-    <hyperlink ref="C114" r:id="rId141" xr:uid="{6FE6A043-A6B1-44FF-8A45-8C3690323458}"/>
-    <hyperlink ref="B113" r:id="rId142" xr:uid="{0F94FF41-1E06-4D7B-B360-1EB377073C87}"/>
-    <hyperlink ref="B112" r:id="rId143" xr:uid="{490A5044-10EC-4082-BEC1-14008171D5CF}"/>
-    <hyperlink ref="B49" r:id="rId144" xr:uid="{836EB236-8BF1-4259-B395-AD9FA9DE0AE0}"/>
-    <hyperlink ref="B74" r:id="rId145" xr:uid="{8AA8904A-1CC5-4D06-93EF-66F7FC625199}"/>
-    <hyperlink ref="B76" r:id="rId146" xr:uid="{5743888C-C74A-41C6-ABC5-E9575351702D}"/>
-    <hyperlink ref="B115" r:id="rId147" xr:uid="{27BDB583-8AD0-4B33-BA19-24E42C9E7CE9}"/>
-    <hyperlink ref="B117" r:id="rId148" xr:uid="{92BA6213-0D94-4C5A-B06A-6FC35C0BECA9}"/>
-    <hyperlink ref="B119" r:id="rId149" xr:uid="{6724AE23-65F5-4D67-ADA6-E20BD420531B}"/>
-    <hyperlink ref="C119" r:id="rId150" xr:uid="{0A5009EB-B388-4AF4-99CE-5813711C2B1E}"/>
-    <hyperlink ref="B120" r:id="rId151" xr:uid="{255CB59B-E711-471E-8ACE-D0ABA408AE96}"/>
-    <hyperlink ref="B39" r:id="rId152" xr:uid="{39FB4A7C-4EA8-4530-9FE6-2842C777350C}"/>
-    <hyperlink ref="B104" r:id="rId153" xr:uid="{FC8A6FB5-FCCF-409E-9D6D-A93D412B2275}"/>
-    <hyperlink ref="C105" r:id="rId154" xr:uid="{988B91BF-CEBD-44F6-A773-3C87D877BE5A}"/>
-    <hyperlink ref="C108" r:id="rId155" xr:uid="{F0593E1B-3EE0-4DF2-B93E-84A02071630B}"/>
-    <hyperlink ref="B109" r:id="rId156" xr:uid="{601C40E0-818B-457C-9FE7-30D06707CEB7}"/>
-    <hyperlink ref="C109" r:id="rId157" xr:uid="{E1D93474-1A3D-49F1-B191-3C3484679D2D}"/>
-    <hyperlink ref="C83" r:id="rId158" xr:uid="{B0D57129-C33F-45FF-B844-E7642495443D}"/>
-    <hyperlink ref="B83" r:id="rId159" xr:uid="{7DCBF3E6-0CD2-475D-AE1F-56469491B512}"/>
-    <hyperlink ref="C120" r:id="rId160" xr:uid="{F24698EA-BA1A-4C92-8B6D-72A40DDDD7A3}"/>
-    <hyperlink ref="C122" r:id="rId161" xr:uid="{BAC9069D-9D63-415D-B933-A4F86CB8C587}"/>
-    <hyperlink ref="C123" r:id="rId162" xr:uid="{140A866C-FAC2-4A61-BA7E-0AFB9A05FD2F}"/>
-    <hyperlink ref="C124" r:id="rId163" xr:uid="{6EA83FA2-D552-4B23-98A9-6C5EFC3BC2CA}"/>
-    <hyperlink ref="C125" r:id="rId164" xr:uid="{E34375AF-4BB2-420C-887F-8D684FC72F4C}"/>
-    <hyperlink ref="C126" r:id="rId165" xr:uid="{CB74A187-1404-4E3B-B1EF-E6C50CF09D3E}"/>
-    <hyperlink ref="C127" r:id="rId166" xr:uid="{B0565FA3-8BDF-4E3B-9814-B9F51432FA7D}"/>
-    <hyperlink ref="C128" r:id="rId167" xr:uid="{8504A7CE-7DD9-4C74-83D8-90E0745EAB21}"/>
-    <hyperlink ref="C130" r:id="rId168" xr:uid="{D3DDF4DA-6F84-4EAF-BA60-77D926C7C2AC}"/>
-    <hyperlink ref="C131" r:id="rId169" xr:uid="{060B4F44-BF89-4037-9E74-C61E23C6AAC9}"/>
-    <hyperlink ref="C132" r:id="rId170" xr:uid="{8FD9E395-82BD-4EEA-89E9-166FDA928F87}"/>
-    <hyperlink ref="C133" r:id="rId171" xr:uid="{3669E93D-A9CE-4C72-B1DD-98E95312A18C}"/>
-    <hyperlink ref="C136" r:id="rId172" xr:uid="{E14EBE84-3FBA-44D8-B082-69967148B456}"/>
-    <hyperlink ref="C137" r:id="rId173" xr:uid="{CC0D1827-F782-476A-9312-1BAA88B7D496}"/>
-    <hyperlink ref="C141" r:id="rId174" xr:uid="{1528B515-167A-4838-B645-B63CD0312C05}"/>
-    <hyperlink ref="B143" r:id="rId175" xr:uid="{50B775B1-8A20-4A55-90CA-EC152D3C2098}"/>
-    <hyperlink ref="B144" r:id="rId176" xr:uid="{F6EFF9E5-8AC0-4C40-A2A8-62DF9BB671E9}"/>
-    <hyperlink ref="C145" r:id="rId177" xr:uid="{DE56B3AC-2F1A-494E-A9CD-9C972DA863E2}"/>
-    <hyperlink ref="B145" r:id="rId178" xr:uid="{F783979B-F441-49BC-98C4-8448098CBBC1}"/>
-    <hyperlink ref="C17" r:id="rId179" xr:uid="{DBE3D417-C525-4AE7-BA26-A27F8BD7B6D3}"/>
-    <hyperlink ref="B121" r:id="rId180" xr:uid="{BF1CBD80-282B-4284-A960-458EE8D86966}"/>
-    <hyperlink ref="C146" r:id="rId181" xr:uid="{3FA9DCB7-198C-457D-99E0-AF0A29EDEAF1}"/>
-    <hyperlink ref="B146" r:id="rId182" xr:uid="{6B057403-173E-478A-AFE1-5BA96D6006F7}"/>
-    <hyperlink ref="C147" r:id="rId183" xr:uid="{FBD8EA4A-7B80-4D87-BD4D-6D3DDE043E14}"/>
-    <hyperlink ref="B147" r:id="rId184" xr:uid="{F9D4FD4A-592C-4041-AD52-AAD4E4FECD78}"/>
-    <hyperlink ref="C148" r:id="rId185" xr:uid="{EF3F39F0-4058-49A5-8980-E800B6F200B5}"/>
-    <hyperlink ref="B148" r:id="rId186" xr:uid="{513D1B27-06CF-4F01-AD66-B1DDDB3DF171}"/>
-    <hyperlink ref="C149" r:id="rId187" xr:uid="{BFCDD610-AD9F-445C-AAE8-66DB3CD722A6}"/>
-    <hyperlink ref="B149" r:id="rId188" xr:uid="{1567BEF7-2918-4A3A-89A1-A37D6C6B5419}"/>
-    <hyperlink ref="B150" r:id="rId189" xr:uid="{233679EA-F519-4185-AA17-F008EE8DA109}"/>
-    <hyperlink ref="C153" r:id="rId190" xr:uid="{D979C888-F3D2-4FAE-9C96-C32136017BEF}"/>
-    <hyperlink ref="B153" r:id="rId191" xr:uid="{F7FA0B04-B8E5-4470-AA22-DE86ABDF6874}"/>
+    <hyperlink r:id="rId1" ref="B2" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
+    <hyperlink r:id="rId2" ref="B3" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
+    <hyperlink r:id="rId3" ref="B4" xr:uid="{00000000-0004-0000-0000-000002000000}"/>
+    <hyperlink r:id="rId4" ref="B5" xr:uid="{00000000-0004-0000-0000-000003000000}"/>
+    <hyperlink r:id="rId5" ref="B6" xr:uid="{00000000-0004-0000-0000-000004000000}"/>
+    <hyperlink r:id="rId6" ref="H6" xr:uid="{00000000-0004-0000-0000-000005000000}"/>
+    <hyperlink r:id="rId7" ref="B7" xr:uid="{00000000-0004-0000-0000-000006000000}"/>
+    <hyperlink r:id="rId8" ref="B8" xr:uid="{00000000-0004-0000-0000-000007000000}"/>
+    <hyperlink r:id="rId9" ref="B9" xr:uid="{00000000-0004-0000-0000-000008000000}"/>
+    <hyperlink r:id="rId10" ref="B10" xr:uid="{00000000-0004-0000-0000-000009000000}"/>
+    <hyperlink r:id="rId11" ref="B11" xr:uid="{00000000-0004-0000-0000-00000A000000}"/>
+    <hyperlink r:id="rId12" ref="B12" xr:uid="{00000000-0004-0000-0000-00000B000000}"/>
+    <hyperlink r:id="rId13" ref="B13" xr:uid="{00000000-0004-0000-0000-00000C000000}"/>
+    <hyperlink r:id="rId14" ref="B14" xr:uid="{00000000-0004-0000-0000-00000D000000}"/>
+    <hyperlink r:id="rId15" ref="B15" xr:uid="{00000000-0004-0000-0000-00000E000000}"/>
+    <hyperlink r:id="rId16" ref="B16" xr:uid="{00000000-0004-0000-0000-00000F000000}"/>
+    <hyperlink r:id="rId17" ref="B17" xr:uid="{00000000-0004-0000-0000-000010000000}"/>
+    <hyperlink r:id="rId18" ref="B18" xr:uid="{00000000-0004-0000-0000-000011000000}"/>
+    <hyperlink r:id="rId19" ref="B19" xr:uid="{00000000-0004-0000-0000-000012000000}"/>
+    <hyperlink r:id="rId20" ref="B20" xr:uid="{00000000-0004-0000-0000-000013000000}"/>
+    <hyperlink r:id="rId21" ref="B21" xr:uid="{00000000-0004-0000-0000-000014000000}"/>
+    <hyperlink r:id="rId22" ref="B22" xr:uid="{00000000-0004-0000-0000-000015000000}"/>
+    <hyperlink r:id="rId23" ref="B23" xr:uid="{00000000-0004-0000-0000-000016000000}"/>
+    <hyperlink r:id="rId24" ref="B24" xr:uid="{00000000-0004-0000-0000-000017000000}"/>
+    <hyperlink r:id="rId25" ref="B25" xr:uid="{00000000-0004-0000-0000-000018000000}"/>
+    <hyperlink r:id="rId26" ref="H25" xr:uid="{00000000-0004-0000-0000-000019000000}"/>
+    <hyperlink r:id="rId27" ref="B26" xr:uid="{00000000-0004-0000-0000-00001A000000}"/>
+    <hyperlink r:id="rId28" ref="H26" xr:uid="{00000000-0004-0000-0000-00001B000000}"/>
+    <hyperlink r:id="rId29" ref="B27" xr:uid="{00000000-0004-0000-0000-00001C000000}"/>
+    <hyperlink r:id="rId30" ref="H27" xr:uid="{00000000-0004-0000-0000-00001D000000}"/>
+    <hyperlink r:id="rId31" ref="B28" xr:uid="{00000000-0004-0000-0000-00001E000000}"/>
+    <hyperlink r:id="rId32" ref="H28" xr:uid="{00000000-0004-0000-0000-00001F000000}"/>
+    <hyperlink r:id="rId33" ref="B29" xr:uid="{00000000-0004-0000-0000-000020000000}"/>
+    <hyperlink r:id="rId34" ref="H29" xr:uid="{00000000-0004-0000-0000-000021000000}"/>
+    <hyperlink r:id="rId35" ref="B30" xr:uid="{00000000-0004-0000-0000-000022000000}"/>
+    <hyperlink r:id="rId36" ref="H30" xr:uid="{00000000-0004-0000-0000-000023000000}"/>
+    <hyperlink r:id="rId37" ref="B31" xr:uid="{00000000-0004-0000-0000-000024000000}"/>
+    <hyperlink r:id="rId38" ref="H31" xr:uid="{00000000-0004-0000-0000-000025000000}"/>
+    <hyperlink r:id="rId39" ref="B32" xr:uid="{00000000-0004-0000-0000-000026000000}"/>
+    <hyperlink r:id="rId40" ref="H32" xr:uid="{00000000-0004-0000-0000-000027000000}"/>
+    <hyperlink r:id="rId41" ref="B33" xr:uid="{00000000-0004-0000-0000-000028000000}"/>
+    <hyperlink r:id="rId42" ref="B34" xr:uid="{00000000-0004-0000-0000-000029000000}"/>
+    <hyperlink r:id="rId43" ref="B38" xr:uid="{00000000-0004-0000-0000-00002A000000}"/>
+    <hyperlink r:id="rId44" ref="B45" xr:uid="{00000000-0004-0000-0000-00002B000000}"/>
+    <hyperlink r:id="rId45" ref="B48" xr:uid="{00000000-0004-0000-0000-00002C000000}"/>
+    <hyperlink r:id="rId46" ref="B35" xr:uid="{00000000-0004-0000-0000-00002D000000}"/>
+    <hyperlink r:id="rId47" ref="B52" xr:uid="{00000000-0004-0000-0000-00002E000000}"/>
+    <hyperlink r:id="rId48" ref="B53" xr:uid="{00000000-0004-0000-0000-00002F000000}"/>
+    <hyperlink r:id="rId49" ref="B55" xr:uid="{00000000-0004-0000-0000-000030000000}"/>
+    <hyperlink r:id="rId50" ref="B56" xr:uid="{00000000-0004-0000-0000-000031000000}"/>
+    <hyperlink r:id="rId51" ref="B57" xr:uid="{00000000-0004-0000-0000-000032000000}"/>
+    <hyperlink r:id="rId52" ref="B58" xr:uid="{00000000-0004-0000-0000-000033000000}"/>
+    <hyperlink r:id="rId53" ref="B61" xr:uid="{00000000-0004-0000-0000-000034000000}"/>
+    <hyperlink r:id="rId54" ref="B62" xr:uid="{00000000-0004-0000-0000-000035000000}"/>
+    <hyperlink r:id="rId55" ref="B63" xr:uid="{00000000-0004-0000-0000-000036000000}"/>
+    <hyperlink r:id="rId56" ref="B64" xr:uid="{00000000-0004-0000-0000-000037000000}"/>
+    <hyperlink r:id="rId57" ref="B65" xr:uid="{00000000-0004-0000-0000-000038000000}"/>
+    <hyperlink r:id="rId58" ref="B66" xr:uid="{00000000-0004-0000-0000-000039000000}"/>
+    <hyperlink r:id="rId59" ref="B67" xr:uid="{00000000-0004-0000-0000-00003A000000}"/>
+    <hyperlink display="https://www.allhomes.com.au/agency/trusted-realtors-570129/" r:id="rId60" ref="H7:H24" xr:uid="{00000000-0004-0000-0000-00003B000000}"/>
+    <hyperlink r:id="rId61" ref="B43" xr:uid="{00000000-0004-0000-0000-00003C000000}"/>
+    <hyperlink r:id="rId62" ref="B44" xr:uid="{00000000-0004-0000-0000-00003D000000}"/>
+    <hyperlink r:id="rId63" ref="B46" xr:uid="{00000000-0004-0000-0000-00003E000000}"/>
+    <hyperlink r:id="rId64" ref="B54" xr:uid="{00000000-0004-0000-0000-00003F000000}"/>
+    <hyperlink r:id="rId65" ref="B42" xr:uid="{00000000-0004-0000-0000-000040000000}"/>
+    <hyperlink r:id="rId66" ref="J2" xr:uid="{00000000-0004-0000-0000-000041000000}"/>
+    <hyperlink r:id="rId67" ref="C69" xr:uid="{9DAE03A7-93E8-4507-BD6C-AC4013ECD47F}"/>
+    <hyperlink r:id="rId68" ref="C68" xr:uid="{66B9A9CA-DF82-46B6-9C5A-C5709E2FF1AE}"/>
+    <hyperlink r:id="rId69" ref="B75" xr:uid="{57E7BFEF-6F05-4DA9-A3DE-5B0A0EFED4D9}"/>
+    <hyperlink r:id="rId70" ref="C75" xr:uid="{F4755F93-6E59-4C38-BF66-16746869FDF3}"/>
+    <hyperlink r:id="rId71" ref="H75" xr:uid="{5BFAFD71-42C4-487F-B5E7-1697975992B4}"/>
+    <hyperlink r:id="rId72" ref="B78" xr:uid="{D3DE0D76-2479-4283-B7C7-F11B85797022}"/>
+    <hyperlink r:id="rId73" ref="C78" xr:uid="{FC1D9146-2FDC-4F13-A3C3-51CAB46DEC08}"/>
+    <hyperlink r:id="rId74" ref="B68" xr:uid="{3ED6FAA1-2B0F-4DB9-878E-9640A9C2850D}"/>
+    <hyperlink r:id="rId75" ref="B69" xr:uid="{12DE6CA8-DDC5-4E7B-BD2E-14B105A0DE3B}"/>
+    <hyperlink r:id="rId76" ref="C70" xr:uid="{0419758C-286A-4B76-B8B2-31CC336DEDF1}"/>
+    <hyperlink r:id="rId77" ref="B70" xr:uid="{AC18D1D2-FA3D-4352-A402-35B7AAFE27C0}"/>
+    <hyperlink r:id="rId78" ref="B71" xr:uid="{E8BCA1EF-4E17-4AA7-A2CE-5674FC05ABC3}"/>
+    <hyperlink r:id="rId79" ref="C71" xr:uid="{949AE606-DF4A-48F4-93A0-F148D80842CB}"/>
+    <hyperlink r:id="rId80" ref="B72" xr:uid="{69A93BB5-0295-46D6-8334-45444356E6E9}"/>
+    <hyperlink r:id="rId81" ref="C72" xr:uid="{CA171BC7-126F-4175-8A03-123D5A2C2D8A}"/>
+    <hyperlink r:id="rId82" ref="C73" xr:uid="{FACC205D-E563-4266-8E0D-0794F3D76E98}"/>
+    <hyperlink r:id="rId83" ref="B85" xr:uid="{7ABCABC0-A765-435B-AE52-9D27F653E00F}"/>
+    <hyperlink r:id="rId84" ref="C4" xr:uid="{2CD58DBE-98E3-4EDC-898F-088D5F0FCB81}"/>
+    <hyperlink r:id="rId85" ref="C29" xr:uid="{CB7CAD83-ACA3-4309-B102-B0F536FC97E6}"/>
+    <hyperlink r:id="rId86" ref="C90" xr:uid="{B4F55488-2B40-4078-ABF0-4B4254363237}"/>
+    <hyperlink r:id="rId87" ref="B90" xr:uid="{09FEE7FE-E667-40E8-BC22-3FDC999B614F}"/>
+    <hyperlink r:id="rId88" ref="C15" xr:uid="{34F25BA9-B460-46CF-85C0-4AC9D6288B41}"/>
+    <hyperlink r:id="rId89" ref="C3" xr:uid="{EBAAEE7A-83B2-457B-8600-89427BF11448}"/>
+    <hyperlink r:id="rId90" ref="C8" xr:uid="{3D3D678C-8F1B-47BC-ACA2-D1CBF5A76F0B}"/>
+    <hyperlink r:id="rId91" ref="C19" xr:uid="{ED2C9A9B-3440-4B4A-91A1-7CAF84972535}"/>
+    <hyperlink r:id="rId92" ref="C20" xr:uid="{E47C999F-11AE-4F93-9032-6E51EB582635}"/>
+    <hyperlink r:id="rId93" ref="C21" xr:uid="{E59411CC-EC13-4665-969A-8D9238CCD0C2}"/>
+    <hyperlink r:id="rId94" ref="C33" xr:uid="{9C953AB9-0076-4477-B52F-C393846B1211}"/>
+    <hyperlink r:id="rId95" ref="C38" xr:uid="{D349EA20-36BF-44C7-A16B-E85B8FE53B2A}"/>
+    <hyperlink r:id="rId96" ref="C39" xr:uid="{DE18DA3B-1A3D-4613-888E-7F506CC87091}"/>
+    <hyperlink r:id="rId97" ref="C40" xr:uid="{0C71282B-049B-4CD1-A090-B66647F2B29B}"/>
+    <hyperlink r:id="rId98" ref="C42" xr:uid="{AD0DC851-DEC5-4ACE-B928-50149068BB70}"/>
+    <hyperlink r:id="rId99" ref="C45" xr:uid="{EB51DFC2-D28F-4E0C-B019-F9954D6C9832}"/>
+    <hyperlink r:id="rId100" ref="C52" xr:uid="{9E5146F6-8EC8-4A2C-B192-C1CCB11CAB8A}"/>
+    <hyperlink r:id="rId101" ref="C48" xr:uid="{31B308E4-DA3E-401B-B796-7D03404228FB}"/>
+    <hyperlink r:id="rId102" ref="C49" xr:uid="{EBAAB9CE-7F91-4628-AF75-32C4EEF948C2}"/>
+    <hyperlink r:id="rId103" ref="C53" xr:uid="{2FF7EB1F-CD56-4E71-AD0F-0D12E8347603}"/>
+    <hyperlink r:id="rId104" ref="C55" xr:uid="{9BD44DCD-EEBB-4649-9792-F3DAC40B3960}"/>
+    <hyperlink r:id="rId105" ref="C63" xr:uid="{9929BCF4-32FD-4143-99F6-FEB21B90BCD7}"/>
+    <hyperlink r:id="rId106" ref="C64" xr:uid="{80B3DEC9-506E-4F3A-B171-A2D71B731577}"/>
+    <hyperlink r:id="rId107" ref="C66" xr:uid="{011D2C70-C541-49D4-894E-FF670D6C19BB}"/>
+    <hyperlink r:id="rId108" ref="C67" xr:uid="{B62DFA3B-60A0-44AA-BF1D-BCA2A049E46C}"/>
+    <hyperlink r:id="rId109" ref="C56" xr:uid="{C98B5D5D-65AB-489D-8160-8F1B41CDE6A7}"/>
+    <hyperlink r:id="rId110" ref="B103" xr:uid="{4D81C408-B745-40E2-B9C7-6E36C45175A7}"/>
+    <hyperlink r:id="rId111" ref="C26" xr:uid="{6A9C6F44-3E7F-47CF-8514-B6609EBEE668}"/>
+    <hyperlink r:id="rId112" ref="C23" xr:uid="{F99F350A-C378-4940-B611-41F47BC3B4B0}"/>
+    <hyperlink r:id="rId113" ref="C103" xr:uid="{3E9C8DCE-ABC0-49DA-B64B-B569BAAE6ED0}"/>
+    <hyperlink r:id="rId114" ref="C104" xr:uid="{E96AA061-2DED-4A35-BE99-8E7E156527EB}"/>
+    <hyperlink r:id="rId115" ref="C102" xr:uid="{4DAA7E56-3BCD-4AF1-B6E7-A26B02A0DA6C}"/>
+    <hyperlink r:id="rId116" ref="C101" xr:uid="{EBE0EC7F-0880-4F4A-991C-2C7C53889923}"/>
+    <hyperlink r:id="rId117" ref="C100" xr:uid="{7AA4A2D0-C18F-4625-A776-6EDD2415E1BC}"/>
+    <hyperlink r:id="rId118" ref="C99" xr:uid="{15BFB680-4225-425B-8826-841A35922C8A}"/>
+    <hyperlink r:id="rId119" ref="B99" xr:uid="{1EF2BF94-D92B-41EF-8B1F-0585F1910B74}"/>
+    <hyperlink r:id="rId120" ref="C97" xr:uid="{6687C5A1-CC2B-49FF-B98D-946AA21B8C55}"/>
+    <hyperlink r:id="rId121" ref="B97" xr:uid="{0411E592-2DE8-4D1D-B66C-46CE99CAA412}"/>
+    <hyperlink r:id="rId122" ref="C96" xr:uid="{A7ED7210-DE23-4760-B67F-78027E9B9B73}"/>
+    <hyperlink r:id="rId123" ref="B96" xr:uid="{992F1752-E440-4347-A698-44C8E60F00BE}"/>
+    <hyperlink r:id="rId124" ref="B102" xr:uid="{A0E03FB2-010F-497D-874D-A0A66FB6303C}"/>
+    <hyperlink r:id="rId125" ref="B101" xr:uid="{165FBF6F-9195-42DA-AC37-C49B2308ACA1}"/>
+    <hyperlink r:id="rId126" ref="B94" xr:uid="{7DB2C8A6-8C43-4818-A7C2-D5E14351114B}"/>
+    <hyperlink r:id="rId127" ref="B93" xr:uid="{EFC122F7-44E7-447B-8F21-BA1503A72780}"/>
+    <hyperlink r:id="rId128" ref="B91" xr:uid="{7AC22E1D-6919-43E6-AD91-1551DBBDE570}"/>
+    <hyperlink r:id="rId129" ref="B88" xr:uid="{FB3E9840-E4E3-4E64-8CCF-2BAEC7024AD6}"/>
+    <hyperlink r:id="rId130" ref="B87" xr:uid="{348337ED-A616-4A9D-A8D3-0091262177C6}"/>
+    <hyperlink r:id="rId131" ref="B86" xr:uid="{CF62843D-4B82-47CB-B74F-D3F292E9603A}"/>
+    <hyperlink r:id="rId132" ref="B84" xr:uid="{9CA10EFF-3943-479E-914B-1D6EE04D75FC}"/>
+    <hyperlink r:id="rId133" ref="C84" xr:uid="{1074AAC9-CCB0-4FFC-9AFB-EFD1363D7538}"/>
+    <hyperlink r:id="rId134" ref="B105" xr:uid="{D6DE2797-5A68-4C1E-9E74-0D323B6ADFA2}"/>
+    <hyperlink r:id="rId135" ref="B106" xr:uid="{1FCAF9BA-00B5-4008-B5C8-E822ABD6BCDD}"/>
+    <hyperlink r:id="rId136" ref="C11" xr:uid="{893B2404-B185-41F7-B397-A3E08B386C5F}"/>
+    <hyperlink r:id="rId137" ref="B107" xr:uid="{B0E609F4-D8A3-433A-BE15-17E4804C6EA3}"/>
+    <hyperlink r:id="rId138" ref="C107" xr:uid="{6793ECA4-A034-42EC-A741-3B0FF42BC11B}"/>
+    <hyperlink r:id="rId139" ref="B108" xr:uid="{4DB78F44-0F08-4561-A0E8-0EE92F9FFECB}"/>
+    <hyperlink r:id="rId140" ref="B114" xr:uid="{27750164-38B8-4B5E-9B5A-E6C71FFFC61F}"/>
+    <hyperlink r:id="rId141" ref="C114" xr:uid="{6FE6A043-A6B1-44FF-8A45-8C3690323458}"/>
+    <hyperlink r:id="rId142" ref="B113" xr:uid="{0F94FF41-1E06-4D7B-B360-1EB377073C87}"/>
+    <hyperlink r:id="rId143" ref="B112" xr:uid="{490A5044-10EC-4082-BEC1-14008171D5CF}"/>
+    <hyperlink r:id="rId144" ref="B49" xr:uid="{836EB236-8BF1-4259-B395-AD9FA9DE0AE0}"/>
+    <hyperlink r:id="rId145" ref="B74" xr:uid="{8AA8904A-1CC5-4D06-93EF-66F7FC625199}"/>
+    <hyperlink r:id="rId146" ref="B76" xr:uid="{5743888C-C74A-41C6-ABC5-E9575351702D}"/>
+    <hyperlink r:id="rId147" ref="B115" xr:uid="{27BDB583-8AD0-4B33-BA19-24E42C9E7CE9}"/>
+    <hyperlink r:id="rId148" ref="B117" xr:uid="{92BA6213-0D94-4C5A-B06A-6FC35C0BECA9}"/>
+    <hyperlink r:id="rId149" ref="B119" xr:uid="{6724AE23-65F5-4D67-ADA6-E20BD420531B}"/>
+    <hyperlink r:id="rId150" ref="C119" xr:uid="{0A5009EB-B388-4AF4-99CE-5813711C2B1E}"/>
+    <hyperlink r:id="rId151" ref="B120" xr:uid="{255CB59B-E711-471E-8ACE-D0ABA408AE96}"/>
+    <hyperlink r:id="rId152" ref="B39" xr:uid="{39FB4A7C-4EA8-4530-9FE6-2842C777350C}"/>
+    <hyperlink r:id="rId153" ref="B104" xr:uid="{FC8A6FB5-FCCF-409E-9D6D-A93D412B2275}"/>
+    <hyperlink r:id="rId154" ref="C105" xr:uid="{988B91BF-CEBD-44F6-A773-3C87D877BE5A}"/>
+    <hyperlink r:id="rId155" ref="C108" xr:uid="{F0593E1B-3EE0-4DF2-B93E-84A02071630B}"/>
+    <hyperlink r:id="rId156" ref="B109" xr:uid="{601C40E0-818B-457C-9FE7-30D06707CEB7}"/>
+    <hyperlink r:id="rId157" ref="C109" xr:uid="{E1D93474-1A3D-49F1-B191-3C3484679D2D}"/>
+    <hyperlink r:id="rId158" ref="C83" xr:uid="{B0D57129-C33F-45FF-B844-E7642495443D}"/>
+    <hyperlink r:id="rId159" ref="B83" xr:uid="{7DCBF3E6-0CD2-475D-AE1F-56469491B512}"/>
+    <hyperlink r:id="rId160" ref="C120" xr:uid="{F24698EA-BA1A-4C92-8B6D-72A40DDDD7A3}"/>
+    <hyperlink r:id="rId161" ref="C122" xr:uid="{BAC9069D-9D63-415D-B933-A4F86CB8C587}"/>
+    <hyperlink r:id="rId162" ref="C123" xr:uid="{140A866C-FAC2-4A61-BA7E-0AFB9A05FD2F}"/>
+    <hyperlink r:id="rId163" ref="C124" xr:uid="{6EA83FA2-D552-4B23-98A9-6C5EFC3BC2CA}"/>
+    <hyperlink r:id="rId164" ref="C125" xr:uid="{E34375AF-4BB2-420C-887F-8D684FC72F4C}"/>
+    <hyperlink r:id="rId165" ref="C126" xr:uid="{CB74A187-1404-4E3B-B1EF-E6C50CF09D3E}"/>
+    <hyperlink r:id="rId166" ref="C127" xr:uid="{B0565FA3-8BDF-4E3B-9814-B9F51432FA7D}"/>
+    <hyperlink r:id="rId167" ref="C128" xr:uid="{8504A7CE-7DD9-4C74-83D8-90E0745EAB21}"/>
+    <hyperlink r:id="rId168" ref="C130" xr:uid="{D3DDF4DA-6F84-4EAF-BA60-77D926C7C2AC}"/>
+    <hyperlink r:id="rId169" ref="C131" xr:uid="{060B4F44-BF89-4037-9E74-C61E23C6AAC9}"/>
+    <hyperlink r:id="rId170" ref="C132" xr:uid="{8FD9E395-82BD-4EEA-89E9-166FDA928F87}"/>
+    <hyperlink r:id="rId171" ref="C133" xr:uid="{3669E93D-A9CE-4C72-B1DD-98E95312A18C}"/>
+    <hyperlink r:id="rId172" ref="C136" xr:uid="{E14EBE84-3FBA-44D8-B082-69967148B456}"/>
+    <hyperlink r:id="rId173" ref="C137" xr:uid="{CC0D1827-F782-476A-9312-1BAA88B7D496}"/>
+    <hyperlink r:id="rId174" ref="C141" xr:uid="{1528B515-167A-4838-B645-B63CD0312C05}"/>
+    <hyperlink r:id="rId175" ref="B143" xr:uid="{50B775B1-8A20-4A55-90CA-EC152D3C2098}"/>
+    <hyperlink r:id="rId176" ref="B144" xr:uid="{F6EFF9E5-8AC0-4C40-A2A8-62DF9BB671E9}"/>
+    <hyperlink r:id="rId177" ref="C145" xr:uid="{DE56B3AC-2F1A-494E-A9CD-9C972DA863E2}"/>
+    <hyperlink r:id="rId178" ref="B145" xr:uid="{F783979B-F441-49BC-98C4-8448098CBBC1}"/>
+    <hyperlink r:id="rId179" ref="C17" xr:uid="{DBE3D417-C525-4AE7-BA26-A27F8BD7B6D3}"/>
+    <hyperlink r:id="rId180" ref="B121" xr:uid="{BF1CBD80-282B-4284-A960-458EE8D86966}"/>
+    <hyperlink r:id="rId181" ref="C146" xr:uid="{3FA9DCB7-198C-457D-99E0-AF0A29EDEAF1}"/>
+    <hyperlink r:id="rId182" ref="B146" xr:uid="{6B057403-173E-478A-AFE1-5BA96D6006F7}"/>
+    <hyperlink r:id="rId183" ref="C147" xr:uid="{FBD8EA4A-7B80-4D87-BD4D-6D3DDE043E14}"/>
+    <hyperlink r:id="rId184" ref="B147" xr:uid="{F9D4FD4A-592C-4041-AD52-AAD4E4FECD78}"/>
+    <hyperlink r:id="rId185" ref="C148" xr:uid="{EF3F39F0-4058-49A5-8980-E800B6F200B5}"/>
+    <hyperlink r:id="rId186" ref="B148" xr:uid="{513D1B27-06CF-4F01-AD66-B1DDDB3DF171}"/>
+    <hyperlink r:id="rId187" ref="C149" xr:uid="{BFCDD610-AD9F-445C-AAE8-66DB3CD722A6}"/>
+    <hyperlink r:id="rId188" ref="B149" xr:uid="{1567BEF7-2918-4A3A-89A1-A37D6C6B5419}"/>
+    <hyperlink r:id="rId189" ref="B150" xr:uid="{233679EA-F519-4185-AA17-F008EE8DA109}"/>
+    <hyperlink r:id="rId190" ref="C153" xr:uid="{D979C888-F3D2-4FAE-9C96-C32136017BEF}"/>
+    <hyperlink r:id="rId191" ref="B153" xr:uid="{F7FA0B04-B8E5-4470-AA22-DE86ABDF6874}"/>
+    <hyperlink r:id="rId192" ref="C93" xr:uid="{0FE1A0D7-D827-4F54-A7B7-45C810922AB8}"/>
+    <hyperlink r:id="rId193" ref="H94" xr:uid="{119834D6-06DC-4C3A-A3DB-668C11E66CDD}"/>
+    <hyperlink r:id="rId194" ref="B157" xr:uid="{476413B0-EB8B-4009-A520-C52327E9DB14}"/>
+    <hyperlink r:id="rId195" ref="B158" xr:uid="{E393AAFE-C1C9-42C1-82B6-E0BF95C57871}"/>
+    <hyperlink r:id="rId196" ref="B154" xr:uid="{6ACA5AA2-08BB-438D-AA2D-656B3CF595C8}"/>
+    <hyperlink r:id="rId197" ref="B155" xr:uid="{09BFA21C-B573-43CD-A621-D848720D45A2}"/>
+    <hyperlink r:id="rId198" ref="B156" xr:uid="{64BD9576-B17E-4000-AF00-7BFD7270B1E0}"/>
   </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId192"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageSetup orientation="portrait" paperSize="9" r:id="rId199"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:AI153"/>
+  <dimension ref="A1:AJ157"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C19" sqref="C19"/>
+    <sheetView workbookViewId="0">
+      <pane activePane="bottomLeft" state="frozen" topLeftCell="A143" ySplit="1"/>
+      <selection activeCell="H169" pane="bottomLeft" sqref="H169"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1"/>
+  <sheetFormatPr customHeight="1" defaultColWidth="14.42578125" defaultRowHeight="15.75"/>
   <cols>
-    <col min="1" max="1" width="14.85546875" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="18.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="55.5703125" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="25.140625" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="19.5703125" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="19.85546875" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="18.5703125" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="32.140625" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="20.5703125" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="21.140625" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="28.85546875" customWidth="1" collapsed="1"/>
-    <col min="12" max="12" width="37.5703125" customWidth="1" collapsed="1"/>
-    <col min="16" max="17" width="18.85546875" customWidth="1" collapsed="1"/>
-    <col min="18" max="18" width="47.85546875" customWidth="1" collapsed="1"/>
-    <col min="19" max="19" width="77.5703125" customWidth="1" collapsed="1"/>
-    <col min="20" max="20" width="24" customWidth="1" collapsed="1"/>
-    <col min="21" max="21" width="18.85546875" customWidth="1" collapsed="1"/>
-    <col min="22" max="31" width="19.140625" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="14.85546875" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="18.140625" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="55.5703125" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="25.140625" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="19.5703125" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" width="19.85546875" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" width="18.5703125" collapsed="true"/>
+    <col min="8" max="8" customWidth="true" width="32.140625" collapsed="true"/>
+    <col min="9" max="9" customWidth="true" width="20.5703125" collapsed="true"/>
+    <col min="10" max="10" customWidth="true" width="21.140625" collapsed="true"/>
+    <col min="11" max="11" customWidth="true" width="28.85546875" collapsed="true"/>
+    <col min="12" max="12" customWidth="true" width="37.5703125" collapsed="true"/>
+    <col min="16" max="17" customWidth="true" width="18.85546875" collapsed="true"/>
+    <col min="18" max="18" customWidth="true" width="47.85546875" collapsed="true"/>
+    <col min="19" max="19" customWidth="true" width="77.5703125" collapsed="true"/>
+    <col min="20" max="20" customWidth="true" width="24.0" collapsed="true"/>
+    <col min="21" max="21" customWidth="true" width="18.85546875" collapsed="true"/>
+    <col min="22" max="31" customWidth="true" width="19.140625" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:35" ht="30">
+    <row ht="30" r="1" spans="1:35">
       <c r="A1" s="1" t="s">
         <v>46</v>
       </c>
@@ -10566,7 +10790,7 @@
       <c r="AH1" s="23"/>
       <c r="AI1" s="23"/>
     </row>
-    <row r="2" spans="1:35" ht="15" customHeight="1">
+    <row customHeight="1" ht="15" r="2" spans="1:35">
       <c r="A2" s="24">
         <v>1</v>
       </c>
@@ -10637,7 +10861,7 @@
       <c r="AH2" s="24"/>
       <c r="AI2" s="24"/>
     </row>
-    <row r="3" spans="1:35" ht="15" customHeight="1">
+    <row customHeight="1" ht="15" r="3" spans="1:35">
       <c r="A3" s="24">
         <v>2</v>
       </c>
@@ -10708,7 +10932,7 @@
       <c r="AH3" s="24"/>
       <c r="AI3" s="24"/>
     </row>
-    <row r="4" spans="1:35" s="24" customFormat="1" ht="15" customHeight="1">
+    <row customFormat="1" customHeight="1" ht="15" r="4" s="24" spans="1:35">
       <c r="A4" s="24">
         <v>3</v>
       </c>
@@ -10770,7 +10994,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="5" spans="1:35" ht="15" customHeight="1">
+    <row customHeight="1" ht="15" r="5" spans="1:35">
       <c r="A5" s="24">
         <v>4</v>
       </c>
@@ -10843,7 +11067,7 @@
       <c r="AH5" s="24"/>
       <c r="AI5" s="24"/>
     </row>
-    <row r="6" spans="1:35" s="24" customFormat="1" ht="15" customHeight="1">
+    <row customFormat="1" customHeight="1" ht="15" r="6" s="24" spans="1:35">
       <c r="A6" s="24">
         <v>5</v>
       </c>
@@ -10902,7 +11126,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="7" spans="1:35" s="24" customFormat="1" ht="15" customHeight="1">
+    <row customFormat="1" customHeight="1" ht="15" r="7" s="24" spans="1:35">
       <c r="A7" s="24">
         <v>6</v>
       </c>
@@ -10961,7 +11185,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="8" spans="1:35" s="24" customFormat="1" ht="15" customHeight="1">
+    <row customFormat="1" customHeight="1" ht="15" r="8" s="24" spans="1:35">
       <c r="A8" s="24">
         <v>7</v>
       </c>
@@ -11017,7 +11241,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="9" spans="1:35" s="24" customFormat="1" ht="15" customHeight="1">
+    <row customFormat="1" customHeight="1" ht="15" r="9" s="24" spans="1:35">
       <c r="A9" s="24">
         <v>8</v>
       </c>
@@ -11076,7 +11300,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="10" spans="1:35" s="24" customFormat="1" ht="15" customHeight="1">
+    <row customFormat="1" customHeight="1" ht="15" r="10" s="24" spans="1:35">
       <c r="A10" s="24">
         <v>9</v>
       </c>
@@ -11132,12 +11356,12 @@
         <v>16</v>
       </c>
     </row>
-    <row r="11" spans="1:35" s="24" customFormat="1" ht="15" customHeight="1">
+    <row customFormat="1" customHeight="1" ht="15" r="11" s="24" spans="1:35">
       <c r="A11" s="24">
         <v>10</v>
       </c>
-      <c r="B11" s="46" t="s">
-        <v>1123</v>
+      <c r="B11" s="24" t="s">
+        <v>7</v>
       </c>
       <c r="C11" s="24" t="s">
         <v>110</v>
@@ -11178,7 +11402,7 @@
       <c r="R11" s="24" t="s">
         <v>113</v>
       </c>
-      <c r="S11" s="47" t="s">
+      <c r="S11" s="24" t="s">
         <v>1093</v>
       </c>
       <c r="T11" s="24" t="s">
@@ -11197,7 +11421,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="12" spans="1:35" s="24" customFormat="1" ht="15" customHeight="1">
+    <row customFormat="1" customHeight="1" ht="15" r="12" s="24" spans="1:35">
       <c r="A12" s="24">
         <v>11</v>
       </c>
@@ -11253,7 +11477,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="13" spans="1:35" s="24" customFormat="1" ht="15" customHeight="1">
+    <row customFormat="1" customHeight="1" ht="15" r="13" s="24" spans="1:35">
       <c r="A13" s="24">
         <v>12</v>
       </c>
@@ -11312,7 +11536,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="14" spans="1:35" s="24" customFormat="1" ht="15" customHeight="1">
+    <row customFormat="1" customHeight="1" ht="15" r="14" s="24" spans="1:35">
       <c r="A14" s="24">
         <v>13</v>
       </c>
@@ -11377,7 +11601,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="15" spans="1:35" s="24" customFormat="1" ht="15" customHeight="1">
+    <row customFormat="1" customHeight="1" ht="15" r="15" s="24" spans="1:35">
       <c r="A15" s="24">
         <v>14</v>
       </c>
@@ -11436,7 +11660,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="16" spans="1:35" s="24" customFormat="1" ht="15" customHeight="1">
+    <row customFormat="1" customHeight="1" ht="15" r="16" s="24" spans="1:35">
       <c r="A16" s="24">
         <v>15</v>
       </c>
@@ -11495,7 +11719,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="17" spans="1:35" s="24" customFormat="1" ht="15" customHeight="1">
+    <row customFormat="1" customHeight="1" ht="15" r="17" s="24" spans="1:35">
       <c r="A17" s="24">
         <v>16</v>
       </c>
@@ -11551,7 +11775,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="18" spans="1:35" s="24" customFormat="1" ht="15" customHeight="1">
+    <row customFormat="1" customHeight="1" ht="15" r="18" s="24" spans="1:35">
       <c r="A18" s="24">
         <v>17</v>
       </c>
@@ -11610,7 +11834,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="19" spans="1:35" s="24" customFormat="1" ht="15" customHeight="1">
+    <row customFormat="1" customHeight="1" ht="15" r="19" s="24" spans="1:35">
       <c r="A19" s="24">
         <v>18</v>
       </c>
@@ -11666,7 +11890,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="20" spans="1:35" ht="15" customHeight="1">
+    <row customHeight="1" ht="15" r="20" spans="1:35">
       <c r="A20" s="24">
         <v>19</v>
       </c>
@@ -11741,7 +11965,7 @@
       <c r="AH20" s="24"/>
       <c r="AI20" s="24"/>
     </row>
-    <row r="21" spans="1:35" s="24" customFormat="1" ht="15" customHeight="1">
+    <row customFormat="1" customHeight="1" ht="15" r="21" s="24" spans="1:35">
       <c r="A21" s="24">
         <v>20</v>
       </c>
@@ -11797,7 +12021,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="22" spans="1:35" s="24" customFormat="1" ht="15" customHeight="1">
+    <row customFormat="1" customHeight="1" ht="15" r="22" s="24" spans="1:35">
       <c r="A22" s="24">
         <v>21</v>
       </c>
@@ -11862,7 +12086,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="23" spans="1:35" s="24" customFormat="1" ht="15" customHeight="1">
+    <row customFormat="1" customHeight="1" ht="15" r="23" s="24" spans="1:35">
       <c r="A23" s="24">
         <v>22</v>
       </c>
@@ -11915,7 +12139,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="24" spans="1:35" s="24" customFormat="1" ht="15" customHeight="1">
+    <row customFormat="1" customHeight="1" ht="15" r="24" s="24" spans="1:35">
       <c r="A24" s="24">
         <v>23</v>
       </c>
@@ -11974,7 +12198,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="25" spans="1:35" ht="15" customHeight="1">
+    <row customHeight="1" ht="15" r="25" spans="1:35">
       <c r="A25" s="24">
         <v>24</v>
       </c>
@@ -12045,7 +12269,7 @@
       <c r="AH25" s="24"/>
       <c r="AI25" s="24"/>
     </row>
-    <row r="26" spans="1:35" s="24" customFormat="1" ht="15" customHeight="1">
+    <row customFormat="1" customHeight="1" ht="15" r="26" s="24" spans="1:35">
       <c r="A26" s="24">
         <v>25</v>
       </c>
@@ -12104,7 +12328,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="27" spans="1:35" s="24" customFormat="1" ht="15" customHeight="1">
+    <row customFormat="1" customHeight="1" ht="15" r="27" s="24" spans="1:35">
       <c r="A27" s="24">
         <v>26</v>
       </c>
@@ -12163,7 +12387,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="28" spans="1:35" s="24" customFormat="1" ht="15" customHeight="1">
+    <row customFormat="1" customHeight="1" ht="15" r="28" s="24" spans="1:35">
       <c r="A28" s="24">
         <v>27</v>
       </c>
@@ -12222,7 +12446,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="29" spans="1:35" s="24" customFormat="1" ht="15" customHeight="1">
+    <row customFormat="1" customHeight="1" ht="15" r="29" s="24" spans="1:35">
       <c r="A29" s="24">
         <v>28</v>
       </c>
@@ -12281,7 +12505,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="30" spans="1:35" s="24" customFormat="1" ht="15" customHeight="1">
+    <row customFormat="1" customHeight="1" ht="15" r="30" s="24" spans="1:35">
       <c r="A30" s="24">
         <v>29</v>
       </c>
@@ -12340,7 +12564,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="31" spans="1:35" s="24" customFormat="1" ht="15" customHeight="1">
+    <row customFormat="1" customHeight="1" ht="15" r="31" s="24" spans="1:35">
       <c r="A31" s="24">
         <v>30</v>
       </c>
@@ -12396,7 +12620,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="32" spans="1:35" s="24" customFormat="1" ht="15" customHeight="1">
+    <row customFormat="1" customHeight="1" ht="15" r="32" s="24" spans="1:35">
       <c r="A32" s="24">
         <v>31</v>
       </c>
@@ -12455,7 +12679,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="33" spans="1:21" s="24" customFormat="1" ht="14.25">
+    <row customFormat="1" ht="14.25" r="33" s="24" spans="1:21">
       <c r="A33" s="24" t="s">
         <v>195</v>
       </c>
@@ -12514,7 +12738,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="34" spans="1:21" s="24" customFormat="1" ht="14.25">
+    <row customFormat="1" ht="14.25" r="34" s="24" spans="1:21">
       <c r="A34" s="24" t="s">
         <v>206</v>
       </c>
@@ -12573,7 +12797,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="35" spans="1:21" s="24" customFormat="1" ht="14.25">
+    <row customFormat="1" ht="14.25" r="35" s="24" spans="1:21">
       <c r="A35" s="24" t="s">
         <v>213</v>
       </c>
@@ -12632,7 +12856,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="36" spans="1:21" s="24" customFormat="1" ht="14.25">
+    <row customFormat="1" ht="14.25" r="36" s="24" spans="1:21">
       <c r="A36" s="24" t="s">
         <v>219</v>
       </c>
@@ -12691,7 +12915,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="37" spans="1:21" s="24" customFormat="1" ht="14.25">
+    <row customFormat="1" ht="14.25" r="37" s="24" spans="1:21">
       <c r="A37" s="24" t="s">
         <v>226</v>
       </c>
@@ -12750,7 +12974,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="38" spans="1:21" s="24" customFormat="1" ht="14.25">
+    <row customFormat="1" ht="14.25" r="38" s="24" spans="1:21">
       <c r="A38" s="24" t="s">
         <v>232</v>
       </c>
@@ -12809,7 +13033,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="39" spans="1:21" s="24" customFormat="1" ht="14.25">
+    <row customFormat="1" ht="14.25" r="39" s="24" spans="1:21">
       <c r="A39" s="24" t="s">
         <v>240</v>
       </c>
@@ -12868,7 +13092,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="40" spans="1:21" s="24" customFormat="1" ht="14.25">
+    <row customFormat="1" ht="14.25" r="40" s="24" spans="1:21">
       <c r="A40" s="24" t="s">
         <v>243</v>
       </c>
@@ -12927,7 +13151,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="41" spans="1:21" s="24" customFormat="1" ht="14.25">
+    <row customFormat="1" ht="14.25" r="41" s="24" spans="1:21">
       <c r="A41" s="24" t="s">
         <v>246</v>
       </c>
@@ -12986,7 +13210,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="42" spans="1:21" s="24" customFormat="1" ht="14.25">
+    <row customFormat="1" ht="14.25" r="42" s="24" spans="1:21">
       <c r="A42" s="24" t="s">
         <v>255</v>
       </c>
@@ -13045,7 +13269,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="43" spans="1:21" s="24" customFormat="1" ht="14.25">
+    <row customFormat="1" ht="14.25" r="43" s="24" spans="1:21">
       <c r="A43" s="24" t="s">
         <v>259</v>
       </c>
@@ -13104,7 +13328,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="44" spans="1:21" s="24" customFormat="1" ht="14.25">
+    <row customFormat="1" ht="14.25" r="44" s="24" spans="1:21">
       <c r="A44" s="24" t="s">
         <v>268</v>
       </c>
@@ -13163,7 +13387,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="45" spans="1:21" s="24" customFormat="1" ht="14.25">
+    <row customFormat="1" ht="14.25" r="45" s="24" spans="1:21">
       <c r="A45" s="24" t="s">
         <v>275</v>
       </c>
@@ -13222,7 +13446,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="46" spans="1:21" s="24" customFormat="1" ht="14.25">
+    <row customFormat="1" ht="14.25" r="46" s="24" spans="1:21">
       <c r="A46" s="24" t="s">
         <v>281</v>
       </c>
@@ -13281,7 +13505,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="47" spans="1:21" s="24" customFormat="1" ht="14.25">
+    <row customFormat="1" ht="14.25" r="47" s="24" spans="1:21">
       <c r="A47" s="24" t="s">
         <v>287</v>
       </c>
@@ -13340,7 +13564,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="48" spans="1:21" s="24" customFormat="1" ht="14.25">
+    <row customFormat="1" ht="14.25" r="48" s="24" spans="1:21">
       <c r="A48" s="24" t="s">
         <v>293</v>
       </c>
@@ -13399,7 +13623,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="49" spans="1:21" s="24" customFormat="1" ht="14.25">
+    <row customFormat="1" ht="14.25" r="49" s="24" spans="1:21">
       <c r="A49" s="24" t="s">
         <v>298</v>
       </c>
@@ -13458,7 +13682,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="50" spans="1:21" s="24" customFormat="1" ht="14.25">
+    <row customFormat="1" ht="14.25" r="50" s="24" spans="1:21">
       <c r="A50" s="24" t="s">
         <v>304</v>
       </c>
@@ -13517,7 +13741,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="51" spans="1:21" s="24" customFormat="1" ht="14.25">
+    <row customFormat="1" ht="14.25" r="51" s="24" spans="1:21">
       <c r="A51" s="24" t="s">
         <v>310</v>
       </c>
@@ -13576,7 +13800,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="52" spans="1:21" s="24" customFormat="1" ht="14.25">
+    <row customFormat="1" ht="14.25" r="52" s="24" spans="1:21">
       <c r="A52" s="24" t="s">
         <v>316</v>
       </c>
@@ -13635,7 +13859,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="53" spans="1:21" s="24" customFormat="1" ht="14.25">
+    <row customFormat="1" ht="14.25" r="53" s="24" spans="1:21">
       <c r="A53" s="24" t="s">
         <v>343</v>
       </c>
@@ -13694,7 +13918,7 @@
         <v>325</v>
       </c>
     </row>
-    <row r="54" spans="1:21" s="24" customFormat="1" ht="14.25">
+    <row customFormat="1" ht="14.25" r="54" s="24" spans="1:21">
       <c r="A54" s="24" t="s">
         <v>349</v>
       </c>
@@ -13753,7 +13977,7 @@
         <v>325</v>
       </c>
     </row>
-    <row r="55" spans="1:21" s="24" customFormat="1" ht="14.25">
+    <row customFormat="1" ht="14.25" r="55" s="24" spans="1:21">
       <c r="A55" s="24" t="s">
         <v>353</v>
       </c>
@@ -13812,7 +14036,7 @@
         <v>325</v>
       </c>
     </row>
-    <row r="56" spans="1:21" s="24" customFormat="1" ht="14.25">
+    <row customFormat="1" ht="14.25" r="56" s="24" spans="1:21">
       <c r="A56" s="24" t="s">
         <v>359</v>
       </c>
@@ -13871,7 +14095,7 @@
         <v>325</v>
       </c>
     </row>
-    <row r="57" spans="1:21" s="24" customFormat="1" ht="14.25">
+    <row customFormat="1" ht="14.25" r="57" s="24" spans="1:21">
       <c r="A57" s="24" t="s">
         <v>364</v>
       </c>
@@ -13930,7 +14154,7 @@
         <v>325</v>
       </c>
     </row>
-    <row r="58" spans="1:21" s="24" customFormat="1" ht="14.25">
+    <row customFormat="1" ht="14.25" r="58" s="24" spans="1:21">
       <c r="A58" s="24" t="s">
         <v>371</v>
       </c>
@@ -13989,7 +14213,7 @@
         <v>325</v>
       </c>
     </row>
-    <row r="59" spans="1:21" s="24" customFormat="1" ht="14.25">
+    <row customFormat="1" ht="14.25" r="59" s="24" spans="1:21">
       <c r="A59" s="24" t="s">
         <v>377</v>
       </c>
@@ -14048,7 +14272,7 @@
         <v>325</v>
       </c>
     </row>
-    <row r="60" spans="1:21" s="24" customFormat="1" ht="14.25">
+    <row customFormat="1" ht="14.25" r="60" s="24" spans="1:21">
       <c r="A60" s="24" t="s">
         <v>384</v>
       </c>
@@ -14107,7 +14331,7 @@
         <v>325</v>
       </c>
     </row>
-    <row r="61" spans="1:21" s="24" customFormat="1" ht="14.25">
+    <row customFormat="1" ht="14.25" r="61" s="24" spans="1:21">
       <c r="A61" s="24" t="s">
         <v>391</v>
       </c>
@@ -14166,7 +14390,7 @@
         <v>325</v>
       </c>
     </row>
-    <row r="62" spans="1:21" s="24" customFormat="1" ht="14.25">
+    <row customFormat="1" ht="14.25" r="62" s="24" spans="1:21">
       <c r="A62" s="24" t="s">
         <v>397</v>
       </c>
@@ -14225,7 +14449,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="63" spans="1:21" s="24" customFormat="1" ht="14.25">
+    <row customFormat="1" ht="14.25" r="63" s="24" spans="1:21">
       <c r="A63" s="24" t="s">
         <v>400</v>
       </c>
@@ -14284,7 +14508,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="64" spans="1:21" s="24" customFormat="1" ht="14.25">
+    <row customFormat="1" ht="14.25" r="64" s="24" spans="1:21">
       <c r="A64" s="24" t="s">
         <v>405</v>
       </c>
@@ -14343,7 +14567,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="65" spans="1:21" s="24" customFormat="1" ht="14.25">
+    <row customFormat="1" ht="14.25" r="65" s="24" spans="1:21">
       <c r="A65" s="24" t="s">
         <v>411</v>
       </c>
@@ -14402,7 +14626,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="66" spans="1:21" s="24" customFormat="1" ht="14.25">
+    <row customFormat="1" ht="14.25" r="66" s="24" spans="1:21">
       <c r="A66" s="24" t="s">
         <v>416</v>
       </c>
@@ -14461,7 +14685,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="67" spans="1:21" s="24" customFormat="1" ht="14.25">
+    <row customFormat="1" ht="14.25" r="67" s="24" spans="1:21">
       <c r="A67" s="24" t="s">
         <v>422</v>
       </c>
@@ -14520,7 +14744,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="68" spans="1:21" s="24" customFormat="1" ht="14.25">
+    <row customFormat="1" ht="14.25" r="68" s="24" spans="1:21">
       <c r="A68" s="24" t="s">
         <v>483</v>
       </c>
@@ -14579,7 +14803,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="69" spans="1:21" s="24" customFormat="1" ht="14.25">
+    <row customFormat="1" ht="14.25" r="69" s="24" spans="1:21">
       <c r="A69" s="24" t="s">
         <v>488</v>
       </c>
@@ -14638,7 +14862,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="70" spans="1:21" s="24" customFormat="1" ht="14.25">
+    <row customFormat="1" ht="14.25" r="70" s="24" spans="1:21">
       <c r="A70" s="24" t="s">
         <v>490</v>
       </c>
@@ -14697,7 +14921,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="71" spans="1:21" s="24" customFormat="1" ht="14.25">
+    <row customFormat="1" ht="14.25" r="71" s="24" spans="1:21">
       <c r="A71" s="24" t="s">
         <v>496</v>
       </c>
@@ -14756,7 +14980,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="72" spans="1:21" s="24" customFormat="1" ht="14.25">
+    <row customFormat="1" ht="14.25" r="72" s="24" spans="1:21">
       <c r="A72" s="24" t="s">
         <v>501</v>
       </c>
@@ -14815,7 +15039,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="73" spans="1:21" s="24" customFormat="1" ht="14.25">
+    <row customFormat="1" ht="14.25" r="73" s="24" spans="1:21">
       <c r="A73" s="24" t="s">
         <v>503</v>
       </c>
@@ -14874,7 +15098,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="74" spans="1:21" s="24" customFormat="1" ht="14.25">
+    <row customFormat="1" ht="14.25" r="74" s="24" spans="1:21">
       <c r="A74" s="24" t="s">
         <v>507</v>
       </c>
@@ -14933,7 +15157,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="75" spans="1:21" s="24" customFormat="1" ht="14.25">
+    <row customFormat="1" ht="14.25" r="75" s="24" spans="1:21">
       <c r="A75" s="24" t="s">
         <v>513</v>
       </c>
@@ -14992,7 +15216,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="76" spans="1:21" s="24" customFormat="1" ht="14.25">
+    <row customFormat="1" ht="14.25" r="76" s="24" spans="1:21">
       <c r="A76" s="24" t="s">
         <v>519</v>
       </c>
@@ -15051,7 +15275,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="77" spans="1:21" s="24" customFormat="1" ht="14.25">
+    <row customFormat="1" ht="14.25" r="77" s="24" spans="1:21">
       <c r="A77" s="24" t="s">
         <v>524</v>
       </c>
@@ -15110,7 +15334,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="78" spans="1:21" s="24" customFormat="1" ht="14.25">
+    <row customFormat="1" ht="14.25" r="78" s="24" spans="1:21">
       <c r="A78" s="24" t="s">
         <v>531</v>
       </c>
@@ -15169,7 +15393,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="79" spans="1:21" s="24" customFormat="1" ht="14.25">
+    <row customFormat="1" ht="14.25" r="79" s="24" spans="1:21">
       <c r="A79" s="24" t="s">
         <v>534</v>
       </c>
@@ -15228,7 +15452,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="80" spans="1:21" s="24" customFormat="1" ht="14.25">
+    <row customFormat="1" ht="14.25" r="80" s="24" spans="1:21">
       <c r="A80" s="24" t="s">
         <v>540</v>
       </c>
@@ -15287,7 +15511,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="81" spans="1:21" s="24" customFormat="1" ht="14.25">
+    <row customFormat="1" ht="14.25" r="81" s="24" spans="1:21">
       <c r="A81" s="24" t="s">
         <v>547</v>
       </c>
@@ -15346,7 +15570,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="82" spans="1:21" s="24" customFormat="1" ht="14.25">
+    <row customFormat="1" ht="14.25" r="82" s="24" spans="1:21">
       <c r="A82" s="24" t="s">
         <v>552</v>
       </c>
@@ -15405,7 +15629,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="83" spans="1:21" s="24" customFormat="1" ht="14.25">
+    <row customFormat="1" ht="14.25" r="83" s="24" spans="1:21">
       <c r="A83" s="24" t="s">
         <v>557</v>
       </c>
@@ -15464,7 +15688,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="84" spans="1:21" s="24" customFormat="1" ht="14.25">
+    <row customFormat="1" ht="14.25" r="84" s="24" spans="1:21">
       <c r="A84" s="24" t="s">
         <v>560</v>
       </c>
@@ -15523,7 +15747,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="85" spans="1:21" s="24" customFormat="1" ht="14.25">
+    <row customFormat="1" ht="14.25" r="85" s="24" spans="1:21">
       <c r="A85" s="24" t="s">
         <v>564</v>
       </c>
@@ -15582,7 +15806,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="86" spans="1:21" s="24" customFormat="1" ht="14.25">
+    <row customFormat="1" ht="14.25" r="86" s="24" spans="1:21">
       <c r="A86" s="24" t="s">
         <v>605</v>
       </c>
@@ -15641,7 +15865,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="87" spans="1:21" s="24" customFormat="1" ht="14.25">
+    <row customFormat="1" ht="14.25" r="87" s="24" spans="1:21">
       <c r="A87" s="24" t="s">
         <v>609</v>
       </c>
@@ -15700,7 +15924,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="88" spans="1:21" s="24" customFormat="1" ht="14.25">
+    <row customFormat="1" ht="14.25" r="88" s="24" spans="1:21">
       <c r="A88" s="24" t="s">
         <v>614</v>
       </c>
@@ -15759,7 +15983,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="89" spans="1:21" s="24" customFormat="1" ht="14.25">
+    <row customFormat="1" ht="14.25" r="89" s="24" spans="1:21">
       <c r="A89" s="24" t="s">
         <v>618</v>
       </c>
@@ -15818,7 +16042,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="90" spans="1:21" s="24" customFormat="1" ht="14.25">
+    <row customFormat="1" ht="14.25" r="90" s="24" spans="1:21">
       <c r="A90" s="24" t="s">
         <v>624</v>
       </c>
@@ -15877,7 +16101,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="91" spans="1:21" s="24" customFormat="1" ht="14.25">
+    <row customFormat="1" ht="14.25" r="91" s="24" spans="1:21">
       <c r="A91" s="24" t="s">
         <v>628</v>
       </c>
@@ -15936,7 +16160,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="92" spans="1:21" s="24" customFormat="1" ht="14.25">
+    <row customFormat="1" ht="14.25" r="92" s="24" spans="1:21">
       <c r="A92" s="24" t="s">
         <v>632</v>
       </c>
@@ -15995,7 +16219,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="93" spans="1:21" s="24" customFormat="1" ht="14.25">
+    <row customFormat="1" ht="14.25" r="93" s="24" spans="1:21">
       <c r="A93" s="24" t="s">
         <v>635</v>
       </c>
@@ -16054,7 +16278,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="94" spans="1:21" s="24" customFormat="1" ht="14.25">
+    <row customFormat="1" ht="14.25" r="94" s="24" spans="1:21">
       <c r="A94" s="24" t="s">
         <v>664</v>
       </c>
@@ -16113,7 +16337,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="95" spans="1:21" s="24" customFormat="1" ht="14.25">
+    <row customFormat="1" ht="14.25" r="95" s="24" spans="1:21">
       <c r="A95" s="24" t="s">
         <v>669</v>
       </c>
@@ -16172,7 +16396,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="96" spans="1:21" s="24" customFormat="1" ht="14.25">
+    <row customFormat="1" ht="14.25" r="96" s="24" spans="1:21">
       <c r="A96" s="24" t="s">
         <v>673</v>
       </c>
@@ -16231,7 +16455,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="97" spans="1:21" s="24" customFormat="1" ht="14.25">
+    <row customFormat="1" ht="14.25" r="97" s="24" spans="1:21">
       <c r="A97" s="24" t="s">
         <v>675</v>
       </c>
@@ -16290,7 +16514,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="98" spans="1:21" s="24" customFormat="1" ht="14.25">
+    <row customFormat="1" ht="14.25" r="98" s="24" spans="1:21">
       <c r="A98" s="24" t="s">
         <v>689</v>
       </c>
@@ -16349,7 +16573,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="99" spans="1:21" s="24" customFormat="1" ht="14.25">
+    <row customFormat="1" ht="14.25" r="99" s="24" spans="1:21">
       <c r="A99" s="24" t="s">
         <v>706</v>
       </c>
@@ -16408,7 +16632,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="100" spans="1:21" s="24" customFormat="1" ht="14.25">
+    <row customFormat="1" ht="14.25" r="100" s="24" spans="1:21">
       <c r="A100" s="24" t="s">
         <v>710</v>
       </c>
@@ -16467,7 +16691,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="101" spans="1:21" s="24" customFormat="1" ht="14.25">
+    <row customFormat="1" ht="14.25" r="101" s="24" spans="1:21">
       <c r="A101" s="24" t="s">
         <v>714</v>
       </c>
@@ -16526,7 +16750,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="102" spans="1:21" s="24" customFormat="1" ht="14.25">
+    <row customFormat="1" ht="14.25" r="102" s="24" spans="1:21">
       <c r="A102" s="24" t="s">
         <v>744</v>
       </c>
@@ -16585,7 +16809,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="103" spans="1:21" s="24" customFormat="1" ht="14.25">
+    <row customFormat="1" ht="14.25" r="103" s="24" spans="1:21">
       <c r="A103" s="24" t="s">
         <v>750</v>
       </c>
@@ -16644,7 +16868,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="104" spans="1:21" s="24" customFormat="1" ht="14.25">
+    <row customFormat="1" ht="14.25" r="104" s="24" spans="1:21">
       <c r="A104" s="24" t="s">
         <v>759</v>
       </c>
@@ -16703,7 +16927,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="105" spans="1:21" s="24" customFormat="1" ht="14.25">
+    <row customFormat="1" ht="14.25" r="105" s="24" spans="1:21">
       <c r="A105" s="24" t="s">
         <v>769</v>
       </c>
@@ -16762,7 +16986,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="106" spans="1:21" s="24" customFormat="1" ht="14.25">
+    <row customFormat="1" ht="14.25" r="106" s="24" spans="1:21">
       <c r="A106" s="24" t="s">
         <v>775</v>
       </c>
@@ -16821,7 +17045,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="107" spans="1:21" s="24" customFormat="1" ht="14.25">
+    <row customFormat="1" ht="14.25" r="107" s="24" spans="1:21">
       <c r="A107" s="24" t="s">
         <v>785</v>
       </c>
@@ -16880,7 +17104,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="108" spans="1:21" s="24" customFormat="1" ht="14.25">
+    <row customFormat="1" ht="14.25" r="108" s="24" spans="1:21">
       <c r="A108" s="24" t="s">
         <v>790</v>
       </c>
@@ -16939,7 +17163,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="109" spans="1:21" s="24" customFormat="1" ht="14.25">
+    <row customFormat="1" ht="14.25" r="109" s="24" spans="1:21">
       <c r="A109" s="24" t="s">
         <v>799</v>
       </c>
@@ -16998,7 +17222,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="110" spans="1:21" s="24" customFormat="1" ht="14.25">
+    <row customFormat="1" ht="14.25" r="110" s="24" spans="1:21">
       <c r="A110" s="24" t="s">
         <v>807</v>
       </c>
@@ -17057,7 +17281,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="111" spans="1:21" s="24" customFormat="1" ht="14.25">
+    <row customFormat="1" ht="14.25" r="111" s="24" spans="1:21">
       <c r="A111" s="24" t="s">
         <v>812</v>
       </c>
@@ -17116,7 +17340,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="112" spans="1:21" s="24" customFormat="1" ht="14.25">
+    <row customFormat="1" ht="14.25" r="112" s="24" spans="1:21">
       <c r="A112" s="24" t="s">
         <v>817</v>
       </c>
@@ -17175,7 +17399,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="113" spans="1:21" s="24" customFormat="1" ht="14.25">
+    <row customFormat="1" ht="14.25" r="113" s="24" spans="1:21">
       <c r="A113" s="24" t="s">
         <v>822</v>
       </c>
@@ -17234,7 +17458,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="114" spans="1:21" s="24" customFormat="1" ht="14.25">
+    <row customFormat="1" ht="14.25" r="114" s="24" spans="1:21">
       <c r="A114" s="24" t="s">
         <v>833</v>
       </c>
@@ -17293,7 +17517,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="115" spans="1:21" s="24" customFormat="1" ht="14.25">
+    <row customFormat="1" ht="14.25" r="115" s="24" spans="1:21">
       <c r="A115" s="24" t="s">
         <v>842</v>
       </c>
@@ -17352,7 +17576,7 @@
         <v>325</v>
       </c>
     </row>
-    <row r="116" spans="1:21" s="24" customFormat="1" ht="14.25">
+    <row customFormat="1" ht="14.25" r="116" s="24" spans="1:21">
       <c r="A116" s="24" t="s">
         <v>850</v>
       </c>
@@ -17411,7 +17635,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="117" spans="1:21" s="24" customFormat="1" ht="14.25">
+    <row customFormat="1" ht="14.25" r="117" s="24" spans="1:21">
       <c r="A117" s="24" t="s">
         <v>857</v>
       </c>
@@ -17470,7 +17694,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="118" spans="1:21" s="24" customFormat="1" ht="14.25">
+    <row customFormat="1" ht="14.25" r="118" s="24" spans="1:21">
       <c r="A118" s="24" t="s">
         <v>866</v>
       </c>
@@ -17529,7 +17753,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="119" spans="1:21" s="24" customFormat="1" ht="14.25">
+    <row customFormat="1" ht="14.25" r="119" s="24" spans="1:21">
       <c r="A119" s="24" t="s">
         <v>870</v>
       </c>
@@ -17588,7 +17812,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="120" spans="1:21" s="24" customFormat="1" ht="14.25">
+    <row customFormat="1" ht="14.25" r="120" s="24" spans="1:21">
       <c r="A120" s="24">
         <v>119</v>
       </c>
@@ -17647,7 +17871,7 @@
         <v>1044</v>
       </c>
     </row>
-    <row r="121" spans="1:21" s="24" customFormat="1" ht="14.25">
+    <row customFormat="1" ht="14.25" r="121" s="24" spans="1:21">
       <c r="A121" s="24" t="s">
         <v>910</v>
       </c>
@@ -17706,7 +17930,7 @@
         <v>1044</v>
       </c>
     </row>
-    <row r="122" spans="1:21" s="24" customFormat="1" ht="14.25">
+    <row customFormat="1" ht="14.25" r="122" s="24" spans="1:21">
       <c r="A122" s="24" t="s">
         <v>915</v>
       </c>
@@ -17765,7 +17989,7 @@
         <v>1044</v>
       </c>
     </row>
-    <row r="123" spans="1:21" s="24" customFormat="1" ht="14.25">
+    <row customFormat="1" ht="14.25" r="123" s="24" spans="1:21">
       <c r="A123" s="24" t="s">
         <v>922</v>
       </c>
@@ -17824,7 +18048,7 @@
         <v>1044</v>
       </c>
     </row>
-    <row r="124" spans="1:21" s="24" customFormat="1" ht="14.25">
+    <row customFormat="1" ht="14.25" r="124" s="24" spans="1:21">
       <c r="A124" s="24" t="s">
         <v>927</v>
       </c>
@@ -17883,7 +18107,7 @@
         <v>1044</v>
       </c>
     </row>
-    <row r="125" spans="1:21" s="24" customFormat="1" ht="14.25">
+    <row customFormat="1" ht="14.25" r="125" s="24" spans="1:21">
       <c r="A125" s="24" t="s">
         <v>930</v>
       </c>
@@ -17942,7 +18166,7 @@
         <v>1044</v>
       </c>
     </row>
-    <row r="126" spans="1:21" s="24" customFormat="1" ht="14.25">
+    <row customFormat="1" ht="14.25" r="126" s="24" spans="1:21">
       <c r="A126" s="24" t="s">
         <v>934</v>
       </c>
@@ -18001,7 +18225,7 @@
         <v>1044</v>
       </c>
     </row>
-    <row r="127" spans="1:21" s="24" customFormat="1" ht="14.25">
+    <row customFormat="1" ht="14.25" r="127" s="24" spans="1:21">
       <c r="A127" s="24" t="s">
         <v>940</v>
       </c>
@@ -18060,7 +18284,7 @@
         <v>1044</v>
       </c>
     </row>
-    <row r="128" spans="1:21" s="24" customFormat="1" ht="14.25">
+    <row customFormat="1" ht="14.25" r="128" s="24" spans="1:21">
       <c r="A128" s="24" t="s">
         <v>946</v>
       </c>
@@ -18119,7 +18343,7 @@
         <v>1044</v>
       </c>
     </row>
-    <row r="129" spans="1:21" s="24" customFormat="1" ht="14.25">
+    <row customFormat="1" ht="14.25" r="129" s="24" spans="1:21">
       <c r="A129" s="24" t="s">
         <v>951</v>
       </c>
@@ -18178,7 +18402,7 @@
         <v>1044</v>
       </c>
     </row>
-    <row r="130" spans="1:21" s="24" customFormat="1" ht="14.25">
+    <row customFormat="1" ht="14.25" r="130" s="24" spans="1:21">
       <c r="A130" s="24" t="s">
         <v>956</v>
       </c>
@@ -18237,7 +18461,7 @@
         <v>1044</v>
       </c>
     </row>
-    <row r="131" spans="1:21" s="24" customFormat="1" ht="14.25">
+    <row customFormat="1" ht="14.25" r="131" s="24" spans="1:21">
       <c r="A131" s="24" t="s">
         <v>960</v>
       </c>
@@ -18296,7 +18520,7 @@
         <v>1044</v>
       </c>
     </row>
-    <row r="132" spans="1:21" s="24" customFormat="1" ht="14.25">
+    <row customFormat="1" ht="14.25" r="132" s="24" spans="1:21">
       <c r="A132" s="24" t="s">
         <v>963</v>
       </c>
@@ -18355,7 +18579,7 @@
         <v>1044</v>
       </c>
     </row>
-    <row r="133" spans="1:21" s="24" customFormat="1" ht="14.25">
+    <row customFormat="1" ht="14.25" r="133" s="24" spans="1:21">
       <c r="A133" s="24" t="s">
         <v>967</v>
       </c>
@@ -18414,7 +18638,7 @@
         <v>1044</v>
       </c>
     </row>
-    <row r="134" spans="1:21" s="24" customFormat="1" ht="14.25">
+    <row customFormat="1" ht="14.25" r="134" s="24" spans="1:21">
       <c r="A134" s="24" t="s">
         <v>972</v>
       </c>
@@ -18473,7 +18697,7 @@
         <v>1044</v>
       </c>
     </row>
-    <row r="135" spans="1:21" s="24" customFormat="1" ht="14.25">
+    <row customFormat="1" ht="14.25" r="135" s="24" spans="1:21">
       <c r="A135" s="24" t="s">
         <v>975</v>
       </c>
@@ -18532,7 +18756,7 @@
         <v>1044</v>
       </c>
     </row>
-    <row r="136" spans="1:21" s="24" customFormat="1" ht="14.25">
+    <row customFormat="1" ht="14.25" r="136" s="24" spans="1:21">
       <c r="A136" s="24" t="s">
         <v>980</v>
       </c>
@@ -18591,7 +18815,7 @@
         <v>1044</v>
       </c>
     </row>
-    <row r="137" spans="1:21" s="24" customFormat="1" ht="14.25">
+    <row customFormat="1" ht="14.25" r="137" s="24" spans="1:21">
       <c r="A137" s="24" t="s">
         <v>986</v>
       </c>
@@ -18650,7 +18874,7 @@
         <v>1044</v>
       </c>
     </row>
-    <row r="138" spans="1:21" s="24" customFormat="1" ht="14.25">
+    <row customFormat="1" ht="14.25" r="138" s="24" spans="1:21">
       <c r="A138" s="24" t="s">
         <v>992</v>
       </c>
@@ -18709,7 +18933,7 @@
         <v>1044</v>
       </c>
     </row>
-    <row r="139" spans="1:21" s="24" customFormat="1" ht="14.25">
+    <row customFormat="1" ht="14.25" r="139" s="24" spans="1:21">
       <c r="A139" s="24" t="s">
         <v>997</v>
       </c>
@@ -18768,7 +18992,7 @@
         <v>1044</v>
       </c>
     </row>
-    <row r="140" spans="1:21" s="24" customFormat="1" ht="14.25">
+    <row customFormat="1" ht="14.25" r="140" s="24" spans="1:21">
       <c r="A140" s="24" t="s">
         <v>1001</v>
       </c>
@@ -18827,7 +19051,7 @@
         <v>1044</v>
       </c>
     </row>
-    <row r="141" spans="1:21" s="24" customFormat="1" ht="14.25">
+    <row customFormat="1" ht="14.25" r="141" s="24" spans="1:21">
       <c r="A141" s="24" t="s">
         <v>1007</v>
       </c>
@@ -18886,7 +19110,7 @@
         <v>1044</v>
       </c>
     </row>
-    <row r="142" spans="1:21" s="24" customFormat="1" ht="14.25">
+    <row customFormat="1" ht="14.25" r="142" s="24" spans="1:21">
       <c r="A142" s="24" t="s">
         <v>1012</v>
       </c>
@@ -18945,7 +19169,7 @@
         <v>1044</v>
       </c>
     </row>
-    <row r="143" spans="1:21" s="24" customFormat="1" ht="14.25">
+    <row customFormat="1" ht="14.25" r="143" s="24" spans="1:21">
       <c r="A143" s="24" t="s">
         <v>1017</v>
       </c>
@@ -19004,7 +19228,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="144" spans="1:21" s="24" customFormat="1" ht="14.25">
+    <row customFormat="1" ht="14.25" r="144" s="24" spans="1:21">
       <c r="A144" s="24" t="s">
         <v>1051</v>
       </c>
@@ -19063,7 +19287,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="145" spans="1:21" s="24" customFormat="1" ht="14.25">
+    <row customFormat="1" ht="14.25" r="145" s="24" spans="1:21">
       <c r="A145" s="24" t="s">
         <v>1056</v>
       </c>
@@ -19122,7 +19346,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="146" spans="1:21" s="24" customFormat="1" ht="14.25">
+    <row customFormat="1" ht="14.25" r="146" s="24" spans="1:21">
       <c r="A146" s="24" t="s">
         <v>1073</v>
       </c>
@@ -19181,7 +19405,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="147" spans="1:21" s="24" customFormat="1" ht="14.25">
+    <row customFormat="1" ht="14.25" r="147" s="24" spans="1:21">
       <c r="A147" s="24" t="s">
         <v>1078</v>
       </c>
@@ -19240,7 +19464,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="148" spans="1:21" s="24" customFormat="1" ht="14.25">
+    <row customFormat="1" ht="14.25" r="148" s="24" spans="1:21">
       <c r="A148" s="24" t="s">
         <v>1082</v>
       </c>
@@ -19299,7 +19523,7 @@
         <v>1044</v>
       </c>
     </row>
-    <row r="149" spans="1:21" s="24" customFormat="1" ht="14.25">
+    <row customFormat="1" ht="14.25" r="149" s="24" spans="1:21">
       <c r="A149" s="24" t="s">
         <v>1096</v>
       </c>
@@ -19358,7 +19582,7 @@
         <v>1044</v>
       </c>
     </row>
-    <row r="150" spans="1:21" s="24" customFormat="1" ht="14.25">
+    <row customFormat="1" ht="14.25" r="150" s="24" spans="1:21">
       <c r="A150" s="24" t="s">
         <v>1101</v>
       </c>
@@ -19417,7 +19641,7 @@
         <v>1044</v>
       </c>
     </row>
-    <row r="151" spans="1:21" s="24" customFormat="1" ht="14.25">
+    <row customFormat="1" ht="14.25" r="151" s="24" spans="1:21">
       <c r="A151" s="24" t="s">
         <v>1108</v>
       </c>
@@ -19476,7 +19700,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="152" spans="1:21" s="24" customFormat="1" ht="14.25">
+    <row customFormat="1" ht="14.25" r="152" s="24" spans="1:21">
       <c r="A152" s="24" t="s">
         <v>1113</v>
       </c>
@@ -19535,15 +19759,15 @@
         <v>1044</v>
       </c>
     </row>
-    <row r="153" spans="1:21" s="24" customFormat="1" ht="14.25">
+    <row customFormat="1" ht="14.25" r="153" s="24" spans="1:21">
       <c r="A153" s="24" t="s">
-        <v>1124</v>
+        <v>1123</v>
       </c>
       <c r="B153" s="24" t="s">
         <v>7</v>
       </c>
       <c r="C153" s="24" t="s">
-        <v>1125</v>
+        <v>1124</v>
       </c>
       <c r="D153" s="24" t="s">
         <v>77</v>
@@ -19555,7 +19779,7 @@
         <v>906</v>
       </c>
       <c r="G153" s="24" t="s">
-        <v>1126</v>
+        <v>1125</v>
       </c>
       <c r="H153" s="24" t="s">
         <v>199</v>
@@ -19582,28 +19806,264 @@
         <v>204</v>
       </c>
       <c r="R153" s="24" t="s">
-        <v>1125</v>
+        <v>1124</v>
       </c>
       <c r="S153" s="24" t="s">
-        <v>1127</v>
+        <v>1126</v>
       </c>
       <c r="T153" s="24" t="s">
         <v>687</v>
       </c>
       <c r="U153" s="24" t="s">
         <v>1044</v>
+      </c>
+    </row>
+    <row ht="12.75" r="154" spans="1:21">
+      <c r="A154" t="s">
+        <v>1132</v>
+      </c>
+      <c r="B154" t="s">
+        <v>1145</v>
+      </c>
+      <c r="C154" t="s">
+        <v>1133</v>
+      </c>
+      <c r="D154" t="s">
+        <v>261</v>
+      </c>
+      <c r="E154" t="s">
+        <v>78</v>
+      </c>
+      <c r="F154" t="s">
+        <v>79</v>
+      </c>
+      <c r="G154" t="s">
+        <v>116</v>
+      </c>
+      <c r="H154" t="s">
+        <v>1134</v>
+      </c>
+      <c r="I154" t="s">
+        <v>198</v>
+      </c>
+      <c r="K154" t="s">
+        <v>199</v>
+      </c>
+      <c r="L154" t="s">
+        <v>237</v>
+      </c>
+      <c r="M154" t="s">
+        <v>202</v>
+      </c>
+      <c r="N154" t="s">
+        <v>204</v>
+      </c>
+      <c r="P154">
+        <v>5.5</v>
+      </c>
+      <c r="Q154" t="s">
+        <v>204</v>
+      </c>
+      <c r="R154" t="s">
+        <v>1133</v>
+      </c>
+      <c r="S154" t="s">
+        <v>1135</v>
+      </c>
+      <c r="T154" t="s">
+        <v>1046</v>
+      </c>
+      <c r="U154" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row ht="14.25" r="155" spans="1:21">
+      <c r="A155" t="s">
+        <v>1136</v>
+      </c>
+      <c r="B155" s="43" t="s">
+        <v>172</v>
+      </c>
+      <c r="C155" t="s">
+        <v>1137</v>
+      </c>
+      <c r="D155" t="s">
+        <v>77</v>
+      </c>
+      <c r="E155" s="43" t="s">
+        <v>172</v>
+      </c>
+      <c r="F155" t="s">
+        <v>270</v>
+      </c>
+      <c r="G155" t="s">
+        <v>149</v>
+      </c>
+      <c r="H155" t="s">
+        <v>199</v>
+      </c>
+      <c r="I155" t="s">
+        <v>198</v>
+      </c>
+      <c r="K155" t="s">
+        <v>361</v>
+      </c>
+      <c r="L155" t="s">
+        <v>1138</v>
+      </c>
+      <c r="M155" t="s">
+        <v>266</v>
+      </c>
+      <c r="N155" t="s">
+        <v>266</v>
+      </c>
+      <c r="P155" t="s">
+        <v>199</v>
+      </c>
+      <c r="Q155" t="s">
+        <v>199</v>
+      </c>
+      <c r="R155" t="s">
+        <v>1137</v>
+      </c>
+      <c r="S155" t="s">
+        <v>662</v>
+      </c>
+      <c r="T155" t="s">
+        <v>1046</v>
+      </c>
+      <c r="U155" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row ht="12.75" r="156" spans="1:21">
+      <c r="A156" t="s">
+        <v>1139</v>
+      </c>
+      <c r="B156" t="s">
+        <v>1145</v>
+      </c>
+      <c r="C156" t="s">
+        <v>1140</v>
+      </c>
+      <c r="D156" t="s">
+        <v>261</v>
+      </c>
+      <c r="E156" t="s">
+        <v>78</v>
+      </c>
+      <c r="F156" t="s">
+        <v>235</v>
+      </c>
+      <c r="G156" t="s">
+        <v>1009</v>
+      </c>
+      <c r="H156" t="s">
+        <v>199</v>
+      </c>
+      <c r="I156" t="s">
+        <v>198</v>
+      </c>
+      <c r="K156" t="s">
+        <v>1141</v>
+      </c>
+      <c r="L156" t="s">
+        <v>1142</v>
+      </c>
+      <c r="M156" t="s">
+        <v>202</v>
+      </c>
+      <c r="N156" t="s">
+        <v>204</v>
+      </c>
+      <c r="P156" t="s">
+        <v>203</v>
+      </c>
+      <c r="Q156" t="s">
+        <v>199</v>
+      </c>
+      <c r="R156" t="s">
+        <v>1140</v>
+      </c>
+      <c r="S156" t="s">
+        <v>1143</v>
+      </c>
+      <c r="T156" t="s">
+        <v>687</v>
+      </c>
+      <c r="U156" t="s">
+        <v>1044</v>
+      </c>
+    </row>
+    <row ht="12.75" r="157" spans="1:21">
+      <c r="A157" t="s">
+        <v>1144</v>
+      </c>
+      <c r="B157" t="s">
+        <v>1145</v>
+      </c>
+      <c r="C157" t="s">
+        <v>98</v>
+      </c>
+      <c r="D157" t="s">
+        <v>84</v>
+      </c>
+      <c r="E157" t="s">
+        <v>173</v>
+      </c>
+      <c r="F157" t="s">
+        <v>207</v>
+      </c>
+      <c r="G157" t="s">
+        <v>100</v>
+      </c>
+      <c r="H157" t="s">
+        <v>592</v>
+      </c>
+      <c r="I157" t="s">
+        <v>198</v>
+      </c>
+      <c r="K157" t="s">
+        <v>426</v>
+      </c>
+      <c r="L157" t="s">
+        <v>125</v>
+      </c>
+      <c r="M157" t="s">
+        <v>201</v>
+      </c>
+      <c r="N157" t="s">
+        <v>204</v>
+      </c>
+      <c r="P157" t="s">
+        <v>203</v>
+      </c>
+      <c r="Q157" t="s">
+        <v>204</v>
+      </c>
+      <c r="R157" t="s">
+        <v>211</v>
+      </c>
+      <c r="S157" t="s">
+        <v>591</v>
+      </c>
+      <c r="T157" t="s">
+        <v>687</v>
+      </c>
+      <c r="U157" t="s">
+        <v>16</v>
       </c>
     </row>
   </sheetData>
   <autoFilter ref="E1:E145" xr:uid="{00000000-0001-0000-0100-000000000000}"/>
   <customSheetViews>
-    <customSheetView guid="{C25CEB9E-BEC1-4982-90C4-50C84EE1B82A}" filter="1" showAutoFilter="1">
-      <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-      <autoFilter ref="A1:AD33" xr:uid="{90701E33-9B9E-47AF-9FB1-DF354111A6C2}"/>
+    <customSheetView filter="1" guid="{C25CEB9E-BEC1-4982-90C4-50C84EE1B82A}" showAutoFilter="1">
+      <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+      <autoFilter ref="A1:AD33" xr:uid="{9BC960B4-F463-4F2F-8485-BEC59714BC46}"/>
     </customSheetView>
-    <customSheetView guid="{A7754112-A52F-4ABC-8778-92F04773E53C}" filter="1" showAutoFilter="1">
-      <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-      <autoFilter ref="A1:AD33" xr:uid="{1C0CC383-E312-4807-81FF-2D69453F21A9}">
+    <customSheetView filter="1" guid="{A7754112-A52F-4ABC-8778-92F04773E53C}" showAutoFilter="1">
+      <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+      <autoFilter ref="A1:AD33" xr:uid="{FB0B4DA2-62AD-478B-B2D5-CB2BBE1D4ED3}">
         <filterColumn colId="5">
           <filters blank="1">
             <filter val="Strathnairn"/>
@@ -19613,76 +20073,76 @@
     </customSheetView>
   </customSheetViews>
   <conditionalFormatting sqref="A1:AI1">
-    <cfRule type="notContainsBlanks" dxfId="1" priority="1">
+    <cfRule dxfId="1" priority="1" type="notContainsBlanks">
       <formula>LEN(TRIM(A1))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <hyperlinks>
-    <hyperlink ref="S2" r:id="rId1" xr:uid="{00000000-0004-0000-0100-000000000000}"/>
-    <hyperlink ref="S3" r:id="rId2" xr:uid="{00000000-0004-0000-0100-000001000000}"/>
-    <hyperlink ref="S4" r:id="rId3" xr:uid="{00000000-0004-0000-0100-000002000000}"/>
-    <hyperlink ref="S5" r:id="rId4" xr:uid="{00000000-0004-0000-0100-000003000000}"/>
-    <hyperlink ref="S6" r:id="rId5" xr:uid="{00000000-0004-0000-0100-000004000000}"/>
-    <hyperlink ref="S7" r:id="rId6" xr:uid="{00000000-0004-0000-0100-000006000000}"/>
-    <hyperlink ref="S8" r:id="rId7" xr:uid="{00000000-0004-0000-0100-000008000000}"/>
-    <hyperlink ref="S9" r:id="rId8" xr:uid="{00000000-0004-0000-0100-00000A000000}"/>
-    <hyperlink ref="S10" r:id="rId9" xr:uid="{00000000-0004-0000-0100-00000C000000}"/>
-    <hyperlink ref="S11" r:id="rId10" xr:uid="{00000000-0004-0000-0100-00000E000000}"/>
-    <hyperlink ref="S12" r:id="rId11" xr:uid="{00000000-0004-0000-0100-000010000000}"/>
-    <hyperlink ref="S14" r:id="rId12" xr:uid="{00000000-0004-0000-0100-000014000000}"/>
-    <hyperlink ref="S15" r:id="rId13" xr:uid="{00000000-0004-0000-0100-000016000000}"/>
-    <hyperlink ref="S16" r:id="rId14" xr:uid="{00000000-0004-0000-0100-000018000000}"/>
-    <hyperlink ref="S17" r:id="rId15" xr:uid="{00000000-0004-0000-0100-00001A000000}"/>
-    <hyperlink ref="S18" r:id="rId16" xr:uid="{00000000-0004-0000-0100-00001C000000}"/>
-    <hyperlink ref="S19" r:id="rId17" display="https://www.allhomes.com.au/strathnairn-act-2615?tid=178720657" xr:uid="{00000000-0004-0000-0100-00001E000000}"/>
-    <hyperlink ref="S20" r:id="rId18" xr:uid="{00000000-0004-0000-0100-000020000000}"/>
-    <hyperlink ref="S21" r:id="rId19" xr:uid="{00000000-0004-0000-0100-000022000000}"/>
-    <hyperlink ref="S22" r:id="rId20" xr:uid="{00000000-0004-0000-0100-000024000000}"/>
-    <hyperlink ref="S32" r:id="rId21" xr:uid="{00000000-0004-0000-0100-000031000000}"/>
-    <hyperlink ref="S31" r:id="rId22" xr:uid="{00000000-0004-0000-0100-000030000000}"/>
-    <hyperlink ref="S30" r:id="rId23" xr:uid="{00000000-0004-0000-0100-00002F000000}"/>
-    <hyperlink ref="S29" r:id="rId24" xr:uid="{00000000-0004-0000-0100-00002E000000}"/>
-    <hyperlink ref="S28" r:id="rId25" xr:uid="{00000000-0004-0000-0100-00002D000000}"/>
-    <hyperlink ref="S27" r:id="rId26" xr:uid="{00000000-0004-0000-0100-00002C000000}"/>
-    <hyperlink ref="S26" r:id="rId27" xr:uid="{00000000-0004-0000-0100-00002B000000}"/>
-    <hyperlink ref="S25" r:id="rId28" xr:uid="{00000000-0004-0000-0100-00002A000000}"/>
-    <hyperlink ref="S24" r:id="rId29" xr:uid="{00000000-0004-0000-0100-000028000000}"/>
-    <hyperlink ref="S23" r:id="rId30" display="https://www.allhomes.com.au/ginninderra-estate-act-2615?tid=174799089" xr:uid="{00000000-0004-0000-0100-000026000000}"/>
-    <hyperlink ref="F145" r:id="rId31" display="https://www.allhomes.com.au/browse-sale/greater-queanbeyan-queanbeyan-region-nsw/" xr:uid="{4A50D1D1-69A3-4F14-AFDA-4A60EE9976C1}"/>
+    <hyperlink r:id="rId1" ref="S2" xr:uid="{00000000-0004-0000-0100-000000000000}"/>
+    <hyperlink r:id="rId2" ref="S3" xr:uid="{00000000-0004-0000-0100-000001000000}"/>
+    <hyperlink r:id="rId3" ref="S4" xr:uid="{00000000-0004-0000-0100-000002000000}"/>
+    <hyperlink r:id="rId4" ref="S5" xr:uid="{00000000-0004-0000-0100-000003000000}"/>
+    <hyperlink r:id="rId5" ref="S6" xr:uid="{00000000-0004-0000-0100-000004000000}"/>
+    <hyperlink r:id="rId6" ref="S7" xr:uid="{00000000-0004-0000-0100-000006000000}"/>
+    <hyperlink r:id="rId7" ref="S8" xr:uid="{00000000-0004-0000-0100-000008000000}"/>
+    <hyperlink r:id="rId8" ref="S9" xr:uid="{00000000-0004-0000-0100-00000A000000}"/>
+    <hyperlink r:id="rId9" ref="S10" xr:uid="{00000000-0004-0000-0100-00000C000000}"/>
+    <hyperlink r:id="rId10" ref="S11" xr:uid="{00000000-0004-0000-0100-00000E000000}"/>
+    <hyperlink r:id="rId11" ref="S12" xr:uid="{00000000-0004-0000-0100-000010000000}"/>
+    <hyperlink r:id="rId12" ref="S14" xr:uid="{00000000-0004-0000-0100-000014000000}"/>
+    <hyperlink r:id="rId13" ref="S15" xr:uid="{00000000-0004-0000-0100-000016000000}"/>
+    <hyperlink r:id="rId14" ref="S16" xr:uid="{00000000-0004-0000-0100-000018000000}"/>
+    <hyperlink r:id="rId15" ref="S17" xr:uid="{00000000-0004-0000-0100-00001A000000}"/>
+    <hyperlink r:id="rId16" ref="S18" xr:uid="{00000000-0004-0000-0100-00001C000000}"/>
+    <hyperlink display="https://www.allhomes.com.au/strathnairn-act-2615?tid=178720657" r:id="rId17" ref="S19" xr:uid="{00000000-0004-0000-0100-00001E000000}"/>
+    <hyperlink r:id="rId18" ref="S20" xr:uid="{00000000-0004-0000-0100-000020000000}"/>
+    <hyperlink r:id="rId19" ref="S21" xr:uid="{00000000-0004-0000-0100-000022000000}"/>
+    <hyperlink r:id="rId20" ref="S22" xr:uid="{00000000-0004-0000-0100-000024000000}"/>
+    <hyperlink r:id="rId21" ref="S32" xr:uid="{00000000-0004-0000-0100-000031000000}"/>
+    <hyperlink r:id="rId22" ref="S31" xr:uid="{00000000-0004-0000-0100-000030000000}"/>
+    <hyperlink r:id="rId23" ref="S30" xr:uid="{00000000-0004-0000-0100-00002F000000}"/>
+    <hyperlink r:id="rId24" ref="S29" xr:uid="{00000000-0004-0000-0100-00002E000000}"/>
+    <hyperlink r:id="rId25" ref="S28" xr:uid="{00000000-0004-0000-0100-00002D000000}"/>
+    <hyperlink r:id="rId26" ref="S27" xr:uid="{00000000-0004-0000-0100-00002C000000}"/>
+    <hyperlink r:id="rId27" ref="S26" xr:uid="{00000000-0004-0000-0100-00002B000000}"/>
+    <hyperlink r:id="rId28" ref="S25" xr:uid="{00000000-0004-0000-0100-00002A000000}"/>
+    <hyperlink r:id="rId29" ref="S24" xr:uid="{00000000-0004-0000-0100-000028000000}"/>
+    <hyperlink display="https://www.allhomes.com.au/ginninderra-estate-act-2615?tid=174799089" r:id="rId30" ref="S23" xr:uid="{00000000-0004-0000-0100-000026000000}"/>
+    <hyperlink display="https://www.allhomes.com.au/browse-sale/greater-queanbeyan-queanbeyan-region-nsw/" r:id="rId31" ref="F145" xr:uid="{4A50D1D1-69A3-4F14-AFDA-4A60EE9976C1}"/>
   </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId32"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageSetup orientation="portrait" paperSize="9" r:id="rId32"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:AI1"/>
+  <dimension ref="A1:AJ1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1"/>
+  <sheetFormatPr customHeight="1" defaultColWidth="14.42578125" defaultRowHeight="15.75"/>
   <cols>
-    <col min="1" max="1" width="16" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="14.5703125" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="16.85546875" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="14.5703125" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="13.140625" customWidth="1" collapsed="1"/>
-    <col min="15" max="15" width="20.85546875" customWidth="1" collapsed="1"/>
-    <col min="21" max="22" width="19.140625" customWidth="1" collapsed="1"/>
-    <col min="23" max="23" width="20.140625" customWidth="1" collapsed="1"/>
-    <col min="24" max="24" width="19.85546875" customWidth="1" collapsed="1"/>
-    <col min="26" max="26" width="15.85546875" customWidth="1" collapsed="1"/>
-    <col min="27" max="27" width="13.42578125" customWidth="1" collapsed="1"/>
-    <col min="28" max="28" width="15.140625" customWidth="1" collapsed="1"/>
-    <col min="29" max="29" width="16.140625" customWidth="1" collapsed="1"/>
-    <col min="30" max="30" width="15.85546875" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="16.0" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="14.5703125" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="16.85546875" collapsed="true"/>
+    <col min="8" max="8" customWidth="true" width="14.5703125" collapsed="true"/>
+    <col min="9" max="9" customWidth="true" width="13.140625" collapsed="true"/>
+    <col min="15" max="15" customWidth="true" width="20.85546875" collapsed="true"/>
+    <col min="21" max="22" customWidth="true" width="19.140625" collapsed="true"/>
+    <col min="23" max="23" customWidth="true" width="20.140625" collapsed="true"/>
+    <col min="24" max="24" customWidth="true" width="19.85546875" collapsed="true"/>
+    <col min="26" max="26" customWidth="true" width="15.85546875" collapsed="true"/>
+    <col min="27" max="27" customWidth="true" width="13.42578125" collapsed="true"/>
+    <col min="28" max="28" customWidth="true" width="15.140625" collapsed="true"/>
+    <col min="29" max="29" customWidth="true" width="16.140625" collapsed="true"/>
+    <col min="30" max="30" customWidth="true" width="15.85546875" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:35" ht="15.75" customHeight="1">
+    <row customHeight="1" ht="15.75" r="1" spans="1:35">
       <c r="A1" s="1" t="s">
         <v>46</v>
       </c>
@@ -19781,37 +20241,37 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A1:AI1">
-    <cfRule type="notContainsBlanks" dxfId="0" priority="1">
+    <cfRule dxfId="0" priority="1" type="notContainsBlanks">
       <formula>LEN(TRIM(A1))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageSetup orientation="portrait" paperSize="9" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:G7"/>
+  <dimension ref="A1:H7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D18" sqref="D18"/>
+      <pane activePane="bottomLeft" state="frozen" topLeftCell="A2" ySplit="1"/>
+      <selection activeCell="D18" pane="bottomLeft" sqref="D18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1"/>
+  <sheetFormatPr customHeight="1" defaultColWidth="14.42578125" defaultRowHeight="15.75"/>
   <cols>
-    <col min="1" max="1" width="44.85546875" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="19.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="26.42578125" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="36.140625" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="53.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="44.85546875" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="19.5703125" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="26.42578125" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="36.140625" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="53.7109375" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="15">
+    <row ht="15" r="1" spans="1:7">
       <c r="A1" s="29" t="s">
         <v>152</v>
       </c>
@@ -19834,7 +20294,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="2" spans="1:7" s="30" customFormat="1" ht="15.75" customHeight="1">
+    <row customFormat="1" customHeight="1" ht="15.75" r="2" s="30" spans="1:7">
       <c r="A2" s="30" t="s">
         <v>158</v>
       </c>
@@ -19857,7 +20317,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:7" ht="15.75" customHeight="1">
+    <row customHeight="1" ht="15.75" r="3" spans="1:7">
       <c r="A3" s="30" t="s">
         <v>161</v>
       </c>
@@ -19874,7 +20334,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="4" spans="1:7" ht="15.75" customHeight="1">
+    <row customHeight="1" ht="15.75" r="4" spans="1:7">
       <c r="A4" s="30" t="s">
         <v>164</v>
       </c>
@@ -19891,7 +20351,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="5" spans="1:7" ht="15.75" customHeight="1">
+    <row customHeight="1" ht="15.75" r="5" spans="1:7">
       <c r="A5" s="34" t="s">
         <v>167</v>
       </c>
@@ -19908,7 +20368,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="6" spans="1:7" ht="15.75" customHeight="1">
+    <row customHeight="1" ht="15.75" r="6" spans="1:7">
       <c r="A6" t="s">
         <v>328</v>
       </c>
@@ -19925,7 +20385,7 @@
         <v>323</v>
       </c>
     </row>
-    <row r="7" spans="1:7" ht="15.75" customHeight="1">
+    <row customHeight="1" ht="15.75" r="7" spans="1:7">
       <c r="A7" s="45" t="s">
         <v>877</v>
       </c>
@@ -19944,16 +20404,16 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="E2" r:id="rId1" xr:uid="{00000000-0004-0000-0300-000000000000}"/>
-    <hyperlink ref="E3" r:id="rId2" xr:uid="{00000000-0004-0000-0300-000001000000}"/>
-    <hyperlink ref="E4" r:id="rId3" xr:uid="{00000000-0004-0000-0300-000002000000}"/>
-    <hyperlink ref="E5" r:id="rId4" xr:uid="{00000000-0004-0000-0300-000003000000}"/>
-    <hyperlink ref="D6" r:id="rId5" xr:uid="{00000000-0004-0000-0300-000004000000}"/>
-    <hyperlink ref="E6" r:id="rId6" xr:uid="{00000000-0004-0000-0300-000005000000}"/>
-    <hyperlink ref="D7" r:id="rId7" xr:uid="{B34712F5-65E4-4DA3-B4D8-B5E126A91A19}"/>
-    <hyperlink ref="E7" r:id="rId8" xr:uid="{FAD2E722-F8D2-45E6-8DA2-DA530385A188}"/>
+    <hyperlink r:id="rId1" ref="E2" xr:uid="{00000000-0004-0000-0300-000000000000}"/>
+    <hyperlink r:id="rId2" ref="E3" xr:uid="{00000000-0004-0000-0300-000001000000}"/>
+    <hyperlink r:id="rId3" ref="E4" xr:uid="{00000000-0004-0000-0300-000002000000}"/>
+    <hyperlink r:id="rId4" ref="E5" xr:uid="{00000000-0004-0000-0300-000003000000}"/>
+    <hyperlink r:id="rId5" ref="D6" xr:uid="{00000000-0004-0000-0300-000004000000}"/>
+    <hyperlink r:id="rId6" ref="E6" xr:uid="{00000000-0004-0000-0300-000005000000}"/>
+    <hyperlink r:id="rId7" ref="D7" xr:uid="{B34712F5-65E4-4DA3-B4D8-B5E126A91A19}"/>
+    <hyperlink r:id="rId8" ref="E7" xr:uid="{FAD2E722-F8D2-45E6-8DA2-DA530385A188}"/>
   </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId9"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageSetup orientation="portrait" paperSize="9" r:id="rId9"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
New property check script run
</commit_message>
<xml_diff>
--- a/src/main/resources/InputTestdata/Listing details.xlsx
+++ b/src/main/resources/InputTestdata/Listing details.xlsx
@@ -1,39 +1,39 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" mc:Ignorable="x15 xr xr6 xr10 xr2">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24326"/>
   <workbookPr/>
-  <mc:AlternateContent>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Athavan\git\777Homes-2\777Homes-business\src\main\resources\InputTestdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr documentId="13_ncr:1_{16A0ED6F-F3BD-429C-A218-CCE48E772B31}" revIDLastSave="0" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A1DDF13E-91F9-471B-A670-1C608B9CBB12}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView windowHeight="15840" windowWidth="29040" xWindow="-120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}" yWindow="-120"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Backlog" r:id="rId1" sheetId="1"/>
-    <sheet name="Listing" r:id="rId2" sheetId="2"/>
-    <sheet name="Tobe-executed" r:id="rId3" sheetId="3"/>
-    <sheet name="Agency login" r:id="rId4" sheetId="4"/>
+    <sheet name="Backlog" sheetId="1" r:id="rId1"/>
+    <sheet name="Listing" sheetId="2" r:id="rId2"/>
+    <sheet name="Tobe-executed" sheetId="3" r:id="rId3"/>
+    <sheet name="Agency login" sheetId="4" r:id="rId4"/>
   </sheets>
   <definedNames>
-    <definedName hidden="1" localSheetId="0" name="_xlnm._FilterDatabase">Backlog!$A$1:$AB$52</definedName>
-    <definedName hidden="1" localSheetId="1" name="_xlnm._FilterDatabase">Listing!$E$1:$E$145</definedName>
-    <definedName hidden="1" localSheetId="1" name="Z_A7754112_A52F_4ABC_8778_92F04773E53C_.wvu.FilterData">Listing!$A$1:$AE$32</definedName>
-    <definedName hidden="1" localSheetId="1" name="Z_C25CEB9E_BEC1_4982_90C4_50C84EE1B82A_.wvu.FilterData">Listing!$A$1:$AE$32</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Backlog!$A$1:$AB$52</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Listing!$E$1:$E$145</definedName>
+    <definedName name="Z_A7754112_A52F_4ABC_8778_92F04773E53C_.wvu.FilterData" localSheetId="1" hidden="1">Listing!$A$1:$AE$32</definedName>
+    <definedName name="Z_C25CEB9E_BEC1_4982_90C4_50C84EE1B82A_.wvu.FilterData" localSheetId="1" hidden="1">Listing!$A$1:$AE$32</definedName>
   </definedNames>
   <calcPr calcId="181029"/>
   <customWorkbookViews>
-    <customWorkbookView activeSheetId="0" guid="{C25CEB9E-BEC1-4982-90C4-50C84EE1B82A}" maximized="1" name="Filter 2" windowHeight="0" windowWidth="0"/>
-    <customWorkbookView activeSheetId="0" guid="{A7754112-A52F-4ABC-8778-92F04773E53C}" maximized="1" name="Filter 1" windowHeight="0" windowWidth="0"/>
+    <customWorkbookView name="Filter 2" guid="{C25CEB9E-BEC1-4982-90C4-50C84EE1B82A}" maximized="1" windowWidth="0" windowHeight="0" activeSheetId="0"/>
+    <customWorkbookView name="Filter 1" guid="{A7754112-A52F-4ABC-8778-92F04773E53C}" maximized="1" windowWidth="0" windowHeight="0" activeSheetId="0"/>
   </customWorkbookViews>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3881" uniqueCount="1167">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3975" uniqueCount="1194">
   <si>
     <t>ID</t>
   </si>
@@ -5668,9 +5668,6 @@
     <t>56 Carr Crescent, Wanniassa ACT 2903</t>
   </si>
   <si>
-    <t>NEW</t>
-  </si>
-  <si>
     <t>Wanniassa</t>
   </si>
   <si>
@@ -5729,24 +5726,273 @@
     <t>$490,000+</t>
   </si>
   <si>
-    <t>A spacious awe-inspiring proportions, this home is ready to meet the needs of a modern family, with spacious living spaces and year-round entertaining opportunities. A simple 3 bedroom sanctuary, 2 bathroom and 2 carport space that you will surely enjoy every corner of it with the touch of modern full timber- flooring and a grand kitchen designed with style.
-The apartment located in the Synergy complex close to the Franklin Shops, Gungahlin Town Centre and a tram stop.</t>
+    <t>https://www.777homes.com.au/?post_type=property&amp;p=9094&amp;preview=true</t>
+  </si>
+  <si>
+    <t>https://www.777homes.com.au/?post_type=property&amp;p=9096&amp;preview=true</t>
+  </si>
+  <si>
+    <t>Don't miss this perfect apartment located in 105/311 Flemington Road Franklin ACT 2913
+A spacious awe-inspiring proportions, this home is ready to meet the needs of a modern family, with spacious living spaces and year-round entertaining opportunities. A simple 3 bedroom sanctuary, 2 bathroom and 2 carport space that you will surely enjoy every corner of it with the touch of modern full timber- flooring and a grand kitchen designed with style.
+The apartment located in the Synergy complex close to the Franklin Shops, Gungahlin Town Centre and a tram stop.
+The kitchen includes modern stainless steel appliances and dishwasher and looks out to the combined living/dining area with split system.
+The large master bedroom with ensuite and master bedroom next with wide balcony with open views. Let the morning sun and birdsong start your every lovely day.
+Access via intercom and 2 parking space with storage shed. Complex includes swimming pool and BBQ area.
+Additional features: location is very accessible to the following:
+- 4 min walk to Gungahlin Village and market place
+- 4 min walk to Gubur Dhaura Heritage Park
+- 5 min walk to Franklin School
+- 4 min drive to Woolworths metro franklin
+- 4 min drive to Coffee Guru
+- 4 min drive to Fresco seafood and Franklin Discount Drug Store
+- 20 min drive to Canberra center and ANU
+This property available now, booking the private inspection with us now.
+Please feel free to contact us if you are interested and need more information.
+Paco Yip
+Paco@trustedrealtor.com.au
+Give me a call on: 0451 660 619</t>
+  </si>
+  <si>
+    <t>https://www.allhomes.com.au/16-packham-place-charnwood-act-2615</t>
+  </si>
+  <si>
+    <t>https://www.allhomes.com.au/4-keith-bain-crest-whitlam-act-2611?tid=179967283</t>
+  </si>
+  <si>
+    <t>https://www.allhomes.com.au/78-churcher-crescent-whitlam-act-2611</t>
+  </si>
+  <si>
+    <t>https://www.allhomes.com.au/32-winsome-street-taylor-act-2913</t>
+  </si>
+  <si>
+    <t>160</t>
+  </si>
+  <si>
+    <t>16 Packham Place, Charnwood ACT 2615</t>
+  </si>
+  <si>
+    <t>Charnwood</t>
+  </si>
+  <si>
+    <t>Block/House: 475/ -</t>
+  </si>
+  <si>
+    <t>Auction 30/10/21</t>
+  </si>
+  <si>
+    <t>Look no further! This delightful 3-bedroom home with two separate living areas and covered outdoor entertaining area is a must see.
+The property has been tastefully renovated with brand new carpets in the bedrooms, brand new flooring in both living areas and the kitchen. Full internal repaint in a wonderful neutral colour has also been completed, leaving you with a fresh new look.
+Modern colour combinations, light filled kitchen and generous room sizes make this home ideal for first home buyers or those wishing to scale down.
+There is absolutely nothing to do, you can just move in and enjoy the easy-care gardens or take the kids (or the dog) for a stroll out the back gate into the park. Pedestrian bridge nearby also provides you with direct access to the oval and Charnwood Primary School.
+Features include:
+* Two living areas, both with ceiling fans
+* Freshly repainted in neutral colour
+* Large skylights in the kitchen &amp; bathroom areas
+* Spacious, well-proportioned bedrooms
+* Main bedroom with BiR
+* Brand new carpets in all bedrooms
+* Ceiling fans in all bedrooms
+* Ducted gas heating throughout
+* R/C Airconditioning in the living area
+* Deadlocks on doors &amp; windows
+* Private covered timber deck
+* Direct access to the playground through the back gate
+* Easy access to the oval &amp; Charnwood Primary School
+* Instantaneous gas hot water
+* Single garage plus studio, workshop or hobby room with water connection</t>
+  </si>
+  <si>
+    <t>161</t>
+  </si>
+  <si>
+    <t>4 Keith Bain Crest, Whitlam ACT 2611</t>
+  </si>
+  <si>
+    <t>Offers over $799,000</t>
+  </si>
+  <si>
+    <t>A home should be a reflection of self. A place to recharge from daily life. It should suit your stage of life and be your escape. Confidence Real Estate is proud to present these well thought out homes in the popular suburb of Whitlam.
+Carefully curated to capture the surrounding native vistas, these homes will bask in natural light, creating a relaxed oasis. The generous open plan living/dining is overlooked by the well-appointed kitchen with 900mm appliances. The bedrooms are segregated to maximise privacy.
+The master bedroom with built-in robe and ensuite has a segregated study right outside.
+Features include;
+- Quality design and execution of space for growing families
+- Architecturally curated to capture surrounding native vistas
+- Generously proportioned interiors with quality inclusions
+- Open plan living/dining with engineered vinyl flooring
+- Laundry and tandem double garage downstairs
+- Modern kitchen with 40mm granite benchtops &amp; 900mm Bosch appliances
+- Designer bathrooms including ensuite to master and common bath with seperate powder.
+- Reverse cycle heating/cooling throughout
+- Min 6 star, energy efficient windows &amp; sliding doors.
+Call Anish on 0450865524 for more details
+Land- 150 sqm
+House - 167.5 sqm</t>
+  </si>
+  <si>
+    <t>162</t>
+  </si>
+  <si>
+    <t>78 Churcher Crescent, Whitlam ACT 2611</t>
+  </si>
+  <si>
+    <t>Expression of Interest</t>
+  </si>
+  <si>
+    <t>Confidence Real Estate is proud to present this once in a life time opportunity to secure a massive block and top build home in the popular suburb of Whitlam.
+This home and land package has a block size of 600 sqm and an amazing outlook of Whitlam Valley.
+The house which has been designed works with the block's contours and provides fantastic living areas. With a huge balcony off the living room upstairs to take maximum advantage of the views.This home provides five great size bedrooms, three of them with ensuites. Two bedrooms are on the lower floor and master with ensuite on its upper floor along with the other two bedrooms. A huge
+open plan and versatile family room and meals area downstairs opens out an exciting outdoor space with a swimming pool.
+Guest master downstairs is very versatile and can be used as a home office or alternatively as a self contained flat with its own
+private entry.
+Please note some inclusions can still be worked to the taste of the buyer. We are
+happy to work with you to customise it to your
+requirements.
+Our level of inclusions offered with this package will also be of very high in order to fit with the profile of the home.
+The residence includes:
+-Four bedrooms plus an extra bedroom on the ground floor level with seperate access
+-264.5 sqm of living only and a total house size of 346.8 sqm.
+-600 sqm of land
+-Swimming pool
+-Three separate living areas
+-Large open main living area combining kitchen with semi defined meals &amp; family
+-Segregated lounge room
+-Alfresco area under roof line
+-Bathroom Plus 3 x ensuites and powder room
+-LED down lights throughout the house
+-Colour bond roof
+-An oversized Master bedroom with views
+-A Huge Walk in robe to the master bedroom
+-Ensuite with double basin vanity and tiled to the ceiling
+-Kitchen is a great sized "Island" style design which overlooks the meals area and includes;
+-Stone bench tops - 40mm
+-Huge walk in Pantry
+-900mm cook top
+-900mm range hood
+-600mm oven
+-Loads of cupboards and benches
+-Double lock up garage with internal access and remote control entry
+-Reverse cycle heating and cooling ducted throughout the house
+(electric)
+-Tiles from floor to ceiling in the bathroom and ensuite
+-Bedrooms are all of a great size
+-Attractive front facade with decorative feature , cladding and render
+Call Anish on Confidence Real Estate is proud to present this once in a life time opportunity to secure a massive block and top build home in the popular suburb of Whitlam.
+This home and land package has a block size of 600 sqm and an amazing outlook of Whitlam Valley.
+The house which has been designed works with the block's contours and provides fantastic living areas. With a huge balcony off the living room upstairs to take maximum advantage of the views.This home provides five great size bedrooms, three of them with ensuites. Two bedrooms are on the lower floor and master with ensuite on its upper floor along with the other two bedrooms. A huge
+open plan and versatile family room and meals area downstairs opens out an exciting outdoor space with a swimming pool.
+Guest master downstairs is very versatile and can be used as a home office or alternatively as a self contained flat with its own
+private entry.
+Please note some inclusions can still be worked to the taste of the buyer. We are
+happy to work with you to customise it to your
+requirements.
+Our level of inclusions offered with this package will also be of very high in order to fit with the profile of the home.
+The residence includes:
+-Four bedrooms plus an extra bedroom on the ground floor level with seperate access
+-264.5 sqm of living only and a total house size of 346.8 sqm.
+-600 sqm of land
+-Swimming pool
+-Three separate living areas
+-Large open main living area combining kitchen with semi defined meals &amp; family
+-Segregated lounge room
+-Alfresco area under roof line
+-Bathroom Plus 3 x ensuites and powder room
+-LED down lights throughout the house
+-Colour bond roof
+-An oversized Master bedroom with views
+-A Huge Walk in robe to the master bedroom
+-Ensuite with double basin vanity and tiled to the ceiling
+-Kitchen is a great sized "Island" style design which overlooks the meals area and includes;
+-Stone bench tops - 40mm
+-Huge walk in Pantry
+-900mm cook top
+-900mm range hood
+-600mm oven
+-Loads of cupboards and benches
+-Double lock up garage with internal access and remote control entry
+-Reverse cycle heating and cooling ducted throughout the house
+(electric)
+-Tiles from floor to ceiling in the bathroom and ensuite
+-Bedrooms are all of a great size
+-Attractive front facade with decorative feature , cladding and render
+Call Anish on 0450 865 524 for more information and to register your interest.</t>
+  </si>
+  <si>
+    <t>163</t>
+  </si>
+  <si>
+    <t>32 Winsome Street, Taylor ACT 2913</t>
+  </si>
+  <si>
+    <t>Block/House: 525/ 238</t>
+  </si>
+  <si>
+    <t>Auction 24/10/21</t>
+  </si>
+  <si>
+    <t>Due to the current ACT lockdown restrictions we are only doing opens by private appointments. Please Call Alvin on 0426 146 118 to book your appointment. First viewing appointment available on Saturday 9 October from 11 am.
+Price guide: Offers over $1,050,000.
+Directly beside the Nature park, facing the Taylor water creek and surrounded by other quality homes, this four bedroom executive ensuite residence is sure to pull at the heart strings of family orientated buyers searching for luxury in an unrivalled setting.
+The cleverly designed, expansive single level floor plan provides formal and informal living options to accommodate the needs of growing families on a day to day basis.
+The sun drenched oversized main bedroom with spacious walk in robe and instantly impressive ensuite is located at the back of the property, allowing for privacy and offers uninterrupted views across the reserve that's sure to change your outlook on life and promote relaxation and contemplation on a lazy Sunday morning whilst having breakfast in bed.
+The visually exciting kitchen with ultra-modern bosch appliances acts as the hub of the home and connects effortlessly with the open plan family/meals area.
+All bedrooms are generously sized with the fourth bedroom acting as a second master.
+A large alfresco area with extended merbau decking provides the ultimate setting for all seasons entertaining with loved ones on a grand or small scale!
+If you have been searching for something truly special inspect today to see why we believe your search will end here!
+- Four bedroom executive residence directly besides Nature Reserve and across from water Creek
+- Double garage with internal access
+- Ducted reverse cycle heating and cooling with three zones.
+- Electric fireplace feature with remote
+- Hybrid Vinyl waterproof flooring all throughout
+- Study Nook
+- Sheer curtains in living areas and blinds in bedrooms
+- Recessed eight off street car park spots with no neighbours to share
+- 2.7 metre ceilings throughout
+- Large island with Calacatta 40mm stone waterfall benchtop and recessed kitchen sink
+- Calacatta large format splashback
+- Bosch Series 8 600mm oven
+- Bosch 900mm tempered glass gas cooktop with wok burner
+- Smeg 900 mm rangehood
+- Plumbed water to fridge
+- Bosch silence plus dishwasher
+- Polyurethane Soft closing draws and doors throughout kitchen
+- Walk in pantry with large pot sink.
+- NBN connected
+- Swann video intercom
+- 4 camera surveillance system
+- Rinnai instantaneous gas hot water system
+- 6.6 KW solar system with feed in tariff plan
+- 2000 litre water tank
+- Fully landscaped gardens
+- 400 m Walking distance to Taylor School, children's park, lake and playing fields.
+EER - 6.0
+Block size - 525 sqm.
+House Size - 238sqm+ 12 sqm deck
+Call Alvin on 0426146118 to book your appointment now.
+A member of the agency has financial interest in this property.</t>
   </si>
   <si>
     <t>Draft</t>
   </si>
   <si>
-    <t>https://www.777homes.com.au/?post_type=property&amp;p=9094&amp;preview=true</t>
-  </si>
-  <si>
-    <t>https://www.777homes.com.au/?post_type=property&amp;p=9096&amp;preview=true</t>
+    <t>https://www.777homes.com.au/?post_type=property&amp;p=9143&amp;preview=true</t>
+  </si>
+  <si>
+    <t>https://www.777homes.com.au/?post_type=property&amp;p=9145&amp;preview=true</t>
+  </si>
+  <si>
+    <t>https://www.777homes.com.au/?post_type=property&amp;p=9147&amp;preview=true</t>
+  </si>
+  <si>
+    <t>iqrealestate</t>
+  </si>
+  <si>
+    <t>https://www.777homes.com.au/?post_type=property&amp;p=9152&amp;preview=true</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="0"/>
   <fonts count="28">
     <font>
       <sz val="10"/>
@@ -5907,7 +6153,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="13">
+  <fills count="11">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -5966,16 +6212,6 @@
         <bgColor indexed="2"/>
       </patternFill>
     </fill>
-    <fill>
-      <patternFill patternType="none">
-        <bgColor indexed="2"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="mediumGray">
-        <bgColor indexed="2"/>
-      </patternFill>
-    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -5987,113 +6223,112 @@
     </border>
   </borders>
   <cellStyleXfs count="2">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
-    <xf applyAlignment="0" applyBorder="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="0" fontId="25" numFmtId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="49">
-    <xf applyAlignment="1" applyFont="1" borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyAlignment="1" applyFill="1" applyFont="1" borderId="0" fillId="3" fontId="1" numFmtId="0" xfId="0">
+  <cellXfs count="48">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf applyAlignment="1" applyFill="1" applyFont="1" borderId="0" fillId="2" fontId="2" numFmtId="0" xfId="0">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf applyAlignment="1" applyFill="1" applyFont="1" borderId="0" fillId="2" fontId="3" numFmtId="0" xfId="0"/>
-    <xf applyAlignment="1" applyFill="1" applyFont="1" borderId="0" fillId="2" fontId="4" numFmtId="0" xfId="0">
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf applyAlignment="1" applyFill="1" applyFont="1" borderId="0" fillId="2" fontId="6" numFmtId="0" xfId="0">
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf applyFill="1" applyFont="1" borderId="0" fillId="2" fontId="4" numFmtId="0" xfId="0"/>
-    <xf applyAlignment="1" applyFill="1" applyFont="1" borderId="0" fillId="2" fontId="7" numFmtId="0" xfId="0"/>
-    <xf applyAlignment="1" applyFill="1" applyFont="1" borderId="0" fillId="2" fontId="8" numFmtId="0" xfId="0"/>
-    <xf applyAlignment="1" applyFill="1" applyFont="1" borderId="0" fillId="2" fontId="5" numFmtId="0" xfId="0">
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf applyAlignment="1" applyFill="1" applyFont="1" borderId="0" fillId="4" fontId="4" numFmtId="0" xfId="0">
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf applyAlignment="1" applyFill="1" applyFont="1" borderId="0" fillId="5" fontId="4" numFmtId="0" xfId="0">
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf applyAlignment="1" applyFill="1" applyFont="1" borderId="0" fillId="2" fontId="9" numFmtId="0" xfId="0">
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf applyAlignment="1" applyFill="1" applyFont="1" borderId="0" fillId="2" fontId="10" numFmtId="0" xfId="0"/>
-    <xf applyAlignment="1" applyFill="1" applyFont="1" borderId="0" fillId="2" fontId="11" numFmtId="0" xfId="0"/>
-    <xf applyAlignment="1" applyFill="1" applyFont="1" borderId="0" fillId="2" fontId="4" numFmtId="0" xfId="0">
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="11" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf applyAlignment="1" applyFill="1" applyFont="1" borderId="0" fillId="2" fontId="12" numFmtId="0" xfId="0"/>
-    <xf applyAlignment="1" applyFill="1" applyFont="1" borderId="0" fillId="2" fontId="13" numFmtId="0" xfId="0"/>
-    <xf applyAlignment="1" applyFill="1" applyFont="1" borderId="0" fillId="2" fontId="14" numFmtId="0" xfId="0"/>
-    <xf applyAlignment="1" applyFill="1" applyFont="1" borderId="0" fillId="2" fontId="15" numFmtId="0" xfId="0"/>
-    <xf applyAlignment="1" applyFill="1" applyFont="1" borderId="0" fillId="2" fontId="16" numFmtId="0" xfId="0"/>
-    <xf applyAlignment="1" applyFill="1" applyFont="1" borderId="0" fillId="2" fontId="17" numFmtId="0" xfId="0"/>
-    <xf applyAlignment="1" applyFill="1" applyFont="1" borderId="0" fillId="3" fontId="1" numFmtId="0" xfId="0">
+    <xf numFmtId="0" fontId="12" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="13" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="14" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="15" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="16" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="17" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf applyFill="1" applyFont="1" borderId="0" fillId="3" fontId="7" numFmtId="0" xfId="0"/>
-    <xf applyAlignment="1" applyFill="1" applyFont="1" borderId="0" fillId="2" fontId="18" numFmtId="0" xfId="0">
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="18" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf applyAlignment="1" applyFill="1" applyFont="1" borderId="0" fillId="2" fontId="19" numFmtId="0" xfId="0">
+    <xf numFmtId="0" fontId="19" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf applyAlignment="1" applyFill="1" applyFont="1" borderId="0" fillId="2" fontId="20" numFmtId="0" xfId="0">
+    <xf numFmtId="0" fontId="20" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf applyAlignment="1" applyFill="1" applyFont="1" borderId="0" fillId="2" fontId="18" numFmtId="0" xfId="0">
+    <xf numFmtId="0" fontId="18" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf applyAlignment="1" applyFill="1" applyFont="1" borderId="0" fillId="2" fontId="21" numFmtId="0" xfId="0">
+    <xf numFmtId="0" fontId="21" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf applyAlignment="1" applyFont="1" borderId="0" fillId="0" fontId="7" numFmtId="0" xfId="0">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf applyAlignment="1" applyFill="1" applyFont="1" borderId="0" fillId="3" fontId="17" numFmtId="0" xfId="0"/>
-    <xf applyAlignment="1" applyFill="1" applyFont="1" borderId="0" fillId="3" fontId="12" numFmtId="0" xfId="0"/>
-    <xf applyAlignment="1" applyFill="1" applyFont="1" borderId="0" fillId="3" fontId="22" numFmtId="0" xfId="0">
+    <xf numFmtId="0" fontId="17" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="12" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="22" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf applyAlignment="1" applyFill="1" applyFont="1" borderId="0" fillId="3" fontId="23" numFmtId="0" xfId="0"/>
-    <xf applyAlignment="1" applyFont="1" borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0"/>
-    <xf applyAlignment="1" applyFill="1" applyFont="1" borderId="0" fillId="3" fontId="24" numFmtId="0" xfId="0">
+    <xf numFmtId="0" fontId="23" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="24" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf applyAlignment="1" applyFill="1" applyFont="1" borderId="0" fillId="3" fontId="1" numFmtId="0" xfId="0">
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf applyAlignment="1" applyFont="1" borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf applyAlignment="1" applyFill="1" borderId="0" fillId="2" fontId="25" numFmtId="0" xfId="1">
+    <xf numFmtId="0" fontId="25" fillId="2" borderId="0" xfId="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf applyAlignment="1" applyFill="1" applyFont="1" borderId="0" fillId="6" fontId="2" numFmtId="0" xfId="0">
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf applyAlignment="1" applyFill="1" applyFont="1" borderId="0" fillId="7" fontId="5" numFmtId="0" xfId="0">
+    <xf numFmtId="0" fontId="5" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf applyAlignment="1" borderId="0" fillId="0" fontId="25" numFmtId="0" xfId="1"/>
-    <xf applyAlignment="1" applyFill="1" borderId="0" fillId="2" fontId="25" numFmtId="0" xfId="1"/>
-    <xf applyAlignment="1" applyFill="1" applyFont="1" borderId="0" fillId="8" fontId="18" numFmtId="0" xfId="0">
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" xfId="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="25" fillId="2" borderId="0" xfId="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="18" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf applyAlignment="1" applyFill="1" applyFont="1" borderId="0" fillId="2" fontId="26" numFmtId="0" xfId="0">
+    <xf numFmtId="0" fontId="26" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf applyAlignment="1" applyFont="1" borderId="0" fillId="0" fontId="27" numFmtId="0" xfId="0"/>
-    <xf applyFill="1" borderId="0" fillId="9" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyFill="1" borderId="0" fillId="10" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyFill="true" borderId="0" fillId="12" fontId="0" numFmtId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
-    <cellStyle builtinId="8" name="Hyperlink" xfId="1"/>
-    <cellStyle builtinId="0" name="Normal" xfId="0"/>
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="2">
     <dxf>
@@ -6113,7 +6348,7 @@
       </fill>
     </dxf>
   </dxfs>
-  <tableStyles count="0" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium2"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -6237,21 +6472,21 @@
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
-        <a:ln algn="ctr" cap="flat" cmpd="sng" w="6350">
+        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
           <a:miter lim="800000"/>
         </a:ln>
-        <a:ln algn="ctr" cap="flat" cmpd="sng" w="12700">
+        <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
           <a:miter lim="800000"/>
         </a:ln>
-        <a:ln algn="ctr" cap="flat" cmpd="sng" w="19050">
+        <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
@@ -6268,7 +6503,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw algn="ctr" blurRad="57150" dir="5400000" dist="19050" rotWithShape="0">
+            <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="63000"/>
               </a:srgbClr>
@@ -6322,32 +6557,32 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:AC160"/>
+  <dimension ref="A1:AB164"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane activePane="bottomLeft" state="frozen" topLeftCell="A139" ySplit="1"/>
-      <selection activeCell="F163" pane="bottomLeft" sqref="F163"/>
+      <pane ySplit="1" topLeftCell="A131" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D162" sqref="D162"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="14.42578125" defaultRowHeight="15.75"/>
+  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="9.140625" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" width="74.85546875" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="75.0" collapsed="true"/>
-    <col min="4" max="4" customWidth="true" width="14.5703125" collapsed="true"/>
-    <col min="6" max="6" bestFit="true" customWidth="true" style="37" width="22.140625" collapsed="true"/>
-    <col min="7" max="7" customWidth="true" width="21.85546875" collapsed="true"/>
-    <col min="8" max="8" customWidth="true" width="56.85546875" collapsed="true"/>
-    <col min="9" max="9" customWidth="true" width="10.85546875" collapsed="true"/>
-    <col min="10" max="10" customWidth="true" width="17.85546875" collapsed="true"/>
-    <col min="11" max="11" customWidth="true" width="22.5703125" collapsed="true"/>
+    <col min="1" max="1" width="9.140625" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="74.85546875" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="75" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="14.5703125" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="22.140625" style="37" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="21.85546875" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="56.85546875" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="10.85546875" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="17.85546875" customWidth="1" collapsed="1"/>
+    <col min="11" max="11" width="22.5703125" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row ht="15" r="1" spans="1:28">
+    <row r="1" spans="1:28" ht="15">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -6374,7 +6609,7 @@
       </c>
       <c r="J1" s="1"/>
     </row>
-    <row customHeight="1" ht="15.75" r="2" spans="1:28">
+    <row r="2" spans="1:28" ht="15.75" customHeight="1">
       <c r="A2" s="2">
         <v>1</v>
       </c>
@@ -6420,7 +6655,7 @@
       <c r="AA2" s="6"/>
       <c r="AB2" s="6"/>
     </row>
-    <row ht="14.25" r="3" spans="1:28">
+    <row r="3" spans="1:28" ht="14.25">
       <c r="A3" s="2">
         <v>2</v>
       </c>
@@ -6466,7 +6701,7 @@
       <c r="AA3" s="6"/>
       <c r="AB3" s="6"/>
     </row>
-    <row customHeight="1" ht="15.75" r="4" spans="1:28">
+    <row r="4" spans="1:28" ht="15.75" customHeight="1">
       <c r="A4" s="9">
         <v>3</v>
       </c>
@@ -6512,7 +6747,7 @@
       <c r="AA4" s="6"/>
       <c r="AB4" s="6"/>
     </row>
-    <row ht="14.25" r="5" spans="1:28">
+    <row r="5" spans="1:28" ht="14.25">
       <c r="A5" s="9">
         <v>4</v>
       </c>
@@ -6556,7 +6791,7 @@
       <c r="AA5" s="6"/>
       <c r="AB5" s="6"/>
     </row>
-    <row ht="14.25" r="6" spans="1:28">
+    <row r="6" spans="1:28" ht="14.25">
       <c r="A6" s="9">
         <v>5</v>
       </c>
@@ -6600,7 +6835,7 @@
       <c r="AA6" s="9"/>
       <c r="AB6" s="9"/>
     </row>
-    <row ht="14.25" r="7" spans="1:28">
+    <row r="7" spans="1:28" ht="14.25">
       <c r="A7" s="9">
         <v>6</v>
       </c>
@@ -6644,7 +6879,7 @@
       <c r="AA7" s="6"/>
       <c r="AB7" s="6"/>
     </row>
-    <row ht="14.25" r="8" spans="1:28">
+    <row r="8" spans="1:28" ht="14.25">
       <c r="A8" s="9">
         <v>7</v>
       </c>
@@ -6688,7 +6923,7 @@
       <c r="AA8" s="6"/>
       <c r="AB8" s="6"/>
     </row>
-    <row ht="14.25" r="9" spans="1:28">
+    <row r="9" spans="1:28" ht="14.25">
       <c r="A9" s="9">
         <v>8</v>
       </c>
@@ -6730,7 +6965,7 @@
       <c r="AA9" s="6"/>
       <c r="AB9" s="6"/>
     </row>
-    <row ht="14.25" r="10" spans="1:28">
+    <row r="10" spans="1:28" ht="14.25">
       <c r="A10" s="9">
         <v>9</v>
       </c>
@@ -6772,7 +7007,7 @@
       <c r="AA10" s="6"/>
       <c r="AB10" s="6"/>
     </row>
-    <row ht="14.25" r="11" spans="1:28">
+    <row r="11" spans="1:28" ht="14.25">
       <c r="A11" s="9">
         <v>10</v>
       </c>
@@ -6816,7 +7051,7 @@
       <c r="AA11" s="6"/>
       <c r="AB11" s="6"/>
     </row>
-    <row ht="14.25" r="12" spans="1:28">
+    <row r="12" spans="1:28" ht="14.25">
       <c r="A12" s="9">
         <v>11</v>
       </c>
@@ -6858,7 +7093,7 @@
       <c r="AA12" s="6"/>
       <c r="AB12" s="6"/>
     </row>
-    <row ht="14.25" r="13" spans="1:28">
+    <row r="13" spans="1:28" ht="14.25">
       <c r="A13" s="9">
         <v>12</v>
       </c>
@@ -6900,7 +7135,7 @@
       <c r="AA13" s="6"/>
       <c r="AB13" s="6"/>
     </row>
-    <row ht="14.25" r="14" spans="1:28">
+    <row r="14" spans="1:28" ht="14.25">
       <c r="A14" s="9">
         <v>13</v>
       </c>
@@ -6942,7 +7177,7 @@
       <c r="AA14" s="6"/>
       <c r="AB14" s="6"/>
     </row>
-    <row ht="14.25" r="15" spans="1:28">
+    <row r="15" spans="1:28" ht="14.25">
       <c r="A15" s="9">
         <v>14</v>
       </c>
@@ -6986,7 +7221,7 @@
       <c r="AA15" s="6"/>
       <c r="AB15" s="6"/>
     </row>
-    <row ht="14.25" r="16" spans="1:28">
+    <row r="16" spans="1:28" ht="14.25">
       <c r="A16" s="9">
         <v>15</v>
       </c>
@@ -7028,7 +7263,7 @@
       <c r="AA16" s="6"/>
       <c r="AB16" s="6"/>
     </row>
-    <row ht="14.25" r="17" spans="1:28">
+    <row r="17" spans="1:28" ht="14.25">
       <c r="A17" s="9">
         <v>16</v>
       </c>
@@ -7072,7 +7307,7 @@
       <c r="AA17" s="6"/>
       <c r="AB17" s="6"/>
     </row>
-    <row ht="14.25" r="18" spans="1:28">
+    <row r="18" spans="1:28" ht="14.25">
       <c r="A18" s="9">
         <v>17</v>
       </c>
@@ -7114,7 +7349,7 @@
       <c r="AA18" s="6"/>
       <c r="AB18" s="6"/>
     </row>
-    <row ht="14.25" r="19" spans="1:28">
+    <row r="19" spans="1:28" ht="14.25">
       <c r="A19" s="9">
         <v>18</v>
       </c>
@@ -7158,7 +7393,7 @@
       <c r="AA19" s="6"/>
       <c r="AB19" s="6"/>
     </row>
-    <row ht="14.25" r="20" spans="1:28">
+    <row r="20" spans="1:28" ht="14.25">
       <c r="A20" s="9">
         <v>19</v>
       </c>
@@ -7202,7 +7437,7 @@
       <c r="AA20" s="6"/>
       <c r="AB20" s="6"/>
     </row>
-    <row ht="14.25" r="21" spans="1:28">
+    <row r="21" spans="1:28" ht="14.25">
       <c r="A21" s="9">
         <v>20</v>
       </c>
@@ -7246,7 +7481,7 @@
       <c r="AA21" s="6"/>
       <c r="AB21" s="6"/>
     </row>
-    <row ht="14.25" r="22" spans="1:28">
+    <row r="22" spans="1:28" ht="14.25">
       <c r="A22" s="9">
         <v>21</v>
       </c>
@@ -7288,7 +7523,7 @@
       <c r="AA22" s="6"/>
       <c r="AB22" s="6"/>
     </row>
-    <row ht="14.25" r="23" spans="1:28">
+    <row r="23" spans="1:28" ht="14.25">
       <c r="A23" s="9">
         <v>22</v>
       </c>
@@ -7332,7 +7567,7 @@
       <c r="AA23" s="6"/>
       <c r="AB23" s="6"/>
     </row>
-    <row ht="14.25" r="24" spans="1:28">
+    <row r="24" spans="1:28" ht="14.25">
       <c r="A24" s="9">
         <v>23</v>
       </c>
@@ -7374,7 +7609,7 @@
       <c r="AA24" s="6"/>
       <c r="AB24" s="6"/>
     </row>
-    <row ht="14.25" r="25" spans="1:28">
+    <row r="25" spans="1:28" ht="14.25">
       <c r="A25" s="9">
         <v>24</v>
       </c>
@@ -7416,7 +7651,7 @@
       <c r="AA25" s="6"/>
       <c r="AB25" s="6"/>
     </row>
-    <row ht="14.25" r="26" spans="1:28">
+    <row r="26" spans="1:28" ht="14.25">
       <c r="A26" s="9">
         <v>25</v>
       </c>
@@ -7460,7 +7695,7 @@
       <c r="AA26" s="6"/>
       <c r="AB26" s="6"/>
     </row>
-    <row ht="14.25" r="27" spans="1:28">
+    <row r="27" spans="1:28" ht="14.25">
       <c r="A27" s="9">
         <v>26</v>
       </c>
@@ -7504,7 +7739,7 @@
       <c r="AA27" s="6"/>
       <c r="AB27" s="6"/>
     </row>
-    <row ht="14.25" r="28" spans="1:28">
+    <row r="28" spans="1:28" ht="14.25">
       <c r="A28" s="9">
         <v>27</v>
       </c>
@@ -7546,7 +7781,7 @@
       <c r="AA28" s="6"/>
       <c r="AB28" s="6"/>
     </row>
-    <row ht="14.25" r="29" spans="1:28">
+    <row r="29" spans="1:28" ht="14.25">
       <c r="A29" s="9">
         <v>28</v>
       </c>
@@ -7590,7 +7825,7 @@
       <c r="AA29" s="6"/>
       <c r="AB29" s="6"/>
     </row>
-    <row ht="14.25" r="30" spans="1:28">
+    <row r="30" spans="1:28" ht="14.25">
       <c r="A30" s="9">
         <v>29</v>
       </c>
@@ -7632,7 +7867,7 @@
       <c r="AA30" s="6"/>
       <c r="AB30" s="6"/>
     </row>
-    <row ht="14.25" r="31" spans="1:28">
+    <row r="31" spans="1:28" ht="14.25">
       <c r="A31" s="4">
         <v>30</v>
       </c>
@@ -7676,7 +7911,7 @@
       <c r="AA31" s="6"/>
       <c r="AB31" s="6"/>
     </row>
-    <row ht="14.25" r="32" spans="1:28">
+    <row r="32" spans="1:28" ht="14.25">
       <c r="A32" s="4">
         <v>31</v>
       </c>
@@ -7718,7 +7953,7 @@
       <c r="AA32" s="6"/>
       <c r="AB32" s="6"/>
     </row>
-    <row customFormat="1" ht="14.25" r="33" s="4" spans="1:8">
+    <row r="33" spans="1:8" s="4" customFormat="1" ht="14.25">
       <c r="A33" s="4">
         <v>32</v>
       </c>
@@ -7741,7 +7976,7 @@
         <v>427</v>
       </c>
     </row>
-    <row customFormat="1" ht="14.25" r="34" s="4" spans="1:8">
+    <row r="34" spans="1:8" s="4" customFormat="1" ht="14.25">
       <c r="A34" s="4">
         <v>33</v>
       </c>
@@ -7761,7 +7996,7 @@
         <v>427</v>
       </c>
     </row>
-    <row customFormat="1" ht="14.25" r="35" s="4" spans="1:8">
+    <row r="35" spans="1:8" s="4" customFormat="1" ht="14.25">
       <c r="A35" s="4">
         <v>34</v>
       </c>
@@ -7781,7 +8016,7 @@
         <v>427</v>
       </c>
     </row>
-    <row customFormat="1" ht="14.25" r="36" s="4" spans="1:8">
+    <row r="36" spans="1:8" s="4" customFormat="1" ht="14.25">
       <c r="A36" s="4">
         <v>35</v>
       </c>
@@ -7801,7 +8036,7 @@
         <v>427</v>
       </c>
     </row>
-    <row customFormat="1" ht="14.25" r="37" s="4" spans="1:8">
+    <row r="37" spans="1:8" s="4" customFormat="1" ht="14.25">
       <c r="A37" s="4">
         <v>36</v>
       </c>
@@ -7821,7 +8056,7 @@
         <v>427</v>
       </c>
     </row>
-    <row customFormat="1" ht="14.25" r="38" s="4" spans="1:8">
+    <row r="38" spans="1:8" s="4" customFormat="1" ht="14.25">
       <c r="A38" s="4">
         <v>37</v>
       </c>
@@ -7844,7 +8079,7 @@
         <v>427</v>
       </c>
     </row>
-    <row customFormat="1" ht="14.25" r="39" s="4" spans="1:8">
+    <row r="39" spans="1:8" s="4" customFormat="1" ht="14.25">
       <c r="A39" s="4">
         <v>38</v>
       </c>
@@ -7867,7 +8102,7 @@
         <v>427</v>
       </c>
     </row>
-    <row customFormat="1" ht="14.25" r="40" s="4" spans="1:8">
+    <row r="40" spans="1:8" s="4" customFormat="1" ht="14.25">
       <c r="A40" s="4">
         <v>39</v>
       </c>
@@ -7890,7 +8125,7 @@
         <v>427</v>
       </c>
     </row>
-    <row customFormat="1" ht="14.25" r="41" s="4" spans="1:8">
+    <row r="41" spans="1:8" s="4" customFormat="1" ht="14.25">
       <c r="A41" s="4">
         <v>40</v>
       </c>
@@ -7910,7 +8145,7 @@
         <v>427</v>
       </c>
     </row>
-    <row customFormat="1" ht="14.25" r="42" s="4" spans="1:8">
+    <row r="42" spans="1:8" s="4" customFormat="1" ht="14.25">
       <c r="A42" s="4">
         <v>41</v>
       </c>
@@ -7933,7 +8168,7 @@
         <v>427</v>
       </c>
     </row>
-    <row customFormat="1" ht="14.25" r="43" s="4" spans="1:8">
+    <row r="43" spans="1:8" s="4" customFormat="1" ht="14.25">
       <c r="A43" s="4">
         <v>42</v>
       </c>
@@ -7953,7 +8188,7 @@
         <v>427</v>
       </c>
     </row>
-    <row customFormat="1" ht="14.25" r="44" s="4" spans="1:8">
+    <row r="44" spans="1:8" s="4" customFormat="1" ht="14.25">
       <c r="A44" s="4">
         <v>43</v>
       </c>
@@ -7973,7 +8208,7 @@
         <v>427</v>
       </c>
     </row>
-    <row customFormat="1" ht="14.25" r="45" s="4" spans="1:8">
+    <row r="45" spans="1:8" s="4" customFormat="1" ht="14.25">
       <c r="A45" s="4">
         <v>44</v>
       </c>
@@ -7996,7 +8231,7 @@
         <v>38</v>
       </c>
     </row>
-    <row customFormat="1" ht="14.25" r="46" s="4" spans="1:8">
+    <row r="46" spans="1:8" s="4" customFormat="1" ht="14.25">
       <c r="A46" s="4">
         <v>45</v>
       </c>
@@ -8016,7 +8251,7 @@
         <v>38</v>
       </c>
     </row>
-    <row customFormat="1" ht="14.25" r="47" s="4" spans="1:8">
+    <row r="47" spans="1:8" s="4" customFormat="1" ht="14.25">
       <c r="A47" s="4">
         <v>46</v>
       </c>
@@ -8036,7 +8271,7 @@
         <v>38</v>
       </c>
     </row>
-    <row customFormat="1" ht="12.75" r="48" s="4" spans="1:8">
+    <row r="48" spans="1:8" s="4" customFormat="1" ht="12.75">
       <c r="A48" s="4">
         <v>47</v>
       </c>
@@ -8059,7 +8294,7 @@
         <v>428</v>
       </c>
     </row>
-    <row customFormat="1" ht="12.75" r="49" s="4" spans="1:8">
+    <row r="49" spans="1:8" s="4" customFormat="1" ht="12.75">
       <c r="A49" s="4">
         <v>48</v>
       </c>
@@ -8082,7 +8317,7 @@
         <v>428</v>
       </c>
     </row>
-    <row customFormat="1" ht="12.75" r="50" s="4" spans="1:8">
+    <row r="50" spans="1:8" s="4" customFormat="1" ht="12.75">
       <c r="A50" s="4">
         <v>49</v>
       </c>
@@ -8102,7 +8337,7 @@
         <v>428</v>
       </c>
     </row>
-    <row customFormat="1" ht="12.75" r="51" s="4" spans="1:8">
+    <row r="51" spans="1:8" s="4" customFormat="1" ht="12.75">
       <c r="A51" s="4">
         <v>50</v>
       </c>
@@ -8122,7 +8357,7 @@
         <v>428</v>
       </c>
     </row>
-    <row customFormat="1" ht="12.75" r="52" s="4" spans="1:8">
+    <row r="52" spans="1:8" s="4" customFormat="1" ht="12.75">
       <c r="A52" s="4">
         <v>51</v>
       </c>
@@ -8145,7 +8380,7 @@
         <v>428</v>
       </c>
     </row>
-    <row customFormat="1" customHeight="1" ht="15.75" r="53" s="4" spans="1:8">
+    <row r="53" spans="1:8" s="4" customFormat="1" ht="15.75" customHeight="1">
       <c r="A53" s="4">
         <v>52</v>
       </c>
@@ -8162,13 +8397,13 @@
         <v>686</v>
       </c>
       <c r="G53" s="4" t="s">
-        <v>325</v>
+        <v>1192</v>
       </c>
       <c r="H53" s="4" t="s">
         <v>323</v>
       </c>
     </row>
-    <row customFormat="1" ht="12.75" r="54" s="4" spans="1:8">
+    <row r="54" spans="1:8" s="4" customFormat="1" ht="12.75">
       <c r="A54" s="4">
         <v>53</v>
       </c>
@@ -8182,13 +8417,13 @@
         <v>686</v>
       </c>
       <c r="G54" s="4" t="s">
-        <v>325</v>
+        <v>1192</v>
       </c>
       <c r="H54" s="4" t="s">
         <v>323</v>
       </c>
     </row>
-    <row customFormat="1" ht="12.75" r="55" s="4" spans="1:8">
+    <row r="55" spans="1:8" s="4" customFormat="1" ht="12.75">
       <c r="A55" s="4">
         <v>54</v>
       </c>
@@ -8205,13 +8440,13 @@
         <v>686</v>
       </c>
       <c r="G55" s="4" t="s">
-        <v>325</v>
+        <v>1192</v>
       </c>
       <c r="H55" s="4" t="s">
         <v>323</v>
       </c>
     </row>
-    <row customFormat="1" ht="12.75" r="56" s="4" spans="1:8">
+    <row r="56" spans="1:8" s="4" customFormat="1" ht="12.75">
       <c r="A56" s="4">
         <v>55</v>
       </c>
@@ -8228,13 +8463,13 @@
         <v>686</v>
       </c>
       <c r="G56" s="4" t="s">
-        <v>325</v>
+        <v>1192</v>
       </c>
       <c r="H56" s="4" t="s">
         <v>323</v>
       </c>
     </row>
-    <row customFormat="1" ht="12.75" r="57" s="4" spans="1:8">
+    <row r="57" spans="1:8" s="4" customFormat="1" ht="12.75">
       <c r="A57" s="4">
         <v>56</v>
       </c>
@@ -8248,13 +8483,13 @@
         <v>686</v>
       </c>
       <c r="G57" s="4" t="s">
-        <v>325</v>
+        <v>1192</v>
       </c>
       <c r="H57" s="4" t="s">
         <v>323</v>
       </c>
     </row>
-    <row customFormat="1" ht="12.75" r="58" s="4" spans="1:8">
+    <row r="58" spans="1:8" s="4" customFormat="1" ht="12.75">
       <c r="A58" s="4">
         <v>57</v>
       </c>
@@ -8268,13 +8503,13 @@
         <v>686</v>
       </c>
       <c r="G58" s="4" t="s">
-        <v>325</v>
+        <v>1192</v>
       </c>
       <c r="H58" s="4" t="s">
         <v>323</v>
       </c>
     </row>
-    <row customFormat="1" ht="12.75" r="59" s="4" spans="1:8">
+    <row r="59" spans="1:8" s="4" customFormat="1" ht="12.75">
       <c r="A59" s="4">
         <v>58</v>
       </c>
@@ -8288,13 +8523,13 @@
         <v>686</v>
       </c>
       <c r="G59" s="4" t="s">
-        <v>325</v>
+        <v>1192</v>
       </c>
       <c r="H59" s="4" t="s">
         <v>323</v>
       </c>
     </row>
-    <row customFormat="1" ht="12.75" r="60" s="4" spans="1:8">
+    <row r="60" spans="1:8" s="4" customFormat="1" ht="12.75">
       <c r="A60" s="4">
         <v>59</v>
       </c>
@@ -8308,13 +8543,13 @@
         <v>686</v>
       </c>
       <c r="G60" s="4" t="s">
-        <v>325</v>
+        <v>1192</v>
       </c>
       <c r="H60" s="4" t="s">
         <v>323</v>
       </c>
     </row>
-    <row customFormat="1" ht="12.75" r="61" s="4" spans="1:8">
+    <row r="61" spans="1:8" s="4" customFormat="1" ht="12.75">
       <c r="A61" s="4">
         <v>60</v>
       </c>
@@ -8328,13 +8563,13 @@
         <v>686</v>
       </c>
       <c r="G61" s="4" t="s">
-        <v>325</v>
+        <v>1192</v>
       </c>
       <c r="H61" s="4" t="s">
         <v>323</v>
       </c>
     </row>
-    <row customFormat="1" ht="12.75" r="62" s="4" spans="1:8">
+    <row r="62" spans="1:8" s="4" customFormat="1" ht="12.75">
       <c r="A62" s="4">
         <v>61</v>
       </c>
@@ -8354,7 +8589,7 @@
         <v>427</v>
       </c>
     </row>
-    <row customFormat="1" ht="12.75" r="63" s="4" spans="1:8">
+    <row r="63" spans="1:8" s="4" customFormat="1" ht="12.75">
       <c r="A63" s="4">
         <v>62</v>
       </c>
@@ -8377,7 +8612,7 @@
         <v>427</v>
       </c>
     </row>
-    <row customFormat="1" ht="12.75" r="64" s="4" spans="1:8">
+    <row r="64" spans="1:8" s="4" customFormat="1" ht="12.75">
       <c r="A64" s="4">
         <v>63</v>
       </c>
@@ -8400,7 +8635,7 @@
         <v>427</v>
       </c>
     </row>
-    <row customFormat="1" ht="12.75" r="65" s="4" spans="1:8">
+    <row r="65" spans="1:8" s="4" customFormat="1" ht="12.75">
       <c r="A65" s="4">
         <v>64</v>
       </c>
@@ -8421,7 +8656,7 @@
         <v>427</v>
       </c>
     </row>
-    <row customFormat="1" ht="12.75" r="66" s="4" spans="1:8">
+    <row r="66" spans="1:8" s="4" customFormat="1" ht="12.75">
       <c r="A66" s="4">
         <v>65</v>
       </c>
@@ -8444,7 +8679,7 @@
         <v>38</v>
       </c>
     </row>
-    <row customFormat="1" ht="12.75" r="67" s="4" spans="1:8">
+    <row r="67" spans="1:8" s="4" customFormat="1" ht="12.75">
       <c r="A67" s="4">
         <v>66</v>
       </c>
@@ -8467,7 +8702,7 @@
         <v>428</v>
       </c>
     </row>
-    <row customFormat="1" ht="12.75" r="68" s="4" spans="1:8">
+    <row r="68" spans="1:8" s="4" customFormat="1" ht="12.75">
       <c r="A68" s="4">
         <v>67</v>
       </c>
@@ -8490,7 +8725,7 @@
         <v>427</v>
       </c>
     </row>
-    <row customFormat="1" ht="12.75" r="69" s="4" spans="1:8">
+    <row r="69" spans="1:8" s="4" customFormat="1" ht="12.75">
       <c r="A69" s="4">
         <v>68</v>
       </c>
@@ -8513,7 +8748,7 @@
         <v>427</v>
       </c>
     </row>
-    <row customFormat="1" ht="12.75" r="70" s="4" spans="1:8">
+    <row r="70" spans="1:8" s="4" customFormat="1" ht="12.75">
       <c r="A70" s="4">
         <v>69</v>
       </c>
@@ -8536,7 +8771,7 @@
         <v>427</v>
       </c>
     </row>
-    <row customFormat="1" ht="12.75" r="71" s="4" spans="1:8">
+    <row r="71" spans="1:8" s="4" customFormat="1" ht="12.75">
       <c r="A71" s="4">
         <v>70</v>
       </c>
@@ -8559,7 +8794,7 @@
         <v>427</v>
       </c>
     </row>
-    <row customFormat="1" ht="12.75" r="72" s="4" spans="1:8">
+    <row r="72" spans="1:8" s="4" customFormat="1" ht="12.75">
       <c r="A72" s="4">
         <v>71</v>
       </c>
@@ -8582,7 +8817,7 @@
         <v>427</v>
       </c>
     </row>
-    <row ht="12.75" r="73" spans="1:8">
+    <row r="73" spans="1:8" ht="12.75">
       <c r="A73">
         <v>72</v>
       </c>
@@ -8605,7 +8840,7 @@
         <v>428</v>
       </c>
     </row>
-    <row ht="12.75" r="74" spans="1:8">
+    <row r="74" spans="1:8" ht="12.75">
       <c r="A74">
         <v>73</v>
       </c>
@@ -8628,7 +8863,7 @@
         <v>428</v>
       </c>
     </row>
-    <row customFormat="1" ht="12.75" r="75" s="4" spans="1:8">
+    <row r="75" spans="1:8" s="4" customFormat="1" ht="12.75">
       <c r="A75" s="4">
         <v>74</v>
       </c>
@@ -8651,7 +8886,7 @@
         <v>428</v>
       </c>
     </row>
-    <row ht="12.75" r="76" spans="1:8">
+    <row r="76" spans="1:8" ht="12.75">
       <c r="A76">
         <v>75</v>
       </c>
@@ -8674,7 +8909,7 @@
         <v>428</v>
       </c>
     </row>
-    <row ht="12.75" r="77" spans="1:8">
+    <row r="77" spans="1:8" ht="12.75">
       <c r="A77">
         <v>76</v>
       </c>
@@ -8697,7 +8932,7 @@
         <v>428</v>
       </c>
     </row>
-    <row ht="12.75" r="78" spans="1:8">
+    <row r="78" spans="1:8" ht="12.75">
       <c r="A78">
         <v>77</v>
       </c>
@@ -8720,7 +8955,7 @@
         <v>428</v>
       </c>
     </row>
-    <row ht="12.75" r="79" spans="1:8">
+    <row r="79" spans="1:8" ht="12.75">
       <c r="A79">
         <v>78</v>
       </c>
@@ -8743,7 +8978,7 @@
         <v>428</v>
       </c>
     </row>
-    <row ht="12.75" r="80" spans="1:8">
+    <row r="80" spans="1:8" ht="12.75">
       <c r="A80">
         <v>79</v>
       </c>
@@ -8766,7 +9001,7 @@
         <v>428</v>
       </c>
     </row>
-    <row ht="12.75" r="81" spans="1:8">
+    <row r="81" spans="1:8" ht="12.75">
       <c r="A81">
         <v>80</v>
       </c>
@@ -8789,7 +9024,7 @@
         <v>428</v>
       </c>
     </row>
-    <row ht="12.75" r="82" spans="1:8">
+    <row r="82" spans="1:8" ht="12.75">
       <c r="A82">
         <v>81</v>
       </c>
@@ -8812,7 +9047,7 @@
         <v>428</v>
       </c>
     </row>
-    <row ht="12.75" r="83" spans="1:8">
+    <row r="83" spans="1:8" ht="12.75">
       <c r="A83">
         <v>82</v>
       </c>
@@ -8835,7 +9070,7 @@
         <v>428</v>
       </c>
     </row>
-    <row ht="12.75" r="84" spans="1:8">
+    <row r="84" spans="1:8" ht="12.75">
       <c r="A84">
         <v>83</v>
       </c>
@@ -8858,7 +9093,7 @@
         <v>428</v>
       </c>
     </row>
-    <row ht="12.75" r="85" spans="1:8">
+    <row r="85" spans="1:8" ht="12.75">
       <c r="A85">
         <v>84</v>
       </c>
@@ -8881,7 +9116,7 @@
         <v>428</v>
       </c>
     </row>
-    <row customFormat="1" ht="12.75" r="86" s="4" spans="1:8">
+    <row r="86" spans="1:8" s="4" customFormat="1" ht="12.75">
       <c r="A86" s="4">
         <v>85</v>
       </c>
@@ -8904,7 +9139,7 @@
         <v>427</v>
       </c>
     </row>
-    <row customFormat="1" ht="12.75" r="87" s="4" spans="1:8">
+    <row r="87" spans="1:8" s="4" customFormat="1" ht="12.75">
       <c r="A87" s="4">
         <v>86</v>
       </c>
@@ -8927,7 +9162,7 @@
         <v>38</v>
       </c>
     </row>
-    <row ht="12.75" r="88" spans="1:8">
+    <row r="88" spans="1:8" ht="12.75">
       <c r="A88">
         <v>87</v>
       </c>
@@ -8950,7 +9185,7 @@
         <v>38</v>
       </c>
     </row>
-    <row ht="12.75" r="89" spans="1:8">
+    <row r="89" spans="1:8" ht="12.75">
       <c r="A89">
         <v>88</v>
       </c>
@@ -8973,7 +9208,7 @@
         <v>38</v>
       </c>
     </row>
-    <row ht="12.75" r="90" spans="1:8">
+    <row r="90" spans="1:8" ht="12.75">
       <c r="A90">
         <v>89</v>
       </c>
@@ -8996,7 +9231,7 @@
         <v>428</v>
       </c>
     </row>
-    <row ht="12.75" r="91" spans="1:8">
+    <row r="91" spans="1:8" ht="12.75">
       <c r="A91">
         <v>90</v>
       </c>
@@ -9019,7 +9254,7 @@
         <v>428</v>
       </c>
     </row>
-    <row ht="12.75" r="92" spans="1:8">
+    <row r="92" spans="1:8" ht="12.75">
       <c r="A92">
         <v>91</v>
       </c>
@@ -9042,7 +9277,7 @@
         <v>428</v>
       </c>
     </row>
-    <row ht="12.75" r="93" spans="1:8">
+    <row r="93" spans="1:8" ht="12.75">
       <c r="A93">
         <v>92</v>
       </c>
@@ -9065,7 +9300,7 @@
         <v>428</v>
       </c>
     </row>
-    <row ht="12.75" r="94" spans="1:8">
+    <row r="94" spans="1:8" ht="12.75">
       <c r="A94">
         <v>93</v>
       </c>
@@ -9088,7 +9323,7 @@
         <v>427</v>
       </c>
     </row>
-    <row ht="12.75" r="95" spans="1:8">
+    <row r="95" spans="1:8" ht="12.75">
       <c r="A95">
         <v>94</v>
       </c>
@@ -9111,7 +9346,7 @@
         <v>427</v>
       </c>
     </row>
-    <row ht="12.75" r="96" spans="1:8">
+    <row r="96" spans="1:8" ht="12.75">
       <c r="A96">
         <v>95</v>
       </c>
@@ -9134,7 +9369,7 @@
         <v>427</v>
       </c>
     </row>
-    <row ht="12.75" r="97" spans="1:8">
+    <row r="97" spans="1:8" ht="12.75">
       <c r="A97">
         <v>96</v>
       </c>
@@ -9157,7 +9392,7 @@
         <v>38</v>
       </c>
     </row>
-    <row ht="12.75" r="98" spans="1:8">
+    <row r="98" spans="1:8" ht="12.75">
       <c r="A98">
         <v>97</v>
       </c>
@@ -9180,7 +9415,7 @@
         <v>428</v>
       </c>
     </row>
-    <row ht="12.75" r="99" spans="1:8">
+    <row r="99" spans="1:8" ht="12.75">
       <c r="A99">
         <v>98</v>
       </c>
@@ -9203,7 +9438,7 @@
         <v>427</v>
       </c>
     </row>
-    <row ht="12.75" r="100" spans="1:8">
+    <row r="100" spans="1:8" ht="12.75">
       <c r="A100">
         <v>99</v>
       </c>
@@ -9226,7 +9461,7 @@
         <v>38</v>
       </c>
     </row>
-    <row ht="12.75" r="101" spans="1:8">
+    <row r="101" spans="1:8" ht="12.75">
       <c r="A101">
         <v>100</v>
       </c>
@@ -9249,7 +9484,7 @@
         <v>428</v>
       </c>
     </row>
-    <row ht="12.75" r="102" spans="1:8">
+    <row r="102" spans="1:8" ht="12.75">
       <c r="A102">
         <v>101</v>
       </c>
@@ -9272,7 +9507,7 @@
         <v>38</v>
       </c>
     </row>
-    <row ht="12.75" r="103" spans="1:8">
+    <row r="103" spans="1:8" ht="12.75">
       <c r="A103">
         <v>102</v>
       </c>
@@ -9295,7 +9530,7 @@
         <v>428</v>
       </c>
     </row>
-    <row ht="12.75" r="104" spans="1:8">
+    <row r="104" spans="1:8" ht="12.75">
       <c r="A104">
         <v>103</v>
       </c>
@@ -9318,7 +9553,7 @@
         <v>38</v>
       </c>
     </row>
-    <row ht="12.75" r="105" spans="1:8">
+    <row r="105" spans="1:8" ht="12.75">
       <c r="A105">
         <v>104</v>
       </c>
@@ -9341,7 +9576,7 @@
         <v>38</v>
       </c>
     </row>
-    <row ht="12.75" r="106" spans="1:8">
+    <row r="106" spans="1:8" ht="12.75">
       <c r="A106">
         <v>105</v>
       </c>
@@ -9364,7 +9599,7 @@
         <v>38</v>
       </c>
     </row>
-    <row ht="12.75" r="107" spans="1:8">
+    <row r="107" spans="1:8" ht="12.75">
       <c r="A107">
         <v>106</v>
       </c>
@@ -9387,7 +9622,7 @@
         <v>427</v>
       </c>
     </row>
-    <row ht="12.75" r="108" spans="1:8">
+    <row r="108" spans="1:8" ht="12.75">
       <c r="A108">
         <v>107</v>
       </c>
@@ -9410,7 +9645,7 @@
         <v>38</v>
       </c>
     </row>
-    <row ht="12.75" r="109" spans="1:8">
+    <row r="109" spans="1:8" ht="12.75">
       <c r="A109">
         <v>108</v>
       </c>
@@ -9433,7 +9668,7 @@
         <v>38</v>
       </c>
     </row>
-    <row ht="12.75" r="110" spans="1:8">
+    <row r="110" spans="1:8" ht="12.75">
       <c r="A110">
         <v>109</v>
       </c>
@@ -9456,7 +9691,7 @@
         <v>428</v>
       </c>
     </row>
-    <row ht="12.75" r="111" spans="1:8">
+    <row r="111" spans="1:8" ht="12.75">
       <c r="A111">
         <v>110</v>
       </c>
@@ -9479,7 +9714,7 @@
         <v>428</v>
       </c>
     </row>
-    <row ht="12.75" r="112" spans="1:8">
+    <row r="112" spans="1:8" ht="12.75">
       <c r="A112">
         <v>111</v>
       </c>
@@ -9502,7 +9737,7 @@
         <v>428</v>
       </c>
     </row>
-    <row ht="12.75" r="113" spans="1:8">
+    <row r="113" spans="1:8" ht="12.75">
       <c r="A113">
         <v>112</v>
       </c>
@@ -9525,7 +9760,7 @@
         <v>428</v>
       </c>
     </row>
-    <row ht="12.75" r="114" spans="1:8">
+    <row r="114" spans="1:8" ht="12.75">
       <c r="A114">
         <v>113</v>
       </c>
@@ -9548,7 +9783,7 @@
         <v>427</v>
       </c>
     </row>
-    <row ht="12.75" r="115" spans="1:8">
+    <row r="115" spans="1:8" ht="12.75">
       <c r="A115">
         <v>114</v>
       </c>
@@ -9565,13 +9800,13 @@
         <v>686</v>
       </c>
       <c r="G115" t="s">
-        <v>325</v>
+        <v>1192</v>
       </c>
       <c r="H115" t="s">
         <v>323</v>
       </c>
     </row>
-    <row ht="12.75" r="116" spans="1:8">
+    <row r="116" spans="1:8" ht="12.75">
       <c r="A116">
         <v>115</v>
       </c>
@@ -9594,7 +9829,7 @@
         <v>427</v>
       </c>
     </row>
-    <row ht="12.75" r="117" spans="1:8">
+    <row r="117" spans="1:8" ht="12.75">
       <c r="A117">
         <v>116</v>
       </c>
@@ -9617,7 +9852,7 @@
         <v>428</v>
       </c>
     </row>
-    <row ht="12.75" r="118" spans="1:8">
+    <row r="118" spans="1:8" ht="12.75">
       <c r="A118">
         <v>117</v>
       </c>
@@ -9637,7 +9872,7 @@
         <v>38</v>
       </c>
     </row>
-    <row ht="12.75" r="119" spans="1:8">
+    <row r="119" spans="1:8" ht="12.75">
       <c r="A119">
         <v>118</v>
       </c>
@@ -9660,7 +9895,7 @@
         <v>428</v>
       </c>
     </row>
-    <row customHeight="1" ht="15.75" r="120" spans="1:8">
+    <row r="120" spans="1:8" ht="15.75" customHeight="1">
       <c r="A120">
         <v>119</v>
       </c>
@@ -9683,7 +9918,7 @@
         <v>881</v>
       </c>
     </row>
-    <row ht="12.75" r="121" spans="1:8">
+    <row r="121" spans="1:8" ht="12.75">
       <c r="A121">
         <v>120</v>
       </c>
@@ -9706,7 +9941,7 @@
         <v>881</v>
       </c>
     </row>
-    <row ht="12.75" r="122" spans="1:8">
+    <row r="122" spans="1:8" ht="12.75">
       <c r="A122">
         <v>121</v>
       </c>
@@ -9729,7 +9964,7 @@
         <v>881</v>
       </c>
     </row>
-    <row ht="12.75" r="123" spans="1:8">
+    <row r="123" spans="1:8" ht="12.75">
       <c r="A123">
         <v>122</v>
       </c>
@@ -9752,7 +9987,7 @@
         <v>881</v>
       </c>
     </row>
-    <row ht="12.75" r="124" spans="1:8">
+    <row r="124" spans="1:8" ht="12.75">
       <c r="A124">
         <v>123</v>
       </c>
@@ -9775,7 +10010,7 @@
         <v>881</v>
       </c>
     </row>
-    <row ht="12.75" r="125" spans="1:8">
+    <row r="125" spans="1:8" ht="12.75">
       <c r="A125">
         <v>124</v>
       </c>
@@ -9798,7 +10033,7 @@
         <v>881</v>
       </c>
     </row>
-    <row ht="12.75" r="126" spans="1:8">
+    <row r="126" spans="1:8" ht="12.75">
       <c r="A126">
         <v>125</v>
       </c>
@@ -9821,7 +10056,7 @@
         <v>881</v>
       </c>
     </row>
-    <row ht="12.75" r="127" spans="1:8">
+    <row r="127" spans="1:8" ht="12.75">
       <c r="A127">
         <v>126</v>
       </c>
@@ -9844,7 +10079,7 @@
         <v>881</v>
       </c>
     </row>
-    <row ht="12.75" r="128" spans="1:8">
+    <row r="128" spans="1:8" ht="12.75">
       <c r="A128">
         <v>127</v>
       </c>
@@ -9867,7 +10102,7 @@
         <v>881</v>
       </c>
     </row>
-    <row ht="12.75" r="129" spans="1:8">
+    <row r="129" spans="1:8" ht="12.75">
       <c r="A129">
         <v>128</v>
       </c>
@@ -9890,7 +10125,7 @@
         <v>881</v>
       </c>
     </row>
-    <row ht="12.75" r="130" spans="1:8">
+    <row r="130" spans="1:8" ht="12.75">
       <c r="A130">
         <v>129</v>
       </c>
@@ -9913,7 +10148,7 @@
         <v>881</v>
       </c>
     </row>
-    <row ht="12.75" r="131" spans="1:8">
+    <row r="131" spans="1:8" ht="12.75">
       <c r="A131">
         <v>130</v>
       </c>
@@ -9936,7 +10171,7 @@
         <v>881</v>
       </c>
     </row>
-    <row ht="12.75" r="132" spans="1:8">
+    <row r="132" spans="1:8" ht="12.75">
       <c r="A132">
         <v>131</v>
       </c>
@@ -9959,7 +10194,7 @@
         <v>881</v>
       </c>
     </row>
-    <row ht="12.75" r="133" spans="1:8">
+    <row r="133" spans="1:8" ht="12.75">
       <c r="A133">
         <v>132</v>
       </c>
@@ -9982,7 +10217,7 @@
         <v>881</v>
       </c>
     </row>
-    <row ht="12.75" r="134" spans="1:8">
+    <row r="134" spans="1:8" ht="12.75">
       <c r="A134">
         <v>133</v>
       </c>
@@ -9993,7 +10228,7 @@
         <v>1033</v>
       </c>
       <c r="D134" s="4" t="s">
-        <v>7</v>
+        <v>14</v>
       </c>
       <c r="F134" s="2" t="s">
         <v>687</v>
@@ -10005,7 +10240,7 @@
         <v>881</v>
       </c>
     </row>
-    <row ht="12.75" r="135" spans="1:8">
+    <row r="135" spans="1:8" ht="12.75">
       <c r="A135">
         <v>134</v>
       </c>
@@ -10028,7 +10263,7 @@
         <v>881</v>
       </c>
     </row>
-    <row ht="12.75" r="136" spans="1:8">
+    <row r="136" spans="1:8" ht="12.75">
       <c r="A136">
         <v>135</v>
       </c>
@@ -10051,7 +10286,7 @@
         <v>881</v>
       </c>
     </row>
-    <row ht="12.75" r="137" spans="1:8">
+    <row r="137" spans="1:8" ht="12.75">
       <c r="A137">
         <v>136</v>
       </c>
@@ -10074,7 +10309,7 @@
         <v>881</v>
       </c>
     </row>
-    <row ht="12.75" r="138" spans="1:8">
+    <row r="138" spans="1:8" ht="12.75">
       <c r="A138">
         <v>137</v>
       </c>
@@ -10097,7 +10332,7 @@
         <v>881</v>
       </c>
     </row>
-    <row ht="12.75" r="139" spans="1:8">
+    <row r="139" spans="1:8" ht="12.75">
       <c r="A139">
         <v>138</v>
       </c>
@@ -10120,7 +10355,7 @@
         <v>881</v>
       </c>
     </row>
-    <row ht="12.75" r="140" spans="1:8">
+    <row r="140" spans="1:8" ht="12.75">
       <c r="A140">
         <v>139</v>
       </c>
@@ -10143,7 +10378,7 @@
         <v>881</v>
       </c>
     </row>
-    <row ht="12.75" r="141" spans="1:8">
+    <row r="141" spans="1:8" ht="12.75">
       <c r="A141">
         <v>140</v>
       </c>
@@ -10166,7 +10401,7 @@
         <v>881</v>
       </c>
     </row>
-    <row ht="12.75" r="142" spans="1:8">
+    <row r="142" spans="1:8" ht="12.75">
       <c r="A142">
         <v>141</v>
       </c>
@@ -10189,7 +10424,7 @@
         <v>881</v>
       </c>
     </row>
-    <row ht="12.75" r="143" spans="1:8">
+    <row r="143" spans="1:8" ht="12.75">
       <c r="A143">
         <v>142</v>
       </c>
@@ -10212,7 +10447,7 @@
         <v>881</v>
       </c>
     </row>
-    <row ht="12.75" r="144" spans="1:8">
+    <row r="144" spans="1:8" ht="12.75">
       <c r="A144">
         <v>143</v>
       </c>
@@ -10235,7 +10470,7 @@
         <v>38</v>
       </c>
     </row>
-    <row ht="12.75" r="145" spans="1:8">
+    <row r="145" spans="1:8" ht="12.75">
       <c r="A145">
         <v>144</v>
       </c>
@@ -10258,7 +10493,7 @@
         <v>428</v>
       </c>
     </row>
-    <row ht="12.75" r="146" spans="1:8">
+    <row r="146" spans="1:8" ht="12.75">
       <c r="A146">
         <v>145</v>
       </c>
@@ -10281,7 +10516,7 @@
         <v>427</v>
       </c>
     </row>
-    <row ht="12.75" r="147" spans="1:8">
+    <row r="147" spans="1:8" ht="12.75">
       <c r="A147">
         <v>146</v>
       </c>
@@ -10304,7 +10539,7 @@
         <v>38</v>
       </c>
     </row>
-    <row ht="12.75" r="148" spans="1:8">
+    <row r="148" spans="1:8" ht="12.75">
       <c r="A148">
         <v>147</v>
       </c>
@@ -10327,7 +10562,7 @@
         <v>881</v>
       </c>
     </row>
-    <row ht="12.75" r="149" spans="1:8">
+    <row r="149" spans="1:8" ht="12.75">
       <c r="A149">
         <v>148</v>
       </c>
@@ -10350,7 +10585,7 @@
         <v>881</v>
       </c>
     </row>
-    <row ht="12.75" r="150" spans="1:8">
+    <row r="150" spans="1:8" ht="12.75">
       <c r="A150">
         <v>149</v>
       </c>
@@ -10373,7 +10608,7 @@
         <v>881</v>
       </c>
     </row>
-    <row ht="12.75" r="151" spans="1:8">
+    <row r="151" spans="1:8" ht="12.75">
       <c r="A151">
         <v>150</v>
       </c>
@@ -10396,7 +10631,7 @@
         <v>427</v>
       </c>
     </row>
-    <row ht="12.75" r="152" spans="1:8">
+    <row r="152" spans="1:8" ht="12.75">
       <c r="A152">
         <v>151</v>
       </c>
@@ -10419,7 +10654,7 @@
         <v>881</v>
       </c>
     </row>
-    <row ht="12.75" r="153" spans="1:8">
+    <row r="153" spans="1:8" ht="12.75">
       <c r="A153">
         <v>152</v>
       </c>
@@ -10442,7 +10677,7 @@
         <v>881</v>
       </c>
     </row>
-    <row ht="12.75" r="154" spans="1:8">
+    <row r="154" spans="1:8" ht="12.75">
       <c r="A154">
         <v>153</v>
       </c>
@@ -10465,7 +10700,7 @@
         <v>427</v>
       </c>
     </row>
-    <row ht="12.75" r="155" spans="1:8">
+    <row r="155" spans="1:8" ht="12.75">
       <c r="A155">
         <v>154</v>
       </c>
@@ -10485,7 +10720,7 @@
         <v>38</v>
       </c>
     </row>
-    <row ht="12.75" r="156" spans="1:8">
+    <row r="156" spans="1:8" ht="12.75">
       <c r="A156">
         <v>155</v>
       </c>
@@ -10508,7 +10743,7 @@
         <v>881</v>
       </c>
     </row>
-    <row ht="12.75" r="157" spans="1:8">
+    <row r="157" spans="1:8" ht="12.75">
       <c r="A157">
         <v>156</v>
       </c>
@@ -10528,7 +10763,7 @@
         <v>881</v>
       </c>
     </row>
-    <row ht="12.75" r="158" spans="1:8">
+    <row r="158" spans="1:8" ht="12.75">
       <c r="A158">
         <v>157</v>
       </c>
@@ -10551,7 +10786,7 @@
         <v>428</v>
       </c>
     </row>
-    <row ht="12.75" r="159" spans="1:8">
+    <row r="159" spans="1:8" ht="12.75">
       <c r="A159">
         <v>158</v>
       </c>
@@ -10559,10 +10794,10 @@
         <v>1148</v>
       </c>
       <c r="C159" t="s">
-        <v>1165</v>
-      </c>
-      <c r="D159" s="46" t="s">
-        <v>1164</v>
+        <v>1162</v>
+      </c>
+      <c r="D159" s="4" t="s">
+        <v>7</v>
       </c>
       <c r="F159" s="2" t="s">
         <v>687</v>
@@ -10574,18 +10809,18 @@
         <v>881</v>
       </c>
     </row>
-    <row ht="12.75" r="160" spans="1:8">
+    <row r="160" spans="1:8" ht="12.75">
       <c r="A160">
         <v>159</v>
       </c>
-      <c r="B160" t="s">
+      <c r="B160" s="41" t="s">
         <v>1149</v>
       </c>
       <c r="C160" t="s">
-        <v>1166</v>
-      </c>
-      <c r="D160" s="47" t="s">
-        <v>1164</v>
+        <v>1163</v>
+      </c>
+      <c r="D160" s="4" t="s">
+        <v>7</v>
       </c>
       <c r="F160" s="2" t="s">
         <v>687</v>
@@ -10597,248 +10832,341 @@
         <v>428</v>
       </c>
     </row>
+    <row r="161" spans="1:8" ht="12.75">
+      <c r="A161">
+        <v>160</v>
+      </c>
+      <c r="B161" t="s">
+        <v>1165</v>
+      </c>
+      <c r="C161" t="s">
+        <v>1193</v>
+      </c>
+      <c r="D161" s="46" t="s">
+        <v>1188</v>
+      </c>
+      <c r="F161" s="2" t="s">
+        <v>1046</v>
+      </c>
+      <c r="G161" t="s">
+        <v>1192</v>
+      </c>
+      <c r="H161" t="s">
+        <v>323</v>
+      </c>
+    </row>
+    <row r="162" spans="1:8" ht="12.75">
+      <c r="A162">
+        <v>161</v>
+      </c>
+      <c r="B162" t="s">
+        <v>1166</v>
+      </c>
+      <c r="C162" t="s">
+        <v>1189</v>
+      </c>
+      <c r="D162" s="47" t="s">
+        <v>1188</v>
+      </c>
+      <c r="F162" s="2" t="s">
+        <v>687</v>
+      </c>
+      <c r="G162" t="s">
+        <v>1044</v>
+      </c>
+      <c r="H162" t="s">
+        <v>881</v>
+      </c>
+    </row>
+    <row r="163" spans="1:8" ht="12.75">
+      <c r="A163">
+        <v>162</v>
+      </c>
+      <c r="B163" t="s">
+        <v>1167</v>
+      </c>
+      <c r="C163" t="s">
+        <v>1190</v>
+      </c>
+      <c r="D163" s="47" t="s">
+        <v>1188</v>
+      </c>
+      <c r="F163" s="2" t="s">
+        <v>687</v>
+      </c>
+      <c r="G163" t="s">
+        <v>1044</v>
+      </c>
+      <c r="H163" t="s">
+        <v>881</v>
+      </c>
+    </row>
+    <row r="164" spans="1:8" ht="12.75">
+      <c r="A164">
+        <v>163</v>
+      </c>
+      <c r="B164" t="s">
+        <v>1168</v>
+      </c>
+      <c r="C164" t="s">
+        <v>1191</v>
+      </c>
+      <c r="D164" s="47" t="s">
+        <v>1188</v>
+      </c>
+      <c r="F164" s="2" t="s">
+        <v>687</v>
+      </c>
+      <c r="G164" t="s">
+        <v>1044</v>
+      </c>
+      <c r="H164" t="s">
+        <v>881</v>
+      </c>
+    </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink r:id="rId1" ref="B2" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
-    <hyperlink r:id="rId2" ref="B3" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
-    <hyperlink r:id="rId3" ref="B4" xr:uid="{00000000-0004-0000-0000-000002000000}"/>
-    <hyperlink r:id="rId4" ref="B5" xr:uid="{00000000-0004-0000-0000-000003000000}"/>
-    <hyperlink r:id="rId5" ref="B6" xr:uid="{00000000-0004-0000-0000-000004000000}"/>
-    <hyperlink r:id="rId6" ref="H6" xr:uid="{00000000-0004-0000-0000-000005000000}"/>
-    <hyperlink r:id="rId7" ref="B7" xr:uid="{00000000-0004-0000-0000-000006000000}"/>
-    <hyperlink r:id="rId8" ref="B8" xr:uid="{00000000-0004-0000-0000-000007000000}"/>
-    <hyperlink r:id="rId9" ref="B9" xr:uid="{00000000-0004-0000-0000-000008000000}"/>
-    <hyperlink r:id="rId10" ref="B10" xr:uid="{00000000-0004-0000-0000-000009000000}"/>
-    <hyperlink r:id="rId11" ref="B11" xr:uid="{00000000-0004-0000-0000-00000A000000}"/>
-    <hyperlink r:id="rId12" ref="B12" xr:uid="{00000000-0004-0000-0000-00000B000000}"/>
-    <hyperlink r:id="rId13" ref="B13" xr:uid="{00000000-0004-0000-0000-00000C000000}"/>
-    <hyperlink r:id="rId14" ref="B14" xr:uid="{00000000-0004-0000-0000-00000D000000}"/>
-    <hyperlink r:id="rId15" ref="B15" xr:uid="{00000000-0004-0000-0000-00000E000000}"/>
-    <hyperlink r:id="rId16" ref="B16" xr:uid="{00000000-0004-0000-0000-00000F000000}"/>
-    <hyperlink r:id="rId17" ref="B17" xr:uid="{00000000-0004-0000-0000-000010000000}"/>
-    <hyperlink r:id="rId18" ref="B18" xr:uid="{00000000-0004-0000-0000-000011000000}"/>
-    <hyperlink r:id="rId19" ref="B19" xr:uid="{00000000-0004-0000-0000-000012000000}"/>
-    <hyperlink r:id="rId20" ref="B20" xr:uid="{00000000-0004-0000-0000-000013000000}"/>
-    <hyperlink r:id="rId21" ref="B21" xr:uid="{00000000-0004-0000-0000-000014000000}"/>
-    <hyperlink r:id="rId22" ref="B22" xr:uid="{00000000-0004-0000-0000-000015000000}"/>
-    <hyperlink r:id="rId23" ref="B23" xr:uid="{00000000-0004-0000-0000-000016000000}"/>
-    <hyperlink r:id="rId24" ref="B24" xr:uid="{00000000-0004-0000-0000-000017000000}"/>
-    <hyperlink r:id="rId25" ref="B25" xr:uid="{00000000-0004-0000-0000-000018000000}"/>
-    <hyperlink r:id="rId26" ref="H25" xr:uid="{00000000-0004-0000-0000-000019000000}"/>
-    <hyperlink r:id="rId27" ref="B26" xr:uid="{00000000-0004-0000-0000-00001A000000}"/>
-    <hyperlink r:id="rId28" ref="H26" xr:uid="{00000000-0004-0000-0000-00001B000000}"/>
-    <hyperlink r:id="rId29" ref="B27" xr:uid="{00000000-0004-0000-0000-00001C000000}"/>
-    <hyperlink r:id="rId30" ref="H27" xr:uid="{00000000-0004-0000-0000-00001D000000}"/>
-    <hyperlink r:id="rId31" ref="B28" xr:uid="{00000000-0004-0000-0000-00001E000000}"/>
-    <hyperlink r:id="rId32" ref="H28" xr:uid="{00000000-0004-0000-0000-00001F000000}"/>
-    <hyperlink r:id="rId33" ref="B29" xr:uid="{00000000-0004-0000-0000-000020000000}"/>
-    <hyperlink r:id="rId34" ref="H29" xr:uid="{00000000-0004-0000-0000-000021000000}"/>
-    <hyperlink r:id="rId35" ref="B30" xr:uid="{00000000-0004-0000-0000-000022000000}"/>
-    <hyperlink r:id="rId36" ref="H30" xr:uid="{00000000-0004-0000-0000-000023000000}"/>
-    <hyperlink r:id="rId37" ref="B31" xr:uid="{00000000-0004-0000-0000-000024000000}"/>
-    <hyperlink r:id="rId38" ref="H31" xr:uid="{00000000-0004-0000-0000-000025000000}"/>
-    <hyperlink r:id="rId39" ref="B32" xr:uid="{00000000-0004-0000-0000-000026000000}"/>
-    <hyperlink r:id="rId40" ref="H32" xr:uid="{00000000-0004-0000-0000-000027000000}"/>
-    <hyperlink r:id="rId41" ref="B33" xr:uid="{00000000-0004-0000-0000-000028000000}"/>
-    <hyperlink r:id="rId42" ref="B34" xr:uid="{00000000-0004-0000-0000-000029000000}"/>
-    <hyperlink r:id="rId43" ref="B38" xr:uid="{00000000-0004-0000-0000-00002A000000}"/>
-    <hyperlink r:id="rId44" ref="B45" xr:uid="{00000000-0004-0000-0000-00002B000000}"/>
-    <hyperlink r:id="rId45" ref="B48" xr:uid="{00000000-0004-0000-0000-00002C000000}"/>
-    <hyperlink r:id="rId46" ref="B35" xr:uid="{00000000-0004-0000-0000-00002D000000}"/>
-    <hyperlink r:id="rId47" ref="B52" xr:uid="{00000000-0004-0000-0000-00002E000000}"/>
-    <hyperlink r:id="rId48" ref="B53" xr:uid="{00000000-0004-0000-0000-00002F000000}"/>
-    <hyperlink r:id="rId49" ref="B55" xr:uid="{00000000-0004-0000-0000-000030000000}"/>
-    <hyperlink r:id="rId50" ref="B56" xr:uid="{00000000-0004-0000-0000-000031000000}"/>
-    <hyperlink r:id="rId51" ref="B57" xr:uid="{00000000-0004-0000-0000-000032000000}"/>
-    <hyperlink r:id="rId52" ref="B58" xr:uid="{00000000-0004-0000-0000-000033000000}"/>
-    <hyperlink r:id="rId53" ref="B61" xr:uid="{00000000-0004-0000-0000-000034000000}"/>
-    <hyperlink r:id="rId54" ref="B62" xr:uid="{00000000-0004-0000-0000-000035000000}"/>
-    <hyperlink r:id="rId55" ref="B63" xr:uid="{00000000-0004-0000-0000-000036000000}"/>
-    <hyperlink r:id="rId56" ref="B64" xr:uid="{00000000-0004-0000-0000-000037000000}"/>
-    <hyperlink r:id="rId57" ref="B65" xr:uid="{00000000-0004-0000-0000-000038000000}"/>
-    <hyperlink r:id="rId58" ref="B66" xr:uid="{00000000-0004-0000-0000-000039000000}"/>
-    <hyperlink r:id="rId59" ref="B67" xr:uid="{00000000-0004-0000-0000-00003A000000}"/>
-    <hyperlink display="https://www.allhomes.com.au/agency/trusted-realtors-570129/" r:id="rId60" ref="H7:H24" xr:uid="{00000000-0004-0000-0000-00003B000000}"/>
-    <hyperlink r:id="rId61" ref="B43" xr:uid="{00000000-0004-0000-0000-00003C000000}"/>
-    <hyperlink r:id="rId62" ref="B44" xr:uid="{00000000-0004-0000-0000-00003D000000}"/>
-    <hyperlink r:id="rId63" ref="B46" xr:uid="{00000000-0004-0000-0000-00003E000000}"/>
-    <hyperlink r:id="rId64" ref="B54" xr:uid="{00000000-0004-0000-0000-00003F000000}"/>
-    <hyperlink r:id="rId65" ref="B42" xr:uid="{00000000-0004-0000-0000-000040000000}"/>
-    <hyperlink r:id="rId66" ref="J2" xr:uid="{00000000-0004-0000-0000-000041000000}"/>
-    <hyperlink r:id="rId67" ref="C69" xr:uid="{9DAE03A7-93E8-4507-BD6C-AC4013ECD47F}"/>
-    <hyperlink r:id="rId68" ref="C68" xr:uid="{66B9A9CA-DF82-46B6-9C5A-C5709E2FF1AE}"/>
-    <hyperlink r:id="rId69" ref="B75" xr:uid="{57E7BFEF-6F05-4DA9-A3DE-5B0A0EFED4D9}"/>
-    <hyperlink r:id="rId70" ref="C75" xr:uid="{F4755F93-6E59-4C38-BF66-16746869FDF3}"/>
-    <hyperlink r:id="rId71" ref="H75" xr:uid="{5BFAFD71-42C4-487F-B5E7-1697975992B4}"/>
-    <hyperlink r:id="rId72" ref="B78" xr:uid="{D3DE0D76-2479-4283-B7C7-F11B85797022}"/>
-    <hyperlink r:id="rId73" ref="C78" xr:uid="{FC1D9146-2FDC-4F13-A3C3-51CAB46DEC08}"/>
-    <hyperlink r:id="rId74" ref="B68" xr:uid="{3ED6FAA1-2B0F-4DB9-878E-9640A9C2850D}"/>
-    <hyperlink r:id="rId75" ref="B69" xr:uid="{12DE6CA8-DDC5-4E7B-BD2E-14B105A0DE3B}"/>
-    <hyperlink r:id="rId76" ref="C70" xr:uid="{0419758C-286A-4B76-B8B2-31CC336DEDF1}"/>
-    <hyperlink r:id="rId77" ref="B70" xr:uid="{AC18D1D2-FA3D-4352-A402-35B7AAFE27C0}"/>
-    <hyperlink r:id="rId78" ref="B71" xr:uid="{E8BCA1EF-4E17-4AA7-A2CE-5674FC05ABC3}"/>
-    <hyperlink r:id="rId79" ref="C71" xr:uid="{949AE606-DF4A-48F4-93A0-F148D80842CB}"/>
-    <hyperlink r:id="rId80" ref="B72" xr:uid="{69A93BB5-0295-46D6-8334-45444356E6E9}"/>
-    <hyperlink r:id="rId81" ref="C72" xr:uid="{CA171BC7-126F-4175-8A03-123D5A2C2D8A}"/>
-    <hyperlink r:id="rId82" ref="C73" xr:uid="{FACC205D-E563-4266-8E0D-0794F3D76E98}"/>
-    <hyperlink r:id="rId83" ref="B85" xr:uid="{7ABCABC0-A765-435B-AE52-9D27F653E00F}"/>
-    <hyperlink r:id="rId84" ref="C4" xr:uid="{2CD58DBE-98E3-4EDC-898F-088D5F0FCB81}"/>
-    <hyperlink r:id="rId85" ref="C29" xr:uid="{CB7CAD83-ACA3-4309-B102-B0F536FC97E6}"/>
-    <hyperlink r:id="rId86" ref="C90" xr:uid="{B4F55488-2B40-4078-ABF0-4B4254363237}"/>
-    <hyperlink r:id="rId87" ref="B90" xr:uid="{09FEE7FE-E667-40E8-BC22-3FDC999B614F}"/>
-    <hyperlink r:id="rId88" ref="C15" xr:uid="{34F25BA9-B460-46CF-85C0-4AC9D6288B41}"/>
-    <hyperlink r:id="rId89" ref="C3" xr:uid="{EBAAEE7A-83B2-457B-8600-89427BF11448}"/>
-    <hyperlink r:id="rId90" ref="C8" xr:uid="{3D3D678C-8F1B-47BC-ACA2-D1CBF5A76F0B}"/>
-    <hyperlink r:id="rId91" ref="C19" xr:uid="{ED2C9A9B-3440-4B4A-91A1-7CAF84972535}"/>
-    <hyperlink r:id="rId92" ref="C20" xr:uid="{E47C999F-11AE-4F93-9032-6E51EB582635}"/>
-    <hyperlink r:id="rId93" ref="C21" xr:uid="{E59411CC-EC13-4665-969A-8D9238CCD0C2}"/>
-    <hyperlink r:id="rId94" ref="C33" xr:uid="{9C953AB9-0076-4477-B52F-C393846B1211}"/>
-    <hyperlink r:id="rId95" ref="C38" xr:uid="{D349EA20-36BF-44C7-A16B-E85B8FE53B2A}"/>
-    <hyperlink r:id="rId96" ref="C39" xr:uid="{DE18DA3B-1A3D-4613-888E-7F506CC87091}"/>
-    <hyperlink r:id="rId97" ref="C40" xr:uid="{0C71282B-049B-4CD1-A090-B66647F2B29B}"/>
-    <hyperlink r:id="rId98" ref="C42" xr:uid="{AD0DC851-DEC5-4ACE-B928-50149068BB70}"/>
-    <hyperlink r:id="rId99" ref="C45" xr:uid="{EB51DFC2-D28F-4E0C-B019-F9954D6C9832}"/>
-    <hyperlink r:id="rId100" ref="C52" xr:uid="{9E5146F6-8EC8-4A2C-B192-C1CCB11CAB8A}"/>
-    <hyperlink r:id="rId101" ref="C48" xr:uid="{31B308E4-DA3E-401B-B796-7D03404228FB}"/>
-    <hyperlink r:id="rId102" ref="C49" xr:uid="{EBAAB9CE-7F91-4628-AF75-32C4EEF948C2}"/>
-    <hyperlink r:id="rId103" ref="C53" xr:uid="{2FF7EB1F-CD56-4E71-AD0F-0D12E8347603}"/>
-    <hyperlink r:id="rId104" ref="C55" xr:uid="{9BD44DCD-EEBB-4649-9792-F3DAC40B3960}"/>
-    <hyperlink r:id="rId105" ref="C63" xr:uid="{9929BCF4-32FD-4143-99F6-FEB21B90BCD7}"/>
-    <hyperlink r:id="rId106" ref="C64" xr:uid="{80B3DEC9-506E-4F3A-B171-A2D71B731577}"/>
-    <hyperlink r:id="rId107" ref="C66" xr:uid="{011D2C70-C541-49D4-894E-FF670D6C19BB}"/>
-    <hyperlink r:id="rId108" ref="C67" xr:uid="{B62DFA3B-60A0-44AA-BF1D-BCA2A049E46C}"/>
-    <hyperlink r:id="rId109" ref="C56" xr:uid="{C98B5D5D-65AB-489D-8160-8F1B41CDE6A7}"/>
-    <hyperlink r:id="rId110" ref="B103" xr:uid="{4D81C408-B745-40E2-B9C7-6E36C45175A7}"/>
-    <hyperlink r:id="rId111" ref="C26" xr:uid="{6A9C6F44-3E7F-47CF-8514-B6609EBEE668}"/>
-    <hyperlink r:id="rId112" ref="C23" xr:uid="{F99F350A-C378-4940-B611-41F47BC3B4B0}"/>
-    <hyperlink r:id="rId113" ref="C103" xr:uid="{3E9C8DCE-ABC0-49DA-B64B-B569BAAE6ED0}"/>
-    <hyperlink r:id="rId114" ref="C104" xr:uid="{E96AA061-2DED-4A35-BE99-8E7E156527EB}"/>
-    <hyperlink r:id="rId115" ref="C102" xr:uid="{4DAA7E56-3BCD-4AF1-B6E7-A26B02A0DA6C}"/>
-    <hyperlink r:id="rId116" ref="C101" xr:uid="{EBE0EC7F-0880-4F4A-991C-2C7C53889923}"/>
-    <hyperlink r:id="rId117" ref="C100" xr:uid="{7AA4A2D0-C18F-4625-A776-6EDD2415E1BC}"/>
-    <hyperlink r:id="rId118" ref="C99" xr:uid="{15BFB680-4225-425B-8826-841A35922C8A}"/>
-    <hyperlink r:id="rId119" ref="B99" xr:uid="{1EF2BF94-D92B-41EF-8B1F-0585F1910B74}"/>
-    <hyperlink r:id="rId120" ref="C97" xr:uid="{6687C5A1-CC2B-49FF-B98D-946AA21B8C55}"/>
-    <hyperlink r:id="rId121" ref="B97" xr:uid="{0411E592-2DE8-4D1D-B66C-46CE99CAA412}"/>
-    <hyperlink r:id="rId122" ref="C96" xr:uid="{A7ED7210-DE23-4760-B67F-78027E9B9B73}"/>
-    <hyperlink r:id="rId123" ref="B96" xr:uid="{992F1752-E440-4347-A698-44C8E60F00BE}"/>
-    <hyperlink r:id="rId124" ref="B102" xr:uid="{A0E03FB2-010F-497D-874D-A0A66FB6303C}"/>
-    <hyperlink r:id="rId125" ref="B101" xr:uid="{165FBF6F-9195-42DA-AC37-C49B2308ACA1}"/>
-    <hyperlink r:id="rId126" ref="B94" xr:uid="{7DB2C8A6-8C43-4818-A7C2-D5E14351114B}"/>
-    <hyperlink r:id="rId127" ref="B93" xr:uid="{EFC122F7-44E7-447B-8F21-BA1503A72780}"/>
-    <hyperlink r:id="rId128" ref="B91" xr:uid="{7AC22E1D-6919-43E6-AD91-1551DBBDE570}"/>
-    <hyperlink r:id="rId129" ref="B88" xr:uid="{FB3E9840-E4E3-4E64-8CCF-2BAEC7024AD6}"/>
-    <hyperlink r:id="rId130" ref="B87" xr:uid="{348337ED-A616-4A9D-A8D3-0091262177C6}"/>
-    <hyperlink r:id="rId131" ref="B86" xr:uid="{CF62843D-4B82-47CB-B74F-D3F292E9603A}"/>
-    <hyperlink r:id="rId132" ref="B84" xr:uid="{9CA10EFF-3943-479E-914B-1D6EE04D75FC}"/>
-    <hyperlink r:id="rId133" ref="C84" xr:uid="{1074AAC9-CCB0-4FFC-9AFB-EFD1363D7538}"/>
-    <hyperlink r:id="rId134" ref="B105" xr:uid="{D6DE2797-5A68-4C1E-9E74-0D323B6ADFA2}"/>
-    <hyperlink r:id="rId135" ref="B106" xr:uid="{1FCAF9BA-00B5-4008-B5C8-E822ABD6BCDD}"/>
-    <hyperlink r:id="rId136" ref="C11" xr:uid="{893B2404-B185-41F7-B397-A3E08B386C5F}"/>
-    <hyperlink r:id="rId137" ref="B107" xr:uid="{B0E609F4-D8A3-433A-BE15-17E4804C6EA3}"/>
-    <hyperlink r:id="rId138" ref="C107" xr:uid="{6793ECA4-A034-42EC-A741-3B0FF42BC11B}"/>
-    <hyperlink r:id="rId139" ref="B108" xr:uid="{4DB78F44-0F08-4561-A0E8-0EE92F9FFECB}"/>
-    <hyperlink r:id="rId140" ref="B114" xr:uid="{27750164-38B8-4B5E-9B5A-E6C71FFFC61F}"/>
-    <hyperlink r:id="rId141" ref="C114" xr:uid="{6FE6A043-A6B1-44FF-8A45-8C3690323458}"/>
-    <hyperlink r:id="rId142" ref="B113" xr:uid="{0F94FF41-1E06-4D7B-B360-1EB377073C87}"/>
-    <hyperlink r:id="rId143" ref="B112" xr:uid="{490A5044-10EC-4082-BEC1-14008171D5CF}"/>
-    <hyperlink r:id="rId144" ref="B49" xr:uid="{836EB236-8BF1-4259-B395-AD9FA9DE0AE0}"/>
-    <hyperlink r:id="rId145" ref="B74" xr:uid="{8AA8904A-1CC5-4D06-93EF-66F7FC625199}"/>
-    <hyperlink r:id="rId146" ref="B76" xr:uid="{5743888C-C74A-41C6-ABC5-E9575351702D}"/>
-    <hyperlink r:id="rId147" ref="B115" xr:uid="{27BDB583-8AD0-4B33-BA19-24E42C9E7CE9}"/>
-    <hyperlink r:id="rId148" ref="B117" xr:uid="{92BA6213-0D94-4C5A-B06A-6FC35C0BECA9}"/>
-    <hyperlink r:id="rId149" ref="B119" xr:uid="{6724AE23-65F5-4D67-ADA6-E20BD420531B}"/>
-    <hyperlink r:id="rId150" ref="C119" xr:uid="{0A5009EB-B388-4AF4-99CE-5813711C2B1E}"/>
-    <hyperlink r:id="rId151" ref="B120" xr:uid="{255CB59B-E711-471E-8ACE-D0ABA408AE96}"/>
-    <hyperlink r:id="rId152" ref="B39" xr:uid="{39FB4A7C-4EA8-4530-9FE6-2842C777350C}"/>
-    <hyperlink r:id="rId153" ref="B104" xr:uid="{FC8A6FB5-FCCF-409E-9D6D-A93D412B2275}"/>
-    <hyperlink r:id="rId154" ref="C105" xr:uid="{988B91BF-CEBD-44F6-A773-3C87D877BE5A}"/>
-    <hyperlink r:id="rId155" ref="C108" xr:uid="{F0593E1B-3EE0-4DF2-B93E-84A02071630B}"/>
-    <hyperlink r:id="rId156" ref="B109" xr:uid="{601C40E0-818B-457C-9FE7-30D06707CEB7}"/>
-    <hyperlink r:id="rId157" ref="C109" xr:uid="{E1D93474-1A3D-49F1-B191-3C3484679D2D}"/>
-    <hyperlink r:id="rId158" ref="C83" xr:uid="{B0D57129-C33F-45FF-B844-E7642495443D}"/>
-    <hyperlink r:id="rId159" ref="B83" xr:uid="{7DCBF3E6-0CD2-475D-AE1F-56469491B512}"/>
-    <hyperlink r:id="rId160" ref="C120" xr:uid="{F24698EA-BA1A-4C92-8B6D-72A40DDDD7A3}"/>
-    <hyperlink r:id="rId161" ref="C122" xr:uid="{BAC9069D-9D63-415D-B933-A4F86CB8C587}"/>
-    <hyperlink r:id="rId162" ref="C123" xr:uid="{140A866C-FAC2-4A61-BA7E-0AFB9A05FD2F}"/>
-    <hyperlink r:id="rId163" ref="C124" xr:uid="{6EA83FA2-D552-4B23-98A9-6C5EFC3BC2CA}"/>
-    <hyperlink r:id="rId164" ref="C125" xr:uid="{E34375AF-4BB2-420C-887F-8D684FC72F4C}"/>
-    <hyperlink r:id="rId165" ref="C126" xr:uid="{CB74A187-1404-4E3B-B1EF-E6C50CF09D3E}"/>
-    <hyperlink r:id="rId166" ref="C127" xr:uid="{B0565FA3-8BDF-4E3B-9814-B9F51432FA7D}"/>
-    <hyperlink r:id="rId167" ref="C128" xr:uid="{8504A7CE-7DD9-4C74-83D8-90E0745EAB21}"/>
-    <hyperlink r:id="rId168" ref="C130" xr:uid="{D3DDF4DA-6F84-4EAF-BA60-77D926C7C2AC}"/>
-    <hyperlink r:id="rId169" ref="C131" xr:uid="{060B4F44-BF89-4037-9E74-C61E23C6AAC9}"/>
-    <hyperlink r:id="rId170" ref="C132" xr:uid="{8FD9E395-82BD-4EEA-89E9-166FDA928F87}"/>
-    <hyperlink r:id="rId171" ref="C133" xr:uid="{3669E93D-A9CE-4C72-B1DD-98E95312A18C}"/>
-    <hyperlink r:id="rId172" ref="C136" xr:uid="{E14EBE84-3FBA-44D8-B082-69967148B456}"/>
-    <hyperlink r:id="rId173" ref="C137" xr:uid="{CC0D1827-F782-476A-9312-1BAA88B7D496}"/>
-    <hyperlink r:id="rId174" ref="C141" xr:uid="{1528B515-167A-4838-B645-B63CD0312C05}"/>
-    <hyperlink r:id="rId175" ref="B143" xr:uid="{50B775B1-8A20-4A55-90CA-EC152D3C2098}"/>
-    <hyperlink r:id="rId176" ref="B144" xr:uid="{F6EFF9E5-8AC0-4C40-A2A8-62DF9BB671E9}"/>
-    <hyperlink r:id="rId177" ref="C145" xr:uid="{DE56B3AC-2F1A-494E-A9CD-9C972DA863E2}"/>
-    <hyperlink r:id="rId178" ref="B145" xr:uid="{F783979B-F441-49BC-98C4-8448098CBBC1}"/>
-    <hyperlink r:id="rId179" ref="C17" xr:uid="{DBE3D417-C525-4AE7-BA26-A27F8BD7B6D3}"/>
-    <hyperlink r:id="rId180" ref="B121" xr:uid="{BF1CBD80-282B-4284-A960-458EE8D86966}"/>
-    <hyperlink r:id="rId181" ref="C146" xr:uid="{3FA9DCB7-198C-457D-99E0-AF0A29EDEAF1}"/>
-    <hyperlink r:id="rId182" ref="B146" xr:uid="{6B057403-173E-478A-AFE1-5BA96D6006F7}"/>
-    <hyperlink r:id="rId183" ref="C147" xr:uid="{FBD8EA4A-7B80-4D87-BD4D-6D3DDE043E14}"/>
-    <hyperlink r:id="rId184" ref="B147" xr:uid="{F9D4FD4A-592C-4041-AD52-AAD4E4FECD78}"/>
-    <hyperlink r:id="rId185" ref="C148" xr:uid="{EF3F39F0-4058-49A5-8980-E800B6F200B5}"/>
-    <hyperlink r:id="rId186" ref="B148" xr:uid="{513D1B27-06CF-4F01-AD66-B1DDDB3DF171}"/>
-    <hyperlink r:id="rId187" ref="C149" xr:uid="{BFCDD610-AD9F-445C-AAE8-66DB3CD722A6}"/>
-    <hyperlink r:id="rId188" ref="B149" xr:uid="{1567BEF7-2918-4A3A-89A1-A37D6C6B5419}"/>
-    <hyperlink r:id="rId189" ref="B150" xr:uid="{233679EA-F519-4185-AA17-F008EE8DA109}"/>
-    <hyperlink r:id="rId190" ref="C153" xr:uid="{D979C888-F3D2-4FAE-9C96-C32136017BEF}"/>
-    <hyperlink r:id="rId191" ref="B153" xr:uid="{F7FA0B04-B8E5-4470-AA22-DE86ABDF6874}"/>
-    <hyperlink r:id="rId192" ref="C93" xr:uid="{0FE1A0D7-D827-4F54-A7B7-45C810922AB8}"/>
-    <hyperlink r:id="rId193" ref="H94" xr:uid="{119834D6-06DC-4C3A-A3DB-668C11E66CDD}"/>
-    <hyperlink r:id="rId194" ref="B157" xr:uid="{476413B0-EB8B-4009-A520-C52327E9DB14}"/>
-    <hyperlink r:id="rId195" ref="B158" xr:uid="{E393AAFE-C1C9-42C1-82B6-E0BF95C57871}"/>
-    <hyperlink r:id="rId196" ref="B154" xr:uid="{6ACA5AA2-08BB-438D-AA2D-656B3CF595C8}"/>
-    <hyperlink r:id="rId197" ref="B155" xr:uid="{09BFA21C-B573-43CD-A621-D848720D45A2}"/>
-    <hyperlink r:id="rId198" ref="B156" xr:uid="{64BD9576-B17E-4000-AF00-7BFD7270B1E0}"/>
-    <hyperlink r:id="rId199" ref="C154" xr:uid="{D6D76F32-CF66-4AA4-86D5-70A2337B29C6}"/>
+    <hyperlink ref="B2" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
+    <hyperlink ref="B3" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
+    <hyperlink ref="B4" r:id="rId3" xr:uid="{00000000-0004-0000-0000-000002000000}"/>
+    <hyperlink ref="B5" r:id="rId4" xr:uid="{00000000-0004-0000-0000-000003000000}"/>
+    <hyperlink ref="B6" r:id="rId5" xr:uid="{00000000-0004-0000-0000-000004000000}"/>
+    <hyperlink ref="H6" r:id="rId6" xr:uid="{00000000-0004-0000-0000-000005000000}"/>
+    <hyperlink ref="B7" r:id="rId7" xr:uid="{00000000-0004-0000-0000-000006000000}"/>
+    <hyperlink ref="B8" r:id="rId8" xr:uid="{00000000-0004-0000-0000-000007000000}"/>
+    <hyperlink ref="B9" r:id="rId9" xr:uid="{00000000-0004-0000-0000-000008000000}"/>
+    <hyperlink ref="B10" r:id="rId10" xr:uid="{00000000-0004-0000-0000-000009000000}"/>
+    <hyperlink ref="B11" r:id="rId11" xr:uid="{00000000-0004-0000-0000-00000A000000}"/>
+    <hyperlink ref="B12" r:id="rId12" xr:uid="{00000000-0004-0000-0000-00000B000000}"/>
+    <hyperlink ref="B13" r:id="rId13" xr:uid="{00000000-0004-0000-0000-00000C000000}"/>
+    <hyperlink ref="B14" r:id="rId14" xr:uid="{00000000-0004-0000-0000-00000D000000}"/>
+    <hyperlink ref="B15" r:id="rId15" xr:uid="{00000000-0004-0000-0000-00000E000000}"/>
+    <hyperlink ref="B16" r:id="rId16" xr:uid="{00000000-0004-0000-0000-00000F000000}"/>
+    <hyperlink ref="B17" r:id="rId17" xr:uid="{00000000-0004-0000-0000-000010000000}"/>
+    <hyperlink ref="B18" r:id="rId18" xr:uid="{00000000-0004-0000-0000-000011000000}"/>
+    <hyperlink ref="B19" r:id="rId19" xr:uid="{00000000-0004-0000-0000-000012000000}"/>
+    <hyperlink ref="B20" r:id="rId20" xr:uid="{00000000-0004-0000-0000-000013000000}"/>
+    <hyperlink ref="B21" r:id="rId21" xr:uid="{00000000-0004-0000-0000-000014000000}"/>
+    <hyperlink ref="B22" r:id="rId22" xr:uid="{00000000-0004-0000-0000-000015000000}"/>
+    <hyperlink ref="B23" r:id="rId23" xr:uid="{00000000-0004-0000-0000-000016000000}"/>
+    <hyperlink ref="B24" r:id="rId24" xr:uid="{00000000-0004-0000-0000-000017000000}"/>
+    <hyperlink ref="B25" r:id="rId25" xr:uid="{00000000-0004-0000-0000-000018000000}"/>
+    <hyperlink ref="H25" r:id="rId26" xr:uid="{00000000-0004-0000-0000-000019000000}"/>
+    <hyperlink ref="B26" r:id="rId27" xr:uid="{00000000-0004-0000-0000-00001A000000}"/>
+    <hyperlink ref="H26" r:id="rId28" xr:uid="{00000000-0004-0000-0000-00001B000000}"/>
+    <hyperlink ref="B27" r:id="rId29" xr:uid="{00000000-0004-0000-0000-00001C000000}"/>
+    <hyperlink ref="H27" r:id="rId30" xr:uid="{00000000-0004-0000-0000-00001D000000}"/>
+    <hyperlink ref="B28" r:id="rId31" xr:uid="{00000000-0004-0000-0000-00001E000000}"/>
+    <hyperlink ref="H28" r:id="rId32" xr:uid="{00000000-0004-0000-0000-00001F000000}"/>
+    <hyperlink ref="B29" r:id="rId33" xr:uid="{00000000-0004-0000-0000-000020000000}"/>
+    <hyperlink ref="H29" r:id="rId34" xr:uid="{00000000-0004-0000-0000-000021000000}"/>
+    <hyperlink ref="B30" r:id="rId35" xr:uid="{00000000-0004-0000-0000-000022000000}"/>
+    <hyperlink ref="H30" r:id="rId36" xr:uid="{00000000-0004-0000-0000-000023000000}"/>
+    <hyperlink ref="B31" r:id="rId37" xr:uid="{00000000-0004-0000-0000-000024000000}"/>
+    <hyperlink ref="H31" r:id="rId38" xr:uid="{00000000-0004-0000-0000-000025000000}"/>
+    <hyperlink ref="B32" r:id="rId39" xr:uid="{00000000-0004-0000-0000-000026000000}"/>
+    <hyperlink ref="H32" r:id="rId40" xr:uid="{00000000-0004-0000-0000-000027000000}"/>
+    <hyperlink ref="B33" r:id="rId41" xr:uid="{00000000-0004-0000-0000-000028000000}"/>
+    <hyperlink ref="B34" r:id="rId42" xr:uid="{00000000-0004-0000-0000-000029000000}"/>
+    <hyperlink ref="B38" r:id="rId43" xr:uid="{00000000-0004-0000-0000-00002A000000}"/>
+    <hyperlink ref="B45" r:id="rId44" xr:uid="{00000000-0004-0000-0000-00002B000000}"/>
+    <hyperlink ref="B48" r:id="rId45" xr:uid="{00000000-0004-0000-0000-00002C000000}"/>
+    <hyperlink ref="B35" r:id="rId46" xr:uid="{00000000-0004-0000-0000-00002D000000}"/>
+    <hyperlink ref="B52" r:id="rId47" xr:uid="{00000000-0004-0000-0000-00002E000000}"/>
+    <hyperlink ref="B53" r:id="rId48" xr:uid="{00000000-0004-0000-0000-00002F000000}"/>
+    <hyperlink ref="B55" r:id="rId49" xr:uid="{00000000-0004-0000-0000-000030000000}"/>
+    <hyperlink ref="B56" r:id="rId50" xr:uid="{00000000-0004-0000-0000-000031000000}"/>
+    <hyperlink ref="B57" r:id="rId51" xr:uid="{00000000-0004-0000-0000-000032000000}"/>
+    <hyperlink ref="B58" r:id="rId52" xr:uid="{00000000-0004-0000-0000-000033000000}"/>
+    <hyperlink ref="B61" r:id="rId53" xr:uid="{00000000-0004-0000-0000-000034000000}"/>
+    <hyperlink ref="B62" r:id="rId54" xr:uid="{00000000-0004-0000-0000-000035000000}"/>
+    <hyperlink ref="B63" r:id="rId55" xr:uid="{00000000-0004-0000-0000-000036000000}"/>
+    <hyperlink ref="B64" r:id="rId56" xr:uid="{00000000-0004-0000-0000-000037000000}"/>
+    <hyperlink ref="B65" r:id="rId57" xr:uid="{00000000-0004-0000-0000-000038000000}"/>
+    <hyperlink ref="B66" r:id="rId58" xr:uid="{00000000-0004-0000-0000-000039000000}"/>
+    <hyperlink ref="B67" r:id="rId59" xr:uid="{00000000-0004-0000-0000-00003A000000}"/>
+    <hyperlink ref="H7:H24" r:id="rId60" display="https://www.allhomes.com.au/agency/trusted-realtors-570129/" xr:uid="{00000000-0004-0000-0000-00003B000000}"/>
+    <hyperlink ref="B43" r:id="rId61" xr:uid="{00000000-0004-0000-0000-00003C000000}"/>
+    <hyperlink ref="B44" r:id="rId62" xr:uid="{00000000-0004-0000-0000-00003D000000}"/>
+    <hyperlink ref="B46" r:id="rId63" xr:uid="{00000000-0004-0000-0000-00003E000000}"/>
+    <hyperlink ref="B54" r:id="rId64" xr:uid="{00000000-0004-0000-0000-00003F000000}"/>
+    <hyperlink ref="B42" r:id="rId65" xr:uid="{00000000-0004-0000-0000-000040000000}"/>
+    <hyperlink ref="J2" r:id="rId66" xr:uid="{00000000-0004-0000-0000-000041000000}"/>
+    <hyperlink ref="C69" r:id="rId67" xr:uid="{9DAE03A7-93E8-4507-BD6C-AC4013ECD47F}"/>
+    <hyperlink ref="C68" r:id="rId68" xr:uid="{66B9A9CA-DF82-46B6-9C5A-C5709E2FF1AE}"/>
+    <hyperlink ref="B75" r:id="rId69" xr:uid="{57E7BFEF-6F05-4DA9-A3DE-5B0A0EFED4D9}"/>
+    <hyperlink ref="C75" r:id="rId70" xr:uid="{F4755F93-6E59-4C38-BF66-16746869FDF3}"/>
+    <hyperlink ref="H75" r:id="rId71" xr:uid="{5BFAFD71-42C4-487F-B5E7-1697975992B4}"/>
+    <hyperlink ref="B78" r:id="rId72" xr:uid="{D3DE0D76-2479-4283-B7C7-F11B85797022}"/>
+    <hyperlink ref="C78" r:id="rId73" xr:uid="{FC1D9146-2FDC-4F13-A3C3-51CAB46DEC08}"/>
+    <hyperlink ref="B68" r:id="rId74" xr:uid="{3ED6FAA1-2B0F-4DB9-878E-9640A9C2850D}"/>
+    <hyperlink ref="B69" r:id="rId75" xr:uid="{12DE6CA8-DDC5-4E7B-BD2E-14B105A0DE3B}"/>
+    <hyperlink ref="C70" r:id="rId76" xr:uid="{0419758C-286A-4B76-B8B2-31CC336DEDF1}"/>
+    <hyperlink ref="B70" r:id="rId77" xr:uid="{AC18D1D2-FA3D-4352-A402-35B7AAFE27C0}"/>
+    <hyperlink ref="B71" r:id="rId78" xr:uid="{E8BCA1EF-4E17-4AA7-A2CE-5674FC05ABC3}"/>
+    <hyperlink ref="C71" r:id="rId79" xr:uid="{949AE606-DF4A-48F4-93A0-F148D80842CB}"/>
+    <hyperlink ref="B72" r:id="rId80" xr:uid="{69A93BB5-0295-46D6-8334-45444356E6E9}"/>
+    <hyperlink ref="C72" r:id="rId81" xr:uid="{CA171BC7-126F-4175-8A03-123D5A2C2D8A}"/>
+    <hyperlink ref="C73" r:id="rId82" xr:uid="{FACC205D-E563-4266-8E0D-0794F3D76E98}"/>
+    <hyperlink ref="B85" r:id="rId83" xr:uid="{7ABCABC0-A765-435B-AE52-9D27F653E00F}"/>
+    <hyperlink ref="C4" r:id="rId84" xr:uid="{2CD58DBE-98E3-4EDC-898F-088D5F0FCB81}"/>
+    <hyperlink ref="C29" r:id="rId85" xr:uid="{CB7CAD83-ACA3-4309-B102-B0F536FC97E6}"/>
+    <hyperlink ref="C90" r:id="rId86" xr:uid="{B4F55488-2B40-4078-ABF0-4B4254363237}"/>
+    <hyperlink ref="B90" r:id="rId87" xr:uid="{09FEE7FE-E667-40E8-BC22-3FDC999B614F}"/>
+    <hyperlink ref="C15" r:id="rId88" xr:uid="{34F25BA9-B460-46CF-85C0-4AC9D6288B41}"/>
+    <hyperlink ref="C3" r:id="rId89" xr:uid="{EBAAEE7A-83B2-457B-8600-89427BF11448}"/>
+    <hyperlink ref="C8" r:id="rId90" xr:uid="{3D3D678C-8F1B-47BC-ACA2-D1CBF5A76F0B}"/>
+    <hyperlink ref="C19" r:id="rId91" xr:uid="{ED2C9A9B-3440-4B4A-91A1-7CAF84972535}"/>
+    <hyperlink ref="C20" r:id="rId92" xr:uid="{E47C999F-11AE-4F93-9032-6E51EB582635}"/>
+    <hyperlink ref="C21" r:id="rId93" xr:uid="{E59411CC-EC13-4665-969A-8D9238CCD0C2}"/>
+    <hyperlink ref="C33" r:id="rId94" xr:uid="{9C953AB9-0076-4477-B52F-C393846B1211}"/>
+    <hyperlink ref="C38" r:id="rId95" xr:uid="{D349EA20-36BF-44C7-A16B-E85B8FE53B2A}"/>
+    <hyperlink ref="C39" r:id="rId96" xr:uid="{DE18DA3B-1A3D-4613-888E-7F506CC87091}"/>
+    <hyperlink ref="C40" r:id="rId97" xr:uid="{0C71282B-049B-4CD1-A090-B66647F2B29B}"/>
+    <hyperlink ref="C42" r:id="rId98" xr:uid="{AD0DC851-DEC5-4ACE-B928-50149068BB70}"/>
+    <hyperlink ref="C45" r:id="rId99" xr:uid="{EB51DFC2-D28F-4E0C-B019-F9954D6C9832}"/>
+    <hyperlink ref="C52" r:id="rId100" xr:uid="{9E5146F6-8EC8-4A2C-B192-C1CCB11CAB8A}"/>
+    <hyperlink ref="C48" r:id="rId101" xr:uid="{31B308E4-DA3E-401B-B796-7D03404228FB}"/>
+    <hyperlink ref="C49" r:id="rId102" xr:uid="{EBAAB9CE-7F91-4628-AF75-32C4EEF948C2}"/>
+    <hyperlink ref="C53" r:id="rId103" xr:uid="{2FF7EB1F-CD56-4E71-AD0F-0D12E8347603}"/>
+    <hyperlink ref="C55" r:id="rId104" xr:uid="{9BD44DCD-EEBB-4649-9792-F3DAC40B3960}"/>
+    <hyperlink ref="C63" r:id="rId105" xr:uid="{9929BCF4-32FD-4143-99F6-FEB21B90BCD7}"/>
+    <hyperlink ref="C64" r:id="rId106" xr:uid="{80B3DEC9-506E-4F3A-B171-A2D71B731577}"/>
+    <hyperlink ref="C66" r:id="rId107" xr:uid="{011D2C70-C541-49D4-894E-FF670D6C19BB}"/>
+    <hyperlink ref="C67" r:id="rId108" xr:uid="{B62DFA3B-60A0-44AA-BF1D-BCA2A049E46C}"/>
+    <hyperlink ref="C56" r:id="rId109" xr:uid="{C98B5D5D-65AB-489D-8160-8F1B41CDE6A7}"/>
+    <hyperlink ref="B103" r:id="rId110" xr:uid="{4D81C408-B745-40E2-B9C7-6E36C45175A7}"/>
+    <hyperlink ref="C26" r:id="rId111" xr:uid="{6A9C6F44-3E7F-47CF-8514-B6609EBEE668}"/>
+    <hyperlink ref="C23" r:id="rId112" xr:uid="{F99F350A-C378-4940-B611-41F47BC3B4B0}"/>
+    <hyperlink ref="C103" r:id="rId113" xr:uid="{3E9C8DCE-ABC0-49DA-B64B-B569BAAE6ED0}"/>
+    <hyperlink ref="C104" r:id="rId114" xr:uid="{E96AA061-2DED-4A35-BE99-8E7E156527EB}"/>
+    <hyperlink ref="C102" r:id="rId115" xr:uid="{4DAA7E56-3BCD-4AF1-B6E7-A26B02A0DA6C}"/>
+    <hyperlink ref="C101" r:id="rId116" xr:uid="{EBE0EC7F-0880-4F4A-991C-2C7C53889923}"/>
+    <hyperlink ref="C100" r:id="rId117" xr:uid="{7AA4A2D0-C18F-4625-A776-6EDD2415E1BC}"/>
+    <hyperlink ref="C99" r:id="rId118" xr:uid="{15BFB680-4225-425B-8826-841A35922C8A}"/>
+    <hyperlink ref="B99" r:id="rId119" xr:uid="{1EF2BF94-D92B-41EF-8B1F-0585F1910B74}"/>
+    <hyperlink ref="C97" r:id="rId120" xr:uid="{6687C5A1-CC2B-49FF-B98D-946AA21B8C55}"/>
+    <hyperlink ref="B97" r:id="rId121" xr:uid="{0411E592-2DE8-4D1D-B66C-46CE99CAA412}"/>
+    <hyperlink ref="C96" r:id="rId122" xr:uid="{A7ED7210-DE23-4760-B67F-78027E9B9B73}"/>
+    <hyperlink ref="B96" r:id="rId123" xr:uid="{992F1752-E440-4347-A698-44C8E60F00BE}"/>
+    <hyperlink ref="B102" r:id="rId124" xr:uid="{A0E03FB2-010F-497D-874D-A0A66FB6303C}"/>
+    <hyperlink ref="B101" r:id="rId125" xr:uid="{165FBF6F-9195-42DA-AC37-C49B2308ACA1}"/>
+    <hyperlink ref="B94" r:id="rId126" xr:uid="{7DB2C8A6-8C43-4818-A7C2-D5E14351114B}"/>
+    <hyperlink ref="B93" r:id="rId127" xr:uid="{EFC122F7-44E7-447B-8F21-BA1503A72780}"/>
+    <hyperlink ref="B91" r:id="rId128" xr:uid="{7AC22E1D-6919-43E6-AD91-1551DBBDE570}"/>
+    <hyperlink ref="B88" r:id="rId129" xr:uid="{FB3E9840-E4E3-4E64-8CCF-2BAEC7024AD6}"/>
+    <hyperlink ref="B87" r:id="rId130" xr:uid="{348337ED-A616-4A9D-A8D3-0091262177C6}"/>
+    <hyperlink ref="B86" r:id="rId131" xr:uid="{CF62843D-4B82-47CB-B74F-D3F292E9603A}"/>
+    <hyperlink ref="B84" r:id="rId132" xr:uid="{9CA10EFF-3943-479E-914B-1D6EE04D75FC}"/>
+    <hyperlink ref="C84" r:id="rId133" xr:uid="{1074AAC9-CCB0-4FFC-9AFB-EFD1363D7538}"/>
+    <hyperlink ref="B105" r:id="rId134" xr:uid="{D6DE2797-5A68-4C1E-9E74-0D323B6ADFA2}"/>
+    <hyperlink ref="B106" r:id="rId135" xr:uid="{1FCAF9BA-00B5-4008-B5C8-E822ABD6BCDD}"/>
+    <hyperlink ref="C11" r:id="rId136" xr:uid="{893B2404-B185-41F7-B397-A3E08B386C5F}"/>
+    <hyperlink ref="B107" r:id="rId137" xr:uid="{B0E609F4-D8A3-433A-BE15-17E4804C6EA3}"/>
+    <hyperlink ref="C107" r:id="rId138" xr:uid="{6793ECA4-A034-42EC-A741-3B0FF42BC11B}"/>
+    <hyperlink ref="B108" r:id="rId139" xr:uid="{4DB78F44-0F08-4561-A0E8-0EE92F9FFECB}"/>
+    <hyperlink ref="B114" r:id="rId140" xr:uid="{27750164-38B8-4B5E-9B5A-E6C71FFFC61F}"/>
+    <hyperlink ref="C114" r:id="rId141" xr:uid="{6FE6A043-A6B1-44FF-8A45-8C3690323458}"/>
+    <hyperlink ref="B113" r:id="rId142" xr:uid="{0F94FF41-1E06-4D7B-B360-1EB377073C87}"/>
+    <hyperlink ref="B112" r:id="rId143" xr:uid="{490A5044-10EC-4082-BEC1-14008171D5CF}"/>
+    <hyperlink ref="B49" r:id="rId144" xr:uid="{836EB236-8BF1-4259-B395-AD9FA9DE0AE0}"/>
+    <hyperlink ref="B74" r:id="rId145" xr:uid="{8AA8904A-1CC5-4D06-93EF-66F7FC625199}"/>
+    <hyperlink ref="B76" r:id="rId146" xr:uid="{5743888C-C74A-41C6-ABC5-E9575351702D}"/>
+    <hyperlink ref="B115" r:id="rId147" xr:uid="{27BDB583-8AD0-4B33-BA19-24E42C9E7CE9}"/>
+    <hyperlink ref="B117" r:id="rId148" xr:uid="{92BA6213-0D94-4C5A-B06A-6FC35C0BECA9}"/>
+    <hyperlink ref="B119" r:id="rId149" xr:uid="{6724AE23-65F5-4D67-ADA6-E20BD420531B}"/>
+    <hyperlink ref="C119" r:id="rId150" xr:uid="{0A5009EB-B388-4AF4-99CE-5813711C2B1E}"/>
+    <hyperlink ref="B120" r:id="rId151" xr:uid="{255CB59B-E711-471E-8ACE-D0ABA408AE96}"/>
+    <hyperlink ref="B39" r:id="rId152" xr:uid="{39FB4A7C-4EA8-4530-9FE6-2842C777350C}"/>
+    <hyperlink ref="B104" r:id="rId153" xr:uid="{FC8A6FB5-FCCF-409E-9D6D-A93D412B2275}"/>
+    <hyperlink ref="C105" r:id="rId154" xr:uid="{988B91BF-CEBD-44F6-A773-3C87D877BE5A}"/>
+    <hyperlink ref="C108" r:id="rId155" xr:uid="{F0593E1B-3EE0-4DF2-B93E-84A02071630B}"/>
+    <hyperlink ref="B109" r:id="rId156" xr:uid="{601C40E0-818B-457C-9FE7-30D06707CEB7}"/>
+    <hyperlink ref="C109" r:id="rId157" xr:uid="{E1D93474-1A3D-49F1-B191-3C3484679D2D}"/>
+    <hyperlink ref="C83" r:id="rId158" xr:uid="{B0D57129-C33F-45FF-B844-E7642495443D}"/>
+    <hyperlink ref="B83" r:id="rId159" xr:uid="{7DCBF3E6-0CD2-475D-AE1F-56469491B512}"/>
+    <hyperlink ref="C120" r:id="rId160" xr:uid="{F24698EA-BA1A-4C92-8B6D-72A40DDDD7A3}"/>
+    <hyperlink ref="C122" r:id="rId161" xr:uid="{BAC9069D-9D63-415D-B933-A4F86CB8C587}"/>
+    <hyperlink ref="C123" r:id="rId162" xr:uid="{140A866C-FAC2-4A61-BA7E-0AFB9A05FD2F}"/>
+    <hyperlink ref="C124" r:id="rId163" xr:uid="{6EA83FA2-D552-4B23-98A9-6C5EFC3BC2CA}"/>
+    <hyperlink ref="C125" r:id="rId164" xr:uid="{E34375AF-4BB2-420C-887F-8D684FC72F4C}"/>
+    <hyperlink ref="C126" r:id="rId165" xr:uid="{CB74A187-1404-4E3B-B1EF-E6C50CF09D3E}"/>
+    <hyperlink ref="C127" r:id="rId166" xr:uid="{B0565FA3-8BDF-4E3B-9814-B9F51432FA7D}"/>
+    <hyperlink ref="C128" r:id="rId167" xr:uid="{8504A7CE-7DD9-4C74-83D8-90E0745EAB21}"/>
+    <hyperlink ref="C130" r:id="rId168" xr:uid="{D3DDF4DA-6F84-4EAF-BA60-77D926C7C2AC}"/>
+    <hyperlink ref="C131" r:id="rId169" xr:uid="{060B4F44-BF89-4037-9E74-C61E23C6AAC9}"/>
+    <hyperlink ref="C132" r:id="rId170" xr:uid="{8FD9E395-82BD-4EEA-89E9-166FDA928F87}"/>
+    <hyperlink ref="C133" r:id="rId171" xr:uid="{3669E93D-A9CE-4C72-B1DD-98E95312A18C}"/>
+    <hyperlink ref="C136" r:id="rId172" xr:uid="{E14EBE84-3FBA-44D8-B082-69967148B456}"/>
+    <hyperlink ref="C137" r:id="rId173" xr:uid="{CC0D1827-F782-476A-9312-1BAA88B7D496}"/>
+    <hyperlink ref="C141" r:id="rId174" xr:uid="{1528B515-167A-4838-B645-B63CD0312C05}"/>
+    <hyperlink ref="B143" r:id="rId175" xr:uid="{50B775B1-8A20-4A55-90CA-EC152D3C2098}"/>
+    <hyperlink ref="B144" r:id="rId176" xr:uid="{F6EFF9E5-8AC0-4C40-A2A8-62DF9BB671E9}"/>
+    <hyperlink ref="C145" r:id="rId177" xr:uid="{DE56B3AC-2F1A-494E-A9CD-9C972DA863E2}"/>
+    <hyperlink ref="B145" r:id="rId178" xr:uid="{F783979B-F441-49BC-98C4-8448098CBBC1}"/>
+    <hyperlink ref="C17" r:id="rId179" xr:uid="{DBE3D417-C525-4AE7-BA26-A27F8BD7B6D3}"/>
+    <hyperlink ref="B121" r:id="rId180" xr:uid="{BF1CBD80-282B-4284-A960-458EE8D86966}"/>
+    <hyperlink ref="C146" r:id="rId181" xr:uid="{3FA9DCB7-198C-457D-99E0-AF0A29EDEAF1}"/>
+    <hyperlink ref="B146" r:id="rId182" xr:uid="{6B057403-173E-478A-AFE1-5BA96D6006F7}"/>
+    <hyperlink ref="C147" r:id="rId183" xr:uid="{FBD8EA4A-7B80-4D87-BD4D-6D3DDE043E14}"/>
+    <hyperlink ref="B147" r:id="rId184" xr:uid="{F9D4FD4A-592C-4041-AD52-AAD4E4FECD78}"/>
+    <hyperlink ref="C148" r:id="rId185" xr:uid="{EF3F39F0-4058-49A5-8980-E800B6F200B5}"/>
+    <hyperlink ref="B148" r:id="rId186" xr:uid="{513D1B27-06CF-4F01-AD66-B1DDDB3DF171}"/>
+    <hyperlink ref="C149" r:id="rId187" xr:uid="{BFCDD610-AD9F-445C-AAE8-66DB3CD722A6}"/>
+    <hyperlink ref="B149" r:id="rId188" xr:uid="{1567BEF7-2918-4A3A-89A1-A37D6C6B5419}"/>
+    <hyperlink ref="B150" r:id="rId189" xr:uid="{233679EA-F519-4185-AA17-F008EE8DA109}"/>
+    <hyperlink ref="C153" r:id="rId190" xr:uid="{D979C888-F3D2-4FAE-9C96-C32136017BEF}"/>
+    <hyperlink ref="B153" r:id="rId191" xr:uid="{F7FA0B04-B8E5-4470-AA22-DE86ABDF6874}"/>
+    <hyperlink ref="C93" r:id="rId192" xr:uid="{0FE1A0D7-D827-4F54-A7B7-45C810922AB8}"/>
+    <hyperlink ref="H94" r:id="rId193" xr:uid="{119834D6-06DC-4C3A-A3DB-668C11E66CDD}"/>
+    <hyperlink ref="B157" r:id="rId194" xr:uid="{476413B0-EB8B-4009-A520-C52327E9DB14}"/>
+    <hyperlink ref="B158" r:id="rId195" xr:uid="{E393AAFE-C1C9-42C1-82B6-E0BF95C57871}"/>
+    <hyperlink ref="B154" r:id="rId196" xr:uid="{6ACA5AA2-08BB-438D-AA2D-656B3CF595C8}"/>
+    <hyperlink ref="B155" r:id="rId197" xr:uid="{09BFA21C-B573-43CD-A621-D848720D45A2}"/>
+    <hyperlink ref="B156" r:id="rId198" xr:uid="{64BD9576-B17E-4000-AF00-7BFD7270B1E0}"/>
+    <hyperlink ref="C154" r:id="rId199" xr:uid="{D6D76F32-CF66-4AA4-86D5-70A2337B29C6}"/>
+    <hyperlink ref="B160" r:id="rId200" xr:uid="{7D226E9C-99B6-4B8B-A61B-E8A9210EF4CD}"/>
   </hyperlinks>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
-  <pageSetup orientation="portrait" paperSize="9" r:id="rId200"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId201"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:AJ159"/>
+  <dimension ref="A1:AI163"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane activePane="bottomLeft" state="frozen" topLeftCell="A143" ySplit="1"/>
-      <selection activeCell="C156" pane="bottomLeft" sqref="C156"/>
+      <pane ySplit="1" topLeftCell="A134" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="W165" sqref="W165"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="14.42578125" defaultRowHeight="15.75"/>
+  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="14.85546875" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="18.140625" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" width="55.5703125" collapsed="true"/>
-    <col min="4" max="4" customWidth="true" width="25.140625" collapsed="true"/>
-    <col min="5" max="5" customWidth="true" width="19.5703125" collapsed="true"/>
-    <col min="6" max="6" customWidth="true" width="19.85546875" collapsed="true"/>
-    <col min="7" max="7" customWidth="true" width="18.5703125" collapsed="true"/>
-    <col min="8" max="8" customWidth="true" width="32.140625" collapsed="true"/>
-    <col min="9" max="9" customWidth="true" width="20.5703125" collapsed="true"/>
-    <col min="10" max="10" customWidth="true" width="21.140625" collapsed="true"/>
-    <col min="11" max="11" customWidth="true" width="28.85546875" collapsed="true"/>
-    <col min="12" max="12" customWidth="true" width="37.5703125" collapsed="true"/>
-    <col min="16" max="17" customWidth="true" width="18.85546875" collapsed="true"/>
-    <col min="18" max="18" customWidth="true" width="47.85546875" collapsed="true"/>
-    <col min="19" max="19" customWidth="true" width="77.5703125" collapsed="true"/>
-    <col min="20" max="20" customWidth="true" width="24.0" collapsed="true"/>
-    <col min="21" max="21" customWidth="true" width="18.85546875" collapsed="true"/>
-    <col min="22" max="31" customWidth="true" width="19.140625" collapsed="true"/>
+    <col min="1" max="1" width="14.85546875" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="18.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="55.5703125" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="25.140625" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="19.5703125" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="19.85546875" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="18.5703125" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="32.140625" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="20.5703125" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="21.140625" customWidth="1" collapsed="1"/>
+    <col min="11" max="11" width="28.85546875" customWidth="1" collapsed="1"/>
+    <col min="12" max="12" width="37.5703125" customWidth="1" collapsed="1"/>
+    <col min="16" max="17" width="18.85546875" customWidth="1" collapsed="1"/>
+    <col min="18" max="18" width="47.85546875" customWidth="1" collapsed="1"/>
+    <col min="19" max="19" width="77.5703125" customWidth="1" collapsed="1"/>
+    <col min="20" max="20" width="24" customWidth="1" collapsed="1"/>
+    <col min="21" max="21" width="18.85546875" customWidth="1" collapsed="1"/>
+    <col min="22" max="31" width="19.140625" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row ht="30" r="1" spans="1:35">
+    <row r="1" spans="1:35" ht="30">
       <c r="A1" s="1" t="s">
         <v>46</v>
       </c>
@@ -10937,7 +11265,7 @@
       <c r="AH1" s="23"/>
       <c r="AI1" s="23"/>
     </row>
-    <row customHeight="1" ht="15" r="2" spans="1:35">
+    <row r="2" spans="1:35" ht="15" customHeight="1">
       <c r="A2" s="24">
         <v>1</v>
       </c>
@@ -11008,7 +11336,7 @@
       <c r="AH2" s="24"/>
       <c r="AI2" s="24"/>
     </row>
-    <row customHeight="1" ht="15" r="3" spans="1:35">
+    <row r="3" spans="1:35" ht="15" customHeight="1">
       <c r="A3" s="24">
         <v>2</v>
       </c>
@@ -11079,7 +11407,7 @@
       <c r="AH3" s="24"/>
       <c r="AI3" s="24"/>
     </row>
-    <row customFormat="1" customHeight="1" ht="15" r="4" s="24" spans="1:35">
+    <row r="4" spans="1:35" s="24" customFormat="1" ht="15" customHeight="1">
       <c r="A4" s="24">
         <v>3</v>
       </c>
@@ -11141,7 +11469,7 @@
         <v>8</v>
       </c>
     </row>
-    <row customHeight="1" ht="15" r="5" spans="1:35">
+    <row r="5" spans="1:35" ht="15" customHeight="1">
       <c r="A5" s="24">
         <v>4</v>
       </c>
@@ -11214,7 +11542,7 @@
       <c r="AH5" s="24"/>
       <c r="AI5" s="24"/>
     </row>
-    <row customFormat="1" customHeight="1" ht="15" r="6" s="24" spans="1:35">
+    <row r="6" spans="1:35" s="24" customFormat="1" ht="15" customHeight="1">
       <c r="A6" s="24">
         <v>5</v>
       </c>
@@ -11273,7 +11601,7 @@
         <v>16</v>
       </c>
     </row>
-    <row customFormat="1" customHeight="1" ht="15" r="7" s="24" spans="1:35">
+    <row r="7" spans="1:35" s="24" customFormat="1" ht="15" customHeight="1">
       <c r="A7" s="24">
         <v>6</v>
       </c>
@@ -11332,7 +11660,7 @@
         <v>16</v>
       </c>
     </row>
-    <row customFormat="1" customHeight="1" ht="15" r="8" s="24" spans="1:35">
+    <row r="8" spans="1:35" s="24" customFormat="1" ht="15" customHeight="1">
       <c r="A8" s="24">
         <v>7</v>
       </c>
@@ -11388,7 +11716,7 @@
         <v>16</v>
       </c>
     </row>
-    <row customFormat="1" customHeight="1" ht="15" r="9" s="24" spans="1:35">
+    <row r="9" spans="1:35" s="24" customFormat="1" ht="15" customHeight="1">
       <c r="A9" s="24">
         <v>8</v>
       </c>
@@ -11447,7 +11775,7 @@
         <v>16</v>
       </c>
     </row>
-    <row customFormat="1" customHeight="1" ht="15" r="10" s="24" spans="1:35">
+    <row r="10" spans="1:35" s="24" customFormat="1" ht="15" customHeight="1">
       <c r="A10" s="24">
         <v>9</v>
       </c>
@@ -11503,7 +11831,7 @@
         <v>16</v>
       </c>
     </row>
-    <row customFormat="1" customHeight="1" ht="15" r="11" s="24" spans="1:35">
+    <row r="11" spans="1:35" s="24" customFormat="1" ht="15" customHeight="1">
       <c r="A11" s="24">
         <v>10</v>
       </c>
@@ -11568,7 +11896,7 @@
         <v>114</v>
       </c>
     </row>
-    <row customFormat="1" customHeight="1" ht="15" r="12" s="24" spans="1:35">
+    <row r="12" spans="1:35" s="24" customFormat="1" ht="15" customHeight="1">
       <c r="A12" s="24">
         <v>11</v>
       </c>
@@ -11624,7 +11952,7 @@
         <v>16</v>
       </c>
     </row>
-    <row customFormat="1" customHeight="1" ht="15" r="13" s="24" spans="1:35">
+    <row r="13" spans="1:35" s="24" customFormat="1" ht="15" customHeight="1">
       <c r="A13" s="24">
         <v>12</v>
       </c>
@@ -11683,7 +12011,7 @@
         <v>114</v>
       </c>
     </row>
-    <row customFormat="1" customHeight="1" ht="15" r="14" s="24" spans="1:35">
+    <row r="14" spans="1:35" s="24" customFormat="1" ht="15" customHeight="1">
       <c r="A14" s="24">
         <v>13</v>
       </c>
@@ -11748,7 +12076,7 @@
         <v>114</v>
       </c>
     </row>
-    <row customFormat="1" customHeight="1" ht="15" r="15" s="24" spans="1:35">
+    <row r="15" spans="1:35" s="24" customFormat="1" ht="15" customHeight="1">
       <c r="A15" s="24">
         <v>14</v>
       </c>
@@ -11807,7 +12135,7 @@
         <v>16</v>
       </c>
     </row>
-    <row customFormat="1" customHeight="1" ht="15" r="16" s="24" spans="1:35">
+    <row r="16" spans="1:35" s="24" customFormat="1" ht="15" customHeight="1">
       <c r="A16" s="24">
         <v>15</v>
       </c>
@@ -11866,7 +12194,7 @@
         <v>16</v>
       </c>
     </row>
-    <row customFormat="1" customHeight="1" ht="15" r="17" s="24" spans="1:35">
+    <row r="17" spans="1:35" s="24" customFormat="1" ht="15" customHeight="1">
       <c r="A17" s="24">
         <v>16</v>
       </c>
@@ -11922,7 +12250,7 @@
         <v>16</v>
       </c>
     </row>
-    <row customFormat="1" customHeight="1" ht="15" r="18" s="24" spans="1:35">
+    <row r="18" spans="1:35" s="24" customFormat="1" ht="15" customHeight="1">
       <c r="A18" s="24">
         <v>17</v>
       </c>
@@ -11981,7 +12309,7 @@
         <v>16</v>
       </c>
     </row>
-    <row customFormat="1" customHeight="1" ht="15" r="19" s="24" spans="1:35">
+    <row r="19" spans="1:35" s="24" customFormat="1" ht="15" customHeight="1">
       <c r="A19" s="24">
         <v>18</v>
       </c>
@@ -12037,7 +12365,7 @@
         <v>16</v>
       </c>
     </row>
-    <row customHeight="1" ht="15" r="20" spans="1:35">
+    <row r="20" spans="1:35" ht="15" customHeight="1">
       <c r="A20" s="24">
         <v>19</v>
       </c>
@@ -12112,7 +12440,7 @@
       <c r="AH20" s="24"/>
       <c r="AI20" s="24"/>
     </row>
-    <row customFormat="1" customHeight="1" ht="15" r="21" s="24" spans="1:35">
+    <row r="21" spans="1:35" s="24" customFormat="1" ht="15" customHeight="1">
       <c r="A21" s="24">
         <v>20</v>
       </c>
@@ -12168,7 +12496,7 @@
         <v>16</v>
       </c>
     </row>
-    <row customFormat="1" customHeight="1" ht="15" r="22" s="24" spans="1:35">
+    <row r="22" spans="1:35" s="24" customFormat="1" ht="15" customHeight="1">
       <c r="A22" s="24">
         <v>21</v>
       </c>
@@ -12233,7 +12561,7 @@
         <v>114</v>
       </c>
     </row>
-    <row customFormat="1" customHeight="1" ht="15" r="23" s="24" spans="1:35">
+    <row r="23" spans="1:35" s="24" customFormat="1" ht="15" customHeight="1">
       <c r="A23" s="24">
         <v>22</v>
       </c>
@@ -12286,7 +12614,7 @@
         <v>16</v>
       </c>
     </row>
-    <row customFormat="1" customHeight="1" ht="15" r="24" s="24" spans="1:35">
+    <row r="24" spans="1:35" s="24" customFormat="1" ht="15" customHeight="1">
       <c r="A24" s="24">
         <v>23</v>
       </c>
@@ -12345,7 +12673,7 @@
         <v>16</v>
       </c>
     </row>
-    <row customHeight="1" ht="15" r="25" spans="1:35">
+    <row r="25" spans="1:35" ht="15" customHeight="1">
       <c r="A25" s="24">
         <v>24</v>
       </c>
@@ -12416,7 +12744,7 @@
       <c r="AH25" s="24"/>
       <c r="AI25" s="24"/>
     </row>
-    <row customFormat="1" customHeight="1" ht="15" r="26" s="24" spans="1:35">
+    <row r="26" spans="1:35" s="24" customFormat="1" ht="15" customHeight="1">
       <c r="A26" s="24">
         <v>25</v>
       </c>
@@ -12475,7 +12803,7 @@
         <v>37</v>
       </c>
     </row>
-    <row customFormat="1" customHeight="1" ht="15" r="27" s="24" spans="1:35">
+    <row r="27" spans="1:35" s="24" customFormat="1" ht="15" customHeight="1">
       <c r="A27" s="24">
         <v>26</v>
       </c>
@@ -12534,7 +12862,7 @@
         <v>37</v>
       </c>
     </row>
-    <row customFormat="1" customHeight="1" ht="15" r="28" s="24" spans="1:35">
+    <row r="28" spans="1:35" s="24" customFormat="1" ht="15" customHeight="1">
       <c r="A28" s="24">
         <v>27</v>
       </c>
@@ -12593,7 +12921,7 @@
         <v>37</v>
       </c>
     </row>
-    <row customFormat="1" customHeight="1" ht="15" r="29" s="24" spans="1:35">
+    <row r="29" spans="1:35" s="24" customFormat="1" ht="15" customHeight="1">
       <c r="A29" s="24">
         <v>28</v>
       </c>
@@ -12652,7 +12980,7 @@
         <v>37</v>
       </c>
     </row>
-    <row customFormat="1" customHeight="1" ht="15" r="30" s="24" spans="1:35">
+    <row r="30" spans="1:35" s="24" customFormat="1" ht="15" customHeight="1">
       <c r="A30" s="24">
         <v>29</v>
       </c>
@@ -12711,7 +13039,7 @@
         <v>37</v>
       </c>
     </row>
-    <row customFormat="1" customHeight="1" ht="15" r="31" s="24" spans="1:35">
+    <row r="31" spans="1:35" s="24" customFormat="1" ht="15" customHeight="1">
       <c r="A31" s="24">
         <v>30</v>
       </c>
@@ -12767,7 +13095,7 @@
         <v>37</v>
       </c>
     </row>
-    <row customFormat="1" customHeight="1" ht="15" r="32" s="24" spans="1:35">
+    <row r="32" spans="1:35" s="24" customFormat="1" ht="15" customHeight="1">
       <c r="A32" s="24">
         <v>31</v>
       </c>
@@ -12826,7 +13154,7 @@
         <v>37</v>
       </c>
     </row>
-    <row customFormat="1" ht="14.25" r="33" s="24" spans="1:21">
+    <row r="33" spans="1:21" s="24" customFormat="1" ht="14.25">
       <c r="A33" s="24" t="s">
         <v>195</v>
       </c>
@@ -12885,7 +13213,7 @@
         <v>8</v>
       </c>
     </row>
-    <row customFormat="1" ht="14.25" r="34" s="24" spans="1:21">
+    <row r="34" spans="1:21" s="24" customFormat="1" ht="14.25">
       <c r="A34" s="24" t="s">
         <v>206</v>
       </c>
@@ -12944,7 +13272,7 @@
         <v>8</v>
       </c>
     </row>
-    <row customFormat="1" ht="14.25" r="35" s="24" spans="1:21">
+    <row r="35" spans="1:21" s="24" customFormat="1" ht="14.25">
       <c r="A35" s="24" t="s">
         <v>213</v>
       </c>
@@ -13003,7 +13331,7 @@
         <v>8</v>
       </c>
     </row>
-    <row customFormat="1" ht="14.25" r="36" s="24" spans="1:21">
+    <row r="36" spans="1:21" s="24" customFormat="1" ht="14.25">
       <c r="A36" s="24" t="s">
         <v>219</v>
       </c>
@@ -13062,7 +13390,7 @@
         <v>8</v>
       </c>
     </row>
-    <row customFormat="1" ht="14.25" r="37" s="24" spans="1:21">
+    <row r="37" spans="1:21" s="24" customFormat="1" ht="14.25">
       <c r="A37" s="24" t="s">
         <v>226</v>
       </c>
@@ -13121,7 +13449,7 @@
         <v>8</v>
       </c>
     </row>
-    <row customFormat="1" ht="14.25" r="38" s="24" spans="1:21">
+    <row r="38" spans="1:21" s="24" customFormat="1" ht="14.25">
       <c r="A38" s="24" t="s">
         <v>232</v>
       </c>
@@ -13180,7 +13508,7 @@
         <v>8</v>
       </c>
     </row>
-    <row customFormat="1" ht="14.25" r="39" s="24" spans="1:21">
+    <row r="39" spans="1:21" s="24" customFormat="1" ht="14.25">
       <c r="A39" s="24" t="s">
         <v>240</v>
       </c>
@@ -13239,7 +13567,7 @@
         <v>8</v>
       </c>
     </row>
-    <row customFormat="1" ht="14.25" r="40" s="24" spans="1:21">
+    <row r="40" spans="1:21" s="24" customFormat="1" ht="14.25">
       <c r="A40" s="24" t="s">
         <v>243</v>
       </c>
@@ -13298,7 +13626,7 @@
         <v>8</v>
       </c>
     </row>
-    <row customFormat="1" ht="14.25" r="41" s="24" spans="1:21">
+    <row r="41" spans="1:21" s="24" customFormat="1" ht="14.25">
       <c r="A41" s="24" t="s">
         <v>246</v>
       </c>
@@ -13357,7 +13685,7 @@
         <v>8</v>
       </c>
     </row>
-    <row customFormat="1" ht="14.25" r="42" s="24" spans="1:21">
+    <row r="42" spans="1:21" s="24" customFormat="1" ht="14.25">
       <c r="A42" s="24" t="s">
         <v>255</v>
       </c>
@@ -13416,7 +13744,7 @@
         <v>8</v>
       </c>
     </row>
-    <row customFormat="1" ht="14.25" r="43" s="24" spans="1:21">
+    <row r="43" spans="1:21" s="24" customFormat="1" ht="14.25">
       <c r="A43" s="24" t="s">
         <v>259</v>
       </c>
@@ -13475,7 +13803,7 @@
         <v>8</v>
       </c>
     </row>
-    <row customFormat="1" ht="14.25" r="44" s="24" spans="1:21">
+    <row r="44" spans="1:21" s="24" customFormat="1" ht="14.25">
       <c r="A44" s="24" t="s">
         <v>268</v>
       </c>
@@ -13534,7 +13862,7 @@
         <v>8</v>
       </c>
     </row>
-    <row customFormat="1" ht="14.25" r="45" s="24" spans="1:21">
+    <row r="45" spans="1:21" s="24" customFormat="1" ht="14.25">
       <c r="A45" s="24" t="s">
         <v>275</v>
       </c>
@@ -13593,7 +13921,7 @@
         <v>37</v>
       </c>
     </row>
-    <row customFormat="1" ht="14.25" r="46" s="24" spans="1:21">
+    <row r="46" spans="1:21" s="24" customFormat="1" ht="14.25">
       <c r="A46" s="24" t="s">
         <v>281</v>
       </c>
@@ -13652,7 +13980,7 @@
         <v>37</v>
       </c>
     </row>
-    <row customFormat="1" ht="14.25" r="47" s="24" spans="1:21">
+    <row r="47" spans="1:21" s="24" customFormat="1" ht="14.25">
       <c r="A47" s="24" t="s">
         <v>287</v>
       </c>
@@ -13711,7 +14039,7 @@
         <v>37</v>
       </c>
     </row>
-    <row customFormat="1" ht="14.25" r="48" s="24" spans="1:21">
+    <row r="48" spans="1:21" s="24" customFormat="1" ht="14.25">
       <c r="A48" s="24" t="s">
         <v>293</v>
       </c>
@@ -13770,7 +14098,7 @@
         <v>16</v>
       </c>
     </row>
-    <row customFormat="1" ht="14.25" r="49" s="24" spans="1:21">
+    <row r="49" spans="1:21" s="24" customFormat="1" ht="14.25">
       <c r="A49" s="24" t="s">
         <v>298</v>
       </c>
@@ -13829,7 +14157,7 @@
         <v>16</v>
       </c>
     </row>
-    <row customFormat="1" ht="14.25" r="50" s="24" spans="1:21">
+    <row r="50" spans="1:21" s="24" customFormat="1" ht="14.25">
       <c r="A50" s="24" t="s">
         <v>304</v>
       </c>
@@ -13888,7 +14216,7 @@
         <v>16</v>
       </c>
     </row>
-    <row customFormat="1" ht="14.25" r="51" s="24" spans="1:21">
+    <row r="51" spans="1:21" s="24" customFormat="1" ht="14.25">
       <c r="A51" s="24" t="s">
         <v>310</v>
       </c>
@@ -13947,7 +14275,7 @@
         <v>16</v>
       </c>
     </row>
-    <row customFormat="1" ht="14.25" r="52" s="24" spans="1:21">
+    <row r="52" spans="1:21" s="24" customFormat="1" ht="14.25">
       <c r="A52" s="24" t="s">
         <v>316</v>
       </c>
@@ -14006,7 +14334,7 @@
         <v>16</v>
       </c>
     </row>
-    <row customFormat="1" ht="14.25" r="53" s="24" spans="1:21">
+    <row r="53" spans="1:21" s="24" customFormat="1" ht="14.25">
       <c r="A53" s="24" t="s">
         <v>343</v>
       </c>
@@ -14065,7 +14393,7 @@
         <v>325</v>
       </c>
     </row>
-    <row customFormat="1" ht="14.25" r="54" s="24" spans="1:21">
+    <row r="54" spans="1:21" s="24" customFormat="1" ht="14.25">
       <c r="A54" s="24" t="s">
         <v>349</v>
       </c>
@@ -14124,7 +14452,7 @@
         <v>325</v>
       </c>
     </row>
-    <row customFormat="1" ht="14.25" r="55" s="24" spans="1:21">
+    <row r="55" spans="1:21" s="24" customFormat="1" ht="14.25">
       <c r="A55" s="24" t="s">
         <v>353</v>
       </c>
@@ -14183,7 +14511,7 @@
         <v>325</v>
       </c>
     </row>
-    <row customFormat="1" ht="14.25" r="56" s="24" spans="1:21">
+    <row r="56" spans="1:21" s="24" customFormat="1" ht="14.25">
       <c r="A56" s="24" t="s">
         <v>359</v>
       </c>
@@ -14242,7 +14570,7 @@
         <v>325</v>
       </c>
     </row>
-    <row customFormat="1" ht="14.25" r="57" s="24" spans="1:21">
+    <row r="57" spans="1:21" s="24" customFormat="1" ht="14.25">
       <c r="A57" s="24" t="s">
         <v>364</v>
       </c>
@@ -14301,7 +14629,7 @@
         <v>325</v>
       </c>
     </row>
-    <row customFormat="1" ht="14.25" r="58" s="24" spans="1:21">
+    <row r="58" spans="1:21" s="24" customFormat="1" ht="14.25">
       <c r="A58" s="24" t="s">
         <v>371</v>
       </c>
@@ -14360,7 +14688,7 @@
         <v>325</v>
       </c>
     </row>
-    <row customFormat="1" ht="14.25" r="59" s="24" spans="1:21">
+    <row r="59" spans="1:21" s="24" customFormat="1" ht="14.25">
       <c r="A59" s="24" t="s">
         <v>377</v>
       </c>
@@ -14419,7 +14747,7 @@
         <v>325</v>
       </c>
     </row>
-    <row customFormat="1" ht="14.25" r="60" s="24" spans="1:21">
+    <row r="60" spans="1:21" s="24" customFormat="1" ht="14.25">
       <c r="A60" s="24" t="s">
         <v>384</v>
       </c>
@@ -14478,7 +14806,7 @@
         <v>325</v>
       </c>
     </row>
-    <row customFormat="1" ht="14.25" r="61" s="24" spans="1:21">
+    <row r="61" spans="1:21" s="24" customFormat="1" ht="14.25">
       <c r="A61" s="24" t="s">
         <v>391</v>
       </c>
@@ -14537,7 +14865,7 @@
         <v>325</v>
       </c>
     </row>
-    <row customFormat="1" ht="14.25" r="62" s="24" spans="1:21">
+    <row r="62" spans="1:21" s="24" customFormat="1" ht="14.25">
       <c r="A62" s="24" t="s">
         <v>397</v>
       </c>
@@ -14596,7 +14924,7 @@
         <v>8</v>
       </c>
     </row>
-    <row customFormat="1" ht="14.25" r="63" s="24" spans="1:21">
+    <row r="63" spans="1:21" s="24" customFormat="1" ht="14.25">
       <c r="A63" s="24" t="s">
         <v>400</v>
       </c>
@@ -14655,7 +14983,7 @@
         <v>8</v>
       </c>
     </row>
-    <row customFormat="1" ht="14.25" r="64" s="24" spans="1:21">
+    <row r="64" spans="1:21" s="24" customFormat="1" ht="14.25">
       <c r="A64" s="24" t="s">
         <v>405</v>
       </c>
@@ -14714,7 +15042,7 @@
         <v>8</v>
       </c>
     </row>
-    <row customFormat="1" ht="14.25" r="65" s="24" spans="1:21">
+    <row r="65" spans="1:21" s="24" customFormat="1" ht="14.25">
       <c r="A65" s="24" t="s">
         <v>411</v>
       </c>
@@ -14773,7 +15101,7 @@
         <v>8</v>
       </c>
     </row>
-    <row customFormat="1" ht="14.25" r="66" s="24" spans="1:21">
+    <row r="66" spans="1:21" s="24" customFormat="1" ht="14.25">
       <c r="A66" s="24" t="s">
         <v>416</v>
       </c>
@@ -14832,7 +15160,7 @@
         <v>37</v>
       </c>
     </row>
-    <row customFormat="1" ht="14.25" r="67" s="24" spans="1:21">
+    <row r="67" spans="1:21" s="24" customFormat="1" ht="14.25">
       <c r="A67" s="24" t="s">
         <v>422</v>
       </c>
@@ -14891,7 +15219,7 @@
         <v>16</v>
       </c>
     </row>
-    <row customFormat="1" ht="14.25" r="68" s="24" spans="1:21">
+    <row r="68" spans="1:21" s="24" customFormat="1" ht="14.25">
       <c r="A68" s="24" t="s">
         <v>483</v>
       </c>
@@ -14950,7 +15278,7 @@
         <v>8</v>
       </c>
     </row>
-    <row customFormat="1" ht="14.25" r="69" s="24" spans="1:21">
+    <row r="69" spans="1:21" s="24" customFormat="1" ht="14.25">
       <c r="A69" s="24" t="s">
         <v>488</v>
       </c>
@@ -15009,7 +15337,7 @@
         <v>8</v>
       </c>
     </row>
-    <row customFormat="1" ht="14.25" r="70" s="24" spans="1:21">
+    <row r="70" spans="1:21" s="24" customFormat="1" ht="14.25">
       <c r="A70" s="24" t="s">
         <v>490</v>
       </c>
@@ -15068,7 +15396,7 @@
         <v>8</v>
       </c>
     </row>
-    <row customFormat="1" ht="14.25" r="71" s="24" spans="1:21">
+    <row r="71" spans="1:21" s="24" customFormat="1" ht="14.25">
       <c r="A71" s="24" t="s">
         <v>496</v>
       </c>
@@ -15127,7 +15455,7 @@
         <v>8</v>
       </c>
     </row>
-    <row customFormat="1" ht="14.25" r="72" s="24" spans="1:21">
+    <row r="72" spans="1:21" s="24" customFormat="1" ht="14.25">
       <c r="A72" s="24" t="s">
         <v>501</v>
       </c>
@@ -15186,7 +15514,7 @@
         <v>8</v>
       </c>
     </row>
-    <row customFormat="1" ht="14.25" r="73" s="24" spans="1:21">
+    <row r="73" spans="1:21" s="24" customFormat="1" ht="14.25">
       <c r="A73" s="24" t="s">
         <v>503</v>
       </c>
@@ -15245,7 +15573,7 @@
         <v>16</v>
       </c>
     </row>
-    <row customFormat="1" ht="14.25" r="74" s="24" spans="1:21">
+    <row r="74" spans="1:21" s="24" customFormat="1" ht="14.25">
       <c r="A74" s="24" t="s">
         <v>507</v>
       </c>
@@ -15304,7 +15632,7 @@
         <v>16</v>
       </c>
     </row>
-    <row customFormat="1" ht="14.25" r="75" s="24" spans="1:21">
+    <row r="75" spans="1:21" s="24" customFormat="1" ht="14.25">
       <c r="A75" s="24" t="s">
         <v>513</v>
       </c>
@@ -15363,7 +15691,7 @@
         <v>16</v>
       </c>
     </row>
-    <row customFormat="1" ht="14.25" r="76" s="24" spans="1:21">
+    <row r="76" spans="1:21" s="24" customFormat="1" ht="14.25">
       <c r="A76" s="24" t="s">
         <v>519</v>
       </c>
@@ -15422,7 +15750,7 @@
         <v>16</v>
       </c>
     </row>
-    <row customFormat="1" ht="14.25" r="77" s="24" spans="1:21">
+    <row r="77" spans="1:21" s="24" customFormat="1" ht="14.25">
       <c r="A77" s="24" t="s">
         <v>524</v>
       </c>
@@ -15481,7 +15809,7 @@
         <v>16</v>
       </c>
     </row>
-    <row customFormat="1" ht="14.25" r="78" s="24" spans="1:21">
+    <row r="78" spans="1:21" s="24" customFormat="1" ht="14.25">
       <c r="A78" s="24" t="s">
         <v>531</v>
       </c>
@@ -15540,7 +15868,7 @@
         <v>16</v>
       </c>
     </row>
-    <row customFormat="1" ht="14.25" r="79" s="24" spans="1:21">
+    <row r="79" spans="1:21" s="24" customFormat="1" ht="14.25">
       <c r="A79" s="24" t="s">
         <v>534</v>
       </c>
@@ -15599,7 +15927,7 @@
         <v>16</v>
       </c>
     </row>
-    <row customFormat="1" ht="14.25" r="80" s="24" spans="1:21">
+    <row r="80" spans="1:21" s="24" customFormat="1" ht="14.25">
       <c r="A80" s="24" t="s">
         <v>540</v>
       </c>
@@ -15658,7 +15986,7 @@
         <v>16</v>
       </c>
     </row>
-    <row customFormat="1" ht="14.25" r="81" s="24" spans="1:21">
+    <row r="81" spans="1:21" s="24" customFormat="1" ht="14.25">
       <c r="A81" s="24" t="s">
         <v>547</v>
       </c>
@@ -15717,7 +16045,7 @@
         <v>16</v>
       </c>
     </row>
-    <row customFormat="1" ht="14.25" r="82" s="24" spans="1:21">
+    <row r="82" spans="1:21" s="24" customFormat="1" ht="14.25">
       <c r="A82" s="24" t="s">
         <v>552</v>
       </c>
@@ -15776,7 +16104,7 @@
         <v>16</v>
       </c>
     </row>
-    <row customFormat="1" ht="14.25" r="83" s="24" spans="1:21">
+    <row r="83" spans="1:21" s="24" customFormat="1" ht="14.25">
       <c r="A83" s="24" t="s">
         <v>557</v>
       </c>
@@ -15835,7 +16163,7 @@
         <v>16</v>
       </c>
     </row>
-    <row customFormat="1" ht="14.25" r="84" s="24" spans="1:21">
+    <row r="84" spans="1:21" s="24" customFormat="1" ht="14.25">
       <c r="A84" s="24" t="s">
         <v>560</v>
       </c>
@@ -15894,7 +16222,7 @@
         <v>16</v>
       </c>
     </row>
-    <row customFormat="1" ht="14.25" r="85" s="24" spans="1:21">
+    <row r="85" spans="1:21" s="24" customFormat="1" ht="14.25">
       <c r="A85" s="24" t="s">
         <v>564</v>
       </c>
@@ -15953,7 +16281,7 @@
         <v>16</v>
       </c>
     </row>
-    <row customFormat="1" ht="14.25" r="86" s="24" spans="1:21">
+    <row r="86" spans="1:21" s="24" customFormat="1" ht="14.25">
       <c r="A86" s="24" t="s">
         <v>605</v>
       </c>
@@ -16012,7 +16340,7 @@
         <v>8</v>
       </c>
     </row>
-    <row customFormat="1" ht="14.25" r="87" s="24" spans="1:21">
+    <row r="87" spans="1:21" s="24" customFormat="1" ht="14.25">
       <c r="A87" s="24" t="s">
         <v>609</v>
       </c>
@@ -16071,7 +16399,7 @@
         <v>37</v>
       </c>
     </row>
-    <row customFormat="1" ht="14.25" r="88" s="24" spans="1:21">
+    <row r="88" spans="1:21" s="24" customFormat="1" ht="14.25">
       <c r="A88" s="24" t="s">
         <v>614</v>
       </c>
@@ -16130,7 +16458,7 @@
         <v>37</v>
       </c>
     </row>
-    <row customFormat="1" ht="14.25" r="89" s="24" spans="1:21">
+    <row r="89" spans="1:21" s="24" customFormat="1" ht="14.25">
       <c r="A89" s="24" t="s">
         <v>618</v>
       </c>
@@ -16189,7 +16517,7 @@
         <v>37</v>
       </c>
     </row>
-    <row customFormat="1" ht="14.25" r="90" s="24" spans="1:21">
+    <row r="90" spans="1:21" s="24" customFormat="1" ht="14.25">
       <c r="A90" s="24" t="s">
         <v>624</v>
       </c>
@@ -16248,7 +16576,7 @@
         <v>16</v>
       </c>
     </row>
-    <row customFormat="1" ht="14.25" r="91" s="24" spans="1:21">
+    <row r="91" spans="1:21" s="24" customFormat="1" ht="14.25">
       <c r="A91" s="24" t="s">
         <v>628</v>
       </c>
@@ -16307,7 +16635,7 @@
         <v>16</v>
       </c>
     </row>
-    <row customFormat="1" ht="14.25" r="92" s="24" spans="1:21">
+    <row r="92" spans="1:21" s="24" customFormat="1" ht="14.25">
       <c r="A92" s="24" t="s">
         <v>632</v>
       </c>
@@ -16366,7 +16694,7 @@
         <v>16</v>
       </c>
     </row>
-    <row customFormat="1" ht="14.25" r="93" s="24" spans="1:21">
+    <row r="93" spans="1:21" s="24" customFormat="1" ht="14.25">
       <c r="A93" s="24" t="s">
         <v>635</v>
       </c>
@@ -16425,7 +16753,7 @@
         <v>16</v>
       </c>
     </row>
-    <row customFormat="1" ht="14.25" r="94" s="24" spans="1:21">
+    <row r="94" spans="1:21" s="24" customFormat="1" ht="14.25">
       <c r="A94" s="24" t="s">
         <v>664</v>
       </c>
@@ -16484,7 +16812,7 @@
         <v>8</v>
       </c>
     </row>
-    <row customFormat="1" ht="14.25" r="95" s="24" spans="1:21">
+    <row r="95" spans="1:21" s="24" customFormat="1" ht="14.25">
       <c r="A95" s="24" t="s">
         <v>669</v>
       </c>
@@ -16543,7 +16871,7 @@
         <v>8</v>
       </c>
     </row>
-    <row customFormat="1" ht="14.25" r="96" s="24" spans="1:21">
+    <row r="96" spans="1:21" s="24" customFormat="1" ht="14.25">
       <c r="A96" s="24" t="s">
         <v>673</v>
       </c>
@@ -16602,7 +16930,7 @@
         <v>8</v>
       </c>
     </row>
-    <row customFormat="1" ht="14.25" r="97" s="24" spans="1:21">
+    <row r="97" spans="1:21" s="24" customFormat="1" ht="14.25">
       <c r="A97" s="24" t="s">
         <v>675</v>
       </c>
@@ -16661,7 +16989,7 @@
         <v>37</v>
       </c>
     </row>
-    <row customFormat="1" ht="14.25" r="98" s="24" spans="1:21">
+    <row r="98" spans="1:21" s="24" customFormat="1" ht="14.25">
       <c r="A98" s="24" t="s">
         <v>689</v>
       </c>
@@ -16720,7 +17048,7 @@
         <v>16</v>
       </c>
     </row>
-    <row customFormat="1" ht="14.25" r="99" s="24" spans="1:21">
+    <row r="99" spans="1:21" s="24" customFormat="1" ht="14.25">
       <c r="A99" s="24" t="s">
         <v>706</v>
       </c>
@@ -16779,7 +17107,7 @@
         <v>8</v>
       </c>
     </row>
-    <row customFormat="1" ht="14.25" r="100" s="24" spans="1:21">
+    <row r="100" spans="1:21" s="24" customFormat="1" ht="14.25">
       <c r="A100" s="24" t="s">
         <v>710</v>
       </c>
@@ -16838,7 +17166,7 @@
         <v>37</v>
       </c>
     </row>
-    <row customFormat="1" ht="14.25" r="101" s="24" spans="1:21">
+    <row r="101" spans="1:21" s="24" customFormat="1" ht="14.25">
       <c r="A101" s="24" t="s">
         <v>714</v>
       </c>
@@ -16897,7 +17225,7 @@
         <v>16</v>
       </c>
     </row>
-    <row customFormat="1" ht="14.25" r="102" s="24" spans="1:21">
+    <row r="102" spans="1:21" s="24" customFormat="1" ht="14.25">
       <c r="A102" s="24" t="s">
         <v>744</v>
       </c>
@@ -16956,7 +17284,7 @@
         <v>37</v>
       </c>
     </row>
-    <row customFormat="1" ht="14.25" r="103" s="24" spans="1:21">
+    <row r="103" spans="1:21" s="24" customFormat="1" ht="14.25">
       <c r="A103" s="24" t="s">
         <v>750</v>
       </c>
@@ -17015,7 +17343,7 @@
         <v>16</v>
       </c>
     </row>
-    <row customFormat="1" ht="14.25" r="104" s="24" spans="1:21">
+    <row r="104" spans="1:21" s="24" customFormat="1" ht="14.25">
       <c r="A104" s="24" t="s">
         <v>759</v>
       </c>
@@ -17074,7 +17402,7 @@
         <v>37</v>
       </c>
     </row>
-    <row customFormat="1" ht="14.25" r="105" s="24" spans="1:21">
+    <row r="105" spans="1:21" s="24" customFormat="1" ht="14.25">
       <c r="A105" s="24" t="s">
         <v>769</v>
       </c>
@@ -17133,7 +17461,7 @@
         <v>37</v>
       </c>
     </row>
-    <row customFormat="1" ht="14.25" r="106" s="24" spans="1:21">
+    <row r="106" spans="1:21" s="24" customFormat="1" ht="14.25">
       <c r="A106" s="24" t="s">
         <v>775</v>
       </c>
@@ -17192,7 +17520,7 @@
         <v>37</v>
       </c>
     </row>
-    <row customFormat="1" ht="14.25" r="107" s="24" spans="1:21">
+    <row r="107" spans="1:21" s="24" customFormat="1" ht="14.25">
       <c r="A107" s="24" t="s">
         <v>785</v>
       </c>
@@ -17251,7 +17579,7 @@
         <v>8</v>
       </c>
     </row>
-    <row customFormat="1" ht="14.25" r="108" s="24" spans="1:21">
+    <row r="108" spans="1:21" s="24" customFormat="1" ht="14.25">
       <c r="A108" s="24" t="s">
         <v>790</v>
       </c>
@@ -17310,7 +17638,7 @@
         <v>37</v>
       </c>
     </row>
-    <row customFormat="1" ht="14.25" r="109" s="24" spans="1:21">
+    <row r="109" spans="1:21" s="24" customFormat="1" ht="14.25">
       <c r="A109" s="24" t="s">
         <v>799</v>
       </c>
@@ -17369,7 +17697,7 @@
         <v>37</v>
       </c>
     </row>
-    <row customFormat="1" ht="14.25" r="110" s="24" spans="1:21">
+    <row r="110" spans="1:21" s="24" customFormat="1" ht="14.25">
       <c r="A110" s="24" t="s">
         <v>807</v>
       </c>
@@ -17428,7 +17756,7 @@
         <v>16</v>
       </c>
     </row>
-    <row customFormat="1" ht="14.25" r="111" s="24" spans="1:21">
+    <row r="111" spans="1:21" s="24" customFormat="1" ht="14.25">
       <c r="A111" s="24" t="s">
         <v>812</v>
       </c>
@@ -17487,7 +17815,7 @@
         <v>16</v>
       </c>
     </row>
-    <row customFormat="1" ht="14.25" r="112" s="24" spans="1:21">
+    <row r="112" spans="1:21" s="24" customFormat="1" ht="14.25">
       <c r="A112" s="24" t="s">
         <v>817</v>
       </c>
@@ -17546,7 +17874,7 @@
         <v>16</v>
       </c>
     </row>
-    <row customFormat="1" ht="14.25" r="113" s="24" spans="1:21">
+    <row r="113" spans="1:21" s="24" customFormat="1" ht="14.25">
       <c r="A113" s="24" t="s">
         <v>822</v>
       </c>
@@ -17605,7 +17933,7 @@
         <v>16</v>
       </c>
     </row>
-    <row customFormat="1" ht="14.25" r="114" s="24" spans="1:21">
+    <row r="114" spans="1:21" s="24" customFormat="1" ht="14.25">
       <c r="A114" s="24" t="s">
         <v>833</v>
       </c>
@@ -17664,7 +17992,7 @@
         <v>8</v>
       </c>
     </row>
-    <row customFormat="1" ht="14.25" r="115" s="24" spans="1:21">
+    <row r="115" spans="1:21" s="24" customFormat="1" ht="14.25">
       <c r="A115" s="24" t="s">
         <v>842</v>
       </c>
@@ -17723,7 +18051,7 @@
         <v>325</v>
       </c>
     </row>
-    <row customFormat="1" ht="14.25" r="116" s="24" spans="1:21">
+    <row r="116" spans="1:21" s="24" customFormat="1" ht="14.25">
       <c r="A116" s="24" t="s">
         <v>850</v>
       </c>
@@ -17782,7 +18110,7 @@
         <v>8</v>
       </c>
     </row>
-    <row customFormat="1" ht="14.25" r="117" s="24" spans="1:21">
+    <row r="117" spans="1:21" s="24" customFormat="1" ht="14.25">
       <c r="A117" s="24" t="s">
         <v>857</v>
       </c>
@@ -17841,7 +18169,7 @@
         <v>16</v>
       </c>
     </row>
-    <row customFormat="1" ht="14.25" r="118" s="24" spans="1:21">
+    <row r="118" spans="1:21" s="24" customFormat="1" ht="14.25">
       <c r="A118" s="24" t="s">
         <v>866</v>
       </c>
@@ -17900,7 +18228,7 @@
         <v>37</v>
       </c>
     </row>
-    <row customFormat="1" ht="14.25" r="119" s="24" spans="1:21">
+    <row r="119" spans="1:21" s="24" customFormat="1" ht="14.25">
       <c r="A119" s="24" t="s">
         <v>870</v>
       </c>
@@ -17959,7 +18287,7 @@
         <v>16</v>
       </c>
     </row>
-    <row customFormat="1" ht="14.25" r="120" s="24" spans="1:21">
+    <row r="120" spans="1:21" s="24" customFormat="1" ht="14.25">
       <c r="A120" s="24">
         <v>119</v>
       </c>
@@ -18018,7 +18346,7 @@
         <v>1044</v>
       </c>
     </row>
-    <row customFormat="1" ht="14.25" r="121" s="24" spans="1:21">
+    <row r="121" spans="1:21" s="24" customFormat="1" ht="14.25">
       <c r="A121" s="24" t="s">
         <v>910</v>
       </c>
@@ -18077,7 +18405,7 @@
         <v>1044</v>
       </c>
     </row>
-    <row customFormat="1" ht="14.25" r="122" s="24" spans="1:21">
+    <row r="122" spans="1:21" s="24" customFormat="1" ht="14.25">
       <c r="A122" s="24" t="s">
         <v>915</v>
       </c>
@@ -18136,7 +18464,7 @@
         <v>1044</v>
       </c>
     </row>
-    <row customFormat="1" ht="14.25" r="123" s="24" spans="1:21">
+    <row r="123" spans="1:21" s="24" customFormat="1" ht="14.25">
       <c r="A123" s="24" t="s">
         <v>922</v>
       </c>
@@ -18195,7 +18523,7 @@
         <v>1044</v>
       </c>
     </row>
-    <row customFormat="1" ht="14.25" r="124" s="24" spans="1:21">
+    <row r="124" spans="1:21" s="24" customFormat="1" ht="14.25">
       <c r="A124" s="24" t="s">
         <v>927</v>
       </c>
@@ -18254,7 +18582,7 @@
         <v>1044</v>
       </c>
     </row>
-    <row customFormat="1" ht="14.25" r="125" s="24" spans="1:21">
+    <row r="125" spans="1:21" s="24" customFormat="1" ht="14.25">
       <c r="A125" s="24" t="s">
         <v>930</v>
       </c>
@@ -18313,7 +18641,7 @@
         <v>1044</v>
       </c>
     </row>
-    <row customFormat="1" ht="14.25" r="126" s="24" spans="1:21">
+    <row r="126" spans="1:21" s="24" customFormat="1" ht="14.25">
       <c r="A126" s="24" t="s">
         <v>934</v>
       </c>
@@ -18372,7 +18700,7 @@
         <v>1044</v>
       </c>
     </row>
-    <row customFormat="1" ht="14.25" r="127" s="24" spans="1:21">
+    <row r="127" spans="1:21" s="24" customFormat="1" ht="14.25">
       <c r="A127" s="24" t="s">
         <v>940</v>
       </c>
@@ -18431,7 +18759,7 @@
         <v>1044</v>
       </c>
     </row>
-    <row customFormat="1" ht="14.25" r="128" s="24" spans="1:21">
+    <row r="128" spans="1:21" s="24" customFormat="1" ht="14.25">
       <c r="A128" s="24" t="s">
         <v>946</v>
       </c>
@@ -18490,7 +18818,7 @@
         <v>1044</v>
       </c>
     </row>
-    <row customFormat="1" ht="14.25" r="129" s="24" spans="1:21">
+    <row r="129" spans="1:21" s="24" customFormat="1" ht="14.25">
       <c r="A129" s="24" t="s">
         <v>951</v>
       </c>
@@ -18549,7 +18877,7 @@
         <v>1044</v>
       </c>
     </row>
-    <row customFormat="1" ht="14.25" r="130" s="24" spans="1:21">
+    <row r="130" spans="1:21" s="24" customFormat="1" ht="14.25">
       <c r="A130" s="24" t="s">
         <v>956</v>
       </c>
@@ -18608,7 +18936,7 @@
         <v>1044</v>
       </c>
     </row>
-    <row customFormat="1" ht="14.25" r="131" s="24" spans="1:21">
+    <row r="131" spans="1:21" s="24" customFormat="1" ht="14.25">
       <c r="A131" s="24" t="s">
         <v>960</v>
       </c>
@@ -18667,7 +18995,7 @@
         <v>1044</v>
       </c>
     </row>
-    <row customFormat="1" ht="14.25" r="132" s="24" spans="1:21">
+    <row r="132" spans="1:21" s="24" customFormat="1" ht="14.25">
       <c r="A132" s="24" t="s">
         <v>963</v>
       </c>
@@ -18726,7 +19054,7 @@
         <v>1044</v>
       </c>
     </row>
-    <row customFormat="1" ht="14.25" r="133" s="24" spans="1:21">
+    <row r="133" spans="1:21" s="24" customFormat="1" ht="14.25">
       <c r="A133" s="24" t="s">
         <v>967</v>
       </c>
@@ -18785,7 +19113,7 @@
         <v>1044</v>
       </c>
     </row>
-    <row customFormat="1" ht="14.25" r="134" s="24" spans="1:21">
+    <row r="134" spans="1:21" s="24" customFormat="1" ht="14.25">
       <c r="A134" s="24" t="s">
         <v>972</v>
       </c>
@@ -18844,7 +19172,7 @@
         <v>1044</v>
       </c>
     </row>
-    <row customFormat="1" ht="14.25" r="135" s="24" spans="1:21">
+    <row r="135" spans="1:21" s="24" customFormat="1" ht="14.25">
       <c r="A135" s="24" t="s">
         <v>975</v>
       </c>
@@ -18903,7 +19231,7 @@
         <v>1044</v>
       </c>
     </row>
-    <row customFormat="1" ht="14.25" r="136" s="24" spans="1:21">
+    <row r="136" spans="1:21" s="24" customFormat="1" ht="14.25">
       <c r="A136" s="24" t="s">
         <v>980</v>
       </c>
@@ -18962,7 +19290,7 @@
         <v>1044</v>
       </c>
     </row>
-    <row customFormat="1" ht="14.25" r="137" s="24" spans="1:21">
+    <row r="137" spans="1:21" s="24" customFormat="1" ht="14.25">
       <c r="A137" s="24" t="s">
         <v>986</v>
       </c>
@@ -19021,7 +19349,7 @@
         <v>1044</v>
       </c>
     </row>
-    <row customFormat="1" ht="14.25" r="138" s="24" spans="1:21">
+    <row r="138" spans="1:21" s="24" customFormat="1" ht="14.25">
       <c r="A138" s="24" t="s">
         <v>992</v>
       </c>
@@ -19080,7 +19408,7 @@
         <v>1044</v>
       </c>
     </row>
-    <row customFormat="1" ht="14.25" r="139" s="24" spans="1:21">
+    <row r="139" spans="1:21" s="24" customFormat="1" ht="14.25">
       <c r="A139" s="24" t="s">
         <v>997</v>
       </c>
@@ -19139,7 +19467,7 @@
         <v>1044</v>
       </c>
     </row>
-    <row customFormat="1" ht="14.25" r="140" s="24" spans="1:21">
+    <row r="140" spans="1:21" s="24" customFormat="1" ht="14.25">
       <c r="A140" s="24" t="s">
         <v>1001</v>
       </c>
@@ -19198,7 +19526,7 @@
         <v>1044</v>
       </c>
     </row>
-    <row customFormat="1" ht="14.25" r="141" s="24" spans="1:21">
+    <row r="141" spans="1:21" s="24" customFormat="1" ht="14.25">
       <c r="A141" s="24" t="s">
         <v>1007</v>
       </c>
@@ -19257,7 +19585,7 @@
         <v>1044</v>
       </c>
     </row>
-    <row customFormat="1" ht="14.25" r="142" s="24" spans="1:21">
+    <row r="142" spans="1:21" s="24" customFormat="1" ht="14.25">
       <c r="A142" s="24" t="s">
         <v>1012</v>
       </c>
@@ -19316,7 +19644,7 @@
         <v>1044</v>
       </c>
     </row>
-    <row customFormat="1" ht="14.25" r="143" s="24" spans="1:21">
+    <row r="143" spans="1:21" s="24" customFormat="1" ht="14.25">
       <c r="A143" s="24" t="s">
         <v>1017</v>
       </c>
@@ -19375,7 +19703,7 @@
         <v>37</v>
       </c>
     </row>
-    <row customFormat="1" ht="14.25" r="144" s="24" spans="1:21">
+    <row r="144" spans="1:21" s="24" customFormat="1" ht="14.25">
       <c r="A144" s="24" t="s">
         <v>1051</v>
       </c>
@@ -19434,7 +19762,7 @@
         <v>37</v>
       </c>
     </row>
-    <row customFormat="1" ht="14.25" r="145" s="24" spans="1:21">
+    <row r="145" spans="1:21" s="24" customFormat="1" ht="14.25">
       <c r="A145" s="24" t="s">
         <v>1056</v>
       </c>
@@ -19493,7 +19821,7 @@
         <v>16</v>
       </c>
     </row>
-    <row customFormat="1" ht="14.25" r="146" s="24" spans="1:21">
+    <row r="146" spans="1:21" s="24" customFormat="1" ht="14.25">
       <c r="A146" s="24" t="s">
         <v>1073</v>
       </c>
@@ -19552,7 +19880,7 @@
         <v>8</v>
       </c>
     </row>
-    <row customFormat="1" ht="14.25" r="147" s="24" spans="1:21">
+    <row r="147" spans="1:21" s="24" customFormat="1" ht="14.25">
       <c r="A147" s="24" t="s">
         <v>1078</v>
       </c>
@@ -19611,7 +19939,7 @@
         <v>37</v>
       </c>
     </row>
-    <row customFormat="1" ht="14.25" r="148" s="24" spans="1:21">
+    <row r="148" spans="1:21" s="24" customFormat="1" ht="14.25">
       <c r="A148" s="24" t="s">
         <v>1082</v>
       </c>
@@ -19670,7 +19998,7 @@
         <v>1044</v>
       </c>
     </row>
-    <row customFormat="1" ht="14.25" r="149" s="24" spans="1:21">
+    <row r="149" spans="1:21" s="24" customFormat="1" ht="14.25">
       <c r="A149" s="24" t="s">
         <v>1096</v>
       </c>
@@ -19729,7 +20057,7 @@
         <v>1044</v>
       </c>
     </row>
-    <row customFormat="1" ht="14.25" r="150" s="24" spans="1:21">
+    <row r="150" spans="1:21" s="24" customFormat="1" ht="14.25">
       <c r="A150" s="24" t="s">
         <v>1101</v>
       </c>
@@ -19788,7 +20116,7 @@
         <v>1044</v>
       </c>
     </row>
-    <row customFormat="1" ht="14.25" r="151" s="24" spans="1:21">
+    <row r="151" spans="1:21" s="24" customFormat="1" ht="14.25">
       <c r="A151" s="24" t="s">
         <v>1108</v>
       </c>
@@ -19847,7 +20175,7 @@
         <v>8</v>
       </c>
     </row>
-    <row customFormat="1" ht="14.25" r="152" s="24" spans="1:21">
+    <row r="152" spans="1:21" s="24" customFormat="1" ht="14.25">
       <c r="A152" s="24" t="s">
         <v>1113</v>
       </c>
@@ -19906,7 +20234,7 @@
         <v>1044</v>
       </c>
     </row>
-    <row customFormat="1" ht="14.25" r="153" s="24" spans="1:21">
+    <row r="153" spans="1:21" s="24" customFormat="1" ht="14.25">
       <c r="A153" s="24" t="s">
         <v>1123</v>
       </c>
@@ -19965,7 +20293,7 @@
         <v>1044</v>
       </c>
     </row>
-    <row customFormat="1" ht="14.25" r="154" s="24" spans="1:21">
+    <row r="154" spans="1:21" s="24" customFormat="1" ht="14.25">
       <c r="A154" s="24" t="s">
         <v>1132</v>
       </c>
@@ -20024,7 +20352,7 @@
         <v>8</v>
       </c>
     </row>
-    <row ht="14.25" r="155" spans="1:21">
+    <row r="155" spans="1:21" ht="14.25">
       <c r="A155" t="s">
         <v>1136</v>
       </c>
@@ -20083,7 +20411,7 @@
         <v>37</v>
       </c>
     </row>
-    <row customFormat="1" ht="14.25" r="156" s="24" spans="1:21">
+    <row r="156" spans="1:21" s="24" customFormat="1" ht="14.25">
       <c r="A156" s="24" t="s">
         <v>1139</v>
       </c>
@@ -20142,7 +20470,7 @@
         <v>1044</v>
       </c>
     </row>
-    <row customFormat="1" ht="14.25" r="157" s="24" spans="1:21">
+    <row r="157" spans="1:21" s="24" customFormat="1" ht="14.25">
       <c r="A157" s="24" t="s">
         <v>1144</v>
       </c>
@@ -20201,134 +20529,370 @@
         <v>16</v>
       </c>
     </row>
-    <row r="158">
-      <c r="A158" t="s">
+    <row r="158" spans="1:21" s="24" customFormat="1" ht="14.25">
+      <c r="A158" s="24" t="s">
         <v>1150</v>
       </c>
-      <c r="B158" t="s">
+      <c r="B158" s="24" t="s">
+        <v>7</v>
+      </c>
+      <c r="C158" s="24" t="s">
+        <v>1151</v>
+      </c>
+      <c r="D158" s="24" t="s">
+        <v>84</v>
+      </c>
+      <c r="E158" s="24" t="s">
+        <v>78</v>
+      </c>
+      <c r="F158" s="24" t="s">
+        <v>906</v>
+      </c>
+      <c r="G158" s="24" t="s">
+        <v>1152</v>
+      </c>
+      <c r="H158" s="24" t="s">
+        <v>1153</v>
+      </c>
+      <c r="I158" s="24" t="s">
+        <v>198</v>
+      </c>
+      <c r="K158" s="24" t="s">
+        <v>199</v>
+      </c>
+      <c r="L158" s="24" t="s">
+        <v>1154</v>
+      </c>
+      <c r="M158" s="24" t="s">
+        <v>202</v>
+      </c>
+      <c r="N158" s="24" t="s">
+        <v>204</v>
+      </c>
+      <c r="P158" s="24" t="s">
+        <v>1155</v>
+      </c>
+      <c r="Q158" s="24" t="s">
+        <v>204</v>
+      </c>
+      <c r="R158" s="24" t="s">
+        <v>1151</v>
+      </c>
+      <c r="S158" s="24" t="s">
+        <v>1156</v>
+      </c>
+      <c r="T158" s="24" t="s">
+        <v>687</v>
+      </c>
+      <c r="U158" s="24" t="s">
+        <v>1044</v>
+      </c>
+    </row>
+    <row r="159" spans="1:21" s="24" customFormat="1" ht="14.25">
+      <c r="A159" s="24" t="s">
+        <v>1157</v>
+      </c>
+      <c r="B159" s="24" t="s">
+        <v>7</v>
+      </c>
+      <c r="C159" s="24" t="s">
+        <v>1158</v>
+      </c>
+      <c r="D159" s="24" t="s">
+        <v>77</v>
+      </c>
+      <c r="E159" s="24" t="s">
+        <v>78</v>
+      </c>
+      <c r="F159" s="24" t="s">
+        <v>79</v>
+      </c>
+      <c r="G159" s="24" t="s">
+        <v>221</v>
+      </c>
+      <c r="H159" s="24" t="s">
+        <v>1159</v>
+      </c>
+      <c r="I159" s="24" t="s">
+        <v>198</v>
+      </c>
+      <c r="K159" s="24" t="s">
+        <v>1160</v>
+      </c>
+      <c r="L159" s="24" t="s">
+        <v>1161</v>
+      </c>
+      <c r="M159" s="24" t="s">
+        <v>202</v>
+      </c>
+      <c r="N159" s="24" t="s">
+        <v>266</v>
+      </c>
+      <c r="P159" s="24" t="s">
+        <v>199</v>
+      </c>
+      <c r="Q159" s="24" t="s">
+        <v>199</v>
+      </c>
+      <c r="R159" s="24" t="s">
+        <v>1158</v>
+      </c>
+      <c r="S159" s="24" t="s">
         <v>1164</v>
       </c>
-      <c r="C158" t="s">
-        <v>1151</v>
-      </c>
-      <c r="D158" t="s">
+      <c r="T159" s="24" t="s">
+        <v>687</v>
+      </c>
+      <c r="U159" s="24" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="160" spans="1:21" ht="14.25">
+      <c r="A160" t="s">
+        <v>1169</v>
+      </c>
+      <c r="B160" t="s">
+        <v>1188</v>
+      </c>
+      <c r="C160" t="s">
+        <v>1170</v>
+      </c>
+      <c r="D160" t="s">
         <v>84</v>
       </c>
-      <c r="E158" t="s">
+      <c r="E160" t="s">
         <v>78</v>
       </c>
-      <c r="F158" t="s">
-        <v>906</v>
-      </c>
-      <c r="G158" t="s">
-        <v>1153</v>
-      </c>
-      <c r="H158" t="s">
-        <v>1154</v>
-      </c>
-      <c r="I158" t="s">
+      <c r="F160" t="s">
+        <v>207</v>
+      </c>
+      <c r="G160" t="s">
+        <v>1171</v>
+      </c>
+      <c r="H160" t="s">
+        <v>1172</v>
+      </c>
+      <c r="I160" t="s">
         <v>198</v>
       </c>
-      <c r="K158" t="s">
+      <c r="K160" t="s">
         <v>199</v>
       </c>
-      <c r="L158" t="s">
+      <c r="L160" t="s">
+        <v>1173</v>
+      </c>
+      <c r="M160" t="s">
+        <v>202</v>
+      </c>
+      <c r="N160" t="s">
+        <v>266</v>
+      </c>
+      <c r="P160" t="s">
         <v>1155</v>
       </c>
-      <c r="M158" t="s">
+      <c r="Q160" t="s">
+        <v>266</v>
+      </c>
+      <c r="R160" t="s">
+        <v>1170</v>
+      </c>
+      <c r="S160" t="s">
+        <v>1174</v>
+      </c>
+      <c r="T160" s="24" t="s">
+        <v>1046</v>
+      </c>
+      <c r="U160" t="s">
+        <v>1192</v>
+      </c>
+    </row>
+    <row r="161" spans="1:21" ht="14.25">
+      <c r="A161" t="s">
+        <v>1175</v>
+      </c>
+      <c r="B161" t="s">
+        <v>1188</v>
+      </c>
+      <c r="C161" t="s">
+        <v>1176</v>
+      </c>
+      <c r="D161" t="s">
+        <v>84</v>
+      </c>
+      <c r="E161" t="s">
+        <v>78</v>
+      </c>
+      <c r="F161" t="s">
+        <v>235</v>
+      </c>
+      <c r="G161" t="s">
+        <v>236</v>
+      </c>
+      <c r="H161" t="s">
+        <v>199</v>
+      </c>
+      <c r="I161" t="s">
+        <v>198</v>
+      </c>
+      <c r="K161" t="s">
+        <v>431</v>
+      </c>
+      <c r="L161" t="s">
+        <v>1177</v>
+      </c>
+      <c r="M161" t="s">
         <v>202</v>
       </c>
-      <c r="N158" t="s">
+      <c r="N161" t="s">
         <v>204</v>
       </c>
-      <c r="P158" t="s">
-        <v>1156</v>
-      </c>
-      <c r="Q158" t="s">
+      <c r="P161" t="s">
+        <v>203</v>
+      </c>
+      <c r="Q161" t="s">
         <v>204</v>
       </c>
-      <c r="R158" t="s">
-        <v>1151</v>
-      </c>
-      <c r="S158" t="s">
-        <v>1157</v>
-      </c>
-      <c r="T158" t="s">
+      <c r="R161" t="s">
+        <v>1176</v>
+      </c>
+      <c r="S161" t="s">
+        <v>1178</v>
+      </c>
+      <c r="T161" s="24" t="s">
         <v>687</v>
       </c>
-      <c r="U158" t="s">
+      <c r="U161" t="s">
         <v>1044</v>
       </c>
     </row>
-    <row r="159">
-      <c r="A159" t="s">
-        <v>1158</v>
-      </c>
-      <c r="B159" t="s">
-        <v>1164</v>
-      </c>
-      <c r="C159" t="s">
-        <v>1159</v>
-      </c>
-      <c r="D159" t="s">
-        <v>77</v>
-      </c>
-      <c r="E159" t="s">
+    <row r="162" spans="1:21" ht="14.25">
+      <c r="A162" t="s">
+        <v>1179</v>
+      </c>
+      <c r="B162" t="s">
+        <v>1188</v>
+      </c>
+      <c r="C162" t="s">
+        <v>1180</v>
+      </c>
+      <c r="D162" t="s">
+        <v>84</v>
+      </c>
+      <c r="E162" t="s">
         <v>78</v>
       </c>
-      <c r="F159" t="s">
+      <c r="F162" t="s">
+        <v>235</v>
+      </c>
+      <c r="G162" t="s">
+        <v>236</v>
+      </c>
+      <c r="H162" t="s">
+        <v>199</v>
+      </c>
+      <c r="I162" t="s">
+        <v>198</v>
+      </c>
+      <c r="K162" t="s">
+        <v>199</v>
+      </c>
+      <c r="L162" t="s">
+        <v>1181</v>
+      </c>
+      <c r="M162" t="s">
+        <v>252</v>
+      </c>
+      <c r="N162" t="s">
+        <v>202</v>
+      </c>
+      <c r="P162" t="s">
+        <v>203</v>
+      </c>
+      <c r="Q162" t="s">
+        <v>204</v>
+      </c>
+      <c r="R162" t="s">
+        <v>1180</v>
+      </c>
+      <c r="S162" t="s">
+        <v>1182</v>
+      </c>
+      <c r="T162" s="24" t="s">
+        <v>687</v>
+      </c>
+      <c r="U162" t="s">
+        <v>1044</v>
+      </c>
+    </row>
+    <row r="163" spans="1:21" ht="14.25">
+      <c r="A163" t="s">
+        <v>1183</v>
+      </c>
+      <c r="B163" t="s">
+        <v>1188</v>
+      </c>
+      <c r="C163" t="s">
+        <v>1184</v>
+      </c>
+      <c r="D163" t="s">
+        <v>84</v>
+      </c>
+      <c r="E163" t="s">
+        <v>78</v>
+      </c>
+      <c r="F163" t="s">
         <v>79</v>
       </c>
-      <c r="G159" t="s">
-        <v>221</v>
-      </c>
-      <c r="H159" t="s">
-        <v>1160</v>
-      </c>
-      <c r="I159" t="s">
+      <c r="G163" t="s">
+        <v>85</v>
+      </c>
+      <c r="H163" t="s">
+        <v>1185</v>
+      </c>
+      <c r="I163" t="s">
         <v>198</v>
       </c>
-      <c r="K159" t="s">
-        <v>1161</v>
-      </c>
-      <c r="L159" t="s">
-        <v>1162</v>
-      </c>
-      <c r="M159" t="s">
+      <c r="K163" t="s">
+        <v>199</v>
+      </c>
+      <c r="L163" t="s">
+        <v>1186</v>
+      </c>
+      <c r="M163" t="s">
+        <v>201</v>
+      </c>
+      <c r="N163" t="s">
         <v>202</v>
       </c>
-      <c r="N159" t="s">
-        <v>266</v>
-      </c>
-      <c r="P159" t="s">
-        <v>199</v>
-      </c>
-      <c r="Q159" t="s">
-        <v>199</v>
-      </c>
-      <c r="R159" t="s">
-        <v>1159</v>
-      </c>
-      <c r="S159" t="s">
-        <v>1163</v>
-      </c>
-      <c r="T159" t="s">
+      <c r="P163" t="s">
+        <v>203</v>
+      </c>
+      <c r="Q163" t="s">
+        <v>204</v>
+      </c>
+      <c r="R163" t="s">
+        <v>1184</v>
+      </c>
+      <c r="S163" t="s">
+        <v>1187</v>
+      </c>
+      <c r="T163" s="24" t="s">
         <v>687</v>
       </c>
-      <c r="U159" t="s">
-        <v>16</v>
+      <c r="U163" t="s">
+        <v>1044</v>
       </c>
     </row>
   </sheetData>
   <autoFilter ref="E1:E145" xr:uid="{00000000-0001-0000-0100-000000000000}"/>
   <customSheetViews>
-    <customSheetView filter="1" guid="{C25CEB9E-BEC1-4982-90C4-50C84EE1B82A}" showAutoFilter="1">
-      <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
-      <autoFilter ref="A1:AD33" xr:uid="{0A09162B-B056-45C1-A5F4-D61AF69BF35A}"/>
+    <customSheetView guid="{C25CEB9E-BEC1-4982-90C4-50C84EE1B82A}" filter="1" showAutoFilter="1">
+      <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+      <autoFilter ref="A1:AD33" xr:uid="{00FAB4A9-34EA-42C1-BA21-FBBF4B768B91}"/>
     </customSheetView>
-    <customSheetView filter="1" guid="{A7754112-A52F-4ABC-8778-92F04773E53C}" showAutoFilter="1">
-      <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
-      <autoFilter ref="A1:AD33" xr:uid="{8908FC95-D4CB-42E8-A173-8FB8D214DC0F}">
+    <customSheetView guid="{A7754112-A52F-4ABC-8778-92F04773E53C}" filter="1" showAutoFilter="1">
+      <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+      <autoFilter ref="A1:AD33" xr:uid="{DFFAF25E-37A5-42AB-A5E0-A5CED9A2DBF7}">
         <filterColumn colId="5">
           <filters blank="1">
             <filter val="Strathnairn"/>
@@ -20338,76 +20902,76 @@
     </customSheetView>
   </customSheetViews>
   <conditionalFormatting sqref="A1:AI1">
-    <cfRule dxfId="1" priority="1" type="notContainsBlanks">
+    <cfRule type="notContainsBlanks" dxfId="1" priority="1">
       <formula>LEN(TRIM(A1))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <hyperlinks>
-    <hyperlink r:id="rId1" ref="S2" xr:uid="{00000000-0004-0000-0100-000000000000}"/>
-    <hyperlink r:id="rId2" ref="S3" xr:uid="{00000000-0004-0000-0100-000001000000}"/>
-    <hyperlink r:id="rId3" ref="S4" xr:uid="{00000000-0004-0000-0100-000002000000}"/>
-    <hyperlink r:id="rId4" ref="S5" xr:uid="{00000000-0004-0000-0100-000003000000}"/>
-    <hyperlink r:id="rId5" ref="S6" xr:uid="{00000000-0004-0000-0100-000004000000}"/>
-    <hyperlink r:id="rId6" ref="S7" xr:uid="{00000000-0004-0000-0100-000006000000}"/>
-    <hyperlink r:id="rId7" ref="S8" xr:uid="{00000000-0004-0000-0100-000008000000}"/>
-    <hyperlink r:id="rId8" ref="S9" xr:uid="{00000000-0004-0000-0100-00000A000000}"/>
-    <hyperlink r:id="rId9" ref="S10" xr:uid="{00000000-0004-0000-0100-00000C000000}"/>
-    <hyperlink r:id="rId10" ref="S11" xr:uid="{00000000-0004-0000-0100-00000E000000}"/>
-    <hyperlink r:id="rId11" ref="S12" xr:uid="{00000000-0004-0000-0100-000010000000}"/>
-    <hyperlink r:id="rId12" ref="S14" xr:uid="{00000000-0004-0000-0100-000014000000}"/>
-    <hyperlink r:id="rId13" ref="S15" xr:uid="{00000000-0004-0000-0100-000016000000}"/>
-    <hyperlink r:id="rId14" ref="S16" xr:uid="{00000000-0004-0000-0100-000018000000}"/>
-    <hyperlink r:id="rId15" ref="S17" xr:uid="{00000000-0004-0000-0100-00001A000000}"/>
-    <hyperlink r:id="rId16" ref="S18" xr:uid="{00000000-0004-0000-0100-00001C000000}"/>
-    <hyperlink display="https://www.allhomes.com.au/strathnairn-act-2615?tid=178720657" r:id="rId17" ref="S19" xr:uid="{00000000-0004-0000-0100-00001E000000}"/>
-    <hyperlink r:id="rId18" ref="S20" xr:uid="{00000000-0004-0000-0100-000020000000}"/>
-    <hyperlink r:id="rId19" ref="S21" xr:uid="{00000000-0004-0000-0100-000022000000}"/>
-    <hyperlink r:id="rId20" ref="S22" xr:uid="{00000000-0004-0000-0100-000024000000}"/>
-    <hyperlink r:id="rId21" ref="S32" xr:uid="{00000000-0004-0000-0100-000031000000}"/>
-    <hyperlink r:id="rId22" ref="S31" xr:uid="{00000000-0004-0000-0100-000030000000}"/>
-    <hyperlink r:id="rId23" ref="S30" xr:uid="{00000000-0004-0000-0100-00002F000000}"/>
-    <hyperlink r:id="rId24" ref="S29" xr:uid="{00000000-0004-0000-0100-00002E000000}"/>
-    <hyperlink r:id="rId25" ref="S28" xr:uid="{00000000-0004-0000-0100-00002D000000}"/>
-    <hyperlink r:id="rId26" ref="S27" xr:uid="{00000000-0004-0000-0100-00002C000000}"/>
-    <hyperlink r:id="rId27" ref="S26" xr:uid="{00000000-0004-0000-0100-00002B000000}"/>
-    <hyperlink r:id="rId28" ref="S25" xr:uid="{00000000-0004-0000-0100-00002A000000}"/>
-    <hyperlink r:id="rId29" ref="S24" xr:uid="{00000000-0004-0000-0100-000028000000}"/>
-    <hyperlink display="https://www.allhomes.com.au/ginninderra-estate-act-2615?tid=174799089" r:id="rId30" ref="S23" xr:uid="{00000000-0004-0000-0100-000026000000}"/>
-    <hyperlink display="https://www.allhomes.com.au/browse-sale/greater-queanbeyan-queanbeyan-region-nsw/" r:id="rId31" ref="F145" xr:uid="{4A50D1D1-69A3-4F14-AFDA-4A60EE9976C1}"/>
+    <hyperlink ref="S2" r:id="rId1" xr:uid="{00000000-0004-0000-0100-000000000000}"/>
+    <hyperlink ref="S3" r:id="rId2" xr:uid="{00000000-0004-0000-0100-000001000000}"/>
+    <hyperlink ref="S4" r:id="rId3" xr:uid="{00000000-0004-0000-0100-000002000000}"/>
+    <hyperlink ref="S5" r:id="rId4" xr:uid="{00000000-0004-0000-0100-000003000000}"/>
+    <hyperlink ref="S6" r:id="rId5" xr:uid="{00000000-0004-0000-0100-000004000000}"/>
+    <hyperlink ref="S7" r:id="rId6" xr:uid="{00000000-0004-0000-0100-000006000000}"/>
+    <hyperlink ref="S8" r:id="rId7" xr:uid="{00000000-0004-0000-0100-000008000000}"/>
+    <hyperlink ref="S9" r:id="rId8" xr:uid="{00000000-0004-0000-0100-00000A000000}"/>
+    <hyperlink ref="S10" r:id="rId9" xr:uid="{00000000-0004-0000-0100-00000C000000}"/>
+    <hyperlink ref="S11" r:id="rId10" xr:uid="{00000000-0004-0000-0100-00000E000000}"/>
+    <hyperlink ref="S12" r:id="rId11" xr:uid="{00000000-0004-0000-0100-000010000000}"/>
+    <hyperlink ref="S14" r:id="rId12" xr:uid="{00000000-0004-0000-0100-000014000000}"/>
+    <hyperlink ref="S15" r:id="rId13" xr:uid="{00000000-0004-0000-0100-000016000000}"/>
+    <hyperlink ref="S16" r:id="rId14" xr:uid="{00000000-0004-0000-0100-000018000000}"/>
+    <hyperlink ref="S17" r:id="rId15" xr:uid="{00000000-0004-0000-0100-00001A000000}"/>
+    <hyperlink ref="S18" r:id="rId16" xr:uid="{00000000-0004-0000-0100-00001C000000}"/>
+    <hyperlink ref="S19" r:id="rId17" display="https://www.allhomes.com.au/strathnairn-act-2615?tid=178720657" xr:uid="{00000000-0004-0000-0100-00001E000000}"/>
+    <hyperlink ref="S20" r:id="rId18" xr:uid="{00000000-0004-0000-0100-000020000000}"/>
+    <hyperlink ref="S21" r:id="rId19" xr:uid="{00000000-0004-0000-0100-000022000000}"/>
+    <hyperlink ref="S22" r:id="rId20" xr:uid="{00000000-0004-0000-0100-000024000000}"/>
+    <hyperlink ref="S32" r:id="rId21" xr:uid="{00000000-0004-0000-0100-000031000000}"/>
+    <hyperlink ref="S31" r:id="rId22" xr:uid="{00000000-0004-0000-0100-000030000000}"/>
+    <hyperlink ref="S30" r:id="rId23" xr:uid="{00000000-0004-0000-0100-00002F000000}"/>
+    <hyperlink ref="S29" r:id="rId24" xr:uid="{00000000-0004-0000-0100-00002E000000}"/>
+    <hyperlink ref="S28" r:id="rId25" xr:uid="{00000000-0004-0000-0100-00002D000000}"/>
+    <hyperlink ref="S27" r:id="rId26" xr:uid="{00000000-0004-0000-0100-00002C000000}"/>
+    <hyperlink ref="S26" r:id="rId27" xr:uid="{00000000-0004-0000-0100-00002B000000}"/>
+    <hyperlink ref="S25" r:id="rId28" xr:uid="{00000000-0004-0000-0100-00002A000000}"/>
+    <hyperlink ref="S24" r:id="rId29" xr:uid="{00000000-0004-0000-0100-000028000000}"/>
+    <hyperlink ref="S23" r:id="rId30" display="https://www.allhomes.com.au/ginninderra-estate-act-2615?tid=174799089" xr:uid="{00000000-0004-0000-0100-000026000000}"/>
+    <hyperlink ref="F145" r:id="rId31" display="https://www.allhomes.com.au/browse-sale/greater-queanbeyan-queanbeyan-region-nsw/" xr:uid="{4A50D1D1-69A3-4F14-AFDA-4A60EE9976C1}"/>
   </hyperlinks>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
-  <pageSetup orientation="portrait" paperSize="9" r:id="rId32"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId32"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:AJ1"/>
+  <dimension ref="A1:AI1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="14.42578125" defaultRowHeight="15.75"/>
+  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="16.0" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" width="14.5703125" collapsed="true"/>
-    <col min="4" max="4" customWidth="true" width="16.85546875" collapsed="true"/>
-    <col min="8" max="8" customWidth="true" width="14.5703125" collapsed="true"/>
-    <col min="9" max="9" customWidth="true" width="13.140625" collapsed="true"/>
-    <col min="15" max="15" customWidth="true" width="20.85546875" collapsed="true"/>
-    <col min="21" max="22" customWidth="true" width="19.140625" collapsed="true"/>
-    <col min="23" max="23" customWidth="true" width="20.140625" collapsed="true"/>
-    <col min="24" max="24" customWidth="true" width="19.85546875" collapsed="true"/>
-    <col min="26" max="26" customWidth="true" width="15.85546875" collapsed="true"/>
-    <col min="27" max="27" customWidth="true" width="13.42578125" collapsed="true"/>
-    <col min="28" max="28" customWidth="true" width="15.140625" collapsed="true"/>
-    <col min="29" max="29" customWidth="true" width="16.140625" collapsed="true"/>
-    <col min="30" max="30" customWidth="true" width="15.85546875" collapsed="true"/>
+    <col min="1" max="1" width="16" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="14.5703125" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="16.85546875" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="14.5703125" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="13.140625" customWidth="1" collapsed="1"/>
+    <col min="15" max="15" width="20.85546875" customWidth="1" collapsed="1"/>
+    <col min="21" max="22" width="19.140625" customWidth="1" collapsed="1"/>
+    <col min="23" max="23" width="20.140625" customWidth="1" collapsed="1"/>
+    <col min="24" max="24" width="19.85546875" customWidth="1" collapsed="1"/>
+    <col min="26" max="26" width="15.85546875" customWidth="1" collapsed="1"/>
+    <col min="27" max="27" width="13.42578125" customWidth="1" collapsed="1"/>
+    <col min="28" max="28" width="15.140625" customWidth="1" collapsed="1"/>
+    <col min="29" max="29" width="16.140625" customWidth="1" collapsed="1"/>
+    <col min="30" max="30" width="15.85546875" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row customHeight="1" ht="15.75" r="1" spans="1:35">
+    <row r="1" spans="1:35" ht="15.75" customHeight="1">
       <c r="A1" s="1" t="s">
         <v>46</v>
       </c>
@@ -20506,37 +21070,37 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A1:AI1">
-    <cfRule dxfId="0" priority="1" type="notContainsBlanks">
+    <cfRule type="notContainsBlanks" dxfId="0" priority="1">
       <formula>LEN(TRIM(A1))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
-  <pageSetup orientation="portrait" paperSize="9" r:id="rId1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:H7"/>
+  <dimension ref="A1:G7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane activePane="bottomLeft" state="frozen" topLeftCell="A2" ySplit="1"/>
-      <selection activeCell="D18" pane="bottomLeft" sqref="D18"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D18" sqref="D18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="14.42578125" defaultRowHeight="15.75"/>
+  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="44.85546875" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="19.5703125" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" width="26.42578125" collapsed="true"/>
-    <col min="4" max="4" customWidth="true" width="36.140625" collapsed="true"/>
-    <col min="5" max="5" bestFit="true" customWidth="true" width="53.7109375" collapsed="true"/>
+    <col min="1" max="1" width="44.85546875" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="19.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="26.42578125" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="36.140625" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="53.7109375" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row ht="15" r="1" spans="1:7">
+    <row r="1" spans="1:7" ht="15">
       <c r="A1" s="29" t="s">
         <v>152</v>
       </c>
@@ -20559,7 +21123,7 @@
         <v>157</v>
       </c>
     </row>
-    <row customFormat="1" customHeight="1" ht="15.75" r="2" s="30" spans="1:7">
+    <row r="2" spans="1:7" s="30" customFormat="1" ht="15.75" customHeight="1">
       <c r="A2" s="30" t="s">
         <v>158</v>
       </c>
@@ -20582,7 +21146,7 @@
         <v>7</v>
       </c>
     </row>
-    <row customHeight="1" ht="15.75" r="3" spans="1:7">
+    <row r="3" spans="1:7" ht="15.75" customHeight="1">
       <c r="A3" s="30" t="s">
         <v>161</v>
       </c>
@@ -20599,7 +21163,7 @@
         <v>17</v>
       </c>
     </row>
-    <row customHeight="1" ht="15.75" r="4" spans="1:7">
+    <row r="4" spans="1:7" ht="15.75" customHeight="1">
       <c r="A4" s="30" t="s">
         <v>164</v>
       </c>
@@ -20616,7 +21180,7 @@
         <v>38</v>
       </c>
     </row>
-    <row customHeight="1" ht="15.75" r="5" spans="1:7">
+    <row r="5" spans="1:7" ht="15.75" customHeight="1">
       <c r="A5" s="34" t="s">
         <v>167</v>
       </c>
@@ -20633,7 +21197,7 @@
         <v>9</v>
       </c>
     </row>
-    <row customHeight="1" ht="15.75" r="6" spans="1:7">
+    <row r="6" spans="1:7" ht="15.75" customHeight="1">
       <c r="A6" t="s">
         <v>328</v>
       </c>
@@ -20650,7 +21214,7 @@
         <v>323</v>
       </c>
     </row>
-    <row customHeight="1" ht="15.75" r="7" spans="1:7">
+    <row r="7" spans="1:7" ht="15.75" customHeight="1">
       <c r="A7" s="45" t="s">
         <v>877</v>
       </c>
@@ -20669,16 +21233,16 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink r:id="rId1" ref="E2" xr:uid="{00000000-0004-0000-0300-000000000000}"/>
-    <hyperlink r:id="rId2" ref="E3" xr:uid="{00000000-0004-0000-0300-000001000000}"/>
-    <hyperlink r:id="rId3" ref="E4" xr:uid="{00000000-0004-0000-0300-000002000000}"/>
-    <hyperlink r:id="rId4" ref="E5" xr:uid="{00000000-0004-0000-0300-000003000000}"/>
-    <hyperlink r:id="rId5" ref="D6" xr:uid="{00000000-0004-0000-0300-000004000000}"/>
-    <hyperlink r:id="rId6" ref="E6" xr:uid="{00000000-0004-0000-0300-000005000000}"/>
-    <hyperlink r:id="rId7" ref="D7" xr:uid="{B34712F5-65E4-4DA3-B4D8-B5E126A91A19}"/>
-    <hyperlink r:id="rId8" ref="E7" xr:uid="{FAD2E722-F8D2-45E6-8DA2-DA530385A188}"/>
+    <hyperlink ref="E2" r:id="rId1" xr:uid="{00000000-0004-0000-0300-000000000000}"/>
+    <hyperlink ref="E3" r:id="rId2" xr:uid="{00000000-0004-0000-0300-000001000000}"/>
+    <hyperlink ref="E4" r:id="rId3" xr:uid="{00000000-0004-0000-0300-000002000000}"/>
+    <hyperlink ref="E5" r:id="rId4" xr:uid="{00000000-0004-0000-0300-000003000000}"/>
+    <hyperlink ref="D6" r:id="rId5" xr:uid="{00000000-0004-0000-0300-000004000000}"/>
+    <hyperlink ref="E6" r:id="rId6" xr:uid="{00000000-0004-0000-0300-000005000000}"/>
+    <hyperlink ref="D7" r:id="rId7" xr:uid="{B34712F5-65E4-4DA3-B4D8-B5E126A91A19}"/>
+    <hyperlink ref="E7" r:id="rId8" xr:uid="{FAD2E722-F8D2-45E6-8DA2-DA530385A188}"/>
   </hyperlinks>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
-  <pageSetup orientation="portrait" paperSize="9" r:id="rId9"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId9"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Update existing listing 12/10/2021
</commit_message>
<xml_diff>
--- a/src/main/resources/InputTestdata/Listing details.xlsx
+++ b/src/main/resources/InputTestdata/Listing details.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Athavan\git\777Homes-2\777Homes-business\src\main\resources\InputTestdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1608F607-FAE3-448C-80C1-D1B35D977F9E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B39E9B6F-C49E-4AD7-A91B-8CCFABB608E6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="20715" windowHeight="13276" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Backlog" sheetId="1" r:id="rId1"/>
@@ -26,8 +26,8 @@
   </definedNames>
   <calcPr calcId="181029"/>
   <customWorkbookViews>
+    <customWorkbookView name="Filter 2" guid="{C25CEB9E-BEC1-4982-90C4-50C84EE1B82A}" maximized="1" windowWidth="0" windowHeight="0" activeSheetId="0"/>
     <customWorkbookView name="Filter 1" guid="{A7754112-A52F-4ABC-8778-92F04773E53C}" maximized="1" windowWidth="0" windowHeight="0" activeSheetId="0"/>
-    <customWorkbookView name="Filter 2" guid="{C25CEB9E-BEC1-4982-90C4-50C84EE1B82A}" maximized="1" windowWidth="0" windowHeight="0" activeSheetId="0"/>
   </customWorkbookViews>
 </workbook>
 </file>
@@ -6548,26 +6548,26 @@
   </sheetPr>
   <dimension ref="A1:AB164"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A131" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E166" sqref="E166"/>
+      <selection pane="bottomLeft" activeCell="D154" sqref="D154"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="14.3984375" defaultRowHeight="15.75" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="9.140625" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="74.85546875" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" width="9.1328125" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="74.86328125" customWidth="1" collapsed="1"/>
     <col min="3" max="3" width="75" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="14.5703125" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="22.140625" style="37" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="21.85546875" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="56.85546875" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="10.85546875" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="17.85546875" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="22.5703125" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="14.59765625" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="22.1328125" style="37" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="21.86328125" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="56.86328125" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="10.86328125" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="17.86328125" customWidth="1" collapsed="1"/>
+    <col min="11" max="11" width="22.59765625" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:28" ht="15">
+    <row r="1" spans="1:28" ht="13.9">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -6640,7 +6640,7 @@
       <c r="AA2" s="6"/>
       <c r="AB2" s="6"/>
     </row>
-    <row r="3" spans="1:28" ht="14.25">
+    <row r="3" spans="1:28" ht="13.9">
       <c r="A3" s="2">
         <v>2</v>
       </c>
@@ -6732,7 +6732,7 @@
       <c r="AA4" s="6"/>
       <c r="AB4" s="6"/>
     </row>
-    <row r="5" spans="1:28" ht="14.25">
+    <row r="5" spans="1:28" ht="13.9">
       <c r="A5" s="9">
         <v>4</v>
       </c>
@@ -6776,7 +6776,7 @@
       <c r="AA5" s="6"/>
       <c r="AB5" s="6"/>
     </row>
-    <row r="6" spans="1:28" ht="14.25">
+    <row r="6" spans="1:28" ht="13.9">
       <c r="A6" s="9">
         <v>5</v>
       </c>
@@ -6820,7 +6820,7 @@
       <c r="AA6" s="9"/>
       <c r="AB6" s="9"/>
     </row>
-    <row r="7" spans="1:28" ht="14.25">
+    <row r="7" spans="1:28" ht="13.9">
       <c r="A7" s="9">
         <v>6</v>
       </c>
@@ -6864,7 +6864,7 @@
       <c r="AA7" s="6"/>
       <c r="AB7" s="6"/>
     </row>
-    <row r="8" spans="1:28" ht="14.25">
+    <row r="8" spans="1:28" ht="13.9">
       <c r="A8" s="9">
         <v>7</v>
       </c>
@@ -6908,7 +6908,7 @@
       <c r="AA8" s="6"/>
       <c r="AB8" s="6"/>
     </row>
-    <row r="9" spans="1:28" ht="14.25">
+    <row r="9" spans="1:28" ht="13.9">
       <c r="A9" s="9">
         <v>8</v>
       </c>
@@ -6950,7 +6950,7 @@
       <c r="AA9" s="6"/>
       <c r="AB9" s="6"/>
     </row>
-    <row r="10" spans="1:28" ht="14.25">
+    <row r="10" spans="1:28" ht="13.9">
       <c r="A10" s="9">
         <v>9</v>
       </c>
@@ -6992,7 +6992,7 @@
       <c r="AA10" s="6"/>
       <c r="AB10" s="6"/>
     </row>
-    <row r="11" spans="1:28" ht="14.25">
+    <row r="11" spans="1:28" ht="13.9">
       <c r="A11" s="9">
         <v>10</v>
       </c>
@@ -7036,7 +7036,7 @@
       <c r="AA11" s="6"/>
       <c r="AB11" s="6"/>
     </row>
-    <row r="12" spans="1:28" ht="14.25">
+    <row r="12" spans="1:28" ht="13.9">
       <c r="A12" s="9">
         <v>11</v>
       </c>
@@ -7078,7 +7078,7 @@
       <c r="AA12" s="6"/>
       <c r="AB12" s="6"/>
     </row>
-    <row r="13" spans="1:28" ht="14.25">
+    <row r="13" spans="1:28" ht="13.9">
       <c r="A13" s="9">
         <v>12</v>
       </c>
@@ -7120,7 +7120,7 @@
       <c r="AA13" s="6"/>
       <c r="AB13" s="6"/>
     </row>
-    <row r="14" spans="1:28" ht="14.25">
+    <row r="14" spans="1:28" ht="13.9">
       <c r="A14" s="9">
         <v>13</v>
       </c>
@@ -7162,7 +7162,7 @@
       <c r="AA14" s="6"/>
       <c r="AB14" s="6"/>
     </row>
-    <row r="15" spans="1:28" ht="14.25">
+    <row r="15" spans="1:28" ht="13.9">
       <c r="A15" s="9">
         <v>14</v>
       </c>
@@ -7206,7 +7206,7 @@
       <c r="AA15" s="6"/>
       <c r="AB15" s="6"/>
     </row>
-    <row r="16" spans="1:28" ht="14.25">
+    <row r="16" spans="1:28" ht="13.9">
       <c r="A16" s="9">
         <v>15</v>
       </c>
@@ -7248,7 +7248,7 @@
       <c r="AA16" s="6"/>
       <c r="AB16" s="6"/>
     </row>
-    <row r="17" spans="1:28" ht="14.25">
+    <row r="17" spans="1:28" ht="13.9">
       <c r="A17" s="9">
         <v>16</v>
       </c>
@@ -7292,7 +7292,7 @@
       <c r="AA17" s="6"/>
       <c r="AB17" s="6"/>
     </row>
-    <row r="18" spans="1:28" ht="14.25">
+    <row r="18" spans="1:28" ht="13.9">
       <c r="A18" s="9">
         <v>17</v>
       </c>
@@ -7334,7 +7334,7 @@
       <c r="AA18" s="6"/>
       <c r="AB18" s="6"/>
     </row>
-    <row r="19" spans="1:28" ht="14.25">
+    <row r="19" spans="1:28" ht="13.9">
       <c r="A19" s="9">
         <v>18</v>
       </c>
@@ -7378,7 +7378,7 @@
       <c r="AA19" s="6"/>
       <c r="AB19" s="6"/>
     </row>
-    <row r="20" spans="1:28" ht="14.25">
+    <row r="20" spans="1:28" ht="13.9">
       <c r="A20" s="9">
         <v>19</v>
       </c>
@@ -7422,7 +7422,7 @@
       <c r="AA20" s="6"/>
       <c r="AB20" s="6"/>
     </row>
-    <row r="21" spans="1:28" ht="14.25">
+    <row r="21" spans="1:28" ht="13.9">
       <c r="A21" s="9">
         <v>20</v>
       </c>
@@ -7466,7 +7466,7 @@
       <c r="AA21" s="6"/>
       <c r="AB21" s="6"/>
     </row>
-    <row r="22" spans="1:28" ht="14.25">
+    <row r="22" spans="1:28" ht="13.9">
       <c r="A22" s="9">
         <v>21</v>
       </c>
@@ -7508,7 +7508,7 @@
       <c r="AA22" s="6"/>
       <c r="AB22" s="6"/>
     </row>
-    <row r="23" spans="1:28" ht="14.25">
+    <row r="23" spans="1:28" ht="13.9">
       <c r="A23" s="9">
         <v>22</v>
       </c>
@@ -7552,7 +7552,7 @@
       <c r="AA23" s="6"/>
       <c r="AB23" s="6"/>
     </row>
-    <row r="24" spans="1:28" ht="14.25">
+    <row r="24" spans="1:28" ht="13.9">
       <c r="A24" s="9">
         <v>23</v>
       </c>
@@ -7594,7 +7594,7 @@
       <c r="AA24" s="6"/>
       <c r="AB24" s="6"/>
     </row>
-    <row r="25" spans="1:28" ht="14.25">
+    <row r="25" spans="1:28" ht="13.9">
       <c r="A25" s="9">
         <v>24</v>
       </c>
@@ -7636,7 +7636,7 @@
       <c r="AA25" s="6"/>
       <c r="AB25" s="6"/>
     </row>
-    <row r="26" spans="1:28" ht="14.25">
+    <row r="26" spans="1:28" ht="13.9">
       <c r="A26" s="9">
         <v>25</v>
       </c>
@@ -7680,7 +7680,7 @@
       <c r="AA26" s="6"/>
       <c r="AB26" s="6"/>
     </row>
-    <row r="27" spans="1:28" ht="14.25">
+    <row r="27" spans="1:28" ht="13.9">
       <c r="A27" s="9">
         <v>26</v>
       </c>
@@ -7724,7 +7724,7 @@
       <c r="AA27" s="6"/>
       <c r="AB27" s="6"/>
     </row>
-    <row r="28" spans="1:28" ht="14.25">
+    <row r="28" spans="1:28" ht="13.9">
       <c r="A28" s="9">
         <v>27</v>
       </c>
@@ -7766,7 +7766,7 @@
       <c r="AA28" s="6"/>
       <c r="AB28" s="6"/>
     </row>
-    <row r="29" spans="1:28" ht="14.25">
+    <row r="29" spans="1:28" ht="13.9">
       <c r="A29" s="9">
         <v>28</v>
       </c>
@@ -7810,7 +7810,7 @@
       <c r="AA29" s="6"/>
       <c r="AB29" s="6"/>
     </row>
-    <row r="30" spans="1:28" ht="14.25">
+    <row r="30" spans="1:28" ht="13.9">
       <c r="A30" s="9">
         <v>29</v>
       </c>
@@ -7852,7 +7852,7 @@
       <c r="AA30" s="6"/>
       <c r="AB30" s="6"/>
     </row>
-    <row r="31" spans="1:28" ht="14.25">
+    <row r="31" spans="1:28" ht="13.9">
       <c r="A31" s="4">
         <v>30</v>
       </c>
@@ -7896,7 +7896,7 @@
       <c r="AA31" s="6"/>
       <c r="AB31" s="6"/>
     </row>
-    <row r="32" spans="1:28" ht="14.25">
+    <row r="32" spans="1:28" ht="13.9">
       <c r="A32" s="4">
         <v>31</v>
       </c>
@@ -7938,7 +7938,7 @@
       <c r="AA32" s="6"/>
       <c r="AB32" s="6"/>
     </row>
-    <row r="33" spans="1:8" s="4" customFormat="1" ht="14.25">
+    <row r="33" spans="1:8" s="4" customFormat="1" ht="13.9">
       <c r="A33" s="4">
         <v>32</v>
       </c>
@@ -7961,7 +7961,7 @@
         <v>427</v>
       </c>
     </row>
-    <row r="34" spans="1:8" s="4" customFormat="1" ht="14.25">
+    <row r="34" spans="1:8" s="4" customFormat="1" ht="13.9">
       <c r="A34" s="4">
         <v>33</v>
       </c>
@@ -7981,7 +7981,7 @@
         <v>427</v>
       </c>
     </row>
-    <row r="35" spans="1:8" s="4" customFormat="1" ht="14.25">
+    <row r="35" spans="1:8" s="4" customFormat="1" ht="13.9">
       <c r="A35" s="4">
         <v>34</v>
       </c>
@@ -8001,7 +8001,7 @@
         <v>427</v>
       </c>
     </row>
-    <row r="36" spans="1:8" s="4" customFormat="1" ht="14.25">
+    <row r="36" spans="1:8" s="4" customFormat="1" ht="13.9">
       <c r="A36" s="4">
         <v>35</v>
       </c>
@@ -8021,7 +8021,7 @@
         <v>427</v>
       </c>
     </row>
-    <row r="37" spans="1:8" s="4" customFormat="1" ht="14.25">
+    <row r="37" spans="1:8" s="4" customFormat="1" ht="13.9">
       <c r="A37" s="4">
         <v>36</v>
       </c>
@@ -8041,7 +8041,7 @@
         <v>427</v>
       </c>
     </row>
-    <row r="38" spans="1:8" s="4" customFormat="1" ht="14.25">
+    <row r="38" spans="1:8" s="4" customFormat="1" ht="13.5">
       <c r="A38" s="4">
         <v>37</v>
       </c>
@@ -8064,7 +8064,7 @@
         <v>427</v>
       </c>
     </row>
-    <row r="39" spans="1:8" s="4" customFormat="1" ht="14.25">
+    <row r="39" spans="1:8" s="4" customFormat="1" ht="13.9">
       <c r="A39" s="4">
         <v>38</v>
       </c>
@@ -8087,7 +8087,7 @@
         <v>427</v>
       </c>
     </row>
-    <row r="40" spans="1:8" s="4" customFormat="1" ht="14.25">
+    <row r="40" spans="1:8" s="4" customFormat="1" ht="13.5">
       <c r="A40" s="4">
         <v>39</v>
       </c>
@@ -8110,7 +8110,7 @@
         <v>427</v>
       </c>
     </row>
-    <row r="41" spans="1:8" s="4" customFormat="1" ht="14.25">
+    <row r="41" spans="1:8" s="4" customFormat="1" ht="13.9">
       <c r="A41" s="4">
         <v>40</v>
       </c>
@@ -8130,7 +8130,7 @@
         <v>427</v>
       </c>
     </row>
-    <row r="42" spans="1:8" s="4" customFormat="1" ht="14.25">
+    <row r="42" spans="1:8" s="4" customFormat="1" ht="13.5">
       <c r="A42" s="4">
         <v>41</v>
       </c>
@@ -8153,7 +8153,7 @@
         <v>427</v>
       </c>
     </row>
-    <row r="43" spans="1:8" s="4" customFormat="1" ht="14.25">
+    <row r="43" spans="1:8" s="4" customFormat="1" ht="13.5">
       <c r="A43" s="4">
         <v>42</v>
       </c>
@@ -8173,7 +8173,7 @@
         <v>427</v>
       </c>
     </row>
-    <row r="44" spans="1:8" s="4" customFormat="1" ht="14.25">
+    <row r="44" spans="1:8" s="4" customFormat="1" ht="13.5">
       <c r="A44" s="4">
         <v>43</v>
       </c>
@@ -8193,7 +8193,7 @@
         <v>427</v>
       </c>
     </row>
-    <row r="45" spans="1:8" s="4" customFormat="1" ht="14.25">
+    <row r="45" spans="1:8" s="4" customFormat="1" ht="13.5">
       <c r="A45" s="4">
         <v>44</v>
       </c>
@@ -8216,7 +8216,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="46" spans="1:8" s="4" customFormat="1" ht="14.25">
+    <row r="46" spans="1:8" s="4" customFormat="1" ht="13.5">
       <c r="A46" s="4">
         <v>45</v>
       </c>
@@ -8236,7 +8236,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="47" spans="1:8" s="4" customFormat="1" ht="14.25">
+    <row r="47" spans="1:8" s="4" customFormat="1" ht="13.5">
       <c r="A47" s="4">
         <v>46</v>
       </c>
@@ -8302,7 +8302,7 @@
         <v>428</v>
       </c>
     </row>
-    <row r="50" spans="1:8" s="4" customFormat="1" ht="12.75">
+    <row r="50" spans="1:8" s="4" customFormat="1" ht="13.15">
       <c r="A50" s="4">
         <v>49</v>
       </c>
@@ -8322,7 +8322,7 @@
         <v>428</v>
       </c>
     </row>
-    <row r="51" spans="1:8" s="4" customFormat="1" ht="12.75">
+    <row r="51" spans="1:8" s="4" customFormat="1" ht="13.15">
       <c r="A51" s="4">
         <v>50</v>
       </c>
@@ -8342,7 +8342,7 @@
         <v>428</v>
       </c>
     </row>
-    <row r="52" spans="1:8" s="4" customFormat="1" ht="12.75">
+    <row r="52" spans="1:8" s="4" customFormat="1" ht="13.15">
       <c r="A52" s="4">
         <v>51</v>
       </c>
@@ -8388,7 +8388,7 @@
         <v>323</v>
       </c>
     </row>
-    <row r="54" spans="1:8" s="4" customFormat="1" ht="12.75">
+    <row r="54" spans="1:8" s="4" customFormat="1" ht="13.15">
       <c r="A54" s="4">
         <v>53</v>
       </c>
@@ -10206,13 +10206,13 @@
       <c r="A134">
         <v>133</v>
       </c>
-      <c r="B134" t="s">
+      <c r="B134" s="41" t="s">
         <v>896</v>
       </c>
-      <c r="C134" t="s">
+      <c r="C134" s="41" t="s">
         <v>1033</v>
       </c>
-      <c r="D134" s="4" t="s">
+      <c r="D134" s="39" t="s">
         <v>14</v>
       </c>
       <c r="F134" s="2" t="s">
@@ -10439,11 +10439,11 @@
       <c r="B144" s="41" t="s">
         <v>1049</v>
       </c>
-      <c r="C144" t="s">
+      <c r="C144" s="41" t="s">
         <v>1060</v>
       </c>
-      <c r="D144" s="4" t="s">
-        <v>7</v>
+      <c r="D144" s="39" t="s">
+        <v>14</v>
       </c>
       <c r="F144" s="2" t="s">
         <v>1046</v>
@@ -10511,8 +10511,8 @@
       <c r="C147" s="41" t="s">
         <v>1091</v>
       </c>
-      <c r="D147" s="4" t="s">
-        <v>7</v>
+      <c r="D147" s="39" t="s">
+        <v>14</v>
       </c>
       <c r="F147" s="2" t="s">
         <v>1046</v>
@@ -10534,8 +10534,8 @@
       <c r="C148" s="41" t="s">
         <v>1088</v>
       </c>
-      <c r="D148" s="4" t="s">
-        <v>7</v>
+      <c r="D148" s="39" t="s">
+        <v>14</v>
       </c>
       <c r="F148" s="2" t="s">
         <v>687</v>
@@ -10672,8 +10672,8 @@
       <c r="C154" s="41" t="s">
         <v>1145</v>
       </c>
-      <c r="D154" s="4" t="s">
-        <v>7</v>
+      <c r="D154" s="39" t="s">
+        <v>14</v>
       </c>
       <c r="F154" s="2" t="s">
         <v>1046</v>
@@ -11118,9 +11118,12 @@
     <hyperlink ref="B163" r:id="rId205" xr:uid="{2BE3F178-27B5-4713-8C5F-C46B5E783D4B}"/>
     <hyperlink ref="C164" r:id="rId206" xr:uid="{9A258B3C-BD23-4F5F-AE50-05C1EFD794FE}"/>
     <hyperlink ref="B164" r:id="rId207" xr:uid="{1CBCDC47-F789-4E9E-A3E5-6986BA7DF67A}"/>
+    <hyperlink ref="B134" r:id="rId208" xr:uid="{62E8D2B3-CF6E-4F5B-8831-F7ABFCBF12C6}"/>
+    <hyperlink ref="C134" r:id="rId209" xr:uid="{67FE63AE-FF52-4665-98A8-947B6D32A39A}"/>
+    <hyperlink ref="C144" r:id="rId210" xr:uid="{DB9C0A49-9F31-4CC1-A80A-79CD0938E90B}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId208"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId211"/>
 </worksheet>
 </file>
 
@@ -11131,34 +11134,34 @@
   </sheetPr>
   <dimension ref="A1:AI163"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A134" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D166" sqref="D166"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A140" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E154" sqref="E154"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="14.3984375" defaultRowHeight="15.75" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="14.85546875" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="18.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="55.5703125" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="25.140625" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="19.5703125" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="19.85546875" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="18.5703125" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="32.140625" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="20.5703125" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="21.140625" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="28.85546875" customWidth="1" collapsed="1"/>
-    <col min="12" max="12" width="37.5703125" customWidth="1" collapsed="1"/>
-    <col min="16" max="17" width="18.85546875" customWidth="1" collapsed="1"/>
-    <col min="18" max="18" width="47.85546875" customWidth="1" collapsed="1"/>
-    <col min="19" max="19" width="77.5703125" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" width="14.86328125" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="18.1328125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="55.59765625" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="25.1328125" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="19.59765625" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="19.86328125" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="18.59765625" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="32.1328125" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="20.59765625" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="21.1328125" customWidth="1" collapsed="1"/>
+    <col min="11" max="11" width="28.86328125" customWidth="1" collapsed="1"/>
+    <col min="12" max="12" width="37.59765625" customWidth="1" collapsed="1"/>
+    <col min="16" max="17" width="18.86328125" customWidth="1" collapsed="1"/>
+    <col min="18" max="18" width="47.86328125" customWidth="1" collapsed="1"/>
+    <col min="19" max="19" width="77.59765625" customWidth="1" collapsed="1"/>
     <col min="20" max="20" width="24" customWidth="1" collapsed="1"/>
-    <col min="21" max="21" width="18.85546875" customWidth="1" collapsed="1"/>
-    <col min="22" max="31" width="19.140625" customWidth="1" collapsed="1"/>
+    <col min="21" max="21" width="18.86328125" customWidth="1" collapsed="1"/>
+    <col min="22" max="31" width="19.1328125" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:35" ht="30">
+    <row r="1" spans="1:35" ht="27.75">
       <c r="A1" s="1" t="s">
         <v>46</v>
       </c>
@@ -13146,7 +13149,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="33" spans="1:21" s="24" customFormat="1" ht="14.25">
+    <row r="33" spans="1:21" s="24" customFormat="1" ht="13.5">
       <c r="A33" s="24" t="s">
         <v>195</v>
       </c>
@@ -13205,7 +13208,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="34" spans="1:21" s="24" customFormat="1" ht="14.25">
+    <row r="34" spans="1:21" s="24" customFormat="1" ht="13.5">
       <c r="A34" s="24" t="s">
         <v>206</v>
       </c>
@@ -13264,7 +13267,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="35" spans="1:21" s="24" customFormat="1" ht="14.25">
+    <row r="35" spans="1:21" s="24" customFormat="1" ht="13.5">
       <c r="A35" s="24" t="s">
         <v>213</v>
       </c>
@@ -13323,7 +13326,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="36" spans="1:21" s="24" customFormat="1" ht="14.25">
+    <row r="36" spans="1:21" s="24" customFormat="1" ht="13.5">
       <c r="A36" s="24" t="s">
         <v>219</v>
       </c>
@@ -13382,7 +13385,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="37" spans="1:21" s="24" customFormat="1" ht="14.25">
+    <row r="37" spans="1:21" s="24" customFormat="1" ht="13.5">
       <c r="A37" s="24" t="s">
         <v>226</v>
       </c>
@@ -13441,7 +13444,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="38" spans="1:21" s="24" customFormat="1" ht="14.25">
+    <row r="38" spans="1:21" s="24" customFormat="1" ht="13.5">
       <c r="A38" s="24" t="s">
         <v>232</v>
       </c>
@@ -13500,7 +13503,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="39" spans="1:21" s="24" customFormat="1" ht="14.25">
+    <row r="39" spans="1:21" s="24" customFormat="1" ht="13.5">
       <c r="A39" s="24" t="s">
         <v>240</v>
       </c>
@@ -13559,7 +13562,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="40" spans="1:21" s="24" customFormat="1" ht="14.25">
+    <row r="40" spans="1:21" s="24" customFormat="1" ht="13.5">
       <c r="A40" s="24" t="s">
         <v>243</v>
       </c>
@@ -13618,7 +13621,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="41" spans="1:21" s="24" customFormat="1" ht="14.25">
+    <row r="41" spans="1:21" s="24" customFormat="1" ht="13.5">
       <c r="A41" s="24" t="s">
         <v>246</v>
       </c>
@@ -13677,7 +13680,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="42" spans="1:21" s="24" customFormat="1" ht="14.25">
+    <row r="42" spans="1:21" s="24" customFormat="1" ht="13.5">
       <c r="A42" s="24" t="s">
         <v>255</v>
       </c>
@@ -13736,7 +13739,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="43" spans="1:21" s="24" customFormat="1" ht="14.25">
+    <row r="43" spans="1:21" s="24" customFormat="1" ht="13.5">
       <c r="A43" s="24" t="s">
         <v>259</v>
       </c>
@@ -13795,7 +13798,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="44" spans="1:21" s="24" customFormat="1" ht="14.25">
+    <row r="44" spans="1:21" s="24" customFormat="1" ht="13.5">
       <c r="A44" s="24" t="s">
         <v>268</v>
       </c>
@@ -13854,7 +13857,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="45" spans="1:21" s="24" customFormat="1" ht="14.25">
+    <row r="45" spans="1:21" s="24" customFormat="1" ht="13.5">
       <c r="A45" s="24" t="s">
         <v>275</v>
       </c>
@@ -13913,7 +13916,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="46" spans="1:21" s="24" customFormat="1" ht="14.25">
+    <row r="46" spans="1:21" s="24" customFormat="1" ht="13.5">
       <c r="A46" s="24" t="s">
         <v>281</v>
       </c>
@@ -13972,7 +13975,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="47" spans="1:21" s="24" customFormat="1" ht="14.25">
+    <row r="47" spans="1:21" s="24" customFormat="1" ht="13.5">
       <c r="A47" s="24" t="s">
         <v>287</v>
       </c>
@@ -14031,7 +14034,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="48" spans="1:21" s="24" customFormat="1" ht="14.25">
+    <row r="48" spans="1:21" s="24" customFormat="1" ht="13.5">
       <c r="A48" s="24" t="s">
         <v>293</v>
       </c>
@@ -14090,7 +14093,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="49" spans="1:21" s="24" customFormat="1" ht="14.25">
+    <row r="49" spans="1:21" s="24" customFormat="1" ht="13.5">
       <c r="A49" s="24" t="s">
         <v>298</v>
       </c>
@@ -14149,7 +14152,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="50" spans="1:21" s="24" customFormat="1" ht="14.25">
+    <row r="50" spans="1:21" s="24" customFormat="1" ht="13.5">
       <c r="A50" s="24" t="s">
         <v>304</v>
       </c>
@@ -14208,7 +14211,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="51" spans="1:21" s="24" customFormat="1" ht="14.25">
+    <row r="51" spans="1:21" s="24" customFormat="1" ht="13.5">
       <c r="A51" s="24" t="s">
         <v>310</v>
       </c>
@@ -14267,7 +14270,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="52" spans="1:21" s="24" customFormat="1" ht="14.25">
+    <row r="52" spans="1:21" s="24" customFormat="1" ht="13.5">
       <c r="A52" s="24" t="s">
         <v>316</v>
       </c>
@@ -14326,7 +14329,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="53" spans="1:21" s="24" customFormat="1" ht="14.25">
+    <row r="53" spans="1:21" s="24" customFormat="1" ht="13.5">
       <c r="A53" s="24" t="s">
         <v>343</v>
       </c>
@@ -14385,7 +14388,7 @@
         <v>325</v>
       </c>
     </row>
-    <row r="54" spans="1:21" s="24" customFormat="1" ht="14.25">
+    <row r="54" spans="1:21" s="24" customFormat="1" ht="13.5">
       <c r="A54" s="24" t="s">
         <v>349</v>
       </c>
@@ -14444,7 +14447,7 @@
         <v>325</v>
       </c>
     </row>
-    <row r="55" spans="1:21" s="24" customFormat="1" ht="14.25">
+    <row r="55" spans="1:21" s="24" customFormat="1" ht="13.5">
       <c r="A55" s="24" t="s">
         <v>353</v>
       </c>
@@ -14503,7 +14506,7 @@
         <v>325</v>
       </c>
     </row>
-    <row r="56" spans="1:21" s="24" customFormat="1" ht="14.25">
+    <row r="56" spans="1:21" s="24" customFormat="1" ht="13.5">
       <c r="A56" s="24" t="s">
         <v>359</v>
       </c>
@@ -14562,7 +14565,7 @@
         <v>325</v>
       </c>
     </row>
-    <row r="57" spans="1:21" s="24" customFormat="1" ht="14.25">
+    <row r="57" spans="1:21" s="24" customFormat="1" ht="13.5">
       <c r="A57" s="24" t="s">
         <v>364</v>
       </c>
@@ -14621,7 +14624,7 @@
         <v>325</v>
       </c>
     </row>
-    <row r="58" spans="1:21" s="24" customFormat="1" ht="14.25">
+    <row r="58" spans="1:21" s="24" customFormat="1" ht="13.5">
       <c r="A58" s="24" t="s">
         <v>371</v>
       </c>
@@ -14680,7 +14683,7 @@
         <v>325</v>
       </c>
     </row>
-    <row r="59" spans="1:21" s="24" customFormat="1" ht="14.25">
+    <row r="59" spans="1:21" s="24" customFormat="1" ht="13.5">
       <c r="A59" s="24" t="s">
         <v>377</v>
       </c>
@@ -14739,7 +14742,7 @@
         <v>325</v>
       </c>
     </row>
-    <row r="60" spans="1:21" s="24" customFormat="1" ht="14.25">
+    <row r="60" spans="1:21" s="24" customFormat="1" ht="13.5">
       <c r="A60" s="24" t="s">
         <v>384</v>
       </c>
@@ -14798,7 +14801,7 @@
         <v>325</v>
       </c>
     </row>
-    <row r="61" spans="1:21" s="24" customFormat="1" ht="14.25">
+    <row r="61" spans="1:21" s="24" customFormat="1" ht="13.5">
       <c r="A61" s="24" t="s">
         <v>391</v>
       </c>
@@ -14857,7 +14860,7 @@
         <v>325</v>
       </c>
     </row>
-    <row r="62" spans="1:21" s="24" customFormat="1" ht="14.25">
+    <row r="62" spans="1:21" s="24" customFormat="1" ht="13.5">
       <c r="A62" s="24" t="s">
         <v>397</v>
       </c>
@@ -14916,7 +14919,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="63" spans="1:21" s="24" customFormat="1" ht="14.25">
+    <row r="63" spans="1:21" s="24" customFormat="1" ht="13.5">
       <c r="A63" s="24" t="s">
         <v>400</v>
       </c>
@@ -14975,7 +14978,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="64" spans="1:21" s="24" customFormat="1" ht="14.25">
+    <row r="64" spans="1:21" s="24" customFormat="1" ht="13.5">
       <c r="A64" s="24" t="s">
         <v>405</v>
       </c>
@@ -15034,7 +15037,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="65" spans="1:21" s="24" customFormat="1" ht="14.25">
+    <row r="65" spans="1:21" s="24" customFormat="1" ht="13.5">
       <c r="A65" s="24" t="s">
         <v>411</v>
       </c>
@@ -15093,7 +15096,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="66" spans="1:21" s="24" customFormat="1" ht="14.25">
+    <row r="66" spans="1:21" s="24" customFormat="1" ht="13.5">
       <c r="A66" s="24" t="s">
         <v>416</v>
       </c>
@@ -15152,7 +15155,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="67" spans="1:21" s="24" customFormat="1" ht="14.25">
+    <row r="67" spans="1:21" s="24" customFormat="1" ht="13.5">
       <c r="A67" s="24" t="s">
         <v>422</v>
       </c>
@@ -15211,7 +15214,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="68" spans="1:21" s="24" customFormat="1" ht="14.25">
+    <row r="68" spans="1:21" s="24" customFormat="1" ht="13.5">
       <c r="A68" s="24" t="s">
         <v>483</v>
       </c>
@@ -15270,7 +15273,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="69" spans="1:21" s="24" customFormat="1" ht="14.25">
+    <row r="69" spans="1:21" s="24" customFormat="1" ht="13.5">
       <c r="A69" s="24" t="s">
         <v>488</v>
       </c>
@@ -15329,7 +15332,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="70" spans="1:21" s="24" customFormat="1" ht="14.25">
+    <row r="70" spans="1:21" s="24" customFormat="1" ht="13.5">
       <c r="A70" s="24" t="s">
         <v>490</v>
       </c>
@@ -15388,7 +15391,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="71" spans="1:21" s="24" customFormat="1" ht="14.25">
+    <row r="71" spans="1:21" s="24" customFormat="1" ht="13.5">
       <c r="A71" s="24" t="s">
         <v>496</v>
       </c>
@@ -15447,7 +15450,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="72" spans="1:21" s="24" customFormat="1" ht="14.25">
+    <row r="72" spans="1:21" s="24" customFormat="1" ht="13.5">
       <c r="A72" s="24" t="s">
         <v>501</v>
       </c>
@@ -15506,7 +15509,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="73" spans="1:21" s="24" customFormat="1" ht="14.25">
+    <row r="73" spans="1:21" s="24" customFormat="1" ht="13.5">
       <c r="A73" s="24" t="s">
         <v>503</v>
       </c>
@@ -15565,7 +15568,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="74" spans="1:21" s="24" customFormat="1" ht="14.25">
+    <row r="74" spans="1:21" s="24" customFormat="1" ht="13.5">
       <c r="A74" s="24" t="s">
         <v>507</v>
       </c>
@@ -15624,7 +15627,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="75" spans="1:21" s="24" customFormat="1" ht="14.25">
+    <row r="75" spans="1:21" s="24" customFormat="1" ht="13.5">
       <c r="A75" s="24" t="s">
         <v>513</v>
       </c>
@@ -15683,7 +15686,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="76" spans="1:21" s="24" customFormat="1" ht="14.25">
+    <row r="76" spans="1:21" s="24" customFormat="1" ht="13.5">
       <c r="A76" s="24" t="s">
         <v>519</v>
       </c>
@@ -15742,7 +15745,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="77" spans="1:21" s="24" customFormat="1" ht="14.25">
+    <row r="77" spans="1:21" s="24" customFormat="1" ht="13.5">
       <c r="A77" s="24" t="s">
         <v>524</v>
       </c>
@@ -15801,7 +15804,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="78" spans="1:21" s="24" customFormat="1" ht="14.25">
+    <row r="78" spans="1:21" s="24" customFormat="1" ht="13.5">
       <c r="A78" s="24" t="s">
         <v>531</v>
       </c>
@@ -15860,7 +15863,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="79" spans="1:21" s="24" customFormat="1" ht="14.25">
+    <row r="79" spans="1:21" s="24" customFormat="1" ht="13.5">
       <c r="A79" s="24" t="s">
         <v>534</v>
       </c>
@@ -15919,7 +15922,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="80" spans="1:21" s="24" customFormat="1" ht="14.25">
+    <row r="80" spans="1:21" s="24" customFormat="1" ht="13.5">
       <c r="A80" s="24" t="s">
         <v>540</v>
       </c>
@@ -15978,7 +15981,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="81" spans="1:21" s="24" customFormat="1" ht="14.25">
+    <row r="81" spans="1:21" s="24" customFormat="1" ht="13.5">
       <c r="A81" s="24" t="s">
         <v>547</v>
       </c>
@@ -16037,7 +16040,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="82" spans="1:21" s="24" customFormat="1" ht="14.25">
+    <row r="82" spans="1:21" s="24" customFormat="1" ht="13.5">
       <c r="A82" s="24" t="s">
         <v>552</v>
       </c>
@@ -16096,7 +16099,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="83" spans="1:21" s="24" customFormat="1" ht="14.25">
+    <row r="83" spans="1:21" s="24" customFormat="1" ht="13.5">
       <c r="A83" s="24" t="s">
         <v>557</v>
       </c>
@@ -16155,7 +16158,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="84" spans="1:21" s="24" customFormat="1" ht="14.25">
+    <row r="84" spans="1:21" s="24" customFormat="1" ht="13.5">
       <c r="A84" s="24" t="s">
         <v>560</v>
       </c>
@@ -16214,7 +16217,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="85" spans="1:21" s="24" customFormat="1" ht="14.25">
+    <row r="85" spans="1:21" s="24" customFormat="1" ht="13.5">
       <c r="A85" s="24" t="s">
         <v>564</v>
       </c>
@@ -16273,7 +16276,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="86" spans="1:21" s="24" customFormat="1" ht="14.25">
+    <row r="86" spans="1:21" s="24" customFormat="1" ht="13.5">
       <c r="A86" s="24" t="s">
         <v>605</v>
       </c>
@@ -16332,7 +16335,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="87" spans="1:21" s="24" customFormat="1" ht="14.25">
+    <row r="87" spans="1:21" s="24" customFormat="1" ht="13.5">
       <c r="A87" s="24" t="s">
         <v>609</v>
       </c>
@@ -16391,7 +16394,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="88" spans="1:21" s="24" customFormat="1" ht="14.25">
+    <row r="88" spans="1:21" s="24" customFormat="1" ht="13.5">
       <c r="A88" s="24" t="s">
         <v>614</v>
       </c>
@@ -16450,7 +16453,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="89" spans="1:21" s="24" customFormat="1" ht="14.25">
+    <row r="89" spans="1:21" s="24" customFormat="1" ht="13.5">
       <c r="A89" s="24" t="s">
         <v>618</v>
       </c>
@@ -16509,7 +16512,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="90" spans="1:21" s="24" customFormat="1" ht="14.25">
+    <row r="90" spans="1:21" s="24" customFormat="1" ht="13.5">
       <c r="A90" s="24" t="s">
         <v>624</v>
       </c>
@@ -16568,7 +16571,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="91" spans="1:21" s="24" customFormat="1" ht="14.25">
+    <row r="91" spans="1:21" s="24" customFormat="1" ht="13.5">
       <c r="A91" s="24" t="s">
         <v>628</v>
       </c>
@@ -16627,7 +16630,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="92" spans="1:21" s="24" customFormat="1" ht="14.25">
+    <row r="92" spans="1:21" s="24" customFormat="1" ht="13.5">
       <c r="A92" s="24" t="s">
         <v>632</v>
       </c>
@@ -16686,7 +16689,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="93" spans="1:21" s="24" customFormat="1" ht="14.25">
+    <row r="93" spans="1:21" s="24" customFormat="1" ht="13.5">
       <c r="A93" s="24" t="s">
         <v>635</v>
       </c>
@@ -16745,7 +16748,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="94" spans="1:21" s="24" customFormat="1" ht="14.25">
+    <row r="94" spans="1:21" s="24" customFormat="1" ht="13.5">
       <c r="A94" s="24" t="s">
         <v>664</v>
       </c>
@@ -16804,7 +16807,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="95" spans="1:21" s="24" customFormat="1" ht="14.25">
+    <row r="95" spans="1:21" s="24" customFormat="1" ht="13.5">
       <c r="A95" s="24" t="s">
         <v>669</v>
       </c>
@@ -16863,7 +16866,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="96" spans="1:21" s="24" customFormat="1" ht="14.25">
+    <row r="96" spans="1:21" s="24" customFormat="1" ht="13.5">
       <c r="A96" s="24" t="s">
         <v>673</v>
       </c>
@@ -16922,7 +16925,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="97" spans="1:21" s="24" customFormat="1" ht="14.25">
+    <row r="97" spans="1:21" s="24" customFormat="1" ht="13.5">
       <c r="A97" s="24" t="s">
         <v>675</v>
       </c>
@@ -16981,7 +16984,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="98" spans="1:21" s="24" customFormat="1" ht="14.25">
+    <row r="98" spans="1:21" s="24" customFormat="1" ht="13.5">
       <c r="A98" s="24" t="s">
         <v>689</v>
       </c>
@@ -17040,7 +17043,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="99" spans="1:21" s="24" customFormat="1" ht="14.25">
+    <row r="99" spans="1:21" s="24" customFormat="1" ht="13.5">
       <c r="A99" s="24" t="s">
         <v>706</v>
       </c>
@@ -17099,7 +17102,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="100" spans="1:21" s="24" customFormat="1" ht="14.25">
+    <row r="100" spans="1:21" s="24" customFormat="1" ht="13.5">
       <c r="A100" s="24" t="s">
         <v>710</v>
       </c>
@@ -17158,7 +17161,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="101" spans="1:21" s="24" customFormat="1" ht="14.25">
+    <row r="101" spans="1:21" s="24" customFormat="1" ht="13.5">
       <c r="A101" s="24" t="s">
         <v>714</v>
       </c>
@@ -17217,7 +17220,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="102" spans="1:21" s="24" customFormat="1" ht="14.25">
+    <row r="102" spans="1:21" s="24" customFormat="1" ht="13.5">
       <c r="A102" s="24" t="s">
         <v>744</v>
       </c>
@@ -17276,7 +17279,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="103" spans="1:21" s="24" customFormat="1" ht="14.25">
+    <row r="103" spans="1:21" s="24" customFormat="1" ht="13.5">
       <c r="A103" s="24" t="s">
         <v>750</v>
       </c>
@@ -17335,7 +17338,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="104" spans="1:21" s="24" customFormat="1" ht="14.25">
+    <row r="104" spans="1:21" s="24" customFormat="1" ht="13.5">
       <c r="A104" s="24" t="s">
         <v>759</v>
       </c>
@@ -17394,7 +17397,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="105" spans="1:21" s="24" customFormat="1" ht="14.25">
+    <row r="105" spans="1:21" s="24" customFormat="1" ht="13.5">
       <c r="A105" s="24" t="s">
         <v>769</v>
       </c>
@@ -17453,7 +17456,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="106" spans="1:21" s="24" customFormat="1" ht="14.25">
+    <row r="106" spans="1:21" s="24" customFormat="1" ht="13.5">
       <c r="A106" s="24" t="s">
         <v>775</v>
       </c>
@@ -17512,7 +17515,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="107" spans="1:21" s="24" customFormat="1" ht="14.25">
+    <row r="107" spans="1:21" s="24" customFormat="1" ht="13.5">
       <c r="A107" s="24" t="s">
         <v>785</v>
       </c>
@@ -17571,7 +17574,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="108" spans="1:21" s="24" customFormat="1" ht="14.25">
+    <row r="108" spans="1:21" s="24" customFormat="1" ht="13.5">
       <c r="A108" s="24" t="s">
         <v>790</v>
       </c>
@@ -17630,7 +17633,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="109" spans="1:21" s="24" customFormat="1" ht="14.25">
+    <row r="109" spans="1:21" s="24" customFormat="1" ht="13.5">
       <c r="A109" s="24" t="s">
         <v>799</v>
       </c>
@@ -17689,7 +17692,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="110" spans="1:21" s="24" customFormat="1" ht="14.25">
+    <row r="110" spans="1:21" s="24" customFormat="1" ht="13.5">
       <c r="A110" s="24" t="s">
         <v>807</v>
       </c>
@@ -17748,7 +17751,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="111" spans="1:21" s="24" customFormat="1" ht="14.25">
+    <row r="111" spans="1:21" s="24" customFormat="1" ht="13.5">
       <c r="A111" s="24" t="s">
         <v>812</v>
       </c>
@@ -17807,7 +17810,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="112" spans="1:21" s="24" customFormat="1" ht="14.25">
+    <row r="112" spans="1:21" s="24" customFormat="1" ht="13.5">
       <c r="A112" s="24" t="s">
         <v>817</v>
       </c>
@@ -17866,7 +17869,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="113" spans="1:21" s="24" customFormat="1" ht="14.25">
+    <row r="113" spans="1:21" s="24" customFormat="1" ht="13.5">
       <c r="A113" s="24" t="s">
         <v>822</v>
       </c>
@@ -17925,7 +17928,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="114" spans="1:21" s="24" customFormat="1" ht="14.25">
+    <row r="114" spans="1:21" s="24" customFormat="1" ht="13.5">
       <c r="A114" s="24" t="s">
         <v>833</v>
       </c>
@@ -17984,7 +17987,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="115" spans="1:21" s="24" customFormat="1" ht="14.25">
+    <row r="115" spans="1:21" s="24" customFormat="1" ht="13.5">
       <c r="A115" s="24" t="s">
         <v>842</v>
       </c>
@@ -18043,7 +18046,7 @@
         <v>325</v>
       </c>
     </row>
-    <row r="116" spans="1:21" s="24" customFormat="1" ht="14.25">
+    <row r="116" spans="1:21" s="24" customFormat="1" ht="13.5">
       <c r="A116" s="24" t="s">
         <v>850</v>
       </c>
@@ -18102,7 +18105,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="117" spans="1:21" s="24" customFormat="1" ht="14.25">
+    <row r="117" spans="1:21" s="24" customFormat="1" ht="13.5">
       <c r="A117" s="24" t="s">
         <v>857</v>
       </c>
@@ -18161,7 +18164,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="118" spans="1:21" s="24" customFormat="1" ht="14.25">
+    <row r="118" spans="1:21" s="24" customFormat="1" ht="13.5">
       <c r="A118" s="24" t="s">
         <v>866</v>
       </c>
@@ -18220,7 +18223,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="119" spans="1:21" s="24" customFormat="1" ht="14.25">
+    <row r="119" spans="1:21" s="24" customFormat="1" ht="13.5">
       <c r="A119" s="24" t="s">
         <v>870</v>
       </c>
@@ -18279,7 +18282,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="120" spans="1:21" s="24" customFormat="1" ht="14.25">
+    <row r="120" spans="1:21" s="24" customFormat="1" ht="13.5">
       <c r="A120" s="24">
         <v>119</v>
       </c>
@@ -18338,7 +18341,7 @@
         <v>1044</v>
       </c>
     </row>
-    <row r="121" spans="1:21" s="24" customFormat="1" ht="14.25">
+    <row r="121" spans="1:21" s="24" customFormat="1" ht="13.5">
       <c r="A121" s="24" t="s">
         <v>910</v>
       </c>
@@ -18397,7 +18400,7 @@
         <v>1044</v>
       </c>
     </row>
-    <row r="122" spans="1:21" s="24" customFormat="1" ht="14.25">
+    <row r="122" spans="1:21" s="24" customFormat="1" ht="13.5">
       <c r="A122" s="24" t="s">
         <v>915</v>
       </c>
@@ -18456,7 +18459,7 @@
         <v>1044</v>
       </c>
     </row>
-    <row r="123" spans="1:21" s="24" customFormat="1" ht="14.25">
+    <row r="123" spans="1:21" s="24" customFormat="1" ht="13.5">
       <c r="A123" s="24" t="s">
         <v>922</v>
       </c>
@@ -18515,7 +18518,7 @@
         <v>1044</v>
       </c>
     </row>
-    <row r="124" spans="1:21" s="24" customFormat="1" ht="14.25">
+    <row r="124" spans="1:21" s="24" customFormat="1" ht="13.5">
       <c r="A124" s="24" t="s">
         <v>927</v>
       </c>
@@ -18574,7 +18577,7 @@
         <v>1044</v>
       </c>
     </row>
-    <row r="125" spans="1:21" s="24" customFormat="1" ht="14.25">
+    <row r="125" spans="1:21" s="24" customFormat="1" ht="13.5">
       <c r="A125" s="24" t="s">
         <v>930</v>
       </c>
@@ -18633,7 +18636,7 @@
         <v>1044</v>
       </c>
     </row>
-    <row r="126" spans="1:21" s="24" customFormat="1" ht="14.25">
+    <row r="126" spans="1:21" s="24" customFormat="1" ht="13.5">
       <c r="A126" s="24" t="s">
         <v>934</v>
       </c>
@@ -18692,7 +18695,7 @@
         <v>1044</v>
       </c>
     </row>
-    <row r="127" spans="1:21" s="24" customFormat="1" ht="14.25">
+    <row r="127" spans="1:21" s="24" customFormat="1" ht="13.5">
       <c r="A127" s="24" t="s">
         <v>940</v>
       </c>
@@ -18751,7 +18754,7 @@
         <v>1044</v>
       </c>
     </row>
-    <row r="128" spans="1:21" s="24" customFormat="1" ht="14.25">
+    <row r="128" spans="1:21" s="24" customFormat="1" ht="13.5">
       <c r="A128" s="24" t="s">
         <v>946</v>
       </c>
@@ -18810,7 +18813,7 @@
         <v>1044</v>
       </c>
     </row>
-    <row r="129" spans="1:21" s="24" customFormat="1" ht="14.25">
+    <row r="129" spans="1:21" s="24" customFormat="1" ht="13.5">
       <c r="A129" s="24" t="s">
         <v>951</v>
       </c>
@@ -18869,7 +18872,7 @@
         <v>1044</v>
       </c>
     </row>
-    <row r="130" spans="1:21" s="24" customFormat="1" ht="14.25">
+    <row r="130" spans="1:21" s="24" customFormat="1" ht="13.5">
       <c r="A130" s="24" t="s">
         <v>956</v>
       </c>
@@ -18928,7 +18931,7 @@
         <v>1044</v>
       </c>
     </row>
-    <row r="131" spans="1:21" s="24" customFormat="1" ht="14.25">
+    <row r="131" spans="1:21" s="24" customFormat="1" ht="13.5">
       <c r="A131" s="24" t="s">
         <v>960</v>
       </c>
@@ -18987,7 +18990,7 @@
         <v>1044</v>
       </c>
     </row>
-    <row r="132" spans="1:21" s="24" customFormat="1" ht="14.25">
+    <row r="132" spans="1:21" s="24" customFormat="1" ht="13.5">
       <c r="A132" s="24" t="s">
         <v>963</v>
       </c>
@@ -19046,7 +19049,7 @@
         <v>1044</v>
       </c>
     </row>
-    <row r="133" spans="1:21" s="24" customFormat="1" ht="14.25">
+    <row r="133" spans="1:21" s="24" customFormat="1" ht="13.5">
       <c r="A133" s="24" t="s">
         <v>967</v>
       </c>
@@ -19105,12 +19108,12 @@
         <v>1044</v>
       </c>
     </row>
-    <row r="134" spans="1:21" s="24" customFormat="1" ht="14.25">
+    <row r="134" spans="1:21" s="24" customFormat="1" ht="13.5">
       <c r="A134" s="24" t="s">
         <v>972</v>
       </c>
-      <c r="B134" s="24" t="s">
-        <v>7</v>
+      <c r="B134" s="43" t="s">
+        <v>172</v>
       </c>
       <c r="C134" s="24" t="s">
         <v>973</v>
@@ -19118,8 +19121,8 @@
       <c r="D134" s="24" t="s">
         <v>84</v>
       </c>
-      <c r="E134" s="24" t="s">
-        <v>78</v>
+      <c r="E134" s="43" t="s">
+        <v>172</v>
       </c>
       <c r="F134" s="24" t="s">
         <v>407</v>
@@ -19164,7 +19167,7 @@
         <v>1044</v>
       </c>
     </row>
-    <row r="135" spans="1:21" s="24" customFormat="1" ht="14.25">
+    <row r="135" spans="1:21" s="24" customFormat="1" ht="13.5">
       <c r="A135" s="24" t="s">
         <v>975</v>
       </c>
@@ -19223,7 +19226,7 @@
         <v>1044</v>
       </c>
     </row>
-    <row r="136" spans="1:21" s="24" customFormat="1" ht="14.25">
+    <row r="136" spans="1:21" s="24" customFormat="1" ht="13.5">
       <c r="A136" s="24" t="s">
         <v>980</v>
       </c>
@@ -19282,7 +19285,7 @@
         <v>1044</v>
       </c>
     </row>
-    <row r="137" spans="1:21" s="24" customFormat="1" ht="14.25">
+    <row r="137" spans="1:21" s="24" customFormat="1" ht="13.5">
       <c r="A137" s="24" t="s">
         <v>986</v>
       </c>
@@ -19341,7 +19344,7 @@
         <v>1044</v>
       </c>
     </row>
-    <row r="138" spans="1:21" s="24" customFormat="1" ht="14.25">
+    <row r="138" spans="1:21" s="24" customFormat="1" ht="13.5">
       <c r="A138" s="24" t="s">
         <v>992</v>
       </c>
@@ -19400,7 +19403,7 @@
         <v>1044</v>
       </c>
     </row>
-    <row r="139" spans="1:21" s="24" customFormat="1" ht="14.25">
+    <row r="139" spans="1:21" s="24" customFormat="1" ht="13.5">
       <c r="A139" s="24" t="s">
         <v>997</v>
       </c>
@@ -19459,7 +19462,7 @@
         <v>1044</v>
       </c>
     </row>
-    <row r="140" spans="1:21" s="24" customFormat="1" ht="14.25">
+    <row r="140" spans="1:21" s="24" customFormat="1" ht="13.5">
       <c r="A140" s="24" t="s">
         <v>1001</v>
       </c>
@@ -19518,7 +19521,7 @@
         <v>1044</v>
       </c>
     </row>
-    <row r="141" spans="1:21" s="24" customFormat="1" ht="14.25">
+    <row r="141" spans="1:21" s="24" customFormat="1" ht="13.5">
       <c r="A141" s="24" t="s">
         <v>1007</v>
       </c>
@@ -19577,7 +19580,7 @@
         <v>1044</v>
       </c>
     </row>
-    <row r="142" spans="1:21" s="24" customFormat="1" ht="14.25">
+    <row r="142" spans="1:21" s="24" customFormat="1" ht="13.5">
       <c r="A142" s="24" t="s">
         <v>1012</v>
       </c>
@@ -19636,7 +19639,7 @@
         <v>1044</v>
       </c>
     </row>
-    <row r="143" spans="1:21" s="24" customFormat="1" ht="14.25">
+    <row r="143" spans="1:21" s="24" customFormat="1" ht="13.5">
       <c r="A143" s="24" t="s">
         <v>1017</v>
       </c>
@@ -19695,12 +19698,12 @@
         <v>37</v>
       </c>
     </row>
-    <row r="144" spans="1:21" s="24" customFormat="1" ht="14.25">
+    <row r="144" spans="1:21" s="24" customFormat="1" ht="13.5">
       <c r="A144" s="24" t="s">
         <v>1051</v>
       </c>
-      <c r="B144" s="24" t="s">
-        <v>7</v>
+      <c r="B144" s="43" t="s">
+        <v>172</v>
       </c>
       <c r="C144" s="24" t="s">
         <v>1052</v>
@@ -19708,8 +19711,8 @@
       <c r="D144" s="24" t="s">
         <v>234</v>
       </c>
-      <c r="E144" s="24" t="s">
-        <v>78</v>
+      <c r="E144" s="43" t="s">
+        <v>172</v>
       </c>
       <c r="F144" s="24" t="s">
         <v>407</v>
@@ -19754,7 +19757,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="145" spans="1:21" s="24" customFormat="1" ht="14.25">
+    <row r="145" spans="1:21" s="24" customFormat="1" ht="13.5">
       <c r="A145" s="24" t="s">
         <v>1056</v>
       </c>
@@ -19813,7 +19816,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="146" spans="1:21" s="24" customFormat="1" ht="14.25">
+    <row r="146" spans="1:21" s="24" customFormat="1" ht="13.5">
       <c r="A146" s="24" t="s">
         <v>1073</v>
       </c>
@@ -19872,12 +19875,12 @@
         <v>8</v>
       </c>
     </row>
-    <row r="147" spans="1:21" s="24" customFormat="1" ht="14.25">
+    <row r="147" spans="1:21" s="24" customFormat="1" ht="13.5">
       <c r="A147" s="24" t="s">
         <v>1078</v>
       </c>
-      <c r="B147" s="24" t="s">
-        <v>7</v>
+      <c r="B147" s="43" t="s">
+        <v>172</v>
       </c>
       <c r="C147" s="24" t="s">
         <v>1079</v>
@@ -19885,8 +19888,8 @@
       <c r="D147" s="24" t="s">
         <v>77</v>
       </c>
-      <c r="E147" s="24" t="s">
-        <v>78</v>
+      <c r="E147" s="43" t="s">
+        <v>172</v>
       </c>
       <c r="F147" s="24" t="s">
         <v>79</v>
@@ -19931,12 +19934,12 @@
         <v>37</v>
       </c>
     </row>
-    <row r="148" spans="1:21" s="24" customFormat="1" ht="14.25">
+    <row r="148" spans="1:21" s="24" customFormat="1" ht="13.5">
       <c r="A148" s="24" t="s">
         <v>1082</v>
       </c>
-      <c r="B148" s="24" t="s">
-        <v>7</v>
+      <c r="B148" s="43" t="s">
+        <v>172</v>
       </c>
       <c r="C148" s="24" t="s">
         <v>1083</v>
@@ -19944,8 +19947,8 @@
       <c r="D148" s="24" t="s">
         <v>84</v>
       </c>
-      <c r="E148" s="24" t="s">
-        <v>78</v>
+      <c r="E148" s="43" t="s">
+        <v>172</v>
       </c>
       <c r="F148" s="24" t="s">
         <v>1084</v>
@@ -19990,7 +19993,7 @@
         <v>1044</v>
       </c>
     </row>
-    <row r="149" spans="1:21" s="24" customFormat="1" ht="14.25">
+    <row r="149" spans="1:21" s="24" customFormat="1" ht="13.5">
       <c r="A149" s="24" t="s">
         <v>1096</v>
       </c>
@@ -20049,7 +20052,7 @@
         <v>1044</v>
       </c>
     </row>
-    <row r="150" spans="1:21" s="24" customFormat="1" ht="14.25">
+    <row r="150" spans="1:21" s="24" customFormat="1" ht="13.5">
       <c r="A150" s="24" t="s">
         <v>1101</v>
       </c>
@@ -20108,7 +20111,7 @@
         <v>1044</v>
       </c>
     </row>
-    <row r="151" spans="1:21" s="24" customFormat="1" ht="14.25">
+    <row r="151" spans="1:21" s="24" customFormat="1" ht="13.5">
       <c r="A151" s="24" t="s">
         <v>1108</v>
       </c>
@@ -20167,7 +20170,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="152" spans="1:21" s="24" customFormat="1" ht="14.25">
+    <row r="152" spans="1:21" s="24" customFormat="1" ht="13.5">
       <c r="A152" s="24" t="s">
         <v>1113</v>
       </c>
@@ -20226,7 +20229,7 @@
         <v>1044</v>
       </c>
     </row>
-    <row r="153" spans="1:21" s="24" customFormat="1" ht="14.25">
+    <row r="153" spans="1:21" s="24" customFormat="1" ht="13.5">
       <c r="A153" s="24" t="s">
         <v>1123</v>
       </c>
@@ -20285,12 +20288,12 @@
         <v>1044</v>
       </c>
     </row>
-    <row r="154" spans="1:21" s="24" customFormat="1" ht="14.25">
+    <row r="154" spans="1:21" s="24" customFormat="1" ht="13.5">
       <c r="A154" s="24" t="s">
         <v>1132</v>
       </c>
-      <c r="B154" s="24" t="s">
-        <v>7</v>
+      <c r="B154" s="43" t="s">
+        <v>172</v>
       </c>
       <c r="C154" s="24" t="s">
         <v>1133</v>
@@ -20298,8 +20301,8 @@
       <c r="D154" s="24" t="s">
         <v>261</v>
       </c>
-      <c r="E154" s="24" t="s">
-        <v>78</v>
+      <c r="E154" s="43" t="s">
+        <v>172</v>
       </c>
       <c r="F154" s="24" t="s">
         <v>79</v>
@@ -20344,7 +20347,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="155" spans="1:21" ht="14.25">
+    <row r="155" spans="1:21" ht="13.5">
       <c r="A155" t="s">
         <v>1136</v>
       </c>
@@ -20403,7 +20406,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="156" spans="1:21" s="24" customFormat="1" ht="14.25">
+    <row r="156" spans="1:21" s="24" customFormat="1" ht="13.5">
       <c r="A156" s="24" t="s">
         <v>1139</v>
       </c>
@@ -20462,7 +20465,7 @@
         <v>1044</v>
       </c>
     </row>
-    <row r="157" spans="1:21" s="24" customFormat="1" ht="14.25">
+    <row r="157" spans="1:21" s="24" customFormat="1" ht="13.5">
       <c r="A157" s="24" t="s">
         <v>1144</v>
       </c>
@@ -20521,7 +20524,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="158" spans="1:21" s="24" customFormat="1" ht="14.25">
+    <row r="158" spans="1:21" s="24" customFormat="1" ht="13.5">
       <c r="A158" s="24" t="s">
         <v>1150</v>
       </c>
@@ -20580,7 +20583,7 @@
         <v>1044</v>
       </c>
     </row>
-    <row r="159" spans="1:21" s="24" customFormat="1" ht="14.25">
+    <row r="159" spans="1:21" s="24" customFormat="1" ht="13.5">
       <c r="A159" s="24" t="s">
         <v>1157</v>
       </c>
@@ -20639,7 +20642,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="160" spans="1:21" s="24" customFormat="1" ht="14.25">
+    <row r="160" spans="1:21" s="24" customFormat="1" ht="13.5">
       <c r="A160" s="24" t="s">
         <v>1169</v>
       </c>
@@ -20698,7 +20701,7 @@
         <v>1191</v>
       </c>
     </row>
-    <row r="161" spans="1:21" s="24" customFormat="1" ht="14.25">
+    <row r="161" spans="1:21" s="24" customFormat="1" ht="13.5">
       <c r="A161" s="24" t="s">
         <v>1175</v>
       </c>
@@ -20757,7 +20760,7 @@
         <v>1044</v>
       </c>
     </row>
-    <row r="162" spans="1:21" s="24" customFormat="1" ht="14.25">
+    <row r="162" spans="1:21" s="24" customFormat="1" ht="13.5">
       <c r="A162" s="24" t="s">
         <v>1179</v>
       </c>
@@ -20816,7 +20819,7 @@
         <v>1044</v>
       </c>
     </row>
-    <row r="163" spans="1:21" s="24" customFormat="1" ht="14.25">
+    <row r="163" spans="1:21" s="24" customFormat="1" ht="13.5">
       <c r="A163" s="24" t="s">
         <v>1183</v>
       </c>
@@ -20878,19 +20881,19 @@
   </sheetData>
   <autoFilter ref="E1:E145" xr:uid="{00000000-0001-0000-0100-000000000000}"/>
   <customSheetViews>
+    <customSheetView guid="{C25CEB9E-BEC1-4982-90C4-50C84EE1B82A}" filter="1" showAutoFilter="1">
+      <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+      <autoFilter ref="A1:AD33" xr:uid="{1B0781F3-8951-4804-84B0-EBB9EA035BC7}"/>
+    </customSheetView>
     <customSheetView guid="{A7754112-A52F-4ABC-8778-92F04773E53C}" filter="1" showAutoFilter="1">
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-      <autoFilter ref="A1:AD33" xr:uid="{8F9995FE-CFC8-4AF1-8AA4-3F597A1BFADF}">
+      <autoFilter ref="A1:AD33" xr:uid="{C32B5D53-ED7A-4EC2-8DB5-10AA08C73AE4}">
         <filterColumn colId="5">
           <filters blank="1">
             <filter val="Strathnairn"/>
           </filters>
         </filterColumn>
       </autoFilter>
-    </customSheetView>
-    <customSheetView guid="{C25CEB9E-BEC1-4982-90C4-50C84EE1B82A}" filter="1" showAutoFilter="1">
-      <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-      <autoFilter ref="A1:AD33" xr:uid="{4BD014B5-09F7-4EF2-99AE-C7201C8EE837}"/>
     </customSheetView>
   </customSheetViews>
   <conditionalFormatting sqref="A1:AI1">
@@ -20945,22 +20948,22 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="14.3984375" defaultRowHeight="15.75" customHeight="1"/>
   <cols>
     <col min="1" max="1" width="16" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="14.5703125" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="16.85546875" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="14.5703125" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="13.140625" customWidth="1" collapsed="1"/>
-    <col min="15" max="15" width="20.85546875" customWidth="1" collapsed="1"/>
-    <col min="21" max="22" width="19.140625" customWidth="1" collapsed="1"/>
-    <col min="23" max="23" width="20.140625" customWidth="1" collapsed="1"/>
-    <col min="24" max="24" width="19.85546875" customWidth="1" collapsed="1"/>
-    <col min="26" max="26" width="15.85546875" customWidth="1" collapsed="1"/>
-    <col min="27" max="27" width="13.42578125" customWidth="1" collapsed="1"/>
-    <col min="28" max="28" width="15.140625" customWidth="1" collapsed="1"/>
-    <col min="29" max="29" width="16.140625" customWidth="1" collapsed="1"/>
-    <col min="30" max="30" width="15.85546875" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="14.59765625" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="16.86328125" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="14.59765625" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="13.1328125" customWidth="1" collapsed="1"/>
+    <col min="15" max="15" width="20.86328125" customWidth="1" collapsed="1"/>
+    <col min="21" max="22" width="19.1328125" customWidth="1" collapsed="1"/>
+    <col min="23" max="23" width="20.1328125" customWidth="1" collapsed="1"/>
+    <col min="24" max="24" width="19.86328125" customWidth="1" collapsed="1"/>
+    <col min="26" max="26" width="15.86328125" customWidth="1" collapsed="1"/>
+    <col min="27" max="27" width="13.3984375" customWidth="1" collapsed="1"/>
+    <col min="28" max="28" width="15.1328125" customWidth="1" collapsed="1"/>
+    <col min="29" max="29" width="16.1328125" customWidth="1" collapsed="1"/>
+    <col min="30" max="30" width="15.86328125" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:35" ht="15.75" customHeight="1">
@@ -21083,16 +21086,16 @@
       <selection pane="bottomLeft" activeCell="D18" sqref="D18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="14.3984375" defaultRowHeight="15.75" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="44.85546875" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="19.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="26.42578125" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="36.140625" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="53.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" width="44.86328125" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="19.59765625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="26.3984375" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="36.1328125" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="53.73046875" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="15">
+    <row r="1" spans="1:7" ht="13.9">
       <c r="A1" s="29" t="s">
         <v>152</v>
       </c>

</xml_diff>

<commit_message>
New listing script run
</commit_message>
<xml_diff>
--- a/src/main/resources/InputTestdata/Listing details.xlsx
+++ b/src/main/resources/InputTestdata/Listing details.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24326"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24430"/>
   <workbookPr/>
   <mc:AlternateContent>
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Athavan\git\777Homes-2\777Homes-business\src\main\resources\InputTestdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr documentId="13_ncr:1_{0EBB6480-9201-49B4-B07B-BA5D8AFD91AE}" revIDLastSave="0" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47"/>
+  <xr:revisionPtr documentId="13_ncr:1_{D5F81294-24D5-46D0-89C4-4C17EC6455A5}" revIDLastSave="0" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47"/>
   <bookViews>
-    <workbookView activeTab="1" windowHeight="15840" windowWidth="29040" xWindow="-120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}" yWindow="-120"/>
+    <workbookView windowHeight="15840" windowWidth="29040" xWindow="-120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}" yWindow="-120"/>
   </bookViews>
   <sheets>
     <sheet name="Backlog" r:id="rId1" sheetId="1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4029" uniqueCount="1207">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4081" uniqueCount="1221">
   <si>
     <t>ID</t>
   </si>
@@ -6056,13 +6056,85 @@
     <t>3	3	5	0	0	0</t>
   </si>
   <si>
+    <t>https://www.777homes.com.au/?post_type=property&amp;p=9258&amp;preview=true</t>
+  </si>
+  <si>
+    <t>https://www.777homes.com.au/?post_type=property&amp;p=9260&amp;preview=true</t>
+  </si>
+  <si>
+    <t>https://www.allhomes.com.au/145-sculthorpe-avenue-whitlam-act-2611</t>
+  </si>
+  <si>
+    <t>https://www.allhomes.com.au/unit-3-109-boddington-crescent-kambah-act-2902</t>
+  </si>
+  <si>
+    <t>166</t>
+  </si>
+  <si>
+    <t>145 Sculthorpe Avenue, Whitlam ACT 2611</t>
+  </si>
+  <si>
+    <t>NEW</t>
+  </si>
+  <si>
+    <t>An amazing opportunity to purchase this luxurious home located among other quality homes in Whitlam. The construction is ready to begin and home shall be ready to move in upon completion.
+This spacious 5-bedroom home is situated on 444 sqm block and boasts a separate lounge room at front of house for intimate gatherings among family and friends. The home will feature a large family &amp; dining area. The stunning kitchen will be large and spacious with all modern comforts including walk in pantry, stone bench tops and quality stainless steel appliances for the home chef to cook healthy meals on daily basis.
+The main bedroom is scheduled from the main living and features large walk-in robe with enough storage for occupants needs. All other bedrooms are spacious and include built-in wardrobes. Bedroom 2 comes with its own Ensuite and is situated away from the other bedrooms ideal for guest visiting.
+Bedroom five has an Ensuite and extra kitchen with separate entry. Provides you with an extra rent out option or studio. Enjoy the weather in all seasons, this home will have double glazed windows, reverse cycle zoned heating &amp; cooling system. The outdoor alfresco area which opens from the family area is under same roof line, fantastic for entertaining or barbecue within a very private backyard. The home is situated in the popular new suburb of Whitlam.
+Call Anish now 0450865524 before you miss the opportunity to purchase this brand house &amp; land package.
+Property features Include:
+Double glazed windows
+LED energy saving down lights throughout
+5 Spacious bedrooms
+Main bedroom with walk-in robe &amp; Ensuite
+Dazzling kitchen with walk-in pantry
+Stone bench tops &amp; ample cupboards
+Stainless-steel appliances
+Walk-in Pantry
+Double automatic garage with internal access
+Colourbond roof
+Alfresco under same roofline
+Alfresco area perfect for entertaining
+Good size backyard with easy-care landscaping
+Rainwater tank</t>
+  </si>
+  <si>
+    <t>167</t>
+  </si>
+  <si>
+    <t>3/109 Boddington Crescent, Kambah ACT 2902</t>
+  </si>
+  <si>
+    <t>Kambah</t>
+  </si>
+  <si>
+    <t xml:space="preserve">7	1	9	0	0	0	</t>
+  </si>
+  <si>
+    <t>Offers over $719,000</t>
+  </si>
+  <si>
+    <t>This modern three bedroom townhouse is ideally located close to a variety of local schools, shops and cafes. Spacious with a sense of privacy they are a must see for your self.
+The property features open-plan living, a stylish kitchen with quality appliances as well as a low-maintenance courtyard area.
+The bedrooms are all spacious with build in robes. The place is freshly painted.
+Features include:
+-Three bedrooms with built-in wardrobes
+-Low-maintenance courtyard
+-Open-plan living
+- Double garage with remote, within secure basement
+- Close to schools and local shops
+- Freshly painted
+- Rental potential of $600 / week approx.
+Call Anish now on 0450 865 524 to view this property.</t>
+  </si>
+  <si>
     <t>Draft</t>
   </si>
   <si>
-    <t>https://www.777homes.com.au/?post_type=property&amp;p=9258&amp;preview=true</t>
-  </si>
-  <si>
-    <t>https://www.777homes.com.au/?post_type=property&amp;p=9260&amp;preview=true</t>
+    <t>https://www.777homes.com.au/?post_type=property&amp;p=9377&amp;preview=true</t>
+  </si>
+  <si>
+    <t>https://www.777homes.com.au/?post_type=property&amp;p=9379&amp;preview=true</t>
   </si>
 </sst>
 </file>
@@ -6230,7 +6302,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="10">
+  <fills count="12">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -6284,6 +6356,16 @@
         <bgColor indexed="2"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor indexed="2"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="mediumGray">
+        <bgColor indexed="2"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -6298,7 +6380,7 @@
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
     <xf applyAlignment="0" applyBorder="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="0" fontId="25" numFmtId="0"/>
   </cellStyleXfs>
-  <cellXfs count="47">
+  <cellXfs count="48">
     <xf applyAlignment="1" applyFont="1" borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
     <xf applyAlignment="1" applyFill="1" applyFont="1" borderId="0" fillId="3" fontId="1" numFmtId="0" xfId="0">
       <alignment horizontal="center"/>
@@ -6396,6 +6478,7 @@
     </xf>
     <xf applyAlignment="1" applyFont="1" borderId="0" fillId="0" fontId="27" numFmtId="0" xfId="0"/>
     <xf applyFill="1" borderId="0" fillId="9" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyFill="true" borderId="0" fillId="11" fontId="0" numFmtId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle builtinId="8" name="Hyperlink" xfId="1"/>
@@ -6632,11 +6715,11 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:AC166"/>
+  <dimension ref="A1:AC168"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane activePane="bottomLeft" state="frozen" topLeftCell="A131" ySplit="1"/>
-      <selection activeCell="F166" pane="bottomLeft" sqref="F166"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane activePane="bottomLeft" state="frozen" topLeftCell="A140" ySplit="1"/>
+      <selection activeCell="E172" pane="bottomLeft" sqref="E172"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr customHeight="1" defaultColWidth="14.42578125" defaultRowHeight="15.75"/>
@@ -9977,7 +10060,7 @@
         <v>1022</v>
       </c>
       <c r="D120" s="4" t="s">
-        <v>7</v>
+        <v>14</v>
       </c>
       <c r="F120" s="2" t="s">
         <v>687</v>
@@ -10069,7 +10152,7 @@
         <v>1026</v>
       </c>
       <c r="D124" s="4" t="s">
-        <v>7</v>
+        <v>14</v>
       </c>
       <c r="F124" s="2" t="s">
         <v>687</v>
@@ -10138,7 +10221,7 @@
         <v>1029</v>
       </c>
       <c r="D127" s="4" t="s">
-        <v>7</v>
+        <v>14</v>
       </c>
       <c r="F127" s="2" t="s">
         <v>687</v>
@@ -10368,7 +10451,7 @@
         <v>1036</v>
       </c>
       <c r="D137" s="4" t="s">
-        <v>7</v>
+        <v>14</v>
       </c>
       <c r="F137" s="2" t="s">
         <v>687</v>
@@ -10644,7 +10727,7 @@
         <v>1089</v>
       </c>
       <c r="D149" s="4" t="s">
-        <v>7</v>
+        <v>14</v>
       </c>
       <c r="F149" s="2" t="s">
         <v>687</v>
@@ -10999,14 +11082,14 @@
       <c r="A165">
         <v>164</v>
       </c>
-      <c r="B165" t="s">
+      <c r="B165" s="41" t="s">
         <v>1193</v>
       </c>
-      <c r="C165" t="s">
-        <v>1205</v>
-      </c>
-      <c r="D165" s="46" t="s">
+      <c r="C165" s="41" t="s">
         <v>1204</v>
+      </c>
+      <c r="D165" s="4" t="s">
+        <v>7</v>
       </c>
       <c r="F165" s="2" t="s">
         <v>1046</v>
@@ -11022,14 +11105,14 @@
       <c r="A166">
         <v>165</v>
       </c>
-      <c r="B166" t="s">
+      <c r="B166" s="41" t="s">
         <v>1194</v>
       </c>
-      <c r="C166" t="s">
-        <v>1206</v>
-      </c>
-      <c r="D166" s="46" t="s">
-        <v>1204</v>
+      <c r="C166" s="41" t="s">
+        <v>1205</v>
+      </c>
+      <c r="D166" s="4" t="s">
+        <v>7</v>
       </c>
       <c r="F166" s="2" t="s">
         <v>1046</v>
@@ -11039,6 +11122,52 @@
       </c>
       <c r="H166" t="s">
         <v>38</v>
+      </c>
+    </row>
+    <row ht="12.75" r="167" spans="1:8">
+      <c r="A167">
+        <v>166</v>
+      </c>
+      <c r="B167" t="s">
+        <v>1206</v>
+      </c>
+      <c r="C167" t="s">
+        <v>1219</v>
+      </c>
+      <c r="D167" s="46" t="s">
+        <v>1218</v>
+      </c>
+      <c r="F167" s="2" t="s">
+        <v>687</v>
+      </c>
+      <c r="G167" t="s">
+        <v>1044</v>
+      </c>
+      <c r="H167" t="s">
+        <v>881</v>
+      </c>
+    </row>
+    <row ht="12.75" r="168" spans="1:8">
+      <c r="A168">
+        <v>167</v>
+      </c>
+      <c r="B168" t="s">
+        <v>1207</v>
+      </c>
+      <c r="C168" t="s">
+        <v>1220</v>
+      </c>
+      <c r="D168" s="46" t="s">
+        <v>1218</v>
+      </c>
+      <c r="F168" s="2" t="s">
+        <v>687</v>
+      </c>
+      <c r="G168" t="s">
+        <v>1044</v>
+      </c>
+      <c r="H168" t="s">
+        <v>881</v>
       </c>
     </row>
   </sheetData>
@@ -11253,9 +11382,13 @@
     <hyperlink r:id="rId208" ref="B134" xr:uid="{62E8D2B3-CF6E-4F5B-8831-F7ABFCBF12C6}"/>
     <hyperlink r:id="rId209" ref="C134" xr:uid="{67FE63AE-FF52-4665-98A8-947B6D32A39A}"/>
     <hyperlink r:id="rId210" ref="C144" xr:uid="{DB9C0A49-9F31-4CC1-A80A-79CD0938E90B}"/>
+    <hyperlink r:id="rId211" ref="C165" xr:uid="{9810966F-0ABF-43E7-9D56-4B9B52DDB64F}"/>
+    <hyperlink r:id="rId212" ref="B165" xr:uid="{54B8C472-92C1-471E-8C07-B776DBF79963}"/>
+    <hyperlink r:id="rId213" ref="C166" xr:uid="{90093A4C-E309-4465-B798-21E88A539310}"/>
+    <hyperlink r:id="rId214" ref="B166" xr:uid="{BF307439-7E40-41B9-80E9-FD464B9A05E3}"/>
   </hyperlinks>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
-  <pageSetup orientation="portrait" paperSize="9" r:id="rId211"/>
+  <pageSetup orientation="portrait" paperSize="9" r:id="rId215"/>
 </worksheet>
 </file>
 
@@ -11264,11 +11397,11 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:AJ165"/>
+  <dimension ref="A1:AJ167"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane activePane="bottomLeft" state="frozen" topLeftCell="A140" ySplit="1"/>
-      <selection activeCell="K171" pane="bottomLeft" sqref="K171"/>
+      <selection activeCell="E170" pane="bottomLeft" sqref="E170"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr customHeight="1" defaultColWidth="14.42578125" defaultRowHeight="15.75"/>
@@ -21010,122 +21143,240 @@
         <v>1044</v>
       </c>
     </row>
-    <row ht="14.25" r="164" spans="1:21">
-      <c r="A164" t="s">
+    <row customFormat="1" ht="14.25" r="164" s="24" spans="1:21">
+      <c r="A164" s="24" t="s">
         <v>1195</v>
       </c>
-      <c r="B164" t="s">
-        <v>1204</v>
-      </c>
-      <c r="C164" t="s">
+      <c r="B164" s="24" t="s">
+        <v>7</v>
+      </c>
+      <c r="C164" s="24" t="s">
         <v>1196</v>
       </c>
-      <c r="D164" t="s">
+      <c r="D164" s="24" t="s">
         <v>77</v>
       </c>
-      <c r="E164" t="s">
+      <c r="E164" s="24" t="s">
         <v>78</v>
       </c>
-      <c r="F164" t="s">
+      <c r="F164" s="24" t="s">
         <v>79</v>
       </c>
-      <c r="G164" t="s">
+      <c r="G164" s="24" t="s">
         <v>221</v>
       </c>
-      <c r="H164" t="s">
+      <c r="H164" s="24" t="s">
         <v>199</v>
       </c>
-      <c r="I164" t="s">
+      <c r="I164" s="24" t="s">
         <v>198</v>
       </c>
       <c r="K164" s="24" t="s">
         <v>1203</v>
       </c>
-      <c r="L164" t="s">
+      <c r="L164" s="24" t="s">
         <v>1197</v>
       </c>
-      <c r="M164" t="s">
+      <c r="M164" s="24" t="s">
         <v>266</v>
       </c>
-      <c r="N164" t="s">
+      <c r="N164" s="24" t="s">
         <v>266</v>
       </c>
-      <c r="P164" t="s">
+      <c r="P164" s="24" t="s">
         <v>201</v>
       </c>
-      <c r="Q164" t="s">
+      <c r="Q164" s="24" t="s">
         <v>266</v>
       </c>
-      <c r="R164" t="s">
+      <c r="R164" s="24" t="s">
         <v>1196</v>
       </c>
-      <c r="S164" t="s">
+      <c r="S164" s="24" t="s">
         <v>1198</v>
       </c>
-      <c r="T164" t="s">
+      <c r="T164" s="24" t="s">
         <v>1046</v>
       </c>
-      <c r="U164" t="s">
+      <c r="U164" s="24" t="s">
         <v>37</v>
       </c>
     </row>
-    <row ht="12.75" r="165" spans="1:21">
-      <c r="A165" t="s">
+    <row customFormat="1" ht="14.25" r="165" s="24" spans="1:21">
+      <c r="A165" s="24" t="s">
         <v>1199</v>
       </c>
-      <c r="B165" t="s">
-        <v>1204</v>
-      </c>
-      <c r="C165" t="s">
+      <c r="B165" s="24" t="s">
+        <v>7</v>
+      </c>
+      <c r="C165" s="24" t="s">
         <v>1200</v>
       </c>
-      <c r="D165" t="s">
+      <c r="D165" s="24" t="s">
         <v>84</v>
       </c>
-      <c r="E165" t="s">
+      <c r="E165" s="24" t="s">
         <v>78</v>
       </c>
-      <c r="F165" t="s">
+      <c r="F165" s="24" t="s">
         <v>79</v>
       </c>
-      <c r="G165" t="s">
+      <c r="G165" s="24" t="s">
         <v>116</v>
       </c>
-      <c r="H165" t="s">
+      <c r="H165" s="24" t="s">
         <v>199</v>
       </c>
-      <c r="I165" t="s">
+      <c r="I165" s="24" t="s">
         <v>198</v>
       </c>
-      <c r="K165" t="s">
+      <c r="K165" s="24" t="s">
         <v>199</v>
       </c>
-      <c r="L165" t="s">
+      <c r="L165" s="24" t="s">
         <v>1201</v>
       </c>
-      <c r="M165" t="s">
+      <c r="M165" s="24" t="s">
         <v>201</v>
       </c>
-      <c r="N165" t="s">
+      <c r="N165" s="24" t="s">
         <v>204</v>
       </c>
-      <c r="P165" t="s">
+      <c r="P165" s="24" t="s">
         <v>201</v>
       </c>
-      <c r="Q165" t="s">
+      <c r="Q165" s="24" t="s">
         <v>204</v>
       </c>
-      <c r="R165" t="s">
+      <c r="R165" s="24" t="s">
         <v>1200</v>
       </c>
-      <c r="S165" t="s">
+      <c r="S165" s="24" t="s">
         <v>1202</v>
       </c>
-      <c r="T165" t="s">
+      <c r="T165" s="24" t="s">
         <v>1046</v>
       </c>
-      <c r="U165" t="s">
+      <c r="U165" s="24" t="s">
         <v>37</v>
+      </c>
+    </row>
+    <row r="166">
+      <c r="A166" t="s">
+        <v>1208</v>
+      </c>
+      <c r="B166" t="s">
+        <v>1218</v>
+      </c>
+      <c r="C166" t="s">
+        <v>1209</v>
+      </c>
+      <c r="D166" t="s">
+        <v>84</v>
+      </c>
+      <c r="E166" t="s">
+        <v>78</v>
+      </c>
+      <c r="F166" t="s">
+        <v>235</v>
+      </c>
+      <c r="G166" t="s">
+        <v>236</v>
+      </c>
+      <c r="H166" t="s">
+        <v>199</v>
+      </c>
+      <c r="I166" t="s">
+        <v>198</v>
+      </c>
+      <c r="K166" t="s">
+        <v>199</v>
+      </c>
+      <c r="L166" t="s">
+        <v>237</v>
+      </c>
+      <c r="M166" t="s">
+        <v>252</v>
+      </c>
+      <c r="N166" t="s">
+        <v>201</v>
+      </c>
+      <c r="P166" t="s">
+        <v>203</v>
+      </c>
+      <c r="Q166" t="s">
+        <v>204</v>
+      </c>
+      <c r="R166" t="s">
+        <v>1209</v>
+      </c>
+      <c r="S166" t="s">
+        <v>1211</v>
+      </c>
+      <c r="T166" t="s">
+        <v>687</v>
+      </c>
+      <c r="U166" t="s">
+        <v>1044</v>
+      </c>
+    </row>
+    <row r="167">
+      <c r="A167" t="s">
+        <v>1212</v>
+      </c>
+      <c r="B167" t="s">
+        <v>1218</v>
+      </c>
+      <c r="C167" t="s">
+        <v>1213</v>
+      </c>
+      <c r="D167" t="s">
+        <v>261</v>
+      </c>
+      <c r="E167" t="s">
+        <v>78</v>
+      </c>
+      <c r="F167" t="s">
+        <v>906</v>
+      </c>
+      <c r="G167" t="s">
+        <v>1214</v>
+      </c>
+      <c r="H167" t="s">
+        <v>199</v>
+      </c>
+      <c r="I167" t="s">
+        <v>198</v>
+      </c>
+      <c r="K167" t="s">
+        <v>1215</v>
+      </c>
+      <c r="L167" t="s">
+        <v>1216</v>
+      </c>
+      <c r="M167" t="s">
+        <v>202</v>
+      </c>
+      <c r="N167" t="s">
+        <v>204</v>
+      </c>
+      <c r="P167" t="s">
+        <v>201</v>
+      </c>
+      <c r="Q167" t="s">
+        <v>204</v>
+      </c>
+      <c r="R167" t="s">
+        <v>1213</v>
+      </c>
+      <c r="S167" t="s">
+        <v>1217</v>
+      </c>
+      <c r="T167" t="s">
+        <v>687</v>
+      </c>
+      <c r="U167" t="s">
+        <v>1044</v>
       </c>
     </row>
   </sheetData>
@@ -21133,11 +21384,11 @@
   <customSheetViews>
     <customSheetView filter="1" guid="{C25CEB9E-BEC1-4982-90C4-50C84EE1B82A}" showAutoFilter="1">
       <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
-      <autoFilter ref="A1:AD33" xr:uid="{B91EE6BC-FFF6-4C33-A187-32776A783144}"/>
+      <autoFilter ref="A1:AD33" xr:uid="{87E59527-CD00-4D58-8812-97F9D7170F43}"/>
     </customSheetView>
     <customSheetView filter="1" guid="{A7754112-A52F-4ABC-8778-92F04773E53C}" showAutoFilter="1">
       <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
-      <autoFilter ref="A1:AD33" xr:uid="{CBFB1478-2647-4EDB-838B-5E3408FC2485}">
+      <autoFilter ref="A1:AD33" xr:uid="{D341ED12-697C-4966-8EB3-B9813302FF17}">
         <filterColumn colId="5">
           <filters blank="1">
             <filter val="Strathnairn"/>

</xml_diff>

<commit_message>
New listings and Sold properties fixed
</commit_message>
<xml_diff>
--- a/src/main/resources/InputTestdata/Listing details.xlsx
+++ b/src/main/resources/InputTestdata/Listing details.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24430"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24527"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Athavan\git\777Homes-2\777Homes-business\src\main\resources\InputTestdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{30F972CA-D404-41EE-BC1D-CA98C3B2D32D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A2E4B4CB-9C93-4221-BE16-5CE895055678}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Backlog" sheetId="1" r:id="rId1"/>
@@ -26,14 +26,14 @@
   </definedNames>
   <calcPr calcId="181029"/>
   <customWorkbookViews>
+    <customWorkbookView name="Filter 1" guid="{A7754112-A52F-4ABC-8778-92F04773E53C}" maximized="1" windowWidth="0" windowHeight="0" activeSheetId="0"/>
     <customWorkbookView name="Filter 2" guid="{C25CEB9E-BEC1-4982-90C4-50C84EE1B82A}" maximized="1" windowWidth="0" windowHeight="0" activeSheetId="0"/>
-    <customWorkbookView name="Filter 1" guid="{A7754112-A52F-4ABC-8778-92F04773E53C}" maximized="1" windowWidth="0" windowHeight="0" activeSheetId="0"/>
   </customWorkbookViews>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4474" uniqueCount="1329">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4623" uniqueCount="1368">
   <si>
     <t>ID</t>
   </si>
@@ -6764,6 +6764,239 @@
   </si>
   <si>
     <t>https://www.777homes.com.au/?post_type=property&amp;p=9551&amp;preview=true</t>
+  </si>
+  <si>
+    <t>https://www.allhomes.com.au/67-mobourne-street-bonner-act-2914</t>
+  </si>
+  <si>
+    <t>https://www.allhomes.com.au/unit-14-90-gozzard-street-gungahlin-act-2912</t>
+  </si>
+  <si>
+    <t>https://www.allhomes.com.au/78-lexcen-avenue-nicholls-act-2913</t>
+  </si>
+  <si>
+    <t>https://www.allhomes.com.au/27-baas-becking-street-whitlam-act-2611</t>
+  </si>
+  <si>
+    <t>https://www.allhomes.com.au/2-keith-bain-crest-whitlam-act-2611</t>
+  </si>
+  <si>
+    <t>https://www.allhomes.com.au/18-rosanove-crescent-denman-prospect-act-2611</t>
+  </si>
+  <si>
+    <t>184</t>
+  </si>
+  <si>
+    <t>67 Mobourne Street, Bonner ACT 2914</t>
+  </si>
+  <si>
+    <t>Block/House: 245/ 122</t>
+  </si>
+  <si>
+    <t>Wonderful opportunity to secure beautiful family home in the beautiful suburb of Bonner. This lovely property is fully packed with stylish features. The spacious floor plan provides room to enjoy and the largish outdoor area is perfect to spend evenings with your loved ones. One of the many features is a large modern kitchen with stone bench tops and a northern aspect from the window, where the whole family can help with the cooking.
+Upstairs, the three bedrooms are a good size with a bathroom. There is a powder room with laundry- allowing space for everyone during the morning rush. Rear lane way access to your secure enclosed garage with automatic roller door, plus to the front there is abundant street parking bays for visitors. Ducted reverse-cycle air conditioning ensures a comfortable ambient temperature all year round.
+This home is a convenient walking distance to a choice of shopping centres, schools, parks, and playgrounds. Buzzing with activity the Bonner Shops offer an array of conveniences like Woolworths, BWS and a hot chocolate at Coffee Guru. Located at the end of the street is Neville Bonner Primary School which opened in 2013. Amaroo School is a 1.1km walk while all within 4kms is Burgmann Anglican School, Gungahlin College and Gungahlin Town Centre.
+This is an excellent opportunity. Don't miss out, call Malkiat Dhillon on 0490 174 554 or Gurjant Singh 0497 000 007
+Property Feature:
+• 3 bedrooms all with built in wardrobes
+• Separate downstairs powder room
+• Spacious fold -European laundry
+• Daikin R/C Air Conditioning
+• Abundant storage options - under-stairs, &amp; walk-in linen cupboard.
+• Kitchen with gas cooktop, electric oven, dishwasher
+• Laminated stone benchtop
+• Open plan living and dining opening out to a private courtyard
+• 3 KW Solar System
+Property Information:
+• Block : 245 m2 (approx.)
+• Living : 122.40 m2 (approx.)
+• Garage : 19.73 m2 (approx.)
+• Year Built : 2012
+• EER : 5.5 Stars
+Disclaimer: New Door Properties and the vendor cannot warrant the accuracy of the information provided and will not accept any liability for loss or damage for any errors or misstatements in the information. Some images may be digitally styled/furnished for illustration purposes. Images and floor plans should be treated as a guide only. Purchasers should rely on their own independent enquiries or contact the agent for more information.</t>
+  </si>
+  <si>
+    <t>185</t>
+  </si>
+  <si>
+    <t>14/90 Gozzard Street, Gungahlin ACT 2912</t>
+  </si>
+  <si>
+    <t xml:space="preserve">3	6	0	0	0	0	</t>
+  </si>
+  <si>
+    <t>$360,000</t>
+  </si>
+  <si>
+    <t>This spacious one-bedroom apartment in the Mirella building is perfectly located for a single or couple looking for a modern lifestyle. The retail center of Gungahlin is a short stroll away with its local cafes, shops, department stores, as well as the public library. The local swimming pool, several places of worship and a choice of medical professionals all at walking distance. Nearby, Yerrabi Pond also offers lots of opportunities to enjoy the outdoors with playground, BMX jumps, beginner’s skate park, walking and bicycle path ways.
+This apartment comes with a large sunny balcony. An open plan design connect with generously sized kitchen, dining and living areas. The kitchen includes a breakfast bar, large fridge space, plenty of cupboard space and ample storage.
+This apartment is perfectly suited to a first home buyer who is looking for a pad of their own. Wide corridors and a lift also make this first-floor apartment suitable for someone with accessibility needs, or down-sizers looking for an apartment without the need to regularly use stairs. The proximity of government offices and the light rail terminus also makes this a great opportunity for the savvy investor.
+Property Features Include:
+6-minute walk (450m) to Yerrabi Pond District Park
+9-minute walk (700m) to light rail terminus
+Secure car parking space
+Lock-up storage cage
+Electric cooktop &amp; oven
+Dishwasher
+Separate laundry with dryer
+Built-in wardrobe
+Window covering/blinds
+Drapes and sheer curtains in living area
+Reverse-cycle heating &amp; cooling system
+Call us now to view this delightful apartment before you miss out.</t>
+  </si>
+  <si>
+    <t>186</t>
+  </si>
+  <si>
+    <t>78 Lexcen Avenue, Nicholls ACT 2913</t>
+  </si>
+  <si>
+    <t>Nicholls</t>
+  </si>
+  <si>
+    <t>Block/House: 827/ -</t>
+  </si>
+  <si>
+    <t>This stylish &amp; substantial 5 bedroom home nestled in the prestigious suburb of Nicholls offers a fantastic combination of space, land &amp; location. If you’re looking for the ultimate lifestyle for a large family, then look no further.
+Upon entering this beautiful family home you'll be welcomed by the grand entrance. The stairs will lead you to the second level. The upper level of the home boasts five generous-sized bedrooms. The huge master bedroom boasts a sitting area, a walk-in-robe and spacious, light filled ensuite. The other four rooms are private and offer views of the local hillside and lovely tree lined street or beautifully manicured backyard. The separate family bathroom is easily accessed from all rooms. There is plenty of storage in the hallway cupboards or bedroom built-ins.
+The lower level is the hub of the home, boasting multiple living areas including formal lounge, formal dining and a large open plan living/dining area. The living area flows onto the rear alfresco area. The large kitchen is the center point of the downstairs level. Featuring quality Tasmanian Blackwood timber cabinetry, walk in pantry and plenty of cupboard space. A great view of the garden can be enjoyed from the kitchen window while preparing the family meals. On the lower level you will also find a separate powder room for guests. The internal laundry has easy access to the outside paved area. There is also plenty of storage area on the lower level including under the stairwell, coat cupboard and laundry built-ins.
+Step outside and you'll find the covered, paved alfresco area surrounded by private, manicured gardens making it a prefect space to entertain family and friends. Sit by a fire pit in winter or cook on the BBQ in Summer.
+The home is perfectly positioned on the large 827 sqm block to maximise the use of the land. There is so much usable space left in the yard the possibilities are endless. Zoned RZ1 Suburban &gt;800 sqm. The lockable garden shed tucked away in the corner of the block is perfect for storing all your bikes &amp; tools. The double garage includes storage nook and internal access to the home. Stay warm in winter with the ducted gas heating. Stay cool in summer with the ducted evaporative cooling system. All this plus much more.
+In regards to location you will be spoilt for choice whether it's proximity to schools, public transport, parks, walking tracks, the list goes on. It's all virtually on your doorstep. Walking distance to the Gold Creek Primary and High schools and John Paul II Catholic college. There is a bus stop conveniently positioned less than 100 metres away. Moments away from Gold Creek Country Club, Gungahlin Lakes Golf Club, Gold Creek Village and Casey Market Town. Easy access to major arterial roads and 5 minutes to Gungahlin Town centre.
+Call Anish now on 0450 865 524 before you miss this fantastic opportunity. So you can be in your new home before Christmas, owners may consider offers before Auction date.
+Features include:
+- 5 Bedrooms, 2.5 bathrooms
+- Multiple living areas including formal lounge &amp; formal dining areas
+- Huge master bedroom with extra-large ensuite &amp; walk in robe to match
+- Tasmanian Blackwood timber kitchen with walk in pantry
+- Alfresco area and paved entertainment area
+- Front &amp; side verandah
+- Ducted vacuum
+- Ducted gas heating &amp; ducted evaporative cooling
+- Double garage with storage and internal access
+- Crimsafe security mesh on lower front &amp; side windows/doors
+- Security cameras with 360 degree CCT coverage of house
+- Lockable garden shed
+- Large usable 827 sqm block of land, plenty of space for boat or caravan.
+- Private fully fenced yard with low maintenance manicured gardens
+- NBN Connected
+- Close to schools, shops, golf, parks, lake &amp; walking trails
+Lower floor - 118.18 sqm
+Upper floor - 128.09 sqm
+Garage – 37.68 sqm
+Verandah - 20.01 sqm
+Pergola – 21.09 sqm
+Total area – 325.05 sqm
+Land Area 827 sqm
+Agency has beneficial interest in this property.</t>
+  </si>
+  <si>
+    <t>187</t>
+  </si>
+  <si>
+    <t>27 Baas Becking Street, Whitlam ACT 2611</t>
+  </si>
+  <si>
+    <t>Block/House: 450/ -</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1	4	9	9	0	0	0	</t>
+  </si>
+  <si>
+    <t>$1,499,000+</t>
+  </si>
+  <si>
+    <t>Commencing construction soon. Split contracts available.
+This stunning 5 bedroom home has been tastefully designed with high-end inclusions and finishes throughout to set it apart from the rest.
+The orientation coupled with the expansive windows ensure natural light pours through every aspect of the home, this helps create a welcoming atmosphere no matter what room you find yourself in. The functional floor plan will allow you to flow freely from one room to the next whilst providing the opportunity for a number of segregated living arrangements designed to appeal to a broad range of families.
+The stylish custom made kitchen is a perfect place for the at home master chef or the everyday family cook to create wonderful meals.The formal dining area is the heart of the home, with an alfresco area to the back setting the perfect scene for entertaining and childrens activities in the back yard.
+As you make your way up the stairs you are greeted with another large family room along with two generous bedrooms. The living opens to large balcony with views to enjoy.
+Impressive properties like this do not come along very often and will definitely not disappoint, enquire now before you miss out.
+-Features Include:
+-Architecturally designed home
+-Stunning views
+-Functional design
+-273.5 m2 home space
+-5 Bedrooms
+-Master with walk-in wardrobe and ensuite
+-All bedrooms feature floor to ceiling built-in wardrobes
+-3 bathrooms
+-3 separate living areas
+-Separate alfresco area
+-Upstairs balcony
+-Double glazed windows
+-Downstairs powder room
+-Custom built kitchen
+-40mm Stone bench tops in kitchen
+-Quality appliances
+-Ducted heating and cooling system throughout
+-Large alfresco
+Land 450 sqm</t>
+  </si>
+  <si>
+    <t>188</t>
+  </si>
+  <si>
+    <t>2 Keith Bain Crest, Whitlam ACT 2611</t>
+  </si>
+  <si>
+    <t>Block/House: 300/ 215</t>
+  </si>
+  <si>
+    <t>Construction commencing early 2022. Split contracts available. Contact Anish or Alvin to arrange a meeting.
+These Land settled ready to build homes offers exceptional versatility thanks to its generous 177m2 of internal living space which includes a downstairs studio/4th bedroom with a bathroom plus kitchenette &amp; double car garage with internal access.
+The open plan living &amp; dining area features timber flooring throughout &amp; is overlooked by the superb kitchen which includes quality Bosch appliances &amp; a large walk-in pantry. Smart floor plan ensuring multiple living spaces adds to the value of the property.
+Located upstairs are the 3 bedrooms which includes the over-sized main bedroom complete with a huge walk-in robe &amp; beautifully finished ensuite. Ideal for families of all ages, the main bathroom is conveniently located nearby to the remaining 2 bedrooms &amp; features a bathtub as well as a separate toilet with vanity.
+Each homes have been crafted to ensure every shape &amp; angle work together cohesively, creating a space that you will be proud to call home. From the dimensions of the floor plans to the size of the windows, each feature has been carefully selected for your home.
+Designed &amp; built by local consultants who understand the Canberra region.
+Features:
+- Expected to commence early 2022
+- Walking distance to the proposed Shops and local school.
+- Spacious 177m2 of living with functional floor plan &amp; multiple living areas
+- Premium Bosch kitchen appliances
+- Ducted reverse-cycle heating &amp; cooling
+- Double-glazed windows
+- Full-height tiling in the bathrooms
+- Semi-frameless shower screens
+- LED downlights
+- Studio downstairs with sepearte entry, ensuite and kitchenette with a rental potential of $400 per week.
+- A short drive to the City, Belconnen &amp; Woden
+Home area- 215 sqm
+Land area - 300 sqm</t>
+  </si>
+  <si>
+    <t>189</t>
+  </si>
+  <si>
+    <t>18 Rosanove Crescent, Denman Prospect ACT 2611</t>
+  </si>
+  <si>
+    <t>The Opportunity
+Take this advantage to purchase land only. Settling in 4th Quarter 2022- buy at today's price!
+The Dream :
+In one of the blue ribbon suburbs, with views, before going to Auction. 
+The Wishlist :
+Design your dream house on this block- designed perfectly for your comfort. Is this your final answer?
+Please enquire for the copy of floorplans and inclusions list.</t>
+  </si>
+  <si>
+    <t>Draft</t>
+  </si>
+  <si>
+    <t>https://www.777homes.com.au/?post_type=property&amp;p=9696&amp;preview=true</t>
+  </si>
+  <si>
+    <t>https://www.777homes.com.au/?post_type=property&amp;p=9698&amp;preview=true</t>
+  </si>
+  <si>
+    <t>https://www.777homes.com.au/?post_type=property&amp;p=9700&amp;preview=true</t>
+  </si>
+  <si>
+    <t>https://www.777homes.com.au/?post_type=property&amp;p=9702&amp;preview=true</t>
+  </si>
+  <si>
+    <t>https://www.777homes.com.au/?post_type=property&amp;p=9704&amp;preview=true</t>
   </si>
 </sst>
 </file>
@@ -6930,7 +7163,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="9">
+  <fills count="12">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -6979,6 +7212,21 @@
         <bgColor rgb="FFD9EAD3"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="mediumGray">
+        <bgColor indexed="2"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="mediumGray">
+        <bgColor indexed="2"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="mediumGray">
+        <bgColor indexed="2"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -6993,7 +7241,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="46">
+  <cellXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -7090,6 +7338,9 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="27" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -7326,11 +7577,11 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:AB184"/>
+  <dimension ref="A1:AB190"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A149" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D184" sqref="D184"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A134" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D164" sqref="D164"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1"/>
@@ -10900,7 +11151,7 @@
       <c r="C130" s="41" t="s">
         <v>1043</v>
       </c>
-      <c r="D130" s="4" t="s">
+      <c r="D130" s="39" t="s">
         <v>14</v>
       </c>
       <c r="F130" s="2" t="s">
@@ -10923,7 +11174,7 @@
       <c r="C131" s="41" t="s">
         <v>1030</v>
       </c>
-      <c r="D131" s="4" t="s">
+      <c r="D131" s="39" t="s">
         <v>14</v>
       </c>
       <c r="F131" s="2" t="s">
@@ -10940,14 +11191,14 @@
       <c r="A132">
         <v>131</v>
       </c>
-      <c r="B132" t="s">
+      <c r="B132" s="41" t="s">
         <v>894</v>
       </c>
       <c r="C132" s="41" t="s">
         <v>1031</v>
       </c>
-      <c r="D132" s="4" t="s">
-        <v>7</v>
+      <c r="D132" s="39" t="s">
+        <v>14</v>
       </c>
       <c r="F132" s="2" t="s">
         <v>687</v>
@@ -11154,7 +11405,7 @@
         <v>1040</v>
       </c>
       <c r="D141" s="4" t="s">
-        <v>7</v>
+        <v>14</v>
       </c>
       <c r="F141" s="2" t="s">
         <v>687</v>
@@ -11561,7 +11812,7 @@
       <c r="C159" t="s">
         <v>1162</v>
       </c>
-      <c r="D159" s="4" t="s">
+      <c r="D159" s="39" t="s">
         <v>14</v>
       </c>
       <c r="F159" s="2" t="s">
@@ -11601,14 +11852,14 @@
       <c r="A161">
         <v>160</v>
       </c>
-      <c r="B161" t="s">
+      <c r="B161" s="41" t="s">
         <v>1165</v>
       </c>
       <c r="C161" s="41" t="s">
         <v>1192</v>
       </c>
-      <c r="D161" s="4" t="s">
-        <v>7</v>
+      <c r="D161" s="39" t="s">
+        <v>14</v>
       </c>
       <c r="F161" s="2" t="s">
         <v>1046</v>
@@ -11676,8 +11927,8 @@
       <c r="C164" s="41" t="s">
         <v>1190</v>
       </c>
-      <c r="D164" s="4" t="s">
-        <v>7</v>
+      <c r="D164" s="39" t="s">
+        <v>14</v>
       </c>
       <c r="F164" s="2" t="s">
         <v>687</v>
@@ -11700,7 +11951,7 @@
         <v>1204</v>
       </c>
       <c r="D165" s="4" t="s">
-        <v>7</v>
+        <v>14</v>
       </c>
       <c r="F165" s="2" t="s">
         <v>1046</v>
@@ -12144,6 +12395,141 @@
       </c>
       <c r="H184" t="s">
         <v>323</v>
+      </c>
+    </row>
+    <row r="185" spans="1:8" ht="12.75">
+      <c r="A185">
+        <v>184</v>
+      </c>
+      <c r="B185" s="41" t="s">
+        <v>1329</v>
+      </c>
+      <c r="C185" t="s">
+        <v>1363</v>
+      </c>
+      <c r="D185" s="46" t="s">
+        <v>1362</v>
+      </c>
+      <c r="F185" s="2" t="s">
+        <v>1046</v>
+      </c>
+      <c r="G185" t="s">
+        <v>8</v>
+      </c>
+      <c r="H185" t="s">
+        <v>427</v>
+      </c>
+    </row>
+    <row r="186" spans="1:8" ht="12.75">
+      <c r="A186">
+        <v>185</v>
+      </c>
+      <c r="B186" s="41" t="s">
+        <v>1330</v>
+      </c>
+      <c r="D186" s="39" t="s">
+        <v>14</v>
+      </c>
+      <c r="F186" s="2" t="s">
+        <v>1046</v>
+      </c>
+      <c r="G186" t="s">
+        <v>37</v>
+      </c>
+      <c r="H186" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="187" spans="1:8" ht="12.75">
+      <c r="A187">
+        <v>186</v>
+      </c>
+      <c r="B187" t="s">
+        <v>1331</v>
+      </c>
+      <c r="C187" t="s">
+        <v>1364</v>
+      </c>
+      <c r="D187" s="47" t="s">
+        <v>1362</v>
+      </c>
+      <c r="F187" s="2" t="s">
+        <v>687</v>
+      </c>
+      <c r="G187" t="s">
+        <v>1044</v>
+      </c>
+      <c r="H187" t="s">
+        <v>881</v>
+      </c>
+    </row>
+    <row r="188" spans="1:8" ht="12.75">
+      <c r="A188">
+        <v>187</v>
+      </c>
+      <c r="B188" t="s">
+        <v>1332</v>
+      </c>
+      <c r="C188" t="s">
+        <v>1365</v>
+      </c>
+      <c r="D188" s="47" t="s">
+        <v>1362</v>
+      </c>
+      <c r="F188" s="2" t="s">
+        <v>687</v>
+      </c>
+      <c r="G188" t="s">
+        <v>1044</v>
+      </c>
+      <c r="H188" t="s">
+        <v>881</v>
+      </c>
+    </row>
+    <row r="189" spans="1:8" ht="12.75">
+      <c r="A189">
+        <v>188</v>
+      </c>
+      <c r="B189" t="s">
+        <v>1333</v>
+      </c>
+      <c r="C189" t="s">
+        <v>1366</v>
+      </c>
+      <c r="D189" s="47" t="s">
+        <v>1362</v>
+      </c>
+      <c r="F189" s="2" t="s">
+        <v>687</v>
+      </c>
+      <c r="G189" t="s">
+        <v>1044</v>
+      </c>
+      <c r="H189" t="s">
+        <v>881</v>
+      </c>
+    </row>
+    <row r="190" spans="1:8" ht="12.75">
+      <c r="A190">
+        <v>189</v>
+      </c>
+      <c r="B190" s="41" t="s">
+        <v>1334</v>
+      </c>
+      <c r="C190" t="s">
+        <v>1367</v>
+      </c>
+      <c r="D190" s="48" t="s">
+        <v>1362</v>
+      </c>
+      <c r="F190" s="2" t="s">
+        <v>687</v>
+      </c>
+      <c r="G190" t="s">
+        <v>16</v>
+      </c>
+      <c r="H190" t="s">
+        <v>428</v>
       </c>
     </row>
   </sheetData>
@@ -12397,9 +12783,14 @@
     <hyperlink ref="B182" r:id="rId247" xr:uid="{E7666688-559A-40B8-8519-A3B1439026D5}"/>
     <hyperlink ref="B183" r:id="rId248" xr:uid="{58A9C96C-C741-4EC7-A2E0-D1E238B541D6}"/>
     <hyperlink ref="B184" r:id="rId249" xr:uid="{F68F145A-A9F7-45A2-A86B-CBB159EB1EA1}"/>
+    <hyperlink ref="B186" r:id="rId250" xr:uid="{659C2299-DE98-4086-870A-5DD4E20F0143}"/>
+    <hyperlink ref="B185" r:id="rId251" xr:uid="{9B3A0160-A4E3-496B-9155-A7641E01D0E0}"/>
+    <hyperlink ref="B190" r:id="rId252" xr:uid="{C1EE2E1B-956B-428A-AC64-0F7B6535D886}"/>
+    <hyperlink ref="B132" r:id="rId253" xr:uid="{F70B080A-D856-4314-83D0-9A89F704485A}"/>
+    <hyperlink ref="B161" r:id="rId254" xr:uid="{6506D93F-CFF8-4EE4-B888-E97278A5B631}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId250"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId255"/>
 </worksheet>
 </file>
 
@@ -12408,11 +12799,11 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:AI183"/>
+  <dimension ref="A1:AI189"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A155" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C177" sqref="C177"/>
+    <sheetView workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A140" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E163" sqref="E163"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1"/>
@@ -20270,8 +20661,8 @@
       <c r="A132" s="24" t="s">
         <v>963</v>
       </c>
-      <c r="B132" s="24" t="s">
-        <v>7</v>
+      <c r="B132" s="43" t="s">
+        <v>172</v>
       </c>
       <c r="C132" s="24" t="s">
         <v>964</v>
@@ -20279,8 +20670,8 @@
       <c r="D132" s="24" t="s">
         <v>84</v>
       </c>
-      <c r="E132" s="24" t="s">
-        <v>78</v>
+      <c r="E132" s="43" t="s">
+        <v>172</v>
       </c>
       <c r="F132" s="24" t="s">
         <v>79</v>
@@ -21922,8 +22313,8 @@
       <c r="A160" s="24" t="s">
         <v>1169</v>
       </c>
-      <c r="B160" s="24" t="s">
-        <v>7</v>
+      <c r="B160" s="43" t="s">
+        <v>172</v>
       </c>
       <c r="C160" s="24" t="s">
         <v>1170</v>
@@ -21931,8 +22322,8 @@
       <c r="D160" s="24" t="s">
         <v>84</v>
       </c>
-      <c r="E160" s="24" t="s">
-        <v>78</v>
+      <c r="E160" s="43" t="s">
+        <v>172</v>
       </c>
       <c r="F160" s="24" t="s">
         <v>207</v>
@@ -22099,8 +22490,8 @@
       <c r="A163" s="24" t="s">
         <v>1183</v>
       </c>
-      <c r="B163" s="24" t="s">
-        <v>7</v>
+      <c r="B163" s="43" t="s">
+        <v>172</v>
       </c>
       <c r="C163" s="24" t="s">
         <v>1184</v>
@@ -22108,8 +22499,8 @@
       <c r="D163" s="24" t="s">
         <v>84</v>
       </c>
-      <c r="E163" s="24" t="s">
-        <v>78</v>
+      <c r="E163" s="43" t="s">
+        <v>172</v>
       </c>
       <c r="F163" s="24" t="s">
         <v>79</v>
@@ -23334,22 +23725,376 @@
         <v>1191</v>
       </c>
     </row>
+    <row r="184" spans="1:21" ht="12.75">
+      <c r="A184" t="s">
+        <v>1335</v>
+      </c>
+      <c r="B184" t="s">
+        <v>1362</v>
+      </c>
+      <c r="C184" t="s">
+        <v>1336</v>
+      </c>
+      <c r="D184" t="s">
+        <v>84</v>
+      </c>
+      <c r="E184" t="s">
+        <v>78</v>
+      </c>
+      <c r="F184" t="s">
+        <v>79</v>
+      </c>
+      <c r="G184" t="s">
+        <v>138</v>
+      </c>
+      <c r="H184" t="s">
+        <v>1337</v>
+      </c>
+      <c r="I184" t="s">
+        <v>198</v>
+      </c>
+      <c r="K184" t="s">
+        <v>199</v>
+      </c>
+      <c r="L184" t="s">
+        <v>1290</v>
+      </c>
+      <c r="M184" t="s">
+        <v>202</v>
+      </c>
+      <c r="N184" t="s">
+        <v>266</v>
+      </c>
+      <c r="P184" t="s">
+        <v>252</v>
+      </c>
+      <c r="Q184" t="s">
+        <v>266</v>
+      </c>
+      <c r="R184" t="s">
+        <v>1336</v>
+      </c>
+      <c r="S184" t="s">
+        <v>1338</v>
+      </c>
+      <c r="T184" t="s">
+        <v>1046</v>
+      </c>
+      <c r="U184" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="185" spans="1:21" ht="14.25">
+      <c r="A185" t="s">
+        <v>1339</v>
+      </c>
+      <c r="B185" s="43" t="s">
+        <v>172</v>
+      </c>
+      <c r="C185" t="s">
+        <v>1340</v>
+      </c>
+      <c r="D185" t="s">
+        <v>77</v>
+      </c>
+      <c r="E185" s="43" t="s">
+        <v>172</v>
+      </c>
+      <c r="F185" t="s">
+        <v>79</v>
+      </c>
+      <c r="G185" t="s">
+        <v>79</v>
+      </c>
+      <c r="H185" t="s">
+        <v>594</v>
+      </c>
+      <c r="I185" t="s">
+        <v>198</v>
+      </c>
+      <c r="K185" t="s">
+        <v>1341</v>
+      </c>
+      <c r="L185" t="s">
+        <v>1342</v>
+      </c>
+      <c r="M185" t="s">
+        <v>266</v>
+      </c>
+      <c r="N185" t="s">
+        <v>266</v>
+      </c>
+      <c r="P185" t="s">
+        <v>203</v>
+      </c>
+      <c r="Q185" t="s">
+        <v>266</v>
+      </c>
+      <c r="R185" t="s">
+        <v>1340</v>
+      </c>
+      <c r="S185" t="s">
+        <v>1343</v>
+      </c>
+      <c r="T185" t="s">
+        <v>1046</v>
+      </c>
+      <c r="U185" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="186" spans="1:21" ht="12.75">
+      <c r="A186" t="s">
+        <v>1344</v>
+      </c>
+      <c r="B186" t="s">
+        <v>1362</v>
+      </c>
+      <c r="C186" t="s">
+        <v>1345</v>
+      </c>
+      <c r="D186" t="s">
+        <v>84</v>
+      </c>
+      <c r="E186" t="s">
+        <v>78</v>
+      </c>
+      <c r="F186" t="s">
+        <v>79</v>
+      </c>
+      <c r="G186" t="s">
+        <v>1346</v>
+      </c>
+      <c r="H186" t="s">
+        <v>1347</v>
+      </c>
+      <c r="I186" t="s">
+        <v>198</v>
+      </c>
+      <c r="K186" t="s">
+        <v>199</v>
+      </c>
+      <c r="L186" t="s">
+        <v>908</v>
+      </c>
+      <c r="M186" t="s">
+        <v>252</v>
+      </c>
+      <c r="N186" t="s">
+        <v>204</v>
+      </c>
+      <c r="P186" t="s">
+        <v>202</v>
+      </c>
+      <c r="Q186" t="s">
+        <v>204</v>
+      </c>
+      <c r="R186" t="s">
+        <v>1345</v>
+      </c>
+      <c r="S186" t="s">
+        <v>1348</v>
+      </c>
+      <c r="T186" t="s">
+        <v>687</v>
+      </c>
+      <c r="U186" t="s">
+        <v>1044</v>
+      </c>
+    </row>
+    <row r="187" spans="1:21" ht="12.75">
+      <c r="A187" t="s">
+        <v>1349</v>
+      </c>
+      <c r="B187" t="s">
+        <v>1362</v>
+      </c>
+      <c r="C187" t="s">
+        <v>1350</v>
+      </c>
+      <c r="D187" t="s">
+        <v>84</v>
+      </c>
+      <c r="E187" t="s">
+        <v>78</v>
+      </c>
+      <c r="F187" t="s">
+        <v>235</v>
+      </c>
+      <c r="G187" t="s">
+        <v>236</v>
+      </c>
+      <c r="H187" t="s">
+        <v>1351</v>
+      </c>
+      <c r="I187" t="s">
+        <v>198</v>
+      </c>
+      <c r="K187" t="s">
+        <v>1352</v>
+      </c>
+      <c r="L187" t="s">
+        <v>1353</v>
+      </c>
+      <c r="M187" t="s">
+        <v>252</v>
+      </c>
+      <c r="N187" t="s">
+        <v>202</v>
+      </c>
+      <c r="P187" t="s">
+        <v>203</v>
+      </c>
+      <c r="Q187" t="s">
+        <v>204</v>
+      </c>
+      <c r="R187" t="s">
+        <v>1350</v>
+      </c>
+      <c r="S187" t="s">
+        <v>1354</v>
+      </c>
+      <c r="T187" t="s">
+        <v>687</v>
+      </c>
+      <c r="U187" t="s">
+        <v>1044</v>
+      </c>
+    </row>
+    <row r="188" spans="1:21" ht="12.75">
+      <c r="A188" t="s">
+        <v>1355</v>
+      </c>
+      <c r="B188" t="s">
+        <v>1362</v>
+      </c>
+      <c r="C188" t="s">
+        <v>1356</v>
+      </c>
+      <c r="D188" t="s">
+        <v>84</v>
+      </c>
+      <c r="E188" t="s">
+        <v>78</v>
+      </c>
+      <c r="F188" t="s">
+        <v>235</v>
+      </c>
+      <c r="G188" t="s">
+        <v>236</v>
+      </c>
+      <c r="H188" t="s">
+        <v>1357</v>
+      </c>
+      <c r="I188" t="s">
+        <v>198</v>
+      </c>
+      <c r="K188" t="s">
+        <v>278</v>
+      </c>
+      <c r="L188" t="s">
+        <v>279</v>
+      </c>
+      <c r="M188" t="s">
+        <v>201</v>
+      </c>
+      <c r="N188" t="s">
+        <v>202</v>
+      </c>
+      <c r="P188" t="s">
+        <v>203</v>
+      </c>
+      <c r="Q188" t="s">
+        <v>204</v>
+      </c>
+      <c r="R188" t="s">
+        <v>1356</v>
+      </c>
+      <c r="S188" t="s">
+        <v>1358</v>
+      </c>
+      <c r="T188" t="s">
+        <v>687</v>
+      </c>
+      <c r="U188" t="s">
+        <v>1044</v>
+      </c>
+    </row>
+    <row r="189" spans="1:21" ht="12.75">
+      <c r="A189" t="s">
+        <v>1359</v>
+      </c>
+      <c r="B189" t="s">
+        <v>1362</v>
+      </c>
+      <c r="C189" t="s">
+        <v>1360</v>
+      </c>
+      <c r="D189" t="s">
+        <v>234</v>
+      </c>
+      <c r="E189" t="s">
+        <v>78</v>
+      </c>
+      <c r="F189" t="s">
+        <v>235</v>
+      </c>
+      <c r="G189" t="s">
+        <v>1009</v>
+      </c>
+      <c r="H189" t="s">
+        <v>872</v>
+      </c>
+      <c r="I189" t="s">
+        <v>198</v>
+      </c>
+      <c r="K189" t="s">
+        <v>199</v>
+      </c>
+      <c r="L189" t="s">
+        <v>1290</v>
+      </c>
+      <c r="M189" t="s">
+        <v>199</v>
+      </c>
+      <c r="N189" t="s">
+        <v>199</v>
+      </c>
+      <c r="P189" t="s">
+        <v>199</v>
+      </c>
+      <c r="Q189" t="s">
+        <v>199</v>
+      </c>
+      <c r="R189" t="s">
+        <v>1360</v>
+      </c>
+      <c r="S189" t="s">
+        <v>1361</v>
+      </c>
+      <c r="T189" t="s">
+        <v>687</v>
+      </c>
+      <c r="U189" t="s">
+        <v>16</v>
+      </c>
+    </row>
   </sheetData>
   <autoFilter ref="E1:E145" xr:uid="{00000000-0001-0000-0100-000000000000}"/>
   <customSheetViews>
-    <customSheetView guid="{C25CEB9E-BEC1-4982-90C4-50C84EE1B82A}" filter="1" showAutoFilter="1">
-      <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-      <autoFilter ref="A1:AD33" xr:uid="{5166EA08-007D-4915-A86F-65CA3448F68C}"/>
-    </customSheetView>
     <customSheetView guid="{A7754112-A52F-4ABC-8778-92F04773E53C}" filter="1" showAutoFilter="1">
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-      <autoFilter ref="A1:AD33" xr:uid="{13B0600A-1985-4657-AE39-6340220251FB}">
+      <autoFilter ref="A1:AD33" xr:uid="{70CEED1F-EDC4-495B-9A60-706864A60681}">
         <filterColumn colId="5">
           <filters blank="1">
             <filter val="Strathnairn"/>
           </filters>
         </filterColumn>
       </autoFilter>
+    </customSheetView>
+    <customSheetView guid="{C25CEB9E-BEC1-4982-90C4-50C84EE1B82A}" filter="1" showAutoFilter="1">
+      <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+      <autoFilter ref="A1:AD33" xr:uid="{46324FE2-865E-40F0-BF1D-A014DB3FB5C1}"/>
     </customSheetView>
   </customSheetViews>
   <conditionalFormatting sqref="A1:AI1">

</xml_diff>

<commit_message>
New property listings 19/11/2021
</commit_message>
<xml_diff>
--- a/src/main/resources/InputTestdata/Listing details.xlsx
+++ b/src/main/resources/InputTestdata/Listing details.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Athavan\git\777Homes-2\777Homes-business\src\main\resources\InputTestdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr documentId="13_ncr:1_{85A68492-E5A8-49F4-99FD-2915FA476FA1}" revIDLastSave="0" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47"/>
+  <xr:revisionPtr documentId="13_ncr:1_{9883F752-EF45-47AF-AEDF-503AD9816390}" revIDLastSave="0" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47"/>
   <bookViews>
     <workbookView activeTab="1" windowHeight="15840" windowWidth="29040" xWindow="-120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}" yWindow="-120"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5004" uniqueCount="1467">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5289" uniqueCount="1536">
   <si>
     <t>ID</t>
   </si>
@@ -7547,19 +7547,488 @@
 Rainwater tanks</t>
   </si>
   <si>
+    <t>https://www.777homes.com.au/?post_type=property&amp;p=9982&amp;preview=true</t>
+  </si>
+  <si>
+    <t>https://www.777homes.com.au/?post_type=property&amp;p=9986&amp;preview=true</t>
+  </si>
+  <si>
+    <t>https://www.777homes.com.au/?post_type=property&amp;p=9988&amp;preview=true</t>
+  </si>
+  <si>
+    <t>https://www.777homes.com.au/?post_type=property&amp;p=9990&amp;preview=true</t>
+  </si>
+  <si>
+    <t>$899,000+</t>
+  </si>
+  <si>
+    <t>https://www.allhomes.com.au/unit-86-235-flemington-road-franklin-act-2913</t>
+  </si>
+  <si>
+    <t>https://www.allhomes.com.au/20-barramundi-street-throsby-act-2914</t>
+  </si>
+  <si>
+    <t>https://www.allhomes.com.au/54-clancy-mckenna-crescent-bonner-act-2914</t>
+  </si>
+  <si>
+    <t>https://www.allhomes.com.au/8-niland-street-whitlam-act-2611</t>
+  </si>
+  <si>
+    <t>https://www.allhomes.com.au/37-corkery-crescent-taylor-act-2913</t>
+  </si>
+  <si>
+    <t>https://www.allhomes.com.au/unit-14-60-copland-drive-evatt-act-2617</t>
+  </si>
+  <si>
+    <t>https://www.allhomes.com.au/3-maclaurin-crescent-chifley-act-2606</t>
+  </si>
+  <si>
+    <t>https://www.allhomes.com.au/34-adventure-street-harrison-act-2914</t>
+  </si>
+  <si>
+    <t>https://www.allhomes.com.au/14-stan-davey-rise-coombs-act-2611</t>
+  </si>
+  <si>
+    <t>https://www.allhomes.com.au/unit-4-3-adventure-street-harrison-act-2914</t>
+  </si>
+  <si>
+    <t>https://www.allhomes.com.au/unit-9-21-samaria-street-crace-act-2911</t>
+  </si>
+  <si>
+    <t>205</t>
+  </si>
+  <si>
+    <t>86/235 Flemington Road, Franklin ACT 2913</t>
+  </si>
+  <si>
+    <t>Block/House: 7612/ 108</t>
+  </si>
+  <si>
+    <t>New Door Properties is proud to present being located in a prime and central location, this spacious Franklin townhouse offers a central lifestyle located just minutes from the light rail, Franklin local school, local shops and the Gungahlin Town Centre!
+Set in a secure building, this property is ideal for those that seek comfort or are simply looking to invest. Bright and light-filled, this immaculate townhouse comes with impressive features and utmost convenience, their first owners have always cared and looked after the property in its best presentation.
+The kitchen has plenty of storage, electric cooking appliances and a dishwasher that overlooks the living area with a split system and much more. The complex includes an in-ground swimming pool, BBQ area and a landscaped courtyard for exclusive use of residents.
+What you get:
+3 Bed | 2 Bath | 2 Car + Storage Cage
+- Three spacious bedrooms with BIR
+- Master Bedroom with En-suite
+- One spacious bedroom on ground floor, and other two on level one
+- Modern kitchen with Bosch stainless steel appliances
+- 20 mm Kitchen stone bench-top
+- Tiles Splash-back in kitchen
+- 600 mm stainless steel appliances
+- Separate toilet on ground floor
+- European style laundry
+- Laminate flooring in living areas
+- Carpet in bedrooms
+- Ducted reverse cycle heating and cooling
+- Two reverse cycle Toshiba units in family living &amp; main bedroom
+- High ceilings throughout the house
+- Secure entrance to the building
+- Under stairs storage
+- Secure and low maintenance front yard and backyard
+- Secure underground parking
+Location:
+- Walking distance to Local shops &amp; Woolworths metro
+- Convenience at its doorstep light rail &amp; bus stop
+- Close proximity to Franklin &amp; Harrison Public School
+- Close proximity to playing fields and walking strips
+Property Details:
+Living Area: 104.7 m2
+Courtyard: 34 m2
+Total Area: 138.7 m2
+EER: 6 Stars
+Strata : $1021.00 pq approx.
+Rates : $391.00 pq approx.
+Rental Estimate: $580 - $600 per week
+Disclaimer: New Door Properties and the vendor cannot warrant the accuracy of the information provided and will not accept any liability for loss or damage for any errors or misstatements in the information. Some images may be digitally styled/furnished for illustration purposes. Images and floor plans should be treated as a guide only. Purchasers should rely on their own independent enquiries or contact the agent for more information.</t>
+  </si>
+  <si>
+    <t>206</t>
+  </si>
+  <si>
+    <t>20 Barramundi Street, Throsby ACT 2914</t>
+  </si>
+  <si>
+    <t>Block/House: 420/ 230</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1	2	9	9	0	0	0	</t>
+  </si>
+  <si>
+    <t>Offers above $1,299,000</t>
+  </si>
+  <si>
+    <t>Please Contact Gurjant or Yash for private inspections.
+This stunning light filled home offers a blend of style, class and unprecedented luxury whilst being set on a generous 420 m2 block. The immaculately presented residence is equipped with 4 spacious bedrooms, 3 bathrooms, multiple living areas in outdoor you are greeted by an entertainment alfresco area with low maintenance yard.
+The modern kitchen boasts quality appliances, walk in pantry. Other features include High ceilings, Reverse-cycle ducted air-conditioning a with zones and a low maintenance yard.
+Separate access to one bedroom with en-suite &amp; extra kitchenette , which can be rent it out and earn second income, or can be used as a teenagers' or parents' retreat or your own home office.
+Conveniently located close to shops, schools, public transportation, parks and only a short drive to Gungahlin shopping centre, this home offers a very comfortable and an enviable lifestyle.
+Features include :
+• Four Bedrooms
+• Two Master bedrooms with en-suites
+• Separate access to one bedroom with extra kitchenette
+• Double glazed windows throughout
+• LED down lights throughout the house
+• Modern kitchen
+• Walk in Pantry
+• Stone bench-tops
+• Cooktop, oven and ducted range-hood
+• Ducted reverse cycle heating and cooling with zones
+• Full length tiles and tub in main bathroom
+• Custom vanities
+• Low maintenance yard
+• Fully landscaped
+Property information
+• Land Size : 420 m2 (approx..)
+• Living : 176.40 (approx..)
+• Garage : 37.50 (approx..)
+• Alfresco : 11.20 (approx..)
+• Porch : 5.40 (approx..)
+• Year built : 2021</t>
+  </si>
+  <si>
+    <t>207</t>
+  </si>
+  <si>
+    <t>54 Clancy McKenna Crescent, Bonner ACT 2914</t>
+  </si>
+  <si>
+    <t>Block/House: 422/ 143</t>
+  </si>
+  <si>
+    <t>Auction 11/12/21</t>
+  </si>
+  <si>
+    <t>New Door Properties is proud to present this amazing opportunity in the finest suburb of Bonner, home is a perfect outlook for a growing family or someone looking to begin their real estate journey.
+The home comprises of three bedrooms, two separate living areas, kitchen features stainless steel appliances, gas cooktop, integrated oven, dishwasher, ducted range hood, tiled splash back, ample of cupboard space, with generous bench-tops and a convenient breakfast bar, the well-maintained space is ready to handle whatever you throw at it.
+Cast your eyes across the landscaped gardens, and it's easy to see that there is something special on offer inside. Within walking distance to local shops and primary schools, this is the perfect place to raise a young family.
+Don't miss out and call to book your inspection!
+3 bed | 2 bath | 2 car garage
+What you get:
+- Single level with two separate living areas
+- Three spacious Bedrooms
+- Main Bedroom with en-suite &amp; WIR
+- Bedroom 2 and 3 with BIR
+- Ceiling fan with lights in main bed and bed 2
+- Floor to ceiling tiles in bathrooms
+- Separate toilet
+- Spacious laundry with outdoor access
+- Modern kitchen with stone bench top
+- 900mm gas cooktop with integrated electric oven
+- 900MM Omega ducted range-hood
+- 600mm Asko dishwasher
+- Spacious open plan family/meals/kitchen areas access to backyard
+- Ducted gas heating and evaporative cooling
+- Double glazed windows
+- Low maintenance front yard and backyard
+- Tiled Pergola
+- Storage shed
+- Double lock up garage with auto door
+- Garage storage loft with pull-down ladder to access
+- Concreted all around the house
+- 26L gas hot water system
+- 1000L rain water tank
+- NBN Connected
+Location:
+- Close proximity to walking strips and playing fields
+- Small drive to Mulligan Flats and Dog park
+- Close proximity to local shops &amp; Woolworths Bonner
+- Small drive to Neville Bonner Primary School
+- Convenient location and easy access to public transport
+Property Information:
+Block : 422 m2 (approx.)
+House : 146 m2 (approx.)
+Garage : 43 m2 (approx.)
+Pergola : 24m2 (approx.)
+Year Built : 2012
+EER : 6 Stars
+Disclaimer: New Door Properties and the vendor cannot warrant the accuracy of the information provided and will not accept any liability for loss or damage for any errors or misstatements in the information. Some images may be digitally styled/furnished for illustration purposes. Images and floor plans should be treated as a guide only. Purchasers should rely on their own independent enquiries or contact the agent for more information.</t>
+  </si>
+  <si>
+    <t>208</t>
+  </si>
+  <si>
+    <t>8 Niland Street, Whitlam ACT 2611</t>
+  </si>
+  <si>
+    <t>Block/House: 641/ 397</t>
+  </si>
+  <si>
+    <t>$1,500,000</t>
+  </si>
+  <si>
+    <t>The home comes with a plethora of parks, recreational areas and within easy commute to local shops, schools and Belconnen Town Centre. This spacious 5-bedroom home is situated on 641sqm block with northerly aspect and boasts a huge formal lounge room at front of house for intimate gatherings among family and friends. The home will feature high ceiling throughout, extra-large family &amp; dining area, wider hallways which adds to the size of the open plan living space to enjoy lifestyle at its best. The large stunning kitchen will be hub of this home and feature all modern comforts including walk in pantry, waterfall edged island bench and quality stainless steel appliances for the home chef to cook healthy meals on daily basis.
+This home features three bedrooms with ensuite and each bedroom is secluded from the other bedrooms. All other bedrooms are spacious and include built-in wardrobes. All 4-bathrooms are modern &amp; well designed for daily comfort. To enjoy the weather in all seasons, this home will have double glazed windows, insulation in external walls &amp; ceiling and ducted multi zoned heating &amp; cooling system. The outdoor alfresco area which opens from the family area is under the same roof line, fantastic for entertaining or barbecue within a very private backyard. The home is situated in one of the best neighbourhood of Whitlam, close to school/s, park with wetlands, beautiful walking and cycling tracks and much more to see and do daily.
+Property Features Include:
+2-Story design with high ceiling
+Double glazed windows
+Multi zoned ducted heating &amp; cooling system
+LED energy saving down lights throughout
+Sensor lights at front
+Local alarm system
+Video doorbell intercom system
+Wider hallways
+3 x Bedroom with ensuite
+Dazzling kitchen with walk-in pantry
+Stone bench tops &amp; ample cupboards
+Stainless-steel appliances
+Storage &amp; bicycle area in garage
+Colorbond roof
+Alfresco under same roofline
+Good size backyard
+Rainwater tank 4000 liters
+Proximity to local schools
+Parks, walking and bicycle tracks nearby
+Minutes to Belconnen Town Centre and the City
+Call Shaun to review this wonderful house and land package.</t>
+  </si>
+  <si>
+    <t>209</t>
+  </si>
+  <si>
+    <t>37 Corkery Crescent, Taylor ACT 2913</t>
+  </si>
+  <si>
+    <t>Block/House: 240/ 180</t>
+  </si>
+  <si>
+    <t xml:space="preserve">8	7	9	0	0	0	</t>
+  </si>
+  <si>
+    <t>$879,000 +</t>
+  </si>
+  <si>
+    <t>Open home held at Builders Display - 2 Quokka St, Throsby.
+Confidence Real Estate is proud to present a wonderful opportunity to provide you with a quality new home in Canberra's most desirable suburb Taylor.
+Taylor has experienced an extensive growth of 28% over the last 6 months. With a new high school announced this region is picking its pace.
+This property represents great value to first home buyers and downsizers and will be ready to move in 6 months from now. This single level design has 4 bedrooms with an abundance of natural light, the main bedroom and guest room with it's own ensuite and a huge main bathroom featuring a luxurious stand alone bath.
+The value does not stop there; double glazed windows and ducted reverse cycle heating/cooling throughout combines to give a 6 star Energy Efficiency Rating (EER) which means you can keep your heating and cooling bills to a minimum while living in comfort all year round.
+A spacious open plan living area and kitchen brings the family together and the generous raked ceiling height adds to the overall ambience of the living space.
+Whether you are buying your first home or downsizing, Taylor has so much to offer. A beautiful bush setting with walking trails and bike paths throughout.
+Act fast as this value packed property won't last long at this price.
+Approx 180.5 sqm of House
+Large bathroom with freestanding bath
+Open plan living with high ceilings
+Ducted reverse cycle air-conditioning
+Double glazing throughout
+2.7m high ceilings
+NBN ready
+Minimum 6.0 EER
+CALL ALVIN NOW ON 0426 146 118 FOR MORE INFORMATION.</t>
+  </si>
+  <si>
+    <t>210</t>
+  </si>
+  <si>
+    <t>14/60 Copland Drive, Evatt ACT 2617</t>
+  </si>
+  <si>
+    <t>Situated in the leafy Woollahra Gardens complex, this spotless and tastefully styled three bedroom ensuite townhouse represents a superb opportunity for first home buyers, professional couples or investors who are searching for something special! If you're in the market for low maintenance living in an ultra-convenient location, this is the one for you.
+Upon your arrival at 14/60 Copland Drive, you are greeted by a peaceful courtyard garden which leads you indoors to a welcoming entry with stunning timber floors. Sure to appeal to buyers is the north facing aspect of the townhouse and sun filled open plan kitchen, dining and living rooms which overlook an enclosed and private courtyard. The outdoor entertaining area comes complete with timber decking adding the summer space to the place. Continuing on this level is a separate laundry and toilet for your convenience, with internal access from the garage and generous under stair storage.
+The upstairs of this delightful townhouse is also blessed with natural light and provides three spacious bedrooms; all with built in robes, sparkling main bathroom and the master bedroom with a modern ensuite. Sure to appeal are bedrooms two and three, both providing access to a shared and expansive north facing balcony offering a leafy and tranquil outlook.
+Walking distance to the popular Ginninderra Creek Nature Reserve and Miles Franklin and St Monica's Primary Schools. Conveniently close to local amenities such as Evatt Shops, Copland College, Belconnen Town Centre and Markets and Lake Ginninderra. Its central location also ensures easy access to all of Belconnen's major facilities including Canberra University, ANU, Calvary Hospital, AIS and Bruce Stadium.
+Features include:
+- Three spacious bedrooms; all with built in robes
+- Main bedroom with ensuite
+- Laminated flooring
+- Tastefully updated kitchen
+- Stunning floating floors
+- Plenty of natural light flooding the place
+- Balcony accessible from second and third bedrooms
+- Separate laundry with third toilet
+- Under stair storage with door access
+- Single garage with remote and internal access
+- Additional allocated parking space
+- Ample off street parking
+- Peaceful and friendly complex
+- Front and rear courtyards are designed for maximum privacy and minimal maintenance</t>
+  </si>
+  <si>
+    <t>211</t>
+  </si>
+  <si>
+    <t>3 MacLaurin Crescent, Chifley ACT 2606</t>
+  </si>
+  <si>
+    <t>Block/House: 700/ -</t>
+  </si>
+  <si>
+    <t>Ready to move in before Christmas!
+An exciting opportunity to secure this aesthetically renovated family home in the highly desirable suburb of Chifley. This extensively renovated home is situated on an easy-care parcel of land close to all amenities within a short stroll to the Woden town centre.
+The front entry door is crafted from natural timber with an incredible steel carved door handle adding to the designer feel of the home. The moment you enter this home you will be welcomed into the beautiful layout of European Oak hardwood floors that draws your attention to the spacious living areas, generously sized kitchen fitted with European appliances &amp; Caesarstone benchtops and family area featuring attractive joinery complete with a study nook. The family room connects to a covered entertaining deck with plenty of space to entertain your loved ones while watching the kids play in the new outdoor deck area.
+Accommodation includes four bedrooms, segregated master with ensuite and walk-in wardrobe and two lovely decks overlooking the backyard. Fully renovated bathroom, brand new kitchen and easy care gardens. To increase the comfort and enjoyment of the home, additional features include double glazed windows and doors, ducted reverse cycle heating and cooling, a double automatic garage and dual circular driveway.
+Within a short stroll to all Woden facilities makes this property an ideal investment opportunity or a family home to live in.
+Features:
+Centrally located
+Secondary potential being located in RZ2
+700 sqm flat block
+Dual Circular driveway
+Four bedrooms
+Segregated master with ensuite
+Built in robes in all bedrooms
+Formal lounge and dining room
+Modern fully renovated bathroom
+Separate toilet
+Large updated kitchen with quality joinery, stone benchtops, gas cooktop, wall-mount range-hood, In built micro-wave and built in Oven
+Double glazed windows and doors
+Ducted reverse cycle heating and cooling
+Open plan living &amp; dining flows through to a covered deck
+Oversize double brick garage
+Secure/easy care gardens with fruiting trees
+Close to schools, shops &amp; public transport
+Walking distance to Woden town Centre, Chifley &amp; Phillip shops, Melrose High School &amp; Marist College
+Minutes to Woden and Canberra City
+Walking distance to reputed schools and Canberra College, Westfield Woden, Woden public transport hub, the soon-to-be-built Light Rail and Woden Canberra Institute of Technology (CIT) campus, Chifley neighbourhood oval, Chifley shops and popular 'A Bite to Eat' café, Phillip shops and Mt Taylor to enjoy at walking proximity. With easy access to major arterial roads, the Tuggeranong Parkway and Hindmarsh drive that allows a short commute to Canberra City, locations don't get much better than this.
+Call Anish now on 0450 865 524 before you miss out.
+Land size: 700 m2
+EER: 3</t>
+  </si>
+  <si>
+    <t>212</t>
+  </si>
+  <si>
+    <t>34 Adventure Street, Harrison ACT 2914</t>
+  </si>
+  <si>
+    <t>Block/House: 329/ 171</t>
+  </si>
+  <si>
+    <t>This beautiful elevated four-bedroom property in Harrison will make the perfect family home for those looking for plenty of space, comfort and a great location. Situated in an ideal spot on Adventure Street you'll enjoy unobstructed views over the city and Black Mountain from the comfort and privacy of the lounge room.
+The kitchen boasts a modern design with its stone island bench and elegant glass splashback. It features a 900 mm gas cooktop and glass canopy range hood to make catering for loved ones a joy.
+The home has two separate living areas while the third and fourth bedroom can be converted to a separate studio with external access.
+As a fantastic family-friendly suburb, getting around Harrison and Canberra is made easy thanks to the light rail network. You will live only a 5-minute drive from Harrison Public School and Wonderschool Early Learning Centre ensuring convenience. The home is also close proximity to pond and DA approved Kenny School. Call Anish now to view on 0450 865 524.
+House size: 171 sqm approx
+Land : 329 sqm approx
+- Family friendly floor plan ( 2 beds at the front of the home and 2 at the back )
+- Generously sized Master bedroom with walk-in-robe and ensuite.
+- Studio option with additional bathroom and separate access.
+- Formal lounge
+- Family/meals area
+- Storage in the bedrooms
+- Large kitchen with stone bench tops, five burner gas cooktop, dishwasher and neutral colour palette
+- Ducted heating and cooling through out
+- Internal access from the double garage
+- Entertaining space includes Spa and outdoor BBQ facilities
+- Low maintenance yard
+- Views to Black Mountain from the front of the home
+- Double glazed windows, high ceilings with rendered exterior
+- Harrison Public Schools and Wonderschool Early Learning Centre a quick drive away
+- DA approved Kenny school is in 5 minutes walk
+- Easy access to Horse Park Drive, Gungahlin drive and Federal highway
+- Walk to light rail terminal.</t>
+  </si>
+  <si>
+    <t>213</t>
+  </si>
+  <si>
+    <t>14 Stan Davey Rise, Coombs ACT 2611</t>
+  </si>
+  <si>
+    <t>Block/House: 557/ 332</t>
+  </si>
+  <si>
+    <t>Flawless in design and craftsmanship, immaculately presented, this architecturally designed home has been built to showcase the latest in contemporary living, featuring spectacular views, beautiful indoor/outdoor living spaces, and the latest state of the art appointments.
+The seamless split-level design features 3 segregated zones for energy efficiency - ideal for families with older children and/or extended families. Its extensive floorplan features four generous bedrooms, main bathroom, powder room, master bathroom and three separate living areas. Key features include the luxurious master suite, featuring a large private balcony with lake views the segregated bedroom wing, which includes a rumpus room.
+The large open plan kitchen, dining and lounge space flow seamlessly to the outdoor areas, perfect for summer entertaining and movie nights. The mind blowing water feature with projector screen is sure to entertain family and friends.
+The homes energy requirements are supported by Solar panels connected to the grid (12.5KW).Situated within close proximity to several parklands, schools, shopping centres and key arterial roads.
+This outstanding, versatile, high quality home has many extras. It is all set up and established for your effortless, harmonic lifestyle in a highly popular suburb. You will be proud to call it home! This property won't last. Please call Anish now on 0450 865 524.
+Features:
+- Spectacular views to lakes and valley.
+- Segregated luxury master suite with exceptional views, private balcony, walk in robe and luxurious bathroom.
+- Three separate living areas
+- Formal lounge room
+- Open-plan kitchen, dining and lounge area with fire place overlooking expansive outdoor living
+- Gourmet kitchen with European appliances, plumbed-in fridge, oven, gas cook top and walk-in-pantry.
+- All Bathrooms feature in-floor heating and floor to ceiling tiles
+- Rumpus room in bedroom wing upstairs
+- Solar panels connected to the grid (12.5 KW) provision for battery
+- Wi Fi controlled Ducted reverse cycle heating and cooling - 3 zones.
+- Automated blinds and curtains.
+- Smart lock with fingerprint, password and tag access.
+- Double garage
+- Built in 2018</t>
+  </si>
+  <si>
+    <t>214</t>
+  </si>
+  <si>
+    <t>4/3 Adventure Street, Harrison ACT 2914</t>
+  </si>
+  <si>
+    <t>Set in one of Harrison's best boutique complex, this single level, free standing, town house is positioned to take advantage of all that the area has to offer. Within walking distance to Harrison schools, public transport, local supermarkets and restaurants.An admired, architect-designed complex that offers a modern, light and bright feel from the street and throughout the home, the property has been presented with lifestyle in mind.
+Enter through the secure double carport with automatic single panel lift door to discover a fully enclosed yard, safe for children and pets to play.
+Entertaining will be a breeze with the spacious kitchen that features stainless steel appliances and overlooks the open plan family and meals area. Large floor to ceiling double glazed windows and sliding door seamlessly connect the indoors with the garden and allow natural light to flood the home throughout the day.
+All three bedrooms offer built in robes and the master features a spacious ensuite for added luxury and convenience.With an amazing list of inclusions to follow please read on and if you have any questions I encourage you to contact me ASAP.
+Features Include:
+- Single level three bedroom home
+- Open plan living/dining
+- Main bedroom with mirrored robe and ensuite
+- Two bedrooms with built in mirrored robes
+- Floor to ceiling glass in living areas
+- Ducted reverse cycle heating and cooling
+- Solar hot water system with electric boost
+- Main bathroom with full size bath
+- Brand new roller blinds
+- Double carport with auto roller door Secure garden ideal for children and pets
+- Brand new Oven and Bosch dishwasher
+- Freshly painted all throughout
+- New flooring through in bedrooms
+- Picturesque location next to pond
+- Located in popular Wells Station division Small boutique complex of 12 townhouses
+- Free-standing sharing no common walls Close to walking tracks and cycle paths Bus stop located immediately outside the complex Fifteen minute drive to city five minute walk to light rail stop
+Located right across from proposed KENNY school and moments from the expanding Gungahlin Market Place, Flemington Rd Retail Precinct and light rail, this opportunity will surely not last long. Call Alvin on 0426146118 to register your interest.
+Pre Auction offers are accepted.
+Living Area: Residence - 106m2
+Carport - 37m2
+Construction: 2014
+EER: 5 Stars
+Body Corp: $ 1870 pa (approx.)
+Rental :$700- $720 per week approx ( figure based on current rental in the complex)</t>
+  </si>
+  <si>
+    <t>215</t>
+  </si>
+  <si>
+    <t>9/21 Samaria Street, Crace ACT 2911</t>
+  </si>
+  <si>
+    <t>The Opportunity: Beautiful family home with courtyards and plenty of living space. Crace shops, medical centre and plenty of parks are close by.
+The Dream: A modern home with an abundance of natural light. A large kitchen, welcoming living and dining rooms, a guest powder room, and a laundry room are all located on the ground floor. There are three lovely bedrooms, a sitting area and a family bathroom waiting for you upstairs.
+This stunning three-bedroom family retreat features a contemporary design and is perfectly situated. It features flowing living spaces, light-filled interiors, and many subtle modern details. This excellent house is complimented by the idyllic outside features, making it an ideal home for the entertainer. It is strategically located to provide quick access to local transportation and urban amenities. This fantastic family home is strongly recommended for inspection. Located in one of the area's most prestigious enclaves , this home is superbly elevated, this property is close to everything you need. Cafe's, restaurants, shops and schools including primary school, high school, private school and early childcare are all within close walking proximity. A bus stop is virtually at your doorstep and next with light rail station, will run right past within a few meters of this home.
+If you interested in that townhouse, feel free to call us on 0497 565 143 Or email us serene@trustedrealtors.com.au</t>
+  </si>
+  <si>
     <t>Draft</t>
   </si>
   <si>
-    <t>https://www.777homes.com.au/?post_type=property&amp;p=9982&amp;preview=true</t>
-  </si>
-  <si>
-    <t>https://www.777homes.com.au/?post_type=property&amp;p=9986&amp;preview=true</t>
-  </si>
-  <si>
-    <t>https://www.777homes.com.au/?post_type=property&amp;p=9988&amp;preview=true</t>
-  </si>
-  <si>
-    <t>https://www.777homes.com.au/?post_type=property&amp;p=9990&amp;preview=true</t>
+    <t>https://www.777homes.com.au/?post_type=property&amp;p=10084&amp;preview=true</t>
+  </si>
+  <si>
+    <t>https://www.777homes.com.au/?post_type=property&amp;p=10086&amp;preview=true</t>
+  </si>
+  <si>
+    <t>https://www.777homes.com.au/?post_type=property&amp;p=10088&amp;preview=true</t>
+  </si>
+  <si>
+    <t>https://www.777homes.com.au/?post_type=property&amp;p=10090&amp;preview=true</t>
+  </si>
+  <si>
+    <t>https://www.777homes.com.au/?post_type=property&amp;p=10092&amp;preview=true</t>
+  </si>
+  <si>
+    <t>https://www.777homes.com.au/?post_type=property&amp;p=10094&amp;preview=true</t>
+  </si>
+  <si>
+    <t>https://www.777homes.com.au/?post_type=property&amp;p=10096&amp;preview=true</t>
+  </si>
+  <si>
+    <t>https://www.777homes.com.au/?post_type=property&amp;p=10098&amp;preview=true</t>
+  </si>
+  <si>
+    <t>https://www.777homes.com.au/?post_type=property&amp;p=10100&amp;preview=true</t>
+  </si>
+  <si>
+    <t>https://www.777homes.com.au/?post_type=property&amp;p=10102&amp;preview=true</t>
   </si>
 </sst>
 </file>
@@ -8141,11 +8610,11 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:AC205"/>
+  <dimension ref="A1:AC216"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane activePane="bottomLeft" state="frozen" topLeftCell="A176" ySplit="1"/>
-      <selection activeCell="F205" pane="bottomLeft" sqref="F205"/>
+      <pane activePane="bottomLeft" state="frozen" topLeftCell="A179" ySplit="1"/>
+      <selection activeCell="D209" pane="bottomLeft" sqref="D209"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr customHeight="1" defaultColWidth="14.42578125" defaultRowHeight="15.75"/>
@@ -12514,7 +12983,7 @@
       <c r="C165" s="41" t="s">
         <v>1204</v>
       </c>
-      <c r="D165" s="4" t="s">
+      <c r="D165" s="39" t="s">
         <v>14</v>
       </c>
       <c r="F165" s="2" t="s">
@@ -12584,7 +13053,7 @@
         <v>1218</v>
       </c>
       <c r="D168" s="4" t="s">
-        <v>7</v>
+        <v>14</v>
       </c>
       <c r="F168" s="2" t="s">
         <v>687</v>
@@ -12698,8 +13167,8 @@
       <c r="C173" s="41" t="s">
         <v>1260</v>
       </c>
-      <c r="D173" s="4" t="s">
-        <v>7</v>
+      <c r="D173" s="39" t="s">
+        <v>14</v>
       </c>
       <c r="F173" s="2" t="s">
         <v>687</v>
@@ -12925,8 +13394,8 @@
       <c r="C183" s="41" t="s">
         <v>1327</v>
       </c>
-      <c r="D183" s="4" t="s">
-        <v>7</v>
+      <c r="D183" s="39" t="s">
+        <v>14</v>
       </c>
       <c r="F183" s="2" t="s">
         <v>1046</v>
@@ -12948,8 +13417,8 @@
       <c r="C184" s="41" t="s">
         <v>1328</v>
       </c>
-      <c r="D184" s="4" t="s">
-        <v>7</v>
+      <c r="D184" s="39" t="s">
+        <v>14</v>
       </c>
       <c r="F184" s="2" t="s">
         <v>1046</v>
@@ -12971,8 +13440,8 @@
       <c r="C185" s="41" t="s">
         <v>1362</v>
       </c>
-      <c r="D185" s="4" t="s">
-        <v>7</v>
+      <c r="D185" s="39" t="s">
+        <v>14</v>
       </c>
       <c r="F185" s="2" t="s">
         <v>1046</v>
@@ -13008,14 +13477,14 @@
       <c r="A187">
         <v>186</v>
       </c>
-      <c r="B187" t="s">
+      <c r="B187" s="41" t="s">
         <v>1331</v>
       </c>
       <c r="C187" s="41" t="s">
         <v>1363</v>
       </c>
-      <c r="D187" s="4" t="s">
-        <v>7</v>
+      <c r="D187" s="39" t="s">
+        <v>14</v>
       </c>
       <c r="F187" s="2" t="s">
         <v>687</v>
@@ -13031,7 +13500,7 @@
       <c r="A188">
         <v>187</v>
       </c>
-      <c r="B188" t="s">
+      <c r="B188" s="41" t="s">
         <v>1332</v>
       </c>
       <c r="C188" s="41" t="s">
@@ -13054,13 +13523,13 @@
       <c r="A189">
         <v>188</v>
       </c>
-      <c r="B189" t="s">
+      <c r="B189" s="41" t="s">
         <v>1333</v>
       </c>
       <c r="C189" s="41" t="s">
         <v>1365</v>
       </c>
-      <c r="D189" s="4" t="s">
+      <c r="D189" s="39" t="s">
         <v>14</v>
       </c>
       <c r="F189" s="2" t="s">
@@ -13175,8 +13644,8 @@
       <c r="C194" s="41" t="s">
         <v>1407</v>
       </c>
-      <c r="D194" s="4" t="s">
-        <v>7</v>
+      <c r="D194" s="39" t="s">
+        <v>14</v>
       </c>
       <c r="F194" s="2" t="s">
         <v>687</v>
@@ -13261,13 +13730,13 @@
       <c r="A198">
         <v>197</v>
       </c>
-      <c r="B198" t="s">
+      <c r="B198" s="41" t="s">
         <v>1414</v>
       </c>
       <c r="C198" s="41" t="s">
         <v>1436</v>
       </c>
-      <c r="D198" s="4" t="s">
+      <c r="D198" s="39" t="s">
         <v>14</v>
       </c>
       <c r="F198" s="2" t="s">
@@ -13284,7 +13753,7 @@
       <c r="A199">
         <v>198</v>
       </c>
-      <c r="B199" t="s">
+      <c r="B199" s="41" t="s">
         <v>1415</v>
       </c>
       <c r="C199" s="41" t="s">
@@ -13350,14 +13819,14 @@
       <c r="A202">
         <v>201</v>
       </c>
-      <c r="B202" t="s">
+      <c r="B202" s="41" t="s">
         <v>1439</v>
       </c>
-      <c r="C202" t="s">
-        <v>1463</v>
-      </c>
-      <c r="D202" s="46" t="s">
+      <c r="C202" s="41" t="s">
         <v>1462</v>
+      </c>
+      <c r="D202" s="4" t="s">
+        <v>7</v>
       </c>
       <c r="F202" s="2" t="s">
         <v>1046</v>
@@ -13373,14 +13842,14 @@
       <c r="A203">
         <v>202</v>
       </c>
-      <c r="B203" t="s">
+      <c r="B203" s="41" t="s">
         <v>1440</v>
       </c>
-      <c r="C203" t="s">
-        <v>1466</v>
-      </c>
-      <c r="D203" s="46" t="s">
-        <v>1462</v>
+      <c r="C203" s="41" t="s">
+        <v>1465</v>
+      </c>
+      <c r="D203" s="4" t="s">
+        <v>7</v>
       </c>
       <c r="F203" s="2" t="s">
         <v>1046</v>
@@ -13396,14 +13865,14 @@
       <c r="A204">
         <v>203</v>
       </c>
-      <c r="B204" t="s">
+      <c r="B204" s="41" t="s">
         <v>1441</v>
       </c>
-      <c r="C204" t="s">
-        <v>1464</v>
-      </c>
-      <c r="D204" s="47" t="s">
-        <v>1462</v>
+      <c r="C204" s="41" t="s">
+        <v>1463</v>
+      </c>
+      <c r="D204" s="4" t="s">
+        <v>7</v>
       </c>
       <c r="F204" s="2" t="s">
         <v>1046</v>
@@ -13419,14 +13888,14 @@
       <c r="A205">
         <v>204</v>
       </c>
-      <c r="B205" t="s">
+      <c r="B205" s="41" t="s">
         <v>1442</v>
       </c>
-      <c r="C205" t="s">
-        <v>1465</v>
-      </c>
-      <c r="D205" s="48" t="s">
-        <v>1462</v>
+      <c r="C205" s="41" t="s">
+        <v>1464</v>
+      </c>
+      <c r="D205" s="39" t="s">
+        <v>14</v>
       </c>
       <c r="F205" s="2" t="s">
         <v>687</v>
@@ -13436,6 +13905,256 @@
       </c>
       <c r="H205" t="s">
         <v>881</v>
+      </c>
+    </row>
+    <row ht="12.75" r="206" spans="1:8">
+      <c r="A206">
+        <v>205</v>
+      </c>
+      <c r="B206" t="s">
+        <v>1467</v>
+      </c>
+      <c r="C206" t="s">
+        <v>1526</v>
+      </c>
+      <c r="D206" s="46" t="s">
+        <v>1525</v>
+      </c>
+      <c r="F206" s="2" t="s">
+        <v>1046</v>
+      </c>
+      <c r="G206" t="s">
+        <v>8</v>
+      </c>
+      <c r="H206" t="s">
+        <v>427</v>
+      </c>
+    </row>
+    <row ht="12.75" r="207" spans="1:8">
+      <c r="A207">
+        <v>206</v>
+      </c>
+      <c r="B207" t="s">
+        <v>1468</v>
+      </c>
+      <c r="C207" t="s">
+        <v>1527</v>
+      </c>
+      <c r="D207" s="46" t="s">
+        <v>1525</v>
+      </c>
+      <c r="F207" s="2" t="s">
+        <v>1046</v>
+      </c>
+      <c r="G207" t="s">
+        <v>8</v>
+      </c>
+      <c r="H207" t="s">
+        <v>427</v>
+      </c>
+    </row>
+    <row ht="12.75" r="208" spans="1:8">
+      <c r="A208">
+        <v>207</v>
+      </c>
+      <c r="B208" t="s">
+        <v>1469</v>
+      </c>
+      <c r="C208" t="s">
+        <v>1528</v>
+      </c>
+      <c r="D208" s="46" t="s">
+        <v>1525</v>
+      </c>
+      <c r="F208" s="2" t="s">
+        <v>1046</v>
+      </c>
+      <c r="G208" t="s">
+        <v>8</v>
+      </c>
+      <c r="H208" t="s">
+        <v>427</v>
+      </c>
+    </row>
+    <row ht="12.75" r="209" spans="1:8">
+      <c r="A209">
+        <v>208</v>
+      </c>
+      <c r="B209" s="41" t="s">
+        <v>1470</v>
+      </c>
+      <c r="D209" s="39" t="s">
+        <v>14</v>
+      </c>
+      <c r="F209" s="2" t="s">
+        <v>1046</v>
+      </c>
+      <c r="G209" t="s">
+        <v>37</v>
+      </c>
+      <c r="H209" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row ht="12.75" r="210" spans="1:8">
+      <c r="A210">
+        <v>209</v>
+      </c>
+      <c r="B210" t="s">
+        <v>1471</v>
+      </c>
+      <c r="C210" t="s">
+        <v>1529</v>
+      </c>
+      <c r="D210" s="47" t="s">
+        <v>1525</v>
+      </c>
+      <c r="F210" s="2" t="s">
+        <v>687</v>
+      </c>
+      <c r="G210" t="s">
+        <v>1044</v>
+      </c>
+      <c r="H210" t="s">
+        <v>881</v>
+      </c>
+    </row>
+    <row ht="12.75" r="211" spans="1:8">
+      <c r="A211">
+        <v>210</v>
+      </c>
+      <c r="B211" t="s">
+        <v>1472</v>
+      </c>
+      <c r="C211" t="s">
+        <v>1530</v>
+      </c>
+      <c r="D211" s="47" t="s">
+        <v>1525</v>
+      </c>
+      <c r="F211" s="2" t="s">
+        <v>687</v>
+      </c>
+      <c r="G211" t="s">
+        <v>1044</v>
+      </c>
+      <c r="H211" t="s">
+        <v>881</v>
+      </c>
+    </row>
+    <row ht="12.75" r="212" spans="1:8">
+      <c r="A212">
+        <v>211</v>
+      </c>
+      <c r="B212" t="s">
+        <v>1473</v>
+      </c>
+      <c r="C212" t="s">
+        <v>1531</v>
+      </c>
+      <c r="D212" s="47" t="s">
+        <v>1525</v>
+      </c>
+      <c r="F212" s="2" t="s">
+        <v>687</v>
+      </c>
+      <c r="G212" t="s">
+        <v>1044</v>
+      </c>
+      <c r="H212" t="s">
+        <v>881</v>
+      </c>
+    </row>
+    <row ht="12.75" r="213" spans="1:8">
+      <c r="A213">
+        <v>212</v>
+      </c>
+      <c r="B213" t="s">
+        <v>1474</v>
+      </c>
+      <c r="C213" t="s">
+        <v>1532</v>
+      </c>
+      <c r="D213" s="47" t="s">
+        <v>1525</v>
+      </c>
+      <c r="F213" s="2" t="s">
+        <v>687</v>
+      </c>
+      <c r="G213" t="s">
+        <v>1044</v>
+      </c>
+      <c r="H213" t="s">
+        <v>881</v>
+      </c>
+    </row>
+    <row ht="12.75" r="214" spans="1:8">
+      <c r="A214">
+        <v>213</v>
+      </c>
+      <c r="B214" t="s">
+        <v>1475</v>
+      </c>
+      <c r="C214" t="s">
+        <v>1533</v>
+      </c>
+      <c r="D214" s="47" t="s">
+        <v>1525</v>
+      </c>
+      <c r="F214" s="2" t="s">
+        <v>687</v>
+      </c>
+      <c r="G214" t="s">
+        <v>1044</v>
+      </c>
+      <c r="H214" t="s">
+        <v>881</v>
+      </c>
+    </row>
+    <row ht="12.75" r="215" spans="1:8">
+      <c r="A215">
+        <v>214</v>
+      </c>
+      <c r="B215" t="s">
+        <v>1476</v>
+      </c>
+      <c r="C215" t="s">
+        <v>1534</v>
+      </c>
+      <c r="D215" s="47" t="s">
+        <v>1525</v>
+      </c>
+      <c r="F215" s="2" t="s">
+        <v>687</v>
+      </c>
+      <c r="G215" t="s">
+        <v>1044</v>
+      </c>
+      <c r="H215" t="s">
+        <v>881</v>
+      </c>
+    </row>
+    <row ht="12.75" r="216" spans="1:8">
+      <c r="A216">
+        <v>215</v>
+      </c>
+      <c r="B216" t="s">
+        <v>1477</v>
+      </c>
+      <c r="C216" t="s">
+        <v>1535</v>
+      </c>
+      <c r="D216" s="48" t="s">
+        <v>1525</v>
+      </c>
+      <c r="F216" s="2" t="s">
+        <v>687</v>
+      </c>
+      <c r="G216" t="s">
+        <v>16</v>
+      </c>
+      <c r="H216" t="s">
+        <v>428</v>
       </c>
     </row>
   </sheetData>
@@ -13716,9 +14435,23 @@
     <hyperlink r:id="rId274" ref="C198" xr:uid="{0EA3339D-CA4A-40E2-87F1-099191AE17A8}"/>
     <hyperlink r:id="rId275" ref="C199" xr:uid="{921809EC-DBAA-4BD8-BE82-0CEB8589B8A1}"/>
     <hyperlink r:id="rId276" ref="C201" xr:uid="{AC7E40E8-606A-43A2-B8C7-610E934907B3}"/>
+    <hyperlink r:id="rId277" ref="C202" xr:uid="{36DDC773-0FEB-457C-9C86-8E44B688F740}"/>
+    <hyperlink r:id="rId278" ref="C203" xr:uid="{FF64A951-3FB0-4007-9C39-2CD3FC6F4721}"/>
+    <hyperlink r:id="rId279" ref="C204" xr:uid="{E23FA518-0E3E-460A-BED6-06C5A8A09C1C}"/>
+    <hyperlink r:id="rId280" ref="C205" xr:uid="{4464FB6F-A499-4FF1-8A14-460C25E3EBE4}"/>
+    <hyperlink r:id="rId281" ref="B198" xr:uid="{8927A608-5F76-4355-96D8-0BF00137DDD5}"/>
+    <hyperlink r:id="rId282" ref="B199" xr:uid="{CB026297-2699-4363-9BC8-B202EFD3179B}"/>
+    <hyperlink r:id="rId283" ref="B202" xr:uid="{A490C9C0-E2E1-4254-8DA6-94EB300FE35D}"/>
+    <hyperlink r:id="rId284" ref="B203" xr:uid="{FFE063F5-3591-40B6-818D-689BA2E21158}"/>
+    <hyperlink r:id="rId285" ref="B204" xr:uid="{17E4DBFE-7BCA-4C3D-B358-2F06813ADCE3}"/>
+    <hyperlink r:id="rId286" ref="B205" xr:uid="{0E3DC333-0BE5-4C61-946D-2A653D5D973C}"/>
+    <hyperlink r:id="rId287" ref="B187" xr:uid="{BF2BE11B-39D0-4E2C-A76A-FF9407D02E11}"/>
+    <hyperlink r:id="rId288" ref="B188" xr:uid="{CBC83D37-047F-4CB7-AF89-AC9490E31386}"/>
+    <hyperlink r:id="rId289" ref="B189" xr:uid="{E5A4143D-9638-4278-97AF-EA9059288D50}"/>
+    <hyperlink r:id="rId290" ref="B209" xr:uid="{B93D9203-052B-4411-80C3-312989FFDF7E}"/>
   </hyperlinks>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
-  <pageSetup orientation="portrait" paperSize="9" r:id="rId277"/>
+  <pageSetup orientation="portrait" paperSize="9" r:id="rId291"/>
 </worksheet>
 </file>
 
@@ -13727,11 +14460,11 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:AJ204"/>
+  <dimension ref="A1:AJ215"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
-      <pane activePane="bottomLeft" state="frozen" topLeftCell="A185" ySplit="1"/>
-      <selection activeCell="K213" pane="bottomLeft" sqref="K213"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane activePane="bottomLeft" state="frozen" topLeftCell="A179" ySplit="1"/>
+      <selection activeCell="E208" pane="bottomLeft" sqref="E208"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr customHeight="1" defaultColWidth="14.42578125" defaultRowHeight="15.75"/>
@@ -23477,8 +24210,8 @@
       <c r="A164" s="24" t="s">
         <v>1195</v>
       </c>
-      <c r="B164" s="24" t="s">
-        <v>7</v>
+      <c r="B164" s="43" t="s">
+        <v>172</v>
       </c>
       <c r="C164" s="24" t="s">
         <v>1196</v>
@@ -23486,8 +24219,8 @@
       <c r="D164" s="24" t="s">
         <v>77</v>
       </c>
-      <c r="E164" s="24" t="s">
-        <v>78</v>
+      <c r="E164" s="43" t="s">
+        <v>172</v>
       </c>
       <c r="F164" s="24" t="s">
         <v>79</v>
@@ -23949,8 +24682,8 @@
       <c r="A172" s="24" t="s">
         <v>1249</v>
       </c>
-      <c r="B172" s="24" t="s">
-        <v>7</v>
+      <c r="B172" s="43" t="s">
+        <v>172</v>
       </c>
       <c r="C172" s="24" t="s">
         <v>1250</v>
@@ -23958,8 +24691,8 @@
       <c r="D172" s="24" t="s">
         <v>84</v>
       </c>
-      <c r="E172" s="24" t="s">
-        <v>78</v>
+      <c r="E172" s="43" t="s">
+        <v>172</v>
       </c>
       <c r="F172" s="24" t="s">
         <v>79</v>
@@ -24136,7 +24869,7 @@
         <v>84</v>
       </c>
       <c r="E175" s="24" t="s">
-        <v>78</v>
+        <v>173</v>
       </c>
       <c r="F175" s="24" t="s">
         <v>79</v>
@@ -24539,8 +25272,8 @@
       <c r="A182" s="24" t="s">
         <v>1312</v>
       </c>
-      <c r="B182" s="24" t="s">
-        <v>7</v>
+      <c r="B182" s="43" t="s">
+        <v>172</v>
       </c>
       <c r="C182" s="24" t="s">
         <v>1313</v>
@@ -24548,8 +25281,8 @@
       <c r="D182" s="24" t="s">
         <v>84</v>
       </c>
-      <c r="E182" s="24" t="s">
-        <v>78</v>
+      <c r="E182" s="43" t="s">
+        <v>172</v>
       </c>
       <c r="F182" s="24" t="s">
         <v>79</v>
@@ -24598,8 +25331,8 @@
       <c r="A183" s="24" t="s">
         <v>1316</v>
       </c>
-      <c r="B183" s="24" t="s">
-        <v>7</v>
+      <c r="B183" s="43" t="s">
+        <v>386</v>
       </c>
       <c r="C183" s="24" t="s">
         <v>1317</v>
@@ -24607,8 +25340,8 @@
       <c r="D183" s="24" t="s">
         <v>261</v>
       </c>
-      <c r="E183" s="24" t="s">
-        <v>848</v>
+      <c r="E183" s="43" t="s">
+        <v>386</v>
       </c>
       <c r="F183" s="24" t="s">
         <v>407</v>
@@ -24657,8 +25390,8 @@
       <c r="A184" s="24" t="s">
         <v>1335</v>
       </c>
-      <c r="B184" s="24" t="s">
-        <v>7</v>
+      <c r="B184" s="43" t="s">
+        <v>172</v>
       </c>
       <c r="C184" s="24" t="s">
         <v>1336</v>
@@ -24666,8 +25399,8 @@
       <c r="D184" s="24" t="s">
         <v>84</v>
       </c>
-      <c r="E184" s="24" t="s">
-        <v>78</v>
+      <c r="E184" s="43" t="s">
+        <v>172</v>
       </c>
       <c r="F184" s="24" t="s">
         <v>79</v>
@@ -24775,8 +25508,8 @@
       <c r="A186" s="24" t="s">
         <v>1344</v>
       </c>
-      <c r="B186" s="24" t="s">
-        <v>7</v>
+      <c r="B186" s="43" t="s">
+        <v>172</v>
       </c>
       <c r="C186" s="24" t="s">
         <v>1345</v>
@@ -24784,8 +25517,8 @@
       <c r="D186" s="24" t="s">
         <v>84</v>
       </c>
-      <c r="E186" s="24" t="s">
-        <v>78</v>
+      <c r="E186" s="43" t="s">
+        <v>172</v>
       </c>
       <c r="F186" s="24" t="s">
         <v>79</v>
@@ -24844,7 +25577,7 @@
         <v>84</v>
       </c>
       <c r="E187" s="24" t="s">
-        <v>78</v>
+        <v>173</v>
       </c>
       <c r="F187" s="24" t="s">
         <v>235</v>
@@ -24893,8 +25626,8 @@
       <c r="A188" s="24" t="s">
         <v>1355</v>
       </c>
-      <c r="B188" s="24" t="s">
-        <v>7</v>
+      <c r="B188" s="43" t="s">
+        <v>172</v>
       </c>
       <c r="C188" s="24" t="s">
         <v>1356</v>
@@ -24902,8 +25635,8 @@
       <c r="D188" s="24" t="s">
         <v>84</v>
       </c>
-      <c r="E188" s="24" t="s">
-        <v>78</v>
+      <c r="E188" s="43" t="s">
+        <v>172</v>
       </c>
       <c r="F188" s="24" t="s">
         <v>235</v>
@@ -24976,11 +25709,11 @@
       <c r="I189" s="24" t="s">
         <v>198</v>
       </c>
-      <c r="K189" s="24" t="s">
-        <v>199</v>
+      <c r="K189" s="24">
+        <v>899000</v>
       </c>
       <c r="L189" s="24" t="s">
-        <v>1290</v>
+        <v>1466</v>
       </c>
       <c r="M189" s="24" t="s">
         <v>199</v>
@@ -25080,7 +25813,7 @@
         <v>77</v>
       </c>
       <c r="E191" s="24" t="s">
-        <v>78</v>
+        <v>173</v>
       </c>
       <c r="F191" s="24" t="s">
         <v>79</v>
@@ -25188,8 +25921,8 @@
       <c r="A193" s="24" t="s">
         <v>1388</v>
       </c>
-      <c r="B193" s="24" t="s">
-        <v>7</v>
+      <c r="B193" s="43" t="s">
+        <v>172</v>
       </c>
       <c r="C193" s="24" t="s">
         <v>1389</v>
@@ -25197,8 +25930,8 @@
       <c r="D193" s="24" t="s">
         <v>261</v>
       </c>
-      <c r="E193" s="24" t="s">
-        <v>78</v>
+      <c r="E193" s="43" t="s">
+        <v>172</v>
       </c>
       <c r="F193" s="24" t="s">
         <v>79</v>
@@ -25257,7 +25990,7 @@
         <v>77</v>
       </c>
       <c r="E194" s="24" t="s">
-        <v>78</v>
+        <v>173</v>
       </c>
       <c r="F194" s="24" t="s">
         <v>684</v>
@@ -25375,7 +26108,7 @@
         <v>84</v>
       </c>
       <c r="E196" s="24" t="s">
-        <v>78</v>
+        <v>173</v>
       </c>
       <c r="F196" s="24" t="s">
         <v>235</v>
@@ -25424,8 +26157,8 @@
       <c r="A197" s="24" t="s">
         <v>1418</v>
       </c>
-      <c r="B197" s="24" t="s">
-        <v>7</v>
+      <c r="B197" s="43" t="s">
+        <v>172</v>
       </c>
       <c r="C197" s="24" t="s">
         <v>1419</v>
@@ -25433,8 +26166,8 @@
       <c r="D197" s="24" t="s">
         <v>234</v>
       </c>
-      <c r="E197" s="24" t="s">
-        <v>78</v>
+      <c r="E197" s="43" t="s">
+        <v>172</v>
       </c>
       <c r="F197" s="24" t="s">
         <v>79</v>
@@ -25493,7 +26226,7 @@
         <v>261</v>
       </c>
       <c r="E198" s="24" t="s">
-        <v>78</v>
+        <v>173</v>
       </c>
       <c r="F198" s="24" t="s">
         <v>79</v>
@@ -25551,7 +26284,7 @@
       <c r="D199" t="s">
         <v>84</v>
       </c>
-      <c r="E199" t="s">
+      <c r="E199" s="43" t="s">
         <v>172</v>
       </c>
       <c r="F199" t="s">
@@ -25656,240 +26389,889 @@
         <v>16</v>
       </c>
     </row>
-    <row ht="12.75" r="201" spans="1:21">
-      <c r="A201" t="s">
+    <row customFormat="1" ht="14.25" r="201" s="24" spans="1:21">
+      <c r="A201" s="24" t="s">
         <v>1443</v>
       </c>
-      <c r="B201" t="s">
-        <v>1462</v>
-      </c>
-      <c r="C201" t="s">
+      <c r="B201" s="24" t="s">
+        <v>7</v>
+      </c>
+      <c r="C201" s="24" t="s">
         <v>1444</v>
       </c>
-      <c r="D201" t="s">
+      <c r="D201" s="24" t="s">
         <v>84</v>
       </c>
-      <c r="E201" t="s">
+      <c r="E201" s="24" t="s">
         <v>78</v>
       </c>
-      <c r="F201" t="s">
+      <c r="F201" s="24" t="s">
         <v>79</v>
       </c>
-      <c r="G201" t="s">
+      <c r="G201" s="24" t="s">
         <v>85</v>
       </c>
-      <c r="H201" t="s">
+      <c r="H201" s="24" t="s">
         <v>1445</v>
       </c>
-      <c r="I201" t="s">
+      <c r="I201" s="24" t="s">
         <v>198</v>
       </c>
-      <c r="K201" t="s">
+      <c r="K201" s="24" t="s">
         <v>199</v>
       </c>
-      <c r="L201" t="s">
+      <c r="L201" s="24" t="s">
         <v>1446</v>
       </c>
-      <c r="M201" t="s">
+      <c r="M201" s="24" t="s">
         <v>201</v>
       </c>
-      <c r="N201" t="s">
+      <c r="N201" s="24" t="s">
         <v>202</v>
       </c>
-      <c r="P201" t="s">
+      <c r="P201" s="24" t="s">
         <v>203</v>
       </c>
-      <c r="Q201" t="s">
+      <c r="Q201" s="24" t="s">
         <v>204</v>
       </c>
-      <c r="R201" t="s">
+      <c r="R201" s="24" t="s">
         <v>1444</v>
       </c>
-      <c r="S201" t="s">
+      <c r="S201" s="24" t="s">
         <v>1447</v>
       </c>
-      <c r="T201" t="s">
+      <c r="T201" s="24" t="s">
         <v>1046</v>
       </c>
-      <c r="U201" t="s">
+      <c r="U201" s="24" t="s">
         <v>8</v>
       </c>
     </row>
-    <row ht="12.75" r="202" spans="1:21">
-      <c r="A202" t="s">
+    <row customFormat="1" ht="14.25" r="202" s="24" spans="1:21">
+      <c r="A202" s="24" t="s">
         <v>1448</v>
       </c>
-      <c r="B202" t="s">
-        <v>1462</v>
-      </c>
-      <c r="C202" t="s">
+      <c r="B202" s="24" t="s">
+        <v>7</v>
+      </c>
+      <c r="C202" s="24" t="s">
         <v>1449</v>
       </c>
-      <c r="D202" t="s">
+      <c r="D202" s="24" t="s">
         <v>84</v>
       </c>
-      <c r="E202" t="s">
+      <c r="E202" s="24" t="s">
         <v>78</v>
       </c>
-      <c r="F202" t="s">
+      <c r="F202" s="24" t="s">
         <v>407</v>
       </c>
-      <c r="G202" t="s">
+      <c r="G202" s="24" t="s">
         <v>1450</v>
       </c>
-      <c r="H202" t="s">
+      <c r="H202" s="24" t="s">
         <v>1451</v>
       </c>
-      <c r="I202" t="s">
+      <c r="I202" s="24" t="s">
         <v>198</v>
       </c>
-      <c r="K202" t="s">
+      <c r="K202" s="24" t="s">
         <v>199</v>
       </c>
-      <c r="L202" t="s">
+      <c r="L202" s="24" t="s">
         <v>1452</v>
       </c>
-      <c r="M202" t="s">
+      <c r="M202" s="24" t="s">
         <v>202</v>
       </c>
-      <c r="N202" t="s">
+      <c r="N202" s="24" t="s">
         <v>266</v>
       </c>
-      <c r="P202" t="s">
+      <c r="P202" s="24" t="s">
         <v>199</v>
       </c>
-      <c r="Q202" t="s">
+      <c r="Q202" s="24" t="s">
         <v>266</v>
       </c>
-      <c r="R202" t="s">
+      <c r="R202" s="24" t="s">
         <v>1449</v>
       </c>
-      <c r="S202" t="s">
+      <c r="S202" s="24" t="s">
         <v>1453</v>
       </c>
-      <c r="T202" t="s">
+      <c r="T202" s="24" t="s">
         <v>1046</v>
       </c>
-      <c r="U202" t="s">
+      <c r="U202" s="24" t="s">
         <v>8</v>
       </c>
     </row>
-    <row ht="12.75" r="203" spans="1:21">
-      <c r="A203" t="s">
+    <row customFormat="1" ht="14.25" r="203" s="24" spans="1:21">
+      <c r="A203" s="24" t="s">
         <v>1454</v>
       </c>
-      <c r="B203" t="s">
-        <v>1462</v>
-      </c>
-      <c r="C203" t="s">
+      <c r="B203" s="24" t="s">
+        <v>7</v>
+      </c>
+      <c r="C203" s="24" t="s">
         <v>1455</v>
       </c>
-      <c r="D203" t="s">
+      <c r="D203" s="24" t="s">
         <v>77</v>
       </c>
-      <c r="E203" t="s">
+      <c r="E203" s="24" t="s">
         <v>78</v>
       </c>
-      <c r="F203" t="s">
+      <c r="F203" s="24" t="s">
         <v>79</v>
       </c>
-      <c r="G203" t="s">
+      <c r="G203" s="24" t="s">
         <v>79</v>
       </c>
-      <c r="H203" t="s">
+      <c r="H203" s="24" t="s">
         <v>771</v>
       </c>
-      <c r="I203" t="s">
+      <c r="I203" s="24" t="s">
         <v>198</v>
       </c>
-      <c r="K203">
+      <c r="K203" s="24">
         <v>520000</v>
       </c>
-      <c r="L203" t="s">
+      <c r="L203" s="24" t="s">
         <v>1456</v>
       </c>
-      <c r="M203" t="s">
+      <c r="M203" s="24" t="s">
         <v>204</v>
       </c>
-      <c r="N203" t="s">
+      <c r="N203" s="24" t="s">
         <v>204</v>
       </c>
-      <c r="P203" t="s">
+      <c r="P203" s="24" t="s">
         <v>203</v>
       </c>
-      <c r="Q203" t="s">
+      <c r="Q203" s="24" t="s">
         <v>204</v>
       </c>
-      <c r="R203" t="s">
+      <c r="R203" s="24" t="s">
         <v>1455</v>
       </c>
-      <c r="S203" t="s">
+      <c r="S203" s="24" t="s">
         <v>1457</v>
       </c>
-      <c r="T203" t="s">
+      <c r="T203" s="24" t="s">
         <v>1046</v>
       </c>
-      <c r="U203" t="s">
+      <c r="U203" s="24" t="s">
         <v>37</v>
       </c>
     </row>
-    <row ht="12.75" r="204" spans="1:21">
-      <c r="A204" t="s">
+    <row customFormat="1" ht="14.25" r="204" s="24" spans="1:21">
+      <c r="A204" s="24" t="s">
         <v>1458</v>
       </c>
-      <c r="B204" t="s">
-        <v>1462</v>
-      </c>
-      <c r="C204" t="s">
+      <c r="B204" s="43" t="s">
+        <v>172</v>
+      </c>
+      <c r="C204" s="24" t="s">
         <v>1459</v>
       </c>
-      <c r="D204" t="s">
+      <c r="D204" s="24" t="s">
         <v>84</v>
       </c>
-      <c r="E204" t="s">
+      <c r="E204" s="43" t="s">
+        <v>172</v>
+      </c>
+      <c r="F204" s="24" t="s">
+        <v>235</v>
+      </c>
+      <c r="G204" s="24" t="s">
+        <v>248</v>
+      </c>
+      <c r="H204" s="24" t="s">
+        <v>1460</v>
+      </c>
+      <c r="I204" s="24" t="s">
+        <v>198</v>
+      </c>
+      <c r="K204" s="24" t="s">
+        <v>199</v>
+      </c>
+      <c r="L204" s="24" t="s">
+        <v>1421</v>
+      </c>
+      <c r="M204" s="24" t="s">
+        <v>252</v>
+      </c>
+      <c r="N204" s="24" t="s">
+        <v>202</v>
+      </c>
+      <c r="P204" s="24" t="s">
+        <v>201</v>
+      </c>
+      <c r="Q204" s="24" t="s">
+        <v>204</v>
+      </c>
+      <c r="R204" s="24" t="s">
+        <v>1459</v>
+      </c>
+      <c r="S204" s="24" t="s">
+        <v>1461</v>
+      </c>
+      <c r="T204" s="24" t="s">
+        <v>687</v>
+      </c>
+      <c r="U204" s="24" t="s">
+        <v>1044</v>
+      </c>
+    </row>
+    <row ht="12.75" r="205" spans="1:21">
+      <c r="A205" t="s">
+        <v>1478</v>
+      </c>
+      <c r="B205" t="s">
+        <v>1525</v>
+      </c>
+      <c r="C205" t="s">
+        <v>1479</v>
+      </c>
+      <c r="D205" t="s">
+        <v>84</v>
+      </c>
+      <c r="E205" t="s">
         <v>78</v>
       </c>
-      <c r="F204" t="s">
+      <c r="F205" t="s">
+        <v>79</v>
+      </c>
+      <c r="G205" t="s">
+        <v>221</v>
+      </c>
+      <c r="H205" t="s">
+        <v>1480</v>
+      </c>
+      <c r="I205" t="s">
+        <v>198</v>
+      </c>
+      <c r="K205" t="s">
+        <v>199</v>
+      </c>
+      <c r="L205" t="s">
+        <v>237</v>
+      </c>
+      <c r="M205" t="s">
+        <v>202</v>
+      </c>
+      <c r="N205" t="s">
+        <v>204</v>
+      </c>
+      <c r="P205" t="s">
+        <v>203</v>
+      </c>
+      <c r="Q205" t="s">
+        <v>204</v>
+      </c>
+      <c r="R205" t="s">
+        <v>1479</v>
+      </c>
+      <c r="S205" t="s">
+        <v>1481</v>
+      </c>
+      <c r="T205" t="s">
+        <v>1046</v>
+      </c>
+      <c r="U205" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row ht="12.75" r="206" spans="1:21">
+      <c r="A206" t="s">
+        <v>1482</v>
+      </c>
+      <c r="B206" t="s">
+        <v>1525</v>
+      </c>
+      <c r="C206" t="s">
+        <v>1483</v>
+      </c>
+      <c r="D206" t="s">
+        <v>84</v>
+      </c>
+      <c r="E206" t="s">
+        <v>78</v>
+      </c>
+      <c r="F206" t="s">
+        <v>79</v>
+      </c>
+      <c r="G206" t="s">
+        <v>120</v>
+      </c>
+      <c r="H206" t="s">
+        <v>1484</v>
+      </c>
+      <c r="I206" t="s">
+        <v>198</v>
+      </c>
+      <c r="K206" t="s">
+        <v>1485</v>
+      </c>
+      <c r="L206" t="s">
+        <v>1486</v>
+      </c>
+      <c r="M206" t="s">
+        <v>201</v>
+      </c>
+      <c r="N206" t="s">
+        <v>202</v>
+      </c>
+      <c r="P206" t="s">
+        <v>203</v>
+      </c>
+      <c r="Q206" t="s">
+        <v>204</v>
+      </c>
+      <c r="R206" t="s">
+        <v>1483</v>
+      </c>
+      <c r="S206" t="s">
+        <v>1487</v>
+      </c>
+      <c r="T206" t="s">
+        <v>1046</v>
+      </c>
+      <c r="U206" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row ht="12.75" r="207" spans="1:21">
+      <c r="A207" t="s">
+        <v>1488</v>
+      </c>
+      <c r="B207" t="s">
+        <v>1525</v>
+      </c>
+      <c r="C207" t="s">
+        <v>1489</v>
+      </c>
+      <c r="D207" t="s">
+        <v>84</v>
+      </c>
+      <c r="E207" t="s">
+        <v>78</v>
+      </c>
+      <c r="F207" t="s">
+        <v>79</v>
+      </c>
+      <c r="G207" t="s">
+        <v>138</v>
+      </c>
+      <c r="H207" t="s">
+        <v>1490</v>
+      </c>
+      <c r="I207" t="s">
+        <v>198</v>
+      </c>
+      <c r="K207" t="s">
+        <v>199</v>
+      </c>
+      <c r="L207" t="s">
+        <v>1491</v>
+      </c>
+      <c r="M207" t="s">
+        <v>202</v>
+      </c>
+      <c r="N207" t="s">
+        <v>204</v>
+      </c>
+      <c r="P207" t="s">
+        <v>203</v>
+      </c>
+      <c r="Q207" t="s">
+        <v>204</v>
+      </c>
+      <c r="R207" t="s">
+        <v>1489</v>
+      </c>
+      <c r="S207" t="s">
+        <v>1492</v>
+      </c>
+      <c r="T207" t="s">
+        <v>1046</v>
+      </c>
+      <c r="U207" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row ht="14.25" r="208" spans="1:21">
+      <c r="A208" t="s">
+        <v>1493</v>
+      </c>
+      <c r="B208" s="43" t="s">
+        <v>172</v>
+      </c>
+      <c r="C208" t="s">
+        <v>1494</v>
+      </c>
+      <c r="D208" t="s">
+        <v>84</v>
+      </c>
+      <c r="E208" s="43" t="s">
+        <v>172</v>
+      </c>
+      <c r="F208" t="s">
         <v>235</v>
       </c>
-      <c r="G204" t="s">
+      <c r="G208" t="s">
+        <v>236</v>
+      </c>
+      <c r="H208" t="s">
+        <v>1495</v>
+      </c>
+      <c r="I208" t="s">
+        <v>198</v>
+      </c>
+      <c r="K208" t="s">
+        <v>778</v>
+      </c>
+      <c r="L208" t="s">
+        <v>1496</v>
+      </c>
+      <c r="M208" t="s">
+        <v>203</v>
+      </c>
+      <c r="N208" t="s">
+        <v>201</v>
+      </c>
+      <c r="P208" t="s">
+        <v>203</v>
+      </c>
+      <c r="Q208" t="s">
+        <v>204</v>
+      </c>
+      <c r="R208" t="s">
+        <v>1494</v>
+      </c>
+      <c r="S208" t="s">
+        <v>1497</v>
+      </c>
+      <c r="T208" t="s">
+        <v>1046</v>
+      </c>
+      <c r="U208" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row ht="12.75" r="209" spans="1:21">
+      <c r="A209" t="s">
+        <v>1498</v>
+      </c>
+      <c r="B209" t="s">
+        <v>1525</v>
+      </c>
+      <c r="C209" t="s">
+        <v>1499</v>
+      </c>
+      <c r="D209" t="s">
+        <v>84</v>
+      </c>
+      <c r="E209" t="s">
+        <v>78</v>
+      </c>
+      <c r="F209" t="s">
+        <v>79</v>
+      </c>
+      <c r="G209" t="s">
+        <v>85</v>
+      </c>
+      <c r="H209" t="s">
+        <v>1500</v>
+      </c>
+      <c r="I209" t="s">
+        <v>198</v>
+      </c>
+      <c r="K209" t="s">
+        <v>1501</v>
+      </c>
+      <c r="L209" t="s">
+        <v>1502</v>
+      </c>
+      <c r="M209" t="s">
+        <v>201</v>
+      </c>
+      <c r="N209" t="s">
+        <v>204</v>
+      </c>
+      <c r="P209" t="s">
+        <v>203</v>
+      </c>
+      <c r="Q209" t="s">
+        <v>204</v>
+      </c>
+      <c r="R209" t="s">
+        <v>1499</v>
+      </c>
+      <c r="S209" t="s">
+        <v>1503</v>
+      </c>
+      <c r="T209" t="s">
+        <v>687</v>
+      </c>
+      <c r="U209" t="s">
+        <v>1044</v>
+      </c>
+    </row>
+    <row ht="12.75" r="210" spans="1:21">
+      <c r="A210" t="s">
+        <v>1504</v>
+      </c>
+      <c r="B210" t="s">
+        <v>1525</v>
+      </c>
+      <c r="C210" t="s">
+        <v>1505</v>
+      </c>
+      <c r="D210" t="s">
+        <v>261</v>
+      </c>
+      <c r="E210" t="s">
+        <v>78</v>
+      </c>
+      <c r="F210" t="s">
+        <v>207</v>
+      </c>
+      <c r="G210" t="s">
+        <v>379</v>
+      </c>
+      <c r="H210" t="s">
+        <v>199</v>
+      </c>
+      <c r="I210" t="s">
+        <v>198</v>
+      </c>
+      <c r="K210" t="s">
+        <v>199</v>
+      </c>
+      <c r="L210" t="s">
+        <v>237</v>
+      </c>
+      <c r="M210" t="s">
+        <v>202</v>
+      </c>
+      <c r="N210" t="s">
+        <v>204</v>
+      </c>
+      <c r="P210" t="s">
+        <v>202</v>
+      </c>
+      <c r="Q210" t="s">
+        <v>204</v>
+      </c>
+      <c r="R210" t="s">
+        <v>1505</v>
+      </c>
+      <c r="S210" t="s">
+        <v>1506</v>
+      </c>
+      <c r="T210" t="s">
+        <v>687</v>
+      </c>
+      <c r="U210" t="s">
+        <v>1044</v>
+      </c>
+    </row>
+    <row ht="12.75" r="211" spans="1:21">
+      <c r="A211" t="s">
+        <v>1507</v>
+      </c>
+      <c r="B211" t="s">
+        <v>1525</v>
+      </c>
+      <c r="C211" t="s">
+        <v>1508</v>
+      </c>
+      <c r="D211" t="s">
+        <v>84</v>
+      </c>
+      <c r="E211" t="s">
+        <v>78</v>
+      </c>
+      <c r="F211" t="s">
+        <v>684</v>
+      </c>
+      <c r="G211" t="s">
+        <v>1115</v>
+      </c>
+      <c r="H211" t="s">
+        <v>1509</v>
+      </c>
+      <c r="I211" t="s">
+        <v>198</v>
+      </c>
+      <c r="K211" t="s">
+        <v>199</v>
+      </c>
+      <c r="L211" t="s">
+        <v>908</v>
+      </c>
+      <c r="M211" t="s">
+        <v>201</v>
+      </c>
+      <c r="N211" t="s">
+        <v>204</v>
+      </c>
+      <c r="P211" t="s">
+        <v>202</v>
+      </c>
+      <c r="Q211" t="s">
+        <v>204</v>
+      </c>
+      <c r="R211" t="s">
+        <v>1508</v>
+      </c>
+      <c r="S211" t="s">
+        <v>1510</v>
+      </c>
+      <c r="T211" t="s">
+        <v>687</v>
+      </c>
+      <c r="U211" t="s">
+        <v>1044</v>
+      </c>
+    </row>
+    <row ht="12.75" r="212" spans="1:21">
+      <c r="A212" t="s">
+        <v>1511</v>
+      </c>
+      <c r="B212" t="s">
+        <v>1525</v>
+      </c>
+      <c r="C212" t="s">
+        <v>1512</v>
+      </c>
+      <c r="D212" t="s">
+        <v>84</v>
+      </c>
+      <c r="E212" t="s">
+        <v>78</v>
+      </c>
+      <c r="F212" t="s">
+        <v>79</v>
+      </c>
+      <c r="G212" t="s">
+        <v>104</v>
+      </c>
+      <c r="H212" t="s">
+        <v>1513</v>
+      </c>
+      <c r="I212" t="s">
+        <v>198</v>
+      </c>
+      <c r="K212" t="s">
+        <v>199</v>
+      </c>
+      <c r="L212" t="s">
+        <v>1446</v>
+      </c>
+      <c r="M212" t="s">
+        <v>201</v>
+      </c>
+      <c r="N212" t="s">
+        <v>202</v>
+      </c>
+      <c r="P212" t="s">
+        <v>201</v>
+      </c>
+      <c r="Q212" t="s">
+        <v>204</v>
+      </c>
+      <c r="R212" t="s">
+        <v>1512</v>
+      </c>
+      <c r="S212" t="s">
+        <v>1514</v>
+      </c>
+      <c r="T212" t="s">
+        <v>687</v>
+      </c>
+      <c r="U212" t="s">
+        <v>1044</v>
+      </c>
+    </row>
+    <row ht="12.75" r="213" spans="1:21">
+      <c r="A213" t="s">
+        <v>1515</v>
+      </c>
+      <c r="B213" t="s">
+        <v>1525</v>
+      </c>
+      <c r="C213" t="s">
+        <v>1516</v>
+      </c>
+      <c r="D213" t="s">
+        <v>84</v>
+      </c>
+      <c r="E213" t="s">
+        <v>78</v>
+      </c>
+      <c r="F213" t="s">
+        <v>235</v>
+      </c>
+      <c r="G213" t="s">
         <v>248</v>
       </c>
-      <c r="H204" t="s">
-        <v>1460</v>
-      </c>
-      <c r="I204" t="s">
+      <c r="H213" t="s">
+        <v>1517</v>
+      </c>
+      <c r="I213" t="s">
         <v>198</v>
       </c>
-      <c r="K204" t="s">
+      <c r="K213" t="s">
         <v>199</v>
       </c>
-      <c r="L204" t="s">
-        <v>1421</v>
-      </c>
-      <c r="M204" t="s">
+      <c r="L213" t="s">
+        <v>1452</v>
+      </c>
+      <c r="M213" t="s">
+        <v>201</v>
+      </c>
+      <c r="N213" t="s">
+        <v>202</v>
+      </c>
+      <c r="P213" t="s">
+        <v>202</v>
+      </c>
+      <c r="Q213" t="s">
+        <v>204</v>
+      </c>
+      <c r="R213" t="s">
+        <v>1516</v>
+      </c>
+      <c r="S213" t="s">
+        <v>1518</v>
+      </c>
+      <c r="T213" t="s">
+        <v>687</v>
+      </c>
+      <c r="U213" t="s">
+        <v>1044</v>
+      </c>
+    </row>
+    <row ht="12.75" r="214" spans="1:21">
+      <c r="A214" t="s">
+        <v>1519</v>
+      </c>
+      <c r="B214" t="s">
+        <v>1525</v>
+      </c>
+      <c r="C214" t="s">
+        <v>1520</v>
+      </c>
+      <c r="D214" t="s">
+        <v>261</v>
+      </c>
+      <c r="E214" t="s">
+        <v>78</v>
+      </c>
+      <c r="F214" t="s">
+        <v>79</v>
+      </c>
+      <c r="G214" t="s">
+        <v>104</v>
+      </c>
+      <c r="H214" t="s">
+        <v>199</v>
+      </c>
+      <c r="I214" t="s">
+        <v>198</v>
+      </c>
+      <c r="K214" t="s">
+        <v>199</v>
+      </c>
+      <c r="L214" t="s">
+        <v>1452</v>
+      </c>
+      <c r="M214" t="s">
+        <v>202</v>
+      </c>
+      <c r="N214" t="s">
+        <v>204</v>
+      </c>
+      <c r="P214" t="s">
         <v>252</v>
       </c>
-      <c r="N204" t="s">
+      <c r="Q214" t="s">
+        <v>204</v>
+      </c>
+      <c r="R214" t="s">
+        <v>1520</v>
+      </c>
+      <c r="S214" t="s">
+        <v>1521</v>
+      </c>
+      <c r="T214" t="s">
+        <v>687</v>
+      </c>
+      <c r="U214" t="s">
+        <v>1044</v>
+      </c>
+    </row>
+    <row ht="12.75" r="215" spans="1:21">
+      <c r="A215" t="s">
+        <v>1522</v>
+      </c>
+      <c r="B215" t="s">
+        <v>1525</v>
+      </c>
+      <c r="C215" t="s">
+        <v>1523</v>
+      </c>
+      <c r="D215" t="s">
+        <v>84</v>
+      </c>
+      <c r="E215" t="s">
+        <v>78</v>
+      </c>
+      <c r="F215" t="s">
+        <v>79</v>
+      </c>
+      <c r="G215" t="s">
+        <v>1245</v>
+      </c>
+      <c r="H215" t="s">
+        <v>199</v>
+      </c>
+      <c r="I215" t="s">
+        <v>198</v>
+      </c>
+      <c r="K215" t="s">
+        <v>431</v>
+      </c>
+      <c r="L215" t="s">
+        <v>140</v>
+      </c>
+      <c r="M215" t="s">
         <v>202</v>
       </c>
-      <c r="P204" t="s">
-        <v>201</v>
-      </c>
-      <c r="Q204" t="s">
-        <v>204</v>
-      </c>
-      <c r="R204" t="s">
-        <v>1459</v>
-      </c>
-      <c r="S204" t="s">
-        <v>1461</v>
-      </c>
-      <c r="T204" t="s">
+      <c r="N215" t="s">
+        <v>266</v>
+      </c>
+      <c r="P215" t="s">
+        <v>199</v>
+      </c>
+      <c r="Q215" t="s">
+        <v>199</v>
+      </c>
+      <c r="R215" t="s">
+        <v>1523</v>
+      </c>
+      <c r="S215" t="s">
+        <v>1524</v>
+      </c>
+      <c r="T215" t="s">
         <v>687</v>
       </c>
-      <c r="U204" t="s">
-        <v>1044</v>
+      <c r="U215" t="s">
+        <v>16</v>
       </c>
     </row>
   </sheetData>
@@ -25897,11 +27279,11 @@
   <customSheetViews>
     <customSheetView filter="1" guid="{C25CEB9E-BEC1-4982-90C4-50C84EE1B82A}" showAutoFilter="1">
       <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
-      <autoFilter ref="A1:AD33" xr:uid="{3B758180-9D8A-452F-8BA2-5915AAF7AE65}"/>
+      <autoFilter ref="A1:AD33" xr:uid="{D4EB5B96-7C28-404B-A032-12EF84F64174}"/>
     </customSheetView>
     <customSheetView filter="1" guid="{A7754112-A52F-4ABC-8778-92F04773E53C}" showAutoFilter="1">
       <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
-      <autoFilter ref="A1:AD33" xr:uid="{A66FFBA3-B8D6-49C9-86CE-96AF0531736C}">
+      <autoFilter ref="A1:AD33" xr:uid="{B700B731-0905-46E0-90BA-3B18AC886C7D}">
         <filterColumn colId="5">
           <filters blank="1">
             <filter val="Strathnairn"/>

</xml_diff>